<commit_message>
pip2 forces added - no logical bugs - 1250 frames
</commit_message>
<xml_diff>
--- a/results_G2/forces/force_results.xlsx
+++ b/results_G2/forces/force_results.xlsx
@@ -467,7 +467,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>{40: {'frame': 40, 'motion_vector': [-0.6262931823730469, -0.466278076171875, 2.1045074462890625], 'ionic_force': [4.294367149472237, 6.8834086656570435, -19.503039240837097], 'ionic_force_magnitude': 21.12324415667585, 'radial_force': 8.11313158237365, 'axial_force': -19.503039240837097, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [6.283811151981354, 0.6723480224609375, -4.648064412176609], 'asn_force_magnitude': 7.844924297710912, 'residue_force': [6.283811151981354, 0.6723480224609375, -4.648064412176609], 'residue_force_magnitude': 7.844924297710912, 'total_force': [10.57817830145359, 7.555756688117981, -24.151103653013706], 'total_force_magnitude': 27.42741553566422, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': -0.7967851539993244, 'cosine_residue_motion': -0.7967851539993244, 'cosine_ionic_motion': -0.9900533422599569, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': -6.25071921466463, 'motion_component_residue': -6.25071921466463, 'motion_component_ionic': -20.91313847669003, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 79.67851539993244, 'motion_component_percent_residue': 79.67851539993244, 'motion_component_percent_ionic': 99.00533422599568, 'ionic_contributions': [{'ion_id': 2397, 'distance': 13.46534252166748, 'force': [0.06721048057079315, 0.29271984100341797, -1.80626380443573], 'magnitude': 1.8310627937316895, 'cosine_ionic_motion': -0.9683026671409607, 'motion_component_ionic': -1.773023009300232, 'motion_component_percent_ionic': 96.83026671409607}, {'ion_id': 2398, 'distance': 8.60761833190918, 'force': [0.4785769283771515, 1.1410447359085083, -4.3067474365234375], 'magnitude': 4.4809699058532715, 'cosine_ionic_motion': -0.9837936162948608, 'motion_component_ionic': -4.408349514007568, 'motion_component_percent_ionic': 98.37936162948608}, {'ion_id': 2399, 'distance': 4.7148919105529785, 'force': [3.748579740524292, 5.449644088745117, -13.39002799987793], 'magnitude': 14.934635162353516, 'cosine_ionic_motion': -0.986416220664978, 'motion_component_ionic': -14.731766700744629, 'motion_component_percent_ionic': 98.6416220664978}], 'glu_contributions': [], 'asn_contributions': [{'resid': 458, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 5.640399932861328, 'force': [5.409074306488037, -2.948438882827759, -1.1765199899673462], 'magnitude': 6.27180814743042, 'cosine_with_motion': -0.3188517093658447, 'motion_component': -1.999776840209961, 'motion_component_percent': 31.885170936584473}, {'resid': 786, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 4.637459754943848, 'force': [-1.6578381061553955, -10.71817684173584, 2.0756356716156006], 'magnitude': 11.042464256286621, 'cosine_with_motion': 0.419744074344635, 'motion_component': 4.635008811950684, 'motion_component_percent': 41.9744074344635}, {'resid': 786, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 3.8657217025756836, 'force': [2.6595325469970703, 12.010087013244629, -5.192760944366455], 'magnitude': 13.352155685424805, 'cosine_with_motion': -0.607042133808136, 'motion_component': -8.105320930480957, 'motion_component_percent': 60.7042133808136}, {'resid': 786, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 5.110611915588379, 'force': [3.557929515838623, 10.984701156616211, 0.10406573861837387], 'magnitude': 11.547005653381348, 'cosine_with_motion': -0.27513089776039124, 'motion_component': -3.176938056945801, 'motion_component_percent': 27.513089776039124}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 4.9544477462768555, 'force': [-2.7461273670196533, -4.893613338470459, -0.13110485672950745], 'magnitude': 5.613007545471191, 'cosine_with_motion': 0.2957080602645874, 'motion_component': 1.6598116159439087, 'motion_component_percent': 29.57080602645874}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 5.950348377227783, 'force': [-0.9387597441673279, -3.7622110843658447, -0.3273800313472748], 'magnitude': 3.891359567642212, 'cosine_with_motion': 0.1892644613981247, 'motion_component': 0.736496090888977, 'motion_component_percent': 18.92644613981247}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': -0.9903907153057547, 'motion_component_pip2': -27.163857691354657, 'motion_component_percent_pip2': 99.03907153057547}, 42: {'frame': 42, 'motion_vector': [-0.06933212280273438, -2.9759140014648438, 0.226318359375], 'ionic_force': [2.3683585077524185, 7.14034366607666, -20.349798798561096], 'ionic_force_magnitude': 21.69580468276858, 'radial_force': 7.522873765451894, 'axial_force': -20.349798798561096, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [6.195552110671997, 3.7248358726501465, -5.933862686157227], 'asn_force_magnitude': 9.352539473982597, 'residue_force': [6.195552110671997, 3.7248358726501465, -5.933862686157227], 'residue_force_magnitude': 9.352539473982597, 'total_force': [8.563910618424416, 10.865179538726807, -26.283661484718323], 'total_force_magnitude': 29.70224827403467, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': -0.4605002387546373, 'cosine_residue_motion': -0.4605002387546373, 'cosine_ionic_motion': -0.4017181196116866, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': -4.306846660731156, 'motion_component_residue': -4.306846660731156, 'motion_component_ionic': -8.715597860624218, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 46.05002387546373, 'motion_component_percent_residue': 46.05002387546373, 'motion_component_percent_ionic': 40.17181196116866, 'ionic_contributions': [{'ion_id': 2397, 'distance': 12.966878890991211, 'force': [0.15900565683841705, 0.345048725605011, -1.9376503229141235], 'magnitude': 1.9745455980300903, 'cosine_ionic_motion': -0.25046253204345703, 'motion_component_ionic': -0.4945496618747711, 'motion_component_percent_ionic': 25.046253204345703}, {'ion_id': 2398, 'distance': 9.182568550109863, 'force': [0.2542445659637451, 0.8576275706291199, -3.834444999694824], 'magnitude': 3.9374020099639893, 'cosine_ionic_motion': -0.2924577295780182, 'motion_component_ionic': -1.1515237092971802, 'motion_component_percent_ionic': 29.24577295780182}, {'ion_id': 2399, 'distance': 4.575058460235596, 'force': [1.9551082849502563, 5.937667369842529, -14.577703475952148], 'magnitude': 15.861518859863281, 'cosine_ionic_motion': -0.4457028806209564, 'motion_component_ionic': -7.069524765014648, 'motion_component_percent_ionic': 44.57028806209564}], 'glu_contributions': [], 'asn_contributions': [{'resid': 458, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 5.975498199462891, 'force': [4.703507423400879, -2.114661693572998, -2.152233362197876], 'magnitude': 5.588101863861084, 'cosine_with_motion': 0.3284846842288971, 'motion_component': 1.8356058597564697, 'motion_component_percent': 32.84846842288971}, {'resid': 786, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 4.833013534545898, 'force': [-1.2233433723449707, -9.516352653503418, 3.3629064559936523], 'magnitude': 10.166940689086914, 'cosine_with_motion': 0.9609329104423523, 'motion_component': 9.769747734069824, 'motion_component_percent': 96.09329104423523}, {'resid': 786, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 4.021487236022949, 'force': [2.2351412773132324, 10.489781379699707, -6.098438262939453], 'magnitude': 12.337841033935547, 'cosine_with_motion': -0.8892149925231934, 'motion_component': -10.970993041992188, 'motion_component_percent': 88.92149925231934}, {'resid': 786, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 5.521584510803223, 'force': [2.6922836303710938, 9.361472129821777, -1.7227236032485962], 'magnitude': 9.892084121704102, 'cosine_with_motion': -0.9629039168357849, 'motion_component': -9.525126457214355, 'motion_component_percent': 96.29039168357849}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 5.220410346984863, 'force': [-2.2120368480682373, -4.495403289794922, 0.6766260862350464], 'magnitude': 5.055648326873779, 'cosine_with_motion': 0.906692624092102, 'motion_component': 4.583919048309326, 'motion_component_percent': 90.6692624092102}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': -0.4384329563610655, 'motion_component_pip2': -13.022444521355375, 'motion_component_percent_pip2': 43.84329563610655}, 46: {'frame': 46, 'motion_vector': [1.4883651733398438, -1.2183418273925781, 1.2192230224609375], 'ionic_force': [7.90682578086853, 7.1081390380859375, -8.699332237243652], 'ionic_force_magnitude': 13.737609540517418, 'radial_force': 10.632193306828489, 'axial_force': -8.699332237243652, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-10.871634006500244, -1.0213706493377686, -9.448031261563301], 'asn_force_magnitude': 14.439560889933551, 'residue_force': [-10.871634006500244, -1.0213706493377686, -9.448031261563301], 'residue_force_magnitude': 14.439560889933551, 'total_force': [-2.964808225631714, 6.086768388748169, -18.147363498806953], 'total_force_magnitude': 19.369193044390578, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': -0.8045396287299343, 'cosine_residue_motion': -0.8045396287299343, 'cosine_ionic_motion': -0.23968063126542874, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': -11.61719895741042, 'motion_component_residue': -11.61719895741042, 'motion_component_ionic': -3.2926389267491913, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 80.45396287299343, 'motion_component_percent_residue': 80.45396287299343, 'motion_component_percent_ionic': 23.968063126542873, 'ionic_contributions': [{'ion_id': 2397, 'distance': 12.625324249267578, 'force': [0.7042213678359985, 0.6977462768554688, -1.8317713737487793], 'magnitude': 2.0828258991241455, 'cosine_ionic_motion': -0.4290952980518341, 'motion_component_ionic': -0.8937308192253113, 'motion_component_percent_ionic': 42.90952980518341}, {'ion_id': 2398, 'distance': 9.481710433959961, 'force': [1.5407878160476685, 1.4651570320129395, -3.019374132156372], 'magnitude': 3.692875862121582, 'cosine_ionic_motion': -0.37731021642684937, 'motion_component_ionic': -1.3933597803115845, 'motion_component_percent_ionic': 37.73102164268494}, {'ion_id': 2399, 'distance': 6.269979476928711, 'force': [5.661816596984863, 4.945235729217529, -3.848186731338501], 'magnitude': 8.445120811462402, 'cosine_ionic_motion': -0.11906857043504715, 'motion_component_ionic': -1.0055484771728516, 'motion_component_percent_ionic': 11.906857043504715}], 'glu_contributions': [], 'asn_contributions': [{'resid': 458, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 4.76320743560791, 'force': [-5.989561080932617, 8.24775505065918, 2.3791494369506836], 'magnitude': 10.467123031616211, 'cosine_with_motion': -0.6738548278808594, 'motion_component': -7.053321361541748, 'motion_component_percent': 67.38548278808594}, {'resid': 458, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 4.5142741203308105, 'force': [3.9843995571136475, -7.883950233459473, -4.223249912261963], 'magnitude': 9.791217803955078, 'cosine_with_motion': 0.4658139944076538, 'motion_component': 4.560886383056641, 'motion_component_percent': 46.58139944076538}, {'resid': 458, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 5.142804145812988, 'force': [5.833247184753418, -9.796405792236328, 0.1724785715341568], 'magnitude': 11.402898788452148, 'cosine_with_motion': 0.8020568490028381, 'motion_component': 9.145772933959961, 'motion_component_percent': 80.20568490028381}, {'resid': 458, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 5.376084804534912, 'force': [-1.6632883548736572, 4.4558610916137695, -0.32246801257133484], 'magnitude': 4.767096996307373, 'cosine_with_motion': -0.7643165588378906, 'motion_component': -3.643571138381958, 'motion_component_percent': 76.43165588378906}, {'resid': 458, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 5.531508922576904, 'force': [-2.742570161819458, 3.5173914432525635, -0.6188658475875854], 'magnitude': 4.502968788146973, 'cosine_with_motion': -0.8895382881164551, 'motion_component': -4.005563259124756, 'motion_component_percent': 88.95382881164551}, {'resid': 786, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 3.7268261909484863, 'force': [11.457611083984375, -12.577831268310547, 1.693105697631836], 'magnitude': 17.098108291625977, 'cosine_with_motion': 0.88453209400177, 'motion_component': 15.123826026916504, 'motion_component_percent': 88.453209400177}, {'resid': 786, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 2.9119558334350586, 'force': [-18.855571746826172, 12.798524856567383, -5.863428592681885], 'magnitude': 23.531143188476562, 'cosine_with_motion': -0.9480908513069153, 'motion_component': -22.309661865234375, 'motion_component_percent': 94.80908513069153}, {'resid': 786, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 3.7182397842407227, 'force': [-10.034814834594727, 19.14767837524414, 2.9207446575164795], 'magnitude': 21.814258575439453, 'cosine_with_motion': -0.6985613107681274, 'motion_component': -15.23859691619873, 'motion_component_percent': 69.85613107681274}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 3.0569589138031006, 'force': [4.639864921569824, -13.245811462402344, -4.516338348388672], 'magnitude': 14.7437162399292, 'cosine_with_motion': 0.5223192572593689, 'motion_component': 7.700926780700684, 'motion_component_percent': 52.23192572593689}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 4.67614221572876, 'force': [2.499049425125122, -5.684582710266113, -1.069158911705017], 'magnitude': 6.301017761230469, 'cosine_with_motion': 0.6510224938392639, 'motion_component': 4.102104187011719, 'motion_component_percent': 65.10224938392639}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': -0.7697707307676186, 'motion_component_pip2': -14.90983788415961, 'motion_component_percent_pip2': 76.97707307676185}, 47: {'frame': 47, 'motion_vector': [0.37799072265625, -0.826751708984375, -0.0462799072265625], 'ionic_force': [11.934091031551361, 3.5142853260040283, -6.645846970379353], 'ionic_force_magnitude': 14.104609603091546, 'radial_force': 12.440768871011223, 'axial_force': -6.645846970379353, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-9.871980369091034, -2.2389142513275146, -8.521904230117798], 'asn_force_magnitude': 13.232217695451348, 'residue_force': [-9.871980369091034, -2.2389142513275146, -8.521904230117798], 'residue_force_magnitude': 13.232217695451348, 'total_force': [2.062110662460327, 1.2753710746765137, -15.16775120049715], 'total_force_magnitude': 15.360323832606422, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': -0.12338397521579754, 'cosine_residue_motion': -0.12338397521579754, 'cosine_ionic_motion': 0.1490120456087327, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': -1.6326436201856067, 'motion_component_residue': -1.6326436201856067, 'motion_component_ionic': 2.1017567294692467, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 12.338397521579754, 'motion_component_percent_residue': 12.338397521579754, 'motion_component_percent_ionic': 14.901204560873271, 'ionic_contributions': [{'ion_id': 2276, 'distance': 14.745076179504395, 'force': [0.6222935318946838, 0.28520452976226807, -1.364987850189209], 'magnitude': 1.527017593383789, 'cosine_ionic_motion': 0.04503704980015755, 'motion_component_ionic': 0.06877236813306808, 'motion_component_percent_ionic': 4.503704980015755}, {'ion_id': 2397, 'distance': 11.65298843383789, 'force': [1.2247580289840698, 0.576052188873291, -2.036106824874878], 'magnitude': 2.444912910461426, 'cosine_ionic_motion': 0.03636369854211807, 'motion_component_ionic': 0.08890607953071594, 'motion_component_percent_ionic': 3.6363698542118073}, {'ion_id': 2398, 'distance': 8.259014129638672, 'force': [3.269360065460205, 1.4678785800933838, -3.293405771255493], 'magnitude': 4.867227554321289, 'cosine_ionic_motion': 0.03941793739795685, 'motion_component_ionic': 0.19185607135295868, 'motion_component_percent_ionic': 3.941793739795685}, {'ion_id': 2399, 'distance': 6.926487445831299, 'force': [6.817679405212402, 1.1851500272750854, 0.04865347594022751], 'magnitude': 6.920094013214111, 'cosine_ionic_motion': 0.25320786237716675, 'motion_component_ionic': 1.7522222995758057, 'motion_component_percent_ionic': 25.320786237716675}], 'glu_contributions': [], 'asn_contributions': [{'resid': 458, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 3.7199745178222656, 'force': [-5.631682872772217, 14.056681632995605, 8.0745849609375], 'magnitude': 17.161149978637695, 'cosine_with_motion': -0.9041681289672852, 'motion_component': -15.51656436920166, 'motion_component_percent': 90.41681289672852}, {'resid': 458, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 2.966031551361084, 'force': [0.9552204012870789, -19.84855079650879, -10.933781623840332], 'magnitude': 22.680938720703125, 'cosine_with_motion': 0.8368524312973022, 'motion_component': 18.98059844970703, 'motion_component_percent': 83.68524312973022}, {'resid': 458, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 4.823035717010498, 'force': [3.9802987575531006, -11.639004707336426, -4.0967488288879395], 'magnitude': 12.965051651000977, 'cosine_with_motion': 0.9589341878890991, 'motion_component': 12.432631492614746, 'motion_component_percent': 95.89341878890991}, {'resid': 458, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 4.967532157897949, 'force': [-0.7541203498840332, 5.383706569671631, 1.2736692428588867], 'magnitude': 5.583477973937988, 'cosine_with_motion': -0.9434663653373718, 'motion_component': -5.267823696136475, 'motion_component_percent': 94.34663653373718}, {'resid': 458, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 5.647162437438965, 'force': [-1.7763100862503052, 3.7039191722869873, 1.3385450839996338], 'magnitude': 4.320416450500488, 'cosine_with_motion': -0.9651583433151245, 'motion_component': -4.169886112213135, 'motion_component_percent': 96.51583433151245}, {'resid': 786, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 5.402390480041504, 'force': [-4.8797502517700195, 3.7242112159729004, -3.009565591812134], 'magnitude': 6.836606979370117, 'cosine_with_motion': -0.7688013911247253, 'motion_component': -5.255992889404297, 'motion_component_percent': 76.88013911247253}, {'resid': 786, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 5.767971515655518, 'force': [-4.209479808807373, 7.480082035064697, -2.9160447120666504], 'magnitude': 9.065024375915527, 'cosine_with_motion': -0.9259529113769531, 'motion_component': -8.39378547668457, 'motion_component_percent': 92.59529113769531}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 4.824652194976807, 'force': [2.4438438415527344, -5.099959373474121, 1.7474372386932373], 'magnitude': 5.919078826904297, 'cosine_with_motion': 0.9390279054641724, 'motion_component': 5.558180332183838, 'motion_component_percent': 93.90279054641724}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': 0.030540574169915673, 'motion_component_pip2': 0.4691131092836398, 'motion_component_percent_pip2': 3.0540574169915673}, 48: {'frame': 48, 'motion_vector': [0.25186920166015625, 0.4375877380371094, 0.5585784912109375], 'ionic_force': [11.552406191825867, 2.412329077720642, -6.972220465540886], 'ionic_force_magnitude': 13.707271012869786, 'radial_force': 11.801585503658107, 'axial_force': -6.972220465540886, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-6.237414240837097, -5.533897638320923, -9.401701241731644], 'asn_force_magnitude': 12.566676001313539, 'residue_force': [-6.237414240837097, -5.533897638320923, -9.401701241731644], 'residue_force_magnitude': 12.566676001313539, 'total_force': [5.3149919509887695, -3.1215685606002808, -16.37392170727253], 'total_force_magnitude': 17.49567494535418, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': -0.9769722228613161, 'cosine_residue_motion': -0.9769722228613161, 'cosine_ionic_motion': 0.0068568632671159105, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': -12.277293386981244, 'motion_component_residue': -12.277293386981244, 'motion_component_ionic': 0.09398888310054954, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 97.69722228613162, 'motion_component_percent_residue': 97.69722228613162, 'motion_component_percent_ionic': 0.685686326711591, 'ionic_contributions': [{'ion_id': 2276, 'distance': 14.279234886169434, 'force': [0.7036464214324951, 0.20887023210525513, -1.4534579515457153], 'magnitude': 1.6282767057418823, 'cosine_ionic_motion': -0.4431001842021942, 'motion_component_ionic': -0.7214897274971008, 'motion_component_percent_ionic': 44.31001842021942}, {'ion_id': 2397, 'distance': 11.222811698913574, 'force': [1.4268983602523804, 0.4878597855567932, -2.16196870803833], 'magnitude': 2.6359353065490723, 'cosine_ionic_motion': -0.31982097029685974, 'motion_component_ionic': -0.8430274128913879, 'motion_component_percent_ionic': 31.982097029685974}, {'ion_id': 2398, 'distance': 8.31759262084961, 'force': [3.404042959213257, 1.0041741132736206, -3.230121374130249], 'magnitude': 4.798912048339844, 'cosine_ionic_motion': -0.14044883847236633, 'motion_component_ionic': -0.6740016341209412, 'motion_component_percent_ionic': 14.044883847236633}, {'ion_id': 2399, 'distance': 7.401081085205078, 'force': [6.017818450927734, 0.7114249467849731, -0.1266724318265915], 'magnitude': 6.06104850769043, 'cosine_ionic_motion': 0.3848356604576111, 'motion_component_ionic': 2.332507610321045, 'motion_component_percent_ionic': 38.48356604576111}], 'glu_contributions': [], 'asn_contributions': [{'resid': 458, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 3.4522414207458496, 'force': [-7.476254940032959, 14.404739379882812, 11.561213493347168], 'magnitude': 19.926177978515625, 'cosine_with_motion': 0.7250462174415588, 'motion_component': 14.447400093078613, 'motion_component_percent': 72.50462174415588}, {'resid': 458, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 2.86439847946167, 'force': [1.4831358194351196, -17.230175018310547, -17.097808837890625], 'magnitude': 24.318998336791992, 'cosine_with_motion': -0.9129306674003601, 'motion_component': -22.20155906677246, 'motion_component_percent': 91.29306674003601}, {'resid': 458, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 4.436764240264893, 'force': [4.484607696533203, -13.104666709899902, -6.5485920906066895], 'magnitude': 15.320837020874023, 'cosine_with_motion': -0.7162755131721497, 'motion_component': -10.9739408493042, 'motion_component_percent': 71.62755131721497}, {'resid': 458, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 4.70457124710083, 'force': [-0.5339769124984741, 5.635095119476318, 2.5908288955688477], 'magnitude': 6.225096225738525, 'cosine_with_motion': 0.8061438202857971, 'motion_component': 5.018322944641113, 'motion_component_percent': 80.61438202857971}, {'resid': 458, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 5.179398536682129, 'force': [-2.122640371322632, 4.312107086181641, 1.8107824325561523], 'magnitude': 5.1360297203063965, 'cosine_with_motion': 0.611238956451416, 'motion_component': 3.139341354370117, 'motion_component_percent': 61.1238956451416}, {'resid': 786, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 5.7807698249816895, 'force': [-3.9585134983062744, 3.9042179584503174, -2.176955223083496], 'magnitude': 5.970919609069824, 'cosine_with_motion': -0.11223604530096054, 'motion_component': -0.6701524257659912, 'motion_component_percent': 11.223604530096054}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 5.896176815032959, 'force': [1.8862279653549194, -3.4552154541015625, 0.4588300883769989], 'magnitude': 3.9631924629211426, 'cosine_with_motion': -0.2615831196308136, 'motion_component': -1.0367043018341064, 'motion_component_percent': 26.15831196308136}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': -0.6963609315978897, 'motion_component_pip2': -12.183304503880695, 'motion_component_percent_pip2': 69.63609315978897}, 49: {'frame': 49, 'motion_vector': [-0.3889617919921875, 1.1154975891113281, -0.8185806274414062], 'ionic_force': [10.422694981098175, 2.216172844171524, -5.677527368068695], 'ionic_force_magnitude': 12.073868881159072, 'radial_force': 10.655702358092233, 'axial_force': -5.677527368068695, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [6.361834019422531, -4.843973159790039, -12.637336492538452], 'asn_force_magnitude': 14.954573938735004, 'residue_force': [6.361834019422531, -4.843973159790039, -12.637336492538452], 'residue_force_magnitude': 14.954573938735004, 'total_force': [16.784529000520706, -2.627800315618515, -18.314863860607147], 'total_force_magnitude': 24.98119265568918, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': 0.1147660670188767, 'cosine_residue_motion': 0.1147660670188767, 'cosine_ionic_motion': 0.17665993113489378, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': 1.7162776348916085, 'motion_component_residue': 1.7162776348916085, 'motion_component_ionic': 2.132968845077299, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 11.47660670188767, 'motion_component_percent_residue': 11.47660670188767, 'motion_component_percent_ionic': 17.665993113489378, 'ionic_contributions': [{'ion_id': 2276, 'distance': 14.36806869506836, 'force': [0.7589524388313293, 0.17289862036705017, -1.407273769378662], 'magnitude': 1.60820472240448, 'cosine_ionic_motion': 0.4541108310222626, 'motion_component_ionic': 0.730303168296814, 'motion_component_percent_ionic': 45.41108310222626}, {'ion_id': 2397, 'distance': 11.255699157714844, 'force': [1.5349833965301514, 0.4721815586090088, -2.070791244506836], 'magnitude': 2.6205544471740723, 'cosine_ionic_motion': 0.4313868582248688, 'motion_component_ionic': 1.1304727792739868, 'motion_component_percent_ionic': 43.13868582248688}, {'ion_id': 2398, 'distance': 8.606088638305664, 'force': [3.3944389820098877, 1.0265886783599854, -2.741765022277832], 'magnitude': 4.482563495635986, 'cosine_ionic_motion': 0.3211763799190521, 'motion_component_ionic': 1.4396934509277344, 'motion_component_percent_ionic': 32.11763799190521}, {'ion_id': 2399, 'distance': 8.319869041442871, 'force': [4.734320163726807, 0.5445039868354797, 0.542302668094635], 'magnitude': 4.796286582946777, 'cosine_ionic_motion': -0.24341759085655212, 'motion_component_ionic': -1.1675004959106445, 'motion_component_percent_ionic': 24.341759085655212}], 'glu_contributions': [], 'asn_contributions': [{'resid': 458, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 3.529278039932251, 'force': [-4.985489368438721, 14.136878967285156, 11.78123664855957], 'magnitude': 19.065780639648438, 'cosine_with_motion': 0.2943148910999298, 'motion_component': 5.6113433837890625, 'motion_component_percent': 29.43148910999298}, {'resid': 458, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 2.623377799987793, 'force': [9.01367473602295, -15.768808364868164, -22.598312377929688], 'magnitude': 28.99285125732422, 'cosine_with_motion': -0.06233493238687515, 'motion_component': -1.807267427444458, 'motion_component_percent': 6.233493238687515}, {'resid': 458, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 3.9403905868530273, 'force': [-0.7967387437820435, -16.442340850830078, -10.31032943725586], 'magnitude': 19.42391014099121, 'cosine_with_motion': -0.3435763120651245, 'motion_component': -6.673595428466797, 'motion_component_percent': 34.35763120651245}, {'resid': 458, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 3.630760431289673, 'force': [2.987987995147705, 8.175934791564941, 5.784988880157471], 'magnitude': 10.451797485351562, 'cosine_with_motion': 0.2145230919122696, 'motion_component': 2.242151975631714, 'motion_component_percent': 21.45230919122696}, {'resid': 458, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 4.901690483093262, 'force': [0.142399400472641, 5.0543622970581055, 2.7050797939300537], 'magnitude': 5.7344841957092285, 'cosine_with_motion': 0.4086933434009552, 'motion_component': 2.3436455726623535, 'motion_component_percent': 40.86933434009552}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': 0.15408577696919068, 'motion_component_pip2': 3.8492464799689072, 'motion_component_percent_pip2': 15.408577696919068}, 50: {'frame': 50, 'motion_vector': [0.4214324951171875, -0.9841651916503906, 1.4104690551757812], 'ionic_force': [9.457020938396454, 3.7250678837299347, -5.476261794567108], 'ionic_force_magnitude': 11.545597386462969, 'radial_force': 10.164220371856622, 'axial_force': -5.476261794567108, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [5.40292501449585, -17.15039348602295, -7.671647407114506], 'asn_force_magnitude': 19.549469797842857, 'residue_force': [5.40292501449585, -17.15039348602295, -7.671647407114506], 'residue_force_magnitude': 19.549469797842857, 'total_force': [14.859945952892303, -13.425325602293015, -13.147909201681614], 'total_force_magnitude': 23.956729276471126, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': 0.24077883487939908, 'cosine_residue_motion': 0.24077883487939908, 'cosine_ionic_motion': -0.3621839066838359, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': 4.707098560434605, 'motion_component_residue': 4.707098560434605, 'motion_component_ionic': -4.181629566427843, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 24.077883487939907, 'motion_component_percent_residue': 24.077883487939907, 'motion_component_percent_ionic': 36.218390668383584, 'ionic_contributions': [{'ion_id': 2276, 'distance': 14.494473457336426, 'force': [0.6689477562904358, 0.31093069911003113, -1.397535800933838], 'magnitude': 1.5802769660949707, 'cosine_ionic_motion': -0.7130301594734192, 'motion_component_ionic': -1.126785159111023, 'motion_component_percent_ionic': 71.30301594734192}, {'ion_id': 2397, 'distance': 11.549384117126465, 'force': [1.3385809659957886, 0.6526557803153992, -1.9943006038665771], 'magnitude': 2.4889743328094482, 'cosine_ionic_motion': -0.6559663414955139, 'motion_component_ionic': -1.6326833963394165, 'motion_component_percent_ionic': 65.59663414955139}, {'ion_id': 2398, 'distance': 8.350281715393066, 'force': [3.314307451248169, 1.5633742809295654, -3.0401113033294678], 'magnitude': 4.761412620544434, 'cosine_ionic_motion': -0.5254019498825073, 'motion_component_ionic': -2.5016555786132812, 'motion_component_percent_ionic': 52.54019498825073}, {'ion_id': 2399, 'distance': 8.676553726196289, 'force': [4.1351847648620605, 1.198107123374939, 0.9556859135627747], 'magnitude': 4.410050868988037, 'cosine_ionic_motion': 0.2447805106639862, 'motion_component_ionic': 1.0794944763183594, 'motion_component_percent_ionic': 24.47805106639862}], 'glu_contributions': [], 'asn_contributions': [{'resid': 458, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 3.733400583267212, 'force': [-7.446679</t>
+          <t>{40: {'frame': 40, 'motion_vector': [-0.6262931823730469, -0.466278076171875, 2.1045074462890625], 'ionic_force': [4.294367149472237, 6.8834086656570435, -19.503039240837097], 'ionic_force_magnitude': 21.12324415667585, 'radial_force': 8.11313158237365, 'axial_force': -19.503039240837097, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [6.283811151981354, 0.6723480224609375, -4.648064412176609], 'asn_force_magnitude': 7.844924297710912, 'residue_force': [6.283811151981354, 0.6723480224609375, -4.648064412176609], 'residue_force_magnitude': 7.844924297710912, 'pip2_force': [0.29895313642919064, 0.04803574737161398, -4.903264417589526], 'pip2_force_magnitude': 4.912604437526591, 'total_force': [10.877131437882781, 7.603792435489595, -29.054368070603232], 'total_force_magnitude': 31.94191527916063, 'cosine_total_motion': -0.9972573457303928, 'cosine_glu_motion': 0, 'cosine_asn_motion': -0.7967851539993244, 'cosine_residue_motion': -0.7967851539993244, 'cosine_pip2_motion': -0.9547790824875996, 'cosine_ionic_motion': -0.9900533422599569, 'motion_component_total': -31.854309648840808, 'motion_component_glu': 0, 'motion_component_asn': -6.25071921466463, 'motion_component_residue': -6.25071921466463, 'motion_component_ionic': -20.91313847669003, 'motion_component_pip2': -4.6904519574861485, 'motion_component_percent_total': 99.72573457303928, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 79.67851539993244, 'motion_component_percent_residue': 79.67851539993244, 'motion_component_percent_ionic': 99.00533422599568, 'motion_component_percent_pip2': 95.47790824875996, 'ionic_contributions': [{'ion_id': 2397, 'distance': 13.46534252166748, 'force': [0.06721048057079315, 0.29271984100341797, -1.80626380443573], 'magnitude': 1.8310627937316895, 'cosine_ionic_motion': -0.9683026671409607, 'motion_component_ionic': -1.773023009300232, 'motion_component_percent_ionic': 96.83026671409607}, {'ion_id': 2398, 'distance': 8.60761833190918, 'force': [0.4785769283771515, 1.1410447359085083, -4.3067474365234375], 'magnitude': 4.4809699058532715, 'cosine_ionic_motion': -0.9837936162948608, 'motion_component_ionic': -4.408349514007568, 'motion_component_percent_ionic': 98.37936162948608}, {'ion_id': 2399, 'distance': 4.7148919105529785, 'force': [3.748579740524292, 5.449644088745117, -13.39002799987793], 'magnitude': 14.934635162353516, 'cosine_ionic_motion': -0.986416220664978, 'motion_component_ionic': -14.731766700744629, 'motion_component_percent_ionic': 98.6416220664978}], 'glu_contributions': [], 'asn_contributions': [{'resid': 458, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 5.640399932861328, 'force': [5.409074306488037, -2.948438882827759, -1.1765199899673462], 'magnitude': 6.27180814743042, 'cosine_with_motion': -0.3188517093658447, 'motion_component': -1.999776840209961, 'motion_component_percent': 31.885170936584473}, {'resid': 786, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 4.637459754943848, 'force': [-1.6578381061553955, -10.71817684173584, 2.0756356716156006], 'magnitude': 11.042464256286621, 'cosine_with_motion': 0.419744074344635, 'motion_component': 4.635008811950684, 'motion_component_percent': 41.9744074344635}, {'resid': 786, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 3.8657217025756836, 'force': [2.6595325469970703, 12.010087013244629, -5.192760944366455], 'magnitude': 13.352155685424805, 'cosine_with_motion': -0.607042133808136, 'motion_component': -8.105320930480957, 'motion_component_percent': 60.7042133808136}, {'resid': 786, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 5.110611915588379, 'force': [3.557929515838623, 10.984701156616211, 0.10406573861837387], 'magnitude': 11.547005653381348, 'cosine_with_motion': -0.27513089776039124, 'motion_component': -3.176938056945801, 'motion_component_percent': 27.513089776039124}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 4.9544477462768555, 'force': [-2.7461273670196533, -4.893613338470459, -0.13110485672950745], 'magnitude': 5.613007545471191, 'cosine_with_motion': 0.2957080602645874, 'motion_component': 1.6598116159439087, 'motion_component_percent': 29.57080602645874}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 5.950348377227783, 'force': [-0.9387597441673279, -3.7622110843658447, -0.3273800313472748], 'magnitude': 3.891359567642212, 'cosine_with_motion': 0.1892644613981247, 'motion_component': 0.736496090888977, 'motion_component_percent': 18.92644613981247}], 'pip2_contributions': [{'resid': 1313, 'atom': 'C1', 'charge': 0.06000000238418579, 'distance': 25.349180221557617, 'force': [-0.020627744495868683, -0.0156398955732584, 0.017055468633770943], 'magnitude': 0.030999986454844475, 'cosine_with_motion': 0.8062765002250671, 'motion_component': 0.024994561448693275, 'motion_component_percent': 80.62765002250671}, {'resid': 1313, 'atom': 'C11', 'charge': 0.17000000178813934, 'distance': 24.34927749633789, 'force': [-0.07222510129213333, -0.04561211168766022, 0.04201413691043854], 'magnitude': 0.09519515931606293, 'cosine_with_motion': 0.725003719329834, 'motion_component': 0.06901684403419495, 'motion_component_percent': 72.5003719329834}, {'resid': 1313, 'atom': 'C12', 'charge': 0.04000000283122063, 'distance': 24.347152709960938, 'force': [-0.01758533902466297, -0.010859603993594646, 0.008643434382975101], 'magnitude': 0.022402768954634666, 'cosine_with_motion': 0.6814333200454712, 'motion_component': 0.015265993773937225, 'motion_component_percent': 68.14333200454712}, {'resid': 1313, 'atom': 'C13', 'charge': -0.05000000074505806, 'distance': 25.171117782592773, 'force': [0.02016681246459484, 0.01389272976666689, -0.009313290007412434], 'magnitude': 0.026200108230113983, 'cosine_with_motion': -0.6581780314445496, 'motion_component': -0.017244335263967514, 'motion_component_percent': 65.81780314445496}, {'resid': 1313, 'atom': 'C2', 'charge': 0.06000000238418579, 'distance': 26.881093978881836, 'force': [-0.01861545629799366, -0.01388173084706068, 0.014856741763651371], 'magnitude': 0.02756737917661667, 'cosine_with_motion': 0.7982795834541321, 'motion_component': 0.022006476297974586, 'motion_component_percent': 79.82795834541321}, {'resid': 1313, 'atom': 'C21', 'charge': 0.6299999952316284, 'distance': 22.404850006103516, 'force': [-0.3425382673740387, -0.1840963214635849, 0.14963898062705994], 'magnitude': 0.4166722297668457, 'cosine_with_motion': 0.6578500866889954, 'motion_component': 0.2741078734397888, 'motion_component_percent': 65.78500866889954}, {'resid': 1313, 'atom': 'C210', 'charge': -0.18000000715255737, 'distance': 21.142786026000977, 'force': [0.12590451538562775, 0.03742505609989166, -0.02488745003938675], 'magnitude': 0.13368608057498932, 'cosine_with_motion': -0.4954608678817749, 'motion_component': -0.0662362203001976, 'motion_component_percent': 49.54608678817749}, {'resid': 1313, 'atom': 'C211', 'charge': -0.15000000596046448, 'distance': 20.2697696685791, 'force': [0.11419277638196945, 0.02941647358238697, -0.02803732454776764], 'magnitude': 0.12120813131332397, 'cosine_with_motion': -0.5301467180252075, 'motion_component': -0.06425809115171432, 'motion_component_percent': 53.01467180252075}, {'resid': 1313, 'atom': 'C212', 'charge': -0.15000000596046448, 'distance': 20.750505447387695, 'force': [0.10746101289987564, 0.026330266147851944, -0.03369562327861786], 'magnitude': 0.1156570240855217, 'cosine_with_motion': -0.5796769857406616, 'motion_component': -0.0670437142252922, 'motion_component_percent': 57.96769857406616}, {'resid': 1313, 'atom': 'C213', 'charge': -0.18000000715255737, 'distance': 22.098243713378906, 'force': [0.11226483434438705, 0.030228592455387115, -0.038192205131053925], 'magnitude': 0.12237567454576492, 'cosine_with_motion': -0.5998708009719849, 'motion_component': -0.07340959459543228, 'motion_component_percent': 59.987080097198486}, {'resid': 1313, 'atom': 'C214', 'charge': -0.15000000596046448, 'distance': 22.210580825805664, 'force': [0.09004440158605576, 0.025229092687368393, -0.03803357481956482], 'magnitude': 0.10095075517892838, 'cosine_with_motion': -0.6540079116821289, 'motion_component': -0.066022589802742, 'motion_component_percent': 65.40079116821289}, {'resid': 1313, 'atom': 'C215', 'charge': -0.15000000596046448, 'distance': 22.781755447387695, 'force': [0.08511880040168762, 0.019903916865587234, -0.03956577181816101], 'magnitude': 0.09595220535993576, 'cosine_with_motion': -0.6771978735923767, 'motion_component': -0.06497862935066223, 'motion_component_percent': 67.71978735923767}, {'resid': 1313, 'atom': 'C216', 'charge': -0.18000000715255737, 'distance': 23.29244613647461, 'force': [0.09981908649206161, 0.016467120498418808, -0.04356349632143974], 'magnitude': 0.11014896631240845, 'cosine_with_motion': -0.6546983122825623, 'motion_component': -0.07211434096097946, 'motion_component_percent': 65.46983122825623}, {'resid': 1313, 'atom': 'C217', 'charge': -0.18000000715255737, 'distance': 22.172033309936523, 'force': [0.11149152368307114, 0.01288951002061367, -0.04670049250125885], 'magnitude': 0.12156247347593307, 'cosine_with_motion': -0.6381000876426697, 'motion_component': -0.07756902277469635, 'motion_component_percent': 63.81000876426697}, {'resid': 1313, 'atom': 'C218', 'charge': -0.18000000715255737, 'distance': 22.748245239257812, 'force': [0.10693046450614929, 0.0049774558283388615, -0.043326955288648605], 'magnitude': 0.1154821366071701, 'cosine_with_motion': -0.6190570592880249, 'motion_component': -0.07149003446102142, 'motion_component_percent': 61.90570592880249}, {'resid': 1313, 'atom': 'C219', 'charge': -0.18000000715255737, 'distance': 23.540712356567383, 'force': [0.0975128561258316, 0.002204304561018944, -0.04599342495203018], 'magnitude': 0.10783789306879044, 'cosine_with_motion': -0.6564140319824219, 'motion_component': -0.07078630477190018, 'motion_component_percent': 65.64140319824219}, {'resid': 1313, 'atom': 'C22', 'charge': -0.08000000566244125, 'distance': 21.06283950805664, 'force': [0.049801550805568695, 0.026753244921565056, -0.019703786820173264], 'magnitude': 0.05986793711781502, 'cosine_with_motion': -0.6334918737411499, 'motion_component': -0.037925850600004196, 'motion_component_percent': 63.34918737411499}, {'resid': 1313, 'atom': 'C220', 'charge': -0.27000001072883606, 'distance': 24.30508041381836, 'force': [0.1383161097764969, -0.0049453191459178925, -0.06220962479710579], 'magnitude': 0.15174266695976257, 'cosine_with_motion': -0.6319201588630676, 'motion_component': -0.09588924795389175, 'motion_component_percent': 63.19201588630676}, {'resid': 1313, 'atom': 'C23', 'charge': -0.18000000715255737, 'distance': 21.25710678100586, 'force': [0.11199240386486053, 0.06150957942008972, -0.03413015231490135], 'magnitude': 0.13225200772285461, 'cosine_with_motion': -0.5748348236083984, 'motion_component': -0.07602305710315704, 'motion_component_percent': 57.483482360839844}, {'resid': 1313, 'atom': 'C24', 'charge': -0.18000000715255737, 'distance': 19.950979232788086, 'force': [0.12821213901042938, 0.07111737877130508, -0.032318875193595886], 'magnitude': 0.1501350849866867, 'cosine_with_motion': -0.5384895205497742, 'motion_component': -0.08084616810083389, 'motion_component_percent': 53.84895205497742}, {'resid': 1313, 'atom': 'C25', 'charge': -0.15000000596046448, 'distance': 19.0755558013916, 'force': [0.1207282692193985, 0.05693156644701958, -0.030232541263103485], 'magnitude': 0.13685950636863708, 'cosine_with_motion': -0.5396430492401123, 'motion_component': -0.07385528087615967, 'motion_component_percent': 53.96430492401123}, {'resid': 1313, 'atom': 'C26', 'charge': -0.15000000596046448, 'distance': 18.948261260986328, 'force': [0.12637273967266083, 0.051721472293138504, -0.024367304518818855], 'magnitude': 0.13870453834533691, 'cosine_with_motion': -0.4963710904121399, 'motion_component': -0.06884892284870148, 'motion_component_percent': 49.63710904121399}, {'resid': 1313, 'atom': 'C27', 'charge': -0.18000000715255737, 'distance': 19.67885398864746, 'force': [0.14194664359092712, 0.05835917592048645, -0.016086911782622337], 'magnitude': 0.1543160080909729, 'cosine_with_motion': -0.43294116854667664, 'motion_component': -0.0668097510933876, 'motion_component_percent': 43.294116854667664}, {'resid': 1313, 'atom': 'C28', 'charge': -0.15000000596046448, 'distance': 20.180278778076172, 'force': [0.11567511409521103, 0.038537513464689255, -0.009374360553920269], 'magnitude': 0.12228552997112274, 'cosine_with_motion': -0.4012646973133087, 'motion_component': -0.049068864434957504, 'motion_component_percent': 40.12646973133087}, {'resid': 1313, 'atom': 'C29', 'charge': -0.15000000596046448, 'distance': 20.729042053222656, 'force': [0.11071113497018814, 0.031530555337667465, -0.013450040481984615], 'magnitude': 0.11589665710926056, 'cosine_with_motion': -0.43184584379196167, 'motion_component': -0.050049491226673126, 'motion_component_percent': 43.18458437919617}, {'resid': 1313, 'atom': 'C3', 'charge': 0.06000000238418579, 'distance': 27.700225830078125, 'force': [-0.017383543774485588, -0.012228383682668209, 0.014908275566995144], 'magnitude': 0.025961080566048622, 'cosine_with_motion': 0.8230640292167664, 'motion_component': 0.0213676318526268, 'motion_component_percent': 82.30640292167664}, {'resid': 1313, 'atom': 'C31', 'charge': 0.6299999952316284, 'distance': 26.12384796142578, 'force': [-0.25041794776916504, -0.15232573449611664, 0.08954697102308273], 'magnitude': 0.3064815402030945, 'cosine_with_motion': 0.6051467657089233, 'motion_component': 0.18546631932258606, 'motion_component_percent': 60.514676570892334}, {'resid': 1313, 'atom': 'C310', 'charge': -0.18000000715255737, 'distance': 23.217395782470703, 'force': [0.09322124719619751, 0.05912939831614494, 0.010195469483733177], 'magnitude': 0.11086223274469376, 'cosine_with_motion': -0.25918394327163696, 'motion_component': -0.028733711689710617, 'motion_component_percent': 25.918394327163696}, {'resid': 1313, 'atom': 'C311', 'charge': -0.18000000715255737, 'distance': 23.134078979492188, 'force': [0.09680936485528946, 0.05377911403775215, 0.014289873652160168], 'magnitude': 0.11166219413280487, 'cosine_with_motion': -0.22196172177791595, 'motion_component': -0.02478473260998726, 'motion_component_percent': 22.196172177791595}, {'resid': 1313, 'atom': 'C312', 'charge': -0.18000000715255737, 'distance': 21.86395835876465, 'force': [0.10944651067256927, 0.05725201591849327, 0.019281180575489998], 'magnitude': 0.1250123828649521, 'cosine_with_motion': -0.1948002725839615, 'motion_component': -0.02435244619846344, 'motion_component_percent': 19.48002725839615}, {'resid': 1313, 'atom': 'C313', 'charge': -0.18000000715255737, 'distance': 21.24875831604004, 'force': [0.11155480891466141, 0.06606439501047134, 0.02662927843630314], 'magnitude': 0.1323559582233429, 'cosine_with_motion': -0.15021631121635437, 'motion_component': -0.019882023334503174, 'motion_component_percent': 15.021631121635437}, {'resid': 1313, 'atom': 'C314', 'charge': -0.18000000715255737, 'distance': 22.05158805847168, 'force': [0.10137556493282318, 0.061754632741212845, 0.03181678056716919], 'magnitude': 0.1228940486907959, 'cosine_with_motion': -0.09181159734725952, 'motion_component': -0.011283098720014095, 'motion_component_percent': 9.181159734725952}, {'resid': 1313, 'atom': 'C315', 'charge': -0.18000000715255737, 'distance': 21.630014419555664, 'force': [0.10036128759384155, 0.06950584799051285, 0.03757404908537865], 'magnitude': 0.12773120403289795, 'cosine_with_motion': -0.05646619200706482, 'motion_component': -0.007212494499981403, 'motion_component_percent': 5.646619200706482}, {'resid': 1313, 'atom': 'C316', 'charge': -0.18000000715255737, 'distance': 22.44887351989746, 'force': [0.09118342399597168, 0.06374425441026688, 0.04103805869817734], 'magnitude': 0.11858275532722473, 'cosine_with_motion': -0.001747677568346262, 'motion_component': -0.0002072444185614586, 'motion_component_percent': 0.1747677568346262}, {'resid': 1313, 'atom': 'C317', 'charge': -0.18000000715255737, 'distance': 22.324893951416016, 'force': [0.08673073351383209, 0.06947783380746841, 0.045027270913124084], 'magnitude': 0.11990348249673843, 'cosine_with_motion': 0.029892288148403168, 'motion_component': 0.0035841893404722214, 'motion_component_percent': 2.9892288148403168}, {'resid': 1313, 'atom': 'C318', 'charge': -0.27000001072883606, 'distance': 23.282550811767578, 'force': [0.11679406464099884, 0.09367932379245758, 0.07020366191864014], 'magnitude': 0.16536390781402588, 'cosine_with_motion': 0.08328942954540253, 'motion_component': 0.013773065060377121, 'motion_component_percent': 8.328942954540253}, {'resid': 1313, 'atom': 'C32', 'charge': -0.08000000566244125, 'distance': 26.098739624023438, 'force': [0.0326407290995121, 0.019235214218497276, -0.009222800843417645], 'magnitude': 0.03899321332573891, 'cosine_with_motion': -0.5577799677848816, 'motion_component': -0.02174963429570198, 'motion_component_percent': 55.77799677848816}, {'resid': 1313, 'atom': 'C33', 'charge': -0.18000000715255737, 'distance': 25.111169815063477, 'force': [0.08159492909908295, 0.04302595555782318, -0.021740052849054337], 'magnitude': 0.09477128088474274, 'cosine_with_motion': -0.5495961904525757, 'motion_component': -0.052085936069488525, 'motion_component_percent': 54.95961904525757}, {'resid': 1313, 'atom': 'C34', 'charge': -0.18000000715255737, 'distance': 24.82367706298828, 'force': [0.08529355376958847, 0.0430118590593338, -0.01673157513141632], 'magnitude': 0.09697915613651276, 'cosine_with_motion': -0.4992749094963074, 'motion_component': -0.04841925948858261, 'motion_component_percent': 49.92749094963074}, {'resid': 1313, 'atom': 'C35', 'charge': -0.18000000715255737, 'distance': 24.317453384399414, 'force': [0.08770979940891266, 0.04850561171770096, -0.012926396913826466], 'magnitude': 0.10105887055397034, 'cosine_with_motion': -0.46178096532821655, 'motion_component': -0.04666706174612045, 'motion_component_percent': 46.178096532821655}, {'resid': 1313, 'atom': 'C36', 'charge': -0.18000000715255737, 'distance': 24.49185562133789, 'force': [0.08818203955888748, 0.04582614451646805, -0.006998721975833178], 'magnitude': 0.09962474554777145, 'cosine_with_motion': -0.40837976336479187, 'motion_component': -0.04068472981452942, 'motion_component_percent': 40.83797633647919}, {'resid': 1313, 'atom': 'C37', 'charge': -0.18000000715255737, 'distance': 24.194231033325195, 'force': [0.08856626600027084, 0.05073058605194092, -0.0022298996336758137], 'magnitude': 0.10209088027477264, 'cosine_with_motion': -0.3657495677471161, 'motion_component': -0.037339694797992706, 'motion_component_percent': 36.57495677471161}, {'resid': 1313, 'atom': 'C38', 'charge': -0.18000000715255737, 'distance': 22.673830032348633, 'force': [0.1008705347776413, 0.05776325985789299, -0.0007786313071846962], 'magnitude': 0.11624141037464142, 'cosine_with_motion': -0.35162127017974854, 'motion_component': -0.040872953832149506, 'motion_component_percent': 35.16212701797485}, {'resid': 1313, 'atom': 'C39', 'charge': -0.18000000715255737, 'distance': 22.330320358276367, 'force': [0.10087825357913971, 0.06454658508300781, 0.0044933767057955265], 'magnitude': 0.11984521150588989, 'cosine_with_motion': -0.31158021092414856, 'motion_component': -0.0373413972556591, 'motion_component_percent': 31.158021092414856}, {'resid': 1313, 'atom': 'C4', 'charge': 0.08000000566244125, 'distance': 27.52768325805664, 'force': [-0.022043120115995407, -0.016745202243328094, 0.021498970687389374], 'magnitude': 0.03505006060004234, 'cosine_with_motion': 0.8497868180274963, 'motion_component': 0.02978507988154888, 'motion_component_percent': 84.97868180274963}, {'resid': 1313, 'atom': 'C5', 'charge': 0.08000000566244125, 'distance': 26.10186767578125, 'force': [-0.024339696392416954, -0.01808541640639305, 0.02449977397918701], 'magnitude': 0.038983866572380066, 'cosine_with_motion': 0.8597826957702637, 'motion_component': 0.03351765498518944, 'motion_component_percent': 85.97826957702637}, {'resid': 1313, 'atom': 'C6', 'charge': 0.06000000238418579, 'distance': 25.121980667114258, 'force': [-0.01979544572532177, -0.01580285094678402, 0.01883210986852646], 'magnitude': 0.03156324103474617, 'cosine_with_motion': 0.8383766412734985, 'motion_component': 0.026461884379386902, 'motion_component_percent': 83.83766412734985}, {'resid': 1313, 'atom': 'H1', 'charge': 0.12000000476837158, 'distance': 24.925737380981445, 'force': [-0.04429272189736366, -0.03035803698003292, 0.03504972159862518], 'magnitude': 0.06412439793348312, 'cosine_with_motion': 0.8035199642181396, 'motion_component': 0.051525235176086426, 'motion_component_percent': 80.35199642181396}, {'resid': 1313, 'atom': 'H10R', 'charge': 0.09000000357627869, 'distance': 21.15948486328125, 'force': [-0.061650991439819336, -0.02179090678691864, 0.013349748216569424], 'magnitude': 0.0667375773191452, 'cosine_with_motion': 0.5131133198738098, 'motion_component': 0.03424394130706787, 'motion_component_percent': 51.31133198738098}, {'resid': 1313, 'atom': 'H10S', 'charge': 0.09000000357627869, 'distance': 22.17120933532715, 'force': [-0.0575135163962841, -0.01599489524960518, 0.011457180604338646], 'magnitude': 0.06078575551509857, 'cosine_with_motion': 0.4953657388687134, 'motion_component': 0.030111180618405342, 'motion_component_percent': 49.53657388687134}, {'resid': 1313, 'atom': 'H10X', 'charge': 0.09000000357627869, 'distance': 23.116687774658203, 'force': [-0.04572857916355133, -0.03146093711256981, -0.006753459107130766], 'magnitude': 0.055915139615535736, 'cosine_with_motion': 0.23182138800621033, 'motion_component': 0.012962325476109982, 'motion_component_percent': 23.182138800621033}, {'resid': 1313, 'atom': 'H10Y', 'charge': 0.09000000357627869, 'distance': 24.25352668762207, 'force': [-0.042655035853385925, -0.027300221845507622, -0.003936361987143755], 'magnitude': 0.050796154886484146, 'cosine_with_motion': 0.27328166365623474, 'motion_component': 0.01388165820389986, 'motion_component_percent': 27.328166365623474}, {'resid': 1313, 'atom': 'H111', 'charge': 0.15000000596046448, 'distance': 19.284683227539062, 'force': [-0.12717151641845703, -0.0302721094340086, 0.02902027778327465], 'magnitude': 0.13390733301639557, 'cosine_with_motion': 0.5151219964027405, 'motion_component': 0.06897861510515213, 'motion_component_percent': 51.51219964027405}, {'resid': 1313, 'atom': 'H11A', 'charge': 0.09000000357627869, 'distance': 25.378955841064453, 'force': [-0.03512468934059143, -0.021811148151755333, 0.021039217710494995], 'magnitude': 0.04639093577861786, 'cosine_with_motion': 0.7341148257255554, 'motion_component': 0.034056272357702255, 'motion_component_percent': 73.41148257255554}, {'resid': 1313, 'atom': 'H11B', 'charge': 0.09000000357627869, 'distance': 23.734375, 'force': [-0.04069747030735016, -0.023722104728221893, 0.024382326751947403], 'magnitude': 0.05304262414574623, 'cosine_with_motion': 0.7379429936408997, 'motion_component': 0.0391424335539341, 'motion_component_percent': 73.79429936408997}, {'resid': 1313, 'atom': 'H11X', 'charge': 0.09000000357627869, 'distance': 23.908754348754883, 'force': [-0.04494696110486984, -0.025340409949421883, -0.008364559151232243], 'magnitude': 0.052271708846092224, 'cosine_with_motion': 0.190588116645813, 'motion_component': 0.00996236689388752, 'motion_component_percent': 19.0588116645813}, {'resid': 1313, 'atom': 'H11Y', 'charge': 0.09000000357627869, 'distance': 23.601634979248047, 'force': [-0.04749711975455284, -0.024315273389220238, -0.0054901838302612305], 'magnitude': 0.0536409467458725, 'cosine_with_motion': 0.24525700509548187, 'motion_component': 0.013155817985534668, 'motion_component_percent': 24.525700509548187}, {'resid': 1313, 'atom': 'H12', 'charge': 0.09000000357627869, 'distance': 24.746625900268555, 'force': [-0.03945346549153328, -0.022035736590623856, 0.018398640677332878], 'magnitude': 0.04879200458526611, 'cosine_with_motion': 0.6729592084884644, 'motion_component': 0.03283502906560898, 'motion_component_percent': 67.29592084884644}, {'resid': 1313, 'atom': 'H121', 'charge': 0.15000000596046448, 'distance': 20.175580978393555, 'force': [-0.11293050646781921, -0.02465069480240345, 0.04008397087454796], 'magnitude': 0.12234247475862503, 'cosine_with_motion': 0.6065782308578491, 'motion_component': 0.0742102786898613, 'motion_component_percent': 60.65782308578491}, {'resid': 1313, 'atom': 'H12X', 'charge': 0.09000000357627869, 'distance': 22.191925048828125, 'force': [-0.05384589359164238, -0.025644056499004364, -0.011141532100737095], 'magnitude': 0.0606723316013813, 'cosine_with_motion': 0.16325056552886963, 'motion_component': 0.009904792532324791, 'motion_component_percent': 16.325056552886963}, {'resid': 1313, 'atom': 'H12Y', 'charge': 0.09000000357627869, 'distance': 21.249271392822266, 'force': [-0.058834951370954514, -0.029275210574269295, -0.0077789779752492905], 'magnitude': 0.06617478281259537, 'cosine_with_motion': 0.2297498732805252, 'motion_component': 0.015203648246824741, 'motion_component_percent': 22.97498732805252}, {'resid': 1313, 'atom': 'H13A', 'charge': 0.09000000357627869, 'distance': 26.141864776611328, 'force': [-0.033331144601106644, -0.023098286241292953, 0.016345731914043427], 'magnitude': 0.04372275248169899, 'cosine_with_motion': 0.6729411482810974, 'motion_component': 0.029422840103507042, 'motion_component_percent': 67.29411482810974}, {'resid': 1313, 'atom': 'H13B', 'charge': 0.09000000357627869, 'distance': 24.752765655517578, 'force': [-0.03632127121090889, -0.02740897238254547, 0.017544561997056007], 'magnitude': 0.04876779764890671, 'cosine_with_motion': 0.6618409752845764, 'motion_component': 0.03227652609348297, 'motion_component_percent': 66.18409752845764}, {'resid': 1313, 'atom': 'H13R', 'charge': 0.09000000357627869, 'distance': 22.833215713500977, 'force': [-0.05325871333479881, -0.01231347769498825, 0.017221104353666306], 'magnitude': 0.05731211602687836, 'cosine_with_motion': 0.585623025894165, 'motion_component': 0.033563293516635895, 'motion_component_percent': 58.562302589416504}, {'resid': 1313, 'atom': 'H13S', 'charge': 0.09000000357627869, 'distance': 22.395423889160156, 'force': [-0.05434586480259895, -0.017211759462952614, 0.01730405166745186], 'magnitude': 0.05957472324371338, 'cosine_with_motion': 0.5868577361106873, 'motion_component': 0.03496188670396805, 'motion_component_percent': 58.685773611068726}, {'resid': 1313, 'atom': 'H13X', 'charge': 0.09000000357627869, 'distance': 20.209503173828125, 'force': [-0.06198037415742874, -0.03563578799366951, -0.01551777869462967], 'magnitude': 0.07315926253795624, 'cosine_with_motion': 0.13869725167751312, 'motion_component': 0.010146988555788994, 'motion_component_percent': 13.869725167751312}, {'resid': 1313, 'atom': 'H13Y', 'charge': 0.09000000357627869, 'distance': 21.163082122802734, 'force': [-0.05486549437046051, -0.03605048358440399, -0.011875058524310589], 'magnitude': 0.06671489030122757, 'cosine_with_motion': 0.17482204735279083, 'motion_component': 0.011663233861327171, 'motion_component_percent': 17.482204735279083}, {'resid': 1313, 'atom': 'H141', 'charge': 0.15000000596046448, 'distance': 21.900493621826172, 'force': [-0.09062059968709946, -0.030129054561257362, 0.040752336382865906], 'magnitude': 0.10382969677448273, 'cosine_with_motion': 0.6717748045921326, 'motion_component': 0.06975017488002777, 'motion_component_percent': 67.17748045921326}, {'resid': 1313, 'atom': 'H14X', 'charge': 0.09000000357627869, 'distance': 22.02593994140625, 'force': [-0.05171218514442444, -0.028492063283920288, -0.017533019185066223], 'magnitude': 0.06159021705389023, 'cosine_with_motion': 0.06346331536769867, 'motion_component': 0.003908719401806593, 'motion_component_percent': 6.346331536769867}, {'resid': 1313, 'atom': 'H14Y', 'charge': 0.09000000357627869, 'distance': 23.098892211914062, 'force': [-0.0459865964949131, -0.02873150072991848, -0.013995789922773838], 'magnitude': 0.05600132420659065, 'cosine_with_motion': 0.10137766599655151, 'motion_component': 0.005677283741533756, 'motion_component_percent': 10.137766599655151}, {'resid': 1313, 'atom': 'H151', 'charge': 0.15000000596046448, 'distance': 23.073305130004883, 'force': [-0.08098272979259491, -0.02008398063480854, 0.04229256138205528], 'magnitude': 0.0935426652431488, 'cosine_with_motion': 0.7100346088409424, 'motion_component': 0.06641852855682373, 'motion_component_percent': 71.00346088409424}, {'resid': 1313, 'atom': 'H15X', 'charge': 0.09000000357627869, 'distance': 20.580276489257812, 'force': [-0.05503208190202713, -0.038420818746089935, -0.0217297300696373], 'magnitude': 0.0705469399690628, 'cosine_with_motion': 0.0419980026781559, 'motion_component': 0.002962830476462841, 'motion_component_percent': 4.19980026781559}, {'resid': 1313, 'atom': 'H15Y', 'charge': 0.09000000357627869, 'distance': 21.824447631835938, 'force': [-0.04826841503381729, -0.03645177558064461, -0.01663796231150627], 'magnitude': 0.06273271143436432, 'cosine_with_motion': 0.08672450482845306, 'motion_component': 0.005440463311970234, 'motion_component_percent': 8.672450482845306}, {'resid': 1313, 'atom': 'H16R', 'charge': 0.09000000357627869, 'distance': 24.058429718017578, 'force': [-0.04732220992445946, -0.008280077017843723, 0.018894901499152184], 'magnitude': 0.05162333324551582, 'cosine_with_motion': 0.6322406530380249, 'motion_component': 0.032638370990753174, 'motion_component_percent': 63.22406530380249}, {'resid': 1313, 'atom': 'H16S', 'charge': 0.09000000357627869, 'distance': 23.78134536743164, 'force': [-0.04719368740916252, -0.006890051998198032, 0.02272973582148552], 'magnitude': 0.052833303809165955, 'cosine_with_motion': 0.6796682476997375, 'motion_component': 0.03590911999344826, 'motion_component_percent': 67.96682476997375}, {'resid': 1313, 'atom': 'H16X', 'charge': 0.09000000357627869, 'distance': 23.5362548828125, 'force': [-0.04168243706226349, -0.028765959665179253, -0.018562056124210358], 'magnitude': 0.053939372301101685, 'cosine_with_motion': 0.0037527866661548615, 'motion_component': 0.00020242296159267426, 'motion_component_percent': 0.37527866661548615}, {'resid': 1313, 'atom': 'H16Y', 'charge': 0.09000000357627869, 'distance': 22.195491790771484, 'force': [-0.04731747880578041, -0.030385848134756088, -0.022727135568857193], 'magnitude': 0.06065283343195915, 'cosine_with_motion': -0.02957518957555294, 'motion_component': -0.0017938190139830112, 'motion_component_percent': 2.957518957555294}, {'resid': 1313, 'atom': 'H17R', 'charge': 0.09000000357627869, 'distance': 21.487606048583984, 'force': [-0.058353859931230545, -0.006627274677157402, 0.02718326449394226], 'magnitude': 0.0647149384021759, 'cosine_with_motion': 0.6666739583015442, 'motion_component': 0.04314376413822174, 'motion_component_percent': 66.66739583015442}, {'resid': 1313, 'atom': 'H17S', 'charge': 0.09000000357627869, 'distance': 21.681516647338867, 'force': [-0.05919909477233887, -0.007594441995024681, 0.021862970665097237], 'magnitude': 0.0635625496506691, 'cosine_with_motion': 0.6071571111679077, 'motion_component': 0.03859245404601097, 'motion_component_percent': 60.71571111679077}, {'resid': 1313, 'atom': 'H17X', 'charge': 0.09000000357627869, 'distance': 22.627771377563477, 'force': [-0.04144328087568283, -0.03578731045126915, -0.020182324573397636], 'magnitude': 0.05835754796862602, 'cosine_with_motion': 0.0012873171363025904, 'motion_component': 7.512466982007027e-05, 'motion_component_percent': 0.12873171363025904}, {'resid': 1313, 'atom': 'H17Y', 'charge': 0.09000000357627869, 'distance': 21.30177879333496, 'force': [-0.046932756900787354, -0.03840772435069084, -0.02565634995698929], 'magnitude': 0.0658489540219307, 'cosine_with_motion': -0.04527180641889572, 'motion_component': -0.0029811011627316475, 'motion_component_percent': 4.527180641889572}, {'resid': 1313, 'atom': 'H18R', 'charge': 0.09000000357627869, 'distance': 21.979440689086914, 'force': [-0.05765325948596001, -0.0007024265360087156, 0.02238672599196434], 'magnitude': 0.06185109168291092, 'cosine_with_motion': 0.601776659488678, 'motion_component': 0.0372205451130867, 'motion_component_percent': 60.1776659488678}, {'resid': 1313, 'atom': 'H18S', 'charge': 0.09000000357627869, 'distance': 23.484834671020508, 'force': [-0.0508478507399559, -0.002325806999579072, 0.01855013705790043], 'magnitude': 0.054175835102796555, 'cosine_with_motion': 0.5918132066726685, 'motion_component': 0.032061975449323654, 'motion_component_percent': 59.181320667266846}, {'resid': 1313, 'atom</t>
         </is>
       </c>
     </row>
@@ -483,7 +483,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>{50: {'frame': 50, 'motion_vector': [-1.7414207458496094, -1.1786270141601562, 2.00604248046875], 'ionic_force': [-6.545310348272324, -0.7018430531024933, -10.480357229709625], 'ionic_force_magnitude': 12.376249790979326, 'radial_force': 6.5828315508137525, 'axial_force': -10.480357229709625, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-7.2292962074279785, 2.4936505556106567, -9.968634337186813], 'asn_force_magnitude': 12.564023531368042, 'residue_force': [-7.2292962074279785, 2.4936505556106567, -9.968634337186813], 'residue_force_magnitude': 12.564023531368042, 'total_force': [-13.774606555700302, 1.7918075025081635, -20.44899156689644], 'total_force_magnitude': 24.72067183539695, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': -0.2833849045886601, 'cosine_residue_motion': -0.2833849045886601, 'cosine_ionic_motion': -0.244627740715776, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': -3.5604546096864134, 'motion_component_residue': -3.5604546096864134, 'motion_component_ionic': -3.0275740249013676, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 28.338490458866012, 'motion_component_percent_residue': 28.338490458866012, 'motion_component_percent_ionic': 24.462774071577602, 'ionic_contributions': [{'ion_id': 2276, 'distance': 14.84231948852539, 'force': [-0.20308879017829895, 0.05022875964641571, -1.4924824237823486], 'magnitude': 1.5070738792419434, 'cosine_ionic_motion': -0.6163520812988281, 'motion_component_ionic': -0.9288880825042725, 'motion_component_percent_ionic': 61.63520812988281}, {'ion_id': 2397, 'distance': 11.31926441192627, 'force': [-0.4405474066734314, 0.15366230905056, -2.54885196685791], 'magnitude': 2.5912044048309326, 'cosine_ionic_motion': -0.6011586785316467, 'motion_component_ionic': -1.557724952697754, 'motion_component_percent_ionic': 60.11586785316467}, {'ion_id': 2398, 'distance': 7.586583137512207, 'force': [-1.7664893865585327, 0.29237300157546997, -5.483336925506592], 'magnitude': 5.768270969390869, 'cosine_ionic_motion': -0.4932217597961426, 'motion_component_ionic': -2.845036745071411, 'motion_component_percent_ionic': 49.32217597961426}, {'ion_id': 2400, 'distance': 8.676553726196289, 'force': [-4.1351847648620605, -1.198107123374939, -0.9556859135627747], 'magnitude': 4.410050868988037, 'cosine_ionic_motion': 0.5224601030349731, 'motion_component_ionic': 2.3040757179260254, 'motion_component_percent_ionic': 52.246010303497314}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 3.536907196044922, 'force': [17.50432777404785, 6.932760238647461, 2.4316861629486084], 'magnitude': 18.983617782592773, 'cosine_with_motion': -0.6122081279754639, 'motion_component': -11.621925354003906, 'motion_component_percent': 61.22081279754639}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 2.6598477363586426, 'force': [-25.585451126098633, -6.123941898345947, -10.163896560668945], 'magnitude': 28.20323944091797, 'cosine_with_motion': 0.3828964829444885, 'motion_component': 10.798921585083008, 'motion_component_percent': 38.28964829444885}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 3.8168246746063232, 'force': [-19.41979217529297, -5.711623191833496, 4.338071346282959], 'magnitude': 20.701927185058594, 'cosine_with_motion': 0.818638265132904, 'motion_component': 16.947389602661133, 'motion_component_percent': 81.8638265132904}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 3.4632747173309326, 'force': [10.508767127990723, 1.0664888620376587, -4.514759540557861], 'magnitude': 11.487151145935059, 'cosine_with_motion': -0.8571218252182007, 'motion_component': -9.845888137817383, 'motion_component_percent': 85.71218252182007}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 4.746883392333984, 'force': [5.515578269958496, 2.1035537719726562, -1.5943527221679688], 'magnitude': 6.114614009857178, 'cosine_with_motion': -0.8600119948387146, 'motion_component': -5.258641242980957, 'motion_component_percent': 86.00119948387146}, {'resid': 786, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 5.7620086669921875, 'force': [4.247273921966553, 4.226412773132324, -0.46538302302360535], 'magnitude': 6.0098652839660645, 'cosine_with_motion': -0.7621320486068726, 'motion_component': -4.580310821533203, 'motion_component_percent': 76.21320486068726}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': -0.26649876987382426, 'motion_component_pip2': -6.588028634587781, 'motion_component_percent_pip2': 26.649876987382427}, 51: {'frame': 51, 'motion_vector': [1.2510223388671875, 0.09128189086914062, -0.7501068115234375], 'ionic_force': [-9.21544224023819, -0.8120492994785309, -11.918546557426453], 'ionic_force_magnitude': 15.087595957921586, 'radial_force': 9.25115126608304, 'axial_force': -11.918546557426453, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-2.755009651184082, 3.5658966302871704, 1.6752006635069847], 'asn_force_magnitude': 4.80749354851622, 'residue_force': [-2.755009651184082, 3.5658966302871704, 1.6752006635069847], 'residue_force_magnitude': 4.80749354851622, 'total_force': [-11.970451891422272, 2.7538473308086395, -10.243345893919468], 'total_force_magnitude': 15.99379656956827, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': -0.6230419473007781, 'cosine_residue_motion': -0.6230419473007781, 'cosine_ionic_motion': -0.12075108929622608, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': -2.9952701421034735, 'motion_component_residue': -2.9952701421034735, 'motion_component_ionic': -1.8218436467803691, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 62.30419473007781, 'motion_component_percent_residue': 62.30419473007781, 'motion_component_percent_ionic': 12.075108929622608, 'ionic_contributions': [{'ion_id': 2276, 'distance': 13.265876770019531, 'force': [-0.5075600743293762, -0.050070032477378845, -1.8162904977798462], 'magnitude': 1.8865405321121216, 'cosine_ionic_motion': 0.262174129486084, 'motion_component_ionic': 0.49460214376449585, 'motion_component_percent_ionic': 26.2174129486084}, {'ion_id': 2397, 'distance': 10.021937370300293, 'force': [-1.0986058712005615, -0.04292032867670059, -3.117279291152954], 'magnitude': 3.305481433868408, 'cosine_ionic_motion': 0.19871388375759125, 'motion_component_ionic': 0.6568450331687927, 'motion_component_percent_ionic': 19.871388375759125}, {'ion_id': 2398, 'distance': 6.365065574645996, 'force': [-4.8084492683410645, -0.025101251900196075, -6.635590553283691], 'magnitude': 8.194685935974121, 'cosine_ionic_motion': -0.08686579018831253, 'motion_component_ionic': -0.711837887763977, 'motion_component_percent_ionic': 8.686579018831253}, {'ion_id': 2400, 'distance': 10.687520980834961, 'force': [-2.8008270263671875, -0.6939576864242554, -0.34938621520996094], 'magnitude': 2.906592607498169, 'cosine_ionic_motion': -0.7780427932739258, 'motion_component_ionic': -2.26145339012146, 'motion_component_percent_ionic': 77.80427932739258}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 3.5729990005493164, 'force': [16.433238983154297, 1.3552528619766235, 8.610907554626465], 'magnitude': 18.60203742980957, 'cosine_with_motion': 0.5231470465660095, 'motion_component': 9.731600761413574, 'motion_component_percent': 52.31470465660095}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 4.275668144226074, 'force': [-10.146831512451172, 1.6897120475769043, -3.648752212524414], 'magnitude': 10.914518356323242, 'cosine_with_motion': -0.6145204305648804, 'motion_component': -6.707194805145264, 'motion_component_percent': 61.45204305648804}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 3.009874105453491, 'force': [-29.88152503967285, -12.14125919342041, -8.24212646484375], 'magnitude': 33.29036331176758, 'cosine_with_motion': -0.6640324592590332, 'motion_component': -22.10588264465332, 'motion_component_percent': 66.40324592590332}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 3.5279111862182617, 'force': [10.470809936523438, 3.5908493995666504, -0.12120798975229263], 'magnitude': 11.070083618164062, 'cosine_with_motion': 0.8355129361152649, 'motion_component': 9.249197959899902, 'motion_component_percent': 83.55129361152649}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 3.0633058547973633, 'force': [10.369297981262207, 9.071341514587402, 5.076379776000977], 'magnitude': 14.682683944702148, 'cosine_with_motion': 0.46565118432044983, 'motion_component': 6.837008953094482, 'motion_component_percent': 46.56511843204498}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': -0.3011863861048142, 'motion_component_pip2': -4.817113788883842, 'motion_component_percent_pip2': 30.11863861048142}, 52: {'frame': 52, 'motion_vector': [0.3236579895019531, -0.5370292663574219, 0.17535400390625], 'ionic_force': [-7.563069611787796, -2.006166153587401, -11.770043104887009], 'ionic_force_magnitude': 14.133599657534024, 'radial_force': 7.824622967820729, 'axial_force': -11.770043104887009, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-12.611527442932129, 0.8868218660354614, -1.0281258821487427], 'asn_force_magnitude': 12.684404609419117, 'residue_force': [-12.611527442932129, 0.8868218660354614, -1.0281258821487427], 'residue_force_magnitude': 12.684404609419117, 'total_force': [-20.174597054719925, -1.1193442875519395, -12.798168987035751], 'total_force_magnitude': 23.917784750580743, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': -0.5737516697540563, 'cosine_residue_motion': -0.5737516697540563, 'cosine_ionic_motion': -0.3732197816864911, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': -7.277698324490267, 'motion_component_residue': -7.277698324490267, 'motion_component_ionic': -5.274938978629114, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 57.375166975405634, 'motion_component_percent_residue': 57.375166975405634, 'motion_component_percent_ionic': 37.32197816864911, 'ionic_contributions': [{'ion_id': 2276, 'distance': 13.700033187866211, 'force': [-0.31668099761009216, 0.012376311235129833, -1.7402429580688477], 'magnitude': 1.7688655853271484, 'cosine_ionic_motion': -0.3597392439842224, 'motion_component_ionic': -0.6363303661346436, 'motion_component_percent_ionic': 35.97392439842224}, {'ion_id': 2397, 'distance': 10.308706283569336, 'force': [-0.737959086894989, -0.020601239055395126, -3.035656452178955], 'magnitude': 3.1241347789764404, 'cosine_ionic_motion': -0.3736850917339325, 'motion_component_ionic': -1.1674425601959229, 'motion_component_percent_ionic': 37.36850917339325}, {'ion_id': 2398, 'distance': 6.783831596374512, 'force': [-2.981602191925049, -0.435778945684433, -6.554752826690674], 'magnitude': 7.214197158813477, 'cosine_ionic_motion': -0.4003385901451111, 'motion_component_ionic': -2.8881216049194336, 'motion_component_percent_ionic': 40.03385901451111}, {'ion_id': 2400, 'distance': 9.247553825378418, 'force': [-3.526827335357666, -1.5621622800827026, -0.4393908679485321], 'magnitude': 3.8822579383850098, 'cosine_ionic_motion': -0.15018175542354584, 'motion_component_ionic': -0.5830442905426025, 'motion_component_percent_ionic': 15.018175542354584}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 3.8028459548950195, 'force': [15.213778495788574, 3.995378255844116, 4.715787410736084], 'magnitude': 16.421350479125977, 'cosine_with_motion': 0.3372141718864441, 'motion_component': 5.537512302398682, 'motion_component_percent': 33.72141718864441}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 2.775726079940796, 'force': [-25.355928421020508, -2.4966883659362793, -4.6398844718933105], 'magnitude': 25.8975887298584, 'cosine_with_motion': -0.4554477334022522, 'motion_component': -11.794998168945312, 'motion_component_percent': 45.54477334022522}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 4.879722595214844, 'force': [-12.16822624206543, -3.2634212970733643, -1.3042912483215332], 'magnitude': 12.665575981140137, 'cosine_with_motion': -0.2927987277507782, 'motion_component': -3.7084643840789795, 'motion_component_percent': 29.27987277507782}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 4.853046417236328, 'force': [5.718878269195557, 1.1074044704437256, -0.5392680168151855], 'magnitude': 5.850019454956055, 'cosine_with_motion': 0.30499932169914246, 'motion_component': 1.7842520475387573, 'motion_component_percent': 30.499932169914246}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 5.639213562011719, 'force': [3.9799704551696777, 1.5441488027572632, 0.7395304441452026], 'magnitude': 4.332604885101318, 'cosine_with_motion': 0.2086505889892578, 'motion_component': 0.9040005803108215, 'motion_component_percent': 20.86505889892578}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': -0.5248244113750791, 'motion_component_pip2': -12.552637303119381, 'motion_component_percent_pip2': 52.482441137507905}, 53: {'frame': 53, 'motion_vector': [5.758647918701172, -2.995861053466797, 0.5327529907226562], 'ionic_force': [-9.539707899093628, -5.161478877067566, -15.843355238437653], 'ionic_force_magnitude': 19.200489478390228, 'radial_force': 10.84651515457587, 'axial_force': -15.843355238437653, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-9.779897212982178, 6.35490345954895, -5.005626350641251], 'asn_force_magnitude': 12.692024371191454, 'residue_force': [-9.779897212982178, 6.35490345954895, -5.005626350641251], 'residue_force_magnitude': 12.692024371191454, 'total_force': [-19.319605112075806, 1.1934245824813843, -20.848981589078903], 'total_force_magnitude': 28.449102573233617, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': -0.9438599026588604, 'cosine_residue_motion': -0.9438599026588604, 'cosine_ionic_motion': -0.38313648679282747, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': -11.97949288753665, 'motion_component_residue': -11.97949288753665, 'motion_component_ionic': -7.35640808345308, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 94.38599026588605, 'motion_component_percent_residue': 94.38599026588605, 'motion_component_percent_ionic': 38.31364867928275, 'ionic_contributions': [{'ion_id': 2276, 'distance': 13.034229278564453, 'force': [-0.3271370530128479, -0.1568824052810669, -1.9202182292938232], 'magnitude': 1.9541926383972168, 'cosine_ionic_motion': -0.19145844876766205, 'motion_component_ionic': -0.3741466999053955, 'motion_component_percent_ionic': 19.145844876766205}, {'ion_id': 2397, 'distance': 9.544228553771973, 'force': [-0.8382934927940369, -0.371917724609375, -3.527385711669922], 'magnitude': 3.6446547508239746, 'cosine_ionic_motion': -0.23558899760246277, 'motion_component_ionic': -0.8586405515670776, 'motion_component_percent_ionic': 23.558899760246277}, {'ion_id': 2398, 'distance': 5.354485511779785, 'force': [-4.838714122772217, -2.53334903717041, -10.210862159729004], 'magnitude': 11.579840660095215, 'cosine_ionic_motion': -0.34094882011413574, 'motion_component_ionic': -3.9481329917907715, 'motion_component_percent_ionic': 34.094882011413574}, {'ion_id': 2400, 'distance': 8.981122016906738, 'force': [-3.5355632305145264, -2.099329710006714, -0.18488913774490356], 'magnitude': 4.11601448059082, 'cosine_ionic_motion': -0.5285422801971436, 'motion_component_ionic': -2.175487756729126, 'motion_component_percent_ionic': 52.854228019714355}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 3.959688663482666, 'force': [13.715808868408203, -4.843451976776123, 4.222024440765381], 'magnitude': 15.146218299865723, 'cosine_with_motion': 0.9705485105514526, 'motion_component': 14.700139999389648, 'motion_component_percent': 97.05485105514526}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 2.8336873054504395, 'force': [-20.997434616088867, 10.525444030761719, -8.111410140991211], 'magnitude': 24.848987579345703, 'cosine_with_motion': -0.9686487317085266, 'motion_component': -24.0699405670166, 'motion_component_percent': 96.86487317085266}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 4.900882244110107, 'force': [-10.844793319702148, 6.044493198394775, -1.8758577108383179], 'magnitude': 12.556443214416504, 'cosine_with_motion': -0.9972764253616333, 'motion_component': -12.522244453430176, 'motion_component_percent': 99.72764253616333}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 4.82323694229126, 'force': [4.598276138305664, -3.727292060852051, 0.1994415819644928], 'magnitude': 5.922552108764648, 'cosine_with_motion': 0.9786937832832336, 'motion_component': 5.796364784240723, 'motion_component_percent': 97.86937832832336}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 5.775038242340088, 'force': [3.7482457160949707, -1.6442897319793701, 0.5601754784584045], 'magnitude': 4.131202220916748, 'cosine_with_motion': 0.9963657855987549, 'motion_component': 4.1161885261535645, 'motion_component_percent': 99.63657855987549}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': -0.6796664647405062, 'motion_component_pip2': -19.33590097098973, 'motion_component_percent_pip2': 67.96664647405062}, 54: {'frame': 54, 'motion_vector': [-0.79925537109375, -0.5596580505371094, -0.49560546875], 'ionic_force': [2.7243117690086365, -10.218597322702408, -10.363595068454742], 'ionic_force_magnitude': 14.806947984010723, 'radial_force': 10.575519176773298, 'axial_force': -10.363595068454742, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [1.5536694526672363, 4.403852224349976, 0.288180947303772], 'asn_force_magnitude': 4.678766016852354, 'residue_force': [1.5536694526672363, 4.403852224349976, 0.288180947303772], 'residue_force_magnitude': 4.678766016852354, 'total_force': [4.277981221675873, -5.814745098352432, -10.07541412115097], 'total_force_magnitude': 12.394609860923957, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': -0.7517615722315798, 'cosine_residue_motion': -0.7517615722315798, 'cosine_ionic_motion': 0.5355211674702611, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': -3.5173164969326116, 'motion_component_residue': -3.5173164969326116, 'motion_component_ionic': 7.929434071068851, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 75.17615722315799, 'motion_component_percent_residue': 75.17615722315799, 'motion_component_percent_ionic': 53.55211674702611, 'ionic_contributions': [{'ion_id': 2276, 'distance': 13.739262580871582, 'force': [0.43902212381362915, -0.4345407783985138, -1.6467351913452148], 'magnitude': 1.7587788105010986, 'cosine_ionic_motion': 0.36806395649909973, 'motion_component_ionic': 0.647343099117279, 'motion_component_percent_ionic': 36.80639564990997}, {'ion_id': 2397, 'distance': 10.359049797058105, 'force': [0.9970773458480835, -1.0642732381820679, -2.7285568714141846], 'magnitude': 3.0938427448272705, 'cosine_ionic_motion': 0.33994677662849426, 'motion_component_ionic': 1.0517418384552002, 'motion_component_percent_ionic': 33.994677662849426}, {'ion_id': 2398, 'distance': 6.714522838592529, 'force': [3.472324848175049, -4.122472286224365, -5.017487525939941], 'magnitude': 7.363898277282715, 'cosine_ionic_motion': 0.25048184394836426, 'motion_component_ionic': 1.8445227146148682, 'motion_component_percent_ionic': 25.048184394836426}, {'ion_id': 2400, 'distance': 8.004618644714355, 'force': [-2.184112548828125, -4.597311019897461, -0.9708154797554016], 'magnitude': 5.181515216827393, 'cosine_ionic_motion': 0.8464369773864746, 'motion_component_ionic': 4.385826110839844, 'motion_component_percent_ionic': 84.64369773864746}], 'glu_contributions': [], 'asn_contributions': [{'resid': 458, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 5.848904609680176, 'force': [6.17788028717041, 6.1426167488098145, -1.3497967720031738], 'magnitude': 8.815888404846191, 'cosine_with_motion': -0.7987779974937439, 'motion_component': -7.041937828063965, 'motion_component_percent': 79.87779974937439}, {'resid': 458, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 5.280088424682617, 'force': [-3.720984697341919, -2.9884397983551025, 1.2833473682403564], 'magnitude': 4.942011833190918, 'cosine_with_motion': 0.7415291666984558, 'motion_component': 3.6646459102630615, 'motion_component_percent': 74.15291666984558}, {'resid': 1114, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 5.25584602355957, 'force': [4.207759857177734, 6.4884490966796875, 3.7551562786102295], 'magnitude': 8.596883773803711, 'cosine_with_motion': -0.941250205039978, 'motion_component': -8.091818809509277, 'motion_component_percent': 94.1250205039978}, {'resid': 1114, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 5.77084493637085, 'force': [-3.90395188331604, -4.017500877380371, -2.1252338886260986], 'magnitude': 5.9914751052856445, 'cosine_with_motion': 0.9794192314147949, 'motion_component': 5.868165969848633, 'motion_component_percent': 97.94192314147949}, {'resid': 1114, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 4.8832573890686035, 'force': [-4.634448051452637, -11.227103233337402, -3.525177478790283], 'magnitude': 12.647246360778809, 'cosine_with_motion': 0.8478227853775024, 'motion_component': 10.722623825073242, 'motion_component_percent': 84.78227853775024}, {'resid': 1114, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 4.934086322784424, 'force': [2.4747731685638428, 5.066349983215332, 0.48656249046325684], 'magnitude': 5.659430027008057, 'cosine_with_motion': -0.8161011934280396, 'motion_component': -4.6186676025390625, 'motion_component_percent': 81.61011934280396}, {'resid': 1114, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 5.083993911743164, 'force': [0.9526407718658447, 4.939480304718018, 1.7633229494094849], 'magnitude': 5.330600261688232, 'cosine_with_motion': -0.754197895526886, 'motion_component': -4.020327568054199, 'motion_component_percent': 75.4197895526886}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': 0.35597066980269904, 'motion_component_pip2': 4.412117574136239, 'motion_component_percent_pip2': 35.5970669802699}, 55: {'frame': 55, 'motion_vector': [-4.003032684326172, 3.991687774658203, -1.4045257568359375], 'ionic_force': [1.2560828030109406, -8.269347667694092, -8.893366515636444], 'ionic_force_magnitude': 12.20867817737289, 'radial_force': 8.36420079010646, 'axial_force': -8.893366515636444, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-2.5737082064151764, -0.5412287712097168, -0.7374037019908428], 'asn_force_magnitude': 2.7314221084013734, 'residue_force': [-2.5737082064151764, -0.5412287712097168, -0.7374037019908428], 'residue_force_magnitude': 2.7314221084013734, 'total_force': [-1.3176254034042358, -8.810576438903809, -9.630770217627287], 'total_force_magnitude': 13.11922744959473, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': 0.5768465343366295, 'cosine_residue_motion': 0.5768465343366295, 'cosine_ionic_motion': -0.35921634306610706, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': 1.5756113770417817, 'motion_component_residue': 1.5756113770417817, 'motion_component_ionic': -4.385556728546875, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 57.684653433662945, 'motion_component_percent_residue': 57.684653433662945, 'motion_component_percent_ionic': 35.921634306610706, 'ionic_contributions': [{'ion_id': 2276, 'distance': 14.350513458251953, 'force': [0.33545854687690735, -0.47075557708740234, -1.5049443244934082], 'magnitude': 1.6121416091918945, 'cosine_ionic_motion': -0.1180131807923317, 'motion_component_ionic': -0.19025395810604095, 'motion_component_percent_ionic': 11.80131807923317}, {'ion_id': 2397, 'distance': 11.072735786437988, 'force': [0.717076301574707, -1.001948356628418, -2.4113221168518066], 'magnitude': 2.7078723907470703, 'cosine_ionic_motion': -0.22082717716693878, 'motion_component_ionic': -0.5979717969894409, 'motion_component_percent_ionic': 22.082717716693878}, {'ion_id': 2398, 'distance': 7.621569633483887, 'force': [2.0875403881073, -3.5012741088867188, -4.006175994873047], 'magnitude': 5.715434551239014, 'cosine_ionic_motion': -0.5017880201339722, 'motion_component_ionic': -2.867936611175537, 'motion_component_percent_ionic': 50.17880201339722}, {'ion_id': 2400, 'distance': 9.205147743225098, 'force': [-1.8839924335479736, -3.2953696250915527, -0.9709240794181824], 'magnitude': 3.91810941696167, 'cosine_ionic_motion': -0.18615977466106415, 'motion_component_ionic': -0.7293943762779236, 'motion_component_percent_ionic': 18.615977466106415}], 'glu_contributions': [], 'asn_contributions': [{'resid': 1114, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 4.610045433044434, 'force': [4.120113372802734, 9.281291961669922, 4.663124084472656], 'magnitude': 11.174186706542969, 'cosine_with_motion': 0.21517425775527954, 'motion_component': 2.4043972492218018, 'motion_component_percent': 21.517425775527954}, {'resid': 1114, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 4.476313591003418, 'force': [-5.87069845199585, -7.2108073234558105, -3.563796043395996], 'magnitude': 9.957985877990723, 'cosine_with_motion': -0.004779744893312454, 'motion_component': -0.047596633434295654, 'motion_component_percent': 0.4779744893312454}, {'resid': 1114, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 4.605300426483154, 'force': [-2.9677417278289795, -13.576927185058594, -3.0112526416778564], 'magnitude': 14.219988822937012, 'cosine_with_motion': -0.45979592204093933, 'motion_component': -6.53829288482666, 'motion_component_percent': 45.97959220409393}, {'resid': 1114, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 4.595030307769775, 'force': [1.80350923538208, 6.2712249755859375, 0.019588876515626907], 'magnitude': 6.5254340171813965, 'cosine_with_motion': 0.4679156243801117, 'motion_component': 3.0533525943756104, 'motion_component_percent': 46.79156243801117}, {'resid': 1114, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 5.3321356773376465, 'force': [0.34110936522483826, 4.693988800048828, 1.1549320220947266], 'magnitude': 4.846004009246826, 'cosine_with_motion': 0.5579343438148499, 'motion_component': 2.703752040863037, 'motion_component_percent': 55.793434381484985}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': -0.21418527594716683, 'motion_component_pip2': -2.809945351505093, 'motion_component_percent_pip2': 21.418527594716682}, 56: {'frame': 56, 'motion_vector': [-0.07032394409179688, 0.9238395690917969, 2.2243270874023438], 'ionic_force': [-5.984475448727608, -2.480348927900195, -11.34298050403595], 'ionic_force_magnitude': 13.062514456087648, 'radial_force': 6.478122968928512, 'axial_force': -11.34298050403595, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-11.193721294403076, 8.06148099899292, 0.7260817885398865], 'asn_force_magnitude': 13.813546506149173, 'residue_force': [-11.193721294403076, 8.06148099899292, 0.7260817885398865], 'residue_force_magnitude': 13.813546506149173, 'total_force': [-17.178196743130684, 5.581132071092725, -10.616898715496063], 'total_force_magnitude': 20.95132494320556, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': 0.2959233170364331, 'cosine_residue_motion': 0.2959233170364331, 'cosine_ionic_motion': -0.8610321677795314, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': 4.087750502136695, 'motion_component_residue': 4.087750502136695, 'motion_component_ionic': -11.247245138776615, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 29.59233170364331, 'motion_component_percent_residue': 29.59233170364331, 'motion_component_percent_ionic': 86.10321677795314, 'ionic_contributions': [{'ion_id': 2276, 'distance': 14.85102653503418, 'force': [-0.15976811945438385, 0.023013589903712273, -1.496627688407898], 'magnitude': 1.5053073167800903, 'cosine_ionic_motion': -0.9088377952575684, 'motion_component_ionic': -1.3680801391601562, 'motion_component_percent_ionic': 90.88377952575684}, {'ion_id': 2397, 'distance': 11.193451881408691, 'force': [-0.29192692041397095, 0.03805402293801308, -2.633376359939575], 'magnitude': 2.6497812271118164, 'cosine_ionic_motion': -0.908683180809021, 'motion_component_ionic': -2.4078116416931152, 'motion_component_percent_ionic': 90.8683180809021}, {'ion_id': 2398, 'distance': 7.468287944793701, 'force': [-1.0910613536834717, -0.1779259592294693, -5.8488993644714355], 'magnitude': 5.952453136444092, 'cosine_ionic_motion': -0.9131712317466736, 'motion_component_ionic': -5.435608863830566, 'motion_component_percent_ionic': 91.31712317466736}, {'ion_id': 2400, 'distance': 7.9803876876831055, 'force': [-4.441719055175781, -2.363490581512451, -1.364077091217041], 'magnitude': 5.213028430938721, 'cosine_ionic_motion': -0.3905108571052551, 'motion_component_ionic': -2.0357441902160645, 'motion_component_percent_ionic': 39.05108571052551}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 3.9731361865997314, 'force': [13.59004020690918, -6.2530903816223145, -1.5898170471191406], 'magnitude': 15.043864250183105, 'cosine_with_motion': -0.2832833230495453, 'motion_component': -4.261675834655762, 'motion_component_percent': 28.32833230495453}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 2.7872426509857178, 'force': [-21.964885711669922, 13.17414379119873, 1.9116986989974976], 'magnitude': 25.684019088745117, 'cosine_with_motion': 0.29032790660858154, 'motion_component': 7.456787586212158, 'motion_component_percent': 29.032790660858154}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 4.980515003204346, 'force': [-9.811515808105469, 6.96938419342041, 1.7268179655075073], 'magnitude': 12.158127784729004, 'cosine_with_motion': 0.37444058060646057, 'motion_component': 4.552496433258057, 'motion_component_percent': 37.44405806064606}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 5.098830223083496, 'force': [3.581787109375, -3.8314223289489746, -0.7596155405044556], 'magnitude': 5.299623966217041, 'cosine_with_motion': -0.4292250871658325, 'motion_component': -2.2747316360473633, 'motion_component_percent': 42.92250871658325}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 5.874406337738037, 'force': [3.4108529090881348, -1.9975342750549316, -0.5630022883415222], 'magnitude': 3.992622137069702, 'cosine_with_motion': -0.34692147374153137, 'motion_component': -1.3851263523101807, 'motion_component_percent': 34.69214737415314}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': -0.34172037596895366, 'motion_component_pip2': -7.15</t>
+          <t>{50: {'frame': 50, 'motion_vector': [-1.7414207458496094, -1.1786270141601562, 2.00604248046875], 'ionic_force': [-6.545310348272324, -0.7018430531024933, -10.480357229709625], 'ionic_force_magnitude': 12.376249790979326, 'radial_force': 6.5828315508137525, 'axial_force': -10.480357229709625, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-7.2292962074279785, 2.4936505556106567, -9.968634337186813], 'asn_force_magnitude': 12.564023531368042, 'residue_force': [-7.2292962074279785, 2.4936505556106567, -9.968634337186813], 'residue_force_magnitude': 12.564023531368042, 'pip2_force': [0.3286649566143751, -0.16861860593780875, -4.935831281458377], 'pip2_force_magnitude': 4.949634666013016, 'total_force': [-13.445941599085927, 1.6231888965703547, -25.384822848354816], 'total_force_magnitude': 28.771814658139576, 'cosine_total_motion': -0.3518590321781765, 'cosine_glu_motion': 0, 'cosine_asn_motion': -0.2833849045886601, 'cosine_residue_motion': -0.2833849045886601, 'cosine_pip2_motion': -0.7143141794509533, 'cosine_ionic_motion': -0.244627740715776, 'motion_component_total': -10.123622859622863, 'motion_component_glu': 0, 'motion_component_asn': -3.5604546096864134, 'motion_component_residue': -3.5604546096864134, 'motion_component_ionic': -3.0275740249013676, 'motion_component_pip2': -3.535594225035081, 'motion_component_percent_total': 35.185903217817646, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 28.338490458866012, 'motion_component_percent_residue': 28.338490458866012, 'motion_component_percent_ionic': 24.462774071577602, 'motion_component_percent_pip2': 71.43141794509533, 'ionic_contributions': [{'ion_id': 2276, 'distance': 14.84231948852539, 'force': [-0.20308879017829895, 0.05022875964641571, -1.4924824237823486], 'magnitude': 1.5070738792419434, 'cosine_ionic_motion': -0.6163520812988281, 'motion_component_ionic': -0.9288880825042725, 'motion_component_percent_ionic': 61.63520812988281}, {'ion_id': 2397, 'distance': 11.31926441192627, 'force': [-0.4405474066734314, 0.15366230905056, -2.54885196685791], 'magnitude': 2.5912044048309326, 'cosine_ionic_motion': -0.6011586785316467, 'motion_component_ionic': -1.557724952697754, 'motion_component_percent_ionic': 60.11586785316467}, {'ion_id': 2398, 'distance': 7.586583137512207, 'force': [-1.7664893865585327, 0.29237300157546997, -5.483336925506592], 'magnitude': 5.768270969390869, 'cosine_ionic_motion': -0.4932217597961426, 'motion_component_ionic': -2.845036745071411, 'motion_component_percent_ionic': 49.32217597961426}, {'ion_id': 2400, 'distance': 8.676553726196289, 'force': [-4.1351847648620605, -1.198107123374939, -0.9556859135627747], 'magnitude': 4.410050868988037, 'cosine_ionic_motion': 0.5224601030349731, 'motion_component_ionic': 2.3040757179260254, 'motion_component_percent_ionic': 52.246010303497314}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 3.536907196044922, 'force': [17.50432777404785, 6.932760238647461, 2.4316861629486084], 'magnitude': 18.983617782592773, 'cosine_with_motion': -0.6122081279754639, 'motion_component': -11.621925354003906, 'motion_component_percent': 61.22081279754639}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 2.6598477363586426, 'force': [-25.585451126098633, -6.123941898345947, -10.163896560668945], 'magnitude': 28.20323944091797, 'cosine_with_motion': 0.3828964829444885, 'motion_component': 10.798921585083008, 'motion_component_percent': 38.28964829444885}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 3.8168246746063232, 'force': [-19.41979217529297, -5.711623191833496, 4.338071346282959], 'magnitude': 20.701927185058594, 'cosine_with_motion': 0.818638265132904, 'motion_component': 16.947389602661133, 'motion_component_percent': 81.8638265132904}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 3.4632747173309326, 'force': [10.508767127990723, 1.0664888620376587, -4.514759540557861], 'magnitude': 11.487151145935059, 'cosine_with_motion': -0.8571218252182007, 'motion_component': -9.845888137817383, 'motion_component_percent': 85.71218252182007}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 4.746883392333984, 'force': [5.515578269958496, 2.1035537719726562, -1.5943527221679688], 'magnitude': 6.114614009857178, 'cosine_with_motion': -0.8600119948387146, 'motion_component': -5.258641242980957, 'motion_component_percent': 86.00119948387146}, {'resid': 786, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 5.7620086669921875, 'force': [4.247273921966553, 4.226412773132324, -0.46538302302360535], 'magnitude': 6.0098652839660645, 'cosine_with_motion': -0.7621320486068726, 'motion_component': -4.580310821533203, 'motion_component_percent': 76.21320486068726}], 'pip2_contributions': [{'resid': 1313, 'atom': 'C1', 'charge': 0.06000000238418579, 'distance': 28.01099967956543, 'force': [-0.018726617097854614, -0.011985673569142818, 0.01225637923926115], 'magnitude': 0.025388214737176895, 'cosine_with_motion': 0.9666793942451477, 'motion_component': 0.02454226464033127, 'motion_component_percent': 96.66793942451477}, {'resid': 1313, 'atom': 'C11', 'charge': 0.17000000178813934, 'distance': 27.12787437438965, 'force': [-0.062194835394620895, -0.03398802503943443, 0.029298905283212662], 'magnitude': 0.07669295370578766, 'cosine_with_motion': 0.9293689131736755, 'motion_component': 0.07127604633569717, 'motion_component_percent': 92.93689131736755}, {'resid': 1313, 'atom': 'C12', 'charge': 0.04000000283122063, 'distance': 26.49906349182129, 'force': [-0.015826033428311348, -0.00811096467077732, 0.006435214076191187], 'magnitude': 0.01891198195517063, 'cosine_with_motion': 0.9102497100830078, 'motion_component': 0.01721462607383728, 'motion_component_percent': 91.02497100830078}, {'resid': 1313, 'atom': 'C13', 'charge': -0.05000000074505806, 'distance': 26.898412704467773, 'force': [0.019192686304450035, 0.010620019398629665, -0.006726689171046019], 'magnitude': 0.022943241521716118, 'cosine_with_motion': -0.891361653804779, 'motion_component': -0.02045072615146637, 'motion_component_percent': 89.1361653804779}, {'resid': 1313, 'atom': 'C2', 'charge': 0.06000000238418579, 'distance': 29.4793643951416, 'force': [-0.016957689076662064, -0.010855847038328648, 0.010954765602946281], 'magnitude': 0.022922031581401825, 'cosine_with_motion': 0.9652561545372009, 'motion_component': 0.02212563157081604, 'motion_component_percent': 96.52561545372009}, {'resid': 1313, 'atom': 'C21', 'charge': 0.6299999952316284, 'distance': 24.434785842895508, 'force': [-0.3013263940811157, -0.13747839629650116, 0.11412396281957626], 'magnitude': 0.3503172695636749, 'cosine_with_motion': 0.899441123008728, 'motion_component': 0.31508976221084595, 'motion_component_percent': 89.9441123008728}, {'resid': 1313, 'atom': 'C210', 'charge': -0.18000000715255737, 'distance': 25.04411506652832, 'force': [0.0915977954864502, 0.024863915517926216, -0.008354746736586094], 'magnitude': 0.09527944773435593, 'cosine_with_motion': -0.7424187064170837, 'motion_component': -0.07073724269866943, 'motion_component_percent': 74.24187064170837}, {'resid': 1313, 'atom': 'C211', 'charge': -0.15000000596046448, 'distance': 24.343381881713867, 'force': [0.08186668902635574, 0.017484353855252266, -0.007366239558905363], 'magnitude': 0.08403641730546951, 'cosine_with_motion': -0.728625476360321, 'motion_component': -0.06123107671737671, 'motion_component_percent': 72.8625476360321}, {'resid': 1313, 'atom': 'C212', 'charge': -0.15000000596046448, 'distance': 24.32572364807129, 'force': [0.08214151859283447, 0.014538208954036236, -0.011138146743178368], 'magnitude': 0.08415846526622772, 'cosine_with_motion': -0.7462652921676636, 'motion_component': -0.06280454248189926, 'motion_component_percent': 74.62652921676636}, {'resid': 1313, 'atom': 'C213', 'charge': -0.18000000715255737, 'distance': 25.113792419433594, 'force': [0.0916767492890358, 0.01665637455880642, -0.01719827763736248], 'magnitude': 0.09475147724151611, 'cosine_with_motion': -0.7763500213623047, 'motion_component': -0.07356031239032745, 'motion_component_percent': 77.63500213623047}, {'resid': 1313, 'atom': 'C214', 'charge': -0.15000000596046448, 'distance': 24.305133819580078, 'force': [0.08038219809532166, 0.01690923050045967, -0.018959373235702515], 'magnitude': 0.08430111408233643, 'cosine_with_motion': -0.8079449534416199, 'motion_component': -0.06811065971851349, 'motion_component_percent': 80.79449534416199}, {'resid': 1313, 'atom': 'C215', 'charge': -0.15000000596046448, 'distance': 24.64800453186035, 'force': [0.0767655223608017, 0.018212785944342613, -0.022243382409214973], 'magnitude': 0.08197206258773804, 'cosine_with_motion': -0.8385663032531738, 'motion_component': -0.06873901188373566, 'motion_component_percent': 83.85663032531738}, {'resid': 1313, 'atom': 'C216', 'charge': -0.18000000715255737, 'distance': 26.089590072631836, 'force': [0.0815596953034401, 0.02018176019191742, -0.025473495945334435], 'magnitude': 0.08779627829790115, 'cosine_with_motion': -0.8501489162445068, 'motion_component': -0.07463990896940231, 'motion_component_percent': 85.01489162445068}, {'resid': 1313, 'atom': 'C217', 'charge': -0.18000000715255737, 'distance': 26.45683479309082, 'force': [0.07854114472866058, 0.017000684514641762, -0.028832167387008667], 'magnitude': 0.08537580817937851, 'cosine_with_motion': -0.8651095032691956, 'motion_component': -0.07385942339897156, 'motion_component_percent': 86.51095032691956}, {'resid': 1313, 'atom': 'C218', 'charge': -0.18000000715255737, 'distance': 26.2915096282959, 'force': [0.08050369471311569, 0.012154463678598404, -0.02907797507941723], 'magnitude': 0.0864529013633728, 'cosine_with_motion': -0.8471624851226807, 'motion_component': -0.07323965430259705, 'motion_component_percent': 84.71624851226807}, {'resid': 1313, 'atom': 'C219', 'charge': -0.18000000715255737, 'distance': 27.025402069091797, 'force': [0.07520081102848053, 0.009123559109866619, -0.030924441292881966], 'magnitude': 0.08182128518819809, 'cosine_with_motion': -0.8568363785743713, 'motion_component': -0.07010745257139206, 'motion_component_percent': 85.68363785743713}, {'resid': 1313, 'atom': 'C22', 'charge': -0.08000000566244125, 'distance': 23.031497955322266, 'force': [0.04273582994937897, 0.01972389407455921, -0.017079012468457222], 'magnitude': 0.050070710480213165, 'cosine_with_motion': -0.9066391587257385, 'motion_component': -0.04539606720209122, 'motion_component_percent': 90.66391587257385}, {'resid': 1313, 'atom': 'C220', 'charge': -0.27000001072883606, 'distance': 26.689979553222656, 'force': [0.11625736951828003, 0.006984170060604811, -0.04764638841152191], 'magnitude': 0.12583613395690918, 'cosine_with_motion': -0.8374699354171753, 'motion_component': -0.1053839772939682, 'motion_component_percent': 83.74699354171753}, {'resid': 1313, 'atom': 'C23', 'charge': -0.18000000715255737, 'distance': 22.057443618774414, 'force': [0.1082642525434494, 0.04371555149555206, -0.038140784949064255], 'magnitude': 0.12282881140708923, 'cosine_with_motion': -0.8868417143821716, 'motion_component': -0.10892971605062485, 'motion_component_percent': 88.68417143821716}, {'resid': 1313, 'atom': 'C24', 'charge': -0.18000000715255737, 'distance': 21.280075073242188, 'force': [0.11705315113067627, 0.05073871091008186, -0.03375423699617386], 'magnitude': 0.13196668028831482, 'cosine_with_motion': -0.8639797568321228, 'motion_component': -0.11401654034852982, 'motion_component_percent': 86.39797568321228}, {'resid': 1313, 'atom': 'C25', 'charge': -0.15000000596046448, 'distance': 20.9041805267334, 'force': [0.10448335856199265, 0.03833189979195595, -0.024523675441741943], 'magnitude': 0.11396279186010361, 'cosine_with_motion': -0.8343191742897034, 'motion_component': -0.09508134424686432, 'motion_component_percent': 83.43191742897034}, {'resid': 1313, 'atom': 'C26', 'charge': -0.15000000596046448, 'distance': 21.6762752532959, 'force': [0.0989554226398468, 0.033233970403671265, -0.018356379121541977], 'magnitude': 0.10598881542682648, 'cosine_with_motion': -0.8061639666557312, 'motion_component': -0.0854443609714508, 'motion_component_percent': 80.61639666557312}, {'resid': 1313, 'atom': 'C27', 'charge': -0.18000000715255737, 'distance': 23.086471557617188, 'force': [0.10429465025663376, 0.03709140792489052, -0.017845582216978073], 'magnitude': 0.11212319135665894, 'cosine_with_motion': -0.8013998866081238, 'motion_component': -0.08985551446676254, 'motion_component_percent': 80.13998866081238}, {'resid': 1313, 'atom': 'C28', 'charge': -0.15000000596046448, 'distance': 23.355907440185547, 'force': [0.08557257801294327, 0.030596930533647537, -0.008689801208674908], 'magnitude': 0.09129266440868378, 'cosine_with_motion': -0.7632946968078613, 'motion_component': -0.06968320906162262, 'motion_component_percent': 76.32946968078613}, {'resid': 1313, 'atom': 'C29', 'charge': -0.15000000596046448, 'distance': 24.276840209960938, 'force': [0.08021902292966843, 0.025942731648683548, -0.005634661763906479], 'magnitude': 0.08449772745370865, 'cosine_with_motion': -0.7394149899482727, 'motion_component': -0.06247888505458832, 'motion_component_percent': 73.94149899482727}, {'resid': 1313, 'atom': 'C3', 'charge': 0.06000000238418579, 'distance': 30.350936889648438, 'force': [-0.01595482788980007, -0.00958431325852871, 0.011009149253368378], 'magnitude': 0.021624453365802765, 'cosine_with_motion': 0.9732761383056641, 'motion_component': 0.021046563982963562, 'motion_component_percent': 97.3276138305664}, {'resid': 1313, 'atom': 'C31', 'charge': 0.6299999952316284, 'distance': 27.743694305419922, 'force': [-0.2386857122182846, -0.11175912618637085, 0.06618499010801315], 'magnitude': 0.2717377841472626, 'cosine_with_motion': 0.8612471222877502, 'motion_component': 0.23403339087963104, 'motion_component_percent': 86.12471222877502}, {'resid': 1313, 'atom': 'C310', 'charge': -0.18000000715255737, 'distance': 25.633176803588867, 'force': [0.07815276086330414, 0.04540754109621048, 0.0101153664290905], 'magnitude': 0.09095063805580139, 'cosine_with_motion': -0.6406019330024719, 'motion_component': -0.058263152837753296, 'motion_component_percent': 64.06019330024719}, {'resid': 1313, 'atom': 'C311', 'charge': -0.18000000715255737, 'distance': 25.352142333984375, 'force': [0.07980728149414062, 0.04505106806755066, 0.0156891867518425], 'magnitude': 0.09297823160886765, 'cosine_with_motion': -0.5943602919578552, 'motion_component': -0.05526256933808327, 'motion_component_percent': 59.43602919578552}, {'resid': 1313, 'atom': 'C312', 'charge': -0.18000000715255737, 'distance': 23.819875717163086, 'force': [0.09041812270879745, 0.05049477145075798, 0.019188668578863144], 'magnitude': 0.10532504320144653, 'cosine_with_motion': -0.5830795168876648, 'motion_component': -0.06141287460923195, 'motion_component_percent': 58.30795168876648}, {'resid': 1313, 'atom': 'C313', 'charge': -0.18000000715255737, 'distance': 23.52074432373047, 'force': [0.09212464839220047, 0.04989314451813698, 0.026311125606298447], 'magnitude': 0.1080210730433464, 'cosine_with_motion': -0.530221164226532, 'motion_component': -0.05727505683898926, 'motion_component_percent': 53.0221164226532}, {'resid': 1313, 'atom': 'C314', 'charge': -0.18000000715255737, 'distance': 24.262231826782227, 'force': [0.08352735638618469, 0.050089456140995026, 0.028642937541007996], 'magnitude': 0.10151941329240799, 'cosine_with_motion': -0.49836283922195435, 'motion_component': -0.050593502819538116, 'motion_component_percent': 49.836283922195435}, {'resid': 1313, 'atom': 'C315', 'charge': -0.18000000715255737, 'distance': 23.7382755279541, 'force': [0.08397702872753143, 0.05794347822666168, 0.02893265150487423], 'magnitude': 0.10605039447546005, 'cosine_with_motion': -0.5077608227729797, 'motion_component': -0.053848233073949814, 'motion_component_percent': 50.776082277297974}, {'resid': 1313, 'atom': 'C316', 'charge': -0.18000000715255737, 'distance': 24.59172821044922, 'force': [0.07493862509727478, 0.05702672898769379, 0.029949825257062912], 'magnitude': 0.09881719201803207, 'cosine_with_motion': -0.4792526066303253, 'motion_component': -0.047358397394418716, 'motion_component_percent': 47.92526066303253}, {'resid': 1313, 'atom': 'C317', 'charge': -0.18000000715255737, 'distance': 25.973957061767578, 'force': [0.06715332716703415, 0.05216098576784134, 0.024819981306791306], 'magnitude': 0.08857972919940948, 'cosine_with_motion': -0.4996738135814667, 'motion_component': -0.04426097124814987, 'motion_component_percent': 49.96738135814667}, {'resid': 1313, 'atom': 'C318', 'charge': -0.27000001072883606, 'distance': 26.061813354492188, 'force': [0.09911034256219864, 0.0816081091761589, 0.03057333268225193], 'magnitude': 0.13197526335716248, 'cosine_with_motion': -0.5408677458763123, 'motion_component': -0.07138116657733917, 'motion_component_percent': 54.086774587631226}, {'resid': 1313, 'atom': 'C32', 'charge': -0.08000000566244125, 'distance': 27.460922241210938, 'force': [0.03170037642121315, 0.013735642656683922, -0.006849483586847782], 'magnitude': 0.035220690071582794, 'cosine_with_motion': -0.8317216038703918, 'motion_component': -0.029293809086084366, 'motion_component_percent': 83.17216038703918}, {'resid': 1313, 'atom': 'C33', 'charge': -0.18000000715255737, 'distance': 28.56014060974121, 'force': [0.06589315086603165, 0.029949842020869255, -0.011344426311552525], 'magnitude': 0.07326388359069824, 'cosine_with_motion': -0.8116008639335632, 'motion_component': -0.05946103110909462, 'motion_component_percent': 81.16008639335632}, {'resid': 1313, 'atom': 'C34', 'charge': -0.18000000715255737, 'distance': 28.655336380004883, 'force': [0.06685290485620499, 0.027629580348730087, -0.007994964718818665], 'magnitude': 0.07277791202068329, 'cosine_with_motion': -0.7802243828773499, 'motion_component': -0.056783102452754974, 'motion_component_percent': 78.02243828773499}, {'resid': 1313, 'atom': 'C35', 'charge': -0.18000000715255737, 'distance': 27.44031524658203, 'force': [0.07309518754482269, 0.030347511172294617, -0.005918057635426521], 'magnitude': 0.07936561852693558, 'cosine_with_motion': -0.7584167718887329, 'motion_component': -0.06019221618771553, 'motion_component_percent': 75.84167718887329}, {'resid': 1313, 'atom': 'C36', 'charge': -0.18000000715255737, 'distance': 27.088674545288086, 'force': [0.07335864007472992, 0.03505804389715195, -0.00467287190258503], 'magnitude': 0.08143950253725052, 'cosine_with_motion': -0.7539457082748413, 'motion_component': -0.06140096113085747, 'motion_component_percent': 75.39457082748413}, {'resid': 1313, 'atom': 'C37', 'charge': -0.18000000715255737, 'distance': 26.33851432800293, 'force': [0.07788114994764328, 0.03680691868066788, -0.0008176924893632531], 'magnitude': 0.0861445963382721, 'cosine_with_motion': -0.7215666770935059, 'motion_component': -0.06215907260775566, 'motion_component_percent': 72.15666770935059}, {'resid': 1313, 'atom': 'C38', 'charge': -0.18000000715255737, 'distance': 26.236770629882812, 'force': [0.07655657082796097, 0.04088493809103966, 0.002046407898887992], 'magnitude': 0.0868140235543251, 'cosine_with_motion': -0.7031381130218506, 'motion_component': -0.06104224920272827, 'motion_component_percent': 70.31381130218506}, {'resid': 1313, 'atom': 'C39', 'charge': -0.18000000715255737, 'distance': 25.605525970458984, 'force': [0.08064118772745132, 0.041913531720638275, 0.0069325692020356655], 'magnitude': 0.09114716947078705, 'cosine_with_motion': -0.6641369462013245, 'motion_component': -0.06053420528769493, 'motion_component_percent': 66.41369462013245}, {'resid': 1313, 'atom': 'C4', 'charge': 0.08000000566244125, 'distance': 30.026735305786133, 'force': [-0.02081386372447014, -0.013145255856215954, 0.01618003286421299], 'magnitude': 0.029458582401275635, 'cosine_with_motion': 0.9834693074226379, 'motion_component': 0.028971612453460693, 'motion_component_percent': 98.3469307422638}, {'resid': 1313, 'atom': 'C5', 'charge': 0.08000000566244125, 'distance': 28.479055404663086, 'force': [-0.02297375351190567, -0.01448468491435051, 0.018297363072633743], 'magnitude': 0.032747410237789154, 'cosine_with_motion': 0.9854391813278198, 'motion_component': 0.032270580530166626, 'motion_component_percent': 98.54391813278198}, {'resid': 1313, 'atom': 'C6', 'charge': 0.06000000238418579, 'distance': 27.64038848876953, 'force': [-0.01839340291917324, -0.012371918186545372, 0.013727754354476929], 'magnitude': 0.026073604822158813, 'cosine_with_motion': 0.9785714149475098, 'motion_component': 0.025514883920550346, 'motion_component_percent': 97.85714149475098}, {'resid': 1313, 'atom': 'H1', 'charge': 0.12000000476837158, 'distance': 27.57379722595215, 'force': [-0.039735376834869385, -0.02319786138832569, 0.025072989985346794], 'magnitude': 0.05239938944578171, 'cosine_with_motion': 0.9642294049263, 'motion_component': 0.050525031983852386, 'motion_component_percent': 96.42294049263}, {'resid': 1313, 'atom': 'H10R', 'charge': 0.09000000357627869, 'distance': 25.50831413269043, 'force': [-0.04384318366646767, -0.01238551177084446, 0.005759193561971188], 'magnitude': 0.045921605080366135, 'cosine_with_motion': 0.7680432200431824, 'motion_component': 0.03526977822184563, 'motion_component_percent': 76.80432200431824}, {'resid': 1313, 'atom': 'H10S', 'charge': 0.09000000357627869, 'distance': 25.93306541442871, 'force': [-0.04283418878912926, -0.011464374139904976, 0.0027918892446905375], 'magnitude': 0.044429656118154526, 'cosine_with_motion': 0.7257172465324402, 'motion_component': 0.03224336728453636, 'motion_component_percent': 72.57172465324402}, {'resid': 1313, 'atom': 'H10X', 'charge': 0.09000000357627869, 'distance': 24.872831344604492, 'force': [-0.0408053882420063, -0.025368912145495415, -0.004903704859316349], 'magnitude': 0.04829811304807663, 'cosine_with_motion': 0.6491925120353699, 'motion_component': 0.03135477378964424, 'motion_component_percent': 64.91925120353699}, {'resid': 1313, 'atom': 'H10Y', 'charge': 0.09000000357627869, 'distance': 26.584863662719727, 'force': [-0.0359291136264801, -0.02183980867266655, -0.00441915774717927], 'magnitude': 0.042277742177248, 'cosine_with_motion': 0.646582841873169, 'motion_component': 0.027336062863469124, 'motion_component_percent': 64.6582841873169}, {'resid': 1313, 'atom': 'H111', 'charge': 0.15000000596046448, 'distance': 23.780059814453125, 'force': [-0.08617128431797028, -0.01762230135500431, 0.00440596416592598], 'magnitude': 0.0880650207400322, 'cosine_with_motion': 0.7020154595375061, 'motion_component': 0.061823006719350815, 'motion_component_percent': 70.20154595375061}, {'resid': 1313, 'atom': 'H11A', 'charge': 0.09000000357627869, 'distance': 28.206741333007812, 'force': [-0.03054092265665531, -0.01670045405626297, 0.014098591171205044], 'magnitude': 0.03755560517311096, 'cosine_with_motion': 0.9267662763595581, 'motion_component': 0.03480526804924011, 'motion_component_percent': 92.67662763595581}, {'resid': 1313, 'atom': 'H11B', 'charge': 0.09000000357627869, 'distance': 26.9195499420166, 'force': [-0.033400338143110275, -0.017198067158460617, 0.016994256526231766], 'magnitude': 0.04123300686478615, 'cosine_with_motion': 0.9390354752540588, 'motion_component': 0.03871925547719002, 'motion_component_percent': 93.90354752540588}, {'resid': 1313, 'atom': 'H11X', 'charge': 0.09000000357627869, 'distance': 25.913667678833008, 'force': [-0.03741530701518059, -0.022495651617646217, -0.008599498309195042], 'magnitude': 0.044496189802885056, 'cosine_with_motion': 0.5754884481430054, 'motion_component': 0.025607042014598846, 'motion_component_percent': 57.54884481430054}, {'resid': 1313, 'atom': 'H11Y', 'charge': 0.09000000357627869, 'distance': 25.818937301635742, 'force': [-0.0391695499420166, -0.02022446319460869, -0.008114578202366829], 'magnitude': 0.044823307543992996, 'cosine_with_motion': 0.581657886505127, 'motion_component': 0.026071829721331596, 'motion_component_percent': 58.165788650512695}, {'resid': 1313, 'atom': 'H12', 'charge': 0.09000000357627869, 'distance': 26.99422836303711, 'force': [-0.03497808054089546, -0.01624063029885292, 0.013935613445937634], 'magnitude': 0.04100519046187401, 'cosine_with_motion': 0.9063506722450256, 'motion_component': 0.0371650829911232, 'motion_component_percent': 90.63506722450256}, {'resid': 1313, 'atom': 'H121', 'charge': 0.15000000596046448, 'distance': 23.742795944213867, 'force': [-0.0867665708065033, -0.011929657310247421, 0.011554078198969364], 'magnitude': 0.08834167569875717, 'cosine_with_motion': 0.7335736155509949, 'motion_component': 0.06480512022972107, 'motion_component_percent': 73.35736155509949}, {'resid': 1313, 'atom': 'H12X', 'charge': 0.09000000357627869, 'distance': 23.2597713470459, 'force': [-0.048462845385074615, -0.024974098429083824, -0.008827529847621918], 'magnitude': 0.05522932484745979, 'cosine_with_motion': 0.5988595485687256, 'motion_component': 0.03307460993528366, 'motion_component_percent': 59.88595485687256}, {'resid': 1313, 'atom': 'H12Y', 'charge': 0.09000000357627869, 'distance': 23.392349243164062, 'force': [-0.04592472314834595, -0.028116824105381966, -0.009059657342731953], 'magnitude': 0.054605066776275635, 'cosine_with_motion': 0.5982607007026672, 'motion_component': 0.032668065279722214, 'motion_component_percent': 59.826070070266724}, {'resid': 1313, 'atom': 'H13A', 'charge': 0.09000000357627869, 'distance': 27.925752639770508, 'force': [-0.031761571764945984, -0.018167991191148758, 0.01136570144444704], 'magnitude': 0.038315173238515854, 'cosine_with_motion': 0.893782913684845, 'motion_component': 0.03424544632434845, 'motion_component_percent': 89.3782913684845}, {'resid': 1313, 'atom': 'H13B', 'charge': 0.09000000357627869, 'distance': 26.280336380004883, 'force': [-0.035424139350652695, -0.0212792307138443, 0.012807426042854786], 'magnitude': 0.043263211846351624, 'cosine_with_motion': 0.8944565653800964, 'motion_component': 0.03869706392288208, 'motion_component_percent': 89.44565653800964}, {'resid': 1313, 'atom': 'H13R', 'charge': 0.09000000357627869, 'distance': 25.559751510620117, 'force': [-0.04444948211312294, -0.006298224441707134, 0.00874333642423153], 'magnitude': 0.04573696479201317, 'cosine_with_motion': 0.770146906375885, 'motion_component': 0.03522418066859245, 'motion_component_percent': 77.0146906375885}, {'resid': 1313, 'atom': 'H13S', 'charge': 0.09000000357627869, 'distance': 25.929399490356445, 'force': [-0.042807649821043015, -0.009044568054378033, 0.007798163685947657], 'magnitude': 0.04444221407175064, 'cosine_with_motion': 0.7808287143707275, 'motion_component': 0.03470175713300705, 'motion_component_percent': 78.08287143707275}, {'resid': 1313, 'atom': 'H13X', 'charge': 0.09000000357627869, 'distance': 23.962055206298828, 'force': [-0.04522915184497833, -0.022081593051552773, -0.013222278095781803], 'magnitude': 0.05203942209482193, 'cosine_with_motion': 0.5174983739852905, 'motion_component': 0.026930315420031548, 'motion_component_percent': 51.74983739852905}, {'resid': 1313, 'atom': 'H13Y', 'charge': 0.09000000357627869, 'distance': 22.491479873657227, 'force': [-0.050232551991939545, -0.027038488537073135, -0.015313912183046341], 'magnitude': 0.059066955000162125, 'cosine_with_motion': 0.5162773728370667, 'motion_component': 0.0304949339479208, 'motion_component_percent': 51.627737283706665}, {'resid': 1313, 'atom': 'H141', 'charge': 0.15000000596046448, 'distance': 23.247333526611328, 'force': [-0.08801519870758057, -0.018781431019306183, 0.019792063161730766], 'magnitude': 0.09214739501476288, 'cosine_with_motion': 0.8032620549201965, 'motion_component': 0.07401850819587708, 'motion_component_percent': 80.32620549201965}, {'resid': 1313, 'atom': 'H14X', 'charge': 0.09000000357627869, 'distance': 24.296720504760742, 'force': [-0.04140184447169304, -0.02408088557422161, -0.01636911928653717], 'magnitude': 0.05061570927500725, 'cosine_with_motion': 0.45984968543052673, 'motion_component': 0.023275617510080338, 'motion_component_percent': 45.98496854305267}, {'resid': 1313, 'atom': 'H14Y', 'charge': 0.09000000357627869, 'distance': 25.319988250732422, 'force': [-0.03844614326953888, -0.023120282217860222, -0.012632647529244423], 'magnitude': 0.04660726338624954, 'cosine_with_motion': 0.5083779692649841, 'motion_component': 0.023694105446338654, 'motion_component_percent': 50.83779692649841}, {'resid': 1313, 'atom': 'H151', 'charge': 0.15000000596046448, 'distance': 23.890975952148438, 'force': [-0.08068130910396576, -0.020908605307340622, 0.025802792981266975], 'magnitude': 0.08724922686815262, 'cosine_with_motion': 0.8554304838180542, 'motion_component': 0.07463564723730087, 'motion_component_percent': 85.54304838180542}, {'resid': 1313, 'atom': 'H15X', 'charge': 0.09000000357627869, 'distance': 22.740198135375977, 'force': [-0.045204512774944305, -0.031882818788290024, -0.01669703610241413], 'magnitude': 0.05778194218873978, 'cosine_with_motion': 0.49309536814689636, 'motion_component': 0.02849200740456581, 'motion_component_percent': 49.309536814689636}, {'resid': 1313, 'atom': 'H15Y', 'charge': 0.09000000357627869, 'distance': 23.719934463500977, 'force': [-0.04237094521522522, -0.029628269374370575, -0.012134508229792118], 'magnitude': 0.05310722813010216, 'cosine_with_motion': 0.5466131567955017, 'motion_component': 0.029029108583927155, 'motion_component_percent': 54.66131567955017}, {'resid': 1313, 'atom': 'H16R', 'charge': 0.09000000357627869, 'distance': 26.72824478149414, 'force': [-0.03931371122598648, -0.009286848828196526, 0.010841937735676765], 'magnitude': 0.04182536527514458, 'cosine_with_motion': 0.8322083950042725, 'motion_component': 0.03480742126703262, 'motion_component_percent': 83.22083950042725}, {'resid': 1313, 'atom': 'H16S', 'charge': 0.09000000357627869, 'distance': 26.319955825805664, 'force': [-0.03954117000102997, -0.011580022051930428, 0.012761666439473629], 'magnitude': 0.04313306510448456, 'cosine_with_motion': 0.862420916557312, 'motion_component': 0.037198856472969055, 'motion_component_percent': 86.2420916557312}, {'resid': 1313, 'atom': 'H16X', 'charge': 0.09000000357627869, 'distance': 24.833810806274414, 'force': [-0.036432985216379166, -0.027262812480330467, -0.01663670688867569], 'magnitude': 0.048450008034706116, 'cosine_with_motion': 0.44177424907684326, 'motion_component': 0.02140396647155285, 'motion_component_percent': 44.177424907684326}, {'resid': 1313, 'atom': 'H16Y', 'charge': 0.09000000357627869, 'distance': 23.93084144592285, 'force': [-0.03833596035838127, -0.03149028867483139, -0.016154693439602852], 'magnitude': 0.052175264805555344, 'cosine_with_motion': 0.47132405638694763, 'motion_component': 0.024591457098722458, 'motion_component_percent': 47.13240563869476}, {'resid': 1313, 'atom': 'H17R', 'charge': 0.09000000357627869, 'distance': 27.533035278320312, 'force': [-0.03620672598481178, -0.008146679028868675, 0.01327873207628727], 'magnitude': 0.03941598907113075, 'cosine_with_motion': 0.8667881488800049, 'motion_component': 0.034165311604738235, 'motion_component_percent': 86.67881488800049}, {'resid': 1313, 'atom': 'H17S', 'charge': 0.09000000357627869, 'distance': 26.234725952148438, 'force': [-0.0392143577337265, -0.009331213310360909, 0.01612197980284691], 'magnitude': 0.04341377317905426, 'cosine_with_motion': 0.8847541809082031, 'motion_component': 0.03841051831841469, 'motion_component_percent': 88.47541809082031}, {'resid': 1313, 'atom': 'H17X', 'charge': 0.09000000357627869, 'distance': 26.714454650878906, 'force': [-0.03102816827595234, -0.02507045678794384, -0.012716165743768215], 'magnitude': 0.041868556290864944, 'cosine_with_motion': 0.47726574540138245, 'motion_component': 0.01998242735862732, 'motion_component_percent': 47.726574540138245}, {'resid': 1313, 'atom': 'H17Y', 'charge': 0.09000000357627869, 'distance': 26.38319206237793, 'force': [-0.0335984006524086, -0.024041427299380302, -0.011655283160507679], 'magnitude': 0.042926546186208725, 'cosine_with_motion': 0.5087178349494934, 'motion_component': 0.021837500855326653, 'motion_component_percent': 50.87178349494934}, {'resid': 1313, 'atom': 'H18R', 'charge': 0.09000000357627869, 'distance': 25.2016544342041, 'force': [-0.043749891221523285, -0.00653818529099226, 0.016016347333788872], 'magnitude': 0.047045979648828506, 'cosine_with_motion': 0.848587155342102, 'motion_component': 0.03992261365056038, 'motion_component_percent': 84.8587155342102}, {'resid': 1313, 'atom': 'H18S', 'charge': 0.09000000357627869, 'distance': 26.64111</t>
         </is>
       </c>
     </row>
@@ -499,7 +499,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>{138: {'frame': 138, 'motion_vector': [2.379444122314453, 2.9537811279296875, 5.88848876953125], 'ionic_force': [2.5273286402225494, -0.9714137520641088, -6.800560832023621], 'ionic_force_magnitude': 7.31974469250412, 'radial_force': 2.707588361141411, 'axial_force': -6.800560832023621, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [6.405253291130066, -6.760278880596161, 5.933797597885132], 'asn_force_magnitude': 11.042580957350252, 'residue_force': [6.405253291130066, -6.760278880596161, 5.933797597885132], 'residue_force_magnitude': 11.042580957350252, 'total_force': [8.932581931352615, -7.73169263266027, -0.8667632341384888], 'total_force_magnitude': 11.845732118797661, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': 0.3906295051309457, 'cosine_residue_motion': 0.3906295051309457, 'cosine_ionic_motion': -0.7197329213971744, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': 4.313557934738133, 'motion_component_residue': 4.313557934738133, 'motion_component_ionic': -5.268261231417452, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 39.06295051309457, 'motion_component_percent_residue': 39.06295051309457, 'motion_component_percent_ionic': 71.97329213971744, 'ionic_contributions': [{'ion_id': 2397, 'distance': 12.146998405456543, 'force': [0.2803648114204407, 0.018578680232167244, -2.2324788570404053], 'magnitude': 2.250091552734375, 'cosine_ionic_motion': -0.7882996797561646, 'motion_component_ionic': -1.7737464904785156, 'motion_component_percent_ionic': 78.82996797561646}, {'ion_id': 2399, 'distance': 13.916149139404297, 'force': [-0.06216016411781311, -0.06396990269422531, 1.7120298147201538], 'magnitude': 1.714351773262024, 'cosine_ionic_motion': 0.811498761177063, 'motion_component_ionic': 1.3911943435668945, 'motion_component_percent_ionic': 81.1498761177063}, {'ion_id': 2400, 'distance': 7.01064395904541, 'force': [2.309123992919922, -0.9260225296020508, -6.280111789703369], 'magnitude': 6.7549519538879395, 'cosine_ionic_motion': -0.7232781052589417, 'motion_component_ionic': -4.885708808898926, 'motion_component_percent_ionic': 72.32781052589417}], 'glu_contributions': [], 'asn_contributions': [{'resid': 458, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 5.213967323303223, 'force': [5.881892204284668, -0.6080090403556824, 4.347905158996582], 'magnitude': 7.339660167694092, 'cosine_with_motion': 0.7353169322013855, 'motion_component': 5.396976470947266, 'motion_component_percent': 73.53169322013855}, {'resid': 1114, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 5.594605922698975, 'force': [0.523361086845398, -6.1522698402404785, 1.5858924388885498], 'magnitude': 6.374903202056885, 'cosine_with_motion': -0.16995061933994293, 'motion_component': -1.0834187269210815, 'motion_component_percent': 16.995061933994293}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': -0.08059470593331476, 'motion_component_pip2': -0.9547032966793192, 'motion_component_percent_pip2': 8.059470593331476}, 139: {'frame': 139, 'motion_vector': [-0.94256591796875, -2.3760528564453125, -1.0450439453125], 'ionic_force': [7.643194556236267, 7.880148112773895, -2.429677963256836], 'ionic_force_magnitude': 11.243597836496535, 'radial_force': 10.97793957460751, 'axial_force': -2.429677963256836, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-1.1356549263000488, -2.2137036323547363, -2.061790406703949], 'asn_force_magnitude': 3.231280793231464, 'residue_force': [-1.1356549263000488, -2.2137036323547363, -2.061790406703949], 'residue_force_magnitude': 3.231280793231464, 'total_force': [6.507539629936218, 5.666444480419159, -4.491468369960785], 'total_force_magnitude': 9.72779282279497, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': 0.9508722310430182, 'cosine_residue_motion': 0.9508722310430182, 'cosine_ionic_motion': -0.7532657723390456, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': 3.072535176986456, 'motion_component_residue': 3.072535176986456, 'motion_component_ionic': -8.469417408178185, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 95.08722310430183, 'motion_component_percent_residue': 95.08722310430183, 'motion_component_percent_ionic': 75.32657723390456, 'ionic_contributions': [{'ion_id': 2276, 'distance': 11.044848442077637, 'force': [1.0126570463180542, 0.7629305720329285, -2.408188819885254], 'magnitude': 2.7215640544891357, 'cosine_ionic_motion': -0.03334284946322441, 'motion_component_ionic': -0.09074470400810242, 'motion_component_percent_ionic': 3.334284946322441}, {'ion_id': 2397, 'distance': 7.7002644538879395, 'force': [3.139317274093628, 2.1036877632141113, -4.131627559661865], 'magnitude': 5.599210739135742, 'cosine_ionic_motion': -0.23539213836193085, 'motion_component_ionic': -1.3180102109909058, 'motion_component_percent_ionic': 23.539213836193085}, {'ion_id': 2400, 'distance': 6.714821815490723, 'force': [3.491220235824585, 5.0135297775268555, 4.110138416290283], 'magnitude': 7.3632426261901855, 'cosine_ionic_motion': -0.9589066505432129, 'motion_component_ionic': -7.060662269592285, 'motion_component_percent_ionic': 95.89066505432129}], 'glu_contributions': [], 'asn_contributions': [{'resid': 458, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 4.5718607902526855, 'force': [-7.33221435546875, 7.092769145965576, 5.00177001953125], 'magnitude': 11.361621856689453, 'cosine_with_motion': -0.4834556579589844, 'motion_component': -5.49284029006958, 'motion_component_percent': 48.34556579589844}, {'resid': 458, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 4.493603706359863, 'force': [4.220494747161865, -6.621179580688477, -5.999292850494385], 'magnitude': 9.881503105163574, 'cosine_with_motion': 0.6604921221733093, 'motion_component': 6.526655197143555, 'motion_component_percent': 66.04921221733093}, {'resid': 458, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 4.668283939361572, 'force': [8.850408554077148, -10.322657585144043, -2.574371099472046], 'magnitude': 13.838871955871582, 'cosine_with_motion': 0.4939039945602417, 'motion_component': 6.835073947906494, 'motion_component_percent': 49.39039945602417}, {'resid': 458, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 4.994819164276123, 'force': [-2.684593439102173, 4.7632060050964355, 0.7774097919464111], 'magnitude': 5.52263879776001, 'cosine_with_motion': -0.6294416189193726, 'motion_component': -3.4761786460876465, 'motion_component_percent': 62.944161891937256}, {'resid': 458, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 5.200928211212158, 'force': [-3.80865216255188, 3.3570291996002197, 0.41139036417007446], 'magnitude': 5.0935959815979, 'cosine_with_motion': -0.34241536259651184, 'motion_component': -1.744125485420227, 'motion_component_percent': 34.241536259651184}, {'resid': 786, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 5.1929216384887695, 'force': [-5.307845115661621, 6.904155254364014, -7.016988277435303], 'magnitude': 11.183858871459961, 'cosine_with_motion': -0.13173407316207886, 'motion_component': -1.4732953310012817, 'motion_component_percent': 13.173407316207886}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 4.621432781219482, 'force': [2.472900629043579, -3.488844633102417, 4.830036640167236], 'magnitude': 6.451087474822998, 'cosine_with_motion': 0.051148250699043274, 'motion_component': 0.3299618363380432, 'motion_component_percent': 5.114825069904327}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 5.125382423400879, 'force': [2.4538462162017822, -3.898181438446045, 2.5082550048828125], 'magnitude': 5.244856834411621, 'cosine_with_motion': 0.29882296919822693, 'motion_component': 1.5672836303710938, 'motion_component_percent': 29.882296919822693}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': -0.5547900052461342, 'motion_component_pip2': -5.396882231191729, 'motion_component_percent_pip2': 55.47900052461342}, 140: {'frame': 140, 'motion_vector': [-2.507404327392578, -0.6652908325195312, -0.67144775390625], 'ionic_force': [4.728224515914917, 0.6357127726078033, -0.928431510925293], 'ionic_force_magnitude': 4.860269835372782, 'radial_force': 4.770769099647933, 'axial_force': -0.928431510925293, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [9.294816076755524, -3.6275479793548584, -6.708367586135864], 'asn_force_magnitude': 12.023098848215163, 'residue_force': [9.294816076755524, -3.6275479793548584, -6.708367586135864], 'residue_force_magnitude': 12.023098848215163, 'total_force': [14.02304059267044, -2.991835206747055, -7.636799097061157], 'total_force_magnitude': 16.24553618126802, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': -0.5086695564331464, 'cosine_residue_motion': -0.5086695564331464, 'cosine_ionic_motion': -0.8949067056997984, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': -6.11578435807348, 'motion_component_residue': -6.11578435807348, 'motion_component_ionic': -4.349488067185558, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 50.86695564331464, 'motion_component_percent_residue': 50.86695564331464, 'motion_component_percent_ionic': 89.49067056997984, 'ionic_contributions': [{'ion_id': 2276, 'distance': 11.146353721618652, 'force': [0.6672391891479492, 0.15043987333774567, -2.5832009315490723], 'magnitude': 2.6722214221954346, 'cosine_ionic_motion': -0.005396207328885794, 'motion_component_ionic': -0.014419861137866974, 'motion_component_percent_ionic': 0.5396207328885794}, {'ion_id': 2397, 'distance': 7.751501083374023, 'force': [2.000823497772217, 0.6351746320724487, -5.111134052276611], 'magnitude': 5.525434970855713, 'cosine_ionic_motion': -0.1355908215045929, 'motion_component_ionic': -0.7491982579231262, 'motion_component_percent_ionic': 13.55908215045929}, {'ion_id': 2400, 'distance': 6.8506317138671875, 'force': [2.060161828994751, -0.14990173280239105, 6.765903472900391], 'magnitude': 7.074191570281982, 'cosine_ionic_motion': -0.5068946480751038, 'motion_component_ionic': -3.5858700275421143, 'motion_component_percent_ionic': 50.689464807510376}], 'glu_contributions': [], 'asn_contributions': [{'resid': 458, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 3.7230935096740723, 'force': [-16.91469383239746, 1.554067611694336, 2.2354938983917236], 'magnitude': 17.132408142089844, 'cosine_with_motion': 0.868613064289093, 'motion_component': 14.881433486938477, 'motion_component_percent': 86.8613064289093}, {'resid': 458, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 2.827564001083374, 'force': [22.825021743774414, -2.897184133529663, -9.667628288269043], 'magnitude': 24.956727981567383, 'cosine_with_motion': -0.7299071550369263, 'motion_component': -18.216094970703125, 'motion_component_percent': 72.99071550369263}, {'resid': 458, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 3.952399492263794, 'force': [18.410274505615234, -4.701493740081787, 3.417818307876587], 'magnitude': 19.306053161621094, 'cosine_with_motion': -0.8762027621269226, 'motion_component': -16.916017532348633, 'motion_component_percent': 87.62027621269226}, {'resid': 458, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 3.4043173789978027, 'force': [-10.2164888381958, 5.089540958404541, -3.3250162601470947], 'magnitude': 11.888474464416504, 'cosine_with_motion': 0.7679142951965332, 'motion_component': 9.129329681396484, 'motion_component_percent': 76.79142951965332}, {'resid': 458, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 4.928169250488281, 'force': [-5.378725528717041, 1.2421607971191406, -1.3075159788131714], 'magnitude': 5.673028469085693, 'cosine_with_motion': 0.8905673027038574, 'motion_component': 5.052213668823242, 'motion_component_percent': 89.05673027038574}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 5.5925140380859375, 'force': [0.569428026676178, -3.914639472961426, 1.9384807348251343], 'magnitude': 4.405264854431152, 'cosine_with_motion': -0.010589201003313065, 'motion_component': -0.046648234128952026, 'motion_component_percent': 1.0589201003313065}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': -0.6441937224162575, 'motion_component_pip2': -10.465272425259037, 'motion_component_percent_pip2': 64.41937224162575}, 141: {'frame': 141, 'motion_vector': [-0.9842605590820312, 0.5642433166503906, -4.0995635986328125], 'ionic_force': [3.7223656959831715, -16.474775947630405, -14.750489234924316], 'ionic_force_magnitude': 22.424343503631757, 'radial_force': 16.89006361442294, 'axial_force': -14.750489234924316, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [2.2445865869522095, 4.586579918861389, -4.961560860276222], 'asn_force_magnitude': 7.1198293847994165, 'residue_force': [2.2445865869522095, 4.586579918861389, -4.961560860276222], 'residue_force_magnitude': 7.1198293847994165, 'total_force': [5.966952282935381, -11.888196028769016, -19.71205009520054], 'total_force_magnitude': 23.780215375832128, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': 0.6841251935299616, 'cosine_residue_motion': 0.6841251935299616, 'cosine_ionic_motion': 0.49809537798298614, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': 4.870854655776208, 'motion_component_residue': 4.870854655776208, 'motion_component_ionic': 11.16946185346178, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 68.41251935299616, 'motion_component_percent_residue': 68.41251935299616, 'motion_component_percent_ionic': 49.809537798298614, 'ionic_contributions': [{'ion_id': 2276, 'distance': 11.13986587524414, 'force': [0.030413765460252762, 0.03557800501585007, -2.6749253273010254], 'magnitude': 2.6753346920013428, 'cosine_ionic_motion': 0.9627609848976135, 'motion_component_ionic': 2.5757079124450684, 'motion_component_percent_ionic': 96.27609848976135}, {'ion_id': 2397, 'distance': 7.386458396911621, 'force': [0.3289110064506531, 0.3385210931301117, -6.066736698150635], 'magnitude': 6.08506965637207, 'cosine_ionic_motion': 0.9557434916496277, 'motion_component_ionic': 5.815765857696533, 'motion_component_percent_ionic': 95.57434916496277}, {'ion_id': 2400, 'distance': 4.270841598510742, 'force': [3.3630409240722656, -16.848875045776367, -6.008827209472656], 'magnitude': 18.2016658782959, 'cosine_ionic_motion': 0.15262272953987122, 'motion_component_ionic': 2.7779879570007324, 'motion_component_percent_ionic': 15.262272953987122}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 5.395811080932617, 'force': [7.916512966156006, -1.714101791381836, 0.9601770043373108], 'magnitude': 8.156669616699219, 'cosine_with_motion': -0.36590734124183655, 'motion_component': -2.9845852851867676, 'motion_component_percent': 36.590734124183655}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 4.219575881958008, 'force': [-10.825837135314941, 2.3067305088043213, -1.7517870664596558], 'magnitude': 11.20662784576416, 'cosine_with_motion': 0.4014878273010254, 'motion_component': 4.499324798583984, 'motion_component_percent': 40.14878273010254}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 5.692919731140137, 'force': [3.5841763019561768, -2.2819156646728516, 0.1400630623102188], 'magnitude': 4.251244068145752, 'cosine_with_motion': -0.2980380952358246, 'motion_component': -1.2670326232910156, 'motion_component_percent': 29.80380952358246}, {'resid': 458, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 5.680197715759277, 'force': [6.0504279136657715, 0.36893242597579956, -1.2251176834106445], 'magnitude': 6.184229850769043, 'cosine_with_motion': -0.027544816955924034, 'motion_component': -0.17034347355365753, 'motion_component_percent': 2.7544816955924034}, {'resid': 458, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 5.956660747528076, 'force': [-3.7763047218322754, 0.8449313044548035, -0.32281407713890076], 'magnitude': 3.8831167221069336, 'cosine_with_motion': 0.3340114951133728, 'motion_component': 1.2970056533813477, 'motion_component_percent': 33.40114951133728}, {'resid': 786, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 5.860579967498779, 'force': [-0.7043887376785278, 5.062003135681152, -2.762082099914551], 'magnitude': 5.809401035308838, 'cosine_with_motion': 0.6018667817115784, 'motion_component': 3.496485471725464, 'motion_component_percent': 60.18667817115784}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': 0.6745236010578689, 'motion_component_pip2': 16.04031650923799, 'motion_component_percent_pip2': 67.4523601057869}, 142: {'frame': 142, 'motion_vector': [1.841552734375, -1.92962646484375, 6.4561614990234375], 'ionic_force': [-4.276970326900482, -1.3154679834842682, -7.215320587158203], 'ionic_force_magnitude': 8.490216862261434, 'radial_force': 4.474699005828144, 'axial_force': -7.215320587158203, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-6.687426978722215, 3.4608835577964783, 4.7408686876297], 'asn_force_magnitude': 8.898046443445633, 'residue_force': [-6.687426978722215, 3.4608835577964783, 4.7408686876297], 'residue_force_magnitude': 8.898046443445633, 'total_force': [-10.964397305622697, 2.14541557431221, -2.4744518995285034], 'total_force_magnitude': 11.443064644802451, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': 0.1868549567387572, 'cosine_residue_motion': 0.1868549567387572, 'cosine_ionic_motion': -0.8754474703093835, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': 1.6626440832494862, 'motion_component_residue': 1.6626440832494862, 'motion_component_ionic': -7.432738874444844, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 18.68549567387572, 'motion_component_percent_residue': 18.68549567387572, 'motion_component_percent_ionic': 87.54474703093835, 'ionic_contributions': [{'ion_id': 2397, 'distance': 11.497966766357422, 'force': [-0.08865207433700562, 0.21174749732017517, -2.5007710456848145], 'magnitude': 2.511284828186035, 'cosine_ionic_motion': -0.9529557824134827, 'motion_component_ionic': -2.39314341545105, 'motion_component_percent_ionic': 95.29557824134827}, {'ion_id': 2400, 'distance': 7.153110980987549, 'force': [-4.188318252563477, -1.5272154808044434, -4.714549541473389], 'magnitude': 6.4885573387146, 'cosine_ionic_motion': -0.7766897082328796, 'motion_component_ionic': -5.039595603942871, 'motion_component_percent_ionic': 77.66897082328796}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 5.308152198791504, 'force': [-5.0682172775268555, -0.3532865643501282, 4.933167457580566], 'magnitude': 7.081509590148926, 'cosine_with_motion': 0.46894556283950806, 'motion_component': 3.3208425045013428, 'motion_component_percent': 46.894556283950806}, {'resid': 786, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 5.071542263031006, 'force': [-0.02059226669371128, 7.565659523010254, 1.715267539024353], 'magnitude': 7.757690906524658, 'cosine_with_motion': -0.06574462354183197, 'motion_component': -0.5100264549255371, 'motion_component_percent': 6.574462354183197}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 5.532100200653076, 'force': [-1.598617434501648, -3.7514894008636475, -1.9075663089752197], 'magnitude': 4.5020060539245605, 'cosine_with_motion': -0.2550356388092041, 'motion_component': -1.1481720209121704, 'motion_component_percent': 25.50356388092041}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': -0.5042438341739326, 'motion_component_pip2': -5.770094791195358, 'motion_component_percent_pip2': 50.42438341739326}, 144: {'frame': 144, 'motion_vector': [-0.438629150390625, -0.26556396484375, 0.38871002197265625], 'ionic_force': [-10.425635397434235, -15.383053839206696, -5.993980288505554], 'ionic_force_magnitude': 19.525880737092468, 'radial_force': 18.583116500204305, 'axial_force': -5.993980288505554, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-5.55267333984375, 10.707819700241089, -7.24886167049408], 'asn_force_magnitude': 14.072511484089857, 'residue_force': [-5.55267333984375, 10.707819700241089, -7.24886167049408], 'residue_force_magnitude': 14.072511484089857, 'total_force': [-15.978308737277985, -4.675234138965607, -13.242841958999634], 'total_force_magnitude': 21.272917700892954, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': -0.356247001389344, 'cosine_residue_motion': -0.356247001389344, 'cosine_ionic_motion': 0.5036919218702878, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': -5.013290018224119, 'motion_component_residue': -5.013290018224119, 'motion_component_ionic': 9.835028394676137, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 35.6247001389344, 'motion_component_percent_residue': 35.6247001389344, 'motion_component_percent_ionic': 50.36919218702878, 'ionic_contributions': [{'ion_id': 2276, 'distance': 11.051673889160156, 'force': [-0.5606434941291809, -0.5012810826301575, -2.6120924949645996], 'magnitude': 2.718203544616699, 'cosine_ionic_motion': -0.36381322145462036, 'motion_component_ionic': -0.9889184236526489, 'motion_component_percent_ionic': 36.381322145462036}, {'ion_id': 2397, 'distance': 7.543346881866455, 'force': [-1.9359514713287354, -1.5789620876312256, -5.272697925567627], 'magnitude': 5.8345842361450195, 'cosine_ionic_motion': -0.2080521285533905, 'motion_component_ionic': -1.213897705078125, 'motion_component_percent_ionic': 20.80521285533905}, {'ion_id': 2400, 'distance': 4.613012313842773, 'force': [-7.929040431976318, -13.302810668945312, 1.8908101320266724], 'magnitude': 15.601590156555176, 'cosine_ionic_motion': 0.7715780735015869, 'motion_component_ionic': 12.03784465789795, 'motion_component_percent_ionic': 77.15780735015869}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 3.654573440551758, 'force': [13.779317855834961, -9.731305122375488, 5.620614528656006], 'magnitude': 17.780866622924805, 'cosine_with_motion': -0.11143654584884644, 'motion_component': -1.981438398361206, 'motion_component_percent': 11.143654584884644}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 2.6744823455810547, 'force': [-16.8614501953125, 18.519262313842773, -12.283468246459961], 'magnitude': 27.895431518554688, 'cosine_with_motion': -0.1279641091823578, 'motion_component': -3.5696139335632324, 'motion_component_percent': 12.796410918235779}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 4.6883344650268555, 'force': [-9.470280647277832, 9.610946655273438, -2.4905078411102295], 'magnitude': 13.720755577087402, 'cosine_with_motion': 0.07176028192043304, 'motion_component': 0.9846053123474121, 'motion_component_percent': 7.176028192043304}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 4.714104175567627, 'force': [3.3111348152160645, -5.184928894042969, 0.7695558071136475], 'magnitude': 6.199944972991943, 'cosine_with_motion': 0.056076113134622574, 'motion_component': 0.3476688265800476, 'motion_component_percent': 5.607611313462257}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 5.547249794006348, 'force': [3.403226852416992, -2.7903780937194824, 0.8242547512054443], 'magnitude': 4.477450370788574, 'cosine_with_motion': -0.14971846342086792, 'motion_component': -0.6703569889068604, 'motion_component_percent': 14.971846342086792}, {'resid': 1114, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 5.604510307312012, 'force': [3.4404242038726807, -6.98671293258667, -5.615911483764648], 'magnitude': 9.601517677307129, 'cosine_with_motion': -0.2972825765609741, 'motion_component': -2.8543639183044434, 'motion_component_percent': 29.728257656097412}, {'resid': 1114, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 4.855534076690674, 'force': [-1.9353364706039429, 3.7937917709350586, 4.001781940460205], 'magnitude': 5.8440260887146, 'cosine_with_motion': 0.37149709463119507, 'motion_component': 2.1710386276245117, 'motion_component_percent': 37.14970946311951}, {'resid': 1114, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 5.756882190704346, 'force': [-1.2197097539901733, 3.4771440029144287, 1.9248188734054565], 'magnitude': 4.15730094909668, 'cosine_with_motion': 0.13450318574905396, 'motion_component': 0.5591702461242676, 'motion_component_percent': 13.450318574905396}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': 0.2266608861204601, 'motion_component_pip2': 4.821738376452018, 'motion_component_percent_pip2': 22.66608861204601}, 145: {'frame': 145, 'motion_vector': [0.6373939514160156, 0.244293212890625, 0.05312347412109375], 'ionic_force': [-7.884051561355591, -4.798625409603119, -4.850839376449585], 'ionic_force_magnitude': 10.426682957677194, 'radial_force': 9.229576092313353, 'axial_force': -4.850839376449585, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-8.360688924789429, 9.444575071334839, -3.1835262775421143], 'asn_force_magnitude': 13.00907210891604, 'residue_force': [-8.360688924789429, 9.444575071334839, -3.1835262775421143], 'residue_force_magnitude': 13.00907210891604, 'total_force': [-16.24474048614502, 4.64594966173172, -8.0343656539917], 'total_force_magnitude': 18.709021171177977, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': -0.35825277730623223, 'cosine_residue_motion': -0.35825277730623223, 'cosine_ionic_motion': -0.9042392465881103, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': -4.660536213196215, 'motion_component_residue': -4.660536213196215, 'motion_component_ionic': -9.428215942063115, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 35.82527773062322, 'motion_component_percent_residue': 35.82527773062322, 'motion_component_percent_ionic': 90.42392465881103, 'ionic_contributions': [{'ion_id': 2276, 'distance': 11.104750633239746, 'force': [-0.7689996957778931, -0.5431862473487854, -2.522294044494629], 'magnitude': 2.6922812461853027, 'cosine_ionic_motion': -0.4105875790119171, 'motion_component_ionic': -1.105417251586914, 'motion_component_percent_ionic': 41.05875790119171}, {'ion_id': 2397, 'distance': 8.041007041931152, 'force': [-1.881825566291809, -1.4822872877120972, -4.541690826416016], 'magnitude': 5.1347246170043945, 'cosine_ionic_motion': -0.5128151178359985, 'motion_component_ionic': -2.633164405822754, 'motion_component_percent_ionic': 51.28151178359985}, {'ion_id': 2400, 'distance': 7.246391773223877, 'force': [-5.233226299285889, -2.7731518745422363, 2.2131454944610596], 'magnitude': 6.322582244873047, 'cosine_ionic_motion': -0.8998908400535583, 'motion_component_ionic': -5.689633846282959, 'motion_component_percent_ionic': 89.98908400535583}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 4.012467861175537, 'force': [11.173873901367188, -8.270788192749023, 4.93074893951416], 'magnitude': 14.75037956237793, 'cosine_with_motion': 0.5310950875282288, 'motion_component': 7.833853721618652, 'motion_component_percent': 53.109508752822876}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 2.987804889678955, 'force': [-14.150491714477539, 14.371257781982422, -9.634489059448242], 'magnitude': 22.351573944091797, 'cosine_with_motion': -0.39340531826019287, 'motion_component': -8.793228149414062, 'motion_component_percent': 39.34053182601929}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 5.097263813018799, 'force': [-7.826177597045898, 8.070252418518066, -2.8909249305725098], 'magnitude': 11.607561111450195, 'cosine_with_motion': -0.39892908930778503, 'motion_component': -4.630593776702881, 'motion_component_percent': 39.8929089307785}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 5.275254726409912, 'force': [2.6153416633605957, -4.049007415771484, 1.1307713985443115], 'magnitude': 4.9510722160339355, 'cosine_with_motion': 0.21768777072429657, 'motion_component': 1.0777878761291504, 'motion_component_percent': 21.768777072429657}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 5.939850807189941, 'force': [2.907025098800659, -2.475907802581787, 0.8179843425750732], 'magnitude': 3.9051265716552734, 'cosine_with_motion': 0.4830447733402252, 'motion_component': 1.8863509893417358, 'motion_component_percent': 48.30447733402252}, {'resid': 1114, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 5.638054847717285, 'force': [-3.0802602767944336, 1.7987682819366455, 2.4623830318450928], 'magnitude': 4.334385871887207, 'cosine_with_motion': -0.46943381428718567, 'motion_component': -2.0347073078155518, 'motion_component_percent': 46.94338142871857}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': -0.753045925083651, 'motion_component_pip2': -14.08875215525933, 'motion_component_percent_pip2': 75.3045925083651}, 146: {'frame': 146, 'motion_vector': [-1.5196418762207031, -1.9833412170410156, 1.7226409912109375], 'ionic_force': [-6.512718200683594, -5.072030991315842, -7.926882565021515], 'ionic_force_magnitude': 11.444494918432433, 'radial_force': 8.254756007198742, 'axial_force': -7.926882565021515, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-3.4557000398635864, 4.09267258644104, -3.3148010969161987], 'asn_force_magnitude': 6.299185501113301, 'residue_force': [-3.4557000398635864, 4.09267258644104, -3.3148010969161987], 'residue_force_magnitude': 6.299185501113301, 'total_force': [-9.96841824054718, -0.9793584048748016, -11.241683661937714], 'total_force_magnitude': 15.056691424703834, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': -0.4485983156486388, 'cosine_residue_motion': -0.4485983156486388, 'cosine_ionic_motion': 0.1814260869933134, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': -2.825804005757753, 'motion_component_residue': -2.825804005757753, 'motion_component_ionic': 2.0763299306660556, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 44.859831564863875, 'motion_component_percent_residue': 44.859831564863875, 'motion_component_percent_ionic': 18.14260869933134, 'ionic_contributions': [{'ion_id': 2276, 'distance': 10.874212265014648, 'force': [-0.6359555721282959, -0.47015663981437683, -2.6939549446105957], 'magnitude': 2.8076467514038086, 'cosine_ionic_motion': -0.3217768967151642, 'motion_component_ionic': -0.9034358263015747, 'motion_component_percent_ionic': 32.17768967151642}, {'ion_id': 2397, 'distance': 7.456031322479248, 'force': [-1.8579390048980713, -1.3600382804870605, -5.510318756103516], 'magnitude': 5.972039699554443, 'cosine_ionic_motion': -0.21912366151809692, 'motion_component_ionic': -1.3086152076721191, 'motion_component_percent_ionic': 21.912366151809692}, {'ion_id': 2400, 'distance': 8.01289176940918, 'force': [-4.018823623657227, -3.2418360710144043, 0.277</t>
+          <t>{138: {'frame': 138, 'motion_vector': [2.379444122314453, 2.9537811279296875, 5.88848876953125], 'ionic_force': [2.5273286402225494, -0.9714137520641088, -6.800560832023621], 'ionic_force_magnitude': 7.31974469250412, 'radial_force': 2.707588361141411, 'axial_force': -6.800560832023621, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [6.405253291130066, -6.760278880596161, 5.933797597885132], 'asn_force_magnitude': 11.042580957350252, 'residue_force': [6.405253291130066, -6.760278880596161, 5.933797597885132], 'residue_force_magnitude': 11.042580957350252, 'pip2_force': [0.8089091824367642, -0.1422158870846033, -4.736720594060898], 'pip2_force_magnitude': 4.807398611533102, 'total_force': [9.74149111378938, -7.873908519744873, -5.603483828199387], 'total_force_magnitude': 13.722030298401197, 'cosine_total_motion': -0.3441180815159799, 'cosine_glu_motion': 0, 'cosine_asn_motion': 0.3906295051309457, 'cosine_residue_motion': 0.3906295051309457, 'cosine_pip2_motion': -0.7836453243283775, 'cosine_ionic_motion': -0.7197329213971744, 'motion_component_total': -4.721998740789969, 'motion_component_glu': 0, 'motion_component_asn': 4.313557934738133, 'motion_component_residue': 4.313557934738133, 'motion_component_ionic': -5.268261231417452, 'motion_component_pip2': -3.76729544411065, 'motion_component_percent_total': 34.41180815159799, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 39.06295051309457, 'motion_component_percent_residue': 39.06295051309457, 'motion_component_percent_ionic': 71.97329213971744, 'motion_component_percent_pip2': 78.36453243283775, 'ionic_contributions': [{'ion_id': 2397, 'distance': 12.146998405456543, 'force': [0.2803648114204407, 0.018578680232167244, -2.2324788570404053], 'magnitude': 2.250091552734375, 'cosine_ionic_motion': -0.7882996797561646, 'motion_component_ionic': -1.7737464904785156, 'motion_component_percent_ionic': 78.82996797561646}, {'ion_id': 2399, 'distance': 13.916149139404297, 'force': [-0.06216016411781311, -0.06396990269422531, 1.7120298147201538], 'magnitude': 1.714351773262024, 'cosine_ionic_motion': 0.811498761177063, 'motion_component_ionic': 1.3911943435668945, 'motion_component_percent_ionic': 81.1498761177063}, {'ion_id': 2400, 'distance': 7.01064395904541, 'force': [2.309123992919922, -0.9260225296020508, -6.280111789703369], 'magnitude': 6.7549519538879395, 'cosine_ionic_motion': -0.7232781052589417, 'motion_component_ionic': -4.885708808898926, 'motion_component_percent_ionic': 72.32781052589417}], 'glu_contributions': [], 'asn_contributions': [{'resid': 458, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 5.213967323303223, 'force': [5.881892204284668, -0.6080090403556824, 4.347905158996582], 'magnitude': 7.339660167694092, 'cosine_with_motion': 0.7353169322013855, 'motion_component': 5.396976470947266, 'motion_component_percent': 73.53169322013855}, {'resid': 1114, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 5.594605922698975, 'force': [0.523361086845398, -6.1522698402404785, 1.5858924388885498], 'magnitude': 6.374903202056885, 'cosine_with_motion': -0.16995061933994293, 'motion_component': -1.0834187269210815, 'motion_component_percent': 16.995061933994293}], 'pip2_contributions': [{'resid': 1313, 'atom': 'C1', 'charge': 0.06000000238418579, 'distance': 24.402841567993164, 'force': [-0.022420506924390793, -0.02128113992512226, 0.012782823294401169], 'magnitude': 0.033450957387685776, 'cosine_with_motion': -0.17471742630004883, 'motion_component': -0.0058444649912416935, 'motion_component_percent': 17.471742630004883}, {'resid': 1313, 'atom': 'C11', 'charge': 0.17000000178813934, 'distance': 24.04247283935547, 'force': [-0.07392477244138718, -0.05795276537537575, 0.02664990723133087], 'magnitude': 0.09764022380113602, 'cosine_with_motion': -0.2780381143093109, 'motion_component': -0.027147704735398293, 'motion_component_percent': 27.80381143093109}, {'resid': 1313, 'atom': 'C12', 'charge': 0.04000000283122063, 'distance': 24.602930068969727, 'force': [-0.017247885465621948, -0.01263332273811102, 0.004924040753394365], 'magnitude': 0.021939383819699287, 'cosine_with_motion': -0.321213960647583, 'motion_component': -0.007047236431390047, 'motion_component_percent': 32.1213960647583}, {'resid': 1313, 'atom': 'C13', 'charge': -0.05000000074505806, 'distance': 25.780147552490234, 'force': [0.019319377839565277, 0.015033502131700516, -0.004959581885486841], 'magnitude': 0.024976829066872597, 'cosine_with_motion': 0.3496534824371338, 'motion_component': 0.00873323529958725, 'motion_component_percent': 34.96534824371338}, {'resid': 1313, 'atom': 'C2', 'charge': 0.06000000238418579, 'distance': 25.88208770751953, 'force': [-0.020231634378433228, -0.01853950135409832, 0.01145560946315527], 'magnitude': 0.029736561700701714, 'cosine_with_motion': -0.17017745971679688, 'motion_component': -0.0050604925490915775, 'motion_component_percent': 17.017745971679688}, {'resid': 1313, 'atom': 'C21', 'charge': 0.6299999952316284, 'distance': 22.660926818847656, 'force': [-0.333642840385437, -0.22080835700035095, 0.07632959634065628], 'magnitude': 0.40730834007263184, 'cosine_with_motion': -0.349338561296463, 'motion_component': -0.14228850603103638, 'motion_component_percent': 34.9338561296463}, {'resid': 1313, 'atom': 'C210', 'charge': -0.18000000715255737, 'distance': 22.375221252441406, 'force': [0.1032874658703804, 0.055836427956819534, 0.021492497995495796], 'magnitude': 0.11936471611261368, 'cosine_with_motion': 0.6425926685333252, 'motion_component': 0.07670289278030396, 'motion_component_percent': 64.25926685333252}, {'resid': 1313, 'atom': 'C211', 'charge': -0.15000000596046448, 'distance': 22.10381507873535, 'force': [0.09119110554456711, 0.04141058027744293, 0.01894017867743969], 'magnitude': 0.10192832350730896, 'cosine_with_motion': 0.6314677596092224, 'motion_component': 0.06436444818973541, 'motion_component_percent': 63.14677596092224}, {'resid': 1313, 'atom': 'C212', 'charge': -0.15000000596046448, 'distance': 21.817134857177734, 'force': [0.09611354768276215, 0.03859924152493477, 0.014785009436309338], 'magnitude': 0.10462462157011032, 'cosine_with_motion': 0.5864573121070862, 'motion_component': 0.06135787442326546, 'motion_component_percent': 58.64573121070862}, {'resid': 1313, 'atom': 'C213', 'charge': -0.18000000715255737, 'distance': 21.773134231567383, 'force': [0.11609593033790588, 0.04831179231405258, 0.008843266405165195], 'magnitude': 0.12605752050876617, 'cosine_with_motion': 0.5334609746932983, 'motion_component': 0.06724676489830017, 'motion_component_percent': 53.346097469329834}, {'resid': 1313, 'atom': 'C214', 'charge': -0.15000000596046448, 'distance': 20.334096908569336, 'force': [0.11114843189716339, 0.046035829931497574, 0.005754346027970314], 'magnitude': 0.1204424500465393, 'cosine_with_motion': 0.5148470401763916, 'motion_component': 0.06200943887233734, 'motion_component_percent': 51.48470401763916}, {'resid': 1313, 'atom': 'C215', 'charge': -0.15000000596046448, 'distance': 19.97473907470703, 'force': [0.11644329875707626, 0.044913630932569504, -0.0015918146818876266], 'magnitude': 0.12481509894132614, 'cosine_with_motion': 0.4579499661922455, 'motion_component': 0.057159069925546646, 'motion_component_percent': 45.79499661922455}, {'resid': 1313, 'atom': 'C216', 'charge': -0.18000000715255737, 'distance': 20.867338180541992, 'force': [0.12942864000797272, 0.0448644794523716, -0.008357933722436428], 'magnitude': 0.13723866641521454, 'cosine_with_motion': 0.4070381820201874, 'motion_component': 0.055861376225948334, 'motion_component_percent': 40.70381820201874}, {'resid': 1313, 'atom': 'C217', 'charge': -0.18000000715255737, 'distance': 20.195837020874023, 'force': [0.13907866179943085, 0.04271954670548439, -0.017299873754382133], 'magnitude': 0.1465166211128235, 'cosine_with_motion': 0.3461562395095825, 'motion_component': 0.05071764439344406, 'motion_component_percent': 34.61562395095825}, {'resid': 1313, 'atom': 'C218', 'charge': -0.18000000715255737, 'distance': 21.173826217651367, 'force': [0.12575942277908325, 0.03788851201534271, -0.022725019603967667], 'magnitude': 0.13329440355300903, 'cosine_with_motion': 0.297047883272171, 'motion_component': 0.03959482163190842, 'motion_component_percent': 29.704788327217102}, {'resid': 1313, 'atom': 'C219', 'charge': -0.18000000715255737, 'distance': 20.60798454284668, 'force': [0.1322927176952362, 0.03534434735774994, -0.03240450844168663], 'magnitude': 0.14071474969387054, 'cosine_with_motion': 0.23170205950737, 'motion_component': 0.03260389715433121, 'motion_component_percent': 23.170205950737}, {'resid': 1313, 'atom': 'C22', 'charge': -0.08000000566244125, 'distance': 21.92666244506836, 'force': [0.04579306021332741, 0.03011610172688961, -0.0069199902936816216], 'magnitude': 0.055243734270334244, 'cosine_with_motion': 0.4061806797981262, 'motion_component': 0.022438937798142433, 'motion_component_percent': 40.61806797981262}, {'resid': 1313, 'atom': 'C220', 'charge': -0.27000001072883606, 'distance': 21.737157821655273, 'force': [0.17669221758842468, 0.04554326832294464, -0.05192851275205612], 'magnitude': 0.18971268832683563, 'cosine_with_motion': 0.18751589953899384, 'motion_component': 0.03557414561510086, 'motion_component_percent': 18.751589953899384}, {'resid': 1313, 'atom': 'C23', 'charge': -0.18000000715255737, 'distance': 20.801536560058594, 'force': [0.11027947813272476, 0.08153290301561356, -0.016270292922854424], 'magnitude': 0.1381082832813263, 'cosine_with_motion': 0.421174556016922, 'motion_component': 0.05816769599914551, 'motion_component_percent': 42.1174556016922}, {'resid': 1313, 'atom': 'C24', 'charge': -0.18000000715255737, 'distance': 20.108715057373047, 'force': [0.11853664368391037, 0.08794492483139038, -0.0075054350309073925], 'magnitude': 0.14778897166252136, 'cosine_with_motion': 0.48072102665901184, 'motion_component': 0.07104526460170746, 'motion_component_percent': 48.072102665901184}, {'resid': 1313, 'atom': 'C25', 'charge': -0.15000000596046448, 'distance': 21.12590980529785, 'force': [0.08920259773731232, 0.06703309714794159, 0.0005030279862694442], 'magnitude': 0.11158312112092972, 'cosine_with_motion': 0.5287017226219177, 'motion_component': 0.05899418517947197, 'motion_component_percent': 52.87017226219177}, {'resid': 1313, 'atom': 'C26', 'charge': -0.15000000596046448, 'distance': 21.136337280273438, 'force': [0.09052691608667374, 0.06466934084892273, 0.006999703589826822], 'magnitude': 0.11147305369377136, 'cosine_with_motion': 0.5733129978179932, 'motion_component': 0.06390894949436188, 'motion_component_percent': 57.331299781799316}, {'resid': 1313, 'atom': 'C27', 'charge': -0.18000000715255737, 'distance': 20.118284225463867, 'force': [0.12313391268253326, 0.08028484135866165, 0.013872077688574791], 'magnitude': 0.1476484090089798, 'cosine_with_motion': 0.591598391532898, 'motion_component': 0.0873485580086708, 'motion_component_percent': 59.159839153289795}, {'resid': 1313, 'atom': 'C28', 'charge': -0.15000000596046448, 'distance': 20.349971771240234, 'force': [0.09935349225997925, 0.06463831663131714, 0.020296355709433556], 'magnitude': 0.12025460600852966, 'cosine_with_motion': 0.6492284536361694, 'motion_component': 0.07807271182537079, 'motion_component_percent': 64.92284536361694}, {'resid': 1313, 'atom': 'C29', 'charge': -0.15000000596046448, 'distance': 21.334993362426758, 'force': [0.09173980355262756, 0.055397652089595795, 0.022017236799001694], 'magnitude': 0.10940681397914886, 'cosine_with_motion': 0.6675648093223572, 'motion_component': 0.07303614169359207, 'motion_component_percent': 66.75648093223572}, {'resid': 1313, 'atom': 'C3', 'charge': 0.06000000238418579, 'distance': 26.375789642333984, 'force': [-0.01954292319715023, -0.016916828230023384, 0.012320205569267273], 'magnitude': 0.028633764013648033, 'cosine_with_motion': -0.11927808821201324, 'motion_component': -0.0034153806045651436, 'motion_component_percent': 11.927808821201324}, {'resid': 1313, 'atom': 'C31', 'charge': 0.6299999952316284, 'distance': 27.533588409423828, 'force': [-0.21990327537059784, -0.1620675027370453, 0.03870305418968201], 'magnitude': 0.27590081095695496, 'cosine_with_motion': -0.4005458652973175, 'motion_component': -0.1105109304189682, 'motion_component_percent': 40.05458652973175}, {'resid': 1313, 'atom': 'C310', 'charge': -0.18000000715255737, 'distance': 26.378376007080078, 'force': [0.06367551535367966, 0.05446280539035797, 0.01885124109685421], 'magnitude': 0.0858844444155693, 'cosine_with_motion': 0.7038129568099976, 'motion_component': 0.06044658273458481, 'motion_component_percent': 70.38129568099976}, {'resid': 1313, 'atom': 'C311', 'charge': -0.18000000715255737, 'distance': 26.79759407043457, 'force': [0.06133041903376579, 0.051465462893247604, 0.022697491571307182], 'magnitude': 0.08321832865476608, 'cosine_with_motion': 0.740455150604248, 'motion_component': 0.061619438230991364, 'motion_component_percent': 74.0455150604248}, {'resid': 1313, 'atom': 'C312', 'charge': -0.18000000715255737, 'distance': 27.45832633972168, 'force': [0.055643778294324875, 0.05150832608342171, 0.023087939247488976], 'magnitude': 0.07926153391599655, 'cosine_with_motion': 0.7574160099029541, 'motion_component': 0.06003395467996597, 'motion_component_percent': 75.74160099029541}, {'resid': 1313, 'atom': 'C313', 'charge': -0.18000000715255737, 'distance': 27.953580856323242, 'force': [0.05311553552746773, 0.048519477248191833, 0.025951147079467773], 'magnitude': 0.07647784799337387, 'cosine_with_motion': 0.7887478470802307, 'motion_component': 0.060321737080812454, 'motion_component_percent': 78.87478470802307}, {'resid': 1313, 'atom': 'C314', 'charge': -0.18000000715255737, 'distance': 28.83768081665039, 'force': [0.047449976205825806, 0.04746103286743164, 0.025688041001558304], 'magnitude': 0.07186045497655869, 'cosine_with_motion': 0.8033562898635864, 'motion_component': 0.05772954970598221, 'motion_component_percent': 80.33562898635864}, {'resid': 1313, 'atom': 'C315', 'charge': -0.18000000715255737, 'distance': 29.904394149780273, 'force': [0.04445531591773033, 0.04272693023085594, 0.025763316079974174], 'magnitude': 0.0668252557516098, 'cosine_with_motion': 0.819736659526825, 'motion_component': 0.054779112339019775, 'motion_component_percent': 81.9736659526825}, {'resid': 1313, 'atom': 'C316', 'charge': -0.18000000715255737, 'distance': 30.961219787597656, 'force': [0.03960398957133293, 0.04120268300175667, 0.024905338883399963], 'magnitude': 0.062341101467609406, 'cosine_with_motion': 0.8303830027580261, 'motion_component': 0.05176699161529541, 'motion_component_percent': 83.03830027580261}, {'resid': 1313, 'atom': 'C317', 'charge': -0.18000000715255737, 'distance': 32.03162384033203, 'force': [0.03698249161243439, 0.0374426506459713, 0.024954555556178093], 'magnitude': 0.05824419856071472, 'cosine_with_motion': 0.8469889163970947, 'motion_component': 0.04933219030499458, 'motion_component_percent': 84.69889163970947}, {'resid': 1313, 'atom': 'C318', 'charge': -0.27000001072883606, 'distance': 33.09305191040039, 'force': [0.049864139407873154, 0.054316502064466476, 0.03553872928023338], 'magnitude': 0.0818517878651619, 'cosine_with_motion': 0.8518084287643433, 'motion_component': 0.06972204148769379, 'motion_component_percent': 85.18084287643433}, {'resid': 1313, 'atom': 'C32', 'charge': -0.08000000566244125, 'distance': 28.054248809814453, 'force': [0.02776786871254444, 0.018834667280316353, -0.0036107683554291725], 'magnitude': 0.03374665603041649, 'cosine_with_motion': 0.42493635416030884, 'motion_component': 0.014340180903673172, 'motion_component_percent': 42.493635416030884}, {'resid': 1313, 'atom': 'C33', 'charge': -0.18000000715255737, 'distance': 27.763357162475586, 'force': [0.06357120722532272, 0.04419083520770073, -0.004084730986505747], 'magnitude': 0.0775294378399849, 'cosine_with_motion': 0.47462400794029236, 'motion_component': 0.036797333508729935, 'motion_component_percent': 47.462400794029236}, {'resid': 1313, 'atom': 'C34', 'charge': -0.18000000715255737, 'distance': 26.25332260131836, 'force': [0.07069101929664612, 0.05011456832289696, -0.002999091288074851], 'magnitude': 0.08670458197593689, 'cosine_with_motion': 0.49163225293159485, 'motion_component': 0.042626768350601196, 'motion_component_percent': 49.163225293159485}, {'resid': 1313, 'atom': 'C35', 'charge': -0.18000000715255737, 'distance': 26.383501052856445, 'force': [0.0700334683060646, 0.04961637780070305, 0.0019840041641145945], 'magnitude': 0.08585108071565628, 'cosine_with_motion': 0.5402674078941345, 'motion_component': 0.046382542699575424, 'motion_component_percent': 54.02674078941345}, {'resid': 1313, 'atom': 'C36', 'charge': -0.18000000715255737, 'distance': 25.057512283325195, 'force': [0.07743663340806961, 0.05513899773359299, 0.004693910479545593], 'magnitude': 0.09517759084701538, 'cosine_with_motion': 0.5621553063392639, 'motion_component': 0.0535045862197876, 'motion_component_percent': 56.21553063392639}, {'resid': 1313, 'atom': 'C37', 'charge': -0.18000000715255737, 'distance': 25.17207908630371, 'force': [0.07662482559680939, 0.05397293344140053, 0.010513661429286003], 'magnitude': 0.09431319683790207, 'cosine_with_motion': 0.611045777797699, 'motion_component': 0.05762968212366104, 'motion_component_percent': 61.1045777797699}, {'resid': 1313, 'atom': 'C38', 'charge': -0.18000000715255737, 'distance': 25.80702018737793, 'force': [0.07003919035196304, 0.0547550730407238, 0.012155810371041298], 'magnitude': 0.0897294282913208, 'cosine_with_motion': 0.6363893151283264, 'motion_component': 0.05710284784436226, 'motion_component_percent': 63.63893151283264}, {'resid': 1313, 'atom': 'C39', 'charge': -0.18000000715255737, 'distance': 25.790361404418945, 'force': [0.0696246400475502, 0.05397447198629379, 0.017645329236984253], 'magnitude': 0.08984537422657013, 'cosine_with_motion': 0.6817025542259216, 'motion_component': 0.061247821897268295, 'motion_component_percent': 68.17025542259216}, {'resid': 1313, 'atom': 'C4', 'charge': 0.08000000566244125, 'distance': 26.21433448791504, 'force': [-0.024888942018151283, -0.023258890956640244, 0.018259065225720406], 'magnitude': 0.03865008056163788, 'cosine_with_motion': -0.0753742977976799, 'motion_component': -0.002913222648203373, 'motion_component_percent': 7.53742977976799}, {'resid': 1313, 'atom': 'C5', 'charge': 0.08000000566244125, 'distance': 24.719451904296875, 'force': [-0.027550406754016876, -0.02643880434334278, 0.020766904577612877], 'magnitude': 0.04346607252955437, 'cosine_with_motion': -0.07017014920711517, 'motion_component': -0.003050020895898342, 'motion_component_percent': 7.017014920711517}, {'resid': 1313, 'atom': 'C6', 'charge': 0.06000000238418579, 'distance': 24.10930824279785, 'force': [-0.021670158952474594, -0.022014115005731583, 0.014840723015367985], 'magnitude': 0.034270454198122025, 'cosine_with_motion': -0.12163854390382767, 'motion_component': -0.004168608225882053, 'motion_component_percent': 12.163854390382767}, {'resid': 1313, 'atom': 'H1', 'charge': 0.12000000476837158, 'distance': 23.959632873535156, 'force': [-0.04838799312710762, -0.04197182506322861, 0.026708029210567474], 'magnitude': 0.06939993053674698, 'cosine_with_motion': -0.1683645099401474, 'motion_component': -0.011684484779834747, 'motion_component_percent': 16.83645099401474}, {'resid': 1313, 'atom': 'H10R', 'charge': 0.09000000357627869, 'distance': 22.654399871826172, 'force': [-0.0503530390560627, -0.028139790520071983, -0.007895772345364094], 'magnitude': 0.05822044238448143, 'cosine_with_motion': -0.6116417646408081, 'motion_component': -0.035610053688287735, 'motion_component_percent': 61.16417646408081}, {'resid': 1313, 'atom': 'H10S', 'charge': 0.09000000357627869, 'distance': 23.199026107788086, 'force': [-0.047447189688682556, -0.026391709223389626, -0.011601462960243225], 'magnitude': 0.05551893264055252, 'cosine_with_motion': -0.6664586067199707, 'motion_component': -0.03700106963515282, 'motion_component_percent': 66.64586067199707}, {'resid': 1313, 'atom': 'H10X', 'charge': 0.09000000357627869, 'distance': 25.809343338012695, 'force': [-0.03220544755458832, -0.02966183051466942, -0.009752064011991024], 'magnitude': 0.044856633991003036, 'cosine_with_motion': -0.7055269479751587, 'motion_component': -0.031647562980651855, 'motion_component_percent': 70.55269479751587}, {'resid': 1313, 'atom': 'H10Y', 'charge': 0.09000000357627869, 'distance': 27.297189712524414, 'force': [-0.029690125957131386, -0.025749001652002335, -0.007968570105731487], 'magnitude': 0.040100034326314926, 'cosine_with_motion': -0.6893672943115234, 'motion_component': -0.027643652632832527, 'motion_component_percent': 68.93672943115234}, {'resid': 1313, 'atom': 'H111', 'charge': 0.15000000596046448, 'distance': 22.09762191772461, 'force': [-0.09088128060102463, -0.03976454213261604, -0.02367294952273369], 'magnitude': 0.10198546200990677, 'cosine_with_motion': -0.662289023399353, 'motion_component': -0.06754384934902191, 'motion_component_percent': 66.2289023399353}, {'resid': 1313, 'atom': 'H11A', 'charge': 0.09000000357627869, 'distance': 24.88187026977539, 'force': [-0.036379072815179825, -0.028213350102305412, 0.01448756642639637], 'magnitude': 0.04826302453875542, 'cosine_with_motion': -0.2502231001853943, 'motion_component': -0.012076523154973984, 'motion_component_percent': 25.02231001853943}, {'resid': 1313, 'atom': 'H11B', 'charge': 0.09000000357627869, 'distance': 23.178268432617188, 'force': [-0.04250072315335274, -0.031956348568201065, 0.016306092962622643], 'magnitude': 0.055618416517972946, 'cosine_with_motion': -0.2554142475128174, 'motion_component': -0.014205736108124256, 'motion_component_percent': 25.54142475128174}, {'resid': 1313, 'atom': 'H11X', 'charge': 0.09000000357627869, 'distance': 27.51233673095703, 'force': [-0.02982335351407528, -0.023458512499928474, -0.010888819582760334], 'magnitude': 0.03947531804442406, 'cosine_with_motion': -0.7391459941864014, 'motion_component': -0.02917802333831787, 'motion_component_percent': 73.91459941864014}, {'resid': 1313, 'atom': 'H11Y', 'charge': 0.09000000357627869, 'distance': 25.961076736450195, 'force': [-0.03285747393965721, -0.026746319606900215, -0.013057917356491089], 'magnitude': 0.04433382675051689, 'cosine_with_motion': -0.7537985444068909, 'motion_component': -0.03341877460479736, 'motion_component_percent': 75.37985444068909}, {'resid': 1313, 'atom': 'H12', 'charge': 0.09000000357627869, 'distance': 24.953998565673828, 'force': [-0.03868640214204788, -0.025988509878516197, 0.011422136798501015], 'magnitude': 0.04798442870378494, 'cosine_with_motion': -0.3021645247936249, 'motion_component': -0.014499192126095295, 'motion_component_percent': 30.216452479362488}, {'resid': 1313, 'atom': 'H121', 'charge': 0.15000000596046448, 'distance': 21.802772521972656, 'force': [-0.0977754145860672, -0.03389129415154457, -0.016325855627655983], 'magnitude': 0.10476251691579819, 'cosine_with_motion': -0.5844879746437073, 'motion_component': -0.06123242899775505, 'motion_component_percent': 58.44879746437073}, {'resid': 1313, 'atom': 'H12X', 'charge': 0.09000000357627869, 'distance': 26.814260482788086, 'force': [-0.028241539373993874, -0.027993325144052505, -0.012075244449079037], 'magnitude': 0.04155745729804039, 'cosine_with_motion': -0.7592005729675293, 'motion_component': -0.03155044466257095, 'motion_component_percent': 75.92005729675293}, {'resid': 1313, 'atom': 'H12Y', 'charge': 0.09000000357627869, 'distance': 28.362220764160156, 'force': [-0.026039570569992065, -0.02449766919016838, -0.01007743552327156], 'magnitude': 0.0371449813246727, 'cosine_with_motion': -0.7443463802337646, 'motion_component': -0.02764873206615448, 'motion_component_percent': 74.43463802337646}, {'resid': 1313, 'atom': 'H13A', 'charge': 0.09000000357627869, 'distance': 26.420774459838867, 'force': [-0.03264874592423439, -0.025857795029878616, 0.009882310405373573], 'magnitude': 0.04280451312661171, 'cosine_with_motion': -0.3197685480117798, 'motion_component': -0.013687537051737309, 'motion_component_percent': 31.97685480117798}, {'resid': 1313, 'atom': 'H13B', 'charge': 0.09000000357627869, 'distance': 25.522319793701172, 'force': [-0.03454909101128578, -0.02902820147573948, 0.00823972001671791], 'magnitude': 0.045871224254369736, 'cosine_with_motion': -0.37171441316604614, 'motion_component': -0.01705099456012249, 'motion_component_percent': 37.171441316604614}, {'resid': 1313, 'atom': 'H13R', 'charge': 0.09000000357627869, 'distance': 22.43419647216797, 'force': [-0.055473849177360535, -0.020952580496668816, -0.0028839786536991596], 'magnitude': 0.059368982911109924, 'cosine_with_motion': -0.507089376449585, 'motion_component': -0.030105380341410637, 'motion_component_percent': 50.708937644958496}, {'resid': 1313, 'atom': 'H13S', 'charge': 0.09000000357627869, 'distance': 22.190671920776367, 'force': [-0.05479662865400314, -0.02578824944794178, -0.0037760513368993998], 'magnitude': 0.06067918241024017, 'cosine_with_motion': -0.5383149981498718, 'motion_component': -0.03266451507806778, 'motion_component_percent': 53.83149981498718}, {'resid': 1313, 'atom': 'H13X', 'charge': 0.09000000357627869, 'distance': 28.53708839416504, 'force': [-0.026252789422869682, -0.022354695945978165, -0.012541885487735271], 'magnitude': 0.036691147834062576, 'cosine_with_motion': -0.7873641848564148, 'motion_component': -0.02888929657638073, 'motion_component_percent': 78.73641848564148}, {'resid': 1313, 'atom': 'H13Y', 'charge': 0.09000000357627869, 'distance': 27.138227462768555, 'force': [-0.028070077300071716, -0.025308331474661827, -0.014750590547919273], 'magnitude': 0.0405711829662323, 'cosine_with_motion': -0.803749144077301, 'motion_component': -0.03260905295610428, 'motion_component_percent': 80.3749144077301}, {'resid': 1313, 'atom': 'H141', 'charge': 0.15000000596046448, 'distance': 19.557283401489258, 'force': [-0.11905485391616821, -0.05160800367593765, -0.01070986408740282], 'magnitude': 0.13020040094852448, 'cosine_with_motion': -0.5469354391098022, 'motion_component': -0.07121121138334274, 'motion_component_percent': 54.693543910980225}, {'resid': 1313, 'atom': 'H14X', 'charge': 0.09000000357627869, 'distance': 29.41438102722168, 'force': [-0.02283059060573578, -0.023293225094676018, -0.011351890861988068], 'magnitude': 0.034535136073827744, 'cosine_with_motion': -0.7853482961654663, 'motion_component': -0.02712211012840271, 'motion_component_percent': 78.53482961654663}, {'resid': 1313, 'atom': 'H14Y', 'charge': 0.09000000357627869, 'distance': 28.174394607543945, 'force': [-0.023991376161575317, -0.02541259117424488, -0.01398305781185627], 'magnitude': 0.03764189034700394, 'cosine_with_motion': -0.8135135769844055, 'motion_component': -0.03062218800187111, 'motion_component_percent': 81.35135769844055}, {'resid': 1313, 'atom': 'H151', 'charge': 0.15000000596046448, 'distance': 18.937761306762695, 'force': [-0.12922175228595734, -0.050669725984334946, 0.003995672333985567], 'magnitude': 0.1388583779335022, 'cosine_with_motion': -0.44582486152648926, 'motion_component': -0.061906516551971436, 'motion_component_percent': 44.582486152648926}, {'resid': 1313, 'atom': 'H15X', 'charge': 0.09000000357627869, 'distance': 30.463045120239258, 'force': [-0.02215442806482315, -0.02007484622299671, -0.011954805813729763], 'magnitude': 0.03219837695360184, 'cosine_with_motion': -0.8088005185127258, 'motion_component': -0.026042064651846886, 'motion_component_percent': 80.88005185127258}, {'resid': 1313, 'atom': 'H15Y', 'charge': 0.09000000357627869, 'distance': 29.527122497558594, 'force': [-0.022922471165657043, -0.021189795807003975, -0.014146269299089909], 'magnitude': 0.03427191451191902, 'cosine_with_motion': -0.8349548578262329, 'motion_component': -0.028615500777959824, 'motion_component_percent': 83.49548578262329}, {'resid': 1313, 'atom': 'H16R', 'charge': 0.09000000357627869, 'distance': 21.477821350097656, 'force': [-0.06182751804590225, -0.01919594593346119, 0.002129355911165476], 'magnitude': 0.06477391719818115, 'cosine_with_motion': -0.42159461975097656, 'motion_component': -0.027308335527777672, 'motion_component_percent': 42.159461975097656}, {'resid': 1313, 'atom': 'H16S', 'charge': 0.09000000357627869, 'distance': 21.56916046142578, 'force': [-0.05973763018846512, -0.022996943444013596, 0.005253229755908251], 'magnitude': 0.06422647833824158, 'cosine_with_motion': -0.3982014060020447, 'motion_component': -0.025575073435902596, 'motion_component_percent': 39.82014060020447}, {'resid': 1313, 'atom': 'H16X', 'charge': 0.09000000357627869, 'distance': 30.419422149658203, 'force': [-0.019739046692848206, -0.02178863063454628, -0.013353673741221428], 'magnitude': 0.03229079023003578, 'cosine_with_motion': -0.8398761749267578, 'motion_component': -0.02712026610970497, 'motion_component_percent': 83.98761749267578}, {'resid': 1313, 'atom': 'H16Y', 'charge': 0.09000000357627869, 'distance': 31.46310806274414, 'force': [-0.019147105515003204, -0.02044018730521202, -0.011254476383328438], 'magnitude': 0.03018403798341751, 'cosine_with_motion': -0.8145283460617065, 'motion_component': -0.024585753679275513, 'motion_component_percent': 81.45283460617065}, {'resid': 1313, 'atom': 'H17R', 'charge': 0.09000000357627869, 'distance': 19.27764320373535, 'force': [-0.0755210816860199, -0.025500932708382607, 0.010532153770327568], 'magnitude': 0.08040309697389603, 'cosine_with_motion': -0.34270909428596497, 'motion_component': -0.027554873377084732, 'motion_component_percent': 34.2709094285965}, {'resid': 1313, 'atom': 'H17S', 'charge': 0.09000000357627869, 'distance': 19.895538330078125, 'force': [-0.07280360907316208, -0.0185097549110651, 0.007431911304593086], 'magnitude': 0.07548648864030838, 'cosine_with_motion': -0.34827208518981934, 'motion_component': -0.026289837434887886, 'motion_component_percent': 34.827208518981934}, {'resid': 1313, 'atom': 'H17X', 'charge': 0.09000000357627869, 'distance': 31.552570343017578, 'force': [-0.018984591588377953, -0.018813924863934517, -0.013653156347572803], 'magnitude': 0.03001311607658863, 'cosine_with_motion': -0.861666202545166, 'motion_component': -0.025861287489533424, 'motion_component_percent': 86.1666202545166}, {'resid': 1313, 'atom': 'H17Y', 'charge': 0.09000000357627869, 'distance': 32.61537170410156, 'force': [-0.01845063827931881, -0.017614614218473434, -0.011759682558476925], 'magnitude': 0.028088979423046112, 'cosine_with_motion': -0.8395576477050781, 'motion_component': -0.02358231693506241, 'motion_component_percent': 83.95576477050781}, {'resid': 1313, 'atom': 'H18R', 'charge': 0.09000000357627869, 'distance': 22.00615882873535, 'force': [-0.058856312185525894, -0.015930963680148125, 0.009441986680030823], 'magnitude': 0.06170099228620529, 'cosine_with_motion': -0.3042813539505005, 'motion_component': -0.01877446100115776, 'motion_component_percent': 30.42813539505005}, {'resid': 1313, 'atom': 'H18S', 'charge': 0.09000000357627869, 'distance': 21.613483428955078, 'force': [-0.059337906539440155, -0.0209550429135561, 0.011454535648226738], 'magnitude': 0.06396333128213882, 'cosine_with_motion': -0.30274879932403564, 'motion_component': -0.019364822655916214, 'motion_component_percent': 30.274879932403564}, {'resid': 1313, 'atom': 'H18X', 'charge': 0.09000000357627869, 'distance': 32.69791030883789, 'force': [-0.016357624903321266, -0.019097700715065002, -0.012196734547615051], 'magnitude': 0.027947349473834038, 'cosine_with_motion': -0.8538968563079834, 'motion_component': -0.023864153772592545, 'motion_component_percent': 85.38968563079834}, {'resid': 1313, 'atom': 'H18Y', 'charge': 0.09000000357627869, 'distance': 33.70170974731445, 'force': [-0.01624273508787155, -0.017670026049017906, -0.010771224275231361], 'magnitude': 0.026307327672839165, 'cosine_with_motion': -0.8372058868408203, 'motion_component': -0.022024650126695633, 'motion_component_percent': 83.72058868408203}, {'resid': 1313, 'atom': 'H18Z', 'charge': 0.09000000357627869, 'distance': 33.87209701538086, 'force': [-0.015853945165872574, -0.01695406064391136, -0.01180961262434721], 'magnitude': 0.026043323799967766, 'cosine_with_motion': -0.862547755241394, 'motion_component': -0.022463610395789146, 'motion_component_percent': 86.2547755241394}, {'resid': 1313, 'atom': 'H19R', 'charge': 0.09000000357627869, 'distance': 19.881628036499023, 'force': [-0.06997542083263397, -0.021369077265262604, 0.018999386578798294], 'magnitude': 0.07559215277433395, 'cosine_with_motion': -0.22238029539585114, 'motion_component': -0.016810204833745956, 'motion_component_percent': 22.238029539585114}, {'resid': 1313, 'ato</t>
         </is>
       </c>
     </row>
@@ -515,7 +515,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>{574: {'frame': 574, 'motion_vector': [-5.495319366455078, 2.858715057373047, 2.9860458374023438], 'ionic_force': [9.93061837553978, -6.6990053951740265, 0.2928283214569092], 'ionic_force_magnitude': 11.982470656380775, 'radial_force': 11.978892044140771, 'axial_force': 0.2928283214569092, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-4.0223565101623535, 1.5621775388717651, -0.024718403816223145], 'asn_force_magnitude': 4.315131696401413, 'residue_force': [-4.0223565101623535, 1.5621775388717651, -0.024718403816223145], 'residue_force_magnitude': 4.315131696401413, 'total_force': [5.908261865377426, -5.136827856302261, 0.26810991764068604], 'total_force_magnitude': 7.833673571389947, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': 0.8929282470610925, 'cosine_residue_motion': 0.8929282470610925, 'cosine_ionic_motion': -0.8840963770449431, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': 3.8531029815054723, 'motion_component_residue': 3.8531029815054723, 'motion_component_ionic': -10.593658895353585, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 89.29282470610926, 'motion_component_percent_residue': 89.29282470610926, 'motion_component_percent_ionic': 88.40963770449432, 'ionic_contributions': [{'ion_id': 2276, 'distance': 9.409431457519531, 'force': [1.1248300075531006, -0.7832292914390564, -3.4903464317321777], 'magnitude': 3.7498278617858887, 'cosine_ionic_motion': -0.730733335018158, 'motion_component_ionic': -2.740124225616455, 'motion_component_percent_ionic': 73.0733335018158}, {'ion_id': 2399, 'distance': 5.997857570648193, 'force': [3.4748947620391846, -1.8985097408294678, 8.336169242858887], 'magnitude': 9.22881031036377, 'cosine_ionic_motion': 0.0058180601336061954, 'motion_component_ionic': 0.05369377136230469, 'motion_component_percent_ionic': 0.5818060133606195}, {'ion_id': 2400, 'distance': 7.033089637756348, 'force': [4.853204727172852, -3.7680044174194336, -2.70151948928833], 'magnitude': 6.711904525756836, 'cosine_ionic_motion': -0.9859932661056519, 'motion_component_ionic': -6.617892742156982, 'motion_component_percent_ionic': 98.59932661056519}, {'ion_id': 2520, 'distance': 13.121502876281738, 'force': [0.47768887877464294, -0.24926194548606873, -1.8514750003814697], 'magnitude': 1.92828369140625, 'cosine_ionic_motion': -0.6686441898345947, 'motion_component_ionic': -1.2893357276916504, 'motion_component_percent_ionic': 66.86441898345947}], 'glu_contributions': [], 'asn_contributions': [{'resid': 458, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 5.911613941192627, 'force': [-6.197589874267578, -0.5701797008514404, 2.728013753890991], 'magnitude': 6.795386791229248, 'cosine_with_motion': 0.8682777881622314, 'motion_component': 5.900283336639404, 'motion_component_percent': 86.82777881622314}, {'resid': 458, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 5.043628692626953, 'force': [6.55202054977417, 1.054604411125183, -4.181386470794678], 'magnitude': 7.843797206878662, 'cosine_with_motion': -0.8431174159049988, 'motion_component': -6.613242149353027, 'motion_component_percent': 84.31174159049988}, {'resid': 458, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 5.3979716300964355, 'force': [-4.376787185668945, 1.0777528285980225, 1.4286543130874634], 'magnitude': 4.728516578674316, 'cosine_with_motion': 0.9656436443328857, 'motion_component': 4.566061973571777, 'motion_component_percent': 96.56436443328857}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': -0.860459125903062, 'motion_component_pip2': -6.7405559138481115, 'motion_component_percent_pip2': 86.0459125903062}, 576: {'frame': 576, 'motion_vector': [-1.9796028137207031, 2.7055091857910156, 8.789741516113281], 'ionic_force': [-0.5628997683525085, -0.05939200520515442, -6.551751971244812], 'ionic_force_magnitude': 6.576156738719347, 'radial_force': 0.5660243453188183, 'axial_force': -6.551751971244812, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-2.3665595054626465, 5.099774360656738, 2.3685860633850098], 'asn_force_magnitude': 6.100696875125754, 'residue_force': [-2.3665595054626465, 5.099774360656738, 2.3685860633850098], 'residue_force_magnitude': 6.100696875125754, 'total_force': [-2.929459273815155, 5.040382355451584, -4.183165907859802], 'total_force_magnitude': 7.17537894043024, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': 0.6847997131850782, 'cosine_residue_motion': 0.6847997131850782, 'cosine_ionic_motion': -0.9154662489972331, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': 4.177755470315219, 'motion_component_residue': 4.177755470315219, 'motion_component_ionic': -6.020249542413278, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 68.47997131850782, 'motion_component_percent_residue': 68.47997131850782, 'motion_component_percent_ionic': 91.54662489972331, 'ionic_contributions': [{'ion_id': 2398, 'distance': 13.145548820495605, 'force': [-0.6126810312271118, -0.3671928942203522, 1.7835184335708618], 'magnitude': 1.9212356805801392, 'cosine_ionic_motion': 0.8795133829116821, 'motion_component_ionic': 1.689752459526062, 'motion_component_percent_ionic': 87.95133829116821}, {'ion_id': 2399, 'distance': 10.647246360778809, 'force': [0.6410248279571533, -0.7755661010742188, -2.7503485679626465], 'magnitude': 2.9286229610443115, 'cosine_ionic_motion': -0.9996935725212097, 'motion_component_ionic': -2.9277255535125732, 'motion_component_percent_ionic': 99.96935725212097}, {'ion_id': 2400, 'distance': 7.618748188018799, 'force': [-0.59124356508255, 1.0833669900894165, -5.584921836853027], 'magnitude': 5.719668388366699, 'cosine_ionic_motion': -0.8361108303070068, 'motion_component_ionic': -4.782276630401611, 'motion_component_percent_ionic': 83.61108303070068}], 'glu_contributions': [], 'asn_contributions': [{'resid': 786, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 5.718953609466553, 'force': [-2.3665595054626465, 5.099774360656738, 2.3685860633850098], 'magnitude': 6.100697040557861, 'cosine_with_motion': 0.6847996711730957, 'motion_component': 4.177755355834961, 'motion_component_percent': 68.47996711730957}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': -0.25678003731850035, 'motion_component_pip2': -1.8424940720980585, 'motion_component_percent_pip2': 25.678003731850037}, 581: {'frame': 581, 'motion_vector': [3.5489273071289062, -1.7108230590820312, -7.8467559814453125], 'ionic_force': [-6.194060891866684, 6.701804757118225, -8.132934629917145], 'ionic_force_magnitude': 12.223960202372647, 'radial_force': 9.125819269231929, 'axial_force': -8.132934629917145, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-0.010998680256307125, -3.837313652038574, -6.3393144607543945], 'asn_force_magnitude': 7.410263481646168, 'residue_force': [-0.010998680256307125, -3.837313652038574, -6.3393144607543945], 'residue_force_magnitude': 7.410263481646168, 'total_force': [-6.205059572122991, 2.864491105079651, -14.47224909067154], 'total_force_magnitude': 16.0048138798025, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': 0.8648223531241873, 'cosine_residue_motion': 0.8648223531241873, 'cosine_ionic_motion': 0.28295282210029593, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': 6.408561501467472, 'motion_component_residue': 6.408561501467472, 'motion_component_ionic': 3.458804036503045, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 86.48223531241874, 'motion_component_percent_residue': 86.48223531241874, 'motion_component_percent_ionic': 28.295282210029594, 'ionic_contributions': [{'ion_id': 2276, 'distance': 10.55654239654541, 'force': [-1.18734872341156, 0.6714307069778442, -2.6485495567321777], 'magnitude': 2.979166269302368, 'cosine_ionic_motion': 0.5894966721534729, 'motion_component_ionic': 1.7562086582183838, 'motion_component_percent_ionic': 58.94966721534729}, {'ion_id': 2399, 'distance': 6.965061664581299, 'force': [-2.951920747756958, 5.079656600952148, -3.509826183319092], 'magnitude': 6.843656063079834, 'cosine_ionic_motion': 0.13936278223991394, 'motion_component_ionic': 0.9537509083747864, 'motion_component_percent_ionic': 13.936278223991394}, {'ion_id': 2400, 'distance': 13.888945579528809, 'force': [-1.56355881690979, 0.6279746294021606, -0.35075289011001587], 'magnitude': 1.721074104309082, 'cosine_ionic_motion': -0.2561647295951843, 'motion_component_ionic': -0.4408784806728363, 'motion_component_percent_ionic': 25.616472959518433}, {'ion_id': 2520, 'distance': 13.865456581115723, 'force': [-0.49123260378837585, 0.3227428197860718, -1.6238059997558594], 'magnitude': 1.7269099950790405, 'cosine_ionic_motion': 0.6889316439628601, 'motion_component_ionic': 1.1897228956222534, 'motion_component_percent_ionic': 68.89316439628601}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 5.1890692710876465, 'force': [-0.010998680256307125, -3.837313652038574, -6.3393144607543945], 'magnitude': 7.410263538360596, 'cosine_with_motion': 0.8648223876953125, 'motion_component': 6.408561706542969, 'motion_component_percent': 86.48223876953125}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': 0.616524853839305, 'motion_component_pip2': 9.867365537970517, 'motion_component_percent_pip2': 61.6524853839305}, 582: {'frame': 582, 'motion_vector': [-2.150157928466797, 4.1082763671875, 8.685333251953125], 'ionic_force': [-1.1703637540340424, -0.1612742319703102, -4.11364483833313], 'ionic_force_magnitude': 4.279933942317226, 'radial_force': 1.1814231649389095, 'axial_force': -4.11364483833313, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [0.6357161998748779, -1.5886460542678833, -0.8043994903564453], 'asn_force_magnitude': 1.890764372577921, 'residue_force': [0.6357161998748779, -1.5886460542678833, -0.8043994903564453], 'residue_force_magnitude': 1.890764372577921, 'total_force': [-0.5346475541591644, -1.7499202862381935, -4.918044328689575], 'total_force_magnitude': 5.247402122413722, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': -0.7993218313288966, 'cosine_residue_motion': -0.7993218313288966, 'cosine_ionic_motion': -0.8038825570520771, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': -1.511329240900416, 'motion_component_residue': -1.511329240900416, 'motion_component_ionic': -3.4405642415639486, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 79.93218313288966, 'motion_component_percent_residue': 79.93218313288966, 'motion_component_percent_ionic': 80.38825570520771, 'ionic_contributions': [{'ion_id': 2399, 'distance': 11.272248268127441, 'force': [0.14949455857276917, -0.21502681076526642, -2.59970760345459], 'magnitude': 2.6128652095794678, 'cosine_ionic_motion': -0.924544632434845, 'motion_component_ionic': -2.41571044921875, 'motion_component_percent_ionic': 92.4544632434845}, {'ion_id': 2400, 'distance': 12.854537963867188, 'force': [-1.3198583126068115, 0.05375257879495621, -1.51393723487854], 'magnitude': 2.009209156036377, 'cosine_ionic_motion': -0.5100781321525574, 'motion_component_ionic': -1.0248537063598633, 'motion_component_percent_ionic': 51.00781321525574}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 5.431150436401367, 'force': [3.3828272819519043, 5.6304755210876465, -4.655178070068359], 'magnitude': 8.050867080688477, 'cosine_with_motion': -0.310018390417099, 'motion_component': -2.4959168434143066, 'motion_component_percent': 31.0018390417099}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 5.220830917358398, 'force': [-1.6956610679626465, -5.968802452087402, 3.8840720653533936], 'magnitude': 7.320374488830566, 'cosine_with_motion': 0.17841362953186035, 'motion_component': 1.3060545921325684, 'motion_component_percent': 17.841362953186035}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 5.099922180175781, 'force': [-5.217322826385498, -5.868323802947998, 8.532121658325195], 'magnitude': 11.595463752746582, 'cosine_with_motion': 0.5361886620521545, 'motion_component': 6.217356204986572, 'motion_component_percent': 53.618866205215454}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 4.585880279541016, 'force': [2.014850378036499, 2.9981794357299805, -5.465660572052002], 'magnitude': 6.551499366760254, 'cosine_with_motion': -0.6121522188186646, 'motion_component': -4.010514736175537, 'motion_component_percent': 61.215221881866455}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 5.792736530303955, 'force': [2.151022434234619, 1.6198252439498901, -3.099754571914673], 'magnitude': 4.105996608734131, 'cosine_with_motion': -0.6157599687576294, 'motion_component': -2.528308391571045, 'motion_component_percent': 61.57599687576294}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': -0.9436847733305737, 'motion_component_pip2': -4.951893482464365, 'motion_component_percent_pip2': 94.36847733305737}, 583: {'frame': 583, 'motion_vector': [6.1293487548828125, -4.2521209716796875, 1.9502792358398438], 'ionic_force': [-7.837743371725082, 9.096575856208801, -5.4587215185165405], 'ionic_force_magnitude': 13.189979305726634, 'radial_force': 12.007410772884443, 'axial_force': -5.4587215185165405, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-5.687160491943359, -2.4163736701011658, 3.010814070701599], 'asn_force_magnitude': 6.873693151648125, 'residue_force': [-5.687160491943359, -2.4163736701011658, 3.010814070701599], 'residue_force_magnitude': 6.873693151648125, 'total_force': [-13.524903863668442, 6.6802021861076355, -2.4479074478149414], 'total_force_magnitude': 15.282027896906177, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': -0.3530545861730067, 'cosine_residue_motion': -0.3530545861730067, 'cosine_ionic_motion': -0.9573623652073077, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': -2.4267888911353594, 'motion_component_residue': -2.4267888911353594, 'motion_component_ionic': -12.627589785165892, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 35.30545861730067, 'motion_component_percent_residue': 35.30545861730067, 'motion_component_percent_ionic': 95.73623652073077, 'ionic_contributions': [{'ion_id': 2276, 'distance': 10.01389217376709, 'force': [-0.9421094059944153, 1.5386027097702026, -2.776057243347168], 'magnitude': 3.3107948303222656, 'cosine_ionic_motion': -0.6945639252662659, 'motion_component_ionic': -2.299558639526367, 'motion_component_percent_ionic': 69.45639252662659}, {'ion_id': 2399, 'distance': 8.15213680267334, 'force': [-3.0953996181488037, 3.490309715270996, -1.7869313955307007], 'magnitude': 4.9956865310668945, 'cosine_ionic_motion': -0.9683117270469666, 'motion_component_ionic': -4.837381839752197, 'motion_component_percent_ionic': 96.83117270469666}, {'ion_id': 2400, 'distance': 8.245593070983887, 'force': [-3.45645809173584, 3.355445623397827, 0.7990020513534546], 'magnitude': 4.883085250854492, 'cosine_ionic_motion': -0.9002402424812317, 'motion_component_ionic': -4.395949840545654, 'motion_component_percent_ionic': 90.02402424812317}, {'ion_id': 2520, 'distance': 13.323786735534668, 'force': [-0.34377625584602356, 0.7122178077697754, -1.6947349309921265], 'magnitude': 1.8701772689819336, 'cosine_ionic_motion': -0.5853453278541565, 'motion_component_ionic': -1.094699501991272, 'motion_component_percent_ionic': 58.53453278541565}], 'glu_contributions': [], 'asn_contributions': [{'resid': 786, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 5.387730121612549, 'force': [-6.3974409103393555, -2.519684314727783, 4.433423042297363], 'magnitude': 8.18115520477295, 'cosine_with_motion': -0.31470000743865967, 'motion_component': -2.5746095180511475, 'motion_component_percent': 31.470000743865967}, {'resid': 786, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 5.210433483123779, 'force': [9.893861770629883, 3.6602487564086914, -3.4813380241394043], 'magnitude': 11.108809471130371, 'cosine_with_motion': 0.44701847434043884, 'motion_component': 4.965843200683594, 'motion_component_percent': 44.701847434043884}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 5.647787094116211, 'force': [-4.115983963012695, -0.8550354838371277, 0.9926395416259766], 'magnitude': 4.319460868835449, 'cosine_with_motion': -0.5901918411254883, 'motion_component': -2.5493106842041016, 'motion_component_percent': 59.01918411254883}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 4.856788635253906, 'force': [-5.067597389221191, -2.7019026279449463, 1.0660895109176636], 'magnitude': 5.841007232666016, 'cosine_with_motion': -0.3884110152721405, 'motion_component': -2.268711566925049, 'motion_component_percent': 38.84110152721405}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': -0.9851034678027899, 'motion_component_pip2': -15.054378676301251, 'motion_component_percent_pip2': 98.510346780279}, 588: {'frame': 588, 'motion_vector': [-3.1440467834472656, -1.0689125061035156, -1.0656280517578125], 'ionic_force': [3.358123615384102, 8.453951895236969, -6.7140625193715096], 'ionic_force_magnitude': 11.30596888272785, 'radial_force': 9.096499154245063, 'axial_force': -6.7140625193715096, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-5.200457751750946, -2.040408134460449, -6.035855293273926], 'asn_force_magnitude': 8.224328258542563, 'residue_force': [-5.200457751750946, -2.040408134460449, -6.035855293273926], 'residue_force_magnitude': 8.224328258542563, 'total_force': [-1.8423341363668442, 6.41354376077652, -12.749917812645435], 'total_force_magnitude': 14.39055742042786, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': 0.8703246920625803, 'cosine_residue_motion': 0.8703246920625803, 'cosine_ionic_motion': -0.31549113882850943, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': 7.157835959037634, 'motion_component_residue': 7.157835959037634, 'motion_component_ionic': -3.5669329983714997, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 87.03246920625803, 'motion_component_percent_residue': 87.03246920625803, 'motion_component_percent_ionic': 31.549113882850943, 'ionic_contributions': [{'ion_id': 2276, 'distance': 9.802630424499512, 'force': [0.5881482362747192, 1.5654650926589966, -3.0233571529388428], 'magnitude': 3.455038070678711, 'cosine_ionic_motion': -0.02495802752673626, 'motion_component_ionic': -0.08623093366622925, 'motion_component_percent_ionic': 2.495802752673626}, {'ion_id': 2399, 'distance': 8.010647773742676, 'force': [1.8164281845092773, 4.498349666595459, -1.797999620437622], 'magnitude': 5.173718452453613, 'cosine_ionic_motion': -0.4768018126487732, 'motion_component_ionic': -2.4668383598327637, 'motion_component_percent_ionic': 47.68018126487732}, {'ion_id': 2400, 'distance': 13.280184745788574, 'force': [0.7155779004096985, 1.7390025854110718, -0.08683473616838455], 'magnitude': 1.8824776411056519, 'cosine_ionic_motion': -0.6117209196090698, 'motion_component_ionic': -1.1515510082244873, 'motion_component_percent_ionic': 61.17209196090698}, {'ion_id': 2520, 'distance': 13.10085391998291, 'force': [0.2379692941904068, 0.6511345505714417, -1.8058710098266602], 'magnitude': 1.934367060661316, 'cosine_ionic_motion': 0.07117947936058044, 'motion_component_ionic': 0.13768723607063293, 'motion_component_percent_ionic': 7.117947936058044}], 'glu_contributions': [], 'asn_contributions': [{'resid': 786, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 3.3795905113220215, 'force': [-0.35776108503341675, -10.95163345336914, 17.67045021057129], 'magnitude': 20.792091369628906, 'cosine_with_motion': -0.08272851258516312, 'motion_component': -1.720098853111267, 'motion_component_percent': 8.272851258516312}, {'resid': 786, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 3.149078845977783, 'force': [-4.199350357055664, 4.893367767333984, -19.0595760345459], 'magnitude': 20.12080955505371, 'cosine_with_motion': 0.4030449390411377, 'motion_component': 8.109590530395508, 'motion_component_percent': 40.30449390411377}, {'resid': 786, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 3.4830784797668457, 'force': [9.743487358093262, 11.083256721496582, -20.005250930786133], 'magnitude': 24.85928726196289, 'cosine_with_motion': -0.24409690499305725, 'motion_component': -6.068075180053711, 'motion_component_percent': 24.409690499305725}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 3.3638532161712646, 'force': [-6.603811264038086, -2.3706917762756348, 9.951359748840332], 'magnitude': 12.176209449768066, 'cosine_with_motion': 0.29888567328453064, 'motion_component': 3.639294385910034, 'motion_component_percent': 29.888567328453064}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 4.124634265899658, 'force': [-3.783022403717041, -4.69470739364624, 5.407161712646484], 'magnitude': 8.098699569702148, 'cosine_with_motion': 0.39477020502090454, 'motion_component': 3.197125196456909, 'motion_component_percent': 39.477020502090454}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': 0.24953188787313627, 'motion_component_pip2': 3.590902960666134, 'motion_component_percent_pip2': 24.953188787313625}, 589: {'frame': 589, 'motion_vector': [-0.09171295166015625, -4.009864807128906, 3.2742767333984375], 'ionic_force': [-6.422350153326988, 14.170203149318695, -14.125219106674194], 'ionic_force_magnitude': 21.01340176164855, 'radial_force': 15.55767459438912, 'axial_force': -14.125219106674194, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [7.036518573760986, 3.6094744205474854, -1.2248984575271606], 'asn_force_magnitude': 8.002579300620667, 'residue_force': [7.036518573760986, 3.6094744205474854, -1.2248984575271606], 'residue_force_magnitude': 8.002579300620667, 'total_force': [0.6141684204339981, 17.77967756986618, -15.350117564201355], 'total_force_magnitude': 23.497239126583867, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': -0.4616776839966081, 'cosine_residue_motion': -0.4616776839966081, 'cosine_ionic_motion': -0.941920364529767, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': -3.694612277509745, 'motion_component_residue': -3.694612277509745, 'motion_component_ionic': -19.79295104734245, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 46.16776839966081, 'motion_component_percent_residue': 46.16776839966081, 'motion_component_percent_ionic': 94.19203645297671, 'ionic_contributions': [{'ion_id': 2276, 'distance': 10.057876586914062, 'force': [-0.3927546441555023, 0.9451647996902466, -3.118217706680298], 'magnitude': 3.2819011211395264, 'cosine_ionic_motion': -0.8217610716819763, 'motion_component_ionic': -2.6969385147094727, 'motion_component_percent_ionic': 82.17610716819763}, {'ion_id': 2399, 'distance': 5.531322956085205, 'force': [-5.342945575714111, 6.576251983642578, -6.779057502746582], 'magnitude': 10.85125732421875, 'cosine_ionic_motion': -0.8556908369064331, 'motion_component_ionic': -9.285321235656738, 'motion_component_percent_ionic': 85.56908369064331}, {'ion_id': 2400, 'distance': 7.016615867614746, 'force': [-0.520441472530365, 6.257226943969727, -2.4597721099853516], 'magnitude': 6.743458271026611, 'cosine_ionic_motion': -0.9479153752326965, 'motion_component_ionic': -6.392227649688721, 'motion_component_percent_ionic': 94.79153752326965}, {'ion_id': 2520, 'distance': 13.511331558227539, 'force': [-0.16620846092700958, 0.3915594220161438, -1.768171787261963], 'magnitude': 1.8186191320419312, 'cosine_ionic_motion': -0.7799671292304993, 'motion_component_ionic': -1.418463110923767, 'motion_component_percent_ionic': 77.99671292304993}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 5.742329120635986, 'force': [-2.895430326461792, -5.975179672241211, -6.290154457092285], 'magnitude': 9.146164894104004, 'cosine_with_motion': 0.07664317637681961, 'motion_component': 0.700991153717041, 'motion_component_percent': 7.664317637681961}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 5.3585309982299805, 'force': [0.896080493927002, 2.868612766265869, 3.7406623363494873], 'magnitude': 4.798380374908447, 'cosine_with_motion': 0.02668731100857258, 'motion_component': 0.1280558705329895, 'motion_component_percent': 2.668731100857258}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 5.2741923332214355, 'force': [2.260348081588745, 3.233445167541504, 2.9947509765625], 'magnitude': 4.953067302703857, 'cosine_with_motion': -0.13130389153957367, 'motion_component': -0.6503570079803467, 'motion_component_percent': 13.130389153957367}, {'resid': 786, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 5.224360466003418, 'force': [-6.243102073669434, -5.37437629699707, 2.800708770751953], 'magnitude': 8.700817108154297, 'cosine_with_motion': 0.694636881351471, 'motion_component': 6.043908596038818, 'motion_component_percent': 69.4636881351471}, {'resid': 786, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 5.226183891296387, 'force': [5.591629505157471, 3.199185609817505, -3.444932222366333], 'magnitude': 7.305386066436768, 'cosine_with_motion': -0.6509145498275757, 'motion_component': -4.755182266235352, 'motion_component_percent': 65.09145498275757}, {'resid': 786, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 5.666459083557129, 'force': [7.426992893218994, 5.657786846160889, -1.025933861732483], 'magnitude': 9.39272689819336, 'cosine_with_motion': -0.5495771765708923, 'motion_component': -5.1620283126831055, 'motion_component_percent': 54.95771765708923}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': -0.9995882153780047, 'motion_component_pip2': -23.487563324852193, 'motion_component_percent_pip2': 99.95882153780047}, 591: {'frame': 591, 'motion_vector': [-3.501201629638672, -1.3938102722167969, 5.450614929199219], 'ionic_force': [-1.188488394021988, 3.7774543166160583, -7.4679893255233765], 'ionic_force_magnitude': 8.452959856936348, 'radial_force': 3.9600083051486465, 'axial_force': -7.4679893255233765, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [3.982780933380127, 1.4798874855041504, 14.609102487564087], 'asn_force_magnitude': 15.214417058343026, 'residue_force': [3.982780933380127, 1.4798874855041504, 14.609102487564087], 'residue_force_magnitude': 15.214417058343026, 'total_force': [2.794292539358139, 5.257341802120209, 7.1411131620407104], 'total_force_magnitude': 9.297484112000634, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': 0.631051085787851, 'cosine_residue_motion': 0.631051085787851, 'cosine_ionic_motion': -0.7464112574309749, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': 9.601074404296568, 'motion_component_residue': 9.601074404296568, 'motion_component_ionic': -6.309384395829413, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 63.1051085787851, 'motion_component_percent_residue': 63.1051085787851, 'motion_component_percent_ionic': 74.64112574309749, 'ionic_contributions': [{'ion_id': 2276, 'distance': 11.154449462890625, 'force': [0.3540971577167511, 0.6324486136436462, -2.568011522293091], 'magnitude': 2.6683437824249268, 'cosine_ionic_motion': -0.9115911722183228, 'motion_component_ionic': -2.432438611984253, 'motion_component_percent_ionic': 91.15911722183228}, {'ion_id': 2399, 'distance': 8.533595085144043, 'force': [-0.9546760320663452, 1.9802272319793701, -3.9940202236175537], 'magnitude': 4.559046268463135, 'cosine_ionic_motion': -0.7013271450996399, 'motion_component_ionic': -3.197382926940918, 'motion_component_percent_ionic': 70.13271450996399}, {'ion_id': 2400, 'distance': 14.457233428955078, 'force': [-0.5879095196723938, 1.164778470993042, -0.9059575796127319], 'magnitude': 1.5884286165237427, 'cosine_ionic_motion': -0.4278210401535034, 'motion_component_ionic': -0.6795631647109985, 'motion_component_percent_ionic': 42.78210401535034}], 'glu_contributions': [], 'asn_contributions': [{'resid': 786, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 3.6577396392822266, 'force': [-5.303252696990967, -8.560955047607422, -14.616823196411133], 'magnitude': 17.750097274780273, 'cosine_with_motion': -0.41804322600364685, 'motion_component': -7.4203081130981445, 'motion_component_percent': 41.804322600364685}, {'resid': 786, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 2.6373789310455322, 'force': [8.30610466003418, 7.949903964996338, 26.280881881713867], 'magnitude': 28.685834884643555, 'cosine_with_motion': 0.542306125164032, 'motion_component': 15.556503295898438, 'motion_component_percent': 54.2306125164032}, {'resid': 786, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 4.588602066040039, 'force': [7.176278114318848, 6.267814636230469, 10.695006370544434], 'magnitude': 14.323674201965332, 'cosine_with_motion': 0.2574140429496765, 'motion_component': 3.687114715576172, 'motion_component_percent': 25.74140429496765}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 4.677822589874268, 'force': [-4.089120388031006, -1.7920253276824951, -4.439994812011719], 'magnitude': 6.296492099761963, 'cosine_with_motion': -0.17702500522136688, 'motion_component': -1.1146365404129028, 'motion_component_percent': 17.70250052213669}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 5.477795124053955, 'force': [-2.1072287559509277, -2.3848507404327393, -3.3099677562713623], 'magnitude': 4.591711521148682, 'cosine_with_motion': -0.24121727049350739, 'motion_component': -1.1076000928878784, 'motion_component_percent': 24.12172704935074}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': 0.35404093933523795, 'motion_component_pip2': 3.291690008467155, 'motion_component_percent_pip2': 35.4040939335238}, 592: {'frame': 592, 'motion_vector': [-0.7360458374023438, -2.419464111328125, -1.2374954223632812], 'ionic_force': [-12.649452447891235, 2.285761058330536, -6.635545194149017], 'ionic_force_magnitude': 14.465953507143455, 'radial_force': 12.854312538881334, 'axial_force': -6.635545194149017, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [6.672793388366699, 3.4266207218170166, -2.720718026161194], 'asn_force_magnitude': 7.97936136247097, 'residue_force': [6.672793388366699, 3.4266207218170166, -2.720718026161194], 'residue_force_magnitude': 7.97936136247097, 'total_force': [-5.976659059524536, 5.7123817801475525, -9.356263220310211], 'total_force_magnitude': 12.485648584021899, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': -0.43778533768112665, 'cosine_residue_motion': -0.43778533768112665, 'cosine_ionic_motion': 0.2944291768168729, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': -3.493247408549088, 'motion_component_residue': -3.493247408549088, 'motion_component_ionic': 4.259198782979404, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_com</t>
+          <t>{574: {'frame': 574, 'motion_vector': [-5.495319366455078, 2.858715057373047, 2.9860458374023438], 'ionic_force': [9.93061837553978, -6.6990053951740265, 0.2928283214569092], 'ionic_force_magnitude': 11.982470656380775, 'radial_force': 11.978892044140771, 'axial_force': 0.2928283214569092, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-4.0223565101623535, 1.5621775388717651, -0.024718403816223145], 'asn_force_magnitude': 4.315131696401413, 'residue_force': [-4.0223565101623535, 1.5621775388717651, -0.024718403816223145], 'residue_force_magnitude': 4.315131696401413, 'pip2_force': [0.6445247805677354, 0.1866492098197341, -4.676992440184222], 'pip2_force_magnitude': 4.724881840409618, 'total_force': [6.552786645945162, -4.950178646482527, -4.408882522543536], 'total_force_magnitude': 9.321026046361993, 'cosine_total_motion': -0.9879746607329254, 'cosine_glu_motion': 0, 'cosine_asn_motion': 0.8929282470610925, 'cosine_residue_motion': 0.8929282470610925, 'cosine_pip2_motion': -0.5224218753743789, 'cosine_ionic_motion': -0.8840963770449431, 'motion_component_total': -9.208937545837252, 'motion_component_glu': 0, 'motion_component_asn': 3.8531029815054723, 'motion_component_residue': 3.8531029815054723, 'motion_component_ionic': -10.593658895353585, 'motion_component_pip2': -2.4683816319891396, 'motion_component_percent_total': 98.79746607329254, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 89.29282470610926, 'motion_component_percent_residue': 89.29282470610926, 'motion_component_percent_ionic': 88.40963770449432, 'motion_component_percent_pip2': 52.24218753743789, 'ionic_contributions': [{'ion_id': 2276, 'distance': 9.409431457519531, 'force': [1.1248300075531006, -0.7832292914390564, -3.4903464317321777], 'magnitude': 3.7498278617858887, 'cosine_ionic_motion': -0.730733335018158, 'motion_component_ionic': -2.740124225616455, 'motion_component_percent_ionic': 73.0733335018158}, {'ion_id': 2399, 'distance': 5.997857570648193, 'force': [3.4748947620391846, -1.8985097408294678, 8.336169242858887], 'magnitude': 9.22881031036377, 'cosine_ionic_motion': 0.0058180601336061954, 'motion_component_ionic': 0.05369377136230469, 'motion_component_percent_ionic': 0.5818060133606195}, {'ion_id': 2400, 'distance': 7.033089637756348, 'force': [4.853204727172852, -3.7680044174194336, -2.70151948928833], 'magnitude': 6.711904525756836, 'cosine_ionic_motion': -0.9859932661056519, 'motion_component_ionic': -6.617892742156982, 'motion_component_percent_ionic': 98.59932661056519}, {'ion_id': 2520, 'distance': 13.121502876281738, 'force': [0.47768887877464294, -0.24926194548606873, -1.8514750003814697], 'magnitude': 1.92828369140625, 'cosine_ionic_motion': -0.6686441898345947, 'motion_component_ionic': -1.2893357276916504, 'motion_component_percent_ionic': 66.86441898345947}], 'glu_contributions': [], 'asn_contributions': [{'resid': 458, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 5.911613941192627, 'force': [-6.197589874267578, -0.5701797008514404, 2.728013753890991], 'magnitude': 6.795386791229248, 'cosine_with_motion': 0.8682777881622314, 'motion_component': 5.900283336639404, 'motion_component_percent': 86.82777881622314}, {'resid': 458, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 5.043628692626953, 'force': [6.55202054977417, 1.054604411125183, -4.181386470794678], 'magnitude': 7.843797206878662, 'cosine_with_motion': -0.8431174159049988, 'motion_component': -6.613242149353027, 'motion_component_percent': 84.31174159049988}, {'resid': 458, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 5.3979716300964355, 'force': [-4.376787185668945, 1.0777528285980225, 1.4286543130874634], 'magnitude': 4.728516578674316, 'cosine_with_motion': 0.9656436443328857, 'motion_component': 4.566061973571777, 'motion_component_percent': 96.56436443328857}], 'pip2_contributions': [{'resid': 1313, 'atom': 'C1', 'charge': 0.06000000238418579, 'distance': 27.402389526367188, 'force': [-0.01598701998591423, -0.016060246154665947, 0.013792908750474453], 'magnitude': 0.026528486981987953, 'cosine_with_motion': 0.455685019493103, 'motion_component': 0.012088634073734283, 'motion_component_percent': 45.5685019493103}, {'resid': 1313, 'atom': 'C11', 'charge': 0.17000000178813934, 'distance': 26.513216018676758, 'force': [-0.055607374757528305, -0.04632038623094559, 0.03476704657077789], 'magnitude': 0.08029013872146606, 'cosine_with_motion': 0.5016644597053528, 'motion_component': 0.040278710424900055, 'motion_component_percent': 50.16644597053528}, {'resid': 1313, 'atom': 'C12', 'charge': 0.04000000283122063, 'distance': 26.91480255126953, 'force': [-0.013379307463765144, -0.010296311229467392, 0.00714502390474081], 'magnitude': 0.01833224669098854, 'cosine_with_motion': 0.5189841389656067, 'motion_component': 0.00951414555311203, 'motion_component_percent': 51.89841389656067}, {'resid': 1313, 'atom': 'C13', 'charge': -0.05000000074505806, 'distance': 28.121273040771484, 'force': [0.01517635490745306, 0.012300416827201843, -0.007681811694055796], 'magnitude': 0.020991241559386253, 'cosine_with_motion': -0.49307140707969666, 'motion_component': -0.0103501807898283, 'motion_component_percent': 49.307140707969666}, {'resid': 1313, 'atom': 'C2', 'charge': 0.06000000238418579, 'distance': 28.834280014038086, 'force': [-0.014851991087198257, -0.014281874522566795, 0.01222646702080965], 'magnitude': 0.02395913377404213, 'cosine_with_motion': 0.46916088461875916, 'motion_component': 0.011240688152611256, 'motion_component_percent': 46.916088461875916}, {'resid': 1313, 'atom': 'C21', 'charge': 0.6299999952316284, 'distance': 24.718509674072266, 'force': [-0.25818294286727905, -0.1850576549768448, 0.12758991122245789], 'magnitude': 0.3423214256763458, 'cosine_with_motion': 0.5398304462432861, 'motion_component': 0.1847955286502838, 'motion_component_percent': 53.98304462432861}, {'resid': 1313, 'atom': 'C210', 'charge': -0.18000000715255737, 'distance': 20.989748001098633, 'force': [0.1097487285733223, 0.07970749586820602, 0.0009218301856890321], 'magnitude': 0.1356426179409027, 'cosine_with_motion': -0.3993440270423889, 'motion_component': -0.05416806787252426, 'motion_component_percent': 39.93440270423889}, {'resid': 1313, 'atom': 'C211', 'charge': -0.15000000596046448, 'distance': 21.944766998291016, 'force': [0.08490826189517975, 0.058728888630867004, 0.005947514902800322], 'magnitude': 0.10341116040945053, 'cosine_with_motion': -0.39508315920829773, 'motion_component': -0.0408560074865818, 'motion_component_percent': 39.50831592082977}, {'resid': 1313, 'atom': 'C212', 'charge': -0.15000000596046448, 'distance': 22.32193374633789, 'force': [0.0798613652586937, 0.05907154083251953, 0.011042341589927673], 'magnitude': 0.09994607418775558, 'cosine_with_motion': -0.34486645460128784, 'motion_component': -0.03446804732084274, 'motion_component_percent': 34.486645460128784}, {'resid': 1313, 'atom': 'C213', 'charge': -0.18000000715255737, 'distance': 21.862707138061523, 'force': [0.0949091762304306, 0.07975561171770096, 0.0162160973995924], 'magnitude': 0.12502668797969818, 'cosine_with_motion': -0.2851226031780243, 'motion_component': -0.035647936165332794, 'motion_component_percent': 28.51226031780243}, {'resid': 1313, 'atom': 'C214', 'charge': -0.15000000596046448, 'distance': 21.32759666442871, 'force': [0.08263921737670898, 0.06865246593952179, 0.0210727471858263], 'magnitude': 0.10948270559310913, 'cosine_with_motion': -0.2589397132396698, 'motion_component': -0.02834942191839218, 'motion_component_percent': 25.89397132396698}, {'resid': 1313, 'atom': 'C215', 'charge': -0.15000000596046448, 'distance': 21.243288040161133, 'force': [0.07940758019685745, 0.07188725471496582, 0.026543162763118744], 'magnitude': 0.11035343259572983, 'cosine_with_motion': -0.1997826099395752, 'motion_component': -0.02204669639468193, 'motion_component_percent': 19.97826099395752}, {'resid': 1313, 'atom': 'C216', 'charge': -0.18000000715255737, 'distance': 21.75861358642578, 'force': [0.08496736735105515, 0.08838987350463867, 0.030012227594852448], 'magnitude': 0.1262258142232895, 'cosine_with_motion': -0.14357523620128632, 'motion_component': -0.018122900277376175, 'motion_component_percent': 14.357523620128632}, {'resid': 1313, 'atom': 'C217', 'charge': -0.18000000715255737, 'distance': 22.94518280029297, 'force': [0.07480096071958542, 0.07911965996026993, 0.03207841143012047], 'magnitude': 0.11350827664136887, 'cosine_with_motion': -0.11413389444351196, 'motion_component': -0.012955141253769398, 'motion_component_percent': 11.413389444351196}, {'resid': 1313, 'atom': 'C218', 'charge': -0.18000000715255737, 'distance': 22.520280838012695, 'force': [0.07689394056797028, 0.07943665981292725, 0.04076153412461281], 'magnitude': 0.11783193051815033, 'cosine_with_motion': -0.09102306514978409, 'motion_component': -0.010725423693656921, 'motion_component_percent': 9.102306514978409}, {'resid': 1313, 'atom': 'C219', 'charge': -0.18000000715255737, 'distance': 23.829050064086914, 'force': [0.06805725395679474, 0.06955601274967194, 0.040080681443214417], 'magnitude': 0.10524395108222961, 'cosine_with_motion': -0.0766497328877449, 'motion_component': -0.008066920563578606, 'motion_component_percent': 7.66497328877449}, {'resid': 1313, 'atom': 'C22', 'charge': -0.08000000566244125, 'distance': 23.81096076965332, 'force': [0.036265384405851364, 0.025475643575191498, -0.015178241766989231], 'magnitude': 0.046846188604831696, 'cosine_with_motion': -0.5332604646682739, 'motion_component': -0.024981221184134483, 'motion_component_percent': 53.32604646682739}, {'resid': 1313, 'atom': 'C220', 'charge': -0.27000001072883606, 'distance': 25.01742172241211, 'force': [0.0884084701538086, 0.09920471161603928, 0.05343755707144737], 'magnitude': 0.1432243138551712, 'cosine_with_motion': -0.043322257697582245, 'motion_component': -0.006204800680279732, 'motion_component_percent': 4.3322257697582245}, {'resid': 1313, 'atom': 'C23', 'charge': -0.18000000715255737, 'distance': 22.606430053710938, 'force': [0.08748061954975128, 0.06767256557941437, -0.0379670113325119], 'magnitude': 0.11693557351827621, 'cosine_with_motion': -0.4982472360134125, 'motion_component': -0.05826282501220703, 'motion_component_percent': 49.82472360134125}, {'resid': 1313, 'atom': 'C24', 'charge': -0.18000000715255737, 'distance': 21.731489181518555, 'force': [0.09698843955993652, 0.07352207601070404, -0.03464677184820175], 'magnitude': 0.1265411078929901, 'cosine_with_motion': -0.48985952138900757, 'motion_component': -0.061987366527318954, 'motion_component_percent': 48.98595213890076}, {'resid': 1313, 'atom': 'C25', 'charge': -0.15000000596046448, 'distance': 22.326690673828125, 'force': [0.07700181752443314, 0.05997266620397568, -0.021323855966329575], 'magnitude': 0.09990349411964417, 'cosine_with_motion': -0.45907098054885864, 'motion_component': -0.045862793922424316, 'motion_component_percent': 45.907098054885864}, {'resid': 1313, 'atom': 'C26', 'charge': -0.15000000596046448, 'distance': 21.762929916381836, 'force': [0.08248762786388397, 0.0629764050245285, -0.016897939145565033], 'magnitude': 0.10514645278453827, 'cosine_with_motion': -0.44771942496299744, 'motion_component': -0.047076109796762466, 'motion_component_percent': 44.771942496299744}, {'resid': 1313, 'atom': 'C27', 'charge': -0.18000000715255737, 'distance': 20.253379821777344, 'force': [0.1153358742594719, 0.08644368499517441, -0.021197110414505005], 'magnitude': 0.14568524062633514, 'cosine_with_motion': -0.4491698145866394, 'motion_component': -0.06543741375207901, 'motion_component_percent': 44.91698145866394}, {'resid': 1313, 'atom': 'C28', 'charge': -0.15000000596046448, 'distance': 20.08144187927246, 'force': [0.10253174602985382, 0.06770477443933487, -0.012394802644848824], 'magnitude': 0.12349221110343933, 'cosine_with_motion': -0.47916385531425476, 'motion_component': -0.05917300283908844, 'motion_component_percent': 47.916385531425476}, {'resid': 1313, 'atom': 'C29', 'charge': -0.15000000596046448, 'distance': 20.329374313354492, 'force': [0.10087910294532776, 0.06576956808567047, -0.00419965386390686], 'magnitude': 0.1204984113574028, 'cosine_with_motion': -0.4572524428367615, 'motion_component': -0.055098194628953934, 'motion_component_percent': 45.72524428367615}, {'resid': 1313, 'atom': 'C3', 'charge': 0.06000000238418579, 'distance': 29.434846878051758, 'force': [-0.014295089058578014, -0.012924598529934883, 0.012538362294435501], 'magnitude': 0.022991418838500977, 'cosine_with_motion': 0.49998340010643005, 'motion_component': 0.011495327576994896, 'motion_component_percent': 49.998340010643005}, {'resid': 1313, 'atom': 'C31', 'charge': 0.6299999952316284, 'distance': 29.705068588256836, 'force': [-0.18095967173576355, -0.13007664680480957, 0.08074997365474701], 'magnitude': 0.2370377480983734, 'cosine_with_motion': 0.5298762917518616, 'motion_component': 0.1256006807088852, 'motion_component_percent': 52.98762917518616}, {'resid': 1313, 'atom': 'C310', 'charge': -0.18000000715255737, 'distance': 23.53643226623535, 'force': [0.09357346594333649, 0.051546595990657806, -0.014980881474912167], 'magnitude': 0.10787711292505264, 'cosine_with_motion': -0.5548380613327026, 'motion_component': -0.059854328632354736, 'motion_component_percent': 55.483806133270264}, {'resid': 1313, 'atom': 'C311', 'charge': -0.18000000715255737, 'distance': 23.462108612060547, 'force': [0.09750301390886307, 0.04634115844964981, -0.011458470486104488], 'magnitude': 0.108561672270298, 'cosine_with_motion': -0.5861093997955322, 'motion_component': -0.06362901628017426, 'motion_component_percent': 58.61093997955322}, {'resid': 1313, 'atom': 'C312', 'charge': -0.18000000715255737, 'distance': 22.221818923950195, 'force': [0.1098579540848732, 0.05003775283694267, -0.008538385853171349], 'magnitude': 0.12101838737726212, 'cosine_with_motion': -0.5841884613037109, 'motion_component': -0.07069754600524902, 'motion_component_percent': 58.418846130371094}, {'resid': 1313, 'atom': 'C313', 'charge': -0.18000000715255737, 'distance': 22.356657028198242, 'force': [0.11110129207372665, 0.044062964618206024, -0.003205313580110669], 'magnitude': 0.1195630207657814, 'cosine_with_motion': -0.601015031337738, 'motion_component': -0.07185917347669601, 'motion_component_percent': 60.101503133773804}, {'resid': 1313, 'atom': 'C314', 'charge': -0.18000000715255737, 'distance': 21.08416748046875, 'force': [0.12545935809612274, 0.04822041839361191, 0.002508534351363778], 'magnitude': 0.13443046808242798, 'cosine_with_motion': -0.5885848999023438, 'motion_component': -0.07912374287843704, 'motion_component_percent': 58.858489990234375}, {'resid': 1313, 'atom': 'C315', 'charge': -0.18000000715255737, 'distance': 19.7880916595459, 'force': [0.14417116343975067, 0.050034087151288986, -0.0017885675188153982], 'magnitude': 0.152616947889328, 'cosine_with_motion': -0.623711884021759, 'motion_component': -0.09518900513648987, 'motion_component_percent': 62.3711884021759}, {'resid': 1313, 'atom': 'C316', 'charge': -0.18000000715255737, 'distance': 18.821378707885742, 'force': [0.1562066525220871, 0.06322502344846725, -0.00779768219217658], 'magnitude': 0.16869714856147766, 'cosine_with_motion': -0.6042345762252808, 'motion_component': -0.10193265229463577, 'motion_component_percent': 60.423457622528076}, {'resid': 1313, 'atom': 'C317', 'charge': -0.18000000715255737, 'distance': 17.54347038269043, 'force': [0.177896648645401, 0.07780766487121582, -0.0005468409508466721], 'magnitude': 0.19416886568069458, 'cosine_with_motion': -0.5668008923530579, 'motion_component': -0.11005508899688721, 'motion_component_percent': 56.680089235305786}, {'resid': 1313, 'atom': 'C318', 'charge': -0.27000001072883606, 'distance': 16.768815994262695, 'force': [0.28250983357429504, 0.14683420956134796, -0.015855953097343445], 'magnitude': 0.3187844157218933, 'cosine_with_motion': -0.5383182168006897, 'motion_component': -0.17160744965076447, 'motion_component_percent': 53.83182168006897}, {'resid': 1313, 'atom': 'C32', 'charge': -0.08000000566244125, 'distance': 30.127117156982422, 'force': [0.02311633713543415, 0.015633665025234222, -0.008804736658930779], 'magnitude': 0.02926260232925415, 'cosine_with_motion': -0.5398436784744263, 'motion_component': -0.01579723134636879, 'motion_component_percent': 53.98436784744263}, {'resid': 1313, 'atom': 'C33', 'charge': -0.18000000715255737, 'distance': 29.63701820373535, 'force': [0.05549591779708862, 0.0336141362786293, -0.020475614815950394], 'magnitude': 0.06803644448518753, 'cosine_with_motion': -0.5771322846412659, 'motion_component': -0.03926602751016617, 'motion_component_percent': 57.71322846412659}, {'resid': 1313, 'atom': 'C34', 'charge': -0.18000000715255737, 'distance': 28.112001419067383, 'force': [0.061979737132787704, 0.03677040711045265, -0.02290373481810093], 'magnitude': 0.07561832666397095, 'cosine_with_motion': -0.5843786597251892, 'motion_component': -0.04418973624706268, 'motion_component_percent': 58.43786597251892}, {'resid': 1313, 'atom': 'C35', 'charge': -0.18000000715255737, 'distance': 27.35348892211914, 'force': [0.06513121724128723, 0.04118206351995468, -0.021005263552069664], 'magnitude': 0.07987026870250702, 'cosine_with_motion': -0.5515170097351074, 'motion_component': -0.044049810618162155, 'motion_component_percent': 55.15170097351074}, {'resid': 1313, 'atom': 'C36', 'charge': -0.18000000715255737, 'distance': 27.78740692138672, 'force': [0.06429164111614227, 0.039864808320999146, -0.016352808102965355], 'magnitude': 0.07739529758691788, 'cosine_with_motion': -0.5414569973945618, 'motion_component': -0.04190622642636299, 'motion_component_percent': 54.14569973945618}, {'resid': 1313, 'atom': 'C37', 'charge': -0.18000000715255737, 'distance': 27.4178409576416, 'force': [0.068262480199337, 0.03787865862250328, -0.015000693500041962], 'magnitude': 0.07949578762054443, 'cosine_with_motion': -0.5700680613517761, 'motion_component': -0.045318007469177246, 'motion_component_percent': 57.00680613517761}, {'resid': 1313, 'atom': 'C38', 'charge': -0.18000000715255737, 'distance': 25.86261749267578, 'force': [0.07760042697191238, 0.04102439060807228, -0.016659297049045563], 'magnitude': 0.08934404700994492, 'cosine_with_motion': -0.584177553653717, 'motion_component': -0.05219278857111931, 'motion_component_percent': 58.417755365371704}, {'resid': 1313, 'atom': 'C39', 'charge': -0.18000000715255737, 'distance': 25.00602149963379, 'force': [0.08180726319551468, 0.047219183295965195, -0.014544346369802952], 'magnitude': 0.09556996077299118, 'cosine_with_motion': -0.5447418093681335, 'motion_component': -0.05206095054745674, 'motion_component_percent': 54.474180936813354}, {'resid': 1313, 'atom': 'C4', 'charge': 0.08000000566244125, 'distance': 29.475217819213867, 'force': [-0.017802823334932327, -0.017433788627386093, 0.01771235466003418], 'magnitude': 0.030571309849619865, 'cosine_with_motion': 0.4798832833766937, 'motion_component': 0.014670660719275475, 'motion_component_percent': 47.98832833766937}, {'resid': 1313, 'atom': 'C5', 'charge': 0.08000000566244125, 'distance': 28.110876083374023, 'force': [-0.018982261419296265, -0.019330019131302834, 0.019892528653144836], 'magnitude': 0.033610839396715164, 'cosine_with_motion': 0.46924152970314026, 'motion_component': 0.01577160134911537, 'motion_component_percent': 46.924152970314026}, {'resid': 1313, 'atom': 'C6', 'charge': 0.06000000238418579, 'distance': 27.347814559936523, 'force': [-0.015022143721580505, -0.016221214085817337, 0.014852693304419518], 'magnitude': 0.026634471490979195, 'cosine_with_motion': 0.43968746066093445, 'motion_component': 0.011710843071341515, 'motion_component_percent': 43.968746066093445}, {'resid': 1313, 'atom': 'H1', 'charge': 0.12000000476837158, 'distance': 26.872238159179688, 'force': [-0.03451615199446678, -0.03192678838968277, 0.028864610940217972], 'magnitude': 0.05517110228538513, 'cosine_with_motion': 0.4865696430206299, 'motion_component': 0.026844583451747894, 'motion_component_percent': 48.65696430206299}, {'resid': 1313, 'atom': 'H10R', 'charge': 0.09000000357627869, 'distance': 21.600147247314453, 'force': [-0.05052445828914642, -0.039332713931798935, 0.0012797724921256304], 'magnitude': 0.0640423372387886, 'cosine_with_motion': 0.3838138282299042, 'motion_component': 0.0245803352445364, 'motion_component_percent': 38.38138282299042}, {'resid': 1313, 'atom': 'H10S', 'charge': 0.09000000357627869, 'distance': 20.172346115112305, 'force': [-0.058071963489055634, -0.044898707419633865, -0.0018910818034783006], 'magnitude': 0.07342903316020966, 'cosine_with_motion': 0.36662667989730835, 'motion_component': 0.026921043172478676, 'motion_component_percent': 36.662667989730835}, {'resid': 1313, 'atom': 'H10X', 'charge': 0.09000000357627869, 'distance': 22.991798400878906, 'force': [-0.04890096187591553, -0.026489781215786934, 0.01009838841855526], 'magnitude': 0.05652424320578575, 'cosine_with_motion': 0.5741134285926819, 'motion_component': 0.0324513278901577, 'motion_component_percent': 57.41134285926819}, {'resid': 1313, 'atom': 'H10Y', 'charge': 0.09000000357627869, 'distance': 23.003032684326172, 'force': [-0.04803583398461342, -0.0288775023072958, 0.006884868256747723], 'magnitude': 0.05646904185414314, 'cosine_with_motion': 0.5201421976089478, 'motion_component': 0.02937193028628826, 'motion_component_percent': 52.014219760894775}, {'resid': 1313, 'atom': 'H111', 'charge': 0.15000000596046448, 'distance': 22.47832489013672, 'force': [-0.08321110159158707, -0.05262521654367447, -0.004539594519883394], 'magnitude': 0.09856017678976059, 'cosine_with_motion': 0.4327154755592346, 'motion_component': 0.04264851287007332, 'motion_component_percent': 43.27154755592346}, {'resid': 1313, 'atom': 'H11A', 'charge': 0.09000000357627869, 'distance': 27.334951400756836, 'force': [-0.027288133278489113, -0.02281026728451252, 0.0182810015976429], 'magnitude': 0.03998931869864464, 'cosine_with_motion': 0.5066989064216614, 'motion_component': 0.020262543112039566, 'motion_component_percent': 50.66989064216614}, {'resid': 1313, 'atom': 'H11B', 'charge': 0.09000000357627869, 'distance': 25.559093475341797, 'force': [-0.03164472430944443, -0.025831986218690872, 0.02057681605219841], 'magnitude': 0.045739319175481796, 'cosine_with_motion': 0.5134486556053162, 'motion_component': 0.023484792560338974, 'motion_component_percent': 51.344865560531616}, {'resid': 1313, 'atom': 'H11X', 'charge': 0.09000000357627869, 'distance': 24.339977264404297, 'force': [-0.045453786849975586, -0.02149791643023491, 0.003946943208575249], 'magnitude': 0.050435952842235565, 'cosine_with_motion': 0.5769813656806946, 'motion_component': 0.029100604355335236, 'motion_component_percent': 57.69813656806946}, {'resid': 1313, 'atom': 'H11Y', 'charge': 0.09000000357627869, 'distance': 23.785486221313477, 'force': [-0.04784690588712692, -0.02111019194126129, 0.007378881331533194], 'magnitude': 0.05281490832567215, 'cosine_with_motion': 0.6184708476066589, 'motion_component': 0.03266448155045509, 'motion_component_percent': 61.847084760665894}, {'resid': 1313, 'atom': 'H12', 'charge': 0.09000000357627869, 'distance': 27.21428108215332, 'force': [-0.030063677579164505, -0.021360209211707115, 0.016358934342861176], 'magnitude': 0.040344737470149994, 'cosine_with_motion': 0.5514664053916931, 'motion_component': 0.0222487673163414, 'motion_component_percent': 55.14664053916931}, {'resid': 1313, 'atom': 'H121', 'charge': 0.15000000596046448, 'distance': 23.170303344726562, 'force': [-0.07495530694723129, -0.05322969704866409, -0.012366272509098053], 'magnitude': 0.09276110678911209, 'cosine_with_motion': 0.3492962121963501, 'motion_component': 0.032401103526353836, 'motion_component_percent': 34.92962121963501}, {'resid': 1313, 'atom': 'H12X', 'charge': 0.09000000357627869, 'distance': 21.59376335144043, 'force': [-0.05827166512608528, -0.025715386494994164, 0.0070289187133312225], 'magnitude': 0.06408021599054337, 'cosine_with_motion': 0.6075019240379333, 'motion_component': 0.03892885521054268, 'motion_component_percent': 60.750192403793335}, {'resid': 1313, 'atom': 'H12Y', 'charge': 0.09000000357627869, 'distance': 21.88326072692871, 'force': [-0.055588047951459885, -0.0281803160905838, 0.0030159649904817343], 'magnitude': 0.06239597126841545, 'cosine_with_motion': 0.5451794266700745, 'motion_component': 0.03401700034737587, 'motion_component_percent': 54.517942667007446}, {'resid': 1313, 'atom': 'H13A', 'charge': 0.09000000357627869, 'distance': 28.964584350585938, 'force': [-0.025414682924747467, -0.020764777436852455, 0.013835546560585499], 'magnitude': 0.03561607003211975, 'cosine_with_motion': 0.4965561330318451, 'motion_component': 0.017685377970337868, 'motion_component_percent': 49.65561330318451}, {'resid': 1313, 'atom': 'H13B', 'charge': 0.09000000357627869, 'distance': 27.87356185913086, 'force': [-0.027067841961979866, -0.02370568923652172, 0.013581275008618832], 'magnitude': 0.038458794355392456, 'cosine_with_motion': 0.4595431089401245, 'motion_component': 0.017673473805189133, 'motion_component_percent': 45.95431089401245}, {'resid': 1313, 'atom': 'H13R', 'charge': 0.09000000357627869, 'distance': 21.23004722595215, 'force': [-0.049622129648923874, -0.0435173436999321, -0.0062346430495381355], 'magnitude': 0.06629468500614166, 'cosine_with_motion': 0.2844361960887909, 'motion_component': 0.018856607377529144, 'motion_component_percent': 28.44361960887909}, {'resid': 1313, 'atom': 'H13S', 'charge': 0.09000000357627869, 'distance': 22.71095848083496, 'force': [-0.0427805632352829, -0.03826403617858887, -0.007852829061448574], 'magnitude': 0.05793081969022751, 'cosine_with_motion': 0.25669384002685547, 'motion_component': 0.014870485290884972, 'motion_component_percent': 25.669384002685547}, {'resid': 1313, 'atom': 'H13X', 'charge': 0.09000000357627869, 'distance': 23.276805877685547, 'force': [-0.05104534327983856, -0.020873552188277245, 0.00016215912182815373], 'magnitude': 0.05514851212501526, 'cosine_with_motion': 0.5836076140403748, 'motion_component': 0.03218509256839752, 'motion_component_percent': 58.360761404037476}, {'resid': 1313, 'atom': 'H13Y', 'charge': 0.09000000357627869, 'distance': 22.564701080322266, 'force': [-0.05533658713102341, -0.019312774762511253, 0.002952663926407695], 'magnitude': 0.05868423357605934, 'cosine_with_motion': 0.6385865211486816, 'motion_component': 0.03747496008872986, 'motion_component_percent': 63.858652114868164}, {'resid': 1313, 'atom': 'H141', 'charge': 0.15000000596046448, 'distance': 20.91357421875, 'force': [-0.08912335336208344, -0.06709177792072296, -0.022801753133535385], 'magnitude': 0.11386043578386307, 'cosine_with_motion': 0.2935974895954132, 'motion_component': 0.033429138362407684, 'motion_component_percent': 29.35974895954132}, {'resid': 1313, 'atom': 'H14X', 'charge': 0.09000000357627869, 'distance': 21.595001220703125, 'force': [-0.06038380041718483, -0.021157752722501755, -0.0033878821413964033], 'magnitude': 0.0640728622674942, 'cosine_with_motion': 0.5928890109062195, 'motion_component': 0.037988096475601196, 'motion_component_percent': 59.28890109062195}, {'resid': 1313, 'atom': 'H14Y', 'charge': 0.09000000357627869, 'distance': 20.897918701171875, 'force': [-0.06262236088514328, -0.0274053867906332, -0.002915058983489871], 'magnitude': 0.06841865926980972, 'cosine_with_motion': 0.5464163422584534, 'motion_component': 0.03738507255911827, 'motion_component_percent': 54.64163422584534}, {'resid': 1313, 'atom': 'H151', 'charge': 0.15000000596046448, 'distance': 20.728126525878906, 'force': [-0.08357397466897964, -0.07334715127944946, -0.03271077573299408], 'magnitude': 0.11590689420700073, 'cosine_with_motion': 0.1905936449766159, 'motion_component': 0.02209111675620079, 'motion_component_percent': 19.05936449766159}, {'resid': 1313, 'atom': 'H15X', 'charge': 0.09000000357627869, 'distance': 19.389982223510742, 'force': [-0.0758725255727768, -0.023544710129499435, -0.002268099458888173], 'magnitude': 0.07947413623332977, 'cosine_with_motion': 0.6273694634437561, 'motion_component': 0.04985964670777321, 'motion_component_percent': 62.73694634437561}, {'resid': 1313, 'atom': 'H15Y', 'charge': 0.09000000357627869, 'distance': 20.140121459960938, 'force': [-0.07045387476682663, -0.021265681833028793, 0.0032305517233908176], 'magnitude': 0.07366420328617096, 'cosine_with_motion': 0.663341760635376, 'motion_component': 0.048864543437957764, 'motion_component_percent': 66.3341760635376}, {'resid': 1313, 'atom': 'H16R', 'charge': 0.09000000357627869, 'distance': 20.997169494628906, 'force': [-0.04374101385474205, -0.04902323707938194, -0.016633594408631325], 'magnitude': 0.06777337193489075, 'cosine_with_motion': 0.10848373919725418, 'motion_component': 0.007352308835834265, 'motion_component_percent': 10.848373919725418}, {'resid': 1313, 'atom': 'H16S', 'charge': 0.09000000357627869, 'distance': 22.048635482788086, 'force': [-0.04108754172921181, -0.04414252191781998, -0.011874829418957233], 'magnitude': 0.061463482677936554, 'cosine_with_motion': 0.15175266563892365, 'motion_component': 0.009327247738838196, 'motion_component_percent': 15.175266563892365}, {'resid': 1313, 'atom': 'H16X', 'charge': 0.09000000357627869, 'distance': 18.692665100097656, 'force': [-0.07960584759712219, -0.030061068013310432, 0.008480374701321125], 'magnitude': 0.08551418036222458, 'cosine_with_motion': 0.6408466100692749, 'motion_component': 0.054801471531391144, 'motion_component_percent': 64.08466100692749}, {'resid': 1313, 'atom': 'H16Y', 'charge': 0.09000000357627869, 'distance': 19.445110321044922, 'force': [-0.07168613374233246, -0.033005472272634506, 0.004068424459546804], 'magnitude': 0.07902414351701736, 'cosine_with_motion': 0.5736560225486755, 'motion_component': 0.04533267766237259, 'motion_component_percent': 57.365602254867554}, {'resid': 1313, 'atom': 'H17R', 'charge': 0.09000000357627869, 'distance': 23.531579971313477, 'force': [-0.03404809907078743, -0.03910934552550316, -0.014931663870811462], 'magnitude': 0.053960807621479034, 'cosine_with_motion': 0.08277805149555206, 'motion_component': 0.0044667706824839115, 'motion_component_percent': 8.277805149555206}, {'resid': 1313, 'atom': 'H17S', 'charge': 0.09000000357627869, 'distance': 23.737777709960938, 'force': [-0.03620608150959015, -0.035808272659778595, -0.014791703782975674], 'magnitude': 0.05302741751074791, 'cosine_with_motion': 0.14378191530704498, 'motion_component': 0.007624383550137281, 'motion_component_percent': 14.378191530704498}, {'resid': 1313, 'atom': 'H17X', 'charge': 0.09000000357627869, 'distance': 17.030092239379883, 'force': [-0.09646784514188766, -0.03614608943462372, -0.0013262205757200718], 'magnitude': 0.10302593559026718, 'cosine_with_motion': 0.596825361251831, 'motion_component': 0.06148849427700043, 'motion_component_percent': 59.682536125183105}, {'resid': 1313, 'atom': 'H17Y', 'charge': 0.09000000357627869, 'distance': 18.075403213500977, 'force': [-0.082859568297863, -0.03847616910934448, -0.004217083565890789], 'magnitude': 0.0914544016122818, 'cosine_with_motion': 0.5291123390197754, 'motion_component': 0.048389650881290436, 'motion_component_percent': 52.91123390197754}, {'resid': 1313, 'atom': 'H18R', 'charge': 0.09000000357627869, 'distance': 22.035890579223633, 'force': [-0.04203231260180473, -0.03952266275882721, -0.021395115181803703], 'magnitude': 0.06153460219502449, 'cosine_with_motion': 0.12787552177906036, 'motion_component': 0.007868769578635693, 'motion_component_percent': 12.787552177906036}, {'resid': 1313, 'atom': 'H18S', 'charge': 0.09000000357627869, 'distance': 21.881269454956055, 'force': [-0.03882807120680809, -0.04325619712471962, -0.022714680060744286], 'magnitude': 0.06240732967853546, 'cosine_with_motion': 0.05100433900952339, 'motion_component': 0.0031830444931983948, 'motion_component_percent': 5.100433900952339}, {'resid': 1313, 'atom': 'H18X', 'charge': 0.09000000357627869, 'distance': 15.944635391235352, 'force': [-0.10282272100448608, -0.056905265897512436, 0.0016583347460255027], 'magnitude': 0.11753072589635849, 'cosine_with_motion': 0.5039783120155334, 'motion_component': 0.059232939034700394, 'motion_component_percent': 50.397831201553345}, {'resid': 1313, 'atom': 'H18Y', 'charge': 0.09000000357627869, 'distance': 16.390501022338867, 'force': [-0.09912913292646408, -0.048982057720422745, 0.012033961713314056], 'magnitude': 0.11122339218854904, 'cosine_with_motion': 0.5761426091194153, 'motion_component': 0.06408053636550903, 'motion_component_percent': 57.61426091194153}, {'resid': 1313, 'atom': 'H18Z', 'charge': 0.09000000357627869, '</t>
         </is>
       </c>
     </row>
@@ -531,7 +531,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>{594: {'frame': 594, 'motion_vector': [-1.0011978149414062, -3.098834991455078, -3.3971405029296875], 'ionic_force': [16.41676777601242, 6.264683712273836, 3.169294625520706], 'ionic_force_magnitude': 17.85499802995518, 'radial_force': 17.571469096986423, 'axial_force': 3.169294625520706, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-3.895551025867462, 2.105670690536499, -4.178462982177734], 'asn_force_magnitude': 6.0884086381870866, 'residue_force': [-3.895551025867462, 2.105670690536499, -4.178462982177734], 'residue_force_magnitude': 6.0884086381870866, 'total_force': [12.521216750144958, 8.370354402810335, -1.0091683566570282], 'total_force_magnitude': 15.095102600010206, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': 0.4038140040399918, 'cosine_residue_motion': 0.4038140040399918, 'cosine_ionic_motion': -0.5547941831455198, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': 2.458584670418001, 'motion_component_residue': 2.458584670418001, 'motion_component_ionic': -9.905849047093849, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 40.38140040399918, 'motion_component_percent_residue': 40.38140040399918, 'motion_component_percent_ionic': 55.47941831455198, 'ionic_contributions': [{'ion_id': 2223, 'distance': 11.164527893066406, 'force': [0.9171769022941589, 0.3611668050289154, -2.4744150638580322], 'magnitude': 2.6635286808013916, 'cosine_ionic_motion': 0.5080801248550415, 'motion_component_ionic': 1.3532860279083252, 'motion_component_percent_ionic': 50.80801248550415}, {'ion_id': 2397, 'distance': 12.290963172912598, 'force': [2.1154870986938477, 0.49722781777381897, 0.3275904953479767], 'magnitude': 2.1976888179779053, 'cosine_ionic_motion': -0.4613851010799408, 'motion_component_ionic': -1.0139808654785156, 'motion_component_percent_ionic': 46.13851010799408}, {'ion_id': 2399, 'distance': 6.807759761810303, 'force': [2.3719210624694824, 3.4110326766967773, 5.835718631744385], 'magnitude': 7.163571834564209, 'cosine_ionic_motion': -0.9720718860626221, 'motion_component_ionic': -6.963506698608398, 'motion_component_percent_ionic': 97.2071886062622}, {'ion_id': 2400, 'distance': 6.391457557678223, 'force': [5.8384013175964355, 0.05161558464169502, 5.653402805328369], 'magnitude': 8.12714958190918, 'cosine_ionic_motion': -0.6591774821281433, 'motion_component_ionic': -5.357234001159668, 'motion_component_percent_ionic': 65.91774821281433}, {'ion_id': 2520, 'distance': 6.330036163330078, 'force': [5.173781394958496, 1.9436408281326294, -6.173002243041992], 'magnitude': 8.285633087158203, 'cosine_ionic_motion': 0.2505042552947998, 'motion_component_ionic': 2.0755863189697266, 'motion_component_percent_ionic': 25.05042552947998}], 'glu_contributions': [], 'asn_contributions': [{'resid': 786, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 5.834468841552734, 'force': [-3.124321937561035, 2.2833364009857178, -4.4025397300720215], 'magnitude': 5.861515998840332, 'cosine_with_motion': 0.3990894556045532, 'motion_component': 2.3392691612243652, 'motion_component_percent': 39.90894556045532}, {'resid': 786, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 5.439373016357422, 'force': [-2.8021013736724854, 6.860512733459473, -6.999019145965576], 'magnitude': 10.193364143371582, 'cosine_with_motion': 0.1109568327665329, 'motion_component': 1.1310234069824219, 'motion_component_percent': 11.09568327665329}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 4.63738489151001, 'force': [1.24074125289917, -3.9694223403930664, 4.873508930206299], 'magnitude': 6.40678071975708, 'cosine_with_motion': -0.18234384059906006, 'motion_component': -1.1682369709014893, 'motion_component_percent': 18.234384059906006}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 5.909841537475586, 'force': [0.7901310324668884, -3.068756103515625, 2.3495869636535645], 'magnitude': 3.9448864459991455, 'cosine_with_motion': 0.03967897593975067, 'motion_component': 0.15652905404567719, 'motion_component_percent': 3.967897593975067}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': -0.4933563271488338, 'motion_component_pip2': -7.447264376675847, 'motion_component_percent_pip2': 49.33563271488338}, 595: {'frame': 595, 'motion_vector': [1.0993881225585938, 1.4108772277832031, 3.018280029296875], 'ionic_force': [9.422489553689957, -1.2596474140882492, -5.467212200164795], 'ionic_force_magnitude': 10.966331667373842, 'radial_force': 9.506314795819439, 'axial_force': -5.467212200164795, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [8.536092162132263, -4.010486304759979, -0.9632402956485748], 'asn_force_magnitude': 9.480332360642446, 'residue_force': [8.536092162132263, -4.010486304759979, -0.9632402956485748], 'residue_force_magnitude': 9.480332360642446, 'total_force': [17.95858171582222, -5.2701337188482285, -6.43045249581337], 'total_force_magnitude': 19.789787415718177, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': 0.02461856368892725, 'cosine_residue_motion': 0.02461856368892725, 'cosine_ionic_motion': -0.20584382003476734, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': 0.2333921660126741, 'motion_component_residue': 0.2333921660126741, 'motion_component_ionic': -2.257351602180471, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 2.4618563688927253, 'motion_component_percent_residue': 2.4618563688927253, 'motion_component_percent_ionic': 20.584382003476733, 'ionic_contributions': [{'ion_id': 2223, 'distance': 14.173755645751953, 'force': [0.3429594337940216, -0.2130206674337387, -1.6025272607803345], 'magnitude': 1.652601718902588, 'cosine_ionic_motion': -0.8210269808769226, 'motion_component_ionic': -1.3568305969238281, 'motion_component_percent_ionic': 82.10269808769226}, {'ion_id': 2397, 'distance': 8.791007995605469, 'force': [3.96269154548645, 0.5620447993278503, -1.5609283447265625], 'magnitude': 4.295965194702148, 'cosine_ionic_motion': 0.029072973877191544, 'motion_component_ionic': 0.12489648163318634, 'motion_component_percent_ionic': 2.9072973877191544}, {'ion_id': 2399, 'distance': 9.089923858642578, 'force': [3.4727280139923096, -1.6169264316558838, -1.2126842737197876], 'magnitude': 4.018070697784424, 'cosine_ionic_motion': -0.1506418138742447, 'motion_component_ionic': -0.6052894592285156, 'motion_component_percent_ionic': 15.064181387424469}, {'ion_id': 2400, 'distance': 10.022102355957031, 'force': [0.03414785861968994, 0.9609813094139099, 3.162410020828247], 'magnitude': 3.305372714996338, 'cosine_ionic_motion': 0.9432307481765747, 'motion_component_ionic': 3.1177291870117188, 'motion_component_percent_ionic': 94.32307481765747}, {'ion_id': 2520, 'distance': 8.452729225158691, 'force': [1.6099627017974854, -0.952726423740387, -4.253482341766357], 'magnitude': 4.646695613861084, 'cosine_ionic_motion': -0.7613705992698669, 'motion_component_ionic': -3.5378575325012207, 'motion_component_percent_ionic': 76.1370599269867}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 5.407621383666992, 'force': [-7.954776287078857, -3.755972385406494, -5.383383274078369], 'magnitude': 10.3134183883667, 'cosine_with_motion': -0.8371943235397339, 'motion_component': -8.6343355178833, 'motion_component_percent': 83.71943235397339}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 4.444257736206055, 'force': [5.389721393585205, 2.168998956680298, 3.860922336578369], 'magnitude': 6.975698947906494, 'cosine_with_motion': 0.8433032631874084, 'motion_component': 5.882629871368408, 'motion_component_percent': 84.33032631874084}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 5.665373802185059, 'force': [3.1088201999664307, 2.2309165000915527, 1.945609211921692], 'magnitude': 4.292685508728027, 'cosine_with_motion': 0.8258417248725891, 'motion_component': 3.545078754425049, 'motion_component_percent': 82.58417248725891}, {'resid': 458, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 5.2611613273620605, 'force': [6.9581522941589355, -0.6865848898887634, -1.7539246082305908], 'magnitude': 7.208573341369629, 'cosine_with_motion': 0.054849158972501755, 'motion_component': 0.39538419246673584, 'motion_component_percent': 5.4849158972501755}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 5.785101413726807, 'force': [1.0341745615005493, -3.9678444862365723, 0.3675360381603241], 'magnitude': 4.116842269897461, 'cosine_with_motion': -0.23206272721290588, 'motion_component': -0.9553656578063965, 'motion_component_percent': 23.20627272129059}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': -0.10227292459747461, 'motion_component_pip2': -2.023959436167797, 'motion_component_percent_pip2': 10.227292459747462}, 597: {'frame': 597, 'motion_vector': [2.5267333984375, -4.712158203125, 3.4478759765625], 'ionic_force': [13.717314541339874, 3.188774585723877, -13.480058789253235], 'ionic_force_magnitude': 19.494742536036124, 'radial_force': 14.083075004579534, 'axial_force': -13.480058789253235, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-2.200845956802368, 6.182508230209351, 0.9410785436630249], 'asn_force_magnitude': 6.6296877579206255, 'residue_force': [-2.200845956802368, 6.182508230209351, 0.9410785436630249], 'residue_force_magnitude': 6.6296877579206255, 'total_force': [11.516468584537506, 9.371282815933228, -12.53898024559021], 'total_force_magnitude': 19.433888336463866, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': -0.7456138508337652, 'cosine_residue_motion': -0.7456138508337652, 'cosine_ionic_motion': -0.2164315894605446, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': -4.943187019008668, 'motion_component_residue': -4.943187019008668, 'motion_component_ionic': -4.219278113198387, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 74.56138508337652, 'motion_component_percent_residue': 74.56138508337652, 'motion_component_percent_ionic': 21.64315894605446, 'ionic_contributions': [{'ion_id': 2397, 'distance': 5.1699652671813965, 'force': [9.219123840332031, 2.1843910217285156, -8.032551765441895], 'magnitude': 12.421178817749023, 'cosine_ionic_motion': -0.18594302237033844, 'motion_component_ionic': -2.309631586074829, 'motion_component_percent_ionic': 18.594302237033844}, {'ion_id': 2399, 'distance': 8.66270637512207, 'force': [4.160089015960693, 0.3329230546951294, -1.468340277671814], 'magnitude': 4.424160957336426, 'cosine_ionic_motion': 0.1378471702337265, 'motion_component_ionic': 0.6098580360412598, 'motion_component_percent_ionic': 13.78471702337265}, {'ion_id': 2520, 'distance': 9.054512977600098, 'force': [0.33810168504714966, 0.6714605093002319, -3.9791667461395264], 'magnitude': 4.049560546875, 'cosine_ionic_motion': -0.6221674084663391, 'motion_component_ionic': -2.5195045471191406, 'motion_component_percent_ionic': 62.21674084663391}], 'glu_contributions': [], 'asn_contributions': [{'resid': 786, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 4.84675407409668, 'force': [0.6873879432678223, -9.602895736694336, -3.084052085876465], 'magnitude': 10.109375953674316, 'cosine_with_motion': 0.5652269721031189, 'motion_component': 5.714091777801514, 'motion_component_percent': 56.52269721031189}, {'resid': 786, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 4.179931640625, 'force': [-2.984717607498169, 10.852893829345703, 1.9306544065475464], 'magnitude': 11.420212745666504, 'cosine_with_motion': -0.7160437703132629, 'motion_component': -8.177371978759766, 'motion_component_percent': 71.6043770313263}, {'resid': 786, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 5.432579517364502, 'force': [-0.9277379512786865, 8.739850044250488, 5.2134175300598145], 'magnitude': 10.21887493133545, 'cosine_with_motion': -0.3930317759513855, 'motion_component': -4.016342639923096, 'motion_component_percent': 39.30317759513855}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 5.235164642333984, 'force': [1.024221658706665, -3.807339906692505, -3.118941307067871], 'magnitude': 5.027192115783691, 'cosine_with_motion': 0.3056250512599945, 'motion_component': 1.536435842514038, 'motion_component_percent': 30.56250512599945}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': -0.4714684459216272, 'motion_component_pip2': -9.162465132207055, 'motion_component_percent_pip2': 47.146844592162715}, 598: {'frame': 598, 'motion_vector': [-0.48065185546875, 7.592967987060547, 0.5522689819335938], 'ionic_force': [15.619737327098846, -17.680415898561478, 1.4677928239107132], 'ionic_force_magnitude': 23.63742194672664, 'radial_force': 23.59180579170807, 'axial_force': 1.4677928239107132, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-0.7410640716552734, 0.6431645900011063, -1.6313884258270264], 'asn_force_magnitude': 1.903750205266428, 'residue_force': [-0.7410640716552734, 0.6431645900011063, -1.6313884258270264], 'residue_force_magnitude': 1.903750205266428, 'total_force': [14.878673255443573, -17.03725130856037, -0.16359560191631317], 'total_force_magnitude': 22.62011524095888, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': 0.29876806724399624, 'cosine_residue_motion': 0.29876806724399624, 'cosine_ionic_motion': -0.7816726766274996, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': 0.5687797693428118, 'motion_component_residue': 0.5687797693428118, 'motion_component_ionic': -18.476726881671414, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 29.876806724399625, 'motion_component_percent_residue': 29.876806724399625, 'motion_component_percent_ionic': 78.16726766274996, 'ionic_contributions': [{'ion_id': 2223, 'distance': 12.98253059387207, 'force': [0.4674975275993347, -0.5725309252738953, -1.8258470296859741], 'magnitude': 1.96978759765625, 'cosine_ionic_motion': -0.37137678265571594, 'motion_component_ionic': -0.731533408164978, 'motion_component_percent_ionic': 37.137678265571594}, {'ion_id': 2397, 'distance': 4.158535480499268, 'force': [9.98279094696045, -14.34394359588623, 7.947362899780273], 'magnitude': 19.198057174682617, 'cosine_ionic_motion': -0.7465006709098816, 'motion_component_ionic': -14.3313627243042, 'motion_component_percent_ionic': 74.65006709098816}, {'ion_id': 2399, 'distance': 10.625804901123047, 'force': [2.918034791946411, -0.2730308473110199, -0.23832587897777557], 'magnitude': 2.9404542446136475, 'cosine_ionic_motion': -0.16082215309143066, 'motion_component_ionic': -0.4728901982307434, 'motion_component_percent_ionic': 16.082215309143066}, {'ion_id': 2520, 'distance': 7.736417293548584, 'force': [2.2514140605926514, -2.490910530090332, -4.4153971672058105], 'magnitude': 5.547001838684082, 'cosine_ionic_motion': -0.5301856398582458, 'motion_component_ionic': -2.9409408569335938, 'motion_component_percent_ionic': 53.018563985824585}], 'glu_contributions': [], 'asn_contributions': [{'resid': 458, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 5.38916540145874, 'force': [-6.544113636016846, -1.0811066627502441, 4.7818217277526855], 'magnitude': 8.176798820495605, 'cosine_with_motion': -0.03883847966790199, 'motion_component': -0.3175744414329529, 'motion_component_percent': 3.8838479667901993}, {'resid': 458, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 5.1868815422058105, 'force': [4.804582118988037, 0.8243797421455383, -5.5893731117248535], 'magnitude': 7.416515827178955, 'cosine_with_motion': 0.015259861946105957, 'motion_component': 0.11317500472068787, 'motion_component_percent': 1.5259861946105957}, {'resid': 458, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 5.186418533325195, 'force': [9.845282554626465, -0.6722015142440796, -5.322195053100586], 'magnitude': 11.211922645568848, 'cosine_with_motion': -0.1493738889694214, 'motion_component': -1.6747684478759766, 'motion_component_percent': 14.937388896942139}, {'resid': 458, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 4.844221591949463, 'force': [-4.795882701873779, 1.356716513633728, 3.1034839153289795], 'magnitude': 5.871352672576904, 'cosine_with_motion': 0.31974390149116516, 'motion_component': 1.8773292303085327, 'motion_component_percent': 31.974390149116516}, {'resid': 458, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 5.667299747467041, 'force': [-4.05093240737915, 0.21537651121616364, 1.394874095916748], 'magnitude': 4.289768695831299, 'cosine_with_motion': 0.13301841914653778, 'motion_component': 0.5706182718276978, 'motion_component_percent': 13.301841914653778}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': -0.791682399561881, 'motion_component_pip2': -17.907947112328603, 'motion_component_percent_pip2': 79.1682399561881}, 599: {'frame': 599, 'motion_vector': [1.4785842895507812, -4.815677642822266, 0.07472991943359375], 'ionic_force': [5.2050963789224625, 6.644684374332428, -4.204517247155309], 'ionic_force_magnitude': 9.42988992671684, 'radial_force': 8.440666961109724, 'axial_force': -4.204517247155309, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [3.193006992340088, 2.4221901297569275, -0.9578146934509277], 'asn_force_magnitude': 4.120644083734371, 'residue_force': [3.193006992340088, 2.4221901297569275, -0.9578146934509277], 'residue_force_magnitude': 4.120644083734371, 'total_force': [8.39810337126255, 9.066874504089355, -5.1623319406062365], 'total_force_magnitude': 13.393506806371525, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': -0.3379021168804551, 'cosine_residue_motion': -0.3379021168804551, 'cosine_ionic_motion': -0.5181498826645695, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': -1.392374358804767, 'motion_component_residue': -1.392374358804767, 'motion_component_ionic': -4.886096359068136, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 33.79021168804551, 'motion_component_percent_residue': 33.79021168804551, 'motion_component_percent_ionic': 51.81498826645695, 'ionic_contributions': [{'ion_id': 2223, 'distance': 12.522210121154785, 'force': [0.5072227120399475, 0.7328923344612122, -1.9205267429351807], 'magnitude': 2.117269277572632, 'cosine_ionic_motion': -0.27401456236839294, 'motion_component_ionic': -0.5801625847816467, 'motion_component_percent_ionic': 27.401456236839294}, {'ion_id': 2397, 'distance': 12.536849975585938, 'force': [0.23971302807331085, 1.1431760787963867, 1.760003685951233], 'magnitude': 2.1123273372650146, 'cosine_ionic_motion': -0.47163525223731995, 'motion_component_ionic': -0.9962480068206787, 'motion_component_percent_ionic': 47.163525223731995}, {'ion_id': 2399, 'distance': 11.582659721374512, 'force': [2.1557390689849854, 1.215116024017334, 0.01983618550002575], 'magnitude': 2.47469425201416, 'cosine_ionic_motion': -0.21356509625911713, 'motion_component_ionic': -0.5285083055496216, 'motion_component_percent_ionic': 21.356509625911713}, {'ion_id': 2520, 'distance': 7.521302700042725, 'force': [2.3024215698242188, 3.553499937057495, -4.063830375671387], 'magnitude': 5.868834972381592, 'cosine_ionic_motion': -0.47388917207717896, 'motion_component_ionic': -2.781177282333374, 'motion_component_percent_ionic': 47.388917207717896}], 'glu_contributions': [], 'asn_contributions': [{'resid': 786, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 3.7215044498443604, 'force': [4.655030727386475, -6.849659442901611, 15.014458656311035], 'magnitude': 17.147043228149414, 'cosine_with_motion': 0.47449085116386414, 'motion_component': 8.136115074157715, 'motion_component_percent': 47.449085116386414}, {'resid': 786, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 3.739779233932495, 'force': [0.7748281955718994, 5.929886341094971, -12.95268726348877], 'magnitude': 14.266605377197266, 'cosine_with_motion': -0.3948250114917755, 'motion_component': -5.6328125, 'motion_component_percent': 39.48250114917755}, {'resid': 786, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 3.408511161804199, 'force': [-11.6922025680542, 2.4208154678344727, -23.049837112426758], 'magnitude': 25.95886993408203, 'cosine_with_motion': -0.23449638485908508, 'motion_component': -6.087261199951172, 'motion_component_percent': 23.44963848590851}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 3.186782121658325, 'force': [3.344067335128784, 1.522575855255127, 13.059879302978516], 'magnitude': 13.566925048828125, 'cosine_with_motion': -0.02065473422408104, 'motion_component': -0.28022122383117676, 'motion_component_percent': 2.065473422408104}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 3.85119891166687, 'force': [6.111283302307129, -0.6014280915260315, 6.970371723175049], 'magnitude': 9.289541244506836, 'cosine_with_motion': 0.26608482003211975, 'motion_component': 2.4718058109283447, 'motion_component_percent': 26.608482003211975}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': -0.4687697410872353, 'motion_component_pip2': -6.278470717872903, 'motion_component_percent_pip2': 46.87697410872353}, 602: {'frame': 602, 'motion_vector': [3.1222152709960938, -2.9506759643554688, 4.228553771972656], 'ionic_force': [5.804734170436859, 3.909941703081131, 5.109992742538452], 'ionic_force_magnitude': 8.665714554479965, 'radial_force': 6.998755811637541, 'axial_force': 5.109992742538452, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-9.875576078891754, 5.132661819458008, -3.2755286693573], 'asn_force_magnitude': 11.60173729691733, 'residue_force': [-9.875576078891754, 5.132661819458008, -3.2755286693573], 'residue_force_magnitude': 11.60173729691733, 'total_force': [-4.070841908454895, 9.042603522539139, 1.8344640731811523], 'total_force_magnitude': 10.08492393353873, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': -0.8555110481135088, 'cosine_residue_motion': -0.8555110481135088, 'cosine_ionic_motion': 0.5397538314076231, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': -9.925414434823331, 'motion_component_residue': -9.925414434823331, 'motion_component_ionic': 4.677352632665365, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 85.55110481135088, 'motion_component_percent_residue': 85.55110481135088, 'motion_component_percent_ionic': 53.97538314076231, 'ionic_contributions': [{'ion_id': 2397, 'distance': 5.686462879180908, 'force': [1.8689794540405273, 3.589475154876709, 9.43603515625], 'magnitude': 10.267237663269043, 'cosine_ionic_motion': 0.5678610801696777, 'motion_component_ionic': 5.83036470413208, 'motion_component_percent_ionic': 56.78610801696777}, {'ion_id': 2399, 'distance': 10.064099311828613, 'force': [3.0035958290100098, -0.2214738428592682, -1.293684720993042], 'magnitude': 3.277843713760376, 'cosine_ionic_motion': 0.23083555698394775, 'motion_component_ionic': 0.7566428780555725, 'motion_component_percent_ionic': 23.083555698394775}, {'ion_id': 2520, 'distance': 10.156685829162598, 'force': [0.932158887386322, 0.5419403910636902, -3.032357692718506], 'magnitude': 3.218355655670166, 'cosine_ionic_motion': -0.5933635234832764, 'motion_component_ionic': -1.9096548557281494, 'motion_component_percent_ionic': 59.33635234832764}], 'glu_contributions': [], 'asn_contributions': [{'resid': 458, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 5.8699541091918945, 'force': [-5.561285495758057, 3.793759346008301, -1.4770618677139282], 'magnitude': 6.892185211181641, 'cosine_with_motion': -0.8377247452735901, 'motion_component': -5.773754119873047, 'motion_component_percent': 83.77247452735901}, {'resid': 458, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 4.84424352645874, 'force': [6.28958797454834, -5.535581111907959, 1.4476195573806763], 'magnitude': 8.502775192260742, 'cosine_with_motion': 0.8212569355964661, 'motion_component': 6.9829630851745605, 'motion_component_percent': 82.1256935596466}, {'resid': 786, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 3.702753782272339, 'force': [6.063577175140381, -15.994159698486328, -2.7280075550079346], 'magnitude': 17.32114601135254, 'cosine_with_motion': 0.5228419303894043, 'motion_component': 9.056221008300781, 'motion_component_percent': 52.28419303894043}, {'resid': 786, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 2.79931378364563, 'force': [-14.146187782287598, 21.134859085083008, 1.2518038749694824], 'magnitude': 25.462989807128906, 'cosine_with_motion': -0.6595712900161743, 'motion_component': -16.79465675354004, 'motion_component_percent': 65.95712900161743}, {'resid': 786, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 3.7914412021636963, 'force': [-1.0152881145477295, 19.72212791442871, 7.083037853240967], 'magnitude': 20.980051040649414, 'cosine_with_motion': -0.24838866293430328, 'motion_component': -5.211206912994385, 'motion_component_percent': 24.83886629343033}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 3.1205642223358154, 'force': [-1.6778204441070557, -12.410035133361816, -6.585193634033203], 'magnitude': 14.148810386657715, 'cosine_with_motion': 0.04143202304840088, 'motion_component': 0.5862138271331787, 'motion_component_percent': 4.143202304840088}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 4.782416820526123, 'force': [0.1718406081199646, -5.578308582305908, -2.2677268981933594], 'magnitude': 6.024088382720947, 'cosine_with_motion': 0.20398205518722534, 'motion_component': 1.2288058996200562, 'motion_component_percent': 20.398205518722534}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': -0.5203868503861344, 'motion_component_pip2': -5.248061802157966, 'motion_component_percent_pip2': 52.038685038613444}, 603: {'frame': 603, 'motion_vector': [-4.6690673828125, 0.09506988525390625, -1.2116546630859375], 'ionic_force': [9.731186628341675, 1.9190939664840698, 0.6936365365982056], 'ionic_force_magnitude': 9.94283895538469, 'radial_force': 9.918614562922151, 'axial_force': 0.6936365365982056, 'glu_force': [9.807960987091064, 2.8591824769973755, 4.126516819000244], 'glu_force_magnitude': 11.018128889179009, 'asn_force': [-4.125835657119751, 2.63333797454834, -2.4717745780944824], 'asn_force_magnitude': 5.483307243140154, 'residue_force': [5.6821253299713135, 5.492520451545715, 1.6547422409057617], 'residue_force_magnitude': 8.07418733124191, 'total_force': [15.413311958312988, 7.411614418029785, 2.3483787775039673], 'total_force_magnitude': 17.26317168681503, 'cosine_total_motion': 0, 'cosine_glu_motion': -0.9504014184565998, 'cosine_asn_motion': 0.8508416819482792, 'cosine_residue_motion': -0.7191087758336354, 'cosine_ionic_motion': -0.9608669198266913, 'motion_component_total': 0, 'motion_component_glu': -10.47164532501337, 'motion_component_asn': 4.665426357392551, 'motion_component_residue': -5.8062189676208185, 'motion_component_ionic': -9.553745041393324, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 95.04014184565997, 'motion_component_percent_asn': 85.08416819482792, 'motion_component_percent_residue': 71.91087758336354, 'motion_component_percent_ionic': 96.08669198266912, 'ionic_contributions': [{'ion_id': 2223, 'distance': 13.333165168762207, 'force': [0.899975061416626, -0.16712290048599243, -1.6278350353240967], 'magnitude': 1.8675470352172852, 'cosine_ionic_motion': -0.24922189116477966, 'motion_component_ionic': -0.46543359756469727, 'motion_component_percent_ionic': 24.922189116477966}, {'ion_id': 2397, 'distance': 9.057463645935059, 'force': [3.4987452030181885, 0.641575276851654, 1.9299601316452026], 'magnitude': 4.04692268371582, 'cosine_ionic_motion': -0.953306257724762, 'motion_component_ionic': -3.857956647872925, 'motion_component_percent_ionic': 95.3306257724762}, {'ion_id': 2399, 'distance': 8.554893493652344, 'force': [2.3054611682891846, 2.0024023056030273, 3.354686975479126], 'magnitude': 4.536374092102051, 'cosine_ionic_motion': -0.6688476800918579, 'motion_component_ionic': -3.0341432094573975, 'motion_component_percent_ionic': 66.88476800918579}, {'ion_id': 2520, 'distance': 8.81511402130127, 'force': [3.027005195617676, -0.5577607154846191, -2.9631755352020264], 'magnitude': 4.272500991821289, 'cosine_ionic_motion': -0.5140341520309448, 'motion_component_ionic': -2.196211338043213, 'motion_component_percent_ionic': 51.40341520309448}], 'glu_contributions': [{'resid': 426, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 5.5419230461120605, 'force': [-7.251682758331299, -2.6675777435302734, -4.011866569519043], 'magnitude': 8.706201553344727, 'cosine_with_motion': 0.9157596230506897, 'motion_component': 7.972787857055664, 'motion_component_percent': 91.57596230506897}, {'resid': 426, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 5.33311653137207, 'force': [8.140597343444824, 0.780370831489563, 4.946865558624268], 'magnitude': 9.557707786560059, 'cosine_with_motion': -0.9526380896568298, 'motion_component': -9.105036735534668, 'motion_component_percent': 95.26380896568298}, {'resid': 426, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 5.065221309661865, 'force': [8.919046401977539, 4.746389389038086, 3.1915178298950195], 'magnitude': 10.595441818237305, 'cosine_with_motion': -0.8814541697502136, 'motion_component': -9.339396476745605, 'motion_component_percent': 88.14541697502136}], 'asn_contributions': [{'resid': 458, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 3.4689948558807373, 'force': [-10.49141788482666, 4.036042213439941, 16.21968650817871], 'magnitude': 19.734176635742188, 'cosine_with_motion': 0.3121097981929779, 'motion_component': 6.159229755401611, 'motion_component_percent': 31.21097981929779}, {'resid': 458, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 3.6002485752105713, 'force': [3.405759572982788, -2.315692901611328, -14.832712173461914], 'magnitude': 15.393861770629883, 'cosine_with_motion': 0.02491246908903122, 'motion_component': 0.3834991157054901, 'motion_component_percent': 2.491246908903122}, {'resid': 458, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 3.5082316398620605, 'force': [14.211526870727539, -12.942626953125, -15.197752952575684], 'magnitude': 24.50409698486328, 'cosine_with_motion': -0.4159107804298401, 'motion_component': -10.19151782989502, 'motion_component_percent': 41.59107804298401}, {'resid': 458, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 3.37701678276062, 'force': [-4.208061695098877, 8.50776481628418, 7.47476053237915], 'magnitude': 12.08146858215332, 'cosine_with_motion': 0.1955726146697998, 'motion_component': 2.362804412841797, 'motion_component_percent': 19.55726146697998}, {'resid': 458, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 3.7783610820770264, 'force': [-7.043642520904541, 5.347850799560547, 3.864243507385254], 'magnitude': 9.651154518127441, 'cosine_with_motion': 0.61665278673172, 'motion_component': 5.951411247253418, 'motion_component_percent': 61.665278673172}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': -0.8897533018654684, 'motion_component_pip2': -15.359964009014142, 'motion_component_percent_pip2': 88.97533018654684}, 60</t>
+          <t>{594: {'frame': 594, 'motion_vector': [-1.0011978149414062, -3.098834991455078, -3.3971405029296875], 'ionic_force': [16.41676777601242, 6.264683712273836, 3.169294625520706], 'ionic_force_magnitude': 17.85499802995518, 'radial_force': 17.571469096986423, 'axial_force': 3.169294625520706, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-3.895551025867462, 2.105670690536499, -4.178462982177734], 'asn_force_magnitude': 6.0884086381870866, 'residue_force': [-3.895551025867462, 2.105670690536499, -4.178462982177734], 'residue_force_magnitude': 6.0884086381870866, 'pip2_force': [0.5637558391317725, 0.03709937212988734, -4.52289681466209], 'pip2_force_magnitude': 4.558047016612277, 'total_force': [13.084972589276731, 8.407453774940223, -5.532065171319118], 'total_force_magnitude': 16.50774156871866, 'cosine_total_motion': -0.2620964359109277, 'cosine_glu_motion': 0, 'cosine_asn_motion': 0.4038140040399918, 'cosine_residue_motion': 0.4038140040399918, 'cosine_pip2_motion': 0.684645010286754, 'cosine_ionic_motion': -0.5547941831455198, 'motion_component_total': -4.326620230099827, 'motion_component_glu': 0, 'motion_component_asn': 2.458584670418001, 'motion_component_residue': 2.458584670418001, 'motion_component_ionic': -9.905849047093849, 'motion_component_pip2': 3.1206441465760206, 'motion_component_percent_total': 26.209643591092767, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 40.38140040399918, 'motion_component_percent_residue': 40.38140040399918, 'motion_component_percent_ionic': 55.47941831455198, 'motion_component_percent_pip2': 68.4645010286754, 'ionic_contributions': [{'ion_id': 2223, 'distance': 11.164527893066406, 'force': [0.9171769022941589, 0.3611668050289154, -2.4744150638580322], 'magnitude': 2.6635286808013916, 'cosine_ionic_motion': 0.5080801248550415, 'motion_component_ionic': 1.3532860279083252, 'motion_component_percent_ionic': 50.80801248550415}, {'ion_id': 2397, 'distance': 12.290963172912598, 'force': [2.1154870986938477, 0.49722781777381897, 0.3275904953479767], 'magnitude': 2.1976888179779053, 'cosine_ionic_motion': -0.4613851010799408, 'motion_component_ionic': -1.0139808654785156, 'motion_component_percent_ionic': 46.13851010799408}, {'ion_id': 2399, 'distance': 6.807759761810303, 'force': [2.3719210624694824, 3.4110326766967773, 5.835718631744385], 'magnitude': 7.163571834564209, 'cosine_ionic_motion': -0.9720718860626221, 'motion_component_ionic': -6.963506698608398, 'motion_component_percent_ionic': 97.2071886062622}, {'ion_id': 2400, 'distance': 6.391457557678223, 'force': [5.8384013175964355, 0.05161558464169502, 5.653402805328369], 'magnitude': 8.12714958190918, 'cosine_ionic_motion': -0.6591774821281433, 'motion_component_ionic': -5.357234001159668, 'motion_component_percent_ionic': 65.91774821281433}, {'ion_id': 2520, 'distance': 6.330036163330078, 'force': [5.173781394958496, 1.9436408281326294, -6.173002243041992], 'magnitude': 8.285633087158203, 'cosine_ionic_motion': 0.2505042552947998, 'motion_component_ionic': 2.0755863189697266, 'motion_component_percent_ionic': 25.05042552947998}], 'glu_contributions': [], 'asn_contributions': [{'resid': 786, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 5.834468841552734, 'force': [-3.124321937561035, 2.2833364009857178, -4.4025397300720215], 'magnitude': 5.861515998840332, 'cosine_with_motion': 0.3990894556045532, 'motion_component': 2.3392691612243652, 'motion_component_percent': 39.90894556045532}, {'resid': 786, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 5.439373016357422, 'force': [-2.8021013736724854, 6.860512733459473, -6.999019145965576], 'magnitude': 10.193364143371582, 'cosine_with_motion': 0.1109568327665329, 'motion_component': 1.1310234069824219, 'motion_component_percent': 11.09568327665329}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 4.63738489151001, 'force': [1.24074125289917, -3.9694223403930664, 4.873508930206299], 'magnitude': 6.40678071975708, 'cosine_with_motion': -0.18234384059906006, 'motion_component': -1.1682369709014893, 'motion_component_percent': 18.234384059906006}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 5.909841537475586, 'force': [0.7901310324668884, -3.068756103515625, 2.3495869636535645], 'magnitude': 3.9448864459991455, 'cosine_with_motion': 0.03967897593975067, 'motion_component': 0.15652905404567719, 'motion_component_percent': 3.967897593975067}], 'pip2_contributions': [{'resid': 1313, 'atom': 'C1', 'charge': 0.06000000238418579, 'distance': 26.491159439086914, 'force': [-0.017052076756954193, -0.0143767474219203, 0.017556725069880486], 'magnitude': 0.028384903445839882, 'cosine_with_motion': 0.014830406755208969, 'motion_component': 0.0004209596663713455, 'motion_component_percent': 1.483040675520897}, {'resid': 1313, 'atom': 'C11', 'charge': 0.17000000178813934, 'distance': 25.81676483154297, 'force': [-0.05900741368532181, -0.04110345616936684, 0.04471484199166298], 'magnitude': 0.08468049764633179, 'cosine_with_motion': 0.08669587969779968, 'motion_component': 0.007341450080275536, 'motion_component_percent': 8.669587969779968}, {'resid': 1313, 'atom': 'C12', 'charge': 0.04000000283122063, 'distance': 26.21453857421875, 'force': [-0.014077982865273952, -0.00943086389452219, 0.009290575981140137], 'magnitude': 0.019324740394949913, 'cosine_with_motion': 0.1292944848537445, 'motion_component': 0.0024985824711620808, 'motion_component_percent': 12.92944848537445}, {'resid': 1313, 'atom': 'C13', 'charge': -0.05000000074505806, 'distance': 27.378812789916992, 'force': [0.015966257080435753, 0.011442461982369423, -0.010225307196378708], 'magnitude': 0.022145163267850876, 'cosine_with_motion': -0.1603139340877533, 'motion_component': -0.0035501783713698387, 'motion_component_percent': 16.03139340877533}, {'resid': 1313, 'atom': 'C2', 'charge': 0.06000000238418579, 'distance': 27.95166015625, 'force': [-0.015625115483999252, -0.013014979660511017, 0.015379151329398155], 'magnitude': 0.025496121495962143, 'cosine_with_motion': 0.031087500974535942, 'motion_component': 0.0007926106918603182, 'motion_component_percent': 3.108750097453594}, {'resid': 1313, 'atom': 'C21', 'charge': 0.6299999952316284, 'distance': 24.2667236328125, 'force': [-0.27260878682136536, -0.16287244856357574, 0.15910494327545166], 'magnitude': 0.355186402797699, 'cosine_with_motion': 0.141879141330719, 'motion_component': 0.050393544137477875, 'motion_component_percent': 14.1879141330719}, {'resid': 1313, 'atom': 'C210', 'charge': -0.18000000715255737, 'distance': 19.1586971282959, 'force': [0.133111372590065, 0.08970475941896439, -0.027225283905863762], 'magnitude': 0.1628090739250183, 'cosine_with_motion': -0.41604867577552795, 'motion_component': -0.06773649901151657, 'motion_component_percent': 41.604867577552795}, {'resid': 1313, 'atom': 'C211', 'charge': -0.15000000596046448, 'distance': 18.513385772705078, 'force': [0.12457168847322464, 0.07165678590536118, -0.021412882953882217], 'magnitude': 0.1452973186969757, 'cosine_with_motion': -0.40077149868011475, 'motion_component': -0.05823102220892906, 'motion_component_percent': 40.077149868011475}, {'resid': 1313, 'atom': 'C212', 'charge': -0.15000000596046448, 'distance': 17.994733810424805, 'force': [0.1343480348587036, 0.07378401607275009, -0.01261032186448574], 'magnitude': 0.15379367768764496, 'cosine_with_motion': -0.4425811171531677, 'motion_component': -0.06806617975234985, 'motion_component_percent': 44.25811171531677}, {'resid': 1313, 'atom': 'C213', 'charge': -0.18000000715255737, 'distance': 17.986648559570312, 'force': [0.1571728140115738, 0.09699719399213791, -0.0030221142806112766], 'magnitude': 0.18471838533878326, 'cosine_with_motion': -0.5149979591369629, 'motion_component': -0.09512959420681, 'motion_component_percent': 51.49979591369629}, {'resid': 1313, 'atom': 'C214', 'charge': -0.15000000596046448, 'distance': 19.369552612304688, 'force': [0.11381798982620239, 0.06824129074811935, 0.002749041188508272], 'magnitude': 0.1327364444732666, 'cosine_with_motion': -0.5359206199645996, 'motion_component': -0.07113619893789291, 'motion_component_percent': 53.59206199645996}, {'resid': 1313, 'atom': 'C215', 'charge': -0.15000000596046448, 'distance': 19.82146453857422, 'force': [0.10726690292358398, 0.06669436395168304, 0.010581561364233494], 'magnitude': 0.12675289809703827, 'cosine_with_motion': -0.5867951512336731, 'motion_component': -0.07437798380851746, 'motion_component_percent': 58.67951512336731}, {'resid': 1313, 'atom': 'C216', 'charge': -0.18000000715255737, 'distance': 19.071619033813477, 'force': [0.13475489616394043, 0.09108933806419373, 0.023196522146463394], 'magnitude': 0.16429920494556427, 'cosine_with_motion': -0.6414923071861267, 'motion_component': -0.10539668053388596, 'motion_component_percent': 64.14923071861267}, {'resid': 1313, 'atom': 'C217', 'charge': -0.18000000715255737, 'distance': 19.884531021118164, 'force': [0.11817985773086548, 0.09046903252601624, 0.026310212910175323], 'magnitude': 0.15114016830921173, 'cosine_with_motion': -0.6861813068389893, 'motion_component': -0.10370955616235733, 'motion_component_percent': 68.61813068389893}, {'resid': 1313, 'atom': 'C218', 'charge': -0.18000000715255737, 'distance': 19.588125228881836, 'force': [0.11801009625196457, 0.09393896162509918, 0.03881748393177986], 'magnitude': 0.1557488590478897, 'cosine_with_motion': -0.7382859587669373, 'motion_component': -0.11498719453811646, 'motion_component_percent': 73.82859587669373}, {'resid': 1313, 'atom': 'C219', 'charge': -0.18000000715255737, 'distance': 20.55119514465332, 'force': [0.10154852271080017, 0.09060897678136826, 0.03870806843042374], 'magnitude': 0.14149346947669983, 'cosine_with_motion': -0.7718603014945984, 'motion_component': -0.10921318829059601, 'motion_component_percent': 77.18603014945984}, {'resid': 1313, 'atom': 'C22', 'charge': -0.08000000566244125, 'distance': 22.917572021484375, 'force': [0.03896016627550125, 0.02400871366262436, -0.021517163142561913], 'magnitude': 0.05056976526975632, 'cosine_with_motion': -0.16938169300556183, 'motion_component': -0.00856559257954359, 'motion_component_percent': 16.938169300556183}, {'resid': 1313, 'atom': 'C220', 'charge': -0.27000001072883606, 'distance': 20.84528160095215, 'force': [0.14344924688339233, 0.1300378441810608, 0.07120141386985779], 'magnitude': 0.20629389584064484, 'cosine_with_motion': -0.8121806383132935, 'motion_component': -0.16754791140556335, 'motion_component_percent': 81.21806383132935}, {'resid': 1313, 'atom': 'C23', 'charge': -0.18000000715255737, 'distance': 21.92696762084961, 'force': [0.09204868227243423, 0.06006483733654022, -0.05803867056965828], 'magnitude': 0.1242949366569519, 'cosine_with_motion': -0.13869254291057587, 'motion_component': -0.017238780856132507, 'motion_component_percent': 13.869254291057587}, {'resid': 1313, 'atom': 'C24', 'charge': -0.18000000715255737, 'distance': 20.547983169555664, 'force': [0.10519500821828842, 0.07073067873716354, -0.0629611611366272], 'magnitude': 0.14153772592544556, 'cosine_with_motion': -0.16607330739498138, 'motion_component': -0.023505639284849167, 'motion_component_percent': 16.60733073949814}, {'resid': 1313, 'atom': 'C25', 'charge': -0.15000000596046448, 'distance': 20.803699493408203, 'force': [0.08460602164268494, 0.06353720277547836, -0.04522281512618065], 'magnitude': 0.11506631970405579, 'cosine_with_motion': -0.236328586935997, 'motion_component': -0.02719346061348915, 'motion_component_percent': 23.6328586935997}, {'resid': 1313, 'atom': 'C26', 'charge': -0.15000000596046448, 'distance': 20.841411590576172, 'force': [0.08716646581888199, 0.06379438936710358, -0.03843134269118309], 'magnitude': 0.11465027183294296, 'cosine_with_motion': -0.2861766219139099, 'motion_component': -0.03281022608280182, 'motion_component_percent': 28.61766219139099}, {'resid': 1313, 'atom': 'C27', 'charge': -0.18000000715255737, 'distance': 20.667449951171875, 'force': [0.11263396590948105, 0.07128126174211502, -0.04250064492225647], 'magnitude': 0.1399061530828476, 'cosine_with_motion': -0.28748559951782227, 'motion_component': -0.04022100567817688, 'motion_component_percent': 28.748559951782227}, {'resid': 1313, 'atom': 'C28', 'charge': -0.15000000596046448, 'distance': 21.223026275634766, 'force': [0.09068571776151657, 0.05751761049032211, -0.026311183348298073], 'magnitude': 0.11056425422430038, 'cosine_with_motion': -0.3452751338481903, 'motion_component': -0.03817508742213249, 'motion_component_percent': 34.52751338481903}, {'resid': 1313, 'atom': 'C29', 'charge': -0.15000000596046448, 'distance': 20.56186294555664, 'force': [0.09719741344451904, 0.06296227872371674, -0.02150915563106537], 'magnitude': 0.11778891831636429, 'cosine_with_motion': -0.3957271873950958, 'motion_component': -0.04661227762699127, 'motion_component_percent': 39.57271873950958}, {'resid': 1313, 'atom': 'C3', 'charge': 0.06000000238418579, 'distance': 28.90619468688965, 'force': [-0.014464004896581173, -0.011485214345157146, 0.015074190683662891], 'magnitude': 0.02384006790816784, 'cosine_with_motion': -0.010134901851415634, 'motion_component': -0.00024161674082279205, 'motion_component_percent': 1.0134901851415634}, {'resid': 1313, 'atom': 'C31', 'charge': 0.6299999952316284, 'distance': 28.794885635375977, 'force': [-0.19339044392108917, -0.11927630007266998, 0.10958223789930344], 'magnitude': 0.2522597014904022, 'cosine_with_motion': 0.16087180376052856, 'motion_component': 0.04058147221803665, 'motion_component_percent': 16.087180376052856}, {'resid': 1313, 'atom': 'C310', 'charge': -0.18000000715255737, 'distance': 23.898391723632812, 'force': [0.0930081158876419, 0.04390237480401993, -0.01924494467675686], 'magnitude': 0.1046341061592102, 'cosine_with_motion': -0.3326317071914673, 'motion_component': -0.03480461984872818, 'motion_component_percent': 33.26317071914673}, {'resid': 1313, 'atom': 'C311', 'charge': -0.18000000715255737, 'distance': 23.0015926361084, 'force': [0.10301720350980759, 0.04287240654230118, -0.017539100721478462], 'magnitude': 0.11295223236083984, 'cosine_with_motion': -0.33188602328300476, 'motion_component': -0.03748726844787598, 'motion_component_percent': 33.188602328300476}, {'resid': 1313, 'atom': 'C312', 'charge': -0.18000000715255737, 'distance': 21.698305130004883, 'force': [0.11488749831914902, 0.051510196179151535, -0.016074564307928085], 'magnitude': 0.126928448677063, 'cosine_with_motion': -0.3683798611164093, 'motion_component': -0.046757884323596954, 'motion_component_percent': 36.83798611164093}, {'resid': 1313, 'atom': 'C313', 'charge': -0.18000000715255737, 'distance': 20.982715606689453, 'force': [0.12592166662216187, 0.04934721440076828, -0.01149718090891838], 'magnitude': 0.13573355972766876, 'cosine_with_motion': -0.3756290078163147, 'motion_component': -0.050985462963581085, 'motion_component_percent': 37.56290078163147}, {'resid': 1313, 'atom': 'C314', 'charge': -0.18000000715255737, 'distance': 20.27346420288086, 'force': [0.1371113508939743, 0.04514959827065468, -0.01738402619957924], 'magnitude': 0.14539675414562225, 'cosine_with_motion': -0.31879910826683044, 'motion_component': -0.04635235667228699, 'motion_component_percent': 31.879910826683044}, {'resid': 1313, 'atom': 'C315', 'charge': -0.18000000715255737, 'distance': 20.07476043701172, 'force': [0.14298324286937714, 0.03784162178635597, -0.010655121877789497], 'magnitude': 0.14828933775424957, 'cosine_with_motion': -0.32130998373031616, 'motion_component': -0.047646842896938324, 'motion_component_percent': 32.130998373031616}, {'resid': 1313, 'atom': 'C316', 'charge': -0.18000000715255737, 'distance': 19.378293991088867, 'force': [0.15545998513698578, 0.03073222190141678, -0.014604073017835617], 'magnitude': 0.15914005041122437, 'cosine_with_motion': -0.2687512934207916, 'motion_component': -0.042769093066453934, 'motion_component_percent': 26.875129342079163}, {'resid': 1313, 'atom': 'C317', 'charge': -0.18000000715255737, 'distance': 20.180044174194336, 'force': [0.14329437911510468, 0.022820644080638885, -0.02191665768623352], 'magnitude': 0.14674603939056396, 'cosine_with_motion': -0.20233756303787231, 'motion_component': -0.029692236334085464, 'motion_component_percent': 20.23375630378723}, {'resid': 1313, 'atom': 'C318', 'charge': -0.27000001072883606, 'distance': 19.949909210205078, 'force': [0.22190682590007782, 0.01804368384182453, -0.034042488783597946], 'magnitude': 0.2252267748117447, 'cosine_with_motion': -0.15325959026813507, 'motion_component': -0.03451816365122795, 'motion_component_percent': 15.325959026813507}, {'resid': 1313, 'atom': 'C32', 'charge': -0.08000000566244125, 'distance': 29.07960319519043, 'force': [0.024987589567899704, 0.014480353333055973, -0.012347130104899406], 'magnitude': 0.03140878677368164, 'cosine_with_motion': -0.18906228244304657, 'motion_component': -0.005938217043876648, 'motion_component_percent': 18.906228244304657}, {'resid': 1313, 'atom': 'C33', 'charge': -0.18000000715255737, 'distance': 28.492843627929688, 'force': [0.0604848712682724, 0.031019188463687897, -0.028246736153960228], 'magnitude': 0.07361038029193878, 'cosine_with_motion': -0.1752934604883194, 'motion_component': -0.012903418391942978, 'motion_component_percent': 17.52934604883194}, {'resid': 1313, 'atom': 'C34', 'charge': -0.18000000715255737, 'distance': 26.975563049316406, 'force': [0.06781422346830368, 0.0345173254609108, -0.030888836830854416], 'magnitude': 0.08212389796972275, 'cosine_with_motion': -0.18093357980251312, 'motion_component': -0.014858971349895, 'motion_component_percent': 18.093357980251312}, {'resid': 1313, 'atom': 'C35', 'charge': -0.18000000715255737, 'distance': 26.589866638183594, 'force': [0.07045482099056244, 0.03781762346625328, -0.0273896511644125], 'magnitude': 0.08452364802360535, 'cosine_with_motion': -0.2380400449037552, 'motion_component': -0.020120013505220413, 'motion_component_percent': 23.80400449037552}, {'resid': 1313, 'atom': 'C36', 'charge': -0.18000000715255737, 'distance': 25.12306785583496, 'force': [0.07953671365976334, 0.04229864850640297, -0.029143230989575386], 'magnitude': 0.09468153119087219, 'cosine_with_motion': -0.25070425868034363, 'motion_component': -0.023737061768770218, 'motion_component_percent': 25.070425868034363}, {'resid': 1313, 'atom': 'C37', 'charge': -0.18000000715255737, 'distance': 24.51609992980957, 'force': [0.08604151010513306, 0.039332129061222076, -0.030589720234274864], 'magnitude': 0.09942780435085297, 'cosine_with_motion': -0.22250650823116302, 'motion_component': -0.02212333306670189, 'motion_component_percent': 22.250650823116302}, {'resid': 1313, 'atom': 'C38', 'charge': -0.18000000715255737, 'distance': 25.142972946166992, 'force': [0.08424026519060135, 0.034616705030202866, -0.02532784454524517], 'magnitude': 0.09453167766332626, 'cosine_with_motion': -0.2373119592666626, 'motion_component': -0.02243349701166153, 'motion_component_percent': 23.73119592666626}, {'resid': 1313, 'atom': 'C39', 'charge': -0.18000000715255737, 'distance': 25.2009220123291, 'force': [0.0841837227344513, 0.03688095137476921, -0.02017975226044655], 'magnitude': 0.09409742802381516, 'cosine_with_motion': -0.2936190664768219, 'motion_component': -0.02762879990041256, 'motion_component_percent': 29.36190664768219}, {'resid': 1313, 'atom': 'C4', 'charge': 0.08000000566244125, 'distance': 28.961231231689453, 'force': [-0.01785549893975258, -0.01550876535475254, 0.02105703577399254], 'magnitude': 0.03166606277227402, 'cosine_with_motion': -0.0375639945268631, 'motion_component': -0.0011895038187503815, 'motion_component_percent': 3.75639945268631}, {'resid': 1313, 'atom': 'C5', 'charge': 0.08000000566244125, 'distance': 27.557458877563477, 'force': [-0.019271403551101685, -0.01665729470551014, 0.02396566793322563], 'magnitude': 0.0349743589758873, 'cosine_with_motion': -0.06380857527256012, 'motion_component': -0.0022316640242934227, 'motion_component_percent': 6.380857527256012}, {'resid': 1313, 'atom': 'C6', 'charge': 0.06000000238418579, 'distance': 26.437026977539062, 'force': [-0.015901362523436546, -0.014449967071413994, 0.018726110458374023], 'magnitude': 0.02850126475095749, 'cosine_with_motion': -0.02174658514559269, 'motion_component': -0.0006198051851242781, 'motion_component_percent': 2.174658514559269}, {'resid': 1313, 'atom': 'H1', 'charge': 0.12000000476837158, 'distance': 25.97567367553711, 'force': [-0.036708757281303406, -0.028122611343860626, 0.03671428933739662], 'magnitude': 0.059045348316431046, 'cosine_with_motion': -0.002963850274682045, 'motion_component': -0.00017500156536698341, 'motion_component_percent': 0.2963850274682045}, {'resid': 1313, 'atom': 'H10R', 'charge': 0.09000000357627869, 'distance': 19.15447425842285, 'force': [-0.06529896706342697, -0.04761362820863724, 0.010076320730149746], 'magnitude': 0.08144044131040573, 'cosine_with_motion': 0.46625447273254395, 'motion_component': 0.037971969693899155, 'motion_component_percent': 46.625447273254395}, {'resid': 1313, 'atom': 'H10S', 'charge': 0.09000000357627869, 'distance': 18.675268173217773, 'force': [-0.06817626953125, -0.04861852526664734, 0.01811622641980648], 'magnitude': 0.08567357808351517, 'cosine_with_motion': 0.39034146070480347, 'motion_component': 0.033441949635744095, 'motion_component_percent': 39.03414607048035}, {'resid': 1313, 'atom': 'H10X', 'charge': 0.09000000357627869, 'distance': 23.39503288269043, 'force': [-0.047576628625392914, -0.024077538400888443, 0.011708194389939308], 'magnitude': 0.05459253862500191, 'cosine_with_motion': 0.321015328168869, 'motion_component': 0.017525041475892067, 'motion_component_percent': 32.1015328168869}, {'resid': 1313, 'atom': 'H10Y', 'charge': 0.09000000357627869, 'distance': 24.240501403808594, 'force': [-0.044728197157382965, -0.02287908084690571, 0.007857173681259155], 'magnitude': 0.050850752741098404, 'cosine_with_motion': 0.3718695640563965, 'motion_component': 0.018909847363829613, 'motion_component_percent': 37.18695640563965}, {'resid': 1313, 'atom': 'H111', 'charge': 0.15000000596046448, 'distance': 18.59153938293457, 'force': [-0.12522360682487488, -0.0657220333814621, 0.027535896748304367], 'magnitude': 0.144078329205513, 'cosine_with_motion': 0.34732213616371155, 'motion_component': 0.05004159361124039, 'motion_component_percent': 34.732213616371155}, {'resid': 1313, 'atom': 'H11A', 'charge': 0.09000000357627869, 'distance': 26.74968719482422, 'force': [-0.028570929542183876, -0.02019382081925869, 0.022796278819441795], 'magnitude': 0.04175833612680435, 'cosine_with_motion': 0.06992106884717941, 'motion_component': 0.0029197875410318375, 'motion_component_percent': 6.992106884717941}, {'resid': 1313, 'atom': 'H11B', 'charge': 0.09000000357627869, 'distance': 25.3295955657959, 'force': [-0.03305971249938011, -0.021026913076639175, 0.025176730006933212], 'magnitude': 0.046571917831897736, 'cosine_with_motion': 0.05808141082525253, 'motion_component': 0.002704962622374296, 'motion_component_percent': 5.808141082525253}, {'resid': 1313, 'atom': 'H11X', 'charge': 0.09000000357627869, 'distance': 23.60810661315918, 'force': [-0.049528881907463074, -0.019452590495347977, 0.006533311679959297], 'magnitude': 0.05361154302954674, 'cosine_with_motion': 0.34751009941101074, 'motion_component': 0.018630553036928177, 'motion_component_percent': 34.751009941101074}, {'resid': 1313, 'atom': 'H11Y', 'charge': 0.09000000357627869, 'distance': 22.766159057617188, 'force': [-0.05307473987340927, -0.01983572728931904, 0.010637934319674969], 'magnitude': 0.057650238275527954, 'cosine_with_motion': 0.2892298400402069, 'motion_component': 0.016674168407917023, 'motion_component_percent': 28.92298400402069}, {'resid': 1313, 'atom': 'H12', 'charge': 0.09000000357627869, 'distance': 26.60165023803711, 'force': [-0.03162373602390289, -0.01921144872903824, 0.020341070368885994], 'magnitude': 0.042224396020174026, 'cosine_with_motion': 0.11118625104427338, 'motion_component': 0.0046947724185884, 'motion_component_percent': 11.118625104427338}, {'resid': 1313, 'atom': 'H121', 'charge': 0.15000000596046448, 'distance': 17.702489852905273, 'force': [-0.14311909675598145, -0.06813277304172516, 0.011328306049108505], 'magnitude': 0.15891344845294952, 'cosine_with_motion': 0.42247143387794495, 'motion_component': 0.06713639199733734, 'motion_component_percent': 42.247143387794495}, {'resid': 1313, 'atom': 'H12X', 'charge': 0.09000000357627869, 'distance': 21.212501525878906, 'force': [-0.05909379944205284, -0.028231369331479073, 0.010975229553878307], 'magnitude': 0.06640438735485077, 'cosine_with_motion': 0.3499731123447418, 'motion_component': 0.023239750415086746, 'motion_component_percent': 34.99731123447418}, {'resid': 1313, 'atom': 'H12Y', 'charge': 0.09000000357627869, 'distance': 21.88981819152832, 'force': [-0.05570612847805023, -0.02742418460547924, 0.005773632787168026], 'magnitude': 0.062358587980270386, 'cosine_with_motion': 0.41281312704086304, 'motion_component': 0.025742443278431892, 'motion_component_percent': 41.281312704086304}, {'resid': 1313, 'atom': 'H13A', 'charge': 0.09000000357627869, 'distance': 28.16581153869629, 'force': [-0.026727067306637764, -0.01921745017170906, 0.01830282248556614], 'magnitude': 0.037664834409952164, 'cosine_with_motion': 0.13615688681602478, 'motion_component': 0.0051283263601362705, 'motion_component_percent': 13.615688681602478}, {'resid': 1313, 'atom': 'H13B', 'charge': 0.09000000357627869, 'distance': 27.04791831970215, 'force': [-0.02862551063299179, -0.022416947409510612, 0.018605777993798256], 'magnitude': 0.040842555463314056, 'cosine_with_motion': 0.18168264627456665, 'motion_component': 0.007420383859425783, 'motion_component_percent': 18.168264627456665}, {'resid': 1313, 'atom': 'H13R', 'charge': 0.09000000357627869, 'distance': 17.24496078491211, 'force': [-0.0859355702996254, -0.051980432122945786, -0.00287288473919034], 'magnitude': 0.10047458112239838, 'cosine_with_motion': 0.5432800054550171, 'motion_component': 0.054585833102464676, 'motion_component_percent': 54.32800054550171}, {'resid': 1313, 'atom': 'H13S', 'charge': 0.09000000357627869, 'distance': 17.812740325927734, 'force': [-0.0770445391535759, -0.054081711918115616, 0.002750380663201213], 'magnitude': 0.0941714197397232, 'cosine_with_motion': 0.531143844127655, 'motion_component': 0.05001857131719589, 'motion_component_percent': 53.1143844127655}, {'resid': 1313, 'atom': 'H13X', 'charge': 0.09000000357627869, 'distance': 20.26738166809082, 'force': [-0.06680478900671005, -0.02848099358379841, 0.004165853839367628], 'magnitude': 0.07274201512336731, 'cosine_with_motion': 0.41186994314193726, 'motion_component': 0.029960250481963158, 'motion_component_percent': 41.186994314193726}, {'resid': 1313, 'atom': 'H13Y', 'charge': 0.09000000357627869, 'distance': 21.801342010498047, 'force': [-0.05880223214626312, -0.021968267858028412, 0.0034346485044807196], 'magnitude': 0.06286576390266418, 'cosine_with_motion': 0.38967037200927734, 'motion_component': 0.024496925994753838, 'motion_component_percent': 38.967037200927734}, {'resid': 1313, 'atom': 'H141', 'charge': 0.15000000596046448, 'distance': 20.022850036621094, 'force': [-0.10849572718143463, -0.06047064810991287, 0.0012618802720680833], 'magnitude': 0.1242160052061081, 'cosine_with_motion': 0.499062180519104, 'motion_component': 0.061991509050130844, 'motion_component_percent': 49.9062180519104}, {'resid': 1313, 'atom': 'H14X', 'charge': 0.09000000357627869, 'distance': 19.387605667114258, 'force': [-0.07419595867395401, -0.026099948212504387, 0.011532049626111984], 'magnitude': 0.07949361950159073, 'cosine_with_motion': 0.3100535571575165, 'motion_component': 0.02464728057384491, 'motion_component_percent': 31.005355715751648}, {'resid': 1313, 'atom': 'H14Y', 'charge': 0.09000000357627869, 'distance': 20.905141830444336, 'force': [-0.06456828117370605, -0.019747747108340263, 0.01075221411883831], 'magnitude': 0.06837138533592224, 'cosine_with_motion': 0.2775871455669403, 'motion_component': 0.018979016691446304, 'motion_component_percent': 27.75871455669403}, {'resid': 1313, 'atom': 'H151', 'charge': 0.15000000596046448, 'distance': 20.775087356567383, 'force': [-0.09871416538953781, -0.05862746760249138, -0.01147520262748003], 'magnitude': 0.11538348346948624, 'cosine_with_motion': 0.5883983373641968, 'motion_component': 0.0678914487361908, 'motion_component_percent': 58.83983373641968}, {'resid': 1313, 'atom': 'H15X', 'charge': 0.09000000357627869, 'distance': 19.562753677368164, 'force': [-0.07511989772319794, -0.02118750661611557, 0.002009943826124072], 'magnitude': 0.0780765563249588, 'cosine_with_motion': 0.3648073077201843, 'motion_component': 0.028482897207140923, 'motion_component_percent': 36.48073077201843}, {'resid': 1313, 'atom': 'H15Y', 'charge': 0.09000000357627869, 'distance': 21.062604904174805, 'force': [-0.06522068381309509, -0.0164446122944355, 0.0035003924276679754], 'magnitude': 0.06735292077064514, 'cosine_with_motion': 0.32927602529525757, 'motion_component': 0.02217770181596279, 'motion_component_percent': 32.92760252952576}, {'resid': 1313, 'atom': 'H16R', 'charge': 0.09000000357627869, 'distance': 18.74248504638672, 'force': [-0.07118667662143707, -0.044007446616888046, -0.015199799090623856], 'magnitude': 0.08506017178297043, 'cosine_with_motion': 0.6477344632148743, 'motion_component': 0.05509640648961067, 'motion_component_percent': 64.77344632148743}, {'resid': 1313, 'atom': 'H16S', 'charge': 0.09000000357627869, 'distance': 18.168678283691406, 'force': [-0.07316059619188309, -0.05219555273652077, -0.010799090377986431], 'magnitude': 0.09051778167486191, 'cosine_with_motion': 0.6377906203269958, 'motion_component': 0.05773139372467995, 'motion_component_percent': 63.779062032699585}, {'resid': 1313, 'atom': 'H16X', 'charge': 0.09000000357627869, 'distance': 18.333724975585938, 'force': [-0.08651266992092133, -0.018219878897070885, 0.009272717870771885], 'magnitude': 0.08889538794755936, 'cosine_with_motion': 0.26671433448791504, 'motion_component': 0.023709673434495926, 'motion_component_percent': 26.671433448791504}, {'resid': 1313, 'atom': 'H16Y', 'charge': 0.09000000357627869, 'distance': 19.237173080444336, 'force': [-0.07959923893213272, -0.013007578440010548, 0.003740764921531081], 'magnitude': 0.08074174076318741, 'cosine_with_motion': 0.2823815643787384, 'motion_component': 0.022799979895353317, 'motion_component_percent': 28.23815643787384}, {'resid': 1313, 'atom': 'H17R', 'charge': 0.09000000357627869, 'distance': 19.819623947143555, 'force': [-0.057547423988580704, -0.04850906878709793, -0.011008155532181263], 'magnitude': 0.07606586068868637, 'cosine_with_motion': 0.6853670477867126, 'motion_component': 0.05213303491473198, 'motion_component_percent': 68.53670477867126}, {'resid': 1313, 'atom': 'H17S', 'charge': 0.09000000357627869, 'distance': 20.911418914794922, 'force': [-0.05421173945069313, -0.03988577052950859, -0.01180035900324583], 'magnitude': 0.06833034008741379, 'cosine_with_motion': 0.6778370141983032, 'motion_component': 0.046316832304000854, 'motion_component_percent': 67.78370141983032}, {'resid': 1313, 'atom': 'H17X', 'charge': 0.09000000357627869, 'distance': 20.08522605895996, 'force': [-0.07142814248800278, -0.012949646450579166, 0.014707439579069614], 'magnitude': 0.07406741380691528, 'cosine_with_motion': 0.17695669829845428, 'motion_component': 0.013106725178658962, 'motion_component_percent': 17.69566982984543}, {'resid': 1313, 'atom': 'H17Y', 'charge': 0.09000000357627869, 'distance': 21.2280216217041, 'force': [-0.06475471705198288, -0.010973814874887466, 0.009113973006606102], 'magnitude': 0.06630733609199524, 'cosine_with_motion': 0.21752800047397614, 'motion_component': 0.014423701912164688, 'motion_component_percent': 21.752800047397614}, {'resid': 1313, 'atom': 'H18R', 'charge': 0.09000000357627869, 'distance': 19.80225944519043, 'force': [-0.05969276279211044, -0.04265344515442848, -0.020586268976330757], 'magnitude': 0.07619932293891907, 'cosine_with_motion': 0.730293333530426, 'motion_component': 0.05564785748720169, 'motion_component_percent': 73.0293333530426}, {'resid': 1313, 'atom': 'H18S', 'charge': 0.09000000357627869, 'distance': 18.560165405273438, 'force': [-0.06457874923944473, -0.05352336913347244, -0.022103700786828995], 'magnitude': 0.08673949539661407, 'cosine_with_motion': 0.7486852407455444, 'motion_component': 0.06494057923555374, 'motion_component_percent': 74.86852407455444}, {'resid': 1313, 'atom': 'H18X', 'charge': 0.09000000357627869, 'distance': 20.729679107666016, 'force': [-0.06821741908</t>
         </is>
       </c>
     </row>
@@ -547,7 +547,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>{699: {'frame': 699, 'motion_vector': [5.170875549316406, -1.8740463256835938, 2.9829635620117188], 'ionic_force': [-0.6573584005236626, 7.503577142953873, -3.2780375480651855], 'ionic_force_magnitude': 8.214701465879575, 'radial_force': 7.532316377250682, 'axial_force': -3.2780375480651855, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [3.6204872131347656, -0.4675694704055786, -2.093546688556671], 'asn_force_magnitude': 4.208264084785352, 'residue_force': [3.6204872131347656, -0.4675694704055786, -2.093546688556671], 'residue_force_magnitude': 4.208264084785352, 'total_force': [2.963128812611103, 7.036007672548294, -5.371584236621857], 'total_force_magnitude': 9.334851554224574, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': 0.5071073425746244, 'cosine_residue_motion': 0.5071073425746244, 'cosine_ionic_motion': -0.5299698043165189, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': 2.1340416168877336, 'motion_component_residue': 2.1340416168877336, 'motion_component_ionic': -4.353543728390819, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 50.71073425746244, 'motion_component_percent_residue': 50.71073425746244, 'motion_component_percent_ionic': 52.996980431651885, 'ionic_contributions': [{'ion_id': 2223, 'distance': 7.634133815765381, 'force': [-0.6771345138549805, 0.5627886652946472, -5.628182411193848], 'magnitude': 5.6966376304626465, 'cosine_ionic_motion': -0.5988484025001526, 'motion_component_ionic': -3.4114224910736084, 'motion_component_percent_ionic': 59.88484025001526}, {'ion_id': 2276, 'distance': 9.756134033203125, 'force': [-1.0542205572128296, -3.153040885925293, -1.055195689201355], 'magnitude': 3.488049030303955, 'cosine_ionic_motion': -0.12325363606214523, 'motion_component_ionic': -0.4299147129058838, 'motion_component_percent_ionic': 12.325363606214523}, {'ion_id': 2391, 'distance': 13.279114723205566, 'force': [-0.07784866541624069, 0.08934804797172546, -1.8790479898452759], 'magnitude': 1.8827811479568481, 'cosine_ionic_motion': -0.5241919755935669, 'motion_component_ionic': -0.9869387149810791, 'motion_component_percent_ionic': 52.41919755935669}, {'ion_id': 2397, 'distance': 5.402998447418213, 'force': [1.1518453359603882, 10.004481315612793, 5.284388542175293], 'magnitude': 11.372825622558594, 'cosine_ionic_motion': 0.04174268990755081, 'motion_component_ionic': 0.47473233938217163, 'motion_component_percent_ionic': 4.174268990755081}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 5.283040523529053, 'force': [6.178944110870361, 4.969132423400879, 3.086221933364868], 'magnitude': 8.508606910705566, 'cosine_with_motion': 0.5981600880622864, 'motion_component': 5.089509010314941, 'motion_component_percent': 59.81600880622864}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 4.861706733703613, 'force': [-4.712672233581543, -5.613819122314453, -4.188048362731934], 'magnitude': 8.441800117492676, 'cosine_with_motion': -0.4987007975578308, 'motion_component': -4.209932327270508, 'motion_component_percent': 49.87007975578308}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 4.806948184967041, 'force': [-11.324604034423828, -5.468269348144531, -3.493640184402466], 'magnitude': 13.051979064941406, 'cosine_with_motion': -0.7191859483718872, 'motion_component': -9.386799812316895, 'motion_component_percent': 71.91859483718872}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 3.9989867210388184, 'force': [7.725991249084473, 2.5652873516082764, 2.8208439350128174], 'magnitude': 8.61561393737793, 'cosine_with_motion': 0.8080123066902161, 'motion_component': 6.961522102355957, 'motion_component_percent': 80.8012306690216}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 5.429563522338867, 'force': [4.222662925720215, 1.9278398752212524, 0.5436672568321228], 'magnitude': 4.673652172088623, 'cosine_with_motion': 0.678597092628479, 'motion_component': 3.1715266704559326, 'motion_component_percent': 67.8597092628479}, {'resid': 786, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 5.841325759887695, 'force': [-3.5671839714050293, -5.903143882751465, 0.9318822622299194], 'magnitude': 6.959907531738281, 'cosine_with_motion': -0.10570015013217926, 'motion_component': -0.7356632947921753, 'motion_component_percent': 10.570015013217926}, {'resid': 786, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 4.738321304321289, 'force': [5.097349166870117, 7.055403232574463, -1.7944735288619995], 'magnitude': 8.887171745300293, 'cosine_with_motion': 0.13996343314647675, 'motion_component': 1.2438790798187256, 'motion_component_percent': 13.996343314647675}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': -0.23776512123523044, 'motion_component_pip2': -2.2195021115030853, 'motion_component_percent_pip2': 23.776512123523045}, 700: {'frame': 700, 'motion_vector': [-2.9224395751953125, -4.688472747802734, -0.5789947509765625], 'ionic_force': [17.967689990997314, -4.085069861263037, -4.228372670710087], 'ionic_force_magnitude': 18.90515312887977, 'radial_force': 18.42622260215003, 'axial_force': -4.228372670710087, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [2.696014404296875, -0.2098812758922577, -3.633272647857666], 'asn_force_magnitude': 4.529151570859276, 'residue_force': [2.696014404296875, -0.2098812758922577, -3.633272647857666], 'residue_force_magnitude': 4.529151570859276, 'total_force': [20.66370439529419, -4.294951137155294, -7.861645318567753], 'total_force_magnitude': 22.522005943556852, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': -0.19043743853583078, 'cosine_residue_motion': -0.19043743853583078, 'cosine_ionic_motion': -0.2943180055214915, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': -0.8625200238949748, 'motion_component_residue': -0.8625200238949748, 'motion_component_ionic': -5.564126962970279, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 19.043743853583077, 'motion_component_percent_residue': 19.043743853583077, 'motion_component_percent_ionic': 29.431800552149152, 'ionic_contributions': [{'ion_id': 2223, 'distance': 4.949044227600098, 'force': [11.875652313232422, -2.7374866008758545, -5.933767318725586], 'magnitude': 13.554871559143066, 'cosine_ionic_motion': -0.24483919143676758, 'motion_component_ionic': -3.3187637329101562, 'motion_component_percent_ionic': 24.483919143676758}, {'ion_id': 2276, 'distance': 11.099944114685059, 'force': [0.5994970202445984, -2.6256368160247803, 0.08704712241888046], 'magnitude': 2.6946136951446533, 'cosine_ionic_motion': 0.7019967436790466, 'motion_component_ionic': 1.891610026359558, 'motion_component_percent_ionic': 70.19967436790466}, {'ion_id': 2333, 'distance': 13.529274940490723, 'force': [0.5745435357093811, -0.0620470754802227, -1.7192775011062622], 'magnitude': 1.8137985467910767, 'cosine_ionic_motion': -0.03897637873888016, 'motion_component_ionic': -0.07069529592990875, 'motion_component_percent_ionic': 3.8976378738880157}, {'ion_id': 2391, 'distance': 9.077005386352539, 'force': [2.116797685623169, -0.23552395403385162, -3.420628070831299], 'magnitude': 4.029516220092773, 'cosine_ionic_motion': -0.13855715095996857, 'motion_component_ionic': -0.5583183169364929, 'motion_component_percent_ionic': 13.855715095996857}, {'ion_id': 2397, 'distance': 6.660634994506836, 'force': [2.801199436187744, 1.5756245851516724, 6.75825309753418], 'magnitude': 7.483534812927246, 'cosine_ionic_motion': -0.4687570035457611, 'motion_component_ionic': -3.5079593658447266, 'motion_component_percent_ionic': 46.87570035457611}], 'glu_contributions': [], 'asn_contributions': [{'resid': 458, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 5.652351379394531, 'force': [-5.523664474487305, 0.7174466848373413, 4.921877861022949], 'magnitude': 7.4330668449401855, 'cosine_with_motion': 0.2404697835445404, 'motion_component': 1.7874280214309692, 'motion_component_percent': 24.04697835445404}, {'resid': 458, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 5.068817138671875, 'force': [4.636160850524902, -0.48063430190086365, -6.211787223815918], 'magnitude': 7.766035079956055, 'cosine_with_motion': -0.17846207320690155, 'motion_component': -1.3859426975250244, 'motion_component_percent': 17.846207320690155}, {'resid': 458, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 5.782376289367676, 'force': [7.117760181427002, -2.543402910232544, -4.922142028808594], 'magnitude': 9.019916534423828, 'cosine_with_motion': -0.1202796921133995, 'motion_component': -1.0849127769470215, 'motion_component_percent': 12.02796921133995}, {'resid': 458, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 5.329108715057373, 'force': [-3.5342421531677246, 2.0967092514038086, 2.5787787437438965], 'magnitude': 4.851511001586914, 'cosine_with_motion': -0.03691481798887253, 'motion_component': -0.1790926456451416, 'motion_component_percent': 3.691481798887253}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': -0.28534967102714065, 'motion_component_pip2': -6.426646986865254, 'motion_component_percent_pip2': 28.534967102714067}, 701: {'frame': 701, 'motion_vector': [1.1266822814941406, 5.776737213134766, -1.5197906494140625], 'ionic_force': [5.6327415853738785, -12.49571943283081, -1.979271188378334], 'ionic_force_magnitude': 13.848765156098588, 'radial_force': 13.70659629199116, 'axial_force': -1.979271188378334, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-2.2959251403808594, -0.25035786628723145, -1.9311881065368652], 'asn_force_magnitude': 3.0105545692237845, 'residue_force': [-2.2959251403808594, -0.25035786628723145, -1.9311881065368652], 'residue_force_magnitude': 3.0105545692237845, 'total_force': [3.336816444993019, -12.746077299118042, -3.9104592949151993], 'total_force_magnitude': 13.743672085722098, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': -0.06000127091663598, 'cosine_residue_motion': -0.06000127091663598, 'cosine_ionic_motion': -0.7463632545048614, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': -0.18063710031731262, 'motion_component_residue': -0.18063710031731262, 'motion_component_ionic': -10.336209432779267, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 6.000127091663598, 'motion_component_percent_residue': 6.000127091663598, 'motion_component_percent_ionic': 74.63632545048614, 'ionic_contributions': [{'ion_id': 2223, 'distance': 6.676501274108887, 'force': [1.7502690553665161, -6.3648223876953125, -3.4494123458862305], 'magnitude': 7.448009967803955, 'cosine_ionic_motion': -0.6527735590934753, 'motion_component_ionic': -4.86186408996582, 'motion_component_percent_ionic': 65.27735590934753}, {'ion_id': 2276, 'distance': 12.407637596130371, 'force': [0.2967414855957031, -2.131870985031128, -0.1333691030740738], 'magnitude': 2.1565518379211426, 'cosine_ionic_motion': -0.8984910845756531, 'motion_component_ionic': -1.9376425743103027, 'motion_component_percent_ionic': 89.84910845756531}, {'ion_id': 2333, 'distance': 14.647942543029785, 'force': [0.17381973564624786, -0.5862891674041748, -1.4213734865188599], 'magnitude': 1.5473366975784302, 'cosine_ionic_motion': -0.10959399491548538, 'motion_component_ionic': -0.16957880556583405, 'motion_component_percent_ionic': 10.959399491548538}, {'ion_id': 2391, 'distance': 10.047150611877441, 'force': [0.5118916630744934, -1.7073681354522705, -2.76401948928833], 'magnitude': 3.288912057876587, 'cosine_ionic_motion': -0.2543776333332062, 'motion_component_ionic': -0.8366256952285767, 'motion_component_percent_ionic': 25.437763333320618}, {'ion_id': 2397, 'distance': 7.041697025299072, 'force': [2.900019645690918, -1.7053687572479248, 5.78890323638916], 'magnitude': 6.6955060958862305, 'cosine_ionic_motion': -0.37793976068496704, 'motion_component_ionic': -2.5304980278015137, 'motion_component_percent_ionic': 37.793976068496704}], 'glu_contributions': [], 'asn_contributions': [{'resid': 1114, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 5.195601463317871, 'force': [-2.55672025680542, 5.472430229187012, 6.396096229553223], 'magnitude': 8.797406196594238, 'cosine_with_motion': 0.35551196336746216, 'motion_component': 3.1275832653045654, 'motion_component_percent': 35.551196336746216}, {'resid': 1114, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 4.7219672203063965, 'force': [0.5400452613830566, -5.773468971252441, -6.815944671630859], 'magnitude': 8.948837280273438, 'cosine_with_motion': -0.4115050435066223, 'motion_component': -3.6824917793273926, 'motion_component_percent': 41.15050435066223}, {'resid': 1114, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 5.002505302429199, 'force': [5.523428440093994, -8.375911712646484, -6.676362037658691], 'magnitude': 12.051471710205078, 'cosine_with_motion': -0.43703415989875793, 'motion_component': -5.266904830932617, 'motion_component_percent': 43.70341598987579}, {'resid': 1114, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 4.350222110748291, 'force': [-3.3683207035064697, 5.705446243286133, 3.0180280208587646], 'magnitude': 7.2805352210998535, 'cosine_with_motion': 0.5553417205810547, 'motion_component': 4.043184757232666, 'motion_component_percent': 55.53417205810547}, {'resid': 1114, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 5.703422546386719, 'force': [-2.4343578815460205, 2.72114634513855, 2.1469943523406982], 'magnitude': 4.235601425170898, 'cosine_with_motion': 0.3772762715816498, 'motion_component': 1.597991943359375, 'motion_component_percent': 37.72762715816498}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': -0.7652137265427211, 'motion_component_pip2': -10.51684653309658, 'motion_component_percent_pip2': 76.52137265427211}, 702: {'frame': 702, 'motion_vector': [-5.393394470214844, -3.3414268493652344, 0.5999679565429688], 'ionic_force': [12.869737058877945, 5.931039102375507, -15.014103665947914], 'ionic_force_magnitude': 20.6453545789457, 'radial_force': 14.170651248215927, 'axial_force': -15.014103665947914, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-1.7871383428573608, -2.3242602348327637, -0.18495991826057434], 'asn_force_magnitude': 2.937730291755655, 'residue_force': [-1.7871383428573608, -2.3242602348327637, -0.18495991826057434], 'residue_force_magnitude': 2.937730291755655, 'total_force': [11.082598716020584, 3.6067788675427437, -15.199063584208488], 'total_force_magnitude': 19.153182031623533, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': 0.9237398505646628, 'cosine_residue_motion': 0.9237398505646628, 'cosine_ionic_motion': -0.7466532508809686, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': 2.7136985407056518, 'motion_component_residue': 2.7136985407056518, 'motion_component_ionic': -15.414921111960098, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 92.37398505646628, 'motion_component_percent_residue': 92.37398505646628, 'motion_component_percent_ionic': 74.66532508809685, 'ionic_contributions': [{'ion_id': 2223, 'distance': 5.368613243103027, 'force': [5.837400436401367, 0.7885303497314453, -9.898978233337402], 'magnitude': 11.518975257873535, 'cosine_ionic_motion': -0.5456710457801819, 'motion_component_ionic': -6.285571098327637, 'motion_component_percent_ionic': 54.56710457801819}, {'ion_id': 2276, 'distance': 8.9594087600708, 'force': [1.0416561365127563, -3.9821670055389404, -0.4046080708503723], 'magnitude': 4.135989665985107, 'cosine_ionic_motion': 0.2824660837650299, 'motion_component_ionic': 1.1682767868041992, 'motion_component_percent_ionic': 28.24660837650299}, {'ion_id': 2333, 'distance': 14.5924711227417, 'force': [0.3185061514377594, 0.06636442989110947, -1.5247997045516968], 'magnitude': 1.5591230392456055, 'cosine_ionic_motion': -0.28727608919143677, 'motion_component_ionic': -0.4478987753391266, 'motion_component_percent_ionic': 28.727608919143677}, {'ion_id': 2391, 'distance': 10.231867790222168, 'force': [0.8932098150253296, 0.07281289994716644, -3.0419726371765137], 'magnitude': 3.171233654022217, 'cosine_ionic_motion': -0.34071439504623413, 'motion_component_ionic': -1.0804849863052368, 'motion_component_percent_ionic': 34.07143950462341}, {'ion_id': 2397, 'distance': 5.711245536804199, 'force': [4.778964519500732, 8.985498428344727, -0.14374502003192902], 'magnitude': 10.178327560424805, 'cosine_ionic_motion': -0.8615603446960449, 'motion_component_ionic': -8.769243240356445, 'motion_component_percent_ionic': 86.15603446960449}], 'glu_contributions': [], 'asn_contributions': [{'resid': 458, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 5.999449253082275, 'force': [-6.119142055511475, 1.549550175666809, 1.9201160669326782], 'magnitude': 6.597867488861084, 'cosine_with_motion': 0.6891546845436096, 'motion_component': 4.5469512939453125, 'motion_component_percent': 68.91546845436096}, {'resid': 458, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 5.406852722167969, 'force': [5.832805156707764, -1.6687109470367432, -3.1271204948425293], 'magnitude': 6.8253278732299805, 'cosine_with_motion': -0.6381785273551941, 'motion_component': -4.355777740478516, 'motion_component_percent': 63.81785273551941}, {'resid': 458, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 5.991536617279053, 'force': [-3.2518978118896484, 1.9782205820083618, 0.49231377243995667], 'magnitude': 3.8380422592163086, 'cosine_with_motion': 0.458884596824646, 'motion_component': 1.7612184286117554, 'motion_component_percent': 45.8884596824646}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 5.4932780265808105, 'force': [1.7510963678359985, -4.183320045471191, 0.5297307372093201], 'magnitude': 4.565864562988281, 'cosine_with_motion': 0.16673867404460907, 'motion_component': 0.7613062262535095, 'motion_component_percent': 16.673867404460907}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': -0.663139030907953, 'motion_component_pip2': -12.701222571254448, 'motion_component_percent_pip2': 66.3139030907953}, 703: {'frame': 703, 'motion_vector': [3.0632972717285156, -0.3276176452636719, -7.320182800292969], 'ionic_force': [-10.884252727031708, -8.873130112886429, -8.478539198637009], 'ionic_force_magnitude': 16.403811214743158, 'radial_force': 14.042770219088153, 'axial_force': -8.478539198637009, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-0.5881392955780029, 3.506279945373535, -12.428325653076172], 'asn_force_magnitude': 12.92683973077886, 'residue_force': [-0.5881392955780029, 3.506279945373535, -12.428325653076172], 'residue_force_magnitude': 12.92683973077886, 'total_force': [-11.47239202260971, -5.366850167512894, -20.90686485171318], 'total_force_magnitude': 24.444137484656153, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': 0.8574168517812821, 'cosine_residue_motion': 0.8574168517812821, 'cosine_ionic_motion': 0.24278296141366212, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': 11.083690225445608, 'motion_component_residue': 11.083690225445608, 'motion_component_ionic': 3.982565865185986, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 85.74168517812821, 'motion_component_percent_residue': 85.74168517812821, 'motion_component_percent_ionic': 24.278296141366212, 'ionic_contributions': [{'ion_id': 2223, 'distance': 6.227024555206299, 'force': [-4.3621296882629395, -4.500438690185547, -5.833205699920654], 'magnitude': 8.562032699584961, 'cosine_ionic_motion': 0.453117698431015, 'motion_component_ionic': 3.879608631134033, 'motion_component_percent_ionic': 45.3117698431015}, {'ion_id': 2276, 'distance': 10.741498947143555, 'force': [-0.5151962637901306, -2.8156723976135254, -0.2937663495540619], 'magnitude': 2.877453088760376, 'cosine_ionic_motion': 0.06540478020906448, 'motion_component_ionic': 0.18819919228553772, 'motion_component_percent_ionic': 6.540478020906448}, {'ion_id': 2391, 'distance': 10.110161781311035, 'force': [-0.9791443347930908, -1.0918611288070679, -2.8980860710144043], 'magnitude': 3.2480435371398926, 'cosine_ionic_motion': 0.7199847102165222, 'motion_component_ionic': 2.3385417461395264, 'motion_component_percent_ionic': 71.99847102165222}, {'ion_id': 2397, 'distance': 8.085201263427734, 'force': [-5.027782440185547, -0.4651578962802887, 0.5465189218521118], 'magnitude': 5.078744888305664, 'cosine_ionic_motion': -0.4772407114505768, 'motion_component_ionic': -2.423783779144287, 'motion_component_percent_ionic': 47.72407114505768}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 3.5694756507873535, 'force': [11.040966033935547, -5.19613790512085, 14.08905029296875], 'magnitude': 18.63878059387207, 'cosine_with_motion': -0.4567333161830902, 'motion_component': -8.512951850891113, 'motion_component_percent': 45.67333161830902}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 2.7612595558166504, 'force': [-8.288887977600098, 7.890403747558594, -23.53480339050293], 'magnitude': 26.169658660888672, 'cosine_with_motion': 0.6942943930625916, 'motion_component': 18.16944694519043, 'motion_component_percent': 69.42943930625916}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 4.231830596923828, 'force': [-10.961858749389648, 8.361246109008789, -9.671320915222168], 'magnitude': 16.84064292907715, 'cosine_with_motion': 0.2577742040157318, 'motion_component': 4.341083526611328, 'motion_component_percent': 25.77742040157318}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 4.259246826171875, 'force': [3.9050405025482178, -5.18712854385376, 3.940364122390747], 'magnitude': 7.594874382019043, 'cosine_with_motion': -0.25170373916625977, 'motion_component': -1.9116581678390503, 'motion_component_percent': 25.170373916625977}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 5.151911735534668, 'force': [3.7166008949279785, -2.3621034622192383, 2.7483842372894287], 'magnitude': 5.190979480743408, 'cosine_with_motion': -0.19307124614715576, 'motion_component': -1.002228856086731, 'motion_component_percent': 19.307124614715576}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': 0.6163545799105755, 'motion_component_pip2': 15.066256090631596, 'motion_component_percent_pip2': 61.63545799105755}, 704: {'frame': 704, 'motion_vector': [1.2222709655761719, 5.7140655517578125, 2.1114425659179688], 'ionic_force': [-1.0323635935783386, -1.6051292419433594, -6.714186668395996], 'ionic_force_magnitude': 6.980151652418031, 'radial_force': 1.9084586641286325, 'axial_force': -6.714186668395996, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [0.0, 0.0, 0.0], 'asn_force_magnitude': 0.0, 'residue_force': [0.0, 0.0, 0.0], 'residue_force_magnitude': 0.0, 'total_force': [-1.0323635935783386, -1.6051292419433594, -6.714186668395996], 'total_force_magnitude': 6.980151652418031, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': 0, 'cosine_residue_motion': 0, 'cosine_ionic_motion': -0.5674696344612931, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': 0, 'motion_component_residue': 0, 'motion_component_ionic': -3.961024106682051, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 0, 'motion_component_percent_residue': 0, 'motion_component_percent_ionic': 56.74696344612931, 'ionic_contributions': [{'ion_id': 2223, 'distance': 11.102577209472656, 'force': [0.1368509829044342, -0.7179929614067078, -2.5922603607177734], 'magnitude': 2.69333553314209, 'cosine_ionic_motion': -0.5622571706771851, 'motion_component_ionic': -1.5143471956253052, 'motion_component_percent_ionic': 56.225717067718506}, {'ion_id': 2276, 'distance': 12.323114395141602, 'force': [-0.2669045627117157, -1.699725866317749, -1.348822832107544], 'magnitude': 2.1862363815307617, 'cosine_ionic_motion': -0.9487032294273376, 'motion_component_ionic': -2.074089527130127, 'motion_component_percent_ionic': 94.87032294273376}, {'ion_id': 2397, 'distance': 10.472274780273438, 'force': [-0.9023100137710571, 0.8125895857810974, -2.7731034755706787], 'magnitude': 3.027303695678711, 'cosine_ionic_motion': -0.12307571619749069, 'motion_component_ionic': -0.37258756160736084, 'motion_component_percent_ionic': 12.30757161974907}], 'glu_contributions': [], 'asn_contributions': [], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': -0.5674696344612931, 'motion_component_pip2': -3.961024106682051, 'motion_component_percent_pip2': 56.74696344612931}, 705: {'frame': 705, 'motion_vector': [-2.187335968017578, 4.105712890625, 6.574501037597656], 'ionic_force': [0.4298229217529297, 5.037623256444931, -11.34488558769226], 'ionic_force_magnitude': 12.42050018379963, 'radial_force': 5.055926801085935, 'axial_force': -11.34488558769226, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [2.027644991874695, 6.931445837020874, 8.752003192901611], 'asn_force_magnitude': 11.346975169321052, 'residue_force': [2.027644991874695, 6.931445837020874, 8.752003192901611], 'residue_force_magnitude': 11.346975169321052, 'total_force': [2.4574679136276245, 11.969069093465805, -2.5928823947906494], 'total_force_magnitude': 12.490828740475267, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': 0.892501505038755, 'cosine_residue_motion': 0.892501505038755, 'cosine_ionic_motion': -0.5482571325039005, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': 10.12719241625642, 'motion_component_residue': 10.12719241625642, 'motion_component_ionic': -6.809627815034155, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 89.2501505038755, 'motion_component_percent_residue': 89.2501505038755, 'motion_component_percent_ionic': 54.82571325039005, 'ionic_contributions': [{'ion_id': 2223, 'distance': 7.240665435791016, 'force': [-0.21974420547485352, 1.4698823690414429, -6.155713081359863], 'magnitude': 6.332586288452148, 'cosine_ionic_motion': -0.6657609343528748, 'motion_component_ionic': -4.215988636016846, 'motion_component_percent_ionic': 66.57609343528748}, {'ion_id': 2276, 'distance': 11.737225532531738, 'force': [1.6645290851593018, 1.0498019456863403, -1.3910768032073975], 'magnitude': 2.409945249557495, 'cosine_ionic_motion': -0.43671128153800964, 'motion_component_ionic': -1.0524502992630005, 'motion_component_percent_ionic': 43.671128153800964}, {'ion_id': 2391, 'distance': 12.296820640563965, 'force': [0.34493374824523926, 0.4556065499782562, -2.1199257373809814], 'magnitude': 2.1955959796905518, 'cosine_ionic_motion': -0.7250614762306213, 'motion_component_ionic': -1.5919420719146729, 'motion_component_percent_ionic': 72.50614762306213}, {'ion_id': 2397, 'distance': 10.543689727783203, 'force': [-1.3598957061767578, 2.0623323917388916, -1.6781699657440186], 'magnitude': 2.986433506011963, 'cosine_ionic_motion': 0.016994668170809746, 'motion_component_ionic': 0.05075344443321228, 'motion_component_percent_ionic': 1.6994668170809746}], 'glu_contributions': [], 'asn_contributions': [{'resid': 786, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 4.092828273773193, 'force': [-2.7781386375427246, -11.191267013549805, -8.247431755065918], 'magnitude': 14.176835060119629, 'cosine_with_motion': -0.8240942358970642, 'motion_component': -11.683048248291016, 'motion_component_percent': 82.40942358970642}, {'resid': 786, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 2.9531259536743164, 'force': [4.536352634429932, 15.927152633666992, 15.786826133728027], 'magnitude': 22.879610061645508, 'cosine_with_motion': 0.8642759919166565, 'motion_component': 19.7742977142334, 'motion_component_percent': 86.42759919166565}, {'resid': 786, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 5.023392200469971, 'force': [4.665904521942139, 8.56997013092041, 6.90089750289917], 'magnitude': 11.951461791992188, 'cosine_with_motion': 0.7308629155158997, 'motion_component': 8.734880447387695, 'motion_component_percent': 73.08629155158997}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 4.886438846588135, 'force': [-3.0606086254119873, -3.3347980976104736, -3.578909397125244], 'magnitude': 5.7703375816345215, 'cosine_with_motion': -0.6568587422370911, 'motion_component': -3.790296792984009, 'motion_component_percent': 65.6858742237091}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 5.918309211730957, 'force': [-1.3358649015426636, -3.03961181640625, -2.109379291534424], 'magnitude': 3.933605909347534, 'cosine_with_motion': -0.7394334077835083, 'motion_component': -2.908639669418335, 'motion_component_percent': 73.94334077835083}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': 0.2656000390488129, 'motion_component_pip2': 3.3175646012222657, 'motion_component_percent_pip2': 26.56000390488129}, 706: {'frame': 706, 'motion_vector': [0.23690032958984375, 0.10396194458007812, 0.001068115234375], 'ionic_force': [-3.7625987380743027, 11.041518449783325, -1.7455277107656002], 'ionic_force_magnitude': 11.794877953150447, 'radial_force': 11.665002312072806, 'axial_force': -1.7455277107656002, 'glu_force': [14.573132038116455, 29.557626724243164, 4.808056831359863], 'glu_force_magnitude': 33.30385691573359, 'asn_force': [-1.2439944744110107, -1.2489422410726547, 0.9008800983428955], 'asn_force_magnitude': 1.9796373217059273, 'residue_force': [13.329137563705444, 28.30868448317051, 5.708936929702759], 'residue_force_magnitude': 31.806280609766464, 'total_force': [9.566538825631142, 39.350202932953835, 3.9634092189371586], 'total_force_magnitude': 40.68987280151798, 'cosine_total_motion': 0, 'cosine_glu_motion': 0.757932463396643, 'cosine_asn_motion': -0.8270640628155926, 'cosine_residue_motion': 0.742142337111611, 'cosine_ionic_motion': 0.08345931341469787, 'motion_component_total': 0, 'motion_component_glu': 25.242074312751285, 'motion_component_asn': -1.6372868861914827, 'motion_component_residue': 23.6047874265598, 'motion_component_ionic': 0.9843924157800932, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 75.7932463396643, 'motion_component_percent_asn': 82.70640628155927, 'motion_component_percent_residue': 74.2142337111611, 'motion_component_percent_ionic': 8.345931341469786, 'ionic_contributions': [{'ion_id': 2223, 'distance': 13.435805320739746, 'force': [-0.23350293934345245, 1.793494462966919, 0.33350518345832825], 'magnitude': 1.8391225337982178, 'cosine_ionic_motion': 0.2763650715351105, 'motion_component_ionic': 0.5082692503929138, 'motion_component_percent_ionic': 27.636507153511047}, {'ion_id': 2276, 'distance': 9.607341766357422, 'force': [-0.5958813428878784, 2.4937124252319336, 2.522737741470337], 'magnitude': 3.596926689147949, 'cosine_ionic_motion': 0.1297939121723175, 'motion_component_ionic': 0.46685919165611267, 'motion_component_percent_ionic': 12.97939121723175}, {'ion_id': 2333, 'distance': 13.088068008422852, 'force': [-0.15788444876670837, 1.0021278858184814, -1.651432991027832], 'magnitude': 1.9381483793258667, 'cosine_ionic_motion': 0.12966477870941162, 'motion_component_ionic': 0.2513095736503601, 'motion_component_percent_ionic': 12.966477870941162}, {'ion_id'</t>
+          <t>{699: {'frame': 699, 'motion_vector': [5.170875549316406, -1.8740463256835938, 2.9829635620117188], 'ionic_force': [-0.6573584005236626, 7.503577142953873, -3.2780375480651855], 'ionic_force_magnitude': 8.214701465879575, 'radial_force': 7.532316377250682, 'axial_force': -3.2780375480651855, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [3.6204872131347656, -0.4675694704055786, -2.093546688556671], 'asn_force_magnitude': 4.208264084785352, 'residue_force': [3.6204872131347656, -0.4675694704055786, -2.093546688556671], 'residue_force_magnitude': 4.208264084785352, 'pip2_force': [0.8608761616051197, -0.04523953070292919, -4.586148631235119], 'pip2_force_magnitude': 4.6664669342595735, 'total_force': [3.8240049742162228, 6.990768141845365, -9.957732867856976], 'total_force_magnitude': 12.75344255969617, 'cosine_total_motion': -0.288624046786004, 'cosine_glu_motion': 0, 'cosine_asn_motion': 0.5071073425746244, 'cosine_residue_motion': 0.5071073425746244, 'cosine_pip2_motion': -0.3131808520488668, 'cosine_ionic_motion': -0.5299698043165189, 'motion_component_total': -3.680950202032362, 'motion_component_glu': 0, 'motion_component_asn': 2.1340416168877336, 'motion_component_residue': 2.1340416168877336, 'motion_component_ionic': -4.353543728390819, 'motion_component_pip2': -1.4614480905292766, 'motion_component_percent_total': 28.862404678600402, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 50.71073425746244, 'motion_component_percent_residue': 50.71073425746244, 'motion_component_percent_ionic': 52.996980431651885, 'motion_component_percent_pip2': 31.318085204886682, 'ionic_contributions': [{'ion_id': 2223, 'distance': 7.634133815765381, 'force': [-0.6771345138549805, 0.5627886652946472, -5.628182411193848], 'magnitude': 5.6966376304626465, 'cosine_ionic_motion': -0.5988484025001526, 'motion_component_ionic': -3.4114224910736084, 'motion_component_percent_ionic': 59.88484025001526}, {'ion_id': 2276, 'distance': 9.756134033203125, 'force': [-1.0542205572128296, -3.153040885925293, -1.055195689201355], 'magnitude': 3.488049030303955, 'cosine_ionic_motion': -0.12325363606214523, 'motion_component_ionic': -0.4299147129058838, 'motion_component_percent_ionic': 12.325363606214523}, {'ion_id': 2391, 'distance': 13.279114723205566, 'force': [-0.07784866541624069, 0.08934804797172546, -1.8790479898452759], 'magnitude': 1.8827811479568481, 'cosine_ionic_motion': -0.5241919755935669, 'motion_component_ionic': -0.9869387149810791, 'motion_component_percent_ionic': 52.41919755935669}, {'ion_id': 2397, 'distance': 5.402998447418213, 'force': [1.1518453359603882, 10.004481315612793, 5.284388542175293], 'magnitude': 11.372825622558594, 'cosine_ionic_motion': 0.04174268990755081, 'motion_component_ionic': 0.47473233938217163, 'motion_component_percent_ionic': 4.174268990755081}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 5.283040523529053, 'force': [6.178944110870361, 4.969132423400879, 3.086221933364868], 'magnitude': 8.508606910705566, 'cosine_with_motion': 0.5981600880622864, 'motion_component': 5.089509010314941, 'motion_component_percent': 59.81600880622864}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 4.861706733703613, 'force': [-4.712672233581543, -5.613819122314453, -4.188048362731934], 'magnitude': 8.441800117492676, 'cosine_with_motion': -0.4987007975578308, 'motion_component': -4.209932327270508, 'motion_component_percent': 49.87007975578308}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 4.806948184967041, 'force': [-11.324604034423828, -5.468269348144531, -3.493640184402466], 'magnitude': 13.051979064941406, 'cosine_with_motion': -0.7191859483718872, 'motion_component': -9.386799812316895, 'motion_component_percent': 71.91859483718872}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 3.9989867210388184, 'force': [7.725991249084473, 2.5652873516082764, 2.8208439350128174], 'magnitude': 8.61561393737793, 'cosine_with_motion': 0.8080123066902161, 'motion_component': 6.961522102355957, 'motion_component_percent': 80.8012306690216}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 5.429563522338867, 'force': [4.222662925720215, 1.9278398752212524, 0.5436672568321228], 'magnitude': 4.673652172088623, 'cosine_with_motion': 0.678597092628479, 'motion_component': 3.1715266704559326, 'motion_component_percent': 67.8597092628479}, {'resid': 786, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 5.841325759887695, 'force': [-3.5671839714050293, -5.903143882751465, 0.9318822622299194], 'magnitude': 6.959907531738281, 'cosine_with_motion': -0.10570015013217926, 'motion_component': -0.7356632947921753, 'motion_component_percent': 10.570015013217926}, {'resid': 786, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 4.738321304321289, 'force': [5.097349166870117, 7.055403232574463, -1.7944735288619995], 'magnitude': 8.887171745300293, 'cosine_with_motion': 0.13996343314647675, 'motion_component': 1.2438790798187256, 'motion_component_percent': 13.996343314647675}], 'pip2_contributions': [{'resid': 1313, 'atom': 'C1', 'charge': 0.06000000238418579, 'distance': 27.730552673339844, 'force': [-0.019282139837741852, -0.012298567220568657, 0.012164638377726078], 'magnitude': 0.025904325768351555, 'cosine_with_motion': -0.24908046424388885, 'motion_component': -0.006452261470258236, 'motion_component_percent': 24.908046424388885}, {'resid': 1313, 'atom': 'C11', 'charge': 0.17000000178813934, 'distance': 27.084714889526367, 'force': [-0.06316477060317993, -0.03291052579879761, 0.029094668105244637], 'magnitude': 0.07693757116794586, 'cosine_with_motion': -0.3700832426548004, 'motion_component': -0.028473306447267532, 'motion_component_percent': 37.00832426548004}, {'resid': 1313, 'atom': 'C12', 'charge': 0.04000000283122063, 'distance': 27.32697868347168, 'force': [-0.015079725533723831, -0.007345029152929783, 0.005907777696847916], 'magnitude': 0.017783403396606445, 'cosine_with_motion': -0.4186989367008209, 'motion_component': -0.0074458918534219265, 'motion_component_percent': 41.86989367008209}, {'resid': 1313, 'atom': 'C13', 'charge': -0.05000000074505806, 'distance': 28.46809196472168, 'force': [0.017330802977085114, 0.008962357416749, -0.006234455853700638], 'magnitude': 0.020482895895838737, 'cosine_with_motion': 0.4230894148349762, 'motion_component': 0.00866609625518322, 'motion_component_percent': 42.30894148349762}, {'resid': 1313, 'atom': 'C2', 'charge': 0.06000000238418579, 'distance': 29.24079704284668, 'force': [-0.01730094850063324, -0.011150346137583256, 0.01091441884636879], 'magnitude': 0.023297587409615517, 'cosine_with_motion': -0.2470167577266693, 'motion_component': -0.0057548945769667625, 'motion_component_percent': 24.70167577266693}, {'resid': 1313, 'atom': 'C21', 'charge': 0.6299999952316284, 'distance': 24.86958885192871, 'force': [-0.29014649987220764, -0.13558435440063477, 0.10860106348991394], 'magnitude': 0.3381749391555786, 'cosine_with_motion': -0.4358730614185333, 'motion_component': -0.1474013477563858, 'motion_component_percent': 43.58730614185333}, {'resid': 1313, 'atom': 'C210', 'charge': -0.18000000715255737, 'distance': 23.948673248291016, 'force': [0.0933164581656456, 0.0457383468747139, 0.0075286743231117725], 'magnitude': 0.10419519245624542, 'cosine_with_motion': 0.6431180238723755, 'motion_component': 0.0670098066329956, 'motion_component_percent': 64.31180238723755}, {'resid': 1313, 'atom': 'C211', 'charge': -0.15000000596046448, 'distance': 23.936250686645508, 'force': [0.0761050283908844, 0.04063335806131363, 0.010580644011497498], 'magnitude': 0.08691947162151337, 'cosine_with_motion': 0.6416255235671997, 'motion_component': 0.055769748985767365, 'motion_component_percent': 64.16255235671997}, {'resid': 1313, 'atom': 'C212', 'charge': -0.15000000596046448, 'distance': 24.675167083740234, 'force': [0.06964115798473358, 0.04152088984847069, 0.010770543478429317], 'magnitude': 0.08179168403148651, 'cosine_with_motion': 0.6143959164619446, 'motion_component': 0.05025247856974602, 'motion_component_percent': 61.43959164619446}, {'resid': 1313, 'atom': 'C213', 'charge': -0.18000000715255737, 'distance': 25.70513343811035, 'force': [0.07643406838178635, 0.04761559143662453, 0.008388765156269073], 'magnitude': 0.09044215083122253, 'cosine_with_motion': 0.5849637389183044, 'motion_component': 0.052905380725860596, 'motion_component_percent': 58.496373891830444}, {'resid': 1313, 'atom': 'C214', 'charge': -0.15000000596046448, 'distance': 26.834144592285156, 'force': [0.05729609355330467, 0.0378718301653862, 0.008121744729578495], 'magnitude': 0.06915982067584991, 'cosine_with_motion': 0.5766386389732361, 'motion_component': 0.03988022357225418, 'motion_component_percent': 57.66386389732361}, {'resid': 1313, 'atom': 'C215', 'charge': -0.15000000596046448, 'distance': 27.523487091064453, 'force': [0.053243547677993774, 0.0380367785692215, 0.006319105159491301], 'magnitude': 0.06573890149593353, 'cosine_with_motion': 0.5418745875358582, 'motion_component': 0.035622239112854004, 'motion_component_percent': 54.187458753585815}, {'resid': 1313, 'atom': 'C216', 'charge': -0.18000000715255737, 'distance': 27.519813537597656, 'force': [0.06309903413057327, 0.04724236950278282, 0.00361968157812953], 'magnitude': 0.07890774309635162, 'cosine_with_motion': 0.5034100413322449, 'motion_component': 0.039722949266433716, 'motion_component_percent': 50.34100413322449}, {'resid': 1313, 'atom': 'C217', 'charge': -0.18000000715255737, 'distance': 28.713232040405273, 'force': [0.058729518204927444, 0.04246637597680092, 0.0012183438520878553], 'magnitude': 0.07248471677303314, 'cosine_with_motion': 0.5021401643753052, 'motion_component': 0.03639748692512512, 'motion_component_percent': 50.21401643753052}, {'resid': 1313, 'atom': 'C218', 'charge': -0.18000000715255737, 'distance': 30.014999389648438, 'force': [0.05273507907986641, 0.04018338397145271, 0.0021119527518749237], 'magnitude': 0.06633365154266357, 'cosine_with_motion': 0.4907509684562683, 'motion_component': 0.032553303986787796, 'motion_component_percent': 49.07509684562683}, {'resid': 1313, 'atom': 'C219', 'charge': -0.18000000715255737, 'distance': 31.236278533935547, 'force': [0.04945216700434685, 0.03613151237368584, 0.0005625594640150666], 'magnitude': 0.061248015612363815, 'cosine_with_motion': 0.4949568510055542, 'motion_component': 0.030315125361084938, 'motion_component_percent': 49.49568510055542}, {'resid': 1313, 'atom': 'C22', 'charge': -0.08000000566244125, 'distance': 23.849021911621094, 'force': [0.040408339351415634, 0.019398245960474014, -0.01309441588819027], 'magnitude': 0.04669678211212158, 'cosine_with_motion': 0.4570322334766388, 'motion_component': 0.02134193480014801, 'motion_component_percent': 45.70322334766388}, {'resid': 1313, 'atom': 'C220', 'charge': -0.27000001072883606, 'distance': 31.554725646972656, 'force': [0.07226505130529404, 0.053572751581668854, -0.0035488491412252188], 'magnitude': 0.09002706408500671, 'cosine_with_motion': 0.4663529098033905, 'motion_component': 0.04198438301682472, 'motion_component_percent': 46.63529098033905}, {'resid': 1313, 'atom': 'C23', 'charge': -0.18000000715255737, 'distance': 23.892274856567383, 'force': [0.09378361701965332, 0.039690155535936356, -0.024265944957733154], 'magnitude': 0.10468768328428268, 'cosine_with_motion': 0.5162906646728516, 'motion_component': 0.05404927581548691, 'motion_component_percent': 51.629066467285156}, {'resid': 1313, 'atom': 'C24', 'charge': -0.18000000715255737, 'distance': 23.757366180419922, 'force': [0.09517543017864227, 0.04261760786175728, -0.018329141661524773], 'magnitude': 0.10588002949953079, 'cosine_with_motion': 0.5397908687591553, 'motion_component': 0.05715307593345642, 'motion_component_percent': 53.97908687591553}, {'resid': 1313, 'atom': 'C25', 'charge': -0.15000000596046448, 'distance': 23.89841651916504, 'force': [0.08050385117530823, 0.031496815383434296, -0.011403183452785015], 'magnitude': 0.08719490468502045, 'cosine_with_motion': 0.5924752354621887, 'motion_component': 0.051660820841789246, 'motion_component_percent': 59.24752354621887}, {'resid': 1313, 'atom': 'C26', 'charge': -0.15000000596046448, 'distance': 23.235082626342773, 'force': [0.08569306135177612, 0.03328832983970642, -0.007592818234115839], 'magnitude': 0.09224458783864975, 'cosine_with_motion': 0.6204090714454651, 'motion_component': 0.05722937732934952, 'motion_component_percent': 62.04090714454651}, {'resid': 1313, 'atom': 'C27', 'charge': -0.18000000715255737, 'distance': 22.508872985839844, 'force': [0.10740755498409271, 0.048375945538282394, -0.00599303562194109], 'magnitude': 0.1179513931274414, 'cosine_with_motion': 0.605492353439331, 'motion_component': 0.07141866534948349, 'motion_component_percent': 60.549235343933105}, {'resid': 1313, 'atom': 'C28', 'charge': -0.15000000596046448, 'distance': 22.082761764526367, 'force': [0.09394954890012741, 0.040007561445236206, 0.0013917884789407253], 'magnitude': 0.10212276875972748, 'cosine_with_motion': 0.6494507789611816, 'motion_component': 0.06632371246814728, 'motion_component_percent': 64.94507789611816}, {'resid': 1313, 'atom': 'C29', 'charge': -0.15000000596046448, 'distance': 22.749645233154297, 'force': [0.08777151256799698, 0.03894048184156418, 0.006222316529601812], 'magnitude': 0.09622326493263245, 'cosine_with_motion': 0.66346275806427, 'motion_component': 0.06384055316448212, 'motion_component_percent': 66.346275806427}, {'resid': 1313, 'atom': 'C3', 'charge': 0.06000000238418579, 'distance': 29.984729766845703, 'force': [-0.016188768669962883, -0.010106164962053299, 0.011254881508648396], 'magnitude': 0.0221558827906847, 'cosine_with_motion': -0.22505025565624237, 'motion_component': -0.004986186977475882, 'motion_component_percent': 22.505025565624237}, {'resid': 1313, 'atom': 'C31', 'charge': 0.6299999952316284, 'distance': 29.23139190673828, 'force': [-0.2165512591600418, -0.09601981192827225, 0.061676714569330215], 'magnitude': 0.24478207528591156, 'cosine_with_motion': -0.49350547790527344, 'motion_component': -0.12080129235982895, 'motion_component_percent': 49.350547790527344}, {'resid': 1313, 'atom': 'C310', 'charge': -0.18000000715255737, 'distance': 24.763416290283203, 'force': [0.0953722670674324, 0.01982802152633667, 0.002796048065647483], 'magnitude': 0.09745171666145325, 'cosine_with_motion': 0.7615376710891724, 'motion_component': 0.07421315461397171, 'motion_component_percent': 76.15376710891724}, {'resid': 1313, 'atom': 'C311', 'charge': -0.18000000715255737, 'distance': 25.760116577148438, 'force': [0.08892184495925903, 0.01414494775235653, 0.0017303524073213339], 'magnitude': 0.09005647152662277, 'cosine_with_motion': 0.7781385779380798, 'motion_component': 0.07007641345262527, 'motion_component_percent': 77.81385779380798}, {'resid': 1313, 'atom': 'C312', 'charge': -0.18000000715255737, 'distance': 25.283205032348633, 'force': [0.09298013895750046, 0.00940130464732647, 0.002435517031699419], 'magnitude': 0.09348594397306442, 'cosine_with_motion': 0.8042635321617126, 'motion_component': 0.0751873329281807, 'motion_component_percent': 80.42635321617126}, {'resid': 1313, 'atom': 'C313', 'charge': -0.18000000715255737, 'distance': 26.404399871826172, 'force': [0.08552572876214981, 0.005430405028164387, 0.0017207800410687923], 'magnitude': 0.08571523427963257, 'cosine_with_motion': 0.8152034878730774, 'motion_component': 0.06987535953521729, 'motion_component_percent': 81.52034878730774}, {'resid': 1313, 'atom': 'C314', 'charge': -0.18000000715255737, 'distance': 27.372879028320312, 'force': [0.07943124324083328, 0.004968713968992233, 0.005214711185544729], 'magnitude': 0.07975715398788452, 'cosine_with_motion': 0.8355700373649597, 'motion_component': 0.06664268672466278, 'motion_component_percent': 83.55700373649597}, {'resid': 1313, 'atom': 'C315', 'charge': -0.18000000715255737, 'distance': 28.42221450805664, 'force': [0.07384230941534042, 0.0013943914091214538, 0.004232986830174923], 'magnitude': 0.07397668063640594, 'cosine_with_motion': 0.8465685844421387, 'motion_component': 0.06262633204460144, 'motion_component_percent': 84.65685844421387}, {'resid': 1313, 'atom': 'C316', 'charge': -0.18000000715255737, 'distance': 28.995861053466797, 'force': [0.07106927037239075, 0.0010233749635517597, 0.0005222775507718325], 'magnitude': 0.07107856124639511, 'cosine_with_motion': 0.825518012046814, 'motion_component': 0.05867663398385048, 'motion_component_percent': 82.5518012046814}, {'resid': 1313, 'atom': 'C317', 'charge': -0.18000000715255737, 'distance': 30.07297706604004, 'force': [0.06606361269950867, -0.0013718706322833896, 0.00019109009008388966], 'magnitude': 0.06607813388109207, 'cosine_with_motion': 0.8338508605957031, 'motion_component': 0.055099308490753174, 'motion_component_percent': 83.38508605957031}, {'resid': 1313, 'atom': 'C318', 'charge': -0.27000001072883606, 'distance': 29.75384521484375, 'force': [0.10100200772285461, -0.006806361488997936, 0.0021920434664934874], 'magnitude': 0.10125481337308884, 'cosine_with_motion': 0.8548267483711243, 'motion_component': 0.08655532449483871, 'motion_component_percent': 85.48267483711243}, {'resid': 1313, 'atom': 'C32', 'charge': -0.08000000566244125, 'distance': 29.455713272094727, 'force': [0.027490273118019104, 0.012009941972792149, -0.006093375850468874], 'magnitude': 0.030611811205744743, 'cosine_with_motion': 0.5297527313232422, 'motion_component': 0.016216689720749855, 'motion_component_percent': 52.97527313232422}, {'resid': 1313, 'atom': 'C33', 'charge': -0.18000000715255737, 'distance': 28.387529373168945, 'force': [0.06779313087463379, 0.027059141546487808, -0.01308577973395586], 'magnitude': 0.07415755838155746, 'cosine_with_motion': 0.5620900392532349, 'motion_component': 0.041683223098516464, 'motion_component_percent': 56.209003925323486}, {'resid': 1313, 'atom': 'C34', 'charge': -0.18000000715255737, 'distance': 28.795791625976562, 'force': [0.06651068478822708, 0.02616306021809578, -0.009266158565878868], 'magnitude': 0.0720696821808815, 'cosine_with_motion': 0.5926594138145447, 'motion_component': 0.042712774127721786, 'motion_component_percent': 59.26594138145447}, {'resid': 1313, 'atom': 'C35', 'charge': -0.18000000715255737, 'distance': 27.56857681274414, 'force': [0.07320688664913177, 0.027679694816470146, -0.007555202580988407], 'magnitude': 0.07862884551286697, 'cosine_with_motion': 0.6181979179382324, 'motion_component': 0.04860818758606911, 'motion_component_percent': 61.81979179382324}, {'resid': 1313, 'atom': 'C36', 'charge': -0.18000000715255737, 'distance': 28.069046020507812, 'force': [0.07137943804264069, 0.02540396898984909, -0.0035817893221974373], 'magnitude': 0.07584995031356812, 'cosine_with_motion': 0.65489661693573, 'motion_component': 0.04967387765645981, 'motion_component_percent': 65.489661693573}, {'resid': 1313, 'atom': 'C37', 'charge': -0.18000000715255737, 'distance': 26.985700607299805, 'force': [0.0777549222111702, 0.026227684691548347, -0.0006969001842662692], 'magnitude': 0.08206220716238022, 'cosine_with_motion': 0.6832799911499023, 'motion_component': 0.05607146397233009, 'motion_component_percent': 68.32799911499023}, {'resid': 1313, 'atom': 'C38', 'charge': -0.18000000715255737, 'distance': 26.29918670654297, 'force': [0.08319058269262314, 0.023313380777835846, -0.0010925483657047153], 'magnitude': 0.08640243113040924, 'cosine_with_motion': 0.7088683247566223, 'motion_component': 0.061247944831848145, 'motion_component_percent': 70.88683247566223}, {'resid': 1313, 'atom': 'C39', 'charge': -0.18000000715255737, 'distance': 25.439516067504883, 'force': [0.08919260650873184, 0.023723391816020012, 0.0029453446622937918], 'magnitude': 0.09234064817428589, 'cosine_with_motion': 0.7365175485610962, 'motion_component': 0.06801050901412964, 'motion_component_percent': 73.65175485610962}, {'resid': 1313, 'atom': 'C4', 'charge': 0.08000000566244125, 'distance': 29.406368255615234, 'force': [-0.021480869501829147, -0.01427800115197897, 0.016676316037774086], 'magnitude': 0.03071463108062744, 'cosine_with_motion': -0.1798992156982422, 'motion_component': -0.005525538232177496, 'motion_component_percent': 17.98992156982422}, {'resid': 1313, 'atom': 'C5', 'charge': 0.08000000566244125, 'distance': 27.909412384033203, 'force': [-0.02400991879403591, -0.015430469997227192, 0.01865706779062748], 'magnitude': 0.0340978279709816, 'cosine_with_motion': -0.18552850186824799, 'motion_component': -0.00632611894980073, 'motion_component_percent': 18.5528501868248}, {'resid': 1313, 'atom': 'C6', 'charge': 0.06000000238418579, 'distance': 27.129344940185547, 'force': [-0.019299976527690887, -0.01299662608653307, 0.013824686408042908], 'magnitude': 0.02706516906619072, 'cosine_with_motion': -0.20197506248950958, 'motion_component': -0.0054664891213178635, 'motion_component_percent': 20.19750624895096}, {'resid': 1313, 'atom': 'H1', 'charge': 0.12000000476837158, 'distance': 27.443714141845703, 'force': [-0.040435079485177994, -0.023382920771837234, 0.024826763197779655], 'magnitude': 0.05289730429649353, 'cosine_with_motion': -0.2755740284919739, 'motion_component': -0.014577123336493969, 'motion_component_percent': 27.557402849197388}, {'resid': 1313, 'atom': 'H10R', 'charge': 0.09000000357627869, 'distance': 24.739301681518555, 'force': [-0.04435037821531296, -0.020061038434505463, -0.0037521100603044033], 'magnitude': 0.048820894211530685, 'cosine_with_motion': -0.664323627948761, 'motion_component': -0.03243287280201912, 'motion_component_percent': 66.4323627948761}, {'resid': 1313, 'atom': 'H10S', 'charge': 0.09000000357627869, 'distance': 24.011629104614258, 'force': [-0.045883920043706894, -0.02402385137975216, -0.0018239966593682766], 'magnitude': 0.051824767142534256, 'cosine_with_motion': -0.6096327304840088, 'motion_component': -0.03159407526254654, 'motion_component_percent': 60.96327304840088}, {'resid': 1313, 'atom': 'H10X', 'charge': 0.09000000357627869, 'distance': 24.00147819519043, 'force': [-0.050783902406692505, -0.010550505481660366, 0.0001883870136225596], 'magnitude': 0.05186861753463745, 'cosine_with_motion': -0.7464960217475891, 'motion_component': -0.03871971741318703, 'motion_component_percent': 74.64960217475891}, {'resid': 1313, 'atom': 'H10Y', 'charge': 0.09000000357627869, 'distance': 24.305870056152344, 'force': [-0.049456167966127396, -0.01000219490379095, -0.0034839569125324488], 'magnitude': 0.05057760700583458, 'cosine_with_motion': -0.7817186117172241, 'motion_component': -0.0395374558866024, 'motion_component_percent': 78.17186117172241}, {'resid': 1313, 'atom': 'H111', 'charge': 0.15000000596046448, 'distance': 23.244386672973633, 'force': [-0.08071717619895935, -0.042120009660720825, -0.014355908147990704], 'magnitude': 0.09217076748609543, 'cosine_with_motion': -0.6611204147338867, 'motion_component': -0.06093597412109375, 'motion_component_percent': 66.11204147338867}, {'resid': 1313, 'atom': 'H11A', 'charge': 0.09000000357627869, 'distance': 28.11920166015625, 'force': [-0.030773645266890526, -0.016269151121377945, 0.014709411188960075], 'magnitude': 0.03778980299830437, 'cosine_with_motion': -0.3584764897823334, 'motion_component': -0.013546755537390709, 'motion_component_percent': 35.84764897823334}, {'resid': 1313, 'atom': 'H11B', 'charge': 0.09000000357627869, 'distance': 26.486507415771484, 'force': [-0.03511406481266022, -0.017079874873161316, 0.017011335119605064], 'magnitude': 0.04259231314063072, 'cosine_with_motion': -0.37080761790275574, 'motion_component': -0.015793554484844208, 'motion_component_percent': 37.080761790275574}, {'resid': 1313, 'atom': 'H11X', 'charge': 0.09000000357627869, 'distance': 26.56309700012207, 'force': [-0.04170222952961922, -0.007105013355612755, -0.0019277473911643028], 'magnitude': 0.04234705865383148, 'cosine_with_motion': -0.7853004336357117, 'motion_component': -0.033255163580179214, 'motion_component_percent': 78.53004336357117}, {'resid': 1313, 'atom': 'H11Y', 'charge': 0.09000000357627869, 'distance': 26.286468505859375, 'force': [-0.04269217327237129, -0.006837464869022369, 0.000766381504945457], 'magnitude': 0.043243035674095154, 'cosine_with_motion': -0.7600991129875183, 'motion_component': -0.032868992537260056, 'motion_component_percent': 76.00991129875183}, {'resid': 1313, 'atom': 'H12', 'charge': 0.09000000357627869, 'distance': 27.58008575439453, 'force': [-0.0338219590485096, -0.014826618134975433, 0.013389998115599155], 'magnitude': 0.03928161785006523, 'cosine_with_motion': -0.4360077381134033, 'motion_component': -0.017127089202404022, 'motion_component_percent': 43.60077381134033}, {'resid': 1313, 'atom': 'H121', 'charge': 0.15000000596046448, 'distance': 24.64780616760254, 'force': [-0.06827235966920853, -0.043278515338897705, -0.013619461096823215], 'magnitude': 0.0819733738899231, 'cosine_with_motion': -0.6093812584877014, 'motion_component': -0.04995303601026535, 'motion_component_percent': 60.93812584877014}, {'resid': 1313, 'atom': 'H12X', 'charge': 0.09000000357627869, 'distance': 24.527080535888672, 'force': [-0.04947111755609512, -0.00442988658323884, 0.000183084441232495], 'magnitude': 0.04966939613223076, 'cosine_with_motion': -0.794665515422821, 'motion_component': -0.03947055712342262, 'motion_component_percent': 79.4665515422821}, {'resid': 1313, 'atom': 'H12Y', 'charge': 0.09000000357627869, 'distance': 24.835180282592773, 'force': [-0.04810182750225067, -0.004786095581948757, -0.0031926899682730436], 'magnitude': 0.04844466596841812, 'cosine_with_motion': -0.8224155306816101, 'motion_component': -0.03984164446592331, 'motion_component_percent': 82.24155306816101}, {'resid': 1313, 'atom': 'H13A', 'charge': 0.09000000357627869, 'distance': 29.414493560791016, 'force': [-0.029167240485548973, -0.014795828610658646, 0.01109111588448286], 'magnitude': 0.03453487157821655, 'cosine_with_motion': -0.41654953360557556, 'motion_component': -0.014385484158992767, 'motion_component_percent': 41.654953360557556}, {'resid': 1313, 'atom': 'H13B', 'charge': 0.09000000357627869, 'distance': 28.453506469726562, 'force': [-0.030559668317437172, -0.017403997480869293, 0.011195358820259571], 'magnitude': 0.036907024681568146, 'cosine_with_motion': -0.3984428346157074, 'motion_component': -0.014705339446663857, 'motion_component_percent': 39.84428346157074}, {'resid': 1313, 'atom': 'H13R', 'charge': 0.09000000357627869, 'distance': 25.333044052124023, 'force': [-0.038720812648534775, -0.025681735947728157, -0.00298490934073925], 'magnitude': 0.04655923694372177, 'cosine_with_motion': -0.5526535511016846, 'motion_component': -0.025731127709150314, 'motion_component_percent': 55.26535511016846}, {'resid': 1313, 'atom': 'H13S', 'charge': 0.09000000357627869, 'distance': 26.08206558227539, 'force': [-0.037888988852500916, -0.022021202370524406, -0.002960139187052846], 'magnitude': 0.04392346739768982, 'cosine_with_motion': -0.5948590040206909, 'motion_component': -0.026128269731998444, 'motion_component_percent': 59.48590040206909}, {'resid': 1313, 'atom': 'H13X', 'charge': 0.09000000357627869, 'distance': 26.815200805664062, 'force': [-0.041435521095991135, -0.003065626136958599, 0.0006924846675246954], 'magnitude': 0.041554540395736694, 'cosine_with_motion': -0.794026792049408, 'motion_component': -0.03299541771411896, 'motion_component_percent': 79.4026792049408}, {'resid': 1313, 'atom': 'H13Y', 'charge': 0.09000000357627869, 'distance': 25.94521141052246, 'force': [-0.04436831921339035, -0.0011400912189856172, -0.0006728777079842985], 'magnitude': 0.0443880632519722, 'cosine_with_motion': -0.8256018161773682, 'motion_component': -0.03664686530828476, 'motion_component_percent': 82.56018161773682}, {'resid': 1313, 'atom': 'H141', 'charge': 0.15000000596046448, 'distance': 27.05891227722168, 'force': [-0.05661053955554962, -0.0362214669585228, -0.010458365082740784], 'magnitude': 0.06801562756299973, 'cosine_with_motion': -0.6016552448272705, 'motion_component': -0.04092196002602577, 'motion_component_percent': 60.16552448272705}, {'resid': 1313, 'atom': 'H14X', 'charge': 0.09000000357627869, 'distance': 27.929527282714844, 'force': [-0.03803815692663193, -0.0036863002460449934, -0.0026017564814537764], 'magnitude': 0.03830482065677643, 'cosine_with_motion': -0.8242396712303162, 'motion_component': -0.03157235309481621, 'motion_component_percent': 82.42396712303162}, {'resid': 1313, 'atom': 'H14Y', 'charge': 0.09000000357627869, 'distance': 26.88328742980957, 'force': [-0.04106626287102699, -0.0023411051370203495, -0.004175468347966671], 'magnitude': 0.04134432598948479, 'cosine_with_motion': -0.8520653247833252, 'motion_component': -0.03522806614637375, 'motion_component_percent': 85.20653247833252}, {'resid': 1313, 'atom': 'H151', 'charge': 0.15000000596046448, 'distance': 28.345943450927734, 'force': [-0.049593523144721985, -0.03645175322890282, -0.0072939470410346985], 'magnitude': 0.06197942793369293, 'cosine_with_motion': -0.5412318110466003, 'motion_component': -0.03354523703455925, 'motion_component_percent': 54.123181104660034}, {'resid': 1313, 'atom': 'H15X', 'charge': 0.09000000357627869, 'distance': 27.96762466430664, 'force': [-0.03810669854283333, 0.000560825108550489, -0.002616451121866703], 'magnitude': 0.038200534880161285, 'cosine_with_motion': -0.8614564538002014, 'motion_component': -0.03290809690952301, 'motion_component_percent': 86.14564538002014}, {'resid': 1313, 'atom': 'H15Y', 'charge': 0.09000000357627869, 'distance': 29.295719146728516, 'force': [-0.034695103764534, -0.0009671602747403085, -0.002726068254560232], 'magnitude': 0.0348154716193676, 'cosine_with_motion': -0.8525875210762024, 'motion_component': -0.02968323603272438, 'motion_component_percent': 85.25875210762024}, {'resid': 1313, 'atom': 'H16R', 'charge': 0.09000000357627869, 'distance': 27.431198120117188, 'force': [-0.03078063204884529, -0.025015277788043022, -0.0018996003782376647], 'magnitude': 0.039709191769361496, 'cosine_with_motion': -0.4747333824634552, 'motion_component': -0.018851278349757195, 'motion_component_percent': 47.47333824634552}, {'resid': 1313, 'atom': 'H16S', 'charge': 0.09000000357627869, 'distance': 26.620155334472656, 'force': [-0.03403468430042267, -0.024867556989192963, -0.0010919328778982162], 'magnitude': 0.042165715247392654, 'cosine_with_motion': -0.5027717351913452, 'motion_component': -0.021199729293584824, 'motion_component_percent': 50.27717351913452}, {'resid': 1313, 'atom': 'H16X', 'charge': 0.09000000357627869, 'distance': 29.353063583374023, 'force': [-0.0346391387283802, -0.0016691082855686545, 0.000129871565150097], 'magnitude': 0.03467957302927971, 'cosine_with_motion': -0.8092706799507141, 'motion_component': -0.028065161779522896, 'motion_component_percent': 80.92706799507141}, {'resid': 1313, 'atom': 'H16Y', 'charge': 0.09000000357627869, 'distance': 28.200084686279297, 'force': [-0.03756917268037796, -8.249126949522179e-06, 0.0005591108347289264], 'magnitude': 0.03757333382964134, 'cosine_with_motion': -0.8191837668418884, 'motion_component': -0.030779464170336723, 'motion_component_percent': 81.91837668418884}, {'resid': 1313, 'atom': 'H17R', 'charge': 0.09000000357627869, 'distance': 28.606454849243164, 'force': [-0.029588675126433372, -0.02138078212738037, 0.0007761635351926088], 'magnitude': 0.036513421684503555, 'cosine_with_motion': -0.48418161273002625, 'motion_component': -0.01767912693321705, 'motion_component_percent': 48.418161273002625}, {'resid': 1313, 'atom': 'H17S', 'charge': 0.09000000357627869, 'distance': 28.834047317504883, 'force': [-0.029880594462156296, -0.019951988011598587, -0.0008368762210011482], 'magnitude': 0.035939283668994904, 'cosine_with_motion': -0.5319346785545349, 'motion_component': -0.01911735162138939, 'motion_component_percent': 53.19346785545349}, {'resid': 1313, 'atom': 'H17X', 'charge': 0.09000000357627869, 'distance': 30.27924156188965, 'force': [-0.03256048262119293, 0.0009346695733256638, 0.001039295457303524], 'magnitude': 0.03259047120809555, 'cosine_with_motion': -0.8190614581108093, 'motion_component': -0.026693599298596382, 'motion_component_percent': 81.90614581108093}, {'resid': 1313, 'atom': 'H17Y', 'charge': 0.09000000357627869, 'distance': 31.018585205078125, 'force': [-0.031046107411384583, 0.00044218168477527797, -0.0006159791373647749], 'magnitude': 0.03105536662042141, 'cosine_with_motion': -0.8399099707603455, 'motion_component': -0.02608371153473854, 'motion_component_percent': 8</t>
         </is>
       </c>
     </row>
@@ -563,7 +563,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>{706: {'frame': 706, 'motion_vector': [-1.6462364196777344, 4.194007873535156, 1.78082275390625], 'ionic_force': [-2.4678491204977036, -11.519292116165161, -0.8560818731784821], 'ionic_force_magnitude': 11.811741883086968, 'radial_force': 11.780677830205107, 'axial_force': -0.8560818731784821, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-5.030915379524231, -3.7795519828796387, -7.650073170661926], 'asn_force_magnitude': 9.905490511009754, 'residue_force': [-5.030915379524231, -3.7795519828796387, -7.650073170661926], 'residue_force_magnitude': 9.905490511009754, 'total_force': [-7.4987645000219345, -15.2988440990448, -8.506155043840408], 'total_force_magnitude': 19.043129297033058, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': -0.4416169984765415, 'cosine_residue_motion': -0.4416169984765415, 'cosine_ionic_motion': -0.7999018642793536, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': -4.374432987909991, 'motion_component_residue': -4.374432987909991, 'motion_component_ionic': -9.44823435266779, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 44.16169984765415, 'motion_component_percent_residue': 44.16169984765415, 'motion_component_percent_ionic': 79.99018642793536, 'ionic_contributions': [{'ion_id': 2276, 'distance': 7.746928691864014, 'force': [0.08160331845283508, -4.599984169006348, 3.07181715965271], 'magnitude': 5.531959533691406, 'cosine_ionic_motion': -0.5207458138465881, 'motion_component_ionic': -2.880744695663452, 'motion_component_percent_ionic': 52.07458138465881}, {'ion_id': 2391, 'distance': 10.210418701171875, 'force': [0.22415855526924133, -2.0812742710113525, -2.39990496635437], 'magnitude': 3.1845712661743164, 'cosine_ionic_motion': -0.8666999936103821, 'motion_component_ionic': -2.760067939758301, 'motion_component_percent_ionic': 86.66999936103821}, {'ion_id': 2397, 'distance': 8.644484519958496, 'force': [-3.0071139335632324, -3.044539213180542, -1.1944888830184937], 'magnitude': 4.442831993103027, 'cosine_ionic_motion': -0.4620648920536041, 'motion_component_ionic': -2.0528767108917236, 'motion_component_percent_ionic': 46.20648920536041}, {'ion_id': 2520, 'distance': 13.435805320739746, 'force': [0.23350293934345245, -1.793494462966919, -0.33350518345832825], 'magnitude': 1.8391225337982178, 'cosine_ionic_motion': -0.9540119171142578, 'motion_component_ionic': -1.7545448541641235, 'motion_component_percent_ionic': 95.40119171142578}], 'glu_contributions': [], 'asn_contributions': [{'resid': 1114, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 3.432359457015991, 'force': [-7.456222057342529, 15.6506929397583, 10.285576820373535], 'magnitude': 20.157691955566406, 'cosine_with_motion': 0.9853840470314026, 'motion_component': 19.863067626953125, 'motion_component_percent': 98.53840470314026}, {'resid': 1114, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 2.944586992263794, 'force': [0.87669837474823, -18.019702911376953, -14.28624439239502], 'magnitude': 23.01249885559082, 'cosine_with_motion': -0.9190108180046082, 'motion_component': -21.14873504638672, 'motion_component_percent': 91.90108180046082}, {'resid': 1114, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 3.606640577316284, 'force': [11.241238594055176, -19.941492080688477, -3.6771652698516846], 'magnitude': 23.18512725830078, 'cosine_with_motion': -0.9676286578178406, 'motion_component': -22.434593200683594, 'motion_component_percent': 96.76286578178406}, {'resid': 1114, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 3.16558575630188, 'force': [-4.855937957763672, 12.832906723022461, -0.8816777467727661], 'magnitude': 13.749217987060547, 'cosine_with_motion': 0.9044355750083923, 'motion_component': 12.435281753540039, 'motion_component_percent': 90.44355750083923}, {'resid': 1114, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 4.277791500091553, 'force': [-4.8366923332214355, 5.698043346405029, 0.9094374179840088], 'magnitude': 7.529167652130127, 'cosine_with_motion': 0.9178365468978882, 'motion_component': 6.910545349121094, 'motion_component_percent': 91.78365468978882}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': -0.725861129490486, 'motion_component_pip2': -13.82266734057778, 'motion_component_percent_pip2': 72.5861129490486}, 707: {'frame': 707, 'motion_vector': [-0.55010986328125, -3.9834671020507812, -1.3980331420898438], 'ionic_force': [-10.146550849080086, -8.860189855098724, -1.1158610880374908], 'ionic_force_magnitude': 13.516678747723436, 'radial_force': 13.470540390101734, 'axial_force': -1.1158610880374908, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-0.34980010986328125, 0.45755040645599365, -1.7348904609680176], 'asn_force_magnitude': 1.8279927250583436, 'residue_force': [-0.34980010986328125, 0.45755040645599365, -1.7348904609680176], 'residue_force_magnitude': 1.8279927250583436, 'total_force': [-10.496350958943367, -8.40263944864273, -2.8507515490055084], 'total_force_magnitude': 13.744253983078007, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': 0.10218226837784337, 'cosine_residue_motion': 0.10218226837784337, 'cosine_ionic_motion': 0.7374353820666473, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': 0.18678844322465693, 'motion_component_residue': 0.18678844322465693, 'motion_component_ionic': 9.967677156599564, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 10.218226837784337, 'motion_component_percent_residue': 10.218226837784337, 'motion_component_percent_ionic': 73.74353820666472, 'ionic_contributions': [{'ion_id': 2276, 'distance': 6.0538859367370605, 'force': [-2.146378993988037, -5.052443981170654, 7.206060886383057], 'magnitude': 9.058777809143066, 'cosine_ionic_motion': 0.29125484824180603, 'motion_component_ionic': 2.6384129524230957, 'motion_component_percent_ionic': 29.125484824180603}, {'ion_id': 2333, 'distance': 12.209272384643555, 'force': [-0.08800055831670761, -0.5070242285728455, -2.1669301986694336], 'magnitude': 2.227196455001831, 'cosine_ionic_motion': 0.5376054644584656, 'motion_component_ionic': 1.1973530054092407, 'motion_component_percent_ionic': 53.76054644584656}, {'ion_id': 2391, 'distance': 6.793758869171143, 'force': [-0.8784823417663574, -2.3900206089019775, -6.727344989776611], 'magnitude': 7.19312858581543, 'cosine_ionic_motion': 0.6337853074073792, 'motion_component_ionic': 4.558899402618408, 'motion_component_percent_ionic': 63.378530740737915}, {'ion_id': 2397, 'distance': 6.574862957000732, 'force': [-6.953972816467285, 3.142096757888794, 0.8676580190658569], 'magnitude': 7.680061340332031, 'cosine_ionic_motion': -0.3029043972492218, 'motion_component_ionic': -2.326324462890625, 'motion_component_percent_ionic': 30.29043972492218}, {'ion_id': 2520, 'distance': 9.038052558898926, 'force': [-0.07971613854169846, -4.052797794342041, -0.2953048050403595], 'magnitude': 4.064323902130127, 'cosine_ionic_motion': 0.9594059586524963, 'motion_component_ionic': 3.899336576461792, 'motion_component_percent_ionic': 95.94059586524963}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 5.827349662780762, 'force': [5.088626861572266, -1.4325895309448242, 4.578238010406494], 'magnitude': 6.993332386016846, 'cosine_with_motion': -0.11732585728168488, 'motion_component': -0.8204987049102783, 'motion_component_percent': 11.732585728168488}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 4.832463264465332, 'force': [-5.438426971435547, 1.8901399374008179, -6.313128471374512], 'magnitude': 8.544279098510742, 'cosine_with_motion': 0.11789023131132126, 'motion_component': 1.0072870254516602, 'motion_component_percent': 11.789023131132126}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': 0.7388153341990368, 'motion_component_pip2': 10.15446559982422, 'motion_component_percent_pip2': 73.88153341990368}, 708: {'frame': 708, 'motion_vector': [0.17077255249023438, 2.1774368286132812, 0.35927581787109375], 'ionic_force': [-3.8774969652295113, -10.092415452003479, -2.3113385438919067], 'ionic_force_magnitude': 11.055953972212574, 'radial_force': 10.811652619798819, 'axial_force': -2.3113385438919067, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [3.2459144592285156, -2.9549927711486816, -1.8020532429218292], 'asn_force_magnitude': 4.74503307095902, 'residue_force': [3.2459144592285156, -2.9549927711486816, -1.8020532429218292], 'residue_force_magnitude': 4.74503307095902, 'total_force': [-0.6315825060009956, -13.04740822315216, -4.113391786813736], 'total_force_magnitude': 13.695026462015026, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': -0.6214816855801305, 'cosine_residue_motion': -0.6214816855801305, 'cosine_ionic_motion': -0.9589774190409146, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': -2.948951151073075, 'motion_component_residue': -2.948951151073075, 'motion_component_ionic': -10.602410205307562, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 62.14816855801305, 'motion_component_percent_residue': 62.14816855801305, 'motion_component_percent_ionic': 95.89774190409146, 'ionic_contributions': [{'ion_id': 2276, 'distance': 9.638389587402344, 'force': [-1.3283097743988037, -1.6270325183868408, 2.8914248943328857], 'magnitude': 3.5737907886505127, 'cosine_ionic_motion': -0.34520965814590454, 'motion_component_ionic': -1.233707070350647, 'motion_component_percent_ionic': 34.520965814590454}, {'ion_id': 2333, 'distance': 13.627022743225098, 'force': [-0.1465599238872528, -0.7644345760345459, -1.6095471382141113], 'magnitude': 1.7878707647323608, 'cosine_ionic_motion': -0.573053777217865, 'motion_component_ionic': -1.0245461463928223, 'motion_component_percent_ionic': 57.3053777217865}, {'ion_id': 2391, 'distance': 8.851482391357422, 'force': [-0.5468158721923828, -2.932461977005005, -3.0096118450164795], 'magnitude': 4.237464427947998, 'cosine_ionic_motion': -0.8060017824172974, 'motion_component_ionic': -3.4154038429260254, 'motion_component_percent_ionic': 80.60017824172974}, {'ion_id': 2397, 'distance': 9.911685943603516, 'force': [-1.7836471796035767, -2.8530490398406982, -0.31502169370651245], 'magnitude': 3.3794267177581787, 'cosine_ionic_motion': -0.886345624923706, 'motion_component_ionic': -2.99534010887146, 'motion_component_percent_ionic': 88.6345624923706}, {'ion_id': 2520, 'distance': 13.096944808959961, 'force': [-0.07216421514749527, -1.9154373407363892, -0.2685827612876892], 'magnitude': 1.9355218410491943, 'cosine_ionic_motion': -0.9989105463027954, 'motion_component_ionic': -1.9334131479263306, 'motion_component_percent_ionic': 99.89105463027954}], 'glu_contributions': [], 'asn_contributions': [{'resid': 1114, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 5.6480326652526855, 'force': [-5.772580146789551, 3.4670333862304688, 3.1743741035461426], 'magnitude': 7.4444379806518555, 'cosine_with_motion': 0.46752554178237915, 'motion_component': 3.4804649353027344, 'motion_component_percent': 46.752554178237915}, {'resid': 1114, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 5.037877082824707, 'force': [5.113110542297363, -4.945231914520264, -3.347742795944214], 'magnitude': 7.861717700958252, 'cosine_with_motion': -0.6377251744270325, 'motion_component': -5.013615131378174, 'motion_component_percent': 63.77251744270325}, {'resid': 1114, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 5.99411153793335, 'force': [7.392880439758301, -3.446922540664673, -1.9804470539093018], 'magnitude': 8.39393424987793, 'cosine_with_motion': -0.37430399656295776, 'motion_component': -3.141883134841919, 'motion_component_percent': 37.430399656295776}, {'resid': 1114, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 5.853701114654541, 'force': [-3.4874963760375977, 1.9701282978057861, 0.3517625033855438], 'magnitude': 4.020916938781738, 'cosine_with_motion': 0.4292758107185364, 'motion_component': 1.7260823249816895, 'motion_component_percent': 42.92758107185364}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': -0.9895096876203296, 'motion_component_pip2': -13.551361356380637, 'motion_component_percent_pip2': 98.95096876203297}, 709: {'frame': 709, 'motion_vector': [7.310642242431641, 6.703319549560547, 0.2125701904296875], 'ionic_force': [-7.450491823256016, -5.189851522445679, -7.015001654624939], 'ionic_force_magnitude': 11.474085386113662, 'radial_force': 9.079889164160347, 'axial_force': -7.015001654624939, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-2.2841343879699707, 3.0783824920654297, -3.716277837753296], 'asn_force_magnitude': 5.338953983425801, 'residue_force': [-2.2841343879699707, 3.0783824920654297, -3.716277837753296], 'residue_force_magnitude': 5.338953983425801, 'total_force': [-9.734626211225986, -2.111469030380249, -10.731279492378235], 'total_force_magnitude': 14.641776138231338, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': 0.059412367349464444, 'cosine_residue_motion': 0.059412367349464444, 'cosine_ionic_motion': -0.7972000077097854, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': 0.3171998953251802, 'motion_component_residue': 0.3171998953251802, 'motion_component_ionic': -9.147140958272548, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 5.941236734946444, 'motion_component_percent_residue': 5.941236734946444, 'motion_component_percent_ionic': 79.72000077097854, 'ionic_contributions': [{'ion_id': 2276, 'distance': 14.292695045471191, 'force': [-0.7468556761741638, -0.284122109413147, 1.4152005910873413], 'magnitude': 1.625211238861084, 'cosine_ionic_motion': -0.43809768557548523, 'motion_component_ionic': -0.7120012640953064, 'motion_component_percent_ionic': 43.80976855754852}, {'ion_id': 2333, 'distance': 12.876778602600098, 'force': [-0.07675156742334366, -0.6486190557479858, -1.892750859260559], 'magnitude': 2.002274513244629, 'cosine_ionic_motion': -0.26737940311431885, 'motion_component_ionic': -0.535366952419281, 'motion_component_percent_ionic': 26.737940311431885}, {'ion_id': 2391, 'distance': 7.903709888458252, 'force': [-0.9395467638969421, -2.8548367023468018, -4.383246898651123], 'magnitude': 5.314667701721191, 'cosine_ionic_motion': -0.5108874440193176, 'motion_component_ionic': -2.7151968479156494, 'motion_component_percent_ionic': 51.08874440193176}, {'ion_id': 2397, 'distance': 7.526681423187256, 'force': [-5.480003833770752, 0.9537739753723145, -1.8451972007751465], 'magnitude': 5.860450267791748, 'cosine_ionic_motion': -0.5858345627784729, 'motion_component_ionic': -3.4332542419433594, 'motion_component_percent_ionic': 58.58345627784729}, {'ion_id': 2520, 'distance': 11.797821044921875, 'force': [-0.2073339819908142, -2.3560476303100586, -0.30900728702545166], 'magnitude': 2.385253429412842, 'cosine_ionic_motion': -0.7342289090156555, 'motion_component_ionic': -1.7513220310211182, 'motion_component_percent_ionic': 73.42289090156555}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 4.945583820343018, 'force': [6.2614030838012695, -5.337404251098633, 5.155470371246338], 'magnitude': 9.709373474121094, 'cosine_with_motion': 0.11515505611896515, 'motion_component': 1.1180834770202637, 'motion_component_percent': 11.515505611896515}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 4.558607578277588, 'force': [-4.648519515991211, 4.786935806274414, -6.904287338256836], 'magnitude': 9.601701736450195, 'cosine_with_motion': -0.035303592681884766, 'motion_component': -0.33897456526756287, 'motion_component_percent': 3.5303592681884766}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 5.4912872314453125, 'force': [-5.758846759796143, 7.184171676635742, -3.9056577682495117], 'magnitude': 10.001540184020996, 'cosine_with_motion': 0.052675455808639526, 'motion_component': 0.5268356800079346, 'motion_component_percent': 5.267545580863953}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 5.560068130493164, 'force': [1.8618288040161133, -3.5553207397460938, 1.9381968975067139], 'magnitude': 4.456828594207764, 'cosine_with_motion': -0.22184942662715912, 'motion_component': -0.988744854927063, 'motion_component_percent': 22.184942662715912}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': -0.603064886362481, 'motion_component_pip2': -8.829941062947368, 'motion_component_percent_pip2': 60.306488636248105}, 710: {'frame': 710, 'motion_vector': [-7.800167083740234, -1.7639541625976562, 2.1779327392578125], 'ionic_force': [8.9276821911335, 4.941914975643158, -3.1694294810295105], 'ionic_force_magnitude': 10.68509785484379, 'radial_force': 10.204216429122246, 'axial_force': -3.1694294810295105, 'glu_force': [4.224793434143066, -0.09057199954986572, 0.5486898422241211], 'glu_force_magnitude': 4.261237307548215, 'asn_force': [7.761636734008789, -10.032618522644043, -0.7592096924781799], 'asn_force_magnitude': 12.70719632998435, 'residue_force': [11.986430168151855, -10.123190522193909, -0.21051985025405884], 'residue_force_magnitude': 15.690691926488407, 'total_force': [20.914112359285355, -5.181275546550751, -3.3799493312835693], 'total_force_magnitude': 21.809854872239328, 'cosine_total_motion': 0, 'cosine_glu_motion': -0.8946876473746518, 'cosine_asn_motion': -0.42249830613006145, 'cosine_residue_motion': -0.5851396069523559, 'cosine_ionic_motion': -0.9626837760498828, 'motion_component_total': 0, 'motion_component_glu': -3.812476381595408, 'motion_component_asn': -5.368768925080522, 'motion_component_residue': -9.18124530667593, 'motion_component_ionic': -10.286370350363521, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 89.46876473746518, 'motion_component_percent_asn': 42.24983061300615, 'motion_component_percent_residue': 58.51396069523559, 'motion_component_percent_ionic': 96.26837760498827, 'ionic_contributions': [{'ion_id': 2276, 'distance': 14.493760108947754, 'force': [0.3473559319972992, 0.8600876927375793, 1.279593586921692], 'magnitude': 1.580432415008545, 'cosine_ionic_motion': -0.10990864038467407, 'motion_component_ionic': -0.1737031787633896, 'motion_component_percent_ionic': 10.990864038467407}, {'ion_id': 2333, 'distance': 13.539588928222656, 'force': [0.8468308448791504, 0.35124027729034424, -1.5618451833724976], 'magnitude': 1.8110363483428955, 'cosine_ionic_motion': -0.7079393267631531, 'motion_component_ionic': -1.2821038961410522, 'motion_component_percent_ionic': 70.79393267631531}, {'ion_id': 2391, 'distance': 8.410918235778809, 'force': [3.2061233520507812, 1.4390449523925781, -3.110344409942627], 'magnitude': 4.693007469177246, 'cosine_ionic_motion': -0.8823399543762207, 'motion_component_ionic': -4.1408281326293945, 'motion_component_percent_ionic': 88.23399543762207}, {'ion_id': 2397, 'distance': 7.536571502685547, 'force': [0.9619972109794617, 5.69840145111084, 0.8762056231498718], 'magnitude': 5.84507942199707, 'cosine_ionic_motion': -0.32297879457473755, 'motion_component_ionic': -1.8878366947174072, 'motion_component_percent_ionic': 32.297879457473755}, {'ion_id': 2520, 'distance': 8.169528007507324, 'force': [3.5653748512268066, -3.4068593978881836, -0.6530390977859497], 'magnitude': 4.97443962097168, 'cosine_ionic_motion': -0.5632591843605042, 'motion_component_ionic': -2.801898717880249, 'motion_component_percent_ionic': 56.325918436050415}], 'glu_contributions': [{'resid': 426, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 5.7110724449157715, 'force': [-7.096174240112305, 1.391594648361206, -3.8622512817382812], 'magnitude': 8.19812297821045, 'cosine_with_motion': 0.6546779870986938, 'motion_component': 5.367130756378174, 'motion_component_percent': 65.46779870986938}, {'resid': 426, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 4.712672710418701, 'force': [11.320967674255371, -1.4821666479110718, 4.410941123962402], 'magnitude': 12.239996910095215, 'cosine_with_motion': -0.7499680519104004, 'motion_component': -9.179606437683105, 'motion_component_percent': 74.99680519104004}], 'asn_contributions': [{'resid': 458, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 5.769043445587158, 'force': [2.603990077972412, -4.500880718231201, -2.983947515487671], 'magnitude': 5.995217800140381, 'cosine_with_motion': -0.37976986169815063, 'motion_component': -2.2768030166625977, 'motion_component_percent': 37.97698616981506}, {'resid': 786, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 5.948239326477051, 'force': [4.54271125793457, -4.605401992797852, 1.7901057004928589], 'magnitude': 6.71196174621582, 'cosine_with_motion': -0.42083171010017395, 'motion_component': -2.824606418609619, 'motion_component_percent': 42.083171010017395}, {'resid': 786, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 4.604506492614746, 'force': [-9.891304969787598, 9.445505142211914, -3.9105138778686523], 'magnitude': 14.224893569946289, 'cosine_with_motion': 0.4408385753631592, 'motion_component': 6.270881652832031, 'motion_component_percent': 44.08385753631592}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 4.102363586425781, 'force': [5.15669059753418, -6.288483619689941, 0.942524254322052], 'magnitude': 8.186869621276855, 'cosine_with_motion': -0.39904630184173584, 'motion_component': -3.266940116882324, 'motion_component_percent': 39.904630184173584}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 4.274384498596191, 'force': [5.349549770355225, -4.083357334136963, 3.4026217460632324], 'magnitude': 7.541175365447998, 'cosine_with_motion': -0.43379196524620056, 'motion_component': -3.27130126953125, 'motion_component_percent': 43.379196524620056}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': -0.8926063823477708, 'motion_component_pip2': -19.46761565703945, 'motion_component_percent_pip2': 89.26063823477708}, 713: {'frame': 713, 'motion_vector': [-8.089969635009766, 0.6659736633300781, 3.9828720092773438], 'ionic_force': [-4.70893632620573, -0.5403179824352264, -25.043581306934357], 'ionic_force_magnitude': 25.488173522703324, 'radial_force': 4.739833841644957, 'axial_force': -25.043581306934357, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-3.3072566986083984, 0.08558881282806396, 0.14399833977222443], 'asn_force_magnitude': 3.311496313938549, 'residue_force': [-3.3072566986083984, 0.08558881282806396, 0.14399833977222443], 'residue_force_magnitude': 3.311496313938549, 'total_force': [-8.016193024814129, -0.4547291696071625, -24.899582967162132], 'total_force_magnitude': 26.162097797526883, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': 0.9146414266807238, 'cosine_residue_motion': 0.9146414266807238, 'cosine_ionic_motion': -0.2690716349241095, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': 3.0288317130287123, 'motion_component_residue': 3.0288317130287123, 'motion_component_ionic': -6.858144520983183, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 91.46414266807238, 'motion_component_percent_residue': 91.46414266807238, 'motion_component_percent_ionic': 26.90716349241095, 'ionic_contributions': [{'ion_id': 2333, 'distance': 14.769694328308105, 'force': [0.12457332760095596, -0.2599804103374481, -1.4943784475326538], 'magnitude': 1.5219314098358154, 'cosine_ionic_motion': -0.5183374881744385, 'motion_component_ionic': -0.788874089717865, 'motion_component_percent_ionic': 51.83374881744385}, {'ion_id': 2391, 'distance': 8.746967315673828, 'force': [0.5294503569602966, -1.1319589614868164, -4.15549898147583], 'magnitude': 4.339334011077881, 'cosine_ionic_motion': -0.5502144694328308, 'motion_component_ionic': -2.3875644207000732, 'motion_component_percent_ionic': 55.02144694328308}, {'ion_id': 2397, 'distance': 4.105687618255615, 'force': [-5.648669242858887, 3.1414291858673096, -18.60471534729004], 'magnitude': 19.69546890258789, 'cosine_ionic_motion': -0.14774323999881744, 'motion_component_ionic': -2.90987229347229, 'motion_component_percent_ionic': 14.774323999881744}, {'ion_id': 2520, 'distance': 11.667777061462402, 'force': [0.2857092320919037, -2.2898077964782715, -0.7889885306358337], 'magnitude': 2.4387195110321045, 'cosine_ionic_motion': -0.31649112701416016, 'motion_component_ionic': -0.771833062171936, 'motion_component_percent_ionic': 31.649112701416016}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 5.9359283447265625, 'force': [-8.473396301269531, -1.1594915390014648, 0.34444698691368103], 'magnitude': 8.559293746948242, 'cosine_with_motion': 0.8934983015060425, 'motion_component': 7.647714614868164, 'motion_component_percent': 89.34983015060425}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 5.090090751647949, 'force': [5.166139602661133, 1.2450803518295288, -0.2004486471414566], 'magnitude': 5.317838191986084, 'cosine_with_motion': -0.8685640692710876, 'motion_component': -4.61888313293457, 'motion_component_percent': 86.85640692710876}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': -0.14636872156010586, 'motion_component_pip2': -3.829312807954471, 'motion_component_percent_pip2': 14.636872156010586}, 714: {'frame': 714, 'motion_vector': [5.6610260009765625, 0.8312492370605469, 1.1868896484375], 'ionic_force': [-9.038275361061096, -3.6551905646920204, -4.149604534730315], 'ionic_force_magnitude': 10.595756573328403, 'radial_force': 9.749402010717256, 'axial_force': -4.149604534730315, 'glu_force': [-8.38670825958252, -3.640471935272217, 2.6357030868530273], 'glu_force_magnitude': 9.51508497623121, 'asn_force': [0.0, 0.0, 0.0], 'asn_force_magnitude': 0.0, 'residue_force': [-8.38670825958252, -3.640471935272217, 2.6357030868530273], 'residue_force_magnitude': 9.51508497623121, 'total_force': [-17.424983620643616, -7.295662499964237, -1.5139014478772879], 'total_force_magnitude': 18.95121745659016, 'cosine_total_motion': 0, 'cosine_glu_motion': -0.8520459233505032, 'cosine_asn_motion': 0, 'cosine_residue_motion': -0.8520459233505032, 'cosine_ionic_motion': -0.95498370105965, 'motion_component_total': 0, 'motion_component_glu': -8.107289364331422, 'motion_component_asn': 0, 'motion_component_residue': -8.107289364331422, 'motion_component_ionic': -10.118774827924273, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 85.20459233505032, 'motion_component_percent_asn': 0, 'motion_component_percent_residue': 85.20459233505032, 'motion_component_percent_ionic': 95.49837010596501, 'ionic_contributions': [{'ion_id': 2333, 'distance': 12.729681015014648, 'force': [-1.093157410621643, -0.28498053550720215, -1.7092225551605225], 'magnitude': 2.048816442489624, 'cosine_ionic_motion': -0.7061232924461365, 'motion_component_ionic': -1.4467170238494873, 'motion_component_percent_ionic': 70.61232924461365}, {'ion_id': 2391, 'distance': 8.473782539367676, 'force': [-3.773362874984741, -1.1170190572738647, -2.427342414855957], 'magnitude': 4.623633861541748, 'cosine_ionic_motion': -0.9316113591194153, 'motion_component_ionic': -4.307429790496826, 'motion_component_percent_ionic': 93.16113591194153}, {'ion_id': 2397, 'distance': 11.313549041748047, 'force': [-2.593719244003296, 0.022573016583919525, -0.005453906487673521], 'magnitude': 2.593823194503784, 'cosine_ionic_motion': -0.9679177403450012, 'motion_component_ionic': -2.5106074810028076, 'motion_component_percent_ionic': 96.79177403450012}, {'ion_id': 2520, 'distance': 10.949122428894043, 'force': [-1.578035831451416, -2.275763988494873, -0.007585658226162195], 'magnitude': 2.769360303878784, 'cosine_ionic_motion': -0.6694760918617249, 'motion_component_ionic': -1.8540204763412476, 'motion_component_percent_ionic': 66.94760918617249}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 5.607813835144043, 'force': [7.338040828704834, 2.280733346939087, -3.639946699142456], 'magnitude': 8.502811431884766, 'cosine_with_motion': 0.7872663140296936, 'motion_component': 6.693976879119873, 'motion_component_percent': 78.72663140296936}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 5.179501056671143, 'force': [-9.59361457824707, -2.3317854404449463, 2.281223773956299], 'magnitude': 10.133047103881836, 'cosine_with_motion': -0.9042035341262817, 'motion_component': -9.162337303161621, 'motion_component_percent': 90.42035341262817}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 5.77519416809082, 'force': [-6.131134510040283, -3.5894198417663574, 3.9944260120391846], 'magnitude': 8.150471687316895, 'cosine_with_motion': -0.6918529868125916, 'motion_component': -5.638928413391113, 'motion_component_percent': 69.18529868125916}], 'asn_contributions': [], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': -0.9617357952862124, 'motion_component_pip2': -18.22606419225569, 'motion_component_percent_pip2': 96.17357952862125}, 716: {'frame': 716, 'motion_vector': [3.1058502197265625, -0.7333259582519531, 1.9380264282226562], 'ionic_force': [-2.2645527720451355, -0.8714849054813385, 0.5113887786865234], 'ionic_force_magnitude': 2.4797587948882485, 'radial_force': 2.4264552742342325, 'axial_force': 0.5113887786865234, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [0.0, 0.0, 0.0], 'asn_force_magnitude': 0.0, 'residue_force': [0.0, 0.0, 0.0], 'residue_force_magnitude': 0.0, 'total_force': [-2.2645527720451355, -0.8714849054813385, 0.5113887786865234], 'total_force_magnitude': 2.4797587948882485, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': 0, 'cosine_residue_motion': 0, 'cosine_ionic_motion': -0.5835921567666872, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': 0, 'motion_component_residue': 0, 'motion_component_ionic': -1.447167783369994, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 0, 'motion_component_percent_residue': 0, 'motion_component_percent_ionic': 58.35921567666872, 'ionic_contributions': [{'ion_id': 2276, 'distance': 10.230752944946289, 'force': [-1.6533632278442383, -1.300869345664978, 2.3738651275634766], 'magnitude': 3.1719248294830322, 'cosine_ionic_motion': 0.035420335829257965, 'motion_component_ionic': 0.11235064268112183, 'motion_component_percent_ionic': 3.5420335829257965}, {'ion_id': 2397, 'distance': 12.862654685974121, 'force': [-0.6111895442008972, 0.4293844401836395, -1.8624763488769531], 'magnitude': 2.006674289703369, 'cosine_ionic_motion': -0.7771656513214111, 'motion_component_ionic': -1.5595183372497559, 'motion_component_percent_ionic': 77.71656513214111}], 'glu_contributions': [], 'asn_contributions': [], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': -0.5835921567666872, 'motion_component_pip2': -1.447167783369994, 'motion_component_percent_pip2': 58.35921567666872}, 717: {'frame': 717, 'motion_vector': [-8.451229095458984, -4.797367095947266, 10.97705078125], 'ionic_force': [0.23044559732079506, 0.6678301393985748, 0.8032693862915039], 'ionic_force_magnitude': 1.0697401438512006, 'radial_force': 0.7064717039016197, 'axial_force': 0.8032693862915039, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-1.8471208810806274, -4.467878341674805, 3.7691712379455566], 'asn_force_m</t>
+          <t>{706: {'frame': 706, 'motion_vector': [-1.6462364196777344, 4.194007873535156, 1.78082275390625], 'ionic_force': [-2.4678491204977036, -11.519292116165161, -0.8560818731784821], 'ionic_force_magnitude': 11.811741883086968, 'radial_force': 11.780677830205107, 'axial_force': -0.8560818731784821, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-5.030915379524231, -3.7795519828796387, -7.650073170661926], 'asn_force_magnitude': 9.905490511009754, 'residue_force': [-5.030915379524231, -3.7795519828796387, -7.650073170661926], 'residue_force_magnitude': 9.905490511009754, 'pip2_force': [0.7980182208120823, 0.1757741943001747, -4.670473291504095], 'pip2_force_magnitude': 4.741418607841228, 'total_force': [-6.700746279209852, -15.123069904744625, -13.176628335344503], 'total_force_magnitude': 21.147831527840886, 'cosine_total_motion': -0.7404281186684233, 'cosine_glu_motion': 0, 'cosine_asn_motion': -0.4416169984765415, 'cosine_residue_motion': -0.4416169984765415, 'cosine_pip2_motion': -0.3871798555103845, 'cosine_ionic_motion': -0.7999018642793536, 'motion_component_total': -15.658449112075996, 'motion_component_glu': 0, 'motion_component_asn': -4.374432987909991, 'motion_component_residue': -4.374432987909991, 'motion_component_ionic': -9.44823435266779, 'motion_component_pip2': -1.835781771498215, 'motion_component_percent_total': 74.04281186684233, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 44.16169984765415, 'motion_component_percent_residue': 44.16169984765415, 'motion_component_percent_ionic': 79.99018642793536, 'motion_component_percent_pip2': 38.717985551038446, 'ionic_contributions': [{'ion_id': 2276, 'distance': 7.746928691864014, 'force': [0.08160331845283508, -4.599984169006348, 3.07181715965271], 'magnitude': 5.531959533691406, 'cosine_ionic_motion': -0.5207458138465881, 'motion_component_ionic': -2.880744695663452, 'motion_component_percent_ionic': 52.07458138465881}, {'ion_id': 2391, 'distance': 10.210418701171875, 'force': [0.22415855526924133, -2.0812742710113525, -2.39990496635437], 'magnitude': 3.1845712661743164, 'cosine_ionic_motion': -0.8666999936103821, 'motion_component_ionic': -2.760067939758301, 'motion_component_percent_ionic': 86.66999936103821}, {'ion_id': 2397, 'distance': 8.644484519958496, 'force': [-3.0071139335632324, -3.044539213180542, -1.1944888830184937], 'magnitude': 4.442831993103027, 'cosine_ionic_motion': -0.4620648920536041, 'motion_component_ionic': -2.0528767108917236, 'motion_component_percent_ionic': 46.20648920536041}, {'ion_id': 2520, 'distance': 13.435805320739746, 'force': [0.23350293934345245, -1.793494462966919, -0.33350518345832825], 'magnitude': 1.8391225337982178, 'cosine_ionic_motion': -0.9540119171142578, 'motion_component_ionic': -1.7545448541641235, 'motion_component_percent_ionic': 95.40119171142578}], 'glu_contributions': [], 'asn_contributions': [{'resid': 1114, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 3.432359457015991, 'force': [-7.456222057342529, 15.6506929397583, 10.285576820373535], 'magnitude': 20.157691955566406, 'cosine_with_motion': 0.9853840470314026, 'motion_component': 19.863067626953125, 'motion_component_percent': 98.53840470314026}, {'resid': 1114, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 2.944586992263794, 'force': [0.87669837474823, -18.019702911376953, -14.28624439239502], 'magnitude': 23.01249885559082, 'cosine_with_motion': -0.9190108180046082, 'motion_component': -21.14873504638672, 'motion_component_percent': 91.90108180046082}, {'resid': 1114, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 3.606640577316284, 'force': [11.241238594055176, -19.941492080688477, -3.6771652698516846], 'magnitude': 23.18512725830078, 'cosine_with_motion': -0.9676286578178406, 'motion_component': -22.434593200683594, 'motion_component_percent': 96.76286578178406}, {'resid': 1114, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 3.16558575630188, 'force': [-4.855937957763672, 12.832906723022461, -0.8816777467727661], 'magnitude': 13.749217987060547, 'cosine_with_motion': 0.9044355750083923, 'motion_component': 12.435281753540039, 'motion_component_percent': 90.44355750083923}, {'resid': 1114, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 4.277791500091553, 'force': [-4.8366923332214355, 5.698043346405029, 0.9094374179840088], 'magnitude': 7.529167652130127, 'cosine_with_motion': 0.9178365468978882, 'motion_component': 6.910545349121094, 'motion_component_percent': 91.78365468978882}], 'pip2_contributions': [{'resid': 1313, 'atom': 'C1', 'charge': 0.06000000238418579, 'distance': 30.871591567993164, 'force': [-0.012777435593307018, -0.013791536912322044, 0.009131867438554764], 'magnitude': 0.020901205018162727, 'cosine_with_motion': -0.20289234817028046, 'motion_component': -0.004240694455802441, 'motion_component_percent': 20.289234817028046}, {'resid': 1313, 'atom': 'C11', 'charge': 0.17000000178813934, 'distance': 29.140981674194336, 'force': [-0.04518341273069382, -0.0424593985080719, 0.02393662929534912], 'magnitude': 0.06646279990673065, 'cosine_with_motion': -0.18964910507202148, 'motion_component': -0.012604610994458199, 'motion_component_percent': 18.96491050720215}, {'resid': 1313, 'atom': 'C12', 'charge': 0.04000000283122063, 'distance': 29.30089569091797, 'force': [-0.010950606316328049, -0.009779006242752075, 0.0048699751496315], 'magnitude': 0.015468076802790165, 'cosine_with_motion': -0.19100242853164673, 'motion_component': -0.00295444019138813, 'motion_component_percent': 19.100242853164673}, {'resid': 1313, 'atom': 'C13', 'charge': -0.05000000074505806, 'distance': 30.720081329345703, 'force': [0.012458797544240952, 0.011285570450127125, -0.00517869321629405], 'magnitude': 0.017589900642633438, 'cosine_with_motion': 0.20652152597904205, 'motion_component': 0.003632693085819483, 'motion_component_percent': 20.652152597904205}, {'resid': 1313, 'atom': 'C2', 'charge': 0.06000000238418579, 'distance': 32.439369201660156, 'force': [-0.011616370640695095, -0.012433290481567383, 0.008295061066746712], 'magnitude': 0.01892973482608795, 'cosine_with_motion': -0.19899912178516388, 'motion_component': -0.0037670007441192865, 'motion_component_percent': 19.899912178516388}, {'resid': 1313, 'atom': 'C21', 'charge': 0.6299999952316284, 'distance': 26.897424697875977, 'force': [-0.20379726588726044, -0.18704572319984436, 0.08404095470905304], 'magnitude': 0.2891060709953308, 'cosine_with_motion': -0.21369686722755432, 'motion_component': -0.061781059950590134, 'motion_component_percent': 21.369686722755432}, {'resid': 1313, 'atom': 'C210', 'charge': -0.18000000715255737, 'distance': 26.280900955200195, 'force': [0.06060691922903061, 0.061420634388923645, 0.006362891755998135], 'magnitude': 0.08652271330356598, 'cosine_with_motion': 0.4035446047782898, 'motion_component': 0.034915775060653687, 'motion_component_percent': 40.35446047782898}, {'resid': 1313, 'atom': 'C211', 'charge': -0.15000000596046448, 'distance': 26.54500961303711, 'force': [0.04955738037824631, 0.049580954015254974, 0.00898327399045229], 'magnitude': 0.07067463546991348, 'cosine_with_motion': 0.4157664477825165, 'motion_component': 0.02938414178788662, 'motion_component_percent': 41.57664477825165}, {'resid': 1313, 'atom': 'C212', 'charge': -0.15000000596046448, 'distance': 27.366361618041992, 'force': [0.045162416994571686, 0.04772859066724777, 0.01020051259547472], 'magnitude': 0.06649596244096756, 'cosine_with_motion': 0.4469657242298126, 'motion_component': 0.029721416532993317, 'motion_component_percent': 44.69657242298126}, {'resid': 1313, 'atom': 'C213', 'charge': -0.18000000715255737, 'distance': 28.250181198120117, 'force': [0.04855861887335777, 0.05609775707125664, 0.010108225978910923], 'magnitude': 0.07488039880990982, 'cosine_with_motion': 0.47780942916870117, 'motion_component': 0.03577855974435806, 'motion_component_percent': 47.78094291687012}, {'resid': 1313, 'atom': 'C214', 'charge': -0.15000000596046448, 'distance': 29.025863647460938, 'force': [0.03708170726895332, 0.04481186717748642, 0.01052639540284872], 'magnitude': 0.05910973995923996, 'cosine_with_motion': 0.5085805654525757, 'motion_component': 0.03006206452846527, 'motion_component_percent': 50.85805654525757}, {'resid': 1313, 'atom': 'C215', 'charge': -0.15000000596046448, 'distance': 30.319215774536133, 'force': [0.033522699028253555, 0.041435789316892624, 0.009703636169433594], 'magnitude': 0.05417431518435478, 'cosine_with_motion': 0.5177057385444641, 'motion_component': 0.02804635278880596, 'motion_component_percent': 51.77057385444641}, {'resid': 1313, 'atom': 'C216', 'charge': -0.18000000715255737, 'distance': 31.41595458984375, 'force': [0.03806298226118088, 0.04622479900717735, 0.00898392777889967], 'magnitude': 0.060549430549144745, 'cosine_with_motion': 0.5018181800842285, 'motion_component': 0.03038480505347252, 'motion_component_percent': 50.18181800842285}, {'resid': 1313, 'atom': 'C217', 'charge': -0.18000000715255737, 'distance': 32.33197021484375, 'force': [0.037526801228523254, 0.04216400161385536, 0.0090562142431736], 'magnitude': 0.057167112827301025, 'cosine_with_motion': 0.47366711497306824, 'motion_component': 0.027078181505203247, 'motion_component_percent': 47.366711497306824}, {'resid': 1313, 'atom': 'C218', 'charge': -0.18000000715255737, 'distance': 33.42985153198242, 'force': [0.03576917573809624, 0.039154283702373505, 0.0068530552089214325], 'magnitude': 0.053473882377147675, 'cosine_with_motion': 0.4536813199520111, 'motion_component': 0.024260101839900017, 'motion_component_percent': 45.36813199520111}, {'resid': 1313, 'atom': 'C219', 'charge': -0.18000000715255737, 'distance': 34.67770767211914, 'force': [0.03219810500741005, 0.037287984043359756, 0.0065152691677212715], 'magnitude': 0.04969467222690582, 'cosine_with_motion': 0.47759154438972473, 'motion_component': 0.023733755573630333, 'motion_component_percent': 47.75915443897247}, {'resid': 1313, 'atom': 'C22', 'charge': -0.08000000566244125, 'distance': 26.081235885620117, 'force': [0.02697880193591118, 0.026440219953656197, -0.00988005381077528], 'magnitude': 0.03904556855559349, 'cosine_with_motion': 0.25841253995895386, 'motion_component': 0.010089864954352379, 'motion_component_percent': 25.841253995895386}, {'resid': 1313, 'atom': 'C220', 'charge': -0.27000001072883606, 'distance': 35.90643310546875, 'force': [0.046037644147872925, 0.051552895456552505, 0.007544830907136202], 'magnitude': 0.06952761858701706, 'cosine_with_motion': 0.4567752480506897, 'motion_component': 0.031758494675159454, 'motion_component_percent': 45.67752480506897}, {'resid': 1313, 'atom': 'C23', 'charge': -0.18000000715255737, 'distance': 25.583881378173828, 'force': [0.06574978679418564, 0.06047460064291954, -0.01886121928691864], 'magnitude': 0.09130146354436874, 'cosine_with_motion': 0.252759724855423, 'motion_component': 0.023077331483364105, 'motion_component_percent': 25.275972485542297}, {'resid': 1313, 'atom': 'C24', 'charge': -0.18000000715255737, 'distance': 24.669618606567383, 'force': [0.0690130665898323, 0.06791236251592636, -0.01634638011455536], 'magnitude': 0.0981941744685173, 'cosine_with_motion': 0.2987108826637268, 'motion_component': 0.029331667348742485, 'motion_component_percent': 29.87108826637268}, {'resid': 1313, 'atom': 'C25', 'charge': -0.15000000596046448, 'distance': 24.13797950744629, 'force': [0.06257786601781845, 0.05729309096932411, -0.010348780080676079], 'magnitude': 0.0854727104306221, 'cosine_with_motion': 0.28699183464050293, 'motion_component': 0.024529971182346344, 'motion_component_percent': 28.699183464050293}, {'resid': 1313, 'atom': 'C26', 'charge': -0.15000000596046448, 'distance': 24.40784454345703, 'force': [0.06148529425263405, 0.05635734274983406, -0.005587219260632992], 'magnitude': 0.08359311521053314, 'cosine_with_motion': 0.309133380651474, 'motion_component': 0.025841422379016876, 'motion_component_percent': 30.9133380651474}, {'resid': 1313, 'atom': 'C27', 'charge': -0.18000000715255737, 'distance': 25.61045265197754, 'force': [0.06526360660791397, 0.06343422085046768, -0.004263507667928934], 'magnitude': 0.09111210703849792, 'cosine_with_motion': 0.3421114981174469, 'motion_component': 0.031170500442385674, 'motion_component_percent': 34.21114981174469}, {'resid': 1313, 'atom': 'C28', 'charge': -0.15000000596046448, 'distance': 26.32105255126953, 'force': [0.05319497361779213, 0.0483437106013298, -0.0005160813452675939], 'magnitude': 0.07188244163990021, 'cosine_with_motion': 0.3281082808971405, 'motion_component': 0.023585224524140358, 'motion_component_percent': 32.81082808971405}, {'resid': 1313, 'atom': 'C29', 'charge': -0.15000000596046448, 'distance': 26.616243362426758, 'force': [0.051523543894290924, 0.04773855209350586, 0.0028287440072745085], 'magnitude': 0.07029684633016586, 'cosine_with_motion': 0.3536260426044464, 'motion_component': 0.02485879510641098, 'motion_component_percent': 35.36260426044464}, {'resid': 1313, 'atom': 'C3', 'charge': 0.06000000238418579, 'distance': 33.056644439697266, 'force': [-0.011219675652682781, -0.011483876965939999, 0.008634214289486408], 'magnitude': 0.018229378387331963, 'cosine_with_motion': -0.16211383044719696, 'motion_component': -0.0029552343767136335, 'motion_component_percent': 16.211383044719696}, {'resid': 1313, 'atom': 'C31', 'charge': 0.6299999952316284, 'distance': 30.87660789489746, 'force': [-0.16680125892162323, -0.13154959678649902, 0.05481423810124397], 'magnitude': 0.219391331076622, 'cosine_with_motion': -0.1688905507326126, 'motion_component': -0.037053123116493225, 'motion_component_percent': 16.88905507326126}, {'resid': 1313, 'atom': 'C310', 'charge': -0.18000000715255737, 'distance': 24.349313735961914, 'force': [0.08501981943845749, 0.054110486060380936, 0.0017981564160436392], 'magnitude': 0.10079458355903625, 'cosine_with_motion': 0.18467263877391815, 'motion_component': 0.01861400157213211, 'motion_component_percent': 18.467263877391815}, {'resid': 1313, 'atom': 'C311', 'charge': -0.18000000715255737, 'distance': 24.591760635375977, 'force': [0.08662640303373337, 0.04753498733043671, 0.0010384190827608109], 'magnitude': 0.09881693869829178, 'cosine_with_motion': 0.12241298705339432, 'motion_component': 0.01209647674113512, 'motion_component_percent': 12.241298705339432}, {'resid': 1313, 'atom': 'C312', 'charge': -0.18000000715255737, 'distance': 25.23893928527832, 'force': [0.08325960487127304, 0.042853180319070816, 0.005704394541680813], 'magnitude': 0.09381416440010071, 'cosine_with_motion': 0.11621542274951935, 'motion_component': 0.010902652516961098, 'motion_component_percent': 11.621542274951935}, {'resid': 1313, 'atom': 'C313', 'charge': -0.18000000715255737, 'distance': 25.5270938873291, 'force': [0.08386556804180145, 0.03678889200091362, 0.004850334022194147], 'magnitude': 0.09170813113451004, 'cosine_with_motion': 0.05597124993801117, 'motion_component': 0.005133018828928471, 'motion_component_percent': 5.597124993801117}, {'resid': 1313, 'atom': 'C314', 'charge': -0.18000000715255737, 'distance': 26.660707473754883, 'force': [0.07745377719402313, 0.032685209065675735, 0.001099324319511652], 'magnitude': 0.08407507836818695, 'cosine_with_motion': 0.02831321768462658, 'motion_component': 0.0023804360534995794, 'motion_component_percent': 2.831321768462658}, {'resid': 1313, 'atom': 'C315', 'charge': -0.18000000715255737, 'distance': 28.008888244628906, 'force': [0.06953367590904236, 0.031072890385985374, 0.0015312492614611983], 'magnitude': 0.07617612183094025, 'cosine_with_motion': 0.050339892506599426, 'motion_component': 0.003834697650745511, 'motion_component_percent': 5.033989250659943}, {'resid': 1313, 'atom': 'C316', 'charge': -0.18000000715255737, 'distance': 29.034423828125, 'force': [0.0651281401515007, 0.027974171563982964, -0.0010699608828872442], 'magnitude': 0.07088986784219742, 'cosine_with_motion': 0.023882387205958366, 'motion_component': 0.001693019294179976, 'motion_component_percent': 2.3882387205958366}, {'resid': 1313, 'atom': 'C317', 'charge': -0.18000000715255737, 'distance': 30.49674415588379, 'force': [0.05889902263879776, 0.02568022347986698, 0.0002715804148465395], 'magnitude': 0.0642545148730278, 'cosine_with_motion': 0.03605911135673523, 'motion_component': 0.0023169605992734432, 'motion_component_percent': 3.605911135673523}, {'resid': 1313, 'atom': 'C318', 'charge': -0.27000001072883606, 'distance': 30.96392059326172, 'force': [0.08709965646266937, 0.033848363906145096, 0.003052136395126581], 'magnitude': 0.09349533915519714, 'cosine_with_motion': 0.008850702084600925, 'motion_component': 0.0008274994324892759, 'motion_component_percent': 0.8850702084600925}, {'resid': 1313, 'atom': 'C32', 'charge': -0.08000000566244125, 'distance': 30.80122184753418, 'force': [0.021788673475384712, 0.01661793701350689, -0.005732379853725433], 'magnitude': 0.027995755895972252, 'cosine_with_motion': 0.17413486540317535, 'motion_component': 0.004875037353485823, 'motion_component_percent': 17.413486540317535}, {'resid': 1313, 'atom': 'C33', 'charge': -0.18000000715255737, 'distance': 29.734411239624023, 'force': [0.05403773859143257, 0.03858604654669762, -0.012635162100195885], 'magnitude': 0.06759147346019745, 'cosine_with_motion': 0.15382103621959686, 'motion_component': 0.010396989993751049, 'motion_component_percent': 15.382103621959686}, {'resid': 1313, 'atom': 'C34', 'charge': -0.18000000715255737, 'distance': 28.275243759155273, 'force': [0.05878765136003494, 0.04379208758473396, -0.01461113803088665], 'magnitude': 0.0747477114200592, 'cosine_with_motion': 0.1680780053138733, 'motion_component': 0.012563446536660194, 'motion_component_percent': 16.80780053138733}, {'resid': 1313, 'atom': 'C35', 'charge': -0.18000000715255737, 'distance': 27.127731323242188, 'force': [0.06528566777706146, 0.046227987855672836, -0.01396546233445406], 'magnitude': 0.08120516687631607, 'cosine_with_motion': 0.1564122587442398, 'motion_component': 0.012701483443379402, 'motion_component_percent': 15.64122587442398}, {'resid': 1313, 'atom': 'C36', 'charge': -0.18000000715255737, 'distance': 27.177398681640625, 'force': [0.06517570465803146, 0.04699496552348137, -0.009476622566580772], 'magnitude': 0.0809086263179779, 'cosine_with_motion': 0.1860472708940506, 'motion_component': 0.015052828937768936, 'motion_component_percent': 18.60472708940506}, {'resid': 1313, 'atom': 'C37', 'charge': -0.18000000715255737, 'distance': 26.01606559753418, 'force': [0.07237086445093155, 0.05005890876054764, -0.007228906266391277], 'magnitude': 0.08829322457313538, 'cosine_with_motion': 0.18219460546970367, 'motion_component': 0.016086548566818237, 'motion_component_percent': 18.219460546970367}, {'resid': 1313, 'atom': 'C38', 'charge': -0.18000000715255737, 'distance': 26.635732650756836, 'force': [0.06961414217948914, 0.047370851039886475, -0.002245035022497177], 'magnitude': 0.08423281461000443, 'cosine_with_motion': 0.19622090458869934, 'motion_component': 0.016528239473700523, 'motion_component_percent': 19.622090458869934}, {'resid': 1313, 'atom': 'C39', 'charge': -0.18000000715255737, 'distance': 25.719600677490234, 'force': [0.0745873749256134, 0.050939761102199554, 0.0018051366787403822], 'magnitude': 0.09034043550491333, 'cosine_with_motion': 0.2149277627468109, 'motion_component': 0.01941666752099991, 'motion_component_percent': 21.49277627468109}, {'resid': 1313, 'atom': 'C4', 'charge': 0.08000000566244125, 'distance': 32.4375, 'force': [-0.014824322424829006, -0.015932179987430573, 0.012790302745997906], 'magnitude': 0.025242557749152184, 'cosine_with_motion': -0.16058272123336792, 'motion_component': -0.004053518641740084, 'motion_component_percent': 16.058272123336792}, {'resid': 1313, 'atom': 'C5', 'charge': 0.08000000566244125, 'distance': 30.889232635498047, 'force': [-0.016304943710565567, -0.017505086958408356, 0.014233367517590523], 'magnitude': 0.027836451306939125, 'cosine_with_motion': -0.15740536153316498, 'motion_component': -0.004381606820970774, 'motion_component_percent': 15.740536153316498}, {'resid': 1313, 'atom': 'C6', 'charge': 0.06000000238418579, 'distance': 30.28729248046875, 'force': [-0.01267993450164795, -0.014297918416559696, 0.010312550701200962], 'magnitude': 0.021715430542826653, 'cosine_with_motion': -0.19701185822486877, 'motion_component': -0.004278197418898344, 'motion_component_percent': 19.701185822486877}, {'resid': 1313, 'atom': 'H1', 'charge': 0.12000000476837158, 'distance': 30.431459426879883, 'force': [-0.027386467903852463, -0.027536364272236824, 0.018506193533539772], 'magnitude': 0.0430203340947628, 'cosine_with_motion': -0.17966970801353455, 'motion_component': -0.007729451172053814, 'motion_component_percent': 17.966970801353455}, {'resid': 1313, 'atom': 'H10R', 'charge': 0.09000000357627869, 'distance': 27.04370880126953, 'force': [-0.027875486761331558, -0.02976829558610916, -0.0024411578197032213], 'magnitude': 0.040855273604393005, 'cosine_with_motion': -0.42088332772254944, 'motion_component': -0.01719530299305916, 'motion_component_percent': 42.088332772254944}, {'resid': 1313, 'atom': 'H10S', 'charge': 0.09000000357627869, 'distance': 25.320392608642578, 'force': [-0.03203672915697098, -0.03371163085103035, -0.003045052522793412], 'magnitude': 0.046605776995420456, 'cosine_with_motion': -0.41662198305130005, 'motion_component': -0.019416991621255875, 'motion_component_percent': 41.662198305130005}, {'resid': 1313, 'atom': 'H10X', 'charge': 0.09000000357627869, 'distance': 23.665489196777344, 'force': [-0.04452395811676979, -0.02938535436987877, 0.0007345876656472683], 'magnitude': 0.05335186421871185, 'cosine_with_motion': -0.18817096948623657, 'motion_component': -0.010039271786808968, 'motion_component_percent': 18.817096948623657}, {'resid': 1313, 'atom': 'H10Y', 'charge': 0.09000000357627869, 'distance': 23.94359016418457, 'force': [-0.0437014102935791, -0.02823217771947384, -0.0030977539718151093], 'magnitude': 0.052119720727205276, 'cosine_with_motion': -0.20585644245147705, 'motion_component': -0.01072918064892292, 'motion_component_percent': 20.585644245147705}, {'resid': 1313, 'atom': 'H111', 'charge': 0.15000000596046448, 'distance': 25.904460906982422, 'force': [-0.053369540721178055, -0.05043250694870949, -0.010762450285255909], 'magnitude': 0.07421304285526276, 'cosine_with_motion': -0.39723390340805054, 'motion_component': -0.02947993576526642, 'motion_component_percent': 39.723390340805054}, {'resid': 1313, 'atom': 'H11A', 'charge': 0.09000000357627869, 'distance': 30.00301742553711, 'force': [-0.022577131167054176, -0.020812135189771652, 0.012606541626155376], 'magnitude': 0.03319332376122475, 'cosine_with_motion': -0.17205803096294403, 'motion_component': -0.005711177829653025, 'motion_component_percent': 17.205803096294403}, {'resid': 1313, 'atom': 'H11B', 'charge': 0.09000000357627869, 'distance': 28.334535598754883, 'force': [-0.025550024583935738, -0.023120393976569176, 0.014063918963074684], 'magnitude': 0.037217605859041214, 'cosine_with_motion': -0.1656075417995453, 'motion_component': -0.006163516081869602, 'motion_component_percent': 16.56075417995453}, {'resid': 1313, 'atom': 'H11X', 'charge': 0.09000000357627869, 'distance': 25.35992431640625, 'force': [-0.04087144508957863, -0.022073522210121155, 0.0009331740438938141], 'magnitude': 0.0464605875313282, 'cosine_with_motion': -0.10498421639204025, 'motion_component': -0.004877628292888403, 'motion_component_percent': 10.498421639204025}, {'resid': 1313, 'atom': 'H11Y', 'charge': 0.09000000357627869, 'distance': 23.66026496887207, 'force': [-0.04724038764834404, -0.024843357503414154, 0.000299440958769992], 'magnitude': 0.053375426679849625, 'cosine_with_motion': -0.10012506693601608, 'motion_component': -0.005344218108803034, 'motion_component_percent': 10.012506693601608}, {'resid': 1313, 'atom': 'H12', 'charge': 0.09000000357627869, 'distance': 29.15144920349121, 'force': [-0.025621669366955757, -0.021200941875576973, 0.011416689492762089], 'magnitude': 0.03516092523932457, 'cosine_with_motion': -0.15501846373081207, 'motion_component': -0.005450592376291752, 'motion_component_percent': 15.501846373081207}, {'resid': 1313, 'atom': 'H121', 'charge': 0.15000000596046448, 'distance': 27.540822982788086, 'force': [-0.044464413076639175, -0.04663824290037155, -0.012590569444000721], 'magnitude': 0.06565617024898529, 'cosine_with_motion': -0.4552997648715973, 'motion_component': -0.029893238097429276, 'motion_component_percent': 45.52997648715973}, {'resid': 1313, 'atom': 'H12X', 'charge': 0.09000000357627869, 'distance': 24.60243797302246, 'force': [-0.043623119592666626, -0.022612854838371277, -0.004758533556014299], 'magnitude': 0.049365587532520294, 'cosine_with_motion': -0.1317044198513031, 'motion_component': -0.006501666270196438, 'motion_component_percent': 13.17044198513031}, {'resid': 1313, 'atom': 'H12Y', 'charge': 0.09000000357627869, 'distance': 26.167081832885742, 'force': [-0.03830613195896149, -0.02066091261804104, -0.0031760523561388254], 'magnitude': 0.04363851994276047, 'cosine_with_motion': -0.13833922147750854, 'motion_component': -0.006036918610334396, 'motion_component_percent': 13.833922147750854}, {'resid': 1313, 'atom': 'H13A', 'charge': 0.09000000357627869, 'distance': 31.576297760009766, 'force': [-0.02137819491326809, -0.018820306286215782, 0.00931942742317915], 'magnitude': 0.029968030750751495, 'cosine_with_motion': -0.18695104122161865, 'motion_component': -0.00560255441814661, 'motion_component_percent': 18.695104122161865}, {'resid': 1313, 'atom': 'H13B', 'charge': 0.09000000357627869, 'distance': 31.007465362548828, 'force': [-0.021320922300219536, -0.020738385617733, 0.009008746594190598], 'magnitude': 0.031077641993761063, 'cosine_with_motion': -0.23800644278526306, 'motion_component': -0.007396678905934095, 'motion_component_percent': 23.800644278526306}, {'resid': 1313, 'atom': 'H13R', 'charge': 0.09000000357627869, 'distance': 27.522254943847656, 'force': [-0.02485325001180172, -0.030260080471634865, -0.004764355719089508], 'magnitude': 0.039446871727705, 'cosine_with_motion': -0.4943854510784149, 'motion_component': -0.019501959905028343, 'motion_component_percent': 49.43854510784149}, {'resid': 1313, 'atom': 'H13S', 'charge': 0.09000000357627869, 'distance': 28.93377685546875, 'force': [-0.023425396531820297, -0.026661094278097153, -0.0037884931080043316], 'magnitude': 0.03569195792078972, 'cosine_with_motion': -0.46264851093292236, 'motion_component': -0.016512831673026085, 'motion_component_percent': 46.264851093292236}, {'resid': 1313, 'atom': 'H13X', 'charge': 0.09000000357627869, 'distance': 24.672168731689453, 'force': [-0.045381806790828705, -0.018603293225169182, -0.0019841636531054974], 'magnitude': 0.04908693954348564, 'cosine_with_motion': -0.028790097683668137, 'motion_component': -0.0014132177457213402, 'motion_component_percent': 2.8790097683668137}, {'resid': 1313, 'atom': 'H13Y', 'charge': 0.09000000357627869, 'distance': 25.7319278717041, 'force': [-0.04136393964290619, -0.01754576712846756, -0.004196654073894024], 'magnitude': 0.04512694850564003, 'cosine_with_motion': -0.059305500239133835, 'motion_component': -0.002676276257261634, 'motion_component_percent': 5.9305500239133835}, {'resid': 1313, 'atom': 'H141', 'charge': 0.15000000596046448, 'distance': 28.47825050354004, 'force': [-0.03770130127668381, -0.046759359538555145, -0.012756617739796638], 'magnitude': 0.06140486150979996, 'cosine_with_motion': -0.5269491076469421, 'motion_component': -0.03235723823308945, 'motion_component_percent': 52.694910764694214}, {'resid': 1313, 'atom': 'H14X', 'charge': 0.09000000357627869, 'distance': 26.869997024536133, 'force': [-0.038729406893253326, -0.014563619159162045, -0.0008191490196622908], 'magnitude': 0.0413852259516716, 'cosine_with_motion': 0.006080150604248047, 'motion_component': 0.00025162840029224753, 'motion_component_percent': 0.6080150604248047}, {'resid': 1313, 'atom': 'H14Y', 'charge': 0.09000000357627869, 'distance': 26.35749626159668, 'force': [-0.03947075083851814, -0.017050428315997124, 0.00110778515227139], 'magnitude': 0.04301028326153755, 'cosine_with_motion': -0.021877596154808998, 'motion_component': -0.000940961588639766, 'motion_component_percent': 2.1877596154809}, {'resid': 1313, 'atom': 'H151', 'charge': 0.15000000596046448, 'distance': 30.776256561279297, 'force': [-0.03195129334926605, -0.04027647525072098, -0.011012999340891838], 'magnitude': 0.05257723852992058, 'cosine_with_motion': -0.533653199672699, 'motion_component': -0.028058012947440147, 'motion_component_percent': 53.3653199672699}, {'resid': 1313, 'atom': 'H15X', 'charge': 0.09000000357627869, 'distance': 28.318819046020508, 'force': [-0.03416506201028824, -0.014723613858222961, -0.002047311281785369], 'magnitude': 0.03725893050432205, 'cosine_with_motion': -0.05070723593235016, 'motion_component': -0.0018892973894253373, 'motion_component_percent': 5.070723593235016}, {'resid': 1313, 'atom': 'H15Y', 'charge': 0.09000000357627869, 'distance': 27.89134979248047, 'force': [-0.03442322090268135, -0.01701470836997032, -0.0009224476525560021], 'magnitude': 0.0384097546339035, 'cosine_with_motion': -0.08777648210525513, 'motion_component': -0.003371473168954253, 'motion_component_percent': 8.777648210525513}, {'resid': 1313, 'atom': 'H16R', 'charge': 0.09000000357627869, 'distance': 31.920364379882812, 'force': [-0.01775466836988926, -0.022959193214774132, -0.004198820795863867], 'magnitude': 0.029325464740395546, 'cosine_with_motion': -0.5246595144271851, 'motion_component': -0.015385884791612625, 'motion_component_percent': 52.465951442718506}, {'resid': 1313, 'atom': 'H16S', 'charge': 0.09000000357627869, 'distance': 30.8035945892334, 'force': [-0.02000165358185768, -0.024027565494179726, -0.0037753924261778593], 'magnitude': 0.031490374356508255, 'cosine_with_motion': -0.4887712895870209, 'motion_component': -0.015391591005027294, 'motion_component_percent': 48.87712895870209}, {'resid': 1313, 'atom': 'H16X', 'charge': 0.09000000357627869, 'distance': 29.03134536743164, 'force': [-0.03221026062965393, -0.014725311659276485, 0.001593898981809616], 'magnitude': 0.035452451556921005, 'cosine_with_motion': -0.034315530210733414, 'motion_component': -0.0012165696825832129, 'motion_component_percent': 3.4315530210733414}, {'resid': 1313, 'atom': 'H16Y', 'charge': 0.09000000357627869, 'distance': 28.824186325073242, 'force': [-0.03347402065992355, -0.01309612113982439, 0.0011756662279367447], 'magnitude': 0.03596387803554535, 'cosine_with_motion': 0.013054667972028255, 'motion_component': 0.0004694964736700058, 'motion_component_percent': 1.3054667972028255}, {'resid': 1313, 'atom': 'H17R', 'charge': 0.09000000357627869, 'distance': 31.67473030090332, 'force': [-0.02015385404229164, -0.021416446194052696, -0.004704182036221027], 'magnitude': 0.029782064259052277, 'cosine_with_motion': -0.4506356716156006, 'motion_component': -0.013420860283076763, 'motion_component_percent': 45.06356716156006}, {'resid': 1313, 'atom': 'H17S', 'charge': 0.09000000357627869, 'distance': 32.81387710571289, 'force': [-0.0180695578455925, -0.020403897389769554, -0.005219538230448961], 'magnitude': 0.027750162407755852, 'cosine_with_motion': -0.4843931794166565, 'motion_component': -0.013441989198327065, 'motion_component_percent': 48.43931794166565}, {'resid': 1313, 'atom': 'H17X', 'charge': 0.09000000357627869, 'distance': 31.151042938232422, 'force': [-0.028181837871670723, -0.012384139932692051, 0.0007439682958647609], 'magnitude': 0.03079182468354702, 'cosine_with_motion': -0.028290774673223495, 'motion_component': -0.000871124560944736, 'motion_component_percent': 2.8290774673223495}, {'resid': 1313, 'atom': 'H17Y', 'charge': 0.09000000357627869, 'distance': 30.681467056274414, 'force': [-0.028679896146059036, -0.013585150241851807, -0.0006590737029910088], 'magnitude': 0.03174156695604324, 'cosine_with_motion': -0.07111553102731705, 'motion_component': -0.0022573184687644243, 'motion_component_percent': 7.111553102731705}, {'resid': 1313, 'atom': 'H18R', 'charge': 0.09000000357627869, 'distance': 33.015933990478516, 'force': [-0.018315039575099945, -0.020216915756464005, -0.0026885257102549076], 'magnitude': 0.02741154097020626, 'cosine_with_motion': -0.4474886357784271, 'motion_component': -0.012266352772712708, 'motion_component_percent': 44.74886357784271}, {'resid': 1313, 'atom': 'H18S', 'charge': 0.09000000357627869, 'distance': 33.758949279785156, 'force': [-0.018112797290086746, -0.01863238774240017, -0.0034863357432186604], 'magnitude': 0.026218196377158165, 'cosine_with_motio</t>
         </is>
       </c>
     </row>
@@ -579,7 +579,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>{738: {'frame': 738, 'motion_vector': [3.9510536193847656, 2.28570556640625, 2.43267822265625], 'ionic_force': [-11.174644649028778, -4.503437966108322, -3.206464245915413], 'ionic_force_magnitude': 12.46735936383432, 'radial_force': 12.047972300211075, 'axial_force': -3.206464245915413, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [2.5245158076286316, -0.6213562488555908, -1.643681526184082], 'asn_force_magnitude': 3.075866156138392, 'residue_force': [2.5245158076286316, -0.6213562488555908, -1.643681526184082], 'residue_force_magnitude': 3.075866156138392, 'total_force': [-8.650128841400146, -5.124794214963913, -4.850145772099495], 'total_force_magnitude': 11.16298162361494, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': 0.28635248657478535, 'cosine_residue_motion': 0.28635248657478535, 'cosine_ionic_motion': -0.9652621561538086, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': 0.8807819221814555, 'motion_component_residue': 0.8807819221814555, 'motion_component_ionic': -12.03427018107909, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 28.635248657478535, 'motion_component_percent_residue': 28.635248657478535, 'motion_component_percent_ionic': 96.52621561538086, 'ionic_contributions': [{'ion_id': 2223, 'distance': 9.962797164916992, 'force': [-1.0856294631958008, -3.158844232559204, -0.17628346383571625], 'magnitude': 3.344841480255127, 'cosine_ionic_motion': -0.6900539398193359, 'motion_component_ionic': -2.3081209659576416, 'motion_component_percent_ionic': 69.0053939819336}, {'ion_id': 2247, 'distance': 11.992884635925293, 'force': [-0.6279826760292053, -0.30957135558128357, -2.1995489597320557], 'magnitude': 2.3082921504974365, 'cosine_ionic_motion': -0.71524977684021, 'motion_component_ionic': -1.651005506515503, 'motion_component_percent_ionic': 71.524977684021}, {'ion_id': 2333, 'distance': 9.139810562133789, 'force': [-1.6120256185531616, -0.814048707485199, -3.5403358936309814], 'magnitude': 3.974327564239502, 'cosine_ionic_motion': -0.8193166255950928, 'motion_component_ionic': -3.256232738494873, 'motion_component_percent_ionic': 81.93166255950928}, {'ion_id': 2397, 'distance': 11.327360153198242, 'force': [-2.407813787460327, -0.9421482682228088, -0.0997670590877533], 'magnitude': 2.5875015258789062, 'cosine_ionic_motion': -0.8898726105690002, 'motion_component_ionic': -2.302546739578247, 'motion_component_percent_ionic': 88.98726105690002}, {'ion_id': 2520, 'distance': 7.3378119468688965, 'force': [-5.441193103790283, 0.7211745977401733, 2.8094711303710938], 'magnitude': 6.166019916534424, 'cosine_ionic_motion': -0.40810179710388184, 'motion_component_ionic': -2.5163638591766357, 'motion_component_percent_ionic': 40.810179710388184}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 4.469289779663086, 'force': [2.241318941116333, -2.6649277210235596, 11.367741584777832], 'magnitude': 11.889108657836914, 'cosine_with_motion': 0.4946511685848236, 'motion_component': 5.8809614181518555, 'motion_component_percent': 49.46511685848236}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 4.421173572540283, 'force': [0.7530450820922852, 1.4551115036010742, -10.075578689575195], 'magnitude': 10.207923889160156, 'cosine_with_motion': -0.34488117694854736, 'motion_component': -3.5205206871032715, 'motion_component_percent': 34.488117694854736}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 4.762054920196533, 'force': [-3.0721590518951416, 6.360317707061768, -11.26843547821045], 'magnitude': 13.299227714538574, 'cosine_with_motion': -0.36362212896347046, 'motion_component': -4.835893630981445, 'motion_component_percent': 36.362212896347046}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 5.166462421417236, 'force': [0.39000052213668823, -2.9728293418884277, 4.201687812805176], 'magnitude': 5.161782264709473, 'cosine_with_motion': 0.1860496699810028, 'motion_component': 0.9603478908538818, 'motion_component_percent': 18.60496699810028}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 5.024162292480469, 'force': [2.212310314178467, -2.7990283966064453, 4.130903244018555], 'magnitude': 5.45831823348999, 'cosine_with_motion': 0.43894222378730774, 'motion_component': 2.3958864212036133, 'motion_component_percent': 43.894222378730774}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': -0.9991495672896906, 'motion_component_pip2': -11.153488258897635, 'motion_component_percent_pip2': 99.91495672896906}, 768: {'frame': 768, 'motion_vector': [0.32949066162109375, -3.7513046264648438, -1.385498046875], 'ionic_force': [-23.60068789124489, 1.7340425252914429, -2.384157210588455], 'ionic_force_magnitude': 23.784103473208177, 'radial_force': 23.66430587233592, 'axial_force': -2.384157210588455, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-3.418138027191162, 3.4485554695129395, -3.3776590824127197], 'asn_force_magnitude': 5.914793595404918, 'residue_force': [-3.418138027191162, 3.4485554695129395, -3.3776590824127197], 'residue_force_magnitude': 5.914793595404918, 'total_force': [-27.01882591843605, 5.182597994804382, -5.761816293001175], 'total_force_magnitude': 28.108269298923332, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': -0.3953548244042137, 'cosine_residue_motion': -0.3953548244042137, 'cosine_ionic_motion': -0.11503042079137742, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': -2.338442183298479, 'motion_component_residue': -2.338442183298479, 'motion_component_ionic': -2.7358954306687977, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 39.53548244042137, 'motion_component_percent_residue': 39.53548244042137, 'motion_component_percent_ionic': 11.503042079137742, 'ionic_contributions': [{'ion_id': 2223, 'distance': 10.918511390686035, 'force': [0.16074945032596588, -2.7634966373443604, -0.30491331219673157], 'magnitude': 2.7849104404449463, 'cosine_ionic_motion': 0.9702523946762085, 'motion_component_ionic': 2.702065944671631, 'motion_component_percent_ionic': 97.02523946762085}, {'ion_id': 2247, 'distance': 12.822553634643555, 'force': [-0.2080269306898117, -0.6208621263504028, -1.9101324081420898], 'magnitude': 2.019245147705078, 'cosine_ionic_motion': 0.6056288480758667, 'motion_component_ionic': 1.222913146018982, 'motion_component_percent_ionic': 60.56288480758667}, {'ion_id': 2333, 'distance': 7.588874340057373, 'force': [-1.2244848012924194, -2.7473256587982178, -4.9178876876831055], 'magnitude': 5.7647881507873535, 'cosine_ionic_motion': 0.7226670980453491, 'motion_component_ionic': 4.166022777557373, 'motion_component_percent_ionic': 72.26670980453491}, {'ion_id': 2397, 'distance': 6.5271477699279785, 'force': [-6.801201343536377, 2.8943991661071777, -2.4684383869171143], 'magnitude': 7.792757987976074, 'cosine_ionic_motion': -0.3095325231552124, 'motion_component_ionic': -2.41211199760437, 'motion_component_percent_ionic': 30.95325231552124}, {'ion_id': 2520, 'distance': 4.315112590789795, 'force': [-15.527724266052246, 4.971327781677246, 7.217214584350586], 'magnitude': 17.830101013183594, 'cosine_ionic_motion': -0.471942663192749, 'motion_component_ionic': -8.414785385131836, 'motion_component_percent_ionic': 47.1942663192749}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 5.808132171630859, 'force': [-3.418138027191162, 3.4485554695129395, -3.3776590824127197], 'magnitude': 5.914793491363525, 'cosine_with_motion': -0.39535486698150635, 'motion_component': -2.338442325592041, 'motion_component_percent': 39.535486698150635}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': -0.18052828368773477, 'motion_component_pip2': -5.074337613967277, 'motion_component_percent_pip2': 18.052828368773476}, 769: {'frame': 769, 'motion_vector': [2.8237457275390625, 4.965324401855469, -10.554466247558594], 'ionic_force': [-10.16476695239544, -5.904048919677734, -7.335442766547203], 'ionic_force_magnitude': 13.856009577932168, 'radial_force': 11.755010882277322, 'axial_force': -7.335442766547203, 'glu_force': [8.788960456848145, -3.2592599391937256, 4.735965728759766], 'glu_force_magnitude': 10.502284163326587, 'asn_force': [-0.6070623397827148, -0.7854671478271484, -0.03577423095703125], 'asn_force_magnitude': 0.9933595121096626, 'residue_force': [8.18189811706543, -4.044727087020874, 4.700191497802734], 'residue_force_magnitude': 10.266210309677875, 'total_force': [-1.9828688353300095, -9.948776006698608, -2.6352512687444687], 'total_force_magnitude': 10.481147938036377, 'cosine_total_motion': 0, 'cosine_glu_motion': -0.3280836538041921, 'cosine_asn_motion': -0.4392720808629199, 'cosine_residue_motion': -0.37813202188776135, 'cosine_ionic_motion': 0.11668692473909413, 'motion_component_total': 0, 'motion_component_glu': -3.445627761594089, 'motion_component_asn': -0.43635509992938637, 'motion_component_residue': -3.8819828615234755, 'motion_component_ionic': 1.6168151468043384, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 32.80836538041921, 'motion_component_percent_asn': 43.92720808629199, 'motion_component_percent_residue': 37.81320218877614, 'motion_component_percent_ionic': 11.668692473909413, 'ionic_contributions': [{'ion_id': 2223, 'distance': 14.935005187988281, 'force': [-0.35283273458480835, -1.4374568462371826, -0.15697066485881805], 'magnitude': 1.4884263277053833, 'cosine_ionic_motion': -0.3626006245613098, 'motion_component_ionic': -0.5397043228149414, 'motion_component_percent_ionic': 36.26006245613098}, {'ion_id': 2333, 'distance': 12.371369361877441, 'force': [-0.19737492501735687, -1.3311318159103394, -1.7013593912124634], 'magnitude': 2.1692147254943848, 'cosine_ionic_motion': 0.41448086500167847, 'motion_component_ionic': 0.8990979790687561, 'motion_component_percent_ionic': 41.44808650016785}, {'ion_id': 2397, 'distance': 5.8048248291015625, 'force': [-8.31820297241211, -1.5744802951812744, -5.040463447570801], 'magnitude': 9.852804183959961, 'cosine_ionic_motion': 0.18515226244926453, 'motion_component_ionic': 1.8242689371109009, 'motion_component_percent_ionic': 18.515226244926453}, {'ion_id': 2520, 'distance': 12.647469520568848, 'force': [-1.2963563203811646, -1.560979962348938, -0.43664926290512085], 'magnitude': 2.0755386352539062, 'cosine_ionic_motion': -0.2731085419654846, 'motion_component_ionic': -0.5668473243713379, 'motion_component_percent_ionic': 27.310854196548462}], 'glu_contributions': [{'resid': 1082, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 5.087636470794678, 'force': [8.788960456848145, -3.2592599391937256, 4.735965728759766], 'magnitude': 10.502284049987793, 'cosine_with_motion': -0.32808366417884827, 'motion_component': -3.4456276893615723, 'motion_component_percent': 32.80836641788483}], 'asn_contributions': [{'resid': 1114, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 4.9927592277526855, 'force': [7.810905456542969, 3.1000492572784424, -8.703723907470703], 'magnitude': 12.098567962646484, 'cosine_with_motion': 0.8906069397926331, 'motion_component': 10.775068283081055, 'motion_component_percent': 89.0606939792633}, {'resid': 1114, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 5.352012634277344, 'force': [-2.5579113960266113, -1.9048476219177246, 3.600759983062744], 'magnitude': 4.810075759887695, 'cosine_with_motion': -0.9473254084587097, 'motion_component': -4.55670690536499, 'motion_component_percent': 94.73254084587097}, {'resid': 1114, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 4.150977611541748, 'force': [-5.860056400299072, -1.9806687831878662, 5.067189693450928], 'magnitude': 7.996231555938721, 'cosine_with_motion': -0.8322315812110901, 'motion_component': -6.654716491699219, 'motion_component_percent': 83.22315812110901}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': -0.21611828476333023, 'motion_component_pip2': -2.265167714719137, 'motion_component_percent_pip2': 21.611828476333024}, 770: {'frame': 770, 'motion_vector': [-1.4037933349609375, 1.7553596496582031, 6.1800079345703125], 'ionic_force': [-0.7906530499458313, 0.20309751480817795, -0.7585084438323975], 'ionic_force_magnitude': 1.1143230704221054, 'radial_force': 0.8163215334106428, 'axial_force': -0.7585084438323975, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [0.0, 0.0, 0.0], 'asn_force_magnitude': 0.0, 'residue_force': [0.0, 0.0, 0.0], 'residue_force_magnitude': 0.0, 'total_force': [-0.7906530499458313, 0.20309751480817795, -0.7585084438323975], 'total_force_magnitude': 1.1143230704221054, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': 0, 'cosine_residue_motion': 0, 'cosine_ionic_motion': -0.4395789388318885, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': 0, 'motion_component_residue': 0, 'motion_component_ionic': -0.48983295281204087, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 0, 'motion_component_percent_residue': 0, 'motion_component_percent_ionic': 43.957893883188845, 'ionic_contributions': [{'ion_id': 2276, 'distance': 11.977141380310059, 'force': [-0.21493187546730042, -0.039743341505527496, 2.3040196895599365], 'magnitude': 2.314364433288574, 'cosine_ionic_motion': 0.9508154392242432, 'motion_component_ionic': 2.200533390045166, 'motion_component_percent_ionic': 95.08154392242432}, {'ion_id': 2397, 'distance': 13.644583702087402, 'force': [0.01927432417869568, 0.633677065372467, -1.6667752265930176], 'magnitude': 1.7832716703414917, 'cosine_ionic_motion': -0.7858363389968872, 'motion_component_ionic': -1.4013596773147583, 'motion_component_percent_ionic': 78.58363389968872}, {'ion_id': 2520, 'distance': 14.556623458862305, 'force': [-0.5949954986572266, -0.3908362090587616, -1.3957529067993164], 'magnitude': 1.5668116807937622, 'cosine_ionic_motion': -0.8226940631866455, 'motion_component_ionic': -1.2890067100524902, 'motion_component_percent_ionic': 82.26940631866455}], 'glu_contributions': [], 'asn_contributions': [], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': -0.4395789388318885, 'motion_component_pip2': -0.48983295281204087, 'motion_component_percent_pip2': 43.957893883188845}, 771: {'frame': 771, 'motion_vector': [-0.15446853637695312, 0.04920196533203125, -1.93829345703125], 'ionic_force': [-2.7821125388145447, 1.8229446485638618, -9.475971817970276], 'ionic_force_magnitude': 10.042774480457261, 'radial_force': 3.3261505333277888, 'axial_force': -9.475971817970276, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [0.584580734372139, 1.5186805725097656, 0.48087379336357117], 'asn_force_magnitude': 1.6968691527226043, 'residue_force': [0.584580734372139, 1.5186805725097656, 0.48087379336357117], 'residue_force_magnitude': 1.6968691527226043, 'total_force': [-2.1975318044424057, 3.3416252210736275, -8.995098024606705], 'total_force_magnitude': 9.844155302611531, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': -0.28712244687516464, 'cosine_residue_motion': -0.28712244687516464, 'cosine_ionic_motion': 0.966869952561779, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': -0.48720922315670157, 'motion_component_residue': -0.48720922315670157, 'motion_component_ionic': 9.710056885508356, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 28.712244687516463, 'motion_component_percent_residue': 28.712244687516463, 'motion_component_percent_ionic': 96.6869952561779, 'ionic_contributions': [{'ion_id': 2223, 'distance': 10.496794700622559, 'force': [0.13423487544059753, -0.13063877820968628, -3.007349729537964], 'magnitude': 3.0131773948669434, 'cosine_ionic_motion': 0.9899585843086243, 'motion_component_ionic': 2.9829208850860596, 'motion_component_percent_ionic': 98.99585843086243}, {'ion_id': 2333, 'distance': 14.411660194396973, 'force': [0.06691697239875793, -0.07073979824781418, -1.5955218076705933], 'magnitude': 1.5984904766082764, 'cosine_ionic_motion': 0.9902258515357971, 'motion_component_ionic': 1.5828665494918823, 'motion_component_percent_ionic': 99.02258515357971}, {'ion_id': 2397, 'distance': 9.46849250793457, 'force': [-0.7696501612663269, 2.535881519317627, -2.5866167545318604], 'magnitude': 3.703193426132202, 'cosine_ionic_motion': 0.7298798561096191, 'motion_component_ionic': 2.7028863430023193, 'motion_component_percent_ionic': 72.98798561096191}, {'ion_id': 2520, 'distance': 10.148862838745117, 'force': [-2.2136142253875732, -0.5115582942962646, -2.2864835262298584], 'magnitude': 3.2233192920684814, 'cosine_ionic_motion': 0.757412850856781, 'motion_component_ionic': 2.4413833618164062, 'motion_component_percent_ionic': 75.7412850856781}], 'glu_contributions': [], 'asn_contributions': [{'resid': 786, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 5.8245391845703125, 'force': [-0.4651033580303192, -6.939955711364746, -0.7885791659355164], 'magnitude': 7.000082969665527, 'cosine_with_motion': 0.09245888143777847, 'motion_component': 0.6472198367118835, 'motion_component_percent': 9.245888143777847}, {'resid': 786, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 5.103423595428467, 'force': [-0.06566555798053741, 7.652342319488525, -0.35961154103279114], 'magnitude': 7.661068916320801, 'cosine_with_motion': 0.07272452861070633, 'motion_component': 0.5571476221084595, 'motion_component_percent': 7.272452861070633}, {'resid': 786, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 5.832085609436035, 'force': [2.3529744148254395, 8.34213638305664, 1.8688523769378662], 'magnitude': 8.86681079864502, 'cosine_with_motion': -0.2073114812374115, 'motion_component': -1.8381916284561157, 'motion_component_percent': 20.73114812374115}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 5.104055881500244, 'force': [-2.024237871170044, -4.801938056945801, -0.9027857184410095], 'magnitude': 5.288777828216553, 'cosine_with_motion': 0.1775328516960144, 'motion_component': 0.9389318227767944, 'motion_component_percent': 17.75328516960144}, {'resid': 1114, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 5.895115375518799, 'force': [2.145742893218994, -8.231741905212402, 1.7163045406341553], 'magnitude': 8.678218841552734, 'cosine_with_motion': -0.24071383476257324, 'motion_component': -2.0889673233032227, 'motion_component_percent': 24.071383476257324}, {'resid': 1114, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 4.890626430511475, 'force': [-1.359129786491394, 5.497837543487549, -1.0533066987991333], 'magnitude': 5.76046085357666, 'cosine_with_motion': 0.22509492933750153, 'motion_component': 1.2966505289077759, 'motion_component_percent': 22.509492933750153}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': 0.9368856320160807, 'motion_component_pip2': 9.222847662351656, 'motion_component_percent_pip2': 93.68856320160806}, 772: {'frame': 772, 'motion_vector': [2.30718994140625, 0.9747352600097656, -0.522308349609375], 'ionic_force': [-2.966384883970022, 2.0772838294506073, -8.681533813476562], 'ionic_force_magnitude': 9.406570934324565, 'radial_force': 3.621401301698394, 'axial_force': -8.681533813476562, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-0.13139595091342926, 9.8625967502594, 1.6915274858474731], 'asn_force_magnitude': 10.007464453572702, 'residue_force': [-0.13139595091342926, 9.8625967502594, 1.6915274858474731], 'residue_force_magnitude': 10.007464453572702, 'total_force': [-3.0977808348834515, 11.939880579710007, -6.990006327629089], 'total_force_magnitude': 14.178052857109895, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': 0.3291149385982543, 'cosine_residue_motion': 0.3291149385982543, 'cosine_ionic_motion': -0.011832574229604879, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': 3.2936060491617924, 'motion_component_residue': 3.2936060491617924, 'motion_component_ionic': -0.11130394882643913, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 32.91149385982543, 'motion_component_percent_residue': 32.91149385982543, 'motion_component_percent_ionic': 1.183257422960488, 'ionic_contributions': [{'ion_id': 2223, 'distance': 11.32835578918457, 'force': [0.03655296936631203, -0.24212563037872314, -2.575432538986206], 'magnitude': 2.5870473384857178, 'cosine_ionic_motion': 0.1803131252527237, 'motion_component_ionic': 0.4664785861968994, 'motion_component_percent_ionic': 18.03131252527237}, {'ion_id': 2397, 'distance': 9.995550155639648, 'force': [-0.583853542804718, 2.0637731552124023, -2.5381085872650146], 'magnitude': 3.3229565620422363, 'cosine_ionic_motion': 0.23409545421600342, 'motion_component_ionic': 0.7778890132904053, 'motion_component_percent_ionic': 23.409545421600342}, {'ion_id': 2520, 'distance': 8.768223762512207, 'force': [-2.419084310531616, 0.2556363046169281, -3.567992687225342], 'magnitude': 4.318320274353027, 'cosine_ionic_motion': -0.31393495202064514, 'motion_component_ionic': -1.3556716442108154, 'motion_component_percent_ionic': 31.393495202064514}], 'glu_contributions': [], 'asn_contributions': [{'resid': 786, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 5.2409491539001465, 'force': [0.2274695783853531, 6.346110820770264, 3.5277373790740967], 'magnitude': 7.2642822265625, 'cosine_with_motion': 0.26192137598991394, 'motion_component': 1.9026708602905273, 'motion_component_percent': 26.192137598991394}, {'resid': 1114, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 5.8813276290893555, 'force': [-0.35886552929878235, 3.5164859294891357, -1.8362098932266235], 'magnitude': 3.9832303524017334, 'cosine_with_motion': 0.34919777512550354, 'motion_component': 1.3909351825714111, 'motion_component_percent': 34.919777512550354}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': 0.22445268983036118, 'motion_component_pip2': 3.1823021003353533, 'motion_component_percent_pip2': 22.44526898303612}, 773: {'frame': 773, 'motion_vector': [0.31307220458984375, -5.276435852050781, -5.0860748291015625], 'ionic_force': [0.11038517951965332, 1.9843040220439434, -8.569669246673584], 'ionic_force_magnitude': 8.797094880535298, 'radial_force': 1.9873719681421886, 'axial_force': -8.569669246673584, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [0.0, 0.0, 0.0], 'asn_force_magnitude': 0.0, 'residue_force': [0.0, 0.0, 0.0], 'residue_force_magnitude': 0.0, 'total_force': [0.11038517951965332, 1.9843040220439434, -8.569669246673584], 'total_force_magnitude': 8.797094880535298, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': 0, 'cosine_residue_motion': 0, 'cosine_ionic_motion': 0.5137258817007229, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': 0, 'motion_component_residue': 0, 'motion_component_ionic': 4.519295323907911, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 0, 'motion_component_percent_residue': 0, 'motion_component_percent_ionic': 51.372588170072284, 'ionic_contributions': [{'ion_id': 2223, 'distance': 13.123822212219238, 'force': [0.3449285626411438, 0.056850384920835495, -1.8956377506256104], 'magnitude': 1.9276021718978882, 'cosine_ionic_motion': 0.6682924628257751, 'motion_component_ionic': 1.2882020473480225, 'motion_component_percent_ionic': 66.82924628257751}, {'ion_id': 2397, 'distance': 7.465973377227783, 'force': [-1.124179720878601, 2.875206708908081, -5.093629837036133], 'magnitude': 5.9561448097229, 'cosine_ionic_motion': 0.23766843974590302, 'motion_component_ionic': 1.4155876636505127, 'motion_component_percent_ionic': 23.7668439745903}, {'ion_id': 2520, 'distance': 12.737494468688965, 'force': [0.8896363377571106, -0.9477530717849731, -1.5804016590118408], 'magnitude': 2.0463035106658936, 'cosine_ionic_motion': 0.8872123956680298, 'motion_component_ionic': 1.815505862236023, 'motion_component_percent_ionic': 88.72123956680298}], 'glu_contributions': [], 'asn_contributions': [], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': 0.5137258817007229, 'motion_component_pip2': 4.519295323907911, 'motion_component_percent_pip2': 51.372588170072284}, 774: {'frame': 774, 'motion_vector': [-3.9452056884765625, -1.6306838989257812, 12.473564147949219], 'ionic_force': [1.3721685409545898, -2.9143333435058594, -2.604368209838867], 'ionic_force_magnitude': 4.142332569250662, 'radial_force': 3.2212086771669246, 'axial_force': -2.604368209838867, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [0.0, 0.0, 0.0], 'asn_force_magnitude': 0.0, 'residue_force': [0.0, 0.0, 0.0], 'residue_force_magnitude': 0.0, 'total_force': [1.3721685409545898, -2.9143333435058594, -2.604368209838867], 'total_force_magnitude': 4.142332569250662, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': 0, 'cosine_residue_motion': 0, 'cosine_ionic_motion': -0.6069542231578314, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': 0, 'motion_component_residue': 0, 'motion_component_ionic': -2.51420624663092, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 0, 'motion_component_percent_residue': 0, 'motion_component_percent_ionic': 60.69542231578314, 'ionic_contributions': [{'ion_id': 2520, 'distance': 8.952546119689941, 'force': [1.3721685409545898, -2.9143333435058594, -2.604368209838867], 'magnitude': 4.142332553863525, 'cosine_ionic_motion': -0.6069542169570923, 'motion_component_ionic': -2.5142061710357666, 'motion_component_percent_ionic': 60.69542169570923}], 'glu_contributions': [], 'asn_contributions': [], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': -0.6069542231578314, 'motion_component_pip2': -2.51420624663092, 'motion_component_percent_pip2': 60.69542231578314}, 775: {'frame': 775, 'motion_vector': [-2.761241912841797, 6.140499114990234, -0.33094024658203125], 'ionic_force': [-7.207597993314266, -17.517175793647766, -3.341889262199402], 'ionic_force_magnitude': 19.234581889388465, 'radial_force': 18.942040983452312, 'axial_force': -3.341889262199402, 'glu_force': [7.747500896453857, -4.517882347106934, 2.664550542831421], 'glu_force_magnitude': 9.356006660865361, 'asn_force': [0.0, 0.0, 0.0], 'asn_force_magnitude': 0.0, 'residue_force': [7.747500896453857, -4.517882347106934, 2.664550542831421], 'residue_force_magnitude': 9.356006660865361, 'total_force': [0.5399029031395912, -22.0350581407547, -0.677338719367981], 'total_force_magnitude': 22.052076322922826, 'cosine_total_motion': 0, 'cosine_glu_motion': -0.7930594408991761, 'cosine_asn_motion': 0, 'cosine_residue_motion': -0.7930594408991761, 'cosine_ionic_motion': -0.6675721905042908, 'motion_component_total': 0, 'motion_component_glu': -7.419869411514851, 'motion_component_asn': 0, 'motion_component_residue': -7.419869411514851, 'motion_component_ionic': -12.840471965333219, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 79.30594408991762, 'motion_component_percent_asn': 0, 'motion_component_percent_residue': 79.30594408991762, 'motion_component_percent_ionic': 66.75721905042909, 'ionic_contributions': [{'ion_id': 2223, 'distance': 8.029935836791992, 'force': [-1.1830815076828003, -4.209423542022705, -2.7188563346862793], 'magnitude': 5.1488938331604, 'cosine_ionic_motion': -0.6246773600578308, 'motion_component_ionic': -3.216397523880005, 'motion_component_percent_ionic': 62.46773600578308}, {'ion_id': 2247, 'distance': 14.485517501831055, 'force': [-0.0917544737458229, -0.7223514318466187, -1.404723048210144], 'magnitude': 1.5822317600250244, 'cosine_ionic_motion': -0.3485355079174042, 'motion_component_ionic': -0.5514639616012573, 'motion_component_percent_ionic': 34.85355079174042}, {'ion_id': 2333, 'distance': 11.268780708312988, 'force': [-0.2442062944173813, -1.5186725854873657, -2.1141114234924316], 'magnitude': 2.6144731044769287, 'cosine_ionic_motion': -0.4511743485927582, 'motion_component_ionic': -1.179583191871643, 'motion_component_percent_ionic': 45.11743485927582}, {'ion_id': 2397, 'distance': 6.392716407775879, 'force': [-7.397141456604004, -1.1310182809829712, -3.162538528442383], 'magnitude': 8.12394905090332, 'cosine_ionic_motion': 0.26526978611946106, 'motion_component_ionic': 2.1550381183624268, 'motion_component_percent_ionic': 26.526978611946106}, {'ion_id': 2520, 'distance': 5.31289529800415, 'force': [1.7085857391357422, -9.935709953308105, 6.058340072631836], 'magnitude': 11.761848449707031, 'cosine_ionic_motion': -0.8542930483818054, 'motion_component_ionic': -10.048065185546875, 'motion_component_percent_ionic': 85.42930483818054}], 'glu_contributions': [{'resid': 1082, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 5.390296936035156, 'force': [7.747500896453857, -4.517882347106934, 2.664550542831421], 'magnitude': 9.356006622314453, 'cosine_with_motion': -0.7930594682693481, 'motion_component': -7.419869422912598, 'motion_component_percent': 79.30594682693481}], 'asn_contributions': [], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': -0.9187498301821008, 'motion_component_pip2': -20.26034137684807, 'motion_component_percent_pip2': 91.87498301821007}, 776: {'frame': 776, 'motion_vector': [4.808204650878906, -3.38946533203125, -6.290168762207031], 'ionic_force': [-12.472280144691467, 1.2180619817227125, -10.58296886086464], 'ionic_force_magnitude': 16.402459477438555, 'radial_force': 12.531617892314754, 'axial_force': -10.58296886086464, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-5.985246181488037, -5.623289108276367, -13.442573070526123], 'asn_force_magnitude': 15.752692563644821, 'residue_force': [-5.985246181488037, -5.623289108276367, -13.442573070526123], 'residue_force_magnitude': 15.752692563644821, 'total_force': [-18.457526326179504, -4.405227126553655, -24.025541931390762], 'total_force_magnitude': 30.615567432519512, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': 0.5516215124882619, 'cosine_residue_motion': 0.5516215124882619, 'cosine_ionic_motion': 0.01749061810998675, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': 8.689524097720351, 'motion_component_residue': 8.689524097720351, 'motion_component_ionic': 0.28688915478441057, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 55.162151248826184, 'motion_component_percent_residue': 55.162151248826184, 'motion_component_percent_ionic': 1.7490618109986749, 'ionic_contributions': [{'ion_id': 2223, 'distance': 7.332991123199463, 'force': [-3.5842080116271973, -0.38914725184440613, -5.0121750831604], 'magnitude': 6.174129962921143, 'cosine_ionic_motion': 0.2936169505119324, 'motion_component_ionic': 1.8128292560577393, 'motion_component_percent_ionic': 29.361695051193237}, {'ion_id': 2247, 'distance': 13.691793441772461, 'force': [-0.4495840072631836, -0.022694872692227364, -1.7128291130065918], 'magnitude': 1.7709952592849731, 'cosine_ionic_motion': 0.5696901082992554, 'motion_component_ionic': 1.0089185237884521, 'motion_component_percent_ionic': 56.96901082992554}, {'ion_id': 2333, 'distance': 10.492341041564941, 'force': [-1.0754488706588745, -0.07478311657905579, -2.8164660930633545], 'magnitude': 3.0157361030578613, 'cosine_ionic_motion': 0.49276822805404663, 'motion_component_ionic': 1.4860589504241943, 'motion_component_percent_ionic': 49.27682280540466}, {'ion_id': 2397, 'distance': 10.82083797454834</t>
+          <t>{738: {'frame': 738, 'motion_vector': [3.9510536193847656, 2.28570556640625, 2.43267822265625], 'ionic_force': [-11.174644649028778, -4.503437966108322, -3.206464245915413], 'ionic_force_magnitude': 12.46735936383432, 'radial_force': 12.047972300211075, 'axial_force': -3.206464245915413, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [2.5245158076286316, -0.6213562488555908, -1.643681526184082], 'asn_force_magnitude': 3.075866156138392, 'residue_force': [2.5245158076286316, -0.6213562488555908, -1.643681526184082], 'residue_force_magnitude': 3.075866156138392, 'pip2_force': [0.9488086828496307, 0.10459831222397042, -4.263142808493285], 'pip2_force_magnitude': 4.368702934416458, 'total_force': [-7.701320158550516, -5.0201959027399425, -9.11328858059278], 'total_force_magnitude': 12.944679518610965, 'cosine_total_motion': -0.9569604537744364, 'cosine_glu_motion': 0, 'cosine_asn_motion': 0.28635248657478535, 'cosine_residue_motion': 0.28635248657478535, 'cosine_pip2_motion': -0.28247700649891, 'cosine_ionic_motion': -0.9652621561538086, 'motion_component_total': -12.387546386094602, 'motion_component_glu': 0, 'motion_component_asn': 0.8807819221814555, 'motion_component_residue': 0.8807819221814555, 'motion_component_ionic': -12.03427018107909, 'motion_component_pip2': -1.234058127196965, 'motion_component_percent_total': 95.69604537744364, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 28.635248657478535, 'motion_component_percent_residue': 28.635248657478535, 'motion_component_percent_ionic': 96.52621561538086, 'motion_component_percent_pip2': 28.247700649891, 'ionic_contributions': [{'ion_id': 2223, 'distance': 9.962797164916992, 'force': [-1.0856294631958008, -3.158844232559204, -0.17628346383571625], 'magnitude': 3.344841480255127, 'cosine_ionic_motion': -0.6900539398193359, 'motion_component_ionic': -2.3081209659576416, 'motion_component_percent_ionic': 69.0053939819336}, {'ion_id': 2247, 'distance': 11.992884635925293, 'force': [-0.6279826760292053, -0.30957135558128357, -2.1995489597320557], 'magnitude': 2.3082921504974365, 'cosine_ionic_motion': -0.71524977684021, 'motion_component_ionic': -1.651005506515503, 'motion_component_percent_ionic': 71.524977684021}, {'ion_id': 2333, 'distance': 9.139810562133789, 'force': [-1.6120256185531616, -0.814048707485199, -3.5403358936309814], 'magnitude': 3.974327564239502, 'cosine_ionic_motion': -0.8193166255950928, 'motion_component_ionic': -3.256232738494873, 'motion_component_percent_ionic': 81.93166255950928}, {'ion_id': 2397, 'distance': 11.327360153198242, 'force': [-2.407813787460327, -0.9421482682228088, -0.0997670590877533], 'magnitude': 2.5875015258789062, 'cosine_ionic_motion': -0.8898726105690002, 'motion_component_ionic': -2.302546739578247, 'motion_component_percent_ionic': 88.98726105690002}, {'ion_id': 2520, 'distance': 7.3378119468688965, 'force': [-5.441193103790283, 0.7211745977401733, 2.8094711303710938], 'magnitude': 6.166019916534424, 'cosine_ionic_motion': -0.40810179710388184, 'motion_component_ionic': -2.5163638591766357, 'motion_component_percent_ionic': 40.810179710388184}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 4.469289779663086, 'force': [2.241318941116333, -2.6649277210235596, 11.367741584777832], 'magnitude': 11.889108657836914, 'cosine_with_motion': 0.4946511685848236, 'motion_component': 5.8809614181518555, 'motion_component_percent': 49.46511685848236}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 4.421173572540283, 'force': [0.7530450820922852, 1.4551115036010742, -10.075578689575195], 'magnitude': 10.207923889160156, 'cosine_with_motion': -0.34488117694854736, 'motion_component': -3.5205206871032715, 'motion_component_percent': 34.488117694854736}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 4.762054920196533, 'force': [-3.0721590518951416, 6.360317707061768, -11.26843547821045], 'magnitude': 13.299227714538574, 'cosine_with_motion': -0.36362212896347046, 'motion_component': -4.835893630981445, 'motion_component_percent': 36.362212896347046}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 5.166462421417236, 'force': [0.39000052213668823, -2.9728293418884277, 4.201687812805176], 'magnitude': 5.161782264709473, 'cosine_with_motion': 0.1860496699810028, 'motion_component': 0.9603478908538818, 'motion_component_percent': 18.60496699810028}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 5.024162292480469, 'force': [2.212310314178467, -2.7990283966064453, 4.130903244018555], 'magnitude': 5.45831823348999, 'cosine_with_motion': 0.43894222378730774, 'motion_component': 2.3958864212036133, 'motion_component_percent': 43.894222378730774}], 'pip2_contributions': [{'resid': 1313, 'atom': 'C1', 'charge': 0.06000000238418579, 'distance': 32.2686767578125, 'force': [-0.01364963036030531, -0.009803573600947857, 0.009140831418335438], 'magnitude': 0.019130531698465347, 'cosine_with_motion': -0.546760082244873, 'motion_component': -0.010459811426699162, 'motion_component_percent': 54.676008224487305}, {'resid': 1313, 'atom': 'C11', 'charge': 0.17000000178813934, 'distance': 31.708324432373047, 'force': [-0.043726127594709396, -0.027371281757950783, 0.02213761769235134], 'magnitude': 0.0561358667910099, 'cosine_with_motion': -0.6250062584877014, 'motion_component': -0.03508526831865311, 'motion_component_percent': 62.50062584877014}, {'resid': 1313, 'atom': 'C12', 'charge': 0.04000000283122063, 'distance': 31.4923038482666, 'force': [-0.01079852320253849, -0.006259041838347912, 0.004849284887313843], 'magnitude': 0.01339026726782322, 'cosine_with_motion': -0.6522622108459473, 'motion_component': -0.008733965456485748, 'motion_component_percent': 65.22622108459473}, {'resid': 1313, 'atom': 'C13', 'charge': -0.05000000074505806, 'distance': 32.23837661743164, 'force': [0.012941473163664341, 0.0077748228795826435, -0.005213260184973478], 'magnitude': 0.015972090885043144, 'cosine_with_motion': 0.6805353164672852, 'motion_component': 0.010869571939110756, 'motion_component_percent': 68.05353164672852}, {'resid': 1313, 'atom': 'C2', 'charge': 0.06000000238418579, 'distance': 33.752010345458984, 'force': [-0.012598118744790554, -0.008867230266332626, 0.008271592669188976], 'magnitude': 0.017485983669757843, 'cosine_with_motion': -0.5519636869430542, 'motion_component': -0.009651628322899342, 'motion_component_percent': 55.19636869430542}, {'resid': 1313, 'atom': 'C21', 'charge': 0.6299999952316284, 'distance': 29.167911529541016, 'force': [-0.1990124136209488, -0.11013854295015335, 0.0933014452457428], 'magnitude': 0.24584873020648956, 'cosine_with_motion': -0.6378347873687744, 'motion_component': -0.15681087970733643, 'motion_component_percent': 63.78347873687744}, {'resid': 1313, 'atom': 'C210', 'charge': -0.18000000715255737, 'distance': 27.95619773864746, 'force': [0.0699339285492897, 0.030164159834384918, -0.0067854635417461395], 'magnitude': 0.07646354287862778, 'cosine_with_motion': 0.8312399983406067, 'motion_component': 0.06355955451726913, 'motion_component_percent': 83.12399983406067}, {'resid': 1313, 'atom': 'C211', 'charge': -0.15000000596046448, 'distance': 28.275798797607422, 'force': [0.05808063596487045, 0.022223317995667458, -0.0035317311994731426], 'magnitude': 0.062287312000989914, 'cosine_with_motion': 0.8432897329330444, 'motion_component': 0.05252625048160553, 'motion_component_percent': 84.32897329330444}, {'resid': 1313, 'atom': 'C212', 'charge': -0.15000000596046448, 'distance': 29.489391326904297, 'force': [0.053773317486047745, 0.019484978169202805, -0.0028590140864253044], 'magnitude': 0.05726611614227295, 'cosine_with_motion': 0.8441688418388367, 'motion_component': 0.0483422726392746, 'motion_component_percent': 84.41688418388367}, {'resid': 1313, 'atom': 'C213', 'charge': -0.18000000715255737, 'distance': 30.694034576416016, 'force': [0.059049107134342194, 0.022796213626861572, -0.004128837492316961], 'magnitude': 0.06343115866184235, 'cosine_with_motion': 0.839309573173523, 'motion_component': 0.05323837697505951, 'motion_component_percent': 83.9309573173523}, {'resid': 1313, 'atom': 'C214', 'charge': -0.15000000596046448, 'distance': 31.593738555908203, 'force': [0.046252619475126266, 0.018650026991963387, -0.0014289335813373327], 'magnitude': 0.04989158362150192, 'cosine_with_motion': 0.8598843216896057, 'motion_component': 0.042900990694761276, 'motion_component_percent': 85.98843216896057}, {'resid': 1313, 'atom': 'C215', 'charge': -0.15000000596046448, 'distance': 32.72728729248047, 'force': [0.04342417046427727, 0.016601409763097763, -0.0007421249756589532], 'magnitude': 0.046495337039232254, 'cosine_with_motion': 0.8637019991874695, 'motion_component': 0.040158115327358246, 'motion_component_percent': 86.37019991874695}, {'resid': 1313, 'atom': 'C216', 'charge': -0.18000000715255737, 'distance': 33.514137268066406, 'force': [0.050248220562934875, 0.01738337054848671, -0.0019323515007272363], 'magnitude': 0.053205255419015884, 'cosine_with_motion': 0.8487250804901123, 'motion_component': 0.04515663534402847, 'motion_component_percent': 84.87250804901123}, {'resid': 1313, 'atom': 'C217', 'charge': -0.18000000715255737, 'distance': 35.018436431884766, 'force': [0.04588926583528519, 0.016317788511514664, -0.0016564653487876058], 'magnitude': 0.048732317984104156, 'cosine_with_motion': 0.8512991666793823, 'motion_component': 0.04148578271269798, 'motion_component_percent': 85.12991666793823}, {'resid': 1313, 'atom': 'C218', 'charge': -0.18000000715255737, 'distance': 35.97636032104492, 'force': [0.043636519461870193, 0.01477277185767889, -0.003073844127357006], 'magnitude': 0.04617173597216606, 'cosine_with_motion': 0.8320149183273315, 'motion_component': 0.0384155735373497, 'motion_component_percent': 83.20149183273315}, {'resid': 1313, 'atom': 'C219', 'charge': -0.18000000715255737, 'distance': 37.38211441040039, 'force': [0.040294114500284195, 0.014109121635556221, -0.0024728719145059586], 'magnitude': 0.04276444762945175, 'cosine_with_motion': 0.8383541703224182, 'motion_component': 0.03585175424814224, 'motion_component_percent': 83.83541703224182}, {'resid': 1313, 'atom': 'C22', 'charge': -0.08000000566244125, 'distance': 27.787450790405273, 'force': [0.027696259319782257, 0.015860874205827713, -0.012828042730689049], 'magnitude': 0.034397803246974945, 'cosine_with_motion': 0.6434230804443359, 'motion_component': 0.02213234081864357, 'motion_component_percent': 64.3423080444336}, {'resid': 1313, 'atom': 'C220', 'charge': -0.27000001072883606, 'distance': 38.363162994384766, 'force': [0.05758515000343323, 0.019171815365552902, -0.005114133935421705], 'magnitude': 0.060907818377017975, 'cosine_with_motion': 0.8218162059783936, 'motion_component': 0.05005503073334694, 'motion_component_percent': 82.18162059783936}, {'resid': 1313, 'atom': 'C23', 'charge': -0.18000000715255737, 'distance': 26.80002212524414, 'force': [0.06893736869096756, 0.03637990355491638, -0.029101941734552383], 'magnitude': 0.08320324867963791, 'cosine_with_motion': 0.6616223454475403, 'motion_component': 0.05504912883043289, 'motion_component_percent': 66.16223454475403}, {'resid': 1313, 'atom': 'C24', 'charge': -0.18000000715255737, 'distance': 27.144983291625977, 'force': [0.06869611144065857, 0.035692065954208374, -0.024175425991415977], 'magnitude': 0.08110197633504868, 'cosine_with_motion': 0.7013137936592102, 'motion_component': 0.05687793344259262, 'motion_component_percent': 70.13137936592102}, {'resid': 1313, 'atom': 'C25', 'charge': -0.15000000596046448, 'distance': 26.613140106201172, 'force': [0.06146484240889549, 0.02823011577129364, -0.019211623817682266], 'magnitude': 0.07031324505805969, 'cosine_with_motion': 0.7166672945022583, 'motion_component': 0.05039120465517044, 'motion_component_percent': 71.66672945022583}, {'resid': 1313, 'atom': 'C26', 'charge': -0.15000000596046448, 'distance': 26.34966278076172, 'force': [0.063740573823452, 0.028609002009034157, -0.01622791215777397], 'magnitude': 0.07172643393278122, 'cosine_with_motion': 0.7486826181411743, 'motion_component': 0.05370033532381058, 'motion_component_percent': 74.86826181411743}, {'resid': 1313, 'atom': 'C27', 'charge': -0.18000000715255737, 'distance': 26.667734146118164, 'force': [0.07405754178762436, 0.036603160202503204, -0.015390302985906601], 'magnitude': 0.08403078466653824, 'cosine_with_motion': 0.7795701026916504, 'motion_component': 0.06550788879394531, 'motion_component_percent': 77.95701026916504}, {'resid': 1313, 'atom': 'C28', 'charge': -0.15000000596046448, 'distance': 25.925893783569336, 'force': [0.06626832485198975, 0.031602926552295685, -0.009957410395145416], 'magnitude': 0.0740903913974762, 'cosine_with_motion': 0.8085183501243591, 'motion_component': 0.05990343913435936, 'motion_component_percent': 80.85183501243591}, {'resid': 1313, 'atom': 'C29', 'charge': -0.15000000596046448, 'distance': 26.527738571166992, 'force': [0.0642482191324234, 0.02889658510684967, -0.0067140813916921616], 'magnitude': 0.07076669484376907, 'cosine_with_motion': 0.8293418288230896, 'motion_component': 0.05868978053331375, 'motion_component_percent': 82.93418288230896}, {'resid': 1313, 'atom': 'C3', 'charge': 0.06000000238418579, 'distance': 34.38382339477539, 'force': [-0.01209657359868288, -0.008094634860754013, 0.008488084189593792], 'magnitude': 0.01684926636517048, 'cosine_with_motion': -0.5237777233123779, 'motion_component': -0.0088252704590559, 'motion_component_percent': 52.37777233123779}, {'resid': 1313, 'atom': 'C31', 'charge': 0.6299999952316284, 'distance': 32.3895378112793, 'force': [-0.1699219048023224, -0.08544665575027466, 0.05979568138718605], 'magnitude': 0.19937428832054138, 'cosine_with_motion': -0.6993690729141235, 'motion_component': -0.13943621516227722, 'motion_component_percent': 69.93690729141235}, {'resid': 1313, 'atom': 'C310', 'charge': -0.18000000715255737, 'distance': 27.356794357299805, 'force': [0.0775734931230545, 0.017701594159007072, -0.006721942685544491], 'magnitude': 0.07985097169876099, 'cosine_with_motion': 0.8004640340805054, 'motion_component': 0.06391783058643341, 'motion_component_percent': 80.04640340805054}, {'resid': 1313, 'atom': 'C311', 'charge': -0.18000000715255737, 'distance': 28.505828857421875, 'force': [0.07148876041173935, 0.016906891018152237, -0.003483446314930916], 'magnitude': 0.07354331761598587, 'cosine_with_motion': 0.8218527436256409, 'motion_component': 0.06044177711009979, 'motion_component_percent': 82.18527436256409}, {'resid': 1313, 'atom': 'C312', 'charge': -0.18000000715255737, 'distance': 29.401470184326172, 'force': [0.0678325742483139, 0.013002971187233925, -0.0029585217125713825], 'magnitude': 0.06913094967603683, 'cosine_with_motion': 0.812524676322937, 'motion_component': 0.05617060139775276, 'motion_component_percent': 81.2524676322937}, {'resid': 1313, 'atom': 'C313', 'charge': -0.18000000715255737, 'distance': 28.82352638244629, 'force': [0.07107935100793839, 0.0110196927562356, -0.0006062230095267296], 'magnitude': 0.07193104177713394, 'cosine_with_motion': 0.8185709714889526, 'motion_component': 0.05888066440820694, 'motion_component_percent': 81.85709714889526}, {'resid': 1313, 'atom': 'C314', 'charge': -0.18000000715255737, 'distance': 29.964962005615234, 'force': [0.06605400145053864, 0.008124123327434063, 0.0006967732333578169], 'magnitude': 0.06655537337064743, 'cosine_with_motion': 0.8169911503791809, 'motion_component': 0.05437515303492546, 'motion_component_percent': 81.69911503791809}, {'resid': 1313, 'atom': 'C315', 'charge': -0.18000000715255737, 'distance': 29.642515182495117, 'force': [0.06774254143238068, 0.00547688128426671, 0.0025448030792176723], 'magnitude': 0.06801120936870575, 'cosine_with_motion': 0.81404709815979, 'motion_component': 0.055364325642585754, 'motion_component_percent': 81.404709815979}, {'resid': 1313, 'atom': 'C316', 'charge': -0.18000000715255737, 'distance': 30.878904342651367, 'force': [0.06252384930849075, 0.0031795320101082325, 0.0029460471123456955], 'magnitude': 0.06267391890287399, 'cosine_with_motion': 0.8065774440765381, 'motion_component': 0.05055136978626251, 'motion_component_percent': 80.65774440765381}, {'resid': 1313, 'atom': 'C317', 'charge': -0.18000000715255737, 'distance': 30.502714157104492, 'force': [0.06408151984214783, 0.00040984651423059404, 0.004336261656135321], 'magnitude': 0.06422936916351318, 'cosine_with_motion': 0.7966939210891724, 'motion_component': 0.05117114633321762, 'motion_component_percent': 79.66939210891724}, {'resid': 1313, 'atom': 'C318', 'charge': -0.27000001072883606, 'distance': 31.74228286743164, 'force': [0.08864043653011322, -0.0019382693571969867, 0.007356500253081322], 'magnitude': 0.08896629512310028, 'cosine_with_motion': 0.7903447151184082, 'motion_component': 0.07031404227018356, 'motion_component_percent': 79.03447151184082}, {'resid': 1313, 'atom': 'C32', 'charge': -0.08000000566244125, 'distance': 32.1761589050293, 'force': [0.022390151396393776, 0.010560380294919014, -0.006730622611939907], 'magnitude': 0.025654274970293045, 'cosine_with_motion': 0.7252023220062256, 'motion_component': 0.018604539334774017, 'motion_component_percent': 72.52023220062256}, {'resid': 1313, 'atom': 'C33', 'charge': -0.18000000715255737, 'distance': 30.82987403869629, 'force': [0.05554255470633507, 0.024472098797559738, -0.016407573595643044], 'magnitude': 0.06287342309951782, 'cosine_with_motion': 0.7240802049636841, 'motion_component': 0.04552540183067322, 'motion_component_percent': 72.40802049636841}, {'resid': 1313, 'atom': 'C34', 'charge': -0.18000000715255737, 'distance': 30.933849334716797, 'force': [0.05658202990889549, 0.022046059370040894, -0.014581877738237381], 'magnitude': 0.06245146691799164, 'cosine_with_motion': 0.738269567489624, 'motion_component': 0.046106018126010895, 'motion_component_percent': 73.8269567489624}, {'resid': 1313, 'atom': 'C35', 'charge': -0.18000000715255737, 'distance': 29.520999908447266, 'force': [0.06280490010976791, 0.023132503032684326, -0.014919333159923553], 'magnitude': 0.0685722604393959, 'cosine_with_motion': 0.7463796138763428, 'motion_component': 0.05118093639612198, 'motion_component_percent': 74.63796138763428}, {'resid': 1313, 'atom': 'C36', 'charge': -0.18000000715255737, 'distance': 29.754182815551758, 'force': [0.06309910118579865, 0.020143656060099602, -0.013008170761168003], 'magnitude': 0.06750167161226273, 'cosine_with_motion': 0.7552959322929382, 'motion_component': 0.0509837381541729, 'motion_component_percent': 75.52959322929382}, {'resid': 1313, 'atom': 'C37', 'charge': -0.18000000715255737, 'distance': 28.581026077270508, 'force': [0.06918127089738846, 0.01997888833284378, -0.012911980040371418], 'magnitude': 0.07315684109926224, 'cosine_with_motion': 0.7600412368774414, 'motion_component': 0.055602215230464935, 'motion_component_percent': 76.00412368774414}, {'resid': 1313, 'atom': 'C38', 'charge': -0.18000000715255737, 'distance': 28.965662002563477, 'force': [0.06843627989292145, 0.016106652095913887, -0.011415544897317886], 'magnitude': 0.07122684270143509, 'cosine_with_motion': 0.7585029006004333, 'motion_component': 0.054025765508413315, 'motion_component_percent': 75.85029006004333}, {'resid': 1313, 'atom': 'C39', 'charge': -0.18000000715255737, 'distance': 27.767555236816406, 'force': [0.07517866790294647, 0.015607287175953388, -0.010571679100394249], 'magnitude': 0.07750599831342697, 'cosine_with_motion': 0.765777587890625, 'motion_component': 0.05935235694050789, 'motion_component_percent': 76.5777587890625}, {'resid': 1313, 'atom': 'C4', 'charge': 0.08000000566244125, 'distance': 34.34451675415039, 'force': [-0.015508313663303852, -0.010995155200362206, 0.012067332863807678], 'magnitude': 0.022517144680023193, 'cosine_with_motion': -0.48983967304229736, 'motion_component': -0.011029791086912155, 'motion_component_percent': 48.983967304229736}, {'resid': 1313, 'atom': 'C5', 'charge': 0.08000000566244125, 'distance': 32.831119537353516, 'force': [-0.01671004295349121, -0.012121847830712795, 0.013453979976475239], 'magnitude': 0.02464090660214424, 'cosine_with_motion': -0.47861427068710327, 'motion_component': -0.011793489567935467, 'motion_component_percent': 47.86142706871033}, {'resid': 1313, 'atom': 'C6', 'charge': 0.06000000238418579, 'distance': 32.076236724853516, 'force': [-0.013217628002166748, -0.010062860324978828, 0.009943461045622826], 'magnitude': 0.019360767677426338, 'cosine_with_motion': -0.5096337199211121, 'motion_component': -0.009866899810731411, 'motion_component_percent': 50.963371992111206}, {'resid': 1313, 'atom': 'H1', 'charge': 0.12000000476837158, 'distance': 31.82754135131836, 'force': [-0.028716349974274635, -0.01911492832005024, 0.018888160586357117], 'magnitude': 0.03932902216911316, 'cosine_with_motion': -0.5466534495353699, 'motion_component': -0.02149934507906437, 'motion_component_percent': 54.66534495353699}, {'resid': 1313, 'atom': 'H10R', 'charge': 0.09000000357627869, 'distance': 28.422040939331055, 'force': [-0.03384503722190857, -0.01421846728771925, 0.0045297821052372456], 'magnitude': 0.03698878735303879, 'cosine_with_motion': -0.8112280368804932, 'motion_component': -0.030006341636180878, 'motion_component_percent': 81.12280368804932}, {'resid': 1313, 'atom': 'H10S', 'charge': 0.09000000357627869, 'distance': 28.548137664794922, 'force': [-0.03308939188718796, -0.015518661588430405, 0.002901833737269044], 'magnitude': 0.0366627536714077, 'cosine_with_motion': -0.8392536640167236, 'motion_component': -0.0307693500071764, 'motion_component_percent': 83.92536640167236}, {'resid': 1313, 'atom': 'H10X', 'charge': 0.09000000357627869, 'distance': 26.652446746826172, 'force': [-0.041149552911520004, -0.008231795392930508, 0.0028807285707443953], 'magnitude': 0.042063601315021515, 'cosine_with_motion': -0.8015514612197876, 'motion_component': -0.03371614217758179, 'motion_component_percent': 80.15514612197876}, {'resid': 1313, 'atom': 'H10Y', 'charge': 0.09000000357627869, 'distance': 26.78232192993164, 'force': [-0.04012057185173035, -0.010627595707774162, 0.0035593367647379637], 'magnitude': 0.04165663197636604, 'cosine_with_motion': -0.8082670569419861, 'motion_component': -0.03366968408226967, 'motion_component_percent': 80.82670569419861}, {'resid': 1313, 'atom': 'H111', 'charge': 0.15000000596046448, 'distance': 27.443374633789062, 'force': [-0.062141645699739456, -0.02244311012327671, 0.002647517016157508], 'magnitude': 0.06612326949834824, 'cosine_with_motion': -0.8490410447120667, 'motion_component': -0.05614136904478073, 'motion_component_percent': 84.90410447120667}, {'resid': 1313, 'atom': 'H11A', 'charge': 0.09000000357627869, 'distance': 32.7114372253418, 'force': [-0.02163558453321457, -0.013510347343981266, 0.011363763362169266], 'magnitude': 0.02792423963546753, 'cosine_with_motion': -0.6142577528953552, 'motion_component': -0.017152680084109306, 'motion_component_percent': 61.42577528953552}, {'resid': 1313, 'atom': 'H11B', 'charge': 0.09000000357627869, 'distance': 31.148235321044922, 'force': [-0.02391369268298149, -0.014494625851511955, 0.012904242612421513], 'magnitude': 0.030797375366091728, 'cosine_with_motion': -0.6040552854537964, 'motion_component': -0.018603317439556122, 'motion_component_percent': 60.40552854537964}, {'resid': 1313, 'atom': 'H11X', 'charge': 0.09000000357627869, 'distance': 28.095693588256836, 'force': [-0.03674684837460518, -0.00907130166888237, 0.0004852105339523405], 'magnitude': 0.037853069603443146, 'cosine_with_motion': -0.8414286971092224, 'motion_component': -0.0318506583571434, 'motion_component_percent': 84.14286971092224}, {'resid': 1313, 'atom': 'H11Y', 'charge': 0.09000000357627869, 'distance': 29.04039192199707, 'force': [-0.03416035696864128, -0.009121538139879704, 0.002275618724524975], 'magnitude': 0.035430364310741425, 'cosine_with_motion': -0.8200598359107971, 'motion_component': -0.029055017977952957, 'motion_component_percent': 82.00598359107971}, {'resid': 1313, 'atom': 'H12', 'charge': 0.09000000357627869, 'distance': 31.88133430480957, 'force': [-0.024082589894533157, -0.012893855571746826, 0.010861827060580254], 'magnitude': 0.029397310689091682, 'cosine_with_motion': -0.6458256840705872, 'motion_component': -0.018985537812113762, 'motion_component_percent': 64.58256840705872}, {'resid': 1313, 'atom': 'H121', 'charge': 0.15000000596046448, 'distance': 29.766626358032227, 'force': [-0.0533113069832325, -0.017738981172442436, 0.0014713853597640991], 'magnitude': 0.05620437487959862, 'cosine_with_motion': -0.8517204523086548, 'motion_component': -0.047870416194200516, 'motion_component_percent': 85.17204523086548}, {'resid': 1313, 'atom': 'H12X', 'charge': 0.09000000357627869, 'distance': 30.411907196044922, 'force': [-0.03164880722761154, -0.006399625446647406, 0.0010601987596601248], 'magnitude': 0.03230675309896469, 'cosine_with_motion': -0.8204260468482971, 'motion_component': -0.026505300775170326, 'motion_component_percent': 82.04260468482971}, {'resid': 1313, 'atom': 'H12Y', 'charge': 0.09000000357627869, 'distance': 29.54867935180664, 'force': [-0.033617403358221054, -0.005859051365405321, 0.002584976376965642], 'magnitude': 0.03422192856669426, 'cosine_with_motion': -0.7905179262161255, 'motion_component': -0.027053048834204674, 'motion_component_percent': 79.05179262161255}, {'resid': 1313, 'atom': 'H13A', 'charge': 0.09000000357627869, 'distance': 33.284339904785156, 'force': [-0.02176963910460472, -0.013093952089548111, 0.00905971322208643], 'magnitude': 0.026971230283379555, 'cosine_with_motion': -0.6731143593788147, 'motion_component': -0.018154721707105637, 'motion_component_percent': 67.31143593788147}, {'resid': 1313, 'atom': 'H13B', 'charge': 0.09000000357627869, 'distance': 31.912220001220703, 'force': [-0.023397354409098625, -0.015098423697054386, 0.009244604967534542], 'magnitude': 0.029340438544750214, 'cosine_with_motion': -0.6883652210235596, 'motion_component': -0.020196937024593353, 'motion_component_percent': 68.83652210235596}, {'resid': 1313, 'atom': 'H13R', 'charge': 0.09000000357627869, 'distance': 30.52679443359375, 'force': [-0.029471339657902718, -0.012315167114138603, 0.0028069838881492615], 'magnitude': 0.032064035534858704, 'cosine_with_motion': -0.8306674957275391, 'motion_component': -0.02663455158472061, 'motion_component_percent': 83.0667495727539}, {'resid': 1313, 'atom': 'H13S', 'charge': 0.09000000357627869, 'distance': 31.25628662109375, 'force': [-0.02869509905576706, -0.010275103151798248, 0.0025385813787579536], 'magnitude': 0.03058481402695179, 'cosine_with_motion': -0.8261064291000366, 'motion_component': -0.025266312062740326, 'motion_component_percent': 82.61064291000366}, {'resid': 1313, 'atom': 'H13X', 'charge': 0.09000000357627869, 'distance': 28.0063419342041, 'force': [-0.037741273641586304, -0.005091314669698477, 0.0009500585729256272], 'magnitude': 0.038094982504844666, 'cosine_with_motion': -0.8041179776191711, 'motion_component': -0.030632860958576202, 'motion_component_percent': 80.41179776191711}, {'resid': 1313, 'atom': 'H13Y', 'charge': 0.09000000357627869, 'distance': 28.320268630981445, 'force': [-0.036677099764347076, -0.00650308933109045, -0.0006661770748905838], 'magnitude': 0.03725511580705643, 'cosine_with_motion': -0.8375759720802307, 'motion_component': -0.031203988939523697, 'motion_component_percent': 83.75759720802307}, {'resid': 1313, 'atom': 'H141', 'charge': 0.15000000596046448, 'distance': 31.147912979125977, 'force': [-0.04708423465490341, -0.020433694124221802, 0.0005568877677433193], 'magnitude': 0.051330022513866425, 'cosine_with_motion': -0.8715096116065979, 'motion_component': -0.04473460838198662, 'motion_component_percent': 87.15096116065979}, {'resid': 1313, 'atom': 'H14X', 'charge': 0.09000000357627869, 'distance': 30.6032657623291, 'force': [-0.031710345298051834, -0.003473429474979639, 0.0005039442330598831], 'magnitude': 0.03190399333834648, 'cosine_with_motion': -0.7999254465103149, 'motion_component': -0.025520816445350647, 'motion_component_percent': 79.9925446510315}, {'resid': 1313, 'atom': 'H14Y', 'charge': 0.09000000357627869, 'distance': 30.655122756958008, 'force': [-0.03146345540881157, -0.004479513503611088, -0.000989891355857253], 'magnitude': 0.03179614618420601, 'cosine_with_motion': -0.8327866792678833, 'motion_component': -0.026479406282305717, 'motion_component_percent': 83.27866792678833}, {'resid': 1313, 'atom': 'H151', 'charge': 0.15000000596046448, 'distance': 33.212886810302734, 'force': [-0.04205583408474922, -0.0164044089615345, -0.0005776677862741053], 'magnitude': 0.0451456680893898, 'cosine_with_motion': -0.8781915903091431, 'motion_component': -0.03964654728770256, 'motion_component_percent': 87.8191590309143}, {'resid': 1313, 'atom': 'H15X', 'charge': 0.09000000357627869, 'distance': 28.859060287475586, 'force': [-0.035800717771053314, -0.0022425889037549496, -0.0006625639507547021], 'magnitude': 0.03587700426578522, 'cosine_with_motion': -0.7985641360282898, 'motion_component': -0.028650088235735893, 'motion_component_percent': 79.85641360282898}, {'resid': 1313, 'atom': 'H15Y', 'charge': 0.09000000357627869, 'distance': 29.268531799316406, 'force': [-0.03464149683713913, -0.003268714528530836, -0.0024308753199875355], 'magnitude': 0.03488017991185188, 'cosine_with_motion': -0.832843005657196, 'motion_component': -0.029049713164567947, 'motion_component_percent': 83.2843005657196}, {'resid': 1313, 'atom': 'H16R', 'charge': 0.09000000357627869, 'distance': 33.31593322753906, 'force': [-0.025415221229195595, -0.008681993931531906, 0.0018388000316917896], 'magnitude': 0.026920098811388016, 'cosine_with_motion': -0.8315717577934265, 'motion_component': -0.022385993972420692, 'motion_component_percent': 83.15717577934265}, {'resid': 1313, 'atom': 'H16S', 'charge': 0.09000000357627869, 'distance': 33.26375961303711, 'force': [-0.025772444903850555, -0.008025415241718292, 0.0007892564754001796], 'magnitude': 0.027004612609744072, 'cosine_with_motion': -0.8466089367866516, 'motion_component': -0.022862346842885017, 'motion_component_percent': 84.66089367866516}, {'resid': 1313, 'atom': 'H16X', 'charge': 0.09000000357627869, 'distance': 31.64946937561035, 'force': [-0.029698947444558144, -0.001922423834912479, -0.002020688261836767], 'magnitude': 0.02982962317764759, 'cosine_with_motion': -0.8208733201026917, 'motion_component': -0.024486342445015907, 'motion_component_percent': 82.08733201026917}, {'resid': 1313, 'atom': 'H16Y', 'charge': 0.09000000357627869, 'distance': 31.313846588134766, 'force': [-0.030440619215369225, -0.0013091892469674349, -0.00047604518476873636], 'magnitude': 0.03047247789800167, 'cosine_with_motion': -0.7894144058227539, 'motion_component': -0.024055413901805878, 'motion_component_percent': 78.94144058227539}, {'resid': 1313, 'atom': 'H17R', 'charge': 0.09000000357627869, 'distance': 35.31849670410156, 'force': [-0.02266635373234749, -0.007745970971882343, 0.00015994219575077295], 'magnitude': 0.02395389787852764, 'cosine_with_motion': -0.8625802397727966, 'motion_component': -0.020662158727645874, 'motion_component_percent': 86.25802397727966}, {'resid': 1313, 'atom': 'H17S', 'charge': 0.09000000357627869, 'distance': 35.14371871948242, 'force': [-0.022529244422912598, -0.008790812455117702, 0.0006661732331849635], 'magnitude': 0.024192746728658676, 'cosine_with_motion': -0.8589787483215332, 'motion_component': -0.020781055092811584, 'motion_component_percent': 85.89787483215332}, {'resid': 1313, 'atom': 'H17X', 'charge': 0.09000000357627869, 'distance': 30.026493072509766, 'force': [-0.032974254339933395, -0.00033222007914446294, -0.0033080705907195807], 'magnitude': 0.03314144164323807, 'cosine_with_motion': -0.8114023804664612, 'motion_component': -0.02689104527235031, 'motion_component_percent': 81.14023804664612}, {'resid': 1313, 'atom': 'H17Y', 'charge': 0.09000000357627869, 'distance': 29.90862464904785, 'force': [-0.03337058424949646, 0.0003774126525968313, -0.0014260868774726987], 'magnitude': 0.033403173089027405, 'cosine_with_motion': -0.7782212495803833, 'motion_component': -0.025995058938860893, 'motion_component_percent': 77.82212495803833}, {'resid': 1313, 'atom': 'H18R', 'charge': 0.09000000357627869, 'distance': 35.67620849609375, 'force': [-0.022067764773964882, -0.007695077918469906, 0.0022180890664458275], 'magnitude': 0.023475952446460724, 'cosine_with_motion': -0.8184725046157837, 'motion_component': -0.01921442151069641, 'motion_component_percent': 81.84725046157837}, {'res</t>
         </is>
       </c>
     </row>
@@ -595,7 +595,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>{789: {'frame': 789, 'motion_vector': [-0.7640838623046875, -0.2713966369628906, -2.7751007080078125], 'ionic_force': [1.7615902721881866, 3.541439116001129, -9.729321956634521], 'ionic_force_magnitude': 10.50260429775689, 'radial_force': 3.9553749884696026, 'axial_force': -9.729321956634521, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-7.713208436965942, 5.550417900085449, 1.8187412023544312], 'asn_force_magnitude': 9.675150790494854, 'residue_force': [-7.713208436965942, 5.550417900085449, 1.8187412023544312], 'residue_force_magnitude': 9.675150790494854, 'total_force': [-5.951618164777756, 9.091857016086578, -7.91058075428009], 'total_force_magnitude': 13.441015982814015, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': -0.023595462164669713, 'cosine_residue_motion': -0.023595462164669713, 'cosine_ionic_motion': 0.813211150887596, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': -0.2282896544145956, 'motion_component_residue': -0.2282896544145956, 'motion_component_ionic': 8.540834928295892, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 2.3595462164669714, 'motion_component_percent_residue': 2.3595462164669714, 'motion_component_percent_ionic': 81.3211150887596, 'ionic_contributions': [{'ion_id': 2223, 'distance': 10.327621459960938, 'force': [-0.2378109097480774, 2.686925172805786, -1.5533154010772705], 'magnitude': 3.112701416015625, 'cosine_ionic_motion': 0.41815653443336487, 'motion_component_ionic': 1.3015964031219482, 'motion_component_percent_ionic': 41.81565344333649}, {'ion_id': 2333, 'distance': 7.631259441375732, 'force': [0.2259296029806137, 1.732958197593689, -5.426454067230225], 'magnitude': 5.700929164886475, 'cosine_ionic_motion': 0.8746433258056641, 'motion_component_ionic': 4.986279487609863, 'motion_component_percent_ionic': 87.4643325805664}, {'ion_id': 2372, 'distance': 13.513449668884277, 'force': [0.18907205760478973, 0.2547174096107483, -1.7901601791381836], 'magnitude': 1.8180490732192993, 'cosine_ionic_motion': 0.9045041799545288, 'motion_component_ionic': 1.6444330215454102, 'motion_component_percent_ionic': 90.45041799545288}, {'ion_id': 2397, 'distance': 8.486930847167969, 'force': [2.124591588973999, -2.658017873764038, -3.109158992767334], 'magnitude': 4.609318733215332, 'cosine_ionic_motion': 0.5797797441482544, 'motion_component_ionic': 2.6723897457122803, 'motion_component_percent_ionic': 57.97797441482544}, {'ion_id': 2520, 'distance': 11.108541488647461, 'force': [-0.5401920676231384, 1.5248562097549438, 2.149766683578491], 'magnitude': 2.690444231033325, 'cosine_ionic_motion': -0.7671087384223938, 'motion_component_ionic': -2.0638632774353027, 'motion_component_percent_ionic': 76.71087384223938}], 'glu_contributions': [], 'asn_contributions': [{'resid': 786, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 3.9632208347320557, 'force': [1.5947648286819458, -14.72599983215332, -3.031982898712158], 'magnitude': 15.119235038757324, 'cosine_with_motion': 0.2560434937477112, 'motion_component': 3.8711817264556885, 'motion_component_percent': 25.604349374771118}, {'resid': 786, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 3.0943763256073, 'force': [-6.973222732543945, 19.09194564819336, 4.59505558013916], 'magnitude': 20.838491439819336, 'cosine_with_motion': -0.20922410488128662, 'motion_component': -4.359914779663086, 'motion_component_percent': 20.922410488128662}, {'resid': 786, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 4.144586563110352, 'force': [3.7976768016815186, 16.522083282470703, 4.566196918487549], 'magnitude': 17.557100296020508, 'cosine_with_motion': -0.39514291286468506, 'motion_component': -6.937563896179199, 'motion_component_percent': 39.514291286468506}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 3.4154815673828125, 'force': [-4.642576217651367, -10.45011043548584, -2.9561102390289307], 'magnitude': 11.810881614685059, 'cosine_with_motion': 0.427182674407959, 'motion_component': 5.045403957366943, 'motion_component_percent': 42.7182674407959}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 5.105398178100586, 'force': [-1.4898511171340942, -4.887500762939453, -1.354418158531189], 'magnitude': 5.28599739074707, 'cosine_with_motion': 0.4072275757789612, 'motion_component': 2.1526038646698, 'motion_component_percent': 40.72275757789612}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': 0.6184462011286872, 'motion_component_pip2': 8.312545273881296, 'motion_component_percent_pip2': 61.84462011286872}, 790: {'frame': 790, 'motion_vector': [2.9487457275390625, -1.4932975769042969, -1.8421783447265625], 'ionic_force': [1.4451133608818054, 5.125002205371857, -8.040021538734436], 'ionic_force_magnitude': 9.643440598364215, 'radial_force': 5.324847437332407, 'axial_force': -8.040021538734436, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [1.793839454650879, 5.60133695602417, 5.983039379119873], 'asn_force_magnitude': 8.389850767211739, 'residue_force': [1.793839454650879, 5.60133695602417, 5.983039379119873], 'residue_force_magnitude': 8.389850767211739, 'total_force': [3.2389528155326843, 10.726339161396027, -2.056982159614563], 'total_force_magnitude': 11.391942009662694, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': -0.44403007828425356, 'cosine_residue_motion': -0.44403007828425356, 'cosine_ionic_motion': 0.31293576408105, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': -3.725346092958233, 'motion_component_residue': -3.725346092958233, 'motion_component_ionic': 3.017777452019324, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 44.40300782842536, 'motion_component_percent_residue': 44.40300782842536, 'motion_component_percent_ionic': 31.293576408105, 'ionic_contributions': [{'ion_id': 2223, 'distance': 11.961237907409668, 'force': [-0.41270458698272705, 1.7766833305358887, -1.4345372915267944], 'magnitude': 2.3205227851867676, 'cosine_ionic_motion': -0.13978178799152374, 'motion_component_ionic': -0.32436680793762207, 'motion_component_percent_ionic': 13.978178799152374}, {'ion_id': 2333, 'distance': 10.727517127990723, 'force': [-0.4385051131248474, 0.661516010761261, -2.7736434936523438], 'magnitude': 2.8849589824676514, 'cosine_ionic_motion': 0.2591139078140259, 'motion_component_ionic': 0.7475330233573914, 'motion_component_percent_ionic': 25.911390781402588}, {'ion_id': 2397, 'distance': 7.980435848236084, 'force': [2.29632306098938, 2.686802864074707, -3.831840753555298], 'magnitude': 5.212965965270996, 'cosine_ionic_motion': 0.4977226257324219, 'motion_component_ionic': 2.594611167907715, 'motion_component_percent_ionic': 49.77226257324219}], 'glu_contributions': [], 'asn_contributions': [{'resid': 786, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 4.876735210418701, 'force': [1.793839454650879, 5.60133695602417, 5.983039379119873], 'magnitude': 8.389850616455078, 'cosine_with_motion': -0.4440300762653351, 'motion_component': -3.725346088409424, 'motion_component_percent': 44.40300762653351}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': -0.062111327492603674, 'motion_component_pip2': -0.7075686409389093, 'motion_component_percent_pip2': 6.211132749260368}, 791: {'frame': 791, 'motion_vector': [-4.2862701416015625, -3.1073150634765625, 4.852760314941406], 'ionic_force': [3.6236579790711403, 1.26600182056427, -4.881911516189575], 'ionic_force_magnitude': 6.210210770244629, 'radial_force': 3.8384447057314746, 'axial_force': -4.881911516189575, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [0.0, 0.0, 0.0], 'asn_force_magnitude': 0.0, 'residue_force': [0.0, 0.0, 0.0], 'residue_force_magnitude': 0.0, 'total_force': [3.6236579790711403, 1.26600182056427, -4.881911516189575], 'total_force_magnitude': 6.210210770244629, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': 0, 'cosine_residue_motion': 0, 'cosine_ionic_motion': -0.9676394641737002, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': 0, 'motion_component_residue': 0, 'motion_component_ionic': -6.0092450221252545, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 0, 'motion_component_percent_residue': 0, 'motion_component_percent_ionic': 96.76394641737002, 'ionic_contributions': [{'ion_id': 2223, 'distance': 12.490010261535645, 'force': [0.27115827798843384, 1.3588730096817017, -1.6152938604354858], 'magnitude': 2.1282002925872803, 'cosine_ionic_motion': -0.865169882774353, 'motion_component_ionic': -1.8412548303604126, 'motion_component_percent_ionic': 86.5169882774353}, {'ion_id': 2333, 'distance': 12.180445671081543, 'force': [0.3829460144042969, -0.4483475685119629, -2.1586720943450928], 'magnitude': 2.237750768661499, 'cosine_ionic_motion': -0.6672807931900024, 'motion_component_ionic': -1.4932080507278442, 'motion_component_percent_ionic': 66.72807931900024}, {'ion_id': 2397, 'distance': 9.022244453430176, 'force': [3.0376453399658203, -0.2374657392501831, -2.711297035217285], 'magnitude': 4.078579425811768, 'cosine_ionic_motion': -0.8685073256492615, 'motion_component_ionic': -3.54227614402771, 'motion_component_percent_ionic': 86.85073256492615}, {'ion_id': 2520, 'distance': 13.930449485778809, 'force': [-0.06809165328741074, 0.5929421186447144, 1.6033514738082886], 'magnitude': 1.7108339071273804, 'cosine_ionic_motion': 0.5070592164993286, 'motion_component_ionic': 0.8674941062927246, 'motion_component_percent_ionic': 50.70592164993286}], 'glu_contributions': [], 'asn_contributions': [], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': -0.9676394641737002, 'motion_component_pip2': -6.0092450221252545, 'motion_component_percent_pip2': 96.76394641737002}, 792: {'frame': 792, 'motion_vector': [1.8702239990234375, 1.3981132507324219, -0.47312164306640625], 'ionic_force': [0.25185398757457733, -1.647958219051361, -12.273043394088745], 'ionic_force_magnitude': 12.385749508042762, 'radial_force': 1.667092295824124, 'axial_force': -12.273043394088745, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-0.2777770757675171, 2.4765875339508057, -2.649211972951889], 'asn_force_magnitude': 3.6371651041400535, 'residue_force': [-0.2777770757675171, 2.4765875339508057, -2.649211972951889], 'residue_force_magnitude': 3.6371651041400535, 'total_force': [-0.02592308819293976, 0.8286293148994446, -14.922255367040634], 'total_force_magnitude': 14.945266935962877, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': 0.48426787074380123, 'cosine_residue_motion': 0.48426787074380123, 'cosine_ionic_motion': 0.13465819205244994, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': 1.7613622005255598, 'motion_component_residue': 1.7613622005255598, 'motion_component_ionic': 1.6678426359675598, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 48.42678707438012, 'motion_component_percent_residue': 48.42678707438012, 'motion_component_percent_ionic': 13.465819205244994, 'ionic_contributions': [{'ion_id': 2223, 'distance': 7.982341766357422, 'force': [-3.0752804279327393, 2.9511165618896484, -2.997102737426758], 'magnitude': 5.210476398468018, 'cosine_ionic_motion': -0.01671295240521431, 'motion_component_ionic': -0.08708244562149048, 'motion_component_percent_ionic': 1.671295240521431}, {'ion_id': 2333, 'distance': 8.011151313781738, 'force': [-0.6063924431800842, -2.2778372764587402, -4.604821681976318], 'magnitude': 5.173068523406982, 'cosine_ionic_motion': -0.17364321649074554, 'motion_component_ionic': -0.8982682228088379, 'motion_component_percent_ionic': 17.364321649074554}, {'ion_id': 2372, 'distance': 12.56301212310791, 'force': [-0.1652175337076187, -0.4457704424858093, -2.0491137504577637], 'magnitude': 2.103538751602173, 'cosine_ionic_motion': 0.0074323867447674274, 'motion_component_ionic': 0.015634313225746155, 'motion_component_percent_ionic': 0.7432386744767427}, {'ion_id': 2397, 'distance': 7.979189395904541, 'force': [4.0987443923950195, -1.87546706199646, -2.6220052242279053], 'magnitude': 5.21459436416626, 'cosine_ionic_motion': 0.5058032870292664, 'motion_component_ionic': 2.637558937072754, 'motion_component_percent_ionic': 50.580328702926636}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 5.719515323638916, 'force': [6.612668514251709, -2.8987932205200195, -0.7551400661468506], 'magnitude': 7.259519577026367, 'cosine_with_motion': 0.5013704895973206, 'motion_component': 3.6397087574005127, 'motion_component_percent': 50.137048959732056}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 4.613062381744385, 'force': [-8.090315818786621, 4.625004768371582, 1.0354187488555908], 'magnitude': 9.376351356506348, 'cosine_with_motion': -0.4097873866558075, 'motion_component': -3.8423104286193848, 'motion_component_percent': 40.97873866558075}, {'resid': 1114, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 5.2532525062561035, 'force': [-5.506649017333984, 6.597408294677734, 0.45109352469444275], 'magnitude': 8.605374336242676, 'cosine_with_motion': -0.06283027678728104, 'motion_component': -0.5406780242919922, 'motion_component_percent': 6.283027678728104}, {'resid': 1114, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 4.607603549957275, 'force': [6.715373992919922, -6.228845596313477, -2.106794595718384], 'magnitude': 9.398582458496094, 'cosine_with_motion': 0.2164776623249054, 'motion_component': 2.03458309173584, 'motion_component_percent': 21.64776623249054}, {'resid': 1114, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 4.961211681365967, 'force': [5.857586860656738, -10.694486618041992, 1.2044787406921387], 'magnitude': 12.252923965454102, 'cosine_with_motion': -0.1564428061246872, 'motion_component': -1.916881799697876, 'motion_component_percent': 15.64428061246872}, {'resid': 1114, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 4.018673896789551, 'force': [-3.9445571899414062, 7.410848140716553, -1.518121600151062], 'magnitude': 8.53140640258789, 'cosine_with_motion': 0.1821431964635849, 'motion_component': 1.5539376735687256, 'motion_component_percent': 18.21431964635849}, {'resid': 1114, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 5.694654941558838, 'force': [-1.9218844175338745, 3.665451765060425, -0.9601467251777649], 'magnitude': 4.248653411865234, 'cosine_with_motion': 0.19606277346611023, 'motion_component': 0.8330027461051941, 'motion_component_percent': 19.606277346611023}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': 0.2294508924588965, 'motion_component_pip2': 3.4292048364931196, 'motion_component_percent_pip2': 22.945089245889648}, 793: {'frame': 793, 'motion_vector': [-0.4285240173339844, 3.8867568969726562, -4.724609375], 'ionic_force': [-1.4666863232851028, -0.13524457812309265, -14.093934535980225], 'ionic_force_magnitude': 14.170689841052884, 'radial_force': 1.4729086417097519, 'axial_force': -14.093934535980225, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-2.4507861603051424, 1.7706725299358368, -1.1950036138296127], 'asn_force_magnitude': 3.251102528201538, 'residue_force': [-2.4507861603051424, 1.7706725299358368, -1.1950036138296127], 'residue_force_magnitude': 3.251102528201538, 'total_force': [-3.9174724835902452, 1.6354279518127441, -15.288938149809837], 'total_force_magnitude': 15.867351543151988, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': 0.6810038461616016, 'cosine_residue_motion': 0.6810038461616016, 'cosine_ionic_motion': 0.7673820294395889, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': 2.2140133259709542, 'motion_component_residue': 2.2140133259709542, 'motion_component_ionic': 10.874332728786127, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 68.10038461616016, 'motion_component_percent_residue': 68.10038461616016, 'motion_component_percent_ionic': 76.73820294395888, 'ionic_contributions': [{'ion_id': 2223, 'distance': 7.717455863952637, 'force': [-0.6692728400230408, 4.413219451904297, -3.3389081954956055], 'magnitude': 5.5742926597595215, 'cosine_ionic_motion': 0.9715787172317505, 'motion_component_ionic': 5.415863990783691, 'motion_component_percent_ionic': 97.15787172317505}, {'ion_id': 2333, 'distance': 5.9145026206970215, 'force': [-4.392226696014404, -4.7174577713012695, -6.966256618499756], 'magnitude': 9.490774154663086, 'cosine_ionic_motion': 0.28277871012687683, 'motion_component_ionic': 2.683788776397705, 'motion_component_percent_ionic': 28.277871012687683}, {'ion_id': 2372, 'distance': 12.76153564453125, 'force': [0.12021027505397797, -0.1753276288509369, -2.02748703956604], 'magnitude': 2.0386009216308594, 'cosine_ionic_motion': 0.7075458765029907, 'motion_component_ionic': 1.4424036741256714, 'motion_component_percent_ionic': 70.75458765029907}, {'ion_id': 2397, 'distance': 9.213869094848633, 'force': [3.4746029376983643, 0.3443213701248169, -1.7612826824188232], 'magnitude': 3.9106955528259277, 'cosine_ionic_motion': 0.3406749963760376, 'motion_component_ionic': 1.3322762250900269, 'motion_component_percent_ionic': 34.06749963760376}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 5.695321083068848, 'force': [7.086710453033447, -1.121163010597229, -1.4571805000305176], 'magnitude': 7.321328163146973, 'cosine_with_motion': -0.011356223374605179, 'motion_component': -0.08314263820648193, 'motion_component_percent': 1.1356223374605179}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 4.527876853942871, 'force': [-9.292401313781738, 1.3447635173797607, 2.5620243549346924], 'magnitude': 9.732476234436035, 'cosine_with_motion': -0.04851501062512398, 'motion_component': -0.47217118740081787, 'motion_component_percent': 4.851501062512398}, {'resid': 458, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 5.948486328125, 'force': [-3.656846523284912, 0.2103463113307953, -1.3209383487701416], 'magnitude': 3.89379620552063, 'cosine_with_motion': 0.36119917035102844, 'motion_component': 1.4064359664916992, 'motion_component_percent': 36.119917035102844}, {'resid': 786, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 5.8059000968933105, 'force': [1.2495111227035522, -6.931521892547607, 0.16176150739192963], 'magnitude': 7.045100688934326, 'cosine_with_motion': -0.6536190509796143, 'motion_component': -4.604812145233154, 'motion_component_percent': 65.36190509796143}, {'resid': 786, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 5.554823398590088, 'force': [0.02254597656428814, 6.408270835876465, -0.8658595681190491], 'magnitude': 6.466541290283203, 'cosine_with_motion': 0.7309523820877075, 'motion_component': 4.726733684539795, 'motion_component_percent': 73.09523820877075}, {'resid': 786, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 5.122107028961182, 'force': [-4.158714771270752, 10.71290111541748, 0.2815915644168854], 'magnitude': 11.49523639678955, 'cosine_with_motion': 0.597030758857727, 'motion_component': 6.863009452819824, 'motion_component_percent': 59.703075885772705}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 4.210773468017578, 'force': [3.1524949073791504, -7.089216709136963, 0.43494728207588196], 'magnitude': 7.770739555358887, 'cosine_with_motion': -0.6496387124061584, 'motion_component': -5.048173427581787, 'motion_component_percent': 64.96387124061584}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 5.717676162719727, 'force': [2.0617167949676514, -3.6622838973999023, -0.31478893756866455], 'magnitude': 4.2145094871521, 'cosine_with_motion': -0.5273557305335999, 'motion_component': -2.222545623779297, 'motion_component_percent': 52.735573053359985}, {'resid': 1114, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 5.960616111755371, 'force': [-2.1367669105529785, 6.260311126708984, 0.9592458605766296], 'magnitude': 6.684116840362549, 'cosine_with_motion': 0.5053520202636719, 'motion_component': 3.3778319358825684, 'motion_component_percent': 50.53520202636719}, {'resid': 1114, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 5.901364326477051, 'force': [2.3585755825042725, -4.916697025299072, -1.7575600147247314], 'magnitude': 5.729381084442139, 'cosine_with_motion': -0.3363032341003418, 'motion_component': -1.9268094301223755, 'motion_component_percent': 33.63032341003418}, {'resid': 1114, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 5.1495232582092285, 'force': [1.733738899230957, -11.209312438964844, -0.8332070708274841], 'magnitude': 11.373160362243652, 'cosine_with_motion': -0.578838586807251, 'motion_component': -6.583223819732666, 'motion_component_percent': 57.8838586807251}, {'resid': 1114, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 4.341142177581787, 'force': [-0.6122412085533142, 7.163901329040527, 1.3246649503707886], 'magnitude': 7.311023235321045, 'cosine_with_motion': 0.487271785736084, 'motion_component': 3.562455415725708, 'motion_component_percent': 48.7271785736084}, {'resid': 1114, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 5.459538459777832, 'force': [-0.25910916924476624, 4.600373268127441, -0.3697046935558319], 'magnitude': 4.622472763061523, 'cosine_with_motion': 0.6962562203407288, 'motion_component': 3.2184255123138428, 'motion_component_percent': 69.62562203407288}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': 0.8248601550903266, 'motion_component_pip2': 13.088346054757082, 'motion_component_percent_pip2': 82.48601550903267}, 794: {'frame': 794, 'motion_vector': [2.0873985290527344, -2.63055419921875, -3.9116897583007812], 'ionic_force': [0.25486694276332855, 3.973426640033722, -6.730924963951111], 'ionic_force_magnitude': 7.820385367268257, 'radial_force': 3.9815921968784296, 'axial_force': -6.730924963951111, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [0.780780553817749, 6.535667300224304, 8.923847675323486], 'asn_force_magnitude': 11.088716006139647, 'residue_force': [0.780780553817749, 6.535667300224304, 8.923847675323486], 'residue_force_magnitude': 11.088716006139647, 'total_force': [1.0356474965810776, 10.509093940258026, 2.1929227113723755], 'total_force_magnitude': 10.785292355814718, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': -0.8828511790277765, 'cosine_residue_motion': -0.8828511790277765, 'cosine_ionic_motion': 0.40699534637881285, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': -9.789685999924565, 'motion_component_residue': -9.789685999924565, 'motion_component_ionic': 3.1828604513671435, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 88.28511790277766, 'motion_component_percent_residue': 88.28511790277766, 'motion_component_percent_ionic': 40.699534637881285, 'ionic_contributions': [{'ion_id': 2223, 'distance': 14.259329795837402, 'force': [-0.1769786924123764, 1.197727918624878, -1.0955578088760376], 'magnitude': 1.6328259706497192, 'cosine_ionic_motion': 0.0909215584397316, 'motion_component_ionic': 0.1484590768814087, 'motion_component_percent_ionic': 9.09215584397316}, {'ion_id': 2333, 'distance': 7.373826026916504, 'force': [-0.6715062856674194, 1.7658628225326538, -5.8063130378723145], 'magnitude': 6.105936527252197, 'cosine_ionic_motion': 0.5294250249862671, 'motion_component_ionic': 3.232635498046875, 'motion_component_percent_ionic': 52.94250249862671}, {'ion_id': 2397, 'distance': 12.446090698242188, 'force': [1.2916356325149536, 0.7320946455001831, -1.5457106828689575], 'magnitude': 2.14324688911438, 'cosine_ionic_motion': 0.6169313788414001, 'motion_component_ionic': 1.3222362995147705, 'motion_component_percent_ionic': 61.693137884140015}, {'ion_id': 2520, 'distance': 13.777055740356445, 'force': [-0.18828371167182922, 0.2777412533760071, 1.7166565656661987], 'magnitude': 1.7491428852081299, 'cosine_ionic_motion': -0.8692659735679626, 'motion_component_ionic': -1.520470380783081, 'motion_component_percent_ionic': 86.92659735679626}], 'glu_contributions': [], 'asn_contributions': [{'resid': 786, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 4.635568141937256, 'force': [-1.0707740783691406, -6.6548075675964355, -8.757976531982422], 'magnitude': 11.051478385925293, 'cosine_with_motion': 0.8693140745162964, 'motion_component': 9.607205390930176, 'motion_component_percent': 86.93140745162964}, {'resid': 786, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 3.43974232673645, 'force': [1.4465851783752441, 10.284523010253906, 13.286484718322754], 'magnitude': 16.86400604248047, 'cosine_with_motion': -0.8742360472679138, 'motion_component': -14.743122100830078, 'motion_component_percent': 87.42360472679138}, {'resid': 786, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 5.321551322937012, 'force': [2.5824410915374756, 4.817376136779785, 9.140058517456055], 'magnitude': 10.649731636047363, 'cosine_with_motion': -0.7838222980499268, 'motion_component': -8.34749698638916, 'motion_component_percent': 78.38222980499268}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 4.9782633781433105, 'force': [-2.17747163772583, -1.9114242792129517, -4.7447190284729], 'magnitude': 5.559432029724121, 'cosine_with_motion': 0.6644074320793152, 'motion_component': 3.693727970123291, 'motion_component_percent': 66.44074320793152}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': -0.6125773257315048, 'motion_component_pip2': -6.606825548557421, 'motion_component_percent_pip2': 61.25773257315048}}</t>
+          <t>{789: {'frame': 789, 'motion_vector': [-0.7640838623046875, -0.2713966369628906, -2.7751007080078125], 'ionic_force': [1.7615902721881866, 3.541439116001129, -9.729321956634521], 'ionic_force_magnitude': 10.50260429775689, 'radial_force': 3.9553749884696026, 'axial_force': -9.729321956634521, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-7.713208436965942, 5.550417900085449, 1.8187412023544312], 'asn_force_magnitude': 9.675150790494854, 'residue_force': [-7.713208436965942, 5.550417900085449, 1.8187412023544312], 'residue_force_magnitude': 9.675150790494854, 'pip2_force': [0.847271473146975, 0.1475509395240806, -4.499001910447987], 'pip2_force_magnitude': 4.580464869331247, 'total_force': [-5.104346691630781, 9.239407955610659, -12.409582664728077], 'total_force_magnitude': 16.291677520479073, 'cosine_total_motion': 0.7607079828858798, 'cosine_glu_motion': 0, 'cosine_asn_motion': -0.023595462164669713, 'cosine_residue_motion': -0.023595462164669713, 'cosine_pip2_motion': 0.8908842196065903, 'cosine_ionic_motion': 0.813211150887596, 'motion_component_total': 12.393209144430868, 'motion_component_glu': 0, 'motion_component_asn': -0.2282896544145956, 'motion_component_residue': -0.2282896544145956, 'motion_component_ionic': 8.540834928295892, 'motion_component_pip2': 4.080663870549571, 'motion_component_percent_total': 76.07079828858798, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 2.3595462164669714, 'motion_component_percent_residue': 2.3595462164669714, 'motion_component_percent_ionic': 81.3211150887596, 'motion_component_percent_pip2': 89.08842196065902, 'ionic_contributions': [{'ion_id': 2223, 'distance': 10.327621459960938, 'force': [-0.2378109097480774, 2.686925172805786, -1.5533154010772705], 'magnitude': 3.112701416015625, 'cosine_ionic_motion': 0.41815653443336487, 'motion_component_ionic': 1.3015964031219482, 'motion_component_percent_ionic': 41.81565344333649}, {'ion_id': 2333, 'distance': 7.631259441375732, 'force': [0.2259296029806137, 1.732958197593689, -5.426454067230225], 'magnitude': 5.700929164886475, 'cosine_ionic_motion': 0.8746433258056641, 'motion_component_ionic': 4.986279487609863, 'motion_component_percent_ionic': 87.4643325805664}, {'ion_id': 2372, 'distance': 13.513449668884277, 'force': [0.18907205760478973, 0.2547174096107483, -1.7901601791381836], 'magnitude': 1.8180490732192993, 'cosine_ionic_motion': 0.9045041799545288, 'motion_component_ionic': 1.6444330215454102, 'motion_component_percent_ionic': 90.45041799545288}, {'ion_id': 2397, 'distance': 8.486930847167969, 'force': [2.124591588973999, -2.658017873764038, -3.109158992767334], 'magnitude': 4.609318733215332, 'cosine_ionic_motion': 0.5797797441482544, 'motion_component_ionic': 2.6723897457122803, 'motion_component_percent_ionic': 57.97797441482544}, {'ion_id': 2520, 'distance': 11.108541488647461, 'force': [-0.5401920676231384, 1.5248562097549438, 2.149766683578491], 'magnitude': 2.690444231033325, 'cosine_ionic_motion': -0.7671087384223938, 'motion_component_ionic': -2.0638632774353027, 'motion_component_percent_ionic': 76.71087384223938}], 'glu_contributions': [], 'asn_contributions': [{'resid': 786, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 3.9632208347320557, 'force': [1.5947648286819458, -14.72599983215332, -3.031982898712158], 'magnitude': 15.119235038757324, 'cosine_with_motion': 0.2560434937477112, 'motion_component': 3.8711817264556885, 'motion_component_percent': 25.604349374771118}, {'resid': 786, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 3.0943763256073, 'force': [-6.973222732543945, 19.09194564819336, 4.59505558013916], 'magnitude': 20.838491439819336, 'cosine_with_motion': -0.20922410488128662, 'motion_component': -4.359914779663086, 'motion_component_percent': 20.922410488128662}, {'resid': 786, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 4.144586563110352, 'force': [3.7976768016815186, 16.522083282470703, 4.566196918487549], 'magnitude': 17.557100296020508, 'cosine_with_motion': -0.39514291286468506, 'motion_component': -6.937563896179199, 'motion_component_percent': 39.514291286468506}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 3.4154815673828125, 'force': [-4.642576217651367, -10.45011043548584, -2.9561102390289307], 'magnitude': 11.810881614685059, 'cosine_with_motion': 0.427182674407959, 'motion_component': 5.045403957366943, 'motion_component_percent': 42.7182674407959}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 5.105398178100586, 'force': [-1.4898511171340942, -4.887500762939453, -1.354418158531189], 'magnitude': 5.28599739074707, 'cosine_with_motion': 0.4072275757789612, 'motion_component': 2.1526038646698, 'motion_component_percent': 40.72275757789612}], 'pip2_contributions': [{'resid': 1313, 'atom': 'C1', 'charge': 0.06000000238418579, 'distance': 25.27534294128418, 'force': [-0.022676624357700348, -0.01718645729124546, 0.012754387222230434], 'magnitude': 0.031181372702121735, 'cosine_with_motion': -0.1486808955669403, 'motion_component': -0.004636074416339397, 'motion_component_percent': 14.86808955669403}, {'resid': 1313, 'atom': 'C11', 'charge': 0.17000000178813934, 'distance': 24.14469337463379, 'force': [-0.07957837730646133, -0.04626452177762985, 0.03000103309750557], 'magnitude': 0.09681521356105804, 'cosine_with_motion': -0.035352230072021484, 'motion_component': -0.003422633744776249, 'motion_component_percent': 3.5352230072021484}, {'resid': 1313, 'atom': 'C12', 'charge': 0.04000000283122063, 'distance': 24.405574798583984, 'force': [-0.018933849409222603, -0.010321058332920074, 0.0056639970280230045], 'magnitude': 0.022295644506812096, 'cosine_with_motion': 0.024045834317803383, 'motion_component': 0.000536117353476584, 'motion_component_percent': 2.4045834317803383}, {'resid': 1313, 'atom': 'C13', 'charge': -0.05000000074505806, 'distance': 25.52105140686035, 'force': [0.021475007757544518, 0.01244976557791233, -0.005778530612587929], 'magnitude': 0.025486545637249947, 'cosine_with_motion': -0.050912998616695404, 'motion_component': -0.0012975964928045869, 'motion_component_percent': 5.09129986166954}, {'resid': 1313, 'atom': 'C2', 'charge': 0.06000000238418579, 'distance': 26.769166946411133, 'force': [-0.019931046292185783, -0.015637120231986046, 0.011444843374192715], 'magnitude': 0.02779839187860489, 'cosine_with_motion': -0.15289171040058136, 'motion_component': -0.004250143654644489, 'motion_component_percent': 15.289171040058136}, {'resid': 1313, 'atom': 'C21', 'charge': 0.6299999952316284, 'distance': 22.003755569458008, 'force': [-0.37328338623046875, -0.19256089627742767, 0.10101927071809769], 'magnitude': 0.4320012629032135, 'cosine_with_motion': 0.04575078561902046, 'motion_component': 0.01976439729332924, 'motion_component_percent': 4.575078561902046}, {'resid': 1313, 'atom': 'C210', 'charge': -0.18000000715255737, 'distance': 21.02984619140625, 'force': [0.11328990757465363, 0.06762255728244781, 0.029181860387325287], 'magnitude': 0.13512584567070007, 'cosine_with_motion': -0.47584792971611023, 'motion_component': -0.06429935246706009, 'motion_component_percent': 47.58479297161102}, {'resid': 1313, 'atom': 'C211', 'charge': -0.15000000596046448, 'distance': 22.154693603515625, 'force': [0.08401113748550415, 0.050087910145521164, 0.02697412297129631], 'magnitude': 0.10146070271730423, 'cosine_with_motion': -0.5203617215156555, 'motion_component': -0.052796266973018646, 'motion_component_percent': 52.03617215156555}, {'resid': 1313, 'atom': 'C212', 'charge': -0.15000000596046448, 'distance': 22.889408111572266, 'force': [0.07601042091846466, 0.05075792968273163, 0.026093831285834312], 'magnitude': 0.09505177289247513, 'cosine_with_motion': -0.5249742269515991, 'motion_component': -0.04989973083138466, 'motion_component_percent': 52.49742269515991}, {'resid': 1313, 'atom': 'C213', 'charge': -0.18000000715255737, 'distance': 22.94007682800293, 'force': [0.08804772794246674, 0.0663875862956047, 0.02712731622159481], 'magnitude': 0.1135588213801384, 'cosine_with_motion': -0.4890875220298767, 'motion_component': -0.05554020404815674, 'motion_component_percent': 48.90875220298767}, {'resid': 1313, 'atom': 'C214', 'charge': -0.15000000596046448, 'distance': 24.376596450805664, 'force': [0.06373637914657593, 0.05037802457809448, 0.020577579736709595], 'magnitude': 0.0838075652718544, 'cosine_with_motion': -0.49309825897216797, 'motion_component': -0.041325364261865616, 'motion_component_percent': 49.3098258972168}, {'resid': 1313, 'atom': 'C215', 'charge': -0.15000000596046448, 'distance': 24.778676986694336, 'force': [0.05915984883904457, 0.050696443766355515, 0.022556085139513016], 'magnitude': 0.08110976964235306, 'cosine_with_motion': -0.5183696746826172, 'motion_component': -0.04204484447836876, 'motion_component_percent': 51.83696746826172}, {'resid': 1313, 'atom': 'C216', 'charge': -0.18000000715255737, 'distance': 24.066883087158203, 'force': [0.07180164754390717, 0.0667029470205307, 0.03225129097700119], 'magnitude': 0.10317414999008179, 'cosine_with_motion': -0.5446571111679077, 'motion_component': -0.05619453638792038, 'motion_component_percent': 54.46571111679077}, {'resid': 1313, 'atom': 'C217', 'charge': -0.18000000715255737, 'distance': 23.413986206054688, 'force': [0.07321666181087494, 0.07485445588827133, 0.030314302071928978], 'magnitude': 0.10900837928056717, 'cosine_with_motion': -0.5089008212089539, 'motion_component': -0.055474456399679184, 'motion_component_percent': 50.890082120895386}, {'resid': 1313, 'atom': 'C218', 'charge': -0.18000000715255737, 'distance': 23.188087463378906, 'force': [0.06934080272912979, 0.07974733412265778, 0.03442244976758957], 'magnitude': 0.11114265024662018, 'cosine_with_motion': -0.5295239686965942, 'motion_component': -0.05885269492864609, 'motion_component_percent': 52.952396869659424}, {'resid': 1313, 'atom': 'C219', 'charge': -0.18000000715255737, 'distance': 23.04113006591797, 'force': [0.06620558351278305, 0.08570046722888947, 0.03071010112762451], 'magnitude': 0.11256491392850876, 'cosine_with_motion': -0.4887808859348297, 'motion_component': -0.05501957982778549, 'motion_component_percent': 48.87808859348297}, {'resid': 1313, 'atom': 'C22', 'charge': -0.08000000566244125, 'distance': 21.00526237487793, 'force': [0.05247148498892784, 0.027455942705273628, -0.010795521549880505], 'magnitude': 0.060196585953235626, 'cosine_with_motion': -0.10104437172412872, 'motion_component': -0.006082526408135891, 'motion_component_percent': 10.104437172412872}, {'resid': 1313, 'atom': 'C220', 'charge': -0.27000001072883606, 'distance': 23.598533630371094, 'force': [0.08668050915002823, 0.12676912546157837, 0.04822714254260063], 'magnitude': 0.16096514463424683, 'cosine_with_motion': -0.5038357377052307, 'motion_component': -0.0810999944806099, 'motion_component_percent': 50.38357377052307}, {'resid': 1313, 'atom': 'C23', 'charge': -0.18000000715255737, 'distance': 21.51387596130371, 'force': [0.11597149819135666, 0.054385196417570114, -0.016226045787334442], 'magnitude': 0.12911398708820343, 'cosine_with_motion': -0.15629570186138153, 'motion_component': -0.020179960876703262, 'motion_component_percent': 15.629570186138153}, {'resid': 1313, 'atom': 'C24', 'charge': -0.18000000715255737, 'distance': 20.584579467773438, 'force': [0.1276913583278656, 0.059051625430583954, -0.009933060966432095], 'magnitude': 0.14103490114212036, 'cosine_with_motion': -0.21098187565803528, 'motion_component': -0.029755808413028717, 'motion_component_percent': 21.098187565803528}, {'resid': 1313, 'atom': 'C25', 'charge': -0.15000000596046448, 'distance': 21.254419326782227, 'force': [0.10148036479949951, 0.04302442818880081, -0.001739401021040976], 'magnitude': 0.11023788899183273, 'cosine_with_motion': -0.2647813856601715, 'motion_component': -0.029188942164182663, 'motion_component_percent': 26.47813856601715}, {'resid': 1313, 'atom': 'C26', 'charge': -0.15000000596046448, 'distance': 21.25423240661621, 'force': [0.10094067454338074, 0.044033233076334, 0.004987322259694338], 'magnitude': 0.11023982614278793, 'cosine_with_motion': -0.32291194796562195, 'motion_component': -0.03559775650501251, 'motion_component_percent': 32.291194796562195}, {'resid': 1313, 'atom': 'C27', 'charge': -0.18000000715255737, 'distance': 20.582904815673828, 'force': [0.1258016675710678, 0.06264136731624603, 0.012137382291257381], 'magnitude': 0.1410578489303589, 'cosine_with_motion': -0.35998013615608215, 'motion_component': -0.05077802389860153, 'motion_component_percent': 35.998013615608215}, {'resid': 1313, 'atom': 'C28', 'charge': -0.15000000596046448, 'distance': 20.216615676879883, 'force': [0.10904069244861603, 0.05096860229969025, 0.01894347555935383], 'magnitude': 0.12184632569551468, 'cosine_with_motion': -0.4250069260597229, 'motion_component': -0.051785532385110855, 'motion_component_percent': 42.50069260597229}, {'resid': 1313, 'atom': 'C29', 'charge': -0.15000000596046448, 'distance': 20.418916702270508, 'force': [0.10414750874042511, 0.05286802724003792, 0.0250022541731596], 'magnitude': 0.11944389343261719, 'cosine_with_motion': -0.4729103446006775, 'motion_component': -0.05648625269532204, 'motion_component_percent': 47.29103446006775}, {'resid': 1313, 'atom': 'C3', 'charge': 0.06000000238418579, 'distance': 27.445035934448242, 'force': [-0.01869869790971279, -0.01428994070738554, 0.012064528651535511], 'magnitude': 0.026446107774972916, 'cosine_with_motion': -0.20029833912849426, 'motion_component': -0.005297111347317696, 'motion_component_percent': 20.029833912849426}, {'resid': 1313, 'atom': 'C31', 'charge': 0.6299999952316284, 'distance': 26.4655818939209, 'force': [-0.263563334941864, -0.13033615052700043, 0.05214845761656761], 'magnitude': 0.29861781001091003, 'cosine_with_motion': 0.10660873353481293, 'motion_component': 0.03183526545763016, 'motion_component_percent': 10.660873353481293}, {'resid': 1313, 'atom': 'C310', 'charge': -0.18000000715255737, 'distance': 22.58210563659668, 'force': [0.11292384564876556, 0.02506452240049839, 0.01878596469759941], 'magnitude': 0.11718761920928955, 'cosine_with_motion': -0.4286198318004608, 'motion_component': -0.05022893846035004, 'motion_component_percent': 42.86198318004608}, {'resid': 1313, 'atom': 'C311', 'charge': -0.18000000715255737, 'distance': 22.35918426513672, 'force': [0.11632254719734192, 0.01761123351752758, 0.0211604256182909], 'magnitude': 0.11953599750995636, 'cosine_with_motion': -0.4409271776676178, 'motion_component': -0.05270667001605034, 'motion_component_percent': 44.09271776676178}, {'resid': 1313, 'atom': 'C312', 'charge': -0.18000000715255737, 'distance': 23.65790557861328, 'force': [0.10427509248256683, 0.012051895260810852, 0.019538454711437225], 'magnitude': 0.10677216202020645, 'cosine_with_motion': -0.4443477690219879, 'motion_component': -0.047443971037864685, 'motion_component_percent': 44.43477690219879}, {'resid': 1313, 'atom': 'C313', 'charge': -0.18000000715255737, 'distance': 24.75435447692871, 'force': [0.0942249596118927, 0.012365276925265789, 0.021897679194808006], 'magnitude': 0.09752307832241058, 'cosine_with_motion': -0.4827762246131897, 'motion_component': -0.04708182439208031, 'motion_component_percent': 48.27762246131897}, {'resid': 1313, 'atom': 'C314', 'charge': -0.18000000715255737, 'distance': 24.716970443725586, 'force': [0.09393756091594696, 0.00819451455026865, 0.026019340381026268], 'magnitude': 0.09781831502914429, 'cosine_with_motion': -0.5169848799705505, 'motion_component': -0.050570592284202576, 'motion_component_percent': 51.698487997055054}, {'resid': 1313, 'atom': 'C315', 'charge': -0.18000000715255737, 'distance': 25.827590942382812, 'force': [0.08485684543848038, 0.008348367176949978, 0.027484014630317688], 'magnitude': 0.08958655595779419, 'cosine_with_motion': -0.553554356098175, 'motion_component': -0.049591027200222015, 'motion_component_percent': 55.355435609817505}, {'resid': 1313, 'atom': 'C316', 'charge': -0.18000000715255737, 'distance': 25.758502960205078, 'force': [0.08419010788202286, 0.00536088552325964, 0.03155134245753288], 'magnitude': 0.09006775170564651, 'cosine_with_motion': -0.5888729691505432, 'motion_component': -0.05303846299648285, 'motion_component_percent': 58.88729691505432}, {'resid': 1313, 'atom': 'C317', 'charge': -0.18000000715255737, 'distance': 26.83822250366211, 'force': [0.0762835219502449, 0.006158046890050173, 0.032036758959293365], 'magnitude': 0.08296656608581543, 'cosine_with_motion': -0.6206070780754089, 'motion_component': -0.051489636301994324, 'motion_component_percent': 62.060707807540894}, {'resid': 1313, 'atom': 'C318', 'charge': -0.27000001072883606, 'distance': 28.247459411621094, 'force': [0.10423076152801514, 0.007922106422483921, 0.04115782305598259], 'magnitude': 0.1123422384262085, 'cosine_with_motion': -0.6034796833992004, 'motion_component': -0.0677962601184845, 'motion_component_percent': 60.347968339920044}, {'resid': 1313, 'atom': 'C32', 'charge': -0.08000000566244125, 'distance': 26.769617080688477, 'force': [0.0332757942378521, 0.015667302533984184, -0.004576403181999922], 'magnitude': 0.037063274532556534, 'cosine_with_motion': -0.15843947231769562, 'motion_component': -0.005872285924851894, 'motion_component_percent': 15.843947231769562}, {'resid': 1313, 'atom': 'C33', 'charge': -0.18000000715255737, 'distance': 26.077802658081055, 'force': [0.08087404072284698, 0.03311450034379959, -0.009216935373842716], 'magnitude': 0.08787566423416138, 'cosine_with_motion': -0.17792534828186035, 'motion_component': -0.015635307878255844, 'motion_component_percent': 17.792534828186035}, {'resid': 1313, 'atom': 'C34', 'charge': -0.18000000715255737, 'distance': 26.809768676757812, 'force': [0.07749311625957489, 0.02973167411983013, -0.004854184575378895], 'magnitude': 0.08314275741577148, 'cosine_with_motion': -0.22385451197624207, 'motion_component': -0.018611881881952286, 'motion_component_percent': 22.385451197624207}, {'resid': 1313, 'atom': 'C35', 'charge': -0.18000000715255737, 'distance': 26.25811767578125, 'force': [0.08237410336732864, 0.026729309931397438, -0.0034992729779332876], 'magnitude': 0.08667290955781937, 'cosine_with_motion': -0.24137353897094727, 'motion_component': -0.02092054672539234, 'motion_component_percent': 24.137353897094727}, {'resid': 1313, 'atom': 'C36', 'charge': -0.18000000715255737, 'distance': 25.405567169189453, 'force': [0.08797577023506165, 0.028843313455581665, 0.0008879622910171747], 'magnitude': 0.09258758276700974, 'cosine_with_motion': -0.28957000374794006, 'motion_component': -0.02681058645248413, 'motion_component_percent': 28.957000374794006}, {'resid': 1313, 'atom': 'C37', 'charge': -0.18000000715255737, 'distance': 24.555288314819336, 'force': [0.0955711305141449, 0.02612404339015484, 0.002573790028691292], 'magnitude': 0.09911070019006729, 'cosine_with_motion': -0.30451634526252747, 'motion_component': -0.030180828645825386, 'motion_component_percent': 30.451634526252747}, {'resid': 1313, 'atom': 'C38', 'charge': -0.18000000715255737, 'distance': 23.899070739746094, 'force': [0.1003129705786705, 0.02842947654426098, 0.008724972605705261], 'magnitude': 0.10462816059589386, 'cosine_with_motion': -0.3589353859424591, 'motion_component': -0.037554748356342316, 'motion_component_percent': 35.89353859424591}, {'resid': 1313, 'atom': 'C39', 'charge': -0.18000000715255737, 'distance': 23.15266990661621, 'force': [0.10819603502750397, 0.024372555315494537, 0.011315678246319294], 'magnitude': 0.11148294806480408, 'cosine_with_motion': -0.3744431138038635, 'motion_component': -0.04174402356147766, 'motion_component_percent': 37.44431138038635}, {'resid': 1313, 'atom': 'C4', 'charge': 0.08000000566244125, 'distance': 26.739046096801758, 'force': [-0.02510295808315277, -0.020180175080895424, 0.018508953973650932], 'magnitude': 0.03714807331562042, 'cosine_with_motion': -0.24866466224193573, 'motion_component': -0.009237413294613361, 'motion_component_percent': 24.866466224193573}, {'resid': 1313, 'atom': 'C5', 'charge': 0.08000000566244125, 'distance': 25.34132194519043, 'force': [-0.028456343337893486, -0.021694401279091835, 0.020740117877721786], 'magnitude': 0.04135895147919655, 'cosine_with_motion': -0.2502635419368744, 'motion_component': -0.010350637137889862, 'motion_component_percent': 25.02635419368744}, {'resid': 1313, 'atom': 'C6', 'charge': 0.06000000238418579, 'distance': 24.480422973632812, 'force': [-0.023157740011811256, -0.018398720771074295, 0.01516757719218731], 'magnitude': 0.033239271491765976, 'cosine_with_motion': -0.20191362500190735, 'motion_component': -0.0067114620469510555, 'motion_component_percent': 20.191362500190735}, {'resid': 1313, 'atom': 'H1', 'charge': 0.12000000476837158, 'distance': 25.37667465209961, 'force': [-0.046510323882102966, -0.03190808743238449, 0.025417083874344826], 'magnitude': 0.06186569482088089, 'cosine_with_motion': -0.14724992215633392, 'motion_component': -0.009109718725085258, 'motion_component_percent': 14.724992215633392}, {'resid': 1313, 'atom': 'H10R', 'charge': 0.09000000357627869, 'distance': 21.397281646728516, 'force': [-0.05472002550959587, -0.03378196433186531, -0.01112136896699667], 'magnitude': 0.06526245176792145, 'cosine_with_motion': 0.43375447392463684, 'motion_component': 0.028307881206274033, 'motion_component_percent': 43.375447392463684}, {'resid': 1313, 'atom': 'H10S', 'charge': 0.09000000357627869, 'distance': 20.238534927368164, 'force': [-0.05965800583362579, -0.038559526205062866, -0.016604777425527573], 'magnitude': 0.07294952124357224, 'cosine_with_motion': 0.4842352569103241, 'motion_component': 0.03532472997903824, 'motion_component_percent': 48.42352569103241}, {'resid': 1313, 'atom': 'H10X', 'charge': 0.09000000357627869, 'distance': 21.67898941040039, 'force': [-0.06078709661960602, -0.015236293897032738, -0.010717526078224182], 'magnitude': 0.06357736140489578, 'cosine_with_motion': 0.43699145317077637, 'motion_component': 0.02778276428580284, 'motion_component_percent': 43.69914531707764}, {'resid': 1313, 'atom': 'H10Y', 'charge': 0.09000000357627869, 'distance': 23.419334411621094, 'force': [-0.052049506455659866, -0.012533596716821194, -0.010087216272950172], 'magnitude': 0.05447929725050926, 'cosine_with_motion': 0.45181986689567566, 'motion_component': 0.024614829570055008, 'motion_component_percent': 45.181986689567566}, {'resid': 1313, 'atom': 'H111', 'charge': 0.15000000596046448, 'distance': 22.339914321899414, 'force': [-0.08386557549238205, -0.04548488184809685, -0.029236765578389168], 'magnitude': 0.09978525340557098, 'cosine_with_motion': 0.5461481809616089, 'motion_component': 0.05449753254652023, 'motion_component_percent': 54.61481809616089}, {'resid': 1313, 'atom': 'H11A', 'charge': 0.09000000357627869, 'distance': 24.940025329589844, 'force': [-0.03947716951370239, -0.022127924486994743, 0.016111426055431366], 'magnitude': 0.048038214445114136, 'cosine_with_motion': -0.06150064617395401, 'motion_component': -0.0029543812852352858, 'motion_component_percent': 6.150064617395401}, {'resid': 1313, 'atom': 'H11B', 'charge': 0.09000000357627869, 'distance': 23.315750122070312, 'force': [-0.045325275510549545, -0.02515977993607521, 0.0182673130184412], 'magnitude': 0.05496444180607796, 'cosine_with_motion': -0.05810246244072914, 'motion_component': -0.0031935693696141243, 'motion_component_percent': 5.810246244072914}, {'resid': 1313, 'atom': 'H11X', 'charge': 0.09000000357627869, 'distance': 21.70240592956543, 'force': [-0.06225941330194473, -0.00811767578125, -0.009084763936698437], 'magnitude': 0.06344024091959, 'cosine_with_motion': 0.4088320732116699, 'motion_component': 0.02593640610575676, 'motion_component_percent': 40.88320732116699}, {'resid': 1313, 'atom': 'H11Y', 'charge': 0.09000000357627869, 'distance': 21.90745735168457, 'force': [-0.06006093695759773, -0.008900129236280918, -0.01376796793192625], 'magnitude': 0.06225821375846863, 'cosine_with_motion': 0.4806446433067322, 'motion_component': 0.029924076050519943, 'motion_component_percent': 48.06446433067322}, {'resid': 1313, 'atom': 'H12', 'charge': 0.09000000357627869, 'distance': 24.674724578857422, 'force': [-0.04253276810050011, -0.02081781066954136, 0.012888426892459393], 'magnitude': 0.04907676950097084, 'cosine_with_motion': 0.016786547377705574, 'motion_component': 0.0008238295558840036, 'motion_component_percent': 1.6786547377705574}, {'resid': 1313, 'atom': 'H121', 'charge': 0.15000000596046448, 'distance': 23.686283111572266, 'force': [-0.0703335851430893, -0.04689730331301689, -0.02707083150744438], 'magnitude': 0.08876372873783112, 'cosine_with_motion': 0.5517435073852539, 'motion_component': 0.048974812030792236, 'motion_component_percent': 55.17435073852539}, {'resid': 1313, 'atom': 'H12X', 'charge': 0.09000000357627869, 'distance': 24.246295928955078, 'force': [-0.04992233216762543, -0.006047288421541452, -0.007383708842098713], 'magnitude': 0.05082645267248154, 'cosine_with_motion': 0.41019514203071594, 'motion_component': 0.02084876410663128, 'motion_component_percent': 41.019514203071594}, {'resid': 1313, 'atom': 'H12Y', 'charge': 0.09000000357627869, 'distance': 23.438549041748047, 'force': [-0.05331629514694214, -0.003671312239021063, -0.01010782178491354], 'magnitude': 0.054390016943216324, 'cosine_with_motion': 0.443785160779953, 'motion_component': 0.024137482047080994, 'motion_component_percent': 44.3785160779953}, {'resid': 1313, 'atom': 'H13A', 'charge': 0.09000000357627869, 'distance': 26.42348861694336, 'force': [-0.0357477068901062, -0.020964404568076134, 0.010680285282433033], 'magnitude': 0.04279571771621704, 'cosine_with_motion': 0.02719710022211075, 'motion_component': 0.0011639194563031197, 'motion_component_percent': 2.719710022211075}, {'resid': 1313, 'atom': 'H13B', 'charge': 0.09000000357627869, 'distance': 25.20548439025879, 'force': [-0.03872540220618248, -0.024647096171975136, 0.010239271447062492], 'magnitude': 0.04703167825937271, 'cosine_with_motion': 0.05783113092184067, 'motion_component': 0.002719895215705037, 'motion_component_percent': 5.783113092184067}, {'resid': 1313, 'atom': 'H13R', 'charge': 0.09000000357627869, 'distance': 22.165023803710938, 'force': [-0.045816484838724136, -0.03693843632936478, -0.015343938954174519], 'magnitude': 0.06081969290971756, 'cosine_with_motion': 0.4982631504535675, 'motion_component': 0.030304212123155594, 'motion_component_percent': 49.82631504535675}, {'resid': 1313, 'atom': 'H13S', 'charge': 0.09000000357627869, 'distance': 22.807205200195312, 'force': [-0.045363206416368484, -0.03343940153717995, -0.01112090703099966], 'magnitude': 0.05744291841983795, 'cosine_with_motion': 0.44918355345726013, 'motion_component': 0.02580241486430168, 'motion_component_percent': 44.91835534572601}, {'resid': 1313, 'atom': 'H13X', 'charge': 0.09000000357627869, 'distance': 24.7167911529541, 'force': [-0.046792320907115936, -0.008217798545956612, -0.011624171398580074], 'magnitude': 0.04890986159443855, 'cosine_with_motion': 0.49674180150032043, 'motion_component': 0.024295572191476822, 'motion_component_percent': 49.67418015003204}, {'resid': 1313, 'atom': 'H13Y', 'charge': 0.09000000357627869, 'distance': 25.645816802978516, 'force': [-0.04416908696293831, -0.005449919495731592, -0.009128015488386154], 'magnitude': 0.0454305000603199, 'cosine_with_motion': 0.46106666326522827, 'motion_component': 0.02094648964703083, 'motion_component_percent': 46.10666632652283}, {'resid': 1313, 'atom': 'H141', 'charge': 0.15000000596046448, 'distance': 25.06597137451172, 'force': [-0.06171484291553497, -0.046577516943216324, -0.01743963547050953], 'magnitude': 0.07926113903522491, 'cosine_with_motion': 0.47213977575302124, 'motion_component': 0.037422336637973785, 'motion_component_percent': 47.213977575302124}, {'resid': 1313, 'atom': 'H14X', 'charge': 0.09000000357627869, 'distance': 23.714794158935547, 'force': [-0.050795335322618484, -0.004123025573790073, -0.015021935105323792], 'magnitude': 0.05313025414943695, 'cosine_with_motion': 0.5313454866409302, 'motion_component': 0.028230519965291023, 'motion_component_percent': 53.13454866409302}, {'resid': 1313, 'atom': 'H14Y', 'charge': 0.09000000357627869, 'distance': 25.023344039916992, 'force': [-0.04615321010351181, -0.0021567512303590775, -0.01192969735711813], 'magnitude': 0.047718845307826996, 'cosine_with_motion': 0.499822735786438, 'motion_component': 0.02385096438229084, 'motion_component_percent': 49.9822735786438}, {'resid': 1313, 'atom': 'H151', 'charge': 0.15000000596046448, 'distance': 25.855365753173828, 'force': [-0.05402318760752678, -0.04690302535891533, -0.020763656124472618], 'magnitude': 0.07449515163898468, 'cosine_with_motion': 0.5182983875274658, 'motion_component': 0.03861071541905403, 'motion_component_percent': 51.82983875274658}, {'resid': 1313, 'atom': 'H15X', 'charge': 0.09000000357627869, 'distance': 25.63323211669922, 'force': [-0.042694948613643646, -0.0060399919748306274, -0.014444601722061634], 'magnitude': 0.04547512158751488, 'cosine_with_motion': 0.565484881401062, 'motion_component': 0.02571549452841282, 'motion_component_percent': 56.5484881401062}, {'resid': 1313, 'atom': 'H15Y', 'charge': 0.09000000357627869, 'distance': 26.812896728515625, 'force': [-0.03960096463561058, -0.0037836600095033646, -0.01203417032957077], 'magnitude': 0.041561685502529144, 'cosine_with_motion': 0.5382915735244751, 'motion_component': 0.022372305393218994, 'motion_component_percent': 53.82915735244751}, {'resid': 1313, 'atom': 'H16R', 'charge': 0.09000000357627869, 'distance': 24.88914680480957, 'force': [-0.032903384417295456, -0.03125625476241112, -0.016340473666787148], 'magnitude': 0.048234812915325165, 'cosine_with_motion': 0.5662842392921448, 'motion_component': 0.02731461450457573, 'motion_component_percent': 56.62842392921448}, {'resid': 1313, 'atom': 'H16S', 'charge': 0.09000000357627869, 'distance': 23.263376235961914, 'force': [-0.038966450840234756, -0.03451082110404968, -0.018412137404084206], 'magnitude': 0.05521220713853836, 'cosine_with_motion': 0.5652920603752136, 'motion_component': 0.031211022287607193, 'motion_component_percent': 56.52920603752136}, {'resid': 1313, 'atom': 'H16X', 'charge': 0.09000000357627869, 'distance': 25.80626106262207, 'force': [-0.04223889485001564, -0.0008907602750696242, -0.01510501466691494], 'magnitude': 0.04486735165119171, 'cosine_with_motion': 0.573813796043396, 'motion_component': 0.025745505467057228, 'motion_component_percent': 57.3813796043396}, {'resid': 1313, 'atom': 'H16Y', 'charge': 0.09000000357627869, 'distance': 24.779163360595703, 'force': [-0.04514994099736214, -0.003236297518014908, -0.0178658626973629], 'magnitude': 0.048663947731256485, 'cosine_with_motion': 0.6038366556167603, 'motion_component': 0.029385074973106384, 'motion_component_percent': 60.383665561676025}, {'resid': 1313, 'atom': 'H17R', 'charge': 0.09000000357627869, 'distance': 22.465389251708984, 'force': [-0.040438588708639145, -0.040471211075782776, -0.015229661948978901], 'magnitude': 0.059204231947660446, 'cosine_with_motion': 0.491600900888443, 'motion_component': 0.02910485304892063, 'motion_component_percent': 49.1600900888443}, {'resid': 1313, 'atom': 'H17S', 'charge': 0.09000000357627869, 'distance': 24.21015167236328, 'force': [-0.034239307045936584, -0.035580310970544815, -0.012668912298977375], 'magnitude': 0.05097832903265953, 'cosine_with_motion': 0.48156502842903137, 'motion_component': 0.02454937994480133, 'motion_component_percent': 48.15650284290314}, {'resid': 1313, 'atom': 'H17X', 'charge': 0.09000000357627869, 'distance': 26.652952194213867, 'force': [-0.03829847276210785, -0.004701498430222273, -0.016743212938308716], 'magnitude': 0.042062003165483475, 'cosine_with_motion': 0.6332148313522339, 'motion_component': 0.026634283363819122, 'motion_component_percent': 63.32148313522339}, {'resid': 1313, 'atom': 'H17Y', 'charge': 0.09000000357627869, 'distance': 26.818923950195312, 'force': [-0.03779064118862152, -0.0018663987284526229, -0.017152419313788414], 'magnitude': 0.041543006896972656, 'cosine_with_motion': 0.6409434080123901, 'motion_component': 0.026626715436577797, 'motion_component_percent': 64.09434080123901}, {'resid': 1313, 'atom': 'H18R', 'charge': 0.09000000357627869, 'distance': 24.025501251220703, 'force': [-0.0316954106092453, -0.03701687231659889, -0.017457397654652596], 'magnitude': 0.05176493525505066, 'cosine_with_motion': 0.552656352519989, 'motion_component': 0.02860822156071663, 'motion_component_percent': 55.2656352519989}, {'resid': 1313, 'atom': 'H18S', 'charge': 0.090000003576</t>
         </is>
       </c>
     </row>
@@ -627,7 +627,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>{939: {'frame': 939, 'motion_vector': [-4.074672698974609, -0.7788047790527344, 1.4778213500976562], 'ionic_force': [6.851991251111031, 8.000294297933578, -4.192061893641949], 'ionic_force_magnitude': 11.337013534391478, 'radial_force': 10.533493862857217, 'axial_force': -4.192061893641949, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [6.12185263633728, -7.080075323581696, 1.0930774211883545], 'asn_force_magnitude': 9.423341474091446, 'residue_force': [6.12185263633728, -7.080075323581696, 1.0930774211883545], 'residue_force_magnitude': 9.423341474091446, 'total_force': [12.97384388744831, 0.9202189743518829, -3.098984472453594], 'total_force_magnitude': 13.370532260801946, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': -0.4292968054055065, 'cosine_residue_motion': -0.4292968054055065, 'cosine_ionic_motion': -0.8081052008199872, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': -4.045410391072674, 'motion_component_residue': -4.045410391072674, 'motion_component_ionic': -9.161499598908337, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 42.92968054055065, 'motion_component_percent_residue': 42.92968054055065, 'motion_component_percent_ionic': 80.81052008199872, 'ionic_contributions': [{'ion_id': 2333, 'distance': 9.940918922424316, 'force': [0.5586365461349487, 3.312108039855957, -0.06815715879201889], 'magnitude': 3.3595802783966064, 'cosine_ionic_motion': -0.33501172065734863, 'motion_component_ionic': -1.1254987716674805, 'motion_component_percent_ionic': 33.50117206573486}, {'ion_id': 2334, 'distance': 13.11501407623291, 'force': [0.7408196330070496, 0.6163527965545654, -1.6724047660827637], 'magnitude': 1.930192232131958, 'cosine_ionic_motion': -0.7023535966873169, 'motion_component_ionic': -1.3556774854660034, 'motion_component_percent_ionic': 70.23535966873169}, {'ion_id': 2343, 'distance': 7.49332857131958, 'force': [3.0116941928863525, 2.9080581665039062, -4.175325870513916], 'magnitude': 5.912736415863037, 'cosine_ionic_motion': -0.7952401041984558, 'motion_component_ionic': -4.70204496383667, 'motion_component_percent_ionic': 79.52401041984558}, {'ion_id': 2372, 'distance': 14.712966918945312, 'force': [0.21832038462162018, 0.3984614908695221, 1.4648445844650269], 'magnitude': 1.5336899757385254, 'cosine_ionic_motion': 0.14285781979560852, 'motion_component_ionic': 0.21909961104393005, 'motion_component_percent_ionic': 14.285781979560852}, {'ion_id': 2397, 'distance': 11.619467735290527, 'force': [2.3225204944610596, 0.7653138041496277, 0.258981317281723], 'magnitude': 2.4590401649475098, 'cosine_ionic_motion': -0.8935918211936951, 'motion_component_ionic': -2.197378158569336, 'motion_component_percent_ionic': 89.3591821193695}], 'glu_contributions': [], 'asn_contributions': [{'resid': 458, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 5.998406887054443, 'force': [4.847882270812988, -6.2280755043029785, -2.82234787940979], 'magnitude': 8.381916999816895, 'cosine_with_motion': -0.5167387127876282, 'motion_component': -4.331261157989502, 'motion_component_percent': 51.67387127876282}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 5.7243452072143555, 'force': [1.273970365524292, -0.851999819278717, 3.9154253005981445], 'magnitude': 4.204694747924805, 'cosine_with_motion': 0.06798364222049713, 'motion_component': 0.285850465297699, 'motion_component_percent': 6.798364222049713}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': -0.9877624714088142, 'motion_component_pip2': -13.20690998998101, 'motion_component_percent_pip2': 98.77624714088142}, 941: {'frame': 941, 'motion_vector': [4.546348571777344, 6.662361145019531, -8.480491638183594], 'ionic_force': [-16.01090270280838, -7.945226639509201, -3.352786064147949], 'ionic_force_magnitude': 18.185620861106393, 'radial_force': 17.873881271619865, 'axial_force': -3.352786064147949, 'glu_force': [-11.130061149597168, 3.2417352199554443, 2.021413668990135], 'glu_force_magnitude': 11.767464537922006, 'asn_force': [1.3882538974285126, -1.0301260948181152, 0.6585688591003418], 'asn_force_magnitude': 1.8498977261263396, 'residue_force': [-9.741807252168655, 2.211609125137329, 2.679982528090477], 'residue_force_magnitude': 10.342936227767565, 'total_force': [-25.752709954977036, -5.733617514371872, -0.6728035360574722], 'total_force_magnitude': 26.391837837187783, 'cosine_total_motion': 0, 'cosine_glu_motion': -0.3350668111411967, 'cosine_asn_motion': -0.28343760662259465, 'cosine_residue_motion': -0.4319099821901041, 'cosine_ionic_motion': -0.4571171356848527, 'motion_component_total': 0, 'motion_component_glu': -3.942886817938642, 'motion_component_asn': -0.5243305839898298, 'motion_component_residue': -4.467217401928472, 'motion_component_ionic': -8.312958918679659, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 33.506681114119665, 'motion_component_percent_asn': 28.343760662259466, 'motion_component_percent_residue': 43.19099821901041, 'motion_component_percent_ionic': 45.711713568485266, 'ionic_contributions': [{'ion_id': 2333, 'distance': 6.778547286987305, 'force': [-7.040979385375977, 1.0157924890518188, -1.26486337184906], 'magnitude': 7.225448131561279, 'cosine_ionic_motion': -0.17166294157505035, 'motion_component_ionic': -1.2403416633605957, 'motion_component_percent_ionic': 17.166294157505035}, {'ion_id': 2334, 'distance': 14.690794944763184, 'force': [-0.33608192205429077, -0.49903711676597595, -1.4157851934432983], 'magnitude': 1.5383226871490479, 'cosine_ionic_motion': 0.39734816551208496, 'motion_component_ionic': 0.6112496852874756, 'motion_component_percent_ionic': 39.734816551208496}, {'ion_id': 2343, 'distance': 11.003790855407715, 'force': [-1.0358814001083374, -1.159320592880249, -2.258540153503418], 'magnitude': 2.7419114112854004, 'cosine_ionic_motion': 0.20941640436649323, 'motion_component_ionic': 0.574201226234436, 'motion_component_percent_ionic': 20.941640436649323}, {'ion_id': 2372, 'distance': 6.887856483459473, 'force': [-3.8972530364990234, -3.206509590148926, 4.8477630615234375], 'magnitude': 6.997934818267822, 'cosine_ionic_motion': -0.9791375398635864, 'motion_component_ionic': -6.851940631866455, 'motion_component_percent_ionic': 97.91375398635864}, {'ion_id': 2397, 'distance': 7.1958441734313965, 'force': [-3.700706958770752, -4.096151828765869, -3.2613604068756104], 'magnitude': 6.4117207527160645, 'cosine_ionic_motion': -0.2193058282136917, 'motion_component_ionic': -1.406127691268921, 'motion_component_percent_ionic': 21.93058282136917}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 5.483707427978516, 'force': [8.001100540161133, -3.2710275650024414, -2.0859203338623047], 'magnitude': 8.892035484313965, 'cosine_with_motion': 0.3101078271865845, 'motion_component': 2.7574896812438965, 'motion_component_percent': 31.010782718658447}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 5.310659885406494, 'force': [-8.652483940124512, 4.243757724761963, 0.17253552377223969], 'magnitude': 9.638710021972656, 'cosine_with_motion': -0.11104666441679001, 'motion_component': -1.0703465938568115, 'motion_component_percent': 11.104666441679}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 4.878771781921387, 'force': [-10.478677749633789, 2.269005060195923, 3.9347984790802], 'magnitude': 11.420758247375488, 'cosine_with_motion': -0.49296465516090393, 'motion_component': -5.630030155181885, 'motion_component_percent': 49.29646551609039}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 5.763005256652832, 'force': [1.0724196434020996, -4.680352687835693, 5.298296928405762], 'magnitude': 7.150366306304932, 'cosine_with_motion': -0.8512700200080872, 'motion_component': -6.086892604827881, 'motion_component_percent': 85.12700200080872}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 5.809535980224609, 'force': [0.31583425402641296, 3.650226593017578, -4.63972806930542], 'magnitude': 5.911935329437256, 'cosine_with_motion': 0.9409037232398987, 'motion_component': 5.562561988830566, 'motion_component_percent': 94.09037232398987}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': -0.484247304013063, 'motion_component_pip2': -12.780176320608131, 'motion_component_percent_pip2': 48.4247304013063}, 942: {'frame': 942, 'motion_vector': [1.8070106506347656, -2.3379135131835938, 12.137763977050781], 'ionic_force': [1.4651539772748947, 1.3210062682628632, -4.856406569480896], 'ionic_force_magnitude': 5.241795351405034, 'radial_force': 1.9727477633783337, 'axial_force': -4.856406569480896, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-6.971011847257614, 8.266367197036743, 10.463233470916748], 'asn_force_magnitude': 15.04682981487342, 'residue_force': [-6.971011847257614, 8.266367197036743, 10.463233470916748], 'residue_force_magnitude': 15.04682981487342, 'total_force': [-5.505857869982719, 9.587373465299606, 5.606826901435852], 'total_force_magnitude': 12.396318354666693, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': 0.5058153030156746, 'cosine_residue_motion': 0.5058153030156746, 'cosine_ionic_motion': -0.9069195619929794, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': 7.610916782235485, 'motion_component_residue': 7.610916782235485, 'motion_component_ionic': -4.753886744153089, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 50.581530301567454, 'motion_component_percent_residue': 50.581530301567454, 'motion_component_percent_ionic': 90.69195619929793, 'ionic_contributions': [{'ion_id': 2223, 'distance': 14.830791473388672, 'force': [-0.24479390680789948, 0.4347176253795624, 1.4245835542678833], 'magnitude': 1.5094176530838013, 'cosine_ionic_motion': 0.8396561145782471, 'motion_component_ionic': 1.2673918008804321, 'motion_component_percent_ionic': 83.9656114578247}, {'ion_id': 2333, 'distance': 14.580857276916504, 'force': [-0.5634464621543884, 0.8605449795722961, -1.1749935150146484], 'magnitude': 1.5616079568862915, 'cosine_ionic_motion': -0.8863965272903442, 'motion_component_ionic': -1.3842039108276367, 'motion_component_percent_ionic': 88.63965272903442}, {'ion_id': 2372, 'distance': 12.797574996948242, 'force': [1.0505107641220093, 0.7881307601928711, -1.5441999435424805], 'magnitude': 2.027134895324707, 'cosine_ionic_motion': -0.7379485964775085, 'motion_component_ionic': -1.4959213733673096, 'motion_component_percent_ionic': 73.79485964775085}, {'ion_id': 2397, 'distance': 9.295544624328613, 'force': [1.2228835821151733, -0.7623870968818665, -3.5617966651916504], 'magnitude': 3.8422746658325195, 'cosine_ionic_motion': -0.8175244331359863, 'motion_component_ionic': -3.141153335571289, 'motion_component_percent_ionic': 81.75244331359863}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 5.621132850646973, 'force': [-4.571839809417725, -3.430217981338501, 2.685060501098633], 'magnitude': 6.314876556396484, 'cosine_with_motion': 0.41006505489349365, 'motion_component': 2.589510202407837, 'motion_component_percent': 41.006505489349365}, {'resid': 786, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 3.8380484580993652, 'force': [-0.35663309693336487, -10.945160865783691, -11.83127212524414], 'magnitude': 16.12150001525879, 'cosine_with_motion': -0.58919757604599, 'motion_component': -9.498748779296875, 'motion_component_percent': 58.919757604599}, {'resid': 786, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 2.74065899848938, 'force': [-1.4760031700134277, 20.094148635864258, 17.31248664855957], 'magnitude': 26.564556121826172, 'cosine_with_motion': 0.4836183786392212, 'motion_component': 12.847107887268066, 'motion_component_percent': 48.36183786392212}, {'resid': 786, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 4.422964096069336, 'force': [2.9860057830810547, 7.733495712280273, 12.998003959655762], 'magnitude': 15.41659164428711, 'cosine_with_motion': 0.7533293962478638, 'motion_component': 11.613771438598633, 'motion_component_percent': 75.33293962478638}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 4.204389572143555, 'force': [-2.886963367462158, -2.784243583679199, -6.683220386505127], 'magnitude': 7.7943572998046875, 'cosine_with_motion': -0.8198370933532715, 'motion_component': -6.390103340148926, 'motion_component_percent': 81.98370933532715}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 5.3982744216918945, 'force': [-0.6655781865119934, -2.4016547203063965, -4.017825126647949], 'magnitude': 4.727986812591553, 'cosine_with_motion': -0.7509793639183044, 'motion_component': -3.5506205558776855, 'motion_component_percent': 75.09793639183044}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': 0.2304740775721402, 'motion_component_pip2': 2.8570300380823968, 'motion_component_percent_pip2': 23.04740775721402}, 944: {'frame': 944, 'motion_vector': [-1.093109130859375, -4.443397521972656, -2.5691909790039062], 'ionic_force': [10.705962538719177, -0.14524871110916138, -2.504377245903015], 'ionic_force_magnitude': 10.995937270571073, 'radial_force': 10.706947794237966, 'axial_force': -2.504377245903015, 'glu_force': [7.598659038543701, 2.049821436405182, -0.012096736580133438], 'glu_force_magnitude': 7.870294367825385, 'asn_force': [-0.6847988367080688, -4.282110929489136, -6.883615970611572], 'asn_force_magnitude': 8.135698635646833, 'residue_force': [6.913860201835632, -2.232289493083954, -6.895712707191706], 'residue_force_magnitude': 10.01675760970509, 'total_force': [17.61982274055481, -2.3775382041931152, -9.40008995309472], 'total_force_magnitude': 20.111502491043343, 'cosine_total_motion': 0, 'cosine_glu_motion': -0.42088438353902685, 'cosine_asn_motion': 0.8774193880616797, 'cosine_residue_motion': 0.38195350972291986, 'cosine_ionic_motion': -0.08011793219755858, 'motion_component_total': 0, 'motion_component_glu': -3.312483993272862, 'motion_component_asn': 7.138419718343487, 'motion_component_residue': 3.8259357250706247, 'motion_component_ionic': -0.8809717566922206, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 42.08843835390269, 'motion_component_percent_asn': 87.74193880616798, 'motion_component_percent_residue': 38.19535097229198, 'motion_component_percent_ionic': 8.011793219755859, 'ionic_contributions': [{'ion_id': 2333, 'distance': 13.44190502166748, 'force': [0.40863609313964844, 0.444547563791275, 1.7354049682617188], 'magnitude': 1.8374537229537964, 'cosine_ionic_motion': -0.7135604619979858, 'motion_component_ionic': -1.3111343383789062, 'motion_component_percent_ionic': 71.35604619979858}, {'ion_id': 2334, 'distance': 12.843454360961914, 'force': [1.1176952123641968, 0.2648090422153473, -1.652727484703064], 'magnitude': 2.012678384780884, 'cosine_ionic_motion': 0.17494170367717743, 'motion_component_ionic': 0.3521013855934143, 'motion_component_percent_ionic': 17.494170367717743}, {'ion_id': 2343, 'distance': 8.127030372619629, 'force': [3.9056527614593506, 0.6693278551101685, -3.092665910720825], 'magnitude': 5.026599884033203, 'cosine_ionic_motion': 0.026622144505381584, 'motion_component_ionic': 0.1338188648223877, 'motion_component_percent_ionic': 2.6622144505381584}, {'ion_id': 2372, 'distance': 13.263224601745605, 'force': [1.6295294761657715, 0.9496340751647949, 0.06864747405052185], 'magnitude': 1.8872953653335571, 'cosine_ionic_motion': -0.6237004995346069, 'motion_component_ionic': -1.1771070957183838, 'motion_component_percent_ionic': 62.37004995346069}, {'ion_id': 2397, 'distance': 8.660684585571289, 'force': [3.64444899559021, -2.473567247390747, 0.4369637072086334], 'magnitude': 4.426226615905762, 'cosine_ionic_motion': 0.2533420920372009, 'motion_component_ionic': 1.1213494539260864, 'motion_component_percent_ionic': 25.334209203720093}], 'glu_contributions': [{'resid': 426, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 5.3482513427734375, 'force': [-9.051460266113281, -1.040523886680603, -2.091996192932129], 'magnitude': 9.348158836364746, 'cosine_with_motion': 0.4054940342903137, 'motion_component': 3.7906227111816406, 'motion_component_percent': 40.54940342903137}, {'resid': 426, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 5.9007887840271, 'force': [7.1462321281433105, 2.320293664932251, 2.121345281600952], 'magnitude': 7.80720853805542, 'cosine_with_motion': -0.57533198595047, 'motion_component': -4.491736888885498, 'motion_component_percent': 57.533198595047}, {'resid': 426, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 5.339428901672363, 'force': [9.503887176513672, 0.7700516581535339, -0.04144582524895668], 'magnitude': 9.535122871398926, 'cosine_with_motion': -0.27386850118637085, 'motion_component': -2.6113698482513428, 'motion_component_percent': 27.386850118637085}], 'asn_contributions': [{'resid': 458, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 5.357764720916748, 'force': [-0.899056077003479, 3.345669746398926, 7.512620449066162], 'magnitude': 8.272923469543457, 'cosine_with_motion': -0.7643670439720154, 'motion_component': -6.323550224304199, 'motion_component_percent': 76.43670439720154}, {'resid': 458, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 4.971437931060791, 'force': [-0.8431729078292847, -2.605689764022827, -7.5945281982421875], 'magnitude': 8.07325267791748, 'cosine_with_motion': 0.7555815577507019, 'motion_component': 6.100000858306885, 'motion_component_percent': 75.55815577507019}, {'resid': 458, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 5.949346542358398, 'force': [1.0574301481246948, -5.022090911865234, -6.801708221435547], 'magnitude': 8.520727157592773, 'cosine_with_motion': 0.8640071153640747, 'motion_component': 7.361968994140625, 'motion_component_percent': 86.40071153640747}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': 0.14643182276858452, 'motion_component_pip2': 2.9449639683784046, 'motion_component_percent_pip2': 14.643182276858452}, 945: {'frame': 945, 'motion_vector': [-0.9502105712890625, -3.343677520751953, 2.6476211547851562], 'ionic_force': [12.936512351036072, -18.47074380517006, -5.592387393116951], 'ionic_force_magnitude': 23.233521585834342, 'radial_force': 22.550426349067926, 'axial_force': -5.592387393116951, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [3.519810199737549, 7.553614020347595, -10.368144989013672], 'asn_force_magnitude': 13.302051688509467, 'residue_force': [3.519810199737549, 7.553614020347595, -10.368144989013672], 'residue_force_magnitude': 13.302051688509467, 'total_force': [16.45632255077362, -10.917129784822464, -15.960532382130623], 'total_force_magnitude': 25.39159050856796, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': -0.9643578355755451, 'cosine_residue_motion': -0.9643578355755451, 'cosine_ionic_motion': 0.34142293019608333, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': -12.827937775045015, 'motion_component_residue': -12.827937775045015, 'motion_component_ionic': 7.932457018609513, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 96.43578355755452, 'motion_component_percent_residue': 96.43578355755452, 'motion_component_percent_ionic': 34.14229301960833, 'ionic_contributions': [{'ion_id': 2333, 'distance': 4.540952205657959, 'force': [5.747335910797119, -15.038304328918457, -0.22236128151416779], 'magnitude': 16.10068130493164, 'cosine_ionic_motion': 0.6287363767623901, 'motion_component_ionic': 10.12308406829834, 'motion_component_percent_ionic': 62.873637676239014}, {'ion_id': 2334, 'distance': 14.638409614562988, 'force': [0.659042239189148, -0.2530182898044586, -1.3791804313659668], 'magnitude': 1.5493526458740234, 'cosine_ionic_motion': -0.5069094300270081, 'motion_component_ionic': -0.7853814959526062, 'motion_component_percent_ionic': 50.690943002700806}, {'ion_id': 2343, 'distance': 8.974699020385742, 'force': [2.517314910888672, -1.1983013153076172, -3.0360047817230225], 'magnitude': 4.121908187866211, 'cosine_ionic_motion': -0.35664188861846924, 'motion_component_ionic': -1.4700450897216797, 'motion_component_percent_ionic': 35.664188861846924}, {'ion_id': 2372, 'distance': 11.224454879760742, 'force': [2.5090982913970947, 0.6923329830169678, -0.4113236665725708], 'magnitude': 2.6351633071899414, 'cosine_ionic_motion': -0.5026834607124329, 'motion_component_ionic': -1.3246530294418335, 'motion_component_percent_ionic': 50.268346071243286}, {'ion_id': 2397, 'distance': 10.323620796203613, 'force': [1.503720998764038, -2.673452854156494, -0.5435172319412231], 'magnitude': 3.115114450454712, 'cosine_ionic_motion': 0.44603583216667175, 'motion_component_ionic': 1.3894526958465576, 'motion_component_percent_ionic': 44.603583216667175}], 'glu_contributions': [], 'asn_contributions': [{'resid': 458, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 3.5457613468170166, 'force': [-14.692557334899902, -6.301402568817139, 10.06045150756836], 'magnitude': 18.888927459716797, 'cosine_with_motion': 0.7471532821655273, 'motion_component': 14.112924575805664, 'motion_component_percent': 74.71532821655273}, {'resid': 458, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 2.735792398452759, 'force': [15.180482864379883, 11.374526023864746, -18.73188018798828], 'magnitude': 26.659149169921875, 'cosine_with_motion': -0.8760719895362854, 'motion_component': -23.35533332824707, 'motion_component_percent': 87.60719895362854}, {'resid': 458, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 3.938117742538452, 'force': [17.225242614746094, 0.4772137403488159, -9.012396812438965], 'magnitude': 19.44633674621582, 'cosine_with_motion': -0.4922184646129608, 'motion_component': -9.571846008300781, 'motion_component_percent': 49.22184646129608}, {'resid': 458, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 3.6525635719299316, 'force': [-8.630203247070312, 2.3025553226470947, 5.183899402618408], 'magnitude': 10.32738971710205, 'cosine_with_motion': 0.31526151299476624, 'motion_component': 3.255828619003296, 'motion_component_percent': 31.526151299476624}, {'resid': 458, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 4.805994033813477, 'force': [-5.563154697418213, -0.29927849769592285, 2.1317811012268066], 'magnitude': 5.965127468109131, 'cosine_with_motion': 0.4577418267726898, 'motion_component': 2.7304883003234863, 'motion_component_percent': 45.77418267726898}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': -0.19279929529359752, 'motion_component_pip2': -4.895480756435502, 'motion_component_percent_pip2': 19.27992952935975}, 946: {'frame': 946, 'motion_vector': [-0.46352386474609375, 6.322200775146484, -12.438140869140625], 'ionic_force': [9.601044237613678, -11.661227107048035, -1.7264618799090385], 'ionic_force_magnitude': 15.203451539619078, 'radial_force': 15.105107351315537, 'axial_force': -1.7264618799090385, 'glu_force': [8.861327886581421, -22.45647621154785, 0.6762290000915527], 'glu_force_magnitude': 24.15106087553681, 'asn_force': [-2.4940197095274925, -0.9710111618041992, 7.1500608921051025], 'asn_force_magnitude': 7.6345509199081745, 'residue_force': [6.367308177053928, -23.42748737335205, 7.826289892196655], 'residue_force_magnitude': 25.507657507635763, 'total_force': [15.968352414667606, -35.088714480400085, 6.099828012287617], 'total_force_magnitude': 39.0309372742386, 'cosine_total_motion': 0, 'cosine_glu_motion': -0.4582205836752819, 'cosine_asn_motion': -0.8811710557149747, 'cosine_residue_motion': -0.6975888906868197, 'cosine_ionic_motion': -0.2671472464111686, 'motion_component_total': 0, 'motion_component_glu': -11.066513210765741, 'motion_component_asn': -6.727345294005217, 'motion_component_residue': -17.79385850477096, 'motion_component_ionic': -4.061560214754879, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 45.82205836752819, 'motion_component_percent_asn': 88.11710557149746, 'motion_component_percent_residue': 69.75888906868197, 'motion_component_percent_ionic': 26.71472464111686, 'ionic_contributions': [{'ion_id': 2333, 'distance': 6.537381649017334, 'force': [2.106290102005005, -7.2145795822143555, 1.9649690389633179], 'magnitude': 7.7683796882629395, 'cosine_ionic_motion': -0.6549484729766846, 'motion_component_ionic': -5.087888240814209, 'motion_component_percent_ionic': 65.49484729766846}, {'ion_id': 2334, 'distance': 13.697625160217285, 'force': [0.7078378796577454, -0.7629865407943726, -1.4310498237609863], 'magnitude': 1.7694876194000244, 'cosine_ionic_motion': 0.5119978189468384, 'motion_component_ionic': 0.9059737920761108, 'motion_component_percent_ionic': 51.19978189468384}, {'ion_id': 2343, 'distance': 9.615497589111328, 'force': [1.8219869136810303, -2.31147837638855, -2.0570547580718994], 'magnitude': 3.590827703475952, 'cosine_ionic_motion': 0.20203277468681335, 'motion_component_ionic': 0.7254648804664612, 'motion_component_percent_ionic': 20.203277468681335}, {'ion_id': 2372, 'distance': 8.875093460083008, 'force': [4.204627513885498, 0.15687620639801025, -0.24956493079662323], 'magnitude': 4.214947700500488, 'cosine_ionic_motion': 0.03648703545331955, 'motion_component_ionic': 0.15379095077514648, 'motion_component_percent_ionic': 3.648703545331955}, {'ion_id': 2397, 'distance': 13.940861701965332, 'force': [0.7603018283843994, -1.529058814048767, 0.04623859375715256], 'magnitude': 1.7082791328430176, 'cosine_ionic_motion': -0.4442490339279175, 'motion_component_ionic': -0.7589013576507568, 'motion_component_percent_ionic': 44.42490339279175}], 'glu_contributions': [{'resid': 1082, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 3.428219795227051, 'force': [-3.492716073989868, 21.762147903442383, -5.643251895904541], 'magnitude': 22.751625061035156, 'cosine_with_motion': 0.659260094165802, 'motion_component': 14.999238014221191, 'motion_component_percent': 65.9260094165802}, {'resid': 1082, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 3.1431379318237305, 'force': [3.670413017272949, -27.068212509155273, -3.314085006713867], 'magnitude': 27.5162353515625, 'cosine_with_motion': -0.3426142930984497, 'motion_component': -9.42745590209961, 'motion_component_percent': 34.26142930984497}, {'resid': 1082, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 3.5556235313415527, 'force': [8.68363094329834, -17.15041160583496, 9.633565902709961], 'magnitude': 21.50227165222168, 'cosine_with_motion': -0.7737925052642822, 'motion_component': -16.638296127319336, 'motion_component_percent': 77.37925052642822}], 'asn_contributions': [{'resid': 458, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 5.823520183563232, 'force': [-1.3654035329818726, -2.7797718048095703, 2.6294658184051514], 'magnitude': 4.062702178955078, 'cosine_with_motion': -0.8753482699394226, 'motion_component': -3.556279420852661, 'motion_component_percent': 87.53482699394226}, {'resid': 1114, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 5.307500839233398, 'force': [2.2005362510681152, 4.164884090423584, 6.991591453552246], 'magnitude': 8.430359840393066, 'cosine_with_motion': -0.5238388180732727, 'motion_component': -4.416149616241455, 'motion_component_percent': 52.38388180732727}, {'resid': 1114, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 5.613898754119873, 'force': [-2.411193609237671, -3.8650875091552734, -4.396687030792236], 'magnitude': 6.331161975860596, 'cosine_with_motion': 0.354904443025589, 'motion_component': 2.246957540512085, 'motion_component_percent': 35.4904443025589}, {'resid': 1114, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 4.150711536407471, 'force': [-2.8417885303497314, -7.533817291259766, -15.543556213378906], 'magnitude': 17.505321502685547, 'cosine_with_motion': 0.6016008853912354, 'motion_component': 10.531216621398926, 'motion_component_percent': 60.160088539123535}, {'resid': 1114, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 3.331644296646118, 'force': [1.8260784149169922, 7.0495405197143555, 10.052186012268066], 'magnitude': 12.412776947021484, 'cosine_with_motion': -0.4692114293575287, 'motion_component': -5.824216842651367, 'motion_component_percent': 46.92114293575287}, {'resid': 1114, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 4.2353434562683105, 'force': [0.09775129705667496, 1.9932408332824707, 7.417060852050781], 'magnitude': 7.680843353271484, 'cosine_with_motion': -0.7432612776756287, 'motion_component': -5.708873271942139, 'motion_component_percent': 74.32612776756287}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': -0.5599511629957952, 'motion_component_pip2': -21.855418719525836, 'motion_component_percent_pip2': 55.995116299579514}}</t>
+          <t>{939: {'frame': 939, 'motion_vector': [-4.074672698974609, -0.7788047790527344, 1.4778213500976562], 'ionic_force': [6.851991251111031, 8.000294297933578, -4.192061893641949], 'ionic_force_magnitude': 11.337013534391478, 'radial_force': 10.533493862857217, 'axial_force': -4.192061893641949, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [6.12185263633728, -7.080075323581696, 1.0930774211883545], 'asn_force_magnitude': 9.423341474091446, 'residue_force': [6.12185263633728, -7.080075323581696, 1.0930774211883545], 'residue_force_magnitude': 9.423341474091446, 'pip2_force': [0.6937301754951477, -0.07981214637402445, -4.579628557604792], 'pip2_force_magnitude': 4.63256184640105, 'total_force': [13.667574062943459, 0.8404068279778585, -7.678613030058386], 'total_force_magnitude': 15.699361849066955, 'cosine_total_motion': -0.9791164881546054, 'cosine_glu_motion': 0, 'cosine_asn_motion': -0.4292968054055065, 'cosine_residue_motion': -0.4292968054055065, 'cosine_pip2_motion': -0.46725637384149626, 'cosine_ionic_motion': -0.8081052008199872, 'motion_component_total': -15.37150403992683, 'motion_component_glu': 0, 'motion_component_asn': -4.045410391072674, 'motion_component_residue': -4.045410391072674, 'motion_component_ionic': -9.161499598908337, 'motion_component_pip2': -2.164594049945821, 'motion_component_percent_total': 97.91164881546054, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 42.92968054055065, 'motion_component_percent_residue': 42.92968054055065, 'motion_component_percent_ionic': 80.81052008199872, 'motion_component_percent_pip2': 46.72563738414963, 'ionic_contributions': [{'ion_id': 2333, 'distance': 9.940918922424316, 'force': [0.5586365461349487, 3.312108039855957, -0.06815715879201889], 'magnitude': 3.3595802783966064, 'cosine_ionic_motion': -0.33501172065734863, 'motion_component_ionic': -1.1254987716674805, 'motion_component_percent_ionic': 33.50117206573486}, {'ion_id': 2334, 'distance': 13.11501407623291, 'force': [0.7408196330070496, 0.6163527965545654, -1.6724047660827637], 'magnitude': 1.930192232131958, 'cosine_ionic_motion': -0.7023535966873169, 'motion_component_ionic': -1.3556774854660034, 'motion_component_percent_ionic': 70.23535966873169}, {'ion_id': 2343, 'distance': 7.49332857131958, 'force': [3.0116941928863525, 2.9080581665039062, -4.175325870513916], 'magnitude': 5.912736415863037, 'cosine_ionic_motion': -0.7952401041984558, 'motion_component_ionic': -4.70204496383667, 'motion_component_percent_ionic': 79.52401041984558}, {'ion_id': 2372, 'distance': 14.712966918945312, 'force': [0.21832038462162018, 0.3984614908695221, 1.4648445844650269], 'magnitude': 1.5336899757385254, 'cosine_ionic_motion': 0.14285781979560852, 'motion_component_ionic': 0.21909961104393005, 'motion_component_percent_ionic': 14.285781979560852}, {'ion_id': 2397, 'distance': 11.619467735290527, 'force': [2.3225204944610596, 0.7653138041496277, 0.258981317281723], 'magnitude': 2.4590401649475098, 'cosine_ionic_motion': -0.8935918211936951, 'motion_component_ionic': -2.197378158569336, 'motion_component_percent_ionic': 89.3591821193695}], 'glu_contributions': [], 'asn_contributions': [{'resid': 458, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 5.998406887054443, 'force': [4.847882270812988, -6.2280755043029785, -2.82234787940979], 'magnitude': 8.381916999816895, 'cosine_with_motion': -0.5167387127876282, 'motion_component': -4.331261157989502, 'motion_component_percent': 51.67387127876282}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 5.7243452072143555, 'force': [1.273970365524292, -0.851999819278717, 3.9154253005981445], 'magnitude': 4.204694747924805, 'cosine_with_motion': 0.06798364222049713, 'motion_component': 0.285850465297699, 'motion_component_percent': 6.798364222049713}], 'pip2_contributions': [{'resid': 1313, 'atom': 'C1', 'charge': 0.06000000238418579, 'distance': 24.639312744140625, 'force': [-0.020335327833890915, -0.014827649109065533, 0.021053263917565346], 'magnitude': 0.032811958342790604, 'cosine_with_motion': 0.8686710596084595, 'motion_component': 0.028502799570560455, 'motion_component_percent': 86.86710596084595}, {'resid': 1313, 'atom': 'C11', 'charge': 0.17000000178813934, 'distance': 23.087688446044922, 'force': [-0.07590331137180328, -0.04445202648639679, 0.0589398518204689], 'magnitude': 0.10588296502828598, 'cosine_with_motion': 0.9243295192718506, 'motion_component': 0.09787075221538544, 'motion_component_percent': 92.43295192718506}, {'resid': 1313, 'atom': 'C12', 'charge': 0.04000000283122063, 'distance': 22.739980697631836, 'force': [-0.01948999986052513, -0.010492898523807526, 0.013021943159401417], 'magnitude': 0.025681355968117714, 'cosine_with_motion': 0.9446119070053101, 'motion_component': 0.024258915334939957, 'motion_component_percent': 94.461190700531}, {'resid': 1313, 'atom': 'C13', 'charge': -0.05000000074505806, 'distance': 23.34505844116211, 'force': [0.02330896630883217, 0.013698745518922806, -0.014028468169271946], 'magnitude': 0.030459176748991013, 'cosine_with_motion': -0.942152202129364, 'motion_component': -0.02869717963039875, 'motion_component_percent': 94.2152202129364}, {'resid': 1313, 'atom': 'C2', 'charge': 0.06000000238418579, 'distance': 26.224149703979492, 'force': [-0.018320659175515175, -0.013162858784198761, 0.018169039860367775], 'magnitude': 0.028965866193175316, 'cosine_with_motion': 0.8760794997215271, 'motion_component': 0.025376401841640472, 'motion_component_percent': 87.60794997215271}, {'resid': 1313, 'atom': 'C21', 'charge': 0.6299999952316284, 'distance': 20.92860221862793, 'force': [-0.37244027853012085, -0.1659366488456726, 0.24856694042682648], 'magnitude': 0.4775272309780121, 'cosine_with_motion': 0.9577770233154297, 'motion_component': 0.45736461877822876, 'motion_component_percent': 95.77770233154297}, {'resid': 1313, 'atom': 'C210', 'charge': -0.18000000715255737, 'distance': 21.98310089111328, 'force': [0.09677869826555252, 0.06851125508546829, -0.03510170057415962], 'magnitude': 0.12366098165512085, 'cosine_with_motion': -0.9173567295074463, 'motion_component': -0.11344123631715775, 'motion_component_percent': 91.73567295074463}, {'resid': 1313, 'atom': 'C211', 'charge': -0.15000000596046448, 'distance': 23.416135787963867, 'force': [0.07012628763914108, 0.05175080895423889, -0.025555647909641266], 'magnitude': 0.09082364290952682, 'cosine_with_motion': -0.909600555896759, 'motion_component': -0.08261323720216751, 'motion_component_percent': 90.9600555896759}, {'resid': 1313, 'atom': 'C212', 'charge': -0.15000000596046448, 'distance': 23.9794864654541, 'force': [0.06633873283863068, 0.05173797905445099, -0.020567188039422035], 'magnitude': 0.08660632371902466, 'cosine_with_motion': -0.8940739631652832, 'motion_component': -0.07743246108293533, 'motion_component_percent': 89.40739631652832}, {'resid': 1313, 'atom': 'C213', 'charge': -0.18000000715255737, 'distance': 23.289011001586914, 'force': [0.08406686782836914, 0.06830301135778427, -0.020184490829706192], 'magnitude': 0.11018145829439163, 'cosine_with_motion': -0.8770688772201538, 'motion_component': -0.09663672745227814, 'motion_component_percent': 87.70688772201538}, {'resid': 1313, 'atom': 'C214', 'charge': -0.15000000596046448, 'distance': 24.309247970581055, 'force': [0.0626591369509697, 0.05487443134188652, -0.012825705111026764], 'magnitude': 0.0842725858092308, 'cosine_with_motion': -0.8541883826255798, 'motion_component': -0.07198466360569, 'motion_component_percent': 85.41883826255798}, {'resid': 1313, 'atom': 'C215', 'charge': -0.15000000596046448, 'distance': 24.18225860595703, 'force': [0.06265537440776825, 0.05702746659517288, -0.008625385351479053], 'magnitude': 0.08515999466180801, 'cosine_with_motion': -0.8331659436225891, 'motion_component': -0.070952408015728, 'motion_component_percent': 83.31659436225891}, {'resid': 1313, 'atom': 'C216', 'charge': -0.18000000715255737, 'distance': 23.130308151245117, 'force': [0.08315408229827881, 0.07427938282489777, -0.006674831733107567], 'magnitude': 0.11169862002134323, 'cosine_with_motion': -0.8264696598052979, 'motion_component': -0.09231551736593246, 'motion_component_percent': 82.64696598052979}, {'resid': 1313, 'atom': 'C217', 'charge': -0.18000000715255737, 'distance': 23.19447135925293, 'force': [0.07966838777065277, 0.07740402221679688, -0.0008127559558488429], 'magnitude': 0.11108148097991943, 'cosine_with_motion': -0.78929203748703, 'motion_component': -0.08767572790384293, 'motion_component_percent': 78.929203748703}, {'resid': 1313, 'atom': 'C218', 'charge': -0.18000000715255737, 'distance': 22.543895721435547, 'force': [0.0857994481921196, 0.08021186292171478, 0.005549025721848011], 'magnitude': 0.1175852045416832, 'cosine_with_motion': -0.7799472212791443, 'motion_component': -0.09171025454998016, 'motion_component_percent': 77.99472212791443}, {'resid': 1313, 'atom': 'C219', 'charge': -0.18000000715255737, 'distance': 21.019975662231445, 'force': [0.09819309413433075, 0.09277896583080292, 0.006594967097043991], 'magnitude': 0.13525277376174927, 'cosine_with_motion': -0.7766873240470886, 'motion_component': -0.10504911094903946, 'motion_component_percent': 77.66873240470886}, {'resid': 1313, 'atom': 'C22', 'charge': -0.08000000566244125, 'distance': 19.36884117126465, 'force': [0.05585312098264694, 0.024307815358042717, -0.03608202189207077], 'magnitude': 0.07079797238111496, 'cosine_with_motion': -0.9616940021514893, 'motion_component': -0.06808598339557648, 'motion_component_percent': 96.16940021514893}, {'resid': 1313, 'atom': 'C220', 'charge': -0.27000001072883606, 'distance': 20.462318420410156, 'force': [0.15678946673870087, 0.14359845221042633, 0.025103580206632614], 'magnitude': 0.21408793330192566, 'cosine_with_motion': -0.7568964958190918, 'motion_component': -0.16204240918159485, 'motion_component_percent': 75.68964958190918}, {'resid': 1313, 'atom': 'C23', 'charge': -0.18000000715255737, 'distance': 19.14923667907715, 'force': [0.1360931694507599, 0.05079604312777519, -0.07387581467628479], 'magnitude': 0.16297000646591187, 'cosine_with_motion': -0.9799124002456665, 'motion_component': -0.1596963256597519, 'motion_component_percent': 97.99124002456665}, {'resid': 1313, 'atom': 'C24', 'charge': -0.18000000715255737, 'distance': 19.071264266967773, 'force': [0.13982678949832916, 0.057948172092437744, -0.06392747908830643], 'magnitude': 0.16430534422397614, 'cosine_with_motion': -0.9803534150123596, 'motion_component': -0.16107730567455292, 'motion_component_percent': 98.03534150123596}, {'resid': 1313, 'atom': 'C25', 'charge': -0.15000000596046448, 'distance': 17.86975860595703, 'force': [0.13029135763645172, 0.06276167184114456, -0.058363333344459534], 'magnitude': 0.15595237910747528, 'cosine_with_motion': -0.9697740077972412, 'motion_component': -0.1512385606765747, 'motion_component_percent': 96.97740077972412}, {'resid': 1313, 'atom': 'C26', 'charge': -0.15000000596046448, 'distance': 18.004230499267578, 'force': [0.12548945844173431, 0.07146970182657242, -0.05241288244724274], 'magnitude': 0.15363147854804993, 'cosine_with_motion': -0.9525306820869446, 'motion_component': -0.14633870124816895, 'motion_component_percent': 95.25306820869446}, {'resid': 1313, 'atom': 'C27', 'charge': -0.18000000715255737, 'distance': 19.369293212890625, 'force': [0.12989914417266846, 0.0777636468410492, -0.04951459541916847], 'magnitude': 0.15928800404071808, 'cosine_with_motion': -0.9452016949653625, 'motion_component': -0.15055929124355316, 'motion_component_percent': 94.52016949653625}, {'resid': 1313, 'atom': 'C28', 'charge': -0.15000000596046448, 'distance': 20.29339027404785, 'force': [0.09487087279558182, 0.06107473373413086, -0.043503113090991974], 'magnitude': 0.12092611938714981, 'cosine_with_motion': -0.9359449744224548, 'motion_component': -0.11318019032478333, 'motion_component_percent': 93.59449744224548}, {'resid': 1313, 'atom': 'C29', 'charge': -0.15000000596046448, 'distance': 21.375568389892578, 'force': [0.08405409753322601, 0.05839860811829567, -0.03746642917394638], 'magnitude': 0.108991838991642, 'cosine_with_motion': -0.9236726760864258, 'motion_component': -0.10067278146743774, 'motion_component_percent': 92.36726760864258}, {'resid': 1313, 'atom': 'C3', 'charge': 0.06000000238418579, 'distance': 27.02078628540039, 'force': [-0.017152510583400726, -0.011391998268663883, 0.0178991686552763], 'magnitude': 0.02728307992219925, 'cosine_with_motion': 0.8757008910179138, 'motion_component': 0.023891817778348923, 'motion_component_percent': 87.57008910179138}, {'resid': 1313, 'atom': 'C31', 'charge': 0.6299999952316284, 'distance': 23.81771469116211, 'force': [-0.30059126019477844, -0.1625380516052246, 0.13845324516296387], 'magnitude': 0.36870452761650085, 'cosine_with_motion': 0.9583080410957336, 'motion_component': 0.35333251953125, 'motion_component_percent': 95.83080410957336}, {'resid': 1313, 'atom': 'C310', 'charge': -0.18000000715255737, 'distance': 20.125701904296875, 'force': [0.14504267275333405, 0.018797073513269424, -0.019422093406319618], 'magnitude': 0.14753957092761993, 'cosine_with_motion': -0.9763109087944031, 'motion_component': -0.14404448866844177, 'motion_component_percent': 97.63109087944031}, {'resid': 1313, 'atom': 'C311', 'charge': -0.18000000715255737, 'distance': 20.057025909423828, 'force': [0.14667262136936188, 0.021990176290273666, -0.008436302654445171], 'magnitude': 0.14855165779590607, 'cosine_with_motion': -0.9587959051132202, 'motion_component': -0.14243072271347046, 'motion_component_percent': 95.87959051132202}, {'resid': 1313, 'atom': 'C312', 'charge': -0.18000000715255737, 'distance': 20.668659210205078, 'force': [0.13923394680023193, 0.013496112078428268, -0.000954567629378289], 'magnitude': 0.13988977670669556, 'cosine_with_motion': -0.9402768015861511, 'motion_component': -0.1315351128578186, 'motion_component_percent': 94.02768015861511}, {'resid': 1313, 'atom': 'C313', 'charge': -0.18000000715255737, 'distance': 21.046314239501953, 'force': [0.13481798768043518, 0.003995935898274183, -0.003170651849359274], 'magnitude': 0.13491445779800415, 'cosine_with_motion': -0.9377257823944092, 'motion_component': -0.12651276588439941, 'motion_component_percent': 93.77257823944092}, {'resid': 1313, 'atom': 'C314', 'charge': -0.18000000715255737, 'distance': 21.7316951751709, 'force': [0.12645623087882996, -0.0005960842245258391, 0.0045289164409041405], 'magnitude': 0.1265387088060379, 'cosine_with_motion': -0.9118162393569946, 'motion_component': -0.11538004875183105, 'motion_component_percent': 91.18162393569946}, {'resid': 1313, 'atom': 'C315', 'charge': -0.18000000715255737, 'distance': 20.905445098876953, 'force': [0.13607607781887054, -0.001677597756497562, 0.013341237790882587], 'magnitude': 0.13673880696296692, 'cosine_with_motion': -0.8858672976493835, 'motion_component': -0.12113244086503983, 'motion_component_percent': 88.58672976493835}, {'resid': 1313, 'atom': 'C316', 'charge': -0.18000000715255737, 'distance': 21.60270118713379, 'force': [0.12646563351154327, -0.00714101642370224, 0.01879827119410038], 'magnitude': 0.12805438041687012, 'cosine_with_motion': -0.8546587228775024, 'motion_component': -0.10944279283285141, 'motion_component_percent': 85.46587228775024}, {'resid': 1313, 'atom': 'C317', 'charge': -0.18000000715255737, 'distance': 20.944175720214844, 'force': [0.13286277651786804, -0.009005315601825714, 0.02873956225812435], 'magnitude': 0.13623353838920593, 'cosine_with_motion': -0.8198865652084351, 'motion_component': -0.11169604957103729, 'motion_component_percent': 81.9886565208435}, {'resid': 1313, 'atom': 'C318', 'charge': -0.27000001072883606, 'distance': 21.929576873779297, 'force': [0.1792498081922531, -0.01732555776834488, 0.04809950292110443], 'magnitude': 0.18639804422855377, 'cosine_with_motion': -0.7867467403411865, 'motion_component': -0.14664804935455322, 'motion_component_percent': 78.67467403411865}, {'resid': 1313, 'atom': 'C32', 'charge': -0.08000000566244125, 'distance': 23.333284378051758, 'force': [0.04139629006385803, 0.02013884298503399, -0.016144409775733948], 'magnitude': 0.048783887177705765, 'cosine_with_motion': -0.969207227230072, 'motion_component': -0.047281697392463684, 'motion_component_percent': 96.9207227230072}, {'resid': 1313, 'atom': 'C33', 'charge': -0.18000000715255737, 'distance': 24.199308395385742, 'force': [0.08879955857992172, 0.037246059626340866, -0.033781252801418304], 'magnitude': 0.10204804688692093, 'cosine_with_motion': -0.9807745218276978, 'motion_component': -0.10008612275123596, 'motion_component_percent': 98.07745218276978}, {'resid': 1313, 'atom': 'C34', 'charge': -0.18000000715255737, 'distance': 23.733802795410156, 'force': [0.0953674167394638, 0.034145597368478775, -0.031532518565654755], 'magnitude': 0.10609036684036255, 'cosine_with_motion': -0.9884042739868164, 'motion_component': -0.10486017167568207, 'motion_component_percent': 98.84042739868164}, {'resid': 1313, 'atom': 'C35', 'charge': -0.18000000715255737, 'distance': 22.62854766845703, 'force': [0.10542266070842743, 0.03277288377285004, -0.03784898668527603], 'magnitude': 0.11670709401369095, 'cosine_with_motion': -0.9942911863327026, 'motion_component': -0.11604083329439163, 'motion_component_percent': 99.42911863327026}, {'resid': 1313, 'atom': 'C36', 'charge': -0.18000000715255737, 'distance': 22.1077823638916, 'force': [0.11348351836204529, 0.029882656410336494, -0.034329164773225784], 'magnitude': 0.12227008491754532, 'cosine_with_motion': -0.9962120652198792, 'motion_component': -0.12180693447589874, 'motion_component_percent': 99.62120652198792}, {'resid': 1313, 'atom': 'C37', 'charge': -0.18000000715255737, 'distance': 20.74103355407715, 'force': [0.12922166287899017, 0.03022986277937889, -0.04105306789278984], 'magnitude': 0.13891521096229553, 'cosine_with_motion': -0.9983547329902649, 'motion_component': -0.1386866569519043, 'motion_component_percent': 99.83547329902649}, {'resid': 1313, 'atom': 'C38', 'charge': -0.18000000715255737, 'distance': 20.31368064880371, 'force': [0.13818798959255219, 0.023756947368383408, -0.03623517230153084], 'magnitude': 0.14482161402702332, 'cosine_with_motion': -0.9958552718162537, 'motion_component': -0.14422136545181274, 'motion_component_percent': 99.58552718162537}, {'resid': 1313, 'atom': 'C39', 'charge': -0.18000000715255737, 'distance': 20.030624389648438, 'force': [0.14393064379692078, 0.027521591633558273, -0.026659062132239342], 'magnitude': 0.14894352853298187, 'cosine_with_motion': -0.9868643879890442, 'motion_component': -0.14698706567287445, 'motion_component_percent': 98.68643879890442}, {'resid': 1313, 'atom': 'C4', 'charge': 0.08000000566244125, 'distance': 27.09943389892578, 'force': [-0.021163279190659523, -0.015059158205986023, 0.025166647508740425], 'magnitude': 0.03616659715771675, 'cosine_with_motion': 0.8485779762268066, 'motion_component': 0.030690178275108337, 'motion_component_percent': 84.85779762268066}, {'resid': 1313, 'atom': 'C5', 'charge': 0.08000000566244125, 'distance': 25.696643829345703, 'force': [-0.022835662588477135, -0.0164418313652277, 0.028741860762238503], 'magnitude': 0.040223076939582825, 'cosine_with_motion': 0.837376594543457, 'motion_component': 0.03368186205625534, 'motion_component_percent': 83.7376594543457}, {'resid': 1313, 'atom': 'C6', 'charge': 0.06000000238418579, 'distance': 24.525794982910156, 'force': [-0.018977362662553787, -0.01479191891849041, 0.022754233330488205], 'magnitude': 0.033116403967142105, 'cosine_with_motion': 0.8397897481918335, 'motion_component': 0.02781081572175026, 'motion_component_percent': 83.97897481918335}, {'resid': 1313, 'atom': 'H1', 'charge': 0.12000000476837158, 'distance': 24.129514694213867, 'force': [-0.04395900294184685, -0.028680842369794846, 0.043899375945329666], 'magnitude': 0.06842616200447083, 'cosine_with_motion': 0.8838358521461487, 'motion_component': 0.060477495193481445, 'motion_component_percent': 88.38358521461487}, {'resid': 1313, 'atom': 'H10R', 'charge': 0.09000000357627869, 'distance': 21.337480545043945, 'force': [-0.05067255347967148, -0.0381813608109951, 0.01678134873509407], 'magnitude': 0.0656287893652916, 'cosine_with_motion': 0.9030977487564087, 'motion_component': 0.05926921218633652, 'motion_component_percent': 90.30977487564087}, {'resid': 1313, 'atom': 'H10S', 'charge': 0.09000000357627869, 'distance': 22.037206649780273, 'force': [-0.04997966066002846, -0.03212229534983635, 0.015993574634194374], 'magnitude': 0.061527252197265625, 'cosine_with_motion': 0.9311680197715759, 'motion_component': 0.057292208075523376, 'motion_component_percent': 93.11680197715759}, {'resid': 1313, 'atom': 'H10X', 'charge': 0.09000000357627869, 'distance': 21.142837524414062, 'force': [-0.06583354622125626, -0.007219814229756594, 0.00904246885329485], 'magnitude': 0.0668427124619484, 'cosine_with_motion': 0.9757925271987915, 'motion_component': 0.06522461771965027, 'motion_component_percent': 97.57925271987915}, {'resid': 1313, 'atom': 'H10Y', 'charge': 0.09000000357627869, 'distance': 19.46343421936035, 'force': [-0.07778820395469666, -0.0066772811114788055, 0.011213392950594425], 'magnitude': 0.07887541502714157, 'cosine_with_motion': 0.9751883745193481, 'motion_component': 0.07691838592290878, 'motion_component_percent': 97.51883745193481}, {'resid': 1313, 'atom': 'H111', 'charge': 0.15000000596046448, 'distance': 24.06795883178711, 'force': [-0.0658726692199707, -0.048096515238285065, 0.027175189927220345], 'magnitude': 0.08597077429294586, 'cosine_with_motion': 0.9139704704284668, 'motion_component': 0.07857474684715271, 'motion_component_percent': 91.39704704284668}, {'resid': 1313, 'atom': 'H11A', 'charge': 0.09000000357627869, 'distance': 24.1783504486084, 'force': [-0.03650572896003723, -0.02141064777970314, 0.02866017445921898], 'magnitude': 0.051112521439790726, 'cosine_with_motion': 0.9230924844741821, 'motion_component': 0.04718158394098282, 'motion_component_percent': 92.30924844741821}, {'resid': 1313, 'atom': 'H11B', 'charge': 0.09000000357627869, 'distance': 22.667190551757812, 'force': [-0.041346460580825806, -0.022550897672772408, 0.03411601483821869], 'magnitude': 0.05815475061535835, 'cosine_with_motion': 0.92327880859375, 'motion_component': 0.053693048655986786, 'motion_component_percent': 92.327880859375}, {'resid': 1313, 'atom': 'H11X', 'charge': 0.09000000357627869, 'distance': 19.057605743408203, 'force': [-0.08116772025823593, -0.013083504512906075, 0.0030083712190389633], 'magnitude': 0.08227045089006424, 'cosine_with_motion': 0.9532563090324402, 'motion_component': 0.07842482626438141, 'motion_component_percent': 95.32563090324402}, {'resid': 1313, 'atom': 'H11Y', 'charge': 0.09000000357627869, 'distance': 20.589380264282227, 'force': [-0.06906619668006897, -0.013656321913003922, 0.003382262075319886], 'magnitude': 0.07048457115888596, 'cosine_with_motion': 0.9570109844207764, 'motion_component': 0.0674545094370842, 'motion_component_percent': 95.70109844207764}, {'resid': 1313, 'atom': 'H12', 'charge': 0.09000000357627869, 'distance': 23.318710327148438, 'force': [-0.042868368327617645, -0.020587226375937462, 0.02753225341439247], 'magnitude': 0.05495048686861992, 'cosine_with_motion': 0.9562166929244995, 'motion_component': 0.052544571459293365, 'motion_component_percent': 95.62166929244995}, {'resid': 1313, 'atom': 'H121', 'charge': 0.15000000596046448, 'distance': 25.008586883544922, 'force': [-0.06024628505110741, -0.04836283624172211, 0.019277166575193405], 'magnitude': 0.07962529361248016, 'cosine_with_motion': 0.8887321352958679, 'motion_component': 0.07076555490493774, 'motion_component_percent': 88.87321352958679}, {'resid': 1313, 'atom': 'H12X', 'charge': 0.09000000357627869, 'distance': 20.102676391601562, 'force': [-0.07355457544326782, -0.006949625443667173, -0.0028955978341400623], 'magnitude': 0.07393887639045715, 'cosine_with_motion': 0.9239342212677002, 'motion_component': 0.06831465661525726, 'motion_component_percent': 92.39342212677002}, {'resid': 1313, 'atom': 'H12Y', 'charge': 0.09000000357627869, 'distance': 21.63641357421875, 'force': [-0.06339171528816223, -0.00743575906381011, -0.0004382760089356452], 'magnitude': 0.06382783502340317, 'cosine_with_motion': 0.9372389316558838, 'motion_component': 0.05982193350791931, 'motion_component_percent': 93.72389316558838}, {'resid': 1313, 'atom': 'H13A', 'charge': 0.09000000357627869, 'distance': 24.43229103088379, 'force': [-0.03815118223428726, -0.02250312641263008, 0.023316407576203346], 'magnitude': 0.050055552273988724, 'cosine_with_motion': 0.9410346150398254, 'motion_component': 0.04710400849580765, 'motion_component_percent': 94.10346150398254}, {'resid': 1313, 'atom': 'H13B', 'charge': 0.09000000357627869, 'distance': 22.931833267211914, 'force': [-0.042345400899648666, -0.027744876220822334, 0.025799784809350967], 'magnitude': 0.05682024359703064, 'cosine_with_motion': 0.9282805323600769, 'motion_component': 0.05274512618780136, 'motion_component_percent': 92.82805323600769}, {'resid': 1313, 'atom': 'H13R', 'charge': 0.09000000357627869, 'distance': 22.94049835205078, 'force': [-0.04468102753162384, -0.03395114094018936, 0.008636587299406528], 'magnitude': 0.05677732825279236, 'cosine_with_motion': 0.8849335312843323, 'motion_component': 0.05024415999650955, 'motion_component_percent': 88.49335312843323}, {'resid': 1313, 'atom': 'H13S', 'charge': 0.09000000357627869, 'distance': 22.349082946777344, 'force': [-0.044692061841487885, -0.03805166482925415, 0.011548462323844433], 'magnitude': 0.05982203781604767, 'cosine_with_motion': 0.8685210943222046, 'motion_component': 0.05195670202374458, 'motion_component_percent': 86.85210943222046}, {'resid': 1313, 'atom': 'H13X', 'charge': 0.09000000357627869, 'distance': 21.830142974853516, 'force': [-0.06254952400922775, -0.0023318014573305845, 0.0036618083249777555], 'magnitude': 0.06269999593496323, 'cosine_with_motion': 0.9492178559303284, 'motion_component': 0.05951595678925514, 'motion_component_percent': 94.92178559303284}, {'resid': 1313, 'atom': 'H13Y', 'charge': 0.09000000357627869, 'distance': 20.241775512695312, 'force': [-0.07285916060209274, 6.011372897773981e-05, 0.003125089220702648], 'magnitude': 0.07292617112398148, 'cosine_with_motion': 0.938647449016571, 'motion_component': 0.06845196336507797, 'motion_component_percent': 93.8647449016571}, {'resid': 1313, 'atom': 'H141', 'charge': 0.15000000596046448, 'distance': 25.184038162231445, 'force': [-0.05736609548330307, -0.051866933703422546, 0.013575570657849312], 'magnitude': 0.07851970195770264, 'cosine_with_motion': 0.8508307933807373, 'motion_component': 0.06680697947740555, 'motion_component_percent': 85.08307933807373}, {'resid': 1313, 'atom': 'H14X', 'charge': 0.09000000357627869, 'distance': 22.028718948364258, 'force': [-0.06148798018693924, 0.00306149385869503, -0.001138343708589673], 'magnitude': 0.06157467141747475, 'cosine_with_motion': 0.9089634418487549, 'motion_component': 0.055969126522541046, 'motion_component_percent': 90.89634418487549}, {'resid': 1313, 'atom': 'H14Y', 'charge': 0.09000000357627869, 'distance': 22.667308807373047, 'force': [-0.05806950107216835, -0.0009041635203175247, -0.003003334626555443], 'magnitude': 0.0581541433930397, 'cosine_with_motion': 0.9093351364135742, 'motion_component': 0.05288160592317581, 'motion_component_percent': 90.93351364135742}, {'resid': 1313, 'atom': 'H151', 'charge': 0.15000000596046448, 'distance': 24.988792419433594, 'force': [-0.05733231455087662, -0.054999932646751404, 0.006950778421014547], 'magnitude': 0.07975149154663086, 'cosine_with_motion': 0.8163689970970154, 'motion_component': 0.06510664522647858, 'motion_component_percent': 81.63689970970154}, {'resid': 1313, 'atom': 'H15X', 'charge': 0.09000000357627869, 'distance': 19.887939453125, 'force': [-0.07521861791610718, 0.0022465738002210855, -0.0066359140910208225], 'magnitude': 0.07554417848587036, 'cosine_with_motion': 0.886538565158844, 'motion_component': 0.06697282940149307, 'motion_component_percent': 88.6538565158844}, {'resid': 1313, 'atom': 'H15Y', 'charge': 0.09000000357627869, 'distance': 20.813556671142578, 'force': [-0.0684763491153717, -0.002579909050837159, -0.007861553691327572], 'magnitude': 0.06897442042827606, 'cosine_with_motion': 0.8869478702545166, 'motion_component': 0.06117671728134155, 'motion_component_percent': 88.69478702545166}, {'resid': 1313, 'atom': 'H16R', 'charge': 0.09000000357627869, 'distance': 23.38818359375, 'force': [-0.0421663373708725, -0.03465820476412773, 0.0021556608844548464], 'magnitude': 0.0546245202422142, 'cosine_with_motion': 0.8396887183189392, 'motion_component': 0.045867592096328735, 'motion_component_percent': 83.96887183189392}, {'resid': 1313, 'atom': 'H16S', 'charge': 0.09000000357627869, 'distance': 22.115705490112305, 'force': [-0.045379482209682465, -0.040621645748615265, 0.004767152015119791], 'magnitude': 0.06109125539660454, 'cosine_with_motion': 0.8310777544975281, 'motion_component': 0.05077158287167549, 'motion_component_percent': 83.10777544975281}, {'resid': 1313, 'atom': 'H16X', 'charge': 0.09000000357627869, 'distance': 22.603778839111328, 'force': [-0.0577290914952755, 0.00219282740727067, -0.009090056642889977], 'magnitude': 0.058481499552726746, 'cosine_with_motion': 0.8545670509338379, 'motion_component': 0.04997636377811432, 'motion_component_percent': 85.45670509338379}, {'resid': 1313, 'atom': 'H16Y', 'charge': 0.09000000357627869, 'distance': 21.90448570251465, 'force': [-0.061444103717803955, 0.006256175693124533, -0.00797942839562893], 'magnitude': 0.06227510794997215, 'cosine_with_motion': 0.85215163230896, 'motion_component': 0.05306783318519592, 'motion_component_percent': 85.215163230896}, {'resid': 1313, 'atom': 'H17R', 'charge': 0.09000000357627869, 'distance': 22.731294631958008, 'force': [-0.03984002768993378, -0.04188866540789604, 0.0014486905420199037], 'magnitude': 0.057827215641736984, 'cosine_with_motion': 0.7739711403846741, 'motion_component': 0.04475659504532814, 'motion_component_percent': 77.39711403846741}, {'resid': 1313, 'atom': 'H17S', 'charge': 0.09000000357627869, 'distance': 24.230440139770508, 'force': [-0.0361163504421711, -0.03585635870695114, -0.00016574228357058018], 'magnitude': 0.050892990082502365, 'cosine_with_motion': 0.7801200151443481, 'motion_component': 0.0397026389837265, 'motion_component_percent': 78.01200151443481}, {'resid': 1313, 'atom': 'H17X', 'charge': 0.09000000357627869, 'distance': 20.59868049621582, 'force': [-0.06850893795490265, 0.0014138646656647325, -0.016236843541264534], 'magnitude': 0.07042094320058823, 'cosine_with_motion': 0.8192166686058044, 'motion_component': 0.057690009474754333, 'motion_component_percent': 81.92166686058044}, {'resid': 1313, 'atom': 'H17Y', 'charge': 0.09000000357627869, 'distance': 20.1258602142334, 'force': [-0.0718555897474289, 0.007422902155667543, -0.014949467964470387], 'magnitude': 0.07376863807439804, 'cosine_with_motion': 0.8154666423797607, 'motion_component': 0.06015586480498314, 'motion_component_percent': 81.54666423797607}, {'resid': 1313, 'atom': 'H18R', 'charge': 0.09000000357627869, 'distance': 22.869035720825195, 'force': [-0.040217239409685135, -0.04034048318862915, -0.0044007874093949795], 'magnitude': 0.057132720947265625, 'cosine_with_motion': 0.7503381371498108, 'motion_component': 0.04286886006593704, 'motion_component_percent': 75.03381371498108}, {'resid': 1313, 'atom': 'H18S', 'charge': 0.09000000357627869, 'distance': 22.962663650512695, 'force': [-0.042934171855449677, -0.0368291437625885, -0.003392125479876995], 'magnitude': 0.056667763739824295, 'cosine_with_motion': 0.7958713173866272, 'motion_component': 0.04510024935007095, 'motion_component_percent': 79.58713173866272}, {'resid': 1313, 'atom': 'H18X', 'charge': 0.09000000357627869, 'distance': 22.19989776611328, 'force': [-0.05804911255836487, 0.00852067768573761, -0.0152821596711874], 'magnitude': 0.060628753155469894, 'cosine_with_motion': 0.7764543890953064, 'motion_component': 0.047075461596250534, 'motion_component_percent': 77.64543890953064}, {'resid': 1313, 'atom': 'H18Y', 'charge': 0.09000000357627869, 'distance': 21.588253021240234, 'force': [-0.06084006652235985, 0.005482955370098352, -0.019465133547782898], 'magnitude': 0.06411293148994446, 'cosine_with_motion': 0.761021614074707, 'motion_component': 0.04879132658243179, 'motion_component_percent': 76.1021614074707}, {'resid': 1313, 'atom': 'H18Z', 'charge': 0.09000000357627869, 'distance': 22.852102279663086, 'force': [-0.05528092384338379, 0.003927062265574932, -0.014227837324142456], 'magnitude': 0.057217422872781754, 'cosine_with</t>
         </is>
       </c>
     </row>
@@ -643,7 +643,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>{963: {'frame': 963, 'motion_vector': [-6.639595031738281, 1.0836753845214844, 2.0808258056640625], 'ionic_force': [-0.03461587429046631, -3.451846368610859, -26.245480060577393], 'ionic_force_magnitude': 26.47152555523407, 'radial_force': 3.452019932046289, 'axial_force': -26.245480060577393, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [0.6113827228546143, -0.2678259313106537, -0.847156286239624], 'asn_force_magnitude': 1.0785144118660877, 'residue_force': [0.6113827228546143, -0.2678259313106537, -0.847156286239624], 'residue_force_magnitude': 1.0785144118660877, 'total_force': [0.576766848564148, -3.7196722999215126, -27.092636346817017], 'total_force_magnitude': 27.352871261300457, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': -0.8048084027521138, 'cosine_residue_motion': -0.8048084027521138, 'cosine_ionic_motion': -0.311802673918244, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': -0.8679974611590815, 'motion_component_residue': -0.8679974611590815, 'motion_component_ionic': -8.253892450817112, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 80.48084027521139, 'motion_component_percent_residue': 80.48084027521139, 'motion_component_percent_ionic': 31.1802673918244, 'ionic_contributions': [{'ion_id': 2230, 'distance': 14.592389106750488, 'force': [0.16000592708587646, 0.08226221054792404, -1.5487253665924072], 'magnitude': 1.5591405630111694, 'cosine_ionic_motion': -0.3821600377559662, 'motion_component_ionic': -0.5958412289619446, 'motion_component_percent_ionic': 38.21600377559662}, {'ion_id': 2333, 'distance': 4.4050493240356445, 'force': [1.2773457765579224, -5.039449691772461, -16.30049705505371], 'magnitude': 17.109468460083008, 'cosine_ionic_motion': -0.3972393572330475, 'motion_component_ionic': -6.796554088592529, 'motion_component_percent_ionic': 39.72393572330475}, {'ion_id': 2334, 'distance': 9.08781909942627, 'force': [0.15932977199554443, 0.28409475088119507, -4.006714344024658], 'magnitude': 4.019932270050049, 'cosine_ionic_motion': -0.32101526856422424, 'motion_component_ionic': -1.2904596328735352, 'motion_component_percent_ionic': 32.101526856422424}, {'ion_id': 2372, 'distance': 7.211418151855469, 'force': [-5.535534858703613, -1.084515929222107, -2.9896254539489746], 'magnitude': 6.38405704498291, 'cosine_ionic_motion': 0.6530299186706543, 'motion_component_ionic': 4.168980121612549, 'motion_component_percent_ionic': 65.30299186706543}, {'ion_id': 2397, 'distance': 8.364306449890137, 'force': [3.9042375087738037, 2.30576229095459, -1.3999178409576416], 'magnitude': 4.745459079742432, 'cosine_ionic_motion': -0.7881255149841309, 'motion_component_ionic': -3.7400174140930176, 'motion_component_percent_ionic': 78.81255149841309}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 5.723193645477295, 'force': [-7.815121173858643, -2.1620965003967285, -4.361874580383301], 'magnitude': 9.207427978515625, 'cosine_with_motion': 0.6241716742515564, 'motion_component': 5.747015476226807, 'motion_component_percent': 62.41716742515564}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 5.179661750793457, 'force': [4.4384284019470215, 0.4155177175998688, 2.5497331619262695], 'magnitude': 5.135507583618164, 'cosine_with_motion': -0.6557264924049377, 'motion_component': -3.367488384246826, 'motion_component_percent': 65.57264924049377}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 5.5684099197387695, 'force': [3.3907041549682617, 1.6970765590667725, 2.3168129920959473], 'magnitude': 4.443485736846924, 'cosine_with_motion': -0.506635844707489, 'motion_component': -2.2512290477752686, 'motion_component_percent': 50.6635844707489}, {'resid': 786, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 5.938525199890137, 'force': [-2.098083734512329, -5.628914833068848, 3.042907476425171], 'magnitude': 6.733938217163086, 'cosine_with_motion': 0.2986576557159424, 'motion_component': 2.0111422538757324, 'motion_component_percent': 29.86576557159424}, {'resid': 786, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 5.167057991027832, 'force': [2.6954550743103027, 5.410591125488281, -4.394735336303711], 'magnitude': 7.473531246185303, 'cosine_with_motion': -0.4024118483066559, 'motion_component': -3.0074374675750732, 'motion_component_percent': 40.24118483066559}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': -0.3334893008063134, 'motion_component_pip2': -9.121889911976194, 'motion_component_percent_pip2': 33.34893008063134}, 964: {'frame': 964, 'motion_vector': [4.467369079589844, -3.3118934631347656, -0.7404861450195312], 'ionic_force': [-10.332740664482117, 5.494437627494335, -2.3852338194847107], 'ionic_force_magnitude': 11.943354422250122, 'radial_force': 11.702750722879982, 'axial_force': -2.3852338194847107, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [0.8001996278762817, -0.6171016693115234, -5.133657693862915], 'asn_force_magnitude': 5.232167355167293, 'residue_force': [0.8001996278762817, -0.6171016693115234, -5.133657693862915], 'residue_force_magnitude': 5.232167355167293, 'total_force': [-9.532541036605835, 4.877335958182812, -7.518891513347626], 'total_force_magnitude': 13.084015983368724, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': 0.32091446238776433, 'cosine_residue_motion': 0.32091446238776433, 'cosine_ionic_motion': -0.9341286958757883, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': 1.6790781739063227, 'motion_component_residue': 1.6790781739063227, 'motion_component_ionic': -11.156630090838835, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 32.091446238776435, 'motion_component_percent_residue': 32.091446238776435, 'motion_component_percent_ionic': 93.41286958757883, 'ionic_contributions': [{'ion_id': 2230, 'distance': 14.369630813598633, 'force': [-0.5380553007125854, 0.253653883934021, -1.4937716722488403], 'magnitude': 1.607854962348938, 'cosine_ionic_motion': -0.23697973787784576, 'motion_component_ionic': -0.38102903962135315, 'motion_component_percent_ionic': 23.697973787784576}, {'ion_id': 2333, 'distance': 9.151873588562012, 'force': [-3.5885279178619385, -0.26910218596458435, 1.6619921922683716], 'magnitude': 3.963857650756836, 'cosine_ionic_motion': -0.7361587882041931, 'motion_component_ionic': -2.9180285930633545, 'motion_component_percent_ionic': 73.61587882041931}, {'ion_id': 2334, 'distance': 9.51083755493164, 'force': [-2.078768253326416, 0.6810020804405212, -2.9472014904022217], 'magnitude': 3.6702914237976074, 'cosine_ionic_motion': -0.4545499384403229, 'motion_component_ionic': -1.6683307886123657, 'motion_component_percent_ionic': 45.45499384403229}, {'ion_id': 2372, 'distance': 12.222784996032715, 'force': [-2.1967005729675293, 0.11882515996694565, -0.3144724369049072], 'magnitude': 2.2222747802734375, 'cosine_ionic_motion': -0.8000177145004272, 'motion_component_ionic': -1.7778592109680176, 'motion_component_percent_ionic': 80.00177145004272}, {'ion_id': 2397, 'distance': 8.037322044372559, 'force': [-1.9306886196136475, 4.710058689117432, 0.708219587802887], 'magnitude': 5.139434337615967, 'cosine_ionic_motion': -0.8583401441574097, 'motion_component_ionic': -4.411382675170898, 'motion_component_percent_ionic': 85.83401441574097}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 5.273385524749756, 'force': [-1.9003324508666992, 2.7260823249816895, 7.866718292236328], 'magnitude': 8.53979206085205, 'cosine_with_motion': -0.4872303307056427, 'motion_component': -4.160845756530762, 'motion_component_percent': 48.72303307056427}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 4.681761741638184, 'force': [1.0527347326278687, -1.411345362663269, -8.931296348571777], 'magnitude': 9.10319709777832, 'cosine_with_motion': 0.3131083548069, 'motion_component': 2.8502871990203857, 'motion_component_percent': 31.310835480690002}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 5.820265293121338, 'force': [3.8972513675689697, -2.509633779525757, -7.6009297370910645], 'magnitude': 8.902862548828125, 'cosine_with_motion': 0.6276770234107971, 'motion_component': 5.588122367858887, 'motion_component_percent': 62.76770234107971}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 5.709196090698242, 'force': [-2.2494540214538574, 0.577795147895813, 3.5318500995635986], 'magnitude': 4.227038383483887, 'cosine_with_motion': -0.6147295832633972, 'motion_component': -2.5984854698181152, 'motion_component_percent': 61.47295832633972}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': -0.7243610775911281, 'motion_component_pip2': -9.477551916932512, 'motion_component_percent_pip2': 72.43610775911282}, 965: {'frame': 965, 'motion_vector': [6.944755554199219, -5.441310882568359, 2.6126480102539062], 'ionic_force': [6.747662315145135, -9.89717410504818, -11.307039380073547], 'ionic_force_magnitude': 16.472223332853403, 'radial_force': 11.978522529296592, 'axial_force': -11.307039380073547, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-0.24390149116516113, 1.7514587044715881, 1.8951330184936523], 'asn_force_magnitude': 2.5920309968529978, 'residue_force': [-0.24390149116516113, 1.7514587044715881, 1.8951330184936523], 'residue_force_magnitude': 2.5920309968529978, 'total_force': [6.503760823979974, -8.145715400576591, -9.411906361579895], 'total_force_magnitude': 14.044058017605716, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': -0.2630086624045145, 'cosine_residue_motion': -0.2630086624045145, 'cosine_ionic_motion': 0.46958702941708175, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': -0.6817266053933473, 'motion_component_residue': -0.6817266053933473, 'motion_component_ionic': 7.735142422769371, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 26.300866240451448, 'motion_component_percent_residue': 26.300866240451448, 'motion_component_percent_ionic': 46.958702941708175, 'ionic_contributions': [{'ion_id': 2230, 'distance': 13.940370559692383, 'force': [0.025344202294945717, -0.1283198446035385, -1.7033849954605103], 'magnitude': 1.7083994150161743, 'cosine_ionic_motion': -0.22749574482440948, 'motion_component_ionic': -0.38865360617637634, 'motion_component_percent_ionic': 22.74957448244095}, {'ion_id': 2333, 'distance': 8.212841033935547, 'force': [-0.6852325797080994, -4.7515549659729, -1.086434245109558], 'magnitude': 4.922109127044678, 'cosine_ionic_motion': 0.4031260311603546, 'motion_component_ionic': 1.9842302799224854, 'motion_component_percent_ionic': 40.31260311603546}, {'ion_id': 2334, 'distance': 7.9869608879089355, 'force': [-0.9994736909866333, -1.149268627166748, -4.976600170135498], 'magnitude': 5.204451560974121, 'cosine_ionic_motion': -0.28587114810943604, 'motion_component_ionic': -1.487802505493164, 'motion_component_percent_ionic': 28.587114810943604}, {'ion_id': 2372, 'distance': 9.729399681091309, 'force': [-2.949526786804199, -1.665939211845398, -0.90868079662323], 'magnitude': 3.507244348526001, 'cosine_ionic_motion': -0.4274074137210846, 'motion_component_ionic': -1.4990222454071045, 'motion_component_percent_ionic': 42.74074137210846}, {'ion_id': 2397, 'distance': 5.290038108825684, 'force': [11.356551170349121, -2.2020914554595947, -2.631939172744751], 'magnitude': 11.863707542419434, 'cosine_ionic_motion': 0.7692697048187256, 'motion_component_ionic': 9.12639045715332, 'motion_component_percent_ionic': 76.92697048187256}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 4.884537220001221, 'force': [6.379004955291748, -2.195544958114624, 7.318586349487305], 'magnitude': 9.953583717346191, 'cosine_with_motion': 0.8229256272315979, 'motion_component': 8.191059112548828, 'motion_component_percent': 82.29256272315979}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 5.193253040313721, 'force': [-4.454446792602539, 3.333285331726074, -4.876718521118164], 'magnitude': 7.39832878112793, 'cosine_with_motion': -0.9080353379249573, 'motion_component': -6.717944145202637, 'motion_component_percent': 90.80353379249573}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 4.454931259155273, 'force': [-6.7003173828125, 1.895298719406128, -13.506893157958984], 'magnitude': 15.196136474609375, 'cosine_with_motion': -0.6589274406433105, 'motion_component': -10.013151168823242, 'motion_component_percent': 65.89274406433105}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 4.242242813110352, 'force': [1.9323811531066895, -1.8520965576171875, 7.172736644744873], 'magnitude': 7.655880928039551, 'cosine_with_motion': 0.5995922088623047, 'motion_component': 4.59040641784668, 'motion_component_percent': 59.95922088623047}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 4.650750637054443, 'force': [2.5994765758514404, 0.5705161690711975, 5.787421703338623], 'magnitude': 6.370009422302246, 'cosine_with_motion': 0.5130138397216797, 'motion_component': 3.2679030895233154, 'motion_component_percent': 51.30138397216797}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': 0.5022348817224921, 'motion_component_pip2': 7.053415817376024, 'motion_component_percent_pip2': 50.22348817224921}, 966: {'frame': 966, 'motion_vector': [1.954345703125, 3.60467529296875, -1.7191238403320312], 'ionic_force': [4.150573551654816, -10.163548946380615, -2.4668384045362473], 'ionic_force_magnitude': 11.252123342163733, 'radial_force': 10.978387312951341, 'axial_force': -2.4668384045362473, 'glu_force': [-0.4746452271938324, -13.296928405761719, 6.007837295532227], 'glu_force_magnitude': 14.59889386526386, 'asn_force': [0.6581447124481201, -0.9605653584003448, -0.7814178466796875], 'asn_force_magnitude': 1.4023031488917512, 'residue_force': [0.18349948525428772, -14.257493764162064, 5.226419448852539], 'residue_force_magnitude': 15.18635113355255, 'total_force': [4.334073036909103, -24.42104271054268, 2.759581044316292], 'total_force_magnitude': 24.955696818553516, 'cosine_total_motion': 0, 'cosine_glu_motion': -0.911840170937927, 'cosine_asn_motion': -0.13359162150330972, 'cosine_residue_motion': -0.8889030492177631, 'cosine_ionic_motion': -0.4853952943793971, 'motion_component_total': 0, 'motion_component_glu': -13.311857877606851, 'motion_component_asn': -0.1873359514996462, 'motion_component_residue': -13.499193829106495, 'motion_component_ionic': -5.461727722062851, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 91.1840170937927, 'motion_component_percent_asn': 13.359162150330972, 'motion_component_percent_residue': 88.8903049217763, 'motion_component_percent_ionic': 48.53952943793971, 'ionic_contributions': [{'ion_id': 2230, 'distance': 14.374963760375977, 'force': [0.7663649916648865, -0.673296332359314, -1.2412574291229248], 'magnitude': 1.6066621541976929, 'cosine_ionic_motion': 0.16862890124320984, 'motion_component_ionic': 0.2709296643733978, 'motion_component_percent_ionic': 16.862890124320984}, {'ion_id': 2333, 'distance': 14.384037017822266, 'force': [0.511242687702179, -1.5174258947372437, 0.10442951321601868], 'magnitude': 1.6046357154846191, 'cosine_ionic_motion': -0.6517917513847351, 'motion_component_ionic': -1.0458883047103882, 'motion_component_percent_ionic': 65.17917513847351}, {'ion_id': 2334, 'distance': 9.694668769836426, 'force': [1.9925323724746704, -2.33052659034729, -1.7539780139923096], 'magnitude': 3.5324180126190186, 'cosine_ionic_motion': -0.09495801478624344, 'motion_component_ionic': -0.33543139696121216, 'motion_component_percent_ionic': 9.495801478624344}, {'ion_id': 2372, 'distance': 8.244967460632324, 'force': [-0.6521925330162048, -4.834371089935303, 0.23507510125637054], 'magnitude': 4.88382625579834, 'cosine_ionic_motion': -0.8798348903656006, 'motion_component_ionic': -4.296960830688477, 'motion_component_percent_ionic': 87.98348903656006}, {'ion_id': 2397, 'distance': 13.802080154418945, 'force': [1.5326260328292847, -0.8079290390014648, 0.1888924241065979], 'magnitude': 1.7428058385849, 'cosine_ionic_motion': -0.031200869008898735, 'motion_component_ionic': -0.054377056658267975, 'motion_component_percent_ionic': 3.1200869008898735}], 'glu_contributions': [{'resid': 1082, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 4.80486536026001, 'force': [2.3577680587768555, 9.827399253845215, -5.657576560974121], 'magnitude': 11.582098960876465, 'cosine_with_motion': 0.9662582278251648, 'motion_component': 11.191298484802246, 'motion_component_percent': 96.62582278251648}, {'resid': 1082, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 4.299968719482422, 'force': [-2.5012972354888916, -13.982897758483887, 3.7920660972595215], 'magnitude': 14.702301979064941, 'cosine_with_motion': -0.945572555065155, 'motion_component': -13.902092933654785, 'motion_component_percent': 94.5572555065155}, {'resid': 1082, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 4.745906352996826, 'force': [-0.33111605048179626, -9.141429901123047, 7.873347759246826], 'magnitude': 12.069174766540527, 'cosine_with_motion': -0.8783586025238037, 'motion_component': -10.60106372833252, 'motion_component_percent': 87.83586025238037}], 'asn_contributions': [{'resid': 1114, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 4.9302544593811035, 'force': [-6.710339069366455, -3.0844039916992188, -9.969874382019043], 'magnitude': 12.407279968261719, 'cosine_with_motion': -0.1285804957151413, 'motion_component': -1.5953342914581299, 'motion_component_percent': 12.85804957151413}, {'resid': 1114, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 4.7290215492248535, 'force': [4.2160515785217285, 1.8340024948120117, 4.100967884063721], 'magnitude': 6.160892009735107, 'cosine_with_motion': 0.2847695052623749, 'motion_component': 1.7544341087341309, 'motion_component_percent': 28.476950526237488}, {'resid': 1114, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 4.795194625854492, 'force': [3.1524322032928467, 0.2898361384868622, 5.087488651275635], 'magnitude': 5.992026329040527, 'cosine_with_motion': -0.05781610310077667, 'motion_component': -0.3464356064796448, 'motion_component_percent': 5.781610310077667}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': -0.7597832947334373, 'motion_component_pip2': -18.96092155116935, 'motion_component_percent_pip2': 75.97832947334373}, 967: {'frame': 967, 'motion_vector': [-0.01629638671875, 1.2219734191894531, -0.38006591796875], 'ionic_force': [8.670876502990723, -4.813853949308395, -4.00980569422245], 'ionic_force_magnitude': 10.697468433269968, 'radial_force': 9.917524347103397, 'axial_force': -4.00980569422245, 'glu_force': [4.893032550811768, 8.126774787902832, 3.453498363494873], 'glu_force_magnitude': 10.095191278190741, 'asn_force': [1.692199945449829, -0.8650398254394531, 0.405582070350647], 'asn_force_magnitude': 1.943278510859069, 'residue_force': [6.585232496261597, 7.261734962463379, 3.85908043384552], 'residue_force_magnitude': 10.535206855575835, 'total_force': [15.25610899925232, 2.4478810131549835, -0.15072526037693024], 'total_force_magnitude': 15.451980499461808, 'cosine_total_motion': 0, 'cosine_glu_motion': 0.6608669210951875, 'cosine_asn_motion': -0.49809360780851347, 'cosine_residue_motion': 0.5413888357033694, 'cosine_ionic_motion': -0.32866670741297843, 'motion_component_total': 0, 'motion_component_glu': 6.671577977884906, 'motion_component_asn': -0.9679346044505492, 'motion_component_residue': 5.703643373434357, 'motion_component_ionic': -3.515901727617113, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 66.08669210951875, 'motion_component_percent_asn': 49.80936078085135, 'motion_component_percent_residue': 54.13888357033694, 'motion_component_percent_ionic': 32.866670741297845, 'ionic_contributions': [{'ion_id': 2333, 'distance': 13.19642162322998, 'force': [1.3005683422088623, -1.378942847251892, -0.20395071804523468], 'magnitude': 1.9064514636993408, 'cosine_ionic_motion': -0.6675289273262024, 'motion_component_ionic': -1.2726114988327026, 'motion_component_percent_ionic': 66.75289273262024}, {'ion_id': 2334, 'distance': 10.797028541564941, 'force': [1.8927514553070068, -0.8881277441978455, -1.9337624311447144], 'magnitude': 2.8479318618774414, 'cosine_ionic_motion': -0.10457437485456467, 'motion_component_ionic': -0.29782068729400635, 'motion_component_percent_ionic': 10.457437485456467}, {'ion_id': 2372, 'distance': 8.624361991882324, 'force': [3.5139474868774414, -2.145446538925171, -1.7241960763931274], 'magnitude': 4.463588237762451, 'cosine_ionic_motion': -0.3542417883872986, 'motion_component_ionic': -1.581189513206482, 'motion_component_percent_ionic': 35.42417883872986}, {'ion_id': 2397, 'distance': 12.853117942810059, 'force': [1.963609218597412, -0.40133681893348694, -0.14789646863937378], 'magnitude': 2.009653091430664, 'cosine_ionic_motion': -0.18126514554023743, 'motion_component_ionic': -0.3642800748348236, 'motion_component_percent_ionic': 18.126514554023743}], 'glu_contributions': [{'resid': 426, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 5.189203262329102, 'force': [4.893032550811768, 8.126774787902832, 3.453498363494873], 'magnitude': 10.09519100189209, 'cosine_with_motion': 0.660866916179657, 'motion_component': 6.6715779304504395, 'motion_component_percent': 66.0866916179657}], 'asn_contributions': [{'resid': 458, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 4.933333396911621, 'force': [-5.519587516784668, -7.10881233215332, 3.7697129249572754], 'magnitude': 9.75765323638916, 'cosine_with_motion': -0.8031351566314697, 'motion_component': -7.836714267730713, 'motion_component_percent': 80.31351566314697}, {'resid': 458, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 5.276961326599121, 'force': [5.277069568634033, 4.322860240936279, -2.1930325031280518], 'magnitude': 7.165471076965332, 'cosine_with_motion': 0.6575344204902649, 'motion_component': 4.711544036865234, 'motion_component_percent': 65.75344204902649}, {'resid': 458, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 4.734410762786865, 'force': [5.860385417938232, 11.801657676696777, -2.7227680683135986], 'magnitude': 13.454988479614258, 'cosine_with_motion': 0.892026424407959, 'motion_component': 12.002204895019531, 'motion_component_percent': 89.2026424407959}, {'resid': 458, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 5.152702331542969, 'force': [-2.531560182571411, -4.528322696685791, 0.12342345714569092], 'magnitude': 5.18938684463501, 'cosine_with_motion': -0.8340235352516174, 'motion_component': -4.328070640563965, 'motion_component_percent': 83.40235352516174}, {'resid': 458, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 4.911143779754639, 'force': [-1.3941073417663574, -5.352422714233398, 1.428246259689331], 'magnitude': 5.712429523468018, 'cosine_with_motion': -0.9657709002494812, 'motion_component': -5.516898155212402, 'motion_component_percent': 96.57709002494812}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': 0.14158325179697465, 'motion_component_pip2': 2.187741645817243, 'motion_component_percent_pip2': 14.158325179697465}, 968: {'frame': 968, 'motion_vector': [0.02275848388671875, 5.277462005615234, 2.4221115112304688], 'ionic_force': [10.573205828666687, -4.63816025853157, -3.354247186332941], 'ionic_force_magnitude': 12.023152093614856, 'radial_force': 11.545787633555921, 'axial_force': -3.354247186332941, 'glu_force': [2.6785926818847656, 3.2278904914855957, 0.8869214057922363], 'glu_force_magnitude': 4.287279482436644, 'asn_force': [11.029534339904785, -2.318687915802002, -5.595620840787888], 'asn_force_magnitude': 12.583239408033403, 'residue_force': [13.70812702178955, 0.9092025756835938, -4.708699434995651], 'residue_force_magnitude': 14.522783691092934, 'total_force': [24.281332850456238, -3.7289576828479767, -8.062946621328592], 'total_force_magnitude': 25.855354544339754, 'cosine_total_motion': 0, 'cosine_glu_motion': 0.7730071987626678, 'cosine_asn_motion': -0.34952281906469684, 'cosine_residue_motion': -0.0746435002330625, 'cosine_ionic_motion': -0.46352573330703795, 'motion_component_total': 0, 'motion_component_glu': 3.3140979030310103, 'motion_component_asn': -4.3981293108618225, 'motion_component_residue': -1.0840314078308118, 'motion_component_ionic': -5.5730403908548745, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 77.30071987626678, 'motion_component_percent_asn': 34.952281906469686, 'motion_component_percent_residue': 7.46435002330625, 'motion_component_percent_ionic': 46.35257333070379, 'ionic_contributions': [{'ion_id': 2333, 'distance': 11.577263832092285, 'force': [1.7472671270370483, -1.7365859746932983, -0.2585771977901459], 'magnitude': 2.477001428604126, 'cosine_ionic_motion': -0.6779547929763794, 'motion_component_ionic': -1.6792949438095093, 'motion_component_percent_ionic': 67.79547929763794}, {'ion_id': 2334, 'distance': 10.844830513000488, 'force': [1.9372375011444092, -0.6883694529533386, -1.9344027042388916], 'magnitude': 2.822880744934082, 'cosine_ionic_motion': -0.504768431186676, 'motion_component_ionic': -1.4249011278152466, 'motion_component_percent_ionic': 50.4768431186676}, {'ion_id': 2372, 'distance': 7.947305679321289, 'force': [4.489342212677002, -2.4995973110198975, -1.1085189580917358], 'magnitude': 5.256519317626953, 'cosine_ionic_motion': -0.5167929530143738, 'motion_component_ionic': -2.716531991958618, 'motion_component_percent_ionic': 51.67929530143738}, {'ion_id': 2397, 'distance': 11.720165252685547, 'force': [2.3993589878082275, 0.286392480134964, -0.05274832621216774], 'magnitude': 2.416966438293457, 'cosine_ionic_motion': 0.10247873514890671, 'motion_component_ionic': 0.2476876676082611, 'motion_component_percent_ionic': 10.24787351489067}], 'glu_contributions': [{'resid': 426, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 5.782297611236572, 'force': [-4.813831329345703, -4.684009075164795, -4.341140270233154], 'magnitude': 7.997400283813477, 'cosine_with_motion': -0.7610806226730347, 'motion_component': -6.086666584014893, 'motion_component_percent': 76.10806226730347}, {'resid': 426, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 4.742635726928711, 'force': [7.492424011230469, 7.911899566650391, 5.228061676025391], 'magnitude': 12.085826873779297, 'cosine_with_motion': 0.7778337597846985, 'motion_component': 9.400764465332031, 'motion_component_percent': 77.78337597846985}], 'asn_contributions': [{'resid': 458, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 3.5314252376556396, 'force': [-13.5960111618042, -9.933279991149902, 8.893770217895508], 'magnitude': 19.0426025390625, 'cosine_with_motion': -0.28206977248191833, 'motion_component': -5.371342658996582, 'motion_component_percent': 28.206977248191833}, {'resid': 458, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 2.7375664710998535, 'force': [22.64103889465332, 7.002033233642578, -12.133611679077148], 'magnitude': 26.624605178833008, 'cosine_with_motion': 0.05225811153650284, 'motion_component': 1.391351580619812, 'motion_component_percent': 5.225811153650284}, {'resid': 458, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 4.26260232925415, 'force': [12.208147048950195, 10.671919822692871, -3.5464532375335693], 'magnitude': 16.59837532043457, 'cosine_with_motion': 0.49810126423835754, 'motion_component': 8.267671585083008, 'motion_component_percent': 49.810126423835754}, {'resid': 458, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 3.9218902587890625, 'force': [-6.7576470375061035, -5.877832889556885, -0.15883514285087585], 'magnitude': 8.957674980163574, 'cosine_with_motion': -0.6067168116569519, 'motion_component': -5.43477201461792, 'motion_component_percent': 60.67168116569519}, {'resid': 458, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 4.961802959442139, 'force': [-3.4659934043884277, -4.181528091430664, 1.3495090007781982], 'magnitude': 5.596379280090332, 'cosine_with_motion': -0.58091801404953, 'motion_component': -3.25103759765625, 'motion_component_percent': 58.091801404953}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': -0.25747362262116225, 'motion_component_pip2': -6.657071798685687, 'motion_component_percent_pip2': 25.747362262116226}, 969: {'frame': 969, 'motion_vector': [0.06914520263671875, -0.8532905578613281, -0.9558258056640625], 'ionic_force': [23.3188294172287, -6.47792075574398, 9.66217988729477], 'ionic_force_magnitude': 26.059335810452897, 'radial_force': 24.20188551967613, 'axial_force': 9.66217988729477, 'glu_force': [14.73054313659668, -3.699486494064331, -0.67975914478302], 'glu_force_magnitude': 15.203196174285724, 'asn_force': [0.24505117535591125, -4.6175923347473145, -3.315617084503174], 'asn_force_magnitude': 5.689949534003777, 'residue_force': [14.975594311952591, -8.317078828811646, -3.995376229286194], 'residue_force_magnitude': 17.589919171343535, 'total_force': [38.29442372918129, -14.794999584555626, 5.666803658008575], 'total_force_magnitude': 41.44234024708913, 'cosine_total_motion': 0, 'cosine_glu_motion': 0.24733429216344024, 'cosine_asn_motion': 0.9760518715233434, 'cosine_residue_motion': 0.5295054266707716, 'cosine_ionic_motion': -0.06266569172519622, 'motion_component_total': 0, 'motion_component_glu': 3.7602717643888823, 'motion_component_asn': 5.553685891537762, 'motion_component_residue': 9.313957655926643, 'motion_component_ionic': -1.6330263044612074, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 24.733429216344025, 'motion_component_percent_asn': 97.60518715233434, 'motion_component_percent_residue': 52.95054266707716, 'motion_component_percent_ionic': 6.266569172519622, 'ionic_contributions': [{'ion_id': 2230, 'distance': 14.364006996154785, 'force': [0.969893217086792, 0.46612340211868286, -1.1963629722595215], 'magnitude': 1.6091140508651733, 'cosine_ionic_motion': 0.3936755955219269, 'motion_component_ionic': 0.6334689259529114, 'motion_component_percent_ionic': 39.36755955219269}, {'ion_id': 2333, 'distance': 13.319838523864746, 'force': [1.80675208568573, 0.24648697674274445, 0.4202408194541931], 'magnitude': 1.8712859153747559, 'cosine_ionic_motion': -0.2028500884771347, 'motion_component_ionic': -0.3795905113220215, 'motion_component_percent_ionic': 20.28500884771347}, {'ion_id': 2334, 'distance': 8.872391700744629, 'force': [3.355475902557373, 1.4490330219268799, -2.104405641555786], 'magnitude': 4.217515468597412, 'cosine_ionic_motion': 0.18607991933822632, 'motion_component_ionic': 0.7847949266433716, 'motion_component_percent_ionic': 18.607991933822632}, {'ion_id': 2372, 'distance': 3.8736305236816406, 'force': [15.835994720458984, -9.779850959777832, 11.963815689086914], 'magnitude': 22.12593650817871, 'cosine_ionic_motion': -0.07027879357337952, 'motion_component_ionic': -1.5549840927124023, 'motion_component_percent_ionic': 7.027879357337952}, {'ion_id': 2397, 'distance': 13.359997749328613, 'force': [1.3507134914398193, 1.1402868032455444, 0.5788919925689697], 'magnitude': 1.8600529432296753, 'cosine_ionic_motion': -0.6003677845001221, 'motion_component_ionic': -1.116715908050537, 'motion_component_percent_ionic': 60.03677845001221}], 'glu_contributions': [{'resid': 426, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645</t>
+          <t xml:space="preserve">{963: {'frame': 963, 'motion_vector': [-6.639595031738281, 1.0836753845214844, 2.0808258056640625], 'ionic_force': [-0.03461587429046631, -3.451846368610859, -26.245480060577393], 'ionic_force_magnitude': 26.47152555523407, 'radial_force': 3.452019932046289, 'axial_force': -26.245480060577393, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [0.6113827228546143, -0.2678259313106537, -0.847156286239624], 'asn_force_magnitude': 1.0785144118660877, 'residue_force': [0.6113827228546143, -0.2678259313106537, -0.847156286239624], 'residue_force_magnitude': 1.0785144118660877, 'pip2_force': [0.9694522628251434, 0.05543461270281114, -4.4345879283257545], 'pip2_force_magnitude': 4.53965646059642, 'total_force': [1.5462191113892914, -3.6642376872187015, -31.52722427514277], 'total_force_magnitude': 31.777087686948455, 'cosine_total_motion': -0.356792005652496, 'cosine_glu_motion': 0, 'cosine_asn_motion': -0.8048084027521138, 'cosine_residue_motion': -0.8048084027521138, 'cosine_pip2_motion': -0.4881252484365865, 'cosine_ionic_motion': -0.311802673918244, 'motion_component_total': -11.337810849621576, 'motion_component_glu': 0, 'motion_component_asn': -0.8679974611590815, 'motion_component_residue': -0.8679974611590815, 'motion_component_ionic': -8.253892450817112, 'motion_component_pip2': -2.2159209376453823, 'motion_component_percent_total': 35.6792005652496, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 80.48084027521139, 'motion_component_percent_residue': 80.48084027521139, 'motion_component_percent_ionic': 31.1802673918244, 'motion_component_percent_pip2': 48.81252484365865, 'ionic_contributions': [{'ion_id': 2230, 'distance': 14.592389106750488, 'force': [0.16000592708587646, 0.08226221054792404, -1.5487253665924072], 'magnitude': 1.5591405630111694, 'cosine_ionic_motion': -0.3821600377559662, 'motion_component_ionic': -0.5958412289619446, 'motion_component_percent_ionic': 38.21600377559662}, {'ion_id': 2333, 'distance': 4.4050493240356445, 'force': [1.2773457765579224, -5.039449691772461, -16.30049705505371], 'magnitude': 17.109468460083008, 'cosine_ionic_motion': -0.3972393572330475, 'motion_component_ionic': -6.796554088592529, 'motion_component_percent_ionic': 39.72393572330475}, {'ion_id': 2334, 'distance': 9.08781909942627, 'force': [0.15932977199554443, 0.28409475088119507, -4.006714344024658], 'magnitude': 4.019932270050049, 'cosine_ionic_motion': -0.32101526856422424, 'motion_component_ionic': -1.2904596328735352, 'motion_component_percent_ionic': 32.101526856422424}, {'ion_id': 2372, 'distance': 7.211418151855469, 'force': [-5.535534858703613, -1.084515929222107, -2.9896254539489746], 'magnitude': 6.38405704498291, 'cosine_ionic_motion': 0.6530299186706543, 'motion_component_ionic': 4.168980121612549, 'motion_component_percent_ionic': 65.30299186706543}, {'ion_id': 2397, 'distance': 8.364306449890137, 'force': [3.9042375087738037, 2.30576229095459, -1.3999178409576416], 'magnitude': 4.745459079742432, 'cosine_ionic_motion': -0.7881255149841309, 'motion_component_ionic': -3.7400174140930176, 'motion_component_percent_ionic': 78.81255149841309}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 5.723193645477295, 'force': [-7.815121173858643, -2.1620965003967285, -4.361874580383301], 'magnitude': 9.207427978515625, 'cosine_with_motion': 0.6241716742515564, 'motion_component': 5.747015476226807, 'motion_component_percent': 62.41716742515564}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 5.179661750793457, 'force': [4.4384284019470215, 0.4155177175998688, 2.5497331619262695], 'magnitude': 5.135507583618164, 'cosine_with_motion': -0.6557264924049377, 'motion_component': -3.367488384246826, 'motion_component_percent': 65.57264924049377}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 5.5684099197387695, 'force': [3.3907041549682617, 1.6970765590667725, 2.3168129920959473], 'magnitude': 4.443485736846924, 'cosine_with_motion': -0.506635844707489, 'motion_component': -2.2512290477752686, 'motion_component_percent': 50.6635844707489}, {'resid': 786, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 5.938525199890137, 'force': [-2.098083734512329, -5.628914833068848, 3.042907476425171], 'magnitude': 6.733938217163086, 'cosine_with_motion': 0.2986576557159424, 'motion_component': 2.0111422538757324, 'motion_component_percent': 29.86576557159424}, {'resid': 786, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 5.167057991027832, 'force': [2.6954550743103027, 5.410591125488281, -4.394735336303711], 'magnitude': 7.473531246185303, 'cosine_with_motion': -0.4024118483066559, 'motion_component': -3.0074374675750732, 'motion_component_percent': 40.24118483066559}], 'pip2_contributions': [{'resid': 1313, 'atom': 'C1', 'charge': 0.06000000238418579, 'distance': 26.762588500976562, 'force': [-0.019891858100891113, -0.014739428646862507, 0.01267177239060402], 'magnitude': 0.027812058106064796, 'cosine_with_motion': 0.7274393439292908, 'motion_component': 0.020231585949659348, 'motion_component_percent': 72.74393439292908}, {'resid': 1313, 'atom': 'C11', 'charge': 0.17000000178813934, 'distance': 26.427982330322266, 'force': [-0.0638677179813385, -0.04040871933102608, 0.0286028403788805], 'magnitude': 0.0808088630437851, 'cosine_with_motion': 0.7728402614593506, 'motion_component': 0.06245234236121178, 'motion_component_percent': 77.28402614593506}, {'resid': 1313, 'atom': 'C12', 'charge': 0.04000000283122063, 'distance': 26.833744049072266, 'force': [-0.01504645124077797, -0.00906425155699253, 0.005620868876576424], 'magnitude': 0.018443170934915543, 'cosine_with_motion': 0.7836431264877319, 'motion_component': 0.014452864415943623, 'motion_component_percent': 78.3643126487732}, {'resid': 1313, 'atom': 'C13', 'charge': -0.05000000074505806, 'distance': 27.97826385498047, 'force': [0.017085665836930275, 0.011044013313949108, -0.005985010415315628], 'magnitude': 0.021206380799412727, 'cosine_with_motion': -0.762907862663269, 'motion_component': -0.016178514808416367, 'motion_component_percent': 76.2907862663269}, {'resid': 1313, 'atom': 'C2', 'charge': 0.06000000238418579, 'distance': 28.321269989013672, 'force': [-0.017902033403515816, -0.013132689520716667, 0.011127717792987823], 'magnitude': 0.02483498305082321, 'cosine_with_motion': 0.7306807637214661, 'motion_component': 0.018146444112062454, 'motion_component_percent': 73.0680763721466}, {'resid': 1313, 'atom': 'C21', 'charge': 0.6299999952316284, 'distance': 24.583093643188477, 'force': [-0.2893790006637573, -0.16362537443637848, 0.09630119800567627], 'magnitude': 0.34610313177108765, 'cosine_with_motion': 0.7978042960166931, 'motion_component': 0.2761225700378418, 'motion_component_percent': 79.78042960166931}, {'resid': 1313, 'atom': 'C210', 'charge': -0.18000000715255737, 'distance': 25.10736656188965, 'force': [0.06947992742061615, 0.06443540006875992, -0.0027669069822877645], 'magnitude': 0.09479998052120209, 'cosine_with_motion': -0.5950649976730347, 'motion_component': -0.05641215294599533, 'motion_component_percent': 59.50649976730347}, {'resid': 1313, 'atom': 'C211', 'charge': -0.15000000596046448, 'distance': 26.290699005126953, 'force': [0.05240496248006821, 0.04924248903989792, -0.004459430929273367], 'magnitude': 0.07204851508140564, 'cosine_with_motion': -0.598913848400116, 'motion_component': -0.043150853365659714, 'motion_component_percent': 59.8913848400116}, {'resid': 1313, 'atom': 'C212', 'charge': -0.15000000596046448, 'distance': 27.569135665893555, 'force': [0.047940317541360855, 0.044577740132808685, -0.0027571427635848522], 'magnitude': 0.06552137434482574, 'cosine_with_motion': -0.5976083278656006, 'motion_component': -0.039156120270490646, 'motion_component_percent': 59.76083278656006}, {'resid': 1313, 'atom': 'C213', 'charge': -0.18000000715255737, 'distance': 27.952190399169922, 'force': [0.05667218938469887, 0.051358774304389954, 0.0007519636419601738], 'magnitude': 0.07648546248674393, 'cosine_with_motion': -0.5923830270767212, 'motion_component': -0.04530869051814079, 'motion_component_percent': 59.23830270767212}, {'resid': 1313, 'atom': 'C214', 'charge': -0.15000000596046448, 'distance': 28.414627075195312, 'force': [0.04377865046262741, 0.04339771345257759, 0.0021235353779047728], 'magnitude': 0.061680153012275696, 'cosine_with_motion': -0.5507704019546509, 'motion_component': -0.03397160395979881, 'motion_component_percent': 55.07704019546509}, {'resid': 1313, 'atom': 'C215', 'charge': -0.15000000596046448, 'distance': 28.393760681152344, 'force': [0.04319930821657181, 0.043883685022592545, 0.004866094794124365], 'magnitude': 0.06177084147930145, 'cosine_with_motion': -0.5267885327339172, 'motion_component': -0.03254017233848572, 'motion_component_percent': 52.678853273391724}, {'resid': 1313, 'atom': 'C216', 'charge': -0.18000000715255737, 'distance': 28.03108787536621, 'force': [0.05454341322183609, 0.052216220647096634, 0.009106190875172615], 'magnitude': 0.07605551183223724, 'cosine_with_motion': -0.5351482033729553, 'motion_component': -0.04070097208023071, 'motion_component_percent': 53.51482033729553}, {'resid': 1313, 'atom': 'C217', 'charge': -0.18000000715255737, 'distance': 29.268497467041016, 'force': [0.049641840159893036, 0.047776564955711365, 0.010936998762190342], 'magnitude': 0.0697605237364769, 'cosine_with_motion': -0.5192286372184753, 'motion_component': -0.03622166067361832, 'motion_component_percent': 51.922863721847534}, {'resid': 1313, 'atom': 'C218', 'charge': -0.18000000715255737, 'distance': 29.321205139160156, 'force': [0.04684366285800934, 0.04973236843943596, 0.012806112878024578], 'magnitude': 0.06950995326042175, 'cosine_with_motion': -0.47086864709854126, 'motion_component': -0.03273005783557892, 'motion_component_percent': 47.086864709854126}, {'resid': 1313, 'atom': 'C219', 'charge': -0.18000000715255737, 'distance': 29.887514114379883, 'force': [0.04465264454483986, 0.04732326418161392, 0.015567946247756481], 'magnitude': 0.06690075248479843, 'cosine_with_motion': -0.4516966938972473, 'motion_component': -0.03021884895861149, 'motion_component_percent': 45.16966938972473}, {'resid': 1313, 'atom': 'C22', 'charge': -0.08000000566244125, 'distance': 23.702129364013672, 'force': [0.039832428097724915, 0.023036548867821693, -0.01085564587265253], 'magnitude': 0.04727737233042717, 'cosine_with_motion': -0.7872570753097534, 'motion_component': -0.037219446152448654, 'motion_component_percent': 78.72570753097534}, {'resid': 1313, 'atom': 'C220', 'charge': -0.27000001072883606, 'distance': 29.59727668762207, 'force': [0.0644836500287056, 0.07494063675403595, 0.02640010416507721], 'magnitude': 0.10232891142368317, 'cosine_with_motion': -0.4052232801914215, 'motion_component': -0.04146605730056763, 'motion_component_percent': 40.52232801914215}, {'resid': 1313, 'atom': 'C23', 'charge': -0.18000000715255737, 'distance': 22.757890701293945, 'force': [0.09399432688951492, 0.06091022491455078, -0.027722574770450592], 'magnitude': 0.11538427323102951, 'cosine_with_motion': -0.7578391432762146, 'motion_component': -0.08744271844625473, 'motion_component_percent': 75.78391432762146}, {'resid': 1313, 'atom': 'C24', 'charge': -0.18000000715255737, 'distance': 23.43341827392578, 'force': [0.08493218570947647, 0.06298304349184036, -0.025751154869794846], 'magnitude': 0.10882766544818878, 'cosine_with_motion': -0.7166998982429504, 'motion_component': -0.07799677550792694, 'motion_component_percent': 71.66998982429504}, {'resid': 1313, 'atom': 'C25', 'charge': -0.15000000596046448, 'distance': 24.402074813842773, 'force': [0.06551200896501541, 0.049481309950351715, -0.015943532809615135], 'magnitude': 0.08363264799118042, 'cosine_with_motion': -0.7038614153862, 'motion_component': -0.05886579304933548, 'motion_component_percent': 70.38614153862}, {'resid': 1313, 'atom': 'C26', 'charge': -0.15000000596046448, 'distance': 24.217132568359375, 'force': [0.0664040669798851, 0.051584258675575256, -0.01183658093214035], 'magnitude': 0.08491490036249161, 'cosine_with_motion': -0.6850351691246033, 'motion_component': -0.05816969275474548, 'motion_component_percent': 68.50351691246033}, {'resid': 1313, 'atom': 'C27', 'charge': -0.18000000715255737, 'distance': 22.966123580932617, 'force': [0.08796126395463943, 0.07035423070192337, -0.012259798124432564], 'magnitude': 0.11330138891935349, 'cosine_with_motion': -0.6684107184410095, 'motion_component': -0.07573186606168747, 'motion_component_percent': 66.84107184410095}, {'resid': 1313, 'atom': 'C28', 'charge': -0.15000000596046448, 'distance': 22.98751449584961, 'force': [0.06928504258394241, 0.06328228861093521, -0.008747700601816177], 'magnitude': 0.09424217790365219, 'cosine_with_motion': -0.6172727942466736, 'motion_component': -0.05817313492298126, 'motion_component_percent': 61.72727942466736}, {'resid': 1313, 'atom': 'C29', 'charge': -0.15000000596046448, 'distance': 23.79194450378418, 'force': [0.06329765170812607, 0.06089157611131668, -0.005058333743363619], 'magnitude': 0.08797705918550491, 'cosine_with_motion': -0.5888527631759644, 'motion_component': -0.0518055334687233, 'motion_component_percent': 58.885276317596436}, {'resid': 1313, 'atom': 'C3', 'charge': 0.06000000238418579, 'distance': 29.115154266357422, 'force': [-0.016818678006529808, -0.01179804839193821, 0.011408139020204544], 'magnitude': 0.02349909581243992, 'cosine_with_motion': 0.7410171031951904, 'motion_component': 0.01741323247551918, 'motion_component_percent': 74.10171031951904}, {'resid': 1313, 'atom': 'C31', 'charge': 0.6299999952316284, 'distance': 29.007389068603516, 'force': [-0.21095629036426544, -0.11783666908740997, 0.058331817388534546], 'magnitude': 0.24857722222805023, 'cosine_with_motion': 0.7965611815452576, 'motion_component': 0.19800697267055511, 'motion_component_percent': 79.65611815452576}, {'resid': 1313, 'atom': 'C310', 'charge': -0.18000000715255737, 'distance': 25.97843360900879, 'force': [0.08632601797580719, 0.01921309158205986, -0.004431640263646841], 'magnitude': 0.08854921907186508, 'cosine_with_motion': -0.9005948305130005, 'motion_component': -0.07974696904420853, 'motion_component_percent': 90.05948305130005}, {'resid': 1313, 'atom': 'C311', 'charge': -0.18000000715255737, 'distance': 25.659189224243164, 'force': [0.08941670507192612, 0.015544496476650238, -0.0012443121522665024], 'magnitude': 0.09076633304357529, 'cosine_with_motion': -0.9065455794334412, 'motion_component': -0.08228381723165512, 'motion_component_percent': 90.65455794334412}, {'resid': 1313, 'atom': 'C312', 'charge': -0.18000000715255737, 'distance': 26.09272003173828, 'force': [0.08710889518260956, 0.01043660193681717, -0.0027579437009990215], 'magnitude': 0.08777521550655365, 'cosine_with_motion': -0.926698625087738, 'motion_component': -0.08134116977453232, 'motion_component_percent': 92.6698625087738}, {'resid': 1313, 'atom': 'C313', 'charge': -0.18000000715255737, 'distance': 25.839996337890625, 'force': [0.08925434947013855, 0.006611107382923365, 0.0005515532102435827], 'magnitude': 0.0895005539059639, 'cosine_with_motion': -0.9270873069763184, 'motion_component': -0.08297482877969742, 'motion_component_percent': 92.70873069763184}, {'resid': 1313, 'atom': 'C314', 'charge': -0.18000000715255737, 'distance': 26.229080200195312, 'force': [0.08684282749891281, 0.0014933100901544094, -0.001269129803404212], 'magnitude': 0.08686493337154388, 'cosine_with_motion': -0.9443010091781616, 'motion_component': -0.0820266455411911, 'motion_component_percent': 94.43010091781616}, {'resid': 1313, 'atom': 'C315', 'charge': -0.18000000715255737, 'distance': 26.034404754638672, 'force': [0.08811075240373611, -0.0024179653264582157, 0.002097445772960782], 'magnitude': 0.08816887438297272, 'cosine_with_motion': -0.9394385814666748, 'motion_component': -0.08282924443483353, 'motion_component_percent': 93.94385814666748}, {'resid': 1313, 'atom': 'C316', 'charge': -0.18000000715255737, 'distance': 26.812908172607422, 'force': [0.082877516746521, -0.006364058703184128, 0.0005459367530420423], 'magnitude': 0.08312329649925232, 'cosine_with_motion': -0.9499227404594421, 'motion_component': -0.07896070927381516, 'motion_component_percent': 94.99227404594421}, {'resid': 1313, 'atom': 'C317', 'charge': -0.18000000715255737, 'distance': 26.729522705078125, 'force': [0.08298132568597794, -0.009512803517282009, 0.00443989085033536], 'magnitude': 0.08364273607730865, 'cosine_with_motion': -0.9372303485870361, 'motion_component': -0.07839251309633255, 'motion_component_percent': 93.72303485870361}, {'resid': 1313, 'atom': 'C318', 'charge': -0.27000001072883606, 'distance': 27.670429229736328, 'force': [0.11544671654701233, -0.01858649030327797, 0.005790174473077059], 'magnitude': 0.11707659065723419, 'cosine_with_motion': -0.9395599961280823, 'motion_component': -0.11000048369169235, 'motion_component_percent': 93.95599961280823}, {'resid': 1313, 'atom': 'C32', 'charge': -0.08000000566244125, 'distance': 29.195816040039062, 'force': [0.026941383257508278, 0.014539418742060661, -0.005802188068628311], 'magnitude': 0.031159238889813423, 'cosine_with_motion': -0.7984546422958374, 'motion_component': -0.02487923949956894, 'motion_component_percent': 79.84546422958374}, {'resid': 1313, 'atom': 'C33', 'charge': -0.18000000715255737, 'distance': 28.14741325378418, 'force': [0.06660670042037964, 0.03305990993976593, -0.012649143114686012], 'magnitude': 0.07542818039655685, 'cosine_with_motion': -0.8147029280662537, 'motion_component': -0.06145155802369118, 'motion_component_percent': 81.47029280662537}, {'resid': 1313, 'atom': 'C34', 'charge': -0.18000000715255737, 'distance': 28.376157760620117, 'force': [0.06680087745189667, 0.029195137321949005, -0.013908675871789455], 'magnitude': 0.07421700656414032, 'cosine_with_motion': -0.843493640422821, 'motion_component': -0.06260157376527786, 'motion_component_percent': 84.3493640422821}, {'resid': 1313, 'atom': 'C35', 'charge': -0.18000000715255737, 'distance': 27.184528350830078, 'force': [0.07392701506614685, 0.02956741489470005, -0.014138811267912388], 'magnitude': 0.08086619526147842, 'cosine_with_motion': -0.8573582768440247, 'motion_component': -0.06933130323886871, 'motion_component_percent': 85.73582768440247}, {'resid': 1313, 'atom': 'C36', 'charge': -0.18000000715255737, 'distance': 27.032487869262695, 'force': [0.07575861364603043, 0.029172390699386597, -0.009864569641649723], 'magnitude': 0.0817783921957016, 'cosine_with_motion': -0.8542115688323975, 'motion_component': -0.06985604763031006, 'motion_component_percent': 85.42115688323975}, {'resid': 1313, 'atom': 'C37', 'charge': -0.18000000715255737, 'distance': 26.099279403686523, 'force': [0.08267445862293243, 0.02787947840988636, -0.009187712334096432], 'magnitude': 0.08773110061883926, 'cosine_with_motion': -0.8705663681030273, 'motion_component': -0.07637574523687363, 'motion_component_percent': 87.05663681030273}, {'resid': 1313, 'atom': 'C38', 'charge': -0.18000000715255737, 'distance': 26.150400161743164, 'force': [0.08292005956172943, 0.027304742485284805, -0.003930915612727404], 'magnitude': 0.08738842606544495, 'cosine_with_motion': -0.8598669767379761, 'motion_component': -0.07514242082834244, 'motion_component_percent': 85.98669767379761}, {'resid': 1313, 'atom': 'C39', 'charge': -0.18000000715255737, 'distance': 25.37773323059082, 'force': [0.08940848708152771, 0.02473253756761551, -0.0021344078704714775], 'magnitude': 0.09279079735279083, 'cosine_with_motion': -0.8742800354957581, 'motion_component': -0.08112514019012451, 'motion_component_percent': 87.4280035495758}, {'resid': 1313, 'atom': 'C4', 'charge': 0.08000000566244125, 'distance': 28.958219528198242, 'force': [-0.02157505974173546, -0.016244444996118546, 0.016546646133065224], 'magnitude': 0.0316726490855217, 'cosine_with_motion': 0.7177174091339111, 'motion_component': 0.02273201197385788, 'motion_component_percent': 71.77174091339111}, {'resid': 1313, 'atom': 'C5', 'charge': 0.08000000566244125, 'distance': 27.434900283813477, 'force': [-0.023836206644773483, -0.017842208966612816, 0.01893940195441246], 'magnitude': 0.035287536680698395, 'cosine_with_motion': 0.7176793813705444, 'motion_component': 0.025325138121843338, 'motion_component_percent': 71.76793813705444}, {'resid': 1313, 'atom': 'C6', 'charge': 0.06000000238418579, 'distance': 26.474260330200195, 'force': [-0.019330289214849472, -0.01518103014677763, 0.014270185492932796], 'magnitude': 0.028421154245734215, 'cosine_with_motion': 0.7074469327926636, 'motion_component': 0.02010645903646946, 'motion_component_percent': 70.74469327926636}, {'resid': 1313, 'atom': 'H1', 'charge': 0.12000000476837158, 'distance': 26.296268463134766, 'force': [-0.042390353977680206, -0.028736749663949013, 0.026394642889499664], 'magnitude': 0.05761440843343735, 'cosine_with_motion': 0.7523410320281982, 'motion_component': 0.04334568232297897, 'motion_component_percent': 75.23410320281982}, {'resid': 1313, 'atom': 'H10R', 'charge': 0.09000000357627869, 'distance': 25.20809555053711, 'force': [-0.033974312245845795, -0.032504238188266754, -0.0005324145313352346], 'magnitude': 0.04702194035053253, 'cosine_with_motion': 0.5715193152427673, 'motion_component': 0.02687394805252552, 'motion_component_percent': 57.15193152427673}, {'resid': 1313, 'atom': 'H10S', 'charge': 0.09000000357627869, 'distance': 25.097301483154297, 'force': [-0.036136139184236526, -0.030713576823472977, 0.0011052251793444157], 'magnitude': 0.04743802174925804, 'cosine_with_motion': 0.6254844665527344, 'motion_component': 0.029671745374798775, 'motion_component_percent': 62.54844665527344}, {'resid': 1313, 'atom': 'H10X', 'charge': 0.09000000357627869, 'distance': 27.070980072021484, 'force': [-0.03971916064620018, -0.00898080412298441, 0.002042219275608659], 'magnitude': 0.040772996842861176, 'cosine_with_motion': 0.8994037508964539, 'motion_component': 0.036671385169029236, 'motion_component_percent': 89.94037508964539}, {'resid': 1313, 'atom': 'H10Y', 'charge': 0.09000000357627869, 'distance': 25.797964096069336, 'force': [-0.043643224984407425, -0.009694688953459263, 0.0041172681376338005], 'magnitude': 0.044896211475133896, 'cosine_with_motion': 0.9104235172271729, 'motion_component': 0.04087456688284874, 'motion_component_percent': 91.04235172271729}, {'resid': 1313, 'atom': 'H111', 'charge': 0.15000000596046448, 'distance': 26.16447639465332, 'force': [-0.05233442410826683, -0.04997745528817177, 0.0074329255148768425], 'magnitude': 0.07274535298347473, 'cosine_with_motion': 0.6027860045433044, 'motion_component': 0.0438498817384243, 'motion_component_percent': 60.278600454330444}, {'resid': 1313, 'atom': 'H11A', 'charge': 0.09000000357627869, 'distance': 27.372461318969727, 'force': [-0.031167317181825638, -0.01995127461850643, 0.014864152297377586], 'magnitude': 0.03987979516386986, 'cosine_with_motion': 0.7700303196907043, 'motion_component': 0.03070865198969841, 'motion_component_percent': 77.00303196907043}, {'resid': 1313, 'atom': 'H11B', 'charge': 0.09000000357627869, 'distance': 25.84989356994629, 'force': [-0.03565007820725441, -0.021130848675966263, 0.016795270144939423], 'magnitude': 0.044716011732816696, 'cosine_with_motion': 0.7899724245071411, 'motion_component': 0.03532441705465317, 'motion_component_percent': 78.99724245071411}, {'resid': 1313, 'atom': 'H11X', 'charge': 0.09000000357627869, 'distance': 24.572185516357422, 'force': [-0.04877587780356407, -0.0083494633436203, 0.00043011916568502784], 'magnitude': 0.049487218260765076, 'cosine_with_motion': 0.9059203863143921, 'motion_component': 0.04483148083090782, 'motion_component_percent': 90.59203863143921}, {'resid': 1313, 'atom': 'H11Y', 'charge': 0.09000000357627869, 'distance': 26.15770721435547, 'force': [-0.043004684150218964, -0.007520244922488928, -0.0010463681537657976], 'magnitude': 0.04366980493068695, 'cosine_with_motion': 0.8949276804924011, 'motion_component': 0.03908131644129753, 'motion_component_percent': 89.49276804924011}, {'resid': 1313, 'atom': 'H12', 'charge': 0.09000000357627869, 'distance': 27.15093231201172, 'force': [-0.03377176448702812, -0.01853279210627079, 0.012607368640601635], 'magnitude': 0.04053322225809097, 'cosine_with_motion': 0.8071337342262268, 'motion_component': 0.032715730369091034, 'motion_component_percent': 80.71337342262268}, {'resid': 1313, 'atom': 'H121', 'charge': 0.15000000596046448, 'distance': 28.41805076599121, 'force': [-0.04488736391067505, -0.04208515211939812, 0.00407102657482028], 'magnitude': 0.06166529655456543, 'cosine_with_motion': 0.6008145809173584, 'motion_component': 0.03704940900206566, 'motion_component_percent': 60.08145809173584}, {'resid': 1313, 'atom': 'H12X', 'charge': 0.09000000357627869, 'distance': 27.175065994262695, 'force': [-0.04014155641198158, -0.004839177243411541, 0.0015334745403379202], 'magnitude': 0.040461260825395584, 'cosine_with_motion': 0.9282130599021912, 'motion_component': 0.03755667060613632, 'motion_component_percent': 92.82130599021912}, {'resid': 1313, 'atom': 'H12Y', 'charge': 0.09000000357627869, 'distance': 25.660133361816406, 'force': [-0.04497800022363663, -0.005124118644744158, 0.0031703573185950518], 'magnitude': 0.04537982493638992, 'cosine_with_motion': 0.9377877116203308, 'motion_component': 0.04255664348602295, 'motion_component_percent': 93.77877116203308}, {'resid': 1313, 'atom': 'H13A', 'charge': 0.09000000357627869, 'distance': 28.88711929321289, 'force': [-0.02864863909780979, -0.018541911616921425, 0.010845230892300606], 'magnitude': 0.035807348787784576, 'cosine_with_motion': 0.7641781568527222, 'motion_component': 0.027363194152712822, 'motion_component_percent': 76.41781568527222}, {'resid': 1313, 'atom': 'H13B', 'charge': 0.09000000357627869, 'distance': 27.65534782409668, 'force': [-0.030677251517772675, -0.021579217165708542, 0.010934384539723396], 'magnitude': 0.039068110287189484, 'cosine_with_motion': 0.7380660772323608, 'motion_component': 0.02883484587073326, 'motion_component_percent': 73.80660772323608}, {'resid': 1313, 'atom': 'H13R', 'charge': 0.09000000357627869, 'distance': 28.760705947875977, 'force': [-0.027386857196688652, -0.023553140461444855, -0.0002589247014839202], 'magnitude': 0.03612281009554863, 'cosine_with_motion': 0.6123868823051453, 'motion_component': 0.022121135145425797, 'motion_component_percent': 61.238688230514526}, {'resid': 1313, 'atom': 'H13S', 'charge': 0.09000000357627869, 'distance': 27.0929012298584, 'force': [-0.03061833791434765, -0.02680150792002678, -0.0011225523194298148], 'magnitude': 0.040707044303417206, 'cosine_with_motion': 0.5997220873832703, 'motion_component': 0.024412913247942924, 'motion_component_percent': 59.972208738327026}, {'resid': 1313, 'atom': 'H13X', 'charge': 0.09000000357627869, 'distance': 24.788251876831055, 'force': [-0.04848001152276993, -0.003689657198265195, -0.0008851448073983192], 'magnitude': 0.048628270626068115, 'cosine_with_motion': 0.922939658164978, 'motion_component': 0.04488096013665199, 'motion_component_percent': 92.2939658164978}, {'resid': 1313, 'atom': 'H13Y', 'charge': 0.09000000357627869, 'distance': 26.432100296020508, 'force': [-0.04258817806839943, -0.003513163421303034, -0.0017298310995101929], 'magnitude': 0.042767833918333054, 'cosine_with_motion': 0.9143155217170715, 'motion_component': 0.039103295654058456, 'motion_component_percent': 91.43155217170715}, {'resid': 1313, 'atom': 'H141', 'charge': 0.15000000596046448, 'distance': 28.823123931884766, 'force': [-0.0414947085082531, -0.04325687140226364, -0.0005840820958837867], 'magnitude': 0.059944216161966324, 'cosine_with_motion': 0.538746178150177, 'motion_component': 0.03229471668601036, 'motion_component_percent': 53.8746178150177}, {'resid': 1313, 'atom': 'H14X', 'charge': 0.09000000357627869, 'distance': 25.787490844726562, 'force': [-0.04486974701285362, -0.00038726991624571383, 0.0023458064533770084], 'magnitude': 0.04493269696831703, 'cosine_with_motion': 0.9556488394737244, 'motion_component': 0.04293987900018692, 'motion_component_percent': 95.56488394737244}, {'resid': 1313, 'atom': 'H14Y', 'charge': 0.09000000357627869, 'distance': 27.301780700683594, 'force': [-0.040067292749881744, -0.0009459464927203953, 0.0008054838981479406], 'magnitude': 0.04008655250072479, 'cosine_with_motion': 0.9447224140167236, 'motion_component': 0.03787066414952278, 'motion_component_percent': 94.47224140167236}, {'resid': 1313, 'atom': 'H151', 'charge': 0.15000000596046448, 'distance': 28.627288818359375, 'force': [-0.04085644334554672, -0.04468357935547829, -0.005174568388611078], 'magnitude': 0.06076715514063835, 'cosine_with_motion': 0.49561163783073425, 'motion_component': 0.030116910114884377, 'motion_component_percent': 49.561163783073425}, {'resid': 1313, 'atom': 'H15X', 'charge': 0.09000000357627869, 'distance': 24.97854995727539, 'force': [-0.04783531278371811, 0.001748983864672482, -0.0014797872863709927], 'magnitude': 0.04789014533162117, 'cosine_with_motion': 0.9382793307304382, 'motion_component': 0.04493433237075806, 'motion_component_percent': 93.82793307304382}, {'resid': 1313, 'atom': 'H15Y', 'charge': 0.09000000357627869, 'distance': 26.400726318359375, 'force': [-0.04278445616364479, 0.0006426721811294556, -0.002621977822855115], 'magnitude': 0.04286954179406166, 'cosine_with_motion': 0.9252321720123291, 'motion_component': 0.03966427966952324, 'motion_component_percent': 92.52321720123291}, {'resid': 1313, 'atom': 'H16R', 'charge': 0.09000000357627869, 'distance': 27.939992904663086, 'force': [-0.028446994721889496, -0.025280186906456947, -0.0040918029844760895], 'magnitude': 0.038276128470897675, 'cosine_with_motion': 0.5675168037414551, 'motion_component': 0.021722346544265747, 'motion_component_percent': 56.75168037414551}, {'resid': 1313, 'atom': 'H16S', 'charge': 0.09000000357627869, 'distance': 27.117799758911133, 'force': [-0.028651315718889236, -0.02827998250722885, -0.005507360212504864], 'magnitude': 0.040632329881191254, 'cosine_with_motion': 0.5176929831504822, 'motion_component': 0.021035071462392807, 'motion_component_percent': 51.76929831504822}, {'resid': 1313, 'atom': 'H16X', 'charge': 0.09000000357627869, 'distance': 27.834678649902344, 'force': [-0.03847725689411163, 0.002612429205328226, 0.00019136503397021443], 'magnitude': 0.038566313683986664, 'cosine_with_motion': 0.9525824785232544, 'motion_component': 0.0367375947535038, 'motion_component_percent': 95.25824785232544}, {'resid': 1313, 'atom': 'H16Y', 'charge': 0.09000000357627869, 'distance': 26.30425453186035, 'force': [-0.042986027896404266, 0.00397453224286437, 0.0011452377075329423], 'magnitude': 0.04318457096815109, 'cosine_with_motion': 0.9605340361595154, 'motion_component': 0.04148025065660477, 'motion_component_percent': 96.05340361595154}, {'resid': 1313, 'atom': 'H17R', 'charge': 0.09000000357627869, 'distance': 30.24349594116211, 'force': [-0.023321371525526047, -0.02241259068250656, -0.004578051622956991], 'magnitude': 0.032667554914951324, 'cosine_with_motion': 0.5261233448982239, 'motion_component': 0.01718716323375702, 'motion_component_percent': 52.61233448982239}, {'resid': 1313, 'atom': 'H17S', 'charge': 0.09000000357627869, 'distance': 29.127851486206055, 'force': [-0.025671811774373055, -0.02326877973973751, -0.006310627795755863], 'magnitude': 0.03521792218089104, 'cosine_with_motion': 0.5326720476150513, 'motion_component': 0.018759602680802345, 'motion_component_percent': 53.26720476150513}, {'resid': 1313, 'atom': 'H17X', 'charge': 0.09000000357627869, 'distance': 26.983400344848633, 'force': [-0.04068264365196228, 0.003966388292610645, -0.0036491143982857466], 'magnitude': 0.04103809967637062, 'cosine_with_motion': 0.9233010411262512, 'motion_component': 0.03789051994681358, 'motion_component_percent': 92.33010411262512}, {'resid': 1313, 'atom': 'H17Y', 'charge': 0.09000000357627869, 'distance': 25.737140655517578, 'force': [-0.04464470222592354, 0.0058729336597025394, -0.0026742257177829742], 'magnitude': 0.045108672231435776, 'cosine_with_motion': 0.9356889724731445, 'motion_component': 0.042207688093185425, 'motion_component_percent': 93.56889724731445}, {'resid': 1313, 'atom': 'H18R', 'charge': 0.09000000357627869, 'distance': 28.258777618408203, 'force': [-0.024967065081000328, -0.026963235810399055, -0.0070493388921022415], 'magnitude': 0.037417422980070114, 'cosine_with_motion': 0.46257320046424866, 'motion_component': 0.017308296635746956, 'motion_component_percent': 46.257320046424866}, {'resid': 1313, 'atom': 'H18S', 'charge': 0.09000000357627869, </t>
         </is>
       </c>
     </row>
@@ -659,7 +659,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>{1193: {'frame': 1193, 'motion_vector': [-6.644626617431641, -6.532619476318359, 5.509552001953125], 'ionic_force': [3.645001269876957, 0.4808567687869072, -8.289402723312378], 'ionic_force_magnitude': 9.068156096955514, 'radial_force': 3.676582310991121, 'axial_force': -8.289402723312378, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [4.907903671264648, -0.8141872882843018, 5.362216949462891], 'asn_force_magnitude': 7.314628493636834, 'residue_force': [4.907903671264648, -0.8141872882843018, 5.362216949462891], 'residue_force_magnitude': 7.314628493636834, 'total_force': [8.552904941141605, -0.33333051949739456, -2.9271857738494873], 'total_force_magnitude': 9.046088034175861, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': 0.028428536362227374, 'cosine_residue_motion': 0.028428536362227374, 'cosine_ionic_motion': -0.7439845571371395, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': 0.20794418210753918, 'motion_component_residue': 0.20794418210753918, 'motion_component_ionic': -6.7465680978439, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 2.8428536362227375, 'motion_component_percent_residue': 2.8428536362227375, 'motion_component_percent_ionic': 74.39845571371396, 'ionic_contributions': [{'ion_id': 2333, 'distance': 10.030160903930664, 'force': [1.0726981163024902, -2.0107765197753906, -2.386737108230591], 'magnitude': 3.300063371658325, 'cosine_ionic_motion': -0.1999226063489914, 'motion_component_ionic': -0.6597572565078735, 'motion_component_percent_ionic': 19.99226063489914}, {'ion_id': 2334, 'distance': 9.7400541305542, 'force': [-0.11895801872015, 2.5222208499908447, -2.423072099685669], 'magnitude': 3.49957537651062, 'cosine_ionic_motion': -0.7664731740951538, 'motion_component_ionic': -2.68233060836792, 'motion_component_percent_ionic': 76.64731740951538}, {'ion_id': 2372, 'distance': 10.768108367919922, 'force': [2.345862627029419, 0.040280118584632874, -1.6411902904510498], 'magnitude': 2.8632497787475586, 'cosine_ionic_motion': -0.8031269907951355, 'motion_component_ionic': -2.299553155899048, 'motion_component_percent_ionic': 80.31269907951355}, {'ion_id': 2515, 'distance': 13.31761646270752, 'force': [0.34539854526519775, -0.07086768001317978, -1.8384032249450684], 'magnitude': 1.8719104528427124, 'cosine_ionic_motion': -0.59026700258255, 'motion_component_ionic': -1.1049269437789917, 'motion_component_percent_ionic': 59.026700258255005}], 'glu_contributions': [], 'asn_contributions': [{'resid': 458, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 5.222881317138672, 'force': [4.907903671264648, -0.8141872882843018, 5.362216949462891], 'magnitude': 7.314628601074219, 'cosine_with_motion': 0.02842852473258972, 'motion_component': 0.2079440951347351, 'motion_component_percent': 2.842852473258972}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': -0.7228123240713142, 'motion_component_pip2': -6.538623915736361, 'motion_component_percent_pip2': 72.28123240713143}, 1194: {'frame': 1194, 'motion_vector': [9.83700180053711, 4.689785003662109, 0.42656707763671875], 'ionic_force': [-2.721445322036743, -9.564446866512299, -2.5387065913528204], 'ionic_force_magnitude': 10.263037545490656, 'radial_force': 9.944089123855065, 'axial_force': -2.5387065913528204, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [2.643080949783325, -2.555886059999466, 1.979728102684021], 'asn_force_magnitude': 4.17585366354761, 'residue_force': [2.643080949783325, -2.555886059999466, 1.979728102684021], 'residue_force_magnitude': 4.17585366354761, 'total_force': [-0.07836437225341797, -12.120332926511765, -0.5589784886687994], 'total_force_magnitude': 12.133468925872698, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': 0.32624510442478094, 'cosine_residue_motion': 0.32624510442478094, 'cosine_ionic_motion': -0.6495960899584495, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': 1.362351814526694, 'motion_component_residue': 1.362351814526694, 'motion_component_ionic': -6.666829060647493, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 32.6245104424781, 'motion_component_percent_residue': 32.6245104424781, 'motion_component_percent_ionic': 64.95960899584496, 'ionic_contributions': [{'ion_id': 2333, 'distance': 13.527481079101562, 'force': [-0.3991110324859619, -1.7573204040527344, -0.2101089507341385], 'magnitude': 1.814279556274414, 'cosine_ionic_motion': -0.6194639205932617, 'motion_component_ionic': -1.1238807439804077, 'motion_component_percent_ionic': 61.94639205932617}, {'ion_id': 2334, 'distance': 9.919899940490723, 'force': [-3.362597942352295, -0.2749153971672058, 0.0100990179926157], 'magnitude': 3.3738324642181396, 'cosine_ionic_motion': -0.9338929653167725, 'motion_component_ionic': -3.1507983207702637, 'motion_component_percent_ionic': 93.38929653167725}, {'ion_id': 2372, 'distance': 7.453216552734375, 'force': [2.2657206058502197, -5.503379821777344, -0.5463338494300842], 'magnitude': 5.976551055908203, 'cosine_ionic_motion': -0.057606227695941925, 'motion_component_ionic': -0.34428656101226807, 'motion_component_percent_ionic': 5.7606227695941925}, {'ion_id': 2515, 'distance': 10.569954872131348, 'force': [-1.225456953048706, -2.0288312435150146, -1.7923628091812134], 'magnitude': 2.9716098308563232, 'cosine_ionic_motion': -0.6891427040100098, 'motion_component_ionic': -2.047863245010376, 'motion_component_percent_ionic': 68.91427040100098}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 5.670623779296875, 'force': [2.94118332862854, -2.6045713424682617, 1.7101606130599976], 'magnitude': 4.284740447998047, 'cosine_with_motion': 0.37336063385009766, 'motion_component': 1.5997533798217773, 'motion_component_percent': 37.336063385009766}, {'resid': 1114, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 5.966697692871094, 'force': [6.902561664581299, -0.3321591019630432, -4.899620056152344], 'magnitude': 8.471242904663086, 'cosine_with_motion': 0.6954656839370728, 'motion_component': 5.891458988189697, 'motion_component_percent': 69.54656839370728}, {'resid': 1114, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 5.613275527954102, 'force': [-3.2479474544525146, -0.3471299111843109, 2.907090425491333], 'magnitude': 4.372737884521484, 'cosine_with_motion': -0.678094744682312, 'motion_component': -2.965130567550659, 'motion_component_percent': 67.8094744682312}, {'resid': 1114, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 5.465703964233398, 'force': [-3.952716588973999, 0.7279742956161499, 2.262097120285034], 'magnitude': 4.612049102783203, 'cosine_with_motion': -0.6859705448150635, 'motion_component': -3.1637299060821533, 'motion_component_percent': 68.59705448150635}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': -0.4371773050664714, 'motion_component_pip2': -5.3044772461208, 'motion_component_percent_pip2': 43.71773050664714}, 1195: {'frame': 1195, 'motion_vector': [-4.003147125244141, 5.795902252197266, 0.6796417236328125], 'ionic_force': [13.309521913528442, 13.192807465791702, -9.53001996781677], 'ionic_force_magnitude': 21.02414856737674, 'radial_force': 18.74015854778564, 'axial_force': -9.53001996781677, 'glu_force': [8.09528112411499, 4.124099493026733, 5.42849063873291], 'glu_force_magnitude': 10.583491093285176, 'asn_force': [-2.2884345054626465, 2.515419341623783, -6.001652240753174], 'asn_force_magnitude': 6.898122684393536, 'residue_force': [5.806846618652344, 6.6395188346505165, -0.5731616020202637], 'residue_force_magnitude': 8.839185043331966, 'total_force': [19.116368532180786, 19.83232630044222, -10.103181569837034], 'total_force_magnitude': 29.33992144124552, 'cosine_total_motion': 0, 'cosine_glu_motion': -0.06427964799769105, 'cosine_asn_motion': 0.4027600277946461, 'cosine_residue_motion': 0.23735050140361202, 'cosine_ionic_motion': 0.1122938935780104, 'motion_component_total': 0, 'motion_component_glu': -0.6803030820630696, 'motion_component_asn': 2.7782880840972193, 'motion_component_residue': 2.09798500203415, 'motion_component_ionic': 2.3608835017932837, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 6.427964799769105, 'motion_component_percent_asn': 40.27600277946461, 'motion_component_percent_residue': 23.735050140361203, 'motion_component_percent_ionic': 11.22938935780104, 'ionic_contributions': [{'ion_id': 2280, 'distance': 14.251970291137695, 'force': [0.6688594818115234, -0.27617111802101135, -1.4656014442443848], 'magnitude': 1.6345125436782837, 'cosine_ionic_motion': -0.4559794068336487, 'motion_component_ionic': -0.7453040480613708, 'motion_component_percent_ionic': 45.59794068336487}, {'ion_id': 2333, 'distance': 10.763583183288574, 'force': [1.6097712516784668, -2.3318943977355957, -0.4276678264141083], 'magnitude': 2.8656578063964844, 'cosine_ionic_motion': -0.9985632300376892, 'motion_component_ionic': -2.8615405559539795, 'motion_component_percent_ionic': 99.85632300376892}, {'ion_id': 2334, 'distance': 4.185331344604492, 'force': [7.030081272125244, 16.958602905273438, -4.711757659912109], 'magnitude': 18.953018188476562, 'cosine_ionic_motion': 0.49912989139556885, 'motion_component_ionic': 9.460018157958984, 'motion_component_percent_ionic': 49.912989139556885}, {'ion_id': 2372, 'distance': 13.0617094039917, 'force': [1.9330906867980957, -0.2231125831604004, -0.014605998061597347], 'magnitude': 1.9459784030914307, 'cosine_ionic_motion': -0.6565573811531067, 'motion_component_ionic': -1.277646541595459, 'motion_component_percent_ionic': 65.65573811531067}, {'ion_id': 2515, 'distance': 9.484843254089355, 'force': [2.0677192211151123, -0.9346173405647278, -2.9103870391845703], 'magnitude': 3.690437078475952, 'cosine_ionic_motion': -0.6001034379005432, 'motion_component_ionic': -2.214643955230713, 'motion_component_percent_ionic': 60.01034379005432}], 'glu_contributions': [{'resid': 426, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 5.971139907836914, 'force': [-5.622689247131348, -2.964876413345337, -3.979714870452881], 'magnitude': 7.4995503425598145, 'cosine_with_motion': 0.049358200281858444, 'motion_component': 0.37016430497169495, 'motion_component_percent': 4.935820028185844}, {'resid': 426, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 5.993918418884277, 'force': [5.860915660858154, 1.5316591262817383, 4.533805847167969], 'magnitude': 7.56648588180542, 'cosine_with_motion': -0.21483327448368073, 'motion_component': -1.6255329847335815, 'motion_component_percent': 21.483327448368073}, {'resid': 426, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 5.0198564529418945, 'force': [7.857054710388184, 5.557316780090332, 4.874399662017822], 'magnitude': 10.787810325622559, 'cosine_with_motion': 0.053307004272937775, 'motion_component': 0.5750658512115479, 'motion_component_percent': 5.3307004272937775}], 'asn_contributions': [{'resid': 458, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 3.4046123027801514, 'force': [-9.986759185791016, -5.42881965637207, 17.045063018798828], 'magnitude': 20.48759651184082, 'cosine_with_motion': 0.13862244784832, 'motion_component': 2.840040683746338, 'motion_component_percent': 13.862244784832}, {'resid': 458, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 3.371288776397705, 'force': [2.7994704246520996, 3.586435556411743, -16.95602035522461], 'magnitude': 17.555801391601562, 'cosine_with_motion': -0.015648169443011284, 'motion_component': -0.2747161388397217, 'motion_component_percent': 1.5648169443011284}, {'resid': 458, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 2.9977424144744873, 'force': [24.914705276489258, -0.08857294172048569, -22.484375], 'magnitude': 33.56035614013672, 'cosine_with_motion': -0.4864576756954193, 'motion_component': -16.325693130493164, 'motion_component_percent': 48.64576756954193}, {'resid': 458, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 2.9146296977996826, 'force': [-10.366682052612305, 5.288373947143555, 11.2966947555542], 'magnitude': 16.21882438659668, 'cosine_with_motion': 0.6955130696296692, 'motion_component': 11.280404090881348, 'motion_component_percent': 69.55130696296692}, {'resid': 458, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 3.5480008125305176, 'force': [-9.649168968200684, -0.8419975638389587, 5.096985340118408], 'magnitude': 10.945075035095215, 'cosine_with_motion': 0.4804217219352722, 'motion_component': 5.258251667022705, 'motion_component_percent': 48.04217219352722}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': 0.15197274855546264, 'motion_component_pip2': 4.458868503827432, 'motion_component_percent_pip2': 15.197274855546263}, 1197: {'frame': 1197, 'motion_vector': [4.764503479003906, -4.515300750732422, 4.117408752441406], 'ionic_force': [13.96442337334156, 4.133416444063187, -10.322688207030296], 'ionic_force_magnitude': 17.850718290016857, 'radial_force': 14.563318703165843, 'axial_force': -10.322688207030296, 'glu_force': [-6.26883602142334, 4.583555698394775, 5.518628120422363], 'glu_force_magnitude': 9.52693782048033, 'asn_force': [-9.999708652496338, 9.37789011001587, 3.179235816001892], 'asn_force_magnitude': 14.072900782144837, 'residue_force': [-16.268544673919678, 13.961445808410645, 8.697863936424255], 'residue_force_magnitude': 23.135262088964048, 'total_force': [-2.3041213005781174, 18.09486225247383, -1.624824270606041], 'total_force_magnitude': 18.313193845261686, 'cosine_total_motion': 0, 'cosine_glu_motion': -0.3771505661394181, 'cosine_asn_motion': -0.7051840175944477, 'cosine_residue_motion': -0.584262873415989, 'cosine_ionic_motion': 0.03880306848620946, 'motion_component_total': 0, 'motion_component_glu': -3.5930899925691904, 'motion_component_asn': -9.92398471276094, 'motion_component_residue': -13.517074705330131, 'motion_component_ionic': 0.6926626443355559, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 37.71505661394181, 'motion_component_percent_asn': 70.51840175944477, 'motion_component_percent_residue': 58.4262873415989, 'motion_component_percent_ionic': 3.880306848620946, 'ionic_contributions': [{'ion_id': 2333, 'distance': 4.980548858642578, 'force': [11.166749954223633, -0.451259583234787, -7.364077568054199], 'magnitude': 13.383930206298828, 'cosine_ionic_motion': 0.2402981072664261, 'motion_component_ionic': 3.2161331176757812, 'motion_component_percent_ionic': 24.02981072664261}, {'ion_id': 2334, 'distance': 13.607234954833984, 'force': [0.06744308769702911, 1.7748206853866577, -0.24612747132778168], 'magnitude': 1.793074369430542, 'cosine_ionic_motion': -0.6266006827354431, 'motion_component_ionic': -1.1235415935516357, 'motion_component_percent_ionic': 62.66006827354431}, {'ion_id': 2372, 'distance': 11.631612777709961, 'force': [2.0285637378692627, 1.3199659585952759, -0.4053173065185547], 'magnitude': 2.4539077281951904, 'cosine_ionic_motion': 0.10708682984113693, 'motion_component_ionic': 0.26278120279312134, 'motion_component_percent_ionic': 10.708682984113693}, {'ion_id': 2515, 'distance': 10.822334289550781, 'force': [0.7016665935516357, 1.48988938331604, -2.3071658611297607], 'magnitude': 2.8346288204193115, 'cosine_ionic_motion': -0.5865707397460938, 'motion_component_ionic': -1.6627103090286255, 'motion_component_percent_ionic': 58.657073974609375}], 'glu_contributions': [{'resid': 754, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 5.341722011566162, 'force': [-6.26883602142334, 4.583555698394775, 5.518628120422363], 'magnitude': 9.526937484741211, 'cosine_with_motion': -0.37715059518814087, 'motion_component': -3.593090057373047, 'motion_component_percent': 37.71505951881409}], 'asn_contributions': [{'resid': 786, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 3.702939748764038, 'force': [13.48578929901123, -10.717351913452148, 1.7982717752456665], 'magnitude': 17.31941032409668, 'cosine_with_motion': 0.8945426940917969, 'motion_component': 15.492952346801758, 'motion_component_percent': 89.45426940917969}, {'resid': 786, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 2.680222511291504, 'force': [-21.082805633544922, 17.988040924072266, 1.8590011596679688], 'magnitude': 27.776071548461914, 'cosine_with_motion': -0.8085246086120605, 'motion_component': -22.457637786865234, 'motion_component_percent': 80.85246086120605}, {'resid': 786, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 4.783864974975586, 'force': [-10.263946533203125, 8.225749969482422, 0.8089612722396851], 'magnitude': 13.178238868713379, 'cosine_with_motion': -0.8100156188011169, 'motion_component': -10.674579620361328, 'motion_component_percent': 81.0015618801117}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 4.910033702850342, 'force': [4.221772193908691, -3.5438177585601807, -1.5097585916519165], 'magnitude': 5.71501350402832, 'cosine_with_motion': 0.6751879453659058, 'motion_component': 3.858708381652832, 'motion_component_percent': 67.51879453659058}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 5.555781841278076, 'force': [3.639482021331787, -2.5747311115264893, 0.22276020050048828], 'magnitude': 4.463708400726318, 'cosine_with_motion': 0.8639838099479675, 'motion_component': 3.856571912765503, 'motion_component_percent': 86.39838099479675}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': -0.7002826579216676, 'motion_component_pip2': -12.824412060994577, 'motion_component_percent_pip2': 70.02826579216675}, 1198: {'frame': 1198, 'motion_vector': [0.8578109741210938, -1.3552742004394531, 0.159271240234375], 'ionic_force': [11.564920544624329, 1.7491050492972136, -3.153635263442993], 'ionic_force_magnitude': 12.114131048151247, 'radial_force': 11.696442009301412, 'axial_force': -3.153635263442993, 'glu_force': [35.57899475097656, 10.550032138824463, 4.449437618255615], 'glu_force_magnitude': 37.376002203807126, 'asn_force': [-2.8626036047935486, -0.03820037841796875, 0.8289382457733154], 'asn_force_magnitude': 2.9804525298004725, 'residue_force': [32.716391146183014, 10.511831760406494, 5.278375864028931], 'residue_force_magnitude': 34.76668100856186, 'total_force': [44.28131169080734, 12.260936809703708, 2.1247406005859375], 'total_force_magnitude': 45.99651790222556, 'cosine_total_motion': 0, 'cosine_glu_motion': 0.2810349011128164, 'cosine_asn_motion': -0.4728958893553447, 'cosine_residue_motion': 0.26158715959508155, 'cosine_ionic_motion': 0.3609429486140535, 'motion_component_total': 0, 'motion_component_glu': 10.503961083339345, 'motion_component_asn': -1.4094437497613814, 'motion_component_residue': 9.094517333577963, 'motion_component_ionic': 4.372510180416766, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 28.103490111281644, 'motion_component_percent_asn': 47.28958893553447, 'motion_component_percent_residue': 26.158715959508154, 'motion_component_percent_ionic': 36.09429486140535, 'ionic_contributions': [{'ion_id': 2280, 'distance': 12.808772087097168, 'force': [1.187301754951477, 0.14585809409618378, -1.6321663856506348], 'magnitude': 2.023592710494995, 'cosine_ionic_motion': 0.17195017635822296, 'motion_component_ionic': 0.34795713424682617, 'motion_component_percent_ionic': 17.195017635822296}, {'ion_id': 2333, 'distance': 9.69631576538086, 'force': [2.851334571838379, -2.0663959980010986, 0.26344195008277893], 'magnitude': 3.5312182903289795, 'cosine_ionic_motion': 0.9291419386863708, 'motion_component_ionic': 3.281002998352051, 'motion_component_percent_ionic': 92.91419386863708}, {'ion_id': 2334, 'distance': 9.662446022033691, 'force': [1.7558832168579102, 3.050319194793701, 0.5076314806938171], 'magnitude': 3.5560178756713867, 'cosine_ionic_motion': -0.444364458322525, 'motion_component_ionic': -1.5801680088043213, 'motion_component_percent_ionic': 44.4364458322525}, {'ion_id': 2372, 'distance': 14.474692344665527, 'force': [1.5602493286132812, -0.025931449607014656, 0.2755068838596344], 'magnitude': 1.5845991373062134, 'cosine_ionic_motion': 0.5549613237380981, 'motion_component_ionic': 0.8793911933898926, 'motion_component_percent_ionic': 55.496132373809814}, {'ion_id': 2515, 'distance': 8.170225143432617, 'force': [4.210151672363281, 0.6452552080154419, -2.568049192428589], 'magnitude': 4.973591327667236, 'cosine_ionic_motion': 0.2903992235660553, 'motion_component_ionic': 1.4443269968032837, 'motion_component_percent_ionic': 29.03992235660553}], 'glu_contributions': [{'resid': 426, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 3.270718574523926, 'force': [-23.342588424682617, -4.573491096496582, -7.680246829986572], 'magnitude': 24.995588302612305, 'cosine_with_motion': -0.37351709604263306, 'motion_component': -9.33627986907959, 'motion_component_percent': 37.351709604263306}, {'resid': 426, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 3.3780441284179688, 'force': [21.993284225463867, -4.587280750274658, 7.922017574310303], 'magnitude': 23.822385787963867, 'cosine_with_motion': 0.6861088275909424, 'motion_component': 16.344749450683594, 'motion_component_percent': 68.61088275909424}, {'resid': 426, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 2.5419650077819824, 'force': [36.92829895019531, 19.710803985595703, 4.207666873931885], 'magnitude': 42.070411682128906, 'cosine_with_motion': 0.08308669924736023, 'motion_component': 3.4954915046691895, 'motion_component_percent': 8.308669924736023}], 'asn_contributions': [{'resid': 458, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 4.482522487640381, 'force': [-2.0276668071746826, 6.178985595703125, 9.869036674499512], 'magnitude': 11.81901741027832, 'cosine_with_motion': -0.4483802914619446, 'motion_component': -5.29941463470459, 'motion_component_percent': 44.83802914619446}, {'resid': 458, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 4.841651916503906, 'force': [-0.6009505391120911, -4.977391242980957, -6.878700256347656], 'magnitude': 8.511878967285156, 'cosine_with_motion': 0.37425515055656433, 'motion_component': 3.185614585876465, 'motion_component_percent': 37.42551505565643}, {'resid': 458, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 4.768810272216797, 'force': [4.984068870544434, -8.261222839355469, -9.09838581085205], 'magnitude': 13.261574745178223, 'cosine_with_motion': 0.656013548374176, 'motion_component': 8.699772834777832, 'motion_component_percent': 65.6013548374176}, {'resid': 458, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 5.251852035522461, 'force': [-1.6944018602371216, 3.746039628982544, 2.8371059894561768], 'magnitude': 4.995296001434326, 'cosine_with_motion': -0.7549513578414917, 'motion_component': -3.771205425262451, 'motion_component_percent': 75.49513578414917}, {'resid': 458, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 4.668795108795166, 'force': [-3.523653268814087, 3.275388479232788, 4.099881649017334], 'magnitude': 6.320864677429199, 'cosine_with_motion': -0.6682965159416199, 'motion_component': -4.224211692810059, 'motion_component_percent': 66.82965159416199}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': 0.292783630765735, 'motion_component_pip2': 13.46702751399473, 'motion_component_percent_pip2': 29.2783630765735}, 1199: {'frame': 1199, 'motion_vector': [-1.2769699096679688, 0.9562950134277344, -0.24597930908203125], 'ionic_force': [14.924130320549011, -0.6675621723989025, -0.8316913843154907], 'ionic_force_magnitude': 14.962186191780027, 'radial_force': 14.939053018138342, 'axial_force': -0.8316913843154907, 'glu_force': [31.544937133789062, 18.192070960998535, 5.975917235016823], 'glu_force_magnitude': 36.90184401116672, 'asn_force': [0.27594494819641113, -1.6547326892614365, 0.010538101196289062], 'asn_force_magnitude': 1.6776164457116916, 'residue_force': [31.820882081985474, 16.5373382717371, 5.986455336213112], 'residue_force_magnitude': 36.357801653592304, 'total_force': [46.745012402534485, 15.869776099338196, 5.154763951897621], 'total_force_magnitude': 49.63383492493817, 'cosine_total_motion': 0, 'cosine_glu_motion': -0.4088646731940607, 'cosine_asn_motion': -0.715423150934783, 'cosine_residue_motion': -0.44799369859386506, 'cosine_ionic_motion': -0.8070322307759455, 'motion_component_total': 0, 'motion_component_glu': -15.08786039188389, 'motion_component_asn': -1.2002056436510697, 'motion_component_residue': -16.28806603553496, 'motion_component_ionic': -12.074966499637284, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 40.88646731940607, 'motion_component_percent_asn': 71.54231509347831, 'motion_component_percent_residue': 44.79936985938651, 'motion_component_percent_ionic': 80.70322307759456, 'ionic_contributions': [{'ion_id': 2280, 'distance': 9.9583101272583, 'force': [2.719872236251831, 0.12990471720695496, -1.9477063417434692], 'magnitude': 3.347856044769287, 'cosine_ionic_motion': -0.5310520529747009, 'motion_component_ionic': -1.7778857946395874, 'motion_component_percent_ionic': 53.10520529747009}, {'ion_id': 2333, 'distance': 11.239668846130371, 'force': [2.1640069484710693, -1.4824652671813965, 0.16104227304458618], 'magnitude': 2.6280343532562256, 'cosine_ionic_motion': -0.994925320148468, 'motion_component_ionic': -2.6146979331970215, 'motion_component_percent_ionic': 99.4925320148468}, {'ion_id': 2334, 'distance': 8.931973457336426, 'force': [2.5532796382904053, 3.194657325744629, 0.7697257995605469], 'magnitude': 4.161436080932617, 'cosine_ionic_motion': -0.05876713618636131, 'motion_component_ionic': -0.24455568194389343, 'motion_component_percent_ionic': 5.876713618636131}, {'ion_id': 2350, 'distance': 13.668970108032227, 'force': [1.0107733011245728, 0.0013701611896976829, -1.4614238739013672], 'magnitude': 1.776914358139038, 'cosine_ionic_motion': -0.32421132922172546, 'motion_component_ionic': -0.5760957598686218, 'motion_component_percent_ionic': 32.421132922172546}, {'ion_id': 2372, 'distance': 13.845468521118164, 'force': [1.6899943351745605, -0.17396794259548187, 0.33635014295578003], 'magnitude': 1.7318998575210571, 'cosine_ionic_motion': -0.8610445261001587, 'motion_component_ionic': -1.4912428855895996, 'motion_component_percent_ionic': 86.10445261001587}, {'ion_id': 2515, 'distance': 7.779934883117676, 'force': [4.786203861236572, -2.3370611667633057, 1.3103206157684326], 'magnitude': 5.4851202964782715, 'cosine_ionic_motion': -0.9791012406349182, 'motion_component_ionic': -5.370488166809082, 'motion_component_percent_ionic': 97.91012406349182}], 'glu_contributions': [{'resid': 426, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 2.9948697090148926, 'force': [-21.89179229736328, -18.070598602294922, -9.108757972717285], 'magnitude': 29.81218910217285, 'cosine_with_motion': 0.2683728337287903, 'motion_component': 8.000782012939453, 'motion_component_percent': 26.83728337287903}, {'resid': 426, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 2.6095354557037354, 'force': [35.99102020263672, 8.748282432556152, 14.890029907226562], 'magnitude': 39.91990661621094, 'cosine_with_motion': -0.640236496925354, 'motion_component': -25.558181762695312, 'motion_component_percent': 64.0236496925354}, {'resid': 426, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 2.888583183288574, 'force': [17.445709228515625, 27.514387130737305, 0.19464530050754547], 'magnitude': 32.579627990722656, 'cosine_with_motion': 0.07580012828111649, 'motion_component': 2.4695398807525635, 'motion_component_percent': 7.580012828111649}], 'asn_contributions': [{'resid': 458, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 5.39150857925415, 'force': [2.8256638050079346, 0.1512780338525772, 7.663982391357422], 'magnitude': 8.169692993164062, 'cosine_with_motion': -0.40559452772140503, 'motion_component': -3.3135826587677, 'motion_component_percent': 40.5594527721405}, {'resid': 458, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 4.912932395935059, 'force': [-2.5497188568115234, -1.8060107231140137, -7.653444290161133], 'magnitude': 8.266676902770996, 'cosine_with_motion': 0.2556501626968384, 'motion_component': 2.113377332687378, 'motion_component_percent': 25.565016269683838}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': -0.5714455185271498, 'motion_component_pip2': -28.36303253517225, 'motion_component_percent_pip2': 57.144551852714976}, 1200: {'frame': 1200, 'motion_vector': [1.146820068359375, 0.3510093688964844, -0.5641098022460938], 'ionic_force': [16.83685964345932, 1.662515515461564, -5.256872717291117], 'ionic_force_magnitude': 17.716616811866174, 'radial_force': 16.91874110247862, 'axial_force': -5.256872717291117, 'glu_force': [33.94590950012207, 7.575952053070068, 1.7999233677983284], 'glu_force_magnitude': 34.82756875566885, 'asn_force': [0.8998526409268379, -2.322071462869644, -0.18230438232421875], 'asn_force_magnitude': 2.4969953027331044, 'residue_force': [34.84576214104891, 5.253880590200424, 1.6176189854741096], 'residue_force_magnitude': 35.27672166781954, 'total_force': [51.68262178450823, 6.916396105661988, -3.639253731817007], 'total_force_magnitude': 52.27020276730792, 'cosine_total_motion': 0, 'cosine_glu_motion': 0.8789868017447876, 'cosine_asn_motion': 0.09661392524348528, 'cosine_residue_motion': 0.8746339322893989, 'cosine_ionic_motion': 0.973453936444527, 'motion_component_total': 0, 'motion_component_glu': 30.612973273092056, 'motion_component_asn': 0.24124451751159004, 'motion_component_residue': 30.854217790603645, 'motion_component_ionic': 17.246310375990415, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 87.89868017447876, 'motion_component_percent_asn': 9.661392524348528, 'motion_component_percent_residue': 87.46339322893989, 'motion_component_percent_ionic': 97.3453936444527, 'ionic_contributions': [{'ion_id': 2280, 'distance': 10.24962329864502, 'force': [2.2625174522399902, 0.4258801341056824, -2.1649155616760254], 'magnitude': 3.1602561473846436, 'cosine_ionic_motion': 0.9467374682426453, 'motion_component_ionic': 2.9919328689575195, 'motion_component_percent_ionic': 94.67374682426453}, {'ion_id': 2333, 'distance': 6.5021538734436035, 'force': [7.279170513153076, -1.4231845140457153, -2.5796186923980713], 'magnitude': 7.852783679962158, 'cosine_ionic_motion': 0.8938919305801392, 'motion_component_ionic': 7.019539833068848, 'motion_component_percent_ionic': 89.38919305801392}, {'ion_id': 2334, 'distance': 8.849498748779297, 'force': [1.787436842918396, 3.7654314041137695, 0.7738240361213684], 'magnitude': 4.239364147186279, 'cosine_ionic_motion': 0.5223663449287415, 'motion_component_ionic': 2.214501142501831, 'motion_component_percent_ionic': 52.236634492874146}, {'ion_id': 2350, 'distance': 13.509414672851562, 'force': [0.8990116715431213, 0.10901985317468643, -1.5777028799057007], 'magnitude': 1.8191354274749756, 'cosine_ionic_motion': 0.8126241564750671, 'motion_component_ionic': 1.4782733917236328, 'motion_component_percent_ionic': 81.26241564750671}, {'ion_id': 2372, 'distance': 14.054884910583496, 'force': [1.6639764308929443, 0.022963957861065865, 0.23520198464393616], 'magnitude': 1.6806739568710327, 'cosine_ionic_motion': 0.8007368445396423, 'motion_component_ionic': 1.3457775115966797, 'motion_component_percent_ionic': 80.07368445396423}, {'ion_id': 2515, 'distance': 10.194159507751465, 'force': [2.944746732711792, -1.2375953197479248, 0.05633839592337608], 'magnitude': 3.194737672805786, 'cosine_ionic_motion': 0.6874698400497437, 'motion_component_ionic': 2.1962857246398926, 'motion_component_percent_ionic': 68.74698400497437}], 'glu_contributions': [{'resid': 426, 'resname': 'GLU', 'atom': 'CD', 'ch</t>
+          <t>{1193: {'frame': 1193, 'motion_vector': [-6.644626617431641, -6.532619476318359, 5.509552001953125], 'ionic_force': [3.645001269876957, 0.4808567687869072, -8.289402723312378], 'ionic_force_magnitude': 9.068156096955514, 'radial_force': 3.676582310991121, 'axial_force': -8.289402723312378, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [4.907903671264648, -0.8141872882843018, 5.362216949462891], 'asn_force_magnitude': 7.314628493636834, 'residue_force': [4.907903671264648, -0.8141872882843018, 5.362216949462891], 'residue_force_magnitude': 7.314628493636834, 'pip2_force': [0.9515090382192284, 0.19201884046196938, -4.748029754431627], 'pip2_force_magnitude': 4.846238462341004, 'total_force': [9.504413979360834, -0.1413116790354252, -7.6752155282811145], 'total_force_magnitude': 12.217315068674827, 'cosine_total_motion': -0.7902828104054711, 'cosine_glu_motion': 0, 'cosine_asn_motion': 0.028428536362227374, 'cosine_residue_motion': 0.028428536362227374, 'cosine_pip2_motion': -0.643078172187104, 'cosine_ionic_motion': -0.7439845571371395, 'motion_component_total': -9.655134088081454, 'motion_component_glu': 0, 'motion_component_asn': 0.20794418210753918, 'motion_component_residue': 0.20794418210753918, 'motion_component_ionic': -6.7465680978439, 'motion_component_pip2': -3.116510172345094, 'motion_component_percent_total': 79.02828104054711, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 2.8428536362227375, 'motion_component_percent_residue': 2.8428536362227375, 'motion_component_percent_ionic': 74.39845571371396, 'motion_component_percent_pip2': 64.3078172187104, 'ionic_contributions': [{'ion_id': 2333, 'distance': 10.030160903930664, 'force': [1.0726981163024902, -2.0107765197753906, -2.386737108230591], 'magnitude': 3.300063371658325, 'cosine_ionic_motion': -0.1999226063489914, 'motion_component_ionic': -0.6597572565078735, 'motion_component_percent_ionic': 19.99226063489914}, {'ion_id': 2334, 'distance': 9.7400541305542, 'force': [-0.11895801872015, 2.5222208499908447, -2.423072099685669], 'magnitude': 3.49957537651062, 'cosine_ionic_motion': -0.7664731740951538, 'motion_component_ionic': -2.68233060836792, 'motion_component_percent_ionic': 76.64731740951538}, {'ion_id': 2372, 'distance': 10.768108367919922, 'force': [2.345862627029419, 0.040280118584632874, -1.6411902904510498], 'magnitude': 2.8632497787475586, 'cosine_ionic_motion': -0.8031269907951355, 'motion_component_ionic': -2.299553155899048, 'motion_component_percent_ionic': 80.31269907951355}, {'ion_id': 2515, 'distance': 13.31761646270752, 'force': [0.34539854526519775, -0.07086768001317978, -1.8384032249450684], 'magnitude': 1.8719104528427124, 'cosine_ionic_motion': -0.59026700258255, 'motion_component_ionic': -1.1049269437789917, 'motion_component_percent_ionic': 59.026700258255005}], 'glu_contributions': [], 'asn_contributions': [{'resid': 458, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 5.222881317138672, 'force': [4.907903671264648, -0.8141872882843018, 5.362216949462891], 'magnitude': 7.314628601074219, 'cosine_with_motion': 0.02842852473258972, 'motion_component': 0.2079440951347351, 'motion_component_percent': 2.842852473258972}], 'pip2_contributions': [{'resid': 1313, 'atom': 'C1', 'charge': 0.06000000238418579, 'distance': 24.31043243408203, 'force': [-0.02336146868765354, -0.021302517503499985, 0.011684262193739414], 'magnitude': 0.03370574861764908, 'cosine_with_motion': 0.9832779765129089, 'motion_component': 0.03314211964607239, 'motion_component_percent': 98.3277976512909}, {'resid': 1313, 'atom': 'C11', 'charge': 0.17000000178813934, 'distance': 23.78378677368164, 'force': [-0.0771302655339241, -0.059358347207307816, 0.021970687434077263], 'magnitude': 0.0997757613658905, 'cosine_with_motion': 0.94559645652771, 'motion_component': 0.09434760361909866, 'motion_component_percent': 94.559645652771}, {'resid': 1313, 'atom': 'C12', 'charge': 0.04000000283122063, 'distance': 23.867908477783203, 'force': [-0.018453296273946762, -0.013773079961538315, 0.003633467247709632], 'magnitude': 0.02331145480275154, 'cosine_with_motion': 0.921778678894043, 'motion_component': 0.021488001570105553, 'motion_component_percent': 92.1778678894043}, {'resid': 1313, 'atom': 'C13', 'charge': -0.05000000074505806, 'distance': 24.56389617919922, 'force': [0.021045787259936333, 0.01737374998629093, -0.0034796325489878654], 'magnitude': 0.02751145511865616, 'cosine_with_motion': -0.9150347709655762, 'motion_component': -0.025173937901854515, 'motion_component_percent': 91.50347709655762}, {'resid': 1313, 'atom': 'C2', 'charge': 0.06000000238418579, 'distance': 25.856468200683594, 'force': [-0.02093159779906273, -0.01840875670313835, 0.010524202138185501], 'magnitude': 0.029795518144965172, 'cosine_with_motion': 0.9838351011276245, 'motion_component': 0.02931387722492218, 'motion_component_percent': 98.38351011276245}, {'resid': 1313, 'atom': 'C21', 'charge': 0.6299999952316284, 'distance': 21.80260467529297, 'force': [-0.36304256319999695, -0.2405434399843216, 0.06282638013362885], 'magnitude': 0.44000932574272156, 'cosine_with_motion': 0.909028172492981, 'motion_component': 0.3999808728694916, 'motion_component_percent': 90.9028172492981}, {'resid': 1313, 'atom': 'C210', 'charge': -0.18000000715255737, 'distance': 21.178058624267578, 'force': [0.10119704902172089, 0.08647412061691284, 0.005880541168153286], 'magnitude': 0.13324111700057983, 'cosine_with_motion': -0.8353927731513977, 'motion_component': -0.11130866408348083, 'motion_component_percent': 83.53927731513977}, {'resid': 1313, 'atom': 'C211', 'charge': -0.15000000596046448, 'distance': 22.616174697875977, 'force': [0.0749022588133812, 0.06217917427420616, 0.0016819314332678914], 'magnitude': 0.09736234694719315, 'cosine_with_motion': -0.8488288521766663, 'motion_component': -0.08264397084712982, 'motion_component_percent': 84.88288521766663}, {'resid': 1313, 'atom': 'C212', 'charge': -0.15000000596046448, 'distance': 23.789323806762695, 'force': [0.06752216070890427, 0.05631352216005325, 0.0035945430863648653], 'magnitude': 0.0879964530467987, 'cosine_with_motion': -0.836405336856842, 'motion_component': -0.07360070198774338, 'motion_component_percent': 83.6405336856842}, {'resid': 1313, 'atom': 'C213', 'charge': -0.18000000715255737, 'distance': 24.154407501220703, 'force': [0.07778673619031906, 0.06578534841537476, 0.010628370568156242], 'magnitude': 0.10242778062820435, 'cosine_with_motion': -0.8009285926818848, 'motion_component': -0.08203733712434769, 'motion_component_percent': 80.09285926818848}, {'resid': 1313, 'atom': 'C214', 'charge': -0.15000000596046448, 'distance': 25.586666107177734, 'force': [0.05677993223071098, 0.04998605325818062, 0.007985822856426239], 'magnitude': 0.07606799155473709, 'cosine_with_motion': -0.8013020753860474, 'motion_component': -0.06095343828201294, 'motion_component_percent': 80.13020753860474}, {'resid': 1313, 'atom': 'C215', 'charge': -0.15000000596046448, 'distance': 26.1981143951416, 'force': [0.05269364267587662, 0.04880866780877113, 0.010288535617291927], 'magnitude': 0.07255866378545761, 'cosine_with_motion': -0.7795439958572388, 'motion_component': -0.056562669575214386, 'motion_component_percent': 77.95439958572388}, {'resid': 1313, 'atom': 'C216', 'charge': -0.18000000715255737, 'distance': 25.769372940063477, 'force': [0.06317097693681717, 0.061714403331279755, 0.017299804836511612], 'magnitude': 0.08999179303646088, 'cosine_with_motion': -0.7468864917755127, 'motion_component': -0.06721365451812744, 'motion_component_percent': 74.68864917755127}, {'resid': 1313, 'atom': 'C217', 'charge': -0.18000000715255737, 'distance': 26.571901321411133, 'force': [0.05985615774989128, 0.05637393891811371, 0.020070085301995277], 'magnitude': 0.08463798463344574, 'cosine_with_motion': -0.7153543829917908, 'motion_component': -0.0605461522936821, 'motion_component_percent': 71.53543829917908}, {'resid': 1313, 'atom': 'C218', 'charge': -0.18000000715255737, 'distance': 26.61672019958496, 'force': [0.0627153292298317, 0.052537791430950165, 0.020543336868286133], 'magnitude': 0.08435319364070892, 'cosine_with_motion': -0.7082753777503967, 'motion_component': -0.059745289385318756, 'motion_component_percent': 70.82753777503967}, {'resid': 1313, 'atom': 'C219', 'charge': -0.18000000715255737, 'distance': 27.619352340698242, 'force': [0.05839952826499939, 0.047180138528347015, 0.02237604185938835], 'magnitude': 0.07834001630544662, 'cosine_with_motion': -0.6756467819213867, 'motion_component': -0.05293017998337746, 'motion_component_percent': 67.56467819213867}, {'resid': 1313, 'atom': 'C22', 'charge': -0.08000000566244125, 'distance': 20.58021354675293, 'force': [0.052282143384218216, 0.03404370695352554, -0.006324160844087601], 'magnitude': 0.062708780169487, 'cosine_with_motion': -0.8907060623168945, 'motion_component': -0.05585509166121483, 'motion_component_percent': 89.07060623168945}, {'resid': 1313, 'atom': 'C220', 'charge': -0.27000001072883606, 'distance': 27.52238655090332, 'force': [0.09184415638446808, 0.06585609912872314, 0.03509784862399101], 'magnitude': 0.11833948642015457, 'cosine_with_motion': -0.6612728238105774, 'motion_component': -0.07825468480587006, 'motion_component_percent': 66.12728238105774}, {'resid': 1313, 'atom': 'C23', 'charge': -0.18000000715255737, 'distance': 19.492555618286133, 'force': [0.12675201892852783, 0.09121134877204895, -0.01874465122818947], 'magnitude': 0.157279834151268, 'cosine_with_motion': -0.9053096175193787, 'motion_component': -0.14238694310188293, 'motion_component_percent': 90.53096175193787}, {'resid': 1313, 'atom': 'C24', 'charge': -0.18000000715255737, 'distance': 18.188016891479492, 'force': [0.14812391996383667, 0.10247202217578888, -0.013910388574004173], 'magnitude': 0.18065080046653748, 'cosine_with_motion': -0.8848037719726562, 'motion_component': -0.15984050929546356, 'motion_component_percent': 88.48037719726562}, {'resid': 1313, 'atom': 'C25', 'charge': -0.15000000596046448, 'distance': 17.297468185424805, 'force': [0.1298229843378067, 0.10313988476991653, -0.014535147696733475], 'magnitude': 0.16644251346588135, 'cosine_with_motion': -0.8971748352050781, 'motion_component': -0.14932803809642792, 'motion_component_percent': 89.71748352050781}, {'resid': 1313, 'atom': 'C26', 'charge': -0.15000000596046448, 'distance': 17.22696304321289, 'force': [0.12450339645147324, 0.11223719269037247, -0.007819503545761108], 'magnitude': 0.1678077131509781, 'cosine_with_motion': -0.8827646970748901, 'motion_component': -0.1481347233057022, 'motion_component_percent': 88.27646970748901}, {'resid': 1313, 'atom': 'C27', 'charge': -0.18000000715255737, 'distance': 18.05255126953125, 'force': [0.13444188237190247, 0.12462921440601349, 0.004277137108147144], 'magnitude': 0.18337218463420868, 'cosine_with_motion': -0.848311185836792, 'motion_component': -0.15555667877197266, 'motion_component_percent': 84.8311185836792}, {'resid': 1313, 'atom': 'C28', 'charge': -0.15000000596046448, 'distance': 19.30562400817871, 'force': [0.09466619044542313, 0.09429634362459183, -0.00010898772598011419], 'magnitude': 0.13361698389053345, 'cosine_with_motion': -0.861184298992157, 'motion_component': -0.11506884545087814, 'motion_component_percent': 86.1184298992157}, {'resid': 1313, 'atom': 'C29', 'charge': -0.15000000596046448, 'distance': 20.594215393066406, 'force': [0.08454720675945282, 0.08147064596414566, 0.0012468245113268495], 'magnitude': 0.11741912364959717, 'cosine_with_motion': -0.855291485786438, 'motion_component': -0.10042757540941238, 'motion_component_percent': 85.5291485786438}, {'resid': 1313, 'atom': 'C3', 'charge': 0.06000000238418579, 'distance': 26.20241928100586, 'force': [-0.020355889573693275, -0.017082469537854195, 0.01164624560624361], 'magnitude': 0.029013928025960922, 'cosine_with_motion': 0.9902553558349609, 'motion_component': 0.028731197118759155, 'motion_component_percent': 99.0255355834961}, {'resid': 1313, 'atom': 'C31', 'charge': 0.6299999952316284, 'distance': 26.266273498535156, 'force': [-0.24270972609519958, -0.17969416081905365, 0.026685724034905434], 'magnitude': 0.30316683650016785, 'cosine_with_motion': 0.8939067721366882, 'motion_component': 0.2710028886795044, 'motion_component_percent': 89.39067721366882}, {'resid': 1313, 'atom': 'C310', 'charge': -0.18000000715255737, 'distance': 19.322675704956055, 'force': [0.1393395960330963, 0.07528627663850784, 0.023127006366848946], 'magnitude': 0.16005751490592957, 'cosine_with_motion': -0.7446819543838501, 'motion_component': -0.11919194459915161, 'motion_component_percent': 74.46819543838501}, {'resid': 1313, 'atom': 'C311', 'charge': -0.18000000715255737, 'distance': 18.433778762817383, 'force': [0.1465766727924347, 0.09336243569850922, 0.02697371132671833], 'magnitude': 0.1758659929037094, 'cosine_with_motion': -0.7538970708847046, 'motion_component': -0.1325848549604416, 'motion_component_percent': 75.38970708847046}, {'resid': 1313, 'atom': 'C312', 'charge': -0.18000000715255737, 'distance': 17.00487518310547, 'force': [0.1731550246477127, 0.10680568218231201, 0.03632725402712822], 'magnitude': 0.20666345953941345, 'cosine_with_motion': -0.7367108464241028, 'motion_component': -0.1522512137889862, 'motion_component_percent': 73.67108464241028}, {'resid': 1313, 'atom': 'C313', 'charge': -0.18000000715255737, 'distance': 16.26487159729004, 'force': [0.19736237823963165, 0.10635344684123993, 0.027680469676852226], 'magnitude': 0.22589637339115143, 'cosine_with_motion': -0.7580385804176331, 'motion_component': -0.17123816907405853, 'motion_component_percent': 75.8038580417633}, {'resid': 1313, 'atom': 'C314', 'charge': -0.18000000715255737, 'distance': 14.666632652282715, 'force': [0.24252964556217194, 0.13040943443775177, 0.03676721453666687], 'magnitude': 0.2778112292289734, 'cosine_with_motion': -0.7517877221107483, 'motion_component': -0.20885507762432098, 'motion_component_percent': 75.17877221107483}, {'resid': 1313, 'atom': 'C315', 'charge': -0.18000000715255737, 'distance': 14.085083961486816, 'force': [0.25338372588157654, 0.16165512800216675, 0.020027637481689453], 'magnitude': 0.301225483417511, 'cosine_with_motion': -0.8063505291938782, 'motion_component': -0.24289332330226898, 'motion_component_percent': 80.63505291938782}, {'resid': 1313, 'atom': 'C316', 'charge': -0.18000000715255737, 'distance': 14.157875061035156, 'force': [0.2561195492744446, 0.1522083431482315, -0.010976579040288925], 'magnitude': 0.29813602566719055, 'cosine_with_motion': -0.8541463017463684, 'motion_component': -0.2546517848968506, 'motion_component_percent': 85.41463017463684}, {'resid': 1313, 'atom': 'C317', 'charge': -0.18000000715255737, 'distance': 13.096346855163574, 'force': [0.3117147982120514, 0.15388159453868866, -0.023555662482976913], 'magnitude': 0.3484257757663727, 'cosine_with_motion': -0.8500787019729614, 'motion_component': -0.2961893379688263, 'motion_component_percent': 85.00787019729614}, {'resid': 1313, 'atom': 'C318', 'charge': -0.27000001072883606, 'distance': 13.12755298614502, 'force': [0.4633353650569916, 0.21720105409622192, -0.09331206977367401], 'magnitude': 0.5201568007469177, 'cosine_with_motion': -0.8900628685951233, 'motion_component': -0.4629722535610199, 'motion_component_percent': 89.00628685951233}, {'resid': 1313, 'atom': 'C32', 'charge': -0.08000000566244125, 'distance': 26.570009231567383, 'force': [0.030981440097093582, 0.02128210850059986, -0.0016295196255668998], 'magnitude': 0.03762224316596985, 'cosine_with_motion': -0.8688900470733643, 'motion_component': -0.032689593732357025, 'motion_component_percent': 86.88900470733643}, {'resid': 1313, 'atom': 'C33', 'charge': -0.18000000715255737, 'distance': 25.95230484008789, 'force': [0.07560627907514572, 0.04624802991747856, -0.004170975647866726], 'magnitude': 0.08872760087251663, 'cosine_with_motion': -0.8615246415138245, 'motion_component': -0.07644101232290268, 'motion_component_percent': 86.15246415138245}, {'resid': 1313, 'atom': 'C34', 'charge': -0.18000000715255737, 'distance': 24.510116577148438, 'force': [0.0849907398223877, 0.05163923278450966, -0.002347142668440938], 'magnitude': 0.09947635978460312, 'cosine_with_motion': -0.8497150540351868, 'motion_component': -0.08452656120061874, 'motion_component_percent': 84.97150540351868}, {'resid': 1313, 'atom': 'C35', 'charge': -0.18000000715255737, 'distance': 24.74884605407715, 'force': [0.08310867846012115, 0.050951868295669556, 0.0040092458948493], 'magnitude': 0.09756648540496826, 'cosine_with_motion': -0.8170976042747498, 'motion_component': -0.07972133904695511, 'motion_component_percent': 81.70976042747498}, {'resid': 1313, 'atom': 'C36', 'charge': -0.18000000715255737, 'distance': 23.530977249145508, 'force': [0.09245240688323975, 0.055049698799848557, 0.008387674577534199], 'magnitude': 0.10792715102434158, 'cosine_with_motion': -0.7940650582313538, 'motion_component': -0.08570118248462677, 'motion_component_percent': 79.40650582313538}, {'resid': 1313, 'atom': 'C37', 'charge': -0.18000000715255737, 'distance': 22.913257598876953, 'force': [0.10085988789796829, 0.05208780989050865, 0.008380352519452572], 'magnitude': 0.11382480710744858, 'cosine_with_motion': -0.7825900912284851, 'motion_component': -0.08907816559076309, 'motion_component_percent': 78.25900912284851}, {'resid': 1313, 'atom': 'C38', 'charge': -0.18000000715255737, 'distance': 21.666305541992188, 'force': [0.11287448555231094, 0.056986987590789795, 0.014766681008040905], 'magnitude': 0.12730365991592407, 'cosine_with_motion': -0.7553520798683167, 'motion_component': -0.09615908563137054, 'motion_component_percent': 75.53520798683167}, {'resid': 1313, 'atom': 'C39', 'charge': -0.18000000715255737, 'distance': 20.47477149963379, 'force': [0.12379162758588791, 0.0693221166729927, 0.013822847045958042], 'magnitude': 0.1425517201423645, 'cosine_with_motion': -0.7771533727645874, 'motion_component': -0.11078455299139023, 'motion_component_percent': 77.71533727645874}, {'resid': 1313, 'atom': 'C4', 'charge': 0.08000000566244125, 'distance': 25.74843406677246, 'force': [-0.02659017965197563, -0.024199580773711205, 0.017670897766947746], 'magnitude': 0.04006142541766167, 'cosine_with_motion': 0.9964510798454285, 'motion_component': 0.03991924971342087, 'motion_component_percent': 99.64510798454285}, {'resid': 1313, 'atom': 'C5', 'charge': 0.08000000566244125, 'distance': 24.24977684020996, 'force': [-0.029676193371415138, -0.027541300281882286, 0.0200194139033556], 'magnitude': 0.045166101306676865, 'cosine_with_motion': 0.9968859553337097, 'motion_component': 0.045025452971458435, 'motion_component_percent': 99.68859553337097}, {'resid': 1313, 'atom': 'C6', 'charge': 0.06000000238418579, 'distance': 23.91864013671875, 'force': [-0.022895056754350662, -0.022393211722373962, 0.013664687052369118], 'magnitude': 0.03481900691986084, 'cosine_with_motion': 0.9914698004722595, 'motion_component': 0.03452199324965477, 'motion_component_percent': 99.14698004722595}, {'resid': 1313, 'atom': 'H1', 'charge': 0.12000000476837158, 'distance': 23.774044036865234, 'force': [-0.05078874155879021, -0.042554713785648346, 0.024043988436460495], 'magnitude': 0.07048767805099487, 'cosine_with_motion': 0.9802185893058777, 'motion_component': 0.06909333169460297, 'motion_component_percent': 98.02185893058777}, {'resid': 1313, 'atom': 'H10R', 'charge': 0.09000000357627869, 'distance': 21.306676864624023, 'force': [-0.049188487231731415, -0.04330160468816757, -0.006128846202045679], 'magnitude': 0.0658186823129654, 'cosine_with_motion': 0.8083556294441223, 'motion_component': 0.05320490151643753, 'motion_component_percent': 80.83556294441223}, {'resid': 1313, 'atom': 'H10S', 'charge': 0.09000000357627869, 'distance': 20.61307144165039, 'force': [-0.055396582931280136, -0.04324354976415634, -0.002547292737290263], 'magnitude': 0.07032264769077301, 'cosine_with_motion': 0.8361943960189819, 'motion_component': 0.05880340561270714, 'motion_component_percent': 83.6194396018982}, {'resid': 1313, 'atom': 'H10X', 'charge': 0.09000000357627869, 'distance': 19.762853622436523, 'force': [-0.06668905168771744, -0.034490738064050674, -0.014688302762806416], 'magnitude': 0.07650350779294968, 'cosine_with_motion': 0.7094253301620483, 'motion_component': 0.05427352711558342, 'motion_component_percent': 70.94253301620483}, {'resid': 1313, 'atom': 'H10Y', 'charge': 0.09000000357627869, 'distance': 18.800273895263672, 'force': [-0.0755700096487999, -0.036439448595047, -0.010393436066806316], 'magnitude': 0.0845380574464798, 'cosine_with_motion': 0.7462528944015503, 'motion_component': 0.06308677047491074, 'motion_component_percent': 74.62528944015503}, {'resid': 1313, 'atom': 'H111', 'charge': 0.15000000596046448, 'distance': 22.546724319458008, 'force': [-0.07622834295034409, -0.061466459184885025, 0.0028073801659047604], 'magnitude': 0.09796309471130371, 'cosine_with_motion': 0.8708661198616028, 'motion_component': 0.08531273901462555, 'motion_component_percent': 87.08661198616028}, {'resid': 1313, 'atom': 'H11A', 'charge': 0.09000000357627869, 'distance': 24.71796417236328, 'force': [-0.037773728370666504, -0.02870824746787548, 0.011861803010106087], 'magnitude': 0.04890521988272667, 'cosine_with_motion': 0.9518039226531982, 'motion_component': 0.046548180282115936, 'motion_component_percent': 95.18039226531982}, {'resid': 1313, 'atom': 'H11B', 'charge': 0.09000000357627869, 'distance': 23.015155792236328, 'force': [-0.04427701607346535, -0.032213062047958374, 0.013561105355620384], 'magnitude': 0.0564095638692379, 'cosine_with_motion': 0.9487748742103577, 'motion_component': 0.053519975394010544, 'motion_component_percent': 94.87748742103577}, {'resid': 1313, 'atom': 'H11X', 'charge': 0.09000000357627869, 'distance': 18.475353240966797, 'force': [-0.07202382385730743, -0.04894164577126503, -0.008951677940785885], 'magnitude': 0.08753769844770432, 'cosine_with_motion': 0.7903862595558167, 'motion_component': 0.06918859481811523, 'motion_component_percent': 79.03862595558167}, {'resid': 1313, 'atom': 'H11Y', 'charge': 0.09000000357627869, 'distance': 19.080646514892578, 'force': [-0.06652367860078812, -0.04555646702647209, -0.015329870395362377], 'magnitude': 0.08207190036773682, 'cosine_with_motion': 0.7374430894851685, 'motion_component': 0.06052335351705551, 'motion_component_percent': 73.74430894851685}, {'resid': 1313, 'atom': 'H12', 'charge': 0.09000000357627869, 'distance': 24.51384162902832, 'force': [-0.04043230041861534, -0.027905790135264397, 0.00767327519133687], 'magnitude': 0.0497230663895607, 'cosine_with_motion': 0.9163552522659302, 'motion_component': 0.045563992112874985, 'motion_component_percent': 91.63552522659302}, {'resid': 1313, 'atom': 'H121', 'charge': 0.15000000596046448, 'distance': 24.605091094970703, 'force': [-0.06423531472682953, -0.0513584241271019, -0.0015982392942532897], 'magnitude': 0.08225823938846588, 'cosine_with_motion': 0.8462245464324951, 'motion_component': 0.06960894167423248, 'motion_component_percent': 84.62245464324951}, {'resid': 1313, 'atom': 'H12X', 'charge': 0.09000000357627869, 'distance': 16.598892211914062, 'force': [-0.08714701980352402, -0.0614018552005291, -0.019905343651771545], 'magnitude': 0.10844820737838745, 'cosine_with_motion': 0.7415143847465515, 'motion_component': 0.08041590452194214, 'motion_component_percent': 74.15143847465515}, {'resid': 1313, 'atom': 'H12Y', 'charge': 0.09000000357627869, 'distance': 17.034683227539062, 'force': [-0.0867101177573204, -0.05011069402098656, -0.023941220715641975], 'magnitude': 0.1029704213142395, 'cosine_with_motion': 0.6922346353530884, 'motion_component': 0.07127968966960907, 'motion_component_percent': 69.22346353530884}, {'resid': 1313, 'atom': 'H13A', 'charge': 0.09000000357627869, 'distance': 25.331663131713867, 'force': [-0.03501211106777191, -0.029856355860829353, 0.0071404180489480495], 'magnitude': 0.046564314514398575, 'cosine_with_motion': 0.926522433757782, 'motion_component': 0.043142881244421005, 'motion_component_percent': 92.6522433757782}, {'resid': 1313, 'atom': 'H13B', 'charge': 0.09000000357627869, 'distance': 23.783679962158203, 'force': [-0.039392802864313126, -0.03463214263319969, 0.006251708138734102], 'magnitude': 0.05282292887568474, 'cosine_with_motion': 0.913648247718811, 'motion_component': 0.048261575400829315, 'motion_component_percent': 91.3648247718811}, {'resid': 1313, 'atom': 'H13R', 'charge': 0.09000000357627869, 'distance': 24.121492385864258, 'force': [-0.04022905230522156, -0.03128226473927498, -0.006344446446746588], 'magnitude': 0.05135376378893852, 'cosine_with_motion': 0.7855768799781799, 'motion_component': 0.04034233093261719, 'motion_component_percent': 78.557687997818}, {'resid': 1313, 'atom': 'H13S', 'charge': 0.09000000357627869, 'distance': 23.467975616455078, 'force': [-0.040011800825595856, -0.0360405370593071, -0.0066029829904437065], 'magnitude': 0.05425369739532471, 'cosine_with_motion': 0.7916305065155029, 'motion_component': 0.0429488830268383, 'motion_component_percent': 79.1630506515503}, {'resid': 1313, 'atom': 'H13X', 'charge': 0.09000000357627869, 'distance': 16.61972999572754, 'force': [-0.09736301004886627, -0.04485733434557915, -0.014505371451377869], 'magnitude': 0.10817644000053406, 'cosine_with_motion': 0.7344565987586975, 'motion_component': 0.07945089787244797, 'motion_component_percent': 73.44565987586975}, {'resid': 1313, 'atom': 'H13Y', 'charge': 0.09000000357627869, 'distance': 16.57933235168457, 'force': [-0.09481576085090637, -0.05276026576757431, -0.0065528107807040215], 'magnitude': 0.10870425403118134, 'cosine_with_motion': 0.7976148128509521, 'motion_component': 0.08670412003993988, 'motion_component_percent': 79.76148128509521}, {'resid': 1313, 'atom': 'H141', 'charge': 0.15000000596046448, 'distance': 26.236358642578125, 'force': [-0.054575365036726, -0.0472027026116848, -0.005250126589089632], 'magnitude': 0.07234728336334229, 'cosine_with_motion': 0.8198362588882446, 'motion_component': 0.05931292474269867, 'motion_component_percent': 81.98362588882446}, {'resid': 1313, 'atom': 'H14X', 'charge': 0.09000000357627869, 'distance': 14.192992210388184, 'force': [-0.13414235413074493, -0.06087357550859451, -0.017389636486768723], 'magnitude': 0.14833125472068787, 'cosine_with_motion': 0.7430949211120605, 'motion_component': 0.11022420227527618, 'motion_component_percent': 74.30949211120605}, {'resid': 1313, 'atom': 'H14Y', 'charge': 0.09000000357627869, 'distance': 14.462865829467773, 'force': [-0.12248189002275467, -0.06744933873414993, -0.02922515757381916], 'magnitude': 0.1428472399711609, 'cosine_with_motion': 0.7071275115013123, 'motion_component': 0.10101120918989182, 'motion_component_percent': 70.71275115013123}, {'resid': 1313, 'atom': 'H151', 'charge': 0.15000000596046448, 'distance': 27.26563262939453, 'force': [-0.04839329421520233, -0.04540039971470833, -0.00918202567845583], 'magnitude': 0.06698818504810333, 'cosine_with_motion': 0.7826664447784424, 'motion_component': 0.052429404109716415, 'motion_component_percent': 78.26664447784424}, {'resid': 1313, 'atom': 'H15X', 'charge': 0.09000000357627869, 'distance': 14.754046440124512, 'force': [-0.11078603565692902, -0.08045346289873123, -0.009759209118783474], 'magnitude': 0.13726451992988586, 'cosine_with_motion': 0.8129352331161499, 'motion_component': 0.11158716678619385, 'motion_component_percent': 81.29352331161499}, {'resid': 1313, 'atom': 'H15Y', 'charge': 0.09000000357627869, 'distance': 13.072661399841309, 'force': [-0.1446349322795868, -0.09705405682325363, -0.01522914506494999], 'magnitude': 0.17484472692012787, 'cosine_with_motion': 0.798413097858429, 'motion_component': 0.1395983248949051, 'motion_component_percent': 79.8413097858429}, {'resid': 1313, 'atom': 'H16R', 'charge': 0.09000000357627869, 'distance': 24.734949111938477, 'force': [-0.0345904640853405, -0.033044904470443726, -0.009833206422626972], 'magnitude': 0.04883807897567749, 'cosine_with_motion': 0.7405964136123657, 'motion_component': 0.03616930544376373, 'motion_component_percent': 74.05964136123657}, {'resid': 1313, 'atom': 'H16S', 'charge': 0.09000000357627869, 'distance': 25.825212478637695, 'force': [-0.03012959286570549, -0.03207585960626602, -0.00839781854301691], 'magnitude': 0.04480152577161789, 'cosine_with_motion': 0.7494587898254395, 'motion_component': 0.03357689827680588, 'motion_component_percent': 74.94587898254395}, {'resid': 1313, 'atom': 'H16X', 'charge': 0.09000000357627869, 'distance': 15.17619514465332, 'force': [-0.11312244087457657, -0.0632452443242073, 0.005860097706317902], 'magnitude': 0.12973429262638092, 'cosine_with_motion': 0.8524057865142822, 'motion_component': 0.1105862632393837, 'motion_component_percent': 85.24057865142822}, {'resid': 1313, 'atom': 'H16Y', 'charge': 0.09000000357627869, 'distance': 14.053987503051758, 'force': [-0.12466272711753845, -0.0847373902797699, 0.012822404503822327], 'magnitude': 0.1512799859046936, 'cosine_with_motion': 0.8869873881340027, 'motion_component': 0.13418343663215637, 'motion_component_percent': 88.69873881340027}, {'resid': 1313, 'atom': 'H17R', 'charge': 0.09000000357627869, 'distance': 26.280323028564453, 'force': [-0.029784703627228737, -0.02909005433320999, -0.011762215755879879], 'magnitude': 0.043263256549835205, 'cosine_with_motion': 0.6899847984313965, 'motion_component': 0.02985098958015442, 'motion_component_percent': 68.99847984313965}, {'resid': 1313, 'atom': 'H17S', 'charge': 0.09000000357627869, 'distance': 27.56843376159668, 'force': [-0.027466941624879837, -0.026652589440345764, -0.008992358110845089], 'magnitude': 0.03931482881307602, 'cosine_with_motion': 0.721537172794342, 'motion_component': 0.02836710959672928, 'motion_component_percent': 72.1537172794342}, {'resid': 1313, 'atom': 'H17X', 'charge': 0.09000000357627869, 'distance': 13.31406307220459, 'force': [-0.15610508620738983, -0.0633755624294281, 0.005277855321764946], 'magnitude': 0.1685619056224823, 'cosine_with_motion': 0.8112877011299133, 'motion_component': 0.1367522031068802, 'motion_component_percent': 81.12877011299133}, {'resid': 1313, 'atom': 'H17Y', 'charge': 0.09000000357627869, 'distance': 12.066847801208496, 'force': [-0.18239451944828033, -0.09363522380590439, 0.00864578876644373], 'magnitude': 0.20520737767219543, 'cosine_with_motion': 0.8423880338668823, 'motion_component': 0.17286424338817596, 'motion_component_percent': 84.23880338668823}, {'resid': 1313, 'atom': 'H18R', 'charge': 0.09000000357627869, 'distance': 26.981342315673828, 'force': [-0.031199706718325615, -0.025242440402507782, -0.008604487404227257], 'magnitude': 0.041044361889362335, 'cosine_with_motion': 0.7310329675674438, 'motion_component': 0.03000478260219097, 'motion_component_percent': 73.10329675674438}, {'resid': 1313, 'atom': 'H18S', 'charge': 0.09000000357627869, 'distance': 25.62979507446289, 'force': [-0.03431210666894913, -0.02767636999487877, -0.011215786449611187], 'magnitude': 0.04548731446266174, 'cosine_with_motion': 0.704701840877533, 'motion_component': 0.03205499425530434, 'motion_component_percent': 70.4701840877533}, {'resid': 1313, 'atom': 'H18X', 'charge': 0.09000000357627869, 'distance': 12.279669761657715, 'force': [-0.18007756769657135, -0.07302985340356827, 0.03878796473145485], 'magnitude': 0.1981559842824936, 'cosine_with_motion': 0.8798550963401794, 'motion_component': 0.17434854805469513, 'motion_component_percent': 87.98550963401794}, {'resid': 1313, 'atom': 'H18Y', 'charge': 0.09000000357627869, 'distance': 14.027799606323242, 'force': [-0.1373099684715271, -0.057386614382267, 0.030162248760461807], 'magnitude': 0.15184535086154938, 'cosine_with_motion': 0.8842315673828125, 'motion_component': 0.1342664510011673, 'motion_component_percent': 88.42315673828125}, {'resid': 1313, 'atom': 'H18Z', 'charge': 0.09000000357627869, 'distance': 13.16140079498291, 'force': [-0.14678184688091278, -0.08182022720575333, 0.03892360255122185], 'magnitude': 0.17249494791030884, 'cosine_with_motion': 0.9234168529510498, 'motion_component': 0.15928474068641663, 'motion_component_percent': 92.34168529510498}, {'resid': 1313, 'atom': 'H19R', 'charge': 0.09000000357627869, 'distance': 27.39101219177246, 'force': [-0.028836848214268684, -0.024407004937529564, -0.01260270457714796], 'magnitude': 0.039825793355703354, 'cosine_with_motion': 0.6532274484634399, 'motion_component': 0.026015300303697586, 'motion_component_percent': 65.322744846344}, {'resid': 1313, 'atom': 'H19S', 'charge': 0.09000000357627869, 'distance': 28.64765739440918, 'force': [-0.026960480958223343, -0.02228177897632122, -0.010110937990248203], 'magnitude': 0.03640846535563469, 'cosine_with_motion': 0.682512998</t>
         </is>
       </c>
     </row>
@@ -675,7 +675,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>{1199: {'frame': 1199, 'motion_vector': [-3.884815216064453, 1.590545654296875, 1.432769775390625], 'ionic_force': [14.11787834763527, -5.172281384468079, -12.066099643707275], 'ionic_force_magnitude': 19.27842691639068, 'radial_force': 15.035524059996838, 'axial_force': -12.066099643707275, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [0.0, 0.0, 0.0], 'asn_force_magnitude': 0.0, 'residue_force': [0.0, 0.0, 0.0], 'residue_force_magnitude': 0.0, 'total_force': [14.11787834763527, -5.172281384468079, -12.066099643707275], 'total_force_magnitude': 19.27842691639068, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': 0, 'cosine_residue_motion': 0, 'cosine_ionic_motion': -0.9397606145256897, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': 0, 'motion_component_residue': 0, 'motion_component_ionic': -18.117106326035902, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 0, 'motion_component_percent_residue': 0, 'motion_component_percent_ionic': 93.97606145256897, 'ionic_contributions': [{'ion_id': 2230, 'distance': 7.779934883117676, 'force': [-4.786203861236572, 2.3370611667633057, -1.3103206157684326], 'magnitude': 5.4851202964782715, 'cosine_ionic_motion': 0.8398500084877014, 'motion_component_ionic': 4.606678485870361, 'motion_component_percent_ionic': 83.98500084877014}, {'ion_id': 2280, 'distance': 8.599261283874512, 'force': [0.6796392798423767, 1.932413935661316, -3.995137929916382], 'magnitude': 4.489683628082275, 'cosine_ionic_motion': -0.2656768560409546, 'motion_component_ionic': -1.1928050518035889, 'motion_component_percent_ionic': 26.56768560409546}, {'ion_id': 2333, 'distance': 4.074949264526367, 'force': [12.101813316345215, -14.844310760498047, -5.739468097686768], 'magnitude': 19.993722915649414, 'cosine_ionic_motion': -0.8890808820724487, 'motion_component_ionic': -17.776037216186523, 'motion_component_percent_ionic': 88.90808820724487}, {'ion_id': 2334, 'distance': 10.257603645324707, 'force': [-0.4024566113948822, 3.128925085067749, -0.06349241733551025], 'magnitude': 3.1553406715393066, 'cosine_ionic_motion': 0.4607953727245331, 'motion_component_ionic': 1.4539663791656494, 'motion_component_percent_ionic': 46.07953727245331}, {'ion_id': 2350, 'distance': 13.552000999450684, 'force': [0.13162976503372192, 0.44357430934906006, -1.747503399848938], 'magnitude': 1.8077203035354614, 'cosine_ionic_motion': -0.2880411744117737, 'motion_component_ionic': -0.5206978917121887, 'motion_component_percent_ionic': 28.804117441177368}, {'ion_id': 2372, 'distance': 7.040935039520264, 'force': [6.39345645904541, 1.8300548791885376, 0.7898228168487549], 'magnitude': 6.696954727172852, 'cosine_ionic_motion': -0.7000511884689331, 'motion_component_ionic': -4.688210964202881, 'motion_component_percent_ionic': 70.00511884689331}], 'glu_contributions': [], 'asn_contributions': [], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': -0.9397606145256897, 'motion_component_pip2': -18.117106326035902, 'motion_component_percent_pip2': 93.97606145256897}, 1200: {'frame': 1200, 'motion_vector': [4.058921813964844, -2.802806854248047, -3.9130706787109375], 'ionic_force': [-8.569838225841522, 18.851579010486603, -8.785514246672392], 'ionic_force_magnitude': 22.49465311989045, 'radial_force': 20.708069886054414, 'axial_force': -8.785514246672392, 'glu_force': [2.0365245640277863, 9.51301097869873, -2.6995275616645813], 'glu_force_magnitude': 10.096150713857131, 'asn_force': [0.4543800354003906, -0.27001094818115234, -0.5987660884857178], 'asn_force_magnitude': 0.798678882548319, 'residue_force': [2.490904599428177, 9.243000030517578, -3.298293650150299], 'residue_force_magnitude': 10.125038088334392, 'total_force': [-6.078933626413345, 28.09457904100418, -12.083807896822691], 'total_force_magnitude': 31.181360118071897, 'cosine_total_motion': 0, 'cosine_glu_motion': -0.12323207282443684, 'cosine_asn_motion': 0.9831801426691412, 'cosine_residue_motion': -0.045325692439082986, 'cosine_ionic_motion': -0.37592748360644773, 'motion_component_total': 0, 'motion_component_glu': -1.244169580016532, 'motion_component_asn': 0.7852452176906866, 'motion_component_residue': -0.45892436232584544, 'motion_component_ionic': -8.456358341960346, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 12.323207282443684, 'motion_component_percent_asn': 98.31801426691412, 'motion_component_percent_residue': 4.5325692439082985, 'motion_component_percent_ionic': 37.59274836064478, 'ionic_contributions': [{'ion_id': 2230, 'distance': 10.194159507751465, 'force': [-2.944746732711792, 1.2375953197479248, -0.05633839592337608], 'magnitude': 3.194737672805786, 'cosine_ionic_motion': -0.7556994557380676, 'motion_component_ionic': -2.41426157951355, 'motion_component_percent_ionic': 75.56994557380676}, {'ion_id': 2280, 'distance': 9.19277572631836, 'force': [-0.8797121047973633, 2.2779886722564697, -3.077542304992676], 'magnitude': 3.9286630153656006, 'cosine_ionic_motion': 0.08437951654195786, 'motion_component_ionic': 0.3314986824989319, 'motion_component_percent_ionic': 8.437951654195786}, {'ion_id': 2333, 'distance': 4.938725471496582, 'force': [-9.285982131958008, 7.636200428009033, -6.3823113441467285], 'magnitude': 13.611573219299316, 'cosine_ionic_motion': -0.39811810851097107, 'motion_component_ionic': -5.419013977050781, 'motion_component_percent_ionic': 39.81181085109711}, {'ion_id': 2334, 'distance': 13.176281929016113, 'force': [-0.8222029209136963, 1.71388578414917, 0.20834310352802277], 'magnitude': 1.9122836589813232, 'cosine_ionic_motion': -0.7438585758209229, 'motion_component_ionic': -1.4224685430526733, 'motion_component_percent_ionic': 74.38585758209229}, {'ion_id': 2350, 'distance': 13.098273277282715, 'force': [-0.40187186002731323, 0.7030442357063293, -1.7575417757034302], 'magnitude': 1.9351292848587036, 'cosine_ionic_motion': 0.26885339617729187, 'motion_component_ionic': 0.520266056060791, 'motion_component_percent_ionic': 26.885339617729187}, {'ion_id': 2372, 'distance': 6.384522914886475, 'force': [5.76467752456665, 5.282864570617676, 2.279876470565796], 'magnitude': 8.144814491271973, 'cosine_ionic_motion': -0.006430993787944317, 'motion_component_ionic': -0.05237925052642822, 'motion_component_percent_ionic': 0.6430993787944317}], 'glu_contributions': [{'resid': 754, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 5.026372909545898, 'force': [-2.8731915950775146, -10.182400703430176, 0.28219449520111084], 'magnitude': 10.583767890930176, 'cosine_with_motion': 0.2366967499256134, 'motion_component': 2.505143404006958, 'motion_component_percent': 23.66967499256134}, {'resid': 754, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 5.194055080413818, 'force': [0.2995319664478302, 10.04994010925293, -0.6645428538322449], 'magnitude': 10.076339721679688, 'cosine_with_motion': -0.38383781909942627, 'motion_component': -3.867680311203003, 'motion_component_percent': 38.38378190994263}, {'resid': 754, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 4.985082149505615, 'force': [4.610184192657471, 9.645471572875977, -2.3171792030334473], 'magnitude': 10.938840866088867, 'cosine_with_motion': 0.010820849798619747, 'motion_component': 0.11836755275726318, 'motion_component_percent': 1.0820849798619747}], 'asn_contributions': [{'resid': 786, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 5.846755504608154, 'force': [2.5790274143218994, 6.216129779815674, -5.704611301422119], 'magnitude': 8.822371482849121, 'cosine_with_motion': 0.2766627073287964, 'motion_component': 2.4408211708068848, 'motion_component_percent': 27.66627073287964}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 5.538305759429932, 'force': [-1.616061806678772, -3.505422592163086, 2.2973313331604004], 'magnitude': 4.4919233322143555, 'cosine_with_motion': -0.20239081978797913, 'motion_component': -0.9091240167617798, 'motion_component_percent': 20.239081978797913}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 5.7780656814575195, 'force': [-0.5085855722427368, -2.9807181358337402, 2.808513879776001], 'magnitude': 4.126873970031738, 'cosine_with_motion': -0.1808759719133377, 'motion_component': -0.7464523315429688, 'motion_component_percent': 18.08759719133377}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': -0.28591705655325567, 'motion_component_pip2': -8.915282704286193, 'motion_component_percent_pip2': 28.591705655325566}, 1201: {'frame': 1201, 'motion_vector': [-2.4408187866210938, 1.504486083984375, -2.6349411010742188], 'ionic_force': [-0.8328255116939545, 8.29288524389267, -18.137705624103546], 'ionic_force_magnitude': 19.961009726663093, 'radial_force': 8.334599210598016, 'axial_force': -18.137705624103546, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-6.122331857681274, 5.094998836517334, -0.9455718472599983], 'asn_force_magnitude': 8.020976663600432, 'residue_force': [-6.122331857681274, 5.094998836517334, -0.9455718472599983], 'residue_force_magnitude': 8.020976663600432, 'total_force': [-6.955157369375229, 13.387884080410004, -19.083277471363544], 'total_force_magnitude': 24.3265520210391, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': 0.8036119578564771, 'cosine_residue_motion': 0.8036119578564771, 'cosine_ionic_motion': 0.8015053747012245, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': 6.445752760557057, 'motion_component_residue': 6.445752760557057, 'motion_component_ionic': 15.99885658038389, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 80.36119578564771, 'motion_component_percent_residue': 80.36119578564771, 'motion_component_percent_ionic': 80.15053747012246, 'ionic_contributions': [{'ion_id': 2230, 'distance': 7.425042152404785, 'force': [-5.259060382843018, 0.6449811458587646, -2.861936569213867], 'magnitude': 6.0219926834106445, 'cosine_ionic_motion': 0.9103459715843201, 'motion_component_ionic': 5.4820966720581055, 'motion_component_percent_ionic': 91.034597158432}, {'ion_id': 2280, 'distance': 10.684066772460938, 'force': [0.5116040110588074, 0.5324084162712097, -2.813185453414917], 'magnitude': 2.9084720611572266, 'cosine_ionic_motion': 0.6149501800537109, 'motion_component_ionic': 1.7885653972625732, 'motion_component_percent_ionic': 61.495018005371094}, {'ion_id': 2333, 'distance': 5.530528545379639, 'force': [0.676487922668457, 2.61903715133667, -10.511920928955078], 'magnitude': 10.854375839233398, 'cosine_ionic_motion': 0.7094592452049255, 'motion_component_ionic': 7.700736999511719, 'motion_component_percent_ionic': 70.94592452049255}, {'ion_id': 2334, 'distance': 9.29998779296875, 'force': [-0.43175986409187317, 3.7040369510650635, -0.9102612137794495], 'magnitude': 3.838604211807251, 'cosine_ionic_motion': 0.6037642359733582, 'motion_component_ionic': 2.3176119327545166, 'motion_component_percent_ionic': 60.376423597335815}, {'ion_id': 2372, 'distance': 9.231269836425781, 'force': [3.669902801513672, 0.7924215793609619, -1.0404014587402344], 'magnitude': 3.8959662914276123, 'cosine_ionic_motion': -0.33115118741989136, 'motion_component_ionic': -1.2901538610458374, 'motion_component_percent_ionic': 33.115118741989136}], 'glu_contributions': [], 'asn_contributions': [{'resid': 458, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 5.6313581466674805, 'force': [-6.832516670227051, 3.0307743549346924, -0.4583672285079956], 'magnitude': 7.488589763641357, 'cosine_with_motion': 0.769666314125061, 'motion_component': 5.7637152671813965, 'motion_component_percent': 76.9666314125061}, {'resid': 458, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 5.2503886222839355, 'force': [8.992154121398926, -6.170127868652344, -0.8732380270957947], 'magnitude': 10.940377235412598, 'cosine_with_motion': -0.6790657639503479, 'motion_component': -7.429235458374023, 'motion_component_percent': 67.90657639503479}, {'resid': 458, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 5.417903423309326, 'force': [-3.348132610321045, 3.289008855819702, 0.06398200243711472], 'magnitude': 4.693789958953857, 'cosine_with_motion': 0.7086012363433838, 'motion_component': 3.3260254859924316, 'motion_component_percent': 70.86012363433838}, {'resid': 458, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 4.818909168243408, 'force': [-4.851992607116699, 3.0617308616638184, 1.5122122764587402], 'magnitude': 5.9331955909729, 'cosine_with_motion': 0.5394884347915649, 'motion_component': 3.200890302658081, 'motion_component_percent': 53.948843479156494}, {'resid': 786, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 5.746336460113525, 'force': [1.0414265394210815, -7.0297698974609375, 1.1051353216171265], 'magnitude': 7.191909313201904, 'cosine_with_motion': -0.572380781173706, 'motion_component': -4.11651086807251, 'motion_component_percent': 57.238078117370605}, {'resid': 786, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 4.638833522796631, 'force': [-1.1232706308364868, 8.913382530212402, -2.2952961921691895], 'magnitude': 9.272459983825684, 'cosine_with_motion': 0.614817202091217, 'motion_component': 5.700867652893066, 'motion_component_percent': 61.481720209121704}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': 0.9226383303942732, 'motion_component_pip2': 22.444609340940946, 'motion_component_percent_pip2': 92.26383303942733}, 1202: {'frame': 1202, 'motion_vector': [3.7926063537597656, -5.016014099121094, -13.400657653808594], 'ionic_force': [-0.6478393822908401, 4.237316012382507, -17.316235780715942], 'ionic_force_magnitude': 17.838905921255016, 'radial_force': 4.28655372695131, 'axial_force': -17.316235780715942, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [7.699722766876221, 11.615922451019287, -2.109640121459961], 'asn_force_magnitude': 14.094891504262085, 'residue_force': [7.699722766876221, 11.615922451019287, -2.109640121459961], 'residue_force_magnitude': 14.094891504262085, 'total_force': [7.0518833845853806, 15.853238463401794, -19.425875902175903], 'total_force_magnitude': 26.046475454733063, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': -0.0038009741047441087, 'cosine_residue_motion': -0.0038009741047441087, 'cosine_ionic_motion': 0.7889625338413784, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': -0.05357431761687792, 'motion_component_residue': -0.05357431761687792, 'motion_component_ionic': 14.074228416591325, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 0.38009741047441087, 'motion_component_percent_residue': 0.38009741047441087, 'motion_component_percent_ionic': 78.89625338413784, 'ionic_contributions': [{'ion_id': 2230, 'distance': 11.394763946533203, 'force': [-1.9107823371887207, 0.6259081959724426, -1.5796518325805664], 'magnitude': 2.556980609893799, 'cosine_ionic_motion': 0.2848574221134186, 'motion_component_ionic': 0.7283748984336853, 'motion_component_percent_ionic': 28.485742211341858}, {'ion_id': 2280, 'distance': 12.427170753479004, 'force': [-0.2162904292345047, 0.5440843105316162, -2.0685102939605713], 'magnitude': 2.14977765083313, 'cosine_ionic_motion': 0.7595205307006836, 'motion_component_ionic': 1.6328002214431763, 'motion_component_percent_ionic': 75.95205307006836}, {'ion_id': 2333, 'distance': 5.691808700561523, 'force': [-1.1114851236343384, -0.53433758020401, -10.17348575592041], 'magnitude': 10.24796199798584, 'cosine_ionic_motion': 0.8885816335678101, 'motion_component_ionic': 9.10615062713623, 'motion_component_percent_ionic': 88.858163356781}, {'ion_id': 2334, 'distance': 11.886580467224121, 'force': [-0.699772834777832, 2.0069098472595215, -1.0020081996917725], 'magnitude': 2.3497636318206787, 'cosine_ionic_motion': 0.020323658362030983, 'motion_component_ionic': 0.04775579273700714, 'motion_component_percent_ionic': 2.0323658362030983}, {'ion_id': 2372, 'distance': 8.661564826965332, 'force': [3.2904913425445557, 1.594751238822937, -2.492579698562622], 'magnitude': 4.425326824188232, 'cosine_ionic_motion': 0.5782955884933472, 'motion_component_ionic': 2.5591468811035156, 'motion_component_percent_ionic': 57.82955884933472}], 'glu_contributions': [], 'asn_contributions': [{'resid': 786, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 3.7162702083587646, 'force': [-6.212677955627441, -15.210829734802246, -5.070935249328613], 'magnitude': 17.19537925720215, 'cosine_with_motion': 0.4741484820842743, 'motion_component': 8.153162956237793, 'motion_component_percent': 47.41484820842743}, {'resid': 786, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 2.716343402862549, 'force': [13.24149227142334, 23.43450927734375, 2.6021718978881836], 'magnitude': 27.042274475097656, 'cosine_with_motion': -0.2553054392337799, 'motion_component': -6.90403938293457, 'motion_component_percent': 25.53054392337799}, {'resid': 786, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 4.285270690917969, 'force': [8.064279556274414, 11.941207885742188, 7.880201816558838], 'magnitude': 16.423234939575195, 'cosine_with_motion': -0.5549459457397461, 'motion_component': -9.114007949829102, 'motion_component_percent': 55.49459457397461}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 4.084445476531982, 'force': [-5.330751895904541, -4.5744123458862305, -4.343565464019775], 'magnitude': 8.258857727050781, 'cosine_with_motion': 0.49842569231987, 'motion_component': 4.116426944732666, 'motion_component_percent': 49.842569231987}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 5.009314060211182, 'force': [-2.062619209289551, -3.974552631378174, -3.1775131225585938], 'magnitude': 5.490724563598633, 'cosine_with_motion': 0.6729316115379333, 'motion_component': 3.6948821544647217, 'motion_component_percent': 67.29316115379333}], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': 0.5382937174490788, 'motion_component_pip2': 14.020654098974447, 'motion_component_percent_pip2': 53.82937174490788}, 1203: {'frame': 1203, 'motion_vector': [-3.8949356079101562, 6.270046234130859, -1.43634033203125], 'ionic_force': [6.087128639221191, 6.551774024963379, 11.820940017700195], 'ionic_force_magnitude': 14.82273594336341, 'radial_force': 8.943091073259383, 'axial_force': 11.820940017700195, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [0.0, 0.0, 0.0], 'asn_force_magnitude': 0.0, 'residue_force': [0.0, 0.0, 0.0], 'residue_force_magnitude': 0.0, 'total_force': [6.087128639221191, 6.551774024963379, 11.820940017700195], 'total_force_magnitude': 14.82273594336341, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': 0, 'cosine_residue_motion': 0, 'cosine_ionic_motion': 0.003517374897341577, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': 0, 'motion_component_residue': 0, 'motion_component_ionic': 0.05213711931710918, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 0, 'motion_component_percent_residue': 0, 'motion_component_percent_ionic': 0.3517374897341577, 'ionic_contributions': [{'ion_id': 2343, 'distance': 4.732655048370361, 'force': [6.087128639221191, 6.551774024963379, 11.820940017700195], 'magnitude': 14.822735786437988, 'cosine_ionic_motion': 0.003517359960824251, 'motion_component_ionic': 0.052136898040771484, 'motion_component_percent_ionic': 0.3517359960824251}], 'glu_contributions': [], 'asn_contributions': [], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': 0.003517374897341577, 'motion_component_pip2': 0.05213711931710918, 'motion_component_percent_pip2': 0.3517374897341577}, 1204: {'frame': 1204, 'motion_vector': [2.462512969970703, 0.90899658203125, 1.249908447265625], 'ionic_force': [-1.0780160427093506, 2.133450984954834, 2.4368791580200195], 'ionic_force_magnitude': 3.413518964988453, 'radial_force': 2.3903413341076374, 'axial_force': 2.4368791580200195, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [0.0, 0.0, 0.0], 'asn_force_magnitude': 0.0, 'residue_force': [0.0, 0.0, 0.0], 'residue_force_magnitude': 0.0, 'total_force': [-1.0780160427093506, 2.133450984954834, 2.4368791580200195], 'total_force_magnitude': 3.413518964988453, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': 0, 'cosine_residue_motion': 0, 'cosine_ionic_motion': 0.2348348627107997, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': 0, 'motion_component_residue': 0, 'motion_component_ionic': 0.8016132575037744, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 0, 'motion_component_percent_residue': 0, 'motion_component_percent_ionic': 23.483486271079972, 'ionic_contributions': [{'ion_id': 2343, 'distance': 9.862065315246582, 'force': [-1.0780160427093506, 2.133450984954834, 2.4368791580200195], 'magnitude': 3.4135189056396484, 'cosine_ionic_motion': 0.23483486473560333, 'motion_component_ionic': 0.8016132712364197, 'motion_component_percent_ionic': 23.483486473560333}], 'glu_contributions': [], 'asn_contributions': [], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': 0.2348348627107997, 'motion_component_pip2': 0.8016132575037744, 'motion_component_percent_pip2': 23.483486271079972}, 1205: {'frame': 1205, 'motion_vector': [-0.2692909240722656, 0.2013092041015625, -0.2580718994140625], 'ionic_force': [0.029493005946278572, 0.9422394633293152, 1.9188988208770752], 'ionic_force_magnitude': 2.137956437446351, 'radial_force': 0.9427009301230498, 'axial_force': 1.9188988208770752, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [0.0, 0.0, 0.0], 'asn_force_magnitude': 0.0, 'residue_force': [0.0, 0.0, 0.0], 'residue_force_magnitude': 0.0, 'total_force': [0.029493005946278572, 0.9422394633293152, 1.9188988208770752], 'total_force_magnitude': 2.137956437446351, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': 0, 'cosine_residue_motion': 0, 'cosine_ionic_motion': -0.3459370081418998, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': 0, 'motion_component_residue': 0, 'motion_component_ionic': -0.7395982535079055, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 0, 'motion_component_percent_residue': 0, 'motion_component_percent_ionic': 34.59370081418998, 'ionic_contributions': [{'ion_id': 2343, 'distance': 12.461480140686035, 'force': [0.029493005946278572, 0.9422394633293152, 1.9188988208770752], 'magnitude': 2.1379566192626953, 'cosine_ionic_motion': -0.34593698382377625, 'motion_component_ionic': -0.739598274230957, 'motion_component_percent_ionic': 34.593698382377625}], 'glu_contributions': [], 'asn_contributions': [], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': -0.3459370081418998, 'motion_component_pip2': -0.7395982535079055, 'motion_component_percent_pip2': 34.59370081418998}, 1206: {'frame': 1206, 'motion_vector': [-0.7671661376953125, -0.17943572998046875, 0.18552398681640625], 'ionic_force': [0.0, 0.0, 0.0], 'ionic_force_magnitude': 0.0, 'radial_force': 0.0, 'axial_force': 0.0, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [0.0, 0.0, 0.0], 'asn_force_magnitude': 0.0, 'residue_force': [0.0, 0.0, 0.0], 'residue_force_magnitude': 0.0, 'total_force': [0.0, 0.0, 0.0], 'total_force_magnitude': 0.0, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': 0, 'cosine_residue_motion': 0, 'cosine_ionic_motion': 0, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': 0, 'motion_component_residue': 0, 'motion_component_ionic': 0, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 0, 'motion_component_percent_residue': 0, 'motion_component_percent_ionic': 0, 'ionic_contributions': [], 'glu_contributions': [], 'asn_contributions': [], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': []}, 1207: {'frame': 1207, 'motion_vector': [2.8995819091796875, -8.923038482666016, -2.8341140747070312], 'ionic_force': [0.0, 0.0, 0.0], 'ionic_force_magnitude': 0.0, 'radial_force': 0.0, 'axial_force': 0.0, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [0.0, 0.0, 0.0], 'asn_force_magnitude': 0.0, 'residue_force': [0.0, 0.0, 0.0], 'residue_force_magnitude': 0.0, 'total_force': [0.0, 0.0, 0.0], 'total_force_magnitude': 0.0, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': 0, 'cosine_residue_motion': 0, 'cosine_ionic_motion': 0, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': 0, 'motion_component_residue': 0, 'motion_component_ionic': 0, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 0, 'motion_component_percent_residue': 0, 'motion_component_percent_ionic': 0, 'ionic_contributions': [], 'glu_contributions': [], 'asn_contributions': [], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': []}, 1208: {'frame': 1208, 'motion_vector': [-1.0768890380859375, 1.3192253112792969, -1.6772384643554688], 'ionic_force': [0.0, 0.0, 0.0], 'ionic_force_magnitude': 0.0, 'radial_force': 0.0, 'axial_force': 0.0, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [0.0, 0.0, 0.0], 'asn_force_magnitude': 0.0, 'residue_force': [0.0, 0.0, 0.0], 'residue_force_magnitude': 0.0, 'total_force': [0.0, 0.0, 0.0], 'total_force_magnitude': 0.0, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': 0, 'cosine_residue_motion': 0, 'cosine_ionic_motion': 0, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': 0, 'motion_component_residue': 0, 'motion_component_ionic': 0, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 0, 'motion_component_percent_residue': 0, 'motion_component_percent_ionic': 0, 'ionic_contributions': [], 'glu_contributions': [], 'asn_contributions': [], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': []}, 1209: {'frame': 1209, 'motion_vector': [-0.0893402099609375, 0.9161643981933594, 1.8559417724609375], 'ionic_force': [0.011790893040597439, -0.1435059905052185, 1.8912526369094849], 'ionic_force_magnitude': 1.8967260031661555, 'radial_force': 0.14398956375230348, 'axial_force': 1.8912526369094849, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [0.0, 0.0, 0.0], 'asn_force_magnitude': 0.0, 'residue_force': [0.0, 0.0, 0.0], 'residue_force_magnitude': 0.0, 'total_force': [0.011790893040597439, -0.1435059905052185, 1.8912526369094849], 'total_force_magnitude': 1.8967260031661555, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': 0, 'cosine_residue_motion': 0, 'cosine_ionic_motion': 0.8595506026939018, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': 0, 'motion_component_residue': 0, 'motion_component_ionic': 1.6303319791666644, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 0, 'motion_component_percent_residue': 0, 'motion_component_percent_ionic': 85.95506026939019, 'ionic_contributions': [{'ion_id': 2343, 'distance': 13.230210304260254, 'force': [0.011790893040597439, -0.1435059905052185, 1.8912526369094849], 'magnitude': 1.8967260122299194, 'cosine_ionic_motion': 0.8595505952835083, 'motion_component_ionic': 1.6303319931030273, 'motion_component_percent_ionic': 85.95505952835083}], 'glu_contributions': [], 'asn_contributions': [], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': 0.8595506026939018, 'motion_component_pip2': 1.6303319791666644, 'motion_component_percent_pip2': 85.95506026939019}, 1210: {'frame': 1210, 'motion_vector': [0.5050811767578125, 0.5206947326660156, -2.4637680053710938], 'ionic_force': [0.0, 0.0, 0.0], 'ionic_force_magnitude': 0.0, 'radial_force': 0.0, 'axial_force': 0.0, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [0.0, 0.0, 0.0], 'asn_force_magnitude': 0.0, 'residue_force': [0.0, 0.0, 0.0], 'residue_force_magnitude': 0.0, 'total_force': [0.0, 0.0, 0.0], 'total_force_magnitude': 0.0, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': 0, 'cosine_residue_motion': 0, 'cosine_ionic_motion': 0, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': 0, 'motion_component_residue': 0, 'motion_component_ionic': 0, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 0, 'motion_component_percent_residue': 0, 'motion_component_percent_ionic': 0, 'ionic_contributions': [], 'glu_contributions': [], 'asn_contributions': [], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': []}, 1211: {'frame': 1211, 'motion_vector': [-0.0905609130859375, -2.4952964782714844, 2.7269058227539062], 'ionic_force': [0.062217146158218384, -0.09291313588619232, 0.03429150581359863], 'ionic_force_magnitude': 0.11696038417876035, 'radial_force': 0.11182049944567028, 'axial_force': 0.03429150581359863, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [0.0, 0.0, 0.0], 'asn_force_magnitude': 0.0, 'residue_force': [0.0, 0.0, 0.0], 'residue_force_magnitude': 0.0, 'total_force': [0.062217146158218384, -0.09291313588619232, 0.03429150581359863], 'total_force_magnitude': 0.11696038417876035, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': 0, 'cosine_residue_motion': 0, 'cosine_ionic_motion': 0.7393273390055136, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': 0, 'motion_component_residue': 0, 'motion_component_ionic': 0.08647200960394547, 'motion_component_percent_total': 0, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 0, 'motion_component_percent_residue': 0, 'motion_component_percent_ionic': 73.93273390055136, 'ionic_contributions': [{'ion_id': 2245, 'distance': 13.162017822265625, 'force': [-0.3218527138233185, -0.29624900221824646, 1.865838646888733], 'magnitude': 1.9164305925369263, 'cosine_ionic_motion': 0.8264901041984558, 'motion_component_ionic': 1.5839109420776367, 'motion_component_percent_ionic': 82.64901041984558}, {'ion_id': 2334, 'distance': 13.280467987060547, 'force': [0.38406985998153687, 0.20333586633205414, -1.8315471410751343], 'magnitude': 1.8823974132537842, 'cosine_ionic_motion': -0.7954956293106079, 'motion_component_ionic': -1.497438907623291, 'motion_component_percent_ionic': 79.54956293106079}], 'glu_contributions': [], 'asn_contributions': [], 'pip2_force': [0.0, 0.0, 0.0], 'pip2_force_magnitude': 0.0, 'pip2_contributions': [], 'cosine_pip2_motion': 0.7393273390055136, 'motion_component_pip2': 0.08647200960394547, 'motion_component_percent_pip2': 73.93273390055136}, 1212: {'frame': 1212, 'motion_vector': [0.090057373046875, 1.2251663208007812, -2.0446929931640625], 'ionic_force': [1.044351577758789, -0.5711382031440735, -4.79685115814209], 'ionic_force_magnitude': 4.942332455271197, 'radial_force': 1.1903230927180708, 'axial_force': -4.79685115814209, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [0.0, 0.0, 0.0], 'asn_force_magnitude': 0.0, 'residue_force': [0.0, 0.0, 0.0], 'residue_force_magnitude': 0.0, 'total_force': [1.044351577758789, -0.5711382031440735, -4.79685115814209], 'total_force_magnitude': 4.942332455271197, 'cosine_total_motion': 0, 'cosine_glu_motion': 0, 'cosine_asn_motion': 0, 'cosine_residue_motion': 0, 'cosine_ionic_motion': 0.7805780641070944, 'motion_component_total': 0, 'motion_component_glu': 0, 'motion_component_asn': 0, 'motion_component_residue': 0, 'motion_component_ionic': 3.8578763001092</t>
+          <t>{1199: {'frame': 1199, 'motion_vector': [-3.884815216064453, 1.590545654296875, 1.432769775390625], 'ionic_force': [14.11787834763527, -5.172281384468079, -12.066099643707275], 'ionic_force_magnitude': 19.27842691639068, 'radial_force': 15.035524059996838, 'axial_force': -12.066099643707275, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [0.0, 0.0, 0.0], 'asn_force_magnitude': 0.0, 'residue_force': [0.0, 0.0, 0.0], 'residue_force_magnitude': 0.0, 'pip2_force': [0.7719871196895838, -0.11984185688197613, -4.625281474491203], 'pip2_force_magnitude': 4.690794698331942, 'total_force': [14.889865467324853, -5.292123241350055, -16.69138111819848], 'total_force_magnitude': 22.985144456139995, 'cosine_total_motion': -0.8844952873793044, 'cosine_glu_motion': 0, 'cosine_asn_motion': 0, 'cosine_residue_motion': 0, 'cosine_pip2_motion': -0.4718061154839001, 'cosine_ionic_motion': -0.9397606145256897, 'motion_component_total': -20.33025195118837, 'motion_component_glu': 0, 'motion_component_asn': 0, 'motion_component_residue': 0, 'motion_component_ionic': -18.117106326035902, 'motion_component_pip2': -2.2131456251524666, 'motion_component_percent_total': 88.44952873793044, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 0, 'motion_component_percent_residue': 0, 'motion_component_percent_ionic': 93.97606145256897, 'motion_component_percent_pip2': 47.18061154839001, 'ionic_contributions': [{'ion_id': 2230, 'distance': 7.779934883117676, 'force': [-4.786203861236572, 2.3370611667633057, -1.3103206157684326], 'magnitude': 5.4851202964782715, 'cosine_ionic_motion': 0.8398500084877014, 'motion_component_ionic': 4.606678485870361, 'motion_component_percent_ionic': 83.98500084877014}, {'ion_id': 2280, 'distance': 8.599261283874512, 'force': [0.6796392798423767, 1.932413935661316, -3.995137929916382], 'magnitude': 4.489683628082275, 'cosine_ionic_motion': -0.2656768560409546, 'motion_component_ionic': -1.1928050518035889, 'motion_component_percent_ionic': 26.56768560409546}, {'ion_id': 2333, 'distance': 4.074949264526367, 'force': [12.101813316345215, -14.844310760498047, -5.739468097686768], 'magnitude': 19.993722915649414, 'cosine_ionic_motion': -0.8890808820724487, 'motion_component_ionic': -17.776037216186523, 'motion_component_percent_ionic': 88.90808820724487}, {'ion_id': 2334, 'distance': 10.257603645324707, 'force': [-0.4024566113948822, 3.128925085067749, -0.06349241733551025], 'magnitude': 3.1553406715393066, 'cosine_ionic_motion': 0.4607953727245331, 'motion_component_ionic': 1.4539663791656494, 'motion_component_percent_ionic': 46.07953727245331}, {'ion_id': 2350, 'distance': 13.552000999450684, 'force': [0.13162976503372192, 0.44357430934906006, -1.747503399848938], 'magnitude': 1.8077203035354614, 'cosine_ionic_motion': -0.2880411744117737, 'motion_component_ionic': -0.5206978917121887, 'motion_component_percent_ionic': 28.804117441177368}, {'ion_id': 2372, 'distance': 7.040935039520264, 'force': [6.39345645904541, 1.8300548791885376, 0.7898228168487549], 'magnitude': 6.696954727172852, 'cosine_ionic_motion': -0.7000511884689331, 'motion_component_ionic': -4.688210964202881, 'motion_component_percent_ionic': 70.00511884689331}], 'glu_contributions': [], 'asn_contributions': [], 'pip2_contributions': [{'resid': 1313, 'atom': 'C1', 'charge': 0.06000000238418579, 'distance': 26.0665225982666, 'force': [-0.01957365870475769, -0.013995480723679066, 0.016748113557696342], 'magnitude': 0.02931724488735199, 'cosine_with_motion': 0.5980947017669678, 'motion_component': 0.017534488812088966, 'motion_component_percent': 59.80947017669678}, {'resid': 1313, 'atom': 'C11', 'charge': 0.17000000178813934, 'distance': 25.322599411010742, 'force': [-0.06587626785039902, -0.04122985526919365, 0.04132247343659401], 'magnitude': 0.0880177840590477, 'cosine_with_motion': 0.6391851902008057, 'motion_component': 0.05625966191291809, 'motion_component_percent': 63.918519020080566}, {'resid': 1313, 'atom': 'C12', 'charge': 0.04000000283122063, 'distance': 25.24015235900879, 'force': [-0.01629634201526642, -0.00952364131808281, 0.008846919052302837], 'magnitude': 0.02084558643400669, 'cosine_with_motion': 0.6579544544219971, 'motion_component': 0.013715446926653385, 'motion_component_percent': 65.7954454421997}, {'resid': 1313, 'atom': 'C13', 'charge': -0.05000000074505806, 'distance': 26.079870223999023, 'force': [0.01909954659640789, 0.01190575584769249, -0.009440068155527115], 'magnitude': 0.024406036362051964, 'cosine_with_motion': -0.6354155540466309, 'motion_component': -0.015507974661886692, 'motion_component_percent': 63.541555404663086}, {'resid': 1313, 'atom': 'C2', 'charge': 0.06000000238418579, 'distance': 27.571277618408203, 'force': [-0.01775849051773548, -0.012352199293673038, 0.014789661392569542], 'magnitude': 0.026204481720924377, 'cosine_with_motion': 0.6068183779716492, 'motion_component': 0.015901360660791397, 'motion_component_percent': 60.68183779716492}, {'resid': 1313, 'atom': 'C21', 'charge': 0.6299999952316284, 'distance': 22.81819725036621, 'force': [-0.31783321499824524, -0.17262010276317596, 0.17480769753456116], 'magnitude': 0.4017130434513092, 'cosine_with_motion': 0.6794248819351196, 'motion_component': 0.27293384075164795, 'motion_component_percent': 67.94248819351196}, {'resid': 1313, 'atom': 'C210', 'charge': -0.18000000715255737, 'distance': 22.665035247802734, 'force': [0.09244047850370407, 0.06488973647356033, -0.02787701040506363], 'magnitude': 0.11633162945508957, 'cosine_with_motion': -0.5733445882797241, 'motion_component': -0.0666981115937233, 'motion_component_percent': 57.33445882797241}, {'resid': 1313, 'atom': 'C211', 'charge': -0.15000000596046448, 'distance': 24.07269287109375, 'force': [0.06863471865653992, 0.04683786630630493, -0.02192377857863903], 'magnitude': 0.08593696355819702, 'cosine_with_motion': -0.586459219455719, 'motion_component': -0.05039852485060692, 'motion_component_percent': 58.6459219455719}, {'resid': 1313, 'atom': 'C212', 'charge': -0.15000000596046448, 'distance': 25.074344635009766, 'force': [0.06454970687627792, 0.042374201118946075, -0.017655104398727417], 'magnitude': 0.07920821011066437, 'cosine_with_motion': -0.5939096212387085, 'motion_component': -0.047042518854141235, 'motion_component_percent': 59.39096212387085}, {'resid': 1313, 'atom': 'C213', 'charge': -0.18000000715255737, 'distance': 25.018484115600586, 'force': [0.07883255183696747, 0.051574669778347015, -0.015521443448960781], 'magnitude': 0.09547477215528488, 'cosine_with_motion': -0.5819700956344604, 'motion_component': -0.055563461035490036, 'motion_component_percent': 58.197009563446045}, {'resid': 1313, 'atom': 'C214', 'charge': -0.15000000596046448, 'distance': 26.480010986328125, 'force': [0.0592246949672699, 0.03791127726435661, -0.009964889846742153], 'magnitude': 0.07102203369140625, 'cosine_with_motion': -0.5842553377151489, 'motion_component': -0.041495002806186676, 'motion_component_percent': 58.42553377151489}, {'resid': 1313, 'atom': 'C215', 'charge': -0.15000000596046448, 'distance': 26.941884994506836, 'force': [0.058843906968832016, 0.03444577381014824, -0.007609979715198278], 'magnitude': 0.06860778480768204, 'cosine_with_motion': -0.6069793105125427, 'motion_component': -0.04164350405335426, 'motion_component_percent': 60.69793105125427}, {'resid': 1313, 'atom': 'C216', 'charge': -0.18000000715255737, 'distance': 26.1450138092041, 'force': [0.07687947899103165, 0.0409686453640461, -0.007358555682003498], 'magnitude': 0.08742443472146988, 'cosine_with_motion': -0.6293359994888306, 'motion_component': -0.05501934140920639, 'motion_component_percent': 62.93359994888306}, {'resid': 1313, 'atom': 'C217', 'charge': -0.18000000715255737, 'distance': 26.68497085571289, 'force': [0.0742553174495697, 0.0390210784971714, -0.002539152279496193], 'magnitude': 0.08392225205898285, 'cosine_with_motion': -0.617984414100647, 'motion_component': -0.05186264589428902, 'motion_component_percent': 61.7984414100647}, {'resid': 1313, 'atom': 'C218', 'charge': -0.18000000715255737, 'distance': 25.67491912841797, 'force': [0.08127076923847198, 0.04016231372952461, 0.000637041695881635], 'magnitude': 0.09065514802932739, 'cosine_with_motion': -0.624032735824585, 'motion_component': -0.056571781635284424, 'motion_component_percent': 62.403273582458496}, {'resid': 1313, 'atom': 'C219', 'charge': -0.18000000715255737, 'distance': 25.39031219482422, 'force': [0.08545580506324768, 0.03592049330472946, -0.00032528574229218066], 'magnitude': 0.09269887953996658, 'cosine_with_motion': -0.6695773601531982, 'motion_component': -0.06206906959414482, 'motion_component_percent': 66.95773601531982}, {'resid': 1313, 'atom': 'C22', 'charge': -0.08000000566244125, 'distance': 21.493654251098633, 'force': [0.04605632647871971, 0.02505752630531788, -0.023585326969623566], 'magnitude': 0.05749202147126198, 'cosine_with_motion': -0.6778433918952942, 'motion_component': -0.03897058591246605, 'motion_component_percent': 67.78433918952942}, {'resid': 1313, 'atom': 'C220', 'charge': -0.27000001072883606, 'distance': 24.44317626953125, 'force': [0.13973203301429749, 0.05429749935865402, 0.006051207426935434], 'magnitude': 0.1500329226255417, 'cosine_with_motion': -0.6728940606117249, 'motion_component': -0.1009562611579895, 'motion_component_percent': 67.28940606117249}, {'resid': 1313, 'atom': 'C23', 'charge': -0.18000000715255737, 'distance': 21.138935089111328, 'force': [0.11249882727861404, 0.0509958490729332, -0.05126822367310524], 'magnitude': 0.133734792470932, 'cosine_with_motion': -0.7238483428955078, 'motion_component': -0.0968037098646164, 'motion_component_percent': 72.38483428955078}, {'resid': 1313, 'atom': 'C24', 'charge': -0.18000000715255737, 'distance': 19.86398696899414, 'force': [0.12989076972007751, 0.05857183411717415, -0.05133931338787079], 'magnitude': 0.1514529585838318, 'cosine_with_motion': -0.7219560146331787, 'motion_component': -0.10934237390756607, 'motion_component_percent': 72.19560146331787}, {'resid': 1313, 'atom': 'C25', 'charge': -0.15000000596046448, 'distance': 18.801464080810547, 'force': [0.11715246737003326, 0.060481004416942596, -0.04964090511202812], 'magnitude': 0.14087893068790436, 'cosine_with_motion': -0.688197910785675, 'motion_component': -0.09695258736610413, 'motion_component_percent': 68.8197910785675}, {'resid': 1313, 'atom': 'C26', 'charge': -0.15000000596046448, 'distance': 18.753000259399414, 'force': [0.11380141973495483, 0.06990958750247955, -0.0470607727766037], 'magnitude': 0.14160801470279694, 'cosine_with_motion': -0.6341679096221924, 'motion_component': -0.08980325609445572, 'motion_component_percent': 63.41679096221924}, {'resid': 1313, 'atom': 'C27', 'charge': -0.18000000715255737, 'distance': 19.71270751953125, 'force': [0.1229880079627037, 0.08156406879425049, -0.043261051177978516], 'magnitude': 0.15378643572330475, 'cosine_with_motion': -0.6011102795600891, 'motion_component': -0.09244260936975479, 'motion_component_percent': 60.11102795600891}, {'resid': 1313, 'atom': 'C28', 'charge': -0.15000000596046448, 'distance': 20.788883209228516, 'force': [0.08819501847028732, 0.06492965668439865, -0.035830460488796234], 'magnitude': 0.11523039638996124, 'cosine_with_motion': -0.5687267184257507, 'motion_component': -0.06553460657596588, 'motion_component_percent': 56.87267184257507}, {'resid': 1313, 'atom': 'C29', 'charge': -0.15000000596046448, 'distance': 21.98827362060547, 'force': [0.07889336347579956, 0.05902434512972832, -0.030024083331227303], 'magnitude': 0.10300233960151672, 'cosine_with_motion': -0.5595014691352844, 'motion_component': -0.05762995779514313, 'motion_component_percent': 55.95014691352844}, {'resid': 1313, 'atom': 'C3', 'charge': 0.06000000238418579, 'distance': 28.32106590270996, 'force': [-0.016719989478588104, -0.010827700607478619, 0.014832299202680588], 'magnitude': 0.024835342541337013, 'cosine_with_motion': 0.6262143850326538, 'motion_component': 0.015552248805761337, 'motion_component_percent': 62.62143850326538}, {'resid': 1313, 'atom': 'C31', 'charge': 0.6299999952316284, 'distance': 27.1365966796875, 'force': [-0.2361566424369812, -0.12329070270061493, 0.09850811958312988], 'magnitude': 0.28403240442276, 'cosine_with_motion': 0.6845768094062805, 'motion_component': 0.1944420039653778, 'motion_component_percent': 68.45768094062805}, {'resid': 1313, 'atom': 'C310', 'charge': -0.18000000715255737, 'distance': 20.339704513549805, 'force': [0.13286229968070984, 0.056033045053482056, -0.008606718853116035], 'magnitude': 0.14445126056671143, 'cosine_with_motion': -0.6857119798660278, 'motion_component': -0.09905195981264114, 'motion_component_percent': 68.57119798660278}, {'resid': 1313, 'atom': 'C311', 'charge': -0.18000000715255737, 'distance': 18.827796936035156, 'force': [0.15463179349899292, 0.06578080356121063, -0.013484744355082512], 'magnitude': 0.16858215630054474, 'cosine_with_motion': -0.6892696619033813, 'motion_component': -0.11619856208562851, 'motion_component_percent': 68.92696619033813}, {'resid': 1313, 'atom': 'C312', 'charge': -0.18000000715255737, 'distance': 18.4708251953125, 'force': [0.16271767020225525, 0.05958602577447891, -0.02557193860411644], 'magnitude': 0.1751612424850464, 'cosine_with_motion': -0.7387829422950745, 'motion_component': -0.12940613925457, 'motion_component_percent': 73.87829422950745}, {'resid': 1313, 'atom': 'C313', 'charge': -0.18000000715255737, 'distance': 17.093366622924805, 'force': [0.18851545453071594, 0.06968317180871964, -0.03792605549097061], 'magnitude': 0.20452924072742462, 'cosine_with_motion': -0.7449812889099121, 'motion_component': -0.15237045288085938, 'motion_component_percent': 74.49812889099121}, {'resid': 1313, 'atom': 'C314', 'charge': -0.18000000715255737, 'distance': 16.7066707611084, 'force': [0.20063360035419464, 0.05663676932454109, -0.04878753423690796], 'magnitude': 0.214106947183609, 'cosine_with_motion': -0.7994630336761475, 'motion_component': -0.17117059230804443, 'motion_component_percent': 79.94630336761475}, {'resid': 1313, 'atom': 'C315', 'charge': -0.18000000715255737, 'distance': 15.272680282592773, 'force': [0.23758867383003235, 0.06862706691026688, -0.06693781167268753], 'magnitude': 0.25620055198669434, 'cosine_with_motion': -0.800545334815979, 'motion_component': -0.2051001638174057, 'motion_component_percent': 80.0545334815979}, {'resid': 1313, 'atom': 'C316', 'charge': -0.18000000715255737, 'distance': 15.101518630981445, 'force': [0.2322043627500534, 0.08464948832988739, -0.08706961572170258], 'magnitude': 0.2620410621166229, 'cosine_with_motion': -0.7675969004631042, 'motion_component': -0.20114190876483917, 'motion_component_percent': 76.75969004631042}, {'resid': 1313, 'atom': 'C317', 'charge': -0.18000000715255737, 'distance': 15.857123374938965, 'force': [0.20565354824066162, 0.06906475126743317, -0.09705890715122223], 'magnitude': 0.23766310513019562, 'cosine_with_motion': -0.7855790257453918, 'motion_component': -0.1867031455039978, 'motion_component_percent': 78.55790257453918}, {'resid': 1313, 'atom': 'C318', 'charge': -0.27000001072883606, 'distance': 15.803705215454102, 'force': [0.29163336753845215, 0.122316874563694, -0.16971753537654877], 'magnitude': 0.3589087426662445, 'cosine_with_motion': -0.7421974539756775, 'motion_component': -0.2663811445236206, 'motion_component_percent': 74.21974539756775}, {'resid': 1313, 'atom': 'C32', 'charge': -0.08000000566244125, 'distance': 27.52945899963379, 'force': [0.02996961958706379, 0.01487260777503252, -0.01043154951184988], 'magnitude': 0.03504553809762001, 'cosine_with_motion': -0.6929464936256409, 'motion_component': -0.024284683167934418, 'motion_component_percent': 69.29464936256409}, {'resid': 1313, 'atom': 'C33', 'charge': -0.18000000715255737, 'distance': 26.842418670654297, 'force': [0.07298870384693146, 0.03167038783431053, -0.023426136001944542], 'magnitude': 0.08294063061475754, 'cosine_with_motion': -0.7250490188598633, 'motion_component': -0.06013602390885353, 'motion_component_percent': 72.50490188598633}, {'resid': 1313, 'atom': 'C34', 'charge': -0.18000000715255737, 'distance': 25.25910186767578, 'force': [0.08282198756933212, 0.03486067056655884, -0.026425013318657875], 'magnitude': 0.09366445243358612, 'cosine_with_motion': -0.7321131825447083, 'motion_component': -0.0685729831457138, 'motion_component_percent': 73.21131825447083}, {'resid': 1313, 'atom': 'C35', 'charge': -0.18000000715255737, 'distance': 24.524402618408203, 'force': [0.08667964488267899, 0.04143088683485985, -0.025350095704197884], 'magnitude': 0.09936048835515976, 'cosine_with_motion': -0.6969411969184875, 'motion_component': -0.06924841552972794, 'motion_component_percent': 69.69411969184875}, {'resid': 1313, 'atom': 'C36', 'charge': -0.18000000715255737, 'distance': 23.242610931396484, 'force': [0.09796544164419174, 0.04504323750734329, -0.02471969835460186], 'magnitude': 0.11062180995941162, 'cosine_with_motion': -0.7017953395843506, 'motion_component': -0.07763387262821198, 'motion_component_percent': 70.17953395843506}, {'resid': 1313, 'atom': 'C37', 'charge': -0.18000000715255737, 'distance': 23.580490112304688, 'force': [0.09772250056266785, 0.04090532660484314, -0.018105536699295044], 'magnitude': 0.10747438669204712, 'cosine_with_motion': -0.7142949104309082, 'motion_component': -0.0767684057354927, 'motion_component_percent': 71.42949104309082}, {'resid': 1313, 'atom': 'C38', 'charge': -0.18000000715255737, 'distance': 22.334787368774414, 'force': [0.11059410870075226, 0.04310492426156998, -0.01619555614888668], 'magnitude': 0.11979727447032928, 'cosine_with_motion': -0.7231886386871338, 'motion_component': -0.0866360291838646, 'motion_component_percent': 72.31886386871338}, {'resid': 1313, 'atom': 'C39', 'charge': -0.18000000715255737, 'distance': 21.227962493896484, 'force': [0.12034440785646439, 0.053550757467746735, -0.015374788083136082], 'magnitude': 0.13261540234088898, 'cosine_with_motion': -0.687437117099762, 'motion_component': -0.09116475284099579, 'motion_component_percent': 68.7437117099762}, {'resid': 1313, 'atom': 'C4', 'charge': 0.08000000566244125, 'distance': 28.285057067871094, 'force': [-0.021007701754570007, -0.014702563174068928, 0.021086225286126137], 'magnitude': 0.03319815918803215, 'cosine_with_motion': 0.6005814075469971, 'motion_component': 0.01993819698691368, 'motion_component_percent': 60.05814075469971}, {'resid': 1313, 'atom': 'C5', 'charge': 0.08000000566244125, 'distance': 26.80779266357422, 'force': [-0.02293197624385357, -0.016353460028767586, 0.02392837218940258], 'magnitude': 0.036957789212465286, 'cosine_with_motion': 0.5939100384712219, 'motion_component': 0.02194960229098797, 'motion_component_percent': 59.39100384712219}, {'resid': 1313, 'atom': 'C6', 'charge': 0.06000000238418579, 'distance': 25.934951782226562, 'force': [-0.018583258613944054, -0.014154835604131222, 0.01820380426943302], 'magnitude': 0.029615458101034164, 'cosine_with_motion': 0.576730489730835, 'motion_component': 0.017080137506127357, 'motion_component_percent': 57.673048973083496}, {'resid': 1313, 'atom': 'H1', 'charge': 0.12000000476837158, 'distance': 25.48573112487793, 'force': [-0.04227064922451973, -0.027507003396749496, 0.03491174057126045], 'magnitude': 0.061337366700172424, 'cosine_with_motion': 0.6266205906867981, 'motion_component': 0.038435257971286774, 'motion_component_percent': 62.66205906867981}, {'resid': 1313, 'atom': 'H10R', 'charge': 0.09000000357627869, 'distance': 22.724151611328125, 'force': [-0.04543622210621834, -0.03388259559869766, 0.011649568565189838], 'magnitude': 0.057863570749759674, 'cosine_with_motion': 0.5427849292755127, 'motion_component': 0.03140747547149658, 'motion_component_percent': 54.27849292755127}, {'resid': 1313, 'atom': 'H10S', 'charge': 0.09000000357627869, 'distance': 22.147640228271484, 'force': [-0.049937810748815536, -0.03220001235604286, 0.013417757116258144], 'magnitude': 0.060915201902389526, 'cosine_with_motion': 0.5995974540710449, 'motion_component': 0.03652460128068924, 'motion_component_percent': 59.95974540710449}, {'resid': 1313, 'atom': 'H10X', 'charge': 0.09000000357627869, 'distance': 20.647653579711914, 'force': [-0.06370026618242264, -0.02920316904783249, 0.001295369234867394], 'magnitude': 0.07008728384971619, 'cosine_with_motion': 0.652572751045227, 'motion_component': 0.04573705047369003, 'motion_component_percent': 65.2572751045227}, {'resid': 1313, 'atom': 'H10Y', 'charge': 0.09000000357627869, 'distance': 20.6290340423584, 'force': [-0.06588226556777954, -0.024105869233608246, 0.0029017641209065914], 'magnitude': 0.07021386176347733, 'cosine_with_motion': 0.7120363712310791, 'motion_component': 0.0499948225915432, 'motion_component_percent': 71.20363712310791}, {'resid': 1313, 'atom': 'H111', 'charge': 0.15000000596046448, 'distance': 24.27827262878418, 'force': [-0.06651221215724945, -0.045633282512426376, 0.02513784170150757], 'magnitude': 0.08448775857686996, 'cosine_with_motion': 0.5919167399406433, 'motion_component': 0.05000972002744675, 'motion_component_percent': 59.19167399406433}, {'resid': 1313, 'atom': 'H11A', 'charge': 0.09000000357627869, 'distance': 26.35346221923828, 'force': [-0.03189311921596527, -0.020093660801649094, 0.020738638937473297], 'magnitude': 0.043023452162742615, 'cosine_with_motion': 0.6374778747558594, 'motion_component': 0.027426499873399734, 'motion_component_percent': 63.74778747558594}, {'resid': 1313, 'atom': 'H11B', 'charge': 0.09000000357627869, 'distance': 24.788331985473633, 'force': [-0.03628024086356163, -0.02151978760957718, 0.024193402379751205], 'magnitude': 0.048627953976392746, 'cosine_with_motion': 0.655454695224762, 'motion_component': 0.031873419880867004, 'motion_component_percent': 65.5454695224762}, {'resid': 1313, 'atom': 'H11X', 'charge': 0.09000000357627869, 'distance': 18.5936279296875, 'force': [-0.07718507945537567, -0.03818611428141594, 0.007349222432821989], 'magnitude': 0.08642758429050446, 'cosine_with_motion': 0.6512013673782349, 'motion_component': 0.05628176033496857, 'motion_component_percent': 65.12013673782349}, {'resid': 1313, 'atom': 'H11Y', 'charge': 0.09000000357627869, 'distance': 18.29551887512207, 'force': [-0.0826907679438591, -0.03351127356290817, 0.002799592213705182], 'magnitude': 0.0892670527100563, 'cosine_with_motion': 0.686821460723877, 'motion_component': 0.061310529708862305, 'motion_component_percent': 68.6821460723877}, {'resid': 1313, 'atom': 'H12', 'charge': 0.09000000357627869, 'distance': 25.783161163330078, 'force': [-0.035789959132671356, -0.01902729645371437, 0.019425347447395325], 'magnitude': 0.0449477843940258, 'cosine_with_motion': 0.6851868629455566, 'motion_component': 0.030797630548477173, 'motion_component_percent': 68.51868629455566}, {'resid': 1313, 'atom': 'H121', 'charge': 0.15000000596046448, 'distance': 26.05333709716797, 'force': [-0.05992741510272026, -0.03853536397218704, 0.017506983131170273], 'magnitude': 0.07336732000112534, 'cosine_with_motion': 0.6041231751441956, 'motion_component': 0.044322896748781204, 'motion_component_percent': 60.412317514419556}, {'resid': 1313, 'atom': 'H12X', 'charge': 0.09000000357627869, 'distance': 18.650907516479492, 'force': [-0.08150777220726013, -0.025036131963133812, 0.010395251214504242], 'magnitude': 0.0858975350856781, 'cosine_with_motion': 0.7656452059745789, 'motion_component': 0.06576703488826752, 'motion_component_percent': 76.56452059745789}, {'resid': 1313, 'atom': 'H12Y', 'charge': 0.09000000357627869, 'distance': 19.25406265258789, 'force': [-0.074168361723423, -0.027785474434494972, 0.01494674477726221], 'magnitude': 0.08060014247894287, 'cosine_with_motion': 0.7422231435775757, 'motion_component': 0.05982329323887825, 'motion_component_percent': 74.22231435775757}, {'resid': 1313, 'atom': 'H13A', 'charge': 0.09000000357627869, 'distance': 27.0484619140625, 'force': [-0.03160765394568443, -0.01991266757249832, 0.016505219042301178], 'magnitude': 0.04084091633558273, 'cosine_with_motion': 0.6335293054580688, 'motion_component': 0.02587391622364521, 'motion_component_percent': 63.352930545806885}, {'resid': 1313, 'atom': 'H13B', 'charge': 0.09000000357627869, 'distance': 25.7582950592041, 'force': [-0.034413985908031464, -0.023541105911135674, 0.017017913982272148], 'magnitude': 0.04503460228443146, 'cosine_with_motion': 0.6038974523544312, 'motion_component': 0.027196280658245087, 'motion_component_percent': 60.389745235443115}, {'resid': 1313, 'atom': 'H13R', 'charge': 0.09000000357627869, 'distance': 24.3172664642334, 'force': [-0.04266186058521271, -0.02599903754889965, 0.00757082924246788], 'magnitude': 0.05053020641207695, 'cosine_with_motion': 0.60334312915802, 'motion_component': 0.030487053096294403, 'motion_component_percent': 60.334312915802}, {'resid': 1313, 'atom': 'H13S', 'charge': 0.09000000357627869, 'distance': 24.68607521057129, 'force': [-0.03955570608377457, -0.02809516340494156, 0.0070788925513625145], 'magnitude': 0.04903165251016617, 'cosine_with_motion': 0.5477287769317627, 'motion_component': 0.02685604616999626, 'motion_component_percent': 54.77287769317627}, {'resid': 1313, 'atom': 'H13X', 'charge': 0.09000000357627869, 'distance': 17.23996925354004, 'force': [-0.0900525450706482, -0.03867454081773758, 0.0223977193236351], 'magnitude': 0.10053277015686035, 'cosine_with_motion': 0.718544065952301, 'motion_component': 0.07223722338676453, 'motion_component_percent': 71.8544065952301}, {'resid': 1313, 'atom': 'H13Y', 'charge': 0.09000000357627869, 'distance': 16.386131286621094, 'force': [-0.10291828960180283, -0.039466772228479385, 0.01529845129698515], 'magnitude': 0.11128272116184235, 'cosine_with_motion': 0.7272300720214844, 'motion_component': 0.08092813938856125, 'motion_component_percent': 72.72300720214844}, {'resid': 1313, 'atom': 'H141', 'charge': 0.15000000596046448, 'distance': 27.32771110534668, 'force': [-0.054666917771101, -0.036866992712020874, 0.009956613183021545], 'magnitude': 0.06668419390916824, 'cosine_with_motion': 0.5679751038551331, 'motion_component': 0.037874963134527206, 'motion_component_percent': 56.797510385513306}, {'resid': 1313, 'atom': 'H14X', 'charge': 0.09000000357627869, 'distance': 17.43242073059082, 'force': [-0.09122764319181442, -0.02491467073559761, 0.026919083669781685], 'magnitude': 0.09832527488470078, 'cosine_with_motion': 0.8101782202720642, 'motion_component': 0.07966099679470062, 'motion_component_percent': 81.01782202720642}, {'resid': 1313, 'atom': 'H14Y', 'charge': 0.09000000357627869, 'distance': 16.954147338867188, 'force': [-0.09950988739728928, -0.023063721135258675, 0.0192783884704113], 'magnitude': 0.10395099222660065, 'cosine_with_motion': 0.8187558054924011, 'motion_component': 0.08511047810316086, 'motion_component_percent': 81.87558054924011}, {'resid': 1313, 'atom': 'H151', 'charge': 0.15000000596046448, 'distance': 27.998083114624023, 'force': [-0.05472566559910774, -0.03158661350607872, 0.006582955364137888], 'magnitude': 0.0635291114449501, 'cosine_with_motion': 0.6096439957618713, 'motion_component': 0.03873014077544212, 'motion_component_percent': 60.964399576187134}, {'resid': 1313, 'atom': 'H15X', 'charge': 0.09000000357627869, 'distance': 14.59005355834961, 'force': [-0.1320786327123642, -0.03777007386088371, 0.028839489445090294], 'magnitude': 0.14036759734153748, 'cosine_with_motion': 0.7939866185188293, 'motion_component': 0.11144999414682388, 'motion_component_percent': 79.39866185188293}, {'resid': 1313, 'atom': 'H15Y', 'charge': 0.09000000357627869, 'distance': 15.218921661376953, 'force': [-0.12055674940347672, -0.026241250336170197, 0.03768610209226608], 'magnitude': 0.12900687754154205, 'cosine_with_motion': 0.8398815393447876, 'motion_component': 0.1083504930138588, 'motion_component_percent': 83.98815393447876}, {'resid': 1313, 'atom': 'H16R', 'charge': 0.09000000357627869, 'distance': 26.308937072753906, 'force': [-0.03858834132552147, -0.01881631650030613, 0.004523936193436384], 'magnitude': 0.04316920042037964, 'cosine_with_motion': 0.6604427099227905, 'motion_component': 0.02851078473031521, 'motion_component_percent': 66.04427099227905}, {'resid': 1313, 'atom': 'H16S', 'charge': 0.09000000357627869, 'distance': 25.115123748779297, 'force': [-0.04132220521569252, -0.022792475298047066, 0.0041186134330928326], 'magnitude': 0.04737071320414543, 'cosine_with_motion': 0.6195484399795532, 'motion_component': 0.029348451644182205, 'motion_component_percent': 61.95484399795532}, {'resid': 1313, 'atom': 'H16X', 'charge': 0.09000000357627869, 'distance': 15.388519287109375, 'force': [-0.10967576503753662, -0.04872152954339981, 0.038968831300735474], 'magnitude': 0.12617896497249603, 'cosine_with_motion': 0.7225754261016846, 'motion_component': 0.09117382019758224, 'motion_component_percent': 72.25754261016846}, {'resid': 1313, 'atom': 'H16Y', 'charge': 0.09000000357627869, 'distance': 14.047861099243164, 'force': [-0.13302777707576752, -0.0489371232688427, 0.053238626569509506], 'magnitude': 0.1514119654893875, 'cosine_with_motion': 0.7671669125556946, 'motion_component': 0.11615825444459915, 'motion_component_percent': 76.71669125556946}, {'resid': 1313, 'atom': 'H17R', 'charge': 0.09000000357627869, 'distance': 26.96343231201172, 'force': [-0.03563243895769119, -0.020467299968004227, 0.000734166766051203], 'magnitude': 0.041098907589912415, 'cosine_with_motion': 0.5865299105644226, 'motion_component': 0.0241057388484478, 'motion_component_percent': 58.65299105644226}, {'resid': 1313, 'atom': 'H17S', 'charge': 0.09000000357627869, 'distance': 27.551626205444336, 'force': [-0.03527197986841202, -0.01743670366704464, 0.00113133923150599], 'magnitude': 0.03936281427741051, 'cosine_with_motion': 0.6352458596229553, 'motion_component': 0.02500506490468979, 'motion_component_percent': 63.52458596229553}, {'resid': 1313, 'atom': 'H17X', 'charge': 0.09000000357627869, 'distance': 16.933395385742188, 'force': [-0.09070684015750885, -0.030355094000697136, 0.04134872555732727], 'magnitude': 0.10420595109462738, 'cosine_with_motion': 0.7860877513885498, 'motion_component': 0.08191502094268799, 'motion_component_percent': 78.60877513885498}, {'resid': 1313, 'atom': 'H17Y', 'charge': 0.09000000357627869, 'distance': 15.635092735290527, 'force': [-0.10739358514547348, -0.027498789131641388, 0.051485300064086914], 'magnitude': 0.12223052978515625, 'cosine_with_motion': 0.8249024152755737, 'motion_component': 0.10082826018333435, 'motion_component_percent': 82.49024152755737}, {'resid': 1313, 'atom': 'H18R', 'charge': 0.09000000357627869, 'distance': 24.75850486755371, 'force': [-0.043174538761377335, -0.022623401135206223, -0.0004843505739700049], 'magnitude': 0.04874519258737564, 'cosine_with_motion': 0.6061022877693176, 'motion_component': 0.029544571414589882, 'motion_component_percent': 60.61022877693176}, {'resid': 1313, 'atom': 'H18S', 'charge': 0.09000000357627869, 'distance': 26.18132781982422, 'force': [-0.03904598578810692, -0.019282778725028038, -0.0019403358455747366], 'magnitude': 0.04359104856848717, 'cosine_with_motion': 0.611507773399353, 'motion_component': 0.026656264439225197, 'motion_component_percent': 61.1507773399353}, {'resid': 1313, 'atom': 'H18X', 'charge': 0.09000000357627869, 'distance': 16.533538818359375, 'force': [-0.08705775439739227, -0.034690871834754944, 0.056263361126184464], 'magnitude': 0.10930725187063217, 'cosine_with_motion': 0.7500139474868774, 'motion_component': 0.08198196440935135, 'motion_component_percent': 75.00139474868774}, {'resid': 1313, 'atom': 'H18Y', 'charge': 0.09000000357627869, 'distance': 15.99013614654541, 'force': [-0.09365008771419525, -0.046880099922418594, 0.05185393616557121], 'magnitude': 0.11686280369758606, 'cosine_with_motion': 0.7013394236564636, 'motion_component': 0.08196049183607101, 'motion_component_percent': 70.13394236564636}, {'resid': 1313, 'atom': 'H18Z', 'charge': 0.09000000357627869, 'distance': 14.814123153686523, 'force': [-0.10831943154335022, -0.046922095119953156, 0.06784531474113464], 'magnitude': 0.1361534744501114, 'cosine_with_motion': 0.7341623306274414, 'motion_component': 0.09995875507593155, 'motion_component_percent': 73.41623306274414}, {'resid': 1313, 'atom': 'H19R', 'charge': 0.09000000357627869, 'distance': 26.42913818359375, 'force': [-0.03965533524751663, -0.016041897237300873, 0.00014089880278334022], 'magnitude': 0.042777422815561295, 'cosine_with_motion': 0.6784971952438354, 'motion_component': 0.029024362564086914, 'motion_component_percent': 67.84971952438354}, {'resid': 1313, 'atom': 'H19S', 'charge': 0.09000000357627869, 'distance': 24.983367919921875, 'force': [-0.044214192777872086, -0.018234508112072945, 0.0020749480463564396], 'magnitude': 0.</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
sf residues added in forces
</commit_message>
<xml_diff>
--- a/results_G2/forces/force_results.xlsx
+++ b/results_G2/forces/force_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,225 +457,49 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>40</v>
+        <v>900</v>
       </c>
       <c r="B2" t="n">
-        <v>594</v>
+        <v>969</v>
       </c>
       <c r="C2" t="n">
-        <v>2400</v>
+        <v>2397</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>{40: {'frame': 40, 'motion_vector': [-0.6262931823730469, -0.466278076171875, 2.1045074462890625], 'ionic_force': [4.294367149472237, 6.8834086656570435, -19.503039240837097], 'ionic_force_magnitude': 21.12324415667585, 'radial_force': 8.11313158237365, 'axial_force': -19.503039240837097, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [6.283811151981354, 0.6723480224609375, -4.648064412176609], 'asn_force_magnitude': 7.844924297710912, 'residue_force': [6.283811151981354, 0.6723480224609375, -4.648064412176609], 'residue_force_magnitude': 7.844924297710912, 'pip2_force': [0.29895313642919064, 0.04803574737161398, -4.903264417589526], 'pip2_force_magnitude': 4.912604437526591, 'total_force': [10.877131437882781, 7.603792435489595, -29.054368070603232], 'total_force_magnitude': 31.94191527916063, 'cosine_total_motion': -0.9972573457303928, 'cosine_glu_motion': 0, 'cosine_asn_motion': -0.7967851539993244, 'cosine_residue_motion': -0.7967851539993244, 'cosine_pip2_motion': -0.9547790824875996, 'cosine_ionic_motion': -0.9900533422599569, 'motion_component_total': -31.854309648840808, 'motion_component_glu': 0, 'motion_component_asn': -6.25071921466463, 'motion_component_residue': -6.25071921466463, 'motion_component_ionic': -20.91313847669003, 'motion_component_pip2': -4.6904519574861485, 'motion_component_percent_total': 99.72573457303928, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 79.67851539993244, 'motion_component_percent_residue': 79.67851539993244, 'motion_component_percent_ionic': 99.00533422599568, 'motion_component_percent_pip2': 95.47790824875996, 'ionic_contributions': [{'ion_id': 2397, 'distance': 13.46534252166748, 'force': [0.06721048057079315, 0.29271984100341797, -1.80626380443573], 'magnitude': 1.8310627937316895, 'cosine_ionic_motion': -0.9683026671409607, 'motion_component_ionic': -1.773023009300232, 'motion_component_percent_ionic': 96.83026671409607}, {'ion_id': 2398, 'distance': 8.60761833190918, 'force': [0.4785769283771515, 1.1410447359085083, -4.3067474365234375], 'magnitude': 4.4809699058532715, 'cosine_ionic_motion': -0.9837936162948608, 'motion_component_ionic': -4.408349514007568, 'motion_component_percent_ionic': 98.37936162948608}, {'ion_id': 2399, 'distance': 4.7148919105529785, 'force': [3.748579740524292, 5.449644088745117, -13.39002799987793], 'magnitude': 14.934635162353516, 'cosine_ionic_motion': -0.986416220664978, 'motion_component_ionic': -14.731766700744629, 'motion_component_percent_ionic': 98.6416220664978}], 'glu_contributions': [], 'asn_contributions': [{'resid': 458, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 5.640399932861328, 'force': [5.409074306488037, -2.948438882827759, -1.1765199899673462], 'magnitude': 6.27180814743042, 'cosine_with_motion': -0.3188517093658447, 'motion_component': -1.999776840209961, 'motion_component_percent': 31.885170936584473}, {'resid': 786, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 4.637459754943848, 'force': [-1.6578381061553955, -10.71817684173584, 2.0756356716156006], 'magnitude': 11.042464256286621, 'cosine_with_motion': 0.419744074344635, 'motion_component': 4.635008811950684, 'motion_component_percent': 41.9744074344635}, {'resid': 786, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 3.8657217025756836, 'force': [2.6595325469970703, 12.010087013244629, -5.192760944366455], 'magnitude': 13.352155685424805, 'cosine_with_motion': -0.607042133808136, 'motion_component': -8.105320930480957, 'motion_component_percent': 60.7042133808136}, {'resid': 786, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 5.110611915588379, 'force': [3.557929515838623, 10.984701156616211, 0.10406573861837387], 'magnitude': 11.547005653381348, 'cosine_with_motion': -0.27513089776039124, 'motion_component': -3.176938056945801, 'motion_component_percent': 27.513089776039124}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 4.9544477462768555, 'force': [-2.7461273670196533, -4.893613338470459, -0.13110485672950745], 'magnitude': 5.613007545471191, 'cosine_with_motion': 0.2957080602645874, 'motion_component': 1.6598116159439087, 'motion_component_percent': 29.57080602645874}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 5.950348377227783, 'force': [-0.9387597441673279, -3.7622110843658447, -0.3273800313472748], 'magnitude': 3.891359567642212, 'cosine_with_motion': 0.1892644613981247, 'motion_component': 0.736496090888977, 'motion_component_percent': 18.92644613981247}], 'pip2_contributions': [{'resid': 1313, 'atom': 'C1', 'charge': 0.06000000238418579, 'distance': 25.349180221557617, 'force': [-0.020627744495868683, -0.0156398955732584, 0.017055468633770943], 'magnitude': 0.030999986454844475, 'cosine_with_motion': 0.8062765002250671, 'motion_component': 0.024994561448693275, 'motion_component_percent': 80.62765002250671}, {'resid': 1313, 'atom': 'C11', 'charge': 0.17000000178813934, 'distance': 24.34927749633789, 'force': [-0.07222510129213333, -0.04561211168766022, 0.04201413691043854], 'magnitude': 0.09519515931606293, 'cosine_with_motion': 0.725003719329834, 'motion_component': 0.06901684403419495, 'motion_component_percent': 72.5003719329834}, {'resid': 1313, 'atom': 'C12', 'charge': 0.04000000283122063, 'distance': 24.347152709960938, 'force': [-0.01758533902466297, -0.010859603993594646, 0.008643434382975101], 'magnitude': 0.022402768954634666, 'cosine_with_motion': 0.6814333200454712, 'motion_component': 0.015265993773937225, 'motion_component_percent': 68.14333200454712}, {'resid': 1313, 'atom': 'C13', 'charge': -0.05000000074505806, 'distance': 25.171117782592773, 'force': [0.02016681246459484, 0.01389272976666689, -0.009313290007412434], 'magnitude': 0.026200108230113983, 'cosine_with_motion': -0.6581780314445496, 'motion_component': -0.017244335263967514, 'motion_component_percent': 65.81780314445496}, {'resid': 1313, 'atom': 'C2', 'charge': 0.06000000238418579, 'distance': 26.881093978881836, 'force': [-0.01861545629799366, -0.01388173084706068, 0.014856741763651371], 'magnitude': 0.02756737917661667, 'cosine_with_motion': 0.7982795834541321, 'motion_component': 0.022006476297974586, 'motion_component_percent': 79.82795834541321}, {'resid': 1313, 'atom': 'C21', 'charge': 0.6299999952316284, 'distance': 22.404850006103516, 'force': [-0.3425382673740387, -0.1840963214635849, 0.14963898062705994], 'magnitude': 0.4166722297668457, 'cosine_with_motion': 0.6578500866889954, 'motion_component': 0.2741078734397888, 'motion_component_percent': 65.78500866889954}, {'resid': 1313, 'atom': 'C210', 'charge': -0.18000000715255737, 'distance': 21.142786026000977, 'force': [0.12590451538562775, 0.03742505609989166, -0.02488745003938675], 'magnitude': 0.13368608057498932, 'cosine_with_motion': -0.4954608678817749, 'motion_component': -0.0662362203001976, 'motion_component_percent': 49.54608678817749}, {'resid': 1313, 'atom': 'C211', 'charge': -0.15000000596046448, 'distance': 20.2697696685791, 'force': [0.11419277638196945, 0.02941647358238697, -0.02803732454776764], 'magnitude': 0.12120813131332397, 'cosine_with_motion': -0.5301467180252075, 'motion_component': -0.06425809115171432, 'motion_component_percent': 53.01467180252075}, {'resid': 1313, 'atom': 'C212', 'charge': -0.15000000596046448, 'distance': 20.750505447387695, 'force': [0.10746101289987564, 0.026330266147851944, -0.03369562327861786], 'magnitude': 0.1156570240855217, 'cosine_with_motion': -0.5796769857406616, 'motion_component': -0.0670437142252922, 'motion_component_percent': 57.96769857406616}, {'resid': 1313, 'atom': 'C213', 'charge': -0.18000000715255737, 'distance': 22.098243713378906, 'force': [0.11226483434438705, 0.030228592455387115, -0.038192205131053925], 'magnitude': 0.12237567454576492, 'cosine_with_motion': -0.5998708009719849, 'motion_component': -0.07340959459543228, 'motion_component_percent': 59.987080097198486}, {'resid': 1313, 'atom': 'C214', 'charge': -0.15000000596046448, 'distance': 22.210580825805664, 'force': [0.09004440158605576, 0.025229092687368393, -0.03803357481956482], 'magnitude': 0.10095075517892838, 'cosine_with_motion': -0.6540079116821289, 'motion_component': -0.066022589802742, 'motion_component_percent': 65.40079116821289}, {'resid': 1313, 'atom': 'C215', 'charge': -0.15000000596046448, 'distance': 22.781755447387695, 'force': [0.08511880040168762, 0.019903916865587234, -0.03956577181816101], 'magnitude': 0.09595220535993576, 'cosine_with_motion': -0.6771978735923767, 'motion_component': -0.06497862935066223, 'motion_component_percent': 67.71978735923767}, {'resid': 1313, 'atom': 'C216', 'charge': -0.18000000715255737, 'distance': 23.29244613647461, 'force': [0.09981908649206161, 0.016467120498418808, -0.04356349632143974], 'magnitude': 0.11014896631240845, 'cosine_with_motion': -0.6546983122825623, 'motion_component': -0.07211434096097946, 'motion_component_percent': 65.46983122825623}, {'resid': 1313, 'atom': 'C217', 'charge': -0.18000000715255737, 'distance': 22.172033309936523, 'force': [0.11149152368307114, 0.01288951002061367, -0.04670049250125885], 'magnitude': 0.12156247347593307, 'cosine_with_motion': -0.6381000876426697, 'motion_component': -0.07756902277469635, 'motion_component_percent': 63.81000876426697}, {'resid': 1313, 'atom': 'C218', 'charge': -0.18000000715255737, 'distance': 22.748245239257812, 'force': [0.10693046450614929, 0.0049774558283388615, -0.043326955288648605], 'magnitude': 0.1154821366071701, 'cosine_with_motion': -0.6190570592880249, 'motion_component': -0.07149003446102142, 'motion_component_percent': 61.90570592880249}, {'resid': 1313, 'atom': 'C219', 'charge': -0.18000000715255737, 'distance': 23.540712356567383, 'force': [0.0975128561258316, 0.002204304561018944, -0.04599342495203018], 'magnitude': 0.10783789306879044, 'cosine_with_motion': -0.6564140319824219, 'motion_component': -0.07078630477190018, 'motion_component_percent': 65.64140319824219}, {'resid': 1313, 'atom': 'C22', 'charge': -0.08000000566244125, 'distance': 21.06283950805664, 'force': [0.049801550805568695, 0.026753244921565056, -0.019703786820173264], 'magnitude': 0.05986793711781502, 'cosine_with_motion': -0.6334918737411499, 'motion_component': -0.037925850600004196, 'motion_component_percent': 63.34918737411499}, {'resid': 1313, 'atom': 'C220', 'charge': -0.27000001072883606, 'distance': 24.30508041381836, 'force': [0.1383161097764969, -0.0049453191459178925, -0.06220962479710579], 'magnitude': 0.15174266695976257, 'cosine_with_motion': -0.6319201588630676, 'motion_component': -0.09588924795389175, 'motion_component_percent': 63.19201588630676}, {'resid': 1313, 'atom': 'C23', 'charge': -0.18000000715255737, 'distance': 21.25710678100586, 'force': [0.11199240386486053, 0.06150957942008972, -0.03413015231490135], 'magnitude': 0.13225200772285461, 'cosine_with_motion': -0.5748348236083984, 'motion_component': -0.07602305710315704, 'motion_component_percent': 57.483482360839844}, {'resid': 1313, 'atom': 'C24', 'charge': -0.18000000715255737, 'distance': 19.950979232788086, 'force': [0.12821213901042938, 0.07111737877130508, -0.032318875193595886], 'magnitude': 0.1501350849866867, 'cosine_with_motion': -0.5384895205497742, 'motion_component': -0.08084616810083389, 'motion_component_percent': 53.84895205497742}, {'resid': 1313, 'atom': 'C25', 'charge': -0.15000000596046448, 'distance': 19.0755558013916, 'force': [0.1207282692193985, 0.05693156644701958, -0.030232541263103485], 'magnitude': 0.13685950636863708, 'cosine_with_motion': -0.5396430492401123, 'motion_component': -0.07385528087615967, 'motion_component_percent': 53.96430492401123}, {'resid': 1313, 'atom': 'C26', 'charge': -0.15000000596046448, 'distance': 18.948261260986328, 'force': [0.12637273967266083, 0.051721472293138504, -0.024367304518818855], 'magnitude': 0.13870453834533691, 'cosine_with_motion': -0.4963710904121399, 'motion_component': -0.06884892284870148, 'motion_component_percent': 49.63710904121399}, {'resid': 1313, 'atom': 'C27', 'charge': -0.18000000715255737, 'distance': 19.67885398864746, 'force': [0.14194664359092712, 0.05835917592048645, -0.016086911782622337], 'magnitude': 0.1543160080909729, 'cosine_with_motion': -0.43294116854667664, 'motion_component': -0.0668097510933876, 'motion_component_percent': 43.294116854667664}, {'resid': 1313, 'atom': 'C28', 'charge': -0.15000000596046448, 'distance': 20.180278778076172, 'force': [0.11567511409521103, 0.038537513464689255, -0.009374360553920269], 'magnitude': 0.12228552997112274, 'cosine_with_motion': -0.4012646973133087, 'motion_component': -0.049068864434957504, 'motion_component_percent': 40.12646973133087}, {'resid': 1313, 'atom': 'C29', 'charge': -0.15000000596046448, 'distance': 20.729042053222656, 'force': [0.11071113497018814, 0.031530555337667465, -0.013450040481984615], 'magnitude': 0.11589665710926056, 'cosine_with_motion': -0.43184584379196167, 'motion_component': -0.050049491226673126, 'motion_component_percent': 43.18458437919617}, {'resid': 1313, 'atom': 'C3', 'charge': 0.06000000238418579, 'distance': 27.700225830078125, 'force': [-0.017383543774485588, -0.012228383682668209, 0.014908275566995144], 'magnitude': 0.025961080566048622, 'cosine_with_motion': 0.8230640292167664, 'motion_component': 0.0213676318526268, 'motion_component_percent': 82.30640292167664}, {'resid': 1313, 'atom': 'C31', 'charge': 0.6299999952316284, 'distance': 26.12384796142578, 'force': [-0.25041794776916504, -0.15232573449611664, 0.08954697102308273], 'magnitude': 0.3064815402030945, 'cosine_with_motion': 0.6051467657089233, 'motion_component': 0.18546631932258606, 'motion_component_percent': 60.514676570892334}, {'resid': 1313, 'atom': 'C310', 'charge': -0.18000000715255737, 'distance': 23.217395782470703, 'force': [0.09322124719619751, 0.05912939831614494, 0.010195469483733177], 'magnitude': 0.11086223274469376, 'cosine_with_motion': -0.25918394327163696, 'motion_component': -0.028733711689710617, 'motion_component_percent': 25.918394327163696}, {'resid': 1313, 'atom': 'C311', 'charge': -0.18000000715255737, 'distance': 23.134078979492188, 'force': [0.09680936485528946, 0.05377911403775215, 0.014289873652160168], 'magnitude': 0.11166219413280487, 'cosine_with_motion': -0.22196172177791595, 'motion_component': -0.02478473260998726, 'motion_component_percent': 22.196172177791595}, {'resid': 1313, 'atom': 'C312', 'charge': -0.18000000715255737, 'distance': 21.86395835876465, 'force': [0.10944651067256927, 0.05725201591849327, 0.019281180575489998], 'magnitude': 0.1250123828649521, 'cosine_with_motion': -0.1948002725839615, 'motion_component': -0.02435244619846344, 'motion_component_percent': 19.48002725839615}, {'resid': 1313, 'atom': 'C313', 'charge': -0.18000000715255737, 'distance': 21.24875831604004, 'force': [0.11155480891466141, 0.06606439501047134, 0.02662927843630314], 'magnitude': 0.1323559582233429, 'cosine_with_motion': -0.15021631121635437, 'motion_component': -0.019882023334503174, 'motion_component_percent': 15.021631121635437}, {'resid': 1313, 'atom': 'C314', 'charge': -0.18000000715255737, 'distance': 22.05158805847168, 'force': [0.10137556493282318, 0.061754632741212845, 0.03181678056716919], 'magnitude': 0.1228940486907959, 'cosine_with_motion': -0.09181159734725952, 'motion_component': -0.011283098720014095, 'motion_component_percent': 9.181159734725952}, {'resid': 1313, 'atom': 'C315', 'charge': -0.18000000715255737, 'distance': 21.630014419555664, 'force': [0.10036128759384155, 0.06950584799051285, 0.03757404908537865], 'magnitude': 0.12773120403289795, 'cosine_with_motion': -0.05646619200706482, 'motion_component': -0.007212494499981403, 'motion_component_percent': 5.646619200706482}, {'resid': 1313, 'atom': 'C316', 'charge': -0.18000000715255737, 'distance': 22.44887351989746, 'force': [0.09118342399597168, 0.06374425441026688, 0.04103805869817734], 'magnitude': 0.11858275532722473, 'cosine_with_motion': -0.001747677568346262, 'motion_component': -0.0002072444185614586, 'motion_component_percent': 0.1747677568346262}, {'resid': 1313, 'atom': 'C317', 'charge': -0.18000000715255737, 'distance': 22.324893951416016, 'force': [0.08673073351383209, 0.06947783380746841, 0.045027270913124084], 'magnitude': 0.11990348249673843, 'cosine_with_motion': 0.029892288148403168, 'motion_component': 0.0035841893404722214, 'motion_component_percent': 2.9892288148403168}, {'resid': 1313, 'atom': 'C318', 'charge': -0.27000001072883606, 'distance': 23.282550811767578, 'force': [0.11679406464099884, 0.09367932379245758, 0.07020366191864014], 'magnitude': 0.16536390781402588, 'cosine_with_motion': 0.08328942954540253, 'motion_component': 0.013773065060377121, 'motion_component_percent': 8.328942954540253}, {'resid': 1313, 'atom': 'C32', 'charge': -0.08000000566244125, 'distance': 26.098739624023438, 'force': [0.0326407290995121, 0.019235214218497276, -0.009222800843417645], 'magnitude': 0.03899321332573891, 'cosine_with_motion': -0.5577799677848816, 'motion_component': -0.02174963429570198, 'motion_component_percent': 55.77799677848816}, {'resid': 1313, 'atom': 'C33', 'charge': -0.18000000715255737, 'distance': 25.111169815063477, 'force': [0.08159492909908295, 0.04302595555782318, -0.021740052849054337], 'magnitude': 0.09477128088474274, 'cosine_with_motion': -0.5495961904525757, 'motion_component': -0.052085936069488525, 'motion_component_percent': 54.95961904525757}, {'resid': 1313, 'atom': 'C34', 'charge': -0.18000000715255737, 'distance': 24.82367706298828, 'force': [0.08529355376958847, 0.0430118590593338, -0.01673157513141632], 'magnitude': 0.09697915613651276, 'cosine_with_motion': -0.4992749094963074, 'motion_component': -0.04841925948858261, 'motion_component_percent': 49.92749094963074}, {'resid': 1313, 'atom': 'C35', 'charge': -0.18000000715255737, 'distance': 24.317453384399414, 'force': [0.08770979940891266, 0.04850561171770096, -0.012926396913826466], 'magnitude': 0.10105887055397034, 'cosine_with_motion': -0.46178096532821655, 'motion_component': -0.04666706174612045, 'motion_component_percent': 46.178096532821655}, {'resid': 1313, 'atom': 'C36', 'charge': -0.18000000715255737, 'distance': 24.49185562133789, 'force': [0.08818203955888748, 0.04582614451646805, -0.006998721975833178], 'magnitude': 0.09962474554777145, 'cosine_with_motion': -0.40837976336479187, 'motion_component': -0.04068472981452942, 'motion_component_percent': 40.83797633647919}, {'resid': 1313, 'atom': 'C37', 'charge': -0.18000000715255737, 'distance': 24.194231033325195, 'force': [0.08856626600027084, 0.05073058605194092, -0.0022298996336758137], 'magnitude': 0.10209088027477264, 'cosine_with_motion': -0.3657495677471161, 'motion_component': -0.037339694797992706, 'motion_component_percent': 36.57495677471161}, {'resid': 1313, 'atom': 'C38', 'charge': -0.18000000715255737, 'distance': 22.673830032348633, 'force': [0.1008705347776413, 0.05776325985789299, -0.0007786313071846962], 'magnitude': 0.11624141037464142, 'cosine_with_motion': -0.35162127017974854, 'motion_component': -0.040872953832149506, 'motion_component_percent': 35.16212701797485}, {'resid': 1313, 'atom': 'C39', 'charge': -0.18000000715255737, 'distance': 22.330320358276367, 'force': [0.10087825357913971, 0.06454658508300781, 0.0044933767057955265], 'magnitude': 0.11984521150588989, 'cosine_with_motion': -0.31158021092414856, 'motion_component': -0.0373413972556591, 'motion_component_percent': 31.158021092414856}, {'resid': 1313, 'atom': 'C4', 'charge': 0.08000000566244125, 'distance': 27.52768325805664, 'force': [-0.022043120115995407, -0.016745202243328094, 0.021498970687389374], 'magnitude': 0.03505006060004234, 'cosine_with_motion': 0.8497868180274963, 'motion_component': 0.02978507988154888, 'motion_component_percent': 84.97868180274963}, {'resid': 1313, 'atom': 'C5', 'charge': 0.08000000566244125, 'distance': 26.10186767578125, 'force': [-0.024339696392416954, -0.01808541640639305, 0.02449977397918701], 'magnitude': 0.038983866572380066, 'cosine_with_motion': 0.8597826957702637, 'motion_component': 0.03351765498518944, 'motion_component_percent': 85.97826957702637}, {'resid': 1313, 'atom': 'C6', 'charge': 0.06000000238418579, 'distance': 25.121980667114258, 'force': [-0.01979544572532177, -0.01580285094678402, 0.01883210986852646], 'magnitude': 0.03156324103474617, 'cosine_with_motion': 0.8383766412734985, 'motion_component': 0.026461884379386902, 'motion_component_percent': 83.83766412734985}, {'resid': 1313, 'atom': 'H1', 'charge': 0.12000000476837158, 'distance': 24.925737380981445, 'force': [-0.04429272189736366, -0.03035803698003292, 0.03504972159862518], 'magnitude': 0.06412439793348312, 'cosine_with_motion': 0.8035199642181396, 'motion_component': 0.051525235176086426, 'motion_component_percent': 80.35199642181396}, {'resid': 1313, 'atom': 'H10R', 'charge': 0.09000000357627869, 'distance': 21.15948486328125, 'force': [-0.061650991439819336, -0.02179090678691864, 0.013349748216569424], 'magnitude': 0.0667375773191452, 'cosine_with_motion': 0.5131133198738098, 'motion_component': 0.03424394130706787, 'motion_component_percent': 51.31133198738098}, {'resid': 1313, 'atom': 'H10S', 'charge': 0.09000000357627869, 'distance': 22.17120933532715, 'force': [-0.0575135163962841, -0.01599489524960518, 0.011457180604338646], 'magnitude': 0.06078575551509857, 'cosine_with_motion': 0.4953657388687134, 'motion_component': 0.030111180618405342, 'motion_component_percent': 49.53657388687134}, {'resid': 1313, 'atom': 'H10X', 'charge': 0.09000000357627869, 'distance': 23.116687774658203, 'force': [-0.04572857916355133, -0.03146093711256981, -0.006753459107130766], 'magnitude': 0.055915139615535736, 'cosine_with_motion': 0.23182138800621033, 'motion_component': 0.012962325476109982, 'motion_component_percent': 23.182138800621033}, {'resid': 1313, 'atom': 'H10Y', 'charge': 0.09000000357627869, 'distance': 24.25352668762207, 'force': [-0.042655035853385925, -0.027300221845507622, -0.003936361987143755], 'magnitude': 0.050796154886484146, 'cosine_with_motion': 0.27328166365623474, 'motion_component': 0.01388165820389986, 'motion_component_percent': 27.328166365623474}, {'resid': 1313, 'atom': 'H111', 'charge': 0.15000000596046448, 'distance': 19.284683227539062, 'force': [-0.12717151641845703, -0.0302721094340086, 0.02902027778327465], 'magnitude': 0.13390733301639557, 'cosine_with_motion': 0.5151219964027405, 'motion_component': 0.06897861510515213, 'motion_component_percent': 51.51219964027405}, {'resid': 1313, 'atom': 'H11A', 'charge': 0.09000000357627869, 'distance': 25.378955841064453, 'force': [-0.03512468934059143, -0.021811148151755333, 0.021039217710494995], 'magnitude': 0.04639093577861786, 'cosine_with_motion': 0.7341148257255554, 'motion_component': 0.034056272357702255, 'motion_component_percent': 73.41148257255554}, {'resid': 1313, 'atom': 'H11B', 'charge': 0.09000000357627869, 'distance': 23.734375, 'force': [-0.04069747030735016, -0.023722104728221893, 0.024382326751947403], 'magnitude': 0.05304262414574623, 'cosine_with_motion': 0.7379429936408997, 'motion_component': 0.0391424335539341, 'motion_component_percent': 73.79429936408997}, {'resid': 1313, 'atom': 'H11X', 'charge': 0.09000000357627869, 'distance': 23.908754348754883, 'force': [-0.04494696110486984, -0.025340409949421883, -0.008364559151232243], 'magnitude': 0.052271708846092224, 'cosine_with_motion': 0.190588116645813, 'motion_component': 0.00996236689388752, 'motion_component_percent': 19.0588116645813}, {'resid': 1313, 'atom': 'H11Y', 'charge': 0.09000000357627869, 'distance': 23.601634979248047, 'force': [-0.04749711975455284, -0.024315273389220238, -0.0054901838302612305], 'magnitude': 0.0536409467458725, 'cosine_with_motion': 0.24525700509548187, 'motion_component': 0.013155817985534668, 'motion_component_percent': 24.525700509548187}, {'resid': 1313, 'atom': 'H12', 'charge': 0.09000000357627869, 'distance': 24.746625900268555, 'force': [-0.03945346549153328, -0.022035736590623856, 0.018398640677332878], 'magnitude': 0.04879200458526611, 'cosine_with_motion': 0.6729592084884644, 'motion_component': 0.03283502906560898, 'motion_component_percent': 67.29592084884644}, {'resid': 1313, 'atom': 'H121', 'charge': 0.15000000596046448, 'distance': 20.175580978393555, 'force': [-0.11293050646781921, -0.02465069480240345, 0.04008397087454796], 'magnitude': 0.12234247475862503, 'cosine_with_motion': 0.6065782308578491, 'motion_component': 0.0742102786898613, 'motion_component_percent': 60.65782308578491}, {'resid': 1313, 'atom': 'H12X', 'charge': 0.09000000357627869, 'distance': 22.191925048828125, 'force': [-0.05384589359164238, -0.025644056499004364, -0.011141532100737095], 'magnitude': 0.0606723316013813, 'cosine_with_motion': 0.16325056552886963, 'motion_component': 0.009904792532324791, 'motion_component_percent': 16.325056552886963}, {'resid': 1313, 'atom': 'H12Y', 'charge': 0.09000000357627869, 'distance': 21.249271392822266, 'force': [-0.058834951370954514, -0.029275210574269295, -0.0077789779752492905], 'magnitude': 0.06617478281259537, 'cosine_with_motion': 0.2297498732805252, 'motion_component': 0.015203648246824741, 'motion_component_percent': 22.97498732805252}, {'resid': 1313, 'atom': 'H13A', 'charge': 0.09000000357627869, 'distance': 26.141864776611328, 'force': [-0.033331144601106644, -0.023098286241292953, 0.016345731914043427], 'magnitude': 0.04372275248169899, 'cosine_with_motion': 0.6729411482810974, 'motion_component': 0.029422840103507042, 'motion_component_percent': 67.29411482810974}, {'resid': 1313, 'atom': 'H13B', 'charge': 0.09000000357627869, 'distance': 24.752765655517578, 'force': [-0.03632127121090889, -0.02740897238254547, 0.017544561997056007], 'magnitude': 0.04876779764890671, 'cosine_with_motion': 0.6618409752845764, 'motion_component': 0.03227652609348297, 'motion_component_percent': 66.18409752845764}, {'resid': 1313, 'atom': 'H13R', 'charge': 0.09000000357627869, 'distance': 22.833215713500977, 'force': [-0.05325871333479881, -0.01231347769498825, 0.017221104353666306], 'magnitude': 0.05731211602687836, 'cosine_with_motion': 0.585623025894165, 'motion_component': 0.033563293516635895, 'motion_component_percent': 58.562302589416504}, {'resid': 1313, 'atom': 'H13S', 'charge': 0.09000000357627869, 'distance': 22.395423889160156, 'force': [-0.05434586480259895, -0.017211759462952614, 0.01730405166745186], 'magnitude': 0.05957472324371338, 'cosine_with_motion': 0.5868577361106873, 'motion_component': 0.03496188670396805, 'motion_component_percent': 58.685773611068726}, {'resid': 1313, 'atom': 'H13X', 'charge': 0.09000000357627869, 'distance': 20.209503173828125, 'force': [-0.06198037415742874, -0.03563578799366951, -0.01551777869462967], 'magnitude': 0.07315926253795624, 'cosine_with_motion': 0.13869725167751312, 'motion_component': 0.010146988555788994, 'motion_component_percent': 13.869725167751312}, {'resid': 1313, 'atom': 'H13Y', 'charge': 0.09000000357627869, 'distance': 21.163082122802734, 'force': [-0.05486549437046051, -0.03605048358440399, -0.011875058524310589], 'magnitude': 0.06671489030122757, 'cosine_with_motion': 0.17482204735279083, 'motion_component': 0.011663233861327171, 'motion_component_percent': 17.482204735279083}, {'resid': 1313, 'atom': 'H141', 'charge': 0.15000000596046448, 'distance': 21.900493621826172, 'force': [-0.09062059968709946, -0.030129054561257362, 0.040752336382865906], 'magnitude': 0.10382969677448273, 'cosine_with_motion': 0.6717748045921326, 'motion_component': 0.06975017488002777, 'motion_component_percent': 67.17748045921326}, {'resid': 1313, 'atom': 'H14X', 'charge': 0.09000000357627869, 'distance': 22.02593994140625, 'force': [-0.05171218514442444, -0.028492063283920288, -0.017533019185066223], 'magnitude': 0.06159021705389023, 'cosine_with_motion': 0.06346331536769867, 'motion_component': 0.003908719401806593, 'motion_component_percent': 6.346331536769867}, {'resid': 1313, 'atom': 'H14Y', 'charge': 0.09000000357627869, 'distance': 23.098892211914062, 'force': [-0.0459865964949131, -0.02873150072991848, -0.013995789922773838], 'magnitude': 0.05600132420659065, 'cosine_with_motion': 0.10137766599655151, 'motion_component': 0.005677283741533756, 'motion_component_percent': 10.137766599655151}, {'resid': 1313, 'atom': 'H151', 'charge': 0.15000000596046448, 'distance': 23.073305130004883, 'force': [-0.08098272979259491, -0.02008398063480854, 0.04229256138205528], 'magnitude': 0.0935426652431488, 'cosine_with_motion': 0.7100346088409424, 'motion_component': 0.06641852855682373, 'motion_component_percent': 71.00346088409424}, {'resid': 1313, 'atom': 'H15X', 'charge': 0.09000000357627869, 'distance': 20.580276489257812, 'force': [-0.05503208190202713, -0.038420818746089935, -0.0217297300696373], 'magnitude': 0.0705469399690628, 'cosine_with_motion': 0.0419980026781559, 'motion_component': 0.002962830476462841, 'motion_component_percent': 4.19980026781559}, {'resid': 1313, 'atom': 'H15Y', 'charge': 0.09000000357627869, 'distance': 21.824447631835938, 'force': [-0.04826841503381729, -0.03645177558064461, -0.01663796231150627], 'magnitude': 0.06273271143436432, 'cosine_with_motion': 0.08672450482845306, 'motion_component': 0.005440463311970234, 'motion_component_percent': 8.672450482845306}, {'resid': 1313, 'atom': 'H16R', 'charge': 0.09000000357627869, 'distance': 24.058429718017578, 'force': [-0.04732220992445946, -0.008280077017843723, 0.018894901499152184], 'magnitude': 0.05162333324551582, 'cosine_with_motion': 0.6322406530380249, 'motion_component': 0.032638370990753174, 'motion_component_percent': 63.22406530380249}, {'resid': 1313, 'atom': 'H16S', 'charge': 0.09000000357627869, 'distance': 23.78134536743164, 'force': [-0.04719368740916252, -0.006890051998198032, 0.02272973582148552], 'magnitude': 0.052833303809165955, 'cosine_with_motion': 0.6796682476997375, 'motion_component': 0.03590911999344826, 'motion_component_percent': 67.96682476997375}, {'resid': 1313, 'atom': 'H16X', 'charge': 0.09000000357627869, 'distance': 23.5362548828125, 'force': [-0.04168243706226349, -0.028765959665179253, -0.018562056124210358], 'magnitude': 0.053939372301101685, 'cosine_with_motion': 0.0037527866661548615, 'motion_component': 0.00020242296159267426, 'motion_component_percent': 0.37527866661548615}, {'resid': 1313, 'atom': 'H16Y', 'charge': 0.09000000357627869, 'distance': 22.195491790771484, 'force': [-0.04731747880578041, -0.030385848134756088, -0.022727135568857193], 'magnitude': 0.06065283343195915, 'cosine_with_motion': -0.02957518957555294, 'motion_component': -0.0017938190139830112, 'motion_component_percent': 2.957518957555294}, {'resid': 1313, 'atom': 'H17R', 'charge': 0.09000000357627869, 'distance': 21.487606048583984, 'force': [-0.058353859931230545, -0.006627274677157402, 0.02718326449394226], 'magnitude': 0.0647149384021759, 'cosine_with_motion': 0.6666739583015442, 'motion_component': 0.04314376413822174, 'motion_component_percent': 66.66739583015442}, {'resid': 1313, 'atom': 'H17S', 'charge': 0.09000000357627869, 'distance': 21.681516647338867, 'force': [-0.05919909477233887, -0.007594441995024681, 0.021862970665097237], 'magnitude': 0.0635625496506691, 'cosine_with_motion': 0.6071571111679077, 'motion_component': 0.03859245404601097, 'motion_component_percent': 60.71571111679077}, {'resid': 1313, 'atom': 'H17X', 'charge': 0.09000000357627869, 'distance': 22.627771377563477, 'force': [-0.04144328087568283, -0.03578731045126915, -0.020182324573397636], 'magnitude': 0.05835754796862602, 'cosine_with_motion': 0.0012873171363025904, 'motion_component': 7.512466982007027e-05, 'motion_component_percent': 0.12873171363025904}, {'resid': 1313, 'atom': 'H17Y', 'charge': 0.09000000357627869, 'distance': 21.30177879333496, 'force': [-0.046932756900787354, -0.03840772435069084, -0.02565634995698929], 'magnitude': 0.0658489540219307, 'cosine_with_motion': -0.04527180641889572, 'motion_component': -0.0029811011627316475, 'motion_component_percent': 4.527180641889572}, {'resid': 1313, 'atom': 'H18R', 'charge': 0.09000000357627869, 'distance': 21.979440689086914, 'force': [-0.05765325948596001, -0.0007024265360087156, 0.02238672599196434], 'magnitude': 0.06185109168291092, 'cosine_with_motion': 0.601776659488678, 'motion_component': 0.0372205451130867, 'motion_component_percent': 60.1776659488678}, {'resid': 1313, 'atom': 'H18S', 'charge': 0.09000000357627869, 'distance': 23.484834671020508, 'force': [-0.0508478507399559, -0.002325806999579072, 0.01855013705790043], 'magnitude': 0.054175835102796555, 'cosine_with_motion': 0.5918132066726685, 'motion_component': 0.032061975449323654, 'motion_component_percent': 59.181320667266846}, {'resid': 1313, 'atom</t>
+          <t>{932: {'frame': 932, 'motion_vector': [-1.5848350524902344, -3.9648208618164062, -3.029510498046875], 'motion_vector_magnitude': 5.235402584075928, 'ionic_force': [-0.6365109831094742, 8.252115368843079, -3.386303260922432], 'ionic_force_magnitude': 8.94257256427081, 'radial_force': 8.276626987626972, 'axial_force': -3.386303260922432, 'glu_force': [7.704223445462621, 27.834427281033644, 11.325118289149916], 'glu_force_magnitude': 31.022068035899924, 'asn_force': [-0.6925757467836006, 0.1964403156845456, 0.5159840994618445], 'asn_force_magnitude': 0.885714148897124, 'sf_force': [0.17746470871481743, -0.8326530914041984, -0.7279579869851707], 'sf_force_magnitude': 1.1201462959273245, 'residue_force': [7.189112407393833, 27.19821450531399, 11.113144401626599], 'residue_force_magnitude': 30.247779885053067, 'pip2_force': [0.8071239286313593, -0.320149728655873, -4.342038780220539], 'pip2_force_magnitude': 4.428006961813273, 'total_force': [7.359725352915718, 35.1301801455012, 3.3848023604836275], 'total_force_magnitude': 36.05207346804415, 'cosine_total_motion': -0.8540692585971585, 'cosine_glu_motion': -0.965920148310478, 'cosine_asn_motion': -0.2683616116012464, 'cosine_sf_motion': 0.8910390514416046, 'cosine_residue_motion': -0.9655068323206991, 'cosine_pip2_motion': 0.5670004453303256, 'cosine_ionic_motion': -0.4581692131675099, 'motion_component_total': -30.79096765774276, 'motion_component_glu': -29.964840558134195, 'motion_component_asn': -0.2376916764160585, 'motion_component_sf': 0.9980940929989102, 'motion_component_residue': -29.204438141551346, 'motion_component_ionic': -4.097211435465319, 'motion_component_pip2': 2.510681919273908, 'motion_component_percent_total': np.float64(85.40692585971586), 'motion_component_percent_glu': np.float64(96.5920148310478), 'motion_component_percent_asn': np.float64(26.83616116012464), 'motion_component_percent_sf': np.float64(89.10390514416045), 'motion_component_percent_residue': np.float64(96.55068323206991), 'motion_component_percent_ionic': np.float64(45.81692131675099), 'motion_component_percent_pip2': np.float64(56.70004453303255), 'ionic_contributions': [{'ion_id': 2333, 'distance': 14.115193367004395, 'force': [-0.5459778308868408, 1.572485089302063, 0.07680048048496246], 'magnitude': 1.6663432121276855, 'cosine_ionic_motion': -0.6421388387680054, 'motion_component_ionic': -1.0700236558914185, 'motion_component_percent_ionic': 64.21388244628906}, {'ion_id': 2343, 'distance': 13.905966758728027, 'force': [-0.11061801016330719, 1.0146534442901611, -1.380529522895813], 'magnitude': 1.7168632745742798, 'cosine_ionic_motion': 0.037238940596580505, 'motion_component_ionic': 0.06393416970968246, 'motion_component_percent_ionic': 3.7238941192626953}, {'ion_id': 2372, 'distance': 11.306429862976074, 'force': [0.9758355617523193, 2.389859676361084, 0.28494706749916077], 'magnitude': 2.597090482711792, 'cosine_ionic_motion': -0.874113142490387, 'motion_component_ionic': -2.270150899887085, 'motion_component_percent_ionic': 87.41131591796875}, {'ion_id': 2381, 'distance': 8.941351890563965, 'force': [-0.9557507038116455, 3.2751171588897705, -2.367521286010742], 'magnitude': 4.152710914611816, 'cosine_ionic_motion': -0.19769522547721863, 'motion_component_ionic': -0.8209711313247681, 'motion_component_percent_ionic': 19.769521713256836}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 12.590643882751465, 'force': [-0.5854712981385105, -0.8527901613713734, 0.31491593773338206], 'magnitude': 1.081295402799023, 'cosine_with_motion': 0.5926487262973543, 'motion_component': 0.6408283432200256, 'motion_component_percent': 59.264872629735436}, {'resid': 98, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 12.965554237365723, 'force': [0.342371656503943, 0.4299297956870839, -0.18483057141019535], 'magnitude': 0.5798450832115514, 'cosine_with_motion': -0.5557988312793378, 'motion_component': -0.32227721957205063, 'motion_component_percent': 55.57988312793378}, {'resid': 98, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 11.88853645324707, 'force': [0.052649529481906876, 0.07506093625121706, -0.01704012749808002], 'magnitude': 0.09325493579819931, 'cosine_with_motion': -0.6747284346606955, 'motion_component': -0.06292175685550268, 'motion_component_percent': 67.47284346606955}, {'resid': 98, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 12.484599113464355, 'force': [0.12013967702504551, 0.1992203208854665, -0.03573180144848387], 'magnitude': 0.23537000633926228, 'cosine_with_motion': -0.7076646682301561, 'motion_component': -0.16656303744740378, 'motion_component_percent': 70.7664668230156}, {'resid': 98, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 12.415838241577148, 'force': [0.07878682101891384, 0.09000884546282266, -0.015401049610233572], 'magnitude': 0.12060741169975223, 'cosine_with_motion': -0.6890336889394917, 'motion_component': -0.08310256979692429, 'motion_component_percent': 68.90336889394916}, {'resid': 98, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 13.482990264892578, 'force': [-0.02058451780092914, -0.023528545930515725, 0.004571512362061461], 'magnitude': 0.03159451806845038, 'cosine_with_motion': 0.6774685457822437, 'motion_component': 0.021404292210523902, 'motion_component_percent': 67.74685457822437}, {'resid': 98, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 12.036210060119629, 'force': [-0.02775673420901588, -0.02747652788220378, 0.006815276586295851], 'magnitude': 0.039646486267501516, 'cosine_with_motion': 0.6373049314251062, 'motion_component': 0.02526690121195647, 'motion_component_percent': 63.730493142510625}, {'resid': 98, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 12.072093963623047, 'force': [0.020752175122121484, 0.023005103728810747, -8.280506588295213e-05], 'magnitude': 0.03098216303861749, 'cosine_with_motion': -0.7635382253195102, 'motion_component': -0.023656065783065724, 'motion_component_percent': 76.35382253195102}, {'resid': 98, 'resname': 'GLU', 'atom': 'HG2', 'charge': -0.042500000447034836, 'distance': 12.604401588439941, 'force': [-0.06428559206640366, -0.06126937220808316, -0.00118076056267318], 'magnitude': 0.08881423035531558, 'cosine_with_motion': 0.7492420620382658, 'motion_component': 0.06654335708975818, 'motion_component_percent': 74.92420620382659}, {'resid': 98, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 11.000815391540527, 'force': [-0.07836785169315627, -0.08631254825748585, -0.001688229082366012], 'magnitude': 0.11659428066220018, 'cosine_with_motion': 0.7724680602775119, 'motion_component': 0.09006535782258158, 'motion_component_percent': 77.24680602775119}, {'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 12.831777572631836, 'force': [0.983000105740883, 1.2884497682928056, 0.10422738890543091], 'magnitude': 1.623962857302597, 'cosine_with_motion': -0.8212234506736056, 'motion_component': -1.333636381439807, 'motion_component_percent': 82.12234506736056}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 14.030905723571777, 'force': [-0.8159837687866297, -1.1121974465089013, -0.06257971854319708], 'magnitude': 1.380843543677957, 'cosine_with_motion': 0.8150819625479988, 'motion_component': 1.1255006655527624, 'motion_component_percent': 81.50819625479988}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 12.313202857971191, 'force': [-0.9926112620735161, -1.4746372519460373, -0.23435403386295262], 'magnitude': 1.7929734955124064, 'cosine_with_motion': 0.8660732008619162, 'motion_component': 1.5528462943190082, 'motion_component_percent': 86.60732008619162}, {'resid': 98, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 10.381473541259766, 'force': [0.9059989703981168, 1.3448600733640257, -0.32078032954793956], 'magnitude': 1.65299206625925, 'cosine_with_motion': -0.6697628537114597, 'motion_component': -1.1071126834601976, 'motion_component_percent': 66.97628537114598}, {'resid': 98, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 9.912365913391113, 'force': [-0.9915450357370874, -1.6872894982616577, 0.1894933399617171], 'magnitude': 1.966218486010338, 'cosine_with_motion': 0.7467655365548984, 'motion_component': 1.46830420268967, 'motion_component_percent': 74.67655365548984}, {'resid': 426, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 13.699601173400879, 'force': [0.7631991813995468, -0.3121347543103282, 0.392756500424138], 'magnitude': 0.9133229242511781, 'cosine_with_motion': -0.24298211293665034, 'motion_component': -0.2219211339280315, 'motion_component_percent': 24.298211293665034}, {'resid': 426, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 14.704678535461426, 'force': [-0.37601815795928684, 0.15241533687433156, -0.19646817776916267], 'magnitude': 0.45079910703721066, 'cosine_with_motion': 0.24864456071503166, 'motion_component': 0.11208874593999578, 'motion_component_percent': 24.864456071503167}, {'resid': 426, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 13.219758987426758, 'force': [-0.0652462410549228, 0.02824976614235723, -0.02515798783075809], 'magnitude': 0.07541913292121262, 'cosine_with_motion': 0.17124413299328678, 'motion_component': 0.012915084028198508, 'motion_component_percent': 17.12441329932868}, {'resid': 426, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 12.607240676879883, 'force': [-0.20698671199682617, 0.07337791623375711, -0.0710410214311649], 'magnitude': 0.23081300712925293, 'cosine_with_motion': 0.20881268830492664, 'motion_component': 0.0481966845144035, 'motion_component_percent': 20.881268830492665}, {'resid': 426, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 14.587169647216797, 'force': [-0.076649061665319, 0.0339322533663251, -0.024653675315545295], 'magnitude': 0.08737436797628172, 'cosine_with_motion': 0.13472672297298385, 'motion_component': 0.011771662269280059, 'motion_component_percent': 13.472672297298386}, {'resid': 426, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 14.66709041595459, 'force': [-0.01850401279598529, 0.009096018699043223, -0.003923857762737846], 'magnitude': 0.020988870990825814, 'cosine_with_motion': 0.046858851512916036, 'motion_component': 0.0009835143891828576, 'motion_component_percent': 4.685885151291604}, {'resid': 426, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 14.419692993164062, 'force': [0.05746025324632701, -0.033759343426547864, 0.01279177267765144], 'magnitude': 0.0678601755078805, 'cosine_with_motion': 0.01134868706315981, 'motion_component': 0.0007701238958900376, 'motion_component_percent': 1.134868706315981}, {'resid': 426, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 13.837331771850586, 'force': [-1.2806234307173554, 0.5341122071228457, -0.1580395804390395], 'magnitude': 1.3965130611939418, 'cosine_with_motion': 0.0534378199480176, 'motion_component': 0.07462661351913674, 'motion_component_percent': 5.34378199480176}, {'resid': 426, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 13.996736526489258, 'force': [1.313907159013888, -0.41579401563165397, 0.1618009565986073], 'magnitude': 1.3875936853053443, 'cosine_with_motion': -0.1271857583497679, 'motion_component': -0.1764821551469094, 'motion_component_percent': 12.71857583497679}, {'resid': 426, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 13.293813705444336, 'force': [1.3879059347323446, -0.6592024054688912, 0.07260238721751497], 'magnitude': 1.5382138348327639, 'cosine_with_motion': 0.02409829756337943, 'motion_component': 0.03706833470790692, 'motion_component_percent': 2.409829756337943}, {'resid': 426, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 12.535074234008789, 'force': [-0.9347428927544644, 0.5331662494715415, -0.3570476591469983], 'magnitude': 1.13379608220918, 'cosine_with_motion': 0.07567277001117025, 'motion_component': 0.08579749016858114, 'motion_component_percent': 7.5672770011170245}, {'resid': 426, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 11.389250755310059, 'force': [1.242462240970332, -0.715821114489855, 0.40254774122417764], 'magnitude': 1.4893478345071727, 'cosine_with_motion': -0.04495356199594613, 'motion_component': -0.0669514902120463, 'motion_component_percent': 4.495356199594613}, {'resid': 754, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 5.35865592956543, 'force': [0.020703319514658803, 2.2838752867568792, 5.515148220031969], 'magnitude': 5.969369718975323, 'cosine_with_motion': -0.8254231175710813, 'motion_component': -4.927255763371021, 'motion_component_percent': 82.54231175710814}, {'resid': 754, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 6.157289028167725, 'force': [-0.07418722135614916, -1.2259926663803034, -2.2587328689180075], 'magnitude': 2.571076804562906, 'cosine_with_motion': 0.8782113293482567, 'motion_component': 2.257948778391658, 'motion_component_percent': 87.82113293482567}, {'resid': 754, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 4.163855075836182, 'force': [-0.0937809626260669, -0.3895323930342045, -0.6460642806221327], 'magnitude': 0.7602166854718592, 'cosine_with_motion': 0.917154525943418, 'motion_component': 0.6972361737782194, 'motion_component_percent': 91.7154525943418}, {'resid': 754, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 3.6754324436187744, 'force': [0.3131561289876035, -1.5550247962493509, -2.2042946461231456], 'magnitude': 2.715710545142836, 'cosine_with_motion': 0.8684180935509269, 'motion_component': 2.35837217424909, 'motion_component_percent': 86.84180935509269}, {'resid': 754, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 4.9525675773620605, 'force': [-0.1645493054825156, -0.5520489994537412, -0.49266533236022164], 'magnitude': 0.7579932067256688, 'cosine_with_motion': 0.9933711534678179, 'motion_component': 0.7529685860858478, 'motion_component_percent': 99.33711534678179}, {'resid': 754, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 5.692524433135986, 'force': [0.012617718425602407, 0.13557488121928576, 0.11347287280101288], 'magnitude': 0.1772451638200774, 'cosine_with_motion': -0.9712749395122011, 'motion_component': -0.17215378576817586, 'motion_component_percent': 97.12749395122012}, {'resid': 754, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 5.680540084838867, 'force': [0.06363204808069181, 0.11884981872991986, 0.11622171435463714], 'magnitude': 0.17799383091166152, 'cosine_with_motion': -0.991726395635772, 'motion_component': -0.17652118037542514, 'motion_component_percent': 99.1726395635772}, {'resid': 754, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 4.281439781188965, 'force': [-0.06894616805486112, -0.21589170325907106, -0.096488731090526], 'magnitude': 0.2463186490158871, 'cosine_with_motion': 0.9751674813128212, 'motion_component': 0.24020193656119943, 'motion_component_percent': 97.51674813128211}, {'resid': 754, 'resname': 'GLU', 'atom': 'HG2', 'charge': -0.042500000447034836, 'distance': 5.164259910583496, 'force': [0.15852321408147738, 0.48513585308645285, 0.13937600254703064], 'magnitude': 0.5290671747884499, 'cosine_with_motion': -0.9375681386316747, 'motion_component': -0.4960365262775258, 'motion_component_percent': 93.75681386316747}, {'resid': 754, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 4.00267219543457, 'force': [0.4514749819655982, 0.6965424850225095, 0.29432571347938125], 'magnitude': 0.8806978587445963, 'cosine_with_motion': -0.9475221009677314, 'motion_component': -0.8344806854354622, 'motion_component_percent': 94.75221009677314}, {'resid': 754, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 3.3726980686187744, 'force': [0.3710284522075463, -22.758947292934756, -5.870731216030349], 'magnitude': 23.506867698734407, 'cosine_with_motion': 0.8729535126706074, 'motion_component': 20.520402729493437, 'motion_component_percent': 87.29535126706074}, {'resid': 754, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 2.6508326530456543, 'force': [1.8593002507774488, 38.535748047845324, -2.8510234742281186], 'magnitude': 38.68577529118624, 'cosine_with_motion': -0.7262762932861518, 'motion_component': -28.09656148138374, 'motion_component_percent': 72.62762932861519}, {'resid': 754, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 3.987839460372925, 'force': [-5.064040406105003, 15.49842137165313, 5.133715117160847], 'magnitude': 17.09387613012755, 'cosine_with_motion': -0.7707327802636219, 'motion_component': -13.17481067525517, 'motion_component_percent': 77.07327802636219}, {'resid': 754, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 3.6582679748535156, 'force': [-5.316663564019318, -3.8249367912103134, -11.589120268608523], 'magnitude': 13.311827880122163, 'cosine_with_motion': 0.8422764617280754, 'motion_component': 11.212239286002442, 'motion_component_percent': 84.22764617280754}, {'resid': 754, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 2.5428404808044434, 'force': [14.24364672927492, 4.091512003715972, 25.943388079003302], 'magnitude': 29.877773137278933, 'cosine_with_motion': -0.7504800106776884, 'motion_component': -22.422671503090648, 'motion_component_percent': 75.04800106776884}, {'resid': 1082, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 14.737552642822266, 'force': [0.2590510945870284, -0.841529430362989, 0.1260699603891962], 'magnitude': 0.8894789973272712, 'cosine_with_motion': 0.5463065522786793, 'motion_component': 0.4859282043541581, 'motion_component_percent': 54.63065522786793}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'N', 'charge': -0.38210001587867737, 'distance': 13.743213653564453, 'force': [-0.2975036771859053, -0.48339125231553076, -0.35906673912838283], 'magnitude': 0.6716431075374798, 'cosine_with_motion': 0.988490347394267, 'motion_component': 0.6639127286946884, 'motion_component_percent': 98.8490347394267}, {'resid': 130, 'resname': 'ASN', 'atom': 'H', 'charge': 0.2681000232696533, 'distance': 13.688724517822266, 'force': [0.2107472641607138, 0.3613968010253428, 0.22498644333389045], 'magnitude': 0.47501679636262417, 'cosine_with_motion': -0.9845461826406781, 'motion_component': -0.46767597354902596, 'motion_component_percent': 98.4546182640678}, {'resid': 130, 'resname': 'ASN', 'atom': 'CA', 'charge': -0.20800000429153442, 'distance': 12.86524772644043, 'force': [-0.1587586063760088, -0.2968241185305162, -0.2465028426476434], 'magnitude': 0.4172199706069201, 'cosine_with_motion': 0.9958472515198175, 'motion_component': 0.4154873610080804, 'motion_component_percent': 99.58472515198174}, {'resid': 130, 'resname': 'ASN', 'atom': 'HA', 'charge': 0.13580000400543213, 'distance': 12.070148468017578, 'force': [0.13052606816308157, 0.20795411789312887, 0.18838023824471783], 'magnitude': 0.3094658038943227, 'cosine_with_motion': -0.9888190992835311, 'motion_component': -0.30600569746583806, 'motion_component_percent': 98.88190992835311}, {'resid': 130, 'resname': 'ASN', 'atom': 'CB', 'charge': -0.22990000247955322, 'distance': 12.447900772094727, 'force': [-0.15202934164649845, -0.38677682655275775, -0.2644518815552216], 'magnitude': 0.49258911065693156, 'cosine_with_motion': 0.9987202658044341, 'motion_component': 0.49195872752766046, 'motion_component_percent': 99.8720265804434}, {'resid': 130, 'resname': 'ASN', 'atom': 'HB2', 'charge': 0.1023000031709671, 'distance': 11.750934600830078, 'force': [0.0841732808408553, 0.19860764002673276, 0.1181838722249369], 'magnitude': 0.24596252466296967, 'cosine_with_motion': -0.9931435902515982, 'motion_component': -0.24427610481112896, 'motion_component_percent': 99.31435902515982}, {'resid': 130, 'resname': 'ASN', 'atom': 'HB3', 'charge': 0.1023000031709671, 'distance': 13.309401512145996, 'force': [0.05660962357100936, 0.1564254072436499, 0.09533077454484143], 'magnitude': 0.19173292384854637, 'cosine_with_motion': -0.9949413798597232, 'motion_component': -0.19076301981841196, 'motion_component_percent': 99.49413798597232}, {'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 11.908919334411621, 'force': [0.33838407262559916, 1.314687149264351, 0.9803054937400859], 'magnitude': 1.6744864711619818, 'cosine_with_motion': -0.9945266085386434, 'motion_component': -1.6653213512085667, 'motion_component_percent': 99.45266085386434}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 12.681903839111328, 'force': [-0.16058901294356137, -0.9695311124503821, -0.7572270519243304], 'magnitude': 1.2406337965949, 'cosine_with_motion': 0.9841936250966421, 'motion_component': 1.2210238736881447, 'motion_component_percent': 98.41936250966421}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 10.6524658203125, 'force': [-0.4853737210012613, -2.064485389717397, -1.6018652227653978], 'magnitude': 2.6577546473104774, 'cosine_with_motion': 0.9923104143984918, 'motion_component': 2.637317615442177, 'motion_component_percent': 99.23104143984918}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 10.539044380187988, 'force': [0.12520255749318426, 0.9384152748897333, 0.8015289452451034], 'magnitude': 1.2404626389436062, 'cosine_with_motion': -0.9773637442343424, 'motion_component': -1.212383209380736, 'motion_component_percent': 97.73637442343424}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 9.876602172851562, 'force': [0.3349073994920081, 1.1089681137422567, 0.8080983974784651], 'magnitude': 1.4124433664890148, 'cosine_with_motion': -0.9974394908652973, 'motion_component': -1.4088267923468694, 'motion_component_percent': 99.74394908652972}, {'resid': 130, 'resname': 'ASN', 'atom': 'C', 'charge': 0.8050000071525574, 'distance': 13.721765518188477, 'force': [0.4621345499777166, 0.9581136555391653, 0.939803946574249], 'magnitude': 1.4194300184265032, 'cosine_with_motion': -0.9928699263170785, 'motion_component': -1.4093093778073715, 'motion_component_percent': 99.28699263170785}, {'resid': 130, 'resname': 'ASN', 'atom': 'O', 'charge': -0.8147000074386597, 'distance': 13.473051071166992, 'force': [-0.4831179843212489, -0.9089957169283788, -1.0773133658647167], 'magnitude': 1.4900604982481513, 'cosine_with_motion': 0.9785071805802416, 'motion_component': 1.4580348970347885, 'motion_component_percent': 97.85071805802416}, {'resid': 458, 'resname': 'ASN', 'atom': 'H', 'charge': 0.2681000232696533, 'distance': 14.988238334655762, 'force': [-0.35159251474955083, 0.14668083919044975, 0.10888439535121618], 'magnitude': 0.3962175873993072, 'cosine_with_motion': -0.1707580934611865, 'motion_component': -0.06765735982009673, 'motion_component_percent': 17.07580934611865}, {'resid': 458, 'resname': 'ASN', 'atom': 'CB', 'charge': -0.22990000247955322, 'distance': 13.948356628417969, 'force': [0.31966476671883176, -0.20056810612156376, -0.10721534479443566], 'magnitude': 0.3923114304146461, 'cosine_with_motion': 0.29865534120148074, 'motion_component': 0.11716590410772709, 'motion_component_percent': 29.865534120148073}, {'resid': 458, 'resname': 'ASN', 'atom': 'HB2', 'charge': 0.1023000031709671, 'distance': 14.130436897277832, 'force': [-0.14275347537218278, 0.08594429294805073, 0.034187662521375416], 'magnitude': 0.17009930184998473, 'cosine_with_motion': -0.24489107379247274, 'motion_component': -0.041655800681392706, 'motion_component_percent': 24.489107379247272}, {'resid': 458, 'resname': 'ASN', 'atom': 'HB3', 'charge': 0.1023000031709671, 'distance': 13.15825366973877, 'force': [-0.16233101313234155, 0.09212510123298781, 0.06034531667896254], 'magnitude': 0.19616306825405483, 'cosine_with_motion': -0.2831650358996113, 'motion_component': -0.05554652226433733, 'motion_component_percent': 28.31650358996113}, {'resid': 458, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 13.690324783325195, 'force': [-0.9465642293702777, 0.760428180794035, 0.36224098811173583], 'magnitude': 1.2670648728211353, 'cosine_with_motion': -0.3937874199450275, 'motion_component': -0.49895420717120925, 'motion_component_percent': 39.37874199450275}, {'resid': 458, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 14.217873573303223, 'force': [0.7117622174176591, -0.6432120444722279, -0.2322906140921963], 'magnitude': 0.9870593283550771, 'cosine_with_motion': 0.411390164935663, 'motion_component': 0.4060664998932799, 'motion_component_percent': 41.1390164935663}, {'resid': 458, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 13.015183448791504, 'force': [1.2540066958212217, -1.0909152124660622, -0.6380848113828289], 'magnitude': 1.7803878848362769, 'cosine_with_motion': 0.45820753997672314, 'motion_component': 0.8157871529151919, 'motion_component_percent': 45.82075399767231}, {'resid': 458, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 13.103280067443848, 'force': [-0.5230588804372654, 0.5369175221645761, 0.286494548494512], 'magnitude': 0.8024650424340664, 'cosine_with_motion': -0.5159820339304598, 'motion_component': -0.4140575447532223, 'motion_component_percent': 51.598203393045985}, {'resid': 458, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 12.524663925170898, 'force': [-0.6287157102878594, 0.49747715761778505, 0.3587246648105989], 'magnitude': 0.87832246462089, 'cosine_with_motion': -0.44858427188238725, 'motion_component': -0.3940016432699058, 'motion_component_percent': 44.85842718823873}, {'resid': 786, 'resname': 'ASN', 'atom': 'N', 'charge': -0.38210001587867737, 'distance': 7.501667022705078, 'force': [0.49021578820599154, 0.5668397111822048, -2.1260210688329435], 'magnitude': 2.2542369800668958, 'cosine_with_motion': 0.2894866368235599, 'motion_component': 0.652571481962864, 'motion_component_percent': 28.948663682355992}, {'resid': 786, 'resname': 'ASN', 'atom': 'H', 'charge': 0.2681000232696533, 'distance': 6.8839216232299805, 'force': [-0.20239703513274077, -0.4813442562026131, 1.8042514266567378], 'magnitude': 1.8782917939986439, 'cosine_with_motion': -0.32915562588543806, 'motion_component': -0.6182503110491059, 'motion_component_percent': 32.91556258854381}, {'resid': 786, 'resname': 'ASN', 'atom': 'CA', 'charge': -0.20800000429153442, 'distance': 7.886672496795654, 'force': [0.3502795636682051, 0.11349646780592988, -1.0473959700202684], 'magnitude': 1.1102322004620069, 'cosine_with_motion': 0.372983065316697, 'motion_component': 0.41409780934162094, 'motion_component_percent': 37.2983065316697}, {'resid': 786, 'resname': 'ASN', 'atom': 'HA', 'charge': 0.13580000400543213, 'distance': 7.839688777923584, 'force': [-0.3218845655237848, -0.09792861103008875, 0.6518603529085356], 'magnitude': 0.7335677242591572, 'cosine_with_motion': -0.2802781585611422, 'motion_component': -0.2056030109352443, 'motion_component_percent': 28.02781585611422}, {'resid': 786, 'resname': 'ASN', 'atom': 'CB', 'charge': -0.22990000247955322, 'distance': 6.96112060546875, 'force': [0.46226908464725724, -0.10364852128038286, -1.502206986300529], 'magnitude': 1.5751385819267905, 'cosine_with_motion': 0.5128584827137732, 'motion_component': 0.8078231831908981, 'motion_component_percent': 51.28584827137732}, {'resid': 786, 'resname': 'ASN', 'atom': 'HB2', 'charge': 0.1023000031709671, 'distance': 6.013607025146484, 'force': [-0.33747211124980603, 0.018039501246879874, 0.8762562556349363], 'magnitude': 0.939168714883538, 'cosine_with_motion': -0.4456673236820701, 'motion_component': -0.41855680764807557, 'motion_component_percent': 44.56673236820701}, {'resid': 786, 'resname': 'ASN', 'atom': 'HB3', 'charge': 0.1023000031709671, 'distance': 6.96274471282959, 'force': [-0.10062106185782334, 0.06931251980960339, 0.6898350531821371], 'magnitude': 0.7005720691624485, 'cosine_with_motion': -0.60123793258576, 'motion_component': -0.4212105024905586, 'motion_component_percent': 60.123793258576}, {'resid': 786, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 7.618808269500732, 'force': [-1.5405918717261788, 0.8970836658594293, 3.6823709083252574], 'magnitude': 4.091214724902708, 'cosine_with_motion': -0.5728971583608515, 'motion_component': -2.3438452901408344, 'motion_component_percent': 57.28971583608515}, {'resid': 786, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 8.537376403808594, 'force': [0.8568063749077062, -0.7672591809837095, -2.4842370944154095], 'magnitude': 2.7375605483999426, 'cosine_with_motion': 0.642619465539742, 'motion_component': 1.7592096964954542, 'motion_component_percent': 64.2619465539742}, {'resid': 786, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 7.498124122619629, 'force': [2.8456438671293864, -1.303742262918855, -4.356359967345832], 'magnitude': 5.364261838477429, 'cosine_with_motion': 0.4934066475087124, 'motion_component': 2.64676245008207, 'motion_component_percent': 49.34066475087124}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 8.276344299316406, 'force': [-1.1255524830412058, 0.616942602411746, 1.548690415703839], 'magnitude': 2.0114493705892107, 'cosine_with_motion': -0.5084184174269311, 'motion_component': -1.022657905729363, 'motion_component_percent': 50.841841742693106}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 6.944668292999268, 'force': [-1.7222472408920102, 0.4454123847072834, 2.235375709780563], 'magnitude': 2.85682206570303, 'cosine_with_motion': -0.388363104597221, 'motion_component': -1.1094842867182748, 'motion_component_percent': 38.8363104597221}, {'resid': 786, 'resname': 'ASN', 'atom': 'C', 'charge': 0.8050000071525574, 'distance': 9.356072425842285, 'force': [-0.8684994864299833, -0.19316420493079656, 2.920627026247174], 'magnitude': 3.0531403496140004, 'cosine_with_motion': -0.4195198328902142, 'motion_component': -1.2808529292604356, 'motion_component_percent': 41.95198328902142}, {'resid': 786, 'resname': 'ASN', 'atom': 'O', 'charge': -0.8147000074386597, 'distance': 10.098258018493652, 'force': [0.9857451010534671, 0.09695902599048614, -2.46053977526189], 'magnitude': 2.652423503631682, 'cosine_with_motion': 0.39661260318306224, 'motion_component': 1.0519845905193, 'motion_component_percent': 39.661260318306226}], 'sf_contributions': [{'resid': 100, 'resname': 'THR', 'atom': 'N', 'charge': -0.4157000184059143, 'distance': 9.454451560974121, 'force': [-0.500074669765452, -1.2946255848007806, 0.6765984087662246], 'magnitude': 1.54399335714464, 'cosine_with_motion': 0.4794664730217872, 'motion_component': 0.7402930493192091, 'motion_component_percent': 47.94664730217872}, {'resid': 100, 'resname': 'THR', 'atom': 'H', 'charge': 0.2718999981880188, 'distance': 10.196442604064941, 'force': [0.3354068855950018, 0.7176704463771909, -0.3554254424174898], 'magnitude': 0.868260268367408, 'cosine_with_motion': -0.5060250599342219, 'motion_component': -0.43936145433912116, 'motion_component_percent': 50.602505993422184}, {'resid': 100, 'resname': 'THR', 'atom': 'CA', 'charge': -0.03889999911189079, 'distance': 9.98306941986084, 'force': [-0.024337471728129213, -0.11124004078020162, 0.06185452458156919], 'magnitude': 0.12958642449774727, 'cosine_with_motion': 0.43073817257871483, 'motion_component': 0.05581781967916926, 'motion_component_percent': 43.07381725787148}, {'resid': 100, 'resname': 'THR', 'atom': 'HA', 'charge': 0.1007000058889389, 'distance': 11.065008163452148, 'force': [0.05276874339582523, 0.23563609178417558, -0.12749479941589661], 'magnitude': 0.2730637872530786, 'cosine_with_motion': -0.4418286713669041, 'motion_component': -0.1206474103204427, 'motion_component_percent': 44.18286713669041}, {'resid': 100, 'resname': 'THR', 'atom': 'CB', 'charge': 0.3653999865055084, 'distance': 9.628469467163086, 'force': [0.08195224112158213, 1.1948164942284574, -0.5272708750364847</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>50</v>
+        <v>939</v>
       </c>
       <c r="B3" t="n">
-        <v>692</v>
+        <v>946</v>
       </c>
       <c r="C3" t="n">
-        <v>2399</v>
+        <v>2381</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>{50: {'frame': 50, 'motion_vector': [-1.7414207458496094, -1.1786270141601562, 2.00604248046875], 'ionic_force': [-6.545310348272324, -0.7018430531024933, -10.480357229709625], 'ionic_force_magnitude': 12.376249790979326, 'radial_force': 6.5828315508137525, 'axial_force': -10.480357229709625, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-7.2292962074279785, 2.4936505556106567, -9.968634337186813], 'asn_force_magnitude': 12.564023531368042, 'residue_force': [-7.2292962074279785, 2.4936505556106567, -9.968634337186813], 'residue_force_magnitude': 12.564023531368042, 'pip2_force': [0.3286649566143751, -0.16861860593780875, -4.935831281458377], 'pip2_force_magnitude': 4.949634666013016, 'total_force': [-13.445941599085927, 1.6231888965703547, -25.384822848354816], 'total_force_magnitude': 28.771814658139576, 'cosine_total_motion': -0.3518590321781765, 'cosine_glu_motion': 0, 'cosine_asn_motion': -0.2833849045886601, 'cosine_residue_motion': -0.2833849045886601, 'cosine_pip2_motion': -0.7143141794509533, 'cosine_ionic_motion': -0.244627740715776, 'motion_component_total': -10.123622859622863, 'motion_component_glu': 0, 'motion_component_asn': -3.5604546096864134, 'motion_component_residue': -3.5604546096864134, 'motion_component_ionic': -3.0275740249013676, 'motion_component_pip2': -3.535594225035081, 'motion_component_percent_total': 35.185903217817646, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 28.338490458866012, 'motion_component_percent_residue': 28.338490458866012, 'motion_component_percent_ionic': 24.462774071577602, 'motion_component_percent_pip2': 71.43141794509533, 'ionic_contributions': [{'ion_id': 2276, 'distance': 14.84231948852539, 'force': [-0.20308879017829895, 0.05022875964641571, -1.4924824237823486], 'magnitude': 1.5070738792419434, 'cosine_ionic_motion': -0.6163520812988281, 'motion_component_ionic': -0.9288880825042725, 'motion_component_percent_ionic': 61.63520812988281}, {'ion_id': 2397, 'distance': 11.31926441192627, 'force': [-0.4405474066734314, 0.15366230905056, -2.54885196685791], 'magnitude': 2.5912044048309326, 'cosine_ionic_motion': -0.6011586785316467, 'motion_component_ionic': -1.557724952697754, 'motion_component_percent_ionic': 60.11586785316467}, {'ion_id': 2398, 'distance': 7.586583137512207, 'force': [-1.7664893865585327, 0.29237300157546997, -5.483336925506592], 'magnitude': 5.768270969390869, 'cosine_ionic_motion': -0.4932217597961426, 'motion_component_ionic': -2.845036745071411, 'motion_component_percent_ionic': 49.32217597961426}, {'ion_id': 2400, 'distance': 8.676553726196289, 'force': [-4.1351847648620605, -1.198107123374939, -0.9556859135627747], 'magnitude': 4.410050868988037, 'cosine_ionic_motion': 0.5224601030349731, 'motion_component_ionic': 2.3040757179260254, 'motion_component_percent_ionic': 52.246010303497314}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 3.536907196044922, 'force': [17.50432777404785, 6.932760238647461, 2.4316861629486084], 'magnitude': 18.983617782592773, 'cosine_with_motion': -0.6122081279754639, 'motion_component': -11.621925354003906, 'motion_component_percent': 61.22081279754639}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 2.6598477363586426, 'force': [-25.585451126098633, -6.123941898345947, -10.163896560668945], 'magnitude': 28.20323944091797, 'cosine_with_motion': 0.3828964829444885, 'motion_component': 10.798921585083008, 'motion_component_percent': 38.28964829444885}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 3.8168246746063232, 'force': [-19.41979217529297, -5.711623191833496, 4.338071346282959], 'magnitude': 20.701927185058594, 'cosine_with_motion': 0.818638265132904, 'motion_component': 16.947389602661133, 'motion_component_percent': 81.8638265132904}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 3.4632747173309326, 'force': [10.508767127990723, 1.0664888620376587, -4.514759540557861], 'magnitude': 11.487151145935059, 'cosine_with_motion': -0.8571218252182007, 'motion_component': -9.845888137817383, 'motion_component_percent': 85.71218252182007}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 4.746883392333984, 'force': [5.515578269958496, 2.1035537719726562, -1.5943527221679688], 'magnitude': 6.114614009857178, 'cosine_with_motion': -0.8600119948387146, 'motion_component': -5.258641242980957, 'motion_component_percent': 86.00119948387146}, {'resid': 786, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 5.7620086669921875, 'force': [4.247273921966553, 4.226412773132324, -0.46538302302360535], 'magnitude': 6.0098652839660645, 'cosine_with_motion': -0.7621320486068726, 'motion_component': -4.580310821533203, 'motion_component_percent': 76.21320486068726}], 'pip2_contributions': [{'resid': 1313, 'atom': 'C1', 'charge': 0.06000000238418579, 'distance': 28.01099967956543, 'force': [-0.018726617097854614, -0.011985673569142818, 0.01225637923926115], 'magnitude': 0.025388214737176895, 'cosine_with_motion': 0.9666793942451477, 'motion_component': 0.02454226464033127, 'motion_component_percent': 96.66793942451477}, {'resid': 1313, 'atom': 'C11', 'charge': 0.17000000178813934, 'distance': 27.12787437438965, 'force': [-0.062194835394620895, -0.03398802503943443, 0.029298905283212662], 'magnitude': 0.07669295370578766, 'cosine_with_motion': 0.9293689131736755, 'motion_component': 0.07127604633569717, 'motion_component_percent': 92.93689131736755}, {'resid': 1313, 'atom': 'C12', 'charge': 0.04000000283122063, 'distance': 26.49906349182129, 'force': [-0.015826033428311348, -0.00811096467077732, 0.006435214076191187], 'magnitude': 0.01891198195517063, 'cosine_with_motion': 0.9102497100830078, 'motion_component': 0.01721462607383728, 'motion_component_percent': 91.02497100830078}, {'resid': 1313, 'atom': 'C13', 'charge': -0.05000000074505806, 'distance': 26.898412704467773, 'force': [0.019192686304450035, 0.010620019398629665, -0.006726689171046019], 'magnitude': 0.022943241521716118, 'cosine_with_motion': -0.891361653804779, 'motion_component': -0.02045072615146637, 'motion_component_percent': 89.1361653804779}, {'resid': 1313, 'atom': 'C2', 'charge': 0.06000000238418579, 'distance': 29.4793643951416, 'force': [-0.016957689076662064, -0.010855847038328648, 0.010954765602946281], 'magnitude': 0.022922031581401825, 'cosine_with_motion': 0.9652561545372009, 'motion_component': 0.02212563157081604, 'motion_component_percent': 96.52561545372009}, {'resid': 1313, 'atom': 'C21', 'charge': 0.6299999952316284, 'distance': 24.434785842895508, 'force': [-0.3013263940811157, -0.13747839629650116, 0.11412396281957626], 'magnitude': 0.3503172695636749, 'cosine_with_motion': 0.899441123008728, 'motion_component': 0.31508976221084595, 'motion_component_percent': 89.9441123008728}, {'resid': 1313, 'atom': 'C210', 'charge': -0.18000000715255737, 'distance': 25.04411506652832, 'force': [0.0915977954864502, 0.024863915517926216, -0.008354746736586094], 'magnitude': 0.09527944773435593, 'cosine_with_motion': -0.7424187064170837, 'motion_component': -0.07073724269866943, 'motion_component_percent': 74.24187064170837}, {'resid': 1313, 'atom': 'C211', 'charge': -0.15000000596046448, 'distance': 24.343381881713867, 'force': [0.08186668902635574, 0.017484353855252266, -0.007366239558905363], 'magnitude': 0.08403641730546951, 'cosine_with_motion': -0.728625476360321, 'motion_component': -0.06123107671737671, 'motion_component_percent': 72.8625476360321}, {'resid': 1313, 'atom': 'C212', 'charge': -0.15000000596046448, 'distance': 24.32572364807129, 'force': [0.08214151859283447, 0.014538208954036236, -0.011138146743178368], 'magnitude': 0.08415846526622772, 'cosine_with_motion': -0.7462652921676636, 'motion_component': -0.06280454248189926, 'motion_component_percent': 74.62652921676636}, {'resid': 1313, 'atom': 'C213', 'charge': -0.18000000715255737, 'distance': 25.113792419433594, 'force': [0.0916767492890358, 0.01665637455880642, -0.01719827763736248], 'magnitude': 0.09475147724151611, 'cosine_with_motion': -0.7763500213623047, 'motion_component': -0.07356031239032745, 'motion_component_percent': 77.63500213623047}, {'resid': 1313, 'atom': 'C214', 'charge': -0.15000000596046448, 'distance': 24.305133819580078, 'force': [0.08038219809532166, 0.01690923050045967, -0.018959373235702515], 'magnitude': 0.08430111408233643, 'cosine_with_motion': -0.8079449534416199, 'motion_component': -0.06811065971851349, 'motion_component_percent': 80.79449534416199}, {'resid': 1313, 'atom': 'C215', 'charge': -0.15000000596046448, 'distance': 24.64800453186035, 'force': [0.0767655223608017, 0.018212785944342613, -0.022243382409214973], 'magnitude': 0.08197206258773804, 'cosine_with_motion': -0.8385663032531738, 'motion_component': -0.06873901188373566, 'motion_component_percent': 83.85663032531738}, {'resid': 1313, 'atom': 'C216', 'charge': -0.18000000715255737, 'distance': 26.089590072631836, 'force': [0.0815596953034401, 0.02018176019191742, -0.025473495945334435], 'magnitude': 0.08779627829790115, 'cosine_with_motion': -0.8501489162445068, 'motion_component': -0.07463990896940231, 'motion_component_percent': 85.01489162445068}, {'resid': 1313, 'atom': 'C217', 'charge': -0.18000000715255737, 'distance': 26.45683479309082, 'force': [0.07854114472866058, 0.017000684514641762, -0.028832167387008667], 'magnitude': 0.08537580817937851, 'cosine_with_motion': -0.8651095032691956, 'motion_component': -0.07385942339897156, 'motion_component_percent': 86.51095032691956}, {'resid': 1313, 'atom': 'C218', 'charge': -0.18000000715255737, 'distance': 26.2915096282959, 'force': [0.08050369471311569, 0.012154463678598404, -0.02907797507941723], 'magnitude': 0.0864529013633728, 'cosine_with_motion': -0.8471624851226807, 'motion_component': -0.07323965430259705, 'motion_component_percent': 84.71624851226807}, {'resid': 1313, 'atom': 'C219', 'charge': -0.18000000715255737, 'distance': 27.025402069091797, 'force': [0.07520081102848053, 0.009123559109866619, -0.030924441292881966], 'magnitude': 0.08182128518819809, 'cosine_with_motion': -0.8568363785743713, 'motion_component': -0.07010745257139206, 'motion_component_percent': 85.68363785743713}, {'resid': 1313, 'atom': 'C22', 'charge': -0.08000000566244125, 'distance': 23.031497955322266, 'force': [0.04273582994937897, 0.01972389407455921, -0.017079012468457222], 'magnitude': 0.050070710480213165, 'cosine_with_motion': -0.9066391587257385, 'motion_component': -0.04539606720209122, 'motion_component_percent': 90.66391587257385}, {'resid': 1313, 'atom': 'C220', 'charge': -0.27000001072883606, 'distance': 26.689979553222656, 'force': [0.11625736951828003, 0.006984170060604811, -0.04764638841152191], 'magnitude': 0.12583613395690918, 'cosine_with_motion': -0.8374699354171753, 'motion_component': -0.1053839772939682, 'motion_component_percent': 83.74699354171753}, {'resid': 1313, 'atom': 'C23', 'charge': -0.18000000715255737, 'distance': 22.057443618774414, 'force': [0.1082642525434494, 0.04371555149555206, -0.038140784949064255], 'magnitude': 0.12282881140708923, 'cosine_with_motion': -0.8868417143821716, 'motion_component': -0.10892971605062485, 'motion_component_percent': 88.68417143821716}, {'resid': 1313, 'atom': 'C24', 'charge': -0.18000000715255737, 'distance': 21.280075073242188, 'force': [0.11705315113067627, 0.05073871091008186, -0.03375423699617386], 'magnitude': 0.13196668028831482, 'cosine_with_motion': -0.8639797568321228, 'motion_component': -0.11401654034852982, 'motion_component_percent': 86.39797568321228}, {'resid': 1313, 'atom': 'C25', 'charge': -0.15000000596046448, 'distance': 20.9041805267334, 'force': [0.10448335856199265, 0.03833189979195595, -0.024523675441741943], 'magnitude': 0.11396279186010361, 'cosine_with_motion': -0.8343191742897034, 'motion_component': -0.09508134424686432, 'motion_component_percent': 83.43191742897034}, {'resid': 1313, 'atom': 'C26', 'charge': -0.15000000596046448, 'distance': 21.6762752532959, 'force': [0.0989554226398468, 0.033233970403671265, -0.018356379121541977], 'magnitude': 0.10598881542682648, 'cosine_with_motion': -0.8061639666557312, 'motion_component': -0.0854443609714508, 'motion_component_percent': 80.61639666557312}, {'resid': 1313, 'atom': 'C27', 'charge': -0.18000000715255737, 'distance': 23.086471557617188, 'force': [0.10429465025663376, 0.03709140792489052, -0.017845582216978073], 'magnitude': 0.11212319135665894, 'cosine_with_motion': -0.8013998866081238, 'motion_component': -0.08985551446676254, 'motion_component_percent': 80.13998866081238}, {'resid': 1313, 'atom': 'C28', 'charge': -0.15000000596046448, 'distance': 23.355907440185547, 'force': [0.08557257801294327, 0.030596930533647537, -0.008689801208674908], 'magnitude': 0.09129266440868378, 'cosine_with_motion': -0.7632946968078613, 'motion_component': -0.06968320906162262, 'motion_component_percent': 76.32946968078613}, {'resid': 1313, 'atom': 'C29', 'charge': -0.15000000596046448, 'distance': 24.276840209960938, 'force': [0.08021902292966843, 0.025942731648683548, -0.005634661763906479], 'magnitude': 0.08449772745370865, 'cosine_with_motion': -0.7394149899482727, 'motion_component': -0.06247888505458832, 'motion_component_percent': 73.94149899482727}, {'resid': 1313, 'atom': 'C3', 'charge': 0.06000000238418579, 'distance': 30.350936889648438, 'force': [-0.01595482788980007, -0.00958431325852871, 0.011009149253368378], 'magnitude': 0.021624453365802765, 'cosine_with_motion': 0.9732761383056641, 'motion_component': 0.021046563982963562, 'motion_component_percent': 97.3276138305664}, {'resid': 1313, 'atom': 'C31', 'charge': 0.6299999952316284, 'distance': 27.743694305419922, 'force': [-0.2386857122182846, -0.11175912618637085, 0.06618499010801315], 'magnitude': 0.2717377841472626, 'cosine_with_motion': 0.8612471222877502, 'motion_component': 0.23403339087963104, 'motion_component_percent': 86.12471222877502}, {'resid': 1313, 'atom': 'C310', 'charge': -0.18000000715255737, 'distance': 25.633176803588867, 'force': [0.07815276086330414, 0.04540754109621048, 0.0101153664290905], 'magnitude': 0.09095063805580139, 'cosine_with_motion': -0.6406019330024719, 'motion_component': -0.058263152837753296, 'motion_component_percent': 64.06019330024719}, {'resid': 1313, 'atom': 'C311', 'charge': -0.18000000715255737, 'distance': 25.352142333984375, 'force': [0.07980728149414062, 0.04505106806755066, 0.0156891867518425], 'magnitude': 0.09297823160886765, 'cosine_with_motion': -0.5943602919578552, 'motion_component': -0.05526256933808327, 'motion_component_percent': 59.43602919578552}, {'resid': 1313, 'atom': 'C312', 'charge': -0.18000000715255737, 'distance': 23.819875717163086, 'force': [0.09041812270879745, 0.05049477145075798, 0.019188668578863144], 'magnitude': 0.10532504320144653, 'cosine_with_motion': -0.5830795168876648, 'motion_component': -0.06141287460923195, 'motion_component_percent': 58.30795168876648}, {'resid': 1313, 'atom': 'C313', 'charge': -0.18000000715255737, 'distance': 23.52074432373047, 'force': [0.09212464839220047, 0.04989314451813698, 0.026311125606298447], 'magnitude': 0.1080210730433464, 'cosine_with_motion': -0.530221164226532, 'motion_component': -0.05727505683898926, 'motion_component_percent': 53.0221164226532}, {'resid': 1313, 'atom': 'C314', 'charge': -0.18000000715255737, 'distance': 24.262231826782227, 'force': [0.08352735638618469, 0.050089456140995026, 0.028642937541007996], 'magnitude': 0.10151941329240799, 'cosine_with_motion': -0.49836283922195435, 'motion_component': -0.050593502819538116, 'motion_component_percent': 49.836283922195435}, {'resid': 1313, 'atom': 'C315', 'charge': -0.18000000715255737, 'distance': 23.7382755279541, 'force': [0.08397702872753143, 0.05794347822666168, 0.02893265150487423], 'magnitude': 0.10605039447546005, 'cosine_with_motion': -0.5077608227729797, 'motion_component': -0.053848233073949814, 'motion_component_percent': 50.776082277297974}, {'resid': 1313, 'atom': 'C316', 'charge': -0.18000000715255737, 'distance': 24.59172821044922, 'force': [0.07493862509727478, 0.05702672898769379, 0.029949825257062912], 'magnitude': 0.09881719201803207, 'cosine_with_motion': -0.4792526066303253, 'motion_component': -0.047358397394418716, 'motion_component_percent': 47.92526066303253}, {'resid': 1313, 'atom': 'C317', 'charge': -0.18000000715255737, 'distance': 25.973957061767578, 'force': [0.06715332716703415, 0.05216098576784134, 0.024819981306791306], 'magnitude': 0.08857972919940948, 'cosine_with_motion': -0.4996738135814667, 'motion_component': -0.04426097124814987, 'motion_component_percent': 49.96738135814667}, {'resid': 1313, 'atom': 'C318', 'charge': -0.27000001072883606, 'distance': 26.061813354492188, 'force': [0.09911034256219864, 0.0816081091761589, 0.03057333268225193], 'magnitude': 0.13197526335716248, 'cosine_with_motion': -0.5408677458763123, 'motion_component': -0.07138116657733917, 'motion_component_percent': 54.086774587631226}, {'resid': 1313, 'atom': 'C32', 'charge': -0.08000000566244125, 'distance': 27.460922241210938, 'force': [0.03170037642121315, 0.013735642656683922, -0.006849483586847782], 'magnitude': 0.035220690071582794, 'cosine_with_motion': -0.8317216038703918, 'motion_component': -0.029293809086084366, 'motion_component_percent': 83.17216038703918}, {'resid': 1313, 'atom': 'C33', 'charge': -0.18000000715255737, 'distance': 28.56014060974121, 'force': [0.06589315086603165, 0.029949842020869255, -0.011344426311552525], 'magnitude': 0.07326388359069824, 'cosine_with_motion': -0.8116008639335632, 'motion_component': -0.05946103110909462, 'motion_component_percent': 81.16008639335632}, {'resid': 1313, 'atom': 'C34', 'charge': -0.18000000715255737, 'distance': 28.655336380004883, 'force': [0.06685290485620499, 0.027629580348730087, -0.007994964718818665], 'magnitude': 0.07277791202068329, 'cosine_with_motion': -0.7802243828773499, 'motion_component': -0.056783102452754974, 'motion_component_percent': 78.02243828773499}, {'resid': 1313, 'atom': 'C35', 'charge': -0.18000000715255737, 'distance': 27.44031524658203, 'force': [0.07309518754482269, 0.030347511172294617, -0.005918057635426521], 'magnitude': 0.07936561852693558, 'cosine_with_motion': -0.7584167718887329, 'motion_component': -0.06019221618771553, 'motion_component_percent': 75.84167718887329}, {'resid': 1313, 'atom': 'C36', 'charge': -0.18000000715255737, 'distance': 27.088674545288086, 'force': [0.07335864007472992, 0.03505804389715195, -0.00467287190258503], 'magnitude': 0.08143950253725052, 'cosine_with_motion': -0.7539457082748413, 'motion_component': -0.06140096113085747, 'motion_component_percent': 75.39457082748413}, {'resid': 1313, 'atom': 'C37', 'charge': -0.18000000715255737, 'distance': 26.33851432800293, 'force': [0.07788114994764328, 0.03680691868066788, -0.0008176924893632531], 'magnitude': 0.0861445963382721, 'cosine_with_motion': -0.7215666770935059, 'motion_component': -0.06215907260775566, 'motion_component_percent': 72.15666770935059}, {'resid': 1313, 'atom': 'C38', 'charge': -0.18000000715255737, 'distance': 26.236770629882812, 'force': [0.07655657082796097, 0.04088493809103966, 0.002046407898887992], 'magnitude': 0.0868140235543251, 'cosine_with_motion': -0.7031381130218506, 'motion_component': -0.06104224920272827, 'motion_component_percent': 70.31381130218506}, {'resid': 1313, 'atom': 'C39', 'charge': -0.18000000715255737, 'distance': 25.605525970458984, 'force': [0.08064118772745132, 0.041913531720638275, 0.0069325692020356655], 'magnitude': 0.09114716947078705, 'cosine_with_motion': -0.6641369462013245, 'motion_component': -0.06053420528769493, 'motion_component_percent': 66.41369462013245}, {'resid': 1313, 'atom': 'C4', 'charge': 0.08000000566244125, 'distance': 30.026735305786133, 'force': [-0.02081386372447014, -0.013145255856215954, 0.01618003286421299], 'magnitude': 0.029458582401275635, 'cosine_with_motion': 0.9834693074226379, 'motion_component': 0.028971612453460693, 'motion_component_percent': 98.3469307422638}, {'resid': 1313, 'atom': 'C5', 'charge': 0.08000000566244125, 'distance': 28.479055404663086, 'force': [-0.02297375351190567, -0.01448468491435051, 0.018297363072633743], 'magnitude': 0.032747410237789154, 'cosine_with_motion': 0.9854391813278198, 'motion_component': 0.032270580530166626, 'motion_component_percent': 98.54391813278198}, {'resid': 1313, 'atom': 'C6', 'charge': 0.06000000238418579, 'distance': 27.64038848876953, 'force': [-0.01839340291917324, -0.012371918186545372, 0.013727754354476929], 'magnitude': 0.026073604822158813, 'cosine_with_motion': 0.9785714149475098, 'motion_component': 0.025514883920550346, 'motion_component_percent': 97.85714149475098}, {'resid': 1313, 'atom': 'H1', 'charge': 0.12000000476837158, 'distance': 27.57379722595215, 'force': [-0.039735376834869385, -0.02319786138832569, 0.025072989985346794], 'magnitude': 0.05239938944578171, 'cosine_with_motion': 0.9642294049263, 'motion_component': 0.050525031983852386, 'motion_component_percent': 96.42294049263}, {'resid': 1313, 'atom': 'H10R', 'charge': 0.09000000357627869, 'distance': 25.50831413269043, 'force': [-0.04384318366646767, -0.01238551177084446, 0.005759193561971188], 'magnitude': 0.045921605080366135, 'cosine_with_motion': 0.7680432200431824, 'motion_component': 0.03526977822184563, 'motion_component_percent': 76.80432200431824}, {'resid': 1313, 'atom': 'H10S', 'charge': 0.09000000357627869, 'distance': 25.93306541442871, 'force': [-0.04283418878912926, -0.011464374139904976, 0.0027918892446905375], 'magnitude': 0.044429656118154526, 'cosine_with_motion': 0.7257172465324402, 'motion_component': 0.03224336728453636, 'motion_component_percent': 72.57172465324402}, {'resid': 1313, 'atom': 'H10X', 'charge': 0.09000000357627869, 'distance': 24.872831344604492, 'force': [-0.0408053882420063, -0.025368912145495415, -0.004903704859316349], 'magnitude': 0.04829811304807663, 'cosine_with_motion': 0.6491925120353699, 'motion_component': 0.03135477378964424, 'motion_component_percent': 64.91925120353699}, {'resid': 1313, 'atom': 'H10Y', 'charge': 0.09000000357627869, 'distance': 26.584863662719727, 'force': [-0.0359291136264801, -0.02183980867266655, -0.00441915774717927], 'magnitude': 0.042277742177248, 'cosine_with_motion': 0.646582841873169, 'motion_component': 0.027336062863469124, 'motion_component_percent': 64.6582841873169}, {'resid': 1313, 'atom': 'H111', 'charge': 0.15000000596046448, 'distance': 23.780059814453125, 'force': [-0.08617128431797028, -0.01762230135500431, 0.00440596416592598], 'magnitude': 0.0880650207400322, 'cosine_with_motion': 0.7020154595375061, 'motion_component': 0.061823006719350815, 'motion_component_percent': 70.20154595375061}, {'resid': 1313, 'atom': 'H11A', 'charge': 0.09000000357627869, 'distance': 28.206741333007812, 'force': [-0.03054092265665531, -0.01670045405626297, 0.014098591171205044], 'magnitude': 0.03755560517311096, 'cosine_with_motion': 0.9267662763595581, 'motion_component': 0.03480526804924011, 'motion_component_percent': 92.67662763595581}, {'resid': 1313, 'atom': 'H11B', 'charge': 0.09000000357627869, 'distance': 26.9195499420166, 'force': [-0.033400338143110275, -0.017198067158460617, 0.016994256526231766], 'magnitude': 0.04123300686478615, 'cosine_with_motion': 0.9390354752540588, 'motion_component': 0.03871925547719002, 'motion_component_percent': 93.90354752540588}, {'resid': 1313, 'atom': 'H11X', 'charge': 0.09000000357627869, 'distance': 25.913667678833008, 'force': [-0.03741530701518059, -0.022495651617646217, -0.008599498309195042], 'magnitude': 0.044496189802885056, 'cosine_with_motion': 0.5754884481430054, 'motion_component': 0.025607042014598846, 'motion_component_percent': 57.54884481430054}, {'resid': 1313, 'atom': 'H11Y', 'charge': 0.09000000357627869, 'distance': 25.818937301635742, 'force': [-0.0391695499420166, -0.02022446319460869, -0.008114578202366829], 'magnitude': 0.044823307543992996, 'cosine_with_motion': 0.581657886505127, 'motion_component': 0.026071829721331596, 'motion_component_percent': 58.165788650512695}, {'resid': 1313, 'atom': 'H12', 'charge': 0.09000000357627869, 'distance': 26.99422836303711, 'force': [-0.03497808054089546, -0.01624063029885292, 0.013935613445937634], 'magnitude': 0.04100519046187401, 'cosine_with_motion': 0.9063506722450256, 'motion_component': 0.0371650829911232, 'motion_component_percent': 90.63506722450256}, {'resid': 1313, 'atom': 'H121', 'charge': 0.15000000596046448, 'distance': 23.742795944213867, 'force': [-0.0867665708065033, -0.011929657310247421, 0.011554078198969364], 'magnitude': 0.08834167569875717, 'cosine_with_motion': 0.7335736155509949, 'motion_component': 0.06480512022972107, 'motion_component_percent': 73.35736155509949}, {'resid': 1313, 'atom': 'H12X', 'charge': 0.09000000357627869, 'distance': 23.2597713470459, 'force': [-0.048462845385074615, -0.024974098429083824, -0.008827529847621918], 'magnitude': 0.05522932484745979, 'cosine_with_motion': 0.5988595485687256, 'motion_component': 0.03307460993528366, 'motion_component_percent': 59.88595485687256}, {'resid': 1313, 'atom': 'H12Y', 'charge': 0.09000000357627869, 'distance': 23.392349243164062, 'force': [-0.04592472314834595, -0.028116824105381966, -0.009059657342731953], 'magnitude': 0.054605066776275635, 'cosine_with_motion': 0.5982607007026672, 'motion_component': 0.032668065279722214, 'motion_component_percent': 59.826070070266724}, {'resid': 1313, 'atom': 'H13A', 'charge': 0.09000000357627869, 'distance': 27.925752639770508, 'force': [-0.031761571764945984, -0.018167991191148758, 0.01136570144444704], 'magnitude': 0.038315173238515854, 'cosine_with_motion': 0.893782913684845, 'motion_component': 0.03424544632434845, 'motion_component_percent': 89.3782913684845}, {'resid': 1313, 'atom': 'H13B', 'charge': 0.09000000357627869, 'distance': 26.280336380004883, 'force': [-0.035424139350652695, -0.0212792307138443, 0.012807426042854786], 'magnitude': 0.043263211846351624, 'cosine_with_motion': 0.8944565653800964, 'motion_component': 0.03869706392288208, 'motion_component_percent': 89.44565653800964}, {'resid': 1313, 'atom': 'H13R', 'charge': 0.09000000357627869, 'distance': 25.559751510620117, 'force': [-0.04444948211312294, -0.006298224441707134, 0.00874333642423153], 'magnitude': 0.04573696479201317, 'cosine_with_motion': 0.770146906375885, 'motion_component': 0.03522418066859245, 'motion_component_percent': 77.0146906375885}, {'resid': 1313, 'atom': 'H13S', 'charge': 0.09000000357627869, 'distance': 25.929399490356445, 'force': [-0.042807649821043015, -0.009044568054378033, 0.007798163685947657], 'magnitude': 0.04444221407175064, 'cosine_with_motion': 0.7808287143707275, 'motion_component': 0.03470175713300705, 'motion_component_percent': 78.08287143707275}, {'resid': 1313, 'atom': 'H13X', 'charge': 0.09000000357627869, 'distance': 23.962055206298828, 'force': [-0.04522915184497833, -0.022081593051552773, -0.013222278095781803], 'magnitude': 0.05203942209482193, 'cosine_with_motion': 0.5174983739852905, 'motion_component': 0.026930315420031548, 'motion_component_percent': 51.74983739852905}, {'resid': 1313, 'atom': 'H13Y', 'charge': 0.09000000357627869, 'distance': 22.491479873657227, 'force': [-0.050232551991939545, -0.027038488537073135, -0.015313912183046341], 'magnitude': 0.059066955000162125, 'cosine_with_motion': 0.5162773728370667, 'motion_component': 0.0304949339479208, 'motion_component_percent': 51.627737283706665}, {'resid': 1313, 'atom': 'H141', 'charge': 0.15000000596046448, 'distance': 23.247333526611328, 'force': [-0.08801519870758057, -0.018781431019306183, 0.019792063161730766], 'magnitude': 0.09214739501476288, 'cosine_with_motion': 0.8032620549201965, 'motion_component': 0.07401850819587708, 'motion_component_percent': 80.32620549201965}, {'resid': 1313, 'atom': 'H14X', 'charge': 0.09000000357627869, 'distance': 24.296720504760742, 'force': [-0.04140184447169304, -0.02408088557422161, -0.01636911928653717], 'magnitude': 0.05061570927500725, 'cosine_with_motion': 0.45984968543052673, 'motion_component': 0.023275617510080338, 'motion_component_percent': 45.98496854305267}, {'resid': 1313, 'atom': 'H14Y', 'charge': 0.09000000357627869, 'distance': 25.319988250732422, 'force': [-0.03844614326953888, -0.023120282217860222, -0.012632647529244423], 'magnitude': 0.04660726338624954, 'cosine_with_motion': 0.5083779692649841, 'motion_component': 0.023694105446338654, 'motion_component_percent': 50.83779692649841}, {'resid': 1313, 'atom': 'H151', 'charge': 0.15000000596046448, 'distance': 23.890975952148438, 'force': [-0.08068130910396576, -0.020908605307340622, 0.025802792981266975], 'magnitude': 0.08724922686815262, 'cosine_with_motion': 0.8554304838180542, 'motion_component': 0.07463564723730087, 'motion_component_percent': 85.54304838180542}, {'resid': 1313, 'atom': 'H15X', 'charge': 0.09000000357627869, 'distance': 22.740198135375977, 'force': [-0.045204512774944305, -0.031882818788290024, -0.01669703610241413], 'magnitude': 0.05778194218873978, 'cosine_with_motion': 0.49309536814689636, 'motion_component': 0.02849200740456581, 'motion_component_percent': 49.309536814689636}, {'resid': 1313, 'atom': 'H15Y', 'charge': 0.09000000357627869, 'distance': 23.719934463500977, 'force': [-0.04237094521522522, -0.029628269374370575, -0.012134508229792118], 'magnitude': 0.05310722813010216, 'cosine_with_motion': 0.5466131567955017, 'motion_component': 0.029029108583927155, 'motion_component_percent': 54.66131567955017}, {'resid': 1313, 'atom': 'H16R', 'charge': 0.09000000357627869, 'distance': 26.72824478149414, 'force': [-0.03931371122598648, -0.009286848828196526, 0.010841937735676765], 'magnitude': 0.04182536527514458, 'cosine_with_motion': 0.8322083950042725, 'motion_component': 0.03480742126703262, 'motion_component_percent': 83.22083950042725}, {'resid': 1313, 'atom': 'H16S', 'charge': 0.09000000357627869, 'distance': 26.319955825805664, 'force': [-0.03954117000102997, -0.011580022051930428, 0.012761666439473629], 'magnitude': 0.04313306510448456, 'cosine_with_motion': 0.862420916557312, 'motion_component': 0.037198856472969055, 'motion_component_percent': 86.2420916557312}, {'resid': 1313, 'atom': 'H16X', 'charge': 0.09000000357627869, 'distance': 24.833810806274414, 'force': [-0.036432985216379166, -0.027262812480330467, -0.01663670688867569], 'magnitude': 0.048450008034706116, 'cosine_with_motion': 0.44177424907684326, 'motion_component': 0.02140396647155285, 'motion_component_percent': 44.177424907684326}, {'resid': 1313, 'atom': 'H16Y', 'charge': 0.09000000357627869, 'distance': 23.93084144592285, 'force': [-0.03833596035838127, -0.03149028867483139, -0.016154693439602852], 'magnitude': 0.052175264805555344, 'cosine_with_motion': 0.47132405638694763, 'motion_component': 0.024591457098722458, 'motion_component_percent': 47.13240563869476}, {'resid': 1313, 'atom': 'H17R', 'charge': 0.09000000357627869, 'distance': 27.533035278320312, 'force': [-0.03620672598481178, -0.008146679028868675, 0.01327873207628727], 'magnitude': 0.03941598907113075, 'cosine_with_motion': 0.8667881488800049, 'motion_component': 0.034165311604738235, 'motion_component_percent': 86.67881488800049}, {'resid': 1313, 'atom': 'H17S', 'charge': 0.09000000357627869, 'distance': 26.234725952148438, 'force': [-0.0392143577337265, -0.009331213310360909, 0.01612197980284691], 'magnitude': 0.04341377317905426, 'cosine_with_motion': 0.8847541809082031, 'motion_component': 0.03841051831841469, 'motion_component_percent': 88.47541809082031}, {'resid': 1313, 'atom': 'H17X', 'charge': 0.09000000357627869, 'distance': 26.714454650878906, 'force': [-0.03102816827595234, -0.02507045678794384, -0.012716165743768215], 'magnitude': 0.041868556290864944, 'cosine_with_motion': 0.47726574540138245, 'motion_component': 0.01998242735862732, 'motion_component_percent': 47.726574540138245}, {'resid': 1313, 'atom': 'H17Y', 'charge': 0.09000000357627869, 'distance': 26.38319206237793, 'force': [-0.0335984006524086, -0.024041427299380302, -0.011655283160507679], 'magnitude': 0.042926546186208725, 'cosine_with_motion': 0.5087178349494934, 'motion_component': 0.021837500855326653, 'motion_component_percent': 50.87178349494934}, {'resid': 1313, 'atom': 'H18R', 'charge': 0.09000000357627869, 'distance': 25.2016544342041, 'force': [-0.043749891221523285, -0.00653818529099226, 0.016016347333788872], 'magnitude': 0.047045979648828506, 'cosine_with_motion': 0.848587155342102, 'motion_component': 0.03992261365056038, 'motion_component_percent': 84.8587155342102}, {'resid': 1313, 'atom': 'H18S', 'charge': 0.09000000357627869, 'distance': 26.64111</t>
+          <t>{900: {'frame': 900, 'motion_vector': [-0.10789871215820312, -0.40692901611328125, 0.30049896240234375], 'motion_vector_magnitude': 0.5172358751296997, 'ionic_force': [-0.3772927224636078, -0.9863015711307526, 0.1931312084197998], 'ionic_force_magnitude': 1.073517699576809, 'radial_force': 1.056002172175319, 'axial_force': 0.1931312084197998, 'glu_force': [1.0836964549269292, -0.4140640135370064, -6.0729958246576405], 'glu_force_magnitude': 6.182808851973082, 'asn_force': [0.21170830633948057, -0.24680387799194037, 0.10385699331562537], 'asn_force_magnitude': 0.341348555329525, 'sf_force': [-10.820608677178974, 7.172259086665558, 9.646289462732797], 'sf_force_magnitude': 16.173366160132755, 'residue_force': [-9.525203915912567, 6.511391195136613, 3.6771506313907802], 'residue_force_magnitude': 12.109878682371527, 'pip2_force': [0.49183042690526857, -0.0003565226072937966, -3.977347450844225], 'pip2_force_magnitude': 4.007641456102983, 'total_force': [-9.410666211470906, 5.524733101398567, -0.10706561103364498], 'total_force_magnitude': 10.913055366416648, 'cosine_total_motion': -0.22409794066701608, 'cosine_glu_motion': -0.5545278312458517, 'cosine_asn_motion': 0.6162150494520675, 'cosine_sf_motion': 0.13718687366050125, 'cosine_residue_motion': -0.08252947473117336, 'cosine_pip2_motion': -0.6021100770712579, 'cosine_ionic_motion': 0.9006558523483511, 'motion_component_total': -2.4455932339990993, 'motion_component_glu': -3.428539583692287, 'motion_component_asn': 0.21034411690277507, 'motion_component_sf': 2.2187735400751585, 'motion_component_residue': -0.9994219267143559, 'motion_component_ionic': 0.966869998723392, 'motion_component_pip2': -2.4130413060081355, 'motion_component_percent_total': np.float64(22.409794066701608), 'motion_component_percent_glu': np.float64(55.45278312458517), 'motion_component_percent_asn': np.float64(61.62150494520675), 'motion_component_percent_sf': np.float64(13.718687366050125), 'motion_component_percent_residue': np.float64(8.252947473117336), 'motion_component_percent_ionic': np.float64(90.06558523483511), 'motion_component_percent_pip2': np.float64(60.21100770712579), 'ionic_contributions': [{'ion_id': 2333, 'distance': 6.926368236541748, 'force': [-1.8060075044631958, -0.864895761013031, 6.624295711517334], 'magnitude': 6.920332431793213, 'cosine_ionic_motion': 0.708884060382843, 'motion_component_ionic': 4.9057135581970215, 'motion_component_percent_ionic': 70.8884048461914}, {'ion_id': 2334, 'distance': 11.763495445251465, 'force': [0.42012912034988403, 0.16894248127937317, -2.3560731410980225], 'magnitude': 2.39919376373291, 'cosine_ionic_motion': -0.6624578833580017, 'motion_component_ionic': -1.589364767074585, 'motion_component_percent_ionic': 66.24578857421875}, {'ion_id': 2343, 'distance': 6.220857620239258, 'force': [2.2641780376434326, 1.203137993812561, -8.186910629272461], 'magnitude': 8.579017639160156, 'cosine_ionic_motion': -0.7198064923286438, 'motion_component_ionic': -6.175232410430908, 'motion_component_percent_ionic': 71.98065185546875}, {'ion_id': 2372, 'distance': 9.070656776428223, 'force': [0.23220226168632507, -3.1571826934814453, 2.5021557807922363], 'magnitude': 4.035158634185791, 'cosine_ionic_motion': 0.9638074040412903, 'motion_component_ionic': 3.889115810394287, 'motion_component_percent_ionic': 96.3807373046875}, {'ion_id': 2397, 'distance': 10.983990669250488, 'force': [-1.4877946376800537, 1.6636964082717896, 1.609663486480713], 'magnitude': 2.7518057823181152, 'cosine_ionic_motion': -0.023025544360280037, 'motion_component_ionic': -0.06336182355880737, 'motion_component_percent_ionic': 2.3025543689727783}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 9.794252395629883, 'force': [-1.6912314364657115, -0.5363449305728168, -0.21223404431586543], 'magnitude': 1.786889181177082, 'cosine_with_motion': 0.36457925767206445, 'motion_component': 0.6514627312157836, 'motion_component_percent': 36.45792576720645}, {'resid': 98, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 10.564867973327637, 'force': [0.839856165166355, 0.2321867460564613, 0.0582473184474808], 'magnitude': 0.8733051089502142, 'cosine_with_motion': -0.371038092338973, 'motion_component': -0.3240294616547664, 'motion_component_percent': 37.1038092338973}, {'resid': 98, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 9.753364562988281, 'force': [0.12948033267208428, 0.033877143145394154, 0.03583917483159748], 'magnitude': 0.1385541909477189, 'cosine_with_motion': -0.23702884019116058, 'motion_component': -0.03284133918396241, 'motion_component_percent': 23.70288401911606}, {'resid': 98, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 9.974266052246094, 'force': [0.3286353961173335, 0.12000001443910166, 0.11653048938037082], 'magnitude': 0.36875545013166927, 'cosine_with_motion': -0.2583370013631268, 'motion_component': -0.09526317722332549, 'motion_component_percent': 25.833700136312682}, {'resid': 98, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 11.158337593078613, 'force': [0.14054687996821183, 0.02843141434994795, 0.04166092792723658], 'magnitude': 0.14932315194401627, 'cosine_with_motion': -0.18405225143852202, 'motion_component': -0.02748326230719271, 'motion_component_percent': 18.405225143852203}, {'resid': 98, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 11.890153884887695, 'force': [-0.03781662116647783, -0.010442535492399685, -0.010553104842827026], 'magnitude': 0.04062648650551295, 'cosine_with_motion': 0.24548714754085468, 'motion_component': 0.0099732802868454, 'motion_component_percent': 24.54871475408547}, {'resid': 98, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 11.384324073791504, 'force': [-0.04277759304901171, -0.004823325593379556, -0.010526327849482842], 'magnitude': 0.044316932597387684, 'cosine_with_motion': 0.14899231887202333, 'motion_component': 0.006602882552979951, 'motion_component_percent': 14.899231887202333}, {'resid': 98, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 11.482601165771484, 'force': [0.030951320350730154, 0.004759316736403936, 0.013859321535726147], 'magnitude': 0.03424494299428136, 'cosine_with_motion': -0.06275718427772363, 'motion_component': -0.002149116198072256, 'motion_component_percent': 6.275718427772363}, {'resid': 98, 'resname': 'GLU', 'atom': 'HG2', 'charge': -0.042500000447034836, 'distance': 12.534331321716309, 'force': [-0.0818327128359716, -0.01065816558487243, -0.03543507047761366], 'magnitude': 0.08980998610111571, 'cosine_with_motion': 0.05421743004866332, 'motion_component': 0.004869266639108666, 'motion_component_percent': 5.421743004866332}, {'resid': 98, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 11.010310173034668, 'force': [-0.1051160028891296, -0.006313083125582573, -0.04957990290102906], 'magnitude': 0.11639328096420981, 'cosine_with_motion': -0.01640872882140244, 'motion_component': -0.0019098657839750216, 'motion_component_percent': 1.640872882140244}, {'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 11.32984733581543, 'force': [1.7541444257403496, 0.45471198073341057, 1.0273020176160537], 'magnitude': 2.083059069536065, 'cosine_with_motion': -0.06088754062457841, 'motion_component': -0.12683234371977364, 'motion_component_percent': 6.0887540624578405}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 10.929491996765137, 'force': [-1.8186182974258203, -0.399683925633789, -1.3083246616096158], 'magnitude': 2.275704983585953, 'cosine_with_motion': -0.02912354763188504, 'motion_component': -0.06627660248558366, 'motion_component_percent': 2.912354763188504}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 11.783027648925781, 'force': [-1.6012701307782764, -0.6193185470273533, -0.941252210232158], 'magnitude': 1.957952302197802, 'cosine_with_motion': 0.14016502012929455, 'motion_component': 0.27443642384975353, 'motion_component_percent': 14.016502012929454}, {'resid': 98, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 8.622139930725098, 'force': [2.243343121435748, 0.37492584570387505, 0.7546906297972329], 'magnitude': 2.396396398130659, 'cosine_with_motion': -0.13540782032451862, 'motion_component': -0.32449081290439985, 'motion_component_percent': 13.540782032451862}, {'resid': 98, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 8.028939247131348, 'force': [-2.6358951862885744, -0.6077114578016181, -1.2899855704603296], 'magnitude': 2.9968849529200328, 'cosine_with_motion': 0.09293989755182026, 'motion_component': 0.27853018049897954, 'motion_component_percent': 9.293989755182027}, {'resid': 426, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 9.179295539855957, 'force': [1.9888111871948408, 0.4204380919628747, 0.07976194494200896], 'magnitude': 2.034330380087184, 'cosine_with_motion': -0.3437563090849686, 'motion_component': -0.6993139029181917, 'motion_component_percent': 34.37563090849686}, {'resid': 426, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 9.865439414978027, 'force': [-0.9835382134209263, -0.1596321104905322, -0.10109319855855749], 'magnitude': 1.0015236705908097, 'cosine_with_motion': 0.2716149230846442, 'motion_component': 0.2720287747549733, 'motion_component_percent': 27.161492308464418}, {'resid': 426, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 9.253471374511719, 'force': [-0.15103134374319496, -0.02404802712102654, 0.0174707837291117], 'magnitude': 0.1539285635786878, 'cosine_with_motion': 0.39353067337656605, 'motion_component': 0.06057561127700858, 'motion_component_percent': 39.353067337656604}, {'resid': 426, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 9.538516998291016, 'force': [-0.384478143019102, -0.10067015889359553, 0.06801389797855972], 'magnitude': 0.4032168320758904, 'cosine_with_motion': 0.4933318554278778, 'motion_component': 0.19891970790775002, 'motion_component_percent': 49.333185542787774}, {'resid': 426, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 10.51595401763916, 'force': [-0.16642018210231743, -0.011538756262658963, 0.020898310513247385], 'magnitude': 0.1681236428625244, 'cosine_with_motion': 0.3327051282200409, 'motion_component': 0.055935598155396546, 'motion_component_percent': 33.270512822004086}, {'resid': 426, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 11.411300659179688, 'force': [0.043580503796232954, 0.005245314393332241, -0.004325592623034903], 'magnitude': 0.04410764543431022, 'cosine_with_motion': -0.35664796258412396, 'motion_component': -0.015730901878529678, 'motion_component_percent': 35.664796258412395}, {'resid': 426, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 10.471868515014648, 'force': [0.05228685502324891, -0.0005432565611477574, -0.0030132584934193653], 'magnitude': 0.05237642659309284, 'cosine_with_motion': -0.2335132000434727, 'motion_component': -0.012230586980595152, 'motion_component_percent': 23.35132000434727}, {'resid': 426, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 10.749743461608887, 'force': [-0.037813332049282986, -0.0005066676826987014, 0.009829693719373651], 'magnitude': 0.03907336268388884, 'cosine_with_motion': 0.35823593588214225, 'motion_component': 0.013997482649125294, 'motion_component_percent': 35.82359358821422}, {'resid': 426, 'resname': 'GLU', 'atom': 'HG2', 'charge': -0.042500000447034836, 'distance': 11.772629737854004, 'force': [0.0985750757819855, -0.0020783278067231874, -0.02536562270040041], 'magnitude': 0.10180756271945347, 'cosine_with_motion': -0.33067266993751665, 'motion_component': -0.033664978584272864, 'motion_component_percent': 33.067266993751666}, {'resid': 426, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 10.072225570678711, 'force': [0.1331052573985167, -0.008612485631152232, -0.039409155958626756], 'magnitude': 0.1390836655730771, 'cosine_with_motion': -0.3155396368571755, 'motion_component': -0.043886409327693596, 'motion_component_percent': 31.55396368571755}, {'resid': 426, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 10.974818229675293, 'force': [-2.061354363289968, -0.2347083036954666, 0.7900491628910711], 'magnitude': 2.2200106933668304, 'cosine_with_motion': 0.4836287983899193, 'motion_component': 1.0736611040457718, 'motion_component_percent': 48.36287983899193}, {'resid': 426, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 10.883970260620117, 'force': [2.0418802809363505, 0.13817179879856956, -1.0381001666618361], 'magnitude': 2.2947807049222098, 'cosine_with_motion': -0.4958034386874668, 'motion_component': -1.1377601645340807, 'motion_component_percent': 49.58034386874668}, {'resid': 426, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 11.393671035766602, 'force': [1.9280212020691403, 0.42984376168444305, -0.6950140711214874], 'magnitude': 2.0940572996324693, 'cosine_with_motion': -0.5463817918592405, 'motion_component': -1.1441547796291112, 'motion_component_percent': 54.63817918592405}, {'resid': 426, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 8.017501831054688, 'force': [-2.7082841228504257, -0.22946335060595138, 0.5418543619423193], 'magnitude': 2.7714729782032745, 'cosine_with_motion': 0.38257434031782367, 'motion_component': 1.0602944463447919, 'motion_component_percent': 38.25743403178237}, {'resid': 426, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 7.816900730133057, 'force': [2.952436183503714, 0.34288105275400904, -1.0778421502975317], 'magnitude': 3.1616752734836133, 'cosine_with_motion': -0.4781798434169941, 'motion_component': -1.5118493872097762, 'motion_component_percent': 47.81798434169941}, {'resid': 754, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 9.490715026855469, 'force': [-0.49991818264340426, 1.8354018384352946, -0.05339140806470599], 'magnitude': 1.9030156962895168, 'cosine_with_motion': -0.7202845086264466, 'motion_component': -1.3707127257103098, 'motion_component_percent': 72.02845086264466}, {'resid': 754, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 10.18281078338623, 'force': [0.20786038458209863, -0.9162639340426555, -0.03131064547116315], 'magnitude': 0.9400669618839727, 'cosine_with_motion': 0.701341416840595, 'motion_component': 0.659307894972739, 'motion_component_percent': 70.1341416840595}, {'resid': 754, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 9.569018363952637, 'force': [0.029366662192606263, -0.13870477418194074, 0.024869406672579995], 'magnitude': 0.14394409545877174, 'cosine_with_motion': 0.8159182542189619, 'motion_component': 0.11744661507184864, 'motion_component_percent': 81.59182542189619}, {'resid': 754, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 9.79934024810791, 'force': [0.11114156696529708, -0.35475342255563147, 0.08803788930602856], 'magnitude': 0.3820380984612616, 'cosine_with_motion': 0.8037432185040205, 'motion_component': 0.3070605308484103, 'motion_component_percent': 80.37432185040205}, {'resid': 754, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 10.837307929992676, 'force': [0.019498976494413678, -0.1545420052645472, 0.028208621428201575], 'magnitude': 0.15830087744038762, 'cosine_with_motion': 0.845887996522876, 'motion_component': 0.13390481206586283, 'motion_component_percent': 84.5887996522876}, {'resid': 754, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 11.671006202697754, 'force': [-0.007629881870493557, 0.04095177628133637, -0.006538425761399013], 'magnitude': 0.04216650435347513, 'cosine_with_motion': -0.8164134865379614, 'motion_component': -0.03442530283433876, 'motion_component_percent': 81.64134865379614}, {'resid': 754, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 10.82571792602539, 'force': [-0.0024781757371516566, 0.04864537727604569, -0.005414056405201818], 'magnitude': 0.04900842878599289, 'cosine_with_motion': -0.8345422125169447, 'motion_component': -0.040899602591041626, 'motion_component_percent': 83.45422125169448}, {'resid': 754, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 11.212655067443848, 'force': [0.0015855354820513375, -0.034436666155207345, 0.010069537521670203], 'magnitude': 0.03591369494427399, 'cosine_with_motion': 0.9080653405618201, 'motion_component': 0.032611981630405476, 'motion_component_percent': 90.806534056182}, {'resid': 754, 'resname': 'GLU', 'atom': 'HG2', 'charge': -0.042500000447034836, 'distance': 12.176896095275879, 'force': [-0.0009403598246794613, 0.09201342173495762, -0.024249680114769013], 'magnitude': 0.09515987096273126, 'cosine_with_motion': -0.9067123320215187, 'motion_component': -0.08628262851548486, 'motion_component_percent': 90.67123320215187}, {'resid': 754, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 10.634336471557617, 'force': [0.004458908696948805, 0.11865479407829693, -0.038320050901991594], 'magnitude': 0.12476885959910831, 'cosine_with_motion': -0.9340728157675191, 'motion_component': -0.11654320000584135, 'motion_component_percent': 93.40728157675191}, {'resid': 754, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 11.621997833251953, 'force': [0.2385413308065054, -1.8170539303678428, 0.7486134167171752], 'magnitude': 1.9796487062246995, 'cosine_with_motion': 0.9166809809747454, 'motion_component': 1.814706318007443, 'motion_component_percent': 91.66809809747454}, {'resid': 754, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 12.0017671585083, 'force': [-0.4141816541740321, 1.713002373634799, -0.6750736462028799], 'magnitude': 1.887232895678338, 'cosine_with_motion': -0.8761403395267304, 'motion_component': -1.6534808699856336, 'motion_component_percent': 87.61403395267304}, {'resid': 754, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 11.942201614379883, 'force': [-0.1270231554132009, 1.6900292613512808, -0.8723001043739056], 'magnitude': 1.9061063082434329, 'cosine_with_motion': -0.9495236244807177, 'motion_component': -1.8098929704488644, 'motion_component_percent': 94.95236244807177}, {'resid': 754, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 8.353270530700684, 'force': [0.30543989332748156, -2.461480571889178, 0.6052879180993856], 'magnitude': 2.5531458238848925, 'cosine_with_motion': 0.8712693550107334, 'motion_component': 2.224477715224538, 'motion_component_percent': 87.12693550107335}, {'resid': 754, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 7.96753454208374, 'force': [-0.45030735202013866, 2.79134774704702, -1.125615330369201], 'magnitude': 3.043256286971248, 'cosine_with_motion': -0.9056323879191852, 'motion_component': -2.7560714582198447, 'motion_component_percent': 90.56323879191852}, {'resid': 1082, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 9.237896919250488, 'force': [0.640062175090208, -1.9037895140209915, -0.019755420320341995], 'magnitude': 2.0086025934239764, 'cosine_with_motion': 0.6734954907279983, 'motion_component': 1.352784789335611, 'motion_component_percent': 67.34954907279983}, {'resid': 1082, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 10.092041015625, 'force': [-0.27128931372324255, 0.9172813610324976, -0.030790602113582356], 'magnitude': 0.9570533152424561, 'cosine_with_motion': -0.7136025394482601, 'motion_component': -0.6829556761443929, 'motion_component_percent': 71.36025394482601}, {'resid': 1082, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 9.300192832946777, 'force': [-0.04970381876446747, 0.1417574042543397, 0.025609060425514665], 'magnitude': 0.1523858761059468, 'cosine_with_motion': -0.5661893298223963, 'motion_component': -0.08627925706682474, 'motion_component_percent': 56.618932982239635}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 9.226442337036133, 'force': [-0.18598069639100628, 0.3802566992213221, 0.08085890659054511], 'magnitude': 0.43095491586452195, 'cosine_with_motion': -0.4951536305462004, 'motion_component': -0.21338889119205037, 'motion_component_percent': 49.51536305462004}, {'resid': 1082, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 10.684876441955566, 'force': [-0.04860004689727895, 0.15179539893482324, 0.033410122881350826], 'magnitude': 0.16284975900242166, 'cosine_with_motion': -0.5518865465377355, 'motion_component': -0.089874591100349, 'motion_component_percent': 55.18865465377355}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 11.272326469421387, 'force': [0.016393923938443314, -0.04155159828833118, -0.0069223702919127515], 'magnitude': 0.04520193881762891, 'cosine_with_motion': 0.5585742818276466, 'motion_component': 0.025248640512274288, 'motion_component_percent': 55.85742818276466}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 10.886266708374023, 'force': [0.010128615976905573, -0.046636208847887266, -0.008444524069498263], 'magnitude': 0.048464779212039344, 'cosine_with_motion': 0.6122291832096453, 'motion_component': 0.029671552191422642, 'motion_component_percent': 61.222918320964524}, {'resid': 1082, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 11.298821449279785, 'force': [-0.01065056872855115, 0.03168807376972864, 0.011546769689354665], 'magnitude': 0.03536801554704979, 'cosine_with_motion': -0.45238875209945734, 'motion_component': -0.01600009241756406, 'motion_component_percent': 45.23887520994573}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HG2', 'charge': -0.042500000447034836, 'distance': 12.345236778259277, 'force': [0.026400027358840818, -0.08398398679952808, -0.02865689219787967], 'magnitude': 0.09258233607838888, 'cosine_with_motion': 0.47435986294668503, 'motion_component': 0.043917344253428484, 'motion_component_percent': 47.4359862946685}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 10.925708770751953, 'force': [0.026511376237927146, -0.10620712021538732, -0.04459930983760719], 'magnitude': 0.1182028083104016, 'cosine_with_motion': 0.4409016713416817, 'motion_component': 0.05211581574133649, 'motion_component_percent': 44.09016713416817}, {'resid': 1082, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 11.188331604003906, 'force': [-0.8643322615861431, 1.76327437505995, 0.8406324604037971], 'magnitude': 2.136087477994807, 'cosine_with_motion': -0.3363843670720284, 'motion_component': -0.7185464342957686, 'motion_component_percent': 33.63843670720284}, {'resid': 1082, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 11.417867660522461, 'force': [0.7961703531430833, -1.630325447769397, -1.0277032618509665], 'magnitude': 2.08519118818577, 'cosine_with_motion': 0.24913150549471666, 'motion_component': 0.5194868199570379, 'motion_component_percent': 24.913150549471666}, {'resid': 1082, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 10.864042282104492, 'force': [1.1457785455858753, -1.835077095177901, -0.790219585177079], 'magnitude': 2.303207201614497, 'cosine_with_motion': 0.32372826186379067, 'motion_component': 0.7456132640908264, 'motion_component_percent': 32.372826186379065}, {'resid': 1082, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 8.280838012695312, 'force': [-0.6166286793127616, 2.432890197594569, 0.6711554034733834], 'magnitude': 2.5980060079442198, 'cosine_with_motion': -0.5371397467327629, 'motion_component': -1.3954922891173547, 'motion_component_percent': 53.71397467327629}, {'resid': 1082, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 7.981538772583008, 'force': [0.8558458203541431, -2.6566229028419, -1.1859439504901177], 'magnitude': 3.0325864158875815, 'cosine_with_motion': 0.4031317650143247, 'motion_component': 1.2225319143952256, 'motion_component_percent': 40.313176501432466}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'N', 'charge': -0.38210001587867737, 'distance': 14.684907913208008, 'force': [-0.30644213551715715, -0.11022571176500491, -0.48989665726910636], 'magnitude': 0.5882645873736255, 'cosine_with_motion': -0.22773960081746153, 'motion_component': -0.1339711423035182, 'motion_component_percent': 22.773960081746154}, {'resid': 130, 'resname': 'ASN', 'atom': 'H', 'charge': 0.2681000232696533, 'distance': 14.24600601196289, 'force': [0.23787968384980446, 0.10511493125956785, 0.35315208378697116], 'magnitude': 0.4385798525300341, 'cosine_with_motion': 0.16610417526079466, 'motion_component': 0.07284994469050227, 'motion_component_percent': 16.610417526079466}, {'resid': 130, 'resname': 'ASN', 'atom': 'CA', 'charge': -0.20800000429153442, 'distance': 14.188486099243164, 'force': [-0.15423413002753417, -0.05139477448368572, -0.3020570741110674], 'magnitude': 0.34302779148360285, 'cosine_with_motion': -0.29991129734454913, 'motion_component': -0.10287790996908282, 'motion_component_percent': 29.991129734454912}, {'resid': 130, 'resname': 'ASN', 'atom': 'HA', 'charge': 0.13580000400543213, 'distance': 13.974637985229492, 'force': [0.10831773436847286, 0.017658745993615284, 0.2031101781918267], 'magnitude': 0.2308642617944615, 'cosine_with_motion': 0.3530754919193582, 'motion_component': 0.081512512799679, 'motion_component_percent': 35.30754919193582}, {'resid': 130, 'resname': 'ASN', 'atom': 'CB', 'charge': -0.22990000247955322, 'distance': 12.925453186035156, 'force': [-0.1861232680291697, -0.08699308889144941, -0.4080609141118241], 'magnitude': 0.45686253735944604, 'cosine_with_motion': -0.28412097737633535, 'motion_component': -0.12980423064119834, 'motion_component_percent': 28.412097737633534}, {'resid': 130, 'resname': 'ASN', 'atom': 'HB2', 'charge': 0.1023000031709671, 'distance': 12.56251335144043, 'force': [0.09778635239443796, 0.05267624509293006, 0.18433124237497492], 'magnitude': 0.21520911789977995, 'cosine_with_motion': 0.21025978284650274, 'motion_component': 0.045249822396195134, 'motion_component_percent': 21.025978284650275}, {'resid': 130, 'resname': 'ASN', 'atom': 'HB3', 'charge': 0.1023000031709671, 'distance': 13.134596824645996, 'force': [0.06662754984135619, 0.04541128913888128, 0.1796009563035756], 'magnitude': 0.19687031031690977, 'cosine_with_motion': 0.27793528114287375, 'motion_component': 0.05471720504661512, 'motion_component_percent': 27.793528114287376}, {'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 11.912529945373535, 'force': [0.6746663872208002, 0.17444830040496992, 1.5214794702745347], 'magnitude': 1.6734714583842258, 'cosine_with_motion': 0.3620918571384696, 'motion_component': 0.6059503882345675, 'motion_component_percent': 36.209185713846956}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 11.88822078704834, 'force': [-0.4486495881478735, -0.08022210395112599, -1.3362295415201246], 'magnitude': 1.411818482149417, 'cosine_with_motion': -0.4388704722622673, 'motion_component': -0.619605444009512, 'motion_component_percent': 43.88704722622673}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 11.185317039489746, 'force': [-1.1751523878380365, -0.1618621204225067, -2.0984839334914787], 'magnitude': 2.410563689221046, 'cosine_with_motion': -0.3512334459234674, 'motion_component': -0.8466705911830942, 'motion_component_percent': 35.12334459234674}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 10.613048553466797, 'force': [0.585774431568365, -0.010270227239874282, 1.0737964217356821], 'magnitude': 1.223223576284873, 'cosine_with_motion': 0.41670883947462156, 'motion_component': 0.5097280768916657, 'motion_component_percent': 41.67088394746216}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 11.333580017089844, 'force': [0.5901923424335399, 0.12089531068814861, 0.8874698785295475], 'magnitude': 1.0726348225331968, 'cosine_with_motion': 0.27722696877265307, 'motion_component': 0.2973633004508708, 'motion_component_percent': 27.722696877265307}, {'resid': 458, 'resname': 'ASN', 'atom': 'N', 'charge': -0.38210001587867737, 'distance': 14.79377269744873, 'force': [0.4290003775642042, 0.01866155446265605, -0.38934724811130267], 'magnitude': 0.5796385573588395, 'cosine_with_motion': -0.5699644348361221, 'motion_component': -0.3303733627542561, 'motion_component_percent': 56.99644348361221}, {'resid': 458, 'resname': 'ASN', 'atom': 'H', 'charge': 0.2681000232696533, 'distance': 14.367311477661133, 'force': [-0.3214784333264229, -0.04037269739114818, 0.28453392949926365], 'magnitude': 0.4312051655823948, 'cosine_with_motion': 0.6125415828296222, 'motion_component': 0.26413109465014944, 'motion_component_percent': 61.25415828296222}, {'resid': 458, 'resname': 'ASN', 'atom': 'CA', 'charge': -0.20800000429153442, 'distance': 14.033319473266602, 'force': [0.2500669019855908, -0.016809727054512044, -0.24524118244888293], 'magnitude': 0.35065547188265084, 'cosine_with_motion': -0.5173701621052531, 'motion_component': -0.1814186783310211, 'motion_component_percent': 51.73701621052531}, {'resid': 458, 'resname': 'ASN', 'atom': 'HA', 'charge': 0.13580000400543213, 'distance': 14.483201026916504, 'force': [-0.15858570636880845, 0.02243098501170631, 0.1433346466337386], 'magnitude': 0.2149357957128315, 'cosine_with_motion': 0.459243820513455, 'motion_component': 0.09870793598826022, 'motion_component_percent': 45.9243820513455}, {'resid': 458, 'resname': 'ASN', 'atom': 'CB', 'charge': -0.22990000247955322, 'distance': 12.548372268676758, 'force': [0.3508086830985685, -0.012479048351910427, -0.33428022551578424], 'magnitude': 0.48473263553840146, 'cosine_with_motion': -0.5313656101831223, 'motion_component': -0.2575702526585357, 'motion_component_percent': 53.136561018312236}, {'resid': 458, 'resname': 'ASN', 'atom': 'HB2', 'charge': 0.1023000031709671, 'distance': 12.475196838378906, 'force': [-0.1704195073329009, 0.005147275871981465, 0.13622043088486224], 'magnitude': 0.21823223574657452, 'cosine_with_motion': 0.5069880608996924, 'motion_component': 0.11064113802696035, 'motion_component_percent': 50.69880608996924}, {'resid': 458, 'resname': 'ASN', 'atom': 'HB3', 'charge': 0.1023000031709671, 'distance': 12.34305191040039, 'force': [-0.15557571498640452, -0.011702725725303715, 0.1592389384967529], 'magnitude': 0.22293002582986732, 'cosine_with_motion': 0.6018670749716485, 'motion_component': 0.13417424256957627, 'motion_component_percent': 60.186707497164846}, {'resid': 458, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 11.720748901367188, 'force': [-1.1895035215348462, 0.20657456001908733, 1.2372373326545885], 'magnitude': 1.7286838617587428, 'cosine_with_motion': 0.4653348327009306, 'motion_component': 0.8044168156043032, 'motion_component_percent': 46.533483270093065}, {'resid': 458, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 11.923039436340332, 'force': [0.999869171817543, -0.29534140561038524, -0.9397259663966543], 'magnitude': 1.4035846246447496, 'cosine_with_motion': -0.3720304516010255, 'motion_component': -0.5221762217668421, 'motion_component_percent': 37.20304516010255}, {'resid': 458, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 11.022150993347168, 'force': [1.5473385791036198, -0.24580689072078693, -1.9256001718828981], 'magnitude': 2.4824612238388895, 'cosine_with_motion': -0.5027738810925133, 'motion_component': -1.2481166641711487, 'motion_component_percent': 50.27738810925133}, {'resid': 458, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 10.725323677062988, 'force': [-0.6925487711609511, 0.2064081033299143, 0.9551814708873327], 'magnitude': 1.1977477814144697, 'cosine_with_motion': 0.44835283171719936, 'motion_component': 0.5370136094801706, 'motion_component_percent': 44.83528317171994}, {'resid': 458, 'resname':</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>138</v>
+        <v>954</v>
       </c>
       <c r="B4" t="n">
-        <v>565</v>
+        <v>959</v>
       </c>
       <c r="C4" t="n">
-        <v>2398</v>
+        <v>2223</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>{138: {'frame': 138, 'motion_vector': [2.379444122314453, 2.9537811279296875, 5.88848876953125], 'ionic_force': [2.5273286402225494, -0.9714137520641088, -6.800560832023621], 'ionic_force_magnitude': 7.31974469250412, 'radial_force': 2.707588361141411, 'axial_force': -6.800560832023621, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [6.405253291130066, -6.760278880596161, 5.933797597885132], 'asn_force_magnitude': 11.042580957350252, 'residue_force': [6.405253291130066, -6.760278880596161, 5.933797597885132], 'residue_force_magnitude': 11.042580957350252, 'pip2_force': [0.8089091824367642, -0.1422158870846033, -4.736720594060898], 'pip2_force_magnitude': 4.807398611533102, 'total_force': [9.74149111378938, -7.873908519744873, -5.603483828199387], 'total_force_magnitude': 13.722030298401197, 'cosine_total_motion': -0.3441180815159799, 'cosine_glu_motion': 0, 'cosine_asn_motion': 0.3906295051309457, 'cosine_residue_motion': 0.3906295051309457, 'cosine_pip2_motion': -0.7836453243283775, 'cosine_ionic_motion': -0.7197329213971744, 'motion_component_total': -4.721998740789969, 'motion_component_glu': 0, 'motion_component_asn': 4.313557934738133, 'motion_component_residue': 4.313557934738133, 'motion_component_ionic': -5.268261231417452, 'motion_component_pip2': -3.76729544411065, 'motion_component_percent_total': 34.41180815159799, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 39.06295051309457, 'motion_component_percent_residue': 39.06295051309457, 'motion_component_percent_ionic': 71.97329213971744, 'motion_component_percent_pip2': 78.36453243283775, 'ionic_contributions': [{'ion_id': 2397, 'distance': 12.146998405456543, 'force': [0.2803648114204407, 0.018578680232167244, -2.2324788570404053], 'magnitude': 2.250091552734375, 'cosine_ionic_motion': -0.7882996797561646, 'motion_component_ionic': -1.7737464904785156, 'motion_component_percent_ionic': 78.82996797561646}, {'ion_id': 2399, 'distance': 13.916149139404297, 'force': [-0.06216016411781311, -0.06396990269422531, 1.7120298147201538], 'magnitude': 1.714351773262024, 'cosine_ionic_motion': 0.811498761177063, 'motion_component_ionic': 1.3911943435668945, 'motion_component_percent_ionic': 81.1498761177063}, {'ion_id': 2400, 'distance': 7.01064395904541, 'force': [2.309123992919922, -0.9260225296020508, -6.280111789703369], 'magnitude': 6.7549519538879395, 'cosine_ionic_motion': -0.7232781052589417, 'motion_component_ionic': -4.885708808898926, 'motion_component_percent_ionic': 72.32781052589417}], 'glu_contributions': [], 'asn_contributions': [{'resid': 458, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 5.213967323303223, 'force': [5.881892204284668, -0.6080090403556824, 4.347905158996582], 'magnitude': 7.339660167694092, 'cosine_with_motion': 0.7353169322013855, 'motion_component': 5.396976470947266, 'motion_component_percent': 73.53169322013855}, {'resid': 1114, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 5.594605922698975, 'force': [0.523361086845398, -6.1522698402404785, 1.5858924388885498], 'magnitude': 6.374903202056885, 'cosine_with_motion': -0.16995061933994293, 'motion_component': -1.0834187269210815, 'motion_component_percent': 16.995061933994293}], 'pip2_contributions': [{'resid': 1313, 'atom': 'C1', 'charge': 0.06000000238418579, 'distance': 24.402841567993164, 'force': [-0.022420506924390793, -0.02128113992512226, 0.012782823294401169], 'magnitude': 0.033450957387685776, 'cosine_with_motion': -0.17471742630004883, 'motion_component': -0.0058444649912416935, 'motion_component_percent': 17.471742630004883}, {'resid': 1313, 'atom': 'C11', 'charge': 0.17000000178813934, 'distance': 24.04247283935547, 'force': [-0.07392477244138718, -0.05795276537537575, 0.02664990723133087], 'magnitude': 0.09764022380113602, 'cosine_with_motion': -0.2780381143093109, 'motion_component': -0.027147704735398293, 'motion_component_percent': 27.80381143093109}, {'resid': 1313, 'atom': 'C12', 'charge': 0.04000000283122063, 'distance': 24.602930068969727, 'force': [-0.017247885465621948, -0.01263332273811102, 0.004924040753394365], 'magnitude': 0.021939383819699287, 'cosine_with_motion': -0.321213960647583, 'motion_component': -0.007047236431390047, 'motion_component_percent': 32.1213960647583}, {'resid': 1313, 'atom': 'C13', 'charge': -0.05000000074505806, 'distance': 25.780147552490234, 'force': [0.019319377839565277, 0.015033502131700516, -0.004959581885486841], 'magnitude': 0.024976829066872597, 'cosine_with_motion': 0.3496534824371338, 'motion_component': 0.00873323529958725, 'motion_component_percent': 34.96534824371338}, {'resid': 1313, 'atom': 'C2', 'charge': 0.06000000238418579, 'distance': 25.88208770751953, 'force': [-0.020231634378433228, -0.01853950135409832, 0.01145560946315527], 'magnitude': 0.029736561700701714, 'cosine_with_motion': -0.17017745971679688, 'motion_component': -0.0050604925490915775, 'motion_component_percent': 17.017745971679688}, {'resid': 1313, 'atom': 'C21', 'charge': 0.6299999952316284, 'distance': 22.660926818847656, 'force': [-0.333642840385437, -0.22080835700035095, 0.07632959634065628], 'magnitude': 0.40730834007263184, 'cosine_with_motion': -0.349338561296463, 'motion_component': -0.14228850603103638, 'motion_component_percent': 34.9338561296463}, {'resid': 1313, 'atom': 'C210', 'charge': -0.18000000715255737, 'distance': 22.375221252441406, 'force': [0.1032874658703804, 0.055836427956819534, 0.021492497995495796], 'magnitude': 0.11936471611261368, 'cosine_with_motion': 0.6425926685333252, 'motion_component': 0.07670289278030396, 'motion_component_percent': 64.25926685333252}, {'resid': 1313, 'atom': 'C211', 'charge': -0.15000000596046448, 'distance': 22.10381507873535, 'force': [0.09119110554456711, 0.04141058027744293, 0.01894017867743969], 'magnitude': 0.10192832350730896, 'cosine_with_motion': 0.6314677596092224, 'motion_component': 0.06436444818973541, 'motion_component_percent': 63.14677596092224}, {'resid': 1313, 'atom': 'C212', 'charge': -0.15000000596046448, 'distance': 21.817134857177734, 'force': [0.09611354768276215, 0.03859924152493477, 0.014785009436309338], 'magnitude': 0.10462462157011032, 'cosine_with_motion': 0.5864573121070862, 'motion_component': 0.06135787442326546, 'motion_component_percent': 58.64573121070862}, {'resid': 1313, 'atom': 'C213', 'charge': -0.18000000715255737, 'distance': 21.773134231567383, 'force': [0.11609593033790588, 0.04831179231405258, 0.008843266405165195], 'magnitude': 0.12605752050876617, 'cosine_with_motion': 0.5334609746932983, 'motion_component': 0.06724676489830017, 'motion_component_percent': 53.346097469329834}, {'resid': 1313, 'atom': 'C214', 'charge': -0.15000000596046448, 'distance': 20.334096908569336, 'force': [0.11114843189716339, 0.046035829931497574, 0.005754346027970314], 'magnitude': 0.1204424500465393, 'cosine_with_motion': 0.5148470401763916, 'motion_component': 0.06200943887233734, 'motion_component_percent': 51.48470401763916}, {'resid': 1313, 'atom': 'C215', 'charge': -0.15000000596046448, 'distance': 19.97473907470703, 'force': [0.11644329875707626, 0.044913630932569504, -0.0015918146818876266], 'magnitude': 0.12481509894132614, 'cosine_with_motion': 0.4579499661922455, 'motion_component': 0.057159069925546646, 'motion_component_percent': 45.79499661922455}, {'resid': 1313, 'atom': 'C216', 'charge': -0.18000000715255737, 'distance': 20.867338180541992, 'force': [0.12942864000797272, 0.0448644794523716, -0.008357933722436428], 'magnitude': 0.13723866641521454, 'cosine_with_motion': 0.4070381820201874, 'motion_component': 0.055861376225948334, 'motion_component_percent': 40.70381820201874}, {'resid': 1313, 'atom': 'C217', 'charge': -0.18000000715255737, 'distance': 20.195837020874023, 'force': [0.13907866179943085, 0.04271954670548439, -0.017299873754382133], 'magnitude': 0.1465166211128235, 'cosine_with_motion': 0.3461562395095825, 'motion_component': 0.05071764439344406, 'motion_component_percent': 34.61562395095825}, {'resid': 1313, 'atom': 'C218', 'charge': -0.18000000715255737, 'distance': 21.173826217651367, 'force': [0.12575942277908325, 0.03788851201534271, -0.022725019603967667], 'magnitude': 0.13329440355300903, 'cosine_with_motion': 0.297047883272171, 'motion_component': 0.03959482163190842, 'motion_component_percent': 29.704788327217102}, {'resid': 1313, 'atom': 'C219', 'charge': -0.18000000715255737, 'distance': 20.60798454284668, 'force': [0.1322927176952362, 0.03534434735774994, -0.03240450844168663], 'magnitude': 0.14071474969387054, 'cosine_with_motion': 0.23170205950737, 'motion_component': 0.03260389715433121, 'motion_component_percent': 23.170205950737}, {'resid': 1313, 'atom': 'C22', 'charge': -0.08000000566244125, 'distance': 21.92666244506836, 'force': [0.04579306021332741, 0.03011610172688961, -0.0069199902936816216], 'magnitude': 0.055243734270334244, 'cosine_with_motion': 0.4061806797981262, 'motion_component': 0.022438937798142433, 'motion_component_percent': 40.61806797981262}, {'resid': 1313, 'atom': 'C220', 'charge': -0.27000001072883606, 'distance': 21.737157821655273, 'force': [0.17669221758842468, 0.04554326832294464, -0.05192851275205612], 'magnitude': 0.18971268832683563, 'cosine_with_motion': 0.18751589953899384, 'motion_component': 0.03557414561510086, 'motion_component_percent': 18.751589953899384}, {'resid': 1313, 'atom': 'C23', 'charge': -0.18000000715255737, 'distance': 20.801536560058594, 'force': [0.11027947813272476, 0.08153290301561356, -0.016270292922854424], 'magnitude': 0.1381082832813263, 'cosine_with_motion': 0.421174556016922, 'motion_component': 0.05816769599914551, 'motion_component_percent': 42.1174556016922}, {'resid': 1313, 'atom': 'C24', 'charge': -0.18000000715255737, 'distance': 20.108715057373047, 'force': [0.11853664368391037, 0.08794492483139038, -0.0075054350309073925], 'magnitude': 0.14778897166252136, 'cosine_with_motion': 0.48072102665901184, 'motion_component': 0.07104526460170746, 'motion_component_percent': 48.072102665901184}, {'resid': 1313, 'atom': 'C25', 'charge': -0.15000000596046448, 'distance': 21.12590980529785, 'force': [0.08920259773731232, 0.06703309714794159, 0.0005030279862694442], 'magnitude': 0.11158312112092972, 'cosine_with_motion': 0.5287017226219177, 'motion_component': 0.05899418517947197, 'motion_component_percent': 52.87017226219177}, {'resid': 1313, 'atom': 'C26', 'charge': -0.15000000596046448, 'distance': 21.136337280273438, 'force': [0.09052691608667374, 0.06466934084892273, 0.006999703589826822], 'magnitude': 0.11147305369377136, 'cosine_with_motion': 0.5733129978179932, 'motion_component': 0.06390894949436188, 'motion_component_percent': 57.331299781799316}, {'resid': 1313, 'atom': 'C27', 'charge': -0.18000000715255737, 'distance': 20.118284225463867, 'force': [0.12313391268253326, 0.08028484135866165, 0.013872077688574791], 'magnitude': 0.1476484090089798, 'cosine_with_motion': 0.591598391532898, 'motion_component': 0.0873485580086708, 'motion_component_percent': 59.159839153289795}, {'resid': 1313, 'atom': 'C28', 'charge': -0.15000000596046448, 'distance': 20.349971771240234, 'force': [0.09935349225997925, 0.06463831663131714, 0.020296355709433556], 'magnitude': 0.12025460600852966, 'cosine_with_motion': 0.6492284536361694, 'motion_component': 0.07807271182537079, 'motion_component_percent': 64.92284536361694}, {'resid': 1313, 'atom': 'C29', 'charge': -0.15000000596046448, 'distance': 21.334993362426758, 'force': [0.09173980355262756, 0.055397652089595795, 0.022017236799001694], 'magnitude': 0.10940681397914886, 'cosine_with_motion': 0.6675648093223572, 'motion_component': 0.07303614169359207, 'motion_component_percent': 66.75648093223572}, {'resid': 1313, 'atom': 'C3', 'charge': 0.06000000238418579, 'distance': 26.375789642333984, 'force': [-0.01954292319715023, -0.016916828230023384, 0.012320205569267273], 'magnitude': 0.028633764013648033, 'cosine_with_motion': -0.11927808821201324, 'motion_component': -0.0034153806045651436, 'motion_component_percent': 11.927808821201324}, {'resid': 1313, 'atom': 'C31', 'charge': 0.6299999952316284, 'distance': 27.533588409423828, 'force': [-0.21990327537059784, -0.1620675027370453, 0.03870305418968201], 'magnitude': 0.27590081095695496, 'cosine_with_motion': -0.4005458652973175, 'motion_component': -0.1105109304189682, 'motion_component_percent': 40.05458652973175}, {'resid': 1313, 'atom': 'C310', 'charge': -0.18000000715255737, 'distance': 26.378376007080078, 'force': [0.06367551535367966, 0.05446280539035797, 0.01885124109685421], 'magnitude': 0.0858844444155693, 'cosine_with_motion': 0.7038129568099976, 'motion_component': 0.06044658273458481, 'motion_component_percent': 70.38129568099976}, {'resid': 1313, 'atom': 'C311', 'charge': -0.18000000715255737, 'distance': 26.79759407043457, 'force': [0.06133041903376579, 0.051465462893247604, 0.022697491571307182], 'magnitude': 0.08321832865476608, 'cosine_with_motion': 0.740455150604248, 'motion_component': 0.061619438230991364, 'motion_component_percent': 74.0455150604248}, {'resid': 1313, 'atom': 'C312', 'charge': -0.18000000715255737, 'distance': 27.45832633972168, 'force': [0.055643778294324875, 0.05150832608342171, 0.023087939247488976], 'magnitude': 0.07926153391599655, 'cosine_with_motion': 0.7574160099029541, 'motion_component': 0.06003395467996597, 'motion_component_percent': 75.74160099029541}, {'resid': 1313, 'atom': 'C313', 'charge': -0.18000000715255737, 'distance': 27.953580856323242, 'force': [0.05311553552746773, 0.048519477248191833, 0.025951147079467773], 'magnitude': 0.07647784799337387, 'cosine_with_motion': 0.7887478470802307, 'motion_component': 0.060321737080812454, 'motion_component_percent': 78.87478470802307}, {'resid': 1313, 'atom': 'C314', 'charge': -0.18000000715255737, 'distance': 28.83768081665039, 'force': [0.047449976205825806, 0.04746103286743164, 0.025688041001558304], 'magnitude': 0.07186045497655869, 'cosine_with_motion': 0.8033562898635864, 'motion_component': 0.05772954970598221, 'motion_component_percent': 80.33562898635864}, {'resid': 1313, 'atom': 'C315', 'charge': -0.18000000715255737, 'distance': 29.904394149780273, 'force': [0.04445531591773033, 0.04272693023085594, 0.025763316079974174], 'magnitude': 0.0668252557516098, 'cosine_with_motion': 0.819736659526825, 'motion_component': 0.054779112339019775, 'motion_component_percent': 81.9736659526825}, {'resid': 1313, 'atom': 'C316', 'charge': -0.18000000715255737, 'distance': 30.961219787597656, 'force': [0.03960398957133293, 0.04120268300175667, 0.024905338883399963], 'magnitude': 0.062341101467609406, 'cosine_with_motion': 0.8303830027580261, 'motion_component': 0.05176699161529541, 'motion_component_percent': 83.03830027580261}, {'resid': 1313, 'atom': 'C317', 'charge': -0.18000000715255737, 'distance': 32.03162384033203, 'force': [0.03698249161243439, 0.0374426506459713, 0.024954555556178093], 'magnitude': 0.05824419856071472, 'cosine_with_motion': 0.8469889163970947, 'motion_component': 0.04933219030499458, 'motion_component_percent': 84.69889163970947}, {'resid': 1313, 'atom': 'C318', 'charge': -0.27000001072883606, 'distance': 33.09305191040039, 'force': [0.049864139407873154, 0.054316502064466476, 0.03553872928023338], 'magnitude': 0.0818517878651619, 'cosine_with_motion': 0.8518084287643433, 'motion_component': 0.06972204148769379, 'motion_component_percent': 85.18084287643433}, {'resid': 1313, 'atom': 'C32', 'charge': -0.08000000566244125, 'distance': 28.054248809814453, 'force': [0.02776786871254444, 0.018834667280316353, -0.0036107683554291725], 'magnitude': 0.03374665603041649, 'cosine_with_motion': 0.42493635416030884, 'motion_component': 0.014340180903673172, 'motion_component_percent': 42.493635416030884}, {'resid': 1313, 'atom': 'C33', 'charge': -0.18000000715255737, 'distance': 27.763357162475586, 'force': [0.06357120722532272, 0.04419083520770073, -0.004084730986505747], 'magnitude': 0.0775294378399849, 'cosine_with_motion': 0.47462400794029236, 'motion_component': 0.036797333508729935, 'motion_component_percent': 47.462400794029236}, {'resid': 1313, 'atom': 'C34', 'charge': -0.18000000715255737, 'distance': 26.25332260131836, 'force': [0.07069101929664612, 0.05011456832289696, -0.002999091288074851], 'magnitude': 0.08670458197593689, 'cosine_with_motion': 0.49163225293159485, 'motion_component': 0.042626768350601196, 'motion_component_percent': 49.163225293159485}, {'resid': 1313, 'atom': 'C35', 'charge': -0.18000000715255737, 'distance': 26.383501052856445, 'force': [0.0700334683060646, 0.04961637780070305, 0.0019840041641145945], 'magnitude': 0.08585108071565628, 'cosine_with_motion': 0.5402674078941345, 'motion_component': 0.046382542699575424, 'motion_component_percent': 54.02674078941345}, {'resid': 1313, 'atom': 'C36', 'charge': -0.18000000715255737, 'distance': 25.057512283325195, 'force': [0.07743663340806961, 0.05513899773359299, 0.004693910479545593], 'magnitude': 0.09517759084701538, 'cosine_with_motion': 0.5621553063392639, 'motion_component': 0.0535045862197876, 'motion_component_percent': 56.21553063392639}, {'resid': 1313, 'atom': 'C37', 'charge': -0.18000000715255737, 'distance': 25.17207908630371, 'force': [0.07662482559680939, 0.05397293344140053, 0.010513661429286003], 'magnitude': 0.09431319683790207, 'cosine_with_motion': 0.611045777797699, 'motion_component': 0.05762968212366104, 'motion_component_percent': 61.1045777797699}, {'resid': 1313, 'atom': 'C38', 'charge': -0.18000000715255737, 'distance': 25.80702018737793, 'force': [0.07003919035196304, 0.0547550730407238, 0.012155810371041298], 'magnitude': 0.0897294282913208, 'cosine_with_motion': 0.6363893151283264, 'motion_component': 0.05710284784436226, 'motion_component_percent': 63.63893151283264}, {'resid': 1313, 'atom': 'C39', 'charge': -0.18000000715255737, 'distance': 25.790361404418945, 'force': [0.0696246400475502, 0.05397447198629379, 0.017645329236984253], 'magnitude': 0.08984537422657013, 'cosine_with_motion': 0.6817025542259216, 'motion_component': 0.061247821897268295, 'motion_component_percent': 68.17025542259216}, {'resid': 1313, 'atom': 'C4', 'charge': 0.08000000566244125, 'distance': 26.21433448791504, 'force': [-0.024888942018151283, -0.023258890956640244, 0.018259065225720406], 'magnitude': 0.03865008056163788, 'cosine_with_motion': -0.0753742977976799, 'motion_component': -0.002913222648203373, 'motion_component_percent': 7.53742977976799}, {'resid': 1313, 'atom': 'C5', 'charge': 0.08000000566244125, 'distance': 24.719451904296875, 'force': [-0.027550406754016876, -0.02643880434334278, 0.020766904577612877], 'magnitude': 0.04346607252955437, 'cosine_with_motion': -0.07017014920711517, 'motion_component': -0.003050020895898342, 'motion_component_percent': 7.017014920711517}, {'resid': 1313, 'atom': 'C6', 'charge': 0.06000000238418579, 'distance': 24.10930824279785, 'force': [-0.021670158952474594, -0.022014115005731583, 0.014840723015367985], 'magnitude': 0.034270454198122025, 'cosine_with_motion': -0.12163854390382767, 'motion_component': -0.004168608225882053, 'motion_component_percent': 12.163854390382767}, {'resid': 1313, 'atom': 'H1', 'charge': 0.12000000476837158, 'distance': 23.959632873535156, 'force': [-0.04838799312710762, -0.04197182506322861, 0.026708029210567474], 'magnitude': 0.06939993053674698, 'cosine_with_motion': -0.1683645099401474, 'motion_component': -0.011684484779834747, 'motion_component_percent': 16.83645099401474}, {'resid': 1313, 'atom': 'H10R', 'charge': 0.09000000357627869, 'distance': 22.654399871826172, 'force': [-0.0503530390560627, -0.028139790520071983, -0.007895772345364094], 'magnitude': 0.05822044238448143, 'cosine_with_motion': -0.6116417646408081, 'motion_component': -0.035610053688287735, 'motion_component_percent': 61.16417646408081}, {'resid': 1313, 'atom': 'H10S', 'charge': 0.09000000357627869, 'distance': 23.199026107788086, 'force': [-0.047447189688682556, -0.026391709223389626, -0.011601462960243225], 'magnitude': 0.05551893264055252, 'cosine_with_motion': -0.6664586067199707, 'motion_component': -0.03700106963515282, 'motion_component_percent': 66.64586067199707}, {'resid': 1313, 'atom': 'H10X', 'charge': 0.09000000357627869, 'distance': 25.809343338012695, 'force': [-0.03220544755458832, -0.02966183051466942, -0.009752064011991024], 'magnitude': 0.044856633991003036, 'cosine_with_motion': -0.7055269479751587, 'motion_component': -0.031647562980651855, 'motion_component_percent': 70.55269479751587}, {'resid': 1313, 'atom': 'H10Y', 'charge': 0.09000000357627869, 'distance': 27.297189712524414, 'force': [-0.029690125957131386, -0.025749001652002335, -0.007968570105731487], 'magnitude': 0.040100034326314926, 'cosine_with_motion': -0.6893672943115234, 'motion_component': -0.027643652632832527, 'motion_component_percent': 68.93672943115234}, {'resid': 1313, 'atom': 'H111', 'charge': 0.15000000596046448, 'distance': 22.09762191772461, 'force': [-0.09088128060102463, -0.03976454213261604, -0.02367294952273369], 'magnitude': 0.10198546200990677, 'cosine_with_motion': -0.662289023399353, 'motion_component': -0.06754384934902191, 'motion_component_percent': 66.2289023399353}, {'resid': 1313, 'atom': 'H11A', 'charge': 0.09000000357627869, 'distance': 24.88187026977539, 'force': [-0.036379072815179825, -0.028213350102305412, 0.01448756642639637], 'magnitude': 0.04826302453875542, 'cosine_with_motion': -0.2502231001853943, 'motion_component': -0.012076523154973984, 'motion_component_percent': 25.02231001853943}, {'resid': 1313, 'atom': 'H11B', 'charge': 0.09000000357627869, 'distance': 23.178268432617188, 'force': [-0.04250072315335274, -0.031956348568201065, 0.016306092962622643], 'magnitude': 0.055618416517972946, 'cosine_with_motion': -0.2554142475128174, 'motion_component': -0.014205736108124256, 'motion_component_percent': 25.54142475128174}, {'resid': 1313, 'atom': 'H11X', 'charge': 0.09000000357627869, 'distance': 27.51233673095703, 'force': [-0.02982335351407528, -0.023458512499928474, -0.010888819582760334], 'magnitude': 0.03947531804442406, 'cosine_with_motion': -0.7391459941864014, 'motion_component': -0.02917802333831787, 'motion_component_percent': 73.91459941864014}, {'resid': 1313, 'atom': 'H11Y', 'charge': 0.09000000357627869, 'distance': 25.961076736450195, 'force': [-0.03285747393965721, -0.026746319606900215, -0.013057917356491089], 'magnitude': 0.04433382675051689, 'cosine_with_motion': -0.7537985444068909, 'motion_component': -0.03341877460479736, 'motion_component_percent': 75.37985444068909}, {'resid': 1313, 'atom': 'H12', 'charge': 0.09000000357627869, 'distance': 24.953998565673828, 'force': [-0.03868640214204788, -0.025988509878516197, 0.011422136798501015], 'magnitude': 0.04798442870378494, 'cosine_with_motion': -0.3021645247936249, 'motion_component': -0.014499192126095295, 'motion_component_percent': 30.216452479362488}, {'resid': 1313, 'atom': 'H121', 'charge': 0.15000000596046448, 'distance': 21.802772521972656, 'force': [-0.0977754145860672, -0.03389129415154457, -0.016325855627655983], 'magnitude': 0.10476251691579819, 'cosine_with_motion': -0.5844879746437073, 'motion_component': -0.06123242899775505, 'motion_component_percent': 58.44879746437073}, {'resid': 1313, 'atom': 'H12X', 'charge': 0.09000000357627869, 'distance': 26.814260482788086, 'force': [-0.028241539373993874, -0.027993325144052505, -0.012075244449079037], 'magnitude': 0.04155745729804039, 'cosine_with_motion': -0.7592005729675293, 'motion_component': -0.03155044466257095, 'motion_component_percent': 75.92005729675293}, {'resid': 1313, 'atom': 'H12Y', 'charge': 0.09000000357627869, 'distance': 28.362220764160156, 'force': [-0.026039570569992065, -0.02449766919016838, -0.01007743552327156], 'magnitude': 0.0371449813246727, 'cosine_with_motion': -0.7443463802337646, 'motion_component': -0.02764873206615448, 'motion_component_percent': 74.43463802337646}, {'resid': 1313, 'atom': 'H13A', 'charge': 0.09000000357627869, 'distance': 26.420774459838867, 'force': [-0.03264874592423439, -0.025857795029878616, 0.009882310405373573], 'magnitude': 0.04280451312661171, 'cosine_with_motion': -0.3197685480117798, 'motion_component': -0.013687537051737309, 'motion_component_percent': 31.97685480117798}, {'resid': 1313, 'atom': 'H13B', 'charge': 0.09000000357627869, 'distance': 25.522319793701172, 'force': [-0.03454909101128578, -0.02902820147573948, 0.00823972001671791], 'magnitude': 0.045871224254369736, 'cosine_with_motion': -0.37171441316604614, 'motion_component': -0.01705099456012249, 'motion_component_percent': 37.171441316604614}, {'resid': 1313, 'atom': 'H13R', 'charge': 0.09000000357627869, 'distance': 22.43419647216797, 'force': [-0.055473849177360535, -0.020952580496668816, -0.0028839786536991596], 'magnitude': 0.059368982911109924, 'cosine_with_motion': -0.507089376449585, 'motion_component': -0.030105380341410637, 'motion_component_percent': 50.708937644958496}, {'resid': 1313, 'atom': 'H13S', 'charge': 0.09000000357627869, 'distance': 22.190671920776367, 'force': [-0.05479662865400314, -0.02578824944794178, -0.0037760513368993998], 'magnitude': 0.06067918241024017, 'cosine_with_motion': -0.5383149981498718, 'motion_component': -0.03266451507806778, 'motion_component_percent': 53.83149981498718}, {'resid': 1313, 'atom': 'H13X', 'charge': 0.09000000357627869, 'distance': 28.53708839416504, 'force': [-0.026252789422869682, -0.022354695945978165, -0.012541885487735271], 'magnitude': 0.036691147834062576, 'cosine_with_motion': -0.7873641848564148, 'motion_component': -0.02888929657638073, 'motion_component_percent': 78.73641848564148}, {'resid': 1313, 'atom': 'H13Y', 'charge': 0.09000000357627869, 'distance': 27.138227462768555, 'force': [-0.028070077300071716, -0.025308331474661827, -0.014750590547919273], 'magnitude': 0.0405711829662323, 'cosine_with_motion': -0.803749144077301, 'motion_component': -0.03260905295610428, 'motion_component_percent': 80.3749144077301}, {'resid': 1313, 'atom': 'H141', 'charge': 0.15000000596046448, 'distance': 19.557283401489258, 'force': [-0.11905485391616821, -0.05160800367593765, -0.01070986408740282], 'magnitude': 0.13020040094852448, 'cosine_with_motion': -0.5469354391098022, 'motion_component': -0.07121121138334274, 'motion_component_percent': 54.693543910980225}, {'resid': 1313, 'atom': 'H14X', 'charge': 0.09000000357627869, 'distance': 29.41438102722168, 'force': [-0.02283059060573578, -0.023293225094676018, -0.011351890861988068], 'magnitude': 0.034535136073827744, 'cosine_with_motion': -0.7853482961654663, 'motion_component': -0.02712211012840271, 'motion_component_percent': 78.53482961654663}, {'resid': 1313, 'atom': 'H14Y', 'charge': 0.09000000357627869, 'distance': 28.174394607543945, 'force': [-0.023991376161575317, -0.02541259117424488, -0.01398305781185627], 'magnitude': 0.03764189034700394, 'cosine_with_motion': -0.8135135769844055, 'motion_component': -0.03062218800187111, 'motion_component_percent': 81.35135769844055}, {'resid': 1313, 'atom': 'H151', 'charge': 0.15000000596046448, 'distance': 18.937761306762695, 'force': [-0.12922175228595734, -0.050669725984334946, 0.003995672333985567], 'magnitude': 0.1388583779335022, 'cosine_with_motion': -0.44582486152648926, 'motion_component': -0.061906516551971436, 'motion_component_percent': 44.582486152648926}, {'resid': 1313, 'atom': 'H15X', 'charge': 0.09000000357627869, 'distance': 30.463045120239258, 'force': [-0.02215442806482315, -0.02007484622299671, -0.011954805813729763], 'magnitude': 0.03219837695360184, 'cosine_with_motion': -0.8088005185127258, 'motion_component': -0.026042064651846886, 'motion_component_percent': 80.88005185127258}, {'resid': 1313, 'atom': 'H15Y', 'charge': 0.09000000357627869, 'distance': 29.527122497558594, 'force': [-0.022922471165657043, -0.021189795807003975, -0.014146269299089909], 'magnitude': 0.03427191451191902, 'cosine_with_motion': -0.8349548578262329, 'motion_component': -0.028615500777959824, 'motion_component_percent': 83.49548578262329}, {'resid': 1313, 'atom': 'H16R', 'charge': 0.09000000357627869, 'distance': 21.477821350097656, 'force': [-0.06182751804590225, -0.01919594593346119, 0.002129355911165476], 'magnitude': 0.06477391719818115, 'cosine_with_motion': -0.42159461975097656, 'motion_component': -0.027308335527777672, 'motion_component_percent': 42.159461975097656}, {'resid': 1313, 'atom': 'H16S', 'charge': 0.09000000357627869, 'distance': 21.56916046142578, 'force': [-0.05973763018846512, -0.022996943444013596, 0.005253229755908251], 'magnitude': 0.06422647833824158, 'cosine_with_motion': -0.3982014060020447, 'motion_component': -0.025575073435902596, 'motion_component_percent': 39.82014060020447}, {'resid': 1313, 'atom': 'H16X', 'charge': 0.09000000357627869, 'distance': 30.419422149658203, 'force': [-0.019739046692848206, -0.02178863063454628, -0.013353673741221428], 'magnitude': 0.03229079023003578, 'cosine_with_motion': -0.8398761749267578, 'motion_component': -0.02712026610970497, 'motion_component_percent': 83.98761749267578}, {'resid': 1313, 'atom': 'H16Y', 'charge': 0.09000000357627869, 'distance': 31.46310806274414, 'force': [-0.019147105515003204, -0.02044018730521202, -0.011254476383328438], 'magnitude': 0.03018403798341751, 'cosine_with_motion': -0.8145283460617065, 'motion_component': -0.024585753679275513, 'motion_component_percent': 81.45283460617065}, {'resid': 1313, 'atom': 'H17R', 'charge': 0.09000000357627869, 'distance': 19.27764320373535, 'force': [-0.0755210816860199, -0.025500932708382607, 0.010532153770327568], 'magnitude': 0.08040309697389603, 'cosine_with_motion': -0.34270909428596497, 'motion_component': -0.027554873377084732, 'motion_component_percent': 34.2709094285965}, {'resid': 1313, 'atom': 'H17S', 'charge': 0.09000000357627869, 'distance': 19.895538330078125, 'force': [-0.07280360907316208, -0.0185097549110651, 0.007431911304593086], 'magnitude': 0.07548648864030838, 'cosine_with_motion': -0.34827208518981934, 'motion_component': -0.026289837434887886, 'motion_component_percent': 34.827208518981934}, {'resid': 1313, 'atom': 'H17X', 'charge': 0.09000000357627869, 'distance': 31.552570343017578, 'force': [-0.018984591588377953, -0.018813924863934517, -0.013653156347572803], 'magnitude': 0.03001311607658863, 'cosine_with_motion': -0.861666202545166, 'motion_component': -0.025861287489533424, 'motion_component_percent': 86.1666202545166}, {'resid': 1313, 'atom': 'H17Y', 'charge': 0.09000000357627869, 'distance': 32.61537170410156, 'force': [-0.01845063827931881, -0.017614614218473434, -0.011759682558476925], 'magnitude': 0.028088979423046112, 'cosine_with_motion': -0.8395576477050781, 'motion_component': -0.02358231693506241, 'motion_component_percent': 83.95576477050781}, {'resid': 1313, 'atom': 'H18R', 'charge': 0.09000000357627869, 'distance': 22.00615882873535, 'force': [-0.058856312185525894, -0.015930963680148125, 0.009441986680030823], 'magnitude': 0.06170099228620529, 'cosine_with_motion': -0.3042813539505005, 'motion_component': -0.01877446100115776, 'motion_component_percent': 30.42813539505005}, {'resid': 1313, 'atom': 'H18S', 'charge': 0.09000000357627869, 'distance': 21.613483428955078, 'force': [-0.059337906539440155, -0.0209550429135561, 0.011454535648226738], 'magnitude': 0.06396333128213882, 'cosine_with_motion': -0.30274879932403564, 'motion_component': -0.019364822655916214, 'motion_component_percent': 30.274879932403564}, {'resid': 1313, 'atom': 'H18X', 'charge': 0.09000000357627869, 'distance': 32.69791030883789, 'force': [-0.016357624903321266, -0.019097700715065002, -0.012196734547615051], 'magnitude': 0.027947349473834038, 'cosine_with_motion': -0.8538968563079834, 'motion_component': -0.023864153772592545, 'motion_component_percent': 85.38968563079834}, {'resid': 1313, 'atom': 'H18Y', 'charge': 0.09000000357627869, 'distance': 33.70170974731445, 'force': [-0.01624273508787155, -0.017670026049017906, -0.010771224275231361], 'magnitude': 0.026307327672839165, 'cosine_with_motion': -0.8372058868408203, 'motion_component': -0.022024650126695633, 'motion_component_percent': 83.72058868408203}, {'resid': 1313, 'atom': 'H18Z', 'charge': 0.09000000357627869, 'distance': 33.87209701538086, 'force': [-0.015853945165872574, -0.01695406064391136, -0.01180961262434721], 'magnitude': 0.026043323799967766, 'cosine_with_motion': -0.862547755241394, 'motion_component': -0.022463610395789146, 'motion_component_percent': 86.2547755241394}, {'resid': 1313, 'atom': 'H19R', 'charge': 0.09000000357627869, 'distance': 19.881628036499023, 'force': [-0.06997542083263397, -0.021369077265262604, 0.018999386578798294], 'magnitude': 0.07559215277433395, 'cosine_with_motion': -0.22238029539585114, 'motion_component': -0.016810204833745956, 'motion_component_percent': 22.238029539585114}, {'resid': 1313, 'ato</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>574</v>
-      </c>
-      <c r="B5" t="n">
-        <v>969</v>
-      </c>
-      <c r="C5" t="n">
-        <v>2397</v>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>{574: {'frame': 574, 'motion_vector': [-5.495319366455078, 2.858715057373047, 2.9860458374023438], 'ionic_force': [9.93061837553978, -6.6990053951740265, 0.2928283214569092], 'ionic_force_magnitude': 11.982470656380775, 'radial_force': 11.978892044140771, 'axial_force': 0.2928283214569092, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-4.0223565101623535, 1.5621775388717651, -0.024718403816223145], 'asn_force_magnitude': 4.315131696401413, 'residue_force': [-4.0223565101623535, 1.5621775388717651, -0.024718403816223145], 'residue_force_magnitude': 4.315131696401413, 'pip2_force': [0.6445247805677354, 0.1866492098197341, -4.676992440184222], 'pip2_force_magnitude': 4.724881840409618, 'total_force': [6.552786645945162, -4.950178646482527, -4.408882522543536], 'total_force_magnitude': 9.321026046361993, 'cosine_total_motion': -0.9879746607329254, 'cosine_glu_motion': 0, 'cosine_asn_motion': 0.8929282470610925, 'cosine_residue_motion': 0.8929282470610925, 'cosine_pip2_motion': -0.5224218753743789, 'cosine_ionic_motion': -0.8840963770449431, 'motion_component_total': -9.208937545837252, 'motion_component_glu': 0, 'motion_component_asn': 3.8531029815054723, 'motion_component_residue': 3.8531029815054723, 'motion_component_ionic': -10.593658895353585, 'motion_component_pip2': -2.4683816319891396, 'motion_component_percent_total': 98.79746607329254, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 89.29282470610926, 'motion_component_percent_residue': 89.29282470610926, 'motion_component_percent_ionic': 88.40963770449432, 'motion_component_percent_pip2': 52.24218753743789, 'ionic_contributions': [{'ion_id': 2276, 'distance': 9.409431457519531, 'force': [1.1248300075531006, -0.7832292914390564, -3.4903464317321777], 'magnitude': 3.7498278617858887, 'cosine_ionic_motion': -0.730733335018158, 'motion_component_ionic': -2.740124225616455, 'motion_component_percent_ionic': 73.0733335018158}, {'ion_id': 2399, 'distance': 5.997857570648193, 'force': [3.4748947620391846, -1.8985097408294678, 8.336169242858887], 'magnitude': 9.22881031036377, 'cosine_ionic_motion': 0.0058180601336061954, 'motion_component_ionic': 0.05369377136230469, 'motion_component_percent_ionic': 0.5818060133606195}, {'ion_id': 2400, 'distance': 7.033089637756348, 'force': [4.853204727172852, -3.7680044174194336, -2.70151948928833], 'magnitude': 6.711904525756836, 'cosine_ionic_motion': -0.9859932661056519, 'motion_component_ionic': -6.617892742156982, 'motion_component_percent_ionic': 98.59932661056519}, {'ion_id': 2520, 'distance': 13.121502876281738, 'force': [0.47768887877464294, -0.24926194548606873, -1.8514750003814697], 'magnitude': 1.92828369140625, 'cosine_ionic_motion': -0.6686441898345947, 'motion_component_ionic': -1.2893357276916504, 'motion_component_percent_ionic': 66.86441898345947}], 'glu_contributions': [], 'asn_contributions': [{'resid': 458, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 5.911613941192627, 'force': [-6.197589874267578, -0.5701797008514404, 2.728013753890991], 'magnitude': 6.795386791229248, 'cosine_with_motion': 0.8682777881622314, 'motion_component': 5.900283336639404, 'motion_component_percent': 86.82777881622314}, {'resid': 458, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 5.043628692626953, 'force': [6.55202054977417, 1.054604411125183, -4.181386470794678], 'magnitude': 7.843797206878662, 'cosine_with_motion': -0.8431174159049988, 'motion_component': -6.613242149353027, 'motion_component_percent': 84.31174159049988}, {'resid': 458, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 5.3979716300964355, 'force': [-4.376787185668945, 1.0777528285980225, 1.4286543130874634], 'magnitude': 4.728516578674316, 'cosine_with_motion': 0.9656436443328857, 'motion_component': 4.566061973571777, 'motion_component_percent': 96.56436443328857}], 'pip2_contributions': [{'resid': 1313, 'atom': 'C1', 'charge': 0.06000000238418579, 'distance': 27.402389526367188, 'force': [-0.01598701998591423, -0.016060246154665947, 0.013792908750474453], 'magnitude': 0.026528486981987953, 'cosine_with_motion': 0.455685019493103, 'motion_component': 0.012088634073734283, 'motion_component_percent': 45.5685019493103}, {'resid': 1313, 'atom': 'C11', 'charge': 0.17000000178813934, 'distance': 26.513216018676758, 'force': [-0.055607374757528305, -0.04632038623094559, 0.03476704657077789], 'magnitude': 0.08029013872146606, 'cosine_with_motion': 0.5016644597053528, 'motion_component': 0.040278710424900055, 'motion_component_percent': 50.16644597053528}, {'resid': 1313, 'atom': 'C12', 'charge': 0.04000000283122063, 'distance': 26.91480255126953, 'force': [-0.013379307463765144, -0.010296311229467392, 0.00714502390474081], 'magnitude': 0.01833224669098854, 'cosine_with_motion': 0.5189841389656067, 'motion_component': 0.00951414555311203, 'motion_component_percent': 51.89841389656067}, {'resid': 1313, 'atom': 'C13', 'charge': -0.05000000074505806, 'distance': 28.121273040771484, 'force': [0.01517635490745306, 0.012300416827201843, -0.007681811694055796], 'magnitude': 0.020991241559386253, 'cosine_with_motion': -0.49307140707969666, 'motion_component': -0.0103501807898283, 'motion_component_percent': 49.307140707969666}, {'resid': 1313, 'atom': 'C2', 'charge': 0.06000000238418579, 'distance': 28.834280014038086, 'force': [-0.014851991087198257, -0.014281874522566795, 0.01222646702080965], 'magnitude': 0.02395913377404213, 'cosine_with_motion': 0.46916088461875916, 'motion_component': 0.011240688152611256, 'motion_component_percent': 46.916088461875916}, {'resid': 1313, 'atom': 'C21', 'charge': 0.6299999952316284, 'distance': 24.718509674072266, 'force': [-0.25818294286727905, -0.1850576549768448, 0.12758991122245789], 'magnitude': 0.3423214256763458, 'cosine_with_motion': 0.5398304462432861, 'motion_component': 0.1847955286502838, 'motion_component_percent': 53.98304462432861}, {'resid': 1313, 'atom': 'C210', 'charge': -0.18000000715255737, 'distance': 20.989748001098633, 'force': [0.1097487285733223, 0.07970749586820602, 0.0009218301856890321], 'magnitude': 0.1356426179409027, 'cosine_with_motion': -0.3993440270423889, 'motion_component': -0.05416806787252426, 'motion_component_percent': 39.93440270423889}, {'resid': 1313, 'atom': 'C211', 'charge': -0.15000000596046448, 'distance': 21.944766998291016, 'force': [0.08490826189517975, 0.058728888630867004, 0.005947514902800322], 'magnitude': 0.10341116040945053, 'cosine_with_motion': -0.39508315920829773, 'motion_component': -0.0408560074865818, 'motion_component_percent': 39.50831592082977}, {'resid': 1313, 'atom': 'C212', 'charge': -0.15000000596046448, 'distance': 22.32193374633789, 'force': [0.0798613652586937, 0.05907154083251953, 0.011042341589927673], 'magnitude': 0.09994607418775558, 'cosine_with_motion': -0.34486645460128784, 'motion_component': -0.03446804732084274, 'motion_component_percent': 34.486645460128784}, {'resid': 1313, 'atom': 'C213', 'charge': -0.18000000715255737, 'distance': 21.862707138061523, 'force': [0.0949091762304306, 0.07975561171770096, 0.0162160973995924], 'magnitude': 0.12502668797969818, 'cosine_with_motion': -0.2851226031780243, 'motion_component': -0.035647936165332794, 'motion_component_percent': 28.51226031780243}, {'resid': 1313, 'atom': 'C214', 'charge': -0.15000000596046448, 'distance': 21.32759666442871, 'force': [0.08263921737670898, 0.06865246593952179, 0.0210727471858263], 'magnitude': 0.10948270559310913, 'cosine_with_motion': -0.2589397132396698, 'motion_component': -0.02834942191839218, 'motion_component_percent': 25.89397132396698}, {'resid': 1313, 'atom': 'C215', 'charge': -0.15000000596046448, 'distance': 21.243288040161133, 'force': [0.07940758019685745, 0.07188725471496582, 0.026543162763118744], 'magnitude': 0.11035343259572983, 'cosine_with_motion': -0.1997826099395752, 'motion_component': -0.02204669639468193, 'motion_component_percent': 19.97826099395752}, {'resid': 1313, 'atom': 'C216', 'charge': -0.18000000715255737, 'distance': 21.75861358642578, 'force': [0.08496736735105515, 0.08838987350463867, 0.030012227594852448], 'magnitude': 0.1262258142232895, 'cosine_with_motion': -0.14357523620128632, 'motion_component': -0.018122900277376175, 'motion_component_percent': 14.357523620128632}, {'resid': 1313, 'atom': 'C217', 'charge': -0.18000000715255737, 'distance': 22.94518280029297, 'force': [0.07480096071958542, 0.07911965996026993, 0.03207841143012047], 'magnitude': 0.11350827664136887, 'cosine_with_motion': -0.11413389444351196, 'motion_component': -0.012955141253769398, 'motion_component_percent': 11.413389444351196}, {'resid': 1313, 'atom': 'C218', 'charge': -0.18000000715255737, 'distance': 22.520280838012695, 'force': [0.07689394056797028, 0.07943665981292725, 0.04076153412461281], 'magnitude': 0.11783193051815033, 'cosine_with_motion': -0.09102306514978409, 'motion_component': -0.010725423693656921, 'motion_component_percent': 9.102306514978409}, {'resid': 1313, 'atom': 'C219', 'charge': -0.18000000715255737, 'distance': 23.829050064086914, 'force': [0.06805725395679474, 0.06955601274967194, 0.040080681443214417], 'magnitude': 0.10524395108222961, 'cosine_with_motion': -0.0766497328877449, 'motion_component': -0.008066920563578606, 'motion_component_percent': 7.66497328877449}, {'resid': 1313, 'atom': 'C22', 'charge': -0.08000000566244125, 'distance': 23.81096076965332, 'force': [0.036265384405851364, 0.025475643575191498, -0.015178241766989231], 'magnitude': 0.046846188604831696, 'cosine_with_motion': -0.5332604646682739, 'motion_component': -0.024981221184134483, 'motion_component_percent': 53.32604646682739}, {'resid': 1313, 'atom': 'C220', 'charge': -0.27000001072883606, 'distance': 25.01742172241211, 'force': [0.0884084701538086, 0.09920471161603928, 0.05343755707144737], 'magnitude': 0.1432243138551712, 'cosine_with_motion': -0.043322257697582245, 'motion_component': -0.006204800680279732, 'motion_component_percent': 4.3322257697582245}, {'resid': 1313, 'atom': 'C23', 'charge': -0.18000000715255737, 'distance': 22.606430053710938, 'force': [0.08748061954975128, 0.06767256557941437, -0.0379670113325119], 'magnitude': 0.11693557351827621, 'cosine_with_motion': -0.4982472360134125, 'motion_component': -0.05826282501220703, 'motion_component_percent': 49.82472360134125}, {'resid': 1313, 'atom': 'C24', 'charge': -0.18000000715255737, 'distance': 21.731489181518555, 'force': [0.09698843955993652, 0.07352207601070404, -0.03464677184820175], 'magnitude': 0.1265411078929901, 'cosine_with_motion': -0.48985952138900757, 'motion_component': -0.061987366527318954, 'motion_component_percent': 48.98595213890076}, {'resid': 1313, 'atom': 'C25', 'charge': -0.15000000596046448, 'distance': 22.326690673828125, 'force': [0.07700181752443314, 0.05997266620397568, -0.021323855966329575], 'magnitude': 0.09990349411964417, 'cosine_with_motion': -0.45907098054885864, 'motion_component': -0.045862793922424316, 'motion_component_percent': 45.907098054885864}, {'resid': 1313, 'atom': 'C26', 'charge': -0.15000000596046448, 'distance': 21.762929916381836, 'force': [0.08248762786388397, 0.0629764050245285, -0.016897939145565033], 'magnitude': 0.10514645278453827, 'cosine_with_motion': -0.44771942496299744, 'motion_component': -0.047076109796762466, 'motion_component_percent': 44.771942496299744}, {'resid': 1313, 'atom': 'C27', 'charge': -0.18000000715255737, 'distance': 20.253379821777344, 'force': [0.1153358742594719, 0.08644368499517441, -0.021197110414505005], 'magnitude': 0.14568524062633514, 'cosine_with_motion': -0.4491698145866394, 'motion_component': -0.06543741375207901, 'motion_component_percent': 44.91698145866394}, {'resid': 1313, 'atom': 'C28', 'charge': -0.15000000596046448, 'distance': 20.08144187927246, 'force': [0.10253174602985382, 0.06770477443933487, -0.012394802644848824], 'magnitude': 0.12349221110343933, 'cosine_with_motion': -0.47916385531425476, 'motion_component': -0.05917300283908844, 'motion_component_percent': 47.916385531425476}, {'resid': 1313, 'atom': 'C29', 'charge': -0.15000000596046448, 'distance': 20.329374313354492, 'force': [0.10087910294532776, 0.06576956808567047, -0.00419965386390686], 'magnitude': 0.1204984113574028, 'cosine_with_motion': -0.4572524428367615, 'motion_component': -0.055098194628953934, 'motion_component_percent': 45.72524428367615}, {'resid': 1313, 'atom': 'C3', 'charge': 0.06000000238418579, 'distance': 29.434846878051758, 'force': [-0.014295089058578014, -0.012924598529934883, 0.012538362294435501], 'magnitude': 0.022991418838500977, 'cosine_with_motion': 0.49998340010643005, 'motion_component': 0.011495327576994896, 'motion_component_percent': 49.998340010643005}, {'resid': 1313, 'atom': 'C31', 'charge': 0.6299999952316284, 'distance': 29.705068588256836, 'force': [-0.18095967173576355, -0.13007664680480957, 0.08074997365474701], 'magnitude': 0.2370377480983734, 'cosine_with_motion': 0.5298762917518616, 'motion_component': 0.1256006807088852, 'motion_component_percent': 52.98762917518616}, {'resid': 1313, 'atom': 'C310', 'charge': -0.18000000715255737, 'distance': 23.53643226623535, 'force': [0.09357346594333649, 0.051546595990657806, -0.014980881474912167], 'magnitude': 0.10787711292505264, 'cosine_with_motion': -0.5548380613327026, 'motion_component': -0.059854328632354736, 'motion_component_percent': 55.483806133270264}, {'resid': 1313, 'atom': 'C311', 'charge': -0.18000000715255737, 'distance': 23.462108612060547, 'force': [0.09750301390886307, 0.04634115844964981, -0.011458470486104488], 'magnitude': 0.108561672270298, 'cosine_with_motion': -0.5861093997955322, 'motion_component': -0.06362901628017426, 'motion_component_percent': 58.61093997955322}, {'resid': 1313, 'atom': 'C312', 'charge': -0.18000000715255737, 'distance': 22.221818923950195, 'force': [0.1098579540848732, 0.05003775283694267, -0.008538385853171349], 'magnitude': 0.12101838737726212, 'cosine_with_motion': -0.5841884613037109, 'motion_component': -0.07069754600524902, 'motion_component_percent': 58.418846130371094}, {'resid': 1313, 'atom': 'C313', 'charge': -0.18000000715255737, 'distance': 22.356657028198242, 'force': [0.11110129207372665, 0.044062964618206024, -0.003205313580110669], 'magnitude': 0.1195630207657814, 'cosine_with_motion': -0.601015031337738, 'motion_component': -0.07185917347669601, 'motion_component_percent': 60.101503133773804}, {'resid': 1313, 'atom': 'C314', 'charge': -0.18000000715255737, 'distance': 21.08416748046875, 'force': [0.12545935809612274, 0.04822041839361191, 0.002508534351363778], 'magnitude': 0.13443046808242798, 'cosine_with_motion': -0.5885848999023438, 'motion_component': -0.07912374287843704, 'motion_component_percent': 58.858489990234375}, {'resid': 1313, 'atom': 'C315', 'charge': -0.18000000715255737, 'distance': 19.7880916595459, 'force': [0.14417116343975067, 0.050034087151288986, -0.0017885675188153982], 'magnitude': 0.152616947889328, 'cosine_with_motion': -0.623711884021759, 'motion_component': -0.09518900513648987, 'motion_component_percent': 62.3711884021759}, {'resid': 1313, 'atom': 'C316', 'charge': -0.18000000715255737, 'distance': 18.821378707885742, 'force': [0.1562066525220871, 0.06322502344846725, -0.00779768219217658], 'magnitude': 0.16869714856147766, 'cosine_with_motion': -0.6042345762252808, 'motion_component': -0.10193265229463577, 'motion_component_percent': 60.423457622528076}, {'resid': 1313, 'atom': 'C317', 'charge': -0.18000000715255737, 'distance': 17.54347038269043, 'force': [0.177896648645401, 0.07780766487121582, -0.0005468409508466721], 'magnitude': 0.19416886568069458, 'cosine_with_motion': -0.5668008923530579, 'motion_component': -0.11005508899688721, 'motion_component_percent': 56.680089235305786}, {'resid': 1313, 'atom': 'C318', 'charge': -0.27000001072883606, 'distance': 16.768815994262695, 'force': [0.28250983357429504, 0.14683420956134796, -0.015855953097343445], 'magnitude': 0.3187844157218933, 'cosine_with_motion': -0.5383182168006897, 'motion_component': -0.17160744965076447, 'motion_component_percent': 53.83182168006897}, {'resid': 1313, 'atom': 'C32', 'charge': -0.08000000566244125, 'distance': 30.127117156982422, 'force': [0.02311633713543415, 0.015633665025234222, -0.008804736658930779], 'magnitude': 0.02926260232925415, 'cosine_with_motion': -0.5398436784744263, 'motion_component': -0.01579723134636879, 'motion_component_percent': 53.98436784744263}, {'resid': 1313, 'atom': 'C33', 'charge': -0.18000000715255737, 'distance': 29.63701820373535, 'force': [0.05549591779708862, 0.0336141362786293, -0.020475614815950394], 'magnitude': 0.06803644448518753, 'cosine_with_motion': -0.5771322846412659, 'motion_component': -0.03926602751016617, 'motion_component_percent': 57.71322846412659}, {'resid': 1313, 'atom': 'C34', 'charge': -0.18000000715255737, 'distance': 28.112001419067383, 'force': [0.061979737132787704, 0.03677040711045265, -0.02290373481810093], 'magnitude': 0.07561832666397095, 'cosine_with_motion': -0.5843786597251892, 'motion_component': -0.04418973624706268, 'motion_component_percent': 58.43786597251892}, {'resid': 1313, 'atom': 'C35', 'charge': -0.18000000715255737, 'distance': 27.35348892211914, 'force': [0.06513121724128723, 0.04118206351995468, -0.021005263552069664], 'magnitude': 0.07987026870250702, 'cosine_with_motion': -0.5515170097351074, 'motion_component': -0.044049810618162155, 'motion_component_percent': 55.15170097351074}, {'resid': 1313, 'atom': 'C36', 'charge': -0.18000000715255737, 'distance': 27.78740692138672, 'force': [0.06429164111614227, 0.039864808320999146, -0.016352808102965355], 'magnitude': 0.07739529758691788, 'cosine_with_motion': -0.5414569973945618, 'motion_component': -0.04190622642636299, 'motion_component_percent': 54.14569973945618}, {'resid': 1313, 'atom': 'C37', 'charge': -0.18000000715255737, 'distance': 27.4178409576416, 'force': [0.068262480199337, 0.03787865862250328, -0.015000693500041962], 'magnitude': 0.07949578762054443, 'cosine_with_motion': -0.5700680613517761, 'motion_component': -0.045318007469177246, 'motion_component_percent': 57.00680613517761}, {'resid': 1313, 'atom': 'C38', 'charge': -0.18000000715255737, 'distance': 25.86261749267578, 'force': [0.07760042697191238, 0.04102439060807228, -0.016659297049045563], 'magnitude': 0.08934404700994492, 'cosine_with_motion': -0.584177553653717, 'motion_component': -0.05219278857111931, 'motion_component_percent': 58.417755365371704}, {'resid': 1313, 'atom': 'C39', 'charge': -0.18000000715255737, 'distance': 25.00602149963379, 'force': [0.08180726319551468, 0.047219183295965195, -0.014544346369802952], 'magnitude': 0.09556996077299118, 'cosine_with_motion': -0.5447418093681335, 'motion_component': -0.05206095054745674, 'motion_component_percent': 54.474180936813354}, {'resid': 1313, 'atom': 'C4', 'charge': 0.08000000566244125, 'distance': 29.475217819213867, 'force': [-0.017802823334932327, -0.017433788627386093, 0.01771235466003418], 'magnitude': 0.030571309849619865, 'cosine_with_motion': 0.4798832833766937, 'motion_component': 0.014670660719275475, 'motion_component_percent': 47.98832833766937}, {'resid': 1313, 'atom': 'C5', 'charge': 0.08000000566244125, 'distance': 28.110876083374023, 'force': [-0.018982261419296265, -0.019330019131302834, 0.019892528653144836], 'magnitude': 0.033610839396715164, 'cosine_with_motion': 0.46924152970314026, 'motion_component': 0.01577160134911537, 'motion_component_percent': 46.924152970314026}, {'resid': 1313, 'atom': 'C6', 'charge': 0.06000000238418579, 'distance': 27.347814559936523, 'force': [-0.015022143721580505, -0.016221214085817337, 0.014852693304419518], 'magnitude': 0.026634471490979195, 'cosine_with_motion': 0.43968746066093445, 'motion_component': 0.011710843071341515, 'motion_component_percent': 43.968746066093445}, {'resid': 1313, 'atom': 'H1', 'charge': 0.12000000476837158, 'distance': 26.872238159179688, 'force': [-0.03451615199446678, -0.03192678838968277, 0.028864610940217972], 'magnitude': 0.05517110228538513, 'cosine_with_motion': 0.4865696430206299, 'motion_component': 0.026844583451747894, 'motion_component_percent': 48.65696430206299}, {'resid': 1313, 'atom': 'H10R', 'charge': 0.09000000357627869, 'distance': 21.600147247314453, 'force': [-0.05052445828914642, -0.039332713931798935, 0.0012797724921256304], 'magnitude': 0.0640423372387886, 'cosine_with_motion': 0.3838138282299042, 'motion_component': 0.0245803352445364, 'motion_component_percent': 38.38138282299042}, {'resid': 1313, 'atom': 'H10S', 'charge': 0.09000000357627869, 'distance': 20.172346115112305, 'force': [-0.058071963489055634, -0.044898707419633865, -0.0018910818034783006], 'magnitude': 0.07342903316020966, 'cosine_with_motion': 0.36662667989730835, 'motion_component': 0.026921043172478676, 'motion_component_percent': 36.662667989730835}, {'resid': 1313, 'atom': 'H10X', 'charge': 0.09000000357627869, 'distance': 22.991798400878906, 'force': [-0.04890096187591553, -0.026489781215786934, 0.01009838841855526], 'magnitude': 0.05652424320578575, 'cosine_with_motion': 0.5741134285926819, 'motion_component': 0.0324513278901577, 'motion_component_percent': 57.41134285926819}, {'resid': 1313, 'atom': 'H10Y', 'charge': 0.09000000357627869, 'distance': 23.003032684326172, 'force': [-0.04803583398461342, -0.0288775023072958, 0.006884868256747723], 'magnitude': 0.05646904185414314, 'cosine_with_motion': 0.5201421976089478, 'motion_component': 0.02937193028628826, 'motion_component_percent': 52.014219760894775}, {'resid': 1313, 'atom': 'H111', 'charge': 0.15000000596046448, 'distance': 22.47832489013672, 'force': [-0.08321110159158707, -0.05262521654367447, -0.004539594519883394], 'magnitude': 0.09856017678976059, 'cosine_with_motion': 0.4327154755592346, 'motion_component': 0.04264851287007332, 'motion_component_percent': 43.27154755592346}, {'resid': 1313, 'atom': 'H11A', 'charge': 0.09000000357627869, 'distance': 27.334951400756836, 'force': [-0.027288133278489113, -0.02281026728451252, 0.0182810015976429], 'magnitude': 0.03998931869864464, 'cosine_with_motion': 0.5066989064216614, 'motion_component': 0.020262543112039566, 'motion_component_percent': 50.66989064216614}, {'resid': 1313, 'atom': 'H11B', 'charge': 0.09000000357627869, 'distance': 25.559093475341797, 'force': [-0.03164472430944443, -0.025831986218690872, 0.02057681605219841], 'magnitude': 0.045739319175481796, 'cosine_with_motion': 0.5134486556053162, 'motion_component': 0.023484792560338974, 'motion_component_percent': 51.344865560531616}, {'resid': 1313, 'atom': 'H11X', 'charge': 0.09000000357627869, 'distance': 24.339977264404297, 'force': [-0.045453786849975586, -0.02149791643023491, 0.003946943208575249], 'magnitude': 0.050435952842235565, 'cosine_with_motion': 0.5769813656806946, 'motion_component': 0.029100604355335236, 'motion_component_percent': 57.69813656806946}, {'resid': 1313, 'atom': 'H11Y', 'charge': 0.09000000357627869, 'distance': 23.785486221313477, 'force': [-0.04784690588712692, -0.02111019194126129, 0.007378881331533194], 'magnitude': 0.05281490832567215, 'cosine_with_motion': 0.6184708476066589, 'motion_component': 0.03266448155045509, 'motion_component_percent': 61.847084760665894}, {'resid': 1313, 'atom': 'H12', 'charge': 0.09000000357627869, 'distance': 27.21428108215332, 'force': [-0.030063677579164505, -0.021360209211707115, 0.016358934342861176], 'magnitude': 0.040344737470149994, 'cosine_with_motion': 0.5514664053916931, 'motion_component': 0.0222487673163414, 'motion_component_percent': 55.14664053916931}, {'resid': 1313, 'atom': 'H121', 'charge': 0.15000000596046448, 'distance': 23.170303344726562, 'force': [-0.07495530694723129, -0.05322969704866409, -0.012366272509098053], 'magnitude': 0.09276110678911209, 'cosine_with_motion': 0.3492962121963501, 'motion_component': 0.032401103526353836, 'motion_component_percent': 34.92962121963501}, {'resid': 1313, 'atom': 'H12X', 'charge': 0.09000000357627869, 'distance': 21.59376335144043, 'force': [-0.05827166512608528, -0.025715386494994164, 0.0070289187133312225], 'magnitude': 0.06408021599054337, 'cosine_with_motion': 0.6075019240379333, 'motion_component': 0.03892885521054268, 'motion_component_percent': 60.750192403793335}, {'resid': 1313, 'atom': 'H12Y', 'charge': 0.09000000357627869, 'distance': 21.88326072692871, 'force': [-0.055588047951459885, -0.0281803160905838, 0.0030159649904817343], 'magnitude': 0.06239597126841545, 'cosine_with_motion': 0.5451794266700745, 'motion_component': 0.03401700034737587, 'motion_component_percent': 54.517942667007446}, {'resid': 1313, 'atom': 'H13A', 'charge': 0.09000000357627869, 'distance': 28.964584350585938, 'force': [-0.025414682924747467, -0.020764777436852455, 0.013835546560585499], 'magnitude': 0.03561607003211975, 'cosine_with_motion': 0.4965561330318451, 'motion_component': 0.017685377970337868, 'motion_component_percent': 49.65561330318451}, {'resid': 1313, 'atom': 'H13B', 'charge': 0.09000000357627869, 'distance': 27.87356185913086, 'force': [-0.027067841961979866, -0.02370568923652172, 0.013581275008618832], 'magnitude': 0.038458794355392456, 'cosine_with_motion': 0.4595431089401245, 'motion_component': 0.017673473805189133, 'motion_component_percent': 45.95431089401245}, {'resid': 1313, 'atom': 'H13R', 'charge': 0.09000000357627869, 'distance': 21.23004722595215, 'force': [-0.049622129648923874, -0.0435173436999321, -0.0062346430495381355], 'magnitude': 0.06629468500614166, 'cosine_with_motion': 0.2844361960887909, 'motion_component': 0.018856607377529144, 'motion_component_percent': 28.44361960887909}, {'resid': 1313, 'atom': 'H13S', 'charge': 0.09000000357627869, 'distance': 22.71095848083496, 'force': [-0.0427805632352829, -0.03826403617858887, -0.007852829061448574], 'magnitude': 0.05793081969022751, 'cosine_with_motion': 0.25669384002685547, 'motion_component': 0.014870485290884972, 'motion_component_percent': 25.669384002685547}, {'resid': 1313, 'atom': 'H13X', 'charge': 0.09000000357627869, 'distance': 23.276805877685547, 'force': [-0.05104534327983856, -0.020873552188277245, 0.00016215912182815373], 'magnitude': 0.05514851212501526, 'cosine_with_motion': 0.5836076140403748, 'motion_component': 0.03218509256839752, 'motion_component_percent': 58.360761404037476}, {'resid': 1313, 'atom': 'H13Y', 'charge': 0.09000000357627869, 'distance': 22.564701080322266, 'force': [-0.05533658713102341, -0.019312774762511253, 0.002952663926407695], 'magnitude': 0.05868423357605934, 'cosine_with_motion': 0.6385865211486816, 'motion_component': 0.03747496008872986, 'motion_component_percent': 63.858652114868164}, {'resid': 1313, 'atom': 'H141', 'charge': 0.15000000596046448, 'distance': 20.91357421875, 'force': [-0.08912335336208344, -0.06709177792072296, -0.022801753133535385], 'magnitude': 0.11386043578386307, 'cosine_with_motion': 0.2935974895954132, 'motion_component': 0.033429138362407684, 'motion_component_percent': 29.35974895954132}, {'resid': 1313, 'atom': 'H14X', 'charge': 0.09000000357627869, 'distance': 21.595001220703125, 'force': [-0.06038380041718483, -0.021157752722501755, -0.0033878821413964033], 'magnitude': 0.0640728622674942, 'cosine_with_motion': 0.5928890109062195, 'motion_component': 0.037988096475601196, 'motion_component_percent': 59.28890109062195}, {'resid': 1313, 'atom': 'H14Y', 'charge': 0.09000000357627869, 'distance': 20.897918701171875, 'force': [-0.06262236088514328, -0.0274053867906332, -0.002915058983489871], 'magnitude': 0.06841865926980972, 'cosine_with_motion': 0.5464163422584534, 'motion_component': 0.03738507255911827, 'motion_component_percent': 54.64163422584534}, {'resid': 1313, 'atom': 'H151', 'charge': 0.15000000596046448, 'distance': 20.728126525878906, 'force': [-0.08357397466897964, -0.07334715127944946, -0.03271077573299408], 'magnitude': 0.11590689420700073, 'cosine_with_motion': 0.1905936449766159, 'motion_component': 0.02209111675620079, 'motion_component_percent': 19.05936449766159}, {'resid': 1313, 'atom': 'H15X', 'charge': 0.09000000357627869, 'distance': 19.389982223510742, 'force': [-0.0758725255727768, -0.023544710129499435, -0.002268099458888173], 'magnitude': 0.07947413623332977, 'cosine_with_motion': 0.6273694634437561, 'motion_component': 0.04985964670777321, 'motion_component_percent': 62.73694634437561}, {'resid': 1313, 'atom': 'H15Y', 'charge': 0.09000000357627869, 'distance': 20.140121459960938, 'force': [-0.07045387476682663, -0.021265681833028793, 0.0032305517233908176], 'magnitude': 0.07366420328617096, 'cosine_with_motion': 0.663341760635376, 'motion_component': 0.048864543437957764, 'motion_component_percent': 66.3341760635376}, {'resid': 1313, 'atom': 'H16R', 'charge': 0.09000000357627869, 'distance': 20.997169494628906, 'force': [-0.04374101385474205, -0.04902323707938194, -0.016633594408631325], 'magnitude': 0.06777337193489075, 'cosine_with_motion': 0.10848373919725418, 'motion_component': 0.007352308835834265, 'motion_component_percent': 10.848373919725418}, {'resid': 1313, 'atom': 'H16S', 'charge': 0.09000000357627869, 'distance': 22.048635482788086, 'force': [-0.04108754172921181, -0.04414252191781998, -0.011874829418957233], 'magnitude': 0.061463482677936554, 'cosine_with_motion': 0.15175266563892365, 'motion_component': 0.009327247738838196, 'motion_component_percent': 15.175266563892365}, {'resid': 1313, 'atom': 'H16X', 'charge': 0.09000000357627869, 'distance': 18.692665100097656, 'force': [-0.07960584759712219, -0.030061068013310432, 0.008480374701321125], 'magnitude': 0.08551418036222458, 'cosine_with_motion': 0.6408466100692749, 'motion_component': 0.054801471531391144, 'motion_component_percent': 64.08466100692749}, {'resid': 1313, 'atom': 'H16Y', 'charge': 0.09000000357627869, 'distance': 19.445110321044922, 'force': [-0.07168613374233246, -0.033005472272634506, 0.004068424459546804], 'magnitude': 0.07902414351701736, 'cosine_with_motion': 0.5736560225486755, 'motion_component': 0.04533267766237259, 'motion_component_percent': 57.365602254867554}, {'resid': 1313, 'atom': 'H17R', 'charge': 0.09000000357627869, 'distance': 23.531579971313477, 'force': [-0.03404809907078743, -0.03910934552550316, -0.014931663870811462], 'magnitude': 0.053960807621479034, 'cosine_with_motion': 0.08277805149555206, 'motion_component': 0.0044667706824839115, 'motion_component_percent': 8.277805149555206}, {'resid': 1313, 'atom': 'H17S', 'charge': 0.09000000357627869, 'distance': 23.737777709960938, 'force': [-0.03620608150959015, -0.035808272659778595, -0.014791703782975674], 'magnitude': 0.05302741751074791, 'cosine_with_motion': 0.14378191530704498, 'motion_component': 0.007624383550137281, 'motion_component_percent': 14.378191530704498}, {'resid': 1313, 'atom': 'H17X', 'charge': 0.09000000357627869, 'distance': 17.030092239379883, 'force': [-0.09646784514188766, -0.03614608943462372, -0.0013262205757200718], 'magnitude': 0.10302593559026718, 'cosine_with_motion': 0.596825361251831, 'motion_component': 0.06148849427700043, 'motion_component_percent': 59.682536125183105}, {'resid': 1313, 'atom': 'H17Y', 'charge': 0.09000000357627869, 'distance': 18.075403213500977, 'force': [-0.082859568297863, -0.03847616910934448, -0.004217083565890789], 'magnitude': 0.0914544016122818, 'cosine_with_motion': 0.5291123390197754, 'motion_component': 0.048389650881290436, 'motion_component_percent': 52.91123390197754}, {'resid': 1313, 'atom': 'H18R', 'charge': 0.09000000357627869, 'distance': 22.035890579223633, 'force': [-0.04203231260180473, -0.03952266275882721, -0.021395115181803703], 'magnitude': 0.06153460219502449, 'cosine_with_motion': 0.12787552177906036, 'motion_component': 0.007868769578635693, 'motion_component_percent': 12.787552177906036}, {'resid': 1313, 'atom': 'H18S', 'charge': 0.09000000357627869, 'distance': 21.881269454956055, 'force': [-0.03882807120680809, -0.04325619712471962, -0.022714680060744286], 'magnitude': 0.06240732967853546, 'cosine_with_motion': 0.05100433900952339, 'motion_component': 0.0031830444931983948, 'motion_component_percent': 5.100433900952339}, {'resid': 1313, 'atom': 'H18X', 'charge': 0.09000000357627869, 'distance': 15.944635391235352, 'force': [-0.10282272100448608, -0.056905265897512436, 0.0016583347460255027], 'magnitude': 0.11753072589635849, 'cosine_with_motion': 0.5039783120155334, 'motion_component': 0.059232939034700394, 'motion_component_percent': 50.397831201553345}, {'resid': 1313, 'atom': 'H18Y', 'charge': 0.09000000357627869, 'distance': 16.390501022338867, 'force': [-0.09912913292646408, -0.048982057720422745, 0.012033961713314056], 'magnitude': 0.11122339218854904, 'cosine_with_motion': 0.5761426091194153, 'motion_component': 0.06408053636550903, 'motion_component_percent': 57.61426091194153}, {'resid': 1313, 'atom': 'H18Z', 'charge': 0.09000000357627869, '</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>594</v>
-      </c>
-      <c r="B6" t="n">
-        <v>707</v>
-      </c>
-      <c r="C6" t="n">
-        <v>2276</v>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>{594: {'frame': 594, 'motion_vector': [-1.0011978149414062, -3.098834991455078, -3.3971405029296875], 'ionic_force': [16.41676777601242, 6.264683712273836, 3.169294625520706], 'ionic_force_magnitude': 17.85499802995518, 'radial_force': 17.571469096986423, 'axial_force': 3.169294625520706, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-3.895551025867462, 2.105670690536499, -4.178462982177734], 'asn_force_magnitude': 6.0884086381870866, 'residue_force': [-3.895551025867462, 2.105670690536499, -4.178462982177734], 'residue_force_magnitude': 6.0884086381870866, 'pip2_force': [0.5637558391317725, 0.03709937212988734, -4.52289681466209], 'pip2_force_magnitude': 4.558047016612277, 'total_force': [13.084972589276731, 8.407453774940223, -5.532065171319118], 'total_force_magnitude': 16.50774156871866, 'cosine_total_motion': -0.2620964359109277, 'cosine_glu_motion': 0, 'cosine_asn_motion': 0.4038140040399918, 'cosine_residue_motion': 0.4038140040399918, 'cosine_pip2_motion': 0.684645010286754, 'cosine_ionic_motion': -0.5547941831455198, 'motion_component_total': -4.326620230099827, 'motion_component_glu': 0, 'motion_component_asn': 2.458584670418001, 'motion_component_residue': 2.458584670418001, 'motion_component_ionic': -9.905849047093849, 'motion_component_pip2': 3.1206441465760206, 'motion_component_percent_total': 26.209643591092767, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 40.38140040399918, 'motion_component_percent_residue': 40.38140040399918, 'motion_component_percent_ionic': 55.47941831455198, 'motion_component_percent_pip2': 68.4645010286754, 'ionic_contributions': [{'ion_id': 2223, 'distance': 11.164527893066406, 'force': [0.9171769022941589, 0.3611668050289154, -2.4744150638580322], 'magnitude': 2.6635286808013916, 'cosine_ionic_motion': 0.5080801248550415, 'motion_component_ionic': 1.3532860279083252, 'motion_component_percent_ionic': 50.80801248550415}, {'ion_id': 2397, 'distance': 12.290963172912598, 'force': [2.1154870986938477, 0.49722781777381897, 0.3275904953479767], 'magnitude': 2.1976888179779053, 'cosine_ionic_motion': -0.4613851010799408, 'motion_component_ionic': -1.0139808654785156, 'motion_component_percent_ionic': 46.13851010799408}, {'ion_id': 2399, 'distance': 6.807759761810303, 'force': [2.3719210624694824, 3.4110326766967773, 5.835718631744385], 'magnitude': 7.163571834564209, 'cosine_ionic_motion': -0.9720718860626221, 'motion_component_ionic': -6.963506698608398, 'motion_component_percent_ionic': 97.2071886062622}, {'ion_id': 2400, 'distance': 6.391457557678223, 'force': [5.8384013175964355, 0.05161558464169502, 5.653402805328369], 'magnitude': 8.12714958190918, 'cosine_ionic_motion': -0.6591774821281433, 'motion_component_ionic': -5.357234001159668, 'motion_component_percent_ionic': 65.91774821281433}, {'ion_id': 2520, 'distance': 6.330036163330078, 'force': [5.173781394958496, 1.9436408281326294, -6.173002243041992], 'magnitude': 8.285633087158203, 'cosine_ionic_motion': 0.2505042552947998, 'motion_component_ionic': 2.0755863189697266, 'motion_component_percent_ionic': 25.05042552947998}], 'glu_contributions': [], 'asn_contributions': [{'resid': 786, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 5.834468841552734, 'force': [-3.124321937561035, 2.2833364009857178, -4.4025397300720215], 'magnitude': 5.861515998840332, 'cosine_with_motion': 0.3990894556045532, 'motion_component': 2.3392691612243652, 'motion_component_percent': 39.90894556045532}, {'resid': 786, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 5.439373016357422, 'force': [-2.8021013736724854, 6.860512733459473, -6.999019145965576], 'magnitude': 10.193364143371582, 'cosine_with_motion': 0.1109568327665329, 'motion_component': 1.1310234069824219, 'motion_component_percent': 11.09568327665329}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 4.63738489151001, 'force': [1.24074125289917, -3.9694223403930664, 4.873508930206299], 'magnitude': 6.40678071975708, 'cosine_with_motion': -0.18234384059906006, 'motion_component': -1.1682369709014893, 'motion_component_percent': 18.234384059906006}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 5.909841537475586, 'force': [0.7901310324668884, -3.068756103515625, 2.3495869636535645], 'magnitude': 3.9448864459991455, 'cosine_with_motion': 0.03967897593975067, 'motion_component': 0.15652905404567719, 'motion_component_percent': 3.967897593975067}], 'pip2_contributions': [{'resid': 1313, 'atom': 'C1', 'charge': 0.06000000238418579, 'distance': 26.491159439086914, 'force': [-0.017052076756954193, -0.0143767474219203, 0.017556725069880486], 'magnitude': 0.028384903445839882, 'cosine_with_motion': 0.014830406755208969, 'motion_component': 0.0004209596663713455, 'motion_component_percent': 1.483040675520897}, {'resid': 1313, 'atom': 'C11', 'charge': 0.17000000178813934, 'distance': 25.81676483154297, 'force': [-0.05900741368532181, -0.04110345616936684, 0.04471484199166298], 'magnitude': 0.08468049764633179, 'cosine_with_motion': 0.08669587969779968, 'motion_component': 0.007341450080275536, 'motion_component_percent': 8.669587969779968}, {'resid': 1313, 'atom': 'C12', 'charge': 0.04000000283122063, 'distance': 26.21453857421875, 'force': [-0.014077982865273952, -0.00943086389452219, 0.009290575981140137], 'magnitude': 0.019324740394949913, 'cosine_with_motion': 0.1292944848537445, 'motion_component': 0.0024985824711620808, 'motion_component_percent': 12.92944848537445}, {'resid': 1313, 'atom': 'C13', 'charge': -0.05000000074505806, 'distance': 27.378812789916992, 'force': [0.015966257080435753, 0.011442461982369423, -0.010225307196378708], 'magnitude': 0.022145163267850876, 'cosine_with_motion': -0.1603139340877533, 'motion_component': -0.0035501783713698387, 'motion_component_percent': 16.03139340877533}, {'resid': 1313, 'atom': 'C2', 'charge': 0.06000000238418579, 'distance': 27.95166015625, 'force': [-0.015625115483999252, -0.013014979660511017, 0.015379151329398155], 'magnitude': 0.025496121495962143, 'cosine_with_motion': 0.031087500974535942, 'motion_component': 0.0007926106918603182, 'motion_component_percent': 3.108750097453594}, {'resid': 1313, 'atom': 'C21', 'charge': 0.6299999952316284, 'distance': 24.2667236328125, 'force': [-0.27260878682136536, -0.16287244856357574, 0.15910494327545166], 'magnitude': 0.355186402797699, 'cosine_with_motion': 0.141879141330719, 'motion_component': 0.050393544137477875, 'motion_component_percent': 14.1879141330719}, {'resid': 1313, 'atom': 'C210', 'charge': -0.18000000715255737, 'distance': 19.1586971282959, 'force': [0.133111372590065, 0.08970475941896439, -0.027225283905863762], 'magnitude': 0.1628090739250183, 'cosine_with_motion': -0.41604867577552795, 'motion_component': -0.06773649901151657, 'motion_component_percent': 41.604867577552795}, {'resid': 1313, 'atom': 'C211', 'charge': -0.15000000596046448, 'distance': 18.513385772705078, 'force': [0.12457168847322464, 0.07165678590536118, -0.021412882953882217], 'magnitude': 0.1452973186969757, 'cosine_with_motion': -0.40077149868011475, 'motion_component': -0.05823102220892906, 'motion_component_percent': 40.077149868011475}, {'resid': 1313, 'atom': 'C212', 'charge': -0.15000000596046448, 'distance': 17.994733810424805, 'force': [0.1343480348587036, 0.07378401607275009, -0.01261032186448574], 'magnitude': 0.15379367768764496, 'cosine_with_motion': -0.4425811171531677, 'motion_component': -0.06806617975234985, 'motion_component_percent': 44.25811171531677}, {'resid': 1313, 'atom': 'C213', 'charge': -0.18000000715255737, 'distance': 17.986648559570312, 'force': [0.1571728140115738, 0.09699719399213791, -0.0030221142806112766], 'magnitude': 0.18471838533878326, 'cosine_with_motion': -0.5149979591369629, 'motion_component': -0.09512959420681, 'motion_component_percent': 51.49979591369629}, {'resid': 1313, 'atom': 'C214', 'charge': -0.15000000596046448, 'distance': 19.369552612304688, 'force': [0.11381798982620239, 0.06824129074811935, 0.002749041188508272], 'magnitude': 0.1327364444732666, 'cosine_with_motion': -0.5359206199645996, 'motion_component': -0.07113619893789291, 'motion_component_percent': 53.59206199645996}, {'resid': 1313, 'atom': 'C215', 'charge': -0.15000000596046448, 'distance': 19.82146453857422, 'force': [0.10726690292358398, 0.06669436395168304, 0.010581561364233494], 'magnitude': 0.12675289809703827, 'cosine_with_motion': -0.5867951512336731, 'motion_component': -0.07437798380851746, 'motion_component_percent': 58.67951512336731}, {'resid': 1313, 'atom': 'C216', 'charge': -0.18000000715255737, 'distance': 19.071619033813477, 'force': [0.13475489616394043, 0.09108933806419373, 0.023196522146463394], 'magnitude': 0.16429920494556427, 'cosine_with_motion': -0.6414923071861267, 'motion_component': -0.10539668053388596, 'motion_component_percent': 64.14923071861267}, {'resid': 1313, 'atom': 'C217', 'charge': -0.18000000715255737, 'distance': 19.884531021118164, 'force': [0.11817985773086548, 0.09046903252601624, 0.026310212910175323], 'magnitude': 0.15114016830921173, 'cosine_with_motion': -0.6861813068389893, 'motion_component': -0.10370955616235733, 'motion_component_percent': 68.61813068389893}, {'resid': 1313, 'atom': 'C218', 'charge': -0.18000000715255737, 'distance': 19.588125228881836, 'force': [0.11801009625196457, 0.09393896162509918, 0.03881748393177986], 'magnitude': 0.1557488590478897, 'cosine_with_motion': -0.7382859587669373, 'motion_component': -0.11498719453811646, 'motion_component_percent': 73.82859587669373}, {'resid': 1313, 'atom': 'C219', 'charge': -0.18000000715255737, 'distance': 20.55119514465332, 'force': [0.10154852271080017, 0.09060897678136826, 0.03870806843042374], 'magnitude': 0.14149346947669983, 'cosine_with_motion': -0.7718603014945984, 'motion_component': -0.10921318829059601, 'motion_component_percent': 77.18603014945984}, {'resid': 1313, 'atom': 'C22', 'charge': -0.08000000566244125, 'distance': 22.917572021484375, 'force': [0.03896016627550125, 0.02400871366262436, -0.021517163142561913], 'magnitude': 0.05056976526975632, 'cosine_with_motion': -0.16938169300556183, 'motion_component': -0.00856559257954359, 'motion_component_percent': 16.938169300556183}, {'resid': 1313, 'atom': 'C220', 'charge': -0.27000001072883606, 'distance': 20.84528160095215, 'force': [0.14344924688339233, 0.1300378441810608, 0.07120141386985779], 'magnitude': 0.20629389584064484, 'cosine_with_motion': -0.8121806383132935, 'motion_component': -0.16754791140556335, 'motion_component_percent': 81.21806383132935}, {'resid': 1313, 'atom': 'C23', 'charge': -0.18000000715255737, 'distance': 21.92696762084961, 'force': [0.09204868227243423, 0.06006483733654022, -0.05803867056965828], 'magnitude': 0.1242949366569519, 'cosine_with_motion': -0.13869254291057587, 'motion_component': -0.017238780856132507, 'motion_component_percent': 13.869254291057587}, {'resid': 1313, 'atom': 'C24', 'charge': -0.18000000715255737, 'distance': 20.547983169555664, 'force': [0.10519500821828842, 0.07073067873716354, -0.0629611611366272], 'magnitude': 0.14153772592544556, 'cosine_with_motion': -0.16607330739498138, 'motion_component': -0.023505639284849167, 'motion_component_percent': 16.60733073949814}, {'resid': 1313, 'atom': 'C25', 'charge': -0.15000000596046448, 'distance': 20.803699493408203, 'force': [0.08460602164268494, 0.06353720277547836, -0.04522281512618065], 'magnitude': 0.11506631970405579, 'cosine_with_motion': -0.236328586935997, 'motion_component': -0.02719346061348915, 'motion_component_percent': 23.6328586935997}, {'resid': 1313, 'atom': 'C26', 'charge': -0.15000000596046448, 'distance': 20.841411590576172, 'force': [0.08716646581888199, 0.06379438936710358, -0.03843134269118309], 'magnitude': 0.11465027183294296, 'cosine_with_motion': -0.2861766219139099, 'motion_component': -0.03281022608280182, 'motion_component_percent': 28.61766219139099}, {'resid': 1313, 'atom': 'C27', 'charge': -0.18000000715255737, 'distance': 20.667449951171875, 'force': [0.11263396590948105, 0.07128126174211502, -0.04250064492225647], 'magnitude': 0.1399061530828476, 'cosine_with_motion': -0.28748559951782227, 'motion_component': -0.04022100567817688, 'motion_component_percent': 28.748559951782227}, {'resid': 1313, 'atom': 'C28', 'charge': -0.15000000596046448, 'distance': 21.223026275634766, 'force': [0.09068571776151657, 0.05751761049032211, -0.026311183348298073], 'magnitude': 0.11056425422430038, 'cosine_with_motion': -0.3452751338481903, 'motion_component': -0.03817508742213249, 'motion_component_percent': 34.52751338481903}, {'resid': 1313, 'atom': 'C29', 'charge': -0.15000000596046448, 'distance': 20.56186294555664, 'force': [0.09719741344451904, 0.06296227872371674, -0.02150915563106537], 'magnitude': 0.11778891831636429, 'cosine_with_motion': -0.3957271873950958, 'motion_component': -0.04661227762699127, 'motion_component_percent': 39.57271873950958}, {'resid': 1313, 'atom': 'C3', 'charge': 0.06000000238418579, 'distance': 28.90619468688965, 'force': [-0.014464004896581173, -0.011485214345157146, 0.015074190683662891], 'magnitude': 0.02384006790816784, 'cosine_with_motion': -0.010134901851415634, 'motion_component': -0.00024161674082279205, 'motion_component_percent': 1.0134901851415634}, {'resid': 1313, 'atom': 'C31', 'charge': 0.6299999952316284, 'distance': 28.794885635375977, 'force': [-0.19339044392108917, -0.11927630007266998, 0.10958223789930344], 'magnitude': 0.2522597014904022, 'cosine_with_motion': 0.16087180376052856, 'motion_component': 0.04058147221803665, 'motion_component_percent': 16.087180376052856}, {'resid': 1313, 'atom': 'C310', 'charge': -0.18000000715255737, 'distance': 23.898391723632812, 'force': [0.0930081158876419, 0.04390237480401993, -0.01924494467675686], 'magnitude': 0.1046341061592102, 'cosine_with_motion': -0.3326317071914673, 'motion_component': -0.03480461984872818, 'motion_component_percent': 33.26317071914673}, {'resid': 1313, 'atom': 'C311', 'charge': -0.18000000715255737, 'distance': 23.0015926361084, 'force': [0.10301720350980759, 0.04287240654230118, -0.017539100721478462], 'magnitude': 0.11295223236083984, 'cosine_with_motion': -0.33188602328300476, 'motion_component': -0.03748726844787598, 'motion_component_percent': 33.188602328300476}, {'resid': 1313, 'atom': 'C312', 'charge': -0.18000000715255737, 'distance': 21.698305130004883, 'force': [0.11488749831914902, 0.051510196179151535, -0.016074564307928085], 'magnitude': 0.126928448677063, 'cosine_with_motion': -0.3683798611164093, 'motion_component': -0.046757884323596954, 'motion_component_percent': 36.83798611164093}, {'resid': 1313, 'atom': 'C313', 'charge': -0.18000000715255737, 'distance': 20.982715606689453, 'force': [0.12592166662216187, 0.04934721440076828, -0.01149718090891838], 'magnitude': 0.13573355972766876, 'cosine_with_motion': -0.3756290078163147, 'motion_component': -0.050985462963581085, 'motion_component_percent': 37.56290078163147}, {'resid': 1313, 'atom': 'C314', 'charge': -0.18000000715255737, 'distance': 20.27346420288086, 'force': [0.1371113508939743, 0.04514959827065468, -0.01738402619957924], 'magnitude': 0.14539675414562225, 'cosine_with_motion': -0.31879910826683044, 'motion_component': -0.04635235667228699, 'motion_component_percent': 31.879910826683044}, {'resid': 1313, 'atom': 'C315', 'charge': -0.18000000715255737, 'distance': 20.07476043701172, 'force': [0.14298324286937714, 0.03784162178635597, -0.010655121877789497], 'magnitude': 0.14828933775424957, 'cosine_with_motion': -0.32130998373031616, 'motion_component': -0.047646842896938324, 'motion_component_percent': 32.130998373031616}, {'resid': 1313, 'atom': 'C316', 'charge': -0.18000000715255737, 'distance': 19.378293991088867, 'force': [0.15545998513698578, 0.03073222190141678, -0.014604073017835617], 'magnitude': 0.15914005041122437, 'cosine_with_motion': -0.2687512934207916, 'motion_component': -0.042769093066453934, 'motion_component_percent': 26.875129342079163}, {'resid': 1313, 'atom': 'C317', 'charge': -0.18000000715255737, 'distance': 20.180044174194336, 'force': [0.14329437911510468, 0.022820644080638885, -0.02191665768623352], 'magnitude': 0.14674603939056396, 'cosine_with_motion': -0.20233756303787231, 'motion_component': -0.029692236334085464, 'motion_component_percent': 20.23375630378723}, {'resid': 1313, 'atom': 'C318', 'charge': -0.27000001072883606, 'distance': 19.949909210205078, 'force': [0.22190682590007782, 0.01804368384182453, -0.034042488783597946], 'magnitude': 0.2252267748117447, 'cosine_with_motion': -0.15325959026813507, 'motion_component': -0.03451816365122795, 'motion_component_percent': 15.325959026813507}, {'resid': 1313, 'atom': 'C32', 'charge': -0.08000000566244125, 'distance': 29.07960319519043, 'force': [0.024987589567899704, 0.014480353333055973, -0.012347130104899406], 'magnitude': 0.03140878677368164, 'cosine_with_motion': -0.18906228244304657, 'motion_component': -0.005938217043876648, 'motion_component_percent': 18.906228244304657}, {'resid': 1313, 'atom': 'C33', 'charge': -0.18000000715255737, 'distance': 28.492843627929688, 'force': [0.0604848712682724, 0.031019188463687897, -0.028246736153960228], 'magnitude': 0.07361038029193878, 'cosine_with_motion': -0.1752934604883194, 'motion_component': -0.012903418391942978, 'motion_component_percent': 17.52934604883194}, {'resid': 1313, 'atom': 'C34', 'charge': -0.18000000715255737, 'distance': 26.975563049316406, 'force': [0.06781422346830368, 0.0345173254609108, -0.030888836830854416], 'magnitude': 0.08212389796972275, 'cosine_with_motion': -0.18093357980251312, 'motion_component': -0.014858971349895, 'motion_component_percent': 18.093357980251312}, {'resid': 1313, 'atom': 'C35', 'charge': -0.18000000715255737, 'distance': 26.589866638183594, 'force': [0.07045482099056244, 0.03781762346625328, -0.0273896511644125], 'magnitude': 0.08452364802360535, 'cosine_with_motion': -0.2380400449037552, 'motion_component': -0.020120013505220413, 'motion_component_percent': 23.80400449037552}, {'resid': 1313, 'atom': 'C36', 'charge': -0.18000000715255737, 'distance': 25.12306785583496, 'force': [0.07953671365976334, 0.04229864850640297, -0.029143230989575386], 'magnitude': 0.09468153119087219, 'cosine_with_motion': -0.25070425868034363, 'motion_component': -0.023737061768770218, 'motion_component_percent': 25.070425868034363}, {'resid': 1313, 'atom': 'C37', 'charge': -0.18000000715255737, 'distance': 24.51609992980957, 'force': [0.08604151010513306, 0.039332129061222076, -0.030589720234274864], 'magnitude': 0.09942780435085297, 'cosine_with_motion': -0.22250650823116302, 'motion_component': -0.02212333306670189, 'motion_component_percent': 22.250650823116302}, {'resid': 1313, 'atom': 'C38', 'charge': -0.18000000715255737, 'distance': 25.142972946166992, 'force': [0.08424026519060135, 0.034616705030202866, -0.02532784454524517], 'magnitude': 0.09453167766332626, 'cosine_with_motion': -0.2373119592666626, 'motion_component': -0.02243349701166153, 'motion_component_percent': 23.73119592666626}, {'resid': 1313, 'atom': 'C39', 'charge': -0.18000000715255737, 'distance': 25.2009220123291, 'force': [0.0841837227344513, 0.03688095137476921, -0.02017975226044655], 'magnitude': 0.09409742802381516, 'cosine_with_motion': -0.2936190664768219, 'motion_component': -0.02762879990041256, 'motion_component_percent': 29.36190664768219}, {'resid': 1313, 'atom': 'C4', 'charge': 0.08000000566244125, 'distance': 28.961231231689453, 'force': [-0.01785549893975258, -0.01550876535475254, 0.02105703577399254], 'magnitude': 0.03166606277227402, 'cosine_with_motion': -0.0375639945268631, 'motion_component': -0.0011895038187503815, 'motion_component_percent': 3.75639945268631}, {'resid': 1313, 'atom': 'C5', 'charge': 0.08000000566244125, 'distance': 27.557458877563477, 'force': [-0.019271403551101685, -0.01665729470551014, 0.02396566793322563], 'magnitude': 0.0349743589758873, 'cosine_with_motion': -0.06380857527256012, 'motion_component': -0.0022316640242934227, 'motion_component_percent': 6.380857527256012}, {'resid': 1313, 'atom': 'C6', 'charge': 0.06000000238418579, 'distance': 26.437026977539062, 'force': [-0.015901362523436546, -0.014449967071413994, 0.018726110458374023], 'magnitude': 0.02850126475095749, 'cosine_with_motion': -0.02174658514559269, 'motion_component': -0.0006198051851242781, 'motion_component_percent': 2.174658514559269}, {'resid': 1313, 'atom': 'H1', 'charge': 0.12000000476837158, 'distance': 25.97567367553711, 'force': [-0.036708757281303406, -0.028122611343860626, 0.03671428933739662], 'magnitude': 0.059045348316431046, 'cosine_with_motion': -0.002963850274682045, 'motion_component': -0.00017500156536698341, 'motion_component_percent': 0.2963850274682045}, {'resid': 1313, 'atom': 'H10R', 'charge': 0.09000000357627869, 'distance': 19.15447425842285, 'force': [-0.06529896706342697, -0.04761362820863724, 0.010076320730149746], 'magnitude': 0.08144044131040573, 'cosine_with_motion': 0.46625447273254395, 'motion_component': 0.037971969693899155, 'motion_component_percent': 46.625447273254395}, {'resid': 1313, 'atom': 'H10S', 'charge': 0.09000000357627869, 'distance': 18.675268173217773, 'force': [-0.06817626953125, -0.04861852526664734, 0.01811622641980648], 'magnitude': 0.08567357808351517, 'cosine_with_motion': 0.39034146070480347, 'motion_component': 0.033441949635744095, 'motion_component_percent': 39.03414607048035}, {'resid': 1313, 'atom': 'H10X', 'charge': 0.09000000357627869, 'distance': 23.39503288269043, 'force': [-0.047576628625392914, -0.024077538400888443, 0.011708194389939308], 'magnitude': 0.05459253862500191, 'cosine_with_motion': 0.321015328168869, 'motion_component': 0.017525041475892067, 'motion_component_percent': 32.1015328168869}, {'resid': 1313, 'atom': 'H10Y', 'charge': 0.09000000357627869, 'distance': 24.240501403808594, 'force': [-0.044728197157382965, -0.02287908084690571, 0.007857173681259155], 'magnitude': 0.050850752741098404, 'cosine_with_motion': 0.3718695640563965, 'motion_component': 0.018909847363829613, 'motion_component_percent': 37.18695640563965}, {'resid': 1313, 'atom': 'H111', 'charge': 0.15000000596046448, 'distance': 18.59153938293457, 'force': [-0.12522360682487488, -0.0657220333814621, 0.027535896748304367], 'magnitude': 0.144078329205513, 'cosine_with_motion': 0.34732213616371155, 'motion_component': 0.05004159361124039, 'motion_component_percent': 34.732213616371155}, {'resid': 1313, 'atom': 'H11A', 'charge': 0.09000000357627869, 'distance': 26.74968719482422, 'force': [-0.028570929542183876, -0.02019382081925869, 0.022796278819441795], 'magnitude': 0.04175833612680435, 'cosine_with_motion': 0.06992106884717941, 'motion_component': 0.0029197875410318375, 'motion_component_percent': 6.992106884717941}, {'resid': 1313, 'atom': 'H11B', 'charge': 0.09000000357627869, 'distance': 25.3295955657959, 'force': [-0.03305971249938011, -0.021026913076639175, 0.025176730006933212], 'magnitude': 0.046571917831897736, 'cosine_with_motion': 0.05808141082525253, 'motion_component': 0.002704962622374296, 'motion_component_percent': 5.808141082525253}, {'resid': 1313, 'atom': 'H11X', 'charge': 0.09000000357627869, 'distance': 23.60810661315918, 'force': [-0.049528881907463074, -0.019452590495347977, 0.006533311679959297], 'magnitude': 0.05361154302954674, 'cosine_with_motion': 0.34751009941101074, 'motion_component': 0.018630553036928177, 'motion_component_percent': 34.751009941101074}, {'resid': 1313, 'atom': 'H11Y', 'charge': 0.09000000357627869, 'distance': 22.766159057617188, 'force': [-0.05307473987340927, -0.01983572728931904, 0.010637934319674969], 'magnitude': 0.057650238275527954, 'cosine_with_motion': 0.2892298400402069, 'motion_component': 0.016674168407917023, 'motion_component_percent': 28.92298400402069}, {'resid': 1313, 'atom': 'H12', 'charge': 0.09000000357627869, 'distance': 26.60165023803711, 'force': [-0.03162373602390289, -0.01921144872903824, 0.020341070368885994], 'magnitude': 0.042224396020174026, 'cosine_with_motion': 0.11118625104427338, 'motion_component': 0.0046947724185884, 'motion_component_percent': 11.118625104427338}, {'resid': 1313, 'atom': 'H121', 'charge': 0.15000000596046448, 'distance': 17.702489852905273, 'force': [-0.14311909675598145, -0.06813277304172516, 0.011328306049108505], 'magnitude': 0.15891344845294952, 'cosine_with_motion': 0.42247143387794495, 'motion_component': 0.06713639199733734, 'motion_component_percent': 42.247143387794495}, {'resid': 1313, 'atom': 'H12X', 'charge': 0.09000000357627869, 'distance': 21.212501525878906, 'force': [-0.05909379944205284, -0.028231369331479073, 0.010975229553878307], 'magnitude': 0.06640438735485077, 'cosine_with_motion': 0.3499731123447418, 'motion_component': 0.023239750415086746, 'motion_component_percent': 34.99731123447418}, {'resid': 1313, 'atom': 'H12Y', 'charge': 0.09000000357627869, 'distance': 21.88981819152832, 'force': [-0.05570612847805023, -0.02742418460547924, 0.005773632787168026], 'magnitude': 0.062358587980270386, 'cosine_with_motion': 0.41281312704086304, 'motion_component': 0.025742443278431892, 'motion_component_percent': 41.281312704086304}, {'resid': 1313, 'atom': 'H13A', 'charge': 0.09000000357627869, 'distance': 28.16581153869629, 'force': [-0.026727067306637764, -0.01921745017170906, 0.01830282248556614], 'magnitude': 0.037664834409952164, 'cosine_with_motion': 0.13615688681602478, 'motion_component': 0.0051283263601362705, 'motion_component_percent': 13.615688681602478}, {'resid': 1313, 'atom': 'H13B', 'charge': 0.09000000357627869, 'distance': 27.04791831970215, 'force': [-0.02862551063299179, -0.022416947409510612, 0.018605777993798256], 'magnitude': 0.040842555463314056, 'cosine_with_motion': 0.18168264627456665, 'motion_component': 0.007420383859425783, 'motion_component_percent': 18.168264627456665}, {'resid': 1313, 'atom': 'H13R', 'charge': 0.09000000357627869, 'distance': 17.24496078491211, 'force': [-0.0859355702996254, -0.051980432122945786, -0.00287288473919034], 'magnitude': 0.10047458112239838, 'cosine_with_motion': 0.5432800054550171, 'motion_component': 0.054585833102464676, 'motion_component_percent': 54.32800054550171}, {'resid': 1313, 'atom': 'H13S', 'charge': 0.09000000357627869, 'distance': 17.812740325927734, 'force': [-0.0770445391535759, -0.054081711918115616, 0.002750380663201213], 'magnitude': 0.0941714197397232, 'cosine_with_motion': 0.531143844127655, 'motion_component': 0.05001857131719589, 'motion_component_percent': 53.1143844127655}, {'resid': 1313, 'atom': 'H13X', 'charge': 0.09000000357627869, 'distance': 20.26738166809082, 'force': [-0.06680478900671005, -0.02848099358379841, 0.004165853839367628], 'magnitude': 0.07274201512336731, 'cosine_with_motion': 0.41186994314193726, 'motion_component': 0.029960250481963158, 'motion_component_percent': 41.186994314193726}, {'resid': 1313, 'atom': 'H13Y', 'charge': 0.09000000357627869, 'distance': 21.801342010498047, 'force': [-0.05880223214626312, -0.021968267858028412, 0.0034346485044807196], 'magnitude': 0.06286576390266418, 'cosine_with_motion': 0.38967037200927734, 'motion_component': 0.024496925994753838, 'motion_component_percent': 38.967037200927734}, {'resid': 1313, 'atom': 'H141', 'charge': 0.15000000596046448, 'distance': 20.022850036621094, 'force': [-0.10849572718143463, -0.06047064810991287, 0.0012618802720680833], 'magnitude': 0.1242160052061081, 'cosine_with_motion': 0.499062180519104, 'motion_component': 0.061991509050130844, 'motion_component_percent': 49.9062180519104}, {'resid': 1313, 'atom': 'H14X', 'charge': 0.09000000357627869, 'distance': 19.387605667114258, 'force': [-0.07419595867395401, -0.026099948212504387, 0.011532049626111984], 'magnitude': 0.07949361950159073, 'cosine_with_motion': 0.3100535571575165, 'motion_component': 0.02464728057384491, 'motion_component_percent': 31.005355715751648}, {'resid': 1313, 'atom': 'H14Y', 'charge': 0.09000000357627869, 'distance': 20.905141830444336, 'force': [-0.06456828117370605, -0.019747747108340263, 0.01075221411883831], 'magnitude': 0.06837138533592224, 'cosine_with_motion': 0.2775871455669403, 'motion_component': 0.018979016691446304, 'motion_component_percent': 27.75871455669403}, {'resid': 1313, 'atom': 'H151', 'charge': 0.15000000596046448, 'distance': 20.775087356567383, 'force': [-0.09871416538953781, -0.05862746760249138, -0.01147520262748003], 'magnitude': 0.11538348346948624, 'cosine_with_motion': 0.5883983373641968, 'motion_component': 0.0678914487361908, 'motion_component_percent': 58.83983373641968}, {'resid': 1313, 'atom': 'H15X', 'charge': 0.09000000357627869, 'distance': 19.562753677368164, 'force': [-0.07511989772319794, -0.02118750661611557, 0.002009943826124072], 'magnitude': 0.0780765563249588, 'cosine_with_motion': 0.3648073077201843, 'motion_component': 0.028482897207140923, 'motion_component_percent': 36.48073077201843}, {'resid': 1313, 'atom': 'H15Y', 'charge': 0.09000000357627869, 'distance': 21.062604904174805, 'force': [-0.06522068381309509, -0.0164446122944355, 0.0035003924276679754], 'magnitude': 0.06735292077064514, 'cosine_with_motion': 0.32927602529525757, 'motion_component': 0.02217770181596279, 'motion_component_percent': 32.92760252952576}, {'resid': 1313, 'atom': 'H16R', 'charge': 0.09000000357627869, 'distance': 18.74248504638672, 'force': [-0.07118667662143707, -0.044007446616888046, -0.015199799090623856], 'magnitude': 0.08506017178297043, 'cosine_with_motion': 0.6477344632148743, 'motion_component': 0.05509640648961067, 'motion_component_percent': 64.77344632148743}, {'resid': 1313, 'atom': 'H16S', 'charge': 0.09000000357627869, 'distance': 18.168678283691406, 'force': [-0.07316059619188309, -0.05219555273652077, -0.010799090377986431], 'magnitude': 0.09051778167486191, 'cosine_with_motion': 0.6377906203269958, 'motion_component': 0.05773139372467995, 'motion_component_percent': 63.779062032699585}, {'resid': 1313, 'atom': 'H16X', 'charge': 0.09000000357627869, 'distance': 18.333724975585938, 'force': [-0.08651266992092133, -0.018219878897070885, 0.009272717870771885], 'magnitude': 0.08889538794755936, 'cosine_with_motion': 0.26671433448791504, 'motion_component': 0.023709673434495926, 'motion_component_percent': 26.671433448791504}, {'resid': 1313, 'atom': 'H16Y', 'charge': 0.09000000357627869, 'distance': 19.237173080444336, 'force': [-0.07959923893213272, -0.013007578440010548, 0.003740764921531081], 'magnitude': 0.08074174076318741, 'cosine_with_motion': 0.2823815643787384, 'motion_component': 0.022799979895353317, 'motion_component_percent': 28.23815643787384}, {'resid': 1313, 'atom': 'H17R', 'charge': 0.09000000357627869, 'distance': 19.819623947143555, 'force': [-0.057547423988580704, -0.04850906878709793, -0.011008155532181263], 'magnitude': 0.07606586068868637, 'cosine_with_motion': 0.6853670477867126, 'motion_component': 0.05213303491473198, 'motion_component_percent': 68.53670477867126}, {'resid': 1313, 'atom': 'H17S', 'charge': 0.09000000357627869, 'distance': 20.911418914794922, 'force': [-0.05421173945069313, -0.03988577052950859, -0.01180035900324583], 'magnitude': 0.06833034008741379, 'cosine_with_motion': 0.6778370141983032, 'motion_component': 0.046316832304000854, 'motion_component_percent': 67.78370141983032}, {'resid': 1313, 'atom': 'H17X', 'charge': 0.09000000357627869, 'distance': 20.08522605895996, 'force': [-0.07142814248800278, -0.012949646450579166, 0.014707439579069614], 'magnitude': 0.07406741380691528, 'cosine_with_motion': 0.17695669829845428, 'motion_component': 0.013106725178658962, 'motion_component_percent': 17.69566982984543}, {'resid': 1313, 'atom': 'H17Y', 'charge': 0.09000000357627869, 'distance': 21.2280216217041, 'force': [-0.06475471705198288, -0.010973814874887466, 0.009113973006606102], 'magnitude': 0.06630733609199524, 'cosine_with_motion': 0.21752800047397614, 'motion_component': 0.014423701912164688, 'motion_component_percent': 21.752800047397614}, {'resid': 1313, 'atom': 'H18R', 'charge': 0.09000000357627869, 'distance': 19.80225944519043, 'force': [-0.05969276279211044, -0.04265344515442848, -0.020586268976330757], 'magnitude': 0.07619932293891907, 'cosine_with_motion': 0.730293333530426, 'motion_component': 0.05564785748720169, 'motion_component_percent': 73.0293333530426}, {'resid': 1313, 'atom': 'H18S', 'charge': 0.09000000357627869, 'distance': 18.560165405273438, 'force': [-0.06457874923944473, -0.05352336913347244, -0.022103700786828995], 'magnitude': 0.08673949539661407, 'cosine_with_motion': 0.7486852407455444, 'motion_component': 0.06494057923555374, 'motion_component_percent': 74.86852407455444}, {'resid': 1313, 'atom': 'H18X', 'charge': 0.09000000357627869, 'distance': 20.729679107666016, 'force': [-0.06821741908</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>699</v>
-      </c>
-      <c r="B7" t="n">
-        <v>787</v>
-      </c>
-      <c r="C7" t="n">
-        <v>2520</v>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>{699: {'frame': 699, 'motion_vector': [5.170875549316406, -1.8740463256835938, 2.9829635620117188], 'ionic_force': [-0.6573584005236626, 7.503577142953873, -3.2780375480651855], 'ionic_force_magnitude': 8.214701465879575, 'radial_force': 7.532316377250682, 'axial_force': -3.2780375480651855, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [3.6204872131347656, -0.4675694704055786, -2.093546688556671], 'asn_force_magnitude': 4.208264084785352, 'residue_force': [3.6204872131347656, -0.4675694704055786, -2.093546688556671], 'residue_force_magnitude': 4.208264084785352, 'pip2_force': [0.8608761616051197, -0.04523953070292919, -4.586148631235119], 'pip2_force_magnitude': 4.6664669342595735, 'total_force': [3.8240049742162228, 6.990768141845365, -9.957732867856976], 'total_force_magnitude': 12.75344255969617, 'cosine_total_motion': -0.288624046786004, 'cosine_glu_motion': 0, 'cosine_asn_motion': 0.5071073425746244, 'cosine_residue_motion': 0.5071073425746244, 'cosine_pip2_motion': -0.3131808520488668, 'cosine_ionic_motion': -0.5299698043165189, 'motion_component_total': -3.680950202032362, 'motion_component_glu': 0, 'motion_component_asn': 2.1340416168877336, 'motion_component_residue': 2.1340416168877336, 'motion_component_ionic': -4.353543728390819, 'motion_component_pip2': -1.4614480905292766, 'motion_component_percent_total': 28.862404678600402, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 50.71073425746244, 'motion_component_percent_residue': 50.71073425746244, 'motion_component_percent_ionic': 52.996980431651885, 'motion_component_percent_pip2': 31.318085204886682, 'ionic_contributions': [{'ion_id': 2223, 'distance': 7.634133815765381, 'force': [-0.6771345138549805, 0.5627886652946472, -5.628182411193848], 'magnitude': 5.6966376304626465, 'cosine_ionic_motion': -0.5988484025001526, 'motion_component_ionic': -3.4114224910736084, 'motion_component_percent_ionic': 59.88484025001526}, {'ion_id': 2276, 'distance': 9.756134033203125, 'force': [-1.0542205572128296, -3.153040885925293, -1.055195689201355], 'magnitude': 3.488049030303955, 'cosine_ionic_motion': -0.12325363606214523, 'motion_component_ionic': -0.4299147129058838, 'motion_component_percent_ionic': 12.325363606214523}, {'ion_id': 2391, 'distance': 13.279114723205566, 'force': [-0.07784866541624069, 0.08934804797172546, -1.8790479898452759], 'magnitude': 1.8827811479568481, 'cosine_ionic_motion': -0.5241919755935669, 'motion_component_ionic': -0.9869387149810791, 'motion_component_percent_ionic': 52.41919755935669}, {'ion_id': 2397, 'distance': 5.402998447418213, 'force': [1.1518453359603882, 10.004481315612793, 5.284388542175293], 'magnitude': 11.372825622558594, 'cosine_ionic_motion': 0.04174268990755081, 'motion_component_ionic': 0.47473233938217163, 'motion_component_percent_ionic': 4.174268990755081}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 5.283040523529053, 'force': [6.178944110870361, 4.969132423400879, 3.086221933364868], 'magnitude': 8.508606910705566, 'cosine_with_motion': 0.5981600880622864, 'motion_component': 5.089509010314941, 'motion_component_percent': 59.81600880622864}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 4.861706733703613, 'force': [-4.712672233581543, -5.613819122314453, -4.188048362731934], 'magnitude': 8.441800117492676, 'cosine_with_motion': -0.4987007975578308, 'motion_component': -4.209932327270508, 'motion_component_percent': 49.87007975578308}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 4.806948184967041, 'force': [-11.324604034423828, -5.468269348144531, -3.493640184402466], 'magnitude': 13.051979064941406, 'cosine_with_motion': -0.7191859483718872, 'motion_component': -9.386799812316895, 'motion_component_percent': 71.91859483718872}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 3.9989867210388184, 'force': [7.725991249084473, 2.5652873516082764, 2.8208439350128174], 'magnitude': 8.61561393737793, 'cosine_with_motion': 0.8080123066902161, 'motion_component': 6.961522102355957, 'motion_component_percent': 80.8012306690216}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 5.429563522338867, 'force': [4.222662925720215, 1.9278398752212524, 0.5436672568321228], 'magnitude': 4.673652172088623, 'cosine_with_motion': 0.678597092628479, 'motion_component': 3.1715266704559326, 'motion_component_percent': 67.8597092628479}, {'resid': 786, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 5.841325759887695, 'force': [-3.5671839714050293, -5.903143882751465, 0.9318822622299194], 'magnitude': 6.959907531738281, 'cosine_with_motion': -0.10570015013217926, 'motion_component': -0.7356632947921753, 'motion_component_percent': 10.570015013217926}, {'resid': 786, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 4.738321304321289, 'force': [5.097349166870117, 7.055403232574463, -1.7944735288619995], 'magnitude': 8.887171745300293, 'cosine_with_motion': 0.13996343314647675, 'motion_component': 1.2438790798187256, 'motion_component_percent': 13.996343314647675}], 'pip2_contributions': [{'resid': 1313, 'atom': 'C1', 'charge': 0.06000000238418579, 'distance': 27.730552673339844, 'force': [-0.019282139837741852, -0.012298567220568657, 0.012164638377726078], 'magnitude': 0.025904325768351555, 'cosine_with_motion': -0.24908046424388885, 'motion_component': -0.006452261470258236, 'motion_component_percent': 24.908046424388885}, {'resid': 1313, 'atom': 'C11', 'charge': 0.17000000178813934, 'distance': 27.084714889526367, 'force': [-0.06316477060317993, -0.03291052579879761, 0.029094668105244637], 'magnitude': 0.07693757116794586, 'cosine_with_motion': -0.3700832426548004, 'motion_component': -0.028473306447267532, 'motion_component_percent': 37.00832426548004}, {'resid': 1313, 'atom': 'C12', 'charge': 0.04000000283122063, 'distance': 27.32697868347168, 'force': [-0.015079725533723831, -0.007345029152929783, 0.005907777696847916], 'magnitude': 0.017783403396606445, 'cosine_with_motion': -0.4186989367008209, 'motion_component': -0.0074458918534219265, 'motion_component_percent': 41.86989367008209}, {'resid': 1313, 'atom': 'C13', 'charge': -0.05000000074505806, 'distance': 28.46809196472168, 'force': [0.017330802977085114, 0.008962357416749, -0.006234455853700638], 'magnitude': 0.020482895895838737, 'cosine_with_motion': 0.4230894148349762, 'motion_component': 0.00866609625518322, 'motion_component_percent': 42.30894148349762}, {'resid': 1313, 'atom': 'C2', 'charge': 0.06000000238418579, 'distance': 29.24079704284668, 'force': [-0.01730094850063324, -0.011150346137583256, 0.01091441884636879], 'magnitude': 0.023297587409615517, 'cosine_with_motion': -0.2470167577266693, 'motion_component': -0.0057548945769667625, 'motion_component_percent': 24.70167577266693}, {'resid': 1313, 'atom': 'C21', 'charge': 0.6299999952316284, 'distance': 24.86958885192871, 'force': [-0.29014649987220764, -0.13558435440063477, 0.10860106348991394], 'magnitude': 0.3381749391555786, 'cosine_with_motion': -0.4358730614185333, 'motion_component': -0.1474013477563858, 'motion_component_percent': 43.58730614185333}, {'resid': 1313, 'atom': 'C210', 'charge': -0.18000000715255737, 'distance': 23.948673248291016, 'force': [0.0933164581656456, 0.0457383468747139, 0.0075286743231117725], 'magnitude': 0.10419519245624542, 'cosine_with_motion': 0.6431180238723755, 'motion_component': 0.0670098066329956, 'motion_component_percent': 64.31180238723755}, {'resid': 1313, 'atom': 'C211', 'charge': -0.15000000596046448, 'distance': 23.936250686645508, 'force': [0.0761050283908844, 0.04063335806131363, 0.010580644011497498], 'magnitude': 0.08691947162151337, 'cosine_with_motion': 0.6416255235671997, 'motion_component': 0.055769748985767365, 'motion_component_percent': 64.16255235671997}, {'resid': 1313, 'atom': 'C212', 'charge': -0.15000000596046448, 'distance': 24.675167083740234, 'force': [0.06964115798473358, 0.04152088984847069, 0.010770543478429317], 'magnitude': 0.08179168403148651, 'cosine_with_motion': 0.6143959164619446, 'motion_component': 0.05025247856974602, 'motion_component_percent': 61.43959164619446}, {'resid': 1313, 'atom': 'C213', 'charge': -0.18000000715255737, 'distance': 25.70513343811035, 'force': [0.07643406838178635, 0.04761559143662453, 0.008388765156269073], 'magnitude': 0.09044215083122253, 'cosine_with_motion': 0.5849637389183044, 'motion_component': 0.052905380725860596, 'motion_component_percent': 58.496373891830444}, {'resid': 1313, 'atom': 'C214', 'charge': -0.15000000596046448, 'distance': 26.834144592285156, 'force': [0.05729609355330467, 0.0378718301653862, 0.008121744729578495], 'magnitude': 0.06915982067584991, 'cosine_with_motion': 0.5766386389732361, 'motion_component': 0.03988022357225418, 'motion_component_percent': 57.66386389732361}, {'resid': 1313, 'atom': 'C215', 'charge': -0.15000000596046448, 'distance': 27.523487091064453, 'force': [0.053243547677993774, 0.0380367785692215, 0.006319105159491301], 'magnitude': 0.06573890149593353, 'cosine_with_motion': 0.5418745875358582, 'motion_component': 0.035622239112854004, 'motion_component_percent': 54.187458753585815}, {'resid': 1313, 'atom': 'C216', 'charge': -0.18000000715255737, 'distance': 27.519813537597656, 'force': [0.06309903413057327, 0.04724236950278282, 0.00361968157812953], 'magnitude': 0.07890774309635162, 'cosine_with_motion': 0.5034100413322449, 'motion_component': 0.039722949266433716, 'motion_component_percent': 50.34100413322449}, {'resid': 1313, 'atom': 'C217', 'charge': -0.18000000715255737, 'distance': 28.713232040405273, 'force': [0.058729518204927444, 0.04246637597680092, 0.0012183438520878553], 'magnitude': 0.07248471677303314, 'cosine_with_motion': 0.5021401643753052, 'motion_component': 0.03639748692512512, 'motion_component_percent': 50.21401643753052}, {'resid': 1313, 'atom': 'C218', 'charge': -0.18000000715255737, 'distance': 30.014999389648438, 'force': [0.05273507907986641, 0.04018338397145271, 0.0021119527518749237], 'magnitude': 0.06633365154266357, 'cosine_with_motion': 0.4907509684562683, 'motion_component': 0.032553303986787796, 'motion_component_percent': 49.07509684562683}, {'resid': 1313, 'atom': 'C219', 'charge': -0.18000000715255737, 'distance': 31.236278533935547, 'force': [0.04945216700434685, 0.03613151237368584, 0.0005625594640150666], 'magnitude': 0.061248015612363815, 'cosine_with_motion': 0.4949568510055542, 'motion_component': 0.030315125361084938, 'motion_component_percent': 49.49568510055542}, {'resid': 1313, 'atom': 'C22', 'charge': -0.08000000566244125, 'distance': 23.849021911621094, 'force': [0.040408339351415634, 0.019398245960474014, -0.01309441588819027], 'magnitude': 0.04669678211212158, 'cosine_with_motion': 0.4570322334766388, 'motion_component': 0.02134193480014801, 'motion_component_percent': 45.70322334766388}, {'resid': 1313, 'atom': 'C220', 'charge': -0.27000001072883606, 'distance': 31.554725646972656, 'force': [0.07226505130529404, 0.053572751581668854, -0.0035488491412252188], 'magnitude': 0.09002706408500671, 'cosine_with_motion': 0.4663529098033905, 'motion_component': 0.04198438301682472, 'motion_component_percent': 46.63529098033905}, {'resid': 1313, 'atom': 'C23', 'charge': -0.18000000715255737, 'distance': 23.892274856567383, 'force': [0.09378361701965332, 0.039690155535936356, -0.024265944957733154], 'magnitude': 0.10468768328428268, 'cosine_with_motion': 0.5162906646728516, 'motion_component': 0.05404927581548691, 'motion_component_percent': 51.629066467285156}, {'resid': 1313, 'atom': 'C24', 'charge': -0.18000000715255737, 'distance': 23.757366180419922, 'force': [0.09517543017864227, 0.04261760786175728, -0.018329141661524773], 'magnitude': 0.10588002949953079, 'cosine_with_motion': 0.5397908687591553, 'motion_component': 0.05715307593345642, 'motion_component_percent': 53.97908687591553}, {'resid': 1313, 'atom': 'C25', 'charge': -0.15000000596046448, 'distance': 23.89841651916504, 'force': [0.08050385117530823, 0.031496815383434296, -0.011403183452785015], 'magnitude': 0.08719490468502045, 'cosine_with_motion': 0.5924752354621887, 'motion_component': 0.051660820841789246, 'motion_component_percent': 59.24752354621887}, {'resid': 1313, 'atom': 'C26', 'charge': -0.15000000596046448, 'distance': 23.235082626342773, 'force': [0.08569306135177612, 0.03328832983970642, -0.007592818234115839], 'magnitude': 0.09224458783864975, 'cosine_with_motion': 0.6204090714454651, 'motion_component': 0.05722937732934952, 'motion_component_percent': 62.04090714454651}, {'resid': 1313, 'atom': 'C27', 'charge': -0.18000000715255737, 'distance': 22.508872985839844, 'force': [0.10740755498409271, 0.048375945538282394, -0.00599303562194109], 'magnitude': 0.1179513931274414, 'cosine_with_motion': 0.605492353439331, 'motion_component': 0.07141866534948349, 'motion_component_percent': 60.549235343933105}, {'resid': 1313, 'atom': 'C28', 'charge': -0.15000000596046448, 'distance': 22.082761764526367, 'force': [0.09394954890012741, 0.040007561445236206, 0.0013917884789407253], 'magnitude': 0.10212276875972748, 'cosine_with_motion': 0.6494507789611816, 'motion_component': 0.06632371246814728, 'motion_component_percent': 64.94507789611816}, {'resid': 1313, 'atom': 'C29', 'charge': -0.15000000596046448, 'distance': 22.749645233154297, 'force': [0.08777151256799698, 0.03894048184156418, 0.006222316529601812], 'magnitude': 0.09622326493263245, 'cosine_with_motion': 0.66346275806427, 'motion_component': 0.06384055316448212, 'motion_component_percent': 66.346275806427}, {'resid': 1313, 'atom': 'C3', 'charge': 0.06000000238418579, 'distance': 29.984729766845703, 'force': [-0.016188768669962883, -0.010106164962053299, 0.011254881508648396], 'magnitude': 0.0221558827906847, 'cosine_with_motion': -0.22505025565624237, 'motion_component': -0.004986186977475882, 'motion_component_percent': 22.505025565624237}, {'resid': 1313, 'atom': 'C31', 'charge': 0.6299999952316284, 'distance': 29.23139190673828, 'force': [-0.2165512591600418, -0.09601981192827225, 0.061676714569330215], 'magnitude': 0.24478207528591156, 'cosine_with_motion': -0.49350547790527344, 'motion_component': -0.12080129235982895, 'motion_component_percent': 49.350547790527344}, {'resid': 1313, 'atom': 'C310', 'charge': -0.18000000715255737, 'distance': 24.763416290283203, 'force': [0.0953722670674324, 0.01982802152633667, 0.002796048065647483], 'magnitude': 0.09745171666145325, 'cosine_with_motion': 0.7615376710891724, 'motion_component': 0.07421315461397171, 'motion_component_percent': 76.15376710891724}, {'resid': 1313, 'atom': 'C311', 'charge': -0.18000000715255737, 'distance': 25.760116577148438, 'force': [0.08892184495925903, 0.01414494775235653, 0.0017303524073213339], 'magnitude': 0.09005647152662277, 'cosine_with_motion': 0.7781385779380798, 'motion_component': 0.07007641345262527, 'motion_component_percent': 77.81385779380798}, {'resid': 1313, 'atom': 'C312', 'charge': -0.18000000715255737, 'distance': 25.283205032348633, 'force': [0.09298013895750046, 0.00940130464732647, 0.002435517031699419], 'magnitude': 0.09348594397306442, 'cosine_with_motion': 0.8042635321617126, 'motion_component': 0.0751873329281807, 'motion_component_percent': 80.42635321617126}, {'resid': 1313, 'atom': 'C313', 'charge': -0.18000000715255737, 'distance': 26.404399871826172, 'force': [0.08552572876214981, 0.005430405028164387, 0.0017207800410687923], 'magnitude': 0.08571523427963257, 'cosine_with_motion': 0.8152034878730774, 'motion_component': 0.06987535953521729, 'motion_component_percent': 81.52034878730774}, {'resid': 1313, 'atom': 'C314', 'charge': -0.18000000715255737, 'distance': 27.372879028320312, 'force': [0.07943124324083328, 0.004968713968992233, 0.005214711185544729], 'magnitude': 0.07975715398788452, 'cosine_with_motion': 0.8355700373649597, 'motion_component': 0.06664268672466278, 'motion_component_percent': 83.55700373649597}, {'resid': 1313, 'atom': 'C315', 'charge': -0.18000000715255737, 'distance': 28.42221450805664, 'force': [0.07384230941534042, 0.0013943914091214538, 0.004232986830174923], 'magnitude': 0.07397668063640594, 'cosine_with_motion': 0.8465685844421387, 'motion_component': 0.06262633204460144, 'motion_component_percent': 84.65685844421387}, {'resid': 1313, 'atom': 'C316', 'charge': -0.18000000715255737, 'distance': 28.995861053466797, 'force': [0.07106927037239075, 0.0010233749635517597, 0.0005222775507718325], 'magnitude': 0.07107856124639511, 'cosine_with_motion': 0.825518012046814, 'motion_component': 0.05867663398385048, 'motion_component_percent': 82.5518012046814}, {'resid': 1313, 'atom': 'C317', 'charge': -0.18000000715255737, 'distance': 30.07297706604004, 'force': [0.06606361269950867, -0.0013718706322833896, 0.00019109009008388966], 'magnitude': 0.06607813388109207, 'cosine_with_motion': 0.8338508605957031, 'motion_component': 0.055099308490753174, 'motion_component_percent': 83.38508605957031}, {'resid': 1313, 'atom': 'C318', 'charge': -0.27000001072883606, 'distance': 29.75384521484375, 'force': [0.10100200772285461, -0.006806361488997936, 0.0021920434664934874], 'magnitude': 0.10125481337308884, 'cosine_with_motion': 0.8548267483711243, 'motion_component': 0.08655532449483871, 'motion_component_percent': 85.48267483711243}, {'resid': 1313, 'atom': 'C32', 'charge': -0.08000000566244125, 'distance': 29.455713272094727, 'force': [0.027490273118019104, 0.012009941972792149, -0.006093375850468874], 'magnitude': 0.030611811205744743, 'cosine_with_motion': 0.5297527313232422, 'motion_component': 0.016216689720749855, 'motion_component_percent': 52.97527313232422}, {'resid': 1313, 'atom': 'C33', 'charge': -0.18000000715255737, 'distance': 28.387529373168945, 'force': [0.06779313087463379, 0.027059141546487808, -0.01308577973395586], 'magnitude': 0.07415755838155746, 'cosine_with_motion': 0.5620900392532349, 'motion_component': 0.041683223098516464, 'motion_component_percent': 56.209003925323486}, {'resid': 1313, 'atom': 'C34', 'charge': -0.18000000715255737, 'distance': 28.795791625976562, 'force': [0.06651068478822708, 0.02616306021809578, -0.009266158565878868], 'magnitude': 0.0720696821808815, 'cosine_with_motion': 0.5926594138145447, 'motion_component': 0.042712774127721786, 'motion_component_percent': 59.26594138145447}, {'resid': 1313, 'atom': 'C35', 'charge': -0.18000000715255737, 'distance': 27.56857681274414, 'force': [0.07320688664913177, 0.027679694816470146, -0.007555202580988407], 'magnitude': 0.07862884551286697, 'cosine_with_motion': 0.6181979179382324, 'motion_component': 0.04860818758606911, 'motion_component_percent': 61.81979179382324}, {'resid': 1313, 'atom': 'C36', 'charge': -0.18000000715255737, 'distance': 28.069046020507812, 'force': [0.07137943804264069, 0.02540396898984909, -0.0035817893221974373], 'magnitude': 0.07584995031356812, 'cosine_with_motion': 0.65489661693573, 'motion_component': 0.04967387765645981, 'motion_component_percent': 65.489661693573}, {'resid': 1313, 'atom': 'C37', 'charge': -0.18000000715255737, 'distance': 26.985700607299805, 'force': [0.0777549222111702, 0.026227684691548347, -0.0006969001842662692], 'magnitude': 0.08206220716238022, 'cosine_with_motion': 0.6832799911499023, 'motion_component': 0.05607146397233009, 'motion_component_percent': 68.32799911499023}, {'resid': 1313, 'atom': 'C38', 'charge': -0.18000000715255737, 'distance': 26.29918670654297, 'force': [0.08319058269262314, 0.023313380777835846, -0.0010925483657047153], 'magnitude': 0.08640243113040924, 'cosine_with_motion': 0.7088683247566223, 'motion_component': 0.061247944831848145, 'motion_component_percent': 70.88683247566223}, {'resid': 1313, 'atom': 'C39', 'charge': -0.18000000715255737, 'distance': 25.439516067504883, 'force': [0.08919260650873184, 0.023723391816020012, 0.0029453446622937918], 'magnitude': 0.09234064817428589, 'cosine_with_motion': 0.7365175485610962, 'motion_component': 0.06801050901412964, 'motion_component_percent': 73.65175485610962}, {'resid': 1313, 'atom': 'C4', 'charge': 0.08000000566244125, 'distance': 29.406368255615234, 'force': [-0.021480869501829147, -0.01427800115197897, 0.016676316037774086], 'magnitude': 0.03071463108062744, 'cosine_with_motion': -0.1798992156982422, 'motion_component': -0.005525538232177496, 'motion_component_percent': 17.98992156982422}, {'resid': 1313, 'atom': 'C5', 'charge': 0.08000000566244125, 'distance': 27.909412384033203, 'force': [-0.02400991879403591, -0.015430469997227192, 0.01865706779062748], 'magnitude': 0.0340978279709816, 'cosine_with_motion': -0.18552850186824799, 'motion_component': -0.00632611894980073, 'motion_component_percent': 18.5528501868248}, {'resid': 1313, 'atom': 'C6', 'charge': 0.06000000238418579, 'distance': 27.129344940185547, 'force': [-0.019299976527690887, -0.01299662608653307, 0.013824686408042908], 'magnitude': 0.02706516906619072, 'cosine_with_motion': -0.20197506248950958, 'motion_component': -0.0054664891213178635, 'motion_component_percent': 20.19750624895096}, {'resid': 1313, 'atom': 'H1', 'charge': 0.12000000476837158, 'distance': 27.443714141845703, 'force': [-0.040435079485177994, -0.023382920771837234, 0.024826763197779655], 'magnitude': 0.05289730429649353, 'cosine_with_motion': -0.2755740284919739, 'motion_component': -0.014577123336493969, 'motion_component_percent': 27.557402849197388}, {'resid': 1313, 'atom': 'H10R', 'charge': 0.09000000357627869, 'distance': 24.739301681518555, 'force': [-0.04435037821531296, -0.020061038434505463, -0.0037521100603044033], 'magnitude': 0.048820894211530685, 'cosine_with_motion': -0.664323627948761, 'motion_component': -0.03243287280201912, 'motion_component_percent': 66.4323627948761}, {'resid': 1313, 'atom': 'H10S', 'charge': 0.09000000357627869, 'distance': 24.011629104614258, 'force': [-0.045883920043706894, -0.02402385137975216, -0.0018239966593682766], 'magnitude': 0.051824767142534256, 'cosine_with_motion': -0.6096327304840088, 'motion_component': -0.03159407526254654, 'motion_component_percent': 60.96327304840088}, {'resid': 1313, 'atom': 'H10X', 'charge': 0.09000000357627869, 'distance': 24.00147819519043, 'force': [-0.050783902406692505, -0.010550505481660366, 0.0001883870136225596], 'magnitude': 0.05186861753463745, 'cosine_with_motion': -0.7464960217475891, 'motion_component': -0.03871971741318703, 'motion_component_percent': 74.64960217475891}, {'resid': 1313, 'atom': 'H10Y', 'charge': 0.09000000357627869, 'distance': 24.305870056152344, 'force': [-0.049456167966127396, -0.01000219490379095, -0.0034839569125324488], 'magnitude': 0.05057760700583458, 'cosine_with_motion': -0.7817186117172241, 'motion_component': -0.0395374558866024, 'motion_component_percent': 78.17186117172241}, {'resid': 1313, 'atom': 'H111', 'charge': 0.15000000596046448, 'distance': 23.244386672973633, 'force': [-0.08071717619895935, -0.042120009660720825, -0.014355908147990704], 'magnitude': 0.09217076748609543, 'cosine_with_motion': -0.6611204147338867, 'motion_component': -0.06093597412109375, 'motion_component_percent': 66.11204147338867}, {'resid': 1313, 'atom': 'H11A', 'charge': 0.09000000357627869, 'distance': 28.11920166015625, 'force': [-0.030773645266890526, -0.016269151121377945, 0.014709411188960075], 'magnitude': 0.03778980299830437, 'cosine_with_motion': -0.3584764897823334, 'motion_component': -0.013546755537390709, 'motion_component_percent': 35.84764897823334}, {'resid': 1313, 'atom': 'H11B', 'charge': 0.09000000357627869, 'distance': 26.486507415771484, 'force': [-0.03511406481266022, -0.017079874873161316, 0.017011335119605064], 'magnitude': 0.04259231314063072, 'cosine_with_motion': -0.37080761790275574, 'motion_component': -0.015793554484844208, 'motion_component_percent': 37.080761790275574}, {'resid': 1313, 'atom': 'H11X', 'charge': 0.09000000357627869, 'distance': 26.56309700012207, 'force': [-0.04170222952961922, -0.007105013355612755, -0.0019277473911643028], 'magnitude': 0.04234705865383148, 'cosine_with_motion': -0.7853004336357117, 'motion_component': -0.033255163580179214, 'motion_component_percent': 78.53004336357117}, {'resid': 1313, 'atom': 'H11Y', 'charge': 0.09000000357627869, 'distance': 26.286468505859375, 'force': [-0.04269217327237129, -0.006837464869022369, 0.000766381504945457], 'magnitude': 0.043243035674095154, 'cosine_with_motion': -0.7600991129875183, 'motion_component': -0.032868992537260056, 'motion_component_percent': 76.00991129875183}, {'resid': 1313, 'atom': 'H12', 'charge': 0.09000000357627869, 'distance': 27.58008575439453, 'force': [-0.0338219590485096, -0.014826618134975433, 0.013389998115599155], 'magnitude': 0.03928161785006523, 'cosine_with_motion': -0.4360077381134033, 'motion_component': -0.017127089202404022, 'motion_component_percent': 43.60077381134033}, {'resid': 1313, 'atom': 'H121', 'charge': 0.15000000596046448, 'distance': 24.64780616760254, 'force': [-0.06827235966920853, -0.043278515338897705, -0.013619461096823215], 'magnitude': 0.0819733738899231, 'cosine_with_motion': -0.6093812584877014, 'motion_component': -0.04995303601026535, 'motion_component_percent': 60.93812584877014}, {'resid': 1313, 'atom': 'H12X', 'charge': 0.09000000357627869, 'distance': 24.527080535888672, 'force': [-0.04947111755609512, -0.00442988658323884, 0.000183084441232495], 'magnitude': 0.04966939613223076, 'cosine_with_motion': -0.794665515422821, 'motion_component': -0.03947055712342262, 'motion_component_percent': 79.4665515422821}, {'resid': 1313, 'atom': 'H12Y', 'charge': 0.09000000357627869, 'distance': 24.835180282592773, 'force': [-0.04810182750225067, -0.004786095581948757, -0.0031926899682730436], 'magnitude': 0.04844466596841812, 'cosine_with_motion': -0.8224155306816101, 'motion_component': -0.03984164446592331, 'motion_component_percent': 82.24155306816101}, {'resid': 1313, 'atom': 'H13A', 'charge': 0.09000000357627869, 'distance': 29.414493560791016, 'force': [-0.029167240485548973, -0.014795828610658646, 0.01109111588448286], 'magnitude': 0.03453487157821655, 'cosine_with_motion': -0.41654953360557556, 'motion_component': -0.014385484158992767, 'motion_component_percent': 41.654953360557556}, {'resid': 1313, 'atom': 'H13B', 'charge': 0.09000000357627869, 'distance': 28.453506469726562, 'force': [-0.030559668317437172, -0.017403997480869293, 0.011195358820259571], 'magnitude': 0.036907024681568146, 'cosine_with_motion': -0.3984428346157074, 'motion_component': -0.014705339446663857, 'motion_component_percent': 39.84428346157074}, {'resid': 1313, 'atom': 'H13R', 'charge': 0.09000000357627869, 'distance': 25.333044052124023, 'force': [-0.038720812648534775, -0.025681735947728157, -0.00298490934073925], 'magnitude': 0.04655923694372177, 'cosine_with_motion': -0.5526535511016846, 'motion_component': -0.025731127709150314, 'motion_component_percent': 55.26535511016846}, {'resid': 1313, 'atom': 'H13S', 'charge': 0.09000000357627869, 'distance': 26.08206558227539, 'force': [-0.037888988852500916, -0.022021202370524406, -0.002960139187052846], 'magnitude': 0.04392346739768982, 'cosine_with_motion': -0.5948590040206909, 'motion_component': -0.026128269731998444, 'motion_component_percent': 59.48590040206909}, {'resid': 1313, 'atom': 'H13X', 'charge': 0.09000000357627869, 'distance': 26.815200805664062, 'force': [-0.041435521095991135, -0.003065626136958599, 0.0006924846675246954], 'magnitude': 0.041554540395736694, 'cosine_with_motion': -0.794026792049408, 'motion_component': -0.03299541771411896, 'motion_component_percent': 79.4026792049408}, {'resid': 1313, 'atom': 'H13Y', 'charge': 0.09000000357627869, 'distance': 25.94521141052246, 'force': [-0.04436831921339035, -0.0011400912189856172, -0.0006728777079842985], 'magnitude': 0.0443880632519722, 'cosine_with_motion': -0.8256018161773682, 'motion_component': -0.03664686530828476, 'motion_component_percent': 82.56018161773682}, {'resid': 1313, 'atom': 'H141', 'charge': 0.15000000596046448, 'distance': 27.05891227722168, 'force': [-0.05661053955554962, -0.0362214669585228, -0.010458365082740784], 'magnitude': 0.06801562756299973, 'cosine_with_motion': -0.6016552448272705, 'motion_component': -0.04092196002602577, 'motion_component_percent': 60.16552448272705}, {'resid': 1313, 'atom': 'H14X', 'charge': 0.09000000357627869, 'distance': 27.929527282714844, 'force': [-0.03803815692663193, -0.0036863002460449934, -0.0026017564814537764], 'magnitude': 0.03830482065677643, 'cosine_with_motion': -0.8242396712303162, 'motion_component': -0.03157235309481621, 'motion_component_percent': 82.42396712303162}, {'resid': 1313, 'atom': 'H14Y', 'charge': 0.09000000357627869, 'distance': 26.88328742980957, 'force': [-0.04106626287102699, -0.0023411051370203495, -0.004175468347966671], 'magnitude': 0.04134432598948479, 'cosine_with_motion': -0.8520653247833252, 'motion_component': -0.03522806614637375, 'motion_component_percent': 85.20653247833252}, {'resid': 1313, 'atom': 'H151', 'charge': 0.15000000596046448, 'distance': 28.345943450927734, 'force': [-0.049593523144721985, -0.03645175322890282, -0.0072939470410346985], 'magnitude': 0.06197942793369293, 'cosine_with_motion': -0.5412318110466003, 'motion_component': -0.03354523703455925, 'motion_component_percent': 54.123181104660034}, {'resid': 1313, 'atom': 'H15X', 'charge': 0.09000000357627869, 'distance': 27.96762466430664, 'force': [-0.03810669854283333, 0.000560825108550489, -0.002616451121866703], 'magnitude': 0.038200534880161285, 'cosine_with_motion': -0.8614564538002014, 'motion_component': -0.03290809690952301, 'motion_component_percent': 86.14564538002014}, {'resid': 1313, 'atom': 'H15Y', 'charge': 0.09000000357627869, 'distance': 29.295719146728516, 'force': [-0.034695103764534, -0.0009671602747403085, -0.002726068254560232], 'magnitude': 0.0348154716193676, 'cosine_with_motion': -0.8525875210762024, 'motion_component': -0.02968323603272438, 'motion_component_percent': 85.25875210762024}, {'resid': 1313, 'atom': 'H16R', 'charge': 0.09000000357627869, 'distance': 27.431198120117188, 'force': [-0.03078063204884529, -0.025015277788043022, -0.0018996003782376647], 'magnitude': 0.039709191769361496, 'cosine_with_motion': -0.4747333824634552, 'motion_component': -0.018851278349757195, 'motion_component_percent': 47.47333824634552}, {'resid': 1313, 'atom': 'H16S', 'charge': 0.09000000357627869, 'distance': 26.620155334472656, 'force': [-0.03403468430042267, -0.024867556989192963, -0.0010919328778982162], 'magnitude': 0.042165715247392654, 'cosine_with_motion': -0.5027717351913452, 'motion_component': -0.021199729293584824, 'motion_component_percent': 50.27717351913452}, {'resid': 1313, 'atom': 'H16X', 'charge': 0.09000000357627869, 'distance': 29.353063583374023, 'force': [-0.0346391387283802, -0.0016691082855686545, 0.000129871565150097], 'magnitude': 0.03467957302927971, 'cosine_with_motion': -0.8092706799507141, 'motion_component': -0.028065161779522896, 'motion_component_percent': 80.92706799507141}, {'resid': 1313, 'atom': 'H16Y', 'charge': 0.09000000357627869, 'distance': 28.200084686279297, 'force': [-0.03756917268037796, -8.249126949522179e-06, 0.0005591108347289264], 'magnitude': 0.03757333382964134, 'cosine_with_motion': -0.8191837668418884, 'motion_component': -0.030779464170336723, 'motion_component_percent': 81.91837668418884}, {'resid': 1313, 'atom': 'H17R', 'charge': 0.09000000357627869, 'distance': 28.606454849243164, 'force': [-0.029588675126433372, -0.02138078212738037, 0.0007761635351926088], 'magnitude': 0.036513421684503555, 'cosine_with_motion': -0.48418161273002625, 'motion_component': -0.01767912693321705, 'motion_component_percent': 48.418161273002625}, {'resid': 1313, 'atom': 'H17S', 'charge': 0.09000000357627869, 'distance': 28.834047317504883, 'force': [-0.029880594462156296, -0.019951988011598587, -0.0008368762210011482], 'magnitude': 0.035939283668994904, 'cosine_with_motion': -0.5319346785545349, 'motion_component': -0.01911735162138939, 'motion_component_percent': 53.19346785545349}, {'resid': 1313, 'atom': 'H17X', 'charge': 0.09000000357627869, 'distance': 30.27924156188965, 'force': [-0.03256048262119293, 0.0009346695733256638, 0.001039295457303524], 'magnitude': 0.03259047120809555, 'cosine_with_motion': -0.8190614581108093, 'motion_component': -0.026693599298596382, 'motion_component_percent': 81.90614581108093}, {'resid': 1313, 'atom': 'H17Y', 'charge': 0.09000000357627869, 'distance': 31.018585205078125, 'force': [-0.031046107411384583, 0.00044218168477527797, -0.0006159791373647749], 'magnitude': 0.03105536662042141, 'cosine_with_motion': -0.8399099707603455, 'motion_component': -0.02608371153473854, 'motion_component_percent': 8</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>706</v>
-      </c>
-      <c r="B8" t="n">
-        <v>959</v>
-      </c>
-      <c r="C8" t="n">
-        <v>2223</v>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>{706: {'frame': 706, 'motion_vector': [-1.6462364196777344, 4.194007873535156, 1.78082275390625], 'ionic_force': [-2.4678491204977036, -11.519292116165161, -0.8560818731784821], 'ionic_force_magnitude': 11.811741883086968, 'radial_force': 11.780677830205107, 'axial_force': -0.8560818731784821, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-5.030915379524231, -3.7795519828796387, -7.650073170661926], 'asn_force_magnitude': 9.905490511009754, 'residue_force': [-5.030915379524231, -3.7795519828796387, -7.650073170661926], 'residue_force_magnitude': 9.905490511009754, 'pip2_force': [0.7980182208120823, 0.1757741943001747, -4.670473291504095], 'pip2_force_magnitude': 4.741418607841228, 'total_force': [-6.700746279209852, -15.123069904744625, -13.176628335344503], 'total_force_magnitude': 21.147831527840886, 'cosine_total_motion': -0.7404281186684233, 'cosine_glu_motion': 0, 'cosine_asn_motion': -0.4416169984765415, 'cosine_residue_motion': -0.4416169984765415, 'cosine_pip2_motion': -0.3871798555103845, 'cosine_ionic_motion': -0.7999018642793536, 'motion_component_total': -15.658449112075996, 'motion_component_glu': 0, 'motion_component_asn': -4.374432987909991, 'motion_component_residue': -4.374432987909991, 'motion_component_ionic': -9.44823435266779, 'motion_component_pip2': -1.835781771498215, 'motion_component_percent_total': 74.04281186684233, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 44.16169984765415, 'motion_component_percent_residue': 44.16169984765415, 'motion_component_percent_ionic': 79.99018642793536, 'motion_component_percent_pip2': 38.717985551038446, 'ionic_contributions': [{'ion_id': 2276, 'distance': 7.746928691864014, 'force': [0.08160331845283508, -4.599984169006348, 3.07181715965271], 'magnitude': 5.531959533691406, 'cosine_ionic_motion': -0.5207458138465881, 'motion_component_ionic': -2.880744695663452, 'motion_component_percent_ionic': 52.07458138465881}, {'ion_id': 2391, 'distance': 10.210418701171875, 'force': [0.22415855526924133, -2.0812742710113525, -2.39990496635437], 'magnitude': 3.1845712661743164, 'cosine_ionic_motion': -0.8666999936103821, 'motion_component_ionic': -2.760067939758301, 'motion_component_percent_ionic': 86.66999936103821}, {'ion_id': 2397, 'distance': 8.644484519958496, 'force': [-3.0071139335632324, -3.044539213180542, -1.1944888830184937], 'magnitude': 4.442831993103027, 'cosine_ionic_motion': -0.4620648920536041, 'motion_component_ionic': -2.0528767108917236, 'motion_component_percent_ionic': 46.20648920536041}, {'ion_id': 2520, 'distance': 13.435805320739746, 'force': [0.23350293934345245, -1.793494462966919, -0.33350518345832825], 'magnitude': 1.8391225337982178, 'cosine_ionic_motion': -0.9540119171142578, 'motion_component_ionic': -1.7545448541641235, 'motion_component_percent_ionic': 95.40119171142578}], 'glu_contributions': [], 'asn_contributions': [{'resid': 1114, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 3.432359457015991, 'force': [-7.456222057342529, 15.6506929397583, 10.285576820373535], 'magnitude': 20.157691955566406, 'cosine_with_motion': 0.9853840470314026, 'motion_component': 19.863067626953125, 'motion_component_percent': 98.53840470314026}, {'resid': 1114, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 2.944586992263794, 'force': [0.87669837474823, -18.019702911376953, -14.28624439239502], 'magnitude': 23.01249885559082, 'cosine_with_motion': -0.9190108180046082, 'motion_component': -21.14873504638672, 'motion_component_percent': 91.90108180046082}, {'resid': 1114, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 3.606640577316284, 'force': [11.241238594055176, -19.941492080688477, -3.6771652698516846], 'magnitude': 23.18512725830078, 'cosine_with_motion': -0.9676286578178406, 'motion_component': -22.434593200683594, 'motion_component_percent': 96.76286578178406}, {'resid': 1114, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 3.16558575630188, 'force': [-4.855937957763672, 12.832906723022461, -0.8816777467727661], 'magnitude': 13.749217987060547, 'cosine_with_motion': 0.9044355750083923, 'motion_component': 12.435281753540039, 'motion_component_percent': 90.44355750083923}, {'resid': 1114, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 4.277791500091553, 'force': [-4.8366923332214355, 5.698043346405029, 0.9094374179840088], 'magnitude': 7.529167652130127, 'cosine_with_motion': 0.9178365468978882, 'motion_component': 6.910545349121094, 'motion_component_percent': 91.78365468978882}], 'pip2_contributions': [{'resid': 1313, 'atom': 'C1', 'charge': 0.06000000238418579, 'distance': 30.871591567993164, 'force': [-0.012777435593307018, -0.013791536912322044, 0.009131867438554764], 'magnitude': 0.020901205018162727, 'cosine_with_motion': -0.20289234817028046, 'motion_component': -0.004240694455802441, 'motion_component_percent': 20.289234817028046}, {'resid': 1313, 'atom': 'C11', 'charge': 0.17000000178813934, 'distance': 29.140981674194336, 'force': [-0.04518341273069382, -0.0424593985080719, 0.02393662929534912], 'magnitude': 0.06646279990673065, 'cosine_with_motion': -0.18964910507202148, 'motion_component': -0.012604610994458199, 'motion_component_percent': 18.96491050720215}, {'resid': 1313, 'atom': 'C12', 'charge': 0.04000000283122063, 'distance': 29.30089569091797, 'force': [-0.010950606316328049, -0.009779006242752075, 0.0048699751496315], 'magnitude': 0.015468076802790165, 'cosine_with_motion': -0.19100242853164673, 'motion_component': -0.00295444019138813, 'motion_component_percent': 19.100242853164673}, {'resid': 1313, 'atom': 'C13', 'charge': -0.05000000074505806, 'distance': 30.720081329345703, 'force': [0.012458797544240952, 0.011285570450127125, -0.00517869321629405], 'magnitude': 0.017589900642633438, 'cosine_with_motion': 0.20652152597904205, 'motion_component': 0.003632693085819483, 'motion_component_percent': 20.652152597904205}, {'resid': 1313, 'atom': 'C2', 'charge': 0.06000000238418579, 'distance': 32.439369201660156, 'force': [-0.011616370640695095, -0.012433290481567383, 0.008295061066746712], 'magnitude': 0.01892973482608795, 'cosine_with_motion': -0.19899912178516388, 'motion_component': -0.0037670007441192865, 'motion_component_percent': 19.899912178516388}, {'resid': 1313, 'atom': 'C21', 'charge': 0.6299999952316284, 'distance': 26.897424697875977, 'force': [-0.20379726588726044, -0.18704572319984436, 0.08404095470905304], 'magnitude': 0.2891060709953308, 'cosine_with_motion': -0.21369686722755432, 'motion_component': -0.061781059950590134, 'motion_component_percent': 21.369686722755432}, {'resid': 1313, 'atom': 'C210', 'charge': -0.18000000715255737, 'distance': 26.280900955200195, 'force': [0.06060691922903061, 0.061420634388923645, 0.006362891755998135], 'magnitude': 0.08652271330356598, 'cosine_with_motion': 0.4035446047782898, 'motion_component': 0.034915775060653687, 'motion_component_percent': 40.35446047782898}, {'resid': 1313, 'atom': 'C211', 'charge': -0.15000000596046448, 'distance': 26.54500961303711, 'force': [0.04955738037824631, 0.049580954015254974, 0.00898327399045229], 'magnitude': 0.07067463546991348, 'cosine_with_motion': 0.4157664477825165, 'motion_component': 0.02938414178788662, 'motion_component_percent': 41.57664477825165}, {'resid': 1313, 'atom': 'C212', 'charge': -0.15000000596046448, 'distance': 27.366361618041992, 'force': [0.045162416994571686, 0.04772859066724777, 0.01020051259547472], 'magnitude': 0.06649596244096756, 'cosine_with_motion': 0.4469657242298126, 'motion_component': 0.029721416532993317, 'motion_component_percent': 44.69657242298126}, {'resid': 1313, 'atom': 'C213', 'charge': -0.18000000715255737, 'distance': 28.250181198120117, 'force': [0.04855861887335777, 0.05609775707125664, 0.010108225978910923], 'magnitude': 0.07488039880990982, 'cosine_with_motion': 0.47780942916870117, 'motion_component': 0.03577855974435806, 'motion_component_percent': 47.78094291687012}, {'resid': 1313, 'atom': 'C214', 'charge': -0.15000000596046448, 'distance': 29.025863647460938, 'force': [0.03708170726895332, 0.04481186717748642, 0.01052639540284872], 'magnitude': 0.05910973995923996, 'cosine_with_motion': 0.5085805654525757, 'motion_component': 0.03006206452846527, 'motion_component_percent': 50.85805654525757}, {'resid': 1313, 'atom': 'C215', 'charge': -0.15000000596046448, 'distance': 30.319215774536133, 'force': [0.033522699028253555, 0.041435789316892624, 0.009703636169433594], 'magnitude': 0.05417431518435478, 'cosine_with_motion': 0.5177057385444641, 'motion_component': 0.02804635278880596, 'motion_component_percent': 51.77057385444641}, {'resid': 1313, 'atom': 'C216', 'charge': -0.18000000715255737, 'distance': 31.41595458984375, 'force': [0.03806298226118088, 0.04622479900717735, 0.00898392777889967], 'magnitude': 0.060549430549144745, 'cosine_with_motion': 0.5018181800842285, 'motion_component': 0.03038480505347252, 'motion_component_percent': 50.18181800842285}, {'resid': 1313, 'atom': 'C217', 'charge': -0.18000000715255737, 'distance': 32.33197021484375, 'force': [0.037526801228523254, 0.04216400161385536, 0.0090562142431736], 'magnitude': 0.057167112827301025, 'cosine_with_motion': 0.47366711497306824, 'motion_component': 0.027078181505203247, 'motion_component_percent': 47.366711497306824}, {'resid': 1313, 'atom': 'C218', 'charge': -0.18000000715255737, 'distance': 33.42985153198242, 'force': [0.03576917573809624, 0.039154283702373505, 0.0068530552089214325], 'magnitude': 0.053473882377147675, 'cosine_with_motion': 0.4536813199520111, 'motion_component': 0.024260101839900017, 'motion_component_percent': 45.36813199520111}, {'resid': 1313, 'atom': 'C219', 'charge': -0.18000000715255737, 'distance': 34.67770767211914, 'force': [0.03219810500741005, 0.037287984043359756, 0.0065152691677212715], 'magnitude': 0.04969467222690582, 'cosine_with_motion': 0.47759154438972473, 'motion_component': 0.023733755573630333, 'motion_component_percent': 47.75915443897247}, {'resid': 1313, 'atom': 'C22', 'charge': -0.08000000566244125, 'distance': 26.081235885620117, 'force': [0.02697880193591118, 0.026440219953656197, -0.00988005381077528], 'magnitude': 0.03904556855559349, 'cosine_with_motion': 0.25841253995895386, 'motion_component': 0.010089864954352379, 'motion_component_percent': 25.841253995895386}, {'resid': 1313, 'atom': 'C220', 'charge': -0.27000001072883606, 'distance': 35.90643310546875, 'force': [0.046037644147872925, 0.051552895456552505, 0.007544830907136202], 'magnitude': 0.06952761858701706, 'cosine_with_motion': 0.4567752480506897, 'motion_component': 0.031758494675159454, 'motion_component_percent': 45.67752480506897}, {'resid': 1313, 'atom': 'C23', 'charge': -0.18000000715255737, 'distance': 25.583881378173828, 'force': [0.06574978679418564, 0.06047460064291954, -0.01886121928691864], 'magnitude': 0.09130146354436874, 'cosine_with_motion': 0.252759724855423, 'motion_component': 0.023077331483364105, 'motion_component_percent': 25.275972485542297}, {'resid': 1313, 'atom': 'C24', 'charge': -0.18000000715255737, 'distance': 24.669618606567383, 'force': [0.0690130665898323, 0.06791236251592636, -0.01634638011455536], 'magnitude': 0.0981941744685173, 'cosine_with_motion': 0.2987108826637268, 'motion_component': 0.029331667348742485, 'motion_component_percent': 29.87108826637268}, {'resid': 1313, 'atom': 'C25', 'charge': -0.15000000596046448, 'distance': 24.13797950744629, 'force': [0.06257786601781845, 0.05729309096932411, -0.010348780080676079], 'magnitude': 0.0854727104306221, 'cosine_with_motion': 0.28699183464050293, 'motion_component': 0.024529971182346344, 'motion_component_percent': 28.699183464050293}, {'resid': 1313, 'atom': 'C26', 'charge': -0.15000000596046448, 'distance': 24.40784454345703, 'force': [0.06148529425263405, 0.05635734274983406, -0.005587219260632992], 'magnitude': 0.08359311521053314, 'cosine_with_motion': 0.309133380651474, 'motion_component': 0.025841422379016876, 'motion_component_percent': 30.9133380651474}, {'resid': 1313, 'atom': 'C27', 'charge': -0.18000000715255737, 'distance': 25.61045265197754, 'force': [0.06526360660791397, 0.06343422085046768, -0.004263507667928934], 'magnitude': 0.09111210703849792, 'cosine_with_motion': 0.3421114981174469, 'motion_component': 0.031170500442385674, 'motion_component_percent': 34.21114981174469}, {'resid': 1313, 'atom': 'C28', 'charge': -0.15000000596046448, 'distance': 26.32105255126953, 'force': [0.05319497361779213, 0.0483437106013298, -0.0005160813452675939], 'magnitude': 0.07188244163990021, 'cosine_with_motion': 0.3281082808971405, 'motion_component': 0.023585224524140358, 'motion_component_percent': 32.81082808971405}, {'resid': 1313, 'atom': 'C29', 'charge': -0.15000000596046448, 'distance': 26.616243362426758, 'force': [0.051523543894290924, 0.04773855209350586, 0.0028287440072745085], 'magnitude': 0.07029684633016586, 'cosine_with_motion': 0.3536260426044464, 'motion_component': 0.02485879510641098, 'motion_component_percent': 35.36260426044464}, {'resid': 1313, 'atom': 'C3', 'charge': 0.06000000238418579, 'distance': 33.056644439697266, 'force': [-0.011219675652682781, -0.011483876965939999, 0.008634214289486408], 'magnitude': 0.018229378387331963, 'cosine_with_motion': -0.16211383044719696, 'motion_component': -0.0029552343767136335, 'motion_component_percent': 16.211383044719696}, {'resid': 1313, 'atom': 'C31', 'charge': 0.6299999952316284, 'distance': 30.87660789489746, 'force': [-0.16680125892162323, -0.13154959678649902, 0.05481423810124397], 'magnitude': 0.219391331076622, 'cosine_with_motion': -0.1688905507326126, 'motion_component': -0.037053123116493225, 'motion_component_percent': 16.88905507326126}, {'resid': 1313, 'atom': 'C310', 'charge': -0.18000000715255737, 'distance': 24.349313735961914, 'force': [0.08501981943845749, 0.054110486060380936, 0.0017981564160436392], 'magnitude': 0.10079458355903625, 'cosine_with_motion': 0.18467263877391815, 'motion_component': 0.01861400157213211, 'motion_component_percent': 18.467263877391815}, {'resid': 1313, 'atom': 'C311', 'charge': -0.18000000715255737, 'distance': 24.591760635375977, 'force': [0.08662640303373337, 0.04753498733043671, 0.0010384190827608109], 'magnitude': 0.09881693869829178, 'cosine_with_motion': 0.12241298705339432, 'motion_component': 0.01209647674113512, 'motion_component_percent': 12.241298705339432}, {'resid': 1313, 'atom': 'C312', 'charge': -0.18000000715255737, 'distance': 25.23893928527832, 'force': [0.08325960487127304, 0.042853180319070816, 0.005704394541680813], 'magnitude': 0.09381416440010071, 'cosine_with_motion': 0.11621542274951935, 'motion_component': 0.010902652516961098, 'motion_component_percent': 11.621542274951935}, {'resid': 1313, 'atom': 'C313', 'charge': -0.18000000715255737, 'distance': 25.5270938873291, 'force': [0.08386556804180145, 0.03678889200091362, 0.004850334022194147], 'magnitude': 0.09170813113451004, 'cosine_with_motion': 0.05597124993801117, 'motion_component': 0.005133018828928471, 'motion_component_percent': 5.597124993801117}, {'resid': 1313, 'atom': 'C314', 'charge': -0.18000000715255737, 'distance': 26.660707473754883, 'force': [0.07745377719402313, 0.032685209065675735, 0.001099324319511652], 'magnitude': 0.08407507836818695, 'cosine_with_motion': 0.02831321768462658, 'motion_component': 0.0023804360534995794, 'motion_component_percent': 2.831321768462658}, {'resid': 1313, 'atom': 'C315', 'charge': -0.18000000715255737, 'distance': 28.008888244628906, 'force': [0.06953367590904236, 0.031072890385985374, 0.0015312492614611983], 'magnitude': 0.07617612183094025, 'cosine_with_motion': 0.050339892506599426, 'motion_component': 0.003834697650745511, 'motion_component_percent': 5.033989250659943}, {'resid': 1313, 'atom': 'C316', 'charge': -0.18000000715255737, 'distance': 29.034423828125, 'force': [0.0651281401515007, 0.027974171563982964, -0.0010699608828872442], 'magnitude': 0.07088986784219742, 'cosine_with_motion': 0.023882387205958366, 'motion_component': 0.001693019294179976, 'motion_component_percent': 2.3882387205958366}, {'resid': 1313, 'atom': 'C317', 'charge': -0.18000000715255737, 'distance': 30.49674415588379, 'force': [0.05889902263879776, 0.02568022347986698, 0.0002715804148465395], 'magnitude': 0.0642545148730278, 'cosine_with_motion': 0.03605911135673523, 'motion_component': 0.0023169605992734432, 'motion_component_percent': 3.605911135673523}, {'resid': 1313, 'atom': 'C318', 'charge': -0.27000001072883606, 'distance': 30.96392059326172, 'force': [0.08709965646266937, 0.033848363906145096, 0.003052136395126581], 'magnitude': 0.09349533915519714, 'cosine_with_motion': 0.008850702084600925, 'motion_component': 0.0008274994324892759, 'motion_component_percent': 0.8850702084600925}, {'resid': 1313, 'atom': 'C32', 'charge': -0.08000000566244125, 'distance': 30.80122184753418, 'force': [0.021788673475384712, 0.01661793701350689, -0.005732379853725433], 'magnitude': 0.027995755895972252, 'cosine_with_motion': 0.17413486540317535, 'motion_component': 0.004875037353485823, 'motion_component_percent': 17.413486540317535}, {'resid': 1313, 'atom': 'C33', 'charge': -0.18000000715255737, 'distance': 29.734411239624023, 'force': [0.05403773859143257, 0.03858604654669762, -0.012635162100195885], 'magnitude': 0.06759147346019745, 'cosine_with_motion': 0.15382103621959686, 'motion_component': 0.010396989993751049, 'motion_component_percent': 15.382103621959686}, {'resid': 1313, 'atom': 'C34', 'charge': -0.18000000715255737, 'distance': 28.275243759155273, 'force': [0.05878765136003494, 0.04379208758473396, -0.01461113803088665], 'magnitude': 0.0747477114200592, 'cosine_with_motion': 0.1680780053138733, 'motion_component': 0.012563446536660194, 'motion_component_percent': 16.80780053138733}, {'resid': 1313, 'atom': 'C35', 'charge': -0.18000000715255737, 'distance': 27.127731323242188, 'force': [0.06528566777706146, 0.046227987855672836, -0.01396546233445406], 'magnitude': 0.08120516687631607, 'cosine_with_motion': 0.1564122587442398, 'motion_component': 0.012701483443379402, 'motion_component_percent': 15.64122587442398}, {'resid': 1313, 'atom': 'C36', 'charge': -0.18000000715255737, 'distance': 27.177398681640625, 'force': [0.06517570465803146, 0.04699496552348137, -0.009476622566580772], 'magnitude': 0.0809086263179779, 'cosine_with_motion': 0.1860472708940506, 'motion_component': 0.015052828937768936, 'motion_component_percent': 18.60472708940506}, {'resid': 1313, 'atom': 'C37', 'charge': -0.18000000715255737, 'distance': 26.01606559753418, 'force': [0.07237086445093155, 0.05005890876054764, -0.007228906266391277], 'magnitude': 0.08829322457313538, 'cosine_with_motion': 0.18219460546970367, 'motion_component': 0.016086548566818237, 'motion_component_percent': 18.219460546970367}, {'resid': 1313, 'atom': 'C38', 'charge': -0.18000000715255737, 'distance': 26.635732650756836, 'force': [0.06961414217948914, 0.047370851039886475, -0.002245035022497177], 'magnitude': 0.08423281461000443, 'cosine_with_motion': 0.19622090458869934, 'motion_component': 0.016528239473700523, 'motion_component_percent': 19.622090458869934}, {'resid': 1313, 'atom': 'C39', 'charge': -0.18000000715255737, 'distance': 25.719600677490234, 'force': [0.0745873749256134, 0.050939761102199554, 0.0018051366787403822], 'magnitude': 0.09034043550491333, 'cosine_with_motion': 0.2149277627468109, 'motion_component': 0.01941666752099991, 'motion_component_percent': 21.49277627468109}, {'resid': 1313, 'atom': 'C4', 'charge': 0.08000000566244125, 'distance': 32.4375, 'force': [-0.014824322424829006, -0.015932179987430573, 0.012790302745997906], 'magnitude': 0.025242557749152184, 'cosine_with_motion': -0.16058272123336792, 'motion_component': -0.004053518641740084, 'motion_component_percent': 16.058272123336792}, {'resid': 1313, 'atom': 'C5', 'charge': 0.08000000566244125, 'distance': 30.889232635498047, 'force': [-0.016304943710565567, -0.017505086958408356, 0.014233367517590523], 'magnitude': 0.027836451306939125, 'cosine_with_motion': -0.15740536153316498, 'motion_component': -0.004381606820970774, 'motion_component_percent': 15.740536153316498}, {'resid': 1313, 'atom': 'C6', 'charge': 0.06000000238418579, 'distance': 30.28729248046875, 'force': [-0.01267993450164795, -0.014297918416559696, 0.010312550701200962], 'magnitude': 0.021715430542826653, 'cosine_with_motion': -0.19701185822486877, 'motion_component': -0.004278197418898344, 'motion_component_percent': 19.701185822486877}, {'resid': 1313, 'atom': 'H1', 'charge': 0.12000000476837158, 'distance': 30.431459426879883, 'force': [-0.027386467903852463, -0.027536364272236824, 0.018506193533539772], 'magnitude': 0.0430203340947628, 'cosine_with_motion': -0.17966970801353455, 'motion_component': -0.007729451172053814, 'motion_component_percent': 17.966970801353455}, {'resid': 1313, 'atom': 'H10R', 'charge': 0.09000000357627869, 'distance': 27.04370880126953, 'force': [-0.027875486761331558, -0.02976829558610916, -0.0024411578197032213], 'magnitude': 0.040855273604393005, 'cosine_with_motion': -0.42088332772254944, 'motion_component': -0.01719530299305916, 'motion_component_percent': 42.088332772254944}, {'resid': 1313, 'atom': 'H10S', 'charge': 0.09000000357627869, 'distance': 25.320392608642578, 'force': [-0.03203672915697098, -0.03371163085103035, -0.003045052522793412], 'magnitude': 0.046605776995420456, 'cosine_with_motion': -0.41662198305130005, 'motion_component': -0.019416991621255875, 'motion_component_percent': 41.662198305130005}, {'resid': 1313, 'atom': 'H10X', 'charge': 0.09000000357627869, 'distance': 23.665489196777344, 'force': [-0.04452395811676979, -0.02938535436987877, 0.0007345876656472683], 'magnitude': 0.05335186421871185, 'cosine_with_motion': -0.18817096948623657, 'motion_component': -0.010039271786808968, 'motion_component_percent': 18.817096948623657}, {'resid': 1313, 'atom': 'H10Y', 'charge': 0.09000000357627869, 'distance': 23.94359016418457, 'force': [-0.0437014102935791, -0.02823217771947384, -0.0030977539718151093], 'magnitude': 0.052119720727205276, 'cosine_with_motion': -0.20585644245147705, 'motion_component': -0.01072918064892292, 'motion_component_percent': 20.585644245147705}, {'resid': 1313, 'atom': 'H111', 'charge': 0.15000000596046448, 'distance': 25.904460906982422, 'force': [-0.053369540721178055, -0.05043250694870949, -0.010762450285255909], 'magnitude': 0.07421304285526276, 'cosine_with_motion': -0.39723390340805054, 'motion_component': -0.02947993576526642, 'motion_component_percent': 39.723390340805054}, {'resid': 1313, 'atom': 'H11A', 'charge': 0.09000000357627869, 'distance': 30.00301742553711, 'force': [-0.022577131167054176, -0.020812135189771652, 0.012606541626155376], 'magnitude': 0.03319332376122475, 'cosine_with_motion': -0.17205803096294403, 'motion_component': -0.005711177829653025, 'motion_component_percent': 17.205803096294403}, {'resid': 1313, 'atom': 'H11B', 'charge': 0.09000000357627869, 'distance': 28.334535598754883, 'force': [-0.025550024583935738, -0.023120393976569176, 0.014063918963074684], 'magnitude': 0.037217605859041214, 'cosine_with_motion': -0.1656075417995453, 'motion_component': -0.006163516081869602, 'motion_component_percent': 16.56075417995453}, {'resid': 1313, 'atom': 'H11X', 'charge': 0.09000000357627869, 'distance': 25.35992431640625, 'force': [-0.04087144508957863, -0.022073522210121155, 0.0009331740438938141], 'magnitude': 0.0464605875313282, 'cosine_with_motion': -0.10498421639204025, 'motion_component': -0.004877628292888403, 'motion_component_percent': 10.498421639204025}, {'resid': 1313, 'atom': 'H11Y', 'charge': 0.09000000357627869, 'distance': 23.66026496887207, 'force': [-0.04724038764834404, -0.024843357503414154, 0.000299440958769992], 'magnitude': 0.053375426679849625, 'cosine_with_motion': -0.10012506693601608, 'motion_component': -0.005344218108803034, 'motion_component_percent': 10.012506693601608}, {'resid': 1313, 'atom': 'H12', 'charge': 0.09000000357627869, 'distance': 29.15144920349121, 'force': [-0.025621669366955757, -0.021200941875576973, 0.011416689492762089], 'magnitude': 0.03516092523932457, 'cosine_with_motion': -0.15501846373081207, 'motion_component': -0.005450592376291752, 'motion_component_percent': 15.501846373081207}, {'resid': 1313, 'atom': 'H121', 'charge': 0.15000000596046448, 'distance': 27.540822982788086, 'force': [-0.044464413076639175, -0.04663824290037155, -0.012590569444000721], 'magnitude': 0.06565617024898529, 'cosine_with_motion': -0.4552997648715973, 'motion_component': -0.029893238097429276, 'motion_component_percent': 45.52997648715973}, {'resid': 1313, 'atom': 'H12X', 'charge': 0.09000000357627869, 'distance': 24.60243797302246, 'force': [-0.043623119592666626, -0.022612854838371277, -0.004758533556014299], 'magnitude': 0.049365587532520294, 'cosine_with_motion': -0.1317044198513031, 'motion_component': -0.006501666270196438, 'motion_component_percent': 13.17044198513031}, {'resid': 1313, 'atom': 'H12Y', 'charge': 0.09000000357627869, 'distance': 26.167081832885742, 'force': [-0.03830613195896149, -0.02066091261804104, -0.0031760523561388254], 'magnitude': 0.04363851994276047, 'cosine_with_motion': -0.13833922147750854, 'motion_component': -0.006036918610334396, 'motion_component_percent': 13.833922147750854}, {'resid': 1313, 'atom': 'H13A', 'charge': 0.09000000357627869, 'distance': 31.576297760009766, 'force': [-0.02137819491326809, -0.018820306286215782, 0.00931942742317915], 'magnitude': 0.029968030750751495, 'cosine_with_motion': -0.18695104122161865, 'motion_component': -0.00560255441814661, 'motion_component_percent': 18.695104122161865}, {'resid': 1313, 'atom': 'H13B', 'charge': 0.09000000357627869, 'distance': 31.007465362548828, 'force': [-0.021320922300219536, -0.020738385617733, 0.009008746594190598], 'magnitude': 0.031077641993761063, 'cosine_with_motion': -0.23800644278526306, 'motion_component': -0.007396678905934095, 'motion_component_percent': 23.800644278526306}, {'resid': 1313, 'atom': 'H13R', 'charge': 0.09000000357627869, 'distance': 27.522254943847656, 'force': [-0.02485325001180172, -0.030260080471634865, -0.004764355719089508], 'magnitude': 0.039446871727705, 'cosine_with_motion': -0.4943854510784149, 'motion_component': -0.019501959905028343, 'motion_component_percent': 49.43854510784149}, {'resid': 1313, 'atom': 'H13S', 'charge': 0.09000000357627869, 'distance': 28.93377685546875, 'force': [-0.023425396531820297, -0.026661094278097153, -0.0037884931080043316], 'magnitude': 0.03569195792078972, 'cosine_with_motion': -0.46264851093292236, 'motion_component': -0.016512831673026085, 'motion_component_percent': 46.264851093292236}, {'resid': 1313, 'atom': 'H13X', 'charge': 0.09000000357627869, 'distance': 24.672168731689453, 'force': [-0.045381806790828705, -0.018603293225169182, -0.0019841636531054974], 'magnitude': 0.04908693954348564, 'cosine_with_motion': -0.028790097683668137, 'motion_component': -0.0014132177457213402, 'motion_component_percent': 2.8790097683668137}, {'resid': 1313, 'atom': 'H13Y', 'charge': 0.09000000357627869, 'distance': 25.7319278717041, 'force': [-0.04136393964290619, -0.01754576712846756, -0.004196654073894024], 'magnitude': 0.04512694850564003, 'cosine_with_motion': -0.059305500239133835, 'motion_component': -0.002676276257261634, 'motion_component_percent': 5.9305500239133835}, {'resid': 1313, 'atom': 'H141', 'charge': 0.15000000596046448, 'distance': 28.47825050354004, 'force': [-0.03770130127668381, -0.046759359538555145, -0.012756617739796638], 'magnitude': 0.06140486150979996, 'cosine_with_motion': -0.5269491076469421, 'motion_component': -0.03235723823308945, 'motion_component_percent': 52.694910764694214}, {'resid': 1313, 'atom': 'H14X', 'charge': 0.09000000357627869, 'distance': 26.869997024536133, 'force': [-0.038729406893253326, -0.014563619159162045, -0.0008191490196622908], 'magnitude': 0.0413852259516716, 'cosine_with_motion': 0.006080150604248047, 'motion_component': 0.00025162840029224753, 'motion_component_percent': 0.6080150604248047}, {'resid': 1313, 'atom': 'H14Y', 'charge': 0.09000000357627869, 'distance': 26.35749626159668, 'force': [-0.03947075083851814, -0.017050428315997124, 0.00110778515227139], 'magnitude': 0.04301028326153755, 'cosine_with_motion': -0.021877596154808998, 'motion_component': -0.000940961588639766, 'motion_component_percent': 2.1877596154809}, {'resid': 1313, 'atom': 'H151', 'charge': 0.15000000596046448, 'distance': 30.776256561279297, 'force': [-0.03195129334926605, -0.04027647525072098, -0.011012999340891838], 'magnitude': 0.05257723852992058, 'cosine_with_motion': -0.533653199672699, 'motion_component': -0.028058012947440147, 'motion_component_percent': 53.3653199672699}, {'resid': 1313, 'atom': 'H15X', 'charge': 0.09000000357627869, 'distance': 28.318819046020508, 'force': [-0.03416506201028824, -0.014723613858222961, -0.002047311281785369], 'magnitude': 0.03725893050432205, 'cosine_with_motion': -0.05070723593235016, 'motion_component': -0.0018892973894253373, 'motion_component_percent': 5.070723593235016}, {'resid': 1313, 'atom': 'H15Y', 'charge': 0.09000000357627869, 'distance': 27.89134979248047, 'force': [-0.03442322090268135, -0.01701470836997032, -0.0009224476525560021], 'magnitude': 0.0384097546339035, 'cosine_with_motion': -0.08777648210525513, 'motion_component': -0.003371473168954253, 'motion_component_percent': 8.777648210525513}, {'resid': 1313, 'atom': 'H16R', 'charge': 0.09000000357627869, 'distance': 31.920364379882812, 'force': [-0.01775466836988926, -0.022959193214774132, -0.004198820795863867], 'magnitude': 0.029325464740395546, 'cosine_with_motion': -0.5246595144271851, 'motion_component': -0.015385884791612625, 'motion_component_percent': 52.465951442718506}, {'resid': 1313, 'atom': 'H16S', 'charge': 0.09000000357627869, 'distance': 30.8035945892334, 'force': [-0.02000165358185768, -0.024027565494179726, -0.0037753924261778593], 'magnitude': 0.031490374356508255, 'cosine_with_motion': -0.4887712895870209, 'motion_component': -0.015391591005027294, 'motion_component_percent': 48.87712895870209}, {'resid': 1313, 'atom': 'H16X', 'charge': 0.09000000357627869, 'distance': 29.03134536743164, 'force': [-0.03221026062965393, -0.014725311659276485, 0.001593898981809616], 'magnitude': 0.035452451556921005, 'cosine_with_motion': -0.034315530210733414, 'motion_component': -0.0012165696825832129, 'motion_component_percent': 3.4315530210733414}, {'resid': 1313, 'atom': 'H16Y', 'charge': 0.09000000357627869, 'distance': 28.824186325073242, 'force': [-0.03347402065992355, -0.01309612113982439, 0.0011756662279367447], 'magnitude': 0.03596387803554535, 'cosine_with_motion': 0.013054667972028255, 'motion_component': 0.0004694964736700058, 'motion_component_percent': 1.3054667972028255}, {'resid': 1313, 'atom': 'H17R', 'charge': 0.09000000357627869, 'distance': 31.67473030090332, 'force': [-0.02015385404229164, -0.021416446194052696, -0.004704182036221027], 'magnitude': 0.029782064259052277, 'cosine_with_motion': -0.4506356716156006, 'motion_component': -0.013420860283076763, 'motion_component_percent': 45.06356716156006}, {'resid': 1313, 'atom': 'H17S', 'charge': 0.09000000357627869, 'distance': 32.81387710571289, 'force': [-0.0180695578455925, -0.020403897389769554, -0.005219538230448961], 'magnitude': 0.027750162407755852, 'cosine_with_motion': -0.4843931794166565, 'motion_component': -0.013441989198327065, 'motion_component_percent': 48.43931794166565}, {'resid': 1313, 'atom': 'H17X', 'charge': 0.09000000357627869, 'distance': 31.151042938232422, 'force': [-0.028181837871670723, -0.012384139932692051, 0.0007439682958647609], 'magnitude': 0.03079182468354702, 'cosine_with_motion': -0.028290774673223495, 'motion_component': -0.000871124560944736, 'motion_component_percent': 2.8290774673223495}, {'resid': 1313, 'atom': 'H17Y', 'charge': 0.09000000357627869, 'distance': 30.681467056274414, 'force': [-0.028679896146059036, -0.013585150241851807, -0.0006590737029910088], 'magnitude': 0.03174156695604324, 'cosine_with_motion': -0.07111553102731705, 'motion_component': -0.0022573184687644243, 'motion_component_percent': 7.111553102731705}, {'resid': 1313, 'atom': 'H18R', 'charge': 0.09000000357627869, 'distance': 33.015933990478516, 'force': [-0.018315039575099945, -0.020216915756464005, -0.0026885257102549076], 'magnitude': 0.02741154097020626, 'cosine_with_motion': -0.4474886357784271, 'motion_component': -0.012266352772712708, 'motion_component_percent': 44.74886357784271}, {'resid': 1313, 'atom': 'H18S', 'charge': 0.09000000357627869, 'distance': 33.758949279785156, 'force': [-0.018112797290086746, -0.01863238774240017, -0.0034863357432186604], 'magnitude': 0.026218196377158165, 'cosine_with_motio</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>738</v>
-      </c>
-      <c r="B9" t="n">
-        <v>777</v>
-      </c>
-      <c r="C9" t="n">
-        <v>2391</v>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>{738: {'frame': 738, 'motion_vector': [3.9510536193847656, 2.28570556640625, 2.43267822265625], 'ionic_force': [-11.174644649028778, -4.503437966108322, -3.206464245915413], 'ionic_force_magnitude': 12.46735936383432, 'radial_force': 12.047972300211075, 'axial_force': -3.206464245915413, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [2.5245158076286316, -0.6213562488555908, -1.643681526184082], 'asn_force_magnitude': 3.075866156138392, 'residue_force': [2.5245158076286316, -0.6213562488555908, -1.643681526184082], 'residue_force_magnitude': 3.075866156138392, 'pip2_force': [0.9488086828496307, 0.10459831222397042, -4.263142808493285], 'pip2_force_magnitude': 4.368702934416458, 'total_force': [-7.701320158550516, -5.0201959027399425, -9.11328858059278], 'total_force_magnitude': 12.944679518610965, 'cosine_total_motion': -0.9569604537744364, 'cosine_glu_motion': 0, 'cosine_asn_motion': 0.28635248657478535, 'cosine_residue_motion': 0.28635248657478535, 'cosine_pip2_motion': -0.28247700649891, 'cosine_ionic_motion': -0.9652621561538086, 'motion_component_total': -12.387546386094602, 'motion_component_glu': 0, 'motion_component_asn': 0.8807819221814555, 'motion_component_residue': 0.8807819221814555, 'motion_component_ionic': -12.03427018107909, 'motion_component_pip2': -1.234058127196965, 'motion_component_percent_total': 95.69604537744364, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 28.635248657478535, 'motion_component_percent_residue': 28.635248657478535, 'motion_component_percent_ionic': 96.52621561538086, 'motion_component_percent_pip2': 28.247700649891, 'ionic_contributions': [{'ion_id': 2223, 'distance': 9.962797164916992, 'force': [-1.0856294631958008, -3.158844232559204, -0.17628346383571625], 'magnitude': 3.344841480255127, 'cosine_ionic_motion': -0.6900539398193359, 'motion_component_ionic': -2.3081209659576416, 'motion_component_percent_ionic': 69.0053939819336}, {'ion_id': 2247, 'distance': 11.992884635925293, 'force': [-0.6279826760292053, -0.30957135558128357, -2.1995489597320557], 'magnitude': 2.3082921504974365, 'cosine_ionic_motion': -0.71524977684021, 'motion_component_ionic': -1.651005506515503, 'motion_component_percent_ionic': 71.524977684021}, {'ion_id': 2333, 'distance': 9.139810562133789, 'force': [-1.6120256185531616, -0.814048707485199, -3.5403358936309814], 'magnitude': 3.974327564239502, 'cosine_ionic_motion': -0.8193166255950928, 'motion_component_ionic': -3.256232738494873, 'motion_component_percent_ionic': 81.93166255950928}, {'ion_id': 2397, 'distance': 11.327360153198242, 'force': [-2.407813787460327, -0.9421482682228088, -0.0997670590877533], 'magnitude': 2.5875015258789062, 'cosine_ionic_motion': -0.8898726105690002, 'motion_component_ionic': -2.302546739578247, 'motion_component_percent_ionic': 88.98726105690002}, {'ion_id': 2520, 'distance': 7.3378119468688965, 'force': [-5.441193103790283, 0.7211745977401733, 2.8094711303710938], 'magnitude': 6.166019916534424, 'cosine_ionic_motion': -0.40810179710388184, 'motion_component_ionic': -2.5163638591766357, 'motion_component_percent_ionic': 40.810179710388184}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 4.469289779663086, 'force': [2.241318941116333, -2.6649277210235596, 11.367741584777832], 'magnitude': 11.889108657836914, 'cosine_with_motion': 0.4946511685848236, 'motion_component': 5.8809614181518555, 'motion_component_percent': 49.46511685848236}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 4.421173572540283, 'force': [0.7530450820922852, 1.4551115036010742, -10.075578689575195], 'magnitude': 10.207923889160156, 'cosine_with_motion': -0.34488117694854736, 'motion_component': -3.5205206871032715, 'motion_component_percent': 34.488117694854736}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 4.762054920196533, 'force': [-3.0721590518951416, 6.360317707061768, -11.26843547821045], 'magnitude': 13.299227714538574, 'cosine_with_motion': -0.36362212896347046, 'motion_component': -4.835893630981445, 'motion_component_percent': 36.362212896347046}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 5.166462421417236, 'force': [0.39000052213668823, -2.9728293418884277, 4.201687812805176], 'magnitude': 5.161782264709473, 'cosine_with_motion': 0.1860496699810028, 'motion_component': 0.9603478908538818, 'motion_component_percent': 18.60496699810028}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 5.024162292480469, 'force': [2.212310314178467, -2.7990283966064453, 4.130903244018555], 'magnitude': 5.45831823348999, 'cosine_with_motion': 0.43894222378730774, 'motion_component': 2.3958864212036133, 'motion_component_percent': 43.894222378730774}], 'pip2_contributions': [{'resid': 1313, 'atom': 'C1', 'charge': 0.06000000238418579, 'distance': 32.2686767578125, 'force': [-0.01364963036030531, -0.009803573600947857, 0.009140831418335438], 'magnitude': 0.019130531698465347, 'cosine_with_motion': -0.546760082244873, 'motion_component': -0.010459811426699162, 'motion_component_percent': 54.676008224487305}, {'resid': 1313, 'atom': 'C11', 'charge': 0.17000000178813934, 'distance': 31.708324432373047, 'force': [-0.043726127594709396, -0.027371281757950783, 0.02213761769235134], 'magnitude': 0.0561358667910099, 'cosine_with_motion': -0.6250062584877014, 'motion_component': -0.03508526831865311, 'motion_component_percent': 62.50062584877014}, {'resid': 1313, 'atom': 'C12', 'charge': 0.04000000283122063, 'distance': 31.4923038482666, 'force': [-0.01079852320253849, -0.006259041838347912, 0.004849284887313843], 'magnitude': 0.01339026726782322, 'cosine_with_motion': -0.6522622108459473, 'motion_component': -0.008733965456485748, 'motion_component_percent': 65.22622108459473}, {'resid': 1313, 'atom': 'C13', 'charge': -0.05000000074505806, 'distance': 32.23837661743164, 'force': [0.012941473163664341, 0.0077748228795826435, -0.005213260184973478], 'magnitude': 0.015972090885043144, 'cosine_with_motion': 0.6805353164672852, 'motion_component': 0.010869571939110756, 'motion_component_percent': 68.05353164672852}, {'resid': 1313, 'atom': 'C2', 'charge': 0.06000000238418579, 'distance': 33.752010345458984, 'force': [-0.012598118744790554, -0.008867230266332626, 0.008271592669188976], 'magnitude': 0.017485983669757843, 'cosine_with_motion': -0.5519636869430542, 'motion_component': -0.009651628322899342, 'motion_component_percent': 55.19636869430542}, {'resid': 1313, 'atom': 'C21', 'charge': 0.6299999952316284, 'distance': 29.167911529541016, 'force': [-0.1990124136209488, -0.11013854295015335, 0.0933014452457428], 'magnitude': 0.24584873020648956, 'cosine_with_motion': -0.6378347873687744, 'motion_component': -0.15681087970733643, 'motion_component_percent': 63.78347873687744}, {'resid': 1313, 'atom': 'C210', 'charge': -0.18000000715255737, 'distance': 27.95619773864746, 'force': [0.0699339285492897, 0.030164159834384918, -0.0067854635417461395], 'magnitude': 0.07646354287862778, 'cosine_with_motion': 0.8312399983406067, 'motion_component': 0.06355955451726913, 'motion_component_percent': 83.12399983406067}, {'resid': 1313, 'atom': 'C211', 'charge': -0.15000000596046448, 'distance': 28.275798797607422, 'force': [0.05808063596487045, 0.022223317995667458, -0.0035317311994731426], 'magnitude': 0.062287312000989914, 'cosine_with_motion': 0.8432897329330444, 'motion_component': 0.05252625048160553, 'motion_component_percent': 84.32897329330444}, {'resid': 1313, 'atom': 'C212', 'charge': -0.15000000596046448, 'distance': 29.489391326904297, 'force': [0.053773317486047745, 0.019484978169202805, -0.0028590140864253044], 'magnitude': 0.05726611614227295, 'cosine_with_motion': 0.8441688418388367, 'motion_component': 0.0483422726392746, 'motion_component_percent': 84.41688418388367}, {'resid': 1313, 'atom': 'C213', 'charge': -0.18000000715255737, 'distance': 30.694034576416016, 'force': [0.059049107134342194, 0.022796213626861572, -0.004128837492316961], 'magnitude': 0.06343115866184235, 'cosine_with_motion': 0.839309573173523, 'motion_component': 0.05323837697505951, 'motion_component_percent': 83.9309573173523}, {'resid': 1313, 'atom': 'C214', 'charge': -0.15000000596046448, 'distance': 31.593738555908203, 'force': [0.046252619475126266, 0.018650026991963387, -0.0014289335813373327], 'magnitude': 0.04989158362150192, 'cosine_with_motion': 0.8598843216896057, 'motion_component': 0.042900990694761276, 'motion_component_percent': 85.98843216896057}, {'resid': 1313, 'atom': 'C215', 'charge': -0.15000000596046448, 'distance': 32.72728729248047, 'force': [0.04342417046427727, 0.016601409763097763, -0.0007421249756589532], 'magnitude': 0.046495337039232254, 'cosine_with_motion': 0.8637019991874695, 'motion_component': 0.040158115327358246, 'motion_component_percent': 86.37019991874695}, {'resid': 1313, 'atom': 'C216', 'charge': -0.18000000715255737, 'distance': 33.514137268066406, 'force': [0.050248220562934875, 0.01738337054848671, -0.0019323515007272363], 'magnitude': 0.053205255419015884, 'cosine_with_motion': 0.8487250804901123, 'motion_component': 0.04515663534402847, 'motion_component_percent': 84.87250804901123}, {'resid': 1313, 'atom': 'C217', 'charge': -0.18000000715255737, 'distance': 35.018436431884766, 'force': [0.04588926583528519, 0.016317788511514664, -0.0016564653487876058], 'magnitude': 0.048732317984104156, 'cosine_with_motion': 0.8512991666793823, 'motion_component': 0.04148578271269798, 'motion_component_percent': 85.12991666793823}, {'resid': 1313, 'atom': 'C218', 'charge': -0.18000000715255737, 'distance': 35.97636032104492, 'force': [0.043636519461870193, 0.01477277185767889, -0.003073844127357006], 'magnitude': 0.04617173597216606, 'cosine_with_motion': 0.8320149183273315, 'motion_component': 0.0384155735373497, 'motion_component_percent': 83.20149183273315}, {'resid': 1313, 'atom': 'C219', 'charge': -0.18000000715255737, 'distance': 37.38211441040039, 'force': [0.040294114500284195, 0.014109121635556221, -0.0024728719145059586], 'magnitude': 0.04276444762945175, 'cosine_with_motion': 0.8383541703224182, 'motion_component': 0.03585175424814224, 'motion_component_percent': 83.83541703224182}, {'resid': 1313, 'atom': 'C22', 'charge': -0.08000000566244125, 'distance': 27.787450790405273, 'force': [0.027696259319782257, 0.015860874205827713, -0.012828042730689049], 'magnitude': 0.034397803246974945, 'cosine_with_motion': 0.6434230804443359, 'motion_component': 0.02213234081864357, 'motion_component_percent': 64.3423080444336}, {'resid': 1313, 'atom': 'C220', 'charge': -0.27000001072883606, 'distance': 38.363162994384766, 'force': [0.05758515000343323, 0.019171815365552902, -0.005114133935421705], 'magnitude': 0.060907818377017975, 'cosine_with_motion': 0.8218162059783936, 'motion_component': 0.05005503073334694, 'motion_component_percent': 82.18162059783936}, {'resid': 1313, 'atom': 'C23', 'charge': -0.18000000715255737, 'distance': 26.80002212524414, 'force': [0.06893736869096756, 0.03637990355491638, -0.029101941734552383], 'magnitude': 0.08320324867963791, 'cosine_with_motion': 0.6616223454475403, 'motion_component': 0.05504912883043289, 'motion_component_percent': 66.16223454475403}, {'resid': 1313, 'atom': 'C24', 'charge': -0.18000000715255737, 'distance': 27.144983291625977, 'force': [0.06869611144065857, 0.035692065954208374, -0.024175425991415977], 'magnitude': 0.08110197633504868, 'cosine_with_motion': 0.7013137936592102, 'motion_component': 0.05687793344259262, 'motion_component_percent': 70.13137936592102}, {'resid': 1313, 'atom': 'C25', 'charge': -0.15000000596046448, 'distance': 26.613140106201172, 'force': [0.06146484240889549, 0.02823011577129364, -0.019211623817682266], 'magnitude': 0.07031324505805969, 'cosine_with_motion': 0.7166672945022583, 'motion_component': 0.05039120465517044, 'motion_component_percent': 71.66672945022583}, {'resid': 1313, 'atom': 'C26', 'charge': -0.15000000596046448, 'distance': 26.34966278076172, 'force': [0.063740573823452, 0.028609002009034157, -0.01622791215777397], 'magnitude': 0.07172643393278122, 'cosine_with_motion': 0.7486826181411743, 'motion_component': 0.05370033532381058, 'motion_component_percent': 74.86826181411743}, {'resid': 1313, 'atom': 'C27', 'charge': -0.18000000715255737, 'distance': 26.667734146118164, 'force': [0.07405754178762436, 0.036603160202503204, -0.015390302985906601], 'magnitude': 0.08403078466653824, 'cosine_with_motion': 0.7795701026916504, 'motion_component': 0.06550788879394531, 'motion_component_percent': 77.95701026916504}, {'resid': 1313, 'atom': 'C28', 'charge': -0.15000000596046448, 'distance': 25.925893783569336, 'force': [0.06626832485198975, 0.031602926552295685, -0.009957410395145416], 'magnitude': 0.0740903913974762, 'cosine_with_motion': 0.8085183501243591, 'motion_component': 0.05990343913435936, 'motion_component_percent': 80.85183501243591}, {'resid': 1313, 'atom': 'C29', 'charge': -0.15000000596046448, 'distance': 26.527738571166992, 'force': [0.0642482191324234, 0.02889658510684967, -0.0067140813916921616], 'magnitude': 0.07076669484376907, 'cosine_with_motion': 0.8293418288230896, 'motion_component': 0.05868978053331375, 'motion_component_percent': 82.93418288230896}, {'resid': 1313, 'atom': 'C3', 'charge': 0.06000000238418579, 'distance': 34.38382339477539, 'force': [-0.01209657359868288, -0.008094634860754013, 0.008488084189593792], 'magnitude': 0.01684926636517048, 'cosine_with_motion': -0.5237777233123779, 'motion_component': -0.0088252704590559, 'motion_component_percent': 52.37777233123779}, {'resid': 1313, 'atom': 'C31', 'charge': 0.6299999952316284, 'distance': 32.3895378112793, 'force': [-0.1699219048023224, -0.08544665575027466, 0.05979568138718605], 'magnitude': 0.19937428832054138, 'cosine_with_motion': -0.6993690729141235, 'motion_component': -0.13943621516227722, 'motion_component_percent': 69.93690729141235}, {'resid': 1313, 'atom': 'C310', 'charge': -0.18000000715255737, 'distance': 27.356794357299805, 'force': [0.0775734931230545, 0.017701594159007072, -0.006721942685544491], 'magnitude': 0.07985097169876099, 'cosine_with_motion': 0.8004640340805054, 'motion_component': 0.06391783058643341, 'motion_component_percent': 80.04640340805054}, {'resid': 1313, 'atom': 'C311', 'charge': -0.18000000715255737, 'distance': 28.505828857421875, 'force': [0.07148876041173935, 0.016906891018152237, -0.003483446314930916], 'magnitude': 0.07354331761598587, 'cosine_with_motion': 0.8218527436256409, 'motion_component': 0.06044177711009979, 'motion_component_percent': 82.18527436256409}, {'resid': 1313, 'atom': 'C312', 'charge': -0.18000000715255737, 'distance': 29.401470184326172, 'force': [0.0678325742483139, 0.013002971187233925, -0.0029585217125713825], 'magnitude': 0.06913094967603683, 'cosine_with_motion': 0.812524676322937, 'motion_component': 0.05617060139775276, 'motion_component_percent': 81.2524676322937}, {'resid': 1313, 'atom': 'C313', 'charge': -0.18000000715255737, 'distance': 28.82352638244629, 'force': [0.07107935100793839, 0.0110196927562356, -0.0006062230095267296], 'magnitude': 0.07193104177713394, 'cosine_with_motion': 0.8185709714889526, 'motion_component': 0.05888066440820694, 'motion_component_percent': 81.85709714889526}, {'resid': 1313, 'atom': 'C314', 'charge': -0.18000000715255737, 'distance': 29.964962005615234, 'force': [0.06605400145053864, 0.008124123327434063, 0.0006967732333578169], 'magnitude': 0.06655537337064743, 'cosine_with_motion': 0.8169911503791809, 'motion_component': 0.05437515303492546, 'motion_component_percent': 81.69911503791809}, {'resid': 1313, 'atom': 'C315', 'charge': -0.18000000715255737, 'distance': 29.642515182495117, 'force': [0.06774254143238068, 0.00547688128426671, 0.0025448030792176723], 'magnitude': 0.06801120936870575, 'cosine_with_motion': 0.81404709815979, 'motion_component': 0.055364325642585754, 'motion_component_percent': 81.404709815979}, {'resid': 1313, 'atom': 'C316', 'charge': -0.18000000715255737, 'distance': 30.878904342651367, 'force': [0.06252384930849075, 0.0031795320101082325, 0.0029460471123456955], 'magnitude': 0.06267391890287399, 'cosine_with_motion': 0.8065774440765381, 'motion_component': 0.05055136978626251, 'motion_component_percent': 80.65774440765381}, {'resid': 1313, 'atom': 'C317', 'charge': -0.18000000715255737, 'distance': 30.502714157104492, 'force': [0.06408151984214783, 0.00040984651423059404, 0.004336261656135321], 'magnitude': 0.06422936916351318, 'cosine_with_motion': 0.7966939210891724, 'motion_component': 0.05117114633321762, 'motion_component_percent': 79.66939210891724}, {'resid': 1313, 'atom': 'C318', 'charge': -0.27000001072883606, 'distance': 31.74228286743164, 'force': [0.08864043653011322, -0.0019382693571969867, 0.007356500253081322], 'magnitude': 0.08896629512310028, 'cosine_with_motion': 0.7903447151184082, 'motion_component': 0.07031404227018356, 'motion_component_percent': 79.03447151184082}, {'resid': 1313, 'atom': 'C32', 'charge': -0.08000000566244125, 'distance': 32.1761589050293, 'force': [0.022390151396393776, 0.010560380294919014, -0.006730622611939907], 'magnitude': 0.025654274970293045, 'cosine_with_motion': 0.7252023220062256, 'motion_component': 0.018604539334774017, 'motion_component_percent': 72.52023220062256}, {'resid': 1313, 'atom': 'C33', 'charge': -0.18000000715255737, 'distance': 30.82987403869629, 'force': [0.05554255470633507, 0.024472098797559738, -0.016407573595643044], 'magnitude': 0.06287342309951782, 'cosine_with_motion': 0.7240802049636841, 'motion_component': 0.04552540183067322, 'motion_component_percent': 72.40802049636841}, {'resid': 1313, 'atom': 'C34', 'charge': -0.18000000715255737, 'distance': 30.933849334716797, 'force': [0.05658202990889549, 0.022046059370040894, -0.014581877738237381], 'magnitude': 0.06245146691799164, 'cosine_with_motion': 0.738269567489624, 'motion_component': 0.046106018126010895, 'motion_component_percent': 73.8269567489624}, {'resid': 1313, 'atom': 'C35', 'charge': -0.18000000715255737, 'distance': 29.520999908447266, 'force': [0.06280490010976791, 0.023132503032684326, -0.014919333159923553], 'magnitude': 0.0685722604393959, 'cosine_with_motion': 0.7463796138763428, 'motion_component': 0.05118093639612198, 'motion_component_percent': 74.63796138763428}, {'resid': 1313, 'atom': 'C36', 'charge': -0.18000000715255737, 'distance': 29.754182815551758, 'force': [0.06309910118579865, 0.020143656060099602, -0.013008170761168003], 'magnitude': 0.06750167161226273, 'cosine_with_motion': 0.7552959322929382, 'motion_component': 0.0509837381541729, 'motion_component_percent': 75.52959322929382}, {'resid': 1313, 'atom': 'C37', 'charge': -0.18000000715255737, 'distance': 28.581026077270508, 'force': [0.06918127089738846, 0.01997888833284378, -0.012911980040371418], 'magnitude': 0.07315684109926224, 'cosine_with_motion': 0.7600412368774414, 'motion_component': 0.055602215230464935, 'motion_component_percent': 76.00412368774414}, {'resid': 1313, 'atom': 'C38', 'charge': -0.18000000715255737, 'distance': 28.965662002563477, 'force': [0.06843627989292145, 0.016106652095913887, -0.011415544897317886], 'magnitude': 0.07122684270143509, 'cosine_with_motion': 0.7585029006004333, 'motion_component': 0.054025765508413315, 'motion_component_percent': 75.85029006004333}, {'resid': 1313, 'atom': 'C39', 'charge': -0.18000000715255737, 'distance': 27.767555236816406, 'force': [0.07517866790294647, 0.015607287175953388, -0.010571679100394249], 'magnitude': 0.07750599831342697, 'cosine_with_motion': 0.765777587890625, 'motion_component': 0.05935235694050789, 'motion_component_percent': 76.5777587890625}, {'resid': 1313, 'atom': 'C4', 'charge': 0.08000000566244125, 'distance': 34.34451675415039, 'force': [-0.015508313663303852, -0.010995155200362206, 0.012067332863807678], 'magnitude': 0.022517144680023193, 'cosine_with_motion': -0.48983967304229736, 'motion_component': -0.011029791086912155, 'motion_component_percent': 48.983967304229736}, {'resid': 1313, 'atom': 'C5', 'charge': 0.08000000566244125, 'distance': 32.831119537353516, 'force': [-0.01671004295349121, -0.012121847830712795, 0.013453979976475239], 'magnitude': 0.02464090660214424, 'cosine_with_motion': -0.47861427068710327, 'motion_component': -0.011793489567935467, 'motion_component_percent': 47.86142706871033}, {'resid': 1313, 'atom': 'C6', 'charge': 0.06000000238418579, 'distance': 32.076236724853516, 'force': [-0.013217628002166748, -0.010062860324978828, 0.009943461045622826], 'magnitude': 0.019360767677426338, 'cosine_with_motion': -0.5096337199211121, 'motion_component': -0.009866899810731411, 'motion_component_percent': 50.963371992111206}, {'resid': 1313, 'atom': 'H1', 'charge': 0.12000000476837158, 'distance': 31.82754135131836, 'force': [-0.028716349974274635, -0.01911492832005024, 0.018888160586357117], 'magnitude': 0.03932902216911316, 'cosine_with_motion': -0.5466534495353699, 'motion_component': -0.02149934507906437, 'motion_component_percent': 54.66534495353699}, {'resid': 1313, 'atom': 'H10R', 'charge': 0.09000000357627869, 'distance': 28.422040939331055, 'force': [-0.03384503722190857, -0.01421846728771925, 0.0045297821052372456], 'magnitude': 0.03698878735303879, 'cosine_with_motion': -0.8112280368804932, 'motion_component': -0.030006341636180878, 'motion_component_percent': 81.12280368804932}, {'resid': 1313, 'atom': 'H10S', 'charge': 0.09000000357627869, 'distance': 28.548137664794922, 'force': [-0.03308939188718796, -0.015518661588430405, 0.002901833737269044], 'magnitude': 0.0366627536714077, 'cosine_with_motion': -0.8392536640167236, 'motion_component': -0.0307693500071764, 'motion_component_percent': 83.92536640167236}, {'resid': 1313, 'atom': 'H10X', 'charge': 0.09000000357627869, 'distance': 26.652446746826172, 'force': [-0.041149552911520004, -0.008231795392930508, 0.0028807285707443953], 'magnitude': 0.042063601315021515, 'cosine_with_motion': -0.8015514612197876, 'motion_component': -0.03371614217758179, 'motion_component_percent': 80.15514612197876}, {'resid': 1313, 'atom': 'H10Y', 'charge': 0.09000000357627869, 'distance': 26.78232192993164, 'force': [-0.04012057185173035, -0.010627595707774162, 0.0035593367647379637], 'magnitude': 0.04165663197636604, 'cosine_with_motion': -0.8082670569419861, 'motion_component': -0.03366968408226967, 'motion_component_percent': 80.82670569419861}, {'resid': 1313, 'atom': 'H111', 'charge': 0.15000000596046448, 'distance': 27.443374633789062, 'force': [-0.062141645699739456, -0.02244311012327671, 0.002647517016157508], 'magnitude': 0.06612326949834824, 'cosine_with_motion': -0.8490410447120667, 'motion_component': -0.05614136904478073, 'motion_component_percent': 84.90410447120667}, {'resid': 1313, 'atom': 'H11A', 'charge': 0.09000000357627869, 'distance': 32.7114372253418, 'force': [-0.02163558453321457, -0.013510347343981266, 0.011363763362169266], 'magnitude': 0.02792423963546753, 'cosine_with_motion': -0.6142577528953552, 'motion_component': -0.017152680084109306, 'motion_component_percent': 61.42577528953552}, {'resid': 1313, 'atom': 'H11B', 'charge': 0.09000000357627869, 'distance': 31.148235321044922, 'force': [-0.02391369268298149, -0.014494625851511955, 0.012904242612421513], 'magnitude': 0.030797375366091728, 'cosine_with_motion': -0.6040552854537964, 'motion_component': -0.018603317439556122, 'motion_component_percent': 60.40552854537964}, {'resid': 1313, 'atom': 'H11X', 'charge': 0.09000000357627869, 'distance': 28.095693588256836, 'force': [-0.03674684837460518, -0.00907130166888237, 0.0004852105339523405], 'magnitude': 0.037853069603443146, 'cosine_with_motion': -0.8414286971092224, 'motion_component': -0.0318506583571434, 'motion_component_percent': 84.14286971092224}, {'resid': 1313, 'atom': 'H11Y', 'charge': 0.09000000357627869, 'distance': 29.04039192199707, 'force': [-0.03416035696864128, -0.009121538139879704, 0.002275618724524975], 'magnitude': 0.035430364310741425, 'cosine_with_motion': -0.8200598359107971, 'motion_component': -0.029055017977952957, 'motion_component_percent': 82.00598359107971}, {'resid': 1313, 'atom': 'H12', 'charge': 0.09000000357627869, 'distance': 31.88133430480957, 'force': [-0.024082589894533157, -0.012893855571746826, 0.010861827060580254], 'magnitude': 0.029397310689091682, 'cosine_with_motion': -0.6458256840705872, 'motion_component': -0.018985537812113762, 'motion_component_percent': 64.58256840705872}, {'resid': 1313, 'atom': 'H121', 'charge': 0.15000000596046448, 'distance': 29.766626358032227, 'force': [-0.0533113069832325, -0.017738981172442436, 0.0014713853597640991], 'magnitude': 0.05620437487959862, 'cosine_with_motion': -0.8517204523086548, 'motion_component': -0.047870416194200516, 'motion_component_percent': 85.17204523086548}, {'resid': 1313, 'atom': 'H12X', 'charge': 0.09000000357627869, 'distance': 30.411907196044922, 'force': [-0.03164880722761154, -0.006399625446647406, 0.0010601987596601248], 'magnitude': 0.03230675309896469, 'cosine_with_motion': -0.8204260468482971, 'motion_component': -0.026505300775170326, 'motion_component_percent': 82.04260468482971}, {'resid': 1313, 'atom': 'H12Y', 'charge': 0.09000000357627869, 'distance': 29.54867935180664, 'force': [-0.033617403358221054, -0.005859051365405321, 0.002584976376965642], 'magnitude': 0.03422192856669426, 'cosine_with_motion': -0.7905179262161255, 'motion_component': -0.027053048834204674, 'motion_component_percent': 79.05179262161255}, {'resid': 1313, 'atom': 'H13A', 'charge': 0.09000000357627869, 'distance': 33.284339904785156, 'force': [-0.02176963910460472, -0.013093952089548111, 0.00905971322208643], 'magnitude': 0.026971230283379555, 'cosine_with_motion': -0.6731143593788147, 'motion_component': -0.018154721707105637, 'motion_component_percent': 67.31143593788147}, {'resid': 1313, 'atom': 'H13B', 'charge': 0.09000000357627869, 'distance': 31.912220001220703, 'force': [-0.023397354409098625, -0.015098423697054386, 0.009244604967534542], 'magnitude': 0.029340438544750214, 'cosine_with_motion': -0.6883652210235596, 'motion_component': -0.020196937024593353, 'motion_component_percent': 68.83652210235596}, {'resid': 1313, 'atom': 'H13R', 'charge': 0.09000000357627869, 'distance': 30.52679443359375, 'force': [-0.029471339657902718, -0.012315167114138603, 0.0028069838881492615], 'magnitude': 0.032064035534858704, 'cosine_with_motion': -0.8306674957275391, 'motion_component': -0.02663455158472061, 'motion_component_percent': 83.0667495727539}, {'resid': 1313, 'atom': 'H13S', 'charge': 0.09000000357627869, 'distance': 31.25628662109375, 'force': [-0.02869509905576706, -0.010275103151798248, 0.0025385813787579536], 'magnitude': 0.03058481402695179, 'cosine_with_motion': -0.8261064291000366, 'motion_component': -0.025266312062740326, 'motion_component_percent': 82.61064291000366}, {'resid': 1313, 'atom': 'H13X', 'charge': 0.09000000357627869, 'distance': 28.0063419342041, 'force': [-0.037741273641586304, -0.005091314669698477, 0.0009500585729256272], 'magnitude': 0.038094982504844666, 'cosine_with_motion': -0.8041179776191711, 'motion_component': -0.030632860958576202, 'motion_component_percent': 80.41179776191711}, {'resid': 1313, 'atom': 'H13Y', 'charge': 0.09000000357627869, 'distance': 28.320268630981445, 'force': [-0.036677099764347076, -0.00650308933109045, -0.0006661770748905838], 'magnitude': 0.03725511580705643, 'cosine_with_motion': -0.8375759720802307, 'motion_component': -0.031203988939523697, 'motion_component_percent': 83.75759720802307}, {'resid': 1313, 'atom': 'H141', 'charge': 0.15000000596046448, 'distance': 31.147912979125977, 'force': [-0.04708423465490341, -0.020433694124221802, 0.0005568877677433193], 'magnitude': 0.051330022513866425, 'cosine_with_motion': -0.8715096116065979, 'motion_component': -0.04473460838198662, 'motion_component_percent': 87.15096116065979}, {'resid': 1313, 'atom': 'H14X', 'charge': 0.09000000357627869, 'distance': 30.6032657623291, 'force': [-0.031710345298051834, -0.003473429474979639, 0.0005039442330598831], 'magnitude': 0.03190399333834648, 'cosine_with_motion': -0.7999254465103149, 'motion_component': -0.025520816445350647, 'motion_component_percent': 79.9925446510315}, {'resid': 1313, 'atom': 'H14Y', 'charge': 0.09000000357627869, 'distance': 30.655122756958008, 'force': [-0.03146345540881157, -0.004479513503611088, -0.000989891355857253], 'magnitude': 0.03179614618420601, 'cosine_with_motion': -0.8327866792678833, 'motion_component': -0.026479406282305717, 'motion_component_percent': 83.27866792678833}, {'resid': 1313, 'atom': 'H151', 'charge': 0.15000000596046448, 'distance': 33.212886810302734, 'force': [-0.04205583408474922, -0.0164044089615345, -0.0005776677862741053], 'magnitude': 0.0451456680893898, 'cosine_with_motion': -0.8781915903091431, 'motion_component': -0.03964654728770256, 'motion_component_percent': 87.8191590309143}, {'resid': 1313, 'atom': 'H15X', 'charge': 0.09000000357627869, 'distance': 28.859060287475586, 'force': [-0.035800717771053314, -0.0022425889037549496, -0.0006625639507547021], 'magnitude': 0.03587700426578522, 'cosine_with_motion': -0.7985641360282898, 'motion_component': -0.028650088235735893, 'motion_component_percent': 79.85641360282898}, {'resid': 1313, 'atom': 'H15Y', 'charge': 0.09000000357627869, 'distance': 29.268531799316406, 'force': [-0.03464149683713913, -0.003268714528530836, -0.0024308753199875355], 'magnitude': 0.03488017991185188, 'cosine_with_motion': -0.832843005657196, 'motion_component': -0.029049713164567947, 'motion_component_percent': 83.2843005657196}, {'resid': 1313, 'atom': 'H16R', 'charge': 0.09000000357627869, 'distance': 33.31593322753906, 'force': [-0.025415221229195595, -0.008681993931531906, 0.0018388000316917896], 'magnitude': 0.026920098811388016, 'cosine_with_motion': -0.8315717577934265, 'motion_component': -0.022385993972420692, 'motion_component_percent': 83.15717577934265}, {'resid': 1313, 'atom': 'H16S', 'charge': 0.09000000357627869, 'distance': 33.26375961303711, 'force': [-0.025772444903850555, -0.008025415241718292, 0.0007892564754001796], 'magnitude': 0.027004612609744072, 'cosine_with_motion': -0.8466089367866516, 'motion_component': -0.022862346842885017, 'motion_component_percent': 84.66089367866516}, {'resid': 1313, 'atom': 'H16X', 'charge': 0.09000000357627869, 'distance': 31.64946937561035, 'force': [-0.029698947444558144, -0.001922423834912479, -0.002020688261836767], 'magnitude': 0.02982962317764759, 'cosine_with_motion': -0.8208733201026917, 'motion_component': -0.024486342445015907, 'motion_component_percent': 82.08733201026917}, {'resid': 1313, 'atom': 'H16Y', 'charge': 0.09000000357627869, 'distance': 31.313846588134766, 'force': [-0.030440619215369225, -0.0013091892469674349, -0.00047604518476873636], 'magnitude': 0.03047247789800167, 'cosine_with_motion': -0.7894144058227539, 'motion_component': -0.024055413901805878, 'motion_component_percent': 78.94144058227539}, {'resid': 1313, 'atom': 'H17R', 'charge': 0.09000000357627869, 'distance': 35.31849670410156, 'force': [-0.02266635373234749, -0.007745970971882343, 0.00015994219575077295], 'magnitude': 0.02395389787852764, 'cosine_with_motion': -0.8625802397727966, 'motion_component': -0.020662158727645874, 'motion_component_percent': 86.25802397727966}, {'resid': 1313, 'atom': 'H17S', 'charge': 0.09000000357627869, 'distance': 35.14371871948242, 'force': [-0.022529244422912598, -0.008790812455117702, 0.0006661732331849635], 'magnitude': 0.024192746728658676, 'cosine_with_motion': -0.8589787483215332, 'motion_component': -0.020781055092811584, 'motion_component_percent': 85.89787483215332}, {'resid': 1313, 'atom': 'H17X', 'charge': 0.09000000357627869, 'distance': 30.026493072509766, 'force': [-0.032974254339933395, -0.00033222007914446294, -0.0033080705907195807], 'magnitude': 0.03314144164323807, 'cosine_with_motion': -0.8114023804664612, 'motion_component': -0.02689104527235031, 'motion_component_percent': 81.14023804664612}, {'resid': 1313, 'atom': 'H17Y', 'charge': 0.09000000357627869, 'distance': 29.90862464904785, 'force': [-0.03337058424949646, 0.0003774126525968313, -0.0014260868774726987], 'magnitude': 0.033403173089027405, 'cosine_with_motion': -0.7782212495803833, 'motion_component': -0.025995058938860893, 'motion_component_percent': 77.82212495803833}, {'resid': 1313, 'atom': 'H18R', 'charge': 0.09000000357627869, 'distance': 35.67620849609375, 'force': [-0.022067764773964882, -0.007695077918469906, 0.0022180890664458275], 'magnitude': 0.023475952446460724, 'cosine_with_motion': -0.8184725046157837, 'motion_component': -0.01921442151069641, 'motion_component_percent': 81.84725046157837}, {'res</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>789</v>
-      </c>
-      <c r="B10" t="n">
-        <v>794</v>
-      </c>
-      <c r="C10" t="n">
-        <v>2247</v>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>{789: {'frame': 789, 'motion_vector': [-0.7640838623046875, -0.2713966369628906, -2.7751007080078125], 'ionic_force': [1.7615902721881866, 3.541439116001129, -9.729321956634521], 'ionic_force_magnitude': 10.50260429775689, 'radial_force': 3.9553749884696026, 'axial_force': -9.729321956634521, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [-7.713208436965942, 5.550417900085449, 1.8187412023544312], 'asn_force_magnitude': 9.675150790494854, 'residue_force': [-7.713208436965942, 5.550417900085449, 1.8187412023544312], 'residue_force_magnitude': 9.675150790494854, 'pip2_force': [0.847271473146975, 0.1475509395240806, -4.499001910447987], 'pip2_force_magnitude': 4.580464869331247, 'total_force': [-5.104346691630781, 9.239407955610659, -12.409582664728077], 'total_force_magnitude': 16.291677520479073, 'cosine_total_motion': 0.7607079828858798, 'cosine_glu_motion': 0, 'cosine_asn_motion': -0.023595462164669713, 'cosine_residue_motion': -0.023595462164669713, 'cosine_pip2_motion': 0.8908842196065903, 'cosine_ionic_motion': 0.813211150887596, 'motion_component_total': 12.393209144430868, 'motion_component_glu': 0, 'motion_component_asn': -0.2282896544145956, 'motion_component_residue': -0.2282896544145956, 'motion_component_ionic': 8.540834928295892, 'motion_component_pip2': 4.080663870549571, 'motion_component_percent_total': 76.07079828858798, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 2.3595462164669714, 'motion_component_percent_residue': 2.3595462164669714, 'motion_component_percent_ionic': 81.3211150887596, 'motion_component_percent_pip2': 89.08842196065902, 'ionic_contributions': [{'ion_id': 2223, 'distance': 10.327621459960938, 'force': [-0.2378109097480774, 2.686925172805786, -1.5533154010772705], 'magnitude': 3.112701416015625, 'cosine_ionic_motion': 0.41815653443336487, 'motion_component_ionic': 1.3015964031219482, 'motion_component_percent_ionic': 41.81565344333649}, {'ion_id': 2333, 'distance': 7.631259441375732, 'force': [0.2259296029806137, 1.732958197593689, -5.426454067230225], 'magnitude': 5.700929164886475, 'cosine_ionic_motion': 0.8746433258056641, 'motion_component_ionic': 4.986279487609863, 'motion_component_percent_ionic': 87.4643325805664}, {'ion_id': 2372, 'distance': 13.513449668884277, 'force': [0.18907205760478973, 0.2547174096107483, -1.7901601791381836], 'magnitude': 1.8180490732192993, 'cosine_ionic_motion': 0.9045041799545288, 'motion_component_ionic': 1.6444330215454102, 'motion_component_percent_ionic': 90.45041799545288}, {'ion_id': 2397, 'distance': 8.486930847167969, 'force': [2.124591588973999, -2.658017873764038, -3.109158992767334], 'magnitude': 4.609318733215332, 'cosine_ionic_motion': 0.5797797441482544, 'motion_component_ionic': 2.6723897457122803, 'motion_component_percent_ionic': 57.97797441482544}, {'ion_id': 2520, 'distance': 11.108541488647461, 'force': [-0.5401920676231384, 1.5248562097549438, 2.149766683578491], 'magnitude': 2.690444231033325, 'cosine_ionic_motion': -0.7671087384223938, 'motion_component_ionic': -2.0638632774353027, 'motion_component_percent_ionic': 76.71087384223938}], 'glu_contributions': [], 'asn_contributions': [{'resid': 786, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 3.9632208347320557, 'force': [1.5947648286819458, -14.72599983215332, -3.031982898712158], 'magnitude': 15.119235038757324, 'cosine_with_motion': 0.2560434937477112, 'motion_component': 3.8711817264556885, 'motion_component_percent': 25.604349374771118}, {'resid': 786, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 3.0943763256073, 'force': [-6.973222732543945, 19.09194564819336, 4.59505558013916], 'magnitude': 20.838491439819336, 'cosine_with_motion': -0.20922410488128662, 'motion_component': -4.359914779663086, 'motion_component_percent': 20.922410488128662}, {'resid': 786, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 4.144586563110352, 'force': [3.7976768016815186, 16.522083282470703, 4.566196918487549], 'magnitude': 17.557100296020508, 'cosine_with_motion': -0.39514291286468506, 'motion_component': -6.937563896179199, 'motion_component_percent': 39.514291286468506}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 3.4154815673828125, 'force': [-4.642576217651367, -10.45011043548584, -2.9561102390289307], 'magnitude': 11.810881614685059, 'cosine_with_motion': 0.427182674407959, 'motion_component': 5.045403957366943, 'motion_component_percent': 42.7182674407959}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 5.105398178100586, 'force': [-1.4898511171340942, -4.887500762939453, -1.354418158531189], 'magnitude': 5.28599739074707, 'cosine_with_motion': 0.4072275757789612, 'motion_component': 2.1526038646698, 'motion_component_percent': 40.72275757789612}], 'pip2_contributions': [{'resid': 1313, 'atom': 'C1', 'charge': 0.06000000238418579, 'distance': 25.27534294128418, 'force': [-0.022676624357700348, -0.01718645729124546, 0.012754387222230434], 'magnitude': 0.031181372702121735, 'cosine_with_motion': -0.1486808955669403, 'motion_component': -0.004636074416339397, 'motion_component_percent': 14.86808955669403}, {'resid': 1313, 'atom': 'C11', 'charge': 0.17000000178813934, 'distance': 24.14469337463379, 'force': [-0.07957837730646133, -0.04626452177762985, 0.03000103309750557], 'magnitude': 0.09681521356105804, 'cosine_with_motion': -0.035352230072021484, 'motion_component': -0.003422633744776249, 'motion_component_percent': 3.5352230072021484}, {'resid': 1313, 'atom': 'C12', 'charge': 0.04000000283122063, 'distance': 24.405574798583984, 'force': [-0.018933849409222603, -0.010321058332920074, 0.0056639970280230045], 'magnitude': 0.022295644506812096, 'cosine_with_motion': 0.024045834317803383, 'motion_component': 0.000536117353476584, 'motion_component_percent': 2.4045834317803383}, {'resid': 1313, 'atom': 'C13', 'charge': -0.05000000074505806, 'distance': 25.52105140686035, 'force': [0.021475007757544518, 0.01244976557791233, -0.005778530612587929], 'magnitude': 0.025486545637249947, 'cosine_with_motion': -0.050912998616695404, 'motion_component': -0.0012975964928045869, 'motion_component_percent': 5.09129986166954}, {'resid': 1313, 'atom': 'C2', 'charge': 0.06000000238418579, 'distance': 26.769166946411133, 'force': [-0.019931046292185783, -0.015637120231986046, 0.011444843374192715], 'magnitude': 0.02779839187860489, 'cosine_with_motion': -0.15289171040058136, 'motion_component': -0.004250143654644489, 'motion_component_percent': 15.289171040058136}, {'resid': 1313, 'atom': 'C21', 'charge': 0.6299999952316284, 'distance': 22.003755569458008, 'force': [-0.37328338623046875, -0.19256089627742767, 0.10101927071809769], 'magnitude': 0.4320012629032135, 'cosine_with_motion': 0.04575078561902046, 'motion_component': 0.01976439729332924, 'motion_component_percent': 4.575078561902046}, {'resid': 1313, 'atom': 'C210', 'charge': -0.18000000715255737, 'distance': 21.02984619140625, 'force': [0.11328990757465363, 0.06762255728244781, 0.029181860387325287], 'magnitude': 0.13512584567070007, 'cosine_with_motion': -0.47584792971611023, 'motion_component': -0.06429935246706009, 'motion_component_percent': 47.58479297161102}, {'resid': 1313, 'atom': 'C211', 'charge': -0.15000000596046448, 'distance': 22.154693603515625, 'force': [0.08401113748550415, 0.050087910145521164, 0.02697412297129631], 'magnitude': 0.10146070271730423, 'cosine_with_motion': -0.5203617215156555, 'motion_component': -0.052796266973018646, 'motion_component_percent': 52.03617215156555}, {'resid': 1313, 'atom': 'C212', 'charge': -0.15000000596046448, 'distance': 22.889408111572266, 'force': [0.07601042091846466, 0.05075792968273163, 0.026093831285834312], 'magnitude': 0.09505177289247513, 'cosine_with_motion': -0.5249742269515991, 'motion_component': -0.04989973083138466, 'motion_component_percent': 52.49742269515991}, {'resid': 1313, 'atom': 'C213', 'charge': -0.18000000715255737, 'distance': 22.94007682800293, 'force': [0.08804772794246674, 0.0663875862956047, 0.02712731622159481], 'magnitude': 0.1135588213801384, 'cosine_with_motion': -0.4890875220298767, 'motion_component': -0.05554020404815674, 'motion_component_percent': 48.90875220298767}, {'resid': 1313, 'atom': 'C214', 'charge': -0.15000000596046448, 'distance': 24.376596450805664, 'force': [0.06373637914657593, 0.05037802457809448, 0.020577579736709595], 'magnitude': 0.0838075652718544, 'cosine_with_motion': -0.49309825897216797, 'motion_component': -0.041325364261865616, 'motion_component_percent': 49.3098258972168}, {'resid': 1313, 'atom': 'C215', 'charge': -0.15000000596046448, 'distance': 24.778676986694336, 'force': [0.05915984883904457, 0.050696443766355515, 0.022556085139513016], 'magnitude': 0.08110976964235306, 'cosine_with_motion': -0.5183696746826172, 'motion_component': -0.04204484447836876, 'motion_component_percent': 51.83696746826172}, {'resid': 1313, 'atom': 'C216', 'charge': -0.18000000715255737, 'distance': 24.066883087158203, 'force': [0.07180164754390717, 0.0667029470205307, 0.03225129097700119], 'magnitude': 0.10317414999008179, 'cosine_with_motion': -0.5446571111679077, 'motion_component': -0.05619453638792038, 'motion_component_percent': 54.46571111679077}, {'resid': 1313, 'atom': 'C217', 'charge': -0.18000000715255737, 'distance': 23.413986206054688, 'force': [0.07321666181087494, 0.07485445588827133, 0.030314302071928978], 'magnitude': 0.10900837928056717, 'cosine_with_motion': -0.5089008212089539, 'motion_component': -0.055474456399679184, 'motion_component_percent': 50.890082120895386}, {'resid': 1313, 'atom': 'C218', 'charge': -0.18000000715255737, 'distance': 23.188087463378906, 'force': [0.06934080272912979, 0.07974733412265778, 0.03442244976758957], 'magnitude': 0.11114265024662018, 'cosine_with_motion': -0.5295239686965942, 'motion_component': -0.05885269492864609, 'motion_component_percent': 52.952396869659424}, {'resid': 1313, 'atom': 'C219', 'charge': -0.18000000715255737, 'distance': 23.04113006591797, 'force': [0.06620558351278305, 0.08570046722888947, 0.03071010112762451], 'magnitude': 0.11256491392850876, 'cosine_with_motion': -0.4887808859348297, 'motion_component': -0.05501957982778549, 'motion_component_percent': 48.87808859348297}, {'resid': 1313, 'atom': 'C22', 'charge': -0.08000000566244125, 'distance': 21.00526237487793, 'force': [0.05247148498892784, 0.027455942705273628, -0.010795521549880505], 'magnitude': 0.060196585953235626, 'cosine_with_motion': -0.10104437172412872, 'motion_component': -0.006082526408135891, 'motion_component_percent': 10.104437172412872}, {'resid': 1313, 'atom': 'C220', 'charge': -0.27000001072883606, 'distance': 23.598533630371094, 'force': [0.08668050915002823, 0.12676912546157837, 0.04822714254260063], 'magnitude': 0.16096514463424683, 'cosine_with_motion': -0.5038357377052307, 'motion_component': -0.0810999944806099, 'motion_component_percent': 50.38357377052307}, {'resid': 1313, 'atom': 'C23', 'charge': -0.18000000715255737, 'distance': 21.51387596130371, 'force': [0.11597149819135666, 0.054385196417570114, -0.016226045787334442], 'magnitude': 0.12911398708820343, 'cosine_with_motion': -0.15629570186138153, 'motion_component': -0.020179960876703262, 'motion_component_percent': 15.629570186138153}, {'resid': 1313, 'atom': 'C24', 'charge': -0.18000000715255737, 'distance': 20.584579467773438, 'force': [0.1276913583278656, 0.059051625430583954, -0.009933060966432095], 'magnitude': 0.14103490114212036, 'cosine_with_motion': -0.21098187565803528, 'motion_component': -0.029755808413028717, 'motion_component_percent': 21.098187565803528}, {'resid': 1313, 'atom': 'C25', 'charge': -0.15000000596046448, 'distance': 21.254419326782227, 'force': [0.10148036479949951, 0.04302442818880081, -0.001739401021040976], 'magnitude': 0.11023788899183273, 'cosine_with_motion': -0.2647813856601715, 'motion_component': -0.029188942164182663, 'motion_component_percent': 26.47813856601715}, {'resid': 1313, 'atom': 'C26', 'charge': -0.15000000596046448, 'distance': 21.25423240661621, 'force': [0.10094067454338074, 0.044033233076334, 0.004987322259694338], 'magnitude': 0.11023982614278793, 'cosine_with_motion': -0.32291194796562195, 'motion_component': -0.03559775650501251, 'motion_component_percent': 32.291194796562195}, {'resid': 1313, 'atom': 'C27', 'charge': -0.18000000715255737, 'distance': 20.582904815673828, 'force': [0.1258016675710678, 0.06264136731624603, 0.012137382291257381], 'magnitude': 0.1410578489303589, 'cosine_with_motion': -0.35998013615608215, 'motion_component': -0.05077802389860153, 'motion_component_percent': 35.998013615608215}, {'resid': 1313, 'atom': 'C28', 'charge': -0.15000000596046448, 'distance': 20.216615676879883, 'force': [0.10904069244861603, 0.05096860229969025, 0.01894347555935383], 'magnitude': 0.12184632569551468, 'cosine_with_motion': -0.4250069260597229, 'motion_component': -0.051785532385110855, 'motion_component_percent': 42.50069260597229}, {'resid': 1313, 'atom': 'C29', 'charge': -0.15000000596046448, 'distance': 20.418916702270508, 'force': [0.10414750874042511, 0.05286802724003792, 0.0250022541731596], 'magnitude': 0.11944389343261719, 'cosine_with_motion': -0.4729103446006775, 'motion_component': -0.05648625269532204, 'motion_component_percent': 47.29103446006775}, {'resid': 1313, 'atom': 'C3', 'charge': 0.06000000238418579, 'distance': 27.445035934448242, 'force': [-0.01869869790971279, -0.01428994070738554, 0.012064528651535511], 'magnitude': 0.026446107774972916, 'cosine_with_motion': -0.20029833912849426, 'motion_component': -0.005297111347317696, 'motion_component_percent': 20.029833912849426}, {'resid': 1313, 'atom': 'C31', 'charge': 0.6299999952316284, 'distance': 26.4655818939209, 'force': [-0.263563334941864, -0.13033615052700043, 0.05214845761656761], 'magnitude': 0.29861781001091003, 'cosine_with_motion': 0.10660873353481293, 'motion_component': 0.03183526545763016, 'motion_component_percent': 10.660873353481293}, {'resid': 1313, 'atom': 'C310', 'charge': -0.18000000715255737, 'distance': 22.58210563659668, 'force': [0.11292384564876556, 0.02506452240049839, 0.01878596469759941], 'magnitude': 0.11718761920928955, 'cosine_with_motion': -0.4286198318004608, 'motion_component': -0.05022893846035004, 'motion_component_percent': 42.86198318004608}, {'resid': 1313, 'atom': 'C311', 'charge': -0.18000000715255737, 'distance': 22.35918426513672, 'force': [0.11632254719734192, 0.01761123351752758, 0.0211604256182909], 'magnitude': 0.11953599750995636, 'cosine_with_motion': -0.4409271776676178, 'motion_component': -0.05270667001605034, 'motion_component_percent': 44.09271776676178}, {'resid': 1313, 'atom': 'C312', 'charge': -0.18000000715255737, 'distance': 23.65790557861328, 'force': [0.10427509248256683, 0.012051895260810852, 0.019538454711437225], 'magnitude': 0.10677216202020645, 'cosine_with_motion': -0.4443477690219879, 'motion_component': -0.047443971037864685, 'motion_component_percent': 44.43477690219879}, {'resid': 1313, 'atom': 'C313', 'charge': -0.18000000715255737, 'distance': 24.75435447692871, 'force': [0.0942249596118927, 0.012365276925265789, 0.021897679194808006], 'magnitude': 0.09752307832241058, 'cosine_with_motion': -0.4827762246131897, 'motion_component': -0.04708182439208031, 'motion_component_percent': 48.27762246131897}, {'resid': 1313, 'atom': 'C314', 'charge': -0.18000000715255737, 'distance': 24.716970443725586, 'force': [0.09393756091594696, 0.00819451455026865, 0.026019340381026268], 'magnitude': 0.09781831502914429, 'cosine_with_motion': -0.5169848799705505, 'motion_component': -0.050570592284202576, 'motion_component_percent': 51.698487997055054}, {'resid': 1313, 'atom': 'C315', 'charge': -0.18000000715255737, 'distance': 25.827590942382812, 'force': [0.08485684543848038, 0.008348367176949978, 0.027484014630317688], 'magnitude': 0.08958655595779419, 'cosine_with_motion': -0.553554356098175, 'motion_component': -0.049591027200222015, 'motion_component_percent': 55.355435609817505}, {'resid': 1313, 'atom': 'C316', 'charge': -0.18000000715255737, 'distance': 25.758502960205078, 'force': [0.08419010788202286, 0.00536088552325964, 0.03155134245753288], 'magnitude': 0.09006775170564651, 'cosine_with_motion': -0.5888729691505432, 'motion_component': -0.05303846299648285, 'motion_component_percent': 58.88729691505432}, {'resid': 1313, 'atom': 'C317', 'charge': -0.18000000715255737, 'distance': 26.83822250366211, 'force': [0.0762835219502449, 0.006158046890050173, 0.032036758959293365], 'magnitude': 0.08296656608581543, 'cosine_with_motion': -0.6206070780754089, 'motion_component': -0.051489636301994324, 'motion_component_percent': 62.060707807540894}, {'resid': 1313, 'atom': 'C318', 'charge': -0.27000001072883606, 'distance': 28.247459411621094, 'force': [0.10423076152801514, 0.007922106422483921, 0.04115782305598259], 'magnitude': 0.1123422384262085, 'cosine_with_motion': -0.6034796833992004, 'motion_component': -0.0677962601184845, 'motion_component_percent': 60.347968339920044}, {'resid': 1313, 'atom': 'C32', 'charge': -0.08000000566244125, 'distance': 26.769617080688477, 'force': [0.0332757942378521, 0.015667302533984184, -0.004576403181999922], 'magnitude': 0.037063274532556534, 'cosine_with_motion': -0.15843947231769562, 'motion_component': -0.005872285924851894, 'motion_component_percent': 15.843947231769562}, {'resid': 1313, 'atom': 'C33', 'charge': -0.18000000715255737, 'distance': 26.077802658081055, 'force': [0.08087404072284698, 0.03311450034379959, -0.009216935373842716], 'magnitude': 0.08787566423416138, 'cosine_with_motion': -0.17792534828186035, 'motion_component': -0.015635307878255844, 'motion_component_percent': 17.792534828186035}, {'resid': 1313, 'atom': 'C34', 'charge': -0.18000000715255737, 'distance': 26.809768676757812, 'force': [0.07749311625957489, 0.02973167411983013, -0.004854184575378895], 'magnitude': 0.08314275741577148, 'cosine_with_motion': -0.22385451197624207, 'motion_component': -0.018611881881952286, 'motion_component_percent': 22.385451197624207}, {'resid': 1313, 'atom': 'C35', 'charge': -0.18000000715255737, 'distance': 26.25811767578125, 'force': [0.08237410336732864, 0.026729309931397438, -0.0034992729779332876], 'magnitude': 0.08667290955781937, 'cosine_with_motion': -0.24137353897094727, 'motion_component': -0.02092054672539234, 'motion_component_percent': 24.137353897094727}, {'resid': 1313, 'atom': 'C36', 'charge': -0.18000000715255737, 'distance': 25.405567169189453, 'force': [0.08797577023506165, 0.028843313455581665, 0.0008879622910171747], 'magnitude': 0.09258758276700974, 'cosine_with_motion': -0.28957000374794006, 'motion_component': -0.02681058645248413, 'motion_component_percent': 28.957000374794006}, {'resid': 1313, 'atom': 'C37', 'charge': -0.18000000715255737, 'distance': 24.555288314819336, 'force': [0.0955711305141449, 0.02612404339015484, 0.002573790028691292], 'magnitude': 0.09911070019006729, 'cosine_with_motion': -0.30451634526252747, 'motion_component': -0.030180828645825386, 'motion_component_percent': 30.451634526252747}, {'resid': 1313, 'atom': 'C38', 'charge': -0.18000000715255737, 'distance': 23.899070739746094, 'force': [0.1003129705786705, 0.02842947654426098, 0.008724972605705261], 'magnitude': 0.10462816059589386, 'cosine_with_motion': -0.3589353859424591, 'motion_component': -0.037554748356342316, 'motion_component_percent': 35.89353859424591}, {'resid': 1313, 'atom': 'C39', 'charge': -0.18000000715255737, 'distance': 23.15266990661621, 'force': [0.10819603502750397, 0.024372555315494537, 0.011315678246319294], 'magnitude': 0.11148294806480408, 'cosine_with_motion': -0.3744431138038635, 'motion_component': -0.04174402356147766, 'motion_component_percent': 37.44431138038635}, {'resid': 1313, 'atom': 'C4', 'charge': 0.08000000566244125, 'distance': 26.739046096801758, 'force': [-0.02510295808315277, -0.020180175080895424, 0.018508953973650932], 'magnitude': 0.03714807331562042, 'cosine_with_motion': -0.24866466224193573, 'motion_component': -0.009237413294613361, 'motion_component_percent': 24.866466224193573}, {'resid': 1313, 'atom': 'C5', 'charge': 0.08000000566244125, 'distance': 25.34132194519043, 'force': [-0.028456343337893486, -0.021694401279091835, 0.020740117877721786], 'magnitude': 0.04135895147919655, 'cosine_with_motion': -0.2502635419368744, 'motion_component': -0.010350637137889862, 'motion_component_percent': 25.02635419368744}, {'resid': 1313, 'atom': 'C6', 'charge': 0.06000000238418579, 'distance': 24.480422973632812, 'force': [-0.023157740011811256, -0.018398720771074295, 0.01516757719218731], 'magnitude': 0.033239271491765976, 'cosine_with_motion': -0.20191362500190735, 'motion_component': -0.0067114620469510555, 'motion_component_percent': 20.191362500190735}, {'resid': 1313, 'atom': 'H1', 'charge': 0.12000000476837158, 'distance': 25.37667465209961, 'force': [-0.046510323882102966, -0.03190808743238449, 0.025417083874344826], 'magnitude': 0.06186569482088089, 'cosine_with_motion': -0.14724992215633392, 'motion_component': -0.009109718725085258, 'motion_component_percent': 14.724992215633392}, {'resid': 1313, 'atom': 'H10R', 'charge': 0.09000000357627869, 'distance': 21.397281646728516, 'force': [-0.05472002550959587, -0.03378196433186531, -0.01112136896699667], 'magnitude': 0.06526245176792145, 'cosine_with_motion': 0.43375447392463684, 'motion_component': 0.028307881206274033, 'motion_component_percent': 43.375447392463684}, {'resid': 1313, 'atom': 'H10S', 'charge': 0.09000000357627869, 'distance': 20.238534927368164, 'force': [-0.05965800583362579, -0.038559526205062866, -0.016604777425527573], 'magnitude': 0.07294952124357224, 'cosine_with_motion': 0.4842352569103241, 'motion_component': 0.03532472997903824, 'motion_component_percent': 48.42352569103241}, {'resid': 1313, 'atom': 'H10X', 'charge': 0.09000000357627869, 'distance': 21.67898941040039, 'force': [-0.06078709661960602, -0.015236293897032738, -0.010717526078224182], 'magnitude': 0.06357736140489578, 'cosine_with_motion': 0.43699145317077637, 'motion_component': 0.02778276428580284, 'motion_component_percent': 43.69914531707764}, {'resid': 1313, 'atom': 'H10Y', 'charge': 0.09000000357627869, 'distance': 23.419334411621094, 'force': [-0.052049506455659866, -0.012533596716821194, -0.010087216272950172], 'magnitude': 0.05447929725050926, 'cosine_with_motion': 0.45181986689567566, 'motion_component': 0.024614829570055008, 'motion_component_percent': 45.181986689567566}, {'resid': 1313, 'atom': 'H111', 'charge': 0.15000000596046448, 'distance': 22.339914321899414, 'force': [-0.08386557549238205, -0.04548488184809685, -0.029236765578389168], 'magnitude': 0.09978525340557098, 'cosine_with_motion': 0.5461481809616089, 'motion_component': 0.05449753254652023, 'motion_component_percent': 54.61481809616089}, {'resid': 1313, 'atom': 'H11A', 'charge': 0.09000000357627869, 'distance': 24.940025329589844, 'force': [-0.03947716951370239, -0.022127924486994743, 0.016111426055431366], 'magnitude': 0.048038214445114136, 'cosine_with_motion': -0.06150064617395401, 'motion_component': -0.0029543812852352858, 'motion_component_percent': 6.150064617395401}, {'resid': 1313, 'atom': 'H11B', 'charge': 0.09000000357627869, 'distance': 23.315750122070312, 'force': [-0.045325275510549545, -0.02515977993607521, 0.0182673130184412], 'magnitude': 0.05496444180607796, 'cosine_with_motion': -0.05810246244072914, 'motion_component': -0.0031935693696141243, 'motion_component_percent': 5.810246244072914}, {'resid': 1313, 'atom': 'H11X', 'charge': 0.09000000357627869, 'distance': 21.70240592956543, 'force': [-0.06225941330194473, -0.00811767578125, -0.009084763936698437], 'magnitude': 0.06344024091959, 'cosine_with_motion': 0.4088320732116699, 'motion_component': 0.02593640610575676, 'motion_component_percent': 40.88320732116699}, {'resid': 1313, 'atom': 'H11Y', 'charge': 0.09000000357627869, 'distance': 21.90745735168457, 'force': [-0.06006093695759773, -0.008900129236280918, -0.01376796793192625], 'magnitude': 0.06225821375846863, 'cosine_with_motion': 0.4806446433067322, 'motion_component': 0.029924076050519943, 'motion_component_percent': 48.06446433067322}, {'resid': 1313, 'atom': 'H12', 'charge': 0.09000000357627869, 'distance': 24.674724578857422, 'force': [-0.04253276810050011, -0.02081781066954136, 0.012888426892459393], 'magnitude': 0.04907676950097084, 'cosine_with_motion': 0.016786547377705574, 'motion_component': 0.0008238295558840036, 'motion_component_percent': 1.6786547377705574}, {'resid': 1313, 'atom': 'H121', 'charge': 0.15000000596046448, 'distance': 23.686283111572266, 'force': [-0.0703335851430893, -0.04689730331301689, -0.02707083150744438], 'magnitude': 0.08876372873783112, 'cosine_with_motion': 0.5517435073852539, 'motion_component': 0.048974812030792236, 'motion_component_percent': 55.17435073852539}, {'resid': 1313, 'atom': 'H12X', 'charge': 0.09000000357627869, 'distance': 24.246295928955078, 'force': [-0.04992233216762543, -0.006047288421541452, -0.007383708842098713], 'magnitude': 0.05082645267248154, 'cosine_with_motion': 0.41019514203071594, 'motion_component': 0.02084876410663128, 'motion_component_percent': 41.019514203071594}, {'resid': 1313, 'atom': 'H12Y', 'charge': 0.09000000357627869, 'distance': 23.438549041748047, 'force': [-0.05331629514694214, -0.003671312239021063, -0.01010782178491354], 'magnitude': 0.054390016943216324, 'cosine_with_motion': 0.443785160779953, 'motion_component': 0.024137482047080994, 'motion_component_percent': 44.3785160779953}, {'resid': 1313, 'atom': 'H13A', 'charge': 0.09000000357627869, 'distance': 26.42348861694336, 'force': [-0.0357477068901062, -0.020964404568076134, 0.010680285282433033], 'magnitude': 0.04279571771621704, 'cosine_with_motion': 0.02719710022211075, 'motion_component': 0.0011639194563031197, 'motion_component_percent': 2.719710022211075}, {'resid': 1313, 'atom': 'H13B', 'charge': 0.09000000357627869, 'distance': 25.20548439025879, 'force': [-0.03872540220618248, -0.024647096171975136, 0.010239271447062492], 'magnitude': 0.04703167825937271, 'cosine_with_motion': 0.05783113092184067, 'motion_component': 0.002719895215705037, 'motion_component_percent': 5.783113092184067}, {'resid': 1313, 'atom': 'H13R', 'charge': 0.09000000357627869, 'distance': 22.165023803710938, 'force': [-0.045816484838724136, -0.03693843632936478, -0.015343938954174519], 'magnitude': 0.06081969290971756, 'cosine_with_motion': 0.4982631504535675, 'motion_component': 0.030304212123155594, 'motion_component_percent': 49.82631504535675}, {'resid': 1313, 'atom': 'H13S', 'charge': 0.09000000357627869, 'distance': 22.807205200195312, 'force': [-0.045363206416368484, -0.03343940153717995, -0.01112090703099966], 'magnitude': 0.05744291841983795, 'cosine_with_motion': 0.44918355345726013, 'motion_component': 0.02580241486430168, 'motion_component_percent': 44.91835534572601}, {'resid': 1313, 'atom': 'H13X', 'charge': 0.09000000357627869, 'distance': 24.7167911529541, 'force': [-0.046792320907115936, -0.008217798545956612, -0.011624171398580074], 'magnitude': 0.04890986159443855, 'cosine_with_motion': 0.49674180150032043, 'motion_component': 0.024295572191476822, 'motion_component_percent': 49.67418015003204}, {'resid': 1313, 'atom': 'H13Y', 'charge': 0.09000000357627869, 'distance': 25.645816802978516, 'force': [-0.04416908696293831, -0.005449919495731592, -0.009128015488386154], 'magnitude': 0.0454305000603199, 'cosine_with_motion': 0.46106666326522827, 'motion_component': 0.02094648964703083, 'motion_component_percent': 46.10666632652283}, {'resid': 1313, 'atom': 'H141', 'charge': 0.15000000596046448, 'distance': 25.06597137451172, 'force': [-0.06171484291553497, -0.046577516943216324, -0.01743963547050953], 'magnitude': 0.07926113903522491, 'cosine_with_motion': 0.47213977575302124, 'motion_component': 0.037422336637973785, 'motion_component_percent': 47.213977575302124}, {'resid': 1313, 'atom': 'H14X', 'charge': 0.09000000357627869, 'distance': 23.714794158935547, 'force': [-0.050795335322618484, -0.004123025573790073, -0.015021935105323792], 'magnitude': 0.05313025414943695, 'cosine_with_motion': 0.5313454866409302, 'motion_component': 0.028230519965291023, 'motion_component_percent': 53.13454866409302}, {'resid': 1313, 'atom': 'H14Y', 'charge': 0.09000000357627869, 'distance': 25.023344039916992, 'force': [-0.04615321010351181, -0.0021567512303590775, -0.01192969735711813], 'magnitude': 0.047718845307826996, 'cosine_with_motion': 0.499822735786438, 'motion_component': 0.02385096438229084, 'motion_component_percent': 49.9822735786438}, {'resid': 1313, 'atom': 'H151', 'charge': 0.15000000596046448, 'distance': 25.855365753173828, 'force': [-0.05402318760752678, -0.04690302535891533, -0.020763656124472618], 'magnitude': 0.07449515163898468, 'cosine_with_motion': 0.5182983875274658, 'motion_component': 0.03861071541905403, 'motion_component_percent': 51.82983875274658}, {'resid': 1313, 'atom': 'H15X', 'charge': 0.09000000357627869, 'distance': 25.63323211669922, 'force': [-0.042694948613643646, -0.0060399919748306274, -0.014444601722061634], 'magnitude': 0.04547512158751488, 'cosine_with_motion': 0.565484881401062, 'motion_component': 0.02571549452841282, 'motion_component_percent': 56.5484881401062}, {'resid': 1313, 'atom': 'H15Y', 'charge': 0.09000000357627869, 'distance': 26.812896728515625, 'force': [-0.03960096463561058, -0.0037836600095033646, -0.01203417032957077], 'magnitude': 0.041561685502529144, 'cosine_with_motion': 0.5382915735244751, 'motion_component': 0.022372305393218994, 'motion_component_percent': 53.82915735244751}, {'resid': 1313, 'atom': 'H16R', 'charge': 0.09000000357627869, 'distance': 24.88914680480957, 'force': [-0.032903384417295456, -0.03125625476241112, -0.016340473666787148], 'magnitude': 0.048234812915325165, 'cosine_with_motion': 0.5662842392921448, 'motion_component': 0.02731461450457573, 'motion_component_percent': 56.62842392921448}, {'resid': 1313, 'atom': 'H16S', 'charge': 0.09000000357627869, 'distance': 23.263376235961914, 'force': [-0.038966450840234756, -0.03451082110404968, -0.018412137404084206], 'magnitude': 0.05521220713853836, 'cosine_with_motion': 0.5652920603752136, 'motion_component': 0.031211022287607193, 'motion_component_percent': 56.52920603752136}, {'resid': 1313, 'atom': 'H16X', 'charge': 0.09000000357627869, 'distance': 25.80626106262207, 'force': [-0.04223889485001564, -0.0008907602750696242, -0.01510501466691494], 'magnitude': 0.04486735165119171, 'cosine_with_motion': 0.573813796043396, 'motion_component': 0.025745505467057228, 'motion_component_percent': 57.3813796043396}, {'resid': 1313, 'atom': 'H16Y', 'charge': 0.09000000357627869, 'distance': 24.779163360595703, 'force': [-0.04514994099736214, -0.003236297518014908, -0.0178658626973629], 'magnitude': 0.048663947731256485, 'cosine_with_motion': 0.6038366556167603, 'motion_component': 0.029385074973106384, 'motion_component_percent': 60.383665561676025}, {'resid': 1313, 'atom': 'H17R', 'charge': 0.09000000357627869, 'distance': 22.465389251708984, 'force': [-0.040438588708639145, -0.040471211075782776, -0.015229661948978901], 'magnitude': 0.059204231947660446, 'cosine_with_motion': 0.491600900888443, 'motion_component': 0.02910485304892063, 'motion_component_percent': 49.1600900888443}, {'resid': 1313, 'atom': 'H17S', 'charge': 0.09000000357627869, 'distance': 24.21015167236328, 'force': [-0.034239307045936584, -0.035580310970544815, -0.012668912298977375], 'magnitude': 0.05097832903265953, 'cosine_with_motion': 0.48156502842903137, 'motion_component': 0.02454937994480133, 'motion_component_percent': 48.15650284290314}, {'resid': 1313, 'atom': 'H17X', 'charge': 0.09000000357627869, 'distance': 26.652952194213867, 'force': [-0.03829847276210785, -0.004701498430222273, -0.016743212938308716], 'magnitude': 0.042062003165483475, 'cosine_with_motion': 0.6332148313522339, 'motion_component': 0.026634283363819122, 'motion_component_percent': 63.32148313522339}, {'resid': 1313, 'atom': 'H17Y', 'charge': 0.09000000357627869, 'distance': 26.818923950195312, 'force': [-0.03779064118862152, -0.0018663987284526229, -0.017152419313788414], 'magnitude': 0.041543006896972656, 'cosine_with_motion': 0.6409434080123901, 'motion_component': 0.026626715436577797, 'motion_component_percent': 64.09434080123901}, {'resid': 1313, 'atom': 'H18R', 'charge': 0.09000000357627869, 'distance': 24.025501251220703, 'force': [-0.0316954106092453, -0.03701687231659889, -0.017457397654652596], 'magnitude': 0.05176493525505066, 'cosine_with_motion': 0.552656352519989, 'motion_component': 0.02860822156071663, 'motion_component_percent': 55.2656352519989}, {'resid': 1313, 'atom': 'H18S', 'charge': 0.090000003576</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>807</v>
-      </c>
-      <c r="B11" t="n">
-        <v>806</v>
-      </c>
-      <c r="C11" t="n">
-        <v>2231</v>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>{}</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>939</v>
-      </c>
-      <c r="B12" t="n">
-        <v>946</v>
-      </c>
-      <c r="C12" t="n">
-        <v>2381</v>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>{939: {'frame': 939, 'motion_vector': [-4.074672698974609, -0.7788047790527344, 1.4778213500976562], 'ionic_force': [6.851991251111031, 8.000294297933578, -4.192061893641949], 'ionic_force_magnitude': 11.337013534391478, 'radial_force': 10.533493862857217, 'axial_force': -4.192061893641949, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [6.12185263633728, -7.080075323581696, 1.0930774211883545], 'asn_force_magnitude': 9.423341474091446, 'residue_force': [6.12185263633728, -7.080075323581696, 1.0930774211883545], 'residue_force_magnitude': 9.423341474091446, 'pip2_force': [0.6937301754951477, -0.07981214637402445, -4.579628557604792], 'pip2_force_magnitude': 4.63256184640105, 'total_force': [13.667574062943459, 0.8404068279778585, -7.678613030058386], 'total_force_magnitude': 15.699361849066955, 'cosine_total_motion': -0.9791164881546054, 'cosine_glu_motion': 0, 'cosine_asn_motion': -0.4292968054055065, 'cosine_residue_motion': -0.4292968054055065, 'cosine_pip2_motion': -0.46725637384149626, 'cosine_ionic_motion': -0.8081052008199872, 'motion_component_total': -15.37150403992683, 'motion_component_glu': 0, 'motion_component_asn': -4.045410391072674, 'motion_component_residue': -4.045410391072674, 'motion_component_ionic': -9.161499598908337, 'motion_component_pip2': -2.164594049945821, 'motion_component_percent_total': 97.91164881546054, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 42.92968054055065, 'motion_component_percent_residue': 42.92968054055065, 'motion_component_percent_ionic': 80.81052008199872, 'motion_component_percent_pip2': 46.72563738414963, 'ionic_contributions': [{'ion_id': 2333, 'distance': 9.940918922424316, 'force': [0.5586365461349487, 3.312108039855957, -0.06815715879201889], 'magnitude': 3.3595802783966064, 'cosine_ionic_motion': -0.33501172065734863, 'motion_component_ionic': -1.1254987716674805, 'motion_component_percent_ionic': 33.50117206573486}, {'ion_id': 2334, 'distance': 13.11501407623291, 'force': [0.7408196330070496, 0.6163527965545654, -1.6724047660827637], 'magnitude': 1.930192232131958, 'cosine_ionic_motion': -0.7023535966873169, 'motion_component_ionic': -1.3556774854660034, 'motion_component_percent_ionic': 70.23535966873169}, {'ion_id': 2343, 'distance': 7.49332857131958, 'force': [3.0116941928863525, 2.9080581665039062, -4.175325870513916], 'magnitude': 5.912736415863037, 'cosine_ionic_motion': -0.7952401041984558, 'motion_component_ionic': -4.70204496383667, 'motion_component_percent_ionic': 79.52401041984558}, {'ion_id': 2372, 'distance': 14.712966918945312, 'force': [0.21832038462162018, 0.3984614908695221, 1.4648445844650269], 'magnitude': 1.5336899757385254, 'cosine_ionic_motion': 0.14285781979560852, 'motion_component_ionic': 0.21909961104393005, 'motion_component_percent_ionic': 14.285781979560852}, {'ion_id': 2397, 'distance': 11.619467735290527, 'force': [2.3225204944610596, 0.7653138041496277, 0.258981317281723], 'magnitude': 2.4590401649475098, 'cosine_ionic_motion': -0.8935918211936951, 'motion_component_ionic': -2.197378158569336, 'motion_component_percent_ionic': 89.3591821193695}], 'glu_contributions': [], 'asn_contributions': [{'resid': 458, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 5.998406887054443, 'force': [4.847882270812988, -6.2280755043029785, -2.82234787940979], 'magnitude': 8.381916999816895, 'cosine_with_motion': -0.5167387127876282, 'motion_component': -4.331261157989502, 'motion_component_percent': 51.67387127876282}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 5.7243452072143555, 'force': [1.273970365524292, -0.851999819278717, 3.9154253005981445], 'magnitude': 4.204694747924805, 'cosine_with_motion': 0.06798364222049713, 'motion_component': 0.285850465297699, 'motion_component_percent': 6.798364222049713}], 'pip2_contributions': [{'resid': 1313, 'atom': 'C1', 'charge': 0.06000000238418579, 'distance': 24.639312744140625, 'force': [-0.020335327833890915, -0.014827649109065533, 0.021053263917565346], 'magnitude': 0.032811958342790604, 'cosine_with_motion': 0.8686710596084595, 'motion_component': 0.028502799570560455, 'motion_component_percent': 86.86710596084595}, {'resid': 1313, 'atom': 'C11', 'charge': 0.17000000178813934, 'distance': 23.087688446044922, 'force': [-0.07590331137180328, -0.04445202648639679, 0.0589398518204689], 'magnitude': 0.10588296502828598, 'cosine_with_motion': 0.9243295192718506, 'motion_component': 0.09787075221538544, 'motion_component_percent': 92.43295192718506}, {'resid': 1313, 'atom': 'C12', 'charge': 0.04000000283122063, 'distance': 22.739980697631836, 'force': [-0.01948999986052513, -0.010492898523807526, 0.013021943159401417], 'magnitude': 0.025681355968117714, 'cosine_with_motion': 0.9446119070053101, 'motion_component': 0.024258915334939957, 'motion_component_percent': 94.461190700531}, {'resid': 1313, 'atom': 'C13', 'charge': -0.05000000074505806, 'distance': 23.34505844116211, 'force': [0.02330896630883217, 0.013698745518922806, -0.014028468169271946], 'magnitude': 0.030459176748991013, 'cosine_with_motion': -0.942152202129364, 'motion_component': -0.02869717963039875, 'motion_component_percent': 94.2152202129364}, {'resid': 1313, 'atom': 'C2', 'charge': 0.06000000238418579, 'distance': 26.224149703979492, 'force': [-0.018320659175515175, -0.013162858784198761, 0.018169039860367775], 'magnitude': 0.028965866193175316, 'cosine_with_motion': 0.8760794997215271, 'motion_component': 0.025376401841640472, 'motion_component_percent': 87.60794997215271}, {'resid': 1313, 'atom': 'C21', 'charge': 0.6299999952316284, 'distance': 20.92860221862793, 'force': [-0.37244027853012085, -0.1659366488456726, 0.24856694042682648], 'magnitude': 0.4775272309780121, 'cosine_with_motion': 0.9577770233154297, 'motion_component': 0.45736461877822876, 'motion_component_percent': 95.77770233154297}, {'resid': 1313, 'atom': 'C210', 'charge': -0.18000000715255737, 'distance': 21.98310089111328, 'force': [0.09677869826555252, 0.06851125508546829, -0.03510170057415962], 'magnitude': 0.12366098165512085, 'cosine_with_motion': -0.9173567295074463, 'motion_component': -0.11344123631715775, 'motion_component_percent': 91.73567295074463}, {'resid': 1313, 'atom': 'C211', 'charge': -0.15000000596046448, 'distance': 23.416135787963867, 'force': [0.07012628763914108, 0.05175080895423889, -0.025555647909641266], 'magnitude': 0.09082364290952682, 'cosine_with_motion': -0.909600555896759, 'motion_component': -0.08261323720216751, 'motion_component_percent': 90.9600555896759}, {'resid': 1313, 'atom': 'C212', 'charge': -0.15000000596046448, 'distance': 23.9794864654541, 'force': [0.06633873283863068, 0.05173797905445099, -0.020567188039422035], 'magnitude': 0.08660632371902466, 'cosine_with_motion': -0.8940739631652832, 'motion_component': -0.07743246108293533, 'motion_component_percent': 89.40739631652832}, {'resid': 1313, 'atom': 'C213', 'charge': -0.18000000715255737, 'distance': 23.289011001586914, 'force': [0.08406686782836914, 0.06830301135778427, -0.020184490829706192], 'magnitude': 0.11018145829439163, 'cosine_with_motion': -0.8770688772201538, 'motion_component': -0.09663672745227814, 'motion_component_percent': 87.70688772201538}, {'resid': 1313, 'atom': 'C214', 'charge': -0.15000000596046448, 'distance': 24.309247970581055, 'force': [0.0626591369509697, 0.05487443134188652, -0.012825705111026764], 'magnitude': 0.0842725858092308, 'cosine_with_motion': -0.8541883826255798, 'motion_component': -0.07198466360569, 'motion_component_percent': 85.41883826255798}, {'resid': 1313, 'atom': 'C215', 'charge': -0.15000000596046448, 'distance': 24.18225860595703, 'force': [0.06265537440776825, 0.05702746659517288, -0.008625385351479053], 'magnitude': 0.08515999466180801, 'cosine_with_motion': -0.8331659436225891, 'motion_component': -0.070952408015728, 'motion_component_percent': 83.31659436225891}, {'resid': 1313, 'atom': 'C216', 'charge': -0.18000000715255737, 'distance': 23.130308151245117, 'force': [0.08315408229827881, 0.07427938282489777, -0.006674831733107567], 'magnitude': 0.11169862002134323, 'cosine_with_motion': -0.8264696598052979, 'motion_component': -0.09231551736593246, 'motion_component_percent': 82.64696598052979}, {'resid': 1313, 'atom': 'C217', 'charge': -0.18000000715255737, 'distance': 23.19447135925293, 'force': [0.07966838777065277, 0.07740402221679688, -0.0008127559558488429], 'magnitude': 0.11108148097991943, 'cosine_with_motion': -0.78929203748703, 'motion_component': -0.08767572790384293, 'motion_component_percent': 78.929203748703}, {'resid': 1313, 'atom': 'C218', 'charge': -0.18000000715255737, 'distance': 22.543895721435547, 'force': [0.0857994481921196, 0.08021186292171478, 0.005549025721848011], 'magnitude': 0.1175852045416832, 'cosine_with_motion': -0.7799472212791443, 'motion_component': -0.09171025454998016, 'motion_component_percent': 77.99472212791443}, {'resid': 1313, 'atom': 'C219', 'charge': -0.18000000715255737, 'distance': 21.019975662231445, 'force': [0.09819309413433075, 0.09277896583080292, 0.006594967097043991], 'magnitude': 0.13525277376174927, 'cosine_with_motion': -0.7766873240470886, 'motion_component': -0.10504911094903946, 'motion_component_percent': 77.66873240470886}, {'resid': 1313, 'atom': 'C22', 'charge': -0.08000000566244125, 'distance': 19.36884117126465, 'force': [0.05585312098264694, 0.024307815358042717, -0.03608202189207077], 'magnitude': 0.07079797238111496, 'cosine_with_motion': -0.9616940021514893, 'motion_component': -0.06808598339557648, 'motion_component_percent': 96.16940021514893}, {'resid': 1313, 'atom': 'C220', 'charge': -0.27000001072883606, 'distance': 20.462318420410156, 'force': [0.15678946673870087, 0.14359845221042633, 0.025103580206632614], 'magnitude': 0.21408793330192566, 'cosine_with_motion': -0.7568964958190918, 'motion_component': -0.16204240918159485, 'motion_component_percent': 75.68964958190918}, {'resid': 1313, 'atom': 'C23', 'charge': -0.18000000715255737, 'distance': 19.14923667907715, 'force': [0.1360931694507599, 0.05079604312777519, -0.07387581467628479], 'magnitude': 0.16297000646591187, 'cosine_with_motion': -0.9799124002456665, 'motion_component': -0.1596963256597519, 'motion_component_percent': 97.99124002456665}, {'resid': 1313, 'atom': 'C24', 'charge': -0.18000000715255737, 'distance': 19.071264266967773, 'force': [0.13982678949832916, 0.057948172092437744, -0.06392747908830643], 'magnitude': 0.16430534422397614, 'cosine_with_motion': -0.9803534150123596, 'motion_component': -0.16107730567455292, 'motion_component_percent': 98.03534150123596}, {'resid': 1313, 'atom': 'C25', 'charge': -0.15000000596046448, 'distance': 17.86975860595703, 'force': [0.13029135763645172, 0.06276167184114456, -0.058363333344459534], 'magnitude': 0.15595237910747528, 'cosine_with_motion': -0.9697740077972412, 'motion_component': -0.1512385606765747, 'motion_component_percent': 96.97740077972412}, {'resid': 1313, 'atom': 'C26', 'charge': -0.15000000596046448, 'distance': 18.004230499267578, 'force': [0.12548945844173431, 0.07146970182657242, -0.05241288244724274], 'magnitude': 0.15363147854804993, 'cosine_with_motion': -0.9525306820869446, 'motion_component': -0.14633870124816895, 'motion_component_percent': 95.25306820869446}, {'resid': 1313, 'atom': 'C27', 'charge': -0.18000000715255737, 'distance': 19.369293212890625, 'force': [0.12989914417266846, 0.0777636468410492, -0.04951459541916847], 'magnitude': 0.15928800404071808, 'cosine_with_motion': -0.9452016949653625, 'motion_component': -0.15055929124355316, 'motion_component_percent': 94.52016949653625}, {'resid': 1313, 'atom': 'C28', 'charge': -0.15000000596046448, 'distance': 20.29339027404785, 'force': [0.09487087279558182, 0.06107473373413086, -0.043503113090991974], 'magnitude': 0.12092611938714981, 'cosine_with_motion': -0.9359449744224548, 'motion_component': -0.11318019032478333, 'motion_component_percent': 93.59449744224548}, {'resid': 1313, 'atom': 'C29', 'charge': -0.15000000596046448, 'distance': 21.375568389892578, 'force': [0.08405409753322601, 0.05839860811829567, -0.03746642917394638], 'magnitude': 0.108991838991642, 'cosine_with_motion': -0.9236726760864258, 'motion_component': -0.10067278146743774, 'motion_component_percent': 92.36726760864258}, {'resid': 1313, 'atom': 'C3', 'charge': 0.06000000238418579, 'distance': 27.02078628540039, 'force': [-0.017152510583400726, -0.011391998268663883, 0.0178991686552763], 'magnitude': 0.02728307992219925, 'cosine_with_motion': 0.8757008910179138, 'motion_component': 0.023891817778348923, 'motion_component_percent': 87.57008910179138}, {'resid': 1313, 'atom': 'C31', 'charge': 0.6299999952316284, 'distance': 23.81771469116211, 'force': [-0.30059126019477844, -0.1625380516052246, 0.13845324516296387], 'magnitude': 0.36870452761650085, 'cosine_with_motion': 0.9583080410957336, 'motion_component': 0.35333251953125, 'motion_component_percent': 95.83080410957336}, {'resid': 1313, 'atom': 'C310', 'charge': -0.18000000715255737, 'distance': 20.125701904296875, 'force': [0.14504267275333405, 0.018797073513269424, -0.019422093406319618], 'magnitude': 0.14753957092761993, 'cosine_with_motion': -0.9763109087944031, 'motion_component': -0.14404448866844177, 'motion_component_percent': 97.63109087944031}, {'resid': 1313, 'atom': 'C311', 'charge': -0.18000000715255737, 'distance': 20.057025909423828, 'force': [0.14667262136936188, 0.021990176290273666, -0.008436302654445171], 'magnitude': 0.14855165779590607, 'cosine_with_motion': -0.9587959051132202, 'motion_component': -0.14243072271347046, 'motion_component_percent': 95.87959051132202}, {'resid': 1313, 'atom': 'C312', 'charge': -0.18000000715255737, 'distance': 20.668659210205078, 'force': [0.13923394680023193, 0.013496112078428268, -0.000954567629378289], 'magnitude': 0.13988977670669556, 'cosine_with_motion': -0.9402768015861511, 'motion_component': -0.1315351128578186, 'motion_component_percent': 94.02768015861511}, {'resid': 1313, 'atom': 'C313', 'charge': -0.18000000715255737, 'distance': 21.046314239501953, 'force': [0.13481798768043518, 0.003995935898274183, -0.003170651849359274], 'magnitude': 0.13491445779800415, 'cosine_with_motion': -0.9377257823944092, 'motion_component': -0.12651276588439941, 'motion_component_percent': 93.77257823944092}, {'resid': 1313, 'atom': 'C314', 'charge': -0.18000000715255737, 'distance': 21.7316951751709, 'force': [0.12645623087882996, -0.0005960842245258391, 0.0045289164409041405], 'magnitude': 0.1265387088060379, 'cosine_with_motion': -0.9118162393569946, 'motion_component': -0.11538004875183105, 'motion_component_percent': 91.18162393569946}, {'resid': 1313, 'atom': 'C315', 'charge': -0.18000000715255737, 'distance': 20.905445098876953, 'force': [0.13607607781887054, -0.001677597756497562, 0.013341237790882587], 'magnitude': 0.13673880696296692, 'cosine_with_motion': -0.8858672976493835, 'motion_component': -0.12113244086503983, 'motion_component_percent': 88.58672976493835}, {'resid': 1313, 'atom': 'C316', 'charge': -0.18000000715255737, 'distance': 21.60270118713379, 'force': [0.12646563351154327, -0.00714101642370224, 0.01879827119410038], 'magnitude': 0.12805438041687012, 'cosine_with_motion': -0.8546587228775024, 'motion_component': -0.10944279283285141, 'motion_component_percent': 85.46587228775024}, {'resid': 1313, 'atom': 'C317', 'charge': -0.18000000715255737, 'distance': 20.944175720214844, 'force': [0.13286277651786804, -0.009005315601825714, 0.02873956225812435], 'magnitude': 0.13623353838920593, 'cosine_with_motion': -0.8198865652084351, 'motion_component': -0.11169604957103729, 'motion_component_percent': 81.9886565208435}, {'resid': 1313, 'atom': 'C318', 'charge': -0.27000001072883606, 'distance': 21.929576873779297, 'force': [0.1792498081922531, -0.01732555776834488, 0.04809950292110443], 'magnitude': 0.18639804422855377, 'cosine_with_motion': -0.7867467403411865, 'motion_component': -0.14664804935455322, 'motion_component_percent': 78.67467403411865}, {'resid': 1313, 'atom': 'C32', 'charge': -0.08000000566244125, 'distance': 23.333284378051758, 'force': [0.04139629006385803, 0.02013884298503399, -0.016144409775733948], 'magnitude': 0.048783887177705765, 'cosine_with_motion': -0.969207227230072, 'motion_component': -0.047281697392463684, 'motion_component_percent': 96.9207227230072}, {'resid': 1313, 'atom': 'C33', 'charge': -0.18000000715255737, 'distance': 24.199308395385742, 'force': [0.08879955857992172, 0.037246059626340866, -0.033781252801418304], 'magnitude': 0.10204804688692093, 'cosine_with_motion': -0.9807745218276978, 'motion_component': -0.10008612275123596, 'motion_component_percent': 98.07745218276978}, {'resid': 1313, 'atom': 'C34', 'charge': -0.18000000715255737, 'distance': 23.733802795410156, 'force': [0.0953674167394638, 0.034145597368478775, -0.031532518565654755], 'magnitude': 0.10609036684036255, 'cosine_with_motion': -0.9884042739868164, 'motion_component': -0.10486017167568207, 'motion_component_percent': 98.84042739868164}, {'resid': 1313, 'atom': 'C35', 'charge': -0.18000000715255737, 'distance': 22.62854766845703, 'force': [0.10542266070842743, 0.03277288377285004, -0.03784898668527603], 'magnitude': 0.11670709401369095, 'cosine_with_motion': -0.9942911863327026, 'motion_component': -0.11604083329439163, 'motion_component_percent': 99.42911863327026}, {'resid': 1313, 'atom': 'C36', 'charge': -0.18000000715255737, 'distance': 22.1077823638916, 'force': [0.11348351836204529, 0.029882656410336494, -0.034329164773225784], 'magnitude': 0.12227008491754532, 'cosine_with_motion': -0.9962120652198792, 'motion_component': -0.12180693447589874, 'motion_component_percent': 99.62120652198792}, {'resid': 1313, 'atom': 'C37', 'charge': -0.18000000715255737, 'distance': 20.74103355407715, 'force': [0.12922166287899017, 0.03022986277937889, -0.04105306789278984], 'magnitude': 0.13891521096229553, 'cosine_with_motion': -0.9983547329902649, 'motion_component': -0.1386866569519043, 'motion_component_percent': 99.83547329902649}, {'resid': 1313, 'atom': 'C38', 'charge': -0.18000000715255737, 'distance': 20.31368064880371, 'force': [0.13818798959255219, 0.023756947368383408, -0.03623517230153084], 'magnitude': 0.14482161402702332, 'cosine_with_motion': -0.9958552718162537, 'motion_component': -0.14422136545181274, 'motion_component_percent': 99.58552718162537}, {'resid': 1313, 'atom': 'C39', 'charge': -0.18000000715255737, 'distance': 20.030624389648438, 'force': [0.14393064379692078, 0.027521591633558273, -0.026659062132239342], 'magnitude': 0.14894352853298187, 'cosine_with_motion': -0.9868643879890442, 'motion_component': -0.14698706567287445, 'motion_component_percent': 98.68643879890442}, {'resid': 1313, 'atom': 'C4', 'charge': 0.08000000566244125, 'distance': 27.09943389892578, 'force': [-0.021163279190659523, -0.015059158205986023, 0.025166647508740425], 'magnitude': 0.03616659715771675, 'cosine_with_motion': 0.8485779762268066, 'motion_component': 0.030690178275108337, 'motion_component_percent': 84.85779762268066}, {'resid': 1313, 'atom': 'C5', 'charge': 0.08000000566244125, 'distance': 25.696643829345703, 'force': [-0.022835662588477135, -0.0164418313652277, 0.028741860762238503], 'magnitude': 0.040223076939582825, 'cosine_with_motion': 0.837376594543457, 'motion_component': 0.03368186205625534, 'motion_component_percent': 83.7376594543457}, {'resid': 1313, 'atom': 'C6', 'charge': 0.06000000238418579, 'distance': 24.525794982910156, 'force': [-0.018977362662553787, -0.01479191891849041, 0.022754233330488205], 'magnitude': 0.033116403967142105, 'cosine_with_motion': 0.8397897481918335, 'motion_component': 0.02781081572175026, 'motion_component_percent': 83.97897481918335}, {'resid': 1313, 'atom': 'H1', 'charge': 0.12000000476837158, 'distance': 24.129514694213867, 'force': [-0.04395900294184685, -0.028680842369794846, 0.043899375945329666], 'magnitude': 0.06842616200447083, 'cosine_with_motion': 0.8838358521461487, 'motion_component': 0.060477495193481445, 'motion_component_percent': 88.38358521461487}, {'resid': 1313, 'atom': 'H10R', 'charge': 0.09000000357627869, 'distance': 21.337480545043945, 'force': [-0.05067255347967148, -0.0381813608109951, 0.01678134873509407], 'magnitude': 0.0656287893652916, 'cosine_with_motion': 0.9030977487564087, 'motion_component': 0.05926921218633652, 'motion_component_percent': 90.30977487564087}, {'resid': 1313, 'atom': 'H10S', 'charge': 0.09000000357627869, 'distance': 22.037206649780273, 'force': [-0.04997966066002846, -0.03212229534983635, 0.015993574634194374], 'magnitude': 0.061527252197265625, 'cosine_with_motion': 0.9311680197715759, 'motion_component': 0.057292208075523376, 'motion_component_percent': 93.11680197715759}, {'resid': 1313, 'atom': 'H10X', 'charge': 0.09000000357627869, 'distance': 21.142837524414062, 'force': [-0.06583354622125626, -0.007219814229756594, 0.00904246885329485], 'magnitude': 0.0668427124619484, 'cosine_with_motion': 0.9757925271987915, 'motion_component': 0.06522461771965027, 'motion_component_percent': 97.57925271987915}, {'resid': 1313, 'atom': 'H10Y', 'charge': 0.09000000357627869, 'distance': 19.46343421936035, 'force': [-0.07778820395469666, -0.0066772811114788055, 0.011213392950594425], 'magnitude': 0.07887541502714157, 'cosine_with_motion': 0.9751883745193481, 'motion_component': 0.07691838592290878, 'motion_component_percent': 97.51883745193481}, {'resid': 1313, 'atom': 'H111', 'charge': 0.15000000596046448, 'distance': 24.06795883178711, 'force': [-0.0658726692199707, -0.048096515238285065, 0.027175189927220345], 'magnitude': 0.08597077429294586, 'cosine_with_motion': 0.9139704704284668, 'motion_component': 0.07857474684715271, 'motion_component_percent': 91.39704704284668}, {'resid': 1313, 'atom': 'H11A', 'charge': 0.09000000357627869, 'distance': 24.1783504486084, 'force': [-0.03650572896003723, -0.02141064777970314, 0.02866017445921898], 'magnitude': 0.051112521439790726, 'cosine_with_motion': 0.9230924844741821, 'motion_component': 0.04718158394098282, 'motion_component_percent': 92.30924844741821}, {'resid': 1313, 'atom': 'H11B', 'charge': 0.09000000357627869, 'distance': 22.667190551757812, 'force': [-0.041346460580825806, -0.022550897672772408, 0.03411601483821869], 'magnitude': 0.05815475061535835, 'cosine_with_motion': 0.92327880859375, 'motion_component': 0.053693048655986786, 'motion_component_percent': 92.327880859375}, {'resid': 1313, 'atom': 'H11X', 'charge': 0.09000000357627869, 'distance': 19.057605743408203, 'force': [-0.08116772025823593, -0.013083504512906075, 0.0030083712190389633], 'magnitude': 0.08227045089006424, 'cosine_with_motion': 0.9532563090324402, 'motion_component': 0.07842482626438141, 'motion_component_percent': 95.32563090324402}, {'resid': 1313, 'atom': 'H11Y', 'charge': 0.09000000357627869, 'distance': 20.589380264282227, 'force': [-0.06906619668006897, -0.013656321913003922, 0.003382262075319886], 'magnitude': 0.07048457115888596, 'cosine_with_motion': 0.9570109844207764, 'motion_component': 0.0674545094370842, 'motion_component_percent': 95.70109844207764}, {'resid': 1313, 'atom': 'H12', 'charge': 0.09000000357627869, 'distance': 23.318710327148438, 'force': [-0.042868368327617645, -0.020587226375937462, 0.02753225341439247], 'magnitude': 0.05495048686861992, 'cosine_with_motion': 0.9562166929244995, 'motion_component': 0.052544571459293365, 'motion_component_percent': 95.62166929244995}, {'resid': 1313, 'atom': 'H121', 'charge': 0.15000000596046448, 'distance': 25.008586883544922, 'force': [-0.06024628505110741, -0.04836283624172211, 0.019277166575193405], 'magnitude': 0.07962529361248016, 'cosine_with_motion': 0.8887321352958679, 'motion_component': 0.07076555490493774, 'motion_component_percent': 88.87321352958679}, {'resid': 1313, 'atom': 'H12X', 'charge': 0.09000000357627869, 'distance': 20.102676391601562, 'force': [-0.07355457544326782, -0.006949625443667173, -0.0028955978341400623], 'magnitude': 0.07393887639045715, 'cosine_with_motion': 0.9239342212677002, 'motion_component': 0.06831465661525726, 'motion_component_percent': 92.39342212677002}, {'resid': 1313, 'atom': 'H12Y', 'charge': 0.09000000357627869, 'distance': 21.63641357421875, 'force': [-0.06339171528816223, -0.00743575906381011, -0.0004382760089356452], 'magnitude': 0.06382783502340317, 'cosine_with_motion': 0.9372389316558838, 'motion_component': 0.05982193350791931, 'motion_component_percent': 93.72389316558838}, {'resid': 1313, 'atom': 'H13A', 'charge': 0.09000000357627869, 'distance': 24.43229103088379, 'force': [-0.03815118223428726, -0.02250312641263008, 0.023316407576203346], 'magnitude': 0.050055552273988724, 'cosine_with_motion': 0.9410346150398254, 'motion_component': 0.04710400849580765, 'motion_component_percent': 94.10346150398254}, {'resid': 1313, 'atom': 'H13B', 'charge': 0.09000000357627869, 'distance': 22.931833267211914, 'force': [-0.042345400899648666, -0.027744876220822334, 0.025799784809350967], 'magnitude': 0.05682024359703064, 'cosine_with_motion': 0.9282805323600769, 'motion_component': 0.05274512618780136, 'motion_component_percent': 92.82805323600769}, {'resid': 1313, 'atom': 'H13R', 'charge': 0.09000000357627869, 'distance': 22.94049835205078, 'force': [-0.04468102753162384, -0.03395114094018936, 0.008636587299406528], 'magnitude': 0.05677732825279236, 'cosine_with_motion': 0.8849335312843323, 'motion_component': 0.05024415999650955, 'motion_component_percent': 88.49335312843323}, {'resid': 1313, 'atom': 'H13S', 'charge': 0.09000000357627869, 'distance': 22.349082946777344, 'force': [-0.044692061841487885, -0.03805166482925415, 0.011548462323844433], 'magnitude': 0.05982203781604767, 'cosine_with_motion': 0.8685210943222046, 'motion_component': 0.05195670202374458, 'motion_component_percent': 86.85210943222046}, {'resid': 1313, 'atom': 'H13X', 'charge': 0.09000000357627869, 'distance': 21.830142974853516, 'force': [-0.06254952400922775, -0.0023318014573305845, 0.0036618083249777555], 'magnitude': 0.06269999593496323, 'cosine_with_motion': 0.9492178559303284, 'motion_component': 0.05951595678925514, 'motion_component_percent': 94.92178559303284}, {'resid': 1313, 'atom': 'H13Y', 'charge': 0.09000000357627869, 'distance': 20.241775512695312, 'force': [-0.07285916060209274, 6.011372897773981e-05, 0.003125089220702648], 'magnitude': 0.07292617112398148, 'cosine_with_motion': 0.938647449016571, 'motion_component': 0.06845196336507797, 'motion_component_percent': 93.8647449016571}, {'resid': 1313, 'atom': 'H141', 'charge': 0.15000000596046448, 'distance': 25.184038162231445, 'force': [-0.05736609548330307, -0.051866933703422546, 0.013575570657849312], 'magnitude': 0.07851970195770264, 'cosine_with_motion': 0.8508307933807373, 'motion_component': 0.06680697947740555, 'motion_component_percent': 85.08307933807373}, {'resid': 1313, 'atom': 'H14X', 'charge': 0.09000000357627869, 'distance': 22.028718948364258, 'force': [-0.06148798018693924, 0.00306149385869503, -0.001138343708589673], 'magnitude': 0.06157467141747475, 'cosine_with_motion': 0.9089634418487549, 'motion_component': 0.055969126522541046, 'motion_component_percent': 90.89634418487549}, {'resid': 1313, 'atom': 'H14Y', 'charge': 0.09000000357627869, 'distance': 22.667308807373047, 'force': [-0.05806950107216835, -0.0009041635203175247, -0.003003334626555443], 'magnitude': 0.0581541433930397, 'cosine_with_motion': 0.9093351364135742, 'motion_component': 0.05288160592317581, 'motion_component_percent': 90.93351364135742}, {'resid': 1313, 'atom': 'H151', 'charge': 0.15000000596046448, 'distance': 24.988792419433594, 'force': [-0.05733231455087662, -0.054999932646751404, 0.006950778421014547], 'magnitude': 0.07975149154663086, 'cosine_with_motion': 0.8163689970970154, 'motion_component': 0.06510664522647858, 'motion_component_percent': 81.63689970970154}, {'resid': 1313, 'atom': 'H15X', 'charge': 0.09000000357627869, 'distance': 19.887939453125, 'force': [-0.07521861791610718, 0.0022465738002210855, -0.0066359140910208225], 'magnitude': 0.07554417848587036, 'cosine_with_motion': 0.886538565158844, 'motion_component': 0.06697282940149307, 'motion_component_percent': 88.6538565158844}, {'resid': 1313, 'atom': 'H15Y', 'charge': 0.09000000357627869, 'distance': 20.813556671142578, 'force': [-0.0684763491153717, -0.002579909050837159, -0.007861553691327572], 'magnitude': 0.06897442042827606, 'cosine_with_motion': 0.8869478702545166, 'motion_component': 0.06117671728134155, 'motion_component_percent': 88.69478702545166}, {'resid': 1313, 'atom': 'H16R', 'charge': 0.09000000357627869, 'distance': 23.38818359375, 'force': [-0.0421663373708725, -0.03465820476412773, 0.0021556608844548464], 'magnitude': 0.0546245202422142, 'cosine_with_motion': 0.8396887183189392, 'motion_component': 0.045867592096328735, 'motion_component_percent': 83.96887183189392}, {'resid': 1313, 'atom': 'H16S', 'charge': 0.09000000357627869, 'distance': 22.115705490112305, 'force': [-0.045379482209682465, -0.040621645748615265, 0.004767152015119791], 'magnitude': 0.06109125539660454, 'cosine_with_motion': 0.8310777544975281, 'motion_component': 0.05077158287167549, 'motion_component_percent': 83.10777544975281}, {'resid': 1313, 'atom': 'H16X', 'charge': 0.09000000357627869, 'distance': 22.603778839111328, 'force': [-0.0577290914952755, 0.00219282740727067, -0.009090056642889977], 'magnitude': 0.058481499552726746, 'cosine_with_motion': 0.8545670509338379, 'motion_component': 0.04997636377811432, 'motion_component_percent': 85.45670509338379}, {'resid': 1313, 'atom': 'H16Y', 'charge': 0.09000000357627869, 'distance': 21.90448570251465, 'force': [-0.061444103717803955, 0.006256175693124533, -0.00797942839562893], 'magnitude': 0.06227510794997215, 'cosine_with_motion': 0.85215163230896, 'motion_component': 0.05306783318519592, 'motion_component_percent': 85.215163230896}, {'resid': 1313, 'atom': 'H17R', 'charge': 0.09000000357627869, 'distance': 22.731294631958008, 'force': [-0.03984002768993378, -0.04188866540789604, 0.0014486905420199037], 'magnitude': 0.057827215641736984, 'cosine_with_motion': 0.7739711403846741, 'motion_component': 0.04475659504532814, 'motion_component_percent': 77.39711403846741}, {'resid': 1313, 'atom': 'H17S', 'charge': 0.09000000357627869, 'distance': 24.230440139770508, 'force': [-0.0361163504421711, -0.03585635870695114, -0.00016574228357058018], 'magnitude': 0.050892990082502365, 'cosine_with_motion': 0.7801200151443481, 'motion_component': 0.0397026389837265, 'motion_component_percent': 78.01200151443481}, {'resid': 1313, 'atom': 'H17X', 'charge': 0.09000000357627869, 'distance': 20.59868049621582, 'force': [-0.06850893795490265, 0.0014138646656647325, -0.016236843541264534], 'magnitude': 0.07042094320058823, 'cosine_with_motion': 0.8192166686058044, 'motion_component': 0.057690009474754333, 'motion_component_percent': 81.92166686058044}, {'resid': 1313, 'atom': 'H17Y', 'charge': 0.09000000357627869, 'distance': 20.1258602142334, 'force': [-0.0718555897474289, 0.007422902155667543, -0.014949467964470387], 'magnitude': 0.07376863807439804, 'cosine_with_motion': 0.8154666423797607, 'motion_component': 0.06015586480498314, 'motion_component_percent': 81.54666423797607}, {'resid': 1313, 'atom': 'H18R', 'charge': 0.09000000357627869, 'distance': 22.869035720825195, 'force': [-0.040217239409685135, -0.04034048318862915, -0.0044007874093949795], 'magnitude': 0.057132720947265625, 'cosine_with_motion': 0.7503381371498108, 'motion_component': 0.04286886006593704, 'motion_component_percent': 75.03381371498108}, {'resid': 1313, 'atom': 'H18S', 'charge': 0.09000000357627869, 'distance': 22.962663650512695, 'force': [-0.042934171855449677, -0.0368291437625885, -0.003392125479876995], 'magnitude': 0.056667763739824295, 'cosine_with_motion': 0.7958713173866272, 'motion_component': 0.04510024935007095, 'motion_component_percent': 79.58713173866272}, {'resid': 1313, 'atom': 'H18X', 'charge': 0.09000000357627869, 'distance': 22.19989776611328, 'force': [-0.05804911255836487, 0.00852067768573761, -0.0152821596711874], 'magnitude': 0.060628753155469894, 'cosine_with_motion': 0.7764543890953064, 'motion_component': 0.047075461596250534, 'motion_component_percent': 77.64543890953064}, {'resid': 1313, 'atom': 'H18Y', 'charge': 0.09000000357627869, 'distance': 21.588253021240234, 'force': [-0.06084006652235985, 0.005482955370098352, -0.019465133547782898], 'magnitude': 0.06411293148994446, 'cosine_with_motion': 0.761021614074707, 'motion_component': 0.04879132658243179, 'motion_component_percent': 76.1021614074707}, {'resid': 1313, 'atom': 'H18Z', 'charge': 0.09000000357627869, 'distance': 22.852102279663086, 'force': [-0.05528092384338379, 0.003927062265574932, -0.014227837324142456], 'magnitude': 0.057217422872781754, 'cosine_with</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>963</v>
-      </c>
-      <c r="B13" t="n">
-        <v>1186</v>
-      </c>
-      <c r="C13" t="n">
-        <v>2343</v>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t xml:space="preserve">{963: {'frame': 963, 'motion_vector': [-6.639595031738281, 1.0836753845214844, 2.0808258056640625], 'ionic_force': [-0.03461587429046631, -3.451846368610859, -26.245480060577393], 'ionic_force_magnitude': 26.47152555523407, 'radial_force': 3.452019932046289, 'axial_force': -26.245480060577393, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [0.6113827228546143, -0.2678259313106537, -0.847156286239624], 'asn_force_magnitude': 1.0785144118660877, 'residue_force': [0.6113827228546143, -0.2678259313106537, -0.847156286239624], 'residue_force_magnitude': 1.0785144118660877, 'pip2_force': [0.9694522628251434, 0.05543461270281114, -4.4345879283257545], 'pip2_force_magnitude': 4.53965646059642, 'total_force': [1.5462191113892914, -3.6642376872187015, -31.52722427514277], 'total_force_magnitude': 31.777087686948455, 'cosine_total_motion': -0.356792005652496, 'cosine_glu_motion': 0, 'cosine_asn_motion': -0.8048084027521138, 'cosine_residue_motion': -0.8048084027521138, 'cosine_pip2_motion': -0.4881252484365865, 'cosine_ionic_motion': -0.311802673918244, 'motion_component_total': -11.337810849621576, 'motion_component_glu': 0, 'motion_component_asn': -0.8679974611590815, 'motion_component_residue': -0.8679974611590815, 'motion_component_ionic': -8.253892450817112, 'motion_component_pip2': -2.2159209376453823, 'motion_component_percent_total': 35.6792005652496, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 80.48084027521139, 'motion_component_percent_residue': 80.48084027521139, 'motion_component_percent_ionic': 31.1802673918244, 'motion_component_percent_pip2': 48.81252484365865, 'ionic_contributions': [{'ion_id': 2230, 'distance': 14.592389106750488, 'force': [0.16000592708587646, 0.08226221054792404, -1.5487253665924072], 'magnitude': 1.5591405630111694, 'cosine_ionic_motion': -0.3821600377559662, 'motion_component_ionic': -0.5958412289619446, 'motion_component_percent_ionic': 38.21600377559662}, {'ion_id': 2333, 'distance': 4.4050493240356445, 'force': [1.2773457765579224, -5.039449691772461, -16.30049705505371], 'magnitude': 17.109468460083008, 'cosine_ionic_motion': -0.3972393572330475, 'motion_component_ionic': -6.796554088592529, 'motion_component_percent_ionic': 39.72393572330475}, {'ion_id': 2334, 'distance': 9.08781909942627, 'force': [0.15932977199554443, 0.28409475088119507, -4.006714344024658], 'magnitude': 4.019932270050049, 'cosine_ionic_motion': -0.32101526856422424, 'motion_component_ionic': -1.2904596328735352, 'motion_component_percent_ionic': 32.101526856422424}, {'ion_id': 2372, 'distance': 7.211418151855469, 'force': [-5.535534858703613, -1.084515929222107, -2.9896254539489746], 'magnitude': 6.38405704498291, 'cosine_ionic_motion': 0.6530299186706543, 'motion_component_ionic': 4.168980121612549, 'motion_component_percent_ionic': 65.30299186706543}, {'ion_id': 2397, 'distance': 8.364306449890137, 'force': [3.9042375087738037, 2.30576229095459, -1.3999178409576416], 'magnitude': 4.745459079742432, 'cosine_ionic_motion': -0.7881255149841309, 'motion_component_ionic': -3.7400174140930176, 'motion_component_percent_ionic': 78.81255149841309}], 'glu_contributions': [], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 5.723193645477295, 'force': [-7.815121173858643, -2.1620965003967285, -4.361874580383301], 'magnitude': 9.207427978515625, 'cosine_with_motion': 0.6241716742515564, 'motion_component': 5.747015476226807, 'motion_component_percent': 62.41716742515564}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 5.179661750793457, 'force': [4.4384284019470215, 0.4155177175998688, 2.5497331619262695], 'magnitude': 5.135507583618164, 'cosine_with_motion': -0.6557264924049377, 'motion_component': -3.367488384246826, 'motion_component_percent': 65.57264924049377}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 5.5684099197387695, 'force': [3.3907041549682617, 1.6970765590667725, 2.3168129920959473], 'magnitude': 4.443485736846924, 'cosine_with_motion': -0.506635844707489, 'motion_component': -2.2512290477752686, 'motion_component_percent': 50.6635844707489}, {'resid': 786, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 5.938525199890137, 'force': [-2.098083734512329, -5.628914833068848, 3.042907476425171], 'magnitude': 6.733938217163086, 'cosine_with_motion': 0.2986576557159424, 'motion_component': 2.0111422538757324, 'motion_component_percent': 29.86576557159424}, {'resid': 786, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 5.167057991027832, 'force': [2.6954550743103027, 5.410591125488281, -4.394735336303711], 'magnitude': 7.473531246185303, 'cosine_with_motion': -0.4024118483066559, 'motion_component': -3.0074374675750732, 'motion_component_percent': 40.24118483066559}], 'pip2_contributions': [{'resid': 1313, 'atom': 'C1', 'charge': 0.06000000238418579, 'distance': 26.762588500976562, 'force': [-0.019891858100891113, -0.014739428646862507, 0.01267177239060402], 'magnitude': 0.027812058106064796, 'cosine_with_motion': 0.7274393439292908, 'motion_component': 0.020231585949659348, 'motion_component_percent': 72.74393439292908}, {'resid': 1313, 'atom': 'C11', 'charge': 0.17000000178813934, 'distance': 26.427982330322266, 'force': [-0.0638677179813385, -0.04040871933102608, 0.0286028403788805], 'magnitude': 0.0808088630437851, 'cosine_with_motion': 0.7728402614593506, 'motion_component': 0.06245234236121178, 'motion_component_percent': 77.28402614593506}, {'resid': 1313, 'atom': 'C12', 'charge': 0.04000000283122063, 'distance': 26.833744049072266, 'force': [-0.01504645124077797, -0.00906425155699253, 0.005620868876576424], 'magnitude': 0.018443170934915543, 'cosine_with_motion': 0.7836431264877319, 'motion_component': 0.014452864415943623, 'motion_component_percent': 78.3643126487732}, {'resid': 1313, 'atom': 'C13', 'charge': -0.05000000074505806, 'distance': 27.97826385498047, 'force': [0.017085665836930275, 0.011044013313949108, -0.005985010415315628], 'magnitude': 0.021206380799412727, 'cosine_with_motion': -0.762907862663269, 'motion_component': -0.016178514808416367, 'motion_component_percent': 76.2907862663269}, {'resid': 1313, 'atom': 'C2', 'charge': 0.06000000238418579, 'distance': 28.321269989013672, 'force': [-0.017902033403515816, -0.013132689520716667, 0.011127717792987823], 'magnitude': 0.02483498305082321, 'cosine_with_motion': 0.7306807637214661, 'motion_component': 0.018146444112062454, 'motion_component_percent': 73.0680763721466}, {'resid': 1313, 'atom': 'C21', 'charge': 0.6299999952316284, 'distance': 24.583093643188477, 'force': [-0.2893790006637573, -0.16362537443637848, 0.09630119800567627], 'magnitude': 0.34610313177108765, 'cosine_with_motion': 0.7978042960166931, 'motion_component': 0.2761225700378418, 'motion_component_percent': 79.78042960166931}, {'resid': 1313, 'atom': 'C210', 'charge': -0.18000000715255737, 'distance': 25.10736656188965, 'force': [0.06947992742061615, 0.06443540006875992, -0.0027669069822877645], 'magnitude': 0.09479998052120209, 'cosine_with_motion': -0.5950649976730347, 'motion_component': -0.05641215294599533, 'motion_component_percent': 59.50649976730347}, {'resid': 1313, 'atom': 'C211', 'charge': -0.15000000596046448, 'distance': 26.290699005126953, 'force': [0.05240496248006821, 0.04924248903989792, -0.004459430929273367], 'magnitude': 0.07204851508140564, 'cosine_with_motion': -0.598913848400116, 'motion_component': -0.043150853365659714, 'motion_component_percent': 59.8913848400116}, {'resid': 1313, 'atom': 'C212', 'charge': -0.15000000596046448, 'distance': 27.569135665893555, 'force': [0.047940317541360855, 0.044577740132808685, -0.0027571427635848522], 'magnitude': 0.06552137434482574, 'cosine_with_motion': -0.5976083278656006, 'motion_component': -0.039156120270490646, 'motion_component_percent': 59.76083278656006}, {'resid': 1313, 'atom': 'C213', 'charge': -0.18000000715255737, 'distance': 27.952190399169922, 'force': [0.05667218938469887, 0.051358774304389954, 0.0007519636419601738], 'magnitude': 0.07648546248674393, 'cosine_with_motion': -0.5923830270767212, 'motion_component': -0.04530869051814079, 'motion_component_percent': 59.23830270767212}, {'resid': 1313, 'atom': 'C214', 'charge': -0.15000000596046448, 'distance': 28.414627075195312, 'force': [0.04377865046262741, 0.04339771345257759, 0.0021235353779047728], 'magnitude': 0.061680153012275696, 'cosine_with_motion': -0.5507704019546509, 'motion_component': -0.03397160395979881, 'motion_component_percent': 55.07704019546509}, {'resid': 1313, 'atom': 'C215', 'charge': -0.15000000596046448, 'distance': 28.393760681152344, 'force': [0.04319930821657181, 0.043883685022592545, 0.004866094794124365], 'magnitude': 0.06177084147930145, 'cosine_with_motion': -0.5267885327339172, 'motion_component': -0.03254017233848572, 'motion_component_percent': 52.678853273391724}, {'resid': 1313, 'atom': 'C216', 'charge': -0.18000000715255737, 'distance': 28.03108787536621, 'force': [0.05454341322183609, 0.052216220647096634, 0.009106190875172615], 'magnitude': 0.07605551183223724, 'cosine_with_motion': -0.5351482033729553, 'motion_component': -0.04070097208023071, 'motion_component_percent': 53.51482033729553}, {'resid': 1313, 'atom': 'C217', 'charge': -0.18000000715255737, 'distance': 29.268497467041016, 'force': [0.049641840159893036, 0.047776564955711365, 0.010936998762190342], 'magnitude': 0.0697605237364769, 'cosine_with_motion': -0.5192286372184753, 'motion_component': -0.03622166067361832, 'motion_component_percent': 51.922863721847534}, {'resid': 1313, 'atom': 'C218', 'charge': -0.18000000715255737, 'distance': 29.321205139160156, 'force': [0.04684366285800934, 0.04973236843943596, 0.012806112878024578], 'magnitude': 0.06950995326042175, 'cosine_with_motion': -0.47086864709854126, 'motion_component': -0.03273005783557892, 'motion_component_percent': 47.086864709854126}, {'resid': 1313, 'atom': 'C219', 'charge': -0.18000000715255737, 'distance': 29.887514114379883, 'force': [0.04465264454483986, 0.04732326418161392, 0.015567946247756481], 'magnitude': 0.06690075248479843, 'cosine_with_motion': -0.4516966938972473, 'motion_component': -0.03021884895861149, 'motion_component_percent': 45.16966938972473}, {'resid': 1313, 'atom': 'C22', 'charge': -0.08000000566244125, 'distance': 23.702129364013672, 'force': [0.039832428097724915, 0.023036548867821693, -0.01085564587265253], 'magnitude': 0.04727737233042717, 'cosine_with_motion': -0.7872570753097534, 'motion_component': -0.037219446152448654, 'motion_component_percent': 78.72570753097534}, {'resid': 1313, 'atom': 'C220', 'charge': -0.27000001072883606, 'distance': 29.59727668762207, 'force': [0.0644836500287056, 0.07494063675403595, 0.02640010416507721], 'magnitude': 0.10232891142368317, 'cosine_with_motion': -0.4052232801914215, 'motion_component': -0.04146605730056763, 'motion_component_percent': 40.52232801914215}, {'resid': 1313, 'atom': 'C23', 'charge': -0.18000000715255737, 'distance': 22.757890701293945, 'force': [0.09399432688951492, 0.06091022491455078, -0.027722574770450592], 'magnitude': 0.11538427323102951, 'cosine_with_motion': -0.7578391432762146, 'motion_component': -0.08744271844625473, 'motion_component_percent': 75.78391432762146}, {'resid': 1313, 'atom': 'C24', 'charge': -0.18000000715255737, 'distance': 23.43341827392578, 'force': [0.08493218570947647, 0.06298304349184036, -0.025751154869794846], 'magnitude': 0.10882766544818878, 'cosine_with_motion': -0.7166998982429504, 'motion_component': -0.07799677550792694, 'motion_component_percent': 71.66998982429504}, {'resid': 1313, 'atom': 'C25', 'charge': -0.15000000596046448, 'distance': 24.402074813842773, 'force': [0.06551200896501541, 0.049481309950351715, -0.015943532809615135], 'magnitude': 0.08363264799118042, 'cosine_with_motion': -0.7038614153862, 'motion_component': -0.05886579304933548, 'motion_component_percent': 70.38614153862}, {'resid': 1313, 'atom': 'C26', 'charge': -0.15000000596046448, 'distance': 24.217132568359375, 'force': [0.0664040669798851, 0.051584258675575256, -0.01183658093214035], 'magnitude': 0.08491490036249161, 'cosine_with_motion': -0.6850351691246033, 'motion_component': -0.05816969275474548, 'motion_component_percent': 68.50351691246033}, {'resid': 1313, 'atom': 'C27', 'charge': -0.18000000715255737, 'distance': 22.966123580932617, 'force': [0.08796126395463943, 0.07035423070192337, -0.012259798124432564], 'magnitude': 0.11330138891935349, 'cosine_with_motion': -0.6684107184410095, 'motion_component': -0.07573186606168747, 'motion_component_percent': 66.84107184410095}, {'resid': 1313, 'atom': 'C28', 'charge': -0.15000000596046448, 'distance': 22.98751449584961, 'force': [0.06928504258394241, 0.06328228861093521, -0.008747700601816177], 'magnitude': 0.09424217790365219, 'cosine_with_motion': -0.6172727942466736, 'motion_component': -0.05817313492298126, 'motion_component_percent': 61.72727942466736}, {'resid': 1313, 'atom': 'C29', 'charge': -0.15000000596046448, 'distance': 23.79194450378418, 'force': [0.06329765170812607, 0.06089157611131668, -0.005058333743363619], 'magnitude': 0.08797705918550491, 'cosine_with_motion': -0.5888527631759644, 'motion_component': -0.0518055334687233, 'motion_component_percent': 58.885276317596436}, {'resid': 1313, 'atom': 'C3', 'charge': 0.06000000238418579, 'distance': 29.115154266357422, 'force': [-0.016818678006529808, -0.01179804839193821, 0.011408139020204544], 'magnitude': 0.02349909581243992, 'cosine_with_motion': 0.7410171031951904, 'motion_component': 0.01741323247551918, 'motion_component_percent': 74.10171031951904}, {'resid': 1313, 'atom': 'C31', 'charge': 0.6299999952316284, 'distance': 29.007389068603516, 'force': [-0.21095629036426544, -0.11783666908740997, 0.058331817388534546], 'magnitude': 0.24857722222805023, 'cosine_with_motion': 0.7965611815452576, 'motion_component': 0.19800697267055511, 'motion_component_percent': 79.65611815452576}, {'resid': 1313, 'atom': 'C310', 'charge': -0.18000000715255737, 'distance': 25.97843360900879, 'force': [0.08632601797580719, 0.01921309158205986, -0.004431640263646841], 'magnitude': 0.08854921907186508, 'cosine_with_motion': -0.9005948305130005, 'motion_component': -0.07974696904420853, 'motion_component_percent': 90.05948305130005}, {'resid': 1313, 'atom': 'C311', 'charge': -0.18000000715255737, 'distance': 25.659189224243164, 'force': [0.08941670507192612, 0.015544496476650238, -0.0012443121522665024], 'magnitude': 0.09076633304357529, 'cosine_with_motion': -0.9065455794334412, 'motion_component': -0.08228381723165512, 'motion_component_percent': 90.65455794334412}, {'resid': 1313, 'atom': 'C312', 'charge': -0.18000000715255737, 'distance': 26.09272003173828, 'force': [0.08710889518260956, 0.01043660193681717, -0.0027579437009990215], 'magnitude': 0.08777521550655365, 'cosine_with_motion': -0.926698625087738, 'motion_component': -0.08134116977453232, 'motion_component_percent': 92.6698625087738}, {'resid': 1313, 'atom': 'C313', 'charge': -0.18000000715255737, 'distance': 25.839996337890625, 'force': [0.08925434947013855, 0.006611107382923365, 0.0005515532102435827], 'magnitude': 0.0895005539059639, 'cosine_with_motion': -0.9270873069763184, 'motion_component': -0.08297482877969742, 'motion_component_percent': 92.70873069763184}, {'resid': 1313, 'atom': 'C314', 'charge': -0.18000000715255737, 'distance': 26.229080200195312, 'force': [0.08684282749891281, 0.0014933100901544094, -0.001269129803404212], 'magnitude': 0.08686493337154388, 'cosine_with_motion': -0.9443010091781616, 'motion_component': -0.0820266455411911, 'motion_component_percent': 94.43010091781616}, {'resid': 1313, 'atom': 'C315', 'charge': -0.18000000715255737, 'distance': 26.034404754638672, 'force': [0.08811075240373611, -0.0024179653264582157, 0.002097445772960782], 'magnitude': 0.08816887438297272, 'cosine_with_motion': -0.9394385814666748, 'motion_component': -0.08282924443483353, 'motion_component_percent': 93.94385814666748}, {'resid': 1313, 'atom': 'C316', 'charge': -0.18000000715255737, 'distance': 26.812908172607422, 'force': [0.082877516746521, -0.006364058703184128, 0.0005459367530420423], 'magnitude': 0.08312329649925232, 'cosine_with_motion': -0.9499227404594421, 'motion_component': -0.07896070927381516, 'motion_component_percent': 94.99227404594421}, {'resid': 1313, 'atom': 'C317', 'charge': -0.18000000715255737, 'distance': 26.729522705078125, 'force': [0.08298132568597794, -0.009512803517282009, 0.00443989085033536], 'magnitude': 0.08364273607730865, 'cosine_with_motion': -0.9372303485870361, 'motion_component': -0.07839251309633255, 'motion_component_percent': 93.72303485870361}, {'resid': 1313, 'atom': 'C318', 'charge': -0.27000001072883606, 'distance': 27.670429229736328, 'force': [0.11544671654701233, -0.01858649030327797, 0.005790174473077059], 'magnitude': 0.11707659065723419, 'cosine_with_motion': -0.9395599961280823, 'motion_component': -0.11000048369169235, 'motion_component_percent': 93.95599961280823}, {'resid': 1313, 'atom': 'C32', 'charge': -0.08000000566244125, 'distance': 29.195816040039062, 'force': [0.026941383257508278, 0.014539418742060661, -0.005802188068628311], 'magnitude': 0.031159238889813423, 'cosine_with_motion': -0.7984546422958374, 'motion_component': -0.02487923949956894, 'motion_component_percent': 79.84546422958374}, {'resid': 1313, 'atom': 'C33', 'charge': -0.18000000715255737, 'distance': 28.14741325378418, 'force': [0.06660670042037964, 0.03305990993976593, -0.012649143114686012], 'magnitude': 0.07542818039655685, 'cosine_with_motion': -0.8147029280662537, 'motion_component': -0.06145155802369118, 'motion_component_percent': 81.47029280662537}, {'resid': 1313, 'atom': 'C34', 'charge': -0.18000000715255737, 'distance': 28.376157760620117, 'force': [0.06680087745189667, 0.029195137321949005, -0.013908675871789455], 'magnitude': 0.07421700656414032, 'cosine_with_motion': -0.843493640422821, 'motion_component': -0.06260157376527786, 'motion_component_percent': 84.3493640422821}, {'resid': 1313, 'atom': 'C35', 'charge': -0.18000000715255737, 'distance': 27.184528350830078, 'force': [0.07392701506614685, 0.02956741489470005, -0.014138811267912388], 'magnitude': 0.08086619526147842, 'cosine_with_motion': -0.8573582768440247, 'motion_component': -0.06933130323886871, 'motion_component_percent': 85.73582768440247}, {'resid': 1313, 'atom': 'C36', 'charge': -0.18000000715255737, 'distance': 27.032487869262695, 'force': [0.07575861364603043, 0.029172390699386597, -0.009864569641649723], 'magnitude': 0.0817783921957016, 'cosine_with_motion': -0.8542115688323975, 'motion_component': -0.06985604763031006, 'motion_component_percent': 85.42115688323975}, {'resid': 1313, 'atom': 'C37', 'charge': -0.18000000715255737, 'distance': 26.099279403686523, 'force': [0.08267445862293243, 0.02787947840988636, -0.009187712334096432], 'magnitude': 0.08773110061883926, 'cosine_with_motion': -0.8705663681030273, 'motion_component': -0.07637574523687363, 'motion_component_percent': 87.05663681030273}, {'resid': 1313, 'atom': 'C38', 'charge': -0.18000000715255737, 'distance': 26.150400161743164, 'force': [0.08292005956172943, 0.027304742485284805, -0.003930915612727404], 'magnitude': 0.08738842606544495, 'cosine_with_motion': -0.8598669767379761, 'motion_component': -0.07514242082834244, 'motion_component_percent': 85.98669767379761}, {'resid': 1313, 'atom': 'C39', 'charge': -0.18000000715255737, 'distance': 25.37773323059082, 'force': [0.08940848708152771, 0.02473253756761551, -0.0021344078704714775], 'magnitude': 0.09279079735279083, 'cosine_with_motion': -0.8742800354957581, 'motion_component': -0.08112514019012451, 'motion_component_percent': 87.4280035495758}, {'resid': 1313, 'atom': 'C4', 'charge': 0.08000000566244125, 'distance': 28.958219528198242, 'force': [-0.02157505974173546, -0.016244444996118546, 0.016546646133065224], 'magnitude': 0.0316726490855217, 'cosine_with_motion': 0.7177174091339111, 'motion_component': 0.02273201197385788, 'motion_component_percent': 71.77174091339111}, {'resid': 1313, 'atom': 'C5', 'charge': 0.08000000566244125, 'distance': 27.434900283813477, 'force': [-0.023836206644773483, -0.017842208966612816, 0.01893940195441246], 'magnitude': 0.035287536680698395, 'cosine_with_motion': 0.7176793813705444, 'motion_component': 0.025325138121843338, 'motion_component_percent': 71.76793813705444}, {'resid': 1313, 'atom': 'C6', 'charge': 0.06000000238418579, 'distance': 26.474260330200195, 'force': [-0.019330289214849472, -0.01518103014677763, 0.014270185492932796], 'magnitude': 0.028421154245734215, 'cosine_with_motion': 0.7074469327926636, 'motion_component': 0.02010645903646946, 'motion_component_percent': 70.74469327926636}, {'resid': 1313, 'atom': 'H1', 'charge': 0.12000000476837158, 'distance': 26.296268463134766, 'force': [-0.042390353977680206, -0.028736749663949013, 0.026394642889499664], 'magnitude': 0.05761440843343735, 'cosine_with_motion': 0.7523410320281982, 'motion_component': 0.04334568232297897, 'motion_component_percent': 75.23410320281982}, {'resid': 1313, 'atom': 'H10R', 'charge': 0.09000000357627869, 'distance': 25.20809555053711, 'force': [-0.033974312245845795, -0.032504238188266754, -0.0005324145313352346], 'magnitude': 0.04702194035053253, 'cosine_with_motion': 0.5715193152427673, 'motion_component': 0.02687394805252552, 'motion_component_percent': 57.15193152427673}, {'resid': 1313, 'atom': 'H10S', 'charge': 0.09000000357627869, 'distance': 25.097301483154297, 'force': [-0.036136139184236526, -0.030713576823472977, 0.0011052251793444157], 'magnitude': 0.04743802174925804, 'cosine_with_motion': 0.6254844665527344, 'motion_component': 0.029671745374798775, 'motion_component_percent': 62.54844665527344}, {'resid': 1313, 'atom': 'H10X', 'charge': 0.09000000357627869, 'distance': 27.070980072021484, 'force': [-0.03971916064620018, -0.00898080412298441, 0.002042219275608659], 'magnitude': 0.040772996842861176, 'cosine_with_motion': 0.8994037508964539, 'motion_component': 0.036671385169029236, 'motion_component_percent': 89.94037508964539}, {'resid': 1313, 'atom': 'H10Y', 'charge': 0.09000000357627869, 'distance': 25.797964096069336, 'force': [-0.043643224984407425, -0.009694688953459263, 0.0041172681376338005], 'magnitude': 0.044896211475133896, 'cosine_with_motion': 0.9104235172271729, 'motion_component': 0.04087456688284874, 'motion_component_percent': 91.04235172271729}, {'resid': 1313, 'atom': 'H111', 'charge': 0.15000000596046448, 'distance': 26.16447639465332, 'force': [-0.05233442410826683, -0.04997745528817177, 0.0074329255148768425], 'magnitude': 0.07274535298347473, 'cosine_with_motion': 0.6027860045433044, 'motion_component': 0.0438498817384243, 'motion_component_percent': 60.278600454330444}, {'resid': 1313, 'atom': 'H11A', 'charge': 0.09000000357627869, 'distance': 27.372461318969727, 'force': [-0.031167317181825638, -0.01995127461850643, 0.014864152297377586], 'magnitude': 0.03987979516386986, 'cosine_with_motion': 0.7700303196907043, 'motion_component': 0.03070865198969841, 'motion_component_percent': 77.00303196907043}, {'resid': 1313, 'atom': 'H11B', 'charge': 0.09000000357627869, 'distance': 25.84989356994629, 'force': [-0.03565007820725441, -0.021130848675966263, 0.016795270144939423], 'magnitude': 0.044716011732816696, 'cosine_with_motion': 0.7899724245071411, 'motion_component': 0.03532441705465317, 'motion_component_percent': 78.99724245071411}, {'resid': 1313, 'atom': 'H11X', 'charge': 0.09000000357627869, 'distance': 24.572185516357422, 'force': [-0.04877587780356407, -0.0083494633436203, 0.00043011916568502784], 'magnitude': 0.049487218260765076, 'cosine_with_motion': 0.9059203863143921, 'motion_component': 0.04483148083090782, 'motion_component_percent': 90.59203863143921}, {'resid': 1313, 'atom': 'H11Y', 'charge': 0.09000000357627869, 'distance': 26.15770721435547, 'force': [-0.043004684150218964, -0.007520244922488928, -0.0010463681537657976], 'magnitude': 0.04366980493068695, 'cosine_with_motion': 0.8949276804924011, 'motion_component': 0.03908131644129753, 'motion_component_percent': 89.49276804924011}, {'resid': 1313, 'atom': 'H12', 'charge': 0.09000000357627869, 'distance': 27.15093231201172, 'force': [-0.03377176448702812, -0.01853279210627079, 0.012607368640601635], 'magnitude': 0.04053322225809097, 'cosine_with_motion': 0.8071337342262268, 'motion_component': 0.032715730369091034, 'motion_component_percent': 80.71337342262268}, {'resid': 1313, 'atom': 'H121', 'charge': 0.15000000596046448, 'distance': 28.41805076599121, 'force': [-0.04488736391067505, -0.04208515211939812, 0.00407102657482028], 'magnitude': 0.06166529655456543, 'cosine_with_motion': 0.6008145809173584, 'motion_component': 0.03704940900206566, 'motion_component_percent': 60.08145809173584}, {'resid': 1313, 'atom': 'H12X', 'charge': 0.09000000357627869, 'distance': 27.175065994262695, 'force': [-0.04014155641198158, -0.004839177243411541, 0.0015334745403379202], 'magnitude': 0.040461260825395584, 'cosine_with_motion': 0.9282130599021912, 'motion_component': 0.03755667060613632, 'motion_component_percent': 92.82130599021912}, {'resid': 1313, 'atom': 'H12Y', 'charge': 0.09000000357627869, 'distance': 25.660133361816406, 'force': [-0.04497800022363663, -0.005124118644744158, 0.0031703573185950518], 'magnitude': 0.04537982493638992, 'cosine_with_motion': 0.9377877116203308, 'motion_component': 0.04255664348602295, 'motion_component_percent': 93.77877116203308}, {'resid': 1313, 'atom': 'H13A', 'charge': 0.09000000357627869, 'distance': 28.88711929321289, 'force': [-0.02864863909780979, -0.018541911616921425, 0.010845230892300606], 'magnitude': 0.035807348787784576, 'cosine_with_motion': 0.7641781568527222, 'motion_component': 0.027363194152712822, 'motion_component_percent': 76.41781568527222}, {'resid': 1313, 'atom': 'H13B', 'charge': 0.09000000357627869, 'distance': 27.65534782409668, 'force': [-0.030677251517772675, -0.021579217165708542, 0.010934384539723396], 'magnitude': 0.039068110287189484, 'cosine_with_motion': 0.7380660772323608, 'motion_component': 0.02883484587073326, 'motion_component_percent': 73.80660772323608}, {'resid': 1313, 'atom': 'H13R', 'charge': 0.09000000357627869, 'distance': 28.760705947875977, 'force': [-0.027386857196688652, -0.023553140461444855, -0.0002589247014839202], 'magnitude': 0.03612281009554863, 'cosine_with_motion': 0.6123868823051453, 'motion_component': 0.022121135145425797, 'motion_component_percent': 61.238688230514526}, {'resid': 1313, 'atom': 'H13S', 'charge': 0.09000000357627869, 'distance': 27.0929012298584, 'force': [-0.03061833791434765, -0.02680150792002678, -0.0011225523194298148], 'magnitude': 0.040707044303417206, 'cosine_with_motion': 0.5997220873832703, 'motion_component': 0.024412913247942924, 'motion_component_percent': 59.972208738327026}, {'resid': 1313, 'atom': 'H13X', 'charge': 0.09000000357627869, 'distance': 24.788251876831055, 'force': [-0.04848001152276993, -0.003689657198265195, -0.0008851448073983192], 'magnitude': 0.048628270626068115, 'cosine_with_motion': 0.922939658164978, 'motion_component': 0.04488096013665199, 'motion_component_percent': 92.2939658164978}, {'resid': 1313, 'atom': 'H13Y', 'charge': 0.09000000357627869, 'distance': 26.432100296020508, 'force': [-0.04258817806839943, -0.003513163421303034, -0.0017298310995101929], 'magnitude': 0.042767833918333054, 'cosine_with_motion': 0.9143155217170715, 'motion_component': 0.039103295654058456, 'motion_component_percent': 91.43155217170715}, {'resid': 1313, 'atom': 'H141', 'charge': 0.15000000596046448, 'distance': 28.823123931884766, 'force': [-0.0414947085082531, -0.04325687140226364, -0.0005840820958837867], 'magnitude': 0.059944216161966324, 'cosine_with_motion': 0.538746178150177, 'motion_component': 0.03229471668601036, 'motion_component_percent': 53.8746178150177}, {'resid': 1313, 'atom': 'H14X', 'charge': 0.09000000357627869, 'distance': 25.787490844726562, 'force': [-0.04486974701285362, -0.00038726991624571383, 0.0023458064533770084], 'magnitude': 0.04493269696831703, 'cosine_with_motion': 0.9556488394737244, 'motion_component': 0.04293987900018692, 'motion_component_percent': 95.56488394737244}, {'resid': 1313, 'atom': 'H14Y', 'charge': 0.09000000357627869, 'distance': 27.301780700683594, 'force': [-0.040067292749881744, -0.0009459464927203953, 0.0008054838981479406], 'magnitude': 0.04008655250072479, 'cosine_with_motion': 0.9447224140167236, 'motion_component': 0.03787066414952278, 'motion_component_percent': 94.47224140167236}, {'resid': 1313, 'atom': 'H151', 'charge': 0.15000000596046448, 'distance': 28.627288818359375, 'force': [-0.04085644334554672, -0.04468357935547829, -0.005174568388611078], 'magnitude': 0.06076715514063835, 'cosine_with_motion': 0.49561163783073425, 'motion_component': 0.030116910114884377, 'motion_component_percent': 49.561163783073425}, {'resid': 1313, 'atom': 'H15X', 'charge': 0.09000000357627869, 'distance': 24.97854995727539, 'force': [-0.04783531278371811, 0.001748983864672482, -0.0014797872863709927], 'magnitude': 0.04789014533162117, 'cosine_with_motion': 0.9382793307304382, 'motion_component': 0.04493433237075806, 'motion_component_percent': 93.82793307304382}, {'resid': 1313, 'atom': 'H15Y', 'charge': 0.09000000357627869, 'distance': 26.400726318359375, 'force': [-0.04278445616364479, 0.0006426721811294556, -0.002621977822855115], 'magnitude': 0.04286954179406166, 'cosine_with_motion': 0.9252321720123291, 'motion_component': 0.03966427966952324, 'motion_component_percent': 92.52321720123291}, {'resid': 1313, 'atom': 'H16R', 'charge': 0.09000000357627869, 'distance': 27.939992904663086, 'force': [-0.028446994721889496, -0.025280186906456947, -0.0040918029844760895], 'magnitude': 0.038276128470897675, 'cosine_with_motion': 0.5675168037414551, 'motion_component': 0.021722346544265747, 'motion_component_percent': 56.75168037414551}, {'resid': 1313, 'atom': 'H16S', 'charge': 0.09000000357627869, 'distance': 27.117799758911133, 'force': [-0.028651315718889236, -0.02827998250722885, -0.005507360212504864], 'magnitude': 0.040632329881191254, 'cosine_with_motion': 0.5176929831504822, 'motion_component': 0.021035071462392807, 'motion_component_percent': 51.76929831504822}, {'resid': 1313, 'atom': 'H16X', 'charge': 0.09000000357627869, 'distance': 27.834678649902344, 'force': [-0.03847725689411163, 0.002612429205328226, 0.00019136503397021443], 'magnitude': 0.038566313683986664, 'cosine_with_motion': 0.9525824785232544, 'motion_component': 0.0367375947535038, 'motion_component_percent': 95.25824785232544}, {'resid': 1313, 'atom': 'H16Y', 'charge': 0.09000000357627869, 'distance': 26.30425453186035, 'force': [-0.042986027896404266, 0.00397453224286437, 0.0011452377075329423], 'magnitude': 0.04318457096815109, 'cosine_with_motion': 0.9605340361595154, 'motion_component': 0.04148025065660477, 'motion_component_percent': 96.05340361595154}, {'resid': 1313, 'atom': 'H17R', 'charge': 0.09000000357627869, 'distance': 30.24349594116211, 'force': [-0.023321371525526047, -0.02241259068250656, -0.004578051622956991], 'magnitude': 0.032667554914951324, 'cosine_with_motion': 0.5261233448982239, 'motion_component': 0.01718716323375702, 'motion_component_percent': 52.61233448982239}, {'resid': 1313, 'atom': 'H17S', 'charge': 0.09000000357627869, 'distance': 29.127851486206055, 'force': [-0.025671811774373055, -0.02326877973973751, -0.006310627795755863], 'magnitude': 0.03521792218089104, 'cosine_with_motion': 0.5326720476150513, 'motion_component': 0.018759602680802345, 'motion_component_percent': 53.26720476150513}, {'resid': 1313, 'atom': 'H17X', 'charge': 0.09000000357627869, 'distance': 26.983400344848633, 'force': [-0.04068264365196228, 0.003966388292610645, -0.0036491143982857466], 'magnitude': 0.04103809967637062, 'cosine_with_motion': 0.9233010411262512, 'motion_component': 0.03789051994681358, 'motion_component_percent': 92.33010411262512}, {'resid': 1313, 'atom': 'H17Y', 'charge': 0.09000000357627869, 'distance': 25.737140655517578, 'force': [-0.04464470222592354, 0.0058729336597025394, -0.0026742257177829742], 'magnitude': 0.045108672231435776, 'cosine_with_motion': 0.9356889724731445, 'motion_component': 0.042207688093185425, 'motion_component_percent': 93.56889724731445}, {'resid': 1313, 'atom': 'H18R', 'charge': 0.09000000357627869, 'distance': 28.258777618408203, 'force': [-0.024967065081000328, -0.026963235810399055, -0.0070493388921022415], 'magnitude': 0.037417422980070114, 'cosine_with_motion': 0.46257320046424866, 'motion_component': 0.017308296635746956, 'motion_component_percent': 46.257320046424866}, {'resid': 1313, 'atom': 'H18S', 'charge': 0.09000000357627869, </t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>1193</v>
-      </c>
-      <c r="B14" t="n">
-        <v>1225</v>
-      </c>
-      <c r="C14" t="n">
-        <v>2230</v>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>{1193: {'frame': 1193, 'motion_vector': [-6.644626617431641, -6.532619476318359, 5.509552001953125], 'ionic_force': [3.645001269876957, 0.4808567687869072, -8.289402723312378], 'ionic_force_magnitude': 9.068156096955514, 'radial_force': 3.676582310991121, 'axial_force': -8.289402723312378, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [4.907903671264648, -0.8141872882843018, 5.362216949462891], 'asn_force_magnitude': 7.314628493636834, 'residue_force': [4.907903671264648, -0.8141872882843018, 5.362216949462891], 'residue_force_magnitude': 7.314628493636834, 'pip2_force': [0.9515090382192284, 0.19201884046196938, -4.748029754431627], 'pip2_force_magnitude': 4.846238462341004, 'total_force': [9.504413979360834, -0.1413116790354252, -7.6752155282811145], 'total_force_magnitude': 12.217315068674827, 'cosine_total_motion': -0.7902828104054711, 'cosine_glu_motion': 0, 'cosine_asn_motion': 0.028428536362227374, 'cosine_residue_motion': 0.028428536362227374, 'cosine_pip2_motion': -0.643078172187104, 'cosine_ionic_motion': -0.7439845571371395, 'motion_component_total': -9.655134088081454, 'motion_component_glu': 0, 'motion_component_asn': 0.20794418210753918, 'motion_component_residue': 0.20794418210753918, 'motion_component_ionic': -6.7465680978439, 'motion_component_pip2': -3.116510172345094, 'motion_component_percent_total': 79.02828104054711, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 2.8428536362227375, 'motion_component_percent_residue': 2.8428536362227375, 'motion_component_percent_ionic': 74.39845571371396, 'motion_component_percent_pip2': 64.3078172187104, 'ionic_contributions': [{'ion_id': 2333, 'distance': 10.030160903930664, 'force': [1.0726981163024902, -2.0107765197753906, -2.386737108230591], 'magnitude': 3.300063371658325, 'cosine_ionic_motion': -0.1999226063489914, 'motion_component_ionic': -0.6597572565078735, 'motion_component_percent_ionic': 19.99226063489914}, {'ion_id': 2334, 'distance': 9.7400541305542, 'force': [-0.11895801872015, 2.5222208499908447, -2.423072099685669], 'magnitude': 3.49957537651062, 'cosine_ionic_motion': -0.7664731740951538, 'motion_component_ionic': -2.68233060836792, 'motion_component_percent_ionic': 76.64731740951538}, {'ion_id': 2372, 'distance': 10.768108367919922, 'force': [2.345862627029419, 0.040280118584632874, -1.6411902904510498], 'magnitude': 2.8632497787475586, 'cosine_ionic_motion': -0.8031269907951355, 'motion_component_ionic': -2.299553155899048, 'motion_component_percent_ionic': 80.31269907951355}, {'ion_id': 2515, 'distance': 13.31761646270752, 'force': [0.34539854526519775, -0.07086768001317978, -1.8384032249450684], 'magnitude': 1.8719104528427124, 'cosine_ionic_motion': -0.59026700258255, 'motion_component_ionic': -1.1049269437789917, 'motion_component_percent_ionic': 59.026700258255005}], 'glu_contributions': [], 'asn_contributions': [{'resid': 458, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 5.222881317138672, 'force': [4.907903671264648, -0.8141872882843018, 5.362216949462891], 'magnitude': 7.314628601074219, 'cosine_with_motion': 0.02842852473258972, 'motion_component': 0.2079440951347351, 'motion_component_percent': 2.842852473258972}], 'pip2_contributions': [{'resid': 1313, 'atom': 'C1', 'charge': 0.06000000238418579, 'distance': 24.31043243408203, 'force': [-0.02336146868765354, -0.021302517503499985, 0.011684262193739414], 'magnitude': 0.03370574861764908, 'cosine_with_motion': 0.9832779765129089, 'motion_component': 0.03314211964607239, 'motion_component_percent': 98.3277976512909}, {'resid': 1313, 'atom': 'C11', 'charge': 0.17000000178813934, 'distance': 23.78378677368164, 'force': [-0.0771302655339241, -0.059358347207307816, 0.021970687434077263], 'magnitude': 0.0997757613658905, 'cosine_with_motion': 0.94559645652771, 'motion_component': 0.09434760361909866, 'motion_component_percent': 94.559645652771}, {'resid': 1313, 'atom': 'C12', 'charge': 0.04000000283122063, 'distance': 23.867908477783203, 'force': [-0.018453296273946762, -0.013773079961538315, 0.003633467247709632], 'magnitude': 0.02331145480275154, 'cosine_with_motion': 0.921778678894043, 'motion_component': 0.021488001570105553, 'motion_component_percent': 92.1778678894043}, {'resid': 1313, 'atom': 'C13', 'charge': -0.05000000074505806, 'distance': 24.56389617919922, 'force': [0.021045787259936333, 0.01737374998629093, -0.0034796325489878654], 'magnitude': 0.02751145511865616, 'cosine_with_motion': -0.9150347709655762, 'motion_component': -0.025173937901854515, 'motion_component_percent': 91.50347709655762}, {'resid': 1313, 'atom': 'C2', 'charge': 0.06000000238418579, 'distance': 25.856468200683594, 'force': [-0.02093159779906273, -0.01840875670313835, 0.010524202138185501], 'magnitude': 0.029795518144965172, 'cosine_with_motion': 0.9838351011276245, 'motion_component': 0.02931387722492218, 'motion_component_percent': 98.38351011276245}, {'resid': 1313, 'atom': 'C21', 'charge': 0.6299999952316284, 'distance': 21.80260467529297, 'force': [-0.36304256319999695, -0.2405434399843216, 0.06282638013362885], 'magnitude': 0.44000932574272156, 'cosine_with_motion': 0.909028172492981, 'motion_component': 0.3999808728694916, 'motion_component_percent': 90.9028172492981}, {'resid': 1313, 'atom': 'C210', 'charge': -0.18000000715255737, 'distance': 21.178058624267578, 'force': [0.10119704902172089, 0.08647412061691284, 0.005880541168153286], 'magnitude': 0.13324111700057983, 'cosine_with_motion': -0.8353927731513977, 'motion_component': -0.11130866408348083, 'motion_component_percent': 83.53927731513977}, {'resid': 1313, 'atom': 'C211', 'charge': -0.15000000596046448, 'distance': 22.616174697875977, 'force': [0.0749022588133812, 0.06217917427420616, 0.0016819314332678914], 'magnitude': 0.09736234694719315, 'cosine_with_motion': -0.8488288521766663, 'motion_component': -0.08264397084712982, 'motion_component_percent': 84.88288521766663}, {'resid': 1313, 'atom': 'C212', 'charge': -0.15000000596046448, 'distance': 23.789323806762695, 'force': [0.06752216070890427, 0.05631352216005325, 0.0035945430863648653], 'magnitude': 0.0879964530467987, 'cosine_with_motion': -0.836405336856842, 'motion_component': -0.07360070198774338, 'motion_component_percent': 83.6405336856842}, {'resid': 1313, 'atom': 'C213', 'charge': -0.18000000715255737, 'distance': 24.154407501220703, 'force': [0.07778673619031906, 0.06578534841537476, 0.010628370568156242], 'magnitude': 0.10242778062820435, 'cosine_with_motion': -0.8009285926818848, 'motion_component': -0.08203733712434769, 'motion_component_percent': 80.09285926818848}, {'resid': 1313, 'atom': 'C214', 'charge': -0.15000000596046448, 'distance': 25.586666107177734, 'force': [0.05677993223071098, 0.04998605325818062, 0.007985822856426239], 'magnitude': 0.07606799155473709, 'cosine_with_motion': -0.8013020753860474, 'motion_component': -0.06095343828201294, 'motion_component_percent': 80.13020753860474}, {'resid': 1313, 'atom': 'C215', 'charge': -0.15000000596046448, 'distance': 26.1981143951416, 'force': [0.05269364267587662, 0.04880866780877113, 0.010288535617291927], 'magnitude': 0.07255866378545761, 'cosine_with_motion': -0.7795439958572388, 'motion_component': -0.056562669575214386, 'motion_component_percent': 77.95439958572388}, {'resid': 1313, 'atom': 'C216', 'charge': -0.18000000715255737, 'distance': 25.769372940063477, 'force': [0.06317097693681717, 0.061714403331279755, 0.017299804836511612], 'magnitude': 0.08999179303646088, 'cosine_with_motion': -0.7468864917755127, 'motion_component': -0.06721365451812744, 'motion_component_percent': 74.68864917755127}, {'resid': 1313, 'atom': 'C217', 'charge': -0.18000000715255737, 'distance': 26.571901321411133, 'force': [0.05985615774989128, 0.05637393891811371, 0.020070085301995277], 'magnitude': 0.08463798463344574, 'cosine_with_motion': -0.7153543829917908, 'motion_component': -0.0605461522936821, 'motion_component_percent': 71.53543829917908}, {'resid': 1313, 'atom': 'C218', 'charge': -0.18000000715255737, 'distance': 26.61672019958496, 'force': [0.0627153292298317, 0.052537791430950165, 0.020543336868286133], 'magnitude': 0.08435319364070892, 'cosine_with_motion': -0.7082753777503967, 'motion_component': -0.059745289385318756, 'motion_component_percent': 70.82753777503967}, {'resid': 1313, 'atom': 'C219', 'charge': -0.18000000715255737, 'distance': 27.619352340698242, 'force': [0.05839952826499939, 0.047180138528347015, 0.02237604185938835], 'magnitude': 0.07834001630544662, 'cosine_with_motion': -0.6756467819213867, 'motion_component': -0.05293017998337746, 'motion_component_percent': 67.56467819213867}, {'resid': 1313, 'atom': 'C22', 'charge': -0.08000000566244125, 'distance': 20.58021354675293, 'force': [0.052282143384218216, 0.03404370695352554, -0.006324160844087601], 'magnitude': 0.062708780169487, 'cosine_with_motion': -0.8907060623168945, 'motion_component': -0.05585509166121483, 'motion_component_percent': 89.07060623168945}, {'resid': 1313, 'atom': 'C220', 'charge': -0.27000001072883606, 'distance': 27.52238655090332, 'force': [0.09184415638446808, 0.06585609912872314, 0.03509784862399101], 'magnitude': 0.11833948642015457, 'cosine_with_motion': -0.6612728238105774, 'motion_component': -0.07825468480587006, 'motion_component_percent': 66.12728238105774}, {'resid': 1313, 'atom': 'C23', 'charge': -0.18000000715255737, 'distance': 19.492555618286133, 'force': [0.12675201892852783, 0.09121134877204895, -0.01874465122818947], 'magnitude': 0.157279834151268, 'cosine_with_motion': -0.9053096175193787, 'motion_component': -0.14238694310188293, 'motion_component_percent': 90.53096175193787}, {'resid': 1313, 'atom': 'C24', 'charge': -0.18000000715255737, 'distance': 18.188016891479492, 'force': [0.14812391996383667, 0.10247202217578888, -0.013910388574004173], 'magnitude': 0.18065080046653748, 'cosine_with_motion': -0.8848037719726562, 'motion_component': -0.15984050929546356, 'motion_component_percent': 88.48037719726562}, {'resid': 1313, 'atom': 'C25', 'charge': -0.15000000596046448, 'distance': 17.297468185424805, 'force': [0.1298229843378067, 0.10313988476991653, -0.014535147696733475], 'magnitude': 0.16644251346588135, 'cosine_with_motion': -0.8971748352050781, 'motion_component': -0.14932803809642792, 'motion_component_percent': 89.71748352050781}, {'resid': 1313, 'atom': 'C26', 'charge': -0.15000000596046448, 'distance': 17.22696304321289, 'force': [0.12450339645147324, 0.11223719269037247, -0.007819503545761108], 'magnitude': 0.1678077131509781, 'cosine_with_motion': -0.8827646970748901, 'motion_component': -0.1481347233057022, 'motion_component_percent': 88.27646970748901}, {'resid': 1313, 'atom': 'C27', 'charge': -0.18000000715255737, 'distance': 18.05255126953125, 'force': [0.13444188237190247, 0.12462921440601349, 0.004277137108147144], 'magnitude': 0.18337218463420868, 'cosine_with_motion': -0.848311185836792, 'motion_component': -0.15555667877197266, 'motion_component_percent': 84.8311185836792}, {'resid': 1313, 'atom': 'C28', 'charge': -0.15000000596046448, 'distance': 19.30562400817871, 'force': [0.09466619044542313, 0.09429634362459183, -0.00010898772598011419], 'magnitude': 0.13361698389053345, 'cosine_with_motion': -0.861184298992157, 'motion_component': -0.11506884545087814, 'motion_component_percent': 86.1184298992157}, {'resid': 1313, 'atom': 'C29', 'charge': -0.15000000596046448, 'distance': 20.594215393066406, 'force': [0.08454720675945282, 0.08147064596414566, 0.0012468245113268495], 'magnitude': 0.11741912364959717, 'cosine_with_motion': -0.855291485786438, 'motion_component': -0.10042757540941238, 'motion_component_percent': 85.5291485786438}, {'resid': 1313, 'atom': 'C3', 'charge': 0.06000000238418579, 'distance': 26.20241928100586, 'force': [-0.020355889573693275, -0.017082469537854195, 0.01164624560624361], 'magnitude': 0.029013928025960922, 'cosine_with_motion': 0.9902553558349609, 'motion_component': 0.028731197118759155, 'motion_component_percent': 99.0255355834961}, {'resid': 1313, 'atom': 'C31', 'charge': 0.6299999952316284, 'distance': 26.266273498535156, 'force': [-0.24270972609519958, -0.17969416081905365, 0.026685724034905434], 'magnitude': 0.30316683650016785, 'cosine_with_motion': 0.8939067721366882, 'motion_component': 0.2710028886795044, 'motion_component_percent': 89.39067721366882}, {'resid': 1313, 'atom': 'C310', 'charge': -0.18000000715255737, 'distance': 19.322675704956055, 'force': [0.1393395960330963, 0.07528627663850784, 0.023127006366848946], 'magnitude': 0.16005751490592957, 'cosine_with_motion': -0.7446819543838501, 'motion_component': -0.11919194459915161, 'motion_component_percent': 74.46819543838501}, {'resid': 1313, 'atom': 'C311', 'charge': -0.18000000715255737, 'distance': 18.433778762817383, 'force': [0.1465766727924347, 0.09336243569850922, 0.02697371132671833], 'magnitude': 0.1758659929037094, 'cosine_with_motion': -0.7538970708847046, 'motion_component': -0.1325848549604416, 'motion_component_percent': 75.38970708847046}, {'resid': 1313, 'atom': 'C312', 'charge': -0.18000000715255737, 'distance': 17.00487518310547, 'force': [0.1731550246477127, 0.10680568218231201, 0.03632725402712822], 'magnitude': 0.20666345953941345, 'cosine_with_motion': -0.7367108464241028, 'motion_component': -0.1522512137889862, 'motion_component_percent': 73.67108464241028}, {'resid': 1313, 'atom': 'C313', 'charge': -0.18000000715255737, 'distance': 16.26487159729004, 'force': [0.19736237823963165, 0.10635344684123993, 0.027680469676852226], 'magnitude': 0.22589637339115143, 'cosine_with_motion': -0.7580385804176331, 'motion_component': -0.17123816907405853, 'motion_component_percent': 75.8038580417633}, {'resid': 1313, 'atom': 'C314', 'charge': -0.18000000715255737, 'distance': 14.666632652282715, 'force': [0.24252964556217194, 0.13040943443775177, 0.03676721453666687], 'magnitude': 0.2778112292289734, 'cosine_with_motion': -0.7517877221107483, 'motion_component': -0.20885507762432098, 'motion_component_percent': 75.17877221107483}, {'resid': 1313, 'atom': 'C315', 'charge': -0.18000000715255737, 'distance': 14.085083961486816, 'force': [0.25338372588157654, 0.16165512800216675, 0.020027637481689453], 'magnitude': 0.301225483417511, 'cosine_with_motion': -0.8063505291938782, 'motion_component': -0.24289332330226898, 'motion_component_percent': 80.63505291938782}, {'resid': 1313, 'atom': 'C316', 'charge': -0.18000000715255737, 'distance': 14.157875061035156, 'force': [0.2561195492744446, 0.1522083431482315, -0.010976579040288925], 'magnitude': 0.29813602566719055, 'cosine_with_motion': -0.8541463017463684, 'motion_component': -0.2546517848968506, 'motion_component_percent': 85.41463017463684}, {'resid': 1313, 'atom': 'C317', 'charge': -0.18000000715255737, 'distance': 13.096346855163574, 'force': [0.3117147982120514, 0.15388159453868866, -0.023555662482976913], 'magnitude': 0.3484257757663727, 'cosine_with_motion': -0.8500787019729614, 'motion_component': -0.2961893379688263, 'motion_component_percent': 85.00787019729614}, {'resid': 1313, 'atom': 'C318', 'charge': -0.27000001072883606, 'distance': 13.12755298614502, 'force': [0.4633353650569916, 0.21720105409622192, -0.09331206977367401], 'magnitude': 0.5201568007469177, 'cosine_with_motion': -0.8900628685951233, 'motion_component': -0.4629722535610199, 'motion_component_percent': 89.00628685951233}, {'resid': 1313, 'atom': 'C32', 'charge': -0.08000000566244125, 'distance': 26.570009231567383, 'force': [0.030981440097093582, 0.02128210850059986, -0.0016295196255668998], 'magnitude': 0.03762224316596985, 'cosine_with_motion': -0.8688900470733643, 'motion_component': -0.032689593732357025, 'motion_component_percent': 86.88900470733643}, {'resid': 1313, 'atom': 'C33', 'charge': -0.18000000715255737, 'distance': 25.95230484008789, 'force': [0.07560627907514572, 0.04624802991747856, -0.004170975647866726], 'magnitude': 0.08872760087251663, 'cosine_with_motion': -0.8615246415138245, 'motion_component': -0.07644101232290268, 'motion_component_percent': 86.15246415138245}, {'resid': 1313, 'atom': 'C34', 'charge': -0.18000000715255737, 'distance': 24.510116577148438, 'force': [0.0849907398223877, 0.05163923278450966, -0.002347142668440938], 'magnitude': 0.09947635978460312, 'cosine_with_motion': -0.8497150540351868, 'motion_component': -0.08452656120061874, 'motion_component_percent': 84.97150540351868}, {'resid': 1313, 'atom': 'C35', 'charge': -0.18000000715255737, 'distance': 24.74884605407715, 'force': [0.08310867846012115, 0.050951868295669556, 0.0040092458948493], 'magnitude': 0.09756648540496826, 'cosine_with_motion': -0.8170976042747498, 'motion_component': -0.07972133904695511, 'motion_component_percent': 81.70976042747498}, {'resid': 1313, 'atom': 'C36', 'charge': -0.18000000715255737, 'distance': 23.530977249145508, 'force': [0.09245240688323975, 0.055049698799848557, 0.008387674577534199], 'magnitude': 0.10792715102434158, 'cosine_with_motion': -0.7940650582313538, 'motion_component': -0.08570118248462677, 'motion_component_percent': 79.40650582313538}, {'resid': 1313, 'atom': 'C37', 'charge': -0.18000000715255737, 'distance': 22.913257598876953, 'force': [0.10085988789796829, 0.05208780989050865, 0.008380352519452572], 'magnitude': 0.11382480710744858, 'cosine_with_motion': -0.7825900912284851, 'motion_component': -0.08907816559076309, 'motion_component_percent': 78.25900912284851}, {'resid': 1313, 'atom': 'C38', 'charge': -0.18000000715255737, 'distance': 21.666305541992188, 'force': [0.11287448555231094, 0.056986987590789795, 0.014766681008040905], 'magnitude': 0.12730365991592407, 'cosine_with_motion': -0.7553520798683167, 'motion_component': -0.09615908563137054, 'motion_component_percent': 75.53520798683167}, {'resid': 1313, 'atom': 'C39', 'charge': -0.18000000715255737, 'distance': 20.47477149963379, 'force': [0.12379162758588791, 0.0693221166729927, 0.013822847045958042], 'magnitude': 0.1425517201423645, 'cosine_with_motion': -0.7771533727645874, 'motion_component': -0.11078455299139023, 'motion_component_percent': 77.71533727645874}, {'resid': 1313, 'atom': 'C4', 'charge': 0.08000000566244125, 'distance': 25.74843406677246, 'force': [-0.02659017965197563, -0.024199580773711205, 0.017670897766947746], 'magnitude': 0.04006142541766167, 'cosine_with_motion': 0.9964510798454285, 'motion_component': 0.03991924971342087, 'motion_component_percent': 99.64510798454285}, {'resid': 1313, 'atom': 'C5', 'charge': 0.08000000566244125, 'distance': 24.24977684020996, 'force': [-0.029676193371415138, -0.027541300281882286, 0.0200194139033556], 'magnitude': 0.045166101306676865, 'cosine_with_motion': 0.9968859553337097, 'motion_component': 0.045025452971458435, 'motion_component_percent': 99.68859553337097}, {'resid': 1313, 'atom': 'C6', 'charge': 0.06000000238418579, 'distance': 23.91864013671875, 'force': [-0.022895056754350662, -0.022393211722373962, 0.013664687052369118], 'magnitude': 0.03481900691986084, 'cosine_with_motion': 0.9914698004722595, 'motion_component': 0.03452199324965477, 'motion_component_percent': 99.14698004722595}, {'resid': 1313, 'atom': 'H1', 'charge': 0.12000000476837158, 'distance': 23.774044036865234, 'force': [-0.05078874155879021, -0.042554713785648346, 0.024043988436460495], 'magnitude': 0.07048767805099487, 'cosine_with_motion': 0.9802185893058777, 'motion_component': 0.06909333169460297, 'motion_component_percent': 98.02185893058777}, {'resid': 1313, 'atom': 'H10R', 'charge': 0.09000000357627869, 'distance': 21.306676864624023, 'force': [-0.049188487231731415, -0.04330160468816757, -0.006128846202045679], 'magnitude': 0.0658186823129654, 'cosine_with_motion': 0.8083556294441223, 'motion_component': 0.05320490151643753, 'motion_component_percent': 80.83556294441223}, {'resid': 1313, 'atom': 'H10S', 'charge': 0.09000000357627869, 'distance': 20.61307144165039, 'force': [-0.055396582931280136, -0.04324354976415634, -0.002547292737290263], 'magnitude': 0.07032264769077301, 'cosine_with_motion': 0.8361943960189819, 'motion_component': 0.05880340561270714, 'motion_component_percent': 83.6194396018982}, {'resid': 1313, 'atom': 'H10X', 'charge': 0.09000000357627869, 'distance': 19.762853622436523, 'force': [-0.06668905168771744, -0.034490738064050674, -0.014688302762806416], 'magnitude': 0.07650350779294968, 'cosine_with_motion': 0.7094253301620483, 'motion_component': 0.05427352711558342, 'motion_component_percent': 70.94253301620483}, {'resid': 1313, 'atom': 'H10Y', 'charge': 0.09000000357627869, 'distance': 18.800273895263672, 'force': [-0.0755700096487999, -0.036439448595047, -0.010393436066806316], 'magnitude': 0.0845380574464798, 'cosine_with_motion': 0.7462528944015503, 'motion_component': 0.06308677047491074, 'motion_component_percent': 74.62528944015503}, {'resid': 1313, 'atom': 'H111', 'charge': 0.15000000596046448, 'distance': 22.546724319458008, 'force': [-0.07622834295034409, -0.061466459184885025, 0.0028073801659047604], 'magnitude': 0.09796309471130371, 'cosine_with_motion': 0.8708661198616028, 'motion_component': 0.08531273901462555, 'motion_component_percent': 87.08661198616028}, {'resid': 1313, 'atom': 'H11A', 'charge': 0.09000000357627869, 'distance': 24.71796417236328, 'force': [-0.037773728370666504, -0.02870824746787548, 0.011861803010106087], 'magnitude': 0.04890521988272667, 'cosine_with_motion': 0.9518039226531982, 'motion_component': 0.046548180282115936, 'motion_component_percent': 95.18039226531982}, {'resid': 1313, 'atom': 'H11B', 'charge': 0.09000000357627869, 'distance': 23.015155792236328, 'force': [-0.04427701607346535, -0.032213062047958374, 0.013561105355620384], 'magnitude': 0.0564095638692379, 'cosine_with_motion': 0.9487748742103577, 'motion_component': 0.053519975394010544, 'motion_component_percent': 94.87748742103577}, {'resid': 1313, 'atom': 'H11X', 'charge': 0.09000000357627869, 'distance': 18.475353240966797, 'force': [-0.07202382385730743, -0.04894164577126503, -0.008951677940785885], 'magnitude': 0.08753769844770432, 'cosine_with_motion': 0.7903862595558167, 'motion_component': 0.06918859481811523, 'motion_component_percent': 79.03862595558167}, {'resid': 1313, 'atom': 'H11Y', 'charge': 0.09000000357627869, 'distance': 19.080646514892578, 'force': [-0.06652367860078812, -0.04555646702647209, -0.015329870395362377], 'magnitude': 0.08207190036773682, 'cosine_with_motion': 0.7374430894851685, 'motion_component': 0.06052335351705551, 'motion_component_percent': 73.74430894851685}, {'resid': 1313, 'atom': 'H12', 'charge': 0.09000000357627869, 'distance': 24.51384162902832, 'force': [-0.04043230041861534, -0.027905790135264397, 0.00767327519133687], 'magnitude': 0.0497230663895607, 'cosine_with_motion': 0.9163552522659302, 'motion_component': 0.045563992112874985, 'motion_component_percent': 91.63552522659302}, {'resid': 1313, 'atom': 'H121', 'charge': 0.15000000596046448, 'distance': 24.605091094970703, 'force': [-0.06423531472682953, -0.0513584241271019, -0.0015982392942532897], 'magnitude': 0.08225823938846588, 'cosine_with_motion': 0.8462245464324951, 'motion_component': 0.06960894167423248, 'motion_component_percent': 84.62245464324951}, {'resid': 1313, 'atom': 'H12X', 'charge': 0.09000000357627869, 'distance': 16.598892211914062, 'force': [-0.08714701980352402, -0.0614018552005291, -0.019905343651771545], 'magnitude': 0.10844820737838745, 'cosine_with_motion': 0.7415143847465515, 'motion_component': 0.08041590452194214, 'motion_component_percent': 74.15143847465515}, {'resid': 1313, 'atom': 'H12Y', 'charge': 0.09000000357627869, 'distance': 17.034683227539062, 'force': [-0.0867101177573204, -0.05011069402098656, -0.023941220715641975], 'magnitude': 0.1029704213142395, 'cosine_with_motion': 0.6922346353530884, 'motion_component': 0.07127968966960907, 'motion_component_percent': 69.22346353530884}, {'resid': 1313, 'atom': 'H13A', 'charge': 0.09000000357627869, 'distance': 25.331663131713867, 'force': [-0.03501211106777191, -0.029856355860829353, 0.0071404180489480495], 'magnitude': 0.046564314514398575, 'cosine_with_motion': 0.926522433757782, 'motion_component': 0.043142881244421005, 'motion_component_percent': 92.6522433757782}, {'resid': 1313, 'atom': 'H13B', 'charge': 0.09000000357627869, 'distance': 23.783679962158203, 'force': [-0.039392802864313126, -0.03463214263319969, 0.006251708138734102], 'magnitude': 0.05282292887568474, 'cosine_with_motion': 0.913648247718811, 'motion_component': 0.048261575400829315, 'motion_component_percent': 91.3648247718811}, {'resid': 1313, 'atom': 'H13R', 'charge': 0.09000000357627869, 'distance': 24.121492385864258, 'force': [-0.04022905230522156, -0.03128226473927498, -0.006344446446746588], 'magnitude': 0.05135376378893852, 'cosine_with_motion': 0.7855768799781799, 'motion_component': 0.04034233093261719, 'motion_component_percent': 78.557687997818}, {'resid': 1313, 'atom': 'H13S', 'charge': 0.09000000357627869, 'distance': 23.467975616455078, 'force': [-0.040011800825595856, -0.0360405370593071, -0.0066029829904437065], 'magnitude': 0.05425369739532471, 'cosine_with_motion': 0.7916305065155029, 'motion_component': 0.0429488830268383, 'motion_component_percent': 79.1630506515503}, {'resid': 1313, 'atom': 'H13X', 'charge': 0.09000000357627869, 'distance': 16.61972999572754, 'force': [-0.09736301004886627, -0.04485733434557915, -0.014505371451377869], 'magnitude': 0.10817644000053406, 'cosine_with_motion': 0.7344565987586975, 'motion_component': 0.07945089787244797, 'motion_component_percent': 73.44565987586975}, {'resid': 1313, 'atom': 'H13Y', 'charge': 0.09000000357627869, 'distance': 16.57933235168457, 'force': [-0.09481576085090637, -0.05276026576757431, -0.0065528107807040215], 'magnitude': 0.10870425403118134, 'cosine_with_motion': 0.7976148128509521, 'motion_component': 0.08670412003993988, 'motion_component_percent': 79.76148128509521}, {'resid': 1313, 'atom': 'H141', 'charge': 0.15000000596046448, 'distance': 26.236358642578125, 'force': [-0.054575365036726, -0.0472027026116848, -0.005250126589089632], 'magnitude': 0.07234728336334229, 'cosine_with_motion': 0.8198362588882446, 'motion_component': 0.05931292474269867, 'motion_component_percent': 81.98362588882446}, {'resid': 1313, 'atom': 'H14X', 'charge': 0.09000000357627869, 'distance': 14.192992210388184, 'force': [-0.13414235413074493, -0.06087357550859451, -0.017389636486768723], 'magnitude': 0.14833125472068787, 'cosine_with_motion': 0.7430949211120605, 'motion_component': 0.11022420227527618, 'motion_component_percent': 74.30949211120605}, {'resid': 1313, 'atom': 'H14Y', 'charge': 0.09000000357627869, 'distance': 14.462865829467773, 'force': [-0.12248189002275467, -0.06744933873414993, -0.02922515757381916], 'magnitude': 0.1428472399711609, 'cosine_with_motion': 0.7071275115013123, 'motion_component': 0.10101120918989182, 'motion_component_percent': 70.71275115013123}, {'resid': 1313, 'atom': 'H151', 'charge': 0.15000000596046448, 'distance': 27.26563262939453, 'force': [-0.04839329421520233, -0.04540039971470833, -0.00918202567845583], 'magnitude': 0.06698818504810333, 'cosine_with_motion': 0.7826664447784424, 'motion_component': 0.052429404109716415, 'motion_component_percent': 78.26664447784424}, {'resid': 1313, 'atom': 'H15X', 'charge': 0.09000000357627869, 'distance': 14.754046440124512, 'force': [-0.11078603565692902, -0.08045346289873123, -0.009759209118783474], 'magnitude': 0.13726451992988586, 'cosine_with_motion': 0.8129352331161499, 'motion_component': 0.11158716678619385, 'motion_component_percent': 81.29352331161499}, {'resid': 1313, 'atom': 'H15Y', 'charge': 0.09000000357627869, 'distance': 13.072661399841309, 'force': [-0.1446349322795868, -0.09705405682325363, -0.01522914506494999], 'magnitude': 0.17484472692012787, 'cosine_with_motion': 0.798413097858429, 'motion_component': 0.1395983248949051, 'motion_component_percent': 79.8413097858429}, {'resid': 1313, 'atom': 'H16R', 'charge': 0.09000000357627869, 'distance': 24.734949111938477, 'force': [-0.0345904640853405, -0.033044904470443726, -0.009833206422626972], 'magnitude': 0.04883807897567749, 'cosine_with_motion': 0.7405964136123657, 'motion_component': 0.03616930544376373, 'motion_component_percent': 74.05964136123657}, {'resid': 1313, 'atom': 'H16S', 'charge': 0.09000000357627869, 'distance': 25.825212478637695, 'force': [-0.03012959286570549, -0.03207585960626602, -0.00839781854301691], 'magnitude': 0.04480152577161789, 'cosine_with_motion': 0.7494587898254395, 'motion_component': 0.03357689827680588, 'motion_component_percent': 74.94587898254395}, {'resid': 1313, 'atom': 'H16X', 'charge': 0.09000000357627869, 'distance': 15.17619514465332, 'force': [-0.11312244087457657, -0.0632452443242073, 0.005860097706317902], 'magnitude': 0.12973429262638092, 'cosine_with_motion': 0.8524057865142822, 'motion_component': 0.1105862632393837, 'motion_component_percent': 85.24057865142822}, {'resid': 1313, 'atom': 'H16Y', 'charge': 0.09000000357627869, 'distance': 14.053987503051758, 'force': [-0.12466272711753845, -0.0847373902797699, 0.012822404503822327], 'magnitude': 0.1512799859046936, 'cosine_with_motion': 0.8869873881340027, 'motion_component': 0.13418343663215637, 'motion_component_percent': 88.69873881340027}, {'resid': 1313, 'atom': 'H17R', 'charge': 0.09000000357627869, 'distance': 26.280323028564453, 'force': [-0.029784703627228737, -0.02909005433320999, -0.011762215755879879], 'magnitude': 0.043263256549835205, 'cosine_with_motion': 0.6899847984313965, 'motion_component': 0.02985098958015442, 'motion_component_percent': 68.99847984313965}, {'resid': 1313, 'atom': 'H17S', 'charge': 0.09000000357627869, 'distance': 27.56843376159668, 'force': [-0.027466941624879837, -0.026652589440345764, -0.008992358110845089], 'magnitude': 0.03931482881307602, 'cosine_with_motion': 0.721537172794342, 'motion_component': 0.02836710959672928, 'motion_component_percent': 72.1537172794342}, {'resid': 1313, 'atom': 'H17X', 'charge': 0.09000000357627869, 'distance': 13.31406307220459, 'force': [-0.15610508620738983, -0.0633755624294281, 0.005277855321764946], 'magnitude': 0.1685619056224823, 'cosine_with_motion': 0.8112877011299133, 'motion_component': 0.1367522031068802, 'motion_component_percent': 81.12877011299133}, {'resid': 1313, 'atom': 'H17Y', 'charge': 0.09000000357627869, 'distance': 12.066847801208496, 'force': [-0.18239451944828033, -0.09363522380590439, 0.00864578876644373], 'magnitude': 0.20520737767219543, 'cosine_with_motion': 0.8423880338668823, 'motion_component': 0.17286424338817596, 'motion_component_percent': 84.23880338668823}, {'resid': 1313, 'atom': 'H18R', 'charge': 0.09000000357627869, 'distance': 26.981342315673828, 'force': [-0.031199706718325615, -0.025242440402507782, -0.008604487404227257], 'magnitude': 0.041044361889362335, 'cosine_with_motion': 0.7310329675674438, 'motion_component': 0.03000478260219097, 'motion_component_percent': 73.10329675674438}, {'resid': 1313, 'atom': 'H18S', 'charge': 0.09000000357627869, 'distance': 25.62979507446289, 'force': [-0.03431210666894913, -0.02767636999487877, -0.011215786449611187], 'magnitude': 0.04548731446266174, 'cosine_with_motion': 0.704701840877533, 'motion_component': 0.03205499425530434, 'motion_component_percent': 70.4701840877533}, {'resid': 1313, 'atom': 'H18X', 'charge': 0.09000000357627869, 'distance': 12.279669761657715, 'force': [-0.18007756769657135, -0.07302985340356827, 0.03878796473145485], 'magnitude': 0.1981559842824936, 'cosine_with_motion': 0.8798550963401794, 'motion_component': 0.17434854805469513, 'motion_component_percent': 87.98550963401794}, {'resid': 1313, 'atom': 'H18Y', 'charge': 0.09000000357627869, 'distance': 14.027799606323242, 'force': [-0.1373099684715271, -0.057386614382267, 0.030162248760461807], 'magnitude': 0.15184535086154938, 'cosine_with_motion': 0.8842315673828125, 'motion_component': 0.1342664510011673, 'motion_component_percent': 88.42315673828125}, {'resid': 1313, 'atom': 'H18Z', 'charge': 0.09000000357627869, 'distance': 13.16140079498291, 'force': [-0.14678184688091278, -0.08182022720575333, 0.03892360255122185], 'magnitude': 0.17249494791030884, 'cosine_with_motion': 0.9234168529510498, 'motion_component': 0.15928474068641663, 'motion_component_percent': 92.34168529510498}, {'resid': 1313, 'atom': 'H19R', 'charge': 0.09000000357627869, 'distance': 27.39101219177246, 'force': [-0.028836848214268684, -0.024407004937529564, -0.01260270457714796], 'magnitude': 0.039825793355703354, 'cosine_with_motion': 0.6532274484634399, 'motion_component': 0.026015300303697586, 'motion_component_percent': 65.322744846344}, {'resid': 1313, 'atom': 'H19S', 'charge': 0.09000000357627869, 'distance': 28.64765739440918, 'force': [-0.026960480958223343, -0.02228177897632122, -0.010110937990248203], 'magnitude': 0.03640846535563469, 'cosine_with_motion': 0.682512998</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>1199</v>
-      </c>
-      <c r="B15" t="n">
-        <v>1219</v>
-      </c>
-      <c r="C15" t="n">
-        <v>2515</v>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>{1199: {'frame': 1199, 'motion_vector': [-3.884815216064453, 1.590545654296875, 1.432769775390625], 'ionic_force': [14.11787834763527, -5.172281384468079, -12.066099643707275], 'ionic_force_magnitude': 19.27842691639068, 'radial_force': 15.035524059996838, 'axial_force': -12.066099643707275, 'glu_force': [0.0, 0.0, 0.0], 'glu_force_magnitude': 0.0, 'asn_force': [0.0, 0.0, 0.0], 'asn_force_magnitude': 0.0, 'residue_force': [0.0, 0.0, 0.0], 'residue_force_magnitude': 0.0, 'pip2_force': [0.7719871196895838, -0.11984185688197613, -4.625281474491203], 'pip2_force_magnitude': 4.690794698331942, 'total_force': [14.889865467324853, -5.292123241350055, -16.69138111819848], 'total_force_magnitude': 22.985144456139995, 'cosine_total_motion': -0.8844952873793044, 'cosine_glu_motion': 0, 'cosine_asn_motion': 0, 'cosine_residue_motion': 0, 'cosine_pip2_motion': -0.4718061154839001, 'cosine_ionic_motion': -0.9397606145256897, 'motion_component_total': -20.33025195118837, 'motion_component_glu': 0, 'motion_component_asn': 0, 'motion_component_residue': 0, 'motion_component_ionic': -18.117106326035902, 'motion_component_pip2': -2.2131456251524666, 'motion_component_percent_total': 88.44952873793044, 'motion_component_percent_glu': 0, 'motion_component_percent_asn': 0, 'motion_component_percent_residue': 0, 'motion_component_percent_ionic': 93.97606145256897, 'motion_component_percent_pip2': 47.18061154839001, 'ionic_contributions': [{'ion_id': 2230, 'distance': 7.779934883117676, 'force': [-4.786203861236572, 2.3370611667633057, -1.3103206157684326], 'magnitude': 5.4851202964782715, 'cosine_ionic_motion': 0.8398500084877014, 'motion_component_ionic': 4.606678485870361, 'motion_component_percent_ionic': 83.98500084877014}, {'ion_id': 2280, 'distance': 8.599261283874512, 'force': [0.6796392798423767, 1.932413935661316, -3.995137929916382], 'magnitude': 4.489683628082275, 'cosine_ionic_motion': -0.2656768560409546, 'motion_component_ionic': -1.1928050518035889, 'motion_component_percent_ionic': 26.56768560409546}, {'ion_id': 2333, 'distance': 4.074949264526367, 'force': [12.101813316345215, -14.844310760498047, -5.739468097686768], 'magnitude': 19.993722915649414, 'cosine_ionic_motion': -0.8890808820724487, 'motion_component_ionic': -17.776037216186523, 'motion_component_percent_ionic': 88.90808820724487}, {'ion_id': 2334, 'distance': 10.257603645324707, 'force': [-0.4024566113948822, 3.128925085067749, -0.06349241733551025], 'magnitude': 3.1553406715393066, 'cosine_ionic_motion': 0.4607953727245331, 'motion_component_ionic': 1.4539663791656494, 'motion_component_percent_ionic': 46.07953727245331}, {'ion_id': 2350, 'distance': 13.552000999450684, 'force': [0.13162976503372192, 0.44357430934906006, -1.747503399848938], 'magnitude': 1.8077203035354614, 'cosine_ionic_motion': -0.2880411744117737, 'motion_component_ionic': -0.5206978917121887, 'motion_component_percent_ionic': 28.804117441177368}, {'ion_id': 2372, 'distance': 7.040935039520264, 'force': [6.39345645904541, 1.8300548791885376, 0.7898228168487549], 'magnitude': 6.696954727172852, 'cosine_ionic_motion': -0.7000511884689331, 'motion_component_ionic': -4.688210964202881, 'motion_component_percent_ionic': 70.00511884689331}], 'glu_contributions': [], 'asn_contributions': [], 'pip2_contributions': [{'resid': 1313, 'atom': 'C1', 'charge': 0.06000000238418579, 'distance': 26.0665225982666, 'force': [-0.01957365870475769, -0.013995480723679066, 0.016748113557696342], 'magnitude': 0.02931724488735199, 'cosine_with_motion': 0.5980947017669678, 'motion_component': 0.017534488812088966, 'motion_component_percent': 59.80947017669678}, {'resid': 1313, 'atom': 'C11', 'charge': 0.17000000178813934, 'distance': 25.322599411010742, 'force': [-0.06587626785039902, -0.04122985526919365, 0.04132247343659401], 'magnitude': 0.0880177840590477, 'cosine_with_motion': 0.6391851902008057, 'motion_component': 0.05625966191291809, 'motion_component_percent': 63.918519020080566}, {'resid': 1313, 'atom': 'C12', 'charge': 0.04000000283122063, 'distance': 25.24015235900879, 'force': [-0.01629634201526642, -0.00952364131808281, 0.008846919052302837], 'magnitude': 0.02084558643400669, 'cosine_with_motion': 0.6579544544219971, 'motion_component': 0.013715446926653385, 'motion_component_percent': 65.7954454421997}, {'resid': 1313, 'atom': 'C13', 'charge': -0.05000000074505806, 'distance': 26.079870223999023, 'force': [0.01909954659640789, 0.01190575584769249, -0.009440068155527115], 'magnitude': 0.024406036362051964, 'cosine_with_motion': -0.6354155540466309, 'motion_component': -0.015507974661886692, 'motion_component_percent': 63.541555404663086}, {'resid': 1313, 'atom': 'C2', 'charge': 0.06000000238418579, 'distance': 27.571277618408203, 'force': [-0.01775849051773548, -0.012352199293673038, 0.014789661392569542], 'magnitude': 0.026204481720924377, 'cosine_with_motion': 0.6068183779716492, 'motion_component': 0.015901360660791397, 'motion_component_percent': 60.68183779716492}, {'resid': 1313, 'atom': 'C21', 'charge': 0.6299999952316284, 'distance': 22.81819725036621, 'force': [-0.31783321499824524, -0.17262010276317596, 0.17480769753456116], 'magnitude': 0.4017130434513092, 'cosine_with_motion': 0.6794248819351196, 'motion_component': 0.27293384075164795, 'motion_component_percent': 67.94248819351196}, {'resid': 1313, 'atom': 'C210', 'charge': -0.18000000715255737, 'distance': 22.665035247802734, 'force': [0.09244047850370407, 0.06488973647356033, -0.02787701040506363], 'magnitude': 0.11633162945508957, 'cosine_with_motion': -0.5733445882797241, 'motion_component': -0.0666981115937233, 'motion_component_percent': 57.33445882797241}, {'resid': 1313, 'atom': 'C211', 'charge': -0.15000000596046448, 'distance': 24.07269287109375, 'force': [0.06863471865653992, 0.04683786630630493, -0.02192377857863903], 'magnitude': 0.08593696355819702, 'cosine_with_motion': -0.586459219455719, 'motion_component': -0.05039852485060692, 'motion_component_percent': 58.6459219455719}, {'resid': 1313, 'atom': 'C212', 'charge': -0.15000000596046448, 'distance': 25.074344635009766, 'force': [0.06454970687627792, 0.042374201118946075, -0.017655104398727417], 'magnitude': 0.07920821011066437, 'cosine_with_motion': -0.5939096212387085, 'motion_component': -0.047042518854141235, 'motion_component_percent': 59.39096212387085}, {'resid': 1313, 'atom': 'C213', 'charge': -0.18000000715255737, 'distance': 25.018484115600586, 'force': [0.07883255183696747, 0.051574669778347015, -0.015521443448960781], 'magnitude': 0.09547477215528488, 'cosine_with_motion': -0.5819700956344604, 'motion_component': -0.055563461035490036, 'motion_component_percent': 58.197009563446045}, {'resid': 1313, 'atom': 'C214', 'charge': -0.15000000596046448, 'distance': 26.480010986328125, 'force': [0.0592246949672699, 0.03791127726435661, -0.009964889846742153], 'magnitude': 0.07102203369140625, 'cosine_with_motion': -0.5842553377151489, 'motion_component': -0.041495002806186676, 'motion_component_percent': 58.42553377151489}, {'resid': 1313, 'atom': 'C215', 'charge': -0.15000000596046448, 'distance': 26.941884994506836, 'force': [0.058843906968832016, 0.03444577381014824, -0.007609979715198278], 'magnitude': 0.06860778480768204, 'cosine_with_motion': -0.6069793105125427, 'motion_component': -0.04164350405335426, 'motion_component_percent': 60.69793105125427}, {'resid': 1313, 'atom': 'C216', 'charge': -0.18000000715255737, 'distance': 26.1450138092041, 'force': [0.07687947899103165, 0.0409686453640461, -0.007358555682003498], 'magnitude': 0.08742443472146988, 'cosine_with_motion': -0.6293359994888306, 'motion_component': -0.05501934140920639, 'motion_component_percent': 62.93359994888306}, {'resid': 1313, 'atom': 'C217', 'charge': -0.18000000715255737, 'distance': 26.68497085571289, 'force': [0.0742553174495697, 0.0390210784971714, -0.002539152279496193], 'magnitude': 0.08392225205898285, 'cosine_with_motion': -0.617984414100647, 'motion_component': -0.05186264589428902, 'motion_component_percent': 61.7984414100647}, {'resid': 1313, 'atom': 'C218', 'charge': -0.18000000715255737, 'distance': 25.67491912841797, 'force': [0.08127076923847198, 0.04016231372952461, 0.000637041695881635], 'magnitude': 0.09065514802932739, 'cosine_with_motion': -0.624032735824585, 'motion_component': -0.056571781635284424, 'motion_component_percent': 62.403273582458496}, {'resid': 1313, 'atom': 'C219', 'charge': -0.18000000715255737, 'distance': 25.39031219482422, 'force': [0.08545580506324768, 0.03592049330472946, -0.00032528574229218066], 'magnitude': 0.09269887953996658, 'cosine_with_motion': -0.6695773601531982, 'motion_component': -0.06206906959414482, 'motion_component_percent': 66.95773601531982}, {'resid': 1313, 'atom': 'C22', 'charge': -0.08000000566244125, 'distance': 21.493654251098633, 'force': [0.04605632647871971, 0.02505752630531788, -0.023585326969623566], 'magnitude': 0.05749202147126198, 'cosine_with_motion': -0.6778433918952942, 'motion_component': -0.03897058591246605, 'motion_component_percent': 67.78433918952942}, {'resid': 1313, 'atom': 'C220', 'charge': -0.27000001072883606, 'distance': 24.44317626953125, 'force': [0.13973203301429749, 0.05429749935865402, 0.006051207426935434], 'magnitude': 0.1500329226255417, 'cosine_with_motion': -0.6728940606117249, 'motion_component': -0.1009562611579895, 'motion_component_percent': 67.28940606117249}, {'resid': 1313, 'atom': 'C23', 'charge': -0.18000000715255737, 'distance': 21.138935089111328, 'force': [0.11249882727861404, 0.0509958490729332, -0.05126822367310524], 'magnitude': 0.133734792470932, 'cosine_with_motion': -0.7238483428955078, 'motion_component': -0.0968037098646164, 'motion_component_percent': 72.38483428955078}, {'resid': 1313, 'atom': 'C24', 'charge': -0.18000000715255737, 'distance': 19.86398696899414, 'force': [0.12989076972007751, 0.05857183411717415, -0.05133931338787079], 'magnitude': 0.1514529585838318, 'cosine_with_motion': -0.7219560146331787, 'motion_component': -0.10934237390756607, 'motion_component_percent': 72.19560146331787}, {'resid': 1313, 'atom': 'C25', 'charge': -0.15000000596046448, 'distance': 18.801464080810547, 'force': [0.11715246737003326, 0.060481004416942596, -0.04964090511202812], 'magnitude': 0.14087893068790436, 'cosine_with_motion': -0.688197910785675, 'motion_component': -0.09695258736610413, 'motion_component_percent': 68.8197910785675}, {'resid': 1313, 'atom': 'C26', 'charge': -0.15000000596046448, 'distance': 18.753000259399414, 'force': [0.11380141973495483, 0.06990958750247955, -0.0470607727766037], 'magnitude': 0.14160801470279694, 'cosine_with_motion': -0.6341679096221924, 'motion_component': -0.08980325609445572, 'motion_component_percent': 63.41679096221924}, {'resid': 1313, 'atom': 'C27', 'charge': -0.18000000715255737, 'distance': 19.71270751953125, 'force': [0.1229880079627037, 0.08156406879425049, -0.043261051177978516], 'magnitude': 0.15378643572330475, 'cosine_with_motion': -0.6011102795600891, 'motion_component': -0.09244260936975479, 'motion_component_percent': 60.11102795600891}, {'resid': 1313, 'atom': 'C28', 'charge': -0.15000000596046448, 'distance': 20.788883209228516, 'force': [0.08819501847028732, 0.06492965668439865, -0.035830460488796234], 'magnitude': 0.11523039638996124, 'cosine_with_motion': -0.5687267184257507, 'motion_component': -0.06553460657596588, 'motion_component_percent': 56.87267184257507}, {'resid': 1313, 'atom': 'C29', 'charge': -0.15000000596046448, 'distance': 21.98827362060547, 'force': [0.07889336347579956, 0.05902434512972832, -0.030024083331227303], 'magnitude': 0.10300233960151672, 'cosine_with_motion': -0.5595014691352844, 'motion_component': -0.05762995779514313, 'motion_component_percent': 55.95014691352844}, {'resid': 1313, 'atom': 'C3', 'charge': 0.06000000238418579, 'distance': 28.32106590270996, 'force': [-0.016719989478588104, -0.010827700607478619, 0.014832299202680588], 'magnitude': 0.024835342541337013, 'cosine_with_motion': 0.6262143850326538, 'motion_component': 0.015552248805761337, 'motion_component_percent': 62.62143850326538}, {'resid': 1313, 'atom': 'C31', 'charge': 0.6299999952316284, 'distance': 27.1365966796875, 'force': [-0.2361566424369812, -0.12329070270061493, 0.09850811958312988], 'magnitude': 0.28403240442276, 'cosine_with_motion': 0.6845768094062805, 'motion_component': 0.1944420039653778, 'motion_component_percent': 68.45768094062805}, {'resid': 1313, 'atom': 'C310', 'charge': -0.18000000715255737, 'distance': 20.339704513549805, 'force': [0.13286229968070984, 0.056033045053482056, -0.008606718853116035], 'magnitude': 0.14445126056671143, 'cosine_with_motion': -0.6857119798660278, 'motion_component': -0.09905195981264114, 'motion_component_percent': 68.57119798660278}, {'resid': 1313, 'atom': 'C311', 'charge': -0.18000000715255737, 'distance': 18.827796936035156, 'force': [0.15463179349899292, 0.06578080356121063, -0.013484744355082512], 'magnitude': 0.16858215630054474, 'cosine_with_motion': -0.6892696619033813, 'motion_component': -0.11619856208562851, 'motion_component_percent': 68.92696619033813}, {'resid': 1313, 'atom': 'C312', 'charge': -0.18000000715255737, 'distance': 18.4708251953125, 'force': [0.16271767020225525, 0.05958602577447891, -0.02557193860411644], 'magnitude': 0.1751612424850464, 'cosine_with_motion': -0.7387829422950745, 'motion_component': -0.12940613925457, 'motion_component_percent': 73.87829422950745}, {'resid': 1313, 'atom': 'C313', 'charge': -0.18000000715255737, 'distance': 17.093366622924805, 'force': [0.18851545453071594, 0.06968317180871964, -0.03792605549097061], 'magnitude': 0.20452924072742462, 'cosine_with_motion': -0.7449812889099121, 'motion_component': -0.15237045288085938, 'motion_component_percent': 74.49812889099121}, {'resid': 1313, 'atom': 'C314', 'charge': -0.18000000715255737, 'distance': 16.7066707611084, 'force': [0.20063360035419464, 0.05663676932454109, -0.04878753423690796], 'magnitude': 0.214106947183609, 'cosine_with_motion': -0.7994630336761475, 'motion_component': -0.17117059230804443, 'motion_component_percent': 79.94630336761475}, {'resid': 1313, 'atom': 'C315', 'charge': -0.18000000715255737, 'distance': 15.272680282592773, 'force': [0.23758867383003235, 0.06862706691026688, -0.06693781167268753], 'magnitude': 0.25620055198669434, 'cosine_with_motion': -0.800545334815979, 'motion_component': -0.2051001638174057, 'motion_component_percent': 80.0545334815979}, {'resid': 1313, 'atom': 'C316', 'charge': -0.18000000715255737, 'distance': 15.101518630981445, 'force': [0.2322043627500534, 0.08464948832988739, -0.08706961572170258], 'magnitude': 0.2620410621166229, 'cosine_with_motion': -0.7675969004631042, 'motion_component': -0.20114190876483917, 'motion_component_percent': 76.75969004631042}, {'resid': 1313, 'atom': 'C317', 'charge': -0.18000000715255737, 'distance': 15.857123374938965, 'force': [0.20565354824066162, 0.06906475126743317, -0.09705890715122223], 'magnitude': 0.23766310513019562, 'cosine_with_motion': -0.7855790257453918, 'motion_component': -0.1867031455039978, 'motion_component_percent': 78.55790257453918}, {'resid': 1313, 'atom': 'C318', 'charge': -0.27000001072883606, 'distance': 15.803705215454102, 'force': [0.29163336753845215, 0.122316874563694, -0.16971753537654877], 'magnitude': 0.3589087426662445, 'cosine_with_motion': -0.7421974539756775, 'motion_component': -0.2663811445236206, 'motion_component_percent': 74.21974539756775}, {'resid': 1313, 'atom': 'C32', 'charge': -0.08000000566244125, 'distance': 27.52945899963379, 'force': [0.02996961958706379, 0.01487260777503252, -0.01043154951184988], 'magnitude': 0.03504553809762001, 'cosine_with_motion': -0.6929464936256409, 'motion_component': -0.024284683167934418, 'motion_component_percent': 69.29464936256409}, {'resid': 1313, 'atom': 'C33', 'charge': -0.18000000715255737, 'distance': 26.842418670654297, 'force': [0.07298870384693146, 0.03167038783431053, -0.023426136001944542], 'magnitude': 0.08294063061475754, 'cosine_with_motion': -0.7250490188598633, 'motion_component': -0.06013602390885353, 'motion_component_percent': 72.50490188598633}, {'resid': 1313, 'atom': 'C34', 'charge': -0.18000000715255737, 'distance': 25.25910186767578, 'force': [0.08282198756933212, 0.03486067056655884, -0.026425013318657875], 'magnitude': 0.09366445243358612, 'cosine_with_motion': -0.7321131825447083, 'motion_component': -0.0685729831457138, 'motion_component_percent': 73.21131825447083}, {'resid': 1313, 'atom': 'C35', 'charge': -0.18000000715255737, 'distance': 24.524402618408203, 'force': [0.08667964488267899, 0.04143088683485985, -0.025350095704197884], 'magnitude': 0.09936048835515976, 'cosine_with_motion': -0.6969411969184875, 'motion_component': -0.06924841552972794, 'motion_component_percent': 69.69411969184875}, {'resid': 1313, 'atom': 'C36', 'charge': -0.18000000715255737, 'distance': 23.242610931396484, 'force': [0.09796544164419174, 0.04504323750734329, -0.02471969835460186], 'magnitude': 0.11062180995941162, 'cosine_with_motion': -0.7017953395843506, 'motion_component': -0.07763387262821198, 'motion_component_percent': 70.17953395843506}, {'resid': 1313, 'atom': 'C37', 'charge': -0.18000000715255737, 'distance': 23.580490112304688, 'force': [0.09772250056266785, 0.04090532660484314, -0.018105536699295044], 'magnitude': 0.10747438669204712, 'cosine_with_motion': -0.7142949104309082, 'motion_component': -0.0767684057354927, 'motion_component_percent': 71.42949104309082}, {'resid': 1313, 'atom': 'C38', 'charge': -0.18000000715255737, 'distance': 22.334787368774414, 'force': [0.11059410870075226, 0.04310492426156998, -0.01619555614888668], 'magnitude': 0.11979727447032928, 'cosine_with_motion': -0.7231886386871338, 'motion_component': -0.0866360291838646, 'motion_component_percent': 72.31886386871338}, {'resid': 1313, 'atom': 'C39', 'charge': -0.18000000715255737, 'distance': 21.227962493896484, 'force': [0.12034440785646439, 0.053550757467746735, -0.015374788083136082], 'magnitude': 0.13261540234088898, 'cosine_with_motion': -0.687437117099762, 'motion_component': -0.09116475284099579, 'motion_component_percent': 68.7437117099762}, {'resid': 1313, 'atom': 'C4', 'charge': 0.08000000566244125, 'distance': 28.285057067871094, 'force': [-0.021007701754570007, -0.014702563174068928, 0.021086225286126137], 'magnitude': 0.03319815918803215, 'cosine_with_motion': 0.6005814075469971, 'motion_component': 0.01993819698691368, 'motion_component_percent': 60.05814075469971}, {'resid': 1313, 'atom': 'C5', 'charge': 0.08000000566244125, 'distance': 26.80779266357422, 'force': [-0.02293197624385357, -0.016353460028767586, 0.02392837218940258], 'magnitude': 0.036957789212465286, 'cosine_with_motion': 0.5939100384712219, 'motion_component': 0.02194960229098797, 'motion_component_percent': 59.39100384712219}, {'resid': 1313, 'atom': 'C6', 'charge': 0.06000000238418579, 'distance': 25.934951782226562, 'force': [-0.018583258613944054, -0.014154835604131222, 0.01820380426943302], 'magnitude': 0.029615458101034164, 'cosine_with_motion': 0.576730489730835, 'motion_component': 0.017080137506127357, 'motion_component_percent': 57.673048973083496}, {'resid': 1313, 'atom': 'H1', 'charge': 0.12000000476837158, 'distance': 25.48573112487793, 'force': [-0.04227064922451973, -0.027507003396749496, 0.03491174057126045], 'magnitude': 0.061337366700172424, 'cosine_with_motion': 0.6266205906867981, 'motion_component': 0.038435257971286774, 'motion_component_percent': 62.66205906867981}, {'resid': 1313, 'atom': 'H10R', 'charge': 0.09000000357627869, 'distance': 22.724151611328125, 'force': [-0.04543622210621834, -0.03388259559869766, 0.011649568565189838], 'magnitude': 0.057863570749759674, 'cosine_with_motion': 0.5427849292755127, 'motion_component': 0.03140747547149658, 'motion_component_percent': 54.27849292755127}, {'resid': 1313, 'atom': 'H10S', 'charge': 0.09000000357627869, 'distance': 22.147640228271484, 'force': [-0.049937810748815536, -0.03220001235604286, 0.013417757116258144], 'magnitude': 0.060915201902389526, 'cosine_with_motion': 0.5995974540710449, 'motion_component': 0.03652460128068924, 'motion_component_percent': 59.95974540710449}, {'resid': 1313, 'atom': 'H10X', 'charge': 0.09000000357627869, 'distance': 20.647653579711914, 'force': [-0.06370026618242264, -0.02920316904783249, 0.001295369234867394], 'magnitude': 0.07008728384971619, 'cosine_with_motion': 0.652572751045227, 'motion_component': 0.04573705047369003, 'motion_component_percent': 65.2572751045227}, {'resid': 1313, 'atom': 'H10Y', 'charge': 0.09000000357627869, 'distance': 20.6290340423584, 'force': [-0.06588226556777954, -0.024105869233608246, 0.0029017641209065914], 'magnitude': 0.07021386176347733, 'cosine_with_motion': 0.7120363712310791, 'motion_component': 0.0499948225915432, 'motion_component_percent': 71.20363712310791}, {'resid': 1313, 'atom': 'H111', 'charge': 0.15000000596046448, 'distance': 24.27827262878418, 'force': [-0.06651221215724945, -0.045633282512426376, 0.02513784170150757], 'magnitude': 0.08448775857686996, 'cosine_with_motion': 0.5919167399406433, 'motion_component': 0.05000972002744675, 'motion_component_percent': 59.19167399406433}, {'resid': 1313, 'atom': 'H11A', 'charge': 0.09000000357627869, 'distance': 26.35346221923828, 'force': [-0.03189311921596527, -0.020093660801649094, 0.020738638937473297], 'magnitude': 0.043023452162742615, 'cosine_with_motion': 0.6374778747558594, 'motion_component': 0.027426499873399734, 'motion_component_percent': 63.74778747558594}, {'resid': 1313, 'atom': 'H11B', 'charge': 0.09000000357627869, 'distance': 24.788331985473633, 'force': [-0.03628024086356163, -0.02151978760957718, 0.024193402379751205], 'magnitude': 0.048627953976392746, 'cosine_with_motion': 0.655454695224762, 'motion_component': 0.031873419880867004, 'motion_component_percent': 65.5454695224762}, {'resid': 1313, 'atom': 'H11X', 'charge': 0.09000000357627869, 'distance': 18.5936279296875, 'force': [-0.07718507945537567, -0.03818611428141594, 0.007349222432821989], 'magnitude': 0.08642758429050446, 'cosine_with_motion': 0.6512013673782349, 'motion_component': 0.05628176033496857, 'motion_component_percent': 65.12013673782349}, {'resid': 1313, 'atom': 'H11Y', 'charge': 0.09000000357627869, 'distance': 18.29551887512207, 'force': [-0.0826907679438591, -0.03351127356290817, 0.002799592213705182], 'magnitude': 0.0892670527100563, 'cosine_with_motion': 0.686821460723877, 'motion_component': 0.061310529708862305, 'motion_component_percent': 68.6821460723877}, {'resid': 1313, 'atom': 'H12', 'charge': 0.09000000357627869, 'distance': 25.783161163330078, 'force': [-0.035789959132671356, -0.01902729645371437, 0.019425347447395325], 'magnitude': 0.0449477843940258, 'cosine_with_motion': 0.6851868629455566, 'motion_component': 0.030797630548477173, 'motion_component_percent': 68.51868629455566}, {'resid': 1313, 'atom': 'H121', 'charge': 0.15000000596046448, 'distance': 26.05333709716797, 'force': [-0.05992741510272026, -0.03853536397218704, 0.017506983131170273], 'magnitude': 0.07336732000112534, 'cosine_with_motion': 0.6041231751441956, 'motion_component': 0.044322896748781204, 'motion_component_percent': 60.412317514419556}, {'resid': 1313, 'atom': 'H12X', 'charge': 0.09000000357627869, 'distance': 18.650907516479492, 'force': [-0.08150777220726013, -0.025036131963133812, 0.010395251214504242], 'magnitude': 0.0858975350856781, 'cosine_with_motion': 0.7656452059745789, 'motion_component': 0.06576703488826752, 'motion_component_percent': 76.56452059745789}, {'resid': 1313, 'atom': 'H12Y', 'charge': 0.09000000357627869, 'distance': 19.25406265258789, 'force': [-0.074168361723423, -0.027785474434494972, 0.01494674477726221], 'magnitude': 0.08060014247894287, 'cosine_with_motion': 0.7422231435775757, 'motion_component': 0.05982329323887825, 'motion_component_percent': 74.22231435775757}, {'resid': 1313, 'atom': 'H13A', 'charge': 0.09000000357627869, 'distance': 27.0484619140625, 'force': [-0.03160765394568443, -0.01991266757249832, 0.016505219042301178], 'magnitude': 0.04084091633558273, 'cosine_with_motion': 0.6335293054580688, 'motion_component': 0.02587391622364521, 'motion_component_percent': 63.352930545806885}, {'resid': 1313, 'atom': 'H13B', 'charge': 0.09000000357627869, 'distance': 25.7582950592041, 'force': [-0.034413985908031464, -0.023541105911135674, 0.017017913982272148], 'magnitude': 0.04503460228443146, 'cosine_with_motion': 0.6038974523544312, 'motion_component': 0.027196280658245087, 'motion_component_percent': 60.389745235443115}, {'resid': 1313, 'atom': 'H13R', 'charge': 0.09000000357627869, 'distance': 24.3172664642334, 'force': [-0.04266186058521271, -0.02599903754889965, 0.00757082924246788], 'magnitude': 0.05053020641207695, 'cosine_with_motion': 0.60334312915802, 'motion_component': 0.030487053096294403, 'motion_component_percent': 60.334312915802}, {'resid': 1313, 'atom': 'H13S', 'charge': 0.09000000357627869, 'distance': 24.68607521057129, 'force': [-0.03955570608377457, -0.02809516340494156, 0.0070788925513625145], 'magnitude': 0.04903165251016617, 'cosine_with_motion': 0.5477287769317627, 'motion_component': 0.02685604616999626, 'motion_component_percent': 54.77287769317627}, {'resid': 1313, 'atom': 'H13X', 'charge': 0.09000000357627869, 'distance': 17.23996925354004, 'force': [-0.0900525450706482, -0.03867454081773758, 0.0223977193236351], 'magnitude': 0.10053277015686035, 'cosine_with_motion': 0.718544065952301, 'motion_component': 0.07223722338676453, 'motion_component_percent': 71.8544065952301}, {'resid': 1313, 'atom': 'H13Y', 'charge': 0.09000000357627869, 'distance': 16.386131286621094, 'force': [-0.10291828960180283, -0.039466772228479385, 0.01529845129698515], 'magnitude': 0.11128272116184235, 'cosine_with_motion': 0.7272300720214844, 'motion_component': 0.08092813938856125, 'motion_component_percent': 72.72300720214844}, {'resid': 1313, 'atom': 'H141', 'charge': 0.15000000596046448, 'distance': 27.32771110534668, 'force': [-0.054666917771101, -0.036866992712020874, 0.009956613183021545], 'magnitude': 0.06668419390916824, 'cosine_with_motion': 0.5679751038551331, 'motion_component': 0.037874963134527206, 'motion_component_percent': 56.797510385513306}, {'resid': 1313, 'atom': 'H14X', 'charge': 0.09000000357627869, 'distance': 17.43242073059082, 'force': [-0.09122764319181442, -0.02491467073559761, 0.026919083669781685], 'magnitude': 0.09832527488470078, 'cosine_with_motion': 0.8101782202720642, 'motion_component': 0.07966099679470062, 'motion_component_percent': 81.01782202720642}, {'resid': 1313, 'atom': 'H14Y', 'charge': 0.09000000357627869, 'distance': 16.954147338867188, 'force': [-0.09950988739728928, -0.023063721135258675, 0.0192783884704113], 'magnitude': 0.10395099222660065, 'cosine_with_motion': 0.8187558054924011, 'motion_component': 0.08511047810316086, 'motion_component_percent': 81.87558054924011}, {'resid': 1313, 'atom': 'H151', 'charge': 0.15000000596046448, 'distance': 27.998083114624023, 'force': [-0.05472566559910774, -0.03158661350607872, 0.006582955364137888], 'magnitude': 0.0635291114449501, 'cosine_with_motion': 0.6096439957618713, 'motion_component': 0.03873014077544212, 'motion_component_percent': 60.964399576187134}, {'resid': 1313, 'atom': 'H15X', 'charge': 0.09000000357627869, 'distance': 14.59005355834961, 'force': [-0.1320786327123642, -0.03777007386088371, 0.028839489445090294], 'magnitude': 0.14036759734153748, 'cosine_with_motion': 0.7939866185188293, 'motion_component': 0.11144999414682388, 'motion_component_percent': 79.39866185188293}, {'resid': 1313, 'atom': 'H15Y', 'charge': 0.09000000357627869, 'distance': 15.218921661376953, 'force': [-0.12055674940347672, -0.026241250336170197, 0.03768610209226608], 'magnitude': 0.12900687754154205, 'cosine_with_motion': 0.8398815393447876, 'motion_component': 0.1083504930138588, 'motion_component_percent': 83.98815393447876}, {'resid': 1313, 'atom': 'H16R', 'charge': 0.09000000357627869, 'distance': 26.308937072753906, 'force': [-0.03858834132552147, -0.01881631650030613, 0.004523936193436384], 'magnitude': 0.04316920042037964, 'cosine_with_motion': 0.6604427099227905, 'motion_component': 0.02851078473031521, 'motion_component_percent': 66.04427099227905}, {'resid': 1313, 'atom': 'H16S', 'charge': 0.09000000357627869, 'distance': 25.115123748779297, 'force': [-0.04132220521569252, -0.022792475298047066, 0.0041186134330928326], 'magnitude': 0.04737071320414543, 'cosine_with_motion': 0.6195484399795532, 'motion_component': 0.029348451644182205, 'motion_component_percent': 61.95484399795532}, {'resid': 1313, 'atom': 'H16X', 'charge': 0.09000000357627869, 'distance': 15.388519287109375, 'force': [-0.10967576503753662, -0.04872152954339981, 0.038968831300735474], 'magnitude': 0.12617896497249603, 'cosine_with_motion': 0.7225754261016846, 'motion_component': 0.09117382019758224, 'motion_component_percent': 72.25754261016846}, {'resid': 1313, 'atom': 'H16Y', 'charge': 0.09000000357627869, 'distance': 14.047861099243164, 'force': [-0.13302777707576752, -0.0489371232688427, 0.053238626569509506], 'magnitude': 0.1514119654893875, 'cosine_with_motion': 0.7671669125556946, 'motion_component': 0.11615825444459915, 'motion_component_percent': 76.71669125556946}, {'resid': 1313, 'atom': 'H17R', 'charge': 0.09000000357627869, 'distance': 26.96343231201172, 'force': [-0.03563243895769119, -0.020467299968004227, 0.000734166766051203], 'magnitude': 0.041098907589912415, 'cosine_with_motion': 0.5865299105644226, 'motion_component': 0.0241057388484478, 'motion_component_percent': 58.65299105644226}, {'resid': 1313, 'atom': 'H17S', 'charge': 0.09000000357627869, 'distance': 27.551626205444336, 'force': [-0.03527197986841202, -0.01743670366704464, 0.00113133923150599], 'magnitude': 0.03936281427741051, 'cosine_with_motion': 0.6352458596229553, 'motion_component': 0.02500506490468979, 'motion_component_percent': 63.52458596229553}, {'resid': 1313, 'atom': 'H17X', 'charge': 0.09000000357627869, 'distance': 16.933395385742188, 'force': [-0.09070684015750885, -0.030355094000697136, 0.04134872555732727], 'magnitude': 0.10420595109462738, 'cosine_with_motion': 0.7860877513885498, 'motion_component': 0.08191502094268799, 'motion_component_percent': 78.60877513885498}, {'resid': 1313, 'atom': 'H17Y', 'charge': 0.09000000357627869, 'distance': 15.635092735290527, 'force': [-0.10739358514547348, -0.027498789131641388, 0.051485300064086914], 'magnitude': 0.12223052978515625, 'cosine_with_motion': 0.8249024152755737, 'motion_component': 0.10082826018333435, 'motion_component_percent': 82.49024152755737}, {'resid': 1313, 'atom': 'H18R', 'charge': 0.09000000357627869, 'distance': 24.75850486755371, 'force': [-0.043174538761377335, -0.022623401135206223, -0.0004843505739700049], 'magnitude': 0.04874519258737564, 'cosine_with_motion': 0.6061022877693176, 'motion_component': 0.029544571414589882, 'motion_component_percent': 60.61022877693176}, {'resid': 1313, 'atom': 'H18S', 'charge': 0.09000000357627869, 'distance': 26.18132781982422, 'force': [-0.03904598578810692, -0.019282778725028038, -0.0019403358455747366], 'magnitude': 0.04359104856848717, 'cosine_with_motion': 0.611507773399353, 'motion_component': 0.026656264439225197, 'motion_component_percent': 61.1507773399353}, {'resid': 1313, 'atom': 'H18X', 'charge': 0.09000000357627869, 'distance': 16.533538818359375, 'force': [-0.08705775439739227, -0.034690871834754944, 0.056263361126184464], 'magnitude': 0.10930725187063217, 'cosine_with_motion': 0.7500139474868774, 'motion_component': 0.08198196440935135, 'motion_component_percent': 75.00139474868774}, {'resid': 1313, 'atom': 'H18Y', 'charge': 0.09000000357627869, 'distance': 15.99013614654541, 'force': [-0.09365008771419525, -0.046880099922418594, 0.05185393616557121], 'magnitude': 0.11686280369758606, 'cosine_with_motion': 0.7013394236564636, 'motion_component': 0.08196049183607101, 'motion_component_percent': 70.13394236564636}, {'resid': 1313, 'atom': 'H18Z', 'charge': 0.09000000357627869, 'distance': 14.814123153686523, 'force': [-0.10831943154335022, -0.046922095119953156, 0.06784531474113464], 'magnitude': 0.1361534744501114, 'cosine_with_motion': 0.7341623306274414, 'motion_component': 0.09995875507593155, 'motion_component_percent': 73.41623306274414}, {'resid': 1313, 'atom': 'H19R', 'charge': 0.09000000357627869, 'distance': 26.42913818359375, 'force': [-0.03965533524751663, -0.016041897237300873, 0.00014089880278334022], 'magnitude': 0.042777422815561295, 'cosine_with_motion': 0.6784971952438354, 'motion_component': 0.029024362564086914, 'motion_component_percent': 67.84971952438354}, {'resid': 1313, 'atom': 'H19S', 'charge': 0.09000000357627869, 'distance': 24.983367919921875, 'force': [-0.044214192777872086, -0.018234508112072945, 0.0020749480463564396], 'magnitude': 0.</t>
+          <t>{954: {'frame': 954, 'motion_vector': [1.8922004699707031, 2.834430694580078, 1.6804885864257812], 'motion_vector_magnitude': 3.799797773361206, 'ionic_force': [-13.062879800796509, 10.245393350720406, 1.3206260204315186], 'ionic_force_magnitude': 16.65385741162942, 'radial_force': 16.60141300013476, 'axial_force': 1.3206260204315186, 'glu_force': [-3.4732834491090627, -0.0006817424385030524, 6.173598070532544], 'glu_force_magnitude': 7.0835733580665945, 'asn_force': [-2.803661426437605, -7.464392549270752, -13.667343181071297], 'asn_force_magnitude': 15.823209003008175, 'sf_force': [0.9609858171911573, 0.10090089443628744, 0.21813816277665765], 'sf_force_magnitude': 0.9905851752374324, 'residue_force': [-5.315959058355512, -7.364173397272972, -7.275606947762098], 'residue_force_magnitude': 11.637221618304736, 'pip2_force': [1.0214345674631753, 0.057866769957992004, -4.444173763193416], 'pip2_force_magnitude': 4.560411996314674, 'total_force': [-17.357404291688844, 2.939086723405426, -10.399154690523996], 'total_force_magnitude': 20.44651884283199, 'cosine_total_motion': -0.5404464599741138, 'cosine_glu_motion': 0.14120076197809814, 'cosine_asn_motion': -0.8221241108611756, 'cosine_sf_motion': 0.6564659222406606, 'cosine_residue_motion': -0.9760190738651873, 'cosine_pip2_motion': -0.3099841639897148, 'cosine_ionic_motion': 0.10337287010655362, 'motion_component_total': -11.050248727402561, 'motion_component_glu': 1.0002059556867586, 'motion_component_asn': -13.008641632568645, 'motion_component_sf': 0.6502854106201674, 'motion_component_residue': -11.358150266261724, 'motion_component_ionic': 1.7215570389854333, 'motion_component_pip2': -1.4136555001262703, 'motion_component_percent_total': np.float64(54.04464599741138), 'motion_component_percent_glu': np.float64(14.120076197809814), 'motion_component_percent_asn': np.float64(82.21241108611757), 'motion_component_percent_sf': np.float64(65.64659222406605), 'motion_component_percent_residue': np.float64(97.60190738651873), 'motion_component_percent_ionic': np.float64(10.337287010655363), 'motion_component_percent_pip2': np.float64(30.99841639897148), 'ionic_contributions': [{'ion_id': 2333, 'distance': 4.532892227172852, 'force': [-7.505458831787109, 11.556084632873535, 8.438343048095703], 'magnitude': 16.157989501953125, 'cosine_ionic_motion': 0.5331462621688843, 'motion_component_ionic': 8.614571571350098, 'motion_component_percent_ionic': 53.31462478637695}, {'ion_id': 2343, 'distance': 10.870248794555664, 'force': [-1.048344612121582, 0.12879706919193268, -2.603606939315796], 'magnitude': 2.809694528579712, 'cosine_ionic_motion': -0.5614266991615295, 'motion_component_ionic': -1.5774375200271606, 'motion_component_percent_ionic': 56.142669677734375}, {'ion_id': 2372, 'distance': 11.836684226989746, 'force': [-2.105020046234131, -0.3876538872718811, -1.0167081356048584], 'magnitude': 2.3696160316467285, 'cosine_ionic_motion': -0.754155695438385, 'motion_component_ionic': -1.7870594263076782, 'motion_component_percent_ionic': 75.41557312011719}, {'ion_id': 2397, 'distance': 8.713855743408203, 'force': [-2.4040563106536865, -1.0518344640731812, -3.4974019527435303], 'magnitude': 4.372375011444092, 'cosine_ionic_motion': -0.8070024847984314, 'motion_component_ionic': -3.528517484664917, 'motion_component_percent_ionic': 80.70024871826172}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 11.101517677307129, 'force': [-0.6118342356021009, -0.4679971967421453, 1.1580407717395618], 'magnitude': 1.3908346188618088, 'cosine_with_motion': -0.1018269675318201, 'motion_component': -0.1416244715769728, 'motion_component_percent': 10.182696753182011}, {'resid': 98, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 11.804080963134766, 'force': [0.34368596400988916, 0.2119715353786382, -0.571264325487313], 'magnitude': 0.6995676545143141, 'cosine_with_motion': 0.1095239175835094, 'motion_component': 0.07661939013711472, 'motion_component_percent': 10.95239175835094}, {'resid': 98, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 9.696623802185059, 'force': [0.06684634861638612, 0.050255175412280036, -0.11250132094151778], 'magnitude': 0.14018047008285017, 'cosine_with_motion': 0.1499543850265833, 'motion_component': 0.021020676184011156, 'motion_component_percent': 14.99543850265833}, {'resid': 98, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 9.599329948425293, 'force': [0.17222320584251394, 0.18256469013987808, -0.3090504091098022], 'magnitude': 0.3981241691827799, 'cosine_with_motion': 0.21416840895455075, 'motion_component': 0.08526561988022835, 'motion_component_percent': 21.416840895455074}, {'resid': 98, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 9.811277389526367, 'force': [0.11714330170636836, 0.06839869751122221, -0.1374867635085172], 'magnitude': 0.193141256845729, 'cosine_with_motion': 0.2513770460845025, 'motion_component': 0.04855127862292755, 'motion_component_percent': 25.13770460845025}, {'resid': 98, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 10.883131980895996, 'force': [-0.029827604491624776, -0.017710275292658346, 0.03388514046408642], 'magnitude': 0.0484927065126438, 'cosine_with_motion': -0.2696955103990436, 'motion_component': -0.013078265233558496, 'motion_component_percent': 26.96955103990436}, {'resid': 98, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 9.710206031799316, 'force': [-0.0398440560174094, -0.01545055105679506, 0.04340992459984714], 'magnitude': 0.060915432212547777, 'cosine_with_motion': -0.19975507951458898, 'motion_component': -0.012168167005283037, 'motion_component_percent': 19.975507951458898}, {'resid': 98, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 9.141039848327637, 'force': [0.03453950139261121, 0.024804287439036555, -0.03334208578585103], 'magnitude': 0.05403632589619309, 'cosine_with_motion': 0.3878236030686454, 'motion_component': 0.02095656260565315, 'motion_component_percent': 38.78236030686454}, {'resid': 98, 'resname': 'GLU', 'atom': 'HG2', 'charge': -0.042500000447034836, 'distance': 9.435471534729004, 'force': [-0.09027500143909559, -0.08684462295257402, 0.09709417405915863], 'magnitude': 0.15848925218081397, 'cosine_with_motion': -0.4214486738461445, 'motion_component': -0.06679508515047121, 'motion_component_percent': 42.14486738461445}, {'resid': 98, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 9.665505409240723, 'force': [-0.10739296881386894, -0.0666723673512608, 0.08266283667827057], 'magnitude': 0.1510350915733709, 'cosine_with_motion': -0.4413173701221372, 'motion_component': -0.0666544094093162, 'motion_component_percent': 44.13173701221372}, {'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 7.6773295402526855, 'force': [3.0470719329534726, 2.0308755923312485, -2.6779714065782163], 'magnitude': 4.536588353660724, 'cosine_with_motion': 0.40733834976551764, 'motion_component': 1.8479264135456257, 'motion_component_percent': 40.73383497655176}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 7.155954360961914, 'force': [-3.2780821701764085, -3.0935973159412513, 2.8044905054343623], 'magnitude': 5.308609428343629, 'cosine_with_motion': -0.5085585720345993, 'motion_component': -2.6997388303678465, 'motion_component_percent': 50.855857203459934}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 7.240767955780029, 'force': [-3.925662829116496, -1.6311771823457684, 2.9685675442000745], 'magnitude': 5.184974533456309, 'cosine_with_motion': -0.35849192244748407, 'motion_component': -1.8587714883399988, 'motion_component_percent': 35.84919224474841}, {'resid': 98, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 8.60933780670166, 'force': [1.0422424824769074, 0.6478053756543638, -2.066646621678737], 'magnitude': 2.403528542768414, 'cosine_with_motion': 0.0367149829316139, 'motion_component': 0.08824550942338914, 'motion_component_percent': 3.6714982931613895}, {'resid': 98, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 7.461002826690674, 'force': [-1.376939717470447, -1.0556324011818645, 3.005668738996941], 'magnitude': 3.4704995779507084, 'cosine_with_motion': -0.041447085104053455, 'motion_component': -0.14384209136090462, 'motion_component_percent': 4.144708510405345}, {'resid': 426, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 14.792044639587402, 'force': [-0.679038761291151, -0.011073994954437078, -0.4491204391941214], 'magnitude': 0.8142023345594093, 'cosine_with_motion': -0.669404889331913, 'motion_component': -0.5450310236595266, 'motion_component_percent': 66.9404889331913}, {'resid': 426, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 13.805797576904297, 'force': [0.8692284020711004, 0.03875903738801685, 0.5199130786298648], 'magnitude': 1.0135925647303794, 'cosine_with_motion': 0.6824246322959306, 'motion_component': 0.6917005332840185, 'motion_component_percent': 68.24246322959307}, {'resid': 754, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 12.345751762390137, 'force': [0.10634993611285551, 0.7660709778679052, 0.8164503733490442], 'magnitude': 1.1246182748757423, 'cosine_with_motion': 0.8762845554493945, 'motion_component': 0.9854856250497548, 'motion_component_percent': 87.62845554493946}, {'resid': 754, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 13.311304092407227, 'force': [-0.059122478902624676, -0.38183480157774274, -0.391576915978534], 'magnitude': 0.5501143193325959, 'cosine_with_motion': -0.8860813775914391, 'motion_component': -0.48744605390700346, 'motion_component_percent': 88.60813775914391}, {'resid': 754, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 11.351812362670898, 'force': [-0.01523728018460148, -0.07482850414698328, -0.06804468388553474], 'magnitude': 0.10228176154809562, 'cosine_with_motion': -0.9141297020211666, 'motion_component': -0.09349879620616067, 'motion_component_percent': 91.41297020211667}, {'resid': 754, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 10.69538402557373, 'force': [-0.024148969922901622, -0.24240295128093498, -0.20859102952306693], 'magnitude': 0.3207063783829962, 'cosine_with_motion': -0.8889600282431633, 'motion_component': -0.2850951511851109, 'motion_component_percent': 88.89600282431633}, {'resid': 754, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 12.2778902053833, 'force': [-0.02378070079151519, -0.09734864625263034, -0.07189370399721733], 'magnitude': 0.12333282341613214, 'cosine_with_motion': -0.9426054112047709, 'motion_component': -0.11625418673120863, 'motion_component_percent': 94.26054112047709}, {'resid': 754, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 12.774681091308594, 'force': [0.004321825812391217, 0.028739001851861613, 0.019851882129266692], 'magnitude': 0.035195250103788926, 'cosine_with_motion': 0.9197105236193632, 'motion_component': 0.03236944190187016, 'motion_component_percent': 91.97105236193633}, {'resid': 754, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 13.171326637268066, 'force': [0.0076972003671071315, 0.025351319782686756, 0.019853565907964017], 'magnitude': 0.033107406837100825, 'cosine_with_motion': 0.9521742150569453, 'motion_component': 0.03152401911768742, 'motion_component_percent': 95.21742150569453}, {'resid': 754, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 11.773818969726562, 'force': [-0.008779413774780372, -0.026839688196545107, -0.016231992140433516], 'magnitude': 0.0325718365703204, 'cosine_with_motion': -0.9692883839807651, 'motion_component': -0.03157150283253145, 'motion_component_percent': 96.92883839807651}, {'resid': 754, 'resname': 'GLU', 'atom': 'HG2', 'charge': -0.042500000447034836, 'distance': 12.562442779541016, 'force': [0.0240006190195133, 0.07640662525756343, 0.03974768245095525], 'magnitude': 0.08940850270970614, 'cosine_with_motion': 0.9677529360834011, 'motion_component': 0.08652534100813884, 'motion_component_percent': 96.7752936083401}, {'resid': 754, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 11.866691589355469, 'force': [0.03541163229466575, 0.07887442178512095, 0.05064464216177405], 'magnitude': 0.10019998948804296, 'cosine_with_motion': 0.986704932581353, 'motion_component': 0.0988678238724517, 'motion_component_percent': 98.6704932581353}, {'resid': 754, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 10.501465797424316, 'force': [-0.584505585377183, -2.0892070253283026, -1.0828282911075993], 'magnitude': 2.424654590254303, 'cosine_with_motion': -0.9602958535748645, 'motion_component': -2.3283857493724693, 'motion_component_percent': 96.02958535748644}, {'resid': 754, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 9.71003532409668, 'force': [0.9469716506553004, 2.4541647700414915, 1.180315117405826], 'magnitude': 2.8831968025152843, 'cosine_with_motion': 0.9795502644488666, 'motion_component': 2.8242361903619733, 'motion_component_percent': 97.95502644488666}, {'resid': 754, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 10.227750778198242, 'force': [0.3240278422999051, 2.2979013773035066, 1.169564268171948], 'magnitude': 2.598696858000846, 'cosine_with_motion': 0.9207338759046741, 'motion_component': 2.3927082303684175, 'motion_component_percent': 92.07338759046742}, {'resid': 754, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 10.741355895996094, 'force': [-0.4012841693472027, -1.0304868025092822, -1.0776173006690413], 'magnitude': 1.5440826018758549, 'cosine_with_motion': -0.9358937186464773, 'motion_component': -1.445097208166922, 'motion_component_percent': 93.58937186464773}, {'resid': 754, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 9.521649360656738, 'force': [0.5928566956235829, 1.4345679292121825, 1.4598803821278563], 'magnitude': 2.1308953365174035, 'cosine_with_motion': 0.9437231724947317, 'motion_component': 2.010975307232433, 'motion_component_percent': 94.37231724947317}, {'resid': 1082, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 14.161029815673828, 'force': [-0.030794148450555527, 0.04359779630595218, -0.038352236512225676], 'magnitude': 0.06572626162364512, 'cosine_with_motion': 0.0034264319728577576, 'motion_component': 0.00022520656428367145, 'motion_component_percent': 0.34264319728577575}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 14.116772651672363, 'force': [-0.09845966236283543, 0.11592801233707513, -0.10370831890137022], 'magnitude': 0.18408971879596345, 'cosine_with_motion': -0.04574119352809602, 'motion_component': -0.008420483453978939, 'motion_component_percent': 4.574119352809602}, {'resid': 1082, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 14.740365028381348, 'force': [-0.03756780792216476, 0.06256789997126593, -0.044673728542454556], 'magnitude': 0.08556765931574804, 'cosine_with_motion': 0.09591218440486252, 'motion_component': 0.008206981119384478, 'motion_component_percent': 9.591218440486251}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 14.934273719787598, 'force': [0.009610757456709949, -0.01935565323155385, 0.014006171546861429], 'magnitude': 0.025752297223975526, 'cosine_with_motion': -0.1342779320573888, 'motion_component': -0.003457965216962668, 'motion_component_percent': 13.42779320573888}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 14.175175666809082, 'force': [0.012733066405629231, -0.021836152889171675, 0.01334588528702774], 'magnitude': 0.028584282520013472, 'cosine_with_motion': -0.14152754298199788, 'motion_component': -0.004045463272960777, 'motion_component_percent': 14.152754298199788}, {'resid': 1082, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 12.797944068908691, 'force': [-0.46867083793340253, 0.7207792290875749, -0.6662673091538571], 'magnitude': 1.0876981100748488, 'cosine_with_motion': 0.00883735214947409, 'motion_component': 0.00961237123104887, 'motion_component_percent': 0.883735214947409}, {'resid': 1082, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 11.764103889465332, 'force': [0.6610025851623972, -0.9307693612654724, 0.8033742678872617], 'magnitude': 1.395946358484201, 'cosine_with_motion': -0.007049105658438108, 'motion_component': -0.009840173374467052, 'motion_component_percent': 0.7049105658438107}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'N', 'charge': -0.38210001587867737, 'distance': 7.056772708892822, 'force': [-1.990859991079422, -1.2621957887516952, -0.965793324966687], 'magnitude': 2.5474337007611165, 'cosine_with_motion': -0.9264426445270376, 'motion_component': -2.360051214490427, 'motion_component_percent': 92.64426445270377}, {'resid': 130, 'resname': 'ASN', 'atom': 'H', 'charge': 0.2681000232696533, 'distance': 7.155559539794922, 'force': [1.2871761522784675, 1.0482396948144108, 0.5161182387501404], 'magnitude': 1.7383920562259703, 'cosine_with_motion': 0.9498225064156394, 'motion_component': 1.6511638999775882, 'motion_component_percent': 94.98225064156394}, {'resid': 130, 'resname': 'ASN', 'atom': 'CA', 'charge': -0.20800000429153442, 'distance': 5.74471378326416, 'force': [-1.664470807610967, -0.842238334065443, -0.9480037484034185], 'magnitude': 2.0924960185733616, 'cosine_with_motion': -0.8967215128082975, 'motion_component': -1.8763861953204442, 'motion_component_percent': 89.67215128082975}, {'resid': 130, 'resname': 'ASN', 'atom': 'HA', 'charge': 0.13580000400543213, 'distance': 5.777805805206299, 'force': [1.1734635610848527, 0.30901086762123753, 0.5928674367058479], 'magnitude': 1.350554050383818, 'cosine_with_motion': 0.7974939345646911, 'motion_component': 1.0770586634828712, 'motion_component_percent': 79.74939345646911}, {'resid': 130, 'resname': 'ASN', 'atom': 'CB', 'charge': -0.22990000247955322, 'distance': 4.6377949714660645, 'force': [-2.88170732468531, -1.8194730770055791, -0.9887685677624829], 'magnitude': 3.5485747369455516, 'cosine_with_motion': -0.9100915289697018, 'motion_component': -3.2295278080100345, 'motion_component_percent': 91.00915289697018}, {'resid': 130, 'resname': 'ASN', 'atom': 'HB2', 'charge': 0.1023000031709671, 'distance': 5.150431156158447, 'force': [1.1036446185517832, 0.6390136811116076, 0.11362270258184524], 'magnitude': 1.2803437223058973, 'cosine_with_motion': 0.840793175198071, 'motion_component': 1.0765042636224926, 'motion_component_percent': 84.07931751980709}, {'resid': 130, 'resname': 'ASN', 'atom': 'HB3', 'charge': 0.1023000031709671, 'distance': 4.550990581512451, 'force': [1.0818516366750277, 1.1368564314814258, 0.4756415776897816], 'magnitude': 1.6398415838136142, 'cosine_with_motion': 0.973947447720916, 'motion_component': 1.5971195252218942, 'motion_component_percent': 97.3947447720916}, {'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 3.3643245697021484, 'force': [18.62399961091497, 6.617210127612467, 7.040623194958056], 'magnitude': 20.981210793319804, 'cosine_with_motion': 0.8256955885988155, 'motion_component': 17.324093195506016, 'motion_component_percent': 82.56955885988155}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 2.7214157581329346, 'force': [-18.91226771438916, -10.021058728087263, -16.36313925016545], 'magnitude': 26.941562951187624, 'cosine_with_motion': -0.8956299296806501, 'motion_component': -24.12967013145898, 'motion_component_percent': 89.56299296806502}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 3.5599894523620605, 'force': [-23.558061254553685, -0.28141086394501763, -3.350257938254237], 'magnitude': 23.796757560652786, 'cosine_with_motion': -0.5640639934808861, 'motion_component': -13.42289410155828, 'motion_component_percent': 56.40639934808861}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 2.978043556213379, 'force': [14.977237735821305, -3.7149320826182204, 1.7978058406147333], 'magnitude': 15.535458680525796, 'cosine_with_motion': 0.35288573183199906, 'motion_component': 5.482241705823128, 'motion_component_percent': 35.28857318319991}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 4.368221282958984, 'force': [7.218541167665226, 0.15097072801551248, -0.08831743689650587], 'magnitude': 7.220659853479815, 'cosine_with_motion': 0.5080148058908184, 'motion_component': 3.6682021138691736, 'motion_component_percent': 50.80148058908184}, {'resid': 130, 'resname': 'ASN', 'atom': 'C', 'charge': 0.8050000071525574, 'distance': 5.722809791564941, 'force': [5.21594594909254, 3.1816156574598145, 5.409671146454983], 'magnitude': 8.16047255055955, 'cosine_with_motion': 0.9022975950567821, 'motion_component': 7.3631747568967665, 'motion_component_percent': 90.2297595056782}, {'resid': 130, 'resname': 'ASN', 'atom': 'O', 'charge': -0.8147000074386597, 'distance': 5.582760334014893, 'force': [-5.465720837001791, -1.6834690814029243, -6.527313556881053], 'magnitude': 8.678363594936451, 'cosine_with_motion': -0.7909682998172332, 'motion_component': -6.864310497882657, 'motion_component_percent': 79.09682998172332}, {'resid': 458, 'resname': 'ASN', 'atom': 'N', 'charge': -0.38210001587867737, 'distance': 14.284584045410156, 'force': [0.6204192587396681, 0.009200418713643403, -0.03878799215185492], 'magnitude': 0.6216986509996285, 'cosine_with_motion': 0.4803956936569566, 'motion_component': 0.2986613546925607, 'motion_component_percent': 48.03956936569566}, {'resid': 458, 'resname': 'ASN', 'atom': 'H', 'charge': 0.2681000232696533, 'distance': 13.984354972839355, 'force': [-0.45364464901524193, -0.03420460618975189, 0.013921612007887345], 'magnitude': 0.4551452888316611, 'cosine_with_motion': -0.5388630218275791, 'motion_component': -0.2452609657104152, 'motion_component_percent': 53.88630218275791}, {'resid': 458, 'resname': 'ASN', 'atom': 'CA', 'charge': -0.20800000429153442, 'distance': 13.48930549621582, 'force': [0.3776841647582964, -0.027382599483041198, -0.025140624423324827], 'magnitude': 0.3795091383089679, 'cosine_with_motion': 0.41246019707360776, 'motion_component': 0.15653241397815196, 'motion_component_percent': 41.24601970736077}, {'resid': 458, 'resname': 'ASN', 'atom': 'HA', 'charge': 0.13580000400543213, 'distance': 14.201311111450195, 'force': [-0.22138253606298522, 0.028946295971704304, 0.01131088770090804], 'magnitude': 0.2235532408728243, 'cosine_with_motion': -0.37417549884178486, 'motion_component': -0.08364814542128672, 'motion_component_percent': 37.417549884178484}, {'resid': 458, 'resname': 'ASN', 'atom': 'CB', 'charge': -0.22990000247955322, 'distance': 12.448068618774414, 'force': [0.4908851502957036, -0.03812588148179411, 0.014463060495301352], 'magnitude': 0.4925758761231513, 'cosine_with_motion': 0.4515136055698844, 'motion_component': 0.22240470984510877, 'motion_component_percent': 45.15136055698844}, {'resid': 458, 'resname': 'ASN', 'atom': 'HB2', 'charge': 0.1023000031709671, 'distance': 13.041008949279785, 'force': [-0.19855456774396496, 0.009814253315361503, -0.01903393718429191], 'magnitude': 0.19970610082034657, 'cosine_with_motion': -0.5005958143005366, 'motion_component': -0.09997203816094644, 'motion_component_percent': 50.059581430053655}, {'resid': 458, 'resname': 'ASN', 'atom': 'HB3', 'charge': 0.1023000031709671, 'distance': 11.62513256072998, 'force': [-0.25124454184475864, 0.005304853230437846, -0.0026671468059876195], 'magnitude': 0.251314693057656, 'cosine_with_motion': -0.4867828947174185, 'motion_component': -0.12233569377162531, 'motion_component_percent': 48.67828947174185}, {'resid': 458, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 12.04772663116455, 'force': [-1.6031014588707357, 0.32058754436848996, -0.06472922002543406], 'magnitude': 1.6361236300973105, 'cosine_with_motion': -0.35925763226892976, 'motion_component': -0.587789901448006, 'motion_component_percent': 35.925763226892975}, {'resid': 458, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 11.021090507507324, 'force': [1.5929276396834018, -0.4012622169307735, 0.009877539142369532], 'magnitude': 1.6427195128149668, 'cosine_with_motion': 0.3033301609717253, 'motion_component': 0.49828637425355804, 'motion_component_percent': 30.333016097172532}, {'resid': 458, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 12.903711318969727, 'force': [1.7466140745984597, -0.4574234191754285, 0.14437323075978206], 'magnitude': 1.8112814634273688, 'cosine_with_motion': 0.32706507169335386, 'motion_component': 0.5924069016927153, 'motion_component_percent': 32.70650716933539}, {'resid': 458, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 12.750555038452148, 'force': [-0.7972911133658882, 0.2738292990691009, -0.0869591138136345], 'magnitude': 0.8474771335889514, 'cosine_with_motion': -0.27284230689077704, 'motion_component': -0.2312276161655927, 'motion_component_percent': 27.284230689077702}, {'resid': 458, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 13.65030574798584, 'force': [-0.7166903091993166, 0.16041720247898603, -0.0859598712168668], 'magnitude': 0.7394374737670634, 'cosine_with_motion': -0.3722390425229593, 'motion_component': -0.2752474972406475, 'motion_component_percent': 37.22390425229593}, {'resid': 458, 'resname': 'ASN', 'atom': 'C', 'charge': 0.8050000071525574, 'distance': 12.963879585266113, 'force': [-1.5585731756792434, 0.13820385157331996, 0.2839499416378316], 'magnitude': 1.5902447037776009, 'cosine_with_motion': -0.34426009846516137, 'motion_component': -0.5474577983061782, 'motion_component_percent': 34.42600984651614}, {'resid': 458, 'resname': 'ASN', 'atom': 'O', 'charge': -0.8147000074386597, 'distance': 13.169370651245117, 'force': [1.4987809858317307, -0.2610268154012036, -0.343203791716721], 'magnitude': 1.5595731096995624, 'cosine_with_motion': 0.25638972372621305, 'motion_component': 0.3998585187267018, 'motion_component_percent': 25.638972372621303}, {'resid': 786, 'resname': 'ASN', 'atom': 'N', 'charge': -0.38210001587867737, 'distance': 9.022168159484863, 'force': [0.693795755714181, 1.3359560344043375, -0.40328656146545444], 'magnitude': 1.558451515821716, 'cosine_with_motion': 0.7466913108209363, 'motion_component': 1.1636822051997924, 'motion_component_percent': 74.66913108209363}, {'resid': 786, 'resname': 'ASN', 'atom': 'H', 'charge': 0.2681000232696533, 'distance': 8.450684547424316, 'force': [-0.4524481683379314, -1.1228737495297918, 0.29650134327778166], 'magnitude': 1.246381903343021, 'cosine_with_motion': -0.7475853069772175, 'motion_component': -0.931776797821541, 'motion_component_percent': 74.75853069772175}, {'resid': 786, 'resname': 'ASN', 'atom': 'CA', 'charge': -0.20800000429153442, 'distance': 8.650700569152832, 'force': [0.5033222384668197, 0.702543179747126, -0.323458888630123], 'magnitude': 0.9227815818373745, 'cosine_with_motion': 0.6845023244941887, 'motion_component': 0.6316461377681072, 'motion_component_percent': 68.45023244941886}, {'resid': 786, 'resname': 'ASN', 'atom': 'HA', 'charge': 0.13580000400543213, 'distance': 9.319811820983887, 'force': [-0.32247764964247677, -0.37382915202636896, 0.16028297013593726], 'magnitude': 0.5190671439604783, 'cosine_with_motion': -0.7100318744670411, 'motion_component': -0.36855421720051185, 'motion_component_percent': 71.0031874467041}, {'resid': 786, 'resname': 'ASN', 'atom': 'CB', 'charge': -0.22990000247955322, 'distance': 7.201537609100342, 'force': [0.8683585210110811, 1.074564002295936, -0.507187824001675], 'magnitude': 1.4717247721154816, 'cosine_with_motion': 0.6860490527481017, 'motion_component': 1.009675385815742, 'motion_component_percent': 68.60490527481016}, {'resid': 786, 'resname': 'ASN', 'atom': 'HB2', 'charge': 0.1023000031709671, 'distance': 6.547247409820557, 'force': [-0.3847703668035233, -0.6163105935964088, 0.3160243125393421], 'magnitude': 0.7923120275909229, 'cosine_with_motion': -0.6456721785371542, 'motion_component': -0.511573832935821, 'motion_component_percent': 64.56721785371542}, {'resid': 786, 'resname': 'ASN', 'atom': 'HB3', 'charge': 0.1023000031709671, 'distance': 7.263469219207764, 'force': [-0.4373029766828588, -0.3987260839131678, 0.2534038253852242], 'magnitude': 0.6437622869726718, 'cosine_with_motion': -0.6261978152171742, 'motion_component': -0.4031225376214986, 'motion_component_percent': 62.61978152171742}, {'resid': 786, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 6.914964199066162, 'force': [-3.300334697150575, -3.642183510636307, 0.7127114323209186], 'magnitude': 4.96645421041289, 'cosine_with_motion': -0.8144922584580064, 'motion_component': -4.04513850636747, 'motion_component_percent': 81.44922584580064}, {'resid': 786, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 7.3717169761657715, 'force': [2.8396982171025082, 2.3066351287442868, -0.312137580124181], 'magnitude': 3.6717681640182724, 'cosine_with_motion': 0.8161375634590656, 'motion_component': 2.99666792296844, 'motion_component_percent': 81.61375634590657}, {'resid': 786, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 6.510997772216797, 'force': [4.037358161876295, 5.854793469685815, -0.17770886491401944], 'magnitude': 7.114102047385448, 'cosine_with_motion': 0.8854590051783157, 'motion_component': 6.299245721614938, 'motion_component_percent': 88.54590051783157}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 6.6432414054870605, 'force': [-1.8888988645576315, -2.4581384016927266, -0.3690475541982463], 'magnitude': 3.1219512199365465, 'cosine_with_motion': -0.9409072288201904, 'motion_component': -2.937466470862309, 'motion_component_percent': 94.09072288201904}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 6.787649154663086, 'force': [-1.3361667717834749, -2.6672124451350876, 0.20946125901148568], 'magnitude': 2.9905246844873963, 'cosine_with_motion': -0.8568154336070887, 'motion_component': -2.5623277042517705, 'motion_component_percent': 85.68154336070887}, {'resid': 786, 'resname': 'ASN', 'atom': 'C', 'charge': 0.8050000071525574, 'distance': 9.315631866455078, 'force': [-1.522006517179266, -2.2205306472248765, 1.4957713426651746], 'magnitude': 3.0797064962654264, 'cosine_with_motion': -0.5691425437949615, 'motion_component': -1.7527919894263728, 'motion_component_percent': 56.91425437949616}, {'resid': 786, 'resname': 'ASN', 'atom': 'O', 'charge': -0.8147000074386597, 'distance': 10.211404800415039, 'force': [1.4215624726574154, 1.7166046186503947, -1.3270660269963623], 'magnitude': 2.5939690669797204, 'cosine_with_motion': 0.540285849421298, 'motion_component': 1.40148478072571, 'motion_component_percent': 54.0285849421298}, {'resid': 1114, 'resname': 'ASN', 'atom': 'N', 'charge': -0.38210001587867737, 'distance': 13.937173843383789, 'force': [0.3688960083864534, -0.5354636119723595, -0.060882239143519916], 'magnitude': 0.6530790088443148, 'cosine_with_motion': -0.3715478311953988, 'motion_component': -0.24265008933534585, 'motion_component_percent': 37.15478311953988}, {'resid': 1114, 'resname': 'ASN', 'atom': 'H', 'charge': 0.2681000232696533, 'distance': 14.056153297424316, 'force': [-0.26858840256836203, 0.361412553335967, 0.01407835702316637], 'magnitude': 0.4505074514805715, 'cosine_with_motion': 0.3153537568267199, 'motion_component': 0.14206921730282945, 'motion_component_percent': 31.53537568267199}, {'resid': 1114, 'resname': 'ASN', 'atom': 'CA', 'charge': -0.20800000429153442, 'distance': 12.619854927062988, 'force': [0.24292607290203572, -0.35385893908338684, -0.061503643873499006], 'magnitude': 0.4336034177385407, 'cosine_with_motion': -0.39249693024098553, 'motion_component': -0.17018801040437692, 'motion_component_percent': 39.249693024098555}, {'resid': 1114, 'resname': 'ASN', 'atom': 'HA', 'charge': 0.13580000400543213, 'distance': 12.298035621643066, 'force': [-0.1458803125912204,</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
starting analysis when ion is first in SF
</commit_message>
<xml_diff>
--- a/results_G2/forces/force_results.xlsx
+++ b/results_G2/forces/force_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,49 +457,225 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>900</v>
+        <v>40</v>
       </c>
       <c r="B2" t="n">
-        <v>969</v>
+        <v>594</v>
       </c>
       <c r="C2" t="n">
-        <v>2397</v>
+        <v>2400</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>{932: {'frame': 932, 'motion_vector': [-1.5848350524902344, -3.9648208618164062, -3.029510498046875], 'motion_vector_magnitude': 5.235402584075928, 'ionic_force': [-0.6365109831094742, 8.252115368843079, -3.386303260922432], 'ionic_force_magnitude': 8.94257256427081, 'radial_force': 8.276626987626972, 'axial_force': -3.386303260922432, 'glu_force': [7.704223445462621, 27.834427281033644, 11.325118289149916], 'glu_force_magnitude': 31.022068035899924, 'asn_force': [-0.6925757467836006, 0.1964403156845456, 0.5159840994618445], 'asn_force_magnitude': 0.885714148897124, 'sf_force': [0.17746470871481743, -0.8326530914041984, -0.7279579869851707], 'sf_force_magnitude': 1.1201462959273245, 'residue_force': [7.189112407393833, 27.19821450531399, 11.113144401626599], 'residue_force_magnitude': 30.247779885053067, 'pip2_force': [0.8071239286313593, -0.320149728655873, -4.342038780220539], 'pip2_force_magnitude': 4.428006961813273, 'total_force': [7.359725352915718, 35.1301801455012, 3.3848023604836275], 'total_force_magnitude': 36.05207346804415, 'cosine_total_motion': -0.8540692585971585, 'cosine_glu_motion': -0.965920148310478, 'cosine_asn_motion': -0.2683616116012464, 'cosine_sf_motion': 0.8910390514416046, 'cosine_residue_motion': -0.9655068323206991, 'cosine_pip2_motion': 0.5670004453303256, 'cosine_ionic_motion': -0.4581692131675099, 'motion_component_total': -30.79096765774276, 'motion_component_glu': -29.964840558134195, 'motion_component_asn': -0.2376916764160585, 'motion_component_sf': 0.9980940929989102, 'motion_component_residue': -29.204438141551346, 'motion_component_ionic': -4.097211435465319, 'motion_component_pip2': 2.510681919273908, 'motion_component_percent_total': np.float64(85.40692585971586), 'motion_component_percent_glu': np.float64(96.5920148310478), 'motion_component_percent_asn': np.float64(26.83616116012464), 'motion_component_percent_sf': np.float64(89.10390514416045), 'motion_component_percent_residue': np.float64(96.55068323206991), 'motion_component_percent_ionic': np.float64(45.81692131675099), 'motion_component_percent_pip2': np.float64(56.70004453303255), 'ionic_contributions': [{'ion_id': 2333, 'distance': 14.115193367004395, 'force': [-0.5459778308868408, 1.572485089302063, 0.07680048048496246], 'magnitude': 1.6663432121276855, 'cosine_ionic_motion': -0.6421388387680054, 'motion_component_ionic': -1.0700236558914185, 'motion_component_percent_ionic': 64.21388244628906}, {'ion_id': 2343, 'distance': 13.905966758728027, 'force': [-0.11061801016330719, 1.0146534442901611, -1.380529522895813], 'magnitude': 1.7168632745742798, 'cosine_ionic_motion': 0.037238940596580505, 'motion_component_ionic': 0.06393416970968246, 'motion_component_percent_ionic': 3.7238941192626953}, {'ion_id': 2372, 'distance': 11.306429862976074, 'force': [0.9758355617523193, 2.389859676361084, 0.28494706749916077], 'magnitude': 2.597090482711792, 'cosine_ionic_motion': -0.874113142490387, 'motion_component_ionic': -2.270150899887085, 'motion_component_percent_ionic': 87.41131591796875}, {'ion_id': 2381, 'distance': 8.941351890563965, 'force': [-0.9557507038116455, 3.2751171588897705, -2.367521286010742], 'magnitude': 4.152710914611816, 'cosine_ionic_motion': -0.19769522547721863, 'motion_component_ionic': -0.8209711313247681, 'motion_component_percent_ionic': 19.769521713256836}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 12.590643882751465, 'force': [-0.5854712981385105, -0.8527901613713734, 0.31491593773338206], 'magnitude': 1.081295402799023, 'cosine_with_motion': 0.5926487262973543, 'motion_component': 0.6408283432200256, 'motion_component_percent': 59.264872629735436}, {'resid': 98, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 12.965554237365723, 'force': [0.342371656503943, 0.4299297956870839, -0.18483057141019535], 'magnitude': 0.5798450832115514, 'cosine_with_motion': -0.5557988312793378, 'motion_component': -0.32227721957205063, 'motion_component_percent': 55.57988312793378}, {'resid': 98, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 11.88853645324707, 'force': [0.052649529481906876, 0.07506093625121706, -0.01704012749808002], 'magnitude': 0.09325493579819931, 'cosine_with_motion': -0.6747284346606955, 'motion_component': -0.06292175685550268, 'motion_component_percent': 67.47284346606955}, {'resid': 98, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 12.484599113464355, 'force': [0.12013967702504551, 0.1992203208854665, -0.03573180144848387], 'magnitude': 0.23537000633926228, 'cosine_with_motion': -0.7076646682301561, 'motion_component': -0.16656303744740378, 'motion_component_percent': 70.7664668230156}, {'resid': 98, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 12.415838241577148, 'force': [0.07878682101891384, 0.09000884546282266, -0.015401049610233572], 'magnitude': 0.12060741169975223, 'cosine_with_motion': -0.6890336889394917, 'motion_component': -0.08310256979692429, 'motion_component_percent': 68.90336889394916}, {'resid': 98, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 13.482990264892578, 'force': [-0.02058451780092914, -0.023528545930515725, 0.004571512362061461], 'magnitude': 0.03159451806845038, 'cosine_with_motion': 0.6774685457822437, 'motion_component': 0.021404292210523902, 'motion_component_percent': 67.74685457822437}, {'resid': 98, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 12.036210060119629, 'force': [-0.02775673420901588, -0.02747652788220378, 0.006815276586295851], 'magnitude': 0.039646486267501516, 'cosine_with_motion': 0.6373049314251062, 'motion_component': 0.02526690121195647, 'motion_component_percent': 63.730493142510625}, {'resid': 98, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 12.072093963623047, 'force': [0.020752175122121484, 0.023005103728810747, -8.280506588295213e-05], 'magnitude': 0.03098216303861749, 'cosine_with_motion': -0.7635382253195102, 'motion_component': -0.023656065783065724, 'motion_component_percent': 76.35382253195102}, {'resid': 98, 'resname': 'GLU', 'atom': 'HG2', 'charge': -0.042500000447034836, 'distance': 12.604401588439941, 'force': [-0.06428559206640366, -0.06126937220808316, -0.00118076056267318], 'magnitude': 0.08881423035531558, 'cosine_with_motion': 0.7492420620382658, 'motion_component': 0.06654335708975818, 'motion_component_percent': 74.92420620382659}, {'resid': 98, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 11.000815391540527, 'force': [-0.07836785169315627, -0.08631254825748585, -0.001688229082366012], 'magnitude': 0.11659428066220018, 'cosine_with_motion': 0.7724680602775119, 'motion_component': 0.09006535782258158, 'motion_component_percent': 77.24680602775119}, {'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 12.831777572631836, 'force': [0.983000105740883, 1.2884497682928056, 0.10422738890543091], 'magnitude': 1.623962857302597, 'cosine_with_motion': -0.8212234506736056, 'motion_component': -1.333636381439807, 'motion_component_percent': 82.12234506736056}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 14.030905723571777, 'force': [-0.8159837687866297, -1.1121974465089013, -0.06257971854319708], 'magnitude': 1.380843543677957, 'cosine_with_motion': 0.8150819625479988, 'motion_component': 1.1255006655527624, 'motion_component_percent': 81.50819625479988}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 12.313202857971191, 'force': [-0.9926112620735161, -1.4746372519460373, -0.23435403386295262], 'magnitude': 1.7929734955124064, 'cosine_with_motion': 0.8660732008619162, 'motion_component': 1.5528462943190082, 'motion_component_percent': 86.60732008619162}, {'resid': 98, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 10.381473541259766, 'force': [0.9059989703981168, 1.3448600733640257, -0.32078032954793956], 'magnitude': 1.65299206625925, 'cosine_with_motion': -0.6697628537114597, 'motion_component': -1.1071126834601976, 'motion_component_percent': 66.97628537114598}, {'resid': 98, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 9.912365913391113, 'force': [-0.9915450357370874, -1.6872894982616577, 0.1894933399617171], 'magnitude': 1.966218486010338, 'cosine_with_motion': 0.7467655365548984, 'motion_component': 1.46830420268967, 'motion_component_percent': 74.67655365548984}, {'resid': 426, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 13.699601173400879, 'force': [0.7631991813995468, -0.3121347543103282, 0.392756500424138], 'magnitude': 0.9133229242511781, 'cosine_with_motion': -0.24298211293665034, 'motion_component': -0.2219211339280315, 'motion_component_percent': 24.298211293665034}, {'resid': 426, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 14.704678535461426, 'force': [-0.37601815795928684, 0.15241533687433156, -0.19646817776916267], 'magnitude': 0.45079910703721066, 'cosine_with_motion': 0.24864456071503166, 'motion_component': 0.11208874593999578, 'motion_component_percent': 24.864456071503167}, {'resid': 426, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 13.219758987426758, 'force': [-0.0652462410549228, 0.02824976614235723, -0.02515798783075809], 'magnitude': 0.07541913292121262, 'cosine_with_motion': 0.17124413299328678, 'motion_component': 0.012915084028198508, 'motion_component_percent': 17.12441329932868}, {'resid': 426, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 12.607240676879883, 'force': [-0.20698671199682617, 0.07337791623375711, -0.0710410214311649], 'magnitude': 0.23081300712925293, 'cosine_with_motion': 0.20881268830492664, 'motion_component': 0.0481966845144035, 'motion_component_percent': 20.881268830492665}, {'resid': 426, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 14.587169647216797, 'force': [-0.076649061665319, 0.0339322533663251, -0.024653675315545295], 'magnitude': 0.08737436797628172, 'cosine_with_motion': 0.13472672297298385, 'motion_component': 0.011771662269280059, 'motion_component_percent': 13.472672297298386}, {'resid': 426, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 14.66709041595459, 'force': [-0.01850401279598529, 0.009096018699043223, -0.003923857762737846], 'magnitude': 0.020988870990825814, 'cosine_with_motion': 0.046858851512916036, 'motion_component': 0.0009835143891828576, 'motion_component_percent': 4.685885151291604}, {'resid': 426, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 14.419692993164062, 'force': [0.05746025324632701, -0.033759343426547864, 0.01279177267765144], 'magnitude': 0.0678601755078805, 'cosine_with_motion': 0.01134868706315981, 'motion_component': 0.0007701238958900376, 'motion_component_percent': 1.134868706315981}, {'resid': 426, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 13.837331771850586, 'force': [-1.2806234307173554, 0.5341122071228457, -0.1580395804390395], 'magnitude': 1.3965130611939418, 'cosine_with_motion': 0.0534378199480176, 'motion_component': 0.07462661351913674, 'motion_component_percent': 5.34378199480176}, {'resid': 426, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 13.996736526489258, 'force': [1.313907159013888, -0.41579401563165397, 0.1618009565986073], 'magnitude': 1.3875936853053443, 'cosine_with_motion': -0.1271857583497679, 'motion_component': -0.1764821551469094, 'motion_component_percent': 12.71857583497679}, {'resid': 426, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 13.293813705444336, 'force': [1.3879059347323446, -0.6592024054688912, 0.07260238721751497], 'magnitude': 1.5382138348327639, 'cosine_with_motion': 0.02409829756337943, 'motion_component': 0.03706833470790692, 'motion_component_percent': 2.409829756337943}, {'resid': 426, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 12.535074234008789, 'force': [-0.9347428927544644, 0.5331662494715415, -0.3570476591469983], 'magnitude': 1.13379608220918, 'cosine_with_motion': 0.07567277001117025, 'motion_component': 0.08579749016858114, 'motion_component_percent': 7.5672770011170245}, {'resid': 426, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 11.389250755310059, 'force': [1.242462240970332, -0.715821114489855, 0.40254774122417764], 'magnitude': 1.4893478345071727, 'cosine_with_motion': -0.04495356199594613, 'motion_component': -0.0669514902120463, 'motion_component_percent': 4.495356199594613}, {'resid': 754, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 5.35865592956543, 'force': [0.020703319514658803, 2.2838752867568792, 5.515148220031969], 'magnitude': 5.969369718975323, 'cosine_with_motion': -0.8254231175710813, 'motion_component': -4.927255763371021, 'motion_component_percent': 82.54231175710814}, {'resid': 754, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 6.157289028167725, 'force': [-0.07418722135614916, -1.2259926663803034, -2.2587328689180075], 'magnitude': 2.571076804562906, 'cosine_with_motion': 0.8782113293482567, 'motion_component': 2.257948778391658, 'motion_component_percent': 87.82113293482567}, {'resid': 754, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 4.163855075836182, 'force': [-0.0937809626260669, -0.3895323930342045, -0.6460642806221327], 'magnitude': 0.7602166854718592, 'cosine_with_motion': 0.917154525943418, 'motion_component': 0.6972361737782194, 'motion_component_percent': 91.7154525943418}, {'resid': 754, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 3.6754324436187744, 'force': [0.3131561289876035, -1.5550247962493509, -2.2042946461231456], 'magnitude': 2.715710545142836, 'cosine_with_motion': 0.8684180935509269, 'motion_component': 2.35837217424909, 'motion_component_percent': 86.84180935509269}, {'resid': 754, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 4.9525675773620605, 'force': [-0.1645493054825156, -0.5520489994537412, -0.49266533236022164], 'magnitude': 0.7579932067256688, 'cosine_with_motion': 0.9933711534678179, 'motion_component': 0.7529685860858478, 'motion_component_percent': 99.33711534678179}, {'resid': 754, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 5.692524433135986, 'force': [0.012617718425602407, 0.13557488121928576, 0.11347287280101288], 'magnitude': 0.1772451638200774, 'cosine_with_motion': -0.9712749395122011, 'motion_component': -0.17215378576817586, 'motion_component_percent': 97.12749395122012}, {'resid': 754, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 5.680540084838867, 'force': [0.06363204808069181, 0.11884981872991986, 0.11622171435463714], 'magnitude': 0.17799383091166152, 'cosine_with_motion': -0.991726395635772, 'motion_component': -0.17652118037542514, 'motion_component_percent': 99.1726395635772}, {'resid': 754, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 4.281439781188965, 'force': [-0.06894616805486112, -0.21589170325907106, -0.096488731090526], 'magnitude': 0.2463186490158871, 'cosine_with_motion': 0.9751674813128212, 'motion_component': 0.24020193656119943, 'motion_component_percent': 97.51674813128211}, {'resid': 754, 'resname': 'GLU', 'atom': 'HG2', 'charge': -0.042500000447034836, 'distance': 5.164259910583496, 'force': [0.15852321408147738, 0.48513585308645285, 0.13937600254703064], 'magnitude': 0.5290671747884499, 'cosine_with_motion': -0.9375681386316747, 'motion_component': -0.4960365262775258, 'motion_component_percent': 93.75681386316747}, {'resid': 754, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 4.00267219543457, 'force': [0.4514749819655982, 0.6965424850225095, 0.29432571347938125], 'magnitude': 0.8806978587445963, 'cosine_with_motion': -0.9475221009677314, 'motion_component': -0.8344806854354622, 'motion_component_percent': 94.75221009677314}, {'resid': 754, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 3.3726980686187744, 'force': [0.3710284522075463, -22.758947292934756, -5.870731216030349], 'magnitude': 23.506867698734407, 'cosine_with_motion': 0.8729535126706074, 'motion_component': 20.520402729493437, 'motion_component_percent': 87.29535126706074}, {'resid': 754, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 2.6508326530456543, 'force': [1.8593002507774488, 38.535748047845324, -2.8510234742281186], 'magnitude': 38.68577529118624, 'cosine_with_motion': -0.7262762932861518, 'motion_component': -28.09656148138374, 'motion_component_percent': 72.62762932861519}, {'resid': 754, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 3.987839460372925, 'force': [-5.064040406105003, 15.49842137165313, 5.133715117160847], 'magnitude': 17.09387613012755, 'cosine_with_motion': -0.7707327802636219, 'motion_component': -13.17481067525517, 'motion_component_percent': 77.07327802636219}, {'resid': 754, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 3.6582679748535156, 'force': [-5.316663564019318, -3.8249367912103134, -11.589120268608523], 'magnitude': 13.311827880122163, 'cosine_with_motion': 0.8422764617280754, 'motion_component': 11.212239286002442, 'motion_component_percent': 84.22764617280754}, {'resid': 754, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 2.5428404808044434, 'force': [14.24364672927492, 4.091512003715972, 25.943388079003302], 'magnitude': 29.877773137278933, 'cosine_with_motion': -0.7504800106776884, 'motion_component': -22.422671503090648, 'motion_component_percent': 75.04800106776884}, {'resid': 1082, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 14.737552642822266, 'force': [0.2590510945870284, -0.841529430362989, 0.1260699603891962], 'magnitude': 0.8894789973272712, 'cosine_with_motion': 0.5463065522786793, 'motion_component': 0.4859282043541581, 'motion_component_percent': 54.63065522786793}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'N', 'charge': -0.38210001587867737, 'distance': 13.743213653564453, 'force': [-0.2975036771859053, -0.48339125231553076, -0.35906673912838283], 'magnitude': 0.6716431075374798, 'cosine_with_motion': 0.988490347394267, 'motion_component': 0.6639127286946884, 'motion_component_percent': 98.8490347394267}, {'resid': 130, 'resname': 'ASN', 'atom': 'H', 'charge': 0.2681000232696533, 'distance': 13.688724517822266, 'force': [0.2107472641607138, 0.3613968010253428, 0.22498644333389045], 'magnitude': 0.47501679636262417, 'cosine_with_motion': -0.9845461826406781, 'motion_component': -0.46767597354902596, 'motion_component_percent': 98.4546182640678}, {'resid': 130, 'resname': 'ASN', 'atom': 'CA', 'charge': -0.20800000429153442, 'distance': 12.86524772644043, 'force': [-0.1587586063760088, -0.2968241185305162, -0.2465028426476434], 'magnitude': 0.4172199706069201, 'cosine_with_motion': 0.9958472515198175, 'motion_component': 0.4154873610080804, 'motion_component_percent': 99.58472515198174}, {'resid': 130, 'resname': 'ASN', 'atom': 'HA', 'charge': 0.13580000400543213, 'distance': 12.070148468017578, 'force': [0.13052606816308157, 0.20795411789312887, 0.18838023824471783], 'magnitude': 0.3094658038943227, 'cosine_with_motion': -0.9888190992835311, 'motion_component': -0.30600569746583806, 'motion_component_percent': 98.88190992835311}, {'resid': 130, 'resname': 'ASN', 'atom': 'CB', 'charge': -0.22990000247955322, 'distance': 12.447900772094727, 'force': [-0.15202934164649845, -0.38677682655275775, -0.2644518815552216], 'magnitude': 0.49258911065693156, 'cosine_with_motion': 0.9987202658044341, 'motion_component': 0.49195872752766046, 'motion_component_percent': 99.8720265804434}, {'resid': 130, 'resname': 'ASN', 'atom': 'HB2', 'charge': 0.1023000031709671, 'distance': 11.750934600830078, 'force': [0.0841732808408553, 0.19860764002673276, 0.1181838722249369], 'magnitude': 0.24596252466296967, 'cosine_with_motion': -0.9931435902515982, 'motion_component': -0.24427610481112896, 'motion_component_percent': 99.31435902515982}, {'resid': 130, 'resname': 'ASN', 'atom': 'HB3', 'charge': 0.1023000031709671, 'distance': 13.309401512145996, 'force': [0.05660962357100936, 0.1564254072436499, 0.09533077454484143], 'magnitude': 0.19173292384854637, 'cosine_with_motion': -0.9949413798597232, 'motion_component': -0.19076301981841196, 'motion_component_percent': 99.49413798597232}, {'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 11.908919334411621, 'force': [0.33838407262559916, 1.314687149264351, 0.9803054937400859], 'magnitude': 1.6744864711619818, 'cosine_with_motion': -0.9945266085386434, 'motion_component': -1.6653213512085667, 'motion_component_percent': 99.45266085386434}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 12.681903839111328, 'force': [-0.16058901294356137, -0.9695311124503821, -0.7572270519243304], 'magnitude': 1.2406337965949, 'cosine_with_motion': 0.9841936250966421, 'motion_component': 1.2210238736881447, 'motion_component_percent': 98.41936250966421}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 10.6524658203125, 'force': [-0.4853737210012613, -2.064485389717397, -1.6018652227653978], 'magnitude': 2.6577546473104774, 'cosine_with_motion': 0.9923104143984918, 'motion_component': 2.637317615442177, 'motion_component_percent': 99.23104143984918}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 10.539044380187988, 'force': [0.12520255749318426, 0.9384152748897333, 0.8015289452451034], 'magnitude': 1.2404626389436062, 'cosine_with_motion': -0.9773637442343424, 'motion_component': -1.212383209380736, 'motion_component_percent': 97.73637442343424}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 9.876602172851562, 'force': [0.3349073994920081, 1.1089681137422567, 0.8080983974784651], 'magnitude': 1.4124433664890148, 'cosine_with_motion': -0.9974394908652973, 'motion_component': -1.4088267923468694, 'motion_component_percent': 99.74394908652972}, {'resid': 130, 'resname': 'ASN', 'atom': 'C', 'charge': 0.8050000071525574, 'distance': 13.721765518188477, 'force': [0.4621345499777166, 0.9581136555391653, 0.939803946574249], 'magnitude': 1.4194300184265032, 'cosine_with_motion': -0.9928699263170785, 'motion_component': -1.4093093778073715, 'motion_component_percent': 99.28699263170785}, {'resid': 130, 'resname': 'ASN', 'atom': 'O', 'charge': -0.8147000074386597, 'distance': 13.473051071166992, 'force': [-0.4831179843212489, -0.9089957169283788, -1.0773133658647167], 'magnitude': 1.4900604982481513, 'cosine_with_motion': 0.9785071805802416, 'motion_component': 1.4580348970347885, 'motion_component_percent': 97.85071805802416}, {'resid': 458, 'resname': 'ASN', 'atom': 'H', 'charge': 0.2681000232696533, 'distance': 14.988238334655762, 'force': [-0.35159251474955083, 0.14668083919044975, 0.10888439535121618], 'magnitude': 0.3962175873993072, 'cosine_with_motion': -0.1707580934611865, 'motion_component': -0.06765735982009673, 'motion_component_percent': 17.07580934611865}, {'resid': 458, 'resname': 'ASN', 'atom': 'CB', 'charge': -0.22990000247955322, 'distance': 13.948356628417969, 'force': [0.31966476671883176, -0.20056810612156376, -0.10721534479443566], 'magnitude': 0.3923114304146461, 'cosine_with_motion': 0.29865534120148074, 'motion_component': 0.11716590410772709, 'motion_component_percent': 29.865534120148073}, {'resid': 458, 'resname': 'ASN', 'atom': 'HB2', 'charge': 0.1023000031709671, 'distance': 14.130436897277832, 'force': [-0.14275347537218278, 0.08594429294805073, 0.034187662521375416], 'magnitude': 0.17009930184998473, 'cosine_with_motion': -0.24489107379247274, 'motion_component': -0.041655800681392706, 'motion_component_percent': 24.489107379247272}, {'resid': 458, 'resname': 'ASN', 'atom': 'HB3', 'charge': 0.1023000031709671, 'distance': 13.15825366973877, 'force': [-0.16233101313234155, 0.09212510123298781, 0.06034531667896254], 'magnitude': 0.19616306825405483, 'cosine_with_motion': -0.2831650358996113, 'motion_component': -0.05554652226433733, 'motion_component_percent': 28.31650358996113}, {'resid': 458, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 13.690324783325195, 'force': [-0.9465642293702777, 0.760428180794035, 0.36224098811173583], 'magnitude': 1.2670648728211353, 'cosine_with_motion': -0.3937874199450275, 'motion_component': -0.49895420717120925, 'motion_component_percent': 39.37874199450275}, {'resid': 458, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 14.217873573303223, 'force': [0.7117622174176591, -0.6432120444722279, -0.2322906140921963], 'magnitude': 0.9870593283550771, 'cosine_with_motion': 0.411390164935663, 'motion_component': 0.4060664998932799, 'motion_component_percent': 41.1390164935663}, {'resid': 458, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 13.015183448791504, 'force': [1.2540066958212217, -1.0909152124660622, -0.6380848113828289], 'magnitude': 1.7803878848362769, 'cosine_with_motion': 0.45820753997672314, 'motion_component': 0.8157871529151919, 'motion_component_percent': 45.82075399767231}, {'resid': 458, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 13.103280067443848, 'force': [-0.5230588804372654, 0.5369175221645761, 0.286494548494512], 'magnitude': 0.8024650424340664, 'cosine_with_motion': -0.5159820339304598, 'motion_component': -0.4140575447532223, 'motion_component_percent': 51.598203393045985}, {'resid': 458, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 12.524663925170898, 'force': [-0.6287157102878594, 0.49747715761778505, 0.3587246648105989], 'magnitude': 0.87832246462089, 'cosine_with_motion': -0.44858427188238725, 'motion_component': -0.3940016432699058, 'motion_component_percent': 44.85842718823873}, {'resid': 786, 'resname': 'ASN', 'atom': 'N', 'charge': -0.38210001587867737, 'distance': 7.501667022705078, 'force': [0.49021578820599154, 0.5668397111822048, -2.1260210688329435], 'magnitude': 2.2542369800668958, 'cosine_with_motion': 0.2894866368235599, 'motion_component': 0.652571481962864, 'motion_component_percent': 28.948663682355992}, {'resid': 786, 'resname': 'ASN', 'atom': 'H', 'charge': 0.2681000232696533, 'distance': 6.8839216232299805, 'force': [-0.20239703513274077, -0.4813442562026131, 1.8042514266567378], 'magnitude': 1.8782917939986439, 'cosine_with_motion': -0.32915562588543806, 'motion_component': -0.6182503110491059, 'motion_component_percent': 32.91556258854381}, {'resid': 786, 'resname': 'ASN', 'atom': 'CA', 'charge': -0.20800000429153442, 'distance': 7.886672496795654, 'force': [0.3502795636682051, 0.11349646780592988, -1.0473959700202684], 'magnitude': 1.1102322004620069, 'cosine_with_motion': 0.372983065316697, 'motion_component': 0.41409780934162094, 'motion_component_percent': 37.2983065316697}, {'resid': 786, 'resname': 'ASN', 'atom': 'HA', 'charge': 0.13580000400543213, 'distance': 7.839688777923584, 'force': [-0.3218845655237848, -0.09792861103008875, 0.6518603529085356], 'magnitude': 0.7335677242591572, 'cosine_with_motion': -0.2802781585611422, 'motion_component': -0.2056030109352443, 'motion_component_percent': 28.02781585611422}, {'resid': 786, 'resname': 'ASN', 'atom': 'CB', 'charge': -0.22990000247955322, 'distance': 6.96112060546875, 'force': [0.46226908464725724, -0.10364852128038286, -1.502206986300529], 'magnitude': 1.5751385819267905, 'cosine_with_motion': 0.5128584827137732, 'motion_component': 0.8078231831908981, 'motion_component_percent': 51.28584827137732}, {'resid': 786, 'resname': 'ASN', 'atom': 'HB2', 'charge': 0.1023000031709671, 'distance': 6.013607025146484, 'force': [-0.33747211124980603, 0.018039501246879874, 0.8762562556349363], 'magnitude': 0.939168714883538, 'cosine_with_motion': -0.4456673236820701, 'motion_component': -0.41855680764807557, 'motion_component_percent': 44.56673236820701}, {'resid': 786, 'resname': 'ASN', 'atom': 'HB3', 'charge': 0.1023000031709671, 'distance': 6.96274471282959, 'force': [-0.10062106185782334, 0.06931251980960339, 0.6898350531821371], 'magnitude': 0.7005720691624485, 'cosine_with_motion': -0.60123793258576, 'motion_component': -0.4212105024905586, 'motion_component_percent': 60.123793258576}, {'resid': 786, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 7.618808269500732, 'force': [-1.5405918717261788, 0.8970836658594293, 3.6823709083252574], 'magnitude': 4.091214724902708, 'cosine_with_motion': -0.5728971583608515, 'motion_component': -2.3438452901408344, 'motion_component_percent': 57.28971583608515}, {'resid': 786, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 8.537376403808594, 'force': [0.8568063749077062, -0.7672591809837095, -2.4842370944154095], 'magnitude': 2.7375605483999426, 'cosine_with_motion': 0.642619465539742, 'motion_component': 1.7592096964954542, 'motion_component_percent': 64.2619465539742}, {'resid': 786, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 7.498124122619629, 'force': [2.8456438671293864, -1.303742262918855, -4.356359967345832], 'magnitude': 5.364261838477429, 'cosine_with_motion': 0.4934066475087124, 'motion_component': 2.64676245008207, 'motion_component_percent': 49.34066475087124}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 8.276344299316406, 'force': [-1.1255524830412058, 0.616942602411746, 1.548690415703839], 'magnitude': 2.0114493705892107, 'cosine_with_motion': -0.5084184174269311, 'motion_component': -1.022657905729363, 'motion_component_percent': 50.841841742693106}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 6.944668292999268, 'force': [-1.7222472408920102, 0.4454123847072834, 2.235375709780563], 'magnitude': 2.85682206570303, 'cosine_with_motion': -0.388363104597221, 'motion_component': -1.1094842867182748, 'motion_component_percent': 38.8363104597221}, {'resid': 786, 'resname': 'ASN', 'atom': 'C', 'charge': 0.8050000071525574, 'distance': 9.356072425842285, 'force': [-0.8684994864299833, -0.19316420493079656, 2.920627026247174], 'magnitude': 3.0531403496140004, 'cosine_with_motion': -0.4195198328902142, 'motion_component': -1.2808529292604356, 'motion_component_percent': 41.95198328902142}, {'resid': 786, 'resname': 'ASN', 'atom': 'O', 'charge': -0.8147000074386597, 'distance': 10.098258018493652, 'force': [0.9857451010534671, 0.09695902599048614, -2.46053977526189], 'magnitude': 2.652423503631682, 'cosine_with_motion': 0.39661260318306224, 'motion_component': 1.0519845905193, 'motion_component_percent': 39.661260318306226}], 'sf_contributions': [{'resid': 100, 'resname': 'THR', 'atom': 'N', 'charge': -0.4157000184059143, 'distance': 9.454451560974121, 'force': [-0.500074669765452, -1.2946255848007806, 0.6765984087662246], 'magnitude': 1.54399335714464, 'cosine_with_motion': 0.4794664730217872, 'motion_component': 0.7402930493192091, 'motion_component_percent': 47.94664730217872}, {'resid': 100, 'resname': 'THR', 'atom': 'H', 'charge': 0.2718999981880188, 'distance': 10.196442604064941, 'force': [0.3354068855950018, 0.7176704463771909, -0.3554254424174898], 'magnitude': 0.868260268367408, 'cosine_with_motion': -0.5060250599342219, 'motion_component': -0.43936145433912116, 'motion_component_percent': 50.602505993422184}, {'resid': 100, 'resname': 'THR', 'atom': 'CA', 'charge': -0.03889999911189079, 'distance': 9.98306941986084, 'force': [-0.024337471728129213, -0.11124004078020162, 0.06185452458156919], 'magnitude': 0.12958642449774727, 'cosine_with_motion': 0.43073817257871483, 'motion_component': 0.05581781967916926, 'motion_component_percent': 43.07381725787148}, {'resid': 100, 'resname': 'THR', 'atom': 'HA', 'charge': 0.1007000058889389, 'distance': 11.065008163452148, 'force': [0.05276874339582523, 0.23563609178417558, -0.12749479941589661], 'magnitude': 0.2730637872530786, 'cosine_with_motion': -0.4418286713669041, 'motion_component': -0.1206474103204427, 'motion_component_percent': 44.18286713669041}, {'resid': 100, 'resname': 'THR', 'atom': 'CB', 'charge': 0.3653999865055084, 'distance': 9.628469467163086, 'force': [0.08195224112158213, 1.1948164942284574, -0.5272708750364847</t>
+          <t>{22: {'frame': 22, 'motion_vector': [0.21028900146484375, 0.1107177734375, -0.33880615234375], 'motion_vector_magnitude': 0.4138471782207489, 'ionic_force': [-2.899083435535431, 3.592764049768448, -13.504176616668701], 'ionic_force_magnitude': 14.271489914430315, 'radial_force': 4.616561305073777, 'axial_force': -13.504176616668701, 'glu_force': [-1.803526569972746, 1.5313365116307978, 0.8455928799230605], 'glu_force_magnitude': 2.512514063448763, 'asn_force': [-1.8459446895867586, -0.24792473018169403, -3.4486663714051247], 'asn_force_magnitude': 3.9194742262336426, 'sf_force': [3.5290039767423877, -6.570519581455301, 22.610275247017853], 'sf_force_magnitude': 23.80861489847865, 'residue_force': [-0.12046728281711694, -5.287107800006197, 20.00720175553579], 'residue_force_magnitude': 20.69435051751637, 'pip2_force': [0.2742085577920079, -0.16031867498531938, -4.897681090091282], 'pip2_force_magnitude': 4.907970300536991, 'total_force': [-2.74534216056054, -1.8546624252230686, 1.6053440487758053], 'total_force_magnitude': 3.681549375606067, 'cosine_total_motion': -0.8706752883695206, 'cosine_glu_motion': -0.47721601984730977, 'cosine_asn_motion': 0.4640989185209237, 'cosine_sf_motion': -0.7759833223571565, 'cosine_residue_motion': -0.8627995493810828, 'cosine_pip2_motion': 0.8366086790694501, 'cosine_ionic_motion': 0.7387870327602997, 'motion_component_total': -3.205434064252441, 'motion_component_glu': -1.19901196116941, 'motion_component_asn': 1.8190237495656678, 'motion_component_sf': -18.475088089643556, 'motion_component_residue': -17.8550763012473, 'motion_component_ionic': 10.543591686950515, 'motion_component_pip2': 4.106050550044344, 'motion_component_percent_total': 87.06752883695205, 'motion_component_percent_glu': 47.721601984730974, 'motion_component_percent_asn': 46.40989185209237, 'motion_component_percent_sf': 77.59833223571565, 'motion_component_percent_residue': 86.27995493810829, 'motion_component_percent_ionic': 73.87870327602997, 'motion_component_percent_pip2': 83.66086790694501, 'ionic_contributions': [{'ion_id': 2397, 'distance': 13.07612133026123, 'force': [-0.1774052381515503, 0.3195008337497711, -1.9069902896881104], 'magnitude': 1.9416913986206055, 'cosine_ionic_motion': 0.8016393184661865, 'motion_component_ionic': 1.5565361976623535, 'motion_component_percent_ionic': 80.16393184661865}, {'ion_id': 2398, 'distance': 9.430180549621582, 'force': [-0.44737333059310913, 0.7956843376159668, -3.620028257369995], 'magnitude': 3.733344554901123, 'cosine_ionic_motion': 0.789954423904419, 'motion_component_ionic': 2.949172019958496, 'motion_component_percent_ionic': 78.9954423904419}, {'ion_id': 2399, 'distance': 6.192728519439697, 'force': [-2.2743048667907715, 2.47757887840271, -7.977158069610596], 'magnitude': 8.657130241394043, 'cosine_ionic_motion': 0.6974462866783142, 'motion_component_ionic': 6.037883281707764, 'motion_component_percent_ionic': 69.74462866783142}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 9.9072847366333, 'force': [-1.4403156042099, -0.7283158302307129, 0.6669184565544128], 'magnitude': 1.7463486194610596, 'cosine_with_motion': -0.8433071374893188, 'motion_component': -1.4727082252502441, 'motion_component_percent': 84.33071374893188}, {'resid': 98, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 10.88489055633545, 'force': [0.6841881275177002, 0.32507437467575073, -0.3210335075855255], 'magnitude': 0.8227084875106812, 'cosine_with_motion': 0.8477462530136108, 'motion_component': 0.6974480152130127, 'motion_component_percent': 84.77462530136108}, {'resid': 98, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 9.317501068115234, 'force': [0.13188929855823517, 0.06473823636770248, -0.03825654089450836], 'magnitude': 0.15182024240493774, 'cosine_with_motion': 0.7617985606193542, 'motion_component': 0.11565644294023514, 'motion_component_percent': 76.17985606193542}, {'resid': 98, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 9.437228202819824, 'force': [0.3420225977897644, 0.2146041989326477, -0.08150182664394379], 'magnitude': 0.41191864013671875, 'cosine_with_motion': 0.7232734560966492, 'motion_component': 0.2979298233985901, 'motion_component_percent': 72.32734560966492}, {'resid': 98, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 10.324674606323242, 'force': [0.16016104817390442, 0.061865970492362976, -0.030662208795547485], 'magnitude': 0.17441080510616302, 'cosine_with_motion': 0.7054409384727478, 'motion_component': 0.12303651869297028, 'motion_component_percent': 70.54409384727478}, {'resid': 98, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 10.673501014709473, 'force': [-0.04704204946756363, -0.013870565220713615, 0.011681166477501392], 'magnitude': 0.050416234880685806, 'cosine_with_motion': -0.7374109029769897, 'motion_component': -0.03717748075723648, 'motion_component_percent': 73.74109029769897}, {'resid': 98, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 9.9197998046875, 'force': [-0.05516332387924194, -0.01836862973868847, 0.005145839881151915], 'magnitude': 0.05836847051978111, 'cosine_with_motion': -0.6365976929664612, 'motion_component': -0.03715723380446434, 'motion_component_percent': 63.65976929664612}, {'resid': 98, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 11.652201652526855, 'force': [0.029846055433154106, 0.013748987577855587, -0.005108237732201815], 'magnitude': 0.03325531259179115, 'cosine_with_motion': 0.6924015283584595, 'motion_component': 0.023026028648018837, 'motion_component_percent': 69.24015283584595}, {'resid': 98, 'resname': 'GLU', 'atom': 'HG2', 'charge': -0.042500000447034836, 'distance': 12.144301414489746, 'force': [-0.08828218281269073, -0.035946980118751526, 0.00819017831236124], 'magnitude': 0.09567135572433472, 'cosine_with_motion': -0.639492392539978, 'motion_component': -0.06118110194802284, 'motion_component_percent': 63.9492392539978}, {'resid': 98, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 11.521405220031738, 'force': [-0.0915706530213356, -0.05242396891117096, 0.01285847183316946], 'magnitude': 0.10629580169916153, 'cosine_with_motion': -0.6687190532684326, 'motion_component': -0.07108202576637268, 'motion_component_percent': 66.87190532684326}, {'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 12.611715316772461, 'force': [1.4799962043762207, 0.6731756329536438, -0.4273703098297119], 'magnitude': 1.6811304092407227, 'cosine_with_motion': 0.7625864744186401, 'motion_component': 1.2820073366165161, 'motion_component_percent': 76.25864744186401}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 13.542510986328125, 'force': [-1.3441143035888672, -0.5010690689086914, 0.37324461340904236], 'magnitude': 1.4822365045547485, 'cosine_with_motion': -0.757373034954071, 'motion_component': -1.1226059198379517, 'motion_component_percent': 75.7373034954071}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 12.526866912841797, 'force': [-1.4396367073059082, -0.7773059010505676, 0.5693977475166321], 'magnitude': 1.7323315143585205, 'cosine_with_motion': -0.8114105463027954, 'motion_component': -1.4056320190429688, 'motion_component_percent': 81.14105463027954}, {'resid': 98, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 7.987919330596924, 'force': [2.5263421535491943, 0.9910473823547363, -0.6564297080039978], 'magnitude': 2.792038679122925, 'cosine_with_motion': 0.7472158670425415, 'motion_component': 2.0862555503845215, 'motion_component_percent': 74.72158670425415}, {'resid': 98, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 7.4775590896606445, 'force': [-3.17303729057312, -1.3287041187286377, 0.3231578767299652], 'magnitude': 3.455148458480835, 'cosine_with_motion': -0.6460952758789062, 'motion_component': -2.2323551177978516, 'motion_component_percent': 64.60952758789062}, {'resid': 426, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 12.28113842010498, 'force': [1.040393352508545, -0.10682795941829681, 0.4447059631347656], 'magnitude': 1.136483073234558, 'cosine_with_motion': 0.11967422068119049, 'motion_component': 0.13600772619247437, 'motion_component_percent': 11.967422068119049}, {'resid': 426, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 13.25570297241211, 'force': [-0.5039324760437012, 0.04769434779882431, -0.22696365416049957], 'magnitude': 0.5547388792037964, 'cosine_with_motion': -0.10364344716072083, 'motion_component': -0.05749505013227463, 'motion_component_percent': 10.364344716072083}, {'resid': 426, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 12.069356918334961, 'force': [-0.0863146111369133, 0.010007970966398716, -0.02522999420762062], 'magnitude': 0.09048162400722504, 'cosine_with_motion': -0.22685936093330383, 'motion_component': -0.020526602864265442, 'motion_component_percent': 22.685936093330383}, {'resid': 426, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 11.795509338378906, 'force': [-0.2549872100353241, 0.0071264151483774185, -0.06674282252788544], 'magnitude': 0.2636737823486328, 'cosine_with_motion': -0.2769330143928528, 'motion_component': -0.07301997393369675, 'motion_component_percent': 27.69330143928528}, {'resid': 426, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 13.553064346313477, 'force': [-0.09743063151836395, 0.012241625227034092, -0.024539487436413765], 'magnitude': 0.10121645778417587, 'cosine_with_motion': -0.25828540325164795, 'motion_component': -0.026142733171582222, 'motion_component_percent': 25.828540325164795}, {'resid': 426, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 13.978535652160645, 'force': [0.02764272317290306, -0.0046700043603777885, 0.008836670778691769], 'magnitude': 0.02939414605498314, 'cosine_with_motion': 0.18923546373844147, 'motion_component': 0.0055624148808419704, 'motion_component_percent': 18.923546373844147}, {'resid': 426, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 13.727547645568848, 'force': [0.02954879216849804, -0.005102624651044607, 0.005458129569888115], 'magnitude': 0.03047882951796055, 'cosine_with_motion': 0.30122995376586914, 'motion_component': 0.009181136265397072, 'motion_component_percent': 30.122995376586914}, {'resid': 426, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 14.419132232666016, 'force': [-0.02108697034418583, 0.0006993637070991099, -0.005145516246557236], 'magnitude': 0.021716946735978127, 'cosine_with_motion': -0.2908032536506653, 'motion_component': -0.00631535891443491, 'motion_component_percent': 29.08032536506653}, {'resid': 426, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 14.075335502624512, 'force': [0.0701255351305008, 0.00018852631910704076, 0.012443355284631252], 'magnitude': 0.07122122496366501, 'cosine_with_motion': 0.3579889237880707, 'motion_component': 0.025496410205960274, 'motion_component_percent': 35.79889237880707}, {'resid': 426, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 14.466131210327148, 'force': [-1.2125535011291504, -0.04435107484459877, -0.40048083662986755], 'magnitude': 1.2777472734451294, 'cosine_with_motion': -0.23489712178707123, 'motion_component': -0.3001391589641571, 'motion_component_percent': 23.489712178707123}, {'resid': 426, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 13.763877868652344, 'force': [1.3564823865890503, 0.15033943951129913, 0.44318369030952454], 'magnitude': 1.4349418878555298, 'cosine_with_motion': 0.2555293142795563, 'motion_component': 0.3666697144508362, 'motion_component_percent': 25.552931427955627}, {'resid': 426, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 11.22170639038086, 'force': [-1.3402295112609863, 0.3047715127468109, -0.3351660668849945], 'magnitude': 1.4147216081619263, 'cosine_with_motion': -0.2297874093055725, 'motion_component': -0.32508522272109985, 'motion_component_percent': 22.97874093055725}, {'resid': 426, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 11.081021308898926, 'force': [1.5193818807601929, -0.3519764244556427, 0.20745722949504852], 'magnitude': 1.5733554363250732, 'cosine_with_motion': 0.3229031264781952, 'motion_component': 0.5080413818359375, 'motion_component_percent': 32.29031264781952}, {'resid': 754, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 8.998961448669434, 'force': [-0.18735714256763458, 1.7927768230438232, 1.1095890998840332], 'magnitude': 2.1166810989379883, 'cosine_with_motion': -0.24754203855991364, 'motion_component': -0.5239675641059875, 'motion_component_percent': 24.754203855991364}, {'resid': 754, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 9.997176170349121, 'force': [0.07383228838443756, -0.821808397769928, -0.5199952721595764], 'magnitude': 0.9753026962280273, 'cosine_with_motion': 0.24952517449855804, 'motion_component': 0.24336257576942444, 'motion_component_percent': 24.952517449855804}, {'resid': 754, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 8.531595230102539, 'force': [0.011536720208823681, -0.16676555573940277, -0.06961154192686081], 'magnitude': 0.18107903003692627, 'cosine_with_motion': 0.10070788115262985, 'motion_component': 0.018236085772514343, 'motion_component_percent': 10.070788115262985}, {'resid': 754, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 8.179649353027344, 'force': [0.09533262997865677, -0.5089262127876282, -0.18043360114097595], 'magnitude': 0.5483160614967346, 'cosine_with_motion': 0.1094321459531784, 'motion_component': 0.06000340357422829, 'motion_component_percent': 10.94321459531784}, {'resid': 754, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 9.890193939208984, 'force': [0.005508695263415575, -0.18015649914741516, -0.060335610061883926], 'magnitude': 0.19007128477096558, 'cosine_with_motion': 0.02102666161954403, 'motion_component': 0.003996564541012049, 'motion_component_percent': 2.102666161954403}, {'resid': 754, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 10.538607597351074, 'force': [0.001197262667119503, 0.047791969031095505, 0.019721832126379013], 'magnitude': 0.051715146750211716, 'cosine_with_motion': -0.053204245865345, 'motion_component': -0.0027514654211699963, 'motion_component_percent': 5.3204245865345}, {'resid': 754, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 9.840184211730957, 'force': [0.0017438764916732907, 0.05773761123418808, 0.01348370686173439], 'magnitude': 0.05931680276989937, 'cosine_with_motion': 0.08925073593854904, 'motion_component': 0.0052940682508051395, 'motion_component_percent': 8.925073593854904}, {'resid': 754, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 10.591939926147461, 'force': [0.006170731503516436, -0.038103535771369934, -0.01139330305159092], 'magnitude': 0.040246300399303436, 'cosine_with_motion': 0.05637785419821739, 'motion_component': 0.0022690000478178263, 'motion_component_percent': 5.637785419821739}, {'resid': 754, 'resname': 'GLU', 'atom': 'HG2', 'charge': -0.042500000447034836, 'distance': 10.001777648925781, 'force': [-0.029909664765000343, 0.13441844284534454, 0.030531233176589012], 'magnitude': 0.14104986190795898, 'cosine_with_motion': -0.03000238910317421, 'motion_component': -0.004231832921504974, 'motion_component_percent': 3.000238910317421}, {'resid': 754, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 10.663293838500977, 'force': [-0.02641480788588524, 0.11284314841032028, 0.044356975704431534], 'magnitude': 0.12409213930368423, 'cosine_with_motion': -0.15751901268959045, 'motion_component': -0.0195468720048666, 'motion_component_percent': 15.751901268959045}, {'resid': 754, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 11.96501636505127, 'force': [0.2495190054178238, -1.7981024980545044, -0.43946343660354614], 'magnitude': 1.8677688837051392, 'cosine_with_motion': 0.002952382666990161, 'motion_component': 0.005514368414878845, 'motion_component_percent': 0.2952382666990161}, {'resid': 754, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 12.975543975830078, 'force': [-0.23663228750228882, 1.5255662202835083, 0.4728459119796753], 'magnitude': 1.6145991086959839, 'cosine_with_motion': -0.06144439056515694, 'motion_component': -0.0992080569267273, 'motion_component_percent': 6.144439056515694}, {'resid': 754, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 12.149155616760254, 'force': [-0.1484737992286682, 1.815801739692688, 0.2697291374206543], 'magnitude': 1.841720461845398, 'cosine_with_motion': 0.10290498286485672, 'motion_component': 0.18952220678329468, 'motion_component_percent': 10.290498286485672}, {'resid': 754, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 7.604703903198242, 'force': [-0.2983003258705139, -2.867304801940918, -1.0859044790267944], 'magnitude': 3.0805206298828125, 'cosine_with_motion': -0.009632213972508907, 'motion_component': -0.029672235250473022, 'motion_component_percent': 0.9632213972508907}, {'resid': 754, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 6.955353736877441, 'force': [0.44022437930107117, 3.8749775886535645, 0.8592867851257324], 'magnitude': 3.9934473037719727, 'cosine_with_motion': 0.13945351541042328, 'motion_component': 0.5569002628326416, 'motion_component_percent': 13.945351541042328}, {'resid': 1082, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 12.502678871154785, 'force': [0.21006809175014496, -1.0212198495864868, 0.3397563397884369], 'magnitude': 1.0965641736984253, 'cosine_with_motion': -0.4054642617702484, 'motion_component': -0.4446175694465637, 'motion_component_percent': 40.54642617702484}, {'resid': 1082, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 13.41995906829834, 'force': [-0.09114678204059601, 0.5022292137145996, -0.18000364303588867], 'magnitude': 0.5412423014640808, 'cosine_with_motion': 0.4349488317966461, 'motion_component': 0.23541270196437836, 'motion_component_percent': 43.49488317966461}, {'resid': 1082, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 12.326581954956055, 'force': [-0.016597917303442955, 0.08341875672340393, -0.017043299973011017], 'magnitude': 0.0867447629570961, 'cosine_with_motion': 0.3208983540534973, 'motion_component': 0.027836252003908157, 'motion_component_percent': 32.08983540534973}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 12.111675262451172, 'force': [-0.06822269409894943, 0.2369026392698288, -0.042030252516269684], 'magnitude': 0.2500874698162079, 'cosine_with_motion': 0.25240063667297363, 'motion_component': 0.0631222352385521, 'motion_component_percent': 25.240063667297363}, {'resid': 1082, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 13.616605758666992, 'force': [-0.015413270331919193, 0.09795893728733063, -0.014877980574965477], 'magnitude': 0.10027401149272919, 'cosine_with_motion': 0.304720014333725, 'motion_component': 0.030555497854948044, 'motion_component_percent': 30.472001433372498}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 14.050009727478027, 'force': [0.0027233348228037357, -0.02844388596713543, 0.005486073438078165], 'magnitude': 0.02909584529697895, 'cosine_with_motion': -0.36834031343460083, 'motion_component': -0.010717173106968403, 'motion_component_percent': 36.83403134346008}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 13.360235214233398, 'force': [0.004246847238391638, -0.0318077951669693, 0.0023743140045553446], 'magnitude': 0.032177772372961044, 'cosine_with_motion': -0.2578011453151703, 'motion_component': -0.00829546619206667, 'motion_component_percent': 25.78011453151703}, {'resid': 1082, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 14.745377540588379, 'force': [-0.004738328978419304, 0.020009128376841545, -0.0029041976667940617], 'magnitude': 0.020766591653227806, 'cosine_with_motion': 0.2563250958919525, 'motion_component': 0.0053229983896017075, 'motion_component_percent': 25.63250958919525}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 14.400664329528809, 'force': [0.019974056631326675, -0.06455644965171814, 0.00793056283146143], 'magnitude': 0.06803963333368301, 'cosine_with_motion': -0.20009031891822815, 'motion_component': -0.013614071533083916, 'motion_component_percent': 20.009031891822815}, {'resid': 1082, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 11.167755126953125, 'force': [-0.16078132390975952, 1.40010404586792, -0.23292073607444763], 'magnitude': 1.4284236431121826, 'cosine_with_motion': 0.3385285437107086, 'motion_component': 0.483562171459198, 'motion_component_percent': 33.85285437107086}, {'resid': 1082, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 11.120382308959961, 'force': [0.15606072545051575, -1.5523951053619385, 0.07936958968639374], 'magnitude': 1.5622371435165405, 'cosine_with_motion': -0.2566801905632019, 'motion_component': -0.4009953439235687, 'motion_component_percent': 25.66801905632019}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'N', 'charge': -0.38210001587867737, 'distance': 9.349747657775879, 'force': [-1.1254172325134277, -0.49060916900634766, -0.7736954092979431], 'magnitude': 1.4511600732803345, 'cosine_with_motion': -0.04803740978240967, 'motion_component': -0.06970997154712677, 'motion_component_percent': 4.803740978240967}, {'resid': 130, 'resname': 'ASN', 'atom': 'H', 'charge': 0.2681000232696533, 'distance': 9.392038345336914, 'force': [0.7695924639701843, 0.4356437921524048, 0.48593786358833313], 'magnitude': 1.0090558528900146, 'cosine_with_motion': 0.10879349708557129, 'motion_component': 0.10977871716022491, 'motion_component_percent': 10.879349708557129}, {'resid': 130, 'resname': 'ASN', 'atom': 'CA', 'charge': -0.20800000429153442, 'distance': 8.292162895202637, 'force': [-0.7333906888961792, -0.28890159726142883, -0.6223370432853699], 'magnitude': 1.0043054819107056, 'cosine_with_motion': 0.05928623676300049, 'motion_component': 0.0595414936542511, 'motion_component_percent': 5.928623676300049}, {'resid': 130, 'resname': 'ASN', 'atom': 'HA', 'charge': 0.13580000400543213, 'distance': 8.227672576904297, 'force': [0.5146359801292419, 0.10863851010799408, 0.4085623323917389], 'magnitude': 0.6660147905349731, 'cosine_with_motion': -0.0659327283501625, 'motion_component': -0.04391217231750488, 'motion_component_percent': 6.593272835016251}, {'resid': 130, 'resname': 'ASN', 'atom': 'CB', 'charge': -0.22990000247955322, 'distance': 7.0511040687561035, 'force': [-1.1016987562179565, -0.6030988693237305, -0.8828065395355225], 'magnitude': 1.5351924896240234, 'cosine_with_motion': 0.001025246107019484, 'motion_component': 0.0015739500522613525, 'motion_component_percent': 0.1025246107019484}, {'resid': 130, 'resname': 'ASN', 'atom': 'HB2', 'charge': 0.1023000031709671, 'distance': 7.484124183654785, 'force': [0.4117639362812042, 0.31202226877212524, 0.3174383044242859], 'magnitude': 0.6063616871833801, 'cosine_with_motion': 0.05413937196135521, 'motion_component': 0.032828040421009064, 'motion_component_percent': 5.413937196135521}, {'resid': 130, 'resname': 'ASN', 'atom': 'HB3', 'charge': 0.1023000031709671, 'distance': 6.475889205932617, 'force': [0.5061593651771545, 0.31621822714805603, 0.5474458336830139], 'magnitude': 0.8098692297935486, 'cosine_with_motion': -0.131361186504364, 'motion_component': -0.10638538002967834, 'motion_component_percent': 13.136118650436401}, {'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 6.398104190826416, 'force': [4.86035680770874, 1.9953069686889648, 2.4597792625427246], 'magnitude': 5.801278591156006, 'cosine_with_motion': 0.17060977220535278, 'motion_component': 0.9897547960281372, 'motion_component_percent': 17.06097722053528}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 5.659969806671143, 'force': [-5.534719467163086, -1.187404751777649, -2.598329782485962], 'magnitude': 6.228512763977051, 'cosine_with_motion': -0.16100983321666718, 'motion_component': -1.0028518438339233, 'motion_component_percent': 16.100983321666718}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 7.045239448547363, 'force': [-5.309815406799316, -2.435286045074463, -1.6715329885482788], 'magnitude': 6.076082706451416, 'cosine_with_motion': -0.32605963945388794, 'motion_component': -1.9811652898788452, 'motion_component_percent': 32.605963945388794}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 6.821243762969971, 'force': [2.719320774078369, 1.0916513204574585, 0.42655107378959656], 'magnitude': 2.9611406326293945, 'cosine_with_motion': 0.4473344683647156, 'motion_component': 1.324620246887207, 'motion_component_percent': 44.73344683647156}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 7.852840423583984, 'force': [1.8658225536346436, 1.0549464225769043, 0.6306239366531372], 'magnitude': 2.2342543601989746, 'cosine_with_motion': 0.3195882737636566, 'motion_component': 0.7140414714813232, 'motion_component_percent': 31.95882737636566}, {'resid': 130, 'resname': 'ASN', 'atom': 'C', 'charge': 0.8050000071525574, 'distance': 8.933457374572754, 'force': [2.077496290206909, 0.938653290271759, 2.4530980587005615], 'magnitude': 3.3488433361053467, 'cosine_with_motion': -0.2094830423593521, 'motion_component': -0.701525866985321, 'motion_component_percent': 20.94830423593521}, {'resid': 130, 'resname': 'ASN', 'atom': 'O', 'charge': -0.8147000074386597, 'distance': 8.817228317260742, 'force': [-2.0099592208862305, -0.5792006850242615, -2.7801060676574707], 'magnitude': 3.479137659072876, 'cosine_with_motion': 0.31609046459198, 'motion_component': 1.0997222661972046, 'motion_component_percent': 31.609046459197998}, {'resid': 458, 'resname': 'ASN', 'atom': 'N', 'charge': -0.38210001587867737, 'distance': 11.314496994018555, 'force': [0.9139137268066406, -0.15517358481884003, -0.35018929839134216], 'magnitude': 0.9909337162971497, 'cosine_with_motion': 0.7160578370094299, 'motion_component': 0.7095658779144287, 'motion_component_percent': 71.605783700943}, {'resid': 458, 'resname': 'ASN', 'atom': 'H', 'charge': 0.2681000232696533, 'distance': 10.89134693145752, 'force': [-0.7121909260749817, 0.07606340944766998, 0.22370502352714539], 'magnitude': 0.7503635883331299, 'cosine_with_motion': -0.6992332935333252, 'motion_component': -0.5246791839599609, 'motion_component_percent': 69.92332935333252}, {'resid': 458, 'resname': 'ASN', 'atom': 'CA', 'charge': -0.20800000429153442, 'distance': 10.603797912597656, 'force': [0.5396945476531982, -0.1565367728471756, -0.24781718850135803], 'magnitude': 0.6141557693481445, 'cosine_with_motion': 0.7086784243583679, 'motion_component': 0.43523895740509033, 'motion_component_percent': 70.86784243583679}, {'resid': 458, 'resname': 'ASN', 'atom': 'HA', 'charge': 0.13580000400543213, 'distance': 11.259113311767578, 'force': [-0.3057432174682617, 0.11769960075616837, 0.13841493427753448], 'magnitude': 0.3556554615497589, 'cosine_with_motion': -0.666898787021637, 'motion_component': -0.23718619346618652, 'motion_component_percent': 66.6898787021637}, {'resid': 458, 'resname': 'ASN', 'atom': 'CB', 'charge': -0.22990000247955322, 'distance': 9.269780158996582, 'force': [0.7956503033638, -0.2569640874862671, -0.2998482584953308], 'magnitude': 0.8882560729980469, 'cosine_with_motion': 0.6541212201118469, 'motion_component': 0.5810271501541138, 'motion_component_percent': 65.41212201118469}, {'resid': 458, 'resname': 'ASN', 'atom': 'HB2', 'charge': 0.1023000031709671, 'distance': 8.516737937927246, 'force': [-0.4265608489513397, 0.0957050547003746, 0.1677311211824417], 'magnitude': 0.46823856234550476, 'cosine_with_motion': -0.7014846801757812, 'motion_component': -0.3284621834754944, 'motion_component_percent': 70.14846801757812}, {'resid': 458, 'resname': 'ASN', 'atom': 'HB3', 'charge': 0.1023000031709671, 'distance': 8.941164016723633, 'force': [-0.35845959186553955, 0.1629776805639267, 0.15948107838630676], 'magnitude': 0.42484021186828613, 'cosine_with_motion': -0.6334287524223328, 'motion_component': -0.26910600066185, 'motion_component_percent': 63.342875242233276}, {'resid': 458, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 9.72842025756836, 'force': [-2.3188693523406982, 0.8245164155960083, 0.48917120695114136], 'magnitude': 2.509237289428711, 'cosine_with_motion': -0.541271448135376, 'motion_component': -1.3581784963607788, 'motion_component_percent': 54.1271448135376}, {'resid': 458, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 10.556720733642578, 'force': [1.5985348224639893, -0.7368727326393127, -0.3275710344314575], 'magnitude': 1.7904183864593506, 'cosine_with_motion': 0.493350088596344, 'motion_component': 0.8833030462265015, 'motion_component_percent': 49.3350088596344}, {'resid': 458, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 9.691855430603027, 'force': [3.090559244155884, -0.816632866859436, -0.30037611722946167], 'magnitude': 3.21071195602417, 'cosine_with_motion': 0.4976609945297241, 'motion_component': 1.5978461503982544, 'motion_component_percent': 49.76609945297241}, {'resid': 458, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 10.41551399230957, 'force': [-1.223549723625183, 0.33912718296051025, 0.03122817724943161], 'magnitude': 1.2700614929199219, 'cosine_with_motion': -0.43821725249290466, 'motion_component': -0.5565628409385681, 'motion_component_percent': 43.821725249290466}, {'resid': 458, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 9.056745529174805, 'force': [-1.6466480493545532, 0.2896944582462311, 0.16171309351921082], 'magnitude': 1.679739236831665, 'cosine_with_motion': -0.5307979583740234, 'motion_component': -0.8916021585464478, 'motion_component_percent': 53.079795837402344}, {'resid': 458, 'resname': 'ASN', 'atom': 'C', 'charge': 0.8050000071525574, 'distance': 10.648370742797852, 'force': [-1.925833821296692, 0.5351306200027466, 1.2491812705993652], 'magnitude': 2.357043504714966, 'cosine_with_motion': -0.7883119583129883, 'motion_component': -1.8580856323242188, 'motion_component_percent': 78.83119583129883}, {'resid': 458, 'resname': 'ASN', 'atom': 'O', 'charge': -0.8147000074386597, 'distance': 11.130712509155273, 'force': [1.6638708114624023, -0.6610121726989746, -1.2493516206741333], 'magnitude': 2.1831817626953125, 'cosine_with_motion': 0.7747572064399719, 'motion_component': 1.6914358139038086, 'motion_component_percent': 77.47572064399719}, {'resid': 786, 'resname': 'ASN', 'atom': 'N', 'charge': -0.38210001587867737, 'distance': 8.747406959533691, 'force': [0.21616563200950623, 1.4516098499298096, -0.7711744904518127], 'magnitude': 1.6578929424285889, 'cosine_with_motion': 0.6813076734542847, 'motion_component': 1.12953519821167, 'motion_component_percent': 68.13076734542847}, {'resid': 786, 'resname': 'ASN', 'atom': 'H', 'charge': 0.2681000232696533, 'distance': 8.249906539916992, 'force': [-0.06082244589924812, -1.1885802745819092, 0.5421102046966553], 'magnitude': 1.3077867031097412, 'cosine_with_motion': -0.6061402559280396, 'motion_component': -0.7927021384239197, 'motion_component_percent': 60.614025592803955}, {'resid': 786, 'resname': 'ASN', 'atom': 'CA', 'charge': -0.20800000429153442, 'distance': 8.148402214050293, 'force': [0.2879575192928314, 0.8459134697914124, -0.5321899652481079], 'magnitude': 1.0400553941726685, 'cosine_with_motion': 0.7771899104118347, 'motion_component': 0.8083205819129944, 'motion_component_percent': 77.71899104118347}, {'resid': 786, 'resname': 'ASN', 'atom': 'HA', 'charge': 0.13580000400543213, 'distance': 8.84109</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>939</v>
+        <v>50</v>
       </c>
       <c r="B3" t="n">
-        <v>946</v>
+        <v>692</v>
       </c>
       <c r="C3" t="n">
-        <v>2381</v>
+        <v>2399</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>{900: {'frame': 900, 'motion_vector': [-0.10789871215820312, -0.40692901611328125, 0.30049896240234375], 'motion_vector_magnitude': 0.5172358751296997, 'ionic_force': [-0.3772927224636078, -0.9863015711307526, 0.1931312084197998], 'ionic_force_magnitude': 1.073517699576809, 'radial_force': 1.056002172175319, 'axial_force': 0.1931312084197998, 'glu_force': [1.0836964549269292, -0.4140640135370064, -6.0729958246576405], 'glu_force_magnitude': 6.182808851973082, 'asn_force': [0.21170830633948057, -0.24680387799194037, 0.10385699331562537], 'asn_force_magnitude': 0.341348555329525, 'sf_force': [-10.820608677178974, 7.172259086665558, 9.646289462732797], 'sf_force_magnitude': 16.173366160132755, 'residue_force': [-9.525203915912567, 6.511391195136613, 3.6771506313907802], 'residue_force_magnitude': 12.109878682371527, 'pip2_force': [0.49183042690526857, -0.0003565226072937966, -3.977347450844225], 'pip2_force_magnitude': 4.007641456102983, 'total_force': [-9.410666211470906, 5.524733101398567, -0.10706561103364498], 'total_force_magnitude': 10.913055366416648, 'cosine_total_motion': -0.22409794066701608, 'cosine_glu_motion': -0.5545278312458517, 'cosine_asn_motion': 0.6162150494520675, 'cosine_sf_motion': 0.13718687366050125, 'cosine_residue_motion': -0.08252947473117336, 'cosine_pip2_motion': -0.6021100770712579, 'cosine_ionic_motion': 0.9006558523483511, 'motion_component_total': -2.4455932339990993, 'motion_component_glu': -3.428539583692287, 'motion_component_asn': 0.21034411690277507, 'motion_component_sf': 2.2187735400751585, 'motion_component_residue': -0.9994219267143559, 'motion_component_ionic': 0.966869998723392, 'motion_component_pip2': -2.4130413060081355, 'motion_component_percent_total': np.float64(22.409794066701608), 'motion_component_percent_glu': np.float64(55.45278312458517), 'motion_component_percent_asn': np.float64(61.62150494520675), 'motion_component_percent_sf': np.float64(13.718687366050125), 'motion_component_percent_residue': np.float64(8.252947473117336), 'motion_component_percent_ionic': np.float64(90.06558523483511), 'motion_component_percent_pip2': np.float64(60.21100770712579), 'ionic_contributions': [{'ion_id': 2333, 'distance': 6.926368236541748, 'force': [-1.8060075044631958, -0.864895761013031, 6.624295711517334], 'magnitude': 6.920332431793213, 'cosine_ionic_motion': 0.708884060382843, 'motion_component_ionic': 4.9057135581970215, 'motion_component_percent_ionic': 70.8884048461914}, {'ion_id': 2334, 'distance': 11.763495445251465, 'force': [0.42012912034988403, 0.16894248127937317, -2.3560731410980225], 'magnitude': 2.39919376373291, 'cosine_ionic_motion': -0.6624578833580017, 'motion_component_ionic': -1.589364767074585, 'motion_component_percent_ionic': 66.24578857421875}, {'ion_id': 2343, 'distance': 6.220857620239258, 'force': [2.2641780376434326, 1.203137993812561, -8.186910629272461], 'magnitude': 8.579017639160156, 'cosine_ionic_motion': -0.7198064923286438, 'motion_component_ionic': -6.175232410430908, 'motion_component_percent_ionic': 71.98065185546875}, {'ion_id': 2372, 'distance': 9.070656776428223, 'force': [0.23220226168632507, -3.1571826934814453, 2.5021557807922363], 'magnitude': 4.035158634185791, 'cosine_ionic_motion': 0.9638074040412903, 'motion_component_ionic': 3.889115810394287, 'motion_component_percent_ionic': 96.3807373046875}, {'ion_id': 2397, 'distance': 10.983990669250488, 'force': [-1.4877946376800537, 1.6636964082717896, 1.609663486480713], 'magnitude': 2.7518057823181152, 'cosine_ionic_motion': -0.023025544360280037, 'motion_component_ionic': -0.06336182355880737, 'motion_component_percent_ionic': 2.3025543689727783}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 9.794252395629883, 'force': [-1.6912314364657115, -0.5363449305728168, -0.21223404431586543], 'magnitude': 1.786889181177082, 'cosine_with_motion': 0.36457925767206445, 'motion_component': 0.6514627312157836, 'motion_component_percent': 36.45792576720645}, {'resid': 98, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 10.564867973327637, 'force': [0.839856165166355, 0.2321867460564613, 0.0582473184474808], 'magnitude': 0.8733051089502142, 'cosine_with_motion': -0.371038092338973, 'motion_component': -0.3240294616547664, 'motion_component_percent': 37.1038092338973}, {'resid': 98, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 9.753364562988281, 'force': [0.12948033267208428, 0.033877143145394154, 0.03583917483159748], 'magnitude': 0.1385541909477189, 'cosine_with_motion': -0.23702884019116058, 'motion_component': -0.03284133918396241, 'motion_component_percent': 23.70288401911606}, {'resid': 98, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 9.974266052246094, 'force': [0.3286353961173335, 0.12000001443910166, 0.11653048938037082], 'magnitude': 0.36875545013166927, 'cosine_with_motion': -0.2583370013631268, 'motion_component': -0.09526317722332549, 'motion_component_percent': 25.833700136312682}, {'resid': 98, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 11.158337593078613, 'force': [0.14054687996821183, 0.02843141434994795, 0.04166092792723658], 'magnitude': 0.14932315194401627, 'cosine_with_motion': -0.18405225143852202, 'motion_component': -0.02748326230719271, 'motion_component_percent': 18.405225143852203}, {'resid': 98, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 11.890153884887695, 'force': [-0.03781662116647783, -0.010442535492399685, -0.010553104842827026], 'magnitude': 0.04062648650551295, 'cosine_with_motion': 0.24548714754085468, 'motion_component': 0.0099732802868454, 'motion_component_percent': 24.54871475408547}, {'resid': 98, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 11.384324073791504, 'force': [-0.04277759304901171, -0.004823325593379556, -0.010526327849482842], 'magnitude': 0.044316932597387684, 'cosine_with_motion': 0.14899231887202333, 'motion_component': 0.006602882552979951, 'motion_component_percent': 14.899231887202333}, {'resid': 98, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 11.482601165771484, 'force': [0.030951320350730154, 0.004759316736403936, 0.013859321535726147], 'magnitude': 0.03424494299428136, 'cosine_with_motion': -0.06275718427772363, 'motion_component': -0.002149116198072256, 'motion_component_percent': 6.275718427772363}, {'resid': 98, 'resname': 'GLU', 'atom': 'HG2', 'charge': -0.042500000447034836, 'distance': 12.534331321716309, 'force': [-0.0818327128359716, -0.01065816558487243, -0.03543507047761366], 'magnitude': 0.08980998610111571, 'cosine_with_motion': 0.05421743004866332, 'motion_component': 0.004869266639108666, 'motion_component_percent': 5.421743004866332}, {'resid': 98, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 11.010310173034668, 'force': [-0.1051160028891296, -0.006313083125582573, -0.04957990290102906], 'magnitude': 0.11639328096420981, 'cosine_with_motion': -0.01640872882140244, 'motion_component': -0.0019098657839750216, 'motion_component_percent': 1.640872882140244}, {'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 11.32984733581543, 'force': [1.7541444257403496, 0.45471198073341057, 1.0273020176160537], 'magnitude': 2.083059069536065, 'cosine_with_motion': -0.06088754062457841, 'motion_component': -0.12683234371977364, 'motion_component_percent': 6.0887540624578405}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 10.929491996765137, 'force': [-1.8186182974258203, -0.399683925633789, -1.3083246616096158], 'magnitude': 2.275704983585953, 'cosine_with_motion': -0.02912354763188504, 'motion_component': -0.06627660248558366, 'motion_component_percent': 2.912354763188504}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 11.783027648925781, 'force': [-1.6012701307782764, -0.6193185470273533, -0.941252210232158], 'magnitude': 1.957952302197802, 'cosine_with_motion': 0.14016502012929455, 'motion_component': 0.27443642384975353, 'motion_component_percent': 14.016502012929454}, {'resid': 98, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 8.622139930725098, 'force': [2.243343121435748, 0.37492584570387505, 0.7546906297972329], 'magnitude': 2.396396398130659, 'cosine_with_motion': -0.13540782032451862, 'motion_component': -0.32449081290439985, 'motion_component_percent': 13.540782032451862}, {'resid': 98, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 8.028939247131348, 'force': [-2.6358951862885744, -0.6077114578016181, -1.2899855704603296], 'magnitude': 2.9968849529200328, 'cosine_with_motion': 0.09293989755182026, 'motion_component': 0.27853018049897954, 'motion_component_percent': 9.293989755182027}, {'resid': 426, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 9.179295539855957, 'force': [1.9888111871948408, 0.4204380919628747, 0.07976194494200896], 'magnitude': 2.034330380087184, 'cosine_with_motion': -0.3437563090849686, 'motion_component': -0.6993139029181917, 'motion_component_percent': 34.37563090849686}, {'resid': 426, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 9.865439414978027, 'force': [-0.9835382134209263, -0.1596321104905322, -0.10109319855855749], 'magnitude': 1.0015236705908097, 'cosine_with_motion': 0.2716149230846442, 'motion_component': 0.2720287747549733, 'motion_component_percent': 27.161492308464418}, {'resid': 426, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 9.253471374511719, 'force': [-0.15103134374319496, -0.02404802712102654, 0.0174707837291117], 'magnitude': 0.1539285635786878, 'cosine_with_motion': 0.39353067337656605, 'motion_component': 0.06057561127700858, 'motion_component_percent': 39.353067337656604}, {'resid': 426, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 9.538516998291016, 'force': [-0.384478143019102, -0.10067015889359553, 0.06801389797855972], 'magnitude': 0.4032168320758904, 'cosine_with_motion': 0.4933318554278778, 'motion_component': 0.19891970790775002, 'motion_component_percent': 49.333185542787774}, {'resid': 426, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 10.51595401763916, 'force': [-0.16642018210231743, -0.011538756262658963, 0.020898310513247385], 'magnitude': 0.1681236428625244, 'cosine_with_motion': 0.3327051282200409, 'motion_component': 0.055935598155396546, 'motion_component_percent': 33.270512822004086}, {'resid': 426, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 11.411300659179688, 'force': [0.043580503796232954, 0.005245314393332241, -0.004325592623034903], 'magnitude': 0.04410764543431022, 'cosine_with_motion': -0.35664796258412396, 'motion_component': -0.015730901878529678, 'motion_component_percent': 35.664796258412395}, {'resid': 426, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 10.471868515014648, 'force': [0.05228685502324891, -0.0005432565611477574, -0.0030132584934193653], 'magnitude': 0.05237642659309284, 'cosine_with_motion': -0.2335132000434727, 'motion_component': -0.012230586980595152, 'motion_component_percent': 23.35132000434727}, {'resid': 426, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 10.749743461608887, 'force': [-0.037813332049282986, -0.0005066676826987014, 0.009829693719373651], 'magnitude': 0.03907336268388884, 'cosine_with_motion': 0.35823593588214225, 'motion_component': 0.013997482649125294, 'motion_component_percent': 35.82359358821422}, {'resid': 426, 'resname': 'GLU', 'atom': 'HG2', 'charge': -0.042500000447034836, 'distance': 11.772629737854004, 'force': [0.0985750757819855, -0.0020783278067231874, -0.02536562270040041], 'magnitude': 0.10180756271945347, 'cosine_with_motion': -0.33067266993751665, 'motion_component': -0.033664978584272864, 'motion_component_percent': 33.067266993751666}, {'resid': 426, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 10.072225570678711, 'force': [0.1331052573985167, -0.008612485631152232, -0.039409155958626756], 'magnitude': 0.1390836655730771, 'cosine_with_motion': -0.3155396368571755, 'motion_component': -0.043886409327693596, 'motion_component_percent': 31.55396368571755}, {'resid': 426, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 10.974818229675293, 'force': [-2.061354363289968, -0.2347083036954666, 0.7900491628910711], 'magnitude': 2.2200106933668304, 'cosine_with_motion': 0.4836287983899193, 'motion_component': 1.0736611040457718, 'motion_component_percent': 48.36287983899193}, {'resid': 426, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 10.883970260620117, 'force': [2.0418802809363505, 0.13817179879856956, -1.0381001666618361], 'magnitude': 2.2947807049222098, 'cosine_with_motion': -0.4958034386874668, 'motion_component': -1.1377601645340807, 'motion_component_percent': 49.58034386874668}, {'resid': 426, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 11.393671035766602, 'force': [1.9280212020691403, 0.42984376168444305, -0.6950140711214874], 'magnitude': 2.0940572996324693, 'cosine_with_motion': -0.5463817918592405, 'motion_component': -1.1441547796291112, 'motion_component_percent': 54.63817918592405}, {'resid': 426, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 8.017501831054688, 'force': [-2.7082841228504257, -0.22946335060595138, 0.5418543619423193], 'magnitude': 2.7714729782032745, 'cosine_with_motion': 0.38257434031782367, 'motion_component': 1.0602944463447919, 'motion_component_percent': 38.25743403178237}, {'resid': 426, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 7.816900730133057, 'force': [2.952436183503714, 0.34288105275400904, -1.0778421502975317], 'magnitude': 3.1616752734836133, 'cosine_with_motion': -0.4781798434169941, 'motion_component': -1.5118493872097762, 'motion_component_percent': 47.81798434169941}, {'resid': 754, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 9.490715026855469, 'force': [-0.49991818264340426, 1.8354018384352946, -0.05339140806470599], 'magnitude': 1.9030156962895168, 'cosine_with_motion': -0.7202845086264466, 'motion_component': -1.3707127257103098, 'motion_component_percent': 72.02845086264466}, {'resid': 754, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 10.18281078338623, 'force': [0.20786038458209863, -0.9162639340426555, -0.03131064547116315], 'magnitude': 0.9400669618839727, 'cosine_with_motion': 0.701341416840595, 'motion_component': 0.659307894972739, 'motion_component_percent': 70.1341416840595}, {'resid': 754, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 9.569018363952637, 'force': [0.029366662192606263, -0.13870477418194074, 0.024869406672579995], 'magnitude': 0.14394409545877174, 'cosine_with_motion': 0.8159182542189619, 'motion_component': 0.11744661507184864, 'motion_component_percent': 81.59182542189619}, {'resid': 754, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 9.79934024810791, 'force': [0.11114156696529708, -0.35475342255563147, 0.08803788930602856], 'magnitude': 0.3820380984612616, 'cosine_with_motion': 0.8037432185040205, 'motion_component': 0.3070605308484103, 'motion_component_percent': 80.37432185040205}, {'resid': 754, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 10.837307929992676, 'force': [0.019498976494413678, -0.1545420052645472, 0.028208621428201575], 'magnitude': 0.15830087744038762, 'cosine_with_motion': 0.845887996522876, 'motion_component': 0.13390481206586283, 'motion_component_percent': 84.5887996522876}, {'resid': 754, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 11.671006202697754, 'force': [-0.007629881870493557, 0.04095177628133637, -0.006538425761399013], 'magnitude': 0.04216650435347513, 'cosine_with_motion': -0.8164134865379614, 'motion_component': -0.03442530283433876, 'motion_component_percent': 81.64134865379614}, {'resid': 754, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 10.82571792602539, 'force': [-0.0024781757371516566, 0.04864537727604569, -0.005414056405201818], 'magnitude': 0.04900842878599289, 'cosine_with_motion': -0.8345422125169447, 'motion_component': -0.040899602591041626, 'motion_component_percent': 83.45422125169448}, {'resid': 754, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 11.212655067443848, 'force': [0.0015855354820513375, -0.034436666155207345, 0.010069537521670203], 'magnitude': 0.03591369494427399, 'cosine_with_motion': 0.9080653405618201, 'motion_component': 0.032611981630405476, 'motion_component_percent': 90.806534056182}, {'resid': 754, 'resname': 'GLU', 'atom': 'HG2', 'charge': -0.042500000447034836, 'distance': 12.176896095275879, 'force': [-0.0009403598246794613, 0.09201342173495762, -0.024249680114769013], 'magnitude': 0.09515987096273126, 'cosine_with_motion': -0.9067123320215187, 'motion_component': -0.08628262851548486, 'motion_component_percent': 90.67123320215187}, {'resid': 754, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 10.634336471557617, 'force': [0.004458908696948805, 0.11865479407829693, -0.038320050901991594], 'magnitude': 0.12476885959910831, 'cosine_with_motion': -0.9340728157675191, 'motion_component': -0.11654320000584135, 'motion_component_percent': 93.40728157675191}, {'resid': 754, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 11.621997833251953, 'force': [0.2385413308065054, -1.8170539303678428, 0.7486134167171752], 'magnitude': 1.9796487062246995, 'cosine_with_motion': 0.9166809809747454, 'motion_component': 1.814706318007443, 'motion_component_percent': 91.66809809747454}, {'resid': 754, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 12.0017671585083, 'force': [-0.4141816541740321, 1.713002373634799, -0.6750736462028799], 'magnitude': 1.887232895678338, 'cosine_with_motion': -0.8761403395267304, 'motion_component': -1.6534808699856336, 'motion_component_percent': 87.61403395267304}, {'resid': 754, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 11.942201614379883, 'force': [-0.1270231554132009, 1.6900292613512808, -0.8723001043739056], 'magnitude': 1.9061063082434329, 'cosine_with_motion': -0.9495236244807177, 'motion_component': -1.8098929704488644, 'motion_component_percent': 94.95236244807177}, {'resid': 754, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 8.353270530700684, 'force': [0.30543989332748156, -2.461480571889178, 0.6052879180993856], 'magnitude': 2.5531458238848925, 'cosine_with_motion': 0.8712693550107334, 'motion_component': 2.224477715224538, 'motion_component_percent': 87.12693550107335}, {'resid': 754, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 7.96753454208374, 'force': [-0.45030735202013866, 2.79134774704702, -1.125615330369201], 'magnitude': 3.043256286971248, 'cosine_with_motion': -0.9056323879191852, 'motion_component': -2.7560714582198447, 'motion_component_percent': 90.56323879191852}, {'resid': 1082, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 9.237896919250488, 'force': [0.640062175090208, -1.9037895140209915, -0.019755420320341995], 'magnitude': 2.0086025934239764, 'cosine_with_motion': 0.6734954907279983, 'motion_component': 1.352784789335611, 'motion_component_percent': 67.34954907279983}, {'resid': 1082, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 10.092041015625, 'force': [-0.27128931372324255, 0.9172813610324976, -0.030790602113582356], 'magnitude': 0.9570533152424561, 'cosine_with_motion': -0.7136025394482601, 'motion_component': -0.6829556761443929, 'motion_component_percent': 71.36025394482601}, {'resid': 1082, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 9.300192832946777, 'force': [-0.04970381876446747, 0.1417574042543397, 0.025609060425514665], 'magnitude': 0.1523858761059468, 'cosine_with_motion': -0.5661893298223963, 'motion_component': -0.08627925706682474, 'motion_component_percent': 56.618932982239635}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 9.226442337036133, 'force': [-0.18598069639100628, 0.3802566992213221, 0.08085890659054511], 'magnitude': 0.43095491586452195, 'cosine_with_motion': -0.4951536305462004, 'motion_component': -0.21338889119205037, 'motion_component_percent': 49.51536305462004}, {'resid': 1082, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 10.684876441955566, 'force': [-0.04860004689727895, 0.15179539893482324, 0.033410122881350826], 'magnitude': 0.16284975900242166, 'cosine_with_motion': -0.5518865465377355, 'motion_component': -0.089874591100349, 'motion_component_percent': 55.18865465377355}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 11.272326469421387, 'force': [0.016393923938443314, -0.04155159828833118, -0.0069223702919127515], 'magnitude': 0.04520193881762891, 'cosine_with_motion': 0.5585742818276466, 'motion_component': 0.025248640512274288, 'motion_component_percent': 55.85742818276466}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 10.886266708374023, 'force': [0.010128615976905573, -0.046636208847887266, -0.008444524069498263], 'magnitude': 0.048464779212039344, 'cosine_with_motion': 0.6122291832096453, 'motion_component': 0.029671552191422642, 'motion_component_percent': 61.222918320964524}, {'resid': 1082, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 11.298821449279785, 'force': [-0.01065056872855115, 0.03168807376972864, 0.011546769689354665], 'magnitude': 0.03536801554704979, 'cosine_with_motion': -0.45238875209945734, 'motion_component': -0.01600009241756406, 'motion_component_percent': 45.23887520994573}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HG2', 'charge': -0.042500000447034836, 'distance': 12.345236778259277, 'force': [0.026400027358840818, -0.08398398679952808, -0.02865689219787967], 'magnitude': 0.09258233607838888, 'cosine_with_motion': 0.47435986294668503, 'motion_component': 0.043917344253428484, 'motion_component_percent': 47.4359862946685}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 10.925708770751953, 'force': [0.026511376237927146, -0.10620712021538732, -0.04459930983760719], 'magnitude': 0.1182028083104016, 'cosine_with_motion': 0.4409016713416817, 'motion_component': 0.05211581574133649, 'motion_component_percent': 44.09016713416817}, {'resid': 1082, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 11.188331604003906, 'force': [-0.8643322615861431, 1.76327437505995, 0.8406324604037971], 'magnitude': 2.136087477994807, 'cosine_with_motion': -0.3363843670720284, 'motion_component': -0.7185464342957686, 'motion_component_percent': 33.63843670720284}, {'resid': 1082, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 11.417867660522461, 'force': [0.7961703531430833, -1.630325447769397, -1.0277032618509665], 'magnitude': 2.08519118818577, 'cosine_with_motion': 0.24913150549471666, 'motion_component': 0.5194868199570379, 'motion_component_percent': 24.913150549471666}, {'resid': 1082, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 10.864042282104492, 'force': [1.1457785455858753, -1.835077095177901, -0.790219585177079], 'magnitude': 2.303207201614497, 'cosine_with_motion': 0.32372826186379067, 'motion_component': 0.7456132640908264, 'motion_component_percent': 32.372826186379065}, {'resid': 1082, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 8.280838012695312, 'force': [-0.6166286793127616, 2.432890197594569, 0.6711554034733834], 'magnitude': 2.5980060079442198, 'cosine_with_motion': -0.5371397467327629, 'motion_component': -1.3954922891173547, 'motion_component_percent': 53.71397467327629}, {'resid': 1082, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 7.981538772583008, 'force': [0.8558458203541431, -2.6566229028419, -1.1859439504901177], 'magnitude': 3.0325864158875815, 'cosine_with_motion': 0.4031317650143247, 'motion_component': 1.2225319143952256, 'motion_component_percent': 40.313176501432466}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'N', 'charge': -0.38210001587867737, 'distance': 14.684907913208008, 'force': [-0.30644213551715715, -0.11022571176500491, -0.48989665726910636], 'magnitude': 0.5882645873736255, 'cosine_with_motion': -0.22773960081746153, 'motion_component': -0.1339711423035182, 'motion_component_percent': 22.773960081746154}, {'resid': 130, 'resname': 'ASN', 'atom': 'H', 'charge': 0.2681000232696533, 'distance': 14.24600601196289, 'force': [0.23787968384980446, 0.10511493125956785, 0.35315208378697116], 'magnitude': 0.4385798525300341, 'cosine_with_motion': 0.16610417526079466, 'motion_component': 0.07284994469050227, 'motion_component_percent': 16.610417526079466}, {'resid': 130, 'resname': 'ASN', 'atom': 'CA', 'charge': -0.20800000429153442, 'distance': 14.188486099243164, 'force': [-0.15423413002753417, -0.05139477448368572, -0.3020570741110674], 'magnitude': 0.34302779148360285, 'cosine_with_motion': -0.29991129734454913, 'motion_component': -0.10287790996908282, 'motion_component_percent': 29.991129734454912}, {'resid': 130, 'resname': 'ASN', 'atom': 'HA', 'charge': 0.13580000400543213, 'distance': 13.974637985229492, 'force': [0.10831773436847286, 0.017658745993615284, 0.2031101781918267], 'magnitude': 0.2308642617944615, 'cosine_with_motion': 0.3530754919193582, 'motion_component': 0.081512512799679, 'motion_component_percent': 35.30754919193582}, {'resid': 130, 'resname': 'ASN', 'atom': 'CB', 'charge': -0.22990000247955322, 'distance': 12.925453186035156, 'force': [-0.1861232680291697, -0.08699308889144941, -0.4080609141118241], 'magnitude': 0.45686253735944604, 'cosine_with_motion': -0.28412097737633535, 'motion_component': -0.12980423064119834, 'motion_component_percent': 28.412097737633534}, {'resid': 130, 'resname': 'ASN', 'atom': 'HB2', 'charge': 0.1023000031709671, 'distance': 12.56251335144043, 'force': [0.09778635239443796, 0.05267624509293006, 0.18433124237497492], 'magnitude': 0.21520911789977995, 'cosine_with_motion': 0.21025978284650274, 'motion_component': 0.045249822396195134, 'motion_component_percent': 21.025978284650275}, {'resid': 130, 'resname': 'ASN', 'atom': 'HB3', 'charge': 0.1023000031709671, 'distance': 13.134596824645996, 'force': [0.06662754984135619, 0.04541128913888128, 0.1796009563035756], 'magnitude': 0.19687031031690977, 'cosine_with_motion': 0.27793528114287375, 'motion_component': 0.05471720504661512, 'motion_component_percent': 27.793528114287376}, {'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 11.912529945373535, 'force': [0.6746663872208002, 0.17444830040496992, 1.5214794702745347], 'magnitude': 1.6734714583842258, 'cosine_with_motion': 0.3620918571384696, 'motion_component': 0.6059503882345675, 'motion_component_percent': 36.209185713846956}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 11.88822078704834, 'force': [-0.4486495881478735, -0.08022210395112599, -1.3362295415201246], 'magnitude': 1.411818482149417, 'cosine_with_motion': -0.4388704722622673, 'motion_component': -0.619605444009512, 'motion_component_percent': 43.88704722622673}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 11.185317039489746, 'force': [-1.1751523878380365, -0.1618621204225067, -2.0984839334914787], 'magnitude': 2.410563689221046, 'cosine_with_motion': -0.3512334459234674, 'motion_component': -0.8466705911830942, 'motion_component_percent': 35.12334459234674}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 10.613048553466797, 'force': [0.585774431568365, -0.010270227239874282, 1.0737964217356821], 'magnitude': 1.223223576284873, 'cosine_with_motion': 0.41670883947462156, 'motion_component': 0.5097280768916657, 'motion_component_percent': 41.67088394746216}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 11.333580017089844, 'force': [0.5901923424335399, 0.12089531068814861, 0.8874698785295475], 'magnitude': 1.0726348225331968, 'cosine_with_motion': 0.27722696877265307, 'motion_component': 0.2973633004508708, 'motion_component_percent': 27.722696877265307}, {'resid': 458, 'resname': 'ASN', 'atom': 'N', 'charge': -0.38210001587867737, 'distance': 14.79377269744873, 'force': [0.4290003775642042, 0.01866155446265605, -0.38934724811130267], 'magnitude': 0.5796385573588395, 'cosine_with_motion': -0.5699644348361221, 'motion_component': -0.3303733627542561, 'motion_component_percent': 56.99644348361221}, {'resid': 458, 'resname': 'ASN', 'atom': 'H', 'charge': 0.2681000232696533, 'distance': 14.367311477661133, 'force': [-0.3214784333264229, -0.04037269739114818, 0.28453392949926365], 'magnitude': 0.4312051655823948, 'cosine_with_motion': 0.6125415828296222, 'motion_component': 0.26413109465014944, 'motion_component_percent': 61.25415828296222}, {'resid': 458, 'resname': 'ASN', 'atom': 'CA', 'charge': -0.20800000429153442, 'distance': 14.033319473266602, 'force': [0.2500669019855908, -0.016809727054512044, -0.24524118244888293], 'magnitude': 0.35065547188265084, 'cosine_with_motion': -0.5173701621052531, 'motion_component': -0.1814186783310211, 'motion_component_percent': 51.73701621052531}, {'resid': 458, 'resname': 'ASN', 'atom': 'HA', 'charge': 0.13580000400543213, 'distance': 14.483201026916504, 'force': [-0.15858570636880845, 0.02243098501170631, 0.1433346466337386], 'magnitude': 0.2149357957128315, 'cosine_with_motion': 0.459243820513455, 'motion_component': 0.09870793598826022, 'motion_component_percent': 45.9243820513455}, {'resid': 458, 'resname': 'ASN', 'atom': 'CB', 'charge': -0.22990000247955322, 'distance': 12.548372268676758, 'force': [0.3508086830985685, -0.012479048351910427, -0.33428022551578424], 'magnitude': 0.48473263553840146, 'cosine_with_motion': -0.5313656101831223, 'motion_component': -0.2575702526585357, 'motion_component_percent': 53.136561018312236}, {'resid': 458, 'resname': 'ASN', 'atom': 'HB2', 'charge': 0.1023000031709671, 'distance': 12.475196838378906, 'force': [-0.1704195073329009, 0.005147275871981465, 0.13622043088486224], 'magnitude': 0.21823223574657452, 'cosine_with_motion': 0.5069880608996924, 'motion_component': 0.11064113802696035, 'motion_component_percent': 50.69880608996924}, {'resid': 458, 'resname': 'ASN', 'atom': 'HB3', 'charge': 0.1023000031709671, 'distance': 12.34305191040039, 'force': [-0.15557571498640452, -0.011702725725303715, 0.1592389384967529], 'magnitude': 0.22293002582986732, 'cosine_with_motion': 0.6018670749716485, 'motion_component': 0.13417424256957627, 'motion_component_percent': 60.186707497164846}, {'resid': 458, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 11.720748901367188, 'force': [-1.1895035215348462, 0.20657456001908733, 1.2372373326545885], 'magnitude': 1.7286838617587428, 'cosine_with_motion': 0.4653348327009306, 'motion_component': 0.8044168156043032, 'motion_component_percent': 46.533483270093065}, {'resid': 458, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 11.923039436340332, 'force': [0.999869171817543, -0.29534140561038524, -0.9397259663966543], 'magnitude': 1.4035846246447496, 'cosine_with_motion': -0.3720304516010255, 'motion_component': -0.5221762217668421, 'motion_component_percent': 37.20304516010255}, {'resid': 458, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 11.022150993347168, 'force': [1.5473385791036198, -0.24580689072078693, -1.9256001718828981], 'magnitude': 2.4824612238388895, 'cosine_with_motion': -0.5027738810925133, 'motion_component': -1.2481166641711487, 'motion_component_percent': 50.27738810925133}, {'resid': 458, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 10.725323677062988, 'force': [-0.6925487711609511, 0.2064081033299143, 0.9551814708873327], 'magnitude': 1.1977477814144697, 'cosine_with_motion': 0.44835283171719936, 'motion_component': 0.5370136094801706, 'motion_component_percent': 44.83528317171994}, {'resid': 458, 'resname':</t>
+          <t>{22: {'frame': 22, 'motion_vector': [-0.09092330932617188, 0.05826568603515625, -1.2532577514648438], 'motion_vector_magnitude': 1.2579017877578735, 'ionic_force': [6.5744180381298065, -0.26533934473991394, -25.52590274810791], 'ionic_force_magnitude': 26.360293788457984, 'radial_force': 6.5797703233436335, 'axial_force': -25.52590274810791, 'glu_force': [0.24643235304392874, -0.21714882948435843, -1.6785882906988263], 'glu_force_magnitude': 1.710421342372809, 'asn_force': [-0.4506613213743549, -0.1643859190535295, -0.9087930917739868], 'asn_force_magnitude': 1.0276299142308358, 'sf_force': [-7.750800419051302, -1.4640836735234188, 11.466914477292448], 'sf_force_magnitude': 13.91792282521292, 'residue_force': [-7.955029387381728, -1.8456184220613068, 8.879533094819635], 'residue_force_magnitude': 12.06378497387765, 'pip2_force': [0.1236323150806129, -0.0426108087413013, -4.306657396700757], 'pip2_force_magnitude': 4.308642310857461, 'total_force': [-1.2569790341713087, -2.153568575542522, -20.953027049989032], 'total_force_magnitude': 21.100881414279417, 'cosine_total_motion': 0.9889053347173746, 'cosine_glu_motion': 0.9614708474229864, 'cosine_asn_motion': 0.9053825309501597, 'cosine_sf_motion': -0.7854731289055279, 'cosine_residue_motion': -0.6927540549963435, 'cosine_pip2_motion': 0.9933169686312892, 'cosine_ionic_motion': 0.9462778692118305, 'motion_component_total': 20.866774197819616, 'motion_component_glu': 1.6445202575015465, 'motion_component_asn': 0.9303981726264097, 'motion_component_sf': -10.932154389385657, 'motion_component_residue': -8.3572359592577, 'motion_component_ionic': 24.944162637939872, 'motion_component_pip2': 4.279847519137446, 'motion_component_percent_total': 98.89053347173746, 'motion_component_percent_glu': 96.14708474229865, 'motion_component_percent_asn': 90.53825309501597, 'motion_component_percent_sf': 78.54731289055279, 'motion_component_percent_residue': 69.27540549963435, 'motion_component_percent_ionic': 94.62778692118306, 'motion_component_percent_pip2': 99.33169686312891, 'ionic_contributions': [{'ion_id': 2397, 'distance': 7.159240245819092, 'force': [0.39101096987724304, 0.3432261049747467, -6.456523418426514], 'magnitude': 6.477452278137207, 'cosine_ionic_motion': 0.9911800622940063, 'motion_component_ionic': 6.420321464538574, 'motion_component_percent_ionic': 99.11800622940063}, {'ion_id': 2398, 'distance': 3.4814634323120117, 'force': [3.909102201461792, 1.8690134286880493, -27.046537399291992], 'magnitude': 27.39141273498535, 'cosine_ionic_motion': 0.9766089916229248, 'motion_component_ionic': 26.750699996948242, 'motion_component_percent_ionic': 97.66089916229248}, {'ion_id': 2400, 'distance': 6.192728519439697, 'force': [2.2743048667907715, -2.47757887840271, 7.977158069610596], 'magnitude': 8.657130241394043, 'cosine_ionic_motion': -0.9502986669540405, 'motion_component_ionic': -8.226859092712402, 'motion_component_percent_ionic': 95.02986669540405}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 10.259893417358398, 'force': [-1.5550671815872192, -0.37449002265930176, -0.30517250299453735], 'magnitude': 1.62837553024292, 'cosine_with_motion': 0.24509240686893463, 'motion_component': 0.39910247921943665, 'motion_component_percent': 24.509240686893463}, {'resid': 98, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 11.070900917053223, 'force': [0.7671473622322083, 0.18164736032485962, 0.10480011999607086], 'magnitude': 0.7952948808670044, 'cosine_with_motion': -0.190432608127594, 'motion_component': -0.15145008265972137, 'motion_component_percent': 19.0432608127594}, {'resid': 98, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 10.517801284790039, 'force': [0.1101216971874237, 0.024930883198976517, 0.03804450109601021], 'magnitude': 0.11914580315351486, 'cosine_with_motion': -0.37524643540382385, 'motion_component': -0.044709037989377975, 'motion_component_percent': 37.524643540382385}, {'resid': 98, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 10.685016632080078, 'force': [0.28457242250442505, 0.09456046670675278, 0.11545214802026749], 'magnitude': 0.3213290274143219, 'cosine_with_motion': -0.40835174918174744, 'motion_component': -0.13121527433395386, 'motion_component_percent': 40.835174918174744}, {'resid': 98, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 11.92063045501709, 'force': [0.12191712111234665, 0.02074405364692211, 0.04270824417471886], 'magnitude': 0.1308361291885376, 'cosine_with_motion': -0.3852306604385376, 'motion_component': -0.050402089953422546, 'motion_component_percent': 38.52306604385376}, {'resid': 98, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 12.084959030151367, 'force': [-0.03770368546247482, -0.003788614645600319, -0.010522007942199707], 'magnitude': 0.03932727128267288, 'cosine_with_motion': 0.33139756321907043, 'motion_component': 0.013032961636781693, 'motion_component_percent': 33.13975632190704}, {'resid': 98, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 12.091750144958496, 'force': [-0.03574266657233238, -0.0043841260485351086, -0.015697259455919266], 'magnitude': 0.039283111691474915, 'cosine_with_motion': 0.45871561765670776, 'motion_component': 0.018019776791334152, 'motion_component_percent': 45.871561765670776}, {'resid': 98, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 13.063215255737305, 'force': [0.024476906284689903, 0.006167897954583168, 0.007932701148092747], 'magnitude': 0.026459207758307457, 'cosine_with_motion': -0.3547707200050354, 'motion_component': -0.00938695203512907, 'motion_component_percent': 35.47707200050354}, {'resid': 98, 'resname': 'GLU', 'atom': 'HG2', 'charge': -0.042500000447034836, 'distance': 13.937634468078613, 'force': [-0.06687988340854645, -0.014543809927999973, -0.02432023547589779], 'magnitude': 0.07263549417257309, 'cosine_with_motion': 0.390869140625, 'motion_component': 0.028390973806381226, 'motion_component_percent': 39.0869140625}, {'resid': 98, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 12.936001777648926, 'force': [-0.07529959827661514, -0.02548573724925518, -0.028110278770327568], 'magnitude': 0.08431927859783173, 'cosine_with_motion': 0.3826976418495178, 'motion_component': 0.032268788665533066, 'motion_component_percent': 38.26976418495178}, {'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 13.380605697631836, 'force': [1.420825481414795, 0.36585378646850586, 0.27906206250190735], 'magnitude': 1.4934756755828857, 'cosine_with_motion': -0.24358299374580383, 'motion_component': -0.3637852668762207, 'motion_component_percent': 24.358299374580383}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 14.372241973876953, 'force': [-1.2734720706939697, -0.2569155693054199, -0.21025389432907104], 'magnitude': 1.3160332441329956, 'cosine_with_motion': 0.2200751006603241, 'motion_component': 0.2896261513233185, 'motion_component_percent': 22.00751006603241}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 12.73697566986084, 'force': [-1.5835905075073242, -0.5063105821609497, -0.20903004705905914], 'magnitude': 1.6756500005722046, 'cosine_with_motion': 0.17859983444213867, 'motion_component': 0.2992708086967468, 'motion_component_percent': 17.859983444213867}, {'resid': 98, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 9.7052001953125, 'force': [1.725627064704895, 0.20717233419418335, 0.7460728883743286], 'magnitude': 1.8913841247558594, 'cosine_with_motion': -0.4538758397102356, 'motion_component': -0.8584535717964172, 'motion_component_percent': 45.38758397102356}, {'resid': 98, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 9.921347618103027, 'force': [-1.6802805662155151, -0.21824903786182404, -0.9904846549034119], 'magnitude': 1.962660312652588, 'cosine_with_motion': 0.5595324635505676, 'motion_component': 1.0981721878051758, 'motion_component_percent': 55.95324635505676}, {'resid': 426, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 9.677720069885254, 'force': [1.8184871673583984, 0.1168493926525116, -0.1703360378742218], 'magnitude': 1.830181360244751, 'cosine_with_motion': 0.023864420130848885, 'motion_component': 0.043676216155290604, 'motion_component_percent': 2.3864420130848885}, {'resid': 426, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 10.437810897827148, 'force': [-0.8927213549613953, -0.05422597378492355, 0.02425236999988556], 'magnitude': 0.894695520401001, 'cosine_with_motion': 0.042308107018470764, 'motion_component': 0.03785287216305733, 'motion_component_percent': 4.230810701847076}, {'resid': 426, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 10.169393539428711, 'force': [-0.12390588223934174, -0.005480889696627855, 0.029337577521800995], 'magnitude': 0.12744960188865662, 'cosine_with_motion': -0.16105981171131134, 'motion_component': -0.020527008920907974, 'motion_component_percent': 16.105981171131134}, {'resid': 426, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 10.254905700683594, 'force': [-0.332694411277771, -0.049444474279880524, 0.0925474762916565], 'magnitude': 0.3488486111164093, 'cosine_with_motion': -0.20194528996944427, 'motion_component': -0.07044833153486252, 'motion_component_percent': 20.194528996944427}, {'resid': 426, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 11.673710823059082, 'force': [-0.13345563411712646, -0.0015557329170405865, 0.02828744612634182], 'magnitude': 0.13642948865890503, 'cosine_with_motion': -0.13639770448207855, 'motion_component': -0.018608668819069862, 'motion_component_percent': 13.639770448207855}, {'resid': 426, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 11.62518310546875, 'force': [0.04211048409342766, -0.0016398223815485835, -0.005498345009982586], 'magnitude': 0.04249957203865051, 'cosine_with_motion': 0.05548928305506706, 'motion_component': 0.0023582708090543747, 'motion_component_percent': 5.548928305506706}, {'resid': 426, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 12.136310577392578, 'force': [0.03753471374511719, -0.001689799246378243, -0.01043615024536848], 'magnitude': 0.0389951691031456, 'cosine_with_motion': 0.19505687057971954, 'motion_component': 0.007606275379657745, 'motion_component_percent': 19.505687057971954}, {'resid': 426, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 12.651860237121582, 'force': [-0.027588170021772385, -0.0029161067213863134, 0.00510544516146183], 'magnitude': 0.02820773608982563, 'cosine_with_motion': -0.11442069709300995, 'motion_component': -0.0032275489065796137, 'motion_component_percent': 11.442069709300995}, {'resid': 426, 'resname': 'GLU', 'atom': 'HG2', 'charge': -0.042500000447034836, 'distance': 13.657156944274902, 'force': [0.07441750168800354, 0.005930183455348015, -0.01223619095981121], 'magnitude': 0.07564955949783325, 'cosine_with_motion': 0.09367768466472626, 'motion_component': 0.007086675614118576, 'motion_component_percent': 9.367768466472626}, {'resid': 426, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 12.784294128417969, 'force': [0.08260209113359451, 0.012219898402690887, -0.021928085014224052], 'magnitude': 0.08633233606815338, 'cosine_with_motion': 0.19045621156692505, 'motion_component': 0.01644252985715866, 'motion_component_percent': 19.045621156692505}, {'resid': 426, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 12.368709564208984, 'force': [-1.7100279331207275, -0.3214007019996643, 0.16565079987049103], 'magnitude': 1.747836947441101, 'cosine_with_motion': -0.032224204391241074, 'motion_component': -0.05632265657186508, 'motion_component_percent': 3.2224204391241074}, {'resid': 426, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 11.91867733001709, 'force': [1.8278578519821167, 0.5160877704620361, -0.23366473615169525], 'magnitude': 1.9136378765106201, 'cosine_with_motion': 0.06510448455810547, 'motion_component': 0.12458640336990356, 'motion_component_percent': 6.510448455810547}, {'resid': 426, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 12.830193519592285, 'force': [1.62895667552948, 0.2705068588256836, -0.02033010497689247], 'magnitude': 1.651389479637146, 'cosine_with_motion': -0.05144694447517395, 'motion_component': -0.08495894074440002, 'motion_component_percent': 5.144694447517395}, {'resid': 426, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 9.527647972106934, 'force': [-1.8546605110168457, 0.13289691507816315, 0.6277855634689331], 'magnitude': 1.9625345468521118, 'cosine_with_motion': -0.24725884199142456, 'motion_component': -0.4852540194988251, 'motion_component_percent': 24.725884199142456}, {'resid': 426, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 10.042847633361816, 'force': [1.7306723594665527, -0.13477832078933716, -0.8096842169761658], 'magnitude': 1.91545832157135, 'cosine_with_motion': 0.3525819480419159, 'motion_component': 0.6753560304641724, 'motion_component_percent': 35.25819480419159}, {'resid': 754, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 9.752018928527832, 'force': [-0.4479050636291504, 1.7362650632858276, -0.182782843708992], 'magnitude': 1.802399754524231, 'cosine_with_motion': 0.16361893713474274, 'motion_component': 0.29490673542022705, 'motion_component_percent': 16.361893713474274}, {'resid': 754, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 10.47778606414795, 'force': [0.20199252665042877, -0.8640119433403015, 0.03187878802418709], 'magnitude': 0.8878816962242126, 'cosine_with_motion': -0.0972902923822403, 'motion_component': -0.08638226985931396, 'motion_component_percent': 9.72902923822403}, {'resid': 754, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 10.164956092834473, 'force': [0.027237044647336006, -0.12084148079156876, 0.030451005324721336], 'magnitude': 0.12756091356277466, 'cosine_with_motion': -0.29714956879615784, 'motion_component': -0.03790466859936714, 'motion_component_percent': 29.714956879615784}, {'resid': 754, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 10.299296379089355, 'force': [0.10238586366176605, -0.3144521713256836, 0.10123145580291748], 'magnitude': 0.345848023891449, 'cosine_with_motion': -0.35513776540756226, 'motion_component': -0.12282369285821915, 'motion_component_percent': 35.513776540756226}, {'resid': 754, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 11.59725570678711, 'force': [0.02280838042497635, -0.132862389087677, 0.030595265328884125], 'magnitude': 0.1382342427968979, 'cosine_with_motion': -0.27695807814598083, 'motion_component': -0.038285091519355774, 'motion_component_percent': 27.695807814598083}, {'resid': 754, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 11.716341018676758, 'force': [-0.004938559141010046, 0.04110904783010483, -0.00602585356682539], 'magnitude': 0.0418408177793026, 'cosine_with_motion': 0.19752803444862366, 'motion_component': 0.008264734409749508, 'motion_component_percent': 19.752803444862366}, {'resid': 754, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 11.944050788879395, 'force': [-0.004508707206696272, 0.03825994208455086, -0.01169483084231615], 'magnitude': 0.04026065766811371, 'cosine_with_motion': 0.3415181040763855, 'motion_component': 0.0137497428804636, 'motion_component_percent': 34.15181040763855}, {'resid': 754, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 12.53586483001709, 'force': [0.007451019715517759, -0.027046265080571175, 0.006206396501511335], 'magnitude': 0.028732167556881905, 'cosine_with_motion': -0.2775576114654541, 'motion_component': -0.007974831387400627, 'motion_component_percent': 27.75576114654541}, {'resid': 754, 'resname': 'GLU', 'atom': 'HG2', 'charge': -0.042500000447034836, 'distance': 12.424324035644531, 'force': [-0.027572808787226677, 0.08316387981176376, -0.02605431154370308], 'magnitude': 0.0914074257016182, 'cosine_with_motion': 0.34792864322662354, 'motion_component': 0.03180326148867607, 'motion_component_percent': 34.79286432266235}, {'resid': 754, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 12.260150909423828, 'force': [-0.029835881665349007, 0.08781393617391586, -0.014507132582366467], 'magnitude': 0.09387185424566269, 'cosine_with_motion': 0.2202756106853485, 'motion_component': 0.020677680149674416, 'motion_component_percent': 22.02756106853485}, {'resid': 754, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 13.978999137878418, 'force': [0.3157138228416443, -1.3010077476501465, 0.28299859166145325], 'magnitude': 1.3683509826660156, 'cosine_with_motion': -0.2667710781097412, 'motion_component': -0.3650364577770233, 'motion_component_percent': 26.67710781097412}, {'resid': 754, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 14.594219207763672, 'force': [-0.30858156085014343, 1.227165699005127, -0.16671541333198547], 'magnitude': 1.2763041257858276, 'cosine_with_motion': 0.19215382635593414, 'motion_component': 0.24524672329425812, 'motion_component_percent': 19.215382635593414}, {'resid': 754, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 14.535812377929688, 'force': [-0.23068764805793762, 1.2170701026916504, -0.3475847840309143], 'magnitude': 1.2865813970565796, 'cosine_with_motion': 0.3259415924549103, 'motion_component': 0.41935038566589355, 'motion_component_percent': 32.59415924549103}, {'resid': 754, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 9.395806312561035, 'force': [0.19125574827194214, -1.9009093046188354, 0.6498300433158875], 'magnitude': 2.0179975032806396, 'cosine_with_motion': -0.37131109833717346, 'motion_component': -0.7493048906326294, 'motion_component_percent': 37.131109833717346}, {'resid': 754, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 9.543281555175781, 'force': [-0.19119085371494293, 1.8940852880477905, -0.9357186555862427], 'magnitude': 2.1212453842163086, 'cosine_with_motion': 0.48736336827278137, 'motion_component': 1.0338172912597656, 'motion_component_percent': 48.73633682727814}, {'resid': 1082, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 10.069339752197266, 'force': [0.1289844661951065, -1.6573456525802612, -0.30767178535461426], 'magnitude': 1.6905897855758667, 'cosine_with_motion': 0.13039523363113403, 'motion_component': 0.22044485807418823, 'motion_component_percent': 13.039523363113403}, {'resid': 1082, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 10.771077156066895, 'force': [-0.049382418394088745, 0.8331094980239868, 0.09697292000055313], 'magnitude': 0.8401867747306824, 'cosine_with_motion': -0.06481420993804932, 'motion_component': -0.054456040263175964, 'motion_component_percent': 6.481420993804932}, {'resid': 1082, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 10.62839412689209, 'force': [-0.008032741025090218, 0.11067705601453781, 0.036056771874427795], 'magnitude': 0.11667916178703308, 'cosine_with_motion': -0.25897082686424255, 'motion_component': -0.030216500163078308, 'motion_component_percent': 25.897082686424255}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 10.506852149963379, 'force': [-0.05304539203643799, 0.3068259060382843, 0.1161031574010849], 'magnitude': 0.3323189616203308, 'cosine_with_motion': -0.2937786281108856, 'motion_component': -0.09762820601463318, 'motion_component_percent': 29.377862811088562}, {'resid': 1082, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 12.113763809204102, 'force': [-0.004875390790402889, 0.12059126794338226, 0.038551561534404755], 'magnitude': 0.12669746577739716, 'cosine_with_motion': -0.2562882900238037, 'motion_component': -0.032471075654029846, 'motion_component_percent': 25.62882900238037}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 12.351288795471191, 'force': [-0.0009505013003945351, -0.03646562248468399, -0.009318940341472626], 'magnitude': 0.03764953836798668, 'cosine_with_motion': 0.20356588065624237, 'motion_component': 0.007664161268621683, 'motion_component_percent': 20.356588065624237}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 12.371161460876465, 'force': [0.0004138073418289423, -0.03468673303723335, -0.01431993953883648], 'magnitude': 0.03752867504954338, 'cosine_with_motion': 0.3365554213523865, 'motion_component': 0.012630479410290718, 'motion_component_percent': 33.65554213523865}, {'resid': 1082, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 13.074196815490723, 'force': [-0.003510561306029558, 0.025123856961727142, 0.007362626027315855], 'magnitude': 0.02641477808356285, 'cosine_with_motion': -0.22403989732265472, 'motion_component': -0.0059179640375077724, 'motion_component_percent': 22.403989732265472}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HG2', 'charge': -0.042500000447034836, 'distance': 14.055633544921875, 'force': [0.007848832756280899, -0.06757277250289917, -0.021755019202828407], 'magnitude': 0.07142103463411331, 'cosine_with_motion': 0.2517104744911194, 'motion_component': 0.01797742210328579, 'motion_component_percent': 25.17104744911194}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 12.821313858032227, 'force': [0.017410485073924065, -0.07960738241672516, -0.02696487121284008], 'magnitude': 0.08583451807498932, 'cosine_with_motion': 0.2553688883781433, 'motion_component': 0.02191946469247341, 'motion_component_percent': 25.53688883781433}, {'resid': 1082, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 13.314204216003418, 'force': [-0.23572281002998352, 1.468443751335144, 0.2518085241317749], 'magnitude': 1.5084097385406494, 'cosine_with_motion': -0.10993198305368423, 'motion_component': -0.16582247614860535, 'motion_component_percent': 10.993198305368423}, {'resid': 1082, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 12.47976303100586, 'force': [0.3679676651954651, -1.6936020851135254, -0.20700021088123322], 'magnitude': 1.7454333305358887, 'cosine_with_motion': 0.05797497183084488, 'motion_component': 0.101191446185112, 'motion_component_percent': 5.797497183084488}, {'resid': 1082, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 14.301231384277344, 'force': [0.15820501744747162, -1.3074817657470703, -0.17905861139297485], 'magnitude': 1.3291348218917847, 'cosine_with_motion': 0.08005206286907196, 'motion_component': 0.10639998316764832, 'motion_component_percent': 8.005206286907196}, {'resid': 1082, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 9.969731330871582, 'force': [0.06649257242679596, 1.6492999792099, 0.6984930038452148], 'magnitude': 1.7923460006713867, 'cosine_with_motion': -0.34832853078842163, 'motion_component': -0.6243252754211426, 'motion_component_percent': 34.83285307884216}, {'resid': 1082, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 10.619867324829102, 'force': [-0.08323084563016891, -1.4965282678604126, -0.8292897939682007], 'magnitude': 1.7129640579223633, 'cosine_with_motion': 0.4453831911087036, 'motion_component': 0.762925386428833, 'motion_component_percent': 44.53831911087036}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'N', 'charge': -0.38210001587867737, 'distance': 13.965925216674805, 'force': [-0.413442999124527, -0.06467059254646301, -0.4978889226913452], 'magnitude': 0.6503927707672119, 'cosine_with_motion': 0.8040366172790527, 'motion_component': 0.5229396224021912, 'motion_component_percent': 80.40366172790527}, {'resid': 130, 'resname': 'ASN', 'atom': 'H', 'charge': 0.2681000232696533, 'distance': 13.678962707519531, 'force': [0.30568012595176697, 0.07937788963317871, 0.3557310104370117], 'magnitude': 0.47569501399993896, 'cosine_with_motion': -0.7837710976600647, 'motion_component': -0.37283599376678467, 'motion_component_percent': 78.37710976600647}, {'resid': 130, 'resname': 'ASN', 'atom': 'CA', 'charge': -0.20800000429153442, 'distance': 13.30413818359375, 'force': [-0.22528241574764252, -0.01797800324857235, -0.3180237114429474], 'magnitude': 0.3901467025279999, 'cosine_with_motion': 0.851732611656189, 'motion_component': 0.33230066299438477, 'motion_component_percent': 85.1732611656189}, {'resid': 130, 'resname': 'ASN', 'atom': 'HA', 'charge': 0.13580000400543213, 'distance': 13.400580406188965, 'force': [0.14959393441677094, -0.008060376159846783, 0.20147360861301422], 'magnitude': 0.251067578792572, 'cosine_with_motion': -0.8440597653388977, 'motion_component': -0.21191604435443878, 'motion_component_percent': 84.40597653388977}, {'resid': 130, 'resname': 'ASN', 'atom': 'CB', 'charge': -0.22990000247955322, 'distance': 11.873865127563477, 'force': [-0.3048804700374603, -0.0454896055161953, -0.4450373649597168], 'magnitude': 0.541368305683136, 'cosine_with_motion': 0.8558397889137268, 'motion_component': 0.46332454681396484, 'motion_component_percent': 85.58397889137268}, {'resid': 130, 'resname': 'ASN', 'atom': 'HB2', 'charge': 0.1023000031709671, 'distance': 11.914814949035645, 'force': [0.13471609354019165, 0.04174308106303215, 0.1932518482208252], 'magnitude': 0.23924295604228973, 'cosine_with_motion': -0.837401270866394, 'motion_component': -0.2003423571586609, 'motion_component_percent': 83.7401270866394}, {'resid': 130, 'resname': 'ASN', 'atom': 'HB3', 'charge': 0.1023000031709671, 'distance': 11.595357894897461, 'force': [0.12361445277929306, 0.01647518016397953, 0.21967780590057373], 'magnitude': 0.2526070177555084, 'cosine_with_motion': -0.8987823128700256, 'motion_component': -0.22703872621059418, 'motion_component_percent': 89.87823128700256}, {'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 10.949317932128906, 'force': [1.2640738487243652, 0.0774819478392601, 1.5231189727783203], 'magnitude': 1.980852723121643, 'cosine_with_motion': -0.8103965520858765, 'motion_component': -1.6052762269973755, 'motion_component_percent': 81.03965520858765}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 10.482000350952148, 'force': [-1.1532378196716309, 0.1201118603348732, -1.3977118730545044], 'magnitude': 1.8160349130630493, 'cosine_with_motion': 0.8157735466957092, 'motion_component': 1.4814732074737549, 'motion_component_percent': 81.57735466957092}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 10.960309982299805, 'force': [-1.7829086780548096, -0.24083907902240753, -1.7510321140289307], 'magnitude': 2.5105538368225098, 'cosine_with_motion': 0.7417819499969482, 'motion_component': 1.8622835874557495, 'motion_component_percent': 74.17819499969482}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 10.371204376220703, 'force': [0.9746187925338745, 0.09169557690620422, 0.8261417150497437], 'magnitude': 1.2809371948242188, 'cosine_with_motion': -0.6942507028579712, 'motion_component': -0.889291524887085, 'motion_component_percent': 69.42507028579712}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 11.554563522338867, 'force': [0.7310255169868469, 0.17287655174732208, 0.7076272368431091], 'magnitude': 1.0319985151290894, 'cosine_with_motion': -0.7265968918800354, 'motion_component': -0.7498469352722168, 'motion_component_percent': 72.65968918800354}, {'resid': 130, 'resname': 'ASN', 'atom': 'C', 'charge': 0.8050000071525574, 'distance': 14.212565422058105, 'force': [0.6673703789710999, 0.06811437755823135, 1.1404128074645996], 'magnitude': 1.3230888843536377, 'cosine_with_motion': -0.8928244709968567, 'motion_component': -1.181286096572876, 'motion_component_percent': 89.28244709968567}, {'resid': 130, 'resname': 'ASN', 'atom': 'O', 'charge': -0.8147000074386597, 'distance': 14.417845726013184, 'force': [-0.6065304279327393, 0.027472812682390213, -1.1508333683013916], 'magnitude': 1.3011730909347534, 'cosine_with_motion': 0.9158644676208496, 'motion_component': 1.1916981935501099, 'motion_component_percent': 91.58644676208496}, {'resid': 458, 'resname': 'ASN', 'atom': 'N', 'charge': -0.38210001587867737, 'distance': 13.106000900268555, 'force': [0.4963540732860565, 2.9235028705443256e-05, -0.5468782186508179], 'magnitude': 0.7385412454605103, 'cosine_with_motion': 0.689173698425293, 'motion_component': 0.5089831948280334, 'motion_component_percent': 68.9173698425293}, {'resid': 458, 'resname': 'ASN', 'atom': 'H', 'charge': 0.2681000232696533, 'distance': 12.509195327758789, 'force': [-0.3960816264152527, -0.030386904254555702, 0.40712910890579224], 'magnitude': 0.5688216686248779, 'cosine_with_motion': -0.6652420163154602, 'motion_component': -0.37840408086776733, 'motion_component_percent': 66.52420163154602}, {'resid': 458, 'resname': 'ASN', 'atom': 'CA', 'charge': -0.20800000429153442, 'distance': 12.638148307800293, 'force': [0.2631179094314575, -0.03182939067482948, -0.3415868878364563], 'magnitude': 0.4323491156101227, 'cosine_with_motion': 0.7397559285163879, 'motion_component': 0.31983283162117004, 'motion_component_percent': 73.9755928516388}, {'resid': 458, 'resname': 'ASN', 'atom': 'HA', 'charge': 0.13580000400543213, 'distance': 13.054707527160645, 'force': [-0.16317276656627655, 0.039592135697603226, 0.20443201065063477], 'magnitude': 0.2645474076271057, 'cosine_with_motion': -0.7183928489685059, 'motion_component': -0.1900489628314972, 'motion_component_percent': 71.83928489685059}, {'resid': 458, 'resname': 'ASN', 'atom': 'CB', 'charge': -0.22990000247955322, 'distance': 11.111639976501465, 'force': [0.371440589427948, -0.05059197172522545, -0.4915578067302704], 'magnitude': 0.6181882619857788, 'cosine_with_motion': 0.7450016140937805, 'motion_component': 0.46055126190185547, 'motion_component_percent': 74.50016140937805}, {'resid': 458, 'resname': 'ASN', 'atom': 'HB2', 'charge': 0.1023000031709671, 'distance': 10.69054126739502, 'force': [-0.17045173048973083, -0.0008763246587477624, 0.24343226850032806], 'magnitude': 0.29717642068862915, 'cosine_with_motion': -0.7748043537139893, 'motion_component': -0.23025357723236084, 'motion_component_percent': 77.48043537139893}, {'resid': 458, 'resname': 'ASN', 'atom': 'HB3', 'charge': 0.1023000031709671, 'distance': 10.949666976928711, 'force': [-0.15308403968811035, 0.04288681596517563, 0.23446126282215118], 'magnitude': 0.28327739238739014, 'cosine_with_motion': -0.7785441875457764, 'motion_component': -0.2205439656972885, 'motion_component_percent': 77.85441875457764}, {'resid': 458, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 10.679563522338867, 'force': [-1.4356496334075928, 0.2777125835418701, 1.4823228120803833], 'magnitude': 2.0821850299835205, 'cosine_with_motion': -0.6532633900642395, 'motion_component': -1.3602153062820435, 'motion_component_percent': 65.32633900642395}, {'resid': 458, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 11.214666366577148, 'force': [1.103218674659729, -0.36391955614089966, -1.0804864168167114], 'magnitude': 1.5864992141723633, 'cosine_with_motion': 0.6176480054855347, 'motion_component': 0.9798980951309204, 'motion_component_percent': 61.76480054855347}, {'resid': 458, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 10.175329208374023, 'force': [2.2049005031585693, -0.19832362234592438, -1.8930878639221191], 'magnitude': 2.912850856781006, 'cosine_with_motion': 0.5896417498588562, 'motion_component': 1.7175384759902954, 'motion_component_percent': 58.96417498588562}, {'resid': 458, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 10.35611343383789, 'force': [-1.0429103374481201, 0.12514378130435944, 0.739636242389679], 'magnitude': 1.2846729755401611, 'cosine_with_motion': -0.5104221701622009, 'motion_component': -0.6557255983352661, 'motion_component_pe</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>954</v>
+        <v>138</v>
       </c>
       <c r="B4" t="n">
+        <v>565</v>
+      </c>
+      <c r="C4" t="n">
+        <v>2398</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>{47: {'frame': 47, 'motion_vector': [0.02567291259765625, -0.07642364501953125, -0.0362091064453125], 'motion_vector_magnitude': 0.08837857097387314, 'ionic_force': [0.47679272294044495, -2.1543928682804108, -12.768511533737183], 'ionic_force_magnitude': 12.957763183463646, 'radial_force': 2.2065221348417197, 'axial_force': -12.768511533737183, 'glu_force': [0.8293746083509177, -0.3688434709329158, -1.7966726874001324], 'glu_force_magnitude': 2.0129432412953654, 'asn_force': [0.13405996351502836, 0.45151741522931843, -1.838835820555687], 'asn_force_magnitude': 1.8981984156119511, 'sf_force': [-8.690462501705042, 0.5698051544295595, 7.944329462421592], 'sf_force_magnitude': 11.788179970421885, 'residue_force': [-7.727027929839096, 0.6524790987259621, 4.308820954465773], 'residue_force_magnitude': 8.871224696761493, 'pip2_force': [0.2537624528631568, -0.052169503731420264, -4.299649526772555], 'pip2_force_magnitude': 4.307447398712858, 'total_force': [-6.996472754035494, -1.554083273285869, -12.759340106043965], 'total_force_magnitude': 14.634430831432084, 'cosine_total_motion': 0.3101611741682717, 'cosine_glu_motion': 0.6438227227059209, 'cosine_asn_motion': 0.21171728973355425, 'cosine_sf_motion': -0.5320610173207722, 'cosine_residue_motion': -0.515618887085534, 'cosine_pip2_motion': 0.43654942203711466, 'cosine_ionic_motion': 0.5581819547418586, 'motion_component_total': 4.539032249961332, 'motion_component_glu': 1.2959785982632637, 'motion_component_asn': 0.40188142392988907, 'motion_component_sf': -6.272031027423018, 'motion_component_residue': -4.574171005229865, 'motion_component_ionic': 7.232789582827826, 'motion_component_pip2': 1.8804136723633713, 'motion_component_percent_total': 31.01611741682717, 'motion_component_percent_glu': 64.38227227059208, 'motion_component_percent_asn': 21.171728973355425, 'motion_component_percent_sf': 53.206101732077215, 'motion_component_percent_residue': 51.561888708553404, 'motion_component_percent_ionic': 55.81819547418586, 'motion_component_percent_pip2': 43.654942203711464, 'ionic_contributions': [{'ion_id': 2276, 'distance': 7.610594272613525, 'force': [0.3474229872226715, 0.19821712374687195, -5.717957496643066], 'magnitude': 5.731930732727051, 'cosine_ionic_motion': 0.39640942215919495, 'motion_component_ionic': 2.272191286087036, 'motion_component_percent_ionic': 39.640942215919495}, {'ion_id': 2397, 'distance': 4.1341233253479, 'force': [1.3617627620697021, 1.197269320487976, -19.34064483642578], 'magnitude': 19.425457000732422, 'cosine_ionic_motion': 0.3749827742576599, 'motion_component_ionic': 7.2842116355896, 'motion_component_percent_ionic': 37.49827742576599}, {'ion_id': 2399, 'distance': 5.925229072570801, 'force': [2.0369670391082764, -2.082000732421875, 8.996685028076172], 'magnitude': 9.456441879272461, 'cosine_ionic_motion': -0.136827290058136, 'motion_component_ionic': -1.2938992977142334, 'motion_component_percent_ionic': 13.682729005813599}, {'ion_id': 2400, 'distance': 8.259014129638672, 'force': [-3.269360065460205, -1.4678785800933838, 3.293405771255493], 'magnitude': 4.867227554321289, 'cosine_ionic_motion': -0.2115606814622879, 'motion_component_ionic': -1.0297139883041382, 'motion_component_percent_ionic': 21.15606814622879}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 10.12036418914795, 'force': [-1.6104865074157715, -0.41559037566185, -0.18576031923294067], 'magnitude': 1.6735856533050537, 'cosine_with_motion': -0.01932763308286667, 'motion_component': -0.0323464497923851, 'motion_component_percent': 1.9327633082866669}, {'resid': 98, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 10.944183349609375, 'force': [0.7883457541465759, 0.1967654824256897, 0.04576463624835014], 'magnitude': 0.8138182163238525, 'cosine_with_motion': 0.049281127750873566, 'motion_component': 0.04010587930679321, 'motion_component_percent': 4.928112775087357}, {'resid': 98, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 10.389772415161133, 'force': [0.1148063987493515, 0.02838226407766342, 0.030371200293302536], 'magnitude': 0.12210025638341904, 'cosine_with_motion': -0.02978166565299034, 'motion_component': -0.003636348992586136, 'motion_component_percent': 2.978166565299034}, {'resid': 98, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 10.530158042907715, 'force': [0.29908493161201477, 0.10739381611347198, 0.09206629544496536], 'magnitude': 0.3308495581150055, 'cosine_with_motion': -0.13210266828536987, 'motion_component': -0.04370610788464546, 'motion_component_percent': 13.210266828536987}, {'resid': 98, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 11.815164566040039, 'force': [0.12634249031543732, 0.024320926517248154, 0.0344034843146801], 'magnitude': 0.1331823319196701, 'cosine_with_motion': 0.011823365464806557, 'motion_component': 0.001574663445353508, 'motion_component_percent': 1.1823365464806557}, {'resid': 98, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 11.93470573425293, 'force': [-0.03917432948946953, -0.00435563363134861, -0.008509068749845028], 'magnitude': 0.040323738008737564, 'cosine_with_motion': -0.10234709084033966, 'motion_component': -0.004127017222344875, 'motion_component_percent': 10.234709084033966}, {'resid': 98, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 12.005684852600098, 'force': [-0.036900632083415985, -0.006338460836559534, -0.013640305958688259], 'magnitude': 0.03984834626317024, 'cosine_with_motion': 0.008792505599558353, 'motion_component': 0.00035036681219935417, 'motion_component_percent': 0.8792505599558353}, {'resid': 98, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 12.910460472106934, 'force': [0.025364045053720474, 0.007254160940647125, 0.006152902729809284], 'magnitude': 0.027089035138487816, 'cosine_with_motion': -0.05263444781303406, 'motion_component': -0.0014258164446800947, 'motion_component_percent': 5.263444781303406}, {'resid': 98, 'resname': 'GLU', 'atom': 'HG2', 'charge': -0.042500000447034836, 'distance': 13.819144248962402, 'force': [-0.06890402734279633, -0.0180678628385067, -0.019621258601546288], 'magnitude': 0.0738864466547966, 'cosine_with_motion': 0.04935899004340172, 'motion_component': 0.0036469604820013046, 'motion_component_percent': 4.935899004340172}, {'resid': 98, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 12.755399703979492, 'force': [-0.07849442213773727, -0.029589757323265076, -0.022002486512064934], 'magnitude': 0.08672391623258591, 'cosine_with_motion': 0.13606396317481995, 'motion_component': 0.011799999512732029, 'motion_component_percent': 13.606396317481995}, {'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 13.332691192626953, 'force': [1.4338804483413696, 0.41932591795921326, 0.17566648125648499], 'magnitude': 1.5042294263839722, 'cosine_with_motion': -0.011999652720987797, 'motion_component': -0.01805023103952408, 'motion_component_percent': 1.1999652720987797}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 14.268365859985352, 'force': [-1.292931079864502, -0.31294044852256775, -0.11545626074075699], 'magnitude': 1.335265040397644, 'cosine_with_motion': -0.04318905621767044, 'motion_component': -0.057668834924697876, 'motion_component_percent': 4.318905621767044}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 12.711807250976562, 'force': [-1.5830941200256348, -0.5620892643928528, -0.08929818868637085], 'magnitude': 1.6822917461395264, 'cosine_with_motion': 0.037313275039196014, 'motion_component': 0.06277181208133698, 'motion_component_percent': 3.7313275039196014}, {'resid': 98, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 9.532828330993652, 'force': [1.8184361457824707, 0.27635371685028076, 0.6783031821250916], 'magnitude': 1.9604021310806274, 'cosine_with_motion': 0.005793910939246416, 'motion_component': 0.011358395218849182, 'motion_component_percent': 0.5793910939246416}, {'resid': 98, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 9.678016662597656, 'force': [-1.8063404560089111, -0.31904327869415283, -0.9432064890861511], 'magnitude': 2.062593698501587, 'cosine_with_motion': 0.06671323627233505, 'motion_component': 0.137602299451828, 'motion_component_percent': 6.671323627233505}, {'resid': 426, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 9.575953483581543, 'force': [1.8174563646316528, 0.35659369826316833, -0.25284409523010254], 'magnitude': 1.8692877292633057, 'cosine_with_motion': 0.1728910654783249, 'motion_component': 0.32318314909935, 'motion_component_percent': 17.28910654783249}, {'resid': 426, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 10.368783950805664, 'force': [-0.8879621028900146, -0.1707691103219986, 0.06611243635416031], 'magnitude': 0.9066474437713623, 'cosine_with_motion': -0.1515028029680252, 'motion_component': -0.1373596340417862, 'motion_component_percent': 15.15028029680252}, {'resid': 426, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 10.019269943237305, 'force': [-0.12394194304943085, -0.023063143715262413, 0.03668133541941643], 'magnitude': 0.1312974989414215, 'cosine_with_motion': -0.2367810159921646, 'motion_component': -0.031088754534721375, 'motion_component_percent': 23.67810159921646}, {'resid': 426, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 10.223624229431152, 'force': [-0.31877967715263367, -0.09285687655210495, 0.11379249393939972], 'magnitude': 0.35098662972450256, 'cosine_with_motion': -0.16788901388645172, 'motion_component': -0.05892679840326309, 'motion_component_percent': 16.788901388645172}, {'resid': 426, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 11.388359069824219, 'force': [-0.13696534931659698, -0.016612401232123375, 0.03891424462199211], 'magnitude': 0.14335200190544128, 'cosine_with_motion': -0.2885546088218689, 'motion_component': -0.0413648821413517, 'motion_component_percent': 28.85546088218689}, {'resid': 426, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 11.268439292907715, 'force': [0.04420889541506767, 0.0022667604498565197, -0.009298998862504959], 'magnitude': 0.04523313045501709, 'cosine_with_motion': 0.32480302453041077, 'motion_component': 0.014691857621073723, 'motion_component_percent': 32.48030245304108}, {'resid': 426, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 11.821270942687988, 'force': [0.03843894228339195, 0.0031582184601575136, -0.014205371960997581], 'magnitude': 0.041101329028606415, 'cosine_with_motion': 0.3468269407749176, 'motion_component': 0.014255048707127571, 'motion_component_percent': 34.68269407749176}, {'resid': 426, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 12.64444351196289, 'force': [-0.027003541588783264, -0.005055740009993315, 0.00654164794832468], 'magnitude': 0.028240837156772614, 'cosine_with_motion': -0.21785809099674225, 'motion_component': -0.006152494810521603, 'motion_component_percent': 21.785809099674225}, {'resid': 426, 'resname': 'GLU', 'atom': 'HG2', 'charge': -0.042500000447034836, 'distance': 13.289451599121094, 'force': [0.07777147740125656, 0.010324808768928051, -0.015099996700882912], 'magnitude': 0.07989376783370972, 'cosine_with_motion': 0.24845542013645172, 'motion_component': 0.01985003985464573, 'motion_component_percent': 24.845542013645172}, {'resid': 426, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 13.321975708007812, 'force': [0.0744224265217781, 0.015621078200638294, -0.023198984563350677], 'magnitude': 0.07950413972139359, 'cosine_with_motion': 0.22156743705272675, 'motion_component': 0.017615528777241707, 'motion_component_percent': 22.156743705272675}, {'resid': 426, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 12.516448020935059, 'force': [-1.6114705801010132, -0.48342016339302063, 0.2875744104385376], 'magnitude': 1.7068191766738892, 'cosine_with_motion': -0.09837318956851959, 'motion_component': -0.16790524125099182, 'motion_component_percent': 9.83731895685196}, {'resid': 426, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 11.998488426208496, 'force': [1.7139288187026978, 0.6767798662185669, -0.4122622311115265], 'magnitude': 1.888264536857605, 'cosine_with_motion': 0.04318740963935852, 'motion_component': 0.0815492570400238, 'motion_component_percent': 4.318740963935852}, {'resid': 426, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 12.939177513122559, 'force': [1.5507326126098633, 0.46414387226104736, -0.12712809443473816], 'magnitude': 1.623687982559204, 'cosine_with_motion': 0.06232403218746185, 'motion_component': 0.10119478404521942, 'motion_component_percent': 6.232403218746185}, {'resid': 426, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 9.232041358947754, 'force': [-1.9352669715881348, -0.15778151154518127, 0.773881196975708], 'magnitude': 2.090226173400879, 'cosine_with_motion': -0.3553662896156311, 'motion_component': -0.7427959442138672, 'motion_component_percent': 35.53662896156311}, {'resid': 426, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 9.16576862335205, 'force': [1.9981932640075684, 0.23040682077407837, -1.114544153213501], 'magnitude': 2.2995810508728027, 'cosine_with_motion': 0.3643468916416168, 'motion_component': 0.8378452062606812, 'motion_component_percent': 36.43468916416168}, {'resid': 754, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 9.717093467712402, 'force': [-0.44717469811439514, 1.7552942037582397, -0.12074985355138779], 'magnitude': 1.8153797388076782, 'cosine_with_motion': -0.8804126977920532, 'motion_component': -1.5982834100723267, 'motion_component_percent': 88.04126977920532}, {'resid': 754, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 10.360391616821289, 'force': [0.19770756363868713, -0.8863223195075989, -0.004580182954668999], 'magnitude': 0.9081169962882996, 'cosine_with_motion': 0.9092860221862793, 'motion_component': 0.8257380723953247, 'motion_component_percent': 90.92860221862793}, {'resid': 754, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 10.163516998291016, 'force': [0.029088985174894333, -0.12130541354417801, 0.026829665526747704], 'magnitude': 0.12759703397750854, 'cosine_with_motion': 0.8021679520606995, 'motion_component': 0.1023542508482933, 'motion_component_percent': 80.21679520606995}, {'resid': 754, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 10.247382164001465, 'force': [0.10932117700576782, -0.31892338395118713, 0.0915963351726532], 'magnitude': 0.34936103224754333, 'cosine_with_motion': 0.7728732824325562, 'motion_component': 0.2700118124485016, 'motion_component_percent': 77.28732824325562}, {'resid': 754, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 11.621627807617188, 'force': [0.02693774737417698, -0.13215318322181702, 0.027546554803848267], 'magnitude': 0.1376550793647766, 'cosine_with_motion': 0.8050267696380615, 'motion_component': 0.11081602424383163, 'motion_component_percent': 80.50267696380615}, {'resid': 754, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 11.802988052368164, 'force': [-0.004867422394454479, 0.040433648973703384, -0.006421761121600866], 'magnitude': 0.0412287600338459, 'cosine_with_motion': -0.8185332417488098, 'motion_component': -0.0337471105158329, 'motion_component_percent': 81.85332417488098}, {'resid': 754, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 12.13443374633789, 'force': [-0.006637376733124256, 0.03690334036946297, -0.010754232294857502], 'magnitude': 0.039007242769002914, 'cosine_with_motion': -0.754564106464386, 'motion_component': -0.029433464631438255, 'motion_component_percent': 75.4564106464386}, {'resid': 754, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 12.580174446105957, 'force': [0.007880054414272308, -0.02706705406308174, 0.004387169610708952], 'magnitude': 0.028530124574899673, 'cosine_with_motion': 0.8376172184944153, 'motion_component': 0.02389732375741005, 'motion_component_percent': 83.76172184944153}, {'resid': 754, 'resname': 'GLU', 'atom': 'HG2', 'charge': -0.042500000447034836, 'distance': 12.678923606872559, 'force': [-0.029575834050774574, 0.08062666654586792, -0.01813165470957756], 'magnitude': 0.08777326345443726, 'cosine_with_motion': -0.8075709939002991, 'motion_component': -0.0708831399679184, 'motion_component_percent': 80.75709939002991}, {'resid': 754, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 12.253327369689941, 'force': [-0.029578441753983498, 0.0888870507478714, -0.007468468975275755], 'magnitude': 0.09397643059492111, 'cosine_with_motion': -0.8767693638801575, 'motion_component': -0.08239565789699554, 'motion_component_percent': 87.67693638801575}, {'resid': 754, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 13.951192855834961, 'force': [0.30945730209350586, -1.3254096508026123, 0.18676839768886566], 'magnitude': 1.37381112575531, 'cosine_with_motion': 0.843999445438385, 'motion_component': 1.1594958305358887, 'motion_component_percent': 84.3999445438385}, {'resid': 754, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 14.702713966369629, 'force': [-0.32131341099739075, 1.2126072645187378, -0.08798455446958542], 'magnitude': 1.2575372457504272, 'cosine_with_motion': -0.8793922066688538, 'motion_component': -1.1058684587478638, 'motion_component_percent': 87.93922066688538}, {'resid': 754, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 14.343954086303711, 'force': [-0.21540018916130066, 1.2793076038360596, -0.25024208426475525], 'magnitude': 1.321229100227356, 'cosine_with_motion': -0.8070530891418457, 'motion_component': -1.0663020610809326, 'motion_component_percent': 80.70530891418457}, {'resid': 754, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 9.56238842010498, 'force': [0.243622824549675, -1.8401198387145996, 0.5920162200927734], 'magnitude': 1.948300838470459, 'cosine_with_motion': 0.7285453081130981, 'motion_component': 1.4194254875183105, 'motion_component_percent': 72.85453081130981}, {'resid': 754, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 9.96861457824707, 'force': [-0.2102193832397461, 1.7577091455459595, -0.8035923838615417], 'magnitude': 1.9440921545028687, 'cosine_with_motion': -0.6438868641853333, 'motion_component': -1.2517753839492798, 'motion_component_percent': 64.38868641853333}, {'resid': 1082, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 9.629386901855469, 'force': [0.35627803206443787, -1.8064523935317993, -0.16467373073101044], 'magnitude': 1.848599910736084, 'cosine_with_motion': 0.9374968409538269, 'motion_component': 1.7330565452575684, 'motion_component_percent': 93.74968409538269}, {'resid': 1082, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 10.426177024841309, 'force': [-0.15792757272720337, 0.8822723627090454, 0.02670697309076786], 'magnitude': 0.8966933488845825, 'cosine_with_motion': -0.914187490940094, 'motion_component': -0.8197458386421204, 'motion_component_percent': 91.4187490940094}, {'resid': 1082, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 9.969714164733887, 'force': [-0.024433594197034836, 0.12657752633094788, 0.031072162091732025], 'magnitude': 0.13260599970817566, 'cosine_with_motion': -0.9749447107315063, 'motion_component': -0.12928351759910583, 'motion_component_percent': 97.49447107315063}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 9.953929901123047, 'force': [-0.1033705323934555, 0.34052830934524536, 0.10222654044628143], 'magnitude': 0.3702637851238251, 'cosine_with_motion': -0.9894994497299194, 'motion_component': -0.36637580394744873, 'motion_component_percent': 98.94994497299194}, {'resid': 1082, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 11.457404136657715, 'force': [-0.02193998172879219, 0.13588741421699524, 0.033348940312862396], 'magnitude': 0.14162945747375488, 'cosine_with_motion': -0.9711433053016663, 'motion_component': -0.1375425010919571, 'motion_component_percent': 97.11433053016663}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 11.764636039733887, 'force': [0.0038608394097536802, -0.04068620130419731, -0.007198006846010685], 'magnitude': 0.041498005390167236, 'cosine_with_motion': 0.9459052681922913, 'motion_component': 0.03925318270921707, 'motion_component_percent': 94.59052681922913}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 11.732832908630371, 'force': [0.004339642357081175, -0.03943672776222229, -0.012912939302623272], 'magnitude': 0.04172327741980553, 'cosine_with_motion': 0.9743541479110718, 'motion_component': 0.04065324738621712, 'motion_component_percent': 97.43541479110718}, {'resid': 1082, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 12.446666717529297, 'force': [-0.0072038560174405575, 0.02749837562441826, 0.006434401497244835], 'magnitude': 0.029145456850528717, 'cosine_with_motion': -0.9781119227409363, 'motion_component': -0.028507519513368607, 'motion_component_percent': 97.81119227409363}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HG2', 'charge': -0.042500000447034836, 'distance': 13.400782585144043, 'force': [0.016434045508503914, -0.07502120733261108, -0.016591191291809082], 'magnitude': 0.07857179641723633, 'cosine_with_motion': 0.9729254245758057, 'motion_component': 0.07644449919462204, 'motion_component_percent': 97.29254245758057}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 12.453123092651367, 'force': [0.02644253708422184, -0.08296652883291245, -0.02637503109872341], 'magnitude': 0.09098513424396515, 'cosine_with_motion': 0.9917103052139282, 'motion_component': 0.09023089706897736, 'motion_component_percent': 99.17103052139282}, {'resid': 1082, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 12.384073257446289, 'force': [-0.5550512671470642, 1.6386737823486328, 0.21556660532951355], 'magnitude': 1.7435029745101929, 'cosine_with_motion': -0.9558719396591187, 'motion_component': -1.6665655374526978, 'motion_component_percent': 95.58719396591187}, {'resid': 1082, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 11.616856575012207, 'force': [0.792901337146759, -1.8335847854614258, -0.2587472200393677], 'magnitude': 2.0143673419952393, 'cosine_with_motion': 0.9540935754776001, 'motion_component': 1.921894907951355, 'motion_component_percent': 95.40935754776001}, {'resid': 1082, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 13.314166069030762, 'force': [0.46842244267463684, -1.4575704336166382, -0.08795734494924545], 'magnitude': 1.5335148572921753, 'cosine_with_motion': 0.9341371059417725, 'motion_component': 1.4325131177902222, 'motion_component_percent': 93.41371059417725}, {'resid': 1082, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 9.365450859069824, 'force': [-0.14469219744205475, 1.9111684560775757, 0.6722105741500854], 'magnitude': 2.031100034713745, 'cosine_with_motion': -0.9699594378471375, 'motion_component': -1.9700846672058105, 'motion_component_percent': 96.99594378471375}, {'resid': 1082, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 9.529675483703613, 'force': [0.15236856043338776, -1.8977168798446655, -0.9491522312164307], 'magnitude': 2.127307176589966, 'cosine_with_motion': 0.9750105738639832, 'motion_component': 2.0741469860076904, 'motion_component_percent': 97.50105738639832}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'N', 'charge': -0.38210001587867737, 'distance': 12.612298011779785, 'force': [-0.5084488987922668, -0.11954557150602341, -0.6026468276977539], 'magnitude': 0.7974926829338074, 'cosine_with_motion': 0.2540256381034851, 'motion_component': 0.20258358120918274, 'motion_component_percent': 25.40256381034851}, {'resid': 130, 'resname': 'ASN', 'atom': 'H', 'charge': 0.2681000232696533, 'distance': 12.163505554199219, 'force': [0.39036405086517334, 0.13059554994106293, 0.438747376203537], 'magnitude': 0.6016132831573486, 'cosine_with_motion': -0.2980165481567383, 'motion_component': -0.17929071187973022, 'motion_component_percent': 29.801654815673828}, {'resid': 130, 'resname': 'ASN', 'atom': 'CA', 'charge': -0.20800000429153442, 'distance': 12.041388511657715, 'force': [-0.2743021845817566, -0.03837347403168678, -0.3874451518058777], 'magnitude': 0.4762645661830902, 'cosine_with_motion': 0.23566582798957825, 'motion_component': 0.1122392863035202, 'motion_component_percent': 23.566582798957825}, {'resid': 130, 'resname': 'ASN', 'atom': 'HA', 'charge': 0.13580000400543213, 'distance': 12.101244926452637, 'force': [0.18308532238006592, -0.0021865980233997107, 0.24751456081867218], 'magnitude': 0.3078773617744446, 'cosine_with_motion': -0.15049158036708832, 'motion_component': -0.0463329516351223, 'motion_component_percent': 15.049158036708832}, {'resid': 130, 'resname': 'ASN', 'atom': 'CB', 'charge': -0.22990000247955322, 'distance': 10.530930519104004, 'force': [-0.38408949971199036, -0.08233559131622314, -0.5651357769966125], 'magnitude': 0.6882458329200745, 'cosine_with_motion': 0.27775460481643677, 'motion_component': 0.19116345047950745, 'motion_component_percent': 27.775460481643677}, {'resid': 130, 'resname': 'ASN', 'atom': 'HB2', 'charge': 0.1023000031709671, 'distance': 10.474102973937988, 'force': [0.1755073368549347, 0.06788771599531174, 0.24582789838314056], 'magnitude': 0.3095850944519043, 'cosine_with_motion': -0.3502708375453949, 'motion_component': -0.10843862593173981, 'motion_component_percent': 35.02708375453949}, {'resid': 130, 'resname': 'ASN', 'atom': 'HB3', 'charge': 0.1023000031709671, 'distance': 10.35511589050293, 'force': [0.15014395117759705, 0.030093571171164513, 0.27726486325263977], 'magnitude': 0.31674066185951233, 'cosine_with_motion': -0.3031012713909149, 'motion_component': -0.09600450098514557, 'motion_component_percent': 30.31012713909149}, {'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 9.619159698486328, 'force': [1.599961757659912, 0.09735436737537384, 2.0044684410095215], 'magnitude': 2.566563606262207, 'cosine_with_motion': -0.17169089615345, 'motion_component': -0.44065558910369873, 'motion_component_percent': 17.169089615345}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 9.256054878234863, 'force': [-1.3605540990829468, 0.18165095150470734, -1.8814668655395508], 'magnitude': 2.3289530277252197, 'cosine_with_motion': 0.0938369631767273, 'motion_component': 0.21854187548160553, 'motion_component_percent': 9.38369631767273}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 9.45495319366455, 'force': [-2.424013137817383, -0.27659091353416443, -2.3300180435180664], 'magnitude': 3.373622179031372, 'cosine_with_motion': 0.14514043927192688, 'motion_component': 0.4896489977836609, 'motion_component_percent': 14.514043927192688}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 8.841269493103027, 'force': [1.3552641868591309, 0.05735884979367256, 1.1255102157592773], 'magnitude': 1.7626128196716309, 'cosine_with_motion': -0.0664006844162941, 'motion_component': -0.11703869700431824, 'motion_component_percent': 6.64006844162941}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 9.9805269241333, 'force': [1.0100494623184204, 0.2288978099822998, 0.9168410301208496], 'magnitude': 1.3831816911697388, 'cosine_with_motion': -0.20254871249198914, 'motion_component': -0.28016167879104614, 'motion_component_percent': 20.254871249198914}, {'resid': 130, 'resname': 'ASN', 'atom': 'C', 'charge': 0.8050000071525574, 'distance': 12.861124038696289, 'force': [0.7924947142601013, 0.1347309947013855, 1.4015960693359375], 'magnitude': 1.6157574653625488, 'cosine_with_motion': -0.28502801060676575, 'motion_component': -0.4605361223220825, 'motion_component_percent': 28.502801060676575}, {'resid': 130, 'resname': 'ASN', 'atom': 'O', 'charge': -0.8147000074386597, 'distance': 13.295897483825684, 'force': [-0.6972013711929321, -0.007909948006272316, -1.3619271516799927], 'magnitude': 1.5300320386886597, 'cosine_with_motion': 0.23679189383983612, 'motion_component': 0.3622991740703583, 'motion_component_percent': 23.679189383983612}, {'resid': 458, 'resname': 'ASN', 'atom': 'N', 'charge': -0.38210001587867737, 'distance': 13.572711944580078, 'force': [0.4937450885772705, 0.046810854226350784, -0.47773104906082153], 'magnitude': 0.6886235475540161, 'cosine_with_motion': 0.43373021483421326, 'motion_component': 0.29867684841156006, 'motion_component_percent': 43.373021483421326}, {'resid': 458, 'resname': 'ASN', 'atom': 'H', 'charge': 0.2681000232696533, 'distance': 13.21522045135498, 'force': [-0.3754120171070099, -0.06566480547189713, 0.3383989930152893], 'magnitude': 0.5096665024757385, 'cosine_with_motion': -0.3745860159397125, 'motion_component': -0.19091394543647766, 'motion_component_percent': 37.45860159397125}, {'resid': 458, 'resname': 'ASN', 'atom': 'CA', 'charge': -0.20800000429153442, 'distance': 12.651140213012695, 'force': [0.29724815487861633, -0.005706643220037222, -0.31268203258514404], 'magnitude': 0.43146154284477234, 'cosine_with_motion': 0.5084786415100098, 'motion_component': 0.21938899159431458, 'motion_component_percent': 50.84786415100098}, {'resid': 458, 'resname': 'ASN', 'atom': 'HA', 'charge': 0.13580000400543213, 'distance': 12.94201374053955, 'force': [-0.1918502151966095, 0.02325686439871788, 0.1873701959848404], 'magnitude': 0.26917460560798645, 'cosine_with_motion': -0.566946268081665, 'motion_component': -0.1526075303554535, 'motion_component_percent': 56.694626808166504}, {'resid': 458, 'resname': 'ASN', 'atom': 'CB', 'charge': -0.22990000247955322, 'distance': 11.192800521850586, 'force': [0.43525567650794983, 0.01584515906870365, -0.42602089047431946], 'magnitude': 0.6092556118965149, 'cosine_with_motion': 0.4715220630168915, 'motion_component': 0.2872774600982666, 'motion_component_percent': 47.15220630168915}, {'resid': 458, 'resname': 'ASN', 'atom': 'HB2', 'charge': 0.1023000031709671, 'distance': 11.131847381591797, 'force': [-0.2130136638879776, -5.616597263724543e-05, 0.1724693477153778], 'magnitude': 0.27408120036125183, 'cosine_with_motion': -0.4833999276161194, 'motion_component': -0.1324908286333084, 'motion_component_percent': 48.33999276161194}, {'resid': 458, 'resname': 'ASN', 'atom': 'HB3', 'charge': 0.1023000031709671, 'distance': 11.102154731750488, 'force': [-0.19039267301559448, -0.032953087240457535, 0.1964486986398697], 'magnitude': 0.2755492031574249, 'cosine_with_motion': -0.3893938958644867, 'motion_component': -0.10729717463254929, 'motion_component_percent': 38.93938958644867}, {'resid': 458, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 9.998913764953613, 'force': [-1.6078851222991943, 0.13213872909545898, 1.743373990058899], 'magnitude': 2.375312089920044, 'cosine_with_motion': -0.5454457998275757, 'motion_component': -1.2956039905548096, 'motion_component_percent': 54.54457998275757}, {'resid': 458, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 9.024710655212402, 'force': [1.5398999452590942, -0.028462203219532967, -1.9052144289016724], 'magnitude': 2.4498865604400635, 'cosine_with_motion': 0.5112521052360535, 'motion_component': 1.2525097131729126, 'motion_component_percent': 51.12521052360535}, {'resid': 458, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 10.166921615600586, 'force': [2.0169692039489746, -0.5277373790740967, -2.041110038757324], 'magnitude': 2.917670726776123, 'cosine_with_motion': 0.6438382863998413, 'motion_component': 1.8785080909729004, 'motion_component_percent': 64.38382863998413}, {'resid': 458, 'resname': 'ASN', 'atom':</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>574</v>
+      </c>
+      <c r="B5" t="n">
+        <v>969</v>
+      </c>
+      <c r="C5" t="n">
+        <v>2397</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>{132: {'frame': 132, 'motion_vector': [-0.21205520629882812, 0.25970458984375, -0.655731201171875], 'motion_vector_magnitude': 0.7364762425422668, 'ionic_force': [-0.820099301636219, -1.9878737260587513, -14.614980936050415], 'ionic_force_magnitude': 14.772334702964727, 'radial_force': 2.1503964321256945, 'axial_force': -14.614980936050415, 'glu_force': [0.7806158270686865, -1.3751291976077482, -1.9682141751982272], 'glu_force_magnitude': 2.5247194733345517, 'asn_force': [-0.4356897057732567, 0.13725195211009122, -0.03864680230617523], 'asn_force_magnitude': 0.45842904947582713, 'sf_force': [7.286105760503233, -0.9644381203652301, 11.586421602929477], 'sf_force_magnitude': 13.720883484749912, 'residue_force': [7.631031881798663, -2.202315365862887, 9.579560625425074], 'residue_force_magnitude': 12.443907036294423, 'pip2_force': [0.3227406945079565, 0.03660308616235852, -3.9786737558897585], 'pip2_force_magnitude': 3.9919100938791203, 'total_force': [7.1336732746704, -4.15358600575928, -9.0140940665151], 'total_force_magnitude': 12.222743674681588, 'cosine_total_motion': 0.3687483798825749, 'cosine_glu_motion': 0.41301498414238663, 'cosine_asn_motion': 0.4542864608807871, 'cosine_sf_motion': -0.9295404572837763, 'cosine_residue_motion': -0.9243970717160477, 'cosine_pip2_motion': 0.8673651693426568, 'cosine_ionic_motion': 0.8494110531979562, 'motion_component_total': 4.507116927758826, 'motion_component_glu': 1.0427469732432446, 'motion_component_asn': 0.20825811045131676, 'motion_component_sf': -12.754116308751847, 'motion_component_residue': -11.503111225057285, 'motion_component_ionic': 12.547784378237987, 'motion_component_pip2': 3.4624437745781242, 'motion_component_percent_total': 36.87483798825749, 'motion_component_percent_glu': 41.301498414238665, 'motion_component_percent_asn': 45.428646088078715, 'motion_component_percent_sf': 92.95404572837764, 'motion_component_percent_residue': 92.43970717160477, 'motion_component_percent_ionic': 84.94110531979561, 'motion_component_percent_pip2': 86.73651693426568, 'ionic_contributions': [{'ion_id': 2276, 'distance': 3.775073528289795, 'force': [-0.858628511428833, -0.8070741295814514, -23.26649284362793], 'magnitude': 23.296316146850586, 'cosine_ionic_motion': 0.8876189589500427, 'motion_component_ionic': 20.678251266479492, 'motion_component_percent_ionic': 88.76189589500427}, {'ion_id': 2398, 'distance': 6.597342491149902, 'force': [-0.3295109272003174, -2.385207414627075, 7.237799167633057], 'magnitude': 7.62781286239624, 'cosine_ionic_motion': -0.9426673650741577, 'motion_component_ionic': -7.190490245819092, 'motion_component_percent_ionic': 94.26673650741577}, {'ion_id': 2400, 'distance': 7.97969388961792, 'force': [0.2676622271537781, 1.2015414237976074, 5.066534519195557], 'magnitude': 5.213934898376465, 'cosine_ionic_motion': -0.7987101078033447, 'motion_component_ionic': -4.164422512054443, 'motion_component_percent_ionic': 79.87101078033447}, {'ion_id': 2520, 'distance': 9.531752586364746, 'force': [0.10037790983915329, 0.0028663943521678448, -3.6528217792510986], 'magnitude': 3.6542019844055176, 'cosine_ionic_motion': 0.882394015789032, 'motion_component_ionic': 3.2244460582733154, 'motion_component_percent_ionic': 88.2394015789032}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 9.483658790588379, 'force': [-1.8567969799041748, -0.3628678619861603, -0.22997890412807465], 'magnitude': 1.905848503112793, 'cosine_with_motion': 0.3208217918872833, 'motion_component': 0.6114377379417419, 'motion_component_percent': 32.08217918872833}, {'resid': 98, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 10.271308898925781, 'force': [0.90922611951828, 0.15389542281627655, 0.05730922147631645], 'magnitude': 0.9239373803138733, 'cosine_with_motion': -0.27983835339546204, 'motion_component': -0.2585531175136566, 'motion_component_percent': 27.983835339546204}, {'resid': 98, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 9.780869483947754, 'force': [0.13117356598377228, 0.02208089642226696, 0.035891033709049225], 'magnitude': 0.13777604699134827, 'cosine_with_motion': -0.44956088066101074, 'motion_component': -0.06193872168660164, 'motion_component_percent': 44.956088066101074}, {'resid': 98, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 9.82430648803711, 'force': [0.3486294150352478, 0.09717070311307907, 0.11614860594272614], 'magnitude': 0.380098819732666, 'cosine_with_motion': -0.44601720571517944, 'motion_component': -0.16953061521053314, 'motion_component_percent': 44.601720571517944}, {'resid': 98, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 11.262479782104492, 'force': [0.13973581790924072, 0.017263595014810562, 0.04074207693338394], 'magnitude': 0.14657437801361084, 'cosine_with_motion': -0.4804522693157196, 'motion_component': -0.07042199373245239, 'motion_component_percent': 48.04522693157196}, {'resid': 98, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 11.429841995239258, 'force': [-0.04276251047849655, -0.0017051236936822534, -0.010067341849207878], 'magnitude': 0.04396465793251991, 'cosine_with_motion': 0.47026434540748596, 'motion_component': 0.020675010979175568, 'motion_component_percent': 47.026434540748596}, {'resid': 98, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 11.42284870147705, 'force': [-0.04087647423148155, -0.0035675435792654753, -0.01593787595629692], 'magnitude': 0.04401851072907448, 'cosine_with_motion': 0.5611757636070251, 'motion_component': 0.024702120572328568, 'motion_component_percent': 56.117576360702515}, {'resid': 98, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 12.394058227539062, 'force': [0.027667859569191933, 0.005953592713922262, 0.007938304916024208], 'magnitude': 0.029393406584858894, 'cosine_with_motion': -0.4400652348995209, 'motion_component': -0.012935016304254532, 'motion_component_percent': 44.00652348995209}, {'resid': 98, 'resname': 'GLU', 'atom': 'HG2', 'charge': -0.042500000447034836, 'distance': 13.347667694091797, 'force': [-0.0745135247707367, -0.013382897712290287, -0.023259712383151054], 'magnitude': 0.07919836789369583, 'cosine_with_motion': 0.47280269861221313, 'motion_component': 0.037445202469825745, 'motion_component_percent': 47.28026986122131}, {'resid': 98, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 12.189821243286133, 'force': [-0.08629634976387024, -0.024895355105400085, -0.030825573951005936], 'magnitude': 0.09495817124843597, 'cosine_with_motion': 0.4582498073577881, 'motion_component': 0.043514564633369446, 'motion_component_percent': 45.82498073577881}, {'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 12.781437873840332, 'force': [1.5548244714736938, 0.4316798150539398, 0.2742663025856018], 'magnitude': 1.6367799043655396, 'cosine_with_motion': -0.3297063708305359, 'motion_component': -0.5396567583084106, 'motion_component_percent': 32.97063708305359}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 13.859169006347656, 'force': [-1.3604257106781006, -0.3398221433162689, -0.19176118075847626], 'magnitude': 1.4152772426605225, 'cosine_with_motion': 0.31274116039276123, 'motion_component': 0.44261544942855835, 'motion_component_percent': 31.274116039276123}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 12.011533737182617, 'force': [-1.7649953365325928, -0.6192379593849182, -0.22674717009067535], 'magnitude': 1.8841652870178223, 'cosine_with_motion': 0.2609768509864807, 'motion_component': 0.49172353744506836, 'motion_component_percent': 26.09768509864807}, {'resid': 98, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 8.891950607299805, 'force': [2.1089606285095215, 0.12377817183732986, 0.7834257483482361], 'magnitude': 2.253173828125, 'cosine_with_motion': -0.5597095489501953, 'motion_component': -1.2611229419708252, 'motion_component_percent': 55.97095489501953}, {'resid': 98, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 8.827138900756836, 'force': [-2.174696207046509, -0.20420601963996887, -1.1732090711593628], 'magnitude': 2.4793996810913086, 'cosine_with_motion': 0.644808292388916, 'motion_component': 1.5987374782562256, 'motion_component_percent': 64.4808292388916}, {'resid': 426, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 10.046738624572754, 'force': [1.645906686782837, 0.36528950929641724, -0.20360203087329865], 'magnitude': 1.698204755783081, 'cosine_with_motion': -0.09646499156951904, 'motion_component': -0.16381730139255524, 'motion_component_percent': 9.646499156951904}, {'resid': 426, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 10.809086799621582, 'force': [-0.8169401288032532, -0.1614331752061844, 0.050843361765146255], 'magnitude': 0.8342882394790649, 'cosine_with_motion': 0.15945078432559967, 'motion_component': 0.13302791118621826, 'motion_component_percent': 15.945078432559967}, {'resid': 426, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 10.355151176452637, 'force': [-0.11594266444444656, -0.02514464408159256, 0.03215428441762924], 'magnitude': 0.12291806936264038, 'cosine_with_motion': -0.03345438092947006, 'motion_component': -0.004112147726118565, 'motion_component_percent': 3.3454380929470062}, {'resid': 426, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 10.429000854492188, 'force': [-0.30648133158683777, -0.10068976134061813, 0.09849538654088974], 'magnitude': 0.3372989296913147, 'cosine_with_motion': -0.10363855957984924, 'motion_component': -0.034957174211740494, 'motion_component_percent': 10.363855957984924}, {'resid': 426, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 11.842620849609375, 'force': [-0.12620685994625092, -0.021113310009241104, 0.034636177122592926], 'magnitude': 0.1325654834508896, 'cosine_with_motion': -0.014671731740236282, 'motion_component': -0.0019449652172625065, 'motion_component_percent': 1.4671731740236282}, {'resid': 426, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 12.03227424621582, 'force': [0.038631830364465714, 0.0035370243713259697, -0.008304977789521217], 'magnitude': 0.039672426879405975, 'cosine_with_motion': -0.06255318969488144, 'motion_component': -0.0024816368240863085, 'motion_component_percent': 6.255318969488144}, {'resid': 426, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 12.151256561279297, 'force': [0.03625749424099922, 0.0049162013456225395, -0.013205333612859249], 'magnitude': 0.03889930248260498, 'cosine_with_motion': 0.07844479382038116, 'motion_component': 0.003051447682082653, 'motion_component_percent': 7.8444793820381165}, {'resid': 426, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 12.983957290649414, 'force': [-0.025166286155581474, -0.006479703821241856, 0.0064817024394869804], 'magnitude': 0.02678322233259678, 'cosine_with_motion': -0.03023649752140045, 'motion_component': -0.0008098308462649584, 'motion_component_percent': 3.023649752140045}, {'resid': 426, 'resname': 'GLU', 'atom': 'HG2', 'charge': -0.042500000447034836, 'distance': 13.933585166931152, 'force': [0.06915540993213654, 0.015029952861368656, -0.016543297097086906], 'magnitude': 0.07267771661281586, 'cosine_with_motion': 0.001616775756701827, 'motion_component': 0.000117503572255373, 'motion_component_percent': 0.1616775756701827}, {'resid': 426, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 13.199907302856445, 'force': [0.07362157851457596, 0.02293361909687519, -0.024736575782299042], 'magnitude': 0.08098138868808746, 'cosine_with_motion': 0.11007001250982285, 'motion_component': 0.008913622237741947, 'motion_component_percent': 11.007001250982285}, {'resid': 426, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 12.809344291687012, 'force': [-1.529401421546936, -0.5078224539756775, 0.2425411343574524], 'magnitude': 1.6296559572219849, 'cosine_with_motion': 0.02782190591096878, 'motion_component': 0.04534013569355011, 'motion_component_percent': 2.782190591096878}, {'resid': 426, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 12.45824146270752, 'force': [1.581851840019226, 0.6883050799369812, -0.3026948869228363], 'magnitude': 1.7514688968658447, 'cosine_with_motion': 0.03240720182657242, 'motion_component': 0.05676020681858063, 'motion_component_percent': 3.240720182657242}, {'resid': 426, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 13.163908004760742, 'force': [1.501142144203186, 0.4441837668418884, -0.10081933438777924], 'magnitude': 1.5687228441238403, 'cosine_with_motion': -0.11845828592777252, 'motion_component': -0.18582822382450104, 'motion_component_percent': 11.845828592777252}, {'resid': 426, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 9.476447105407715, 'force': [-1.848260521888733, -0.2182982861995697, 0.6868312358856201], 'magnitude': 1.9837989807128906, 'cosine_with_motion': -0.07880548387765884, 'motion_component': -0.15633423626422882, 'motion_component_percent': 7.880548387765884}, {'resid': 426, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 9.422074317932129, 'force': [1.9079746007919312, 0.2926750183105469, -1.0048400163650513], 'magnitude': 2.176172971725464, 'cosine_with_motion': 0.20610100030899048, 'motion_component': 0.44851142168045044, 'motion_component_percent': 20.610100030899048}, {'resid': 754, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 9.87628173828125, 'force': [-0.39602312445640564, 1.7021774053573608, -0.184297114610672], 'magnitude': 1.7573297023773193, 'cosine_with_motion': 0.4998266398906708, 'motion_component': 0.8783602118492126, 'motion_component_percent': 49.98266398906708}, {'resid': 754, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 10.612454414367676, 'force': [0.17125913500785828, -0.847518801689148, 0.03816322609782219], 'magnitude': 0.865490734577179, 'cosine_with_motion': -0.4415435194969177, 'motion_component': -0.3821518123149872, 'motion_component_percent': 44.15435194969177}, {'resid': 754, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 10.224969863891602, 'force': [0.02627972885966301, -0.11937569826841354, 0.030853452160954475], 'magnitude': 0.1260679066181183, 'cosine_with_motion': -0.6118382215499878, 'motion_component': -0.0771331638097763, 'motion_component_percent': 61.18382215499878}, {'resid': 754, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 10.392961502075195, 'force': [0.10070789605379105, -0.30929914116859436, 0.09771819412708282], 'magnitude': 0.3396422863006592, 'cosine_with_motion': -0.6626685857772827, 'motion_component': -0.2250702679157257, 'motion_component_percent': 66.26685857772827}, {'resid': 754, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 11.643477439880371, 'force': [0.021175455302000046, -0.13056142628192902, 0.036227017641067505], 'magnitude': 0.13713891804218292, 'cosine_with_motion': -0.6153784990310669, 'motion_component': -0.08439233899116516, 'motion_component_percent': 61.53784990310669}, {'resid': 754, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 11.626708984375, 'force': [-0.0028870338574051857, 0.04121824726462364, -0.009898851625621319], 'magnitude': 0.042488422244787216, 'cosine_with_motion': 0.5690888166427612, 'motion_component': 0.02417968586087227, 'motion_component_percent': 56.90888166427612}, {'resid': 754, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 11.756912231445312, 'force': [-0.005839797202497721, 0.03845490515232086, -0.014619547873735428], 'magnitude': 0.04155254736542702, 'cosine_with_motion': 0.6800683736801147, 'motion_component': 0.02825857326388359, 'motion_component_percent': 68.00683736801147}, {'resid': 754, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 12.75967025756836, 'force': [0.006287178490310907, -0.026300281286239624, 0.006155505310744047], 'magnitude': 0.027733078226447105, 'cosine_with_motion': -0.5973090529441833, 'motion_component': -0.016565218567848206, 'motion_component_percent': 59.730905294418335}, {'resid': 754, 'resname': 'GLU', 'atom': 'HG2', 'charge': -0.042500000447034836, 'distance': 12.772477149963379, 'force': [-0.025736844167113304, 0.0794697180390358, -0.022429287433624268], 'magnitude': 0.08649216592311859, 'cosine_with_motion': 0.6405688524246216, 'motion_component': 0.0554041862487793, 'motion_component_percent': 64.05688524246216}, {'resid': 754, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 12.823868751525879, 'force': [-0.02081843838095665, 0.0823746845126152, -0.011945684440433979], 'magnitude': 0.08580032736063004, 'cosine_with_motion': 0.5323778390884399, 'motion_component': 0.045678190886974335, 'motion_component_percent': 53.237783908843994}, {'resid': 754, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 14.18630599975586, 'force': [0.25415709614753723, -1.2668944597244263, 0.30934956669807434], 'magnitude': 1.3286514282226562, 'cosine_with_motion': -0.5986220836639404, 'motion_component': -0.7953600883483887, 'motion_component_percent': 59.86220836639404}, {'resid': 754, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 14.552260398864746, 'force': [-0.15421609580516815, 1.2243804931640625, -0.35345518589019775], 'magnitude': 1.283674716949463, 'cosine_with_motion': 0.6160922646522522, 'motion_component': 0.7908620834350586, 'motion_component_percent': 61.60922646522522}, {'resid': 754, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 9.339800834655762, 'force': [0.236037477850914, -1.9085475206375122, 0.6874634623527527], 'magnitude': 2.042271614074707, 'cosine_with_motion': -0.6625310778617859, 'motion_component': -1.353068470954895, 'motion_component_percent': 66.25310778617859}, {'resid': 754, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 9.184541702270508, 'force': [-0.31865647435188293, 2.012669563293457, -1.04526948928833], 'magnitude': 2.290189743041992, 'cosine_with_motion': 0.7563351392745972, 'motion_component': 1.7321510314941406, 'motion_component_percent': 75.63351392745972}, {'resid': 1082, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 9.680215835571289, 'force': [0.4972318708896637, -1.7474712133407593, -0.21263791620731354], 'magnitude': 1.8292375802993774, 'cosine_with_motion': -0.3116365075111389, 'motion_component': -0.570057213306427, 'motion_component_percent': 31.16365075111389}, {'resid': 1082, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 10.375456809997559, 'force': [-0.2017790675163269, 0.8807582259178162, 0.05871343985199928], 'magnitude': 0.9054816961288452, 'cosine_with_motion': 0.34943318367004395, 'motion_component': 0.31640535593032837, 'motion_component_percent': 34.943318367004395}, {'resid': 1082, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 10.046111106872559, 'force': [-0.03528735041618347, 0.1211538091301918, 0.03364656865596771], 'magnitude': 0.1305968314409256, 'cosine_with_motion': 0.17554278671741486, 'motion_component': 0.022925332188606262, 'motion_component_percent': 17.554278671741486}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 10.121879577636719, 'force': [-0.1296529471874237, 0.31674060225486755, 0.10528816282749176], 'magnitude': 0.35807833075523376, 'cosine_with_motion': 0.15437749028205872, 'motion_component': 0.055279236286878586, 'motion_component_percent': 15.437749028205872}, {'resid': 1082, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 11.538230895996094, 'force': [-0.03117317333817482, 0.13058780133724213, 0.03844199702143669], 'magnitude': 0.13965216279029846, 'cosine_with_motion': 0.1489255726337433, 'motion_component': 0.02079777792096138, 'motion_component_percent': 14.892557263374329}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 11.622241020202637, 'force': [0.006095070391893387, -0.040890973061323166, -0.009940920397639275], 'magnitude': 0.04252109304070473, 'cosine_with_motion': -0.17222930490970612, 'motion_component': -0.0073233782313764095, 'motion_component_percent': 17.22293049097061}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 11.701863288879395, 'force': [0.008513454347848892, -0.03815898671746254, -0.01519036665558815], 'magnitude': 0.04194442182779312, 'cosine_with_motion': -0.05679924413561821, 'motion_component': -0.002382411388680339, 'motion_component_percent': 5.679924413561821}, {'resid': 1082, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 12.626124382019043, 'force': [-0.008443578146398067, 0.026241667568683624, 0.006501106545329094], 'magnitude': 0.028322843834757805, 'cosine_with_motion': 0.20818769931793213, 'motion_component': 0.005896467715501785, 'motion_component_percent': 20.818769931793213}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HG2', 'charge': -0.042500000447034836, 'distance': 13.607799530029297, 'force': [0.020311852917075157, -0.07100296765565872, -0.018770884722471237], 'magnitude': 0.07619933784008026, 'cosine_with_motion': -0.18600434064865112, 'motion_component': -0.014173407107591629, 'motion_component_percent': 18.600434064865112}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 12.755013465881348, 'force': [0.030905919149518013, -0.07728847861289978, -0.02435700036585331], 'magnitude': 0.08672916889190674, 'cosine_with_motion': -0.16680175065994263, 'motion_component': -0.014466577209532261, 'motion_component_percent': 16.680175065994263}, {'resid': 1082, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 12.550080299377441, 'force': [-0.5913727879524231, 1.5785022974014282, 0.2018357366323471], 'magnitude': 1.6976834535598755, 'cosine_with_motion': 0.3223201334476471, 'motion_component': 0.5471975803375244, 'motion_component_percent': 32.23201334476471}, {'resid': 1082, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 12.105847358703613, 'force': [0.8085550665855408, -1.6584389209747314, -0.19118669629096985], 'magnitude': 1.8549213409423828, 'cosine_with_motion': -0.34901800751686096, 'motion_component': -0.647400975227356, 'motion_component_percent': 34.901800751686096}, {'resid': 1082, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 13.344992637634277, 'force': [0.48874467611312866, -1.4436589479446411, -0.08361505717039108], 'magnitude': 1.5264383554458618, 'cosine_with_motion': -0.3769277334213257, 'motion_component': -0.5753569602966309, 'motion_component_percent': 37.69277334213257}, {'resid': 1082, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 9.133936882019043, 'force': [-0.3902582824230194, 1.9584839344024658, 0.756198525428772], 'magnitude': 2.1353681087493896, 'cosine_with_motion': 0.06073874980211258, 'motion_component': 0.12969958782196045, 'motion_component_percent': 6.073874980211258}, {'resid': 1082, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 9.183073043823242, 'force': [0.5115017890930176, -1.960960865020752, -1.0683274269104004], 'magnitude': 2.290922164916992, 'cosine_with_motion': 0.04907416179776192, 'motion_component': 0.11242508888244629, 'motion_component_percent': 4.907416179776192}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'N', 'charge': -0.38210001587867737, 'distance': 12.496807098388672, 'force': [-0.5212306380271912, -0.06541899591684341, -0.6195739507675171], 'magnitude': 0.812300980091095, 'cosine_with_motion': 0.8354735374450684, 'motion_component': 0.6786559820175171, 'motion_component_percent': 83.54735374450684}, {'resid': 130, 'resname': 'ASN', 'atom': 'H', 'charge': 0.2681000232696533, 'distance': 12.138741493225098, 'force': [0.39649853110313416, 0.09178170561790466, 0.4463924169540405], 'magnitude': 0.6040704846382141, 'cosine_with_motion': -0.7933691143989563, 'motion_component': -0.47925084829330444, 'motion_component_percent': 79.33691143989563}, {'resid': 130, 'resname': 'ASN', 'atom': 'CA', 'charge': -0.20800000429153442, 'distance': 11.789182662963867, 'force': [-0.2958124577999115, -0.00013681696145795286, -0.3992052376270294], 'magnitude': 0.49685999751091003, 'cosine_with_motion': 0.8866949677467346, 'motion_component': 0.44056326150894165, 'motion_component_percent': 88.66949677467346}, {'resid': 130, 'resname': 'ASN', 'atom': 'HA', 'charge': 0.13580000400543213, 'distance': 12.147562026977539, 'force': [0.19078649580478668, -0.02332831732928753, 0.2375023365020752], 'magnitude': 0.3055340647697449, 'cosine_with_motion': -0.8988299369812012, 'motion_component': -0.27462315559387207, 'motion_component_percent': 89.88299369812012}, {'resid': 130, 'resname': 'ASN', 'atom': 'CB', 'charge': -0.22990000247955322, 'distance': 10.320075035095215, 'force': [-0.4287400245666504, -0.014182431623339653, -0.5740888714790344], 'magnitude': 0.7166569828987122, 'cosine_with_motion': 0.8785156607627869, 'motion_component': 0.6295943856239319, 'motion_component_percent': 87.85156607627869}, {'resid': 130, 'resname': 'ASN', 'atom': 'HB2', 'charge': 0.1023000031709671, 'distance': 9.999173164367676, 'force': [0.22983939945697784, 0.010219573974609375, 0.2499203383922577], 'magnitude': 0.3396921753883362, 'cosine_with_motion': -0.8392723202705383, 'motion_component': -0.2850942313671112, 'motion_component_percent': 83.92723202705383}, {'resid': 130, 'resname': 'ASN', 'atom': 'HB3', 'charge': 0.1023000031709671, 'distance': 10.080110549926758, 'force': [0.18460382521152496, 0.03672175854444504, 0.27622827887535095], 'magnitude': 0.3342590630054474, 'cosine_with_motion': -0.8560652136802673, 'motion_component': -0.2861475646495819, 'motion_component_percent': 85.60652136802673}, {'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 9.725334167480469, 'force': [1.345657229423523, -0.2457275092601776, 2.1054904460906982], 'magnitude': 2.5108296871185303, 'cosine_with_motion': -0.9354516863822937, 'motion_component': -2.348759889602661, 'motion_component_percent': 93.54516863822937}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 9.112768173217773, 'force': [-1.0484338998794556, 0.19763422012329102, -2.1529102325439453], 'magnitude': 2.40276837348938, 'cosine_with_motion': 0.9524186253547668, 'motion_component': 2.2884414196014404, 'motion_component_percent': 95.24186253547668}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 10.101024627685547, 'force': [-1.645513653755188, 0.6352711915969849, -2.3718857765197754], 'magnitude': 2.9558632373809814, 'cosine_with_motion': 0.950535237789154, 'motion_component': 2.809652090072632, 'motion_component_percent': 95.0535237789154}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 10.031545639038086, 'force': [0.6678047180175781, -0.38841715455055237, 1.130369782447815], 'magnitude': 1.3691482543945312, 'cosine_with_motion': -0.9755627512931824, 'motion_component': -1.3356900215148926, 'motion_component_percent': 97.55627512931824}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 10.60934829711914, 'force': [0.7600784301757812, -0.2802553176879883, 0.9176613688468933], 'magnitude': 1.2240771055221558, 'cosine_with_motion': -0.9270082116127014, 'motion_component': -1.1347295045852661, 'motion_component_percent': 92.70082116127014}, {'resid': 130, 'resname': 'ASN', 'atom': 'C', 'charge': 0.8050000071525574, 'distance': 12.400932312011719, 'force': [0.8647244572639465, -0.0042650592513382435, 1.5074937343597412], 'magnitude': 1.7379021644592285, 'cosine_with_motion': -0.9164512753486633, 'motion_component': -1.5927026271820068, 'motion_component_percent': 91.64512753486633}, {'resid': 130, 'resname': 'ASN', 'atom': 'O', 'charge': -0.8147000074386597, 'distance': 12.426905632019043, 'force': [-0.7827314138412476, 0.14578676223754883, -1.5600723028182983], 'magnitude': 1.7514986991882324, 'cosine_with_motion': 0.9510787129402161, 'motion_component': 1.6658130884170532, 'motion_component_percent': 95.1078712940216}, {'resid': 458, 'resname': 'ASN', 'atom': 'N', 'charge': -0.38210001587867737, 'distance': 14.38281536102295, 'force': [0.4346216022968292, 0.09637151658535004, -0.42175158858299255], 'magnitude': 0.6132355332374573, 'cosine_with_motion': 0.46369469165802, 'motion_component': 0.2843540608882904, 'motion_component_percent': 46.369469165802}, {'resid': 458, 'resname': 'ASN', 'atom': 'H', 'charge': 0.2681000232696533, 'distance': 14.061104774475098, 'force': [-0.32625627517700195, -0.0962473526597023, 0.29489749670028687], 'magnitude': 0.4501902461051941, 'cosine_with_motion': -0.44995635747909546, 'motion_component': -0.2025659680366516, 'motion_component_percent': 44.995635747909546}, {'resid': 458, 'resname': 'ASN', 'atom': 'CA', 'charge': -0.20800000429153442, 'distance': 13.37633228302002, 'force': [0.26698482036590576, 0.03246859833598137, -0.2768027186393738], 'magnitude': 0.38594669103622437, 'cosine_with_motion': 0.46905651688575745, 'motion_component': 0.18103080987930298, 'motion_component_percent': 46.905651688575745}, {'resid': 458, 'resname': 'ASN', 'atom': 'HA', 'charge': 0.13580000400543213, 'distance': 13.49803352355957, 'force': [-0.17866121232509613, -0.0034302473068237305, 0.1711799055337906], 'magnitude': 0.24745535850524902, 'cosine_with_motion': -0.41292113065719604, 'motion_component': -0.10217954963445663, 'motion_component_percent': 41.292113065719604}, {'resid': 458, 'resname': 'ASN', 'atom': 'CB', 'charge': -0.22990000247955322, 'distance': 11.916101455688477, 'force': [0.3758048415184021, 0.06681672483682632, -0.37848737835884094], 'magnitude': 0.5375373959541321, 'cosine_with_motion': 0.4694492220878601, 'motion_component': 0.2523465156555176, 'motion_component_percent': 46.94492220878601}, {'resid': 458, 'resname': 'ASN', 'atom': 'HB2', 'charge': 0.1023000031709671, 'distance': 11.7998628616333, 'force': [-0.18486283719539642, -0.03484199568629265, 0.15528079867362976], 'magnitude': 0.24392695724964142, 'cosine_with_motion': -0.39895015954971313, 'motion_component': -0.09731470048427582, 'motion_component_percent': 39.89501595497131}, {'resid': 458, 'resname': 'ASN', 'atom': 'HB3', 'charge': 0.1023000031709671, 'distance': 11.811158180236816, 'force': [-0.15925630927085876, -0.0486336387693882, 0.17760992050170898], 'magnitude': 0.24346064031124115, 'cosine_with_motion': -0.5316342711448669, 'motion_component': -0.12943202257156372, 'motion_component_percent': 53.163427114486694}, {'resid': 458, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 10.860250473022461, 'force': [-1.3759504556655884, -0.061123933643102646, 1.4687113761901855], 'magnitude': 2.013476848602295, 'cosine_with_motion': -0.46340736746788025, 'motion_component': -0.9330599904060364, 'motion_component_percent': 46.340736746788025}, {'resid': 458, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 11.175772666931152, 'force': [1.0124400854110718, -0.0790393203496933, -1.2332555055618286], 'magnitude': 1.597561001777649, 'cosine_with_motion': 0.4874049723148346, 'motion_component': 0.7786591649055481, 'motion_component_percent': 48.74049723148346}, {'resid': 458, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 9.594298362731934, 'force': [2.3353331089019775, 0.13818761706352234, -2.293799877166748], 'magnitude': 3.276338577270508, 'cosine_with_motion': 0.4329913258552551, 'motion_component': 1.4186261892318726, 'motion_component_percent': 43.29913258552551}, {'resid': 458, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 9.055036544799805, 'force': [-1.13761568069458, 0.05803200975060463, 1.2353612184524536], 'magnitude': 1.6803733110427856, 'cosine_with_motion': -0.44745999574661255, 'motion_component': -0.7518998384475708, 'motion_component_percent': 44.745999574661255}, {'resid': 458, 'resname': 'ASN', 'atom'</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>594</v>
+      </c>
+      <c r="B6" t="n">
+        <v>707</v>
+      </c>
+      <c r="C6" t="n">
+        <v>2276</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>{572: {'frame': 572, 'motion_vector': [0.15352249145507812, 0.076873779296875, 0.39681243896484375], 'motion_vector_magnitude': 0.43236425518989563, 'ionic_force': [-0.3125167489051819, -1.289296954870224, -9.502991199493408], 'ionic_force_magnitude': 9.595144349817415, 'radial_force': 1.3266323364760475, 'axial_force': -9.502991199493408, 'glu_force': [0.9554665456525981, -0.30127836768951965, -4.48761841095984], 'glu_force_magnitude': 4.598086991030583, 'asn_force': [0.33605277934111655, 0.08795814258337487, 0.8305616825819016], 'asn_force_magnitude': 0.9002781869638328, 'sf_force': [-1.5402950609513937, 6.563160356687149, 5.1141541545512155], 'sf_force_magnitude': 8.461805685484304, 'residue_force': [-0.248775735957679, 6.349840131581004, 1.4570974261732772], 'residue_force_magnitude': 6.519623606681503, 'pip2_force': [0.5148408971726894, 0.06700416374951601, -3.789991525663936], 'pip2_force_magnitude': 3.8253871009305453, 'total_force': [-0.046451587690171436, 5.127547340460296, -11.835885298984067], 'total_force_magnitude': 12.89891779527909, 'cosine_total_motion': -0.772738052483734, 'cosine_glu_motion': -0.8335901745523787, 'cosine_asn_motion': 0.9966151169827423, 'cosine_sf_motion': 0.6279549963311233, 'cosine_residue_motion': 0.3647363735697491, 'cosine_pip2_motion': -0.8583791320678055, 'cosine_ionic_motion': -0.9444147683160993, 'motion_component_total': -9.967484616271744, 'motion_component_glu': -3.8329201374602055, 'motion_component_asn': 0.8972308506179714, 'motion_component_sf': 5.3136331581829745, 'motion_component_residue': 2.3779438713407397, 'motion_component_ionic': -9.061796028092344, 'motion_component_pip2': -3.28363245952014, 'motion_component_percent_total': 77.27380524837339, 'motion_component_percent_glu': 83.35901745523788, 'motion_component_percent_asn': 99.66151169827423, 'motion_component_percent_sf': 62.79549963311233, 'motion_component_percent_residue': 36.473637356974905, 'motion_component_percent_ionic': 94.44147683160993, 'motion_component_percent_pip2': 85.83791320678054, 'ionic_contributions': [{'ion_id': 2397, 'distance': 6.32469367980957, 'force': [-2.0392518043518066, -2.568722724914551, 7.624112129211426], 'magnitude': 8.299636840820312, 'cosine_ionic_motion': 0.7008019685745239, 'motion_component_ionic': 5.816401958465576, 'motion_component_percent_ionic': 70.08019685745239}, {'ion_id': 2399, 'distance': 12.818243026733398, 'force': [-0.5064868330955505, 0.3477652072906494, 1.9249334335327148], 'magnitude': 2.0206034183502197, 'cosine_ionic_motion': 0.8159163594245911, 'motion_component_ionic': 1.6486433744430542, 'motion_component_percent_ionic': 81.5916359424591}, {'ion_id': 2400, 'distance': 10.611924171447754, 'force': [1.8795051574707031, 0.12723931670188904, 2.267789363861084], 'magnitude': 2.9481515884399414, 'cosine_ionic_motion': 0.9400155544281006, 'motion_component_ionic': 2.771308422088623, 'motion_component_percent_ionic': 94.00155544281006}, {'ion_id': 2520, 'distance': 3.9445085525512695, 'force': [0.35371673107147217, 0.8044212460517883, -21.319826126098633], 'magnitude': 21.337928771972656, 'cosine_ionic_motion': -0.9044058918952942, 'motion_component_ionic': -19.29814910888672, 'motion_component_percent_ionic': 90.44058918952942}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 9.710868835449219, 'force': [-1.7115813493728638, -0.294517457485199, -0.5364797115325928], 'magnitude': 1.817707896232605, 'cosine_with_motion': -0.6340261697769165, 'motion_component': -1.1524744033813477, 'motion_component_percent': 63.40261697769165}, {'resid': 98, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 10.347222328186035, 'force': [0.8783551454544067, 0.12435287237167358, 0.2047225534915924], 'magnitude': 0.9104299545288086, 'cosine_with_motion': 0.5732260346412659, 'motion_component': 0.521882176399231, 'motion_component_percent': 57.32260346412659}, {'resid': 98, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 10.255535125732422, 'force': [0.11331728845834732, 0.014284307137131691, 0.051571737974882126], 'magnitude': 0.12531757354736328, 'cosine_with_motion': 0.7190310955047607, 'motion_component': 0.09010723233222961, 'motion_component_percent': 71.90310955047607}, {'resid': 98, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 10.601941108703613, 'force': [0.28378385305404663, 0.06430863589048386, 0.14784449338912964], 'magnitude': 0.3263845443725586, 'cosine_with_motion': 0.7594929933547974, 'motion_component': 0.2478867769241333, 'motion_component_percent': 75.94929933547974}, {'resid': 98, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 11.543353080749512, 'force': [0.12798471748828888, 0.007167627103626728, 0.05510599911212921], 'magnitude': 0.13952825963497162, 'cosine_with_motion': 0.6973040103912354, 'motion_component': 0.09729361534118652, 'motion_component_percent': 69.73040103912354}, {'resid': 98, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 11.616106033325195, 'force': [-0.04024822637438774, 0.00021770216699223965, -0.013852757401764393], 'magnitude': 0.04256602004170418, 'cosine_with_motion': -0.6335145831108093, 'motion_component': -0.026966193690896034, 'motion_component_percent': 63.35145831108093}, {'resid': 98, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 11.898330688476562, 'force': [-0.0360567644238472, 9.759354725247249e-05, -0.01859782263636589], 'magnitude': 0.040570665150880814, 'cosine_with_motion': -0.7358556985855103, 'motion_component': -0.02985415607690811, 'motion_component_percent': 73.58556985855103}, {'resid': 98, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 12.772038459777832, 'force': [0.02527405135333538, 0.0036276138853281736, 0.010686976835131645], 'magnitude': 0.02767939120531082, 'cosine_with_motion': 0.7018736600875854, 'motion_component': 0.019427435472607613, 'motion_component_percent': 70.18736600875854}, {'resid': 98, 'resname': 'GLU', 'atom': 'HG2', 'charge': -0.042500000447034836, 'distance': 12.720277786254883, 'force': [-0.08114060014486313, -0.015751073136925697, -0.02779485285282135], 'magnitude': 0.0872034803032875, 'cosine_with_motion': -0.6550316214561462, 'motion_component': -0.05712103843688965, 'motion_component_percent': 65.50316214561462}, {'resid': 98, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 13.707199096679688, 'force': [-0.06887738406658173, -0.0066835288889706135, -0.029171524569392204], 'magnitude': 0.07509820908308029, 'cosine_with_motion': -0.6979917287826538, 'motion_component': -0.05241793021559715, 'motion_component_percent': 69.79917287826538}, {'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 13.05179214477539, 'force': [1.3516136407852173, 0.31946444511413574, 0.7314087152481079], 'magnitude': 1.569673776626587, 'cosine_with_motion': 0.7695831060409546, 'motion_component': 1.2079944610595703, 'motion_component_percent': 76.95831060409546}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 13.015609741210938, 'force': [-1.317733645439148, -0.2646907866001129, -0.876639187335968], 'magnitude': 1.604674220085144, 'cosine_with_motion': -0.8222942352294922, 'motion_component': -1.3195143938064575, 'motion_component_percent': 82.22942352294922}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 13.375911712646484, 'force': [-1.2850030660629272, -0.4449901878833771, -0.6777130961418152], 'magnitude': 1.5193893909454346, 'cosine_with_motion': -0.761740505695343, 'motion_component': -1.15738046169281, 'motion_component_percent': 76.1740505695343}, {'resid': 98, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 9.412531852722168, 'force': [1.7474619150161743, 0.049468111246824265, 0.9936683773994446], 'magnitude': 2.0108323097229004, 'cosine_with_motion': 0.7664691209793091, 'motion_component': 1.541240930557251, 'motion_component_percent': 76.64691209793091}, {'resid': 98, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 9.385722160339355, 'force': [-1.7510242462158203, -0.09986753016710281, -1.3166109323501587], 'magnitude': 2.1930625438690186, 'cosine_with_motion': -0.8425911068916321, 'motion_component': -1.8478549718856812, 'motion_component_percent': 84.25911068916321}, {'resid': 426, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 9.691309928894043, 'force': [1.7580598592758179, 0.40326058864593506, -0.27824637293815613], 'magnitude': 1.8250519037246704, 'cosine_with_motion': 0.24140582978725433, 'motion_component': 0.4405781626701355, 'motion_component_percent': 24.140582978725433}, {'resid': 426, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 10.28647518157959, 'force': [-0.9039757251739502, -0.1559552550315857, 0.08451486378908157], 'magnitude': 0.9212149381637573, 'cosine_with_motion': -0.29433292150497437, 'motion_component': -0.2711438834667206, 'motion_component_percent': 29.433292150497437}, {'resid': 426, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 10.159980773925781, 'force': [-0.11892162263393402, -0.02818240411579609, 0.03697407618165016], 'magnitude': 0.12768587470054626, 'cosine_with_motion': -0.10418745875358582, 'motion_component': -0.01330326683819294, 'motion_component_percent': 10.418745875358582}, {'resid': 426, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 10.391952514648438, 'force': [-0.3042597770690918, -0.10696590691804886, 0.10670490562915802], 'magnitude': 0.3397081792354584, 'cosine_with_motion': -0.08572953939437866, 'motion_component': -0.029123026877641678, 'motion_component_percent': 8.572953939437866}, {'resid': 426, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 11.490646362304688, 'force': [-0.13337787985801697, -0.022557809948921204, 0.03910602629184723], 'magnitude': 0.14081120491027832, 'cosine_with_motion': -0.10993197560310364, 'motion_component': -0.01547965407371521, 'motion_component_percent': 10.993197560310364}, {'resid': 426, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 12.016432762145996, 'force': [0.0382157601416111, 0.007521713152527809, -0.008074456825852394], 'magnitude': 0.03977709636092186, 'cosine_with_motion': 0.18845908343791962, 'motion_component': 0.007496355101466179, 'motion_component_percent': 18.84590834379196}, {'resid': 426, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 11.472623825073242, 'force': [0.04185941070318222, 0.0028841495513916016, -0.011987180449068546], 'magnitude': 0.04363738372921944, 'cosine_with_motion': 0.1002485528588295, 'motion_component': 0.004374584648758173, 'motion_component_percent': 10.02485528588295}, {'resid': 426, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 12.531938552856445, 'force': [-0.026234272867441177, -0.005311676766723394, 0.010493883863091469], 'magnitude': 0.02875017561018467, 'cosine_with_motion': -0.02186354249715805, 'motion_component': -0.0006285806884989142, 'motion_component_percent': 2.186354249715805}, {'resid': 426, 'resname': 'GLU', 'atom': 'HG2', 'charge': -0.042500000447034836, 'distance': 12.563004493713379, 'force': [0.07910367846488953, 0.023693175986409187, -0.03425917774438858], 'magnitude': 0.0894005075097084, 'cosine_with_motion': 0.009600886143743992, 'motion_component': 0.0008583241142332554, 'motion_component_percent': 0.9600886143743992}, {'resid': 426, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 13.511012077331543, 'force': [0.07162120938301086, 0.013657618314027786, -0.02565901167690754], 'magnitude': 0.0772949755191803, 'cosine_with_motion': 0.0557626411318779, 'motion_component': 0.00431017205119133, 'motion_component_percent': 5.57626411318779}, {'resid': 426, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 12.534595489501953, 'force': [-1.5038708448410034, -0.18582883477210999, 0.7747501134872437], 'magnitude': 1.7018805742263794, 'cosine_with_motion': 0.08462134748697281, 'motion_component': 0.14401543140411377, 'motion_component_percent': 8.46213474869728}, {'resid': 426, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 12.538514137268066, 'force': [1.4435811042785645, 0.24256344139575958, -0.920366108417511], 'magnitude': 1.7291145324707031, 'cosine_with_motion': -0.1671249270439148, 'motion_component': -0.28897812962532043, 'motion_component_percent': 16.71249270439148}, {'resid': 426, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 12.736300468444824, 'force': [1.5112993717193604, 0.02438542991876602, -0.7237247228622437], 'magnitude': 1.6758275032043457, 'cosine_with_motion': -0.07354722172021866, 'motion_component': -0.12325245887041092, 'motion_component_percent': 7.354722172021866}, {'resid': 426, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 9.315009117126465, 'force': [-1.8697829246520996, -0.2771493196487427, 0.8015949726104736], 'magnitude': 2.053157329559326, 'cosine_with_motion': 0.01095358096063137, 'motion_component': 0.022489424794912338, 'motion_component_percent': 1.095358096063137}, {'resid': 426, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 9.275980949401855, 'force': [1.9034794569015503, 0.41105198860168457, -1.11758553981781], 'magnitude': 2.245260715484619, 'cosine_with_motion': -0.12324830144643784, 'motion_component': -0.27672457695007324, 'motion_component_percent': 12.324830144643784}, {'resid': 754, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 9.585121154785156, 'force': [-0.39680206775665283, 1.8010648488998413, -0.28213635087013245], 'magnitude': 1.8657135963439941, 'cosine_with_motion': -0.042667631059885025, 'motion_component': -0.0796055793762207, 'motion_component_percent': 4.2667631059885025}, {'resid': 754, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 10.1903076171875, 'force': [0.15463583171367645, -0.9222362637519836, 0.08182944357395172], 'magnitude': 0.9386841654777527, 'cosine_with_motion': -0.03618244081735611, 'motion_component': -0.0339638851583004, 'motion_component_percent': 3.618244081735611}, {'resid': 754, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 10.047160148620605, 'force': [0.026302220299839973, -0.1223367303609848, 0.03728709742426872], 'magnitude': 0.13056956231594086, 'cosine_with_motion': 0.16703058779239655, 'motion_component': 0.021809110417962074, 'motion_component_percent': 16.703058779239655}, {'resid': 754, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 10.34400749206543, 'force': [0.10062795877456665, -0.3093695342540741, 0.1082620620727539], 'magnitude': 0.34286466240882874, 'cosine_with_motion': 0.23357674479484558, 'motion_component': 0.08008521050214767, 'motion_component_percent': 23.357674479484558}, {'resid': 754, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 11.345527648925781, 'force': [0.02004973217844963, -0.1374761164188385, 0.03949941322207451], 'magnitude': 0.14443641901016235, 'cosine_with_motion': 0.13104479014873505, 'motion_component': 0.018927641212940216, 'motion_component_percent': 13.104479014873505}, {'resid': 754, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 12.006640434265137, 'force': [-0.007237139157950878, 0.03824581950902939, -0.008500969968736172], 'magnitude': 0.03984200581908226, 'cosine_with_motion': -0.08964532613754272, 'motion_component': -0.0035716495476663113, 'motion_component_percent': 8.964532613754272}, {'resid': 754, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 11.429488182067871, 'force': [-0.001993078738451004, 0.042417097836732864, -0.01139949169009924], 'magnitude': 0.04396738484501839, 'cosine_with_motion': -0.08251899480819702, 'motion_component': -0.003628144273534417, 'motion_component_percent': 8.251899480819702}, {'resid': 754, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 12.30929946899414, 'force': [0.004313956014811993, -0.02735625021159649, 0.011001862585544586], 'magnitude': 0.02979958988726139, 'cosine_with_motion': 0.22701986134052277, 'motion_component': 0.00676509877666831, 'motion_component_percent': 22.701986134052277}, {'resid': 754, 'resname': 'GLU', 'atom': 'HG2', 'charge': -0.042500000447034836, 'distance': 11.921906471252441, 'force': [-0.010349603369832039, 0.0886223167181015, -0.04352356120944023], 'magnitude': 0.09927401691675186, 'cosine_with_motion': -0.2806650698184967, 'motion_component': -0.027862748131155968, 'motion_component_percent': 28.06650698184967}, {'resid': 754, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 12.60661792755127, 'force': [-0.020058395341038704, 0.07969541102647781, -0.03359648212790489], 'magnitude': 0.08878300338983536, 'cosine_with_motion': -0.2679171860218048, 'motion_component': -0.02378649264574051, 'motion_component_percent': 26.79171860218048}, {'resid': 754, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 13.596606254577637, 'force': [0.14411380887031555, -1.3513742685317993, 0.49507009983062744], 'magnitude': 1.4464008808135986, 'cosine_with_motion': 0.1833939552307129, 'motion_component': 0.265261173248291, 'motion_component_percent': 18.33939552307129}, {'resid': 754, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 14.245744705200195, 'force': [-0.164395272731781, 1.278640627861023, -0.3637808561325073], 'magnitude': 1.3395088911056519, 'cosine_with_motion': -0.12310539931058884, 'motion_component': -0.1649007797241211, 'motion_component_percent': 12.310539931058884}, {'resid': 754, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 14.227850914001465, 'force': [-0.05676233768463135, 1.2315584421157837, -0.532324492931366], 'magnitude': 1.3428802490234375, 'cosine_with_motion': -0.2157592922449112, 'motion_component': -0.28973889350891113, 'motion_component_percent': 21.57592922449112}, {'resid': 754, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 9.182231903076172, 'force': [0.24628914892673492, -1.9294217824935913, 0.8254044055938721], 'magnitude': 2.112964630126953, 'cosine_with_motion': 0.23755119740962982, 'motion_component': 0.5019372701644897, 'motion_component_percent': 23.755119740962982}, {'resid': 754, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 9.205208778381348, 'force': [-0.33436155319213867, 1.936800241470337, -1.1554356813430786], 'magnitude': 2.2799177169799805, 'cosine_with_motion': -0.3661499619483948, 'motion_component': -0.8347917795181274, 'motion_component_percent': 36.61499619483948}, {'resid': 1082, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 9.577649116516113, 'force': [0.5019335746765137, -1.7486425638198853, -0.42670249938964844], 'magnitude': 1.8686259984970093, 'cosine_with_motion': -0.28057920932769775, 'motion_component': -0.5242975950241089, 'motion_component_percent': 28.057920932769775}, {'resid': 1082, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 10.034797668457031, 'force': [-0.19872359931468964, 0.9333007335662842, 0.16275542974472046], 'magnitude': 0.9680033922195435, 'cosine_with_motion': 0.252840131521225, 'motion_component': 0.24475009739398956, 'motion_component_percent': 25.284013152122498}, {'resid': 1082, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 10.04581356048584, 'force': [-0.0355733260512352, 0.11625991761684418, 0.04770452901721001], 'magnitude': 0.1306045651435852, 'cosine_with_motion': 0.3967820405960083, 'motion_component': 0.051821544766426086, 'motion_component_percent': 39.67820405960083}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 10.079503059387207, 'force': [-0.13175469636917114, 0.3043353259563446, 0.14286601543426514], 'magnitude': 0.3610955476760864, 'cosine_with_motion': 0.38340550661087036, 'motion_component': 0.13844601809978485, 'motion_component_percent': 38.340550661087036}, {'resid': 1082, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 11.44823932647705, 'force': [-0.030927324667572975, 0.1284281462430954, 0.051700375974178314], 'magnitude': 0.14185631275177002, 'cosine_with_motion': 0.4180428087711334, 'motion_component': 0.059302009642124176, 'motion_component_percent': 41.80428087711334}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 11.581928253173828, 'force': [0.005811235401779413, -0.04000482335686684, -0.014113539829850197], 'magnitude': 0.0428176149725914, 'cosine_with_motion': -0.4204438328742981, 'motion_component': -0.018002402037382126, 'motion_component_percent': 42.04438328742981}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 11.730895042419434, 'force': [0.008423054590821266, -0.03636959567666054, -0.018662452697753906], 'magnitude': 0.041737060993909836, 'cosine_with_motion': -0.4936509430408478, 'motion_component': -0.020603539422154427, 'motion_component_percent': 49.36509430408478}, {'resid': 1082, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 12.537525177001953, 'force': [-0.008322459645569324, 0.02596277929842472, 0.009042724967002869], 'magnitude': 0.028724556788802147, 'cosine_with_motion': 0.34674888849258423, 'motion_component': 0.009960208088159561, 'motion_component_percent': 34.67488884925842}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HG2', 'charge': -0.042500000447034836, 'distance': 12.29879379272461, 'force': [0.02954951301217079, -0.08572143316268921, -0.021917112171649933], 'magnitude': 0.09328289330005646, 'cosine_with_motion': -0.26654142141342163, 'motion_component': -0.024863755330443382, 'motion_component_percent': 26.654142141342163}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 13.469508171081543, 'force': [0.01930593140423298, -0.07129822671413422, -0.024337949231266975], 'magnitude': 0.07777205109596252, 'cosine_with_motion': -0.36206281185150146, 'motion_component': -0.028158366680145264, 'motion_component_percent': 36.20628118515015}, {'resid': 1082, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 12.970206260681152, 'force': [-0.6076231598854065, 1.3521521091461182, 0.5735293626785278], 'magnitude': 1.589483380317688, 'cosine_with_motion': 0.34667113423347473, 'motion_component': 0.5510280132293701, 'motion_component_percent': 34.66711342334747}, {'resid': 1082, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 13.214681625366211, 'force': [0.7138685584068298, -1.297705888748169, -0.47920653223991394], 'magnitude': 1.556691288948059, 'cosine_with_motion': -0.2679113745689392, 'motion_component': -0.41705530881881714, 'motion_component_percent': 26.79113745689392}, {'resid': 1082, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 13.227367401123047, 'force': [0.5676351189613342, -1.2695280313491821, -0.6928878426551819], 'magnitude': 1.5537067651748657, 'cosine_with_motion': -0.42484235763549805, 'motion_component': -0.6600804328918457, 'motion_component_percent': 42.484235763549805}, {'resid': 1082, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 9.171931266784668, 'force': [-0.3836880028247833, 1.8350181579589844, 0.9849880933761597], 'magnitude': 2.117713212966919, 'cosine_with_motion': 0.5166049003601074, 'motion_component': 1.094020962715149, 'motion_component_percent': 51.66049003601074}, {'resid': 1082, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 8.865360260009766, 'force': [0.5782567858695984, -1.9484940767288208, -1.3824187517166138], 'magnitude': 2.458066701889038, 'cosine_with_motion': -0.5735651850700378, 'motion_component': -1.409861445426941, 'motion_component_percent': 57.356518507003784}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CB', 'charge': -0.22990000247955322, 'distance': 14.665119171142578, 'force': [-0.13034234941005707, -0.04954785481095314, -0.326358437538147], 'magnitude': 0.35489991307258606, 'cosine_with_motion': -0.9991949200630188, 'motion_component': -0.3546141982078552, 'motion_component_percent': 99.91949200630188}, {'resid': 130, 'resname': 'ASN', 'atom': 'HB2', 'charge': 0.1023000031709671, 'distance': 14.004157066345215, 'force': [0.07225470244884491, 0.01911095157265663, 0.15622299909591675], 'magnitude': 0.17318081855773926, 'cosine_with_motion': 0.9956713914871216, 'motion_component': 0.17243118584156036, 'motion_component_percent': 99.56713914871216}, {'resid': 130, 'resname': 'ASN', 'atom': 'HB3', 'charge': 0.1023000031709671, 'distance': 14.679009437561035, 'force': [0.05772019922733307, 0.033514104783535004, 0.14279448986053467], 'magnitude': 0.15762323141098022, 'cosine_with_motion': 0.999261736869812, 'motion_component': 0.15750686824321747, 'motion_component_percent': 99.9261736869812}, {'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 14.617785453796387, 'force': [0.31191563606262207, 0.10833314061164856, 1.061198115348816], 'magnitude': 1.1113815307617188, 'cosine_with_motion': 0.9933176636695862, 'motion_component': 1.1039549112319946, 'motion_component_percent': 99.33176636695862}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 13.802395820617676, 'force': [-0.4181118905544281, -0.042038705199956894, -1.526301622390747], 'magnitude': 1.5830923318862915, 'cosine_with_motion': -0.9833509922027588, 'motion_component': -1.5567353963851929, 'motion_component_percent': 98.33509922027588}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 13.879307746887207, 'force': [0.14495591819286346, -0.006711688358336687, 0.7003628015518188], 'magnitude': 0.7152379751205444, 'cosine_with_motion': 0.9689803719520569, 'motion_component': 0.6930515766143799, 'motion_component_percent': 96.89803719520569}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 13.341304779052734, 'force': [0.2455645650625229, -0.0074915471486747265, 0.7340653538703918], 'magnitude': 0.774086594581604, 'cosine_with_motion': 0.9812442064285278, 'motion_component': 0.7595679759979248, 'motion_component_percent': 98.12442064285278}, {'resid': 458, 'resname': 'ASN', 'atom': 'CB', 'charge': -0.22990000247955322, 'distance': 14.670737266540527, 'force': [0.23773688077926636, -0.021059907972812653, -0.2622951865196228], 'magnitude': 0.3546281158924103, 'cosine_with_motion': -0.4513380229473114, 'motion_component': -0.1600571572780609, 'motion_component_percent': 45.13380229473114}, {'resid': 458, 'resname': 'ASN', 'atom': 'HB2', 'charge': 0.1023000031709671, 'distance': 14.456725120544434, 'force': [-0.11747827380895615, 0.008310407400131226, 0.11197562515735626], 'magnitude': 0.16250768303871155, 'cosine_with_motion': 0.38479435443878174, 'motion_component': 0.06253203749656677, 'motion_component_percent': 38.479435443878174}, {'resid': 458, 'resname': 'ASN', 'atom': 'HB3', 'charge': 0.1023000031709671, 'distance': 14.172569274902344, 'force': [-0.1094079241156578, 0.00010253903747070581, 0.12892301380634308], 'magnitude': 0.16908946633338928, 'cosine_with_motion': 0.4701188802719116, 'motion_component': 0.07949215173721313, 'motion_component_percent': 47.01188802719116}, {'resid': 458, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 14.105829238891602, 'force': [-0.7570440769195557, 0.17570717632770538, 0.9058130383491516], 'magnitude': 1.1935184001922607, 'cosine_with_motion': 0.4974896013736725, 'motion_component': 0.593762993812561, 'motion_component_percent': 49.74896013736725}, {'resid': 458, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 13.981952667236328, 'force': [0.5763665437698364, -0.15993249416351318, -0.8270126581192017], 'magnitude': 1.0206501483917236, 'cosine_with_motion': -0.5710005164146423, 'motion_component': -0.5827917456626892, 'motion_component_percent': 57.10005164146423}, {'resid': 458, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 14.164510726928711, 'force': [1.00485360622406, -0.3345543444156647, -1.0667258501052856], 'magnitude': 1.5031838417053223, 'cosine_with_motion': -0.4535013437271118, 'motion_component': -0.6816958785057068, 'motion_component_percent': 45.35013437271118}, {'resid': 458, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 14.098430633544922, 'force': [-0.44370460510253906, 0.19959264993667603, 0.49374526739120483], 'magnitude': 0.6931777596473694, 'cosine_with_motion': 0.4776327908039093, 'motion_component': 0.3310844302177429, 'motion_component_percent': 47.76327908039093}, {'resid': 458, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 14.467889785766602, 'force': [-0.47193485498428345, 0.13638269901275635, 0.438109815120697], 'magnitude': 0.6582271456718445, 'cosine_with_motion': 0.39311835169792175, 'motion_component': 0.2587611675262451, 'motion_component_percent': 39.311835169792175}, {'resid': 786, 'resname': 'ASN', 'atom': 'N', 'charge': -0.38210001587867737, 'distance': 14.986479759216309, 'force': [0.02374161221086979, 0.33377182483673096, -0.45504164695739746], 'magnitude': 0.564827561378479, 'cosine_with_motion': -0.6193941831588745, 'motion_component': -0.3498508930206299, 'motion_component_percent': 61.93941831588745}, {'resid': 786, 'resname': 'ASN', 'atom': 'H', 'charge': 0.2681000232696533, 'distance': 14.536611557006836, 'force': [0.0071253995411098, -0.2547243535518646, 0.33539628982543945], 'magnitude': 0.4212195873260498, 'cosine_with_motion': 0.6292638182640076, 'motion_component': 0.2650582492351532, 'motion_component_percent': 62.92638182640076}, {'resid': 786, 'resname': 'ASN', 'atom': 'CA', 'charge': -0.20800000429153442, 'distance': 14.380319595336914, 'force': [0.03476359695196152, 0.17844092845916748, -0.2801145017147064], 'magnitude': 0.3339368402957916, 'cosine_with_motion': -0.6378791928291321, 'motion_component': -0.21301135420799255, 'motion_component_percent': 63.78791928291321}, {'resid': 786, 'resname': 'ASN', 'atom': 'HA', 'charge': 0.13580000400543213, 'distance': 14.627284049987793, 'force': [-0.036351218819618225, -0.11577250063419342, 0.17227652668952942], 'magnitude': 0.21072229743003845, 'cosine_with_motion': 0.5913904905319214, 'motion_component': 0.12461916357278824, 'motion_component_percent': 59.13904905319214}, {'resid': 786, 'resname': 'ASN', 'atom': 'CB', 'charge': -0.22990000247955322, 'distance': 12.896712303161621, 'force': [0.04079525172710419, 0.24078422784805298, -0.3885214030742645], 'magnitude': 0.458901047706604, 'cosine_with_motion': -0.6521626114845276, 'motion_component': -0.2992781102657318, 'motion_component_percent': 65.21626114845276}, {'resid': 786, 'resname': 'ASN', 'atom': 'HB2', 'charge': 0.1023000031709671, 'distance': 12.373305320739746, 'force': [-0.02529660239815712, -0.12922902405261993, 0.17853142321109772], 'magnitude': 0.2218412309885025, 'cosine_with_motion': 0.594535231590271, 'motion_component': 0.13189242780208588, 'motion_component_percent': 59.4535231590271}, {'resid': 786, 'resname': 'ASN', 'atom': 'HB3', 'charge': 0.1023000031709671, 'distance': 12.658638954162598, 'force': [-0.0017513793427497149, -0.10795798152685165, 0.1823900043964386], 'magnitude': 0.2119530737400055, 'cosine_with_motion': 0.6962676048278809, 'motion_component': 0.14757606387138367, 'motion_component_percent': 69.62676048278809}, {'resid': 786, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 12.32958698272705, 'force': [-0.2533985376358032, -0.6976304054260254, 1.3745859861373901], 'magnitude': 1.5621733665466309, 'cosine_with_motion': 0.6705688834190369, 'motion_component': 1.0475448369979858, 'motion_component_percent': 67.05688834190369}, {'resid': 786, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 12.799765586853027, 'force': [0.3056301772594452, 0.5271573662757874, -1.0544925928115845], 'magnitude': 1.2178913354873657, 'cosine_with_motion': -0.6285744309425354, 'motion_component': -0.7655353546142578, 'motion_component_percent': 62.85744309425354}, {'resid': 786, 'resname': 'ASN', 'atom': 'ND2'</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>699</v>
+      </c>
+      <c r="B7" t="n">
+        <v>787</v>
+      </c>
+      <c r="C7" t="n">
+        <v>2520</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>{594: {'frame': 594, 'motion_vector': [0.022796630859375, 0.11915206909179688, -0.375732421875], 'motion_vector_magnitude': 0.3948312997817993, 'ionic_force': [-3.058868169784546, -1.4938152581453323, 2.6580605506896973], 'ionic_force_magnitude': 4.318963347462176, 'radial_force': 3.404138438076346, 'axial_force': 2.6580605506896973, 'glu_force': [1.1205107644200325, -0.40159851871430874, -3.9068927109474316], 'glu_force_magnitude': 4.084193481982564, 'asn_force': [-0.4061229359358549, 0.18224849039688706, -0.6486099287867546], 'asn_force_magnitude': 0.7866671412140345, 'sf_force': [-9.48588762648751, 3.600470368848619, 16.548227221283014], 'sf_force_magnitude': 19.41106063837105, 'residue_force': [-8.771499798003333, 3.381120340531197, 11.992724581548828], 'residue_force_magnitude': 15.237999420934882, 'pip2_force': [0.5804278971627355, 0.039335550274699926, -3.9027120734317577], 'pip2_force_magnitude': 3.945833924207933, 'total_force': [-11.249940070625144, 1.9266406326605647, 10.748073058806767], 'total_force_magnitude': 15.677824153801566, 'cosine_total_motion': -0.6567421829377594, 'cosine_glu_motion': 0.8964827069032978, 'cosine_asn_motion': 0.824726838327264, 'cosine_sf_motion': -0.7835169975664343, 'cosine_residue_motion': -0.7152317910938658, 'cosine_pip2_motion': 0.9527294662221718, 'cosine_ionic_motion': -0.7309390782921045, 'motion_component_total': -10.296288458481971, 'motion_component_glu': 3.661408828244534, 'motion_component_asn': 0.648785504189398, 'motion_component_sf': -15.20889595095648, 'motion_component_residue': -10.898701618522546, 'motion_component_ionic': -3.156899088371385, 'motion_component_pip2': 3.7593122484119617, 'motion_component_percent_total': 65.67421829377594, 'motion_component_percent_glu': 89.64827069032978, 'motion_component_percent_asn': 82.4726838327264, 'motion_component_percent_sf': 78.35169975664343, 'motion_component_percent_residue': 71.52317910938658, 'motion_component_percent_ionic': 73.09390782921045, 'motion_component_percent_pip2': 95.27294662221718, 'ionic_contributions': [{'ion_id': 2223, 'distance': 5.6569085121154785, 'force': [-0.19841152429580688, 0.05314994603395462, -10.372767448425293], 'magnitude': 10.374800682067871, 'cosine_ionic_motion': 0.9518829584121704, 'motion_component_ionic': 9.875596046447754, 'motion_component_percent_ionic': 95.18829584121704}, {'ion_id': 2276, 'distance': 6.330036163330078, 'force': [-5.173781394958496, -1.9436408281326294, 6.173002243041992], 'magnitude': 8.285633087158203, 'cosine_ionic_motion': -0.815830647945404, 'motion_component_ionic': -6.759673595428467, 'motion_component_percent_ionic': 81.5830647945404}, {'ion_id': 2391, 'distance': 13.529471397399902, 'force': [0.15421754121780396, 0.10575271397829056, -1.804080605506897], 'magnitude': 1.8137457370758057, 'cosine_ionic_motion': 0.969061553478241, 'motion_component_ionic': 1.7576313018798828, 'motion_component_percent_ionic': 96.9061553478241}, {'ion_id': 2397, 'distance': 10.326164245605469, 'force': [2.3755767345428467, 0.39075520634651184, 1.974417805671692], 'magnitude': 3.1135799884796143, 'cosine_ionic_motion': -0.5215309858322144, 'motion_component_ionic': -1.6238285303115845, 'motion_component_percent_ionic': 52.153098583221436}, {'ion_id': 2399, 'distance': 10.54881763458252, 'force': [-0.4804004728794098, 0.49685174226760864, 2.9023799896240234], 'magnitude': 2.9835307598114014, 'cosine_ionic_motion': -0.8847848176956177, 'motion_component_ionic': -2.639782667160034, 'motion_component_percent_ionic': 88.47848176956177}, {'ion_id': 2400, 'distance': 9.297172546386719, 'force': [0.26393094658851624, -0.5966840386390686, 3.7851085662841797], 'magnitude': 3.8409292697906494, 'cosine_ionic_motion': -0.9807112812995911, 'motion_component_ionic': -3.7668426036834717, 'motion_component_percent_ionic': 98.0711281299591}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 9.590046882629395, 'force': [-1.7928144931793213, -0.48158109188079834, -0.16624599695205688], 'magnitude': 1.863797664642334, 'cosine_with_motion': -0.048631880432367325, 'motion_component': -0.09063998609781265, 'motion_component_percent': 4.8631880432367325}, {'resid': 98, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 10.065117835998535, 'force': [0.9421316981315613, 0.19442380964756012, 0.019437531009316444], 'magnitude': 0.9621801376342773, 'cosine_with_motion': 0.09828963875770569, 'motion_component': 0.09457233548164368, 'motion_component_percent': 9.828963875770569}, {'resid': 98, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 9.86525821685791, 'force': [0.12745700776576996, 0.032909732311964035, 0.031822580844163895], 'magnitude': 0.1354290097951889, 'cosine_with_motion': -0.09593729674816132, 'motion_component': -0.012992693111300468, 'motion_component_percent': 9.593729674816132}, {'resid': 98, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 10.005486488342285, 'force': [0.33076760172843933, 0.12490391731262207, 0.09634892642498016], 'magnitude': 0.3664577901363373, 'cosine_with_motion': -0.0952281653881073, 'motion_component': -0.034897103905677795, 'motion_component_percent': 9.52281653881073}, {'resid': 98, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 11.345869064331055, 'force': [0.13721056282520294, 0.025212598964571953, 0.03737584501504898], 'magnitude': 0.14442771673202515, 'cosine_with_motion': -0.13873393833637238, 'motion_component': -0.020037025213241577, 'motion_component_percent': 13.873393833637238}, {'resid': 98, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 12.137920379638672, 'force': [-0.03716716542840004, -0.008428799919784069, -0.008208164013922215], 'magnitude': 0.03898482769727707, 'cosine_with_motion': 0.08007041364908218, 'motion_component': 0.0031215313356369734, 'motion_component_percent': 8.007041364908218}, {'resid': 98, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 11.383199691772461, 'force': [-0.04302111640572548, -0.003878240939229727, -0.009945317171514034], 'magnitude': 0.04432568699121475, 'cosine_with_motion': 0.13107359409332275, 'motion_component': 0.005809927359223366, 'motion_component_percent': 13.107359409332275}, {'resid': 98, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 11.767973899841309, 'force': [0.02969316765666008, 0.005381372757256031, 0.012344663962721825], 'magnitude': 0.03260420262813568, 'cosine_with_motion': -0.25791528820991516, 'motion_component': -0.008409122005105019, 'motion_component_percent': 25.791528820991516}, {'resid': 98, 'resname': 'GLU', 'atom': 'HG2', 'charge': -0.042500000447034836, 'distance': 12.76659870147705, 'force': [-0.07934975624084473, -0.011245482601225376, -0.03273890167474747], 'magnitude': 0.0865718200802803, 'cosine_with_motion': 0.2677559554576874, 'motion_component': 0.023180121555924416, 'motion_component_percent': 26.775595545768738}, {'resid': 98, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 11.049116134643555, 'force': [-0.10351207852363586, -0.013457213528454304, -0.0496208555996418], 'magnitude': 0.11557714641094208, 'cosine_with_motion': 0.32171520590782166, 'motion_component': 0.03718292713165283, 'motion_component_percent': 32.171520590782166}, {'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 12.047611236572266, 'force': [1.5929365158081055, 0.505753755569458, 0.7750096321105957], 'magnitude': 1.8422468900680542, 'cosine_with_motion': -0.26756566762924194, 'motion_component': -0.49292200803756714, 'motion_component_percent': 26.756566762924194}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 12.003085136413574, 'force': [-1.5292519330978394, -0.5395638346672058, -0.9645431041717529], 'magnitude': 1.8868184089660645, 'cosine_with_motion': 0.353378564119339, 'motion_component': 0.6667611598968506, 'motion_component_percent': 35.3378564119339}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 12.415393829345703, 'force': [-1.5277525186538696, -0.6155211329460144, -0.6303304433822632], 'magnitude': 1.7635788917541504, 'cosine_with_motion': 0.1847829520702362, 'motion_component': 0.32587930560112, 'motion_component_percent': 18.47829520702362}, {'resid': 98, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 8.910833358764648, 'force': [2.0850510597229004, 0.3682873249053955, 0.7421742677688599], 'magnitude': 2.2436344623565674, 'cosine_with_motion': -0.21159687638282776, 'motion_component': -0.47474604845046997, 'motion_component_percent': 21.159687638282776}, {'resid': 98, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 8.759810447692871, 'force': [-2.1793127059936523, -0.5478726029396057, -1.1353596448898315], 'magnitude': 2.5176596641540527, 'cosine_with_motion': 0.3134952783584595, 'motion_component': 0.7892744541168213, 'motion_component_percent': 31.349527835845947}, {'resid': 426, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 9.701981544494629, 'force': [1.7478071451187134, 0.5034265518188477, 0.0889742448925972], 'magnitude': 1.8210394382476807, 'cosine_with_motion': 0.0923471674323082, 'motion_component': 0.1681678295135498, 'motion_component_percent': 9.23471674323082}, {'resid': 426, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 10.35847282409668, 'force': [-0.8750235438346863, -0.2197779417037964, -0.106391042470932], 'magnitude': 0.9084534049034119, 'cosine_with_motion': -0.01717386208474636, 'motion_component': -0.01560165360569954, 'motion_component_percent': 1.717386208474636}, {'resid': 426, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 10.146203994750977, 'force': [-0.12246618419885635, -0.03517019748687744, 0.012550054118037224], 'magnitude': 0.1280328631401062, 'cosine_with_motion': -0.23140574991703033, 'motion_component': -0.029627541080117226, 'motion_component_percent': 23.140574991703033}, {'resid': 426, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 10.348739624023438, 'force': [-0.3154398798942566, -0.12589146196842194, 0.04461299628019333], 'magnitude': 0.3425511419773102, 'cosine_with_motion': -0.2880130708217621, 'motion_component': -0.0986592099070549, 'motion_component_percent': 28.80130708217621}, {'resid': 426, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 11.529033660888672, 'force': [-0.1357920616865158, -0.02951723523437977, 0.015946200117468834], 'magnitude': 0.13987505435943604, 'cosine_with_motion': -0.22822412848472595, 'motion_component': -0.03192286193370819, 'motion_component_percent': 22.822412848472595}, {'resid': 426, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 12.193486213684082, 'force': [0.037420690059661865, 0.009404510259628296, -0.001884087803773582], 'magnitude': 0.03863033279776573, 'cosine_with_motion': 0.17581062018871307, 'motion_component': 0.006791622843593359, 'motion_component_percent': 17.581062018871307}, {'resid': 426, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 11.566888809204102, 'force': [0.04241948574781418, 0.005156072787940502, -0.004111414309591055], 'magnitude': 0.0429290309548378, 'cosine_with_motion': 0.1844377964735031, 'motion_component': 0.00791773572564125, 'motion_component_percent': 18.44377964735031}, {'resid': 426, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 12.344389915466309, 'force': [-0.028080208227038383, -0.006961153354495764, 0.006403578910976648], 'magnitude': 0.029630417004227638, 'cosine_with_motion': -0.33127591013908386, 'motion_component': -0.009815843775868416, 'motion_component_percent': 33.127591013908386}, {'resid': 426, 'resname': 'GLU', 'atom': 'HG2', 'charge': -0.042500000447034836, 'distance': 12.504310607910156, 'force': [0.08309367299079895, 0.028571318835020065, -0.020559536293148994], 'magnitude': 0.09024174511432648, 'cosine_with_motion': 0.36551710963249207, 'motion_component': 0.0329849012196064, 'motion_component_percent': 36.55171096324921}, {'resid': 426, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 13.38047981262207, 'force': [0.07531361281871796, 0.017330503091216087, -0.015446572564542294], 'magnitude': 0.0788104236125946, 'cosine_with_motion': 0.30805328488349915, 'motion_component': 0.024277810007333755, 'motion_component_percent': 30.805328488349915}, {'resid': 426, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 12.048078536987305, 'force': [-1.7175227403640747, -0.3143385648727417, 0.5870725512504578], 'magnitude': 1.8421040773391724, 'cosine_with_motion': -0.4086095094680786, 'motion_component': -0.7527012228965759, 'motion_component_percent': 40.86095094680786}, {'resid': 426, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 11.921722412109375, 'force': [1.8096003532409668, 0.13593612611293793, -0.6042662262916565], 'magnitude': 1.9126603603363037, 'cosine_with_motion': 0.3767220675945282, 'motion_component': 0.7205413579940796, 'motion_component_percent': 37.67220675945282}, {'resid': 426, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 12.035977363586426, 'force': [1.6705882549285889, 0.4007371962070465, -0.7548986077308655], 'magnitude': 1.876520037651062, 'cosine_with_motion': 0.4986744821071625, 'motion_component': 0.9357726573944092, 'motion_component_percent': 49.86744821071625}, {'resid': 426, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 9.158407211303711, 'force': [-2.0385968685150146, -0.4331376254558563, 0.4096005856990814], 'magnitude': 2.123972177505493, 'cosine_with_motion': -0.3004762530326843, 'motion_component': -0.6382032036781311, 'motion_component_percent': 30.047625303268433}, {'resid': 426, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 8.989972114562988, 'force': [2.185789108276367, 0.6338819861412048, -0.7311016917228699], 'magnitude': 2.390395402908325, 'cosine_with_motion': 0.42387616634368896, 'motion_component': 1.013231635093689, 'motion_component_percent': 42.3876166343689}, {'resid': 754, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 9.445825576782227, 'force': [-0.6024428606033325, 1.8236416578292847, 0.04686163738369942], 'magnitude': 1.921146035194397, 'cosine_with_motion': 0.24514509737491608, 'motion_component': 0.47095954418182373, 'motion_component_percent': 24.514509737491608}, {'resid': 754, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 10.073192596435547, 'force': [0.24283239245414734, -0.9265748858451843, -0.07291767746210098], 'magnitude': 0.9606381058692932, 'cosine_with_motion': -0.20425009727478027, 'motion_component': -0.19621042907238007, 'motion_component_percent': 20.425009727478027}, {'resid': 754, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 9.66006851196289, 'force': [0.04076177999377251, -0.1340668648481369, 0.01772720366716385], 'magnitude': 0.14124341309070587, 'cosine_with_motion': -0.3892207443714142, 'motion_component': -0.054974865168333054, 'motion_component_percent': 38.92207443714142}, {'resid': 754, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 9.909429550170898, 'force': [0.14185284078121185, -0.3398035168647766, 0.06313369423151016], 'magnitude': 0.37359675765037537, 'cosine_with_motion': -0.4133743643760681, 'motion_component': -0.15443532168865204, 'motion_component_percent': 41.33743643760681}, {'resid': 754, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 10.91507339477539, 'force': [0.03327913582324982, -0.15102563798427582, 0.020889481529593468], 'magnitude': 0.15605324506759644, 'cosine_with_motion': -0.4071304202079773, 'motion_component': -0.06353402137756348, 'motion_component_percent': 40.71304202079773}, {'resid': 754, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 11.676067352294922, 'force': [-0.010561893694102764, 0.040659282356500626, -0.003194146091118455], 'magnitude': 0.04212995991110802, 'cosine_with_motion': 0.34891948103904724, 'motion_component': 0.014699963852763176, 'motion_component_percent': 34.891948103904724}, {'resid': 754, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 10.763864517211914, 'force': [-0.005994264502078295, 0.048948414623737335, -0.005062842275947332], 'magnitude': 0.04957328736782074, 'cosine_with_motion': 0.38818252086639404, 'motion_component': 0.019243484362959862, 'motion_component_percent': 38.818252086639404}, {'resid': 754, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 11.628021240234375, 'force': [0.006528609432280064, -0.0316387414932251, 0.008456393145024776], 'magnitude': 0.03339376300573349, 'cosine_with_motion': -0.5156148672103882, 'motion_component': -0.017218321561813354, 'motion_component_percent': 51.56148672103882}, {'resid': 754, 'resname': 'GLU', 'atom': 'HG2', 'charge': -0.042500000447034836, 'distance': 11.104201316833496, 'force': [-0.017659617587924004, 0.1067647784948349, -0.0372074693441391], 'magnitude': 0.11443328112363815, 'cosine_with_motion': 0.5820638537406921, 'motion_component': 0.06660747528076172, 'motion_component_percent': 58.206385374069214}, {'resid': 754, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 12.02552604675293, 'force': [-0.026712827384471893, 0.08987697213888168, -0.02699206955730915], 'magnitude': 0.09757057577371597, 'cosine_with_motion': 0.5254361629486084, 'motion_component': 0.051267109811306, 'motion_component_percent': 52.54361629486084}, {'resid': 754, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 12.89415168762207, 'force': [0.22279030084609985, -1.5483120679855347, 0.3737497925758362], 'magnitude': 1.608289361000061, 'cosine_with_motion': -0.5036757588386536, 'motion_component': -0.8100563883781433, 'motion_component_percent': 50.367575883865356}, {'resid': 754, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 13.579208374023438, 'force': [-0.2442905753850937, 1.43500554561615, -0.233350932598114], 'magnitude': 1.4742358922958374, 'cosine_with_motion': 0.434810996055603, 'motion_component': 0.6410139799118042, 'motion_component_percent': 43.4810996055603}, {'resid': 754, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 13.298093795776367, 'force': [-0.10438523441553116, 1.4683319330215454, -0.44290193915367126], 'magnitude': 1.5372238159179688, 'cosine_with_motion': 0.5585156679153442, 'motion_component': 0.8585635423660278, 'motion_component_percent': 55.851566791534424}, {'resid': 754, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 8.553815841674805, 'force': [0.5128027200698853, -2.3252127170562744, 0.5087481737136841], 'magnitude': 2.4348318576812744, 'cosine_with_motion': -0.4748717248439789, 'motion_component': -1.1562328338623047, 'motion_component_percent': 47.48717248439789}, {'resid': 754, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 8.290276527404785, 'force': [-0.6740087866783142, 2.5517735481262207, -0.9671778678894043], 'magnitude': 2.8109195232391357, 'cosine_with_motion': 0.5875483155250549, 'motion_component': 1.6515510082244873, 'motion_component_percent': 58.75483155250549}, {'resid': 1082, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 9.724139213562012, 'force': [0.5073971748352051, -1.735087275505066, -0.13447114825248718], 'magnitude': 1.8127498626708984, 'cosine_with_motion': -0.20209722220897675, 'motion_component': -0.3663517236709595, 'motion_component_percent': 20.209722220897675}, {'resid': 1082, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 10.440635681152344, 'force': [-0.2071099579334259, 0.8696102499961853, 0.022308319807052612], 'magnitude': 0.89421147108078, 'cosine_with_motion': 0.25636377930641174, 'motion_component': 0.2292434424161911, 'motion_component_percent': 25.636377930641174}, {'resid': 1082, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 9.92604923248291, 'force': [-0.036896418780088425, 0.12495025992393494, 0.030362853780388832], 'magnitude': 0.1337752491235733, 'cosine_with_motion': 0.04995696619153023, 'motion_component': 0.00668300548568368, 'motion_component_percent': 4.995696619153023}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 9.817631721496582, 'force': [-0.14068229496479034, 0.33904337882995605, 0.10063060373067856], 'magnitude': 0.38061586022377014, 'cosine_with_motion': -0.004122619051486254, 'motion_component': -0.001569134183228016, 'motion_component_percent': 0.4122619051486254}, {'resid': 1082, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 11.378716468811035, 'force': [-0.03374553471803665, 0.13527965545654297, 0.0343540757894516], 'magnitude': 0.14359508454799652, 'cosine_with_motion': 0.043065354228019714, 'motion_component': 0.0061839730478823185, 'motion_component_percent': 4.306535422801971}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 11.483257293701172, 'force': [0.006590817589312792, -0.04214286059141159, -0.008815769106149673], 'magnitude': 0.04355660080909729, 'cosine_with_motion': -0.09064045548439026, 'motion_component': -0.0039479900151491165, 'motion_component_percent': 9.064045548439026}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 11.620668411254883, 'force': [0.009094762615859509, -0.03915766254067421, -0.01389190461486578], 'magnitude': 0.042532604187726974, 'cosine_with_motion': 0.045330993831157684, 'motion_component': 0.0019280451815575361, 'motion_component_percent': 4.533099383115768}, {'resid': 1082, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 12.45029067993164, 'force': [-0.009140818379819393, 0.027086526155471802, 0.005588800646364689], 'magnitude': 0.02912849374115467, 'cosine_with_motion': 0.07991955429315567, 'motion_component': 0.0023279362358152866, 'motion_component_percent': 7.991955429315567}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HG2', 'charge': -0.042500000447034836, 'distance': 12.417304992675781, 'force': [0.02885790914297104, -0.0863056480884552, -0.009632422588765621], 'magnitude': 0.09151080250740051, 'cosine_with_motion': -0.16623854637145996, 'motion_component': -0.01521262340247631, 'motion_component_percent': 16.623854637145996}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 13.437140464782715, 'force': [0.022969571873545647, -0.07265974581241608, -0.01731882616877556], 'magnitude': 0.07814718037843704, 'cosine_with_motion': -0.052720408886671066, 'motion_component': -0.004119951277971268, 'motion_component_percent': 5.272040888667107}, {'resid': 1082, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 12.36180591583252, 'force': [-0.7420474290847778, 1.539110779762268, 0.3771846890449524], 'magnitude': 1.749789834022522, 'cosine_with_motion': 0.035826534032821655, 'motion_component': 0.0626889020204544, 'motion_component_percent': 3.5826534032821655}, {'resid': 1082, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 12.502397537231445, 'force': [0.8502728939056396, -1.497827172279358, -0.24100708961486816], 'magnitude': 1.7391189336776733, 'cosine_with_motion': -0.0998045802116394, 'motion_component': -0.17357203364372253, 'motion_component_percent': 9.98045802116394}, {'resid': 1082, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 12.179191589355469, 'force': [0.8138851523399353, -1.5413901805877686, -0.5659546852111816], 'magnitude': 1.8326475620269775, 'cosine_with_motion': 0.06570260226726532, 'motion_component': 0.12040971219539642, 'motion_component_percent': 6.570260226726532}, {'resid': 1082, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 9.121491432189941, 'force': [-0.4018396735191345, 1.9900614023208618, 0.6803784966468811], 'magnitude': 2.1411993503570557, 'cosine_with_motion': -0.03274247422814369, 'motion_component': -0.07010816782712936, 'motion_component_percent': 3.274247422814369}, {'resid': 1082, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 8.894001007080078, 'force': [0.5659362077713013, -2.12551212310791, -1.0613921880722046], 'magnitude': 2.442260980606079, 'cosine_with_motion': 0.1643107533454895, 'motion_component': 0.4012897312641144, 'motion_component_percent': 16.43107533454895}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'N', 'charge': -0.38210001587867737, 'distance': 14.63835334777832, 'force': [-0.2746018171310425, -0.15320074558258057, -0.5015993118286133], 'magnitude': 0.5920122265815735, 'cosine_with_motion': 0.7014180421829224, 'motion_component': 0.4152480661869049, 'motion_component_percent': 70.14180421829224}, {'resid': 130, 'resname': 'ASN', 'atom': 'H', 'charge': 0.2681000232696533, 'distance': 14.263683319091797, 'force': [0.20724180340766907, 0.1389089971780777, 0.359382301568985], 'magnitude': 0.4374934434890747, 'cosine_with_motion': -0.658552885055542, 'motion_component': -0.2881125807762146, 'motion_component_percent': 65.8552885055542}, {'resid': 130, 'resname': 'ASN', 'atom': 'CA', 'charge': -0.20800000429153442, 'distance': 14.161233901977539, 'force': [-0.13255809247493744, -0.07690223306417465, -0.308368057012558], 'magnitude': 0.34434932470321655, 'cosine_with_motion': 0.7625700235366821, 'motion_component': 0.2625904679298401, 'motion_component_percent': 76.25700235366821}, {'resid': 130, 'resname': 'ASN', 'atom': 'HA', 'charge': 0.13580000400543213, 'distance': 13.826547622680664, 'force': [0.09455857425928116, 0.03570140525698662, 0.21307925879955292], 'magnitude': 0.23583613336086273, 'cosine_with_motion': -0.7909669280052185, 'motion_component': -0.18653857707977295, 'motion_component_percent': 79.09669280052185}, {'resid': 130, 'resname': 'ASN', 'atom': 'CB', 'charge': -0.22990000247955322, 'distance': 13.089225769042969, 'force': [-0.14901243150234222, -0.1278361827135086, -0.3999059200286865], 'magnitude': 0.445501446723938, 'cosine_with_motion': 0.7483243346214294, 'motion_component': 0.3333795666694641, 'motion_component_percent': 74.83243346214294}, {'resid': 130, 'resname': 'ASN', 'atom': 'HB2', 'charge': 0.1023000031709671, 'distance': 13.488924026489258, 'force': [0.05944611132144928, 0.06696931272745132, 0.16378182172775269], 'magnitude': 0.18666337430477142, 'cosine_with_motion': -0.7083181738853455, 'motion_component': -0.13221706449985504, 'motion_component_percent': 70.83181738853455}, {'resid': 130, 'resname': 'ASN', 'atom': 'HB3', 'charge': 0.1023000031709671, 'distance': 12.907281875610352, 'force': [0.053383804857730865, 0.05351732298731804, 0.18933379650115967], 'magnitude': 0.20386570692062378, 'cosine_with_motion': -0.7894539833068848, 'motion_component': -0.16094259917736053, 'motion_component_percent': 78.94539833068848}, {'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 11.749862670898438, 'force': [0.6677812933921814, 0.5050665140151978, 1.5026030540466309], 'magnitude': 1.720127820968628, 'cosine_with_motion': -0.7202626466751099, 'motion_component': -1.2389438152313232, 'motion_component_percent': 72.02626466751099}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 11.683664321899414, 'force': [-0.693419337272644, -0.350850909948349, -1.237983226776123], 'magnitude': 1.4616870880126953, 'cosine_with_motion': 0.7061586976051331, 'motion_component': 1.032183051109314, 'motion_component_percent': 70.6158697605133}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 10.829587936401367, 'force': [-0.8620378375053406, -0.9163658618927002, -2.242748975753784], 'magnitude': 2.571528434753418, 'cosine_with_motion': 0.7030641436576843, 'motion_component': 1.807949423789978, 'motion_component_percent': 70.30641436576843}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 9.961666107177734, 'force': [0.5203132033348083, 0.5200696587562561, 1.1775072813034058], 'magnitude': 1.3884241580963135, 'cosine_with_motion': -0.6723885536193848, 'motion_component': -0.9335604906082153, 'motion_component_percent': 67.23885536193848}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 11.083067893981934, 'force': [0.2863999605178833, 0.4427371621131897, 0.9900043606758118], 'magnitude': 1.1216727495193481, 'cosine_with_motion': -0.7060619592666626, 'motion_component': -0.791970431804657, 'motion_component_percent': 70.60619592666626}, {'resid': 458, 'resname': 'ASN', 'atom': 'CB', 'charge': -0.22990000247955322, 'distance': 13.904709815979004, 'force': [0.29802459478378296, -0.019197944551706314, -0.2581910490989685], 'magnitude': 0.39477822184562683, 'cosine_with_motion': 0.6512908935546875, 'motion_component': 0.2571154534816742, 'motion_component_percent': 65.12908935546875}, {'resid': 458, 'resname': 'ASN', 'atom': 'HB2', 'charge': 0.1023000031709671, 'distance': 13.949250221252441, 'force': [-0.1399165391921997, 0.011723052710294724, 0.10369442403316498], 'magnitude': 0.17454685270786285, 'cosine_with_motion': -0.5913550853729248, 'motion_component': -0.1032191663980484, 'motion_component_percent': 59.13550853729248}, {'resid': 458, 'resname': 'ASN', 'atom': 'HB3', 'charge': 0.1023000031709671, 'distance': 13.25754165649414, 'force': [-0.14469566941261292, -0.0029181218706071377, 0.12804196774959564], 'magnitude': 0.1932358592748642, 'cosine_with_motion': -0.6783591508865356, 'motion_component': -0.13108330965042114, 'motion_component_percent': 67.83591508865356}, {'resid': 458, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 13.13726806640625, 'force': [-0.9858729839324951, 0.18566052615642548, 0.9417755007743835], 'magnitude': 1.3759928941726685, 'cosine_with_motion': -0.6519750952720642, 'motion_component': -0.8971130847930908, 'motion_component_percent': 65.19750952720642}, {'resid': 458, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 12.447216987609863, 'force': [0.8539428114891052, -0.16226720809936523, -0.9502786993980408], 'magnitude': 1.2878581285476685, 'cosine_with_motion': 0.7024432420730591, 'motion_component': 0.9046472311019897, 'motion_component_percent': 70.24432420730591}, {'resid': 458, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 13.491104125976562, 'force': [1.2143737077713013, -0.36442720890045166, -1.0668221712112427], 'magnitude': 1.6569913625717163, 'cosine_with_motion': 0.5886306166648865, 'motion_component': 0.975355863571167, 'motion_component_percent': 58.86306166648865}, {'resid': 458, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 13.036529541015625, 'force': [-0.5740676522254944, 0.2295912206172943, 0.5243804454803467], 'magnitude': 0.8107038140296936, 'cosine_with_motion': -0.5709536671638489, 'motion_component': -0.46287432312965393, 'motion_component_percent': 57.09536671638489}, {'resid': 458, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 13.895878791809082, 'force': [-0.5528053641319275, 0.1603447049856186, 0.4216933250427246], 'magnitude': 0.7135331034660339, 'cosine_with_motion': -0.5393218398094177, 'motion_component': -0.3848239779472351, 'motion_component_percent': 53.93218398094177}, {'resid': 786, 'resname': 'ASN', 'atom': 'N', 'charge': -0.38210001587867737, 'distance': 13.183247566223145, 'force': [0.01366508286446333, 0.4581678509712219, -0.5680374503135681], 'magnitude': 0.7299116849899292, 'cosine_with_motion': 0.9310919642448425, 'motion_component': 0.6796149015426636, 'motion_component_percent': 93.10919642448425}, {'resid': 786, 'resname': 'ASN', 'atom': 'H', 'charge': 0.2681000232696533, 'distance': 12.782675743103027, 'force': [0.025164401158690453, -0.3540955185890198, 0.4131920337677002], 'magnitude': 0.5447426438331604, 'cosine_with_motion': -0.9153145551681519, 'motion_component': -0.49861088395118713, 'motion_component_percent': 91.53145551681519}, {'resid': 786, 'resname': 'ASN', 'atom': 'CA', 'charge': -0.20800000429153442, 'distance': 12.492462158203125, 'force': [0.04039634391665459, 0.2511225938796997, -0.362083792</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>706</v>
+      </c>
+      <c r="B8" t="n">
         <v>959</v>
       </c>
-      <c r="C4" t="n">
+      <c r="C8" t="n">
         <v>2223</v>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>{954: {'frame': 954, 'motion_vector': [1.8922004699707031, 2.834430694580078, 1.6804885864257812], 'motion_vector_magnitude': 3.799797773361206, 'ionic_force': [-13.062879800796509, 10.245393350720406, 1.3206260204315186], 'ionic_force_magnitude': 16.65385741162942, 'radial_force': 16.60141300013476, 'axial_force': 1.3206260204315186, 'glu_force': [-3.4732834491090627, -0.0006817424385030524, 6.173598070532544], 'glu_force_magnitude': 7.0835733580665945, 'asn_force': [-2.803661426437605, -7.464392549270752, -13.667343181071297], 'asn_force_magnitude': 15.823209003008175, 'sf_force': [0.9609858171911573, 0.10090089443628744, 0.21813816277665765], 'sf_force_magnitude': 0.9905851752374324, 'residue_force': [-5.315959058355512, -7.364173397272972, -7.275606947762098], 'residue_force_magnitude': 11.637221618304736, 'pip2_force': [1.0214345674631753, 0.057866769957992004, -4.444173763193416], 'pip2_force_magnitude': 4.560411996314674, 'total_force': [-17.357404291688844, 2.939086723405426, -10.399154690523996], 'total_force_magnitude': 20.44651884283199, 'cosine_total_motion': -0.5404464599741138, 'cosine_glu_motion': 0.14120076197809814, 'cosine_asn_motion': -0.8221241108611756, 'cosine_sf_motion': 0.6564659222406606, 'cosine_residue_motion': -0.9760190738651873, 'cosine_pip2_motion': -0.3099841639897148, 'cosine_ionic_motion': 0.10337287010655362, 'motion_component_total': -11.050248727402561, 'motion_component_glu': 1.0002059556867586, 'motion_component_asn': -13.008641632568645, 'motion_component_sf': 0.6502854106201674, 'motion_component_residue': -11.358150266261724, 'motion_component_ionic': 1.7215570389854333, 'motion_component_pip2': -1.4136555001262703, 'motion_component_percent_total': np.float64(54.04464599741138), 'motion_component_percent_glu': np.float64(14.120076197809814), 'motion_component_percent_asn': np.float64(82.21241108611757), 'motion_component_percent_sf': np.float64(65.64659222406605), 'motion_component_percent_residue': np.float64(97.60190738651873), 'motion_component_percent_ionic': np.float64(10.337287010655363), 'motion_component_percent_pip2': np.float64(30.99841639897148), 'ionic_contributions': [{'ion_id': 2333, 'distance': 4.532892227172852, 'force': [-7.505458831787109, 11.556084632873535, 8.438343048095703], 'magnitude': 16.157989501953125, 'cosine_ionic_motion': 0.5331462621688843, 'motion_component_ionic': 8.614571571350098, 'motion_component_percent_ionic': 53.31462478637695}, {'ion_id': 2343, 'distance': 10.870248794555664, 'force': [-1.048344612121582, 0.12879706919193268, -2.603606939315796], 'magnitude': 2.809694528579712, 'cosine_ionic_motion': -0.5614266991615295, 'motion_component_ionic': -1.5774375200271606, 'motion_component_percent_ionic': 56.142669677734375}, {'ion_id': 2372, 'distance': 11.836684226989746, 'force': [-2.105020046234131, -0.3876538872718811, -1.0167081356048584], 'magnitude': 2.3696160316467285, 'cosine_ionic_motion': -0.754155695438385, 'motion_component_ionic': -1.7870594263076782, 'motion_component_percent_ionic': 75.41557312011719}, {'ion_id': 2397, 'distance': 8.713855743408203, 'force': [-2.4040563106536865, -1.0518344640731812, -3.4974019527435303], 'magnitude': 4.372375011444092, 'cosine_ionic_motion': -0.8070024847984314, 'motion_component_ionic': -3.528517484664917, 'motion_component_percent_ionic': 80.70024871826172}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 11.101517677307129, 'force': [-0.6118342356021009, -0.4679971967421453, 1.1580407717395618], 'magnitude': 1.3908346188618088, 'cosine_with_motion': -0.1018269675318201, 'motion_component': -0.1416244715769728, 'motion_component_percent': 10.182696753182011}, {'resid': 98, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 11.804080963134766, 'force': [0.34368596400988916, 0.2119715353786382, -0.571264325487313], 'magnitude': 0.6995676545143141, 'cosine_with_motion': 0.1095239175835094, 'motion_component': 0.07661939013711472, 'motion_component_percent': 10.95239175835094}, {'resid': 98, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 9.696623802185059, 'force': [0.06684634861638612, 0.050255175412280036, -0.11250132094151778], 'magnitude': 0.14018047008285017, 'cosine_with_motion': 0.1499543850265833, 'motion_component': 0.021020676184011156, 'motion_component_percent': 14.99543850265833}, {'resid': 98, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 9.599329948425293, 'force': [0.17222320584251394, 0.18256469013987808, -0.3090504091098022], 'magnitude': 0.3981241691827799, 'cosine_with_motion': 0.21416840895455075, 'motion_component': 0.08526561988022835, 'motion_component_percent': 21.416840895455074}, {'resid': 98, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 9.811277389526367, 'force': [0.11714330170636836, 0.06839869751122221, -0.1374867635085172], 'magnitude': 0.193141256845729, 'cosine_with_motion': 0.2513770460845025, 'motion_component': 0.04855127862292755, 'motion_component_percent': 25.13770460845025}, {'resid': 98, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 10.883131980895996, 'force': [-0.029827604491624776, -0.017710275292658346, 0.03388514046408642], 'magnitude': 0.0484927065126438, 'cosine_with_motion': -0.2696955103990436, 'motion_component': -0.013078265233558496, 'motion_component_percent': 26.96955103990436}, {'resid': 98, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 9.710206031799316, 'force': [-0.0398440560174094, -0.01545055105679506, 0.04340992459984714], 'magnitude': 0.060915432212547777, 'cosine_with_motion': -0.19975507951458898, 'motion_component': -0.012168167005283037, 'motion_component_percent': 19.975507951458898}, {'resid': 98, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 9.141039848327637, 'force': [0.03453950139261121, 0.024804287439036555, -0.03334208578585103], 'magnitude': 0.05403632589619309, 'cosine_with_motion': 0.3878236030686454, 'motion_component': 0.02095656260565315, 'motion_component_percent': 38.78236030686454}, {'resid': 98, 'resname': 'GLU', 'atom': 'HG2', 'charge': -0.042500000447034836, 'distance': 9.435471534729004, 'force': [-0.09027500143909559, -0.08684462295257402, 0.09709417405915863], 'magnitude': 0.15848925218081397, 'cosine_with_motion': -0.4214486738461445, 'motion_component': -0.06679508515047121, 'motion_component_percent': 42.14486738461445}, {'resid': 98, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 9.665505409240723, 'force': [-0.10739296881386894, -0.0666723673512608, 0.08266283667827057], 'magnitude': 0.1510350915733709, 'cosine_with_motion': -0.4413173701221372, 'motion_component': -0.0666544094093162, 'motion_component_percent': 44.13173701221372}, {'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 7.6773295402526855, 'force': [3.0470719329534726, 2.0308755923312485, -2.6779714065782163], 'magnitude': 4.536588353660724, 'cosine_with_motion': 0.40733834976551764, 'motion_component': 1.8479264135456257, 'motion_component_percent': 40.73383497655176}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 7.155954360961914, 'force': [-3.2780821701764085, -3.0935973159412513, 2.8044905054343623], 'magnitude': 5.308609428343629, 'cosine_with_motion': -0.5085585720345993, 'motion_component': -2.6997388303678465, 'motion_component_percent': 50.855857203459934}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 7.240767955780029, 'force': [-3.925662829116496, -1.6311771823457684, 2.9685675442000745], 'magnitude': 5.184974533456309, 'cosine_with_motion': -0.35849192244748407, 'motion_component': -1.8587714883399988, 'motion_component_percent': 35.84919224474841}, {'resid': 98, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 8.60933780670166, 'force': [1.0422424824769074, 0.6478053756543638, -2.066646621678737], 'magnitude': 2.403528542768414, 'cosine_with_motion': 0.0367149829316139, 'motion_component': 0.08824550942338914, 'motion_component_percent': 3.6714982931613895}, {'resid': 98, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 7.461002826690674, 'force': [-1.376939717470447, -1.0556324011818645, 3.005668738996941], 'magnitude': 3.4704995779507084, 'cosine_with_motion': -0.041447085104053455, 'motion_component': -0.14384209136090462, 'motion_component_percent': 4.144708510405345}, {'resid': 426, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 14.792044639587402, 'force': [-0.679038761291151, -0.011073994954437078, -0.4491204391941214], 'magnitude': 0.8142023345594093, 'cosine_with_motion': -0.669404889331913, 'motion_component': -0.5450310236595266, 'motion_component_percent': 66.9404889331913}, {'resid': 426, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 13.805797576904297, 'force': [0.8692284020711004, 0.03875903738801685, 0.5199130786298648], 'magnitude': 1.0135925647303794, 'cosine_with_motion': 0.6824246322959306, 'motion_component': 0.6917005332840185, 'motion_component_percent': 68.24246322959307}, {'resid': 754, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 12.345751762390137, 'force': [0.10634993611285551, 0.7660709778679052, 0.8164503733490442], 'magnitude': 1.1246182748757423, 'cosine_with_motion': 0.8762845554493945, 'motion_component': 0.9854856250497548, 'motion_component_percent': 87.62845554493946}, {'resid': 754, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 13.311304092407227, 'force': [-0.059122478902624676, -0.38183480157774274, -0.391576915978534], 'magnitude': 0.5501143193325959, 'cosine_with_motion': -0.8860813775914391, 'motion_component': -0.48744605390700346, 'motion_component_percent': 88.60813775914391}, {'resid': 754, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 11.351812362670898, 'force': [-0.01523728018460148, -0.07482850414698328, -0.06804468388553474], 'magnitude': 0.10228176154809562, 'cosine_with_motion': -0.9141297020211666, 'motion_component': -0.09349879620616067, 'motion_component_percent': 91.41297020211667}, {'resid': 754, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 10.69538402557373, 'force': [-0.024148969922901622, -0.24240295128093498, -0.20859102952306693], 'magnitude': 0.3207063783829962, 'cosine_with_motion': -0.8889600282431633, 'motion_component': -0.2850951511851109, 'motion_component_percent': 88.89600282431633}, {'resid': 754, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 12.2778902053833, 'force': [-0.02378070079151519, -0.09734864625263034, -0.07189370399721733], 'magnitude': 0.12333282341613214, 'cosine_with_motion': -0.9426054112047709, 'motion_component': -0.11625418673120863, 'motion_component_percent': 94.26054112047709}, {'resid': 754, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 12.774681091308594, 'force': [0.004321825812391217, 0.028739001851861613, 0.019851882129266692], 'magnitude': 0.035195250103788926, 'cosine_with_motion': 0.9197105236193632, 'motion_component': 0.03236944190187016, 'motion_component_percent': 91.97105236193633}, {'resid': 754, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 13.171326637268066, 'force': [0.0076972003671071315, 0.025351319782686756, 0.019853565907964017], 'magnitude': 0.033107406837100825, 'cosine_with_motion': 0.9521742150569453, 'motion_component': 0.03152401911768742, 'motion_component_percent': 95.21742150569453}, {'resid': 754, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 11.773818969726562, 'force': [-0.008779413774780372, -0.026839688196545107, -0.016231992140433516], 'magnitude': 0.0325718365703204, 'cosine_with_motion': -0.9692883839807651, 'motion_component': -0.03157150283253145, 'motion_component_percent': 96.92883839807651}, {'resid': 754, 'resname': 'GLU', 'atom': 'HG2', 'charge': -0.042500000447034836, 'distance': 12.562442779541016, 'force': [0.0240006190195133, 0.07640662525756343, 0.03974768245095525], 'magnitude': 0.08940850270970614, 'cosine_with_motion': 0.9677529360834011, 'motion_component': 0.08652534100813884, 'motion_component_percent': 96.7752936083401}, {'resid': 754, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 11.866691589355469, 'force': [0.03541163229466575, 0.07887442178512095, 0.05064464216177405], 'magnitude': 0.10019998948804296, 'cosine_with_motion': 0.986704932581353, 'motion_component': 0.0988678238724517, 'motion_component_percent': 98.6704932581353}, {'resid': 754, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 10.501465797424316, 'force': [-0.584505585377183, -2.0892070253283026, -1.0828282911075993], 'magnitude': 2.424654590254303, 'cosine_with_motion': -0.9602958535748645, 'motion_component': -2.3283857493724693, 'motion_component_percent': 96.02958535748644}, {'resid': 754, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 9.71003532409668, 'force': [0.9469716506553004, 2.4541647700414915, 1.180315117405826], 'magnitude': 2.8831968025152843, 'cosine_with_motion': 0.9795502644488666, 'motion_component': 2.8242361903619733, 'motion_component_percent': 97.95502644488666}, {'resid': 754, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 10.227750778198242, 'force': [0.3240278422999051, 2.2979013773035066, 1.169564268171948], 'magnitude': 2.598696858000846, 'cosine_with_motion': 0.9207338759046741, 'motion_component': 2.3927082303684175, 'motion_component_percent': 92.07338759046742}, {'resid': 754, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 10.741355895996094, 'force': [-0.4012841693472027, -1.0304868025092822, -1.0776173006690413], 'magnitude': 1.5440826018758549, 'cosine_with_motion': -0.9358937186464773, 'motion_component': -1.445097208166922, 'motion_component_percent': 93.58937186464773}, {'resid': 754, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 9.521649360656738, 'force': [0.5928566956235829, 1.4345679292121825, 1.4598803821278563], 'magnitude': 2.1308953365174035, 'cosine_with_motion': 0.9437231724947317, 'motion_component': 2.010975307232433, 'motion_component_percent': 94.37231724947317}, {'resid': 1082, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 14.161029815673828, 'force': [-0.030794148450555527, 0.04359779630595218, -0.038352236512225676], 'magnitude': 0.06572626162364512, 'cosine_with_motion': 0.0034264319728577576, 'motion_component': 0.00022520656428367145, 'motion_component_percent': 0.34264319728577575}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 14.116772651672363, 'force': [-0.09845966236283543, 0.11592801233707513, -0.10370831890137022], 'magnitude': 0.18408971879596345, 'cosine_with_motion': -0.04574119352809602, 'motion_component': -0.008420483453978939, 'motion_component_percent': 4.574119352809602}, {'resid': 1082, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 14.740365028381348, 'force': [-0.03756780792216476, 0.06256789997126593, -0.044673728542454556], 'magnitude': 0.08556765931574804, 'cosine_with_motion': 0.09591218440486252, 'motion_component': 0.008206981119384478, 'motion_component_percent': 9.591218440486251}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 14.934273719787598, 'force': [0.009610757456709949, -0.01935565323155385, 0.014006171546861429], 'magnitude': 0.025752297223975526, 'cosine_with_motion': -0.1342779320573888, 'motion_component': -0.003457965216962668, 'motion_component_percent': 13.42779320573888}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 14.175175666809082, 'force': [0.012733066405629231, -0.021836152889171675, 0.01334588528702774], 'magnitude': 0.028584282520013472, 'cosine_with_motion': -0.14152754298199788, 'motion_component': -0.004045463272960777, 'motion_component_percent': 14.152754298199788}, {'resid': 1082, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 12.797944068908691, 'force': [-0.46867083793340253, 0.7207792290875749, -0.6662673091538571], 'magnitude': 1.0876981100748488, 'cosine_with_motion': 0.00883735214947409, 'motion_component': 0.00961237123104887, 'motion_component_percent': 0.883735214947409}, {'resid': 1082, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 11.764103889465332, 'force': [0.6610025851623972, -0.9307693612654724, 0.8033742678872617], 'magnitude': 1.395946358484201, 'cosine_with_motion': -0.007049105658438108, 'motion_component': -0.009840173374467052, 'motion_component_percent': 0.7049105658438107}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'N', 'charge': -0.38210001587867737, 'distance': 7.056772708892822, 'force': [-1.990859991079422, -1.2621957887516952, -0.965793324966687], 'magnitude': 2.5474337007611165, 'cosine_with_motion': -0.9264426445270376, 'motion_component': -2.360051214490427, 'motion_component_percent': 92.64426445270377}, {'resid': 130, 'resname': 'ASN', 'atom': 'H', 'charge': 0.2681000232696533, 'distance': 7.155559539794922, 'force': [1.2871761522784675, 1.0482396948144108, 0.5161182387501404], 'magnitude': 1.7383920562259703, 'cosine_with_motion': 0.9498225064156394, 'motion_component': 1.6511638999775882, 'motion_component_percent': 94.98225064156394}, {'resid': 130, 'resname': 'ASN', 'atom': 'CA', 'charge': -0.20800000429153442, 'distance': 5.74471378326416, 'force': [-1.664470807610967, -0.842238334065443, -0.9480037484034185], 'magnitude': 2.0924960185733616, 'cosine_with_motion': -0.8967215128082975, 'motion_component': -1.8763861953204442, 'motion_component_percent': 89.67215128082975}, {'resid': 130, 'resname': 'ASN', 'atom': 'HA', 'charge': 0.13580000400543213, 'distance': 5.777805805206299, 'force': [1.1734635610848527, 0.30901086762123753, 0.5928674367058479], 'magnitude': 1.350554050383818, 'cosine_with_motion': 0.7974939345646911, 'motion_component': 1.0770586634828712, 'motion_component_percent': 79.74939345646911}, {'resid': 130, 'resname': 'ASN', 'atom': 'CB', 'charge': -0.22990000247955322, 'distance': 4.6377949714660645, 'force': [-2.88170732468531, -1.8194730770055791, -0.9887685677624829], 'magnitude': 3.5485747369455516, 'cosine_with_motion': -0.9100915289697018, 'motion_component': -3.2295278080100345, 'motion_component_percent': 91.00915289697018}, {'resid': 130, 'resname': 'ASN', 'atom': 'HB2', 'charge': 0.1023000031709671, 'distance': 5.150431156158447, 'force': [1.1036446185517832, 0.6390136811116076, 0.11362270258184524], 'magnitude': 1.2803437223058973, 'cosine_with_motion': 0.840793175198071, 'motion_component': 1.0765042636224926, 'motion_component_percent': 84.07931751980709}, {'resid': 130, 'resname': 'ASN', 'atom': 'HB3', 'charge': 0.1023000031709671, 'distance': 4.550990581512451, 'force': [1.0818516366750277, 1.1368564314814258, 0.4756415776897816], 'magnitude': 1.6398415838136142, 'cosine_with_motion': 0.973947447720916, 'motion_component': 1.5971195252218942, 'motion_component_percent': 97.3947447720916}, {'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 3.3643245697021484, 'force': [18.62399961091497, 6.617210127612467, 7.040623194958056], 'magnitude': 20.981210793319804, 'cosine_with_motion': 0.8256955885988155, 'motion_component': 17.324093195506016, 'motion_component_percent': 82.56955885988155}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 2.7214157581329346, 'force': [-18.91226771438916, -10.021058728087263, -16.36313925016545], 'magnitude': 26.941562951187624, 'cosine_with_motion': -0.8956299296806501, 'motion_component': -24.12967013145898, 'motion_component_percent': 89.56299296806502}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 3.5599894523620605, 'force': [-23.558061254553685, -0.28141086394501763, -3.350257938254237], 'magnitude': 23.796757560652786, 'cosine_with_motion': -0.5640639934808861, 'motion_component': -13.42289410155828, 'motion_component_percent': 56.40639934808861}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 2.978043556213379, 'force': [14.977237735821305, -3.7149320826182204, 1.7978058406147333], 'magnitude': 15.535458680525796, 'cosine_with_motion': 0.35288573183199906, 'motion_component': 5.482241705823128, 'motion_component_percent': 35.28857318319991}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 4.368221282958984, 'force': [7.218541167665226, 0.15097072801551248, -0.08831743689650587], 'magnitude': 7.220659853479815, 'cosine_with_motion': 0.5080148058908184, 'motion_component': 3.6682021138691736, 'motion_component_percent': 50.80148058908184}, {'resid': 130, 'resname': 'ASN', 'atom': 'C', 'charge': 0.8050000071525574, 'distance': 5.722809791564941, 'force': [5.21594594909254, 3.1816156574598145, 5.409671146454983], 'magnitude': 8.16047255055955, 'cosine_with_motion': 0.9022975950567821, 'motion_component': 7.3631747568967665, 'motion_component_percent': 90.2297595056782}, {'resid': 130, 'resname': 'ASN', 'atom': 'O', 'charge': -0.8147000074386597, 'distance': 5.582760334014893, 'force': [-5.465720837001791, -1.6834690814029243, -6.527313556881053], 'magnitude': 8.678363594936451, 'cosine_with_motion': -0.7909682998172332, 'motion_component': -6.864310497882657, 'motion_component_percent': 79.09682998172332}, {'resid': 458, 'resname': 'ASN', 'atom': 'N', 'charge': -0.38210001587867737, 'distance': 14.284584045410156, 'force': [0.6204192587396681, 0.009200418713643403, -0.03878799215185492], 'magnitude': 0.6216986509996285, 'cosine_with_motion': 0.4803956936569566, 'motion_component': 0.2986613546925607, 'motion_component_percent': 48.03956936569566}, {'resid': 458, 'resname': 'ASN', 'atom': 'H', 'charge': 0.2681000232696533, 'distance': 13.984354972839355, 'force': [-0.45364464901524193, -0.03420460618975189, 0.013921612007887345], 'magnitude': 0.4551452888316611, 'cosine_with_motion': -0.5388630218275791, 'motion_component': -0.2452609657104152, 'motion_component_percent': 53.88630218275791}, {'resid': 458, 'resname': 'ASN', 'atom': 'CA', 'charge': -0.20800000429153442, 'distance': 13.48930549621582, 'force': [0.3776841647582964, -0.027382599483041198, -0.025140624423324827], 'magnitude': 0.3795091383089679, 'cosine_with_motion': 0.41246019707360776, 'motion_component': 0.15653241397815196, 'motion_component_percent': 41.24601970736077}, {'resid': 458, 'resname': 'ASN', 'atom': 'HA', 'charge': 0.13580000400543213, 'distance': 14.201311111450195, 'force': [-0.22138253606298522, 0.028946295971704304, 0.01131088770090804], 'magnitude': 0.2235532408728243, 'cosine_with_motion': -0.37417549884178486, 'motion_component': -0.08364814542128672, 'motion_component_percent': 37.417549884178484}, {'resid': 458, 'resname': 'ASN', 'atom': 'CB', 'charge': -0.22990000247955322, 'distance': 12.448068618774414, 'force': [0.4908851502957036, -0.03812588148179411, 0.014463060495301352], 'magnitude': 0.4925758761231513, 'cosine_with_motion': 0.4515136055698844, 'motion_component': 0.22240470984510877, 'motion_component_percent': 45.15136055698844}, {'resid': 458, 'resname': 'ASN', 'atom': 'HB2', 'charge': 0.1023000031709671, 'distance': 13.041008949279785, 'force': [-0.19855456774396496, 0.009814253315361503, -0.01903393718429191], 'magnitude': 0.19970610082034657, 'cosine_with_motion': -0.5005958143005366, 'motion_component': -0.09997203816094644, 'motion_component_percent': 50.059581430053655}, {'resid': 458, 'resname': 'ASN', 'atom': 'HB3', 'charge': 0.1023000031709671, 'distance': 11.62513256072998, 'force': [-0.25124454184475864, 0.005304853230437846, -0.0026671468059876195], 'magnitude': 0.251314693057656, 'cosine_with_motion': -0.4867828947174185, 'motion_component': -0.12233569377162531, 'motion_component_percent': 48.67828947174185}, {'resid': 458, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 12.04772663116455, 'force': [-1.6031014588707357, 0.32058754436848996, -0.06472922002543406], 'magnitude': 1.6361236300973105, 'cosine_with_motion': -0.35925763226892976, 'motion_component': -0.587789901448006, 'motion_component_percent': 35.925763226892975}, {'resid': 458, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 11.021090507507324, 'force': [1.5929276396834018, -0.4012622169307735, 0.009877539142369532], 'magnitude': 1.6427195128149668, 'cosine_with_motion': 0.3033301609717253, 'motion_component': 0.49828637425355804, 'motion_component_percent': 30.333016097172532}, {'resid': 458, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 12.903711318969727, 'force': [1.7466140745984597, -0.4574234191754285, 0.14437323075978206], 'magnitude': 1.8112814634273688, 'cosine_with_motion': 0.32706507169335386, 'motion_component': 0.5924069016927153, 'motion_component_percent': 32.70650716933539}, {'resid': 458, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 12.750555038452148, 'force': [-0.7972911133658882, 0.2738292990691009, -0.0869591138136345], 'magnitude': 0.8474771335889514, 'cosine_with_motion': -0.27284230689077704, 'motion_component': -0.2312276161655927, 'motion_component_percent': 27.284230689077702}, {'resid': 458, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 13.65030574798584, 'force': [-0.7166903091993166, 0.16041720247898603, -0.0859598712168668], 'magnitude': 0.7394374737670634, 'cosine_with_motion': -0.3722390425229593, 'motion_component': -0.2752474972406475, 'motion_component_percent': 37.22390425229593}, {'resid': 458, 'resname': 'ASN', 'atom': 'C', 'charge': 0.8050000071525574, 'distance': 12.963879585266113, 'force': [-1.5585731756792434, 0.13820385157331996, 0.2839499416378316], 'magnitude': 1.5902447037776009, 'cosine_with_motion': -0.34426009846516137, 'motion_component': -0.5474577983061782, 'motion_component_percent': 34.42600984651614}, {'resid': 458, 'resname': 'ASN', 'atom': 'O', 'charge': -0.8147000074386597, 'distance': 13.169370651245117, 'force': [1.4987809858317307, -0.2610268154012036, -0.343203791716721], 'magnitude': 1.5595731096995624, 'cosine_with_motion': 0.25638972372621305, 'motion_component': 0.3998585187267018, 'motion_component_percent': 25.638972372621303}, {'resid': 786, 'resname': 'ASN', 'atom': 'N', 'charge': -0.38210001587867737, 'distance': 9.022168159484863, 'force': [0.693795755714181, 1.3359560344043375, -0.40328656146545444], 'magnitude': 1.558451515821716, 'cosine_with_motion': 0.7466913108209363, 'motion_component': 1.1636822051997924, 'motion_component_percent': 74.66913108209363}, {'resid': 786, 'resname': 'ASN', 'atom': 'H', 'charge': 0.2681000232696533, 'distance': 8.450684547424316, 'force': [-0.4524481683379314, -1.1228737495297918, 0.29650134327778166], 'magnitude': 1.246381903343021, 'cosine_with_motion': -0.7475853069772175, 'motion_component': -0.931776797821541, 'motion_component_percent': 74.75853069772175}, {'resid': 786, 'resname': 'ASN', 'atom': 'CA', 'charge': -0.20800000429153442, 'distance': 8.650700569152832, 'force': [0.5033222384668197, 0.702543179747126, -0.323458888630123], 'magnitude': 0.9227815818373745, 'cosine_with_motion': 0.6845023244941887, 'motion_component': 0.6316461377681072, 'motion_component_percent': 68.45023244941886}, {'resid': 786, 'resname': 'ASN', 'atom': 'HA', 'charge': 0.13580000400543213, 'distance': 9.319811820983887, 'force': [-0.32247764964247677, -0.37382915202636896, 0.16028297013593726], 'magnitude': 0.5190671439604783, 'cosine_with_motion': -0.7100318744670411, 'motion_component': -0.36855421720051185, 'motion_component_percent': 71.0031874467041}, {'resid': 786, 'resname': 'ASN', 'atom': 'CB', 'charge': -0.22990000247955322, 'distance': 7.201537609100342, 'force': [0.8683585210110811, 1.074564002295936, -0.507187824001675], 'magnitude': 1.4717247721154816, 'cosine_with_motion': 0.6860490527481017, 'motion_component': 1.009675385815742, 'motion_component_percent': 68.60490527481016}, {'resid': 786, 'resname': 'ASN', 'atom': 'HB2', 'charge': 0.1023000031709671, 'distance': 6.547247409820557, 'force': [-0.3847703668035233, -0.6163105935964088, 0.3160243125393421], 'magnitude': 0.7923120275909229, 'cosine_with_motion': -0.6456721785371542, 'motion_component': -0.511573832935821, 'motion_component_percent': 64.56721785371542}, {'resid': 786, 'resname': 'ASN', 'atom': 'HB3', 'charge': 0.1023000031709671, 'distance': 7.263469219207764, 'force': [-0.4373029766828588, -0.3987260839131678, 0.2534038253852242], 'magnitude': 0.6437622869726718, 'cosine_with_motion': -0.6261978152171742, 'motion_component': -0.4031225376214986, 'motion_component_percent': 62.61978152171742}, {'resid': 786, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 6.914964199066162, 'force': [-3.300334697150575, -3.642183510636307, 0.7127114323209186], 'magnitude': 4.96645421041289, 'cosine_with_motion': -0.8144922584580064, 'motion_component': -4.04513850636747, 'motion_component_percent': 81.44922584580064}, {'resid': 786, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 7.3717169761657715, 'force': [2.8396982171025082, 2.3066351287442868, -0.312137580124181], 'magnitude': 3.6717681640182724, 'cosine_with_motion': 0.8161375634590656, 'motion_component': 2.99666792296844, 'motion_component_percent': 81.61375634590657}, {'resid': 786, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 6.510997772216797, 'force': [4.037358161876295, 5.854793469685815, -0.17770886491401944], 'magnitude': 7.114102047385448, 'cosine_with_motion': 0.8854590051783157, 'motion_component': 6.299245721614938, 'motion_component_percent': 88.54590051783157}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 6.6432414054870605, 'force': [-1.8888988645576315, -2.4581384016927266, -0.3690475541982463], 'magnitude': 3.1219512199365465, 'cosine_with_motion': -0.9409072288201904, 'motion_component': -2.937466470862309, 'motion_component_percent': 94.09072288201904}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 6.787649154663086, 'force': [-1.3361667717834749, -2.6672124451350876, 0.20946125901148568], 'magnitude': 2.9905246844873963, 'cosine_with_motion': -0.8568154336070887, 'motion_component': -2.5623277042517705, 'motion_component_percent': 85.68154336070887}, {'resid': 786, 'resname': 'ASN', 'atom': 'C', 'charge': 0.8050000071525574, 'distance': 9.315631866455078, 'force': [-1.522006517179266, -2.2205306472248765, 1.4957713426651746], 'magnitude': 3.0797064962654264, 'cosine_with_motion': -0.5691425437949615, 'motion_component': -1.7527919894263728, 'motion_component_percent': 56.91425437949616}, {'resid': 786, 'resname': 'ASN', 'atom': 'O', 'charge': -0.8147000074386597, 'distance': 10.211404800415039, 'force': [1.4215624726574154, 1.7166046186503947, -1.3270660269963623], 'magnitude': 2.5939690669797204, 'cosine_with_motion': 0.540285849421298, 'motion_component': 1.40148478072571, 'motion_component_percent': 54.0285849421298}, {'resid': 1114, 'resname': 'ASN', 'atom': 'N', 'charge': -0.38210001587867737, 'distance': 13.937173843383789, 'force': [0.3688960083864534, -0.5354636119723595, -0.060882239143519916], 'magnitude': 0.6530790088443148, 'cosine_with_motion': -0.3715478311953988, 'motion_component': -0.24265008933534585, 'motion_component_percent': 37.15478311953988}, {'resid': 1114, 'resname': 'ASN', 'atom': 'H', 'charge': 0.2681000232696533, 'distance': 14.056153297424316, 'force': [-0.26858840256836203, 0.361412553335967, 0.01407835702316637], 'magnitude': 0.4505074514805715, 'cosine_with_motion': 0.3153537568267199, 'motion_component': 0.14206921730282945, 'motion_component_percent': 31.53537568267199}, {'resid': 1114, 'resname': 'ASN', 'atom': 'CA', 'charge': -0.20800000429153442, 'distance': 12.619854927062988, 'force': [0.24292607290203572, -0.35385893908338684, -0.061503643873499006], 'magnitude': 0.4336034177385407, 'cosine_with_motion': -0.39249693024098553, 'motion_component': -0.17018801040437692, 'motion_component_percent': 39.249693024098555}, {'resid': 1114, 'resname': 'ASN', 'atom': 'HA', 'charge': 0.13580000400543213, 'distance': 12.298035621643066, 'force': [-0.1458803125912204,</t>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>{623: {'frame': 623, 'motion_vector': [0.4919548034667969, 0.13670730590820312, -1.4161605834960938], 'motion_vector_magnitude': 1.5053967237472534, 'ionic_force': [-0.7565615475177765, 0.58968585729599, -11.05220103263855], 'ionic_force_magnitude': 11.093748800623441, 'radial_force': 0.9592261388626768, 'axial_force': -11.05220103263855, 'glu_force': [0.7916474456433207, -0.12158595188520849, -5.622965402901173], 'glu_force_magnitude': 5.679720833290398, 'asn_force': [0.3060680021299049, -0.19012906635180116, 0.4194922372698784], 'asn_force_magnitude': 0.5529922431004679, 'sf_force': [-12.510543377868089, -2.4116257523764943, 7.6270081449183635], 'sf_force_magnitude': 14.849272292664569, 'residue_force': [-11.412827930094863, -2.723340770613504, 2.4235349792870693], 'residue_force_magnitude': 11.980932689514082, 'pip2_force': [0.511644174810499, 0.02534106420353055, -3.736842623562552], 'pip2_force_magnitude': 3.771791977883502, 'total_force': [-11.657745302802141, -2.1083138491139835, -12.365508676914033], 'total_force_magnitude': 17.124655256974005, 'cosine_total_motion': 0.44563646587297423, 'cosine_glu_motion': 0.974927237245802, 'cosine_asn_motion': -0.5639689895808384, 'cosine_sf_motion': -0.7732549738629644, 'cosine_residue_motion': -0.5222322632932115, 'cosine_pip2_motion': 0.9769456048299991, 'cosine_ionic_motion': 0.9197400293685907, 'motion_component_total': 7.6313708480109455, 'motion_component_glu': 5.537314540327232, 'motion_component_asn': -0.31187047658741224, 'motion_component_sf': -11.482273658548383, 'motion_component_residue': -6.256829594808563, 'motion_component_ionic': 10.203364847693171, 'motion_component_pip2': 3.6848355951263367, 'motion_component_percent_total': 44.56364658729742, 'motion_component_percent_glu': 97.4927237245802, 'motion_component_percent_asn': 56.39689895808384, 'motion_component_percent_sf': 77.32549738629643, 'motion_component_percent_residue': 52.22322632932115, 'motion_component_percent_ionic': 91.97400293685907, 'motion_component_percent_pip2': 97.69456048299992, 'ionic_contributions': [{'ion_id': 2276, 'distance': 11.822823524475098, 'force': [-0.802685558795929, 1.3643453121185303, 1.7707951068878174], 'magnitude': 2.3751752376556396, 'cosine_ionic_motion': -0.7596246004104614, 'motion_component_ionic': -1.8042415380477905, 'motion_component_percent_ionic': 75.96246004104614}, {'ion_id': 2391, 'distance': 3.7618348598480225, 'force': [1.3791444301605225, -0.49850088357925415, -23.414695739746094], 'magnitude': 23.460573196411133, 'cosine_ionic_motion': 0.9561640620231628, 'motion_component_ionic': 22.432157516479492, 'motion_component_percent_ionic': 95.61640620231628}, {'ion_id': 2397, 'distance': 10.330368041992188, 'force': [-0.2553107440471649, -0.8818203210830688, 2.972510814666748], 'magnitude': 3.111046552658081, 'cosine_ionic_motion': -0.9513908624649048, 'motion_component_ionic': -2.9598212242126465, 'motion_component_percent_ionic': 95.13908624649048}, {'ion_id': 2520, 'distance': 6.55833101272583, 'force': [-1.077709674835205, 0.6056617498397827, 7.6191887855529785], 'magnitude': 7.718829154968262, 'cosine_ionic_motion': -0.9670807123184204, 'motion_component_ionic': -7.464730739593506, 'motion_component_percent_ionic': 96.70807123184204}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 9.848191261291504, 'force': [-1.6338375806808472, -0.4704136252403259, -0.48257604241371155], 'magnitude': 1.7673691511154175, 'cosine_with_motion': -0.06941238790750504, 'motion_component': -0.12267731130123138, 'motion_component_percent': 6.9412387907505035}, {'resid': 98, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 10.483662605285645, 'force': [0.8411481380462646, 0.2157210260629654, 0.1802830547094345], 'magnitude': 0.8868865370750427, 'cosine_with_motion': 0.1408025324344635, 'motion_component': 0.12487587332725525, 'motion_component_percent': 14.08025324344635}, {'resid': 98, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 10.347125053405762, 'force': [0.11002442240715027, 0.02538670040667057, 0.04905024543404579], 'magnitude': 0.12310883402824402, 'cosine_with_motion': -0.06402412801980972, 'motion_component': -0.007881935685873032, 'motion_component_percent': 6.402412801980972}, {'resid': 98, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 10.629962921142578, 'force': [0.2761877775192261, 0.09297412633895874, 0.14312294125556946], 'magnitude': 0.3246660530567169, 'cosine_with_motion': -0.11069627106189728, 'motion_component': -0.03593932092189789, 'motion_component_percent': 11.069627106189728}, {'resid': 98, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 11.675406455993652, 'force': [0.12480668723583221, 0.019704630598425865, 0.051353808492422104], 'magnitude': 0.1363898664712906, 'cosine_with_motion': -0.04204260930418968, 'motion_component': -0.005734185688197613, 'motion_component_percent': 4.204260930418968}, {'resid': 98, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 12.30247688293457, 'force': [-0.035034336149692535, -0.007600520271807909, -0.012447722256183624], 'magnitude': 0.03794889152050018, 'cosine_with_motion': -0.011314591392874718, 'motion_component': -0.00042937620310112834, 'motion_component_percent': 1.1314591392874718}, {'resid': 98, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 11.597854614257812, 'force': [-0.04012402519583702, -0.002729875035583973, -0.014349515549838543], 'magnitude': 0.04270009696483612, 'cosine_with_motion': 0.0032485437113791704, 'motion_component': 0.00013871313421986997, 'motion_component_percent': 0.32485437113791704}, {'resid': 98, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 12.485617637634277, 'force': [0.02522433176636696, 0.003321676282212138, 0.013842208310961723], 'magnitude': 0.02896389365196228, 'cosine_with_motion': -0.1545671671628952, 'motion_component': -0.004476867150515318, 'motion_component_percent': 15.45671671628952}, {'resid': 98, 'resname': 'GLU', 'atom': 'HG2', 'charge': -0.042500000447034836, 'distance': 13.459403038024902, 'force': [-0.06865337491035461, -0.006280621979385614, -0.03624838963150978], 'magnitude': 0.07788888365030289, 'cosine_with_motion': 0.14243115484714508, 'motion_component': 0.0110938036814332, 'motion_component_percent': 14.243115484714508}, {'resid': 98, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 12.142105102539062, 'force': [-0.08183062076568604, -0.004016639199107885, -0.049469687044620514], 'magnitude': 0.09570597857236862, 'cosine_with_motion': 0.2030252367258072, 'motion_component': 0.019430728629231453, 'motion_component_percent': 20.30252367258072}, {'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 12.741732597351074, 'force': [1.3470180034637451, 0.33357492089271545, 0.8870561718940735], 'magnitude': 1.6469967365264893, 'cosine_with_motion': -0.22099846601486206, 'motion_component': -0.36398375034332275, 'motion_component_percent': 22.099846601486206}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 12.620734214782715, 'force': [-1.3001444339752197, -0.3250887095928192, -1.0567052364349365], 'magnitude': 1.7066588401794434, 'cosine_with_motion': 0.316211462020874, 'motion_component': 0.5396651029586792, 'motion_component_percent': 31.621146202087402}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 13.146772384643555, 'force': [-1.2918938398361206, -0.4442174732685089, -0.779376745223999], 'magnitude': 1.57281494140625, 'cosine_with_motion': 0.17208248376846313, 'motion_component': 0.2706539034843445, 'motion_component_percent': 17.208248376846313}, {'resid': 98, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 9.391639709472656, 'force': [1.7583047151565552, 0.2432488054037094, 0.9637116193771362], 'magnitude': 2.0197885036468506, 'cosine_with_motion': -0.153427854180336, 'motion_component': -0.30989181995391846, 'motion_component_percent': 15.3427854180336}, {'resid': 98, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 9.139359474182129, 'force': [-1.8543591499328613, -0.34552571177482605, -1.3384405374526978], 'magnitude': 2.312889575958252, 'cosine_with_motion': 0.26881080865859985, 'motion_component': 0.6217297315597534, 'motion_component_percent': 26.881080865859985}, {'resid': 426, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 9.656079292297363, 'force': [1.7527222633361816, 0.4445191025733948, -0.3317526578903198], 'magnitude': 1.8383939266204834, 'cosine_with_motion': 0.5032838582992554, 'motion_component': 0.9252339601516724, 'motion_component_percent': 50.32838582992554}, {'resid': 426, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 10.222562789916992, 'force': [-0.9085091948509216, -0.18350285291671753, 0.10486921668052673], 'magnitude': 0.9327700138092041, 'cosine_with_motion': -0.4419229328632355, 'motion_component': -0.41221246123313904, 'motion_component_percent': 44.19229328632355}, {'resid': 426, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 10.171282768249512, 'force': [-0.11747777462005615, -0.029823560267686844, 0.039253804832696915], 'magnitude': 0.12740224599838257, 'cosine_with_motion': -0.6124405860900879, 'motion_component': -0.07802630960941315, 'motion_component_percent': 61.24405860900879}, {'resid': 426, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 10.30409049987793, 'force': [-0.30600887537002563, -0.11466333270072937, 0.11224645376205444], 'magnitude': 0.34552624821662903, 'cosine_with_motion': -0.6251548528671265, 'motion_component': -0.21600741147994995, 'motion_component_percent': 62.51548528671265}, {'resid': 426, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 11.6107816696167, 'force': [-0.12882369756698608, -0.02533780410885811, 0.04221689701080322], 'magnitude': 0.1379123479127884, 'cosine_with_motion': -0.6099104285240173, 'motion_component': -0.0841141790151596, 'motion_component_percent': 60.99104285240173}, {'resid': 426, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 12.182340621948242, 'force': [0.03648070991039276, 0.008857754990458488, -0.00940579455345869], 'magnitude': 0.038701046258211136, 'cosine_with_motion': 0.557460606098175, 'motion_component': 0.02157430909574032, 'motion_component_percent': 55.746060609817505}, {'resid': 426, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 11.579959869384766, 'force': [0.0408303327858448, 0.00401290412992239, -0.012303470633924007], 'magnitude': 0.04283216968178749, 'cosine_with_motion': 0.5902498960494995, 'motion_component': 0.02528168261051178, 'motion_component_percent': 59.02498960494995}, {'resid': 426, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 12.458076477050781, 'force': [-0.026070117950439453, -0.005620276555418968, 0.011623742990195751], 'magnitude': 0.02909209579229355, 'cosine_with_motion': -0.6862573027610779, 'motion_component': -0.019964663311839104, 'motion_component_percent': 68.62573027610779}, {'resid': 426, 'resname': 'GLU', 'atom': 'HG2', 'charge': -0.042500000447034836, 'distance': 12.401857376098633, 'force': [0.07870390266180038, 0.023673441261053085, -0.04075893014669418], 'magnitude': 0.09173890948295593, 'cosine_with_motion': 0.7217509150505066, 'motion_component': 0.06621263921260834, 'motion_component_percent': 72.17509150505066}, {'resid': 426, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 13.49221134185791, 'force': [0.07030345499515533, 0.014779653400182724, -0.029101025313138962], 'magnitude': 0.0775105357170105, 'cosine_with_motion': 0.6669145822525024, 'motion_component': 0.0516929067671299, 'motion_component_percent': 66.69145822525024}, {'resid': 426, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 12.45517635345459, 'force': [-1.510270118713379, -0.16279275715351105, 0.8145940899848938], 'magnitude': 1.7236533164978027, 'cosine_with_motion': -0.7394977807998657, 'motion_component': -1.2746378183364868, 'motion_component_percent': 73.94977807998657}, {'resid': 426, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 12.83794116973877, 'force': [1.4818437099456787, 0.016440600156784058, -0.7241401672363281], 'magnitude': 1.6493968963623047, 'cosine_with_motion': 0.7075106501579285, 'motion_component': 1.1669658422470093, 'motion_component_percent': 70.75106501579285}, {'resid': 426, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 12.562678337097168, 'force': [1.420340657234192, 0.17975187301635742, -0.957716703414917], 'magnitude': 1.7224690914154053, 'cosine_with_motion': 0.8020045757293701, 'motion_component': 1.3814281225204468, 'motion_component_percent': 80.20045757293701}, {'resid': 426, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 9.410491943359375, 'force': [-1.7976493835449219, -0.3310234248638153, 0.840138852596283], 'magnitude': 2.0117039680480957, 'cosine_with_motion': -0.6998343467712402, 'motion_component': -1.4078595638275146, 'motion_component_percent': 69.98343467712402}, {'resid': 426, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 9.421553611755371, 'force': [1.8004015684127808, 0.45885169506073, -1.1334832906723022], 'magnitude': 2.1764132976531982, 'cosine_with_motion': 0.7794121503829956, 'motion_component': 1.6963229179382324, 'motion_component_percent': 77.94121503829956}, {'resid': 754, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 10.169477462768555, 'force': [-0.42397576570510864, 1.5690425634384155, -0.3248421549797058], 'magnitude': 1.6574596166610718, 'cosine_with_motion': 0.18674398958683014, 'motion_component': 0.3095206320285797, 'motion_component_percent': 18.674398958683014}, {'resid': 754, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 10.780922889709473, 'force': [0.17535406351089478, -0.8117992877960205, 0.11649695038795471], 'magnitude': 0.8386529088020325, 'cosine_with_motion': -0.1502496898174286, 'motion_component': -0.1260073333978653, 'motion_component_percent': 15.024968981742859}, {'resid': 754, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 10.489956855773926, 'force': [0.02657802402973175, -0.10997197031974792, 0.03932961821556091], 'magnitude': 0.11977914720773697, 'cosine_with_motion': -0.31975042819976807, 'motion_component': -0.03829943388700485, 'motion_component_percent': 31.975042819976807}, {'resid': 754, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 10.757936477661133, 'force': [0.09651520848274231, -0.27857092022895813, 0.11646564304828644], 'magnitude': 0.31698769330978394, 'cosine_with_motion': -0.3259391188621521, 'motion_component': -0.10331869125366211, 'motion_component_percent': 32.59391188621521}, {'resid': 754, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 11.833998680114746, 'force': [0.020486585795879364, -0.12382595986127853, 0.043270234018564224], 'magnitude': 0.1327587366104126, 'cosine_with_motion': -0.3408830761909485, 'motion_component': -0.045255206525325775, 'motion_component_percent': 34.08830761909485}, {'resid': 754, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 12.546091079711914, 'force': [-0.007764453534036875, 0.03402726724743843, -0.01064604613929987], 'magnitude': 0.03648944944143295, 'cosine_with_motion': 0.28960874676704407, 'motion_component': 0.010567664168775082, 'motion_component_percent': 28.960874676704407}, {'resid': 754, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 11.874349594116211, 'force': [-0.0034034554846584797, 0.03903692588210106, -0.011128823272883892], 'magnitude': 0.04073470085859299, 'cosine_with_motion': 0.3167301118373871, 'motion_component': 0.012901906855404377, 'motion_component_percent': 31.67301118373871}, {'resid': 754, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 12.762782096862793, 'force': [0.003505733795464039, -0.024929670616984367, 0.011601514182984829], 'magnitude': 0.02771955542266369, 'cosine_with_motion': -0.43406373262405396, 'motion_component': -0.01203205343335867, 'motion_component_percent': 43.406373262405396}, {'resid': 754, 'resname': 'GLU', 'atom': 'HG2', 'charge': -0.042500000447034836, 'distance': 12.880111694335938, 'force': [-0.015474319458007812, 0.07341308891773224, -0.04006263241171837], 'magnitude': 0.08505263179540634, 'cosine_with_motion': 0.4620392620563507, 'motion_component': 0.03929765522480011, 'motion_component_percent': 46.20392620563507}, {'resid': 754, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 13.789984703063965, 'force': [-0.009146389551460743, 0.06758776307106018, -0.0292192492634058], 'magnitude': 0.07419923692941666, 'cosine_with_motion': 0.4128878712654114, 'motion_component': 0.03063596412539482, 'motion_component_percent': 41.28878712654114}, {'resid': 754, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 12.543380737304688, 'force': [0.02910444140434265, -1.50430166721344, 0.7902663350105286], 'magnitude': 1.6994973421096802, 'cosine_with_motion': -0.5122208595275879, 'motion_component': -0.8705180287361145, 'motion_component_percent': 51.22208595275879}, {'resid': 754, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 11.717659950256348, 'force': [0.10774537920951843, 1.7785435914993286, -0.8631412982940674], 'magnitude': 1.9798583984375, 'cosine_with_motion': 0.5094804763793945, 'motion_component': 1.0086991786956787, 'motion_component_percent': 50.94804763793945}, {'resid': 754, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 13.30244255065918, 'force': [0.0009784314315766096, 1.301003098487854, -0.8169202208518982], 'magnitude': 1.5362190008163452, 'cosine_with_motion': 0.577366292476654, 'motion_component': 0.886961042881012, 'motion_component_percent': 57.736629247665405}, {'resid': 754, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 9.503018379211426, 'force': [0.2984755039215088, -1.7695717811584473, 0.8192405104637146], 'magnitude': 1.972720742225647, 'cosine_with_motion': -0.42268291115760803, 'motion_component': -0.8338353633880615, 'motion_component_percent': 42.2682911157608}, {'resid': 754, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 9.308195114135742, 'force': [-0.4361191391944885, 1.8541213274002075, -1.159225583076477], 'magnitude': 2.2297465801239014, 'cosine_with_motion': 0.5006685853004456, 'motion_component': 1.1163640022277832, 'motion_component_percent': 50.066858530044556}, {'resid': 1082, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 9.518389701843262, 'force': [0.5507668256759644, -1.7516647577285767, -0.4559178650379181], 'magnitude': 1.8919657468795776, 'cosine_with_motion': 0.23774652183055878, 'motion_component': 0.449808269739151, 'motion_component_percent': 23.774652183055878}, {'resid': 1082, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 10.08830738067627, 'force': [-0.23671184480190277, 0.9130520820617676, 0.1661657989025116], 'magnitude': 0.957761824131012, 'cosine_with_motion': -0.157404825091362, 'motion_component': -0.1507563292980194, 'motion_component_percent': 15.7404825091362}, {'resid': 1082, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 10.002734184265137, 'force': [-0.035393740981817245, 0.11673079431056976, 0.04974447935819626], 'magnitude': 0.13173195719718933, 'cosine_with_motion': -0.3625674843788147, 'motion_component': -0.04776172339916229, 'motion_component_percent': 36.25674843788147}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 10.07710075378418, 'force': [-0.13067308068275452, 0.3030649423599243, 0.14693720638751984], 'magnitude': 0.36126771569252014, 'cosine_with_motion': -0.4246395528316498, 'motion_component': -0.15340855717658997, 'motion_component_percent': 42.46395528316498}, {'resid': 1082, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 11.531974792480469, 'force': [-0.032466474920511246, 0.12581464648246765, 0.051591504365205765], 'magnitude': 0.1398037225008011, 'cosine_with_motion': -0.3413194417953491, 'motion_component': -0.04771772772073746, 'motion_component_percent': 34.13194417953491}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 12.104949951171875, 'force': [0.011382197961211205, -0.03539856895804405, -0.012402812018990517], 'magnitude': 0.03919748589396477, 'cosine_with_motion': 0.31054651737213135, 'motion_component': 0.012172643095254898, 'motion_component_percent': 31.054651737213135}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 11.510330200195312, 'force': [0.006471074651926756, -0.04032835364341736, -0.01453067734837532], 'magnitude': 0.043351948261260986, 'cosine_with_motion': 0.2796129584312439, 'motion_component': 0.012121766805648804, 'motion_component_percent': 27.96129584312439}, {'resid': 1082, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 12.349764823913574, 'force': [-0.006001001223921776, 0.02542121335864067, 0.013934989459812641], 'magnitude': 0.029604628682136536, 'cosine_with_motion': -0.43106478452682495, 'motion_component': -0.012761512771248817, 'motion_component_percent': 43.106478452682495}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HG2', 'charge': -0.042500000447034836, 'distance': 13.407751083374023, 'force': [0.016076654195785522, -0.06811828166246414, -0.03552667051553726], 'magnitude': 0.07849014550447464, 'cosine_with_motion': 0.4139190912246704, 'motion_component': 0.03248856961727142, 'motion_component_percent': 41.39190912246704}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 12.104578971862793, 'force': [0.01199739146977663, -0.08206930011510849, -0.04893304035067558], 'magnitude': 0.09630031138658524, 'cosine_with_motion': 0.4413304328918457, 'motion_component': 0.04250025749206543, 'motion_component_percent': 44.13304328918457}, {'resid': 1082, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 12.355308532714844, 'force': [-0.5024715662002563, 1.3867430686950684, 0.9448152184486389], 'magnitude': 1.7516306638717651, 'cosine_with_motion': -0.5292676687240601, 'motion_component': -0.9270815253257751, 'motion_component_percent': 52.926766872406006}, {'resid': 1082, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 12.39936637878418, 'force': [0.6663650274276733, -1.370016098022461, -0.8974056839942932], 'magnitude': 1.768141269683838, 'cosine_with_motion': 0.5302521586418152, 'motion_component': 0.9375606775283813, 'motion_component_percent': 53.02521586418152}, {'resid': 1082, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 12.404061317443848, 'force': [0.43795451521873474, -1.3138972520828247, -1.0970244407653809], 'magnitude': 1.7668030261993408, 'cosine_with_motion': 0.5975763201713562, 'motion_component': 1.0557996034622192, 'motion_component_percent': 59.75763201713562}, {'resid': 1082, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 9.253911018371582, 'force': [-0.3599926233291626, 1.7999759912490845, 0.978969931602478], 'magnitude': 2.0803582668304443, 'cosine_with_motion': -0.42066025733947754, 'motion_component': -0.8751240372657776, 'motion_component_percent': 42.066025733947754}, {'resid': 1082, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 9.101045608520508, 'force': [0.467830091714859, -1.8508821725845337, -1.3399553298950195], 'magnitude': 2.332404375076294, 'cosine_with_motion': 0.53392493724823, 'motion_component': 1.2453289031982422, 'motion_component_percent': 53.392493724823}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'H', 'charge': 0.2681000232696533, 'distance': 14.670730590820312, 'force': [0.2155623584985733, 0.09190233796834946, 0.3407537639141083], 'magnitude': 0.41355323791503906, 'cosine_with_motion': -0.584602952003479, 'motion_component': -0.24176444113254547, 'motion_component_percent': 58.4602952003479}, {'resid': 130, 'resname': 'ASN', 'atom': 'CA', 'charge': -0.20800000429153442, 'distance': 14.606184959411621, 'force': [-0.1433182656764984, -0.037119463086128235, -0.2878481149673462], 'magnitude': 0.32368892431259155, 'cosine_with_motion': 0.6814529299736023, 'motion_component': 0.22057877480983734, 'motion_component_percent': 68.14529299736023}, {'resid': 130, 'resname': 'ASN', 'atom': 'HA', 'charge': 0.13580000400543213, 'distance': 14.623834609985352, 'force': [0.09867805987596512, 0.009455367922782898, 0.18606191873550415], 'magnitude': 0.210821732878685, 'cosine_with_motion': -0.673206627368927, 'motion_component': -0.1419265866279602, 'motion_component_percent': 67.3206627368927}, {'resid': 130, 'resname': 'ASN', 'atom': 'CB', 'charge': -0.22990000247955322, 'distance': 13.250663757324219, 'force': [-0.18221649527549744, -0.06774066388607025, -0.38882261514663696], 'magnitude': 0.43471217155456543, 'cosine_with_motion': 0.6902849078178406, 'motion_component': 0.3000752627849579, 'motion_component_percent': 69.02849078178406}, {'resid': 130, 'resname': 'ASN', 'atom': 'HB2', 'charge': 0.1023000031709671, 'distance': 12.498743057250977, 'force': [0.10276943445205688, 0.03572894260287285, 0.18822680413722992], 'magnitude': 0.21741077303886414, 'cosine_with_motion': -0.6450468897819519, 'motion_component': -0.1402401477098465, 'motion_component_percent': 64.50468897819519}, {'resid': 130, 'resname': 'ASN', 'atom': 'HB3', 'charge': 0.1023000031709671, 'distance': 13.523523330688477, 'force': [0.07230369001626968, 0.0424843393266201, 0.16569629311561584], 'magnitude': 0.18570946156978607, 'cosine_with_motion': -0.6913366317749023, 'motion_component': -0.12838774919509888, 'motion_component_percent': 69.13366317749023}, {'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 12.657081604003906, 'force': [0.4969075322151184, 0.15136447548866272, 1.388386845588684], 'magnitude': 1.482378602027893, 'cosine_with_motion': -0.7622578144073486, 'motion_component': -1.1299546957015991, 'motion_component_percent': 76.22578144073486}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 13.122559547424316, 'force': [-0.2971903681755066, -0.13989053666591644, -1.1111804246902466], 'magnitude': 1.1587119102478027, 'cosine_with_motion': 0.8073523044586182, 'motion_component': 0.9354887008666992, 'motion_component_percent': 80.73523044586182}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 11.881149291992188, 'force': [-0.7492342591285706, -0.03914029523730278, -2.000412940979004], 'magnitude': 2.136477470397949, 'cosine_with_motion': 0.7645453214645386, 'motion_component': 1.6334338188171387, 'motion_component_percent': 76.45453214645386}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 11.69504165649414, 'force': [0.28595155477523804, -0.028108036145567894, 0.9655082821846008], 'magnitude': 1.0073552131652832, 'cosine_with_motion': -0.811412513256073, 'motion_component': -0.8173806071281433, 'motion_component_percent': 81.1412513256073}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 11.672191619873047, 'force': [0.42575907707214355, -0.016971530392766, 0.9171561002731323], 'magnitude': 1.011303186416626, 'cosine_with_motion': -0.7170896530151367, 'motion_component': -0.725195050239563, 'motion_component_percent': 71.70896530151367}, {'resid': 458, 'resname': 'ASN', 'atom': 'CB', 'charge': -0.22990000247955322, 'distance': 14.439806938171387, 'force': [0.2389569878578186, 0.006877627223730087, -0.27722448110580444], 'magnitude': 0.3660616874694824, 'cosine_with_motion': 0.9274546504020691, 'motion_component': 0.3395056128501892, 'motion_component_percent': 92.74546504020691}, {'resid': 458, 'resname': 'ASN', 'atom': 'HB2', 'charge': 0.1023000031709671, 'distance': 14.210594177246094, 'force': [-0.11895076930522919, -0.002545300405472517, 0.11887257546186447], 'magnitude': 0.1681857705116272, 'cosine_with_motion': -0.8973985314369202, 'motion_component': -0.15092965960502625, 'motion_component_percent': 89.73985314369202}, {'resid': 458, 'resname': 'ASN', 'atom': 'HB3', 'charge': 0.1023000031709671, 'distance': 14.238768577575684, 'force': [-0.10588996112346649, -0.014994175173342228, 0.12894079089164734], 'magnitude': 0.16752085089683533, 'cosine_with_motion': -0.9387689232826233, 'motion_component': -0.1572633683681488, 'motion_component_percent': 93.87689232826233}, {'resid': 458, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 13.79012680053711, 'force': [-0.7500873804092407, 0.06592479348182678, 0.9962440133094788], 'magnitude': 1.2487910985946655, 'cosine_with_motion': -0.9419723153114319, 'motion_component': -1.1763266324996948, 'motion_component_percent': 94.19723153114319}, {'resid': 458, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 13.187884330749512, 'force': [0.6196878552436829, -0.029589442536234856, -0.9650490283966064], 'magnitude': 1.147261142730713, 'cosine_with_motion': 0.9654877781867981, 'motion_component': 1.1076666116714478, 'motion_component_percent': 96.54877781867981}, {'resid': 458, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 13.807275772094727, 'force': [0.9756256937980652, -0.22718214988708496, -1.2244113683700562], 'magnitude': 1.5819735527038574, 'cosine_with_motion': 0.9165952205657959, 'motion_component': 1.4500293731689453, 'motion_component_percent': 91.65952205657959}, {'resid': 458, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 13.38267707824707, 'force': [-0.4436444044113159, 0.14939405024051666, 0.6104879975318909], 'magnitude': 0.7693078517913818, 'cosine_with_motion': -0.9173356294631958, 'motion_component': -0.7057135105133057, 'motion_component_percent': 91.73356294631958}, {'resid': 458, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 14.363139152526855, 'force': [-0.4389684796333313, 0.11011336743831635, 0.4911443591117859], 'magnitude': 0.6678630709648132, 'cosine_with_motion': -0.8916248679161072, 'motion_component': -0.5954833030700684, 'motion_component_percent': 89.16248679161072}, {'resid': 786, 'resname': 'ASN', 'atom': 'H', 'charge': 0.2681000232696533, 'distance': 14.633115768432617, 'force': [0.021768789738416672, -0.24795784056186676, 0.3329183757305145], 'magnitude': 0.4156821072101593, 'cosine_with_motion': -0.790477454662323, 'motion_component': -0.3285873234272003, 'motion_component_percent': 79.0477454662323}, {'resid': 786, 'resname': 'ASN', 'atom': 'CA', 'charge': -0.20800000429153442, 'distance': 14.670220375061035, 'force': [0.026129955425858498, 0.1769164353609085, -0.2664111852645874], 'magnitude': 0.3208692967891693, 'cosine_with_motion': 0.857745349407196, 'motion_component': 0.27522414922714233, 'motion_component_percent': 85.7745349407196}, {'resid': 786, 'resname': 'ASN', 'atom': 'HA', 'charge': 0.13580000400543213, 'distance': 14.85374641418457, 'force': [-0.028111394494771957, -0.11964084208011627, 0.1632576286792755], 'magnitude': 0.20434586703777313, 'cosine_with_motion': -0.8496943712234497, 'motion_component': -0.17363153398036957, 'motion_component_percent': 84.96943712234497}, {'resid': 786, 'resname': 'ASN', 'atom': 'CB', 'charge': -0.22990000247955322, 'distance': 13.186275482177734, 'force': [0.030493682250380516, 0.2359534054994583, -0.36890238523483276], 'magnitude': 0.4389679431915283, 'cosine_with_motion': 0.862083911895752, 'motion_component': 0.3784272074699402, 'motion_component_percent': 86.2083911895752}, {'resid': 786, 'resname': 'ASN', 'atom': 'HB2', 'charge': 0.1023000031709671, 'distance': 12.607373237609863, 'force': [-0.013002250343561172, -0.12742558121681213, 0.17103490233421326], 'magnitude': 0.21368031203746796, 'cosine_with_motion': -0.8270165920257568, 'motion_component': -0.17671716213226318, 'motion_component_percent': 82.70165920257568}, {'resid': 786, 'resname': 'ASN', 'atom': 'HB3', 'charge': 0.1023000</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>738</v>
+      </c>
+      <c r="B9" t="n">
+        <v>777</v>
+      </c>
+      <c r="C9" t="n">
+        <v>2391</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>{700: {'frame': 700, 'motion_vector': [0.28216552734375, -0.00325775146484375, 0.15927886962890625], 'motion_vector_magnitude': 0.32403355836868286, 'ionic_force': [-5.0707626938819885, -1.4347685873508453, 2.822461724281311], 'ionic_force_magnitude': 5.9780837550127295, 'radial_force': 5.269838251494448, 'axial_force': 2.822461724281311, 'glu_force': [0.8746330216526985, 0.11070827406365424, -4.787924962118268], 'glu_force_magnitude': 4.86841500771932, 'asn_force': [0.04523044475354254, -0.21424964256584644, -0.011380806565284729], 'asn_force_magnitude': 0.2192674741731492, 'sf_force': [3.417745786089654, 2.5834525211394066, -5.115120332222432], 'sf_force_magnitude': 6.672306138092771, 'residue_force': [4.337609252495895, 2.4799111526372144, -9.914426100905985], 'residue_force_magnitude': 11.102281669217291, 'pip2_force': [0.5152207929641008, -0.03619463695213199, -3.7013881944003515], 'pip2_force_magnitude': 3.737249935834229, 'total_force': [-0.21793264842199278, 1.008947928334237, -10.793352571025025], 'total_force_magnitude': 10.842597949006072, 'cosine_total_motion': -0.5077561456711301, 'cosine_glu_motion': -0.327210699076102, 'cosine_asn_motion': 0.16393693629493683, 'cosine_sf_motion': 0.06531909844303115, 'cosine_residue_motion': -0.10099026957278355, 'cosine_pip2_motion': -0.36668828934251196, 'cosine_ionic_motion': -0.504136051399118, 'motion_component_total': -5.505395743649023, 'motion_component_glu': -1.5929974780684253, 'motion_component_asn': 0.03594603794507527, 'motion_component_sf': 0.4358290214761227, 'motion_component_residue': -1.1212224186472275, 'motion_component_ionic': -3.01376753918533, 'motion_component_pip2': -1.370405785816466, 'motion_component_percent_total': 50.77561456711302, 'motion_component_percent_glu': 32.7210699076102, 'motion_component_percent_asn': 16.393693629493683, 'motion_component_percent_sf': 6.531909844303114, 'motion_component_percent_residue': 10.099026957278355, 'motion_component_percent_ionic': 50.4136051399118, 'motion_component_percent_pip2': 36.668828934251195, 'ionic_contributions': [{'ion_id': 2223, 'distance': 5.575526714324951, 'force': [-0.8282948136329651, -0.8982522487640381, 10.609752655029297], 'magnitude': 10.679877281188965, 'cosine_ionic_motion': 0.4216329753398895, 'motion_component_ionic': 4.502988338470459, 'motion_component_percent_ionic': 42.16329753398895}, {'ion_id': 2276, 'distance': 13.270231246948242, 'force': [-0.3265973925590515, -1.4612276554107666, 1.1456502676010132], 'magnitude': 1.8853027820587158, 'cosine_ionic_motion': 0.15564486384391785, 'motion_component_ionic': 0.2934376895427704, 'motion_component_percent_ionic': 15.564486384391785}, {'ion_id': 2298, 'distance': 14.560537338256836, 'force': [-0.3472580909729004, 0.2919861972332001, -1.4988049268722534], 'magnitude': 1.565969467163086, 'cosine_ionic_motion': -0.6654428243637085, 'motion_component_ionic': -1.0420631170272827, 'motion_component_percent_ionic': 66.54428243637085}, {'ion_id': 2333, 'distance': 5.141991138458252, 'force': [-1.17897367477417, 0.1654052585363388, -12.500133514404297], 'magnitude': 12.5566987991333, 'cosine_ionic_motion': -0.5712289810180664, 'motion_component_ionic': -7.172749996185303, 'motion_component_percent_ionic': 57.12289810180664}, {'ion_id': 2397, 'distance': 14.041548728942871, 'force': [-0.27284103631973267, 0.23179590702056885, 1.6453691720962524], 'magnitude': 1.6838679313659668, 'cosine_ionic_motion': 0.3378318250179291, 'motion_component_ionic': 0.5688641667366028, 'motion_component_percent_ionic': 33.78318250179291}, {'ion_id': 2520, 'distance': 9.077005386352539, 'force': [-2.116797685623169, 0.23552395403385162, 3.420628070831299], 'magnitude': 4.029516220092773, 'cosine_ionic_motion': -0.04076046124100685, 'motion_component_ionic': -0.16424493491649628, 'motion_component_percent_ionic': 4.076046124100685}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 9.829123497009277, 'force': [-1.6425492763519287, -0.38963988423347473, -0.5459990501403809], 'magnitude': 1.7742328643798828, 'cosine_with_motion': -0.9552218914031982, 'motion_component': -1.6947860717773438, 'motion_component_percent': 95.52218914031982}, {'resid': 98, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 10.518148422241211, 'force': [0.8342220187187195, 0.1904999017715454, 0.209966778755188], 'magnitude': 0.8810803890228271, 'cosine_with_motion': 0.9394456744194031, 'motion_component': 0.8277271389961243, 'motion_component_percent': 93.94456744194031}, {'resid': 98, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 10.435715675354004, 'force': [0.10740598291158676, 0.0212845541536808, 0.051561471074819565], 'magnitude': 0.12102752923965454, 'cosine_with_motion': 0.9804319143295288, 'motion_component': 0.11865925043821335, 'motion_component_percent': 98.04319143295288}, {'resid': 98, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 10.66610336303711, 'force': [0.27163779735565186, 0.08071661740541458, 0.15389731526374817], 'magnitude': 0.3224696218967438, 'cosine_with_motion': 0.9655997157096863, 'motion_component': 0.31137657165527344, 'motion_component_percent': 96.55997157096863}, {'resid': 98, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 11.777254104614258, 'force': [0.12183157354593277, 0.0159214548766613, 0.05357795208692551], 'magnitude': 0.13404111564159393, 'cosine_with_motion': 0.9867572784423828, 'motion_component': 0.13226604461669922, 'motion_component_percent': 98.67572784423828}, {'resid': 98, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 11.698545455932617, 'force': [-0.039287276566028595, -0.0019513614242896438, -0.01462986133992672], 'magnitude': 0.0419682115316391, 'cosine_with_motion': -0.9860488772392273, 'motion_component': -0.04138270765542984, 'motion_component_percent': 98.60488772392273}, {'resid': 98, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 12.2723388671875, 'force': [-0.033586811274290085, -0.003159142564982176, -0.01778378337621689], 'magnitude': 0.03813550993800163, 'cosine_with_motion': -0.9953181147575378, 'motion_component': -0.03795696422457695, 'motion_component_percent': 99.53181147575378}, {'resid': 98, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 12.939962387084961, 'force': [0.024620184674859047, 0.005132756661623716, 0.009728717617690563], 'magnitude': 0.026965657249093056, 'cosine_with_motion': 0.9704784154891968, 'motion_component': 0.026169588789343834, 'motion_component_percent': 97.04784154891968}, {'resid': 98, 'resname': 'GLU', 'atom': 'HG2', 'charge': -0.042500000447034836, 'distance': 12.776798248291016, 'force': [-0.08073645085096359, -0.01870768703520298, -0.02454441413283348], 'magnitude': 0.08643367886543274, 'cosine_with_motion': -0.9508020281791687, 'motion_component': -0.08218131959438324, 'motion_component_percent': 95.08020281791687}, {'resid': 98, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 13.828186988830566, 'force': [-0.06822708249092102, -0.010728725232183933, -0.025978833436965942], 'magnitude': 0.07378983497619629, 'cosine_with_motion': -0.9767413139343262, 'motion_component': -0.07207357883453369, 'motion_component_percent': 97.67413139343262}, {'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 13.326933860778809, 'force': [1.3048772811889648, 0.4148874878883362, 0.6259254813194275], 'magnitude': 1.505529522895813, 'cosine_with_motion': 0.9563268423080444, 'motion_component': 1.4397783279418945, 'motion_component_percent': 95.63268423080444}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 13.49196720123291, 'force': [-1.2349071502685547, -0.3886560797691345, -0.7443680167198181], 'magnitude': 1.4933630228042603, 'cosine_with_motion': -0.9624807238578796, 'motion_component': -1.437333106994629, 'motion_component_percent': 96.24807238578796}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 13.506837844848633, 'force': [-1.2705262899398804, -0.5372384190559387, -0.5634406208992004], 'magnitude': 1.4900764226913452, 'cosine_with_motion': -0.9247319102287292, 'motion_component': -1.377921223640442, 'motion_component_percent': 92.47319102287292}, {'resid': 98, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 9.733694076538086, 'force': [1.6209135055541992, 0.11188095808029175, 0.9464414119720459], 'magnitude': 1.8803268671035767, 'cosine_with_motion': 0.9974732995033264, 'motion_component': 1.8755759000778198, 'motion_component_percent': 99.74732995033264}, {'resid': 98, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 9.945596694946289, 'force': [-1.5492523908615112, -0.11989138275384903, -1.1832362413406372], 'magnitude': 1.953101396560669, 'cosine_with_motion': -0.9879109263420105, 'motion_component': -1.9294902086257935, 'motion_component_percent': 98.79109263420105}, {'resid': 426, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 9.942017555236816, 'force': [1.6399213075637817, 0.44781795144081116, -0.34271880984306335], 'magnitude': 1.7341680526733398, 'cosine_with_motion': 0.7237262725830078, 'motion_component': 1.2550629377365112, 'motion_component_percent': 72.37262725830078}, {'resid': 426, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 10.4567289352417, 'force': [-0.8644874691963196, -0.17774204909801483, 0.12558713555335999], 'magnitude': 0.8914611339569092, 'cosine_with_motion': -0.7731896638870239, 'motion_component': -0.6892685294151306, 'motion_component_percent': 77.31896638870239}, {'resid': 426, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 10.517929077148438, 'force': [-0.1084674745798111, -0.030909476801753044, 0.03839839622378349], 'magnitude': 0.11914288252592087, 'cosine_with_motion': -0.6317372918128967, 'motion_component': -0.0752670019865036, 'motion_component_percent': 63.17372918128967}, {'resid': 426, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 10.569662094116211, 'force': [-0.2853016257286072, -0.11480186134576797, 0.11514188349246979], 'magnitude': 0.32838109135627747, 'cosine_with_motion': -0.5806846618652344, 'motion_component': -0.19068585336208344, 'motion_component_percent': 58.06846618652344}, {'resid': 426, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 11.993595123291016, 'force': [-0.11929990351200104, -0.02845761552453041, 0.040780071169137955], 'magnitude': 0.12924905121326447, 'cosine_with_motion': -0.6464552283287048, 'motion_component': -0.0835537239909172, 'motion_component_percent': 64.64552283287048}, {'resid': 426, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 12.509705543518066, 'force': [0.03439024090766907, 0.009164034388959408, -0.00896496418863535], 'magnitude': 0.036702025681734085, 'cosine_with_motion': 0.693363606929779, 'motion_component': 0.025447849184274673, 'motion_component_percent': 69.3363606929779}, {'resid': 426, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 12.090742111206055, 'force': [0.03702875226736069, 0.00520822498947382, -0.012059158645570278], 'magnitude': 0.03928966075181961, 'cosine_with_motion': 0.6684775948524475, 'motion_component': 0.026264257729053497, 'motion_component_percent': 66.84775948524475}, {'resid': 426, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 12.928864479064941, 'force': [-0.02375052310526371, -0.007048445288091898, 0.010764684528112411], 'magnitude': 0.027011966332793236, 'cosine_with_motion': -0.5671373605728149, 'motion_component': -0.015319494530558586, 'motion_component_percent': 56.713736057281494}, {'resid': 426, 'resname': 'GLU', 'atom': 'HG2', 'charge': -0.042500000447034836, 'distance': 12.893601417541504, 'force': [0.07200954109430313, 0.028779039159417152, -0.034498073160648346], 'magnitude': 0.08487475663423538, 'cosine_with_motion': 0.5355936288833618, 'motion_component': 0.04545838013291359, 'motion_component_percent': 53.55936288833618}, {'resid': 426, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 13.90301513671875, 'force': [0.06526904553174973, 0.0189126618206501, -0.02666313759982586], 'magnitude': 0.07299766689538956, 'cosine_with_motion': 0.5964475870132446, 'motion_component': 0.04353928193449974, 'motion_component_percent': 59.64475870132446}, {'resid': 426, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 12.989089965820312, 'force': [-1.344892978668213, -0.3045932352542877, 0.7812058329582214], 'magnitude': 1.584864854812622, 'cosine_with_motion': -0.4947149157524109, 'motion_component': -0.7840563058853149, 'motion_component_percent': 49.47149157524109}, {'resid': 426, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 13.05612564086914, 'force': [1.2648537158966064, 0.37864598631858826, -0.8943920135498047], 'magnitude': 1.594730257987976, 'cosine_with_motion': 0.4125949740409851, 'motion_component': 0.6579777002334595, 'motion_component_percent': 41.25949740409851}, {'resid': 426, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 13.222417831420898, 'force': [1.3424056768417358, 0.15590791404247284, -0.7689350247383118], 'magnitude': 1.5548702478408813, 'cosine_with_motion': 0.5077059864997864, 'motion_component': 0.7894169688224792, 'motion_component_percent': 50.77059864997864}, {'resid': 426, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 9.767374038696289, 'force': [-1.654188632965088, -0.31788668036460876, 0.8060539364814758], 'magnitude': 1.8673818111419678, 'cosine_with_motion': -0.5574867129325867, 'motion_component': -1.0410405397415161, 'motion_component_percent': 55.74867129325867}, {'resid': 426, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 9.732592582702637, 'force': [1.6758488416671753, 0.4177217185497284, -1.084761619567871], 'magnitude': 2.0395264625549316, 'cosine_with_motion': 0.4520163834095001, 'motion_component': 0.9218993782997131, 'motion_component_percent': 45.20163834095001}, {'resid': 754, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 9.856719970703125, 'force': [-0.4184713661670685, 1.6530767679214478, -0.452786922454834], 'magnitude': 1.7643121480941772, 'cosine_with_motion': -0.3421097695827484, 'motion_component': -0.6035884022712708, 'motion_component_percent': 34.21097695827484}, {'resid': 754, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 10.203563690185547, 'force': [0.1601680964231491, -0.9041222333908081, 0.18294034898281097], 'magnitude': 0.9362467527389526, 'cosine_with_motion': 0.2547268569469452, 'motion_component': 0.23848718404769897, 'motion_component_percent': 25.47268569469452}, {'resid': 754, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 10.327390670776367, 'force': [0.02631239779293537, -0.11070633679628372, 0.048205021768808365], 'magnitude': 0.12357977032661438, 'cosine_with_motion': 0.3861539661884308, 'motion_component': 0.04772081971168518, 'motion_component_percent': 38.61539661884308}, {'resid': 754, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 10.645743370056152, 'force': [0.09729891270399094, -0.27761703729629517, 0.13507825136184692], 'magnitude': 0.32370424270629883, 'cosine_with_motion': 0.47548308968544006, 'motion_component': 0.1539158970117569, 'motion_component_percent': 47.548308968544006}, {'resid': 754, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 11.680184364318848, 'force': [0.020584147423505783, -0.1241200640797615, 0.052366748452186584], 'magnitude': 0.13627830147743225, 'cosine_with_motion': 0.3295702040195465, 'motion_component': 0.044913265854120255, 'motion_component_percent': 32.95702040195465}, {'resid': 754, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 12.381388664245605, 'force': [-0.0069937012158334255, 0.03471186012029648, -0.01224454678595066], 'magnitude': 0.03746670484542847, 'cosine_with_motion': -0.3325045704841614, 'motion_component': -0.012457850389182568, 'motion_component_percent': 33.25045704841614}, {'resid': 754, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 11.605412483215332, 'force': [-0.0028860378079116344, 0.0398513525724411, -0.014902821741998196], 'magnitude': 0.042644500732421875, 'cosine_with_motion': -0.24010790884494781, 'motion_component': -0.010239281691610813, 'motion_component_percent': 24.01079088449478}, {'resid': 754, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 12.540525436401367, 'force': [0.0042021735571324825, -0.02483779564499855, 0.013774490915238857], 'magnitude': 0.02871081605553627, 'cosine_with_motion': 0.371977835893631, 'motion_component': 0.010679787024855614, 'motion_component_percent': 37.1977835893631}, {'resid': 754, 'resname': 'GLU', 'atom': 'HG2', 'charge': -0.042500000447034836, 'distance': 12.252102851867676, 'force': [-0.018733076751232147, 0.0773983895778656, -0.04993657022714615], 'magnitude': 0.09399521350860596, 'cosine_with_motion': -0.44297027587890625, 'motion_component': -0.04163708537817001, 'motion_component_percent': 44.297027587890625}, {'resid': 754, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 13.532191276550293, 'force': [-0.013304135762155056, 0.06718647480010986, -0.03530120477080345], 'magnitude': 0.07705321162939072, 'cosine_with_motion': -0.3843178451061249, 'motion_component': -0.02961292490363121, 'motion_component_percent': 38.43178451061249}, {'resid': 754, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 12.806262016296387, 'force': [0.06001588702201843, -1.389973521232605, 0.850122332572937], 'magnitude': 1.6304404735565186, 'cosine_with_motion': 0.29692211747169495, 'motion_component': 0.4841138422489166, 'motion_component_percent': 29.692211747169495}, {'resid': 754, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 13.912518501281738, 'force': [-0.0332145094871521, 1.1627435684204102, -0.7870112657546997], 'magnitude': 1.4044438600540161, 'cosine_with_motion': -0.30436861515045166, 'motion_component': -0.4274686276912689, 'motion_component_percent': 30.436861515045166}, {'resid': 754, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 12.093122482299805, 'force': [0.08626337349414825, 1.5952537059783936, -0.9502434134483337], 'magnitude': 1.8588271141052246, 'cosine_with_motion': -0.21950054168701172, 'motion_component': -0.40801355242729187, 'motion_component_percent': 21.950054168701172}, {'resid': 754, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 9.385168075561523, 'force': [0.2688106596469879, -1.7524254322052002, 0.9734243750572205], 'magnitude': 2.0225749015808105, 'cosine_with_motion': 0.3610168695449829, 'motion_component': 0.7301836609840393, 'motion_component_percent': 36.10168695449829}, {'resid': 754, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 9.226314544677734, 'force': [-0.3838246464729309, 1.8012278079986572, -1.326228141784668], 'magnitude': 2.269498586654663, 'cosine_with_motion': -0.4424979090690613, 'motion_component': -1.0042483806610107, 'motion_component_percent': 44.24979090690613}, {'resid': 1082, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 9.910117149353027, 'force': [0.5155361294746399, -1.5881778001785278, -0.5080968737602234], 'magnitude': 1.7453505992889404, 'cosine_with_motion': 0.12326240539550781, 'motion_component': 0.2151361107826233, 'motion_component_percent': 12.326240539550781}, {'resid': 1082, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 10.413910865783691, 'force': [-0.22420060634613037, 0.8464642763137817, 0.2026972770690918], 'magnitude': 0.8988069295883179, 'cosine_with_motion': -0.11582694202661514, 'motion_component': -0.10410606116056442, 'motion_component_percent': 11.582694202661514}, {'resid': 1082, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 10.562430381774902, 'force': [-0.032243482768535614, 0.10257790237665176, 0.048943281173706055], 'magnitude': 0.1181410700082779, 'cosine_with_motion': -0.042750030755996704, 'motion_component': -0.0050505343824625015, 'motion_component_percent': 4.27500307559967}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 10.932292938232422, 'force': [-0.10746745020151138, 0.25261643528938293, 0.1373259574174881], 'magnitude': 0.3069572150707245, 'cosine_with_motion': -0.09323382377624512, 'motion_component': -0.028618793934583664, 'motion_component_percent': 9.323382377624512}, {'resid': 1082, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 11.88418960571289, 'force': [-0.028665456920862198, 0.11727669090032578, 0.052473705261945724], 'magnitude': 0.1316397339105606, 'cosine_with_motion': -0.0026376277673989534, 'motion_component': -0.0003472166135907173, 'motion_component_percent': 0.26376277673989534}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 11.889041900634766, 'force': [0.006251147016882896, -0.03764834254980087, -0.0139518603682518], 'magnitude': 0.04063408821821213, 'cosine_with_motion': -0.025498155504465103, 'motion_component': -0.001036094268783927, 'motion_component_percent': 2.5498155504465103}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 12.24971866607666, 'force': [0.006937680300325155, -0.03305521234869957, -0.01800861954689026], 'magnitude': 0.03827647864818573, 'cosine_with_motion': -0.06475380808115005, 'motion_component': -0.002478547627106309, 'motion_component_percent': 6.4753808081150055}, {'resid': 1082, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 13.050354957580566, 'force': [-0.007830827496945858, 0.023419957607984543, 0.009645567275583744], 'magnitude': 0.026511378586292267, 'cosine_with_motion': -0.08725271373987198, 'motion_component': -0.002313189674168825, 'motion_component_percent': 8.725271373987198}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HG2', 'charge': -0.042500000447034836, 'distance': 12.786247253417969, 'force': [0.028376027941703796, -0.07755188643932343, -0.025084372609853745], 'magnitude': 0.08630596846342087, 'cosine_with_motion': 0.152469664812088, 'motion_component': 0.013159042224287987, 'motion_component_percent': 15.246966481208801}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 13.959430694580078, 'force': [0.018437717109918594, -0.0651211366057396, -0.025735724717378616], 'magnitude': 0.07240883260965347, 'cosine_with_motion': 0.05606638267636299, 'motion_component': 0.0040597012266516685, 'motion_component_percent': 5.606638267636299}, {'resid': 1082, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 13.330643653869629, 'force': [-0.5578597187995911, 1.242451548576355, 0.6396897435188293], 'magnitude': 1.5046913623809814, 'cosine_with_motion': -0.12217171490192413, 'motion_component': -0.18383072316646576, 'motion_component_percent': 12.217171490192413}, {'resid': 1082, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 13.754886627197266, 'force': [0.48865780234336853, -1.1431814432144165, -0.7202754616737366], 'magnitude': 1.4368183612823486, 'cosine_with_motion': 0.05773889273405075, 'motion_component': 0.08296030014753342, 'motion_component_percent': 5.773889273405075}, {'resid': 1082, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 13.142038345336914, 'force': [0.718887448310852, -1.2554912567138672, -0.6198834180831909], 'magnitude': 1.5739481449127197, 'cosine_with_motion': 0.212153822183609, 'motion_component': 0.33391910791397095, 'motion_component_percent': 21.2153822183609}, {'resid': 1082, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 9.77890396118164, 'force': [-0.357083797454834, 1.5588886737823486, 0.9555392861366272], 'magnitude': 1.8629809617996216, 'cosine_with_motion': 0.07680045068264008, 'motion_component': 0.1430777758359909, 'motion_component_percent': 7.680045068264008}, {'resid': 1082, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 9.818870544433594, 'force': [0.4628981053829193, -1.5314768552780151, -1.2065175771713257], 'magnitude': 2.0038416385650635, 'cosine_with_motion': -0.08712252974510193, 'motion_component': -0.17457975447177887, 'motion_component_percent': 8.712252974510193}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'CB', 'charge': -0.22990000247955322, 'distance': 13.933757781982422, 'force': [-0.16021452844142914, -0.08001680672168732, -0.3499755859375], 'magnitude': 0.3931339383125305, 'cosine_with_motion': -0.7904166579246521, 'motion_component': -0.3107396066188812, 'motion_component_percent': 79.04166579246521}, {'resid': 130, 'resname': 'ASN', 'atom': 'HB2', 'charge': 0.1023000031709671, 'distance': 13.398519515991211, 'force': [0.08891411870718002, 0.03725716471672058, 0.16278623044490814], 'magnitude': 0.1891908347606659, 'cosine_with_motion': 0.8302130699157715, 'motion_component': 0.15706869959831238, 'motion_component_percent': 83.02130699157715}, {'resid': 130, 'resname': 'ASN', 'atom': 'HB3', 'charge': 0.1023000031709671, 'distance': 14.006364822387695, 'force': [0.06748197972774506, 0.048184383660554886, 0.15197743475437164], 'magnitude': 0.1731262356042862, 'cosine_with_motion': 0.7681266069412231, 'motion_component': 0.13298286497592926, 'motion_component_percent': 76.81266069412231}, {'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 13.4276123046875, 'force': [0.43182173371315, 0.2009008675813675, 1.2280069589614868], 'magnitude': 1.3171303272247314, 'cosine_with_motion': 0.742245614528656, 'motion_component': 0.9776341915130615, 'motion_component_percent': 74.2245614528656}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 13.895955085754395, 'force': [-0.25948894023895264, -0.18953008949756622, -0.9820889234542847], 'magnitude': 1.0333222150802612, 'cosine_with_motion': -0.684008777141571, 'motion_component': -0.7068014740943909, 'motion_component_percent': 68.4008777141571}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 12.774867057800293, 'force': [-0.6256296038627625, -0.12645207345485687, -1.7342747449874878], 'magnitude': 1.8480019569396973, 'cosine_with_motion': -0.7554131746292114, 'motion_component': -1.3960050344467163, 'motion_component_percent': 75.54131746292114}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 12.603804588317871, 'force': [0.24447666108608246, 0.015903739258646965, 0.8320061564445496], 'magnitude': 0.8673269152641296, 'cosine_with_motion': 0.7168015241622925, 'motion_component': 0.6217012405395508, 'motion_component_percent': 71.68015241622925}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 12.535192489624023, 'force': [0.3588235080242157, 0.04589592292904854, 0.7987497448921204], 'magnitude': 0.8768476843833923, 'cosine_with_motion': 0.8035885691642761, 'motion_component': 0.7046247720718384, 'motion_component_percent': 80.35885691642761}, {'resid': 458, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 14.582756996154785, 'force': [-0.6868134140968323, 0.082407645881176, 0.8766845464706421], 'magnitude': 1.1167271137237549, 'cosine_with_motion': -0.15040802955627441, 'motion_component': -0.16796472668647766, 'motion_component_percent': 15.040802955627441}, {'resid': 458, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 14.133539199829102, 'force': [0.5508571863174438, -0.05966679006814957, -0.831110954284668], 'magnitude': 0.9988739490509033, 'cosine_with_motion': 0.07182924449443817, 'motion_component': 0.07174836099147797, 'motion_component_percent': 7.182924449443817}, {'resid': 458, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 14.481070518493652, 'force': [0.9267371296882629, -0.21462300419807434, -1.0786395072937012], 'magnitude': 1.4381821155548096, 'cosine_with_motion': 0.1939576119184494, 'motion_component': 0.2789463698863983, 'motion_component_percent': 19.39576119184494}, {'resid': 458, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 13.925216674804688, 'force': [-0.4413902461528778, 0.14458680152893066, 0.5377005338668823], 'magnitude': 0.7105297446250916, 'cosine_with_motion': -0.17100666463375092, 'motion_component': -0.12150532007217407, 'motion_component_percent': 17.10066646337509}, {'resid': 458, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 14.97500991821289, 'force': [-0.4229383170604706, 0.092687226831913, 0.4359138607978821], 'magnitude': 0.6144010424613953, 'cosine_with_motion': -0.2521953284740448, 'motion_component': -0.15494906902313232, 'motion_component_percent': 25.21953284740448}, {'resid': 786, 'resname': 'ASN', 'atom': 'H', 'charge': 0.2681000232696533, 'distance': 14.847915649414062, 'force': [-0.00245463359169662, -0.2420821338891983, 0.3231064975261688], 'magnitude': 0.4037419855594635, 'cosine_with_motion': 0.3941119313240051, 'motion_component': 0.15911953151226044, 'motion_component_percent': 39.41119313240051}, {'resid': 786, 'resname': 'ASN', 'atom': 'CA', 'charge': -0.20800000429153442, 'distance': 14.854999542236328, 'force': [0.04117432236671448, 0.1677521914243698, -0.2609465420246124], 'magnitude': 0.3129364550113678, 'cosine_with_motion': -0.300702303647995, 'motion_component': -0.0941007137298584, 'motion_component_percent': 30.0702303647995}, {'resid': 786, 'resname': 'ASN', 'atom': 'CB', 'charge': -0.22990000247955322, 'distance': 13.311960220336914, 'force': [0.05321504920721054, 0.22355306148529053, -0.3642940819263458], 'magnitude': 0.43071797490119934, 'cosine_with_motion': -0.3133774697780609, 'motion_component': -0.1349773108959198, 'motion_component_percent': 31.33774697780609}, {'resid': 786, 'resname': 'ASN', 'atom': 'HB2', 'charge': 0.1023000031709671, 'distance': 12.743988037109375, 'force': [-0.027499817311763763, -0.12078683823347092, 0.16848434507846832], 'magnitude': 0.20912359654903412, 'cosine_with_motion': 0.2873244881629944, 'motion_component': 0.06008633226156235, 'motion_component_percent': 28.73244881629944}, {'resid': 786, 'resname': 'ASN', 'atom': 'HB3', 'charge': 0.1023000031709671, 'distance': 13.190842628479004, 'force': [-0.00935207400470972, -0.09686923772096634, 0.16920393705368042], 'magnitude': 0.19519497454166412, 'cosine_with_motion': 0.3893669843673706, 'motion_component': 0.07600247859954834, 'motion_component_percent': 38.93669843673706}, {'resid': 786, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 12.987796783447266, 'force': [-0.28514716029167175, -0.6317389607429504, 1.2254098653793335], 'magnitude': 1.4078466892242432, 'cosine_with_motion': 0.2559927999973297, 'motion_component': 0.36039862036705017, 'motion_component_percent': 25.59927999973297}, {'resid': 786, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 12.773780822753906, 'force': [0.21760711073875427, 0.44804903864860535, -1.1168099641799927], 'magnitude': 1.222851276397705, 'cosine_with_motion': -0.29765090346336365, 'motion_component': -0.36398279666900635, 'motion_component_percent': 29.765090346336365}, {'resid': 786, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 13.178906440734863, 'force': [0.5032789707183838, 0.8089449405670166, -1.4517216682434082], 'magnitude': 1.736426591873169, 'cosine_with_motion': -0.16325289011001587, 'motion_component': -0.28347665071487427, 'motion_component_percent': 16.325289011001587}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 13.067357063293457, 'force': [-0.2754772901535034, -0.33098629117012024, 0.6823641061782837], 'magnitude': 0.8068831562995911, 'cosine_with_motion': 0.12252197414636612, 'motion_component': 0.09886091947555542, 'motion_component_percent': 12.252197414636612}, {'resid': 786, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 13.330060958862305, 'force': [-0.2378445416688919, -0.407608449459</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>789</v>
+      </c>
+      <c r="B10" t="n">
+        <v>794</v>
+      </c>
+      <c r="C10" t="n">
+        <v>2247</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>{735: {'frame': 735, 'motion_vector': [-0.15482711791992188, 0.24771881103515625, 0.11165618896484375], 'motion_vector_magnitude': 0.3127349615097046, 'ionic_force': [0.05034467577934265, 1.278035044670105, 33.2567253112793], 'ionic_force_magnitude': 33.28131137127366, 'radial_force': 1.279026255314661, 'axial_force': 33.2567253112793, 'glu_force': [1.4249044463504106, -0.5858631468145177, -2.7867901055142283], 'glu_force_magnitude': 3.184303283328487, 'asn_force': [0.0, 0.0, 0.0], 'asn_force_magnitude': 0.0, 'sf_force': [2.0691297974080953, -2.4244274701486574, -6.324143321020529], 'sf_force_magnitude': 7.081944324925327, 'residue_force': [3.494034243758506, -3.010290616963175, -9.110933426534757], 'residue_force_magnitude': 10.211720364261938, 'pip2_force': [0.4278039773926139, 0.059453467663843185, -3.340027960948646], 'pip2_force_magnitude': 3.3678387339373845, 'total_force': [3.9721828969304624, -1.672802104629227, 20.805763923795894], 'total_force_magnitude': 21.247501413122567, 'cosine_total_motion': 0.1946934633710557, 'cosine_glu_motion': -0.6797312063593116, 'cosine_asn_motion': 0, 'cosine_sf_motion': -0.7346416446364206, 'cosine_residue_motion': -0.7214417625516292, 'cosine_pip2_motion': -0.4029873088852142, 'cosine_ionic_motion': 0.38643631860099853, 'motion_component_total': 4.136749638102232, 'motion_component_glu': -2.1644703121907893, 'motion_component_asn': 0, 'motion_component_sf': -5.202691226086707, 'motion_component_residue': -7.367161538277497, 'motion_component_ionic': 12.861107444528542, 'motion_component_pip2': -1.3571962681488137, 'motion_component_percent_total': 19.46934633710557, 'motion_component_percent_glu': 67.97312063593117, 'motion_component_percent_asn': 0, 'motion_component_percent_sf': 73.46416446364205, 'motion_component_percent_residue': 72.14417625516292, 'motion_component_percent_ionic': 38.64363186009985, 'motion_component_percent_pip2': 40.29873088852142, 'ionic_contributions': [{'ion_id': 2223, 'distance': 14.000561714172363, 'force': [0.1022900640964508, -0.9547053575515747, 1.3952902555465698], 'magnitude': 1.6937415599822998, 'cosine_ionic_motion': -0.1822623461484909, 'motion_component_ionic': -0.30870530009269714, 'motion_component_percent_ionic': 18.22623461484909}, {'ion_id': 2333, 'distance': 3.664323329925537, 'force': [0.7465257048606873, 0.9109559059143066, 24.697742462158203], 'magnitude': 24.72580909729004, 'cosine_ionic_motion': 0.3708617091178894, 'motion_component_ionic': 9.169856071472168, 'motion_component_percent_ionic': 37.08617091178894}, {'ion_id': 2391, 'distance': 12.038893699645996, 'force': [0.4656803011894226, 0.8973014950752258, 2.0555336475372314], 'magnitude': 2.290682554244995, 'cosine_ionic_motion': 0.5300167798995972, 'motion_component_ionic': 1.2141002416610718, 'motion_component_percent_ionic': 53.00167798995972}, {'ion_id': 2397, 'distance': 9.809953689575195, 'force': [-0.8989313244819641, 0.1696433126926422, 3.326383113861084], 'magnitude': 3.4498813152313232, 'cosine_ionic_motion': 0.5122020840644836, 'motion_component_ionic': 1.7670364379882812, 'motion_component_percent_ionic': 51.220208406448364}, {'ion_id': 2520, 'distance': 13.445075035095215, 'force': [-0.3652200698852539, 0.254839688539505, 1.7817758321762085], 'magnitude': 1.8365875482559204, 'cosine_ionic_motion': 0.5547357201576233, 'motion_component_ionic': 1.0188207626342773, 'motion_component_percent_ionic': 55.47357201576233}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 11.731096267700195, 'force': [-1.004483699798584, -0.26458218693733215, -0.6873260140419006], 'magnitude': 1.2455554008483887, 'cosine_with_motion': 0.03397727757692337, 'motion_component': 0.042320579290390015, 'motion_component_percent': 3.397727757692337}, {'resid': 98, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 12.073562622070312, 'force': [0.5686269402503967, 0.11786603927612305, 0.3315329849720001], 'magnitude': 0.6686875820159912, 'cosine_with_motion': -0.10435784608125687, 'motion_component': -0.0697827935218811, 'motion_component_percent': 10.435784608125687}, {'resid': 98, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 12.468323707580566, 'force': [0.06407091021537781, 0.014702009968459606, 0.053544823080301285], 'magnitude': 0.08478371798992157, 'cosine_with_motion': -0.01128946803510189, 'motion_component': -0.0009571630507707596, 'motion_component_percent': 1.128946803510189}, {'resid': 98, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 12.887487411499023, 'force': [0.15904511511325836, 0.053399261087179184, 0.14367611706256866], 'magnitude': 0.2208838164806366, 'cosine_with_motion': 0.06725478172302246, 'motion_component': 0.014855492860078812, 'motion_component_percent': 6.725478172302246}, {'resid': 98, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 13.588374137878418, 'force': [0.07937899231910706, 0.011139985173940659, 0.06093912199139595], 'magnitude': 0.10069111734628677, 'cosine_with_motion': -0.0865747481584549, 'motion_component': -0.008717307820916176, 'motion_component_percent': 8.65747481584549}, {'resid': 98, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 13.290796279907227, 'force': [-0.026789288967847824, -0.00177772028837353, -0.01834097132086754], 'magnitude': 0.03251488134264946, 'cosine_with_motion': 0.16319458186626434, 'motion_component': 0.0053062522783875465, 'motion_component_percent': 16.319458186626434}, {'resid': 98, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 14.142755508422852, 'force': [-0.02160283736884594, -0.0023084997665137053, -0.018776774406433105], 'magnitude': 0.028715483844280243, 'cosine_with_motion': 0.07530935108661652, 'motion_component': 0.002162544522434473, 'motion_component_percent': 7.530935108661652}, {'resid': 98, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 14.755379676818848, 'force': [0.016718659549951553, 0.003558574477210641, 0.011743348091840744], 'magnitude': 0.020738448947668076, 'cosine_with_motion': -0.06102071702480316, 'motion_component': -0.0012654750607907772, 'motion_component_percent': 6.102071702480316}, {'resid': 98, 'resname': 'GLU', 'atom': 'HG2', 'charge': -0.042500000447034836, 'distance': 14.753222465515137, 'force': [-0.054586250334978104, -0.012364741414785385, -0.03270998224616051], 'magnitude': 0.064826600253582, 'cosine_with_motion': 0.08563777059316635, 'motion_component': 0.005551605485379696, 'motion_component_percent': 8.563777059316635}, {'resid': 98, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 11.69831657409668, 'force': [0.9191528558731079, 0.1413482278585434, 0.9109578728675842], 'magnitude': 1.3017932176589966, 'cosine_with_motion': -0.013708825223147869, 'motion_component': -0.017846055328845978, 'motion_component_percent': 1.370882522314787}, {'resid': 98, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 11.857131958007812, 'force': [-0.8624247908592224, -0.18216408789157867, -1.0541666746139526], 'magnitude': 1.374127984046936, 'cosine_with_motion': -0.06818799674510956, 'motion_component': -0.09369903802871704, 'motion_component_percent': 6.818799674510956}, {'resid': 426, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 10.723194122314453, 'force': [1.2657051086425781, 0.29620856046676636, -0.729694664478302], 'magnitude': 1.4907056093215942, 'cosine_with_motion': -0.4377216398715973, 'motion_component': -0.6525141000747681, 'motion_component_percent': 43.77216398715973}, {'resid': 426, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 11.147733688354492, 'force': [-0.6970469355583191, -0.11863310635089874, 0.3395406901836395], 'magnitude': 0.7843698859214783, 'cosine_with_motion': 0.4747084677219391, 'motion_component': 0.37234702706336975, 'motion_component_percent': 47.47084677219391}, {'resid': 426, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 11.575762748718262, 'force': [-0.07800214737653732, -0.019544798880815506, 0.05664660781621933], 'magnitude': 0.09836245328187943, 'cosine_with_motion': 0.44081827998161316, 'motion_component': 0.043359968811273575, 'motion_component_percent': 44.081827998161316}, {'resid': 426, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 11.568466186523438, 'force': [-0.2077416479587555, -0.07823709398508072, 0.160832017660141], 'magnitude': 0.2741250991821289, 'cosine_with_motion': 0.3585870563983917, 'motion_component': 0.09829771518707275, 'motion_component_percent': 35.85870563983917}, {'resid': 426, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 12.927265167236328, 'force': [-0.09193253517150879, -0.017758311703801155, 0.06008613482117653], 'magnitude': 0.1112532839179039, 'cosine_with_motion': 0.47548848390579224, 'motion_component': 0.05289965495467186, 'motion_component_percent': 47.548848390579224}, {'resid': 426, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 13.256302833557129, 'force': [0.028070777654647827, 0.006260174326598644, -0.015527592971920967], 'magnitude': 0.032684314996004105, 'cosine_with_motion': -0.4430948793888092, 'motion_component': -0.014482252299785614, 'motion_component_percent': 44.30948793888092}, {'resid': 426, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 13.094057083129883, 'force': [0.028140563517808914, 0.0026140070986002684, -0.01798551343381405], 'magnitude': 0.033499300479888916, 'cosine_with_motion': -0.5457577705383301, 'motion_component': -0.01828250288963318, 'motion_component_percent': 54.57577705383301}, {'resid': 426, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 14.262663841247559, 'force': [-0.01748662255704403, -0.004185930360108614, 0.013013862073421478], 'magnitude': 0.022196048870682716, 'cosine_with_motion': 0.44998297095298767, 'motion_component': 0.0099878441542387, 'motion_component_percent': 44.99829709529877}, {'resid': 426, 'resname': 'GLU', 'atom': 'HG2', 'charge': -0.042500000447034836, 'distance': 14.107640266418457, 'force': [0.054048702120780945, 0.018431879580020905, -0.042013879865407944], 'magnitude': 0.07089543342590332, 'cosine_with_motion': -0.3830772936344147, 'motion_component': -0.027158431708812714, 'motion_component_percent': 38.30772936344147}, {'resid': 426, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 14.647502899169922, 'force': [-0.9259982109069824, -0.15302973985671997, 0.8199833035469055], 'magnitude': 1.2462998628616333, 'cosine_with_motion': 0.5054821372032166, 'motion_component': 0.6299823522567749, 'motion_component_percent': 50.548213720321655}, {'resid': 426, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 14.975423812866211, 'force': [0.8327013254165649, 0.18589307367801666, -0.8610275387763977], 'magnitude': 1.2121535539627075, 'cosine_with_motion': -0.47223085165023804, 'motion_component': -0.5724163055419922, 'motion_component_percent': 47.223085165023804}, {'resid': 426, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 14.780047416687012, 'force': [0.9482935667037964, 0.05117681995034218, -0.8041653633117676], 'magnitude': 1.2444121837615967, 'cosine_with_motion': -0.575412929058075, 'motion_component': -0.7160508632659912, 'motion_component_percent': 57.541292905807495}, {'resid': 426, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 11.303415298461914, 'force': [-1.023337960243225, -0.17790468037128448, 0.9302254319190979], 'magnitude': 1.3943421840667725, 'cosine_with_motion': 0.5004719495773315, 'motion_component': 0.6978291273117065, 'motion_component_percent': 50.047194957733154}, {'resid': 426, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 11.693343162536621, 'force': [0.9384178519248962, 0.24427510797977448, -1.027602195739746], 'magnitude': 1.4128923416137695, 'cosine_with_motion': -0.4515429735183716, 'motion_component': -0.6379815936088562, 'motion_component_percent': 45.15429735183716}, {'resid': 754, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 11.153669357299805, 'force': [-0.30229347944259644, 1.1480543613433838, -0.6993459463119507], 'magnitude': 1.3778588771820068, 'cosine_with_motion': 0.5873957872390747, 'motion_component': 0.809348464012146, 'motion_component_percent': 58.73957872390747}, {'resid': 754, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 11.24092960357666, 'force': [0.12894432246685028, -0.6769554615020752, 0.3466845750808716], 'magnitude': 0.7714179158210754, 'cosine_with_motion': -0.6174076199531555, 'motion_component': -0.4762793183326721, 'motion_component_percent': 61.74076199531555}, {'resid': 754, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 11.996248245239258, 'force': [0.016562316566705704, -0.07196850329637527, 0.05417150259017944], 'magnitude': 0.09158781170845032, 'cosine_with_motion': -0.50077885389328, 'motion_component': -0.04586523771286011, 'motion_component_percent': 50.077885389328}, {'resid': 754, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 12.302226066589355, 'force': [0.06052393093705177, -0.1801428496837616, 0.15047678351402283], 'magnitude': 0.24240019917488098, 'cosine_with_motion': -0.4906386435031891, 'motion_component': -0.11893090605735779, 'motion_component_percent': 49.06386435031891}, {'resid': 754, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 13.369449615478516, 'force': [0.01625142991542816, -0.08509419858455658, 0.05756857991218567], 'magnitude': 0.10401573777198792, 'cosine_with_motion': -0.5277603268623352, 'motion_component': -0.05489538237452507, 'motion_component_percent': 52.77603268623352}, {'resid': 754, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 13.71593952178955, 'force': [-0.006336808670312166, 0.025644473731517792, -0.015307306312024593], 'magnitude': 0.03053044155240059, 'cosine_with_motion': 0.5890878438949585, 'motion_component': 0.017985111102461815, 'motion_component_percent': 58.90878438949585}, {'resid': 754, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 13.425566673278809, 'force': [-0.0027077896520495415, 0.026960354298353195, -0.0167692881077528], 'magnitude': 0.03186536952853203, 'cosine_with_motion': 0.5243565440177917, 'motion_component': 0.016708815470337868, 'motion_component_percent': 52.435654401779175}, {'resid': 754, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 14.486411094665527, 'force': [0.00317567796446383, -0.016697069630026817, 0.013192728161811829], 'magnitude': 0.02151569537818432, 'cosine_with_motion': -0.46885794401168823, 'motion_component': -0.01008780486881733, 'motion_component_percent': 46.88579440116882}, {'resid': 754, 'resname': 'GLU', 'atom': 'HG2', 'charge': -0.042500000447034836, 'distance': 14.496532440185547, 'force': [-0.013806643895804882, 0.04956558346748352, -0.043136656284332275], 'magnitude': 0.06714269518852234, 'cosine_with_motion': 0.4571651816368103, 'motion_component': 0.030695302411913872, 'motion_component_percent': 45.71651816368103}, {'resid': 754, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 14.450767517089844, 'force': [0.0815165713429451, -0.9481583833694458, 0.8567044734954834], 'magnitude': 1.2804654836654663, 'cosine_with_motion': -0.37918010354042053, 'motion_component': -0.48552703857421875, 'motion_component_percent': 37.91801035404205}, {'resid': 754, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 14.082502365112305, 'force': [0.02159946598112583, 1.0457407236099243, -0.8859445452690125], 'magnitude': 1.3707436323165894, 'cosine_with_motion': 0.36573776602745056, 'motion_component': 0.501332700252533, 'motion_component_percent': 36.573776602745056}, {'resid': 754, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 11.500566482543945, 'force': [0.1258777230978012, -0.9933637976646423, 0.9009147882461548], 'magnitude': 1.3469462394714355, 'cosine_with_motion': -0.391635537147522, 'motion_component': -0.5275120139122009, 'motion_component_percent': 39.1635537147522}, {'resid': 754, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 11.822552680969238, 'force': [-0.13474401831626892, 0.9224129915237427, -1.0204968452453613], 'magnitude': 1.3821778297424316, 'cosine_with_motion': 0.3132784366607666, 'motion_component': 0.43300649523735046, 'motion_component_percent': 31.32784366607666}, {'resid': 1082, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 11.39023208618164, 'force': [0.3258711099624634, -1.0514187812805176, -0.730717658996582], 'magnitude': 1.321219801902771, 'cosine_with_motion': -0.949920117855072, 'motion_component': -1.2550532817840576, 'motion_component_percent': 94.9920117855072}, {'resid': 1082, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 11.673358917236328, 'force': [-0.15102924406528473, 0.603450357913971, 0.35316503047943115], 'magnitude': 0.7153235077857971, 'cosine_with_motion': 0.9490217566490173, 'motion_component': 0.6788575649261475, 'motion_component_percent': 94.90217566490173}, {'resid': 1082, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 12.330633163452148, 'force': [-0.019816262647509575, 0.06424316018819809, 0.05472569540143013], 'magnitude': 0.08668777346611023, 'cosine_with_motion': 0.9255817532539368, 'motion_component': 0.08023662120103836, 'motion_component_percent': 92.55817532539368}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 12.377656936645508, 'force': [-0.0713832676410675, 0.16595123708248138, 0.15717251598834991], 'magnitude': 0.23945476114749908, 'cosine_with_motion': 0.9308910369873047, 'motion_component': 0.22290629148483276, 'motion_component_percent': 93.08910369873047}, {'resid': 1082, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 13.741291999816895, 'force': [-0.020244339480996132, 0.07575328648090363, 0.05955230072140694], 'magnitude': 0.0984625369310379, 'cosine_with_motion': 0.9271447658538818, 'motion_component': 0.09128902852535248, 'motion_component_percent': 92.71447658538818}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 14.001485824584961, 'force': [0.007517672143876553, -0.02322305552661419, -0.016203057020902634], 'magnitude': 0.02929786406457424, 'cosine_with_motion': -0.9523525238037109, 'motion_component': -0.027901895344257355, 'motion_component_percent': 95.2352523803711}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 13.797815322875977, 'force': [0.004178594332188368, -0.024222007021307945, -0.0174932349473238], 'magnitude': 0.030169183388352394, 'cosine_with_motion': -0.9115497469902039, 'motion_component': -0.027500711381435394, 'motion_component_percent': 91.15497469902039}, {'resid': 1082, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 14.960424423217773, 'force': [-0.004187011159956455, 0.014623490162193775, 0.013251695781946182], 'magnitude': 0.020173868164420128, 'cosine_with_motion': 0.9114507436752319, 'motion_component': 0.018387487158179283, 'motion_component_percent': 91.1450743675232}, {'resid': 1082, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 14.669754981994629, 'force': [0.444660484790802, -0.8409731388092041, -0.8310842514038086], 'magnitude': 1.26319420337677, 'cosine_with_motion': -0.9365163445472717, 'motion_component': -1.18300199508667, 'motion_component_percent': 93.65163445472717}, {'resid': 1082, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 11.98241138458252, 'force': [-0.1741536557674408, 0.8656761646270752, 0.8716934323310852], 'magnitude': 1.2407957315444946, 'cosine_with_motion': 0.8729454874992371, 'motion_component': 1.0831470489501953, 'motion_component_percent': 87.2945487499237}, {'resid': 1082, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 12.283918380737305, 'force': [0.19798922538757324, -0.796104907989502, -0.9829505681991577], 'magnitude': 1.2803025245666504, 'cosine_with_motion': -0.8432084918022156, 'motion_component': -1.0795619487762451, 'motion_component_percent': 84.32084918022156}], 'asn_contributions': [], 'sf_contributions': [{'resid': 100, 'resname': 'THR', 'atom': 'N', 'charge': -0.4157000184059143, 'distance': 8.816055297851562, 'force': [-1.1153616905212402, -0.12437710165977478, -1.376084327697754], 'magnitude': 1.7756996154785156, 'cosine_with_motion': -0.021196018904447556, 'motion_component': -0.03763776272535324, 'motion_component_percent': 2.1196018904447556}, {'resid': 100, 'resname': 'THR', 'atom': 'H', 'charge': 0.2718999981880188, 'distance': 9.158703804016113, 'force': [0.7519910335540771, 0.1178789734840393, 0.7607544660568237], 'magnitude': 1.076166033744812, 'cosine_with_motion': -0.006788854952901602, 'motion_component': -0.007305935025215149, 'motion_component_percent': 0.6788854952901602}, {'resid': 100, 'resname': 'THR', 'atom': 'CA', 'charge': -0.03889999911189079, 'distance': 7.641517162322998, 'force': [-0.12352830916643143, -0.035033468157052994, -0.18008357286453247], 'magnitude': 0.22117115557193756, 'cosine_with_motion': -0.13966530561447144, 'motion_component': -0.030889935791492462, 'motion_component_percent': 13.966530561447144}, {'resid': 100, 'resname': 'THR', 'atom': 'HA', 'charge': 0.1007000058889389, 'distance': 7.5666046142578125, 'force': [0.35627874732017517, 0.15876948833465576, 0.43455642461776733], 'magnitude': 0.5839362740516663, 'cosine_with_motion': 0.1790054738521576, 'motion_component': 0.1045277863740921, 'motion_component_percent': 17.90054738521576}, {'resid': 100, 'resname': 'THR', 'atom': 'CB', 'charge': 0.3653999865055084, 'distance': 8.15181827545166, 'force': [0.7304357886314392, 0.39796310663223267, 1.6250481605529785], 'magnitude': 1.8255664110183716, 'cosine_with_motion': 0.2924031913280487, 'motion_component': 0.5338014364242554, 'motion_component_percent': 29.24031913280487}, {'resid': 100, 'resname': 'THR', 'atom': 'HB', 'charge': 0.00430000014603138, 'distance': 7.593003273010254, 'force': [0.00835275650024414, 0.007897173054516315, 0.02193182148039341], 'magnitude': 0.024761637672781944, 'cosine_with_motion': 0.4018514156341553, 'motion_component': 0.009950499050319195, 'motion_component_percent': 40.18514156341553}, {'resid': 100, 'resname': 'THR', 'atom': 'CG2', 'charge': -0.24380001425743103, 'distance': 9.604183197021484, 'force': [-0.36054062843322754, -0.25149238109588623, -0.7594615817070007], 'magnitude': 0.877507746219635, 'cosine_with_motion': -0.3326072096824646, 'motion_component': -0.29186540842056274, 'motion_component_percent': 33.26072096824646}, {'resid': 100, 'resname': 'THR', 'atom': 'HG21', 'charge': 0.0642000064253807, 'distance': 9.679905891418457, 'force': [0.10999336838722229, 0.07888063788414001, 0.18282099068164825], 'magnitude': 0.22747352719306946, 'cosine_with_motion': 0.3222336769104004, 'motion_component': 0.07329963147640228, 'motion_component_percent': 32.22336769104004}, {'resid': 100, 'resname': 'THR', 'atom': 'HG22', 'charge': 0.0642000064253807, 'distance': 10.360023498535156, 'force': [0.08319679647684097, 0.04177035018801689, 0.17541515827178955], 'magnitude': 0.19858737289905548, 'cosine_with_motion': 0.2745722830295563, 'motion_component': 0.05452658608555794, 'motion_component_percent': 27.457228302955627}, {'resid': 100, 'resname': 'THR', 'atom': 'HG23', 'charge': 0.0642000064253807, 'distance': 9.994627952575684, 'force': [0.06965199112892151, 0.07368990778923035, 0.18774057924747467], 'magnitude': 0.21337321400642395, 'cosine_with_motion': 0.4260912537574768, 'motion_component': 0.0909164622426033, 'motion_component_percent': 42.60912537574768}, {'resid': 100, 'resname': 'THR', 'atom': 'OG1', 'charge': -0.6761000156402588, 'distance': 8.437439918518066, 'force': [-0.9932865500450134, -0.2880045473575592, -2.9785923957824707], 'magnitude': 3.153026819229126, 'cosine_with_motion': -0.25367045402526855, 'motion_component': -0.7998297810554504, 'motion_component_percent': 25.367045402526855}, {'resid': 100, 'resname': 'THR', 'atom': 'HG1', 'charge': 0.41019999980926514, 'distance': 9.101644515991211, 'force': [0.602523684501648, 0.05451073497533798, 1.5286046266555786], 'magnitude': 1.643970251083374, 'cosine_with_motion': 0.1767938733100891, 'motion_component': 0.2906438708305359, 'motion_component_percent': 17.67938733100891}, {'resid': 100, 'resname': 'THR', 'atom': 'C', 'charge': 0.5973000526428223, 'distance': 6.356112957000732, 'force': [2.7432823181152344, 0.2200930118560791, 4.064379692077637], 'magnitude': 4.90848445892334, 'cosine_with_motion': 0.054460491985082626, 'motion_component': 0.2673184871673584, 'motion_component_percent': 5.446049198508263}, {'resid': 100, 'resname': 'THR', 'atom': 'O', 'charge': -0.5679000020027161, 'distance': 5.504797458648682, 'force': [-2.7451915740966797, -0.6719012260437012, -5.543037414550781], 'magnitude': 6.221960544586182, 'cosine_with_motion': -0.18517954647541046, 'motion_component': -1.1521798372268677, 'motion_component_percent': 18.517954647541046}, {'resid': 101, 'resname': 'ILE', 'atom': 'N', 'charge': -0.4157000184059143, 'distance': 6.377499580383301, 'force': [-2.2609503269195557, 0.3860912322998047, -2.5006513595581055], 'magnitude': 3.393260955810547, 'cosine_with_motion': 0.1568852663040161, 'motion_component': 0.5323526263237, 'motion_component_percent': 15.688526630401611}, {'resid': 101, 'resname': 'ILE', 'atom': 'H', 'charge': 0.2718999981880188, 'distance': 7.261749267578125, 'force': [1.2272729873657227, -0.20661857724189758, 1.1753840446472168], 'magnitude': 1.7118463516235352, 'cosine_with_motion': -0.2053958773612976, 'motion_component': -0.35160619020462036, 'motion_component_percent': 20.53958773612976}, {'resid': 101, 'resname': 'ILE', 'atom': 'CA', 'charge': -0.059700001031160355, 'distance': 5.3528618812561035, 'force': [-0.4610254466533661, 0.1987908035516739, -0.4758533239364624], 'magnitude': 0.6917359828948975, 'cosine_with_motion': 0.3119839131832123, 'motion_component': 0.21581050753593445, 'motion_component_percent': 31.198391318321228}, {'resid': 101, 'resname': 'ILE', 'atom': 'HA', 'charge': 0.0869000032544136, 'distance': 5.35119104385376, 'force': [0.5060008764266968, -0.35270726680755615, 0.7966634035110474], 'magnitude': 1.0075275897979736, 'cosine_with_motion': -0.24362146854400635, 'motion_component': -0.24545535445213318, 'motion_component_percent': 24.362146854400635}, {'resid': 101, 'resname': 'ILE', 'atom': 'CB', 'charge': 0.13030001521110535, 'distance': 6.334309101104736, 'force': [0.7683430314064026, -0.48011454939842224, 0.5844419598579407], 'magnitude': 1.0781620740890503, 'cosine_with_motion': -0.512004554271698, 'motion_component': -0.5520238876342773, 'motion_component_percent': 51.2004554271698}, {'resid': 101, 'resname': 'ILE', 'atom': 'HB', 'charge': 0.018699999898672104, 'distance': 6.717626571655273, 'force': [0.11189384013414383, -0.05101283639669418, 0.06168530881404877], 'magnitude': 0.13757768273353577, 'cosine_with_motion': -0.5362766981124878, 'motion_component': -0.07377970218658447, 'motion_component_percent': 53.62766981124878}, {'resid': 101, 'resname': 'ILE', 'atom': 'CG2', 'charge': -0.3203999996185303, 'distance': 5.958845615386963, 'force': [-1.9719668626785278, 1.8992571830749512, -1.216025948524475], 'magnitude': 2.995755434036255, 'cosine_with_motion': 0.6831404566764832, 'motion_component': 2.0465216636657715, 'motion_component_percent': 68.31404566764832}, {'resid': 101, 'resname': 'ILE', 'atom': 'HG21', 'charge': 0.08820000290870667, 'distance': 5.709073543548584, 'force': [0.45939916372299194, -0.6438101530075073, 0.4261508285999298], 'magnitude': 0.898411750793457, 'cosine_with_motion': -0.6514303088188171, 'motion_component': -0.5852526426315308, 'motion_component_percent': 65.14303088188171}, {'resid': 101, 'resname': 'ILE', 'atom': 'HG22', 'charge': 0.08820000290870667, 'distance': 6.872889995574951, 'force': [0.4184933602809906, -0.4120675027370453, 0.19837024807929993], 'magnitude': 0.6199089288711548, 'cosine_with_motion': -0.7464993000030518, 'motion_component': -0.4627615809440613, 'motion_component_percent': 74.64993000030518}, {'resid': 101, 'resname': 'ILE', 'atom': 'HG23', 'charge': 0.08820000290870667, 'distance': 5.270881175994873, 'force': [0.7543463110923767, -0.6802529096603394, 0.28130343556404114], 'magnitude': 1.0539990663528442, 'cosine_with_motion': -0.7702615261077881, 'motion_component': -0.8118549585342407, 'motion_component_percent': 77.02615261077881}, {'resid': 101, 'resname': 'ILE', 'atom': 'CG1', 'charge': -0.0430000014603138, 'distance': 7.552713394165039, 'force': [-0.1551971733570099, 0.12270943820476532, -0.1532609462738037], 'magnitude': 0.2502652406692505, 'cosine_with_motion': 0.47674983739852905, 'motion_component': 0.11931391060352325, 'motion_component_percent': 47.674983739852905}, {'resid': 101, 'resname': 'ILE', 'atom': 'HG12', 'charge': 0.023600000888109207, 'distance': 7.402340412139893, 'force': [0.0716981291770935, -0.07550033926963806, 0.09800924360752106], 'magnitude': 0.1429920792579651, 'cosine_with_motion': -0.4217556118965149, 'motion_component': -0.060307711362838745, 'motion_component_percent': 42.17556118965149}, {'resid': 101, 'resname': 'ILE', 'atom': 'HG13', 'charge': 0.023600000888109207, 'distance': 8.029217720031738, 'force': [0.07620379328727722, -0.04657674580812454, 0.08242876082658768], 'magnitude': 0.12153564393520355, 'cosine_with_motion': -0.37182965874671936, 'motion_component': -0.04519055783748627, 'motion_component_percent': 37.182965874671936}, {'resid': 101, 'resname': 'ILE', 'atom': 'CD1', 'charge': -0.06599999964237213, 'distance': 8.71054458618164, 'force': [-0.18130430579185486, 0.1675182282924652, -0.1498986780643463], 'magnitude': 0.28879615664482117, 'cosine_with_motion': 0.5849544405937195, 'motion_component': 0.16893258690834045, 'motion_component_percent': 58.49544405937195}, {'resid': 101, 'resname': 'ILE', 'atom': 'HD11', 'charge': 0.01860000006854534, 'distance': 9.597696304321289, 'force': [0.04020912945270538, -0.03716468811035156, 0.038678448647260666], 'magnitude': 0.06703738123178482, 'cosine_with_motion': -0.5300835967063904, 'motion_component': -0.03553541749715805, 'motion_component_percent': 53.00835967063904}, {'resid': 101, 'resname': 'ILE', 'atom': 'HD12', 'charge': 0.01860000006854534, 'distance': 8.939000129699707, 'force': [0.05484684556722641, -0.042893487960100174, 0.033531129360198975], 'magnitude': 0.07728107273578644, 'cosine_with_motion': -0.6360903382301331, 'motion_component': -0.04915774241089821, 'motion_component_percent': 63.609033823013306}, {'resid': 101, 'resname': 'ILE', 'atom': 'HD13', 'charge': 0.01860000006854534, 'distance': 8.4950590133667, 'force': [0.047569356858730316, -0.05778821185231209, 0.04147037863731384], 'magnitude': 0.0855693519115448, 'cosine_with_motion': -0.6371260285377502, 'motion_component': -0.05451846122741699, 'motion_component_percent': 63.712602853775024}, {'resid': 101, 'resname': 'ILE', 'atom': 'C', 'charge': 0.5973000526428223, 'distance': 4.095999717712402, 'force': [9.417631149291992, -2.15792179107666, 6.808796405792236], 'magnitude': 11.819818496704102, 'cosine_with_motion': -0.3334040343761444, 'motion_component': -3.940775156021118, 'motion_component_percent': 33.34040343761444}, {'resid': 101, 'resname': 'ILE', 'atom': 'O', 'charge': -0.5679000020027161, 'distance': 3.019723892211914, 'force': [-14.711637496948242, 5.779220104217529, -13.329774856567383], 'magnitude': 20.67642593383789, 'cosine_with_motion': 0.3434808552265167, 'motion_component': 7.101956367492676, 'motion_component_percent': 34.34808552265167}, {'resid': 102, 'resname': 'GLY', 'atom': 'N', 'charge': -0.4157000184059143, 'distance': 4.635801792144775, 'force': [-5.825216770172119, -0.02667613886296749, -2.703305244445801], 'magnitude': 6.421971797943115, 'cosine_with_motion': 0.2954889237880707, 'motion_component': 1.897621512413025, 'motion_component_percent': 29.548892378807068}, {'resid': 102, 'resname': 'GLY', 'atom': 'H', 'charge': 0.2718999981880188, 'distance': 5.627887725830078, 'force': [2.5522286891937256, 0.08771518617868423, 1.2654515504837036], 'magnitude': 2.8500759601593018, 'cosine_with_motion': -0</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>805</v>
+      </c>
+      <c r="B11" t="n">
+        <v>806</v>
+      </c>
+      <c r="C11" t="n">
+        <v>2231</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">{789: {'frame': 789, 'motion_vector': [-0.3777351379394531, -0.5515480041503906, -0.7409820556640625], 'motion_vector_magnitude': 0.9979696273803711, 'ionic_force': [-1.8180436491966248, 1.9862427115440369, 27.112340331077576], 'ionic_force_magnitude': 27.245723353358077, 'radial_force': 2.692664631837019, 'axial_force': 27.112340331077576, 'glu_force': [0.023792091858922504, 0.02174933929927647, -1.4417408108711243], 'glu_force_magnitude': 1.442101127912431, 'asn_force': [0.0, 0.0, 0.0], 'asn_force_magnitude': 0.0, 'sf_force': [0.9993288824625779, 4.147023725021427, -5.690206987084821], 'sf_force_magnitude': 7.111604569088709, 'residue_force': [1.0231209743215004, 4.168773064320703, -7.131947797955945], 'residue_force_magnitude': 8.324069003959005, 'pip2_force': [0.41510902624577284, -0.002843749476596713, -3.223507883492857], 'pip2_force_magnitude': 3.2501271768228395, 'total_force': [-0.3798136486293515, 6.152172026388143, 16.756884649628773], 'total_force_magnitude': 17.85459778911086, 'cosine_total_motion': -0.8792229977191637, 'cosine_glu_motion': 0.727724221232856, 'cosine_asn_motion': 0, 'cosine_sf_motion': 0.21861924764449006, 'cosine_residue_motion': 0.31285006881247773, 'cosine_pip2_motion': 0.6885491719553888, 'cosine_ionic_motion': -0.7538882584198244, 'motion_component_total': -15.698172991212001, 'motion_component_glu': 1.049451920249097, 'motion_component_asn': 0, 'motion_component_sf': 1.5547336404392915, 'motion_component_residue': 2.604185560688388, 'motion_component_ionic': -20.54023092825146, 'motion_component_pip2': 2.2378723763510715, 'motion_component_percent_total': 87.92229977191637, 'motion_component_percent_glu': 72.7724221232856, 'motion_component_percent_asn': 0, 'motion_component_percent_sf': 21.861924764449007, 'motion_component_percent_residue': 31.285006881247774, 'motion_component_percent_ionic': 75.38882584198244, 'motion_component_percent_pip2': 68.85491719553887, 'ionic_contributions': [{'ion_id': 2223, 'distance': 14.149683952331543, 'force': [-0.27153486013412476, 0.8629049062728882, 1.3897439241409302], 'magnitude': 1.6582292318344116, 'cosine_ionic_motion': -0.8478895425796509, 'motion_component_ionic': -1.40599524974823, 'motion_component_percent_ionic': 84.78895425796509}, {'ion_id': 2286, 'distance': 10.174296379089355, 'force': [-0.6761355996131897, -0.4113306701183319, -3.1080434322357178], 'magnitude': 3.207224130630493, 'cosine_ionic_motion': 0.8702041506767273, 'motion_component_ionic': 2.7909398078918457, 'motion_component_percent_ionic': 87.02041506767273}, {'ion_id': 2333, 'distance': 9.855289459228516, 'force': [-0.42506974935531616, 0.2663635313510895, 3.3812062740325928], 'magnitude': 3.4182143211364746, 'cosine_ionic_motion': -0.7304489612579346, 'motion_component_ionic': -2.496831178665161, 'motion_component_percent_ionic': 73.04489612579346}, {'ion_id': 2372, 'distance': 3.7240054607391357, 'force': [-0.7882312536239624, 2.1955366134643555, 23.825708389282227], 'magnitude': 23.939634323120117, 'cosine_ionic_motion': -0.7771797776222229, 'motion_component_ionic': -18.60540008544922, 'motion_component_percent_ionic': 77.71797776222229}, {'ion_id': 2397, 'distance': 13.215291976928711, 'force': [0.34292781352996826, -0.9272316694259644, 1.623725175857544], 'magnitude': 1.9010106325149536, 'cosine_ionic_motion': -0.4328988194465637, 'motion_component_ionic': -0.822945237159729, 'motion_component_percent_ionic': 43.28988194465637}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 11.536504745483398, 'force': [-0.9881191849708557, -0.33167219161987305, -0.7565538287162781], 'magnitude': 1.2879284620285034, 'cosine_with_motion': 0.8688722848892212, 'motion_component': 1.119045376777649, 'motion_component_percent': 86.88722848892212}, {'resid': 98, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 11.968896865844727, 'force': [0.5543110370635986, 0.16041743755340576, 0.3605491518974304], 'magnitude': 0.6804338097572327, 'cosine_with_motion': -0.8320730328559875, 'motion_component': -0.5661706328392029, 'motion_component_percent': 83.20730328559875}, {'resid': 98, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 12.489405632019043, 'force': [0.06042743846774101, 0.019192982465028763, 0.055857159197330475], 'magnitude': 0.08449774235486984, 'cosine_with_motion': -0.88703852891922, 'motion_component': -0.07495275139808655, 'motion_component_percent': 88.703852891922}, {'resid': 98, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 12.912367820739746, 'force': [0.14942587912082672, 0.06530784070491791, 0.14772094786167145], 'magnitude': 0.22003337740898132, 'cosine_with_motion': -0.9195568561553955, 'motion_component': -0.20233319699764252, 'motion_component_percent': 91.95568561553955}, {'resid': 98, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 13.659555435180664, 'force': [0.07503107935190201, 0.016857489943504333, 0.0633653923869133], 'magnitude': 0.09964442253112793, 'cosine_with_motion': -0.8506679534912109, 'motion_component': -0.08476431667804718, 'motion_component_percent': 85.0667953491211}, {'resid': 98, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 14.088735580444336, 'force': [-0.02264069952070713, -0.006128987763077021, -0.016944991424679756], 'magnitude': 0.02893611043691635, 'cosine_with_motion': 0.8480191230773926, 'motion_component': 0.024538375437259674, 'motion_component_percent': 84.80191230773926}, {'resid': 98, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 13.306002616882324, 'force': [-0.025327425450086594, -0.003261546604335308, -0.020006919279694557], 'magnitude': 0.032440606504678726, 'cosine_with_motion': 0.808986485004425, 'motion_component': 0.026244012638926506, 'motion_component_percent': 80.8986485004425}, {'resid': 98, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 14.991434097290039, 'force': [0.014316312037408352, 0.003118240274488926, 0.013745825737714767], 'magnitude': 0.0200904943048954, 'cosine_with_motion': -0.8635062575340271, 'motion_component': -0.017348267138004303, 'motion_component_percent': 86.35062575340271}, {'resid': 98, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 14.884713172912598, 'force': [-0.043783821165561676, -0.00617984076961875, -0.04583375155925751], 'magnitude': 0.0636863112449646, 'cosine_with_motion': 0.8482016324996948, 'motion_component': 0.05401883274316788, 'motion_component_percent': 84.82016324996948}, {'resid': 98, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 11.817391395568848, 'force': [0.8292576670646667, 0.21729496121406555, 0.9447233080863953], 'magnitude': 1.275691032409668, 'cosine_with_motion': -0.8900404572486877, 'motion_component': -1.1354166269302368, 'motion_component_percent': 89.00404572486877}, {'resid': 98, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 12.06009292602539, 'force': [-0.7597703337669373, -0.27221786975860596, -1.0549585819244385], 'magnitude': 1.3282661437988281, 'cosine_with_motion': 0.9194830656051636, 'motion_component': 1.221318244934082, 'motion_component_percent': 91.94830656051636}, {'resid': 426, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 11.047283172607422, 'force': [1.1775567531585693, 0.26510491967201233, -0.7181701064109802], 'magnitude': 1.4045244455337524, 'cosine_with_motion': -0.04200088232755661, 'motion_component': -0.058991268277168274, 'motion_component_percent': 4.200088232755661}, {'resid': 426, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 11.486474990844727, 'force': [-0.6496268510818481, -0.11499711871147156, 0.332520991563797], 'magnitude': 0.7387892603874207, 'cosine_with_motion': 0.08466315269470215, 'motion_component': 0.06254822760820389, 'motion_component_percent': 8.466315269470215}, {'resid': 426, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 11.952422142028809, 'force': [-0.07224062830209732, -0.01667594537138939, 0.05491122230887413], 'magnitude': 0.0922607034444809, 'cosine_with_motion': -0.045646440237760544, 'motion_component': -0.004211372695863247, 'motion_component_percent': 4.564644023776054}, {'resid': 426, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 12.098755836486816, 'force': [-0.18851225078105927, -0.06634119898080826, 0.15123918652534485], 'magnitude': 0.25062185525894165, 'cosine_with_motion': -0.017062125727534294, 'motion_component': -0.00427614152431488, 'motion_component_percent': 1.7062125727534294}, {'resid': 426, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 13.323458671569824, 'force': [-0.08501112461090088, -0.014476417563855648, 0.059438858181238174], 'magnitude': 0.10473507642745972, 'cosine_with_motion': -0.037762220948934555, 'motion_component': -0.00395502895116806, 'motion_component_percent': 3.7762220948934555}, {'resid': 426, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 13.488673210144043, 'force': [0.02671715058386326, 0.005456786602735519, -0.015904389321804047], 'magnitude': 0.03156789764761925, 'cosine_with_motion': -0.04179874435067177, 'motion_component': -0.001319498522207141, 'motion_component_percent': 4.179874435067177}, {'resid': 426, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 13.38994026184082, 'force': [0.026329269632697105, 0.001839134842157364, -0.018155956640839577], 'magnitude': 0.032035160809755325, 'cosine_with_motion': 0.07799084484577179, 'motion_component': 0.0024984492920339108, 'motion_component_percent': 7.799084484577179}, {'resid': 426, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 14.4356050491333, 'force': [-0.016622792929410934, -0.003646475961431861, 0.013411290012300014], 'magnitude': 0.02166741155087948, 'cosine_with_motion': -0.0761815533041954, 'motion_component': -0.0016506570391356945, 'motion_component_percent': 7.61815533041954}, {'resid': 426, 'resname': 'GLU', 'atom': 'HG2', 'charge': -0.042500000447034836, 'distance': 14.237420082092285, 'force': [0.05098053067922592, 0.01606864482164383, -0.04458896443247795], 'magnitude': 0.06960884481668472, 'cosine_with_motion': 0.07082238793373108, 'motion_component': 0.004929864779114723, 'motion_component_percent': 7.082238793373108}, {'resid': 426, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 14.683125495910645, 'force': [-0.9056307077407837, -0.11452068388462067, 0.8396204710006714], 'magnitude': 1.2402598857879639, 'cosine_with_motion': -0.17523163557052612, 'motion_component': -0.21733276546001434, 'motion_component_percent': 17.523163557052612}, {'resid': 426, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 14.585150718688965, 'force': [0.8560543060302734, 0.13424178957939148, -0.939232349395752], 'magnitude': 1.2778916358947754, 'cosine_with_motion': 0.23410367965698242, 'motion_component': 0.29915913939476013, 'motion_component_percent': 23.410367965698242}, {'resid': 426, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 11.581486701965332, 'force': [-0.9682579636573792, -0.13923251628875732, 0.8984312415122986], 'magnitude': 1.3281896114349365, 'cosine_with_motion': -0.16837731003761292, 'motion_component': -0.22363698482513428, 'motion_component_percent': 16.83773100376129}, {'resid': 426, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 11.695866584777832, 'force': [0.9268863797187805, 0.1887303590774536, -1.0487157106399536], 'magnitude': 1.4122825860977173, 'cosine_with_motion': 0.2290794998407364, 'motion_component': 0.32352498173713684, 'motion_component_percent': 22.90794998407364}, {'resid': 754, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 11.435626983642578, 'force': [-0.2747243046760559, 1.0426589250564575, -0.7452903985977173], 'magnitude': 1.31075119972229, 'cosine_with_motion': 0.061879076063632965, 'motion_component': 0.08110807090997696, 'motion_component_percent': 6.1879076063632965}, {'resid': 754, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 11.776670455932617, 'force': [0.12858553230762482, -0.592026948928833, 0.3562823534011841], 'magnitude': 0.702828049659729, 'cosine_with_motion': 0.01990470662713051, 'motion_component': 0.013989586383104324, 'motion_component_percent': 1.9904706627130508}, {'resid': 754, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 12.125195503234863, 'force': [0.013981918804347515, -0.06682492047548294, 0.058104123920202255], 'magnitude': 0.08965017646551132, 'cosine_with_motion': -0.12829621136188507, 'motion_component': -0.011501777917146683, 'motion_component_percent': 12.829621136188507}, {'resid': 754, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 12.605782508850098, 'force': [0.051165591925382614, -0.16336068511009216, 0.1549021452665329], 'magnitude': 0.2308664172887802, 'cosine_with_motion': -0.19099797308444977, 'motion_component': -0.04409501701593399, 'motion_component_percent': 19.099797308444977}, {'resid': 754, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 13.37293815612793, 'force': [0.009996434673666954, -0.08175641298294067, 0.06343460828065872], 'magnitude': 0.10396148264408112, 'cosine_with_motion': -0.054817378520965576, 'motion_component': -0.005698896013200283, 'motion_component_percent': 5.481737852096558}, {'resid': 754, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 13.869071006774902, 'force': [-0.00446094386279583, 0.02415630966424942, -0.016976187005639076], 'magnitude': 0.02985997684299946, 'cosine_with_motion': 0.03156915679574013, 'motion_component': 0.0009426543256267905, 'motion_component_percent': 3.1569156795740128}, {'resid': 754, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 13.03630542755127, 'force': [-0.0009773540077731013, 0.027506038546562195, -0.0196133591234684], 'magnitude': 0.0337967649102211, 'cosine_with_motion': -0.007962866686284542, 'motion_component': -0.000269119133008644, 'motion_component_percent': 0.7962866686284542}, {'resid': 754, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 14.559836387634277, 'force': [0.0013484437949955463, -0.015890711918473244, 0.014118229039013386], 'magnitude': 0.02129923552274704, 'cosine_with_motion': -0.10379280149936676, 'motion_component': -0.002210707403719425, 'motion_component_percent': 10.379280149936676}, {'resid': 754, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 14.365402221679688, 'force': [0.00017817037587519735, 0.049542803317308426, -0.04712209850549698], 'magnitude': 0.06837406754493713, 'cosine_with_motion': 0.11026695370674133, 'motion_component': 0.007539399899542332, 'motion_component_percent': 11.026695370674133}, {'resid': 754, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 14.912007331848145, 'force': [0.16592921316623688, -0.8336456418037415, 0.8505633473396301], 'magnitude': 1.2024788856506348, 'cosine_with_motion': -0.19427217543125153, 'motion_component': -0.2336081862449646, 'motion_component_percent': 19.427217543125153}, {'resid': 754, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 14.46163272857666, 'force': [-0.17741070687770844, 0.8248223662376404, -0.988792359828949], 'magnitude': 1.2998141050338745, 'cosine_with_motion': 0.2657794654369354, 'motion_component': 0.34546390175819397, 'motion_component_percent': 26.577946543693542}, {'resid': 754, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 11.49199104309082, 'force': [0.10095295310020447, -0.9330597519874573, 0.9689652323722839], 'magnitude': 1.3489571809768677, 'cosine_with_motion': -0.17938555777072906, 'motion_component': -0.24198342859745026, 'motion_component_percent': 17.938555777072906}, {'resid': 754, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 11.705488204956055, 'force': [-0.1193489134311676, 0.8646338582038879, -1.1073195934295654], 'magnitude': 1.4099619388580322, 'cosine_with_motion': 0.2762414515018463, 'motion_component': 0.38948994874954224, 'motion_component_percent': 27.62414515018463}, {'resid': 1082, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 11.738513946533203, 'force': [0.3542022407054901, -0.9876286387443542, -0.6682970523834229], 'magnitude': 1.2439817190170288, 'cosine_with_motion': 0.7298898100852966, 'motion_component': 0.90796959400177, 'motion_component_percent': 72.98898100852966}, {'resid': 1082, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 12.25681209564209, 'force': [-0.17257198691368103, 0.5420202016830444, 0.3121365010738373], 'magnitude': 0.6488422155380249, 'cosine_with_motion': -0.7181982398033142, 'motion_component': -0.4659973382949829, 'motion_component_percent': 71.81982398033142}, {'resid': 1082, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 12.486446380615234, 'force': [-0.02191685326397419, 0.06224391236901283, 0.05283923074603081], 'magnitude': 0.08453778922557831, 'cosine_with_motion': -0.7728770971298218, 'motion_component': -0.06533732265233994, 'motion_component_percent': 77.28770971298218}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 12.938920974731445, 'force': [-0.07173819094896317, 0.15330706536769867, 0.1391727775335312], 'magnitude': 0.219131201505661, 'cosine_with_motion': -0.7343062162399292, 'motion_component': -0.16090939939022064, 'motion_component_percent': 73.43062162399292}, {'resid': 1082, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 13.780845642089844, 'force': [-0.020727790892124176, 0.07577775418758392, 0.05841347947716713], 'magnitude': 0.09789813309907913, 'cosine_with_motion': -0.7906785011291504, 'motion_component': -0.07740595191717148, 'motion_component_percent': 79.06785011291504}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 13.88697338104248, 'force': [0.00703989714384079, -0.024198148399591446, -0.01587195321917534], 'magnitude': 0.029783038422465324, 'cosine_with_motion': 0.7552529573440552, 'motion_component': 0.022493727505207062, 'motion_component_percent': 75.52529573440552}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 13.614629745483398, 'force': [0.0041610547341406345, -0.02434946969151497, -0.01870700716972351], 'magnitude': 0.030986499041318893, 'cosine_with_motion': 0.8317173719406128, 'motion_component': 0.025772009044885635, 'motion_component_percent': 83.17173719406128}, {'resid': 1082, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 11.922428131103516, 'force': [-0.23471929132938385, 0.8601911067962646, 0.8807781338691711], 'magnitude': 1.253312349319458, 'cosine_with_motion': -0.8302227258682251, 'motion_component': -1.040528416633606, 'motion_component_percent': 83.02227258682251}, {'resid': 1082, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 12.266879081726074, 'force': [0.26309695839881897, -0.7866494655609131, -0.9799304604530334], 'magnitude': 1.283861756324768, 'cosine_with_motion': 0.827785849571228, 'motion_component': 1.0627626180648804, 'motion_component_percent': 82.7785849571228}], 'asn_contributions': [], 'sf_contributions': [{'resid': 100, 'resname': 'THR', 'atom': 'N', 'charge': -0.4157000184059143, 'distance': 8.692227363586426, 'force': [-1.0912113189697266, -0.24335458874702454, -1.4445401430130005], 'magnitude': 1.8266525268554688, 'cosine_with_motion': 0.8869110345840454, 'motion_component': 1.6200783252716064, 'motion_component_percent': 88.69110345840454}, {'resid': 100, 'resname': 'THR', 'atom': 'H', 'charge': 0.2718999981880188, 'distance': 9.291739463806152, 'force': [0.6784638166427612, 0.1939253807067871, 0.7715548276901245], 'magnitude': 1.0455701351165771, 'cosine_with_motion': -0.8960176110267639, 'motion_component': -0.9368492364883423, 'motion_component_percent': 89.60176110267639}, {'resid': 100, 'resname': 'THR', 'atom': 'CA', 'charge': -0.03889999911189079, 'distance': 7.622952461242676, 'force': [-0.11649254709482193, -0.05002587288618088, -0.18254271149635315], 'magnitude': 0.22224973142147064, 'cosine_with_motion': 0.9326297640800476, 'motion_component': 0.20727671682834625, 'motion_component_percent': 93.26297640800476}, {'resid': 100, 'resname': 'THR', 'atom': 'HA', 'charge': 0.1007000058889389, 'distance': 7.437439918518066, 'force': [0.3423239290714264, 0.20626072585582733, 0.453391432762146], 'magnitude': 0.6043947339057922, 'cosine_with_motion': -0.9599742889404297, 'motion_component': -0.5802034139633179, 'motion_component_percent': 95.99742889404297}, {'resid': 100, 'resname': 'THR', 'atom': 'CB', 'charge': 0.3653999865055084, 'distance': 8.24217700958252, 'force': [0.6539973616600037, 0.4939587414264679, 1.5865768194198608], 'magnitude': 1.7857586145401, 'cosine_with_motion': -0.9511663317680359, 'motion_component': -1.698553442955017, 'motion_component_percent': 95.11663317680359}, {'resid': 100, 'resname': 'THR', 'atom': 'HB', 'charge': 0.00430000014603138, 'distance': 7.693872928619385, 'force': [0.006750338710844517, 0.008620633743703365, 0.02148788794875145], 'magnitude': 0.024116627871990204, 'cosine_with_motion': -0.9650573134422302, 'motion_component': -0.023273928090929985, 'motion_component_percent': 96.50573134422302}, {'resid': 100, 'resname': 'THR', 'atom': 'CG2', 'charge': -0.24380001425743103, 'distance': 9.552233695983887, 'force': [-0.35178494453430176, -0.31482717394828796, -0.7510252594947815], 'magnitude': 0.8870782256126404, 'cosine_with_motion': 0.9748586416244507, 'motion_component': 0.8647758960723877, 'motion_component_percent': 97.48586416244507}, {'resid': 100, 'resname': 'THR', 'atom': 'HG21', 'charge': 0.0642000064253807, 'distance': 9.322653770446777, 'force': [0.10438620299100876, 0.10946699976921082, 0.19303862750530243], 'magnitude': 0.24524153769016266, 'cosine_with_motion': -0.992241621017456, 'motion_component': -0.24333886802196503, 'motion_component_percent': 99.2241621017456}, {'resid': 100, 'resname': 'THR', 'atom': 'HG22', 'charge': 0.0642000064253807, 'distance': 10.199082374572754, 'force': [0.09437168389558792, 0.06022002920508385, 0.17161959409713745], 'magnitude': 0.204904243350029, 'cosine_with_motion': -0.9586312174797058, 'motion_component': -0.1964275985956192, 'motion_component_percent': 95.86312174797058}, {'resid': 100, 'resname': 'THR', 'atom': 'HG23', 'charge': 0.0642000064253807, 'distance': 10.178244590759277, 'force': [0.06418439000844955, 0.0758366659283638, 0.18016603589057922], 'magnitude': 0.20574410259723663, 'cosine_with_motion': -0.971974790096283, 'motion_component': -0.1999780833721161, 'motion_component_percent': 97.1974790096283}, {'resid': 100, 'resname': 'THR', 'atom': 'OG1', 'charge': -0.6761000156402588, 'distance': 8.841397285461426, 'force': [-0.849859356880188, -0.4543907642364502, -2.7049434185028076], 'magnitude': 2.8714892864227295, 'cosine_with_motion': 0.8989047408103943, 'motion_component': 2.58119535446167, 'motion_component_percent': 89.89047408103943}, {'resid': 100, 'resname': 'THR', 'atom': 'HG1', 'charge': 0.41019999980926514, 'distance': 8.35677433013916, 'force': [0.43123430013656616, 0.2030375748872757, 1.8909505605697632], 'magnitude': 1.9500977993011475, 'cosine_with_motion': -0.8612120151519775, 'motion_component': -1.6794476509094238, 'motion_component_percent': 86.12120151519775}, {'resid': 100, 'resname': 'THR', 'atom': 'C', 'charge': 0.5973000526428223, 'distance': 6.393817901611328, 'force': [2.525376558303833, 0.49671608209609985, 4.1116485595703125], 'magnitude': 4.85076379776001, 'cosine_with_motion': -0.8830033540725708, 'motion_component': -4.283240795135498, 'motion_component_percent': 88.30033540725708}, {'resid': 100, 'resname': 'THR', 'atom': 'O', 'charge': -0.5679000020027161, 'distance': 5.716579437255859, 'force': [-2.0607383251190186, -0.6321477293968201, -5.351707458496094], 'magnitude': 5.769490718841553, 'cosine_with_motion': 0.8844720125198364, 'motion_component': 5.10295295715332, 'motion_component_percent': 88.44720125198364}, {'resid': 101, 'resname': 'ILE', 'atom': 'N', 'charge': -0.4157000184059143, 'distance': 6.131131172180176, 'force': [-2.4029712677001953, 0.05564824864268303, -2.775271415710449], 'magnitude': 3.6714437007904053, 'cosine_with_motion': 0.8006082773208618, 'motion_component': 2.9393882751464844, 'motion_component_percent': 80.06082773208618}, {'resid': 101, 'resname': 'ILE', 'atom': 'H', 'charge': 0.2718999981880188, 'distance': 6.906736373901367, 'force': [1.3744909763336182, -0.026414690539240837, 1.3004100322723389], 'magnitude': 1.8923503160476685, 'cosine_with_motion': -0.7774417400360107, 'motion_component': -1.4711921215057373, 'motion_component_percent': 77.74417400360107}, {'resid': 101, 'resname': 'ILE', 'atom': 'CA', 'charge': -0.059700001031160355, 'distance': 5.261504173278809, 'force': [-0.4702218770980835, 0.15720383822917938, -0.5165133476257324], 'magnitude': 0.7159662842750549, 'cosine_with_motion': 0.6628867983818054, 'motion_component': 0.47460460662841797, 'motion_component_percent': 66.28867983818054}, {'resid': 101, 'resname': 'ILE', 'atom': 'HA', 'charge': 0.0869000032544136, 'distance': 5.246748924255371, 'force': [0.5202758312225342, -0.33475351333618164, 0.8459540605545044], 'magnitude': 1.0480387210845947, 'cosine_with_motion': -0.6106932163238525, 'motion_component': -0.6400301456451416, 'motion_component_percent': 61.069321632385254}, {'resid': 101, 'resname': 'ILE', 'atom': 'CB', 'charge': 0.13030001521110535, 'distance': 6.105713844299316, 'force': [0.8358506560325623, -0.4387485384941101, 0.6748284101486206], 'magnitude': 1.1604050397872925, 'cosine_with_motion': -0.495466947555542, 'motion_component': -0.5749423503875732, 'motion_component_percent': 49.5466947555542}, {'resid': 101, 'resname': 'ILE', 'atom': 'HB', 'charge': 0.018699999898672104, 'distance': 6.237673282623291, 'force': [0.13215547800064087, -0.05304427817463875, 0.07198504358530045], 'magnitude': 0.1595638245344162, 'cosine_with_motion': -0.46472620964050293, 'motion_component': -0.07415349036455154, 'motion_component_percent': 46.47262096405029}, {'resid': 101, 'resname': 'ILE', 'atom': 'CG2', 'charge': -0.3203999996185303, 'distance': 5.871387481689453, 'force': [-1.8888449668884277, 1.8551806211471558, -1.584901213645935], 'magnitude': 3.085667133331299, 'cosine_with_motion': 0.2807835042476654, 'motion_component': 0.8664044141769409, 'motion_component_percent': 28.07835042476654}, {'resid': 101, 'resname': 'ILE', 'atom': 'HG21', 'charge': 0.08820000290870667, 'distance': 4.879656791687012, 'force': [0.7220392823219299, -0.8166322112083435, 0.5693284869194031], 'magnitude': 1.229781985282898, 'cosine_with_motion': -0.1989675909280777, 'motion_component': -0.24468675255775452, 'motion_component_percent': 19.89675909280777}, {'resid': 101, 'resname': 'ILE', 'atom': 'HG22', 'charge': 0.08820000290870667, 'distance': 6.3109846115112305, 'force': [0.3510526418685913, -0.474934846162796, 0.43787577748298645], 'magnitude': 0.7352117300033569, 'cosine_with_motion': -0.26592427492141724, 'motion_component': -0.1955106407403946, 'motion_component_percent': 26.592427492141724}, {'resid': 101, 'resname': 'ILE', 'atom': 'HG23', 'charge': 0.08820000290870667, 'distance': 6.509936809539795, 'force': [0.4475732743740082, -0.4535413384437561, 0.2672164738178253], 'magnitude': 0.6909603476524353, 'cosine_with_motion': -0.16955359280109406, 'motion_component': -0.1171548068523407, 'motion_component_percent': 16.955359280109406}, {'resid': 101, 'resname': 'ILE', 'atom': 'CG1', 'charge': -0.0430000014603138, 'distance': 7.529069423675537, 'force': [-0.16990303993225098, 0.0921764150261879, -0.16142992675304413], 'magnitude': 0.2518395483493805, 'cosine_with_motion': 0.5290106534957886, 'motion_component': 0.13322579860687256, 'motion_component_percent': 52.90106534957886}, {'resid': 101, 'resname': 'ILE', 'atom': 'HG12', 'charge': 0.023600000888109207, 'distance': 7.790594100952148, 'force': [0.07369229942560196, -0.04801565036177635, 0.09449563175439835], 'magnitude': 0.12909485399723053, 'cosine_with_motion': -0.5539958477020264, 'motion_component': -0.07151801139116287, 'motion_component_percent': 55.39958477020264}, {'resid': 101, 'resname': 'ILE', 'atom': 'HG13', 'charge': 0.023600000888109207, 'distance': 7.8587751388549805, 'force': [0.09138941764831543, -0.030360709875822067, 0.08258827775716782], 'magnitude': 0.12686458230018616, 'cosine_with_motion': -0.6237573027610779, 'motion_component': -0.07913270592689514, 'motion_component_percent': 62.37573027610779}, {'resid': 101, 'resname': 'ILE', 'atom': 'CD1', 'charge': -0.06599999964237213, 'distance': 8.578559875488281, 'force': [-0.21166619658470154, 0.13621827960014343, -0.15905241668224335], 'magnitude': 0.2977510392665863, 'cosine_with_motion': 0.41285303235054016, 'motion_component': 0.12292741984128952, 'motion_component_percent': 41.285303235054016}, {'resid': 101, 'resname': 'ILE', 'atom': 'HD11', 'charge': 0.01860000006854534, 'distance': 8.62802505493164, 'force': [0.052368536591529846, -0.04609459266066551, 0.04487652704119682], 'magnitude': 0.08295226097106934, 'cosine_with_motion': -0.3335283696651459, 'motion_component': -0.027666931971907616, 'motion_component_percent': 33.35283696651459}, {'resid': 101, 'resname': 'ILE', 'atom': 'HD12', 'charge': 0.01860000006854534, 'distance': 9.605938911437988, 'force': [0.04746038466691971, -0.028604360297322273, 0.0375220887362957], 'magnitude': 0.0669223740696907, 'cosine_with_motion': -0.44850340485572815, 'motion_component': -0.03001491352915764, 'motion_component_percent': 44.850340485572815}, {'resid': 101, 'resname': 'ILE', 'atom': 'HD13', 'charge': 0.01860000006854534, 'distance': 8.529306411743164, 'force': [0.06604080647230148, -0.03918705880641937, 0.03616912290453911], 'magnitude': 0.08488356322050095, 'cosine_with_motion': -0.3557151257991791, 'motion_component': -0.030194366350769997, 'motion_component_percent': 35.57151257991791}, {'resid': 101, 'resname': 'ILE', 'atom': 'C', 'charge': 0.5973000526428223, 'distance': 3.89237904548645, 'force': [9.991813659667969, -1.9817997217178345, 8.219078063964844], 'magnitude': 13.08881664276123, 'cosine_with_motion': -0.6715072989463806, 'motion_component': -8.789236068725586, 'motion_component_percent': 67.15072989463806}, {'resid': 101, 'resname': 'ILE', 'atom': 'O', 'charge': -0.5679000020027161, 'distance': 2.8393607139587402, 'force': [-15.449605941772461, 7.251489162445068, -15.989466667175293], 'magnitude': 23.386693954467773, 'cosine_with_motion': 0.5863189697265625, 'motion_component': 13.71206283569336, 'motion_component_percent': 58.63189697265625}, {'resid': 102, 'resname': 'GLY', 'atom': 'N', 'charge': -0.4157000184059143, 'distance': 4.175678253173828, 'force': [-7.063827991485596, -0.578406035900116, -3.5240321159362793], 'magnitude': 7.9152398109436035, 'cosine_with_motion': 0.7087478637695312, 'motion_component': 5.609909534454346, 'motion_component_percent': 70.87478637695312}, {'resid': 102, 'resname': 'GLY', 'atom': 'H', 'charge': 0.2718999981880188, 'distance': 5.182270050048828, 'force': [3.026263475418091, 0.23385076224803925, 1.4440834522247314], 'magnitude': 3.361299514770508, 'cosine_with_motion': -0.6982153654098511, 'motion_component': -2.3469109535217285, 'motion_component_percent': 69.82153654098511}, {'resid': 102, 'resname': 'GLY', 'atom': 'CA', 'charge': -0.025200000032782555, 'distance': 3.701850414276123, 'force': [-0.5852888226509094, -0.1507231444120407, -0.08634717017412186], 'magnitude': 0.6105213165283203, 'cosine_with_motion': 0.60431307554245, 'motion_component': 0.36894601583480835, 'motion_component_percent': 60.431307554244995}, {'resid': 102, 'resname': 'GLY', 'atom': 'HA2', 'charge': 0.0697999969124794, 'distance': 4.661733627319336, 'force': [1.0202624797821045, 0.3089725971221924, 0.026394162327051163], 'magnitude': 1.0663471221923828, 'cosine_with_motion': -0.5406591892242432, 'motion_component': -0.576530396938324, 'motion_component_percent': 54.065918922424316}, {'resid': 102, 'resname': 'GLY', 'atom': 'HA3', 'charge': 0.0697999969124794, 'distance': 3.1946098804473877, 'force': [1.9236314296722412, 1.1407030820846558, 0.39302873611450195], 'magnitude': 2.2706899642944336, 'cosine_with_motion': </t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>939</v>
+      </c>
+      <c r="B12" t="n">
+        <v>946</v>
+      </c>
+      <c r="C12" t="n">
+        <v>2381</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>{805: {'frame': 805, 'motion_vector': [0.5000572204589844, -0.8116645812988281, 2.552490234375], 'motion_vector_magnitude': 2.7247133255004883, 'ionic_force': [-10.476232096552849, 1.6047565713524818, 11.229859232902527], 'ionic_force_magnitude': 15.441386627662336, 'radial_force': 10.598428307732382, 'axial_force': 11.229859232902527, 'glu_force': [0.4065493914531544, 1.121332980459556, -6.467527237953618], 'glu_force_magnitude': 6.576593239240907, 'asn_force': [-0.1620856230147183, 0.2204859512130497, 3.251880921423435], 'asn_force_magnitude': 3.2633748376470826, 'sf_force': [0.08371658779651625, -4.5646154356436455, 13.080483275756706], 'sf_force_magnitude': 13.85430493636326, 'residue_force': [0.32818035623495234, -3.22279650397104, 9.864836959226523], 'residue_force_magnitude': 10.383117445370058, 'pip2_force': [0.5160131542943418, -0.01927251904271543, -3.689003342704382], 'pip2_force_magnitude': 3.7249680089739226, 'total_force': [-9.632038586023555, -1.6373124516612734, 17.405692849424668], 'total_force_magnitude': 19.960338247522877, 'cosine_total_motion': 0.7527688696363684, 'cosine_glu_motion': -0.9607025943976918, 'cosine_asn_motion': 0.9042507412331336, 'cosine_sf_motion': 0.9837239542860201, 'cosine_residue_motion': 0.9882937969738762, 'cosine_pip2_motion': -0.9007825919020438, 'cosine_ionic_motion': 0.5258165752399018, 'motion_component_total': 15.025521260147366, 'motion_component_glu': -6.318150187237059, 'motion_component_asn': 2.9509091158639316, 'motion_component_sf': 13.628811635883594, 'motion_component_residue': 10.261570564510468, 'motion_component_ionic': 8.119337033512625, 'motion_component_pip2': -3.3553863378757254, 'motion_component_percent_total': 75.27688696363684, 'motion_component_percent_glu': 96.07025943976917, 'motion_component_percent_asn': 90.42507412331337, 'motion_component_percent_sf': 98.372395428602, 'motion_component_percent_residue': 98.82937969738762, 'motion_component_percent_ionic': 52.581657523990174, 'motion_component_percent_pip2': 90.07825919020438, 'ionic_contributions': [{'ion_id': 2223, 'distance': 10.26485538482666, 'force': [-1.4653534889221191, 2.2305703163146973, 1.6749225854873657], 'magnitude': 3.150883913040161, 'cosine_ionic_motion': 0.2017398178577423, 'motion_component_ionic': 0.6356587409973145, 'motion_component_percent_ionic': 20.17398178577423}, {'ion_id': 2231, 'distance': 4.615085124969482, 'force': [-9.639967918395996, 2.9178953170776367, 11.89661693572998], 'magnitude': 15.587577819824219, 'cosine_ionic_motion': 0.5457074046134949, 'motion_component_ionic': 8.506257057189941, 'motion_component_percent_ionic': 54.57074046134949}, {'ion_id': 2333, 'distance': 9.047889709472656, 'force': [0.704569935798645, -2.897843837738037, 2.748289108276367], 'magnitude': 4.0554914474487305, 'cosine_ionic_motion': 0.8795781135559082, 'motion_component_ionic': 3.5671215057373047, 'motion_component_percent_ionic': 87.95781135559082}, {'ion_id': 2343, 'distance': 5.714763641357422, 'force': [0.18896515667438507, -0.07984892278909683, -10.163729667663574], 'magnitude': 10.165800094604492, 'cosine_ionic_motion': -0.9308501482009888, 'motion_component_ionic': -9.462836265563965, 'motion_component_percent_ionic': 93.08501482009888}, {'ion_id': 2372, 'distance': 9.028743743896484, 'force': [-3.2316272258758545, -0.6547687649726868, 2.390570878982544], 'magnitude': 4.072710037231445, 'cosine_ionic_motion': 0.45213818550109863, 'motion_component_ionic': 1.8414276838302612, 'motion_component_percent_ionic': 45.21381855010986}, {'ion_id': 2397, 'distance': 9.108790397644043, 'force': [2.967181444168091, 0.08875246345996857, 2.6831893920898438], 'magnitude': 4.001443386077881, 'cosine_ionic_motion': 0.7576538324356079, 'motion_component_ionic': 3.0317089557647705, 'motion_component_percent_ionic': 75.76538324356079}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 9.917972564697266, 'force': [-1.6660727262496948, -0.44027993083000183, -0.2587750554084778], 'magnitude': 1.7425869703292847, 'cosine_with_motion': -0.23931780457496643, 'motion_component': -0.4170320928096771, 'motion_component_percent': 23.931780457496643}, {'resid': 98, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 10.653299331665039, 'force': [0.8357123136520386, 0.17756567895412445, 0.08779286593198776], 'magnitude': 0.858866810798645, 'cosine_with_motion': 0.2127501517534256, 'motion_component': 0.18272404372692108, 'motion_component_percent': 21.27501517534256}, {'resid': 98, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 10.040849685668945, 'force': [0.12186508625745773, 0.028803955763578415, 0.0375572070479393], 'magnitude': 0.13073372840881348, 'cosine_with_motion': 0.3745656907558441, 'motion_component': 0.048968371003866196, 'motion_component_percent': 37.45656907558441}, {'resid': 98, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 10.243396759033203, 'force': [0.3112889528274536, 0.10491639375686646, 0.11972866207361221], 'magnitude': 0.34963297843933105, 'cosine_with_motion': 0.39480581879615784, 'motion_component': 0.13803713023662567, 'motion_component_percent': 39.480581879615784}, {'resid': 98, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 11.286087036132812, 'force': [0.13748414814472198, 0.02020740881562233, 0.04466128721833229], 'magnitude': 0.14596185088157654, 'cosine_with_motion': 0.41826510429382324, 'motion_component': 0.06105075031518936, 'motion_component_percent': 41.826510429382324}, {'resid': 98, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 12.072796821594238, 'force': [-0.03759440779685974, -0.0065694693475961685, -0.00981726124882698], 'magnitude': 0.03940654918551445, 'cosine_with_motion': -0.3588065207004547, 'motion_component': -0.014139327220618725, 'motion_component_percent': 35.88065207004547}, {'resid': 98, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 11.094642639160156, 'force': [-0.044621020555496216, -0.0021076116245239973, -0.013483568094670773], 'magnitude': 0.046661376953125, 'cosine_with_motion': -0.43274781107902527, 'motion_component': -0.02019260823726654, 'motion_component_percent': 43.27478110790253}, {'resid': 98, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 11.998729705810547, 'force': [0.028199777007102966, 0.004392937757074833, 0.013002379797399044], 'magnitude': 0.03136219456791878, 'cosine_with_motion': 0.5116773247718811, 'motion_component': 0.016047323122620583, 'motion_component_percent': 51.16773247718811}, {'resid': 98, 'resname': 'GLU', 'atom': 'HG2', 'charge': -0.042500000447034836, 'distance': 12.116682052612305, 'force': [-0.08368987590074539, -0.021321119740605354, -0.042168281972408295], 'magnitude': 0.09610801190137863, 'cosine_with_motion': -0.504753828048706, 'motion_component': -0.04851088672876358, 'motion_component_percent': 50.475382804870605}, {'resid': 98, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 13.000343322753906, 'force': [-0.07603708654642105, -0.009408356621861458, -0.03316438943147659], 'magnitude': 0.08348672091960907, 'cosine_with_motion': -0.5057128667831421, 'motion_component': -0.042220309376716614, 'motion_component_percent': 50.57128667831421}, {'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 11.608240127563477, 'force': [1.7178534269332886, 0.11423458904027939, 0.9866870045661926], 'magnitude': 1.9843440055847168, 'cosine_with_motion': 0.6075373291969299, 'motion_component': 1.2055630683898926, 'motion_component_percent': 60.75373291969299}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 11.546860694885254, 'force': [-1.7932460308074951, 0.09556171298027039, -0.9654526710510254], 'magnitude': 2.038862943649292, 'cosine_with_motion': -0.6189742684364319, 'motion_component': -1.2620036602020264, 'motion_component_percent': 61.89742684364319}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 11.299222946166992, 'force': [-1.723423957824707, -0.20408852398395538, -1.233571171760559], 'magnitude': 2.129211187362671, 'cosine_with_motion': -0.6627327799797058, 'motion_component': -1.4110980033874512, 'motion_component_percent': 66.27327799797058}, {'resid': 98, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 8.881653785705566, 'force': [2.0920755863189697, 0.2829519212245941, 0.8022051453590393], 'magnitude': 2.2584009170532227, 'cosine_with_motion': 0.4654454290866852, 'motion_component': 1.0511623620986938, 'motion_component_percent': 46.54454290866852}, {'resid': 98, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 8.48457145690918, 'force': [-2.3224527835845947, -0.43536368012428284, -1.2722705602645874], 'magnitude': 2.683654308319092, 'cosine_with_motion': -0.5546148419380188, 'motion_component': -1.4883944988250732, 'motion_component_percent': 55.46148419380188}, {'resid': 426, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 9.348220825195312, 'force': [1.8786503076553345, 0.5530252456665039, 0.11050964146852493], 'magnitude': 1.961472988128662, 'cosine_with_motion': 0.14456796646118164, 'motion_component': 0.2835661470890045, 'motion_component_percent': 14.456796646118164}, {'resid': 426, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 10.018021583557129, 'force': [-0.9420817494392395, -0.21406064927577972, -0.09991542994976044], 'magnitude': 0.971248209476471, 'cosine_with_motion': -0.20873191952705383, 'motion_component': -0.20273050665855408, 'motion_component_percent': 20.873191952705383}, {'resid': 426, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 9.534235954284668, 'force': [-0.13803811371326447, -0.04201959818601608, 0.014274169690907001], 'magnitude': 0.1449962705373764, 'cosine_with_motion': 0.0038310394156724215, 'motion_component': 0.0005554864183068275, 'motion_component_percent': 0.38310394156724215}, {'resid': 426, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 9.602323532104492, 'force': [-0.36251363158226013, -0.1555292159318924, 0.05195988342165947], 'magnitude': 0.39787596464157104, 'cosine_with_motion': 0.0715683326125145, 'motion_component': 0.028475318104028702, 'motion_component_percent': 7.15683326125145}, {'resid': 426, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 10.923237800598145, 'force': [-0.14994195103645325, -0.03762156888842583, 0.019542662426829338], 'magnitude': 0.15582004189491272, 'cosine_with_motion': 0.012810744345188141, 'motion_component': 0.0019961707293987274, 'motion_component_percent': 1.281074434518814}, {'resid': 426, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 11.594000816345215, 'force': [0.04091249406337738, 0.012046834453940392, -0.002601079409942031], 'magnitude': 0.042728491127491, 'cosine_with_motion': 0.03471285104751587, 'motion_component': 0.001483227824792266, 'motion_component_percent': 3.471285104751587}, {'resid': 426, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 11.06163215637207, 'force': [0.046121131628751755, 0.006838954519480467, -0.005427754484117031], 'magnitude': 0.046940285712480545, 'cosine_with_motion': 0.028600560501217842, 'motion_component': 0.001342518487945199, 'motion_component_percent': 2.860056050121784}, {'resid': 426, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 11.498003959655762, 'force': [-0.03166548162698746, -0.009603610262274742, 0.008456512354314327], 'magnitude': 0.034153252840042114, 'cosine_with_motion': 0.14556024968624115, 'motion_component': 0.004971356131136417, 'motion_component_percent': 14.556024968624115}, {'resid': 426, 'resname': 'GLU', 'atom': 'HG2', 'charge': -0.042500000447034836, 'distance': 11.286779403686523, 'force': [0.09896083176136017, 0.040792278945446014, -0.02847360260784626], 'magnitude': 0.11076101660728455, 'cosine_with_motion': -0.18655945360660553, 'motion_component': -0.020663514733314514, 'motion_component_percent': 18.655945360660553}, {'resid': 426, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 12.557783126831055, 'force': [0.0835874080657959, 0.02446255087852478, -0.020505618304014206], 'magnitude': 0.0894748643040657, 'cosine_with_motion': -0.12468463182449341, 'motion_component': -0.011156140826642513, 'motion_component_percent': 12.46846318244934}, {'resid': 426, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 11.230976104736328, 'force': [-1.9381107091903687, -0.42262881994247437, 0.747712254524231], 'magnitude': 2.119896650314331, 'cosine_with_motion': 0.22201700508594513, 'motion_component': 0.47065311670303345, 'motion_component_percent': 22.201700508594513}, {'resid': 426, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 11.162314414978027, 'force': [2.0371859073638916, 0.19638019800186157, -0.7559065222740173], 'magnitude': 2.181762218475342, 'cosine_with_motion': -0.1800146996974945, 'motion_component': -0.39274927973747253, 'motion_component_percent': 18.00146996974945}, {'resid': 426, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 11.221531867980957, 'force': [1.8625630140304565, 0.5119181275367737, -0.96394944190979], 'magnitude': 2.1587958335876465, 'cosine_with_motion': -0.33059439063072205, 'motion_component': -0.7136858105659485, 'motion_component_percent': 33.059439063072205}, {'resid': 426, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 8.512327194213867, 'force': [-2.3517332077026367, -0.5148625373840332, 0.49909907579421997], 'magnitude': 2.4586241245269775, 'cosine_with_motion': 0.07700201869010925, 'motion_component': 0.18931901454925537, 'motion_component_percent': 7.700201869010925}, {'resid': 426, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 8.231924057006836, 'force': [2.5824615955352783, 0.7667228579521179, -0.933125913143158], 'magnitude': 2.8509113788604736, 'cosine_with_motion': -0.22048872709274292, 'motion_component': -0.6285938024520874, 'motion_component_percent': 22.048872709274292}, {'resid': 754, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 9.160865783691406, 'force': [-0.5175990462303162, 1.967189908027649, -0.18482233583927155], 'magnitude': 2.0425238609313965, 'cosine_with_motion': -0.41817834973335266, 'motion_component': -0.8541392683982849, 'motion_component_percent': 41.817834973335266}, {'resid': 754, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 9.930930137634277, 'force': [0.20976205170154572, -0.9651351571083069, 0.03695066273212433], 'magnitude': 0.9883579015731812, 'cosine_with_motion': 0.3648638129234314, 'motion_component': 0.3606160283088684, 'motion_component_percent': 36.48638129234314}, {'resid': 754, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 9.21467113494873, 'force': [0.030063919723033905, -0.1476738303899765, 0.03720495104789734], 'magnitude': 0.15522760152816772, 'cosine_with_motion': 0.5434688925743103, 'motion_component': 0.08436137437820435, 'motion_component_percent': 54.34688925743103}, {'resid': 754, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 9.382380485534668, 'force': [0.11786408722400665, -0.3794859051704407, 0.12561048567295074], 'magnitude': 0.41674870252609253, 'cosine_with_motion': 0.605513870716095, 'motion_component': 0.25234711170196533, 'motion_component_percent': 60.5513870716095}, {'resid': 754, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 10.575311660766602, 'force': [0.019951002672314644, -0.15958714485168457, 0.04207349941134453], 'magnitude': 0.1662416309118271, 'cosine_with_motion': 0.5450804829597473, 'motion_component': 0.09061506390571594, 'motion_component_percent': 54.50804829597473}, {'resid': 754, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 11.344700813293457, 'force': [-0.008422060869634151, 0.042243946343660355, -0.011665789410471916], 'magnitude': 0.04462704062461853, 'cosine_with_motion': -0.5615012049674988, 'motion_component': -0.025058137252926826, 'motion_component_percent': 56.15012049674988}, {'resid': 754, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 10.750149726867676, 'force': [-0.0028622036334127188, 0.048830628395080566, -0.008800765499472618], 'magnitude': 0.04969985783100128, 'cosine_with_motion': -0.46913471817970276, 'motion_component': -0.023315928876399994, 'motion_component_percent': 46.913471817970276}, {'resid': 754, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 10.833091735839844, 'force': [0.0015707853017374873, -0.03584989160299301, 0.013878014869987965], 'magnitude': 0.0384744256734848, 'cosine_with_motion': 0.6229701042175293, 'motion_component': 0.023968417197465897, 'motion_component_percent': 62.29701042175293}, {'resid': 754, 'resname': 'GLU', 'atom': 'HG2', 'charge': -0.042500000447034836, 'distance': 11.922053337097168, 'force': [-0.0041702198795974255, 0.09235025197267532, -0.03617851808667183], 'magnitude': 0.09927157312631607, 'cosine_with_motion': -0.6262347102165222, 'motion_component': -0.06216730549931526, 'motion_component_percent': 62.62347102165222}, {'resid': 754, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 10.597421646118164, 'force': [0.007162639405578375, 0.11773466318845749, -0.04327306151390076], 'magnitude': 0.12563961744308472, 'cosine_with_motion': -0.5913365483283997, 'motion_component': -0.0742952972650528, 'motion_component_percent': 59.133654832839966}, {'resid': 754, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 10.5279541015625, 'force': [0.1733083724975586, -2.107877254486084, 1.1605278253555298], 'magnitude': 2.4124691486358643, 'cosine_with_motion': 0.724111020565033, 'motion_component': 1.746895432472229, 'motion_component_percent': 72.4111020565033}, {'resid': 754, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 10.520896911621094, 'force': [-0.4599180519580841, 2.0706379413604736, -1.2378894090652466], 'magnitude': 2.4558982849121094, 'cosine_with_motion': -0.7577164173126221, 'motion_component': -1.8608744144439697, 'motion_component_percent': 75.7716417312622}, {'resid': 754, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 10.492804527282715, 'force': [0.028359076008200645, 2.060166358947754, -1.3605875968933105], 'magnitude': 2.4690661430358887, 'cosine_with_motion': -0.7626713514328003, 'motion_component': -1.8830859661102295, 'motion_component_percent': 76.26713514328003}, {'resid': 754, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 8.125082015991211, 'force': [0.27385127544403076, -2.551928997039795, 0.8336242437362671], 'magnitude': 2.6985671520233154, 'cosine_with_motion': 0.5897150039672852, 'motion_component': 1.5913854837417603, 'motion_component_percent': 58.971500396728516}, {'resid': 754, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 7.677719593048096, 'force': [-0.46071118116378784, 2.911374568939209, -1.4326974153518677], 'magnitude': 3.277343273162842, 'cosine_with_motion': -0.6999454498291016, 'motion_component': -2.293961524963379, 'motion_component_percent': 69.99454498291016}, {'resid': 1082, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 10.095779418945312, 'force': [0.565130889415741, -1.5825204849243164, -0.06728389114141464], 'magnitude': 1.681746482849121, 'cosine_with_motion': 0.3045062720775604, 'motion_component': 0.5121023654937744, 'motion_component_percent': 30.450627207756042}, {'resid': 1082, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 10.853769302368164, 'force': [-0.24440865218639374, 0.79049152135849, -0.0057685486972332], 'magnitude': 0.8274332284927368, 'cosine_with_motion': -0.3453315794467926, 'motion_component': -0.28573882579803467, 'motion_component_percent': 34.53315794467926}, {'resid': 1082, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 10.301560401916504, 'force': [-0.041272372007369995, 0.11488018929958344, 0.022909488528966904], 'magnitude': 0.12420029193162918, 'cosine_with_motion': -0.16372579336166382, 'motion_component': -0.020334791392087936, 'motion_component_percent': 16.372579336166382}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 10.47085952758789, 'force': [-0.14230936765670776, 0.29524609446525574, 0.06737929582595825], 'magnitude': 0.3346075117588043, 'cosine_with_motion': -0.1522619128227234, 'motion_component': -0.05094797909259796, 'motion_component_percent': 15.226191282272339}, {'resid': 1082, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 11.658084869384766, 'force': [-0.03874926269054413, 0.1283555030822754, 0.0271359384059906], 'magnitude': 0.13679546117782593, 'cosine_with_motion': -0.14566703140735626, 'motion_component': -0.019926588982343674, 'motion_component_percent': 14.566703140735626}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 12.340296745300293, 'force': [0.011647447943687439, -0.03552410751581192, -0.004991964902728796], 'magnitude': 0.037716638296842575, 'cosine_with_motion': 0.21326009929180145, 'motion_component': 0.00804345402866602, 'motion_component_percent': 21.326009929180145}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 11.762126922607422, 'force': [0.008038308471441269, -0.03991740942001343, -0.008095706813037395], 'magnitude': 0.041515711694955826, 'cosine_with_motion': 0.1392783671617508, 'motion_component': 0.0057822405360639095, 'motion_component_percent': 13.92783671617508}, {'resid': 1082, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 12.318647384643555, 'force': [-0.009601840749382973, 0.02676258608698845, 0.008768812753260136], 'magnitude': 0.029754385352134705, 'cosine_with_motion': -0.05108291655778885, 'motion_component': -0.0015199407935142517, 'motion_component_percent': 5.108291655778885}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HG2', 'charge': -0.042500000447034836, 'distance': 12.22248363494873, 'force': [0.0382230281829834, -0.0818127766251564, -0.027689779177308083], 'magnitude': 0.09445133060216904, 'cosine_with_motion': 0.057665370404720306, 'motion_component': 0.005446570925414562, 'motion_component_percent': 5.766537040472031}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 13.373836517333984, 'force': [0.024066517129540443, -0.07164569199085236, -0.022608192637562752], 'magnitude': 0.07888873666524887, 'cosine_with_motion': 0.05805889889597893, 'motion_component': 0.0045801931992173195, 'motion_component_percent': 5.805889889597893}, {'resid': 1082, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 11.870328903198242, 'force': [-0.5066403150558472, 1.6638699769973755, 0.7589874267578125], 'magnitude': 1.8976852893829346, 'cosine_with_motion': 0.06448987871408463, 'motion_component': 0.12238149344921112, 'motion_component_percent': 6.4489878714084625}, {'resid': 1082, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 11.773313522338867, 'force': [0.31356993317604065, -1.7681353092193604, -0.7884266972541809], 'magnitude': 1.9611846208572388, 'cosine_with_motion': -0.07869424670934677, 'motion_component': -0.1543339490890503, 'motion_component_percent': 7.869424670934677}, {'resid': 1082, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 11.889870643615723, 'force': [0.600310206413269, -1.5827871561050415, -0.9121628999710083], 'magnitude': 1.922921895980835, 'cosine_with_motion': -0.14188715815544128, 'motion_component': -0.27283793687820435, 'motion_component_percent': 14.188715815544128}, {'resid': 1082, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 9.171394348144531, 'force': [-0.5608819127082825, 1.9521459341049194, 0.6002480983734131], 'magnitude': 2.1179614067077637, 'cosine_with_motion': -0.057675063610076904, 'motion_component': -0.12215355783700943, 'motion_component_percent': 5.76750636100769}, {'resid': 1082, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 8.951977729797363, 'force': [0.76751708984375, -2.076422929763794, -0.9544638395309448], 'magnitude': 2.41072940826416, 'cosine_with_motion': -0.05588728189468384, 'motion_component': -0.13472911715507507, 'motion_component_percent': 5.588728189468384}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'N', 'charge': -0.38210001587867737, 'distance': 14.742170333862305, 'force': [-0.32056140899658203, -0.11281135678291321, -0.4745774567127228], 'magnitude': 0.5837035179138184, 'cosine_with_motion': -0.8048720359802246, 'motion_component': -0.46980664134025574, 'motion_component_percent': 80.48720359802246}, {'resid': 130, 'resname': 'ASN', 'atom': 'H', 'charge': 0.2681000232696533, 'distance': 14.272891998291016, 'force': [0.2439701110124588, 0.10927872359752655, 0.3456064462661743], 'magnitude': 0.4369291365146637, 'cosine_with_motion': 0.7689654231071472, 'motion_component': 0.33598339557647705, 'motion_component_percent': 76.89654231071472}, {'resid': 130, 'resname': 'ASN', 'atom': 'CA', 'charge': -0.20800000429153442, 'distance': 13.950506210327148, 'force': [-0.17989890277385712, -0.04545995593070984, -0.30244797468185425], 'magnitude': 0.35483095049858093, 'cosine_with_motion': -0.8533782958984375, 'motion_component': -0.3028050363063812, 'motion_component_percent': 85.33782958984375}, {'resid': 130, 'resname': 'ASN', 'atom': 'HA', 'charge': 0.13580000400543213, 'distance': 14.27078628540039, 'force': [0.11650732159614563, 0.012606868520379066, 0.18782185018062592], 'magnitude': 0.22138187289237976, 'cosine_with_motion': 0.8744021654129028, 'motion_component': 0.19357678294181824, 'motion_component_percent': 87.44021654129028}, {'resid': 130, 'resname': 'ASN', 'atom': 'CB', 'charge': -0.22990000247955322, 'distance': 12.456268310546875, 'force': [-0.25106561183929443, -0.06437169760465622, -0.4181089699268341], 'magnitude': 0.4919275939464569, 'cosine_with_motion': -0.8509031534194946, 'motion_component': -0.4185827374458313, 'motion_component_percent': 85.09031534194946}, {'resid': 130, 'resname': 'ASN', 'atom': 'HB2', 'charge': 0.1023000031709671, 'distance': 12.323342323303223, 'force': [0.10884582996368408, 0.048048410564661026, 0.18936854600906372], 'magnitude': 0.2236437201499939, 'cosine_with_motion': 0.8185427188873291, 'motion_component': 0.18306194245815277, 'motion_component_percent': 81.85427188873291}, {'resid': 130, 'resname': 'ASN', 'atom': 'HB3', 'charge': 0.1023000031709671, 'distance': 12.1511869430542, 'force': [0.10391910374164581, 0.01899905316531658, 0.20433224737644196], 'magnitude': 0.23002567887306213, 'cosine_with_motion': 0.8904620409011841, 'motion_component': 0.204829141497612, 'motion_component_percent': 89.04620409011841}, {'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 11.848848342895508, 'force': [1.0207568407058716, 0.16781796514987946, 1.338316798210144], 'magnitude': 1.6915079355239868, 'cosine_with_motion': 0.8223841786384583, 'motion_component': 1.3910694122314453, 'motion_component_percent': 82.23841786384583}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 11.18601131439209, 'force': [-0.9870704412460327, -0.02388085424900055, -1.2521944046020508], 'magnitude': 1.5946376323699951, 'cosine_with_motion': -0.8447597622871399, 'motion_component': -1.34708571434021, 'motion_component_percent': 84.47597622871399}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 12.134881973266602, 'force': [-1.3555282354354858, -0.33321866393089294, -1.498694658279419], 'magnitude': 2.0480666160583496, 'cosine_with_motion': -0.7585096955299377, 'motion_component': -1.5534783601760864, 'motion_component_percent': 75.85096955299377}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 11.792470932006836, 'force': [0.7120258212089539, 0.13851650059223175, 0.6748884916305542], 'magnitude': 0.9907785058021545, 'cosine_with_motion': 0.7283598184585571, 'motion_component': 0.7216432690620422, 'motion_component_percent': 72.83598184585571}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 12.486884117126465, 'force': [0.5691388845443726, 0.20976173877716064, 0.6425807476043701], 'magnitude': 0.8836453557014465, 'cosine_with_motion': 0.7287209033966064, 'motion_component': 0.6439308524131775, 'motion_component_percent': 72.87209033966064}, {'resid': 130, 'resname': 'ASN', 'atom': 'C', 'charge': 0.8050000071525574, 'distance': 14.61804485321045, 'force': [0.5268728733062744, 0.15555039048194885, 1.1235992908477783], 'magnitude': 1.2507063150405884, 'cosine_with_motion': 0.8818515539169312, 'motion_component': 1.1029373407363892, 'motion_component_percent': 88.18515539169312}, {'resid': 458, 'resname': 'ASN', 'atom': 'H', 'charge': 0.2681000232696533, 'distance': 14.720118522644043, 'force': [-0.302646279335022, -0.03556503728032112, 0.2754685580730438], 'magnitude': 0.4107828736305237, 'cosine_with_motion': 0.5187841057777405, 'motion_component': 0.213107630610466, 'motion_component_percent': 51.87841057777405}, {'resid': 458, 'resname': 'ASN', 'atom': 'CA', 'charge': -0.20800000429153442, 'distance': 14.559157371520996, 'force': [0.22417186200618744, -0.011387579143047333, -0.2361188679933548], 'magnitude': 0.3257834017276764, 'cosine_with_motion': -0.542263925075531, 'motion_component': -0.17666058242321014, 'motion_component_percent': 54.2263925075531}, {'resid': 458, 'resname': 'ASN', 'atom': 'HA', 'charge': 0.13580000400543213, 'distance': 14.729241371154785, 'force': [-0.14786303043365479, 0.020433111116290092, 0.14458954334259033], 'magnitude': 0.20781511068344116, 'cosine_with_motion': 0.49191197752952576, 'motion_component': 0.10222674161195755, 'motion_component_percent': 49.191197752952576}, {'resid': 458, 'resname': 'ASN', 'atom': 'CB', 'charge': -0.22990000247955322, 'distance': 13.00257396697998, 'force': [0.3074222505092621, -0.008526943624019623, -0.330505907535553], 'magnitude': 0.4514590799808502, 'cosine_with_motion': -0.5552111268043518, 'motion_component': -0.2506551146507263, 'motion_component_percent': 55.52111268043518}, {'resid': 458, 'resname': 'ASN', 'atom': 'HB2', 'charge': 0.1023000031709671, 'distance': 12.750468254089355, 'force': [-0.1540869027376175, 4.1251463699154556e-05, 0.1410711258649826], 'magnitude': 0.20891107618808746, 'cosine_with_motion': 0.49716371297836304, 'motion_component': 0.10386300832033157, 'motion_component_percent': 49.716371297836304}, {'resid': 458, 'resname': 'ASN', 'atom': 'HB3', 'charge': 0.1023000031709671, 'distance': 12.791299819946289, 'force': [-0.1342872530221939, -0.010594211518764496, 0.1579364836215973], 'magnitude': 0.20757947862148285, 'cosine_with_motion': 0.6092331409454346, 'motion_component': 0.12646429240703583, 'motion_component_percent': 60.92331409454346}, {'resid': 458, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 12.435599327087402, 'force': [-0.9971124529838562, 0.194014310836792, 1.1516740322113037], 'magnitude': 1.5356522798538208, 'cosine_with_motion': 0.5457535982131958, 'motion_component': 0.8380877375602722, 'motion_component_percent': 54.57535982131958}, {'resid': 458, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 12.545868873596191, 'force': [0.8668451905250549, -0.25857362151145935, -0.8881117105484009], 'magnitude': 1.2676842212677002, 'cosine_with_motion': -0.47003862261772156, 'motion_component': -0.5958605408668518, 'motion_component_percent': 47.003862261772156}, {'resid': 458, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 12.047618865966797, 'force': [1.1808158159255981, -0.2871021628379822, -1.6854313611984253], 'magnitude': 2.077843189239502, 'cosine_with_motion': -0.6144174337387085, 'motion_component': -1.276663064956665, 'motion_component_percent': 61.44174337387085}, {'resid': 458, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 11.821269989013672, 'force': [-0.5218880772590637, 0.20710192620754242, 0.8104644</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>963</v>
+      </c>
+      <c r="B13" t="n">
+        <v>1186</v>
+      </c>
+      <c r="C13" t="n">
+        <v>2343</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>{939: {'frame': 939, 'motion_vector': [-0.11650466918945312, 0.023532867431640625, 2.3374404907226562], 'motion_vector_magnitude': 2.3404605388641357, 'ionic_force': [0.011754631996154785, 1.384194927290082, 1.1702117919921875], 'ionic_force_magnitude': 1.812602936725671, 'radial_force': 1.3842448367644216, 'axial_force': 1.1702117919921875, 'glu_force': [1.185623006566857, -0.2731010753195733, -5.82710570000927], 'glu_force_magnitude': 5.952768007416537, 'asn_force': [0.07152459118515253, 0.1890568340313621, 0.8805094212293625], 'asn_force_magnitude': 0.903413025427369, 'sf_force': [-3.2091511190883466, 2.3061026771829347, 15.226869580335915], 'sf_force_magnitude': 15.73131646364714, 'residue_force': [-1.9520035213363371, 2.2220584358947235, 10.280273301556008], 'residue_force_magnitude': 10.69728379517556, 'pip2_force': [0.6153464145027101, -0.007583370199427009, -3.8775673207710497], 'pip2_force_magnitude': 3.926096922448107, 'total_force': [-1.3249024748374723, 3.5986699929853785, 7.572917772777146], 'total_force_magnitude': 8.488514350549677, 'cosine_total_motion': 0.9030180206820309, 'cosine_glu_motion': -0.9880027321426302, 'cosine_asn_motion': 0.9715531481815293, 'cosine_sf_motion': 0.9783132496752479, 'cosine_residue_motion': 0.9709490973519864, 'cosine_pip2_motion': -0.9941861204345686, 'cosine_ionic_motion': 0.6521199023514099, 'motion_component_total': 7.665281427364383, 'motion_component_glu': -5.88135105513878, 'motion_component_asn': 0.8777137689621604, 'motion_component_sf': 15.390155331220363, 'motion_component_residue': 10.386518045043742, 'motion_component_ionic': 1.1820344500994235, 'motion_component_pip2': -3.9032710677787827, 'motion_component_percent_total': 90.30180206820309, 'motion_component_percent_glu': 98.80027321426303, 'motion_component_percent_asn': 97.15531481815293, 'motion_component_percent_sf': 97.8313249675248, 'motion_component_percent_residue': 97.09490973519864, 'motion_component_percent_ionic': 65.21199023514099, 'motion_component_percent_pip2': 99.41861204345686, 'ionic_contributions': [{'ion_id': 2333, 'distance': 8.245080947875977, 'force': [-1.2816457748413086, 3.622016668319702, 3.014767646789551], 'magnitude': 4.883691787719727, 'cosine_ionic_motion': 0.637037456035614, 'motion_component_ionic': 3.1110944747924805, 'motion_component_percent_ionic': 63.7037456035614}, {'ion_id': 2334, 'distance': 6.21304178237915, 'force': [1.6844559907913208, 0.6955639719963074, -8.405319213867188], 'magnitude': 8.600616455078125, 'cosine_ionic_motion': -0.9849676489830017, 'motion_component_ionic': -8.471328735351562, 'motion_component_percent_ionic': 98.49676489830017}, {'ion_id': 2381, 'distance': 7.49332857131958, 'force': [-3.0116941928863525, -2.9080581665039062, 4.175325870513916], 'magnitude': 5.912736415863037, 'cosine_ionic_motion': 0.7256565690040588, 'motion_component_ionic': 4.290616035461426, 'motion_component_percent_ionic': 72.56565690040588}, {'ion_id': 2397, 'distance': 9.67905330657959, 'force': [2.620638608932495, -0.025327546522021294, 2.385437488555908], 'magnitude': 3.543825626373291, 'cosine_ionic_motion': 0.6353735327720642, 'motion_component_ionic': 2.251652956008911, 'motion_component_percent_ionic': 63.53735327720642}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 9.199265480041504, 'force': [-1.9083045721054077, -0.6243361234664917, -0.2669468820095062], 'magnitude': 2.025507926940918, 'cosine_with_motion': -0.08782360702753067, 'motion_component': -0.17788740992546082, 'motion_component_percent': 8.782360702753067}, {'resid': 98, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 9.992105484008789, 'force': [0.9374246597290039, 0.2596541941165924, 0.08344092220067978], 'magnitude': 0.9762927889823914, 'cosine_with_motion': 0.04023425281047821, 'motion_component': 0.03928041085600853, 'motion_component_percent': 4.023425281047821}, {'resid': 98, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 9.382155418395996, 'force': [0.1368747353553772, 0.04352513328194618, 0.042325474321842194], 'magnitude': 0.14973501861095428, 'cosine_with_motion': 0.23972396552562714, 'motion_component': 0.03589507192373276, 'motion_component_percent': 23.972396552562714}, {'resid': 98, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 9.176970481872559, 'force': [0.3766750991344452, 0.1693359911441803, 0.13856637477874756], 'magnitude': 0.43561387062072754, 'cosine_with_motion': 0.2785491943359375, 'motion_component': 0.12133988738059998, 'motion_component_percent': 27.85491943359375}, {'resid': 98, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 10.865092277526855, 'force': [0.14430376887321472, 0.041361164301633835, 0.04763919115066528], 'magnitude': 0.1574922651052475, 'cosine_with_motion': 0.2591261863708496, 'motion_component': 0.040810368955135345, 'motion_component_percent': 25.91261863708496}, {'resid': 98, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 11.529401779174805, 'force': [-0.03977356478571892, -0.013314453884959221, -0.010381522588431835], 'magnitude': 0.04320864751935005, 'cosine_with_motion': -0.19723208248615265, 'motion_component': -0.008522131480276585, 'motion_component_percent': 19.723208248615265}, {'resid': 98, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 11.006648063659668, 'force': [-0.04478509724140167, -0.00808728951960802, -0.013290642760694027], 'magnitude': 0.04741044342517853, 'cosine_with_motion': -0.23466290533542633, 'motion_component': -0.011125472374260426, 'motion_component_percent': 23.466290533542633}, {'resid': 98, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 11.495786666870117, 'force': [0.02959432266652584, 0.009601333178579807, 0.014118617400527], 'magnitude': 0.034166429191827774, 'cosine_with_motion': 0.3724057972431183, 'motion_component': 0.012723776511847973, 'motion_component_percent': 37.24057972431183}, {'resid': 98, 'resname': 'GLU', 'atom': 'HG2', 'charge': -0.042500000447034836, 'distance': 11.46219253540039, 'force': [-0.08868764340877533, -0.039234209805727005, -0.046143967658281326], 'magnitude': 0.10739687085151672, 'cosine_with_motion': -0.3916704058647156, 'motion_component': -0.04206417500972748, 'motion_component_percent': 39.16704058647156}, {'resid': 98, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 12.533992767333984, 'force': [-0.07893069088459015, -0.02338346280157566, -0.035914722830057144], 'magnitude': 0.08981484919786453, 'cosine_with_motion': -0.3582307696342468, 'motion_component': -0.03217444196343422, 'motion_component_percent': 35.82307696342468}, {'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 11.161053657531738, 'force': [1.790451169013977, 0.43291082978248596, 1.1020495891571045], 'magnitude': 2.1465413570404053, 'cosine_with_motion': 0.47325170040130615, 'motion_component': 1.0158543586730957, 'motion_component_percent': 47.325170040130615}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 11.108824729919434, 'force': [-1.8875830173492432, -0.20632976293563843, -1.1166417598724365], 'magnitude': 2.2028231620788574, 'cosine_with_motion': -0.4645467698574066, 'motion_component': -1.023314356803894, 'motion_component_percent': 46.45467698574066}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 11.341093063354492, 'force': [-1.6234350204467773, -0.5166818499565125, -1.2507838010787964], 'magnitude': 2.113518714904785, 'cosine_with_motion': -0.555260181427002, 'motion_component': -1.1735527515411377, 'motion_component_percent': 55.526018142700195}, {'resid': 98, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 8.451034545898438, 'force': [2.2821638584136963, 0.4437505304813385, 0.9038407802581787], 'magnitude': 2.4944167137145996, 'cosine_with_motion': 0.3181239068508148, 'motion_component': 0.7935335636138916, 'motion_component_percent': 31.812390685081482}, {'resid': 98, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 8.104186058044434, 'force': [-2.503288984298706, -0.5579763650894165, -1.4403407573699951], 'magnitude': 2.9414918422698975, 'cosine_with_motion': -0.4485759437084198, 'motion_component': -1.319482445716858, 'motion_component_percent': 44.85759437084198}, {'resid': 426, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 9.492454528808594, 'force': [1.8387688398361206, 0.4501740634441376, 0.1873168796300888], 'magnitude': 1.9023183584213257, 'cosine_with_motion': 0.05260443314909935, 'motion_component': 0.10007037967443466, 'motion_component_percent': 5.260443314909935}, {'resid': 426, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 10.280620574951172, 'force': [-0.8938426971435547, -0.18140287697315216, -0.13678449392318726], 'magnitude': 0.9222645163536072, 'cosine_with_motion': -0.10185558348894119, 'motion_component': -0.09393779188394547, 'motion_component_percent': 10.18555834889412}, {'resid': 426, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 9.345588684082031, 'force': [-0.14780475199222565, -0.029635310173034668, 0.007003480102866888], 'magnitude': 0.15090906620025635, 'cosine_with_motion': 0.09312871843576431, 'motion_component': 0.014053967781364918, 'motion_component_percent': 9.312871843576431}, {'resid': 426, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 9.587409019470215, 'force': [-0.380105584859848, -0.11330001056194305, 0.04444652795791626], 'magnitude': 0.39911481738090515, 'cosine_with_motion': 0.1557723730802536, 'motion_component': 0.06217106059193611, 'motion_component_percent': 15.57723730802536}, {'resid': 426, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 10.460142135620117, 'force': [-0.16878296434879303, -0.015205669216811657, 0.012440496124327183], 'magnitude': 0.16992254555225372, 'cosine_with_motion': 0.12166319787502289, 'motion_component': 0.020673319697380066, 'motion_component_percent': 12.166319787502289}, {'resid': 426, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 11.381643295288086, 'force': [0.043879199773073196, 0.006014181766659021, -0.0020704942289739847], 'magnitude': 0.044337812811136246, 'cosine_with_motion': -0.094537653028965, 'motion_component': -0.004191592801362276, 'motion_component_percent': 9.4537653028965}, {'resid': 426, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 10.459547996520996, 'force': [0.052495259791612625, 0.0006817938992753625, -0.00014498268137685955], 'magnitude': 0.052499886602163315, 'cosine_with_motion': -0.052401576191186905, 'motion_component': -0.002751076826825738, 'motion_component_percent': 5.2401576191186905}, {'resid': 426, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 10.662495613098145, 'force': [-0.03889516368508339, -0.0013954987516626716, 0.00790787860751152], 'magnitude': 0.03971543535590172, 'cosine_with_motion': 0.2472536414861679, 'motion_component': 0.009819786064326763, 'motion_component_percent': 24.72536414861679}, {'resid': 426, 'resname': 'GLU', 'atom': 'HG2', 'charge': -0.042500000447034836, 'distance': 11.520064353942871, 'force': [0.10423062741756439, -0.0027071302756667137, -0.020801596343517303], 'magnitude': 0.10632054507732391, 'cosine_with_motion': -0.24445341527462006, 'motion_component': -0.025990420952439308, 'motion_component_percent': 24.445341527462006}, {'resid': 426, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 9.866703987121582, 'force': [0.14124901592731476, -0.004889574367552996, -0.03212302178144455], 'magnitude': 0.14493818581104279, 'cosine_with_motion': -0.2701972723007202, 'motion_component': -0.03916190192103386, 'motion_component_percent': 27.01972723007202}, {'resid': 426, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 11.09310245513916, 'force': [-2.061154365539551, -0.2725745439529419, 0.6316059231758118], 'magnitude': 2.172919750213623, 'cosine_with_motion': 0.3362533152103424, 'motion_component': 0.7306514382362366, 'motion_component_percent': 33.62533152103424}, {'resid': 426, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 10.8727388381958, 'force': [2.0926694869995117, 0.26171135902404785, -0.9165444374084473], 'magnitude': 2.2995243072509766, 'cosine_with_motion': -0.4422220289707184, 'motion_component': -1.0169003009796143, 'motion_component_percent': 44.22220289707184}, {'resid': 426, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 11.81359577178955, 'force': [1.8416519165039062, 0.40112221240997314, -0.49139758944511414], 'magnitude': 1.947832703590393, 'cosine_with_motion': -0.29694798588752747, 'motion_component': -0.5784050226211548, 'motion_component_percent': 29.694798588752747}, {'resid': 426, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 8.097832679748535, 'force': [-2.682424306869507, -0.33199700713157654, 0.27414873242378235], 'magnitude': 2.716758966445923, 'cosine_with_motion': 0.14870069921016693, 'motion_component': 0.4039839506149292, 'motion_component_percent': 14.870069921016693}, {'resid': 426, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 7.615781307220459, 'force': [3.181023120880127, 0.6238256692886353, -0.7659109234809875], 'magnitude': 3.3308684825897217, 'cosine_with_motion': -0.27530261874198914, 'motion_component': -0.9169968366622925, 'motion_component_percent': 27.530261874198914}, {'resid': 754, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 9.655570983886719, 'force': [-0.4117690622806549, 1.7917371988296509, 0.022981345653533936], 'magnitude': 1.8385875225067139, 'cosine_with_motion': 0.03343028947710991, 'motion_component': 0.06146451085805893, 'motion_component_percent': 3.343028947710991}, {'resid': 754, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 10.269599914550781, 'force': [0.15227870643138885, -0.9095554947853088, -0.061227601021528244], 'magnitude': 0.9242449998855591, 'cosine_with_motion': -0.0842571035027504, 'motion_component': -0.07787420600652695, 'motion_component_percent': 8.42571035027504}, {'resid': 754, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 9.608550071716309, 'force': [0.025371260941028595, -0.1390833556652069, 0.019827580079436302], 'magnitude': 0.14276207983493805, 'cosine_with_motion': 0.12006406486034393, 'motion_component': 0.017140595242381096, 'motion_component_percent': 12.006406486034393}, {'resid': 754, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 9.770750999450684, 'force': [0.1013266071677208, -0.36243507266044617, 0.07773417979478836], 'magnitude': 0.3842770457267761, 'cosine_with_motion': 0.17941683530807495, 'motion_component': 0.06894577294588089, 'motion_component_percent': 17.941683530807495}, {'resid': 754, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 10.846649169921875, 'force': [0.014315720647573471, -0.15561841428279877, 0.023471621796488762], 'magnitude': 0.15802831947803497, 'cosine_with_motion': 0.1339254081249237, 'motion_component': 0.021164007484912872, 'motion_component_percent': 13.39254081249237}, {'resid': 754, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 11.616758346557617, 'force': [-0.005847268737852573, 0.04194992780685425, -0.0041799768805503845], 'magnitude': 0.04256124049425125, 'cosine_with_motion': -0.08133494853973389, 'motion_component': -0.003461716463789344, 'motion_component_percent': 8.133494853973389}, {'resid': 754, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 10.678483963012695, 'force': [-0.00019002927001565695, 0.05011720210313797, -0.00502846110612154], 'magnitude': 0.05036919191479683, 'cosine_with_motion': -0.0895109549164772, 'motion_component': -0.004508594516664743, 'motion_component_percent': 8.95109549164772}, {'resid': 754, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 11.422403335571289, 'force': [0.002241395879536867, -0.03322039917111397, 0.009434772655367851], 'magnitude': 0.03460684418678284, 'cosine_with_motion': 0.25939956307411194, 'motion_component': 0.00897700060158968, 'motion_component_percent': 25.939956307411194}, {'resid': 754, 'resname': 'GLU', 'atom': 'HG2', 'charge': -0.042500000447034836, 'distance': 12.398606300354004, 'force': [-0.0025069997645914555, 0.08865127712488174, -0.023654257878661156], 'magnitude': 0.09178702533245087, 'cosine_with_motion': -0.24630461633205414, 'motion_component': -0.02260756865143776, 'motion_component_percent': 24.630461633205414}, {'resid': 754, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 10.797303199768066, 'force': [1.2357740160950925e-05, 0.1147245541214943, -0.03855862841010094], 'magnitude': 0.12103094905614853, 'cosine_with_motion': -0.3086479604244232, 'motion_component': -0.03735595569014549, 'motion_component_percent': 30.864796042442322}, {'resid': 754, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 11.807275772094727, 'force': [0.31606778502464294, -1.7790671586990356, 0.6432524919509888], 'magnitude': 1.918007493019104, 'cosine_with_motion': 0.31741318106651306, 'motion_component': 0.6088008880615234, 'motion_component_percent': 31.741318106651306}, {'resid': 754, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 12.593454360961914, 'force': [-0.39206069707870483, 1.5928184986114502, -0.49721333384513855], 'magnitude': 1.7140605449676514, 'cosine_with_motion': -0.2689753770828247, 'motion_component': -0.46104007959365845, 'motion_component_percent': 26.89753770828247}, {'resid': 754, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 11.45733642578125, 'force': [-0.36041393876075745, 1.8318898677825928, -0.89593505859375], 'magnitude': 2.070849657058716, 'cosine_with_motion': -0.41452494263648987, 'motion_component': -0.8584188222885132, 'motion_component_percent': 41.45249426364899}, {'resid': 754, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 8.379273414611816, 'force': [0.2509109377861023, -2.4772024154663086, 0.4883946478366852], 'magnitude': 2.537324905395508, 'cosine_with_motion': 0.17749665677547455, 'motion_component': 0.45036667585372925, 'motion_component_percent': 17.749665677547455}, {'resid': 754, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 7.880489826202393, 'force': [-0.40738847851753235, 2.9164369106292725, -1.0029261112213135], 'magnitude': 3.110856771469116, 'cosine_with_motion': -0.3060342073440552, 'motion_component': -0.9520285725593567, 'motion_component_percent': 30.603420734405518}, {'resid': 1082, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 9.1122465133667, 'force': [0.6341122388839722, -1.9600000381469727, 0.134016215801239], 'magnitude': 2.064378499984741, 'cosine_with_motion': 0.039997849613428116, 'motion_component': 0.08257070183753967, 'motion_component_percent': 3.9997849613428116}, {'resid': 1082, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 9.870962142944336, 'force': [-0.25502654910087585, 0.961002767086029, -0.11064381897449493], 'magnitude': 1.0004034042358398, 'cosine_with_motion': -0.08810795843601227, 'motion_component': -0.08814350515604019, 'motion_component_percent': 8.810795843601227}, {'resid': 1082, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 9.155479431152344, 'force': [-0.05101367086172104, 0.14799262583255768, 0.014852278865873814], 'magnitude': 0.15724122524261475, 'cosine_with_motion': 0.11994650959968567, 'motion_component': 0.018860535696148872, 'motion_component_percent': 11.994650959968567}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 8.998689651489258, 'force': [-0.19556325674057007, 0.40528643131256104, 0.05242258310317993], 'magnitude': 0.45304548740386963, 'cosine_with_motion': 0.14604464173316956, 'motion_component': 0.06616486608982086, 'motion_component_percent': 14.604464173316956}, {'resid': 1082, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 10.687308311462402, 'force': [-0.04949445277452469, 0.15371213853359222, 0.020464451983571053], 'magnitude': 0.1627756655216217, 'cosine_with_motion': 0.15019045770168304, 'motion_component': 0.024447351694107056, 'motion_component_percent': 15.019045770168304}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 11.221848487854004, 'force': [0.017289575189352036, -0.04201029986143112, -0.004053712822496891], 'magnitude': 0.04560950770974159, 'cosine_with_motion': -0.11689529567956924, 'motion_component': -0.005331536754965782, 'motion_component_percent': 11.689529567956924}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 11.172463417053223, 'force': [0.010736677795648575, -0.04460209980607033, -0.003553744638338685], 'magnitude': 0.04601361230015755, 'cosine_with_motion': -0.09849433600902557, 'motion_component': -0.004532080143690109, 'motion_component_percent': 9.849433600902557}, {'resid': 1082, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 11.113289833068848, 'force': [-0.009867429733276367, 0.03395399451255798, 0.009290024638175964], 'magnitude': 0.03655878081917763, 'cosine_with_motion': 0.2765580117702484, 'motion_component': 0.010110623203217983, 'motion_component_percent': 27.65580117702484}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HG2', 'charge': -0.042500000447034836, 'distance': 12.195591926574707, 'force': [0.026175638660788536, -0.08771932870149612, -0.024902913719415665], 'magnitude': 0.09486832469701767, 'cosine_with_motion': -0.2851928174495697, 'motion_component': -0.027055764570832253, 'motion_component_percent': 28.51928174495697}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 10.894660949707031, 'force': [0.021118706092238426, -0.11213364452123642, -0.03334514796733856], 'magnitude': 0.11887747049331665, 'cosine_with_motion': -0.2984658181667328, 'motion_component': -0.035480860620737076, 'motion_component_percent': 29.84658181667328}, {'resid': 1082, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 10.685893058776855, 'force': [-0.8308801651000977, 2.0326671600341797, 0.8132534027099609], 'magnitude': 2.3416829109191895, 'cosine_with_motion': 0.3732367157936096, 'motion_component': 0.8740020394325256, 'motion_component_percent': 37.32367157936096}, {'resid': 1082, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 10.257808685302734, 'force': [0.7718333005905151, -2.184640407562256, -1.1428207159042358], 'magnitude': 2.5834896564483643, 'cosine_with_motion': -0.4651588201522827, 'motion_component': -1.2017329931259155, 'motion_component_percent': 46.51588201522827}, {'resid': 1082, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 10.78917407989502, 'force': [1.0655505657196045, -1.9345152378082275, -0.7588140368461609], 'magnitude': 2.335282802581787, 'cosine_with_motion': -0.3555576205253601, 'motion_component': -0.830327570438385, 'motion_component_percent': 35.55576205253601}, {'resid': 1082, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 8.180293083190918, 'force': [-0.580885648727417, 2.550903558731079, 0.4930616021156311], 'magnitude': 2.6622633934020996, 'cosine_with_motion': 0.20546042919158936, 'motion_component': 0.5469897985458374, 'motion_component_percent': 20.546042919158936}, {'resid': 1082, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 7.709196090698242, 'force': [0.8835325241088867, -2.9663591384887695, -0.9933346509933472], 'magnitude': 3.2506353855133057, 'cosine_with_motion': -0.3278927803039551, 'motion_component': -1.0658599138259888, 'motion_component_percent': 32.78927803039551}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'N', 'charge': -0.38210001587867737, 'distance': 14.952507019042969, 'force': [-0.31295308470726013, -0.09939911216497421, -0.46273064613342285], 'magnitude': 0.5673971176147461, 'cosine_with_motion': -0.7887855768203735, 'motion_component': -0.44755464792251587, 'motion_component_percent': 78.87855768203735}, {'resid': 130, 'resname': 'ASN', 'atom': 'H', 'charge': 0.2681000232696533, 'distance': 14.511523246765137, 'force': [0.23898452520370483, 0.09741833060979843, 0.3347419500350952], 'magnitude': 0.42267730832099915, 'cosine_with_motion': 0.7651066780090332, 'motion_component': 0.32339322566986084, 'motion_component_percent': 76.51066780090332}, {'resid': 130, 'resname': 'ASN', 'atom': 'CA', 'charge': -0.20800000429153442, 'distance': 14.199386596679688, 'force': [-0.1702713668346405, -0.04064358025789261, -0.294385701417923], 'magnitude': 0.34250134229660034, 'cosine_with_motion': -0.8348541259765625, 'motion_component': -0.28593865036964417, 'motion_component_percent': 83.48541259765625}, {'resid': 130, 'resname': 'ASN', 'atom': 'HA', 'charge': 0.13580000400543213, 'distance': 14.034262657165527, 'force': [0.1203593760728836, 0.011144077405333519, 0.1943906992673874], 'magnitude': 0.2289067804813385, 'cosine_with_motion': 0.8224334716796875, 'motion_component': 0.18826059997081757, 'motion_component_percent': 82.24334716796875}, {'resid': 130, 'resname': 'ASN', 'atom': 'CB', 'charge': -0.22990000247955322, 'distance': 12.899147987365723, 'force': [-0.2138560712337494, -0.07863749563694, -0.39813676476478577], 'magnitude': 0.45872777700424194, 'cosine_with_motion': -0.8453122973442078, 'motion_component': -0.3877682387828827, 'motion_component_percent': 84.53122973442078}, {'resid': 130, 'resname': 'ASN', 'atom': 'HB2', 'charge': 0.1023000031709671, 'distance': 12.201788902282715, 'force': [0.1193113625049591, 0.04064180329442024, 0.1901383101940155], 'magnitude': 0.22812175750732422, 'cosine_with_motion': 0.8081757426261902, 'motion_component': 0.1843624711036682, 'motion_component_percent': 80.81757426261902}, {'resid': 130, 'resname': 'ASN', 'atom': 'HB3', 'charge': 0.1023000031709671, 'distance': 13.147619247436523, 'force': [0.0850834995508194, 0.04830826073884964, 0.1703869253396988], 'magnitude': 0.19648052752017975, 'cosine_with_motion': 0.8469921350479126, 'motion_component': 0.1664174646139145, 'motion_component_percent': 84.69921350479126}, {'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 12.195417404174805, 'force': [0.6263405680656433, 0.17742590606212616, 1.4580061435699463], 'magnitude': 1.5967354774475098, 'cosine_with_motion': 0.8935296535491943, 'motion_component': 1.4267305135726929, 'motion_component_percent': 89.35296535491943}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 12.44211196899414, 'force': [-0.38705453276634216, -0.16492900252342224, -1.218314290046692], 'magnitude': 1.2889152765274048, 'cosine_with_motion': -0.9303431510925293, 'motion_component': -1.1991335153579712, 'motion_component_percent': 93.03431510925293}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 11.399138450622559, 'force': [-0.9791609048843384, -0.06634428352117538, -2.1032793521881104], 'magnitude': 2.3209786415100098, 'cosine_with_motion': -0.8843215703964233, 'motion_component': -2.0524914264678955, 'motion_component_percent': 88.43215703964233}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 11.024120330810547, 'force': [0.41022366285324097, -0.026858577504754066, 1.0565376281738281], 'magnitude': 1.1337003707885742, 'cosine_with_motion': 0.9124844074249268, 'motion_component': 1.0344839096069336, 'motion_component_percent': 91.24844074249268}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 11.318466186523438, 'force': [0.5342535376548767, 0.0006608002004213631, 0.933421790599823], 'magnitude': 1.075501561164856, 'cosine_with_motion': 0.842053234577179, 'motion_component': 0.905629575252533, 'motion_component_percent': 84.2053234577179}, {'resid': 130, 'resname': 'ASN', 'atom': 'C', 'charge': 0.8050000071525574, 'distance': 14.996065139770508, 'force': [0.5027453899383545, 0.1283503621816635, 1.0691943168640137], 'magnitude': 1.1884456872940063, 'cosine_with_motion': 0.8785250186920166, 'motion_component': 1.044079303741455, 'motion_component_percent': 87.85250186920166}, {'resid': 458, 'resname': 'ASN', 'atom': 'N', 'charge': -0.38210001587867737, 'distance': 14.472807884216309, 'force': [0.4391495883464813, 0.058707915246486664, -0.412907212972641], 'magnitude': 0.605633020401001, 'cosine_with_motion': -0.7160183191299438, 'motion_component': -0.4336443245410919, 'motion_component_percent': 71.60183191299438}, {'resid': 458, 'resname': 'ASN', 'atom': 'H', 'charge': 0.2681000232696533, 'distance': 14.036032676696777, 'force': [-0.33223992586135864, -0.07044898718595505, 0.29795435070991516], 'magnitude': 0.45179998874664307, 'cosine_with_motion': 0.6936696767807007, 'motion_component': 0.31339994072914124, 'motion_component_percent': 69.36696767807007}, {'resid': 458, 'resname': 'ASN', 'atom': 'CA', 'charge': -0.20800000429153442, 'distance': 13.654990196228027, 'force': [0.25780588388442993, 0.011455586180090904, -0.265646368265152], 'magnitude': 0.37035536766052246, 'cosine_with_motion': -0.7506887316703796, 'motion_component': -0.27802160382270813, 'motion_component_percent': 75.06887316703796}, {'resid': 458, 'resname': 'ASN', 'atom': 'HA', 'charge': 0.13580000400543213, 'distance': 13.818964004516602, 'force': [-0.17079202830791473, 0.008767473511397839, 0.162770077586174], 'magnitude': 0.23609507083892822, 'cosine_with_motion': 0.7249196767807007, 'motion_component': 0.17114996910095215, 'motion_component_percent': 72.49196767807007}, {'resid': 458, 'resname': 'ASN', 'atom': 'CB', 'charge': -0.22990000247955322, 'distance': 12.199490547180176, 'force': [0.3594961166381836, 0.033678602427244186, -0.3642079830169678], 'magnitude': 0.5128539800643921, 'cosine_with_motion': -0.7434759140014648, 'motion_component': -0.3812945783138275, 'motion_component_percent': 74.34759140014648}, {'resid': 458, 'resname': 'ASN', 'atom': 'HB2', 'charge': 0.1023000031709671, 'distance': 11.927542686462402, 'force': [-0.18132825195789337, -0.018161486834287643, 0.15421898663043976], 'magnitude': 0.23873263597488403, 'cosine_with_motion': 0.6822009086608887, 'motion_component': 0.162863627076149, 'motion_component_percent': 68.22009086608887}, {'resid': 458, 'resname': 'ASN', 'atom': 'HB3', 'charge': 0.1023000031709671, 'distance': 12.106386184692383, 'force': [-0.15511678159236908, -0.03413382172584534, 0.16873960196971893], 'magnitude': 0.23173128068447113, 'cosine_with_motion': 0.7590695023536682, 'motion_component': 0.1759001463651657, 'motion_component_percent': 75.90695023536682}, {'resid': 458, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 11.282498359680176, 'force': [-1.2254321575164795, 0.02686131000518799, 1.406418800354004], 'magnitude': 1.8655881881713867, 'cosine_with_motion': 0.7857437133789062, 'motion_component': 1.465874195098877, 'motion_component_percent': 78.57437133789062}, {'resid': 458, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 11.580598831176758, 'force': [0.8566738963127136, -0.060082610696554184, -1.2149524688720703], 'magnitude': 1.4878205060958862, 'cosine_with_motion': -0.8446131944656372, 'motion_component': -1.2566328048706055, 'motion_component_percent': 84.46131944656372}, {'resid': 458, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 10.350701332092285, 'force': [1.9815322160720825, -0.2098444253206253, -1.9883711338043213], 'magnitude': 2.8149821758270264, 'cosine_with_motion': -0.741231381893158, 'motion_component': -2.0865530967712402, 'motion_component_percent': 74.1231381893158}, {'resid': 458, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 9.918787956237793, 'force': [-0.9315465092658997, 0.21294881403446198, 1.0237902402877808], 'magnitude': 1.4004544019699097, 'cosine_with_motion': 0.7647385001182556, 'motion_component': 1.0709813833236694, 'motion_component_percent': 76.47385001182556}, {'resid': 458, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.4149</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>1193</v>
+      </c>
+      <c r="B14" t="n">
+        <v>1225</v>
+      </c>
+      <c r="C14" t="n">
+        <v>2230</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>{963: {'frame': 963, 'motion_vector': [-0.33338165283203125, -0.41335296630859375, 0.9359664916992188], 'motion_vector_magnitude': 1.07612144947052, 'ionic_force': [-2.9778733253479004, -0.732078991830349, 17.99839723110199], 'ionic_force_magnitude': 18.257764706574505, 'radial_force': 3.0665402642225166, 'axial_force': 17.99839723110199, 'glu_force': [-1.2704326654784381, 1.315926321032748, -2.3915896136313677], 'glu_force_magnitude': 3.010873979417084, 'asn_force': [0.0, 0.0, 0.0], 'asn_force_magnitude': 0.0, 'sf_force': [-1.3469595810311148, -0.8255676170156221, 0.3450609624851495], 'sf_force_magnitude': 1.617074231761655, 'residue_force': [-2.617392246509553, 0.490358704017126, -2.046528651146218], 'residue_force_magnitude': 3.358492720054048, 'pip2_force': [0.5142812457925174, -0.010757024552731309, -3.243831784464419], 'pip2_force_magnitude': 3.2843637982496316, 'total_force': [-5.080984326064936, -0.2524773123659543, 12.708036795491353], 'total_force_magnitude': 13.688474922742095, 'cosine_total_motion': 0.9295408398999593, 'cosine_glu_motion': -0.7280255182794085, 'cosine_asn_motion': 0, 'cosine_sf_motion': 0.6397472834746699, 'cosine_residue_motion': -0.3446409859641062, 'cosine_pip2_motion': -0.906277311284571, 'cosine_ionic_motion': 0.9233340106149747, 'motion_component_total': 12.723996476635218, 'motion_component_glu': -2.1919930893391077, 'motion_component_asn': 0, 'motion_component_sf': 1.0345188469464077, 'motion_component_residue': -1.1574742423927, 'motion_component_ionic': 16.858015111385974, 'motion_component_pip2': -2.9765443923580572, 'motion_component_percent_total': 92.95408398999592, 'motion_component_percent_glu': 72.80255182794086, 'motion_component_percent_asn': 0, 'motion_component_percent_sf': 63.97472834746699, 'motion_component_percent_residue': 34.46409859641062, 'motion_component_percent_ionic': 92.33340106149747, 'motion_component_percent_pip2': 90.6277311284571, 'ionic_contributions': [{'ion_id': 2333, 'distance': 10.5684232711792, 'force': [-0.32869887351989746, -0.5814714431762695, 2.8964521884918213], 'magnitude': 2.9724714756011963, 'cosine_ionic_motion': 0.9569132924079895, 'motion_component_ionic': 2.84439754486084, 'motion_component_percent_ionic': 95.69132924079895}, {'ion_id': 2334, 'distance': 5.556124687194824, 'force': [-2.2014694213867188, -0.24710756540298462, 10.523964881896973], 'magnitude': 10.754597663879395, 'cosine_ionic_motion': 0.9233488440513611, 'motion_component_ionic': 9.930245399475098, 'motion_component_percent_ionic': 92.33488440513611}, {'ion_id': 2343, 'distance': 14.592389106750488, 'force': [-0.16000592708587646, -0.08226221054792404, 1.5487253665924072], 'magnitude': 1.5591405630111694, 'cosine_ionic_motion': 0.9160083532333374, 'motion_component_ionic': 1.4281858205795288, 'motion_component_percent_ionic': 91.60083532333374}, {'ion_id': 2372, 'distance': 13.698756217956543, 'force': [-1.0009732246398926, -0.25765180587768555, 1.4358693361282349], 'magnitude': 1.769195556640625, 'cosine_ionic_motion': 0.9371088743209839, 'motion_component_ionic': 1.6579288244247437, 'motion_component_percent_ionic': 93.71088743209839}, {'ion_id': 2397, 'distance': 13.583029747009277, 'force': [0.7132741212844849, 0.43641403317451477, 1.5933854579925537], 'magnitude': 1.7994705438613892, 'cosine_ionic_motion': 0.5541947484016418, 'motion_component_ionic': 0.9972571134567261, 'motion_component_percent_ionic': 55.419474840164185}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 10.86776065826416, 'force': [-1.0503259897232056, -0.42152512073516846, -0.9085326194763184], 'magnitude': 1.4513096809387207, 'cosine_with_motion': -0.20870853960514069, 'motion_component': -0.3029007315635681, 'motion_component_percent': 20.87085396051407}, {'resid': 98, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 11.317855834960938, 'force': [0.591378927230835, 0.20803126692771912, 0.4313521385192871], 'magnitude': 0.760966956615448, 'cosine_with_motion': 0.1472548097372055, 'motion_component': 0.11205604672431946, 'motion_component_percent': 14.72548097372055}, {'resid': 98, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 11.74729061126709, 'force': [0.06363973021507263, 0.024207696318626404, 0.06697995215654373], 'magnitude': 0.09551095217466354, 'cosine_with_motion': 0.3061677813529968, 'motion_component': 0.02924237586557865, 'motion_component_percent': 30.616778135299683}, {'resid': 98, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 12.25554084777832, 'force': [0.15273424983024597, 0.07862593978643417, 0.17363323271274567], 'magnitude': 0.24425046145915985, 'cosine_with_motion': 0.30092403292655945, 'motion_component': 0.07350083440542221, 'motion_component_percent': 30.092403292655945}, {'resid': 98, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 12.973910331726074, 'force': [0.0784071683883667, 0.0208919495344162, 0.07494059950113297], 'magnitude': 0.1104547455906868, 'cosine_with_motion': 0.2975417971611023, 'motion_component': 0.032864902168512344, 'motion_component_percent': 29.75417971611023}, {'resid': 98, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 13.54500961303711, 'force': [-0.02305479347705841, -0.0073945350013673306, -0.01984575018286705], 'magnitude': 0.03130585327744484, 'cosine_with_motion': -0.23249077796936035, 'motion_component': -0.007278322242200375, 'motion_component_percent': 23.249077796936035}, {'resid': 98, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 12.565220832824707, 'force': [-0.02722526527941227, -0.004569114185869694, -0.023691730573773384], 'magnitude': 0.03637842833995819, 'cosine_with_motion': -0.28634199500083923, 'motion_component': -0.010416671633720398, 'motion_component_percent': 28.634199500083923}, {'resid': 98, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 14.106629371643066, 'force': [0.015085669234395027, 0.0034683281555771828, 0.016589753329753876], 'magnitude': 0.02268979139626026, 'cosine_with_motion': 0.37123867869377136, 'motion_component': 0.008423328399658203, 'motion_component_percent': 37.123867869377136}, {'resid': 98, 'resname': 'GLU', 'atom': 'HG2', 'charge': -0.042500000447034836, 'distance': 14.900114059448242, 'force': [-0.0444483645260334, -0.0080315712839365, -0.04471062496304512], 'magnitude': 0.06355472654104233, 'cosine_with_motion': -0.34666764736175537, 'motion_component': -0.022032367065548897, 'motion_component_percent': 34.66676473617554}, {'resid': 98, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 13.780309677124023, 'force': [-0.04689602926373482, -0.007312537170946598, -0.057169001549482346], 'magnitude': 0.07430347055196762, 'cosine_with_motion': -0.4358619749546051, 'motion_component': -0.03238605707883835, 'motion_component_percent': 43.58619749546051}, {'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 14.62722110748291, 'force': [0.7630792856216431, 0.2950676679611206, 0.9447438716888428], 'magnitude': 1.2497583627700806, 'cosine_with_motion': 0.3776399493217468, 'motion_component': 0.4719586968421936, 'motion_component_percent': 37.76399493217468}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 14.734550476074219, 'force': [-0.7800986766815186, -0.38828086853027344, -0.8991445302963257], 'magnitude': 1.2521089315414429, 'cosine_with_motion': -0.31244978308677673, 'motion_component': -0.39122116565704346, 'motion_component_percent': 31.244978308677673}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 14.977458000183105, 'force': [-0.6687812805175781, -0.26243117451667786, -0.9758995175361633], 'magnitude': 1.2118244171142578, 'cosine_with_motion': -0.4462743103504181, 'motion_component': -0.5408061146736145, 'motion_component_percent': 44.62743103504181}, {'resid': 98, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 11.151861190795898, 'force': [0.8692598342895508, 0.25521886348724365, 1.109640121459961], 'magnitude': 1.4324979782104492, 'cosine_with_motion': 0.4173063635826111, 'motion_component': 0.597790539264679, 'motion_component_percent': 41.73063635826111}, {'resid': 98, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 11.473546028137207, 'force': [-0.7614473104476929, -0.2793729901313782, -1.2230429649353027], 'magnitude': 1.4675439596176147, 'cosine_with_motion': -0.490987628698349, 'motion_component': -0.7205459475517273, 'motion_component_percent': 49.0987628698349}, {'resid': 426, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 12.514248847961426, 'force': [0.9354533553123474, 0.1611393392086029, -0.5449526906013489], 'magnitude': 1.0945374965667725, 'cosine_with_motion': -0.7543607950210571, 'motion_component': -0.8256762027740479, 'motion_component_percent': 75.43607950210571}, {'resid': 426, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 12.40679931640625, 'force': [-0.5622939467430115, -0.057530760765075684, 0.28551748394966125], 'magnitude': 0.6332491636276245, 'cosine_with_motion': 0.7021375894546509, 'motion_component': 0.4446280598640442, 'motion_component_percent': 70.21375894546509}, {'resid': 426, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 13.177985191345215, 'force': [-0.061185404658317566, -0.008520259521901608, 0.04409382492303848], 'magnitude': 0.07589805126190186, 'cosine_with_motion': 0.7981621026992798, 'motion_component': 0.06057894974946976, 'motion_component_percent': 79.81621026992798}, {'resid': 426, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 13.699895858764648, 'force': [-0.15214234590530396, -0.033998191356658936, 0.11791028082370758], 'magnitude': 0.19546356797218323, 'cosine_with_motion': 0.8326171040534973, 'motion_component': 0.16274631023406982, 'motion_component_percent': 83.26171040534973}, {'resid': 426, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 14.524916648864746, 'force': [-0.07234460860490799, -0.0051210843957960606, 0.05006033554673195], 'magnitude': 0.08812493830919266, 'cosine_with_motion': 0.7707219123840332, 'motion_component': 0.06791982054710388, 'motion_component_percent': 77.07219123840332}, {'resid': 426, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 14.456986427307129, 'force': [0.023354722186923027, 6.34481621091254e-05, -0.014482568018138409], 'magnitude': 0.027480753138661385, 'cosine_with_motion': -0.7225418090820312, 'motion_component': -0.01985599286854267, 'motion_component_percent': 72.25418090820312}, {'resid': 426, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 14.879989624023438, 'force': [0.048148155212402344, -0.0021670067217200994, -0.041691213846206665], 'magnitude': 0.0637267455458641, 'cosine_with_motion': -0.7900168299674988, 'motion_component': -0.050345201045274734, 'motion_component_percent': 79.00168299674988}, {'resid': 426, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 12.326996803283691, 'force': [-0.8868691325187683, -0.06930432468652725, 0.7636566162109375], 'magnitude': 1.1723955869674683, 'cosine_with_motion': 0.8235867619514465, 'motion_component': 0.9655694961547852, 'motion_component_percent': 82.35867619514465}, {'resid': 426, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 12.37043285369873, 'force': [0.8713492155075073, 0.11467844992876053, -0.9063097238540649], 'magnitude': 1.2624571323394775, 'cosine_with_motion': -0.8731101751327515, 'motion_component': -1.102264165878296, 'motion_component_percent': 87.31101751327515}, {'resid': 754, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 11.723438262939453, 'force': [-0.089572973549366, 1.024742841720581, -0.705226480960846], 'magnitude': 1.247183084487915, 'cosine_with_motion': -0.7851656079292297, 'motion_component': -0.9792452454566956, 'motion_component_percent': 78.51656079292297}, {'resid': 754, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 12.084525108337402, 'force': [0.02844856120646, -0.5757279992103577, 0.33652734756469727], 'magnitude': 0.6674748659133911, 'cosine_with_motion': 0.7566267848014832, 'motion_component': 0.5050293803215027, 'motion_component_percent': 75.66267848014832}, {'resid': 754, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 12.362873077392578, 'force': [0.0025646663270890713, -0.06572017818689346, 0.05577605962753296], 'magnitude': 0.08623623102903366, 'cosine_with_motion': 0.8460623025894165, 'motion_component': 0.07296122610569, 'motion_component_percent': 84.60623025894165}, {'resid': 754, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 12.759586334228516, 'force': [0.02122245728969574, -0.16376015543937683, 0.15332230925559998], 'magnitude': 0.22533422708511353, 'cosine_with_motion': 0.8417776226997375, 'motion_component': 0.1896813064813614, 'motion_component_percent': 84.17776226997375}, {'resid': 754, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 13.535293579101562, 'force': [-0.0035710223019123077, -0.07923327386379242, 0.06330888718366623], 'magnitude': 0.10148241370916367, 'cosine_with_motion': 0.8533928394317627, 'motion_component': 0.08660436421632767, 'motion_component_percent': 85.33928394317627}, {'resid': 754, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 14.226341247558594, 'force': [-0.0004936759360134602, 0.022696074098348618, -0.017029814422130585], 'magnitude': 0.0283790435642004, 'cosine_with_motion': -0.8237335085868835, 'motion_component': -0.023376768454909325, 'motion_component_percent': 82.37335085868835}, {'resid': 754, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 13.294952392578125, 'force': [0.0026894034817814827, 0.02653011493384838, -0.018569229170680046], 'magnitude': 0.03249455615878105, 'cosine_with_motion': -0.8362789750099182, 'motion_component': -0.027174513787031174, 'motion_component_percent': 83.62789750099182}, {'resid': 754, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 14.332968711853027, 'force': [-0.0021138759329915047, -0.016030926257371902, 0.014886578544974327], 'magnitude': 0.021978838369250298, 'cosine_with_motion': 0.8990609049797058, 'motion_component': 0.019760314375162125, 'motion_component_percent': 89.90609049797058}, {'resid': 754, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 13.863022804260254, 'force': [0.011614090763032436, 0.051555708050727844, -0.0509660504758358], 'magnitude': 0.07341945171356201, 'cosine_with_motion': -0.9225003719329834, 'motion_component': -0.06772947311401367, 'motion_component_percent': 92.25003719329834}, {'resid': 754, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 14.775160789489746, 'force': [-0.04666072875261307, 0.8284670114517212, -0.9284808039665222], 'magnitude': 1.2452354431152344, 'cosine_with_motion': -0.8924614787101746, 'motion_component': -1.111324667930603, 'motion_component_percent': 89.24614787101746}, {'resid': 754, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 11.52257251739502, 'force': [-0.04420057684183121, -0.947267472743988, 0.9493024945259094], 'magnitude': 1.341806411743164, 'cosine_with_motion': 0.8967136740684509, 'motion_component': 1.2032161951065063, 'motion_component_percent': 89.67136740684509}, {'resid': 754, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 11.575718879699707, 'force': [0.004107880871742964, 0.9055112600326538, -1.121909499168396], 'magnitude': 1.4417519569396973, 'cosine_with_motion': -0.9189395308494568, 'motion_component': -1.3248828649520874, 'motion_component_percent': 91.89395308494568}, {'resid': 1082, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 11.754955291748047, 'force': [0.41961655020713806, -0.9536443948745728, -0.6733017563819885], 'magnitude': 1.2405043840408325, 'cosine_with_motion': -0.28157851099967957, 'motion_component': -0.3492993712425232, 'motion_component_percent': 28.157851099967957}, {'resid': 1082, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 12.182430267333984, 'force': [-0.20484022796154022, 0.5354126691818237, 0.3205406963825226], 'magnitude': 0.6567896008491516, 'cosine_with_motion': 0.20797109603881836, 'motion_component': 0.13659325242042542, 'motion_component_percent': 20.797109603881836}, {'resid': 1082, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 12.527904510498047, 'force': [-0.026916079223155975, 0.05991619452834129, 0.05232667550444603], 'magnitude': 0.08397920429706573, 'cosine_with_motion': 0.36718085408210754, 'motion_component': 0.030835555866360664, 'motion_component_percent': 36.718085408210754}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 12.712896347045898, 'force': [-0.08867650479078293, 0.1513332724571228, 0.14408425986766815], 'magnitude': 0.2269924134016037, 'cosine_with_motion': 0.41702425479888916, 'motion_component': 0.09466134011745453, 'motion_component_percent': 41.702425479888916}, {'resid': 1082, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 13.952410697937012, 'force': [-0.027796639129519463, 0.07117858529090881, 0.057290706783533096], 'magnitude': 0.09550533443689346, 'cosine_with_motion': 0.3256344497203827, 'motion_component': 0.031099826097488403, 'motion_component_percent': 32.56344497203827}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 13.927240371704102, 'force': [0.006952587049454451, -0.02336389198899269, -0.016810866072773933], 'magnitude': 0.02961106412112713, 'cosine_with_motion': -0.2634461224079132, 'motion_component': -0.0078009204007685184, 'motion_component_percent': 26.34461224079132}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 14.621319770812988, 'force': [0.007113732397556305, -0.019242972135543823, -0.017346801236271858], 'magnitude': 0.026866497471928596, 'cosine_with_motion': -0.3684841990470886, 'motion_component': -0.009899879805743694, 'motion_component_percent': 36.84841990470886}, {'resid': 1082, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 14.895257949829102, 'force': [-0.007434107828885317, 0.01526541169732809, 0.011218524537980556], 'magnitude': 0.020350774750113487, 'cosine_with_motion': 0.30450156331062317, 'motion_component': 0.0061968425288796425, 'motion_component_percent': 30.450156331062317}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HG2', 'charge': -0.042500000447034836, 'distance': 14.590117454528809, 'force': [0.024592861533164978, -0.05222650244832039, -0.03257555887103081], 'magnitude': 0.06628411263227463, 'cosine_with_motion': -0.23973813652992249, 'motion_component': -0.015890829265117645, 'motion_component_percent': 23.97381365299225}, {'resid': 1082, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 14.872492790222168, 'force': [-0.5387159585952759, 0.8356070518493652, 0.6876991987228394], 'magnitude': 1.2088773250579834, 'cosine_with_motion': 0.36733123660087585, 'motion_component': 0.4440584182739258, 'motion_component_percent': 36.733123660087585}, {'resid': 1082, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 12.101154327392578, 'force': [-0.28299471735954285, 0.8217833638191223, 0.8512433171272278], 'magnitude': 1.216564416885376, 'cosine_with_motion': 0.42117786407470703, 'motion_component': 0.5123900175094604, 'motion_component_percent': 42.1177864074707}, {'resid': 1082, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 12.568724632263184, 'force': [0.2898544669151306, -0.7436888813972473, -0.9265450835227966], 'magnitude': 1.2229368686676025, 'cosine_with_motion': -0.4988047182559967, 'motion_component': -0.6100066900253296, 'motion_component_percent': 49.88047182559967}], 'asn_contributions': [], 'sf_contributions': [{'resid': 100, 'resname': 'THR', 'atom': 'N', 'charge': -0.4157000184059143, 'distance': 7.820949554443359, 'force': [-1.2037780284881592, -0.256264865398407, -1.8910820484161377], 'magnitude': 2.256312131881714, 'cosine_with_motion': -0.5200616717338562, 'motion_component': -1.1734215021133423, 'motion_component_percent': 52.00616717338562}, {'resid': 100, 'resname': 'THR', 'atom': 'H', 'charge': 0.2718999981880188, 'distance': 7.973606109619141, 'force': [0.8916993141174316, 0.21528609097003937, 1.083722472190857], 'magnitude': 1.4198346138000488, 'cosine_with_motion': 0.4110587239265442, 'motion_component': 0.5836353898048401, 'motion_component_percent': 41.10587239265442}, {'resid': 100, 'resname': 'THR', 'atom': 'CA', 'charge': -0.03889999911189079, 'distance': 6.690989017486572, 'force': [-0.12442974001169205, -0.05742783099412918, -0.2538437843322754], 'magnitude': 0.2884742319583893, 'cosine_with_motion': -0.555251955986023, 'motion_component': -0.1601758897304535, 'motion_component_percent': 55.525195598602295}, {'resid': 100, 'resname': 'THR', 'atom': 'HA', 'charge': 0.1007000058889389, 'distance': 6.763186454772949, 'force': [0.3409338891506195, 0.2507391571998596, 0.5959242582321167], 'magnitude': 0.7309116125106812, 'cosine_with_motion': 0.4328528046607971, 'motion_component': 0.3163771331310272, 'motion_component_percent': 43.28528046607971}, {'resid': 100, 'resname': 'THR', 'atom': 'CB', 'charge': 0.3653999865055084, 'distance': 7.15402364730835, 'force': [0.5500074028968811, 0.4888582229614258, 2.253197193145752], 'magnitude': 2.370313882827759, 'cosine_with_motion': 0.6756783723831177, 'motion_component': 1.6015697717666626, 'motion_component_percent': 67.56783723831177}, {'resid': 100, 'resname': 'THR', 'atom': 'HB', 'charge': 0.00430000014603138, 'distance': 6.687530994415283, 'force': [0.004259211011230946, 0.009851723909378052, 0.030062364414334297], 'magnitude': 0.031920887529850006, 'cosine_with_motion': 0.6592339277267456, 'motion_component': 0.021043332293629646, 'motion_component_percent': 65.92339277267456}, {'resid': 100, 'resname': 'THR', 'atom': 'CG2', 'charge': -0.24380001425743103, 'distance': 8.670187950134277, 'force': [-0.2400764524936676, -0.27756354212760925, -1.0122805833816528], 'magnitude': 1.0767498016357422, 'cosine_with_motion': -0.6495926976203918, 'motion_component': -0.699448823928833, 'motion_component_percent': 64.95926976203918}, {'resid': 100, 'resname': 'THR', 'atom': 'HG21', 'charge': 0.0642000064253807, 'distance': 9.070099830627441, 'force': [0.028791505843400955, 0.06445559114217758, 0.24928627908229828], 'magnitude': 0.25908902287483215, 'cosine_with_motion': 0.7068657279014587, 'motion_component': 0.18314115703105927, 'motion_component_percent': 70.68657279014587}, {'resid': 100, 'resname': 'THR', 'atom': 'HG22', 'charge': 0.0642000064253807, 'distance': 8.903556823730469, 'force': [0.06965973973274231, 0.09790084511041641, 0.24053123593330383], 'magnitude': 0.26887232065200806, 'cosine_with_motion': 0.5579549670219421, 'motion_component': 0.15001864731311798, 'motion_component_percent': 55.795496702194214}, {'resid': 100, 'resname': 'THR', 'atom': 'HG23', 'charge': 0.0642000064253807, 'distance': 9.173186302185059, 'force': [0.07741741091012955, 0.04760519042611122, 0.2364327609539032], 'magnitude': 0.2532985508441925, 'cosine_with_motion': 0.6449697017669678, 'motion_component': 0.16336989402770996, 'motion_component_percent': 64.49697017669678}, {'resid': 100, 'resname': 'THR', 'atom': 'OG1', 'charge': -0.6761000156402588, 'distance': 7.207488059997559, 'force': [-0.6522688269615173, -0.16313524544239044, -4.268337726593018], 'magnitude': 4.320969104766846, 'cosine_with_motion': -0.7978975772857666, 'motion_component': -3.447690725326538, 'motion_component_percent': 79.78975772857666}, {'resid': 100, 'resname': 'THR', 'atom': 'HG1', 'charge': 0.41019999980926514, 'distance': 7.929015636444092, 'force': [0.4567595422267914, -0.042990297079086304, 2.1170432567596436], 'magnitude': 2.1661832332611084, 'cosine_with_motion': 0.7923278212547302, 'motion_component': 1.71632719039917, 'motion_component_percent': 79.23278212547302}, {'resid': 100, 'resname': 'THR', 'atom': 'C', 'charge': 0.5973000526428223, 'distance': 5.372811794281006, 'force': [3.2526018619537354, 0.5898107290267944, 6.021894931793213], 'magnitude': 6.869534969329834, 'cosine_with_motion': 0.5827745199203491, 'motion_component': 4.003389835357666, 'motion_component_percent': 58.27745199203491}, {'resid': 100, 'resname': 'THR', 'atom': 'O', 'charge': -0.5679000020027161, 'distance': 4.354108810424805, 'force': [-3.645887851715088, -1.648386001586914, -9.104743003845215], 'magnitude': 9.945150375366211, 'cosine_with_motion': -0.6190225481987, 'motion_component': -6.1562724113464355, 'motion_component_percent': 61.902254819869995}, {'resid': 101, 'resname': 'ILE', 'atom': 'N', 'charge': -0.4157000184059143, 'distance': 5.576398849487305, 'force': [-2.652541160583496, 0.46372851729393005, -3.528020143508911], 'magnitude': 4.438236713409424, 'cosine_with_motion': -0.5463649034500122, 'motion_component': -2.424896717071533, 'motion_component_percent': 54.63649034500122}, {'resid': 101, 'resname': 'ILE', 'atom': 'H', 'charge': 0.2718999981880188, 'distance': 6.568813800811768, 'force': [1.301344633102417, -0.2056732326745987, 1.6250847578048706], 'magnitude': 2.0920562744140625, 'cosine_with_motion': 0.5206736922264099, 'motion_component': 1.0892786979675293, 'motion_component_percent': 52.06736922264099}, {'resid': 101, 'resname': 'ILE', 'atom': 'CA', 'charge': -0.059700001031160355, 'distance': 4.9365434646606445, 'force': [-0.5521948337554932, 0.24094648659229279, -0.5463793277740479], 'magnitude': 0.8133293986320496, 'cosine_with_motion': -0.4877478778362274, 'motion_component': -0.3966996967792511, 'motion_component_percent': 48.77478778362274}, {'resid': 101, 'resname': 'ILE', 'atom': 'HA', 'charge': 0.0869000032544136, 'distance': 4.675082206726074, 'force': [0.6819103956222534, -0.5644811391830444, 0.9791848659515381], 'magnitude': 1.320016622543335, 'cosine_with_motion': 0.6494044065475464, 'motion_component': 0.8572245836257935, 'motion_component_percent': 64.94044065475464}, {'resid': 101, 'resname': 'ILE', 'atom': 'CB', 'charge': 0.13030001521110535, 'distance': 6.186561107635498, 'force': [0.8347606658935547, -0.44436824321746826, 0.6190574169158936], 'magnitude': 1.1302745342254639, 'cosine_with_motion': 0.3985850512981415, 'motion_component': 0.45051053166389465, 'motion_component_percent': 39.85850512981415}, {'resid': 101, 'resname': 'ILE', 'atom': 'HB', 'charge': 0.018699999898672104, 'distance': 6.786393642425537, 'force': [0.10788610577583313, -0.03605930507183075, 0.07233487069606781], 'magnitude': 0.1348036229610443, 'cosine_with_motion': 0.321517676115036, 'motion_component': 0.0433417484164238, 'motion_component_percent': 32.1517676115036}, {'resid': 101, 'resname': 'ILE', 'atom': 'CG2', 'charge': -0.3203999996185303, 'distance': 6.139284610748291, 'force': [-2.250354766845703, 1.412636399269104, -0.9515464305877686], 'magnitude': 2.82224702835083, 'cosine_with_motion': -0.2384876012802124, 'motion_component': -0.6730709075927734, 'motion_component_percent': 23.84876012802124}, {'resid': 101, 'resname': 'ILE', 'atom': 'HG21', 'charge': 0.08820000290870667, 'distance': 5.865858554840088, 'force': [0.7568936944007874, -0.33534035086631775, 0.19724667072296143], 'magnitude': 0.8510273098945618, 'cosine_with_motion': 0.07741325348615646, 'motion_component': 0.06588079035282135, 'motion_component_percent': 7.741325348615646}, {'resid': 101, 'resname': 'ILE', 'atom': 'HG22', 'charge': 0.08820000290870667, 'distance': 5.539966106414795, 'force': [0.6854344010353088, -0.6001872420310974, 0.28329458832740784], 'magnitude': 0.9540968537330627, 'cosine_with_motion': 0.2773210108280182, 'motion_component': 0.2645910978317261, 'motion_component_percent': 27.73210108280182}, {'resid': 101, 'resname': 'ILE', 'atom': 'HG23', 'charge': 0.08820000290870667, 'distance': 7.160867691040039, 'force': [0.4553391933441162, -0.30280566215515137, 0.16454458236694336], 'magnitude': 0.5710516571998596, 'cosine_with_motion': 0.2072705626487732, 'motion_component': 0.118362195789814, 'motion_component_percent': 20.72705626487732}, {'resid': 101, 'resname': 'ILE', 'atom': 'CG1', 'charge': -0.0430000014603138, 'distance': 7.120519638061523, 'force': [-0.16999652981758118, 0.13743750751018524, -0.17746157944202423], 'magnitude': 0.28156793117523193, 'cosine_with_motion': -0.5486266016960144, 'motion_component': -0.15447565913200378, 'motion_component_percent': 54.86266016960144}, {'resid': 101, 'resname': 'ILE', 'atom': 'HG12', 'charge': 0.023600000888109207, 'distance': 6.7671990394592285, 'force': [0.08585306257009506, -0.10198681056499481, 0.10724156349897385], 'magnitude': 0.17109298706054688, 'cosine_with_motion': 0.6186790466308594, 'motion_component': 0.10585164278745651, 'motion_component_percent': 61.86790466308594}, {'resid': 101, 'resname': 'ILE', 'atom': 'HG13', 'charge': 0.023600000888109207, 'distance': 7.405676364898682, 'force': [0.07932671159505844, -0.05660579726099968, 0.10446518659591675], 'magnitude': 0.14286328852176666, 'cosine_with_motion': 0.6161642670631409, 'motion_component': 0.08802725374698639, 'motion_component_percent': 61.61642670631409}, {'resid': 101, 'resname': 'ILE', 'atom': 'CD1', 'charge': -0.06599999964237213, 'distance': 8.505878448486328, 'force': [-0.1966281682252884, 0.15703420341014862, -0.16853055357933044], 'magnitude': 0.3028612434864044, 'cosine_with_motion': -0.48201847076416016, 'motion_component': -0.1459847092628479, 'motion_component_percent': 48.201847076416016}, {'resid': 101, 'resname': 'ILE', 'atom': 'HD11', 'charge': 0.01860000006854534, 'distance': 9.071434020996094, 'force': [0.04240606352686882, -0.042479049414396286, 0.045037999749183655], 'magnitude': 0.07504109293222427, 'cosine_with_motion': 0.564379096031189, 'motion_component': 0.042351625859737396, 'motion_component_percent': 56.4379096031189}, {'resid': 101, 'resname': 'ILE', 'atom': 'HD12', 'charge': 0.01860000006854534, 'distance': 9.135123252868652, 'force': [0.05194074288010597, -0.03203073516488075, 0.0418563112616539], 'magnitude': 0.07399837672710419, 'cosine_with_motion': 0.4407818913459778, 'motion_component': 0.03261714428663254, 'motion_component_percent': 44.07818913459778}, {'resid': 101, 'resname': 'ILE', 'atom': 'HD13', 'charge': 0.01860000006854534, 'distance': 8.557930946350098, 'force': [0.057194098830223083, -0.049020372331142426, 0.037883248180150986], 'magnitude': 0.0843166783452034, 'cosine_with_motion': 0.4039534032344818, 'motion_component': 0.03406000882387161, 'motion_component_percent': 40.39534032344818}, {'resid': 101, 'resname': 'ILE', 'atom': 'C', 'charge': 0.5973000526428223, 'distance': 3.7527668476104736, 'force': [11.681468963623047, -2.6854379177093506, 7.389233589172363], 'magnitude': 14.080804824829102, 'cosine_with_motion': 0.2726730704307556, 'motion_component': 3.83945631980896, 'motion_component_percent': 27.26730704307556}, {'resid': 101, 'resname': 'ILE', 'atom': 'O', 'charge': -0.5679000020027161, 'distance': 2.7742443084716797, 'force': [-19.51871109008789, 9.42858600616455, -11.412528991699219], 'magnitude': 24.4974308013916, 'cosine_with_motion': -0.306192010641098, 'motion_component': -7.500917434692383, 'motion_component_percent': 30.619201064109802}, {'resid': 102, 'resname': 'GLY', 'atom': 'N', 'charge': -0.4157000184059143, 'distance': 4.283140182495117, 'force': [-6.92142391204834, -0.6764242649078369, -2.869236707687378], 'magnitude': 7.523043155670166, 'cosine_with_motion': -0.01215851679444313, 'motion_component': -0.09146904945373535, 'motion_component_percent': 1.215851679444313}, {'resid': 102, 'resname': 'GLY', 'atom': 'H', 'charge': 0.2718999981880188, 'distance': 5.210223197937012, 'force': [2.9379777908325195, 0.3638745844364166, 1.5144950151443481], 'magnitude': 3.325329065322876, 'cosine_with_motion': 0.08038098365068436, 'motion_component': 0.26729321479797363, 'motion_component_percent': 8.038098365068436}, {'resid': 102, 'resname': 'GLY', 'atom': 'CA', 'charge': -0.025200000032782555, 'distance': 3.887051582336426, 'force': [-0.5182666182518005, -0.18146352469921112, -0.07132749259471893], 'magnitude': 0.5537300109863281, 'cosine_with_motion': 0.3038005828857422, 'motion_component':</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>1199</v>
+      </c>
+      <c r="B15" t="n">
+        <v>1219</v>
+      </c>
+      <c r="C15" t="n">
+        <v>2515</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>{1192: {'frame': 1192, 'motion_vector': [0.06830596923828125, 0.3096580505371094, 0.7273101806640625], 'motion_vector_magnitude': 0.7934316992759705, 'ionic_force': [-9.001857563853264, 1.1696378886699677, 8.737475156784058], 'ionic_force_magnitude': 12.599403339282903, 'radial_force': 9.077526777185213, 'axial_force': 8.737475156784058, 'glu_force': [1.4068490621866658, 0.43748429929837584, -6.2748513472033665], 'glu_force_magnitude': 6.445492706179102, 'asn_force': [0.38773764204233885, 0.3511815653182566, 0.1291203498840332], 'asn_force_magnitude': 0.5388330313094298, 'sf_force': [-8.828848069504602, -4.08640664255654, 17.43584824638674], 'sf_force_magnitude': 19.966373770761503, 'residue_force': [-7.034261365275597, -3.2977407779399073, 11.290117249067407], 'residue_force_magnitude': 13.704841286610582, 'pip2_force': [0.6345773222346907, 0.015990155283361673, -4.095811611972749], 'pip2_force_magnitude': 4.144709498110977, 'total_force': [-15.40154160689417, -2.112112733986578, 15.931780793878715], 'total_force_magnitude': 22.259607888149404, 'cosine_total_motion': 0.5594829694916092, 'cosine_glu_motion': -0.8471152196624777, 'cosine_asn_motion': 0.5359694908520551, 'cosine_sf_motion': 0.6825432224905922, 'cosine_residue_motion': 0.6170546607516405, 'cosine_pip2_motion': -0.8911629843221197, 'cosine_ionic_motion': 0.6104135893262582, 'motion_component_total': 12.453871520980677, 'motion_component_glu': -5.460074969627808, 'motion_component_asn': 0.2887980654451846, 'motion_component_sf': 13.627913094947193, 'motion_component_residue': 8.45663619076457, 'motion_component_ionic': 7.69084701570092, 'motion_component_pip2': -3.6936116854848136, 'motion_component_percent_total': 55.94829694916093, 'motion_component_percent_glu': 84.71152196624777, 'motion_component_percent_asn': 53.596949085205516, 'motion_component_percent_sf': 68.25432224905921, 'motion_component_percent_residue': 61.705466075164054, 'motion_component_percent_ionic': 61.04135893262582, 'motion_component_percent_pip2': 89.11629843221198, 'ionic_contributions': [{'ion_id': 2230, 'distance': 4.5025715827941895, 'force': [-10.962936401367188, 0.6812362670898438, 12.146373748779297], 'magnitude': 16.376338958740234, 'cosine_ionic_motion': 0.638495683670044, 'motion_component_ionic': 10.456221580505371, 'motion_component_percent_ionic': 63.849568367004395}, {'ion_id': 2280, 'distance': 6.140703201293945, 'force': [0.5102397203445435, 0.8216593861579895, -8.751155853271484], 'magnitude': 8.804441452026367, 'cosine_ionic_motion': -0.8697051405906677, 'motion_component_ionic': -7.657268047332764, 'motion_component_percent_ionic': 86.97051405906677}, {'ion_id': 2333, 'distance': 9.456350326538086, 'force': [0.7882878184318542, -2.834900140762329, 2.2641022205352783], 'magnitude': 3.71271014213562, 'cosine_ionic_motion': 0.2792806327342987, 'motion_component_ionic': 1.0368880033493042, 'motion_component_percent_ionic': 27.92806327342987}, {'ion_id': 2334, 'distance': 8.861929893493652, 'force': [-1.48007333278656, 2.9500322341918945, 2.641641855239868], 'magnitude': 4.227478981018066, 'cosine_ionic_motion': 0.8150030970573425, 'motion_component_ionic': 3.445408582687378, 'motion_component_percent_ionic': 81.50030970573425}, {'ion_id': 2350, 'distance': 10.950079917907715, 'force': [0.1739748865365982, 0.13303831219673157, -2.7602007389068604], 'magnitude': 2.768876075744629, 'cosine_ionic_motion': -0.8896307349205017, 'motion_component_ionic': -2.4632773399353027, 'motion_component_percent_ionic': 88.96307349205017}, {'ion_id': 2372, 'distance': 9.348301887512207, 'force': [1.9686497449874878, -0.5814281702041626, 3.196713924407959], 'magnitude': 3.7990288734436035, 'cosine_ionic_motion': 0.7562126517295837, 'motion_component_ionic': 2.8728737831115723, 'motion_component_percent_ionic': 75.62126517295837}], 'glu_contributions': [{'resid': 98, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 9.30593204498291, 'force': [-1.8800134658813477, -0.5865165591239929, -0.19833369553089142], 'magnitude': 1.9793404340744019, 'cosine_with_motion': -0.2892671823501587, 'motion_component': -0.5725582242012024, 'motion_component_percent': 28.92671823501587}, {'resid': 98, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 9.529297828674316, 'force': [1.047460913658142, 0.23074355721473694, 0.04274715855717659], 'magnitude': 1.0734264850616455, 'cosine_with_motion': 0.2044050693511963, 'motion_component': 0.21941381692886353, 'motion_component_percent': 20.44050693511963}, {'resid': 98, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 9.545154571533203, 'force': [0.1350836455821991, 0.03729020804166794, 0.035912882536649704], 'magnitude': 0.1446647346019745, 'cosine_with_motion': 0.4085501730442047, 'motion_component': 0.059102803468704224, 'motion_component_percent': 40.85501730442047}, {'resid': 98, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 9.724564552307129, 'force': [0.3451806306838989, 0.13587792217731476, 0.11349811404943466], 'magnitude': 0.38793596625328064, 'cosine_with_motion': 0.4814866781234741, 'motion_component': 0.1867859959602356, 'motion_component_percent': 48.14866781234741}, {'resid': 98, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 10.946259498596191, 'force': [0.14725756645202637, 0.0287980604916811, 0.0395241342484951], 'magnitude': 0.15516531467437744, 'cosine_with_motion': 0.3876308500766754, 'motion_component': 0.060146864503622055, 'motion_component_percent': 38.76308500766754}, {'resid': 98, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 11.623629570007324, 'force': [-0.04030655696988106, -0.010321050882339478, -0.008719928562641144], 'magnitude': 0.04251093789935112, 'cosine_with_motion': -0.3644067943096161, 'motion_component': -0.015491274185478687, 'motion_component_percent': 36.44067943096161}, {'resid': 98, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 11.04062271118164, 'force': [-0.04573037475347519, -0.004481717944145203, -0.010433453135192394], 'magnitude': 0.047119103372097015, 'cosine_with_motion': -0.3236474096775055, 'motion_component': -0.015249975956976414, 'motion_component_percent': 32.36474096775055}, {'resid': 98, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 11.527336120605469, 'force': [0.030888570472598076, 0.006229001563042402, 0.012716654688119888], 'magnitude': 0.033979661762714386, 'cosine_with_motion': 0.49285680055618286, 'motion_component': 0.016747107729315758, 'motion_component_percent': 49.285680055618286}, {'resid': 98, 'resname': 'GLU', 'atom': 'HG2', 'charge': -0.042500000447034836, 'distance': 11.434142112731934, 'force': [-0.09442152082920074, -0.02872082218527794, -0.0436735525727272], 'magnitude': 0.1079244539141655, 'cosine_with_motion': -0.5501229763031006, 'motion_component': -0.05937172472476959, 'motion_component_percent': 55.01229763031006}, {'resid': 98, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 12.57211971282959, 'force': [-0.08204638212919235, -0.01490713655948639, -0.03186638653278351], 'magnitude': 0.0892709270119667, 'cosine_with_motion': -0.4715083837509155, 'motion_component': -0.04209199175238609, 'motion_component_percent': 47.15083837509155}, {'resid': 98, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 11.06985092163086, 'force': [1.9387092590332031, 0.166052907705307, 0.9875257015228271], 'magnitude': 2.1820573806762695, 'cosine_with_motion': 0.5210393667221069, 'motion_component': 1.1369378566741943, 'motion_component_percent': 52.10393667221069}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 11.293594360351562, 'force': [-1.9376713037490845, 0.05538715049624443, -0.8859726786613464], 'magnitude': 2.131334066390991, 'cosine_with_motion': -0.4491719901561737, 'motion_component': -0.9573355913162231, 'motion_component_percent': 44.91719901561737}, {'resid': 98, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 10.858089447021484, 'force': [-1.9157603979110718, -0.21605199575424194, -1.2647488117218018], 'magnitude': 2.3057332038879395, 'cosine_with_motion': -0.6109102964401245, 'motion_component': -1.408596158027649, 'motion_component_percent': 61.09102964401245}, {'resid': 98, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 8.4381103515625, 'force': [2.321110725402832, 0.42634621262550354, 0.8312619924545288], 'magnitude': 2.502063751220703, 'cosine_with_motion': 0.450909286737442, 'motion_component': 1.1282037496566772, 'motion_component_percent': 45.0909286737442}, {'resid': 98, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 8.027008056640625, 'force': [-2.6003973484039307, -0.6437756419181824, -1.3466447591781616], 'magnitude': 2.9983270168304443, 'cosine_with_motion': -0.5701638460159302, 'motion_component': -1.7095377445220947, 'motion_component_percent': 57.01638460159302}, {'resid': 426, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 9.952709197998047, 'force': [1.6504729986190796, 0.4279140830039978, 0.2954069674015045], 'magnitude': 1.730444073677063, 'cosine_with_motion': 0.335105836391449, 'motion_component': 0.5798819065093994, 'motion_component_percent': 33.5105836391449}, {'resid': 426, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 10.720279693603516, 'force': [-0.811874270439148, -0.16808368265628815, -0.178877055644989], 'magnitude': 0.8481680154800415, 'cosine_with_motion': -0.35307037830352783, 'motion_component': -0.2994630038738251, 'motion_component_percent': 35.30703783035278}, {'resid': 426, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 9.827038764953613, 'force': [-0.13290564715862274, -0.030779877677559853, -0.004086641129106283], 'magnitude': 0.13648447394371033, 'cosine_with_motion': -0.19929374754428864, 'motion_component': -0.027200503274798393, 'motion_component_percent': 19.929374754428864}, {'resid': 426, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 9.902549743652344, 'force': [-0.353653222322464, -0.12201997637748718, 0.0018225208623334765], 'magnitude': 0.3741160035133362, 'cosine_with_motion': -0.20420588552951813, 'motion_component': -0.07639668881893158, 'motion_component_percent': 20.420588552951813}, {'resid': 426, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 11.058089256286621, 'force': [-0.14999614655971527, -0.02466600202023983, 0.0031253937631845474], 'magnitude': 0.15204283595085144, 'cosine_with_motion': -0.12940232455730438, 'motion_component': -0.019674696028232574, 'motion_component_percent': 12.940232455730438}, {'resid': 426, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 11.964774131774902, 'force': [0.03930804505944252, 0.00801249872893095, 0.0006305065471678972], 'magnitude': 0.04012131690979004, 'cosine_with_motion': 0.17669054865837097, 'motion_component': 0.007089057471603155, 'motion_component_percent': 17.669054865837097}, {'resid': 426, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 11.2313871383667, 'force': [0.04541143402457237, 0.003269999288022518, 0.0005274112336337566], 'magnitude': 0.045532066375017166, 'cosine_with_motion': 0.12450788915157318, 'motion_component': 0.005669101607054472, 'motion_component_percent': 12.450788915157318}, {'resid': 426, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 11.313941955566406, 'force': [-0.03429904580116272, -0.006118502467870712, 0.005510194227099419], 'magnitude': 0.03527354449033737, 'cosine_with_motion': -0.008212808519601822, 'motion_component': -0.0002896948717534542, 'motion_component_percent': 0.8212808519601822}, {'resid': 426, 'resname': 'GLU', 'atom': 'HG2', 'charge': -0.042500000447034836, 'distance': 11.196883201599121, 'force': [0.10664205253124237, 0.02958657220005989, -0.02046618051826954], 'magnitude': 0.11254668980836868, 'cosine_with_motion': 0.01747795008122921, 'motion_component': 0.001967085525393486, 'motion_component_percent': 1.747795008122921}, {'resid': 426, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 12.391651153564453, 'force': [0.0895036980509758, 0.014728764072060585, -0.014694847166538239], 'magnitude': 0.09189008176326752, 'cosine_with_motion': -0.00018096872372552752, 'motion_component': -1.6629230231046677e-05, 'motion_component_percent': 0.018096872372552752}, {'resid': 426, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 10.904159545898438, 'force': [-2.179901361465454, -0.16413989663124084, 0.5277570486068726], 'magnitude': 2.248875141143799, 'cosine_with_motion': 0.1031847596168518, 'motion_component': 0.23204964399337769, 'motion_component_percent': 10.31847596168518}, {'resid': 426, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 11.222975730895996, 'force': [2.114912271499634, -0.057231560349464417, -0.4264666736125946], 'magnitude': 2.158240795135498, 'cosine_with_motion': -0.1071203276515007, 'motion_component': -0.2311914563179016, 'motion_component_percent': 10.71203276515007}, {'resid': 426, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 10.573806762695312, 'force': [2.278928518295288, 0.22599922120571136, -0.8167170882225037], 'magnitude': 2.431381940841675, 'cosine_with_motion': -0.19094550609588623, 'motion_component': -0.4642614722251892, 'motion_component_percent': 19.094550609588623}, {'resid': 426, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 8.536748886108398, 'force': [-2.418163776397705, -0.3542819619178772, 0.054065950214862823], 'magnitude': 2.4445767402648926, 'cosine_with_motion': -0.12144669145345688, 'motion_component': -0.29688575863838196, 'motion_component_percent': 12.144669145345688}, {'resid': 426, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 8.000861167907715, 'force': [2.9285941123962402, 0.5769820213317871, -0.44552096724510193], 'magnitude': 3.017956256866455, 'cosine_with_motion': 0.02283344231545925, 'motion_component': 0.06891033053398132, 'motion_component_percent': 2.283344231545925}, {'resid': 754, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 9.297966003417969, 'force': [-0.5872825980186462, 1.8924018144607544, -0.07173582166433334], 'magnitude': 1.9827333688735962, 'cosine_with_motion': 0.3138315677642822, 'motion_component': 0.6222442984580994, 'motion_component_percent': 31.383156776428223}, {'resid': 754, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 10.035107612609863, 'force': [0.24401409924030304, -0.9365096092224121, -0.017934590578079224], 'magnitude': 0.967943549156189, 'cosine_with_motion': -0.3728843927383423, 'motion_component': -0.36093103885650635, 'motion_component_percent': 37.28843927383423}, {'resid': 754, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 9.251741409301758, 'force': [0.034829363226890564, -0.1473216861486435, 0.028195222839713097], 'magnitude': 0.1539861410856247, 'cosine_with_motion': -0.18607045710086823, 'motion_component': -0.028652271255850792, 'motion_component_percent': 18.607045710086823}, {'resid': 754, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 9.496588706970215, 'force': [0.12196919322013855, -0.3733828663825989, 0.10574924200773239], 'magnitude': 0.40678513050079346, 'cosine_with_motion': -0.09411836415529251, 'motion_component': -0.03828595206141472, 'motion_component_percent': 9.411836415529251}, {'resid': 754, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 10.440937995910645, 'force': [0.022625962272286415, -0.16610610485076904, 0.031360965222120285], 'magnitude': 0.1705481857061386, 'cosine_with_motion': -0.20013147592544556, 'motion_component': -0.034132059663534164, 'motion_component_percent': 20.013147592544556}, {'resid': 754, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 11.35075569152832, 'force': [-0.008280569687485695, 0.04314054548740387, -0.007592879701405764], 'magnitude': 0.044579438865184784, 'cosine_with_motion': 0.20556046068668365, 'motion_component': 0.009163769893348217, 'motion_component_percent': 20.556046068668365}, {'resid': 754, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 10.428926467895508, 'force': [-0.0035444567911326885, 0.05239896848797798, -0.005526064895093441], 'magnitude': 0.05280864238739014, 'cosine_with_motion': 0.2855483591556549, 'motion_component': 0.015079421922564507, 'motion_component_percent': 28.55483591556549}, {'resid': 754, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 10.862405776977539, 'force': [0.0017927699955180287, -0.03648218512535095, 0.011410657316446304], 'magnitude': 0.038267046213150024, 'cosine_with_motion': -0.09470491856336594, 'motion_component': -0.003624077420681715, 'motion_component_percent': 9.470491856336594}, {'resid': 754, 'resname': 'GLU', 'atom': 'HG2', 'charge': -0.042500000447034836, 'distance': 11.93215274810791, 'force': [-0.0029489565640687943, 0.09434272348880768, -0.03020389936864376], 'magnitude': 0.09910358488559723, 'cosine_with_motion': 0.08959398418664932, 'motion_component': 0.008879085071384907, 'motion_component_percent': 8.959398418664932}, {'resid': 754, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 10.301401138305664, 'force': [0.005514923017472029, 0.1267174929380417, -0.03989636152982712], 'magnitude': 0.1329641193151474, 'cosine_with_motion': 0.10046417266130447, 'motion_component': 0.013358130119740963, 'motion_component_percent': 10.046417266130447}, {'resid': 754, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 10.666695594787598, 'force': [0.237155944108963, -2.1211535930633545, 0.9836291670799255], 'magnitude': 2.3501195907592773, 'cosine_with_motion': 0.040098682045936584, 'motion_component': 0.09423670172691345, 'motion_component_percent': 4.0098682045936584}, {'resid': 754, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 11.041523933410645, 'force': [-0.46476924419403076, 1.9567521810531616, -0.9627745747566223], 'magnitude': 2.2297589778900146, 'cosine_with_motion': -0.07125308364629745, 'motion_component': -0.1588772088289261, 'motion_component_percent': 7.1253083646297455}, {'resid': 754, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 10.246249198913574, 'force': [-0.07158733159303665, 2.244502067565918, -1.2890598773956299], 'magnitude': 2.589322090148926, 'cosine_with_motion': -0.12042545527219772, 'motion_component': -0.31182029843330383, 'motion_component_percent': 12.042545527219772}, {'resid': 754, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 7.996084690093994, 'force': [0.3817600607872009, -2.693377733230591, 0.6030440330505371], 'magnitude': 2.786339282989502, 'cosine_with_motion': -0.16706828773021698, 'motion_component': -0.46550893783569336, 'motion_component_percent': 16.706828773021698}, {'resid': 754, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 7.55982780456543, 'force': [-0.4796859920024872, 3.118093490600586, -1.2141706943511963], 'magnitude': 3.380357503890991, 'cosine_with_motion': 0.018529847264289856, 'motion_component': 0.06263750791549683, 'motion_component_percent': 1.8529847264289856}, {'resid': 1082, 'resname': 'GLU', 'atom': 'N', 'charge': -0.5163000226020813, 'distance': 9.281804084777832, 'force': [0.7117884755134583, -1.8572328090667725, -0.05222923308610916], 'magnitude': 1.9896442890167236, 'cosine_with_motion': -0.3575685918331146, 'motion_component': -0.7114343047142029, 'motion_component_percent': 35.75685918331146}, {'resid': 1082, 'resname': 'GLU', 'atom': 'H', 'charge': 0.2935999929904938, 'distance': 9.824446678161621, 'force': [-0.2828369736671448, 0.9694440960884094, -0.008782923221588135], 'magnitude': 1.0098989009857178, 'cosine_with_motion': 0.34256044030189514, 'motion_component': 0.3459514081478119, 'motion_component_percent': 34.256044030189514}, {'resid': 1082, 'resname': 'GLU', 'atom': 'CA', 'charge': 0.03970000147819519, 'distance': 9.36844253540039, 'force': [-0.05690574273467064, 0.13640613853931427, 0.02659389190375805], 'magnitude': 0.15017367899417877, 'cosine_with_motion': 0.4842049777507782, 'motion_component': 0.07271484285593033, 'motion_component_percent': 48.42049777507782}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HA', 'charge': 0.11050000041723251, 'distance': 9.475604057312012, 'force': [-0.19655084609985352, 0.3498712182044983, 0.07682936638593674], 'magnitude': 0.40858885645866394, 'cosine_with_motion': 0.4651434123516083, 'motion_component': 0.19005241990089417, 'motion_component_percent': 46.51434123516083}, {'resid': 1082, 'resname': 'GLU', 'atom': 'CB', 'charge': 0.0560000017285347, 'distance': 10.7530517578125, 'force': [-0.05244738608598709, 0.1479753702878952, 0.03473348543047905], 'magnitude': 0.1607913374900818, 'cosine_with_motion': 0.5291027426719666, 'motion_component': 0.08507513999938965, 'motion_component_percent': 52.910274267196655}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HB2', 'charge': -0.01730000041425228, 'distance': 11.376656532287598, 'force': [0.014023988507688046, -0.041654959321022034, -0.006122339051216841], 'magnitude': 0.04437669366598129, 'cosine_with_motion': -0.46559977531433105, 'motion_component': -0.02066177874803543, 'motion_component_percent': 46.559977531433105}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HB3', 'charge': -0.01730000041425228, 'distance': 10.570362091064453, 'force': [0.012201236560940742, -0.048098381608724594, -0.013421578332781792], 'magnitude': 0.05140489712357521, 'cosine_with_motion': -0.5840759873390198, 'motion_component': -0.030024366453289986, 'motion_component_percent': 58.40759873390198}, {'resid': 1082, 'resname': 'GLU', 'atom': 'CG', 'charge': 0.01360000018030405, 'distance': 11.596389770507812, 'force': [-0.013123448006808758, 0.029296617954969406, 0.009840917773544788], 'magnitude': 0.03357618674635887, 'cosine_with_motion': 0.5755512714385986, 'motion_component': 0.01932481676340103, 'motion_component_percent': 57.55512714385986}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HG2', 'charge': -0.042500000447034836, 'distance': 11.758992195129395, 'force': [0.04753455892205238, -0.0867975503206253, -0.024891680106520653], 'magnitude': 0.10204383730888367, 'cosine_with_motion': -0.5154663920402527, 'motion_component': -0.05260016769170761, 'motion_component_percent': 51.54663920402527}, {'resid': 1082, 'resname': 'GLU', 'atom': 'HG3', 'charge': -0.042500000447034836, 'distance': 12.577237129211426, 'force': [0.031622275710105896, -0.07894755154848099, -0.02690075896680355], 'magnitude': 0.0891982838511467, 'cosine_with_motion': -0.5913568735122681, 'motion_component': -0.052748020738363266, 'motion_component_percent': 59.13568735122681}, {'resid': 1082, 'resname': 'GLU', 'atom': 'CD', 'charge': 0.805400013923645, 'distance': 11.08047103881836, 'force': [-0.8382714986801147, 1.798356533050537, 0.8979766964912415], 'magnitude': 2.1778767108917236, 'cosine_with_motion': 0.667087197303772, 'motion_component': 1.452833652496338, 'motion_component_percent': 66.7087197303772}, {'resid': 1082, 'resname': 'GLU', 'atom': 'OE1', 'charge': -0.8187999725341797, 'distance': 11.009544372558594, 'force': [1.0557866096496582, -1.7048646211624146, -1.0042877197265625], 'magnitude': 2.2427310943603516, 'cosine_with_motion': -0.6666299104690552, 'motion_component': -1.4950716495513916, 'motion_component_percent': 66.66299104690552}, {'resid': 1082, 'resname': 'GLU', 'atom': 'OE2', 'charge': -0.8187999725341797, 'distance': 11.08823013305664, 'force': [0.6398348808288574, -1.8383842706680298, -1.0485880374908447], 'magnitude': 2.2110137939453125, 'cosine_with_motion': -0.7343232035636902, 'motion_component': -1.6235986948013306, 'motion_component_percent': 73.43232035636902}, {'resid': 1082, 'resname': 'GLU', 'atom': 'C', 'charge': 0.5365999937057495, 'distance': 8.249771118164062, 'force': [-0.773941159248352, 2.3973007202148438, 0.7112287878990173], 'magnitude': 2.617609977722168, 'cosine_with_motion': 0.5810418128967285, 'motion_component': 1.5209407806396484, 'motion_component_percent': 58.10418128967285}, {'resid': 1082, 'resname': 'GLU', 'atom': 'O', 'charge': -0.5819000005722046, 'distance': 7.769079685211182, 'force': [1.1342473030090332, -2.730323553085327, -1.2261346578598022], 'magnitude': 3.200716972351074, 'cosine_with_motion': -0.6535688638687134, 'motion_component': -2.091888904571533, 'motion_component_percent': 65.35688638687134}], 'asn_contributions': [{'resid': 130, 'resname': 'ASN', 'atom': 'N', 'charge': -0.38210001587867737, 'distance': 14.697056770324707, 'force': [-0.33479511737823486, -0.11388297379016876, -0.4688872992992401], 'magnitude': 0.5872924327850342, 'cosine_with_motion': -0.8566093444824219, 'motion_component': -0.5030801892280579, 'motion_component_percent': 85.66093444824219}, {'resid': 130, 'resname': 'ASN', 'atom': 'H', 'charge': 0.2681000232696533, 'distance': 14.261276245117188, 'force': [0.254459947347641, 0.10975749790668488, 0.3387228548526764], 'magnitude': 0.43764111399650574, 'cosine_with_motion': 0.8574082851409912, 'motion_component': 0.3752371072769165, 'motion_component_percent': 85.74082851409912}, {'resid': 130, 'resname': 'ASN', 'atom': 'CA', 'charge': -0.20800000429153442, 'distance': 14.11490535736084, 'force': [-0.1807497888803482, -0.043637391179800034, -0.2925170361995697], 'magnitude': 0.34661349654197693, 'cosine_with_motion': -0.8676266074180603, 'motion_component': -0.3007310926914215, 'motion_component_percent': 86.76266074180603}, {'resid': 130, 'resname': 'ASN', 'atom': 'HA', 'charge': 0.13580000400543213, 'distance': 14.363728523254395, 'force': [0.1223364993929863, 0.014101493172347546, 0.18052318692207336], 'magnitude': 0.2185261845588684, 'cosine_with_motion': 0.8306301236152649, 'motion_component': 0.1815144270658493, 'motion_component_percent': 83.06301236152649}, {'resid': 130, 'resname': 'ASN', 'atom': 'CB', 'charge': -0.22990000247955322, 'distance': 12.5274658203125, 'force': [-0.24792854487895966, -0.06613067537546158, -0.41315415501594543], 'magnitude': 0.4863519072532654, 'cosine_with_motion': -0.8756555914878845, 'motion_component': -0.42587676644325256, 'motion_component_percent': 87.56555914878845}, {'resid': 130, 'resname': 'ASN', 'atom': 'HB2', 'charge': 0.1023000031709671, 'distance': 12.274458885192871, 'force': [0.11270757764577866, 0.049611058086156845, 0.18882213532924652], 'magnitude': 0.22542861104011536, 'cosine_with_motion': 0.8967424631118774, 'motion_component': 0.20215140283107758, 'motion_component_percent': 89.67424631118774}, {'resid': 130, 'resname': 'ASN', 'atom': 'HB3', 'charge': 0.1023000031709671, 'distance': 12.1663179397583, 'force': [0.1050616055727005, 0.018702134490013123, 0.20312893390655518], 'magnitude': 0.22945386171340942, 'cosine_with_motion': 0.882724940776825, 'motion_component': 0.20254464447498322, 'motion_component_percent': 88.2724940776825}, {'resid': 130, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 11.815363883972168, 'force': [1.0143647193908691, 0.1467275470495224, 1.3576844930648804], 'magnitude': 1.7011090517044067, 'cosine_with_motion': 0.816602885723114, 'motion_component': 1.3891305923461914, 'motion_component_percent': 81.6602885723114}, {'resid': 130, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 11.330058097839355, 'force': [-0.9241240620613098, 0.016134286299347878, -1.2496927976608276], 'magnitude': 1.5543479919433594, 'cosine_with_motion': -0.7841284871101379, 'motion_component': -1.2188085317611694, 'motion_component_percent': 78.4128487110138}, {'resid': 130, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 11.90491771697998, 'force': [-1.4207782745361328, -0.29905760288238525, -1.555681824684143], 'magnitude': 2.1279549598693848, 'cosine_with_motion': -0.782472550868988, 'motion_component': -1.6650663614273071, 'motion_component_percent': 78.2472550868988}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD21', 'charge': 0.41499999165534973, 'distance': 11.448018074035645, 'force': [0.7560954093933105, 0.1090112179517746, 0.722261905670166], 'magnitude': 1.0512973070144653, 'cosine_with_motion': 0.7321503162384033, 'motion_component': 0.7697076797485352, 'motion_component_percent': 73.21503162384033}, {'resid': 130, 'resname': 'ASN', 'atom': 'HD22', 'charge': 0.41499999165534973, 'distance': 12.444681167602539, 'force': [0.588836133480072, 0.18638892471790314, 0.6403173208236694], 'magnitude': 0.8896488547325134, 'cosine_with_motion': 0.798507809638977, 'motion_component': 0.7103915810585022, 'motion_component_percent': 79.8507809638977}, {'resid': 130, 'resname': 'ASN', 'atom': 'C', 'charge': 0.8050000071525574, 'distance': 14.994108200073242, 'force': [0.5302886962890625, 0.14876145124435425, 1.0534725189208984], 'magnitude': 1.1887558698654175, 'cosine_with_motion': 0.8995879888534546, 'motion_component': 1.0693905353546143, 'motion_component_percent': 89.95879888534546}, {'resid': 458, 'resname': 'ASN', 'atom': 'N', 'charge': -0.38210001587867737, 'distance': 14.31051254272461, 'force': [0.43778181076049805, 0.046791624277830124, -0.4357445240020752], 'magnitude': 0.6194478869438171, 'cosine_with_motion': -0.5544958114624023, 'motion_component': -0.34348124265670776, 'motion_component_percent': 55.449581146240234}, {'resid': 458, 'resname': 'ASN', 'atom': 'H', 'charge': 0.2681000232696533, 'distance': 13.908805847167969, 'force': [-0.33554744720458984, -0.05917762592434883, 0.309193879365921], 'magnitude': 0.46010318398475647, 'cosine_with_motion': 0.5030266046524048, 'motion_component': 0.23144415020942688, 'motion_component_percent': 50.30266046524048}, {'resid': 458, 'resname': 'ASN', 'atom': 'CA', 'charge': -0.20800000429153442, 'distance': 13.539936065673828, 'force': [0.2564440965652466, -0.0021190745756030083, -0.2758929431438446], 'magnitude': 0.3766762316226959, 'cosine_with_motion': -0.6149871349334717, 'motion_component': -0.23165103793144226, 'motion_component_percent': 61.49871349334717}, {'resid': 458, 'resname': 'ASN', 'atom': 'HA', 'charge': 0.13580000400543213, 'distance': 13.890741348266602, 'force': [-0.16633442044258118, 0.015327856875956059, 0.16338780522346497], 'magnitude': 0.23366141319274902, 'cosine_with_motion': 0.6052955389022827, 'motion_component': 0.1414342075586319, 'motion_component_percent': 60.52955389022827}, {'resid': 458, 'resname': 'ASN', 'atom': 'CB', 'charge': -0.22990000247955322, 'distance': 12.058449745178223, 'force': [0.36390525102615356, 0.006227548699826002, -0.37825441360473633], 'magnitude': 0.524921178817749, 'cosine_with_motion': -0.5962292551994324, 'motion_component': -0.31297335028648376, 'motion_component_percent': 59.62292551994324}, {'resid': 458, 'resname': 'ASN', 'atom': 'HB2', 'charge': 0.1023000031709671, 'distance': 11.923460960388184, 'force': [-0.18003728985786438, -0.007557373493909836, 0.15684643387794495], 'magnitude': 0.23889608681201935, 'cosine_with_motion': 0.5246075987815857, 'motion_component': 0.1253267079591751, 'motion_component_percent': 52.46075987815857}, {'resid': 458, 'resname': 'ASN', 'atom': 'HB3', 'charge': 0.1023000031709671, 'distance': 11.682769775390625, 'force': [-0.16300424933433533, -0.020629342645406723, 0.1868848204612732], 'magnitude': 0.24884110689163208, 'cosine_with_motion': 0.5996858477592468, 'motion_component': 0.14922648668289185, 'motion_component_percent': 59.96858477592468}, {'resid': 458, 'resname': 'ASN', 'atom': 'CG', 'charge': 0.7153000235557556, 'distance': 11.204047203063965, 'force': [-1.2627500295639038, 0.1748153120279312, 1.3977946043014526], 'magnitude': 1.8918054103851318, 'cosine_with_motion': 0.6558945775032043, 'motion_component': 1.2408249378204346, 'motion_component_percent': 65.58945775032043}, {'resid': 458, 'resname': 'ASN', 'atom': 'OD1', 'charge': -0.6010000109672546, 'distance': 10.998223304748535, 'force': [0.9607732892036438, -0.17265233397483826, -1.3297165632247925], 'magnitude': 1.6495575904846191, 'cosine_with_motion': -0.7296338677406311, 'motion_component': -1.2035731077194214, 'motion_component_percent': 72.96338677406311}, {'resid': 458, 'resname': 'ASN', 'atom': 'ND2', 'charge': -0.9083999991416931, 'distance': 11.281820297241211, 'force': [1.686111569404602, -0.40592342615127563, -1.6145553588867188], 'magnit</t>
         </is>
       </c>
     </row>

</xml_diff>